<commit_message>
Update from Judi's spreadsheet 1-28-2024
</commit_message>
<xml_diff>
--- a/data/pct_supersite.xlsx
+++ b/data/pct_supersite.xlsx
@@ -513,7 +513,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>Platt MS</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>Monarch K8</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>Monarch K8</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>Monarch K8</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>Monarch K8</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>Monarch K8</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>Monarch K8</t>
         </is>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>Monarch K8</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>Monarch K8</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>Monarch K8</t>
         </is>
       </c>
     </row>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>Monarch K8</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>Monarch K8</t>
         </is>
       </c>
     </row>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>Monarch K8</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>Monarch K8</t>
         </is>
       </c>
     </row>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -3873,7 +3873,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -3915,7 +3915,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -3999,7 +3999,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -4419,7 +4419,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -4503,7 +4503,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -4545,7 +4545,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -4587,7 +4587,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -4671,7 +4671,7 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -4713,7 +4713,7 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -5175,7 +5175,7 @@
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>Timberline K-8</t>
         </is>
       </c>
     </row>
@@ -6897,7 +6897,7 @@
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>Platt MS</t>
         </is>
       </c>
     </row>
@@ -6939,7 +6939,7 @@
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>Platt MS</t>
         </is>
       </c>
     </row>
@@ -6981,7 +6981,7 @@
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>Platt MS</t>
         </is>
       </c>
     </row>
@@ -7023,7 +7023,7 @@
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>Platt MS</t>
         </is>
       </c>
     </row>
@@ -7065,7 +7065,7 @@
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>Platt MS</t>
         </is>
       </c>
     </row>
@@ -7107,7 +7107,7 @@
       </c>
       <c r="H159" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>Platt MS</t>
         </is>
       </c>
     </row>
@@ -7149,7 +7149,7 @@
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>Platt MS</t>
         </is>
       </c>
     </row>
@@ -7191,7 +7191,7 @@
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>Platt MS</t>
         </is>
       </c>
     </row>
@@ -7233,7 +7233,7 @@
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>Platt MS</t>
         </is>
       </c>
     </row>
@@ -7485,7 +7485,7 @@
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>Platt MS</t>
         </is>
       </c>
     </row>
@@ -7527,7 +7527,7 @@
       </c>
       <c r="H169" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>Platt MS</t>
         </is>
       </c>
     </row>
@@ -8241,7 +8241,7 @@
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>Ward Community Center</t>
+          <t>Ward Town Hall</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update branch to version 0.5.0
</commit_message>
<xml_diff>
--- a/data/pct_supersite.xlsx
+++ b/data/pct_supersite.xlsx
@@ -933,7 +933,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Monarch K8</t>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Monarch K8</t>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Monarch K8</t>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Monarch K8</t>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Monarch K8</t>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Monarch K8</t>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Monarch K8</t>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Monarch K8</t>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Monarch K8</t>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Monarch K8</t>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Monarch K8</t>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Monarch K8</t>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Monarch K8</t>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>
@@ -7149,7 +7149,7 @@
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>Platt MS</t>
+          <t>New Horizon</t>
         </is>
       </c>
     </row>
@@ -7233,7 +7233,7 @@
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>Platt MS</t>
+          <t>New Horizon</t>
         </is>
       </c>
     </row>
@@ -7485,7 +7485,7 @@
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>Platt MS</t>
+          <t>New Horizon</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor supersite_area_sdhd.ipynb - remove unneccessary code - rewrite header markdown to match final code
</commit_message>
<xml_diff>
--- a/data/pct_supersite.xlsx
+++ b/data/pct_supersite.xlsx
@@ -2193,7 +2193,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Erie MS</t>
+          <t>Erie Elementary</t>
         </is>
       </c>
     </row>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Erie MS</t>
+          <t>Erie Elementary</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Erie MS</t>
+          <t>Erie Elementary</t>
         </is>
       </c>
     </row>
@@ -2319,7 +2319,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Erie MS</t>
+          <t>Erie Elementary</t>
         </is>
       </c>
     </row>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Erie MS</t>
+          <t>Erie Elementary</t>
         </is>
       </c>
     </row>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Erie MS</t>
+          <t>Erie Elementary</t>
         </is>
       </c>
     </row>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Erie MS</t>
+          <t>Erie Elementary</t>
         </is>
       </c>
     </row>
@@ -2487,7 +2487,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Erie MS</t>
+          <t>Erie Elementary</t>
         </is>
       </c>
     </row>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Erie MS</t>
+          <t>Erie Elementary</t>
         </is>
       </c>
     </row>
@@ -7149,7 +7149,7 @@
       </c>
       <c r="H160" t="inlineStr">
         <is>
-          <t>New Horizon</t>
+          <t>Horizon K-8</t>
         </is>
       </c>
     </row>
@@ -7233,7 +7233,7 @@
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>New Horizon</t>
+          <t>Horizon K-8</t>
         </is>
       </c>
     </row>
@@ -7485,7 +7485,7 @@
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>New Horizon</t>
+          <t>Horizon K-8</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update for final supersite list Final 2-9 - Erie moved to Meadowlark - Ward name changed to Ward Town Hall - Southern Hills moved to Fairview - Judi's Forecast column name changed to Fcst  Turn Out
</commit_message>
<xml_diff>
--- a/data/pct_supersite.xlsx
+++ b/data/pct_supersite.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H194"/>
+  <dimension ref="A1:H205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1309,11 +1309,7 @@
           <t>POLYGON ((-105.1278491696992 39.98669844549102, -105.1278929800003 39.98688710210271, -105.1278529946731 39.98947786494407, -105.1278595500547 39.99060939569144, -105.1280717529826 39.99060563213883, -105.1282287101203 39.990606162723, -105.1307358058815 39.99061460499159, -105.1307415269931 39.98829279039961, -105.131057485362 39.98813023334419, -105.131771009591 39.98813583993596, -105.1311695131819 39.98706498517915, -105.1311069093307 39.98692138552279, -105.1319496864446 39.9869269236389, -105.1333510646578 39.98693611959428, -105.1349481206317 39.98693405035077, -105.1358909917806 39.98693593439277, -105.1380400749165 39.98694709482201, -105.1380400266357 39.98688889589904, -105.1380419916548 39.98611502626242, -105.1380518736492 39.9856651169243, -105.1380488539903 39.98515806618041, -105.1380459539424 39.98503205218287, -105.1380169493754 39.98491611294507, -105.1379600767696 39.98480612599635, -105.1378400755192 39.98468907677978, -105.1373158899584 39.9843429050377, -105.1371601067108 39.98424413577549, -105.137043097014 39.98416909736873, -105.136991932848 39.98412693492242, -105.1369150197316 39.98402786426627, -105.1368760086788 39.9839149131145, -105.1368760662072 39.98363599987925, -105.1368658968665 39.98320002809678, -105.1368710296304 39.98263809867464, -105.1368619200536 39.98166791044249, -105.1368601054013 39.98066809809995, -105.136862070902 39.98029887266666, -105.1368509912206 39.9799669411584, -105.1368547160319 39.97965870039376, -105.1368970054142 39.97868457762276, -105.1391939833452 39.9786950285204, -105.1398623998234 39.97870544999949, -105.1399528897068 39.9787119508487, -105.1403200008789 39.97879408159125, -105.1404369659418 39.97880899577163, -105.1409293598499 39.97880895007127, -105.1409456587332 39.97776151773809, -105.1420770432057 39.97776765748668, -105.1432885288381 39.97773242539142, -105.1432943712138 39.977650378093, -105.1433036870691 39.9771906058965, -105.1433117063147 39.97673384507582, -105.1433105828532 39.97615496704697, -105.1433054578167 39.97603468882662, -105.1409958621201 39.97603391013515, -105.1409831119745 39.97681055059026, -105.1402610830722 39.97681347542572, -105.1402610924567 39.97681258380209, -105.1367812813878 39.97680764905088, -105.1367812462675 39.97680764894022, -105.1367811807096 39.97680764873362, -105.13678106013 39.97680764835362, -105.1357531011968 39.97680290928571, -105.1345908763852 39.97680911350178, -105.1333829314064 39.97682394561945, -105.1321378796018 39.97683809725402, -105.1307808317385 39.97684309169715, -105.130198828228 39.97684589219254, -105.1300746618064 39.97685388159796, -105.1299589906039 39.976864768547, -105.1298379006302 39.97687795087256, -105.1297750609442 39.97688488677507, -105.129713999398 39.97689292626037, -105.1296518574046 39.97690288425013, -105.1295918539046 39.97691312287947, -105.1295311225317 39.97692610525043, -105.1292929066513 39.97696487020448, -105.1290571708148 39.97700693726274, -105.1288189364574 39.97704899579355, -105.1285810424273 39.97709407394184, -105.1278751389853 39.97724196051531, -105.1273435143957 39.97735082326365, -105.1271320977502 39.97739411515896, -105.1251821045501 39.97776690536398, -105.1220440922178 39.97834907560969, -105.1218390971384 39.97837997317655, -105.1212738234645 39.9784519641494, -105.1209279925593 39.97846208286956, -105.1206690055671 39.97844805327635, -105.1204351430655 39.97840802722106, -105.120213921188 39.9783408640164, -105.1199982265585 39.97824241435777, -105.1201190479548 39.97979700902974, -105.120230166672 39.98108244243971, -105.1219081678686 39.98099644262695, -105.1225391670139 39.98073944211418, -105.1232421681502 39.98033144190374, -105.1235891680376 39.98066744275177, -105.1243405817918 39.98021614971381, -105.1255771679067 39.97947344233817, -105.1253541688852 39.97925444189506, -105.1255304415947 39.97914450912447, -105.1260051674357 39.97884844174765, -105.1262311691111 39.97870844220219, -105.1271081689285 39.97816144152506, -105.1276701687788 39.97808644191434, -105.1276742985784 39.97835509150174, -105.1276812036791 39.97880423869458, -105.1276880805791 39.97925149078886, -105.12769489113 39.97973687298536, -105.1276979486562 39.98011536714193, -105.1276992570783 39.98027720192252, -105.1277006654453 39.98045161563807, -105.1277022727454 39.98065050362139, -105.1277031693758 39.98076144258219, -105.1275471685854 39.9807554418902, -105.1274521692765 39.98074644262105, -105.1273271684002 39.98072644199087, -105.1273066551089 39.98072157695184, -105.127214375739 39.98069969063391, -105.1271711685487 39.98068944278467, -105.127139392241 39.98068334791111, -105.1270981684207 39.98067544186095, -105.1269711680979 39.98065844167844, -105.1268901681804 39.98065044284952, -105.1267971687024 39.98065044260115, -105.1266971688295 39.98065244248855, -105.1266091684414 39.98065844226225, -105.1264991677584 39.98067244239655, -105.126331169116 39.98070644271509, -105.1261481677718 39.9807394421338, -105.1259671694033 39.98075344203813, -105.1258431687578 39.98075244156166, -105.1256331685554 39.98073244235897, -105.1254741692224 39.98069944174981, -105.1253301685872 39.98066944203719, -105.1250891674626 39.98064744247992, -105.12468924775 39.98064430008328, -105.1239441684502 39.98063844197828, -105.1239481684561 39.98099044193104, -105.123848168531 39.98109744278342, -105.1237131684662 39.98127144197014, -105.1236411680837 39.98141344271861, -105.123586168347 39.98161144252593, -105.1235830349789 39.98201442443881, -105.1235781685477 39.98264044277064, -105.1236691677244 39.98278344313378, -105.123744168235 39.98286744302084, -105.1238561683382 39.98296444303244, -105.1240021678686 39.98305844296069, -105.1242251688294 39.98315444282675, -105.1249263230647 39.98314996424318, -105.1258921445311 39.98314315953377, -105.1268441685182 39.98313644257139, -105.1268601685777 39.98365144197767, -105.1278411686021 39.98365144210749, -105.1278251690041 39.98379744319919, -105.1278173436443 39.98417719271642, -105.1278081691162 39.98462244192449, -105.1278341691096 39.98513544239999, -105.1278368922283 39.98539987307798, -105.127841169928 39.98581544210798, -105.1278438505662 39.98611127501945, -105.1278491696992 39.98669844549102))</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Louisville MS</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1855,11 +1851,7 @@
           <t>POLYGON ((-105.0744840001105 40.00754717649394, -105.0744840004529 40.00754899853014, -105.0744840014802 40.00754920928831, -105.0744959994806 40.00913899920532, -105.0744850002892 40.01025499937742, -105.0744939996588 40.01117199953493, -105.0744939994117 40.01312199935634, -105.0744879997328 40.01486699832747, -105.0750330000281 40.01486599880874, -105.0776729999707 40.01487699919728, -105.0778080003735 40.01487099884424, -105.0780740000252 40.01483699883885, -105.0785220001667 40.0147389989032, -105.0787519998548 40.01470499815898, -105.0790640003765 40.0146869983785, -105.0798880004663 40.01470099918091, -105.0827519996697 40.0147379995101, -105.083827279062 40.01474776707985, -105.0838636006166 40.01474809629242, -105.0838678605798 40.01474813508104, -105.0839630017275 40.01474899892437, -105.084275999784 40.01475199921421, -105.084343261355 40.01475098794224, -105.0844090000323 40.01474999906352, -105.0863749999974 40.01472599885857, -105.0865649991523 40.01472399889266, -105.0905288819658 40.01468199225995, -105.0905289991035 40.0146819917752, -105.0905557415763 40.01468189398261, -105.0924409249201 40.01467444931598, -105.0932924249816 40.01467107691634, -105.0933139431195 40.01248606893635, -105.0933140887827 40.01198287150529, -105.0933129151652 40.01122189458499, -105.0933126135376 40.01105094940586, -105.0933099689575 40.0108779091348, -105.0933099762549 40.01069699925051, -105.0933091657515 40.01035411921701, -105.093309443264 40.01025378320853, -105.0933088726542 40.01016387563778, -105.0933051569746 40.00994891221197, -105.0933161589406 40.00948089214382, -105.0932939057928 40.00908193347691, -105.0932830467683 40.00826903791486, -105.0932839692943 40.00739606304989, -105.0932938828004 40.00699090412751, -105.0932959870564 40.00538111757357, -105.0932939383563 40.00512608058885, -105.0933018889842 40.00385287724529, -105.0933040871278 40.00360389412218, -105.093300989612 40.00340513019348, -105.0933119971037 40.00293601104079, -105.0933390080789 40.00214126804693, -105.0931508052644 40.00213842182832, -105.0903574852876 40.00212367809764, -105.0882204212901 40.00211118790698, -105.08822934821 40.00271429971438, -105.0858460122409 40.00271024910187, -105.0840693395224 40.00271148340227, -105.0839257284982 40.00271103102219, -105.0838931675961 40.00576387712228, -105.0838750855414 40.00747700408438, -105.0834530015145 40.00748030588483, -105.0785867684244 40.00751825042298, -105.0751311968962 40.00754507131038, -105.0744840001105 40.00754717649394))</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Centaurus HS</t>
-        </is>
-      </c>
+      <c r="H34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2193,7 +2185,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Erie Elementary</t>
+          <t>Meadowlark</t>
         </is>
       </c>
     </row>
@@ -2235,7 +2227,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Erie Elementary</t>
+          <t>Meadowlark</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2269,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Erie Elementary</t>
+          <t>Meadowlark</t>
         </is>
       </c>
     </row>
@@ -2319,7 +2311,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Erie Elementary</t>
+          <t>Meadowlark</t>
         </is>
       </c>
     </row>
@@ -2361,7 +2353,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Erie Elementary</t>
+          <t>Meadowlark</t>
         </is>
       </c>
     </row>
@@ -2403,7 +2395,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Erie Elementary</t>
+          <t>Meadowlark</t>
         </is>
       </c>
     </row>
@@ -2445,7 +2437,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Erie Elementary</t>
+          <t>Meadowlark</t>
         </is>
       </c>
     </row>
@@ -2487,7 +2479,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Erie Elementary</t>
+          <t>Meadowlark</t>
         </is>
       </c>
     </row>
@@ -2529,7 +2521,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Erie Elementary</t>
+          <t>Meadowlark</t>
         </is>
       </c>
     </row>
@@ -2611,11 +2603,7 @@
           <t>POLYGON ((-105.1782688488585 40.01463291530548, -105.1782689995687 40.01463299858616, -105.179412999948 40.01461999874561, -105.1808354543097 40.01462562931187, -105.1827040007133 40.01463299831895, -105.1834549992717 40.0146349225061, -105.1838739999368 40.01463599886635, -105.1841701799736 40.01463570346134, -105.1858630004019 40.01463399899924, -105.1864974973728 40.01463462047163, -105.1868859994811 40.01463499863746, -105.1879306387029 40.01464043574966, -105.1880389993641 40.01464099911838, -105.1886723010191 40.01463892504425, -105.1895639999455 40.01463599872144, -105.1942429993284 40.01465399917136, -105.1943553939693 40.01465460062421, -105.1951779999087 40.01465899884218, -105.1966359998847 40.01466699895634, -105.1967699330014 40.01466790959612, -105.1967830001021 40.0146679988932, -105.1983059994697 40.01466299922393, -105.1988599995382 40.01467899903977, -105.2006159994158 40.01467999898198, -105.2009300000826 40.01468399931195, -105.201182717144 40.01468616479592, -105.2012799993588 40.01468699864344, -105.2020565681202 40.01468240032865, -105.2020579655673 40.01468239223043, -105.2027989994621 40.01467799882614, -105.2028090273656 40.01467798954275, -105.2027581900902 40.01266844174256, -105.2038051899005 40.01281044069496, -105.2043981908388 40.01288544030034, -105.2045691898613 40.01294644116913, -105.2048331905392 40.01297844102542, -105.2050351910883 40.01296044132123, -105.2050398702081 40.01392145197964, -105.2050431900852 40.0146034419073, -105.2069742231526 40.01462497172324, -105.2078121909381 40.01462344028587, -105.2078361910397 40.01348944102689, -105.2075011914237 40.01348844053171, -105.2074681901274 40.01104044140051, -105.2098111911977 40.01104044022411, -105.2098292659196 40.01246736656677, -105.2098311921049 40.01261944051893, -105.2101881770135 40.0126180919686, -105.2101880793582 40.01262205279892, -105.2121356176559 40.01262468172177, -105.2130646768166 40.01262642336378, -105.213064157268 40.01258789120162, -105.2130592574697 40.01222416348261, -105.2130589996108 40.01220499962974, -105.2130529986013 40.01186999911342, -105.2130460006044 40.01138699885649, -105.2130454473815 40.01133281594282, -105.2130440003177 40.01119099898076, -105.2130312388504 40.01016524665692, -105.2130280004494 40.00990499912331, -105.2130180708937 40.00983143781237, -105.2130060003659 40.00974199894547, -105.2129829999123 40.00961299956395, -105.2129829986977 40.0095865752715, -105.2129829998411 40.0095709993631, -105.2130219997471 40.00935599951865, -105.2130219996678 40.00906603303326, -105.2130219999797 40.00890899948654, -105.2130189997407 40.00870099855842, -105.2130112852478 40.00853642174128, -105.213003999585 40.0083809993364, -105.2129869521706 40.00829726722127, -105.2129700000606 40.00821399827627, -105.2129235378465 40.00809508272722, -105.2128859992807 40.00799899844429, -105.2126530118967 40.00758899420312, -105.2126529828366 40.00758894189271, -105.2125739999607 40.00741399830913, -105.2125429989301 40.00731899837689, -105.2125049987698 40.00709399945863, -105.2125054826385 40.00647891950867, -105.2125059976708 40.00582199879766, -105.2125107894076 40.00369755140002, -105.2110311909939 40.00371343942365, -105.21103119153 40.00352344002083, -105.2111551901976 40.00343643944229, -105.2111711906653 40.00325443919979, -105.2111441915764 40.00300243863417, -105.2117761908399 40.0030044389501, -105.2117791909032 40.00354043954807, -105.2125117588774 40.00352564947486, -105.2125161427577 40.00307331652181, -105.2125269999105 40.00195299848955, -105.212566988398 40.00156499793533, -105.2125669991999 40.00156493581707, -105.2125852425582 40.00147525356017, -105.2127399996955 40.00071399866724, -105.2127818519077 40.00052534458408, -105.2128050001144 40.00042099923211, -105.2128159972606 40.00024511251258, -105.2128159836817 40.00024499989686, -105.2127969995393 40.00008999943838, -105.2127928656112 40.00007553362977, -105.2127829993984 40.00004099865892, -105.2127459994442 39.99984399810055, -105.2127392146961 39.99881852246104, -105.2127389991961 39.99878599927126, -105.2127455277946 39.99746149416151, -105.2127469993367 39.99716299909484, -105.2127440001071 39.99692699925155, -105.2127449818323 39.99692495901152, -105.2126844006306 39.99661445128344, -105.2126006533221 39.99626870887596, -105.2125139076481 39.9958991302809, -105.2124961767938 39.99569533982743, -105.2124925687887 39.99544869177733, -105.2124983315102 39.99518419448454, -105.2124740351865 39.99470038739478, -105.2124601767598 39.99431311694229, -105.2124779991473 39.99348899860376, -105.2125093588739 39.99318486329975, -105.2033772696824 39.99340858016221, -105.2029582688417 39.99342377712174, -105.1990257041367 39.99355631287658, -105.1964298760536 39.99604846059979, -105.1934576319139 39.99892492757701, -105.1934732468954 39.99998381946754, -105.193474990138 40.00010170190278, -105.1908131549582 40.00010201071742, -105.1906400392679 40.00010099696486, -105.1840981545727 40.00011510349158, -105.1811590475376 40.00011113122423, -105.1801420832138 40.00011407962215, -105.1793810524402 40.00011690691521, -105.1781569577279 40.00014094854438, -105.1781831559926 40.00056488123449, -105.1781969902901 40.00081006671814, -105.1782380691662 40.00148495285106, -105.1782610216749 40.00532089112599, -105.1782459979963 40.00585698788481, -105.1782109170462 40.00640702843349, -105.1781838615073 40.00729886938524, -105.1781999993325 40.00796407729013, -105.1782029610038 40.0085468924531, -105.1782108321747 40.00884586714735, -105.1782329229247 40.00968705887914, -105.1782201536082 40.01239296866031, -105.1782518670392 40.01369208709981, -105.1782688488585 40.01463291530548))</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>Centaurus HS</t>
-        </is>
-      </c>
+      <c r="H52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3703,11 +3691,7 @@
           <t>POLYGON ((-105.093035412355 40.17395404356559, -105.0930355022931 40.17396373747397, -105.0930905495083 40.1739629603663, -105.0933063695626 40.17394767675843, -105.0947811388498 40.17392604651604, -105.0950699350661 40.17392596063161, -105.0955101015059 40.1739269531794, -105.0957541527641 40.17392890476933, -105.0963270854283 40.17393008282001, -105.0964931512326 40.17392709427654, -105.0974990948966 40.17392895400177, -105.0977370735687 40.17392895919532, -105.0979528772734 40.17392696481058, -105.0981518434555 40.1739279313386, -105.0989699184054 40.17392802714794, -105.0998391512321 40.17393103942207, -105.1001161310761 40.17393199790583, -105.101211927436 40.17392892050625, -105.1023799809039 40.17393102219533, -105.1024508498185 40.17392907018132, -105.1024948495252 40.17393196664215, -105.1024899190531 40.17355092136356, -105.1024980637468 40.17289211231032, -105.102497972706 40.17264610216935, -105.1024978523519 40.17231590278406, -105.1025021205653 40.17066690196754, -105.1025081247895 40.16902696535896, -105.1025060264547 40.16736503926331, -105.1025141437187 40.1657308741228, -105.1025160379682 40.1639369188412, -105.1025170800547 40.16388092145418, -105.1025181698239 40.1638169634628, -105.1025169988298 40.16187393466532, -105.1025209099907 40.16157198012871, -105.1025371099835 40.16033012490647, -105.1025380469332 40.16023102782011, -105.1025380471068 40.16023099809953, -105.1025380465539 40.16023089182191, -105.1024143180025 40.16022903062637, -105.101072318054 40.16022203122495, -105.1010700959203 40.16022203616376, -105.1010699280626 40.16022203558438, -105.1010630001934 40.16022199906198, -105.0998739874729 40.16022399957189, -105.0967180002406 40.1602330001241, -105.0960982895062 40.16023918860394, -105.0960170000153 40.16023999516622, -105.0960168884854 40.16023999747829, -105.095906860969 40.16024372245906, -105.0951589994661 40.16026899899504, -105.0948714164467 40.16027221347903, -105.0946219991399 40.16027500002095, -105.0944589999225 40.16027599890212, -105.0943463028096 40.16027599968295, -105.0942474912358 40.16027599866759, -105.0941529994326 40.16027600012808, -105.0933151831979 40.16027514992445, -105.0931679955306 40.16027501197318, -105.0931099998072 40.16041499996014, -105.0931024819559 40.16045158549526, -105.0930949991611 40.1604880000312, -105.0930969990843 40.16066999982127, -105.093074999123 40.16093800027746, -105.0930749994591 40.16106100006206, -105.0930749990154 40.16110699945172, -105.0931069998108 40.1613119217147, -105.0931069993422 40.16131200006891, -105.0931149989175 40.16163199930823, -105.0931129997678 40.16178000016573, -105.0931070642517 40.16237164155648, -105.0931070011848 40.1623778683723, -105.0931070004038 40.1623779989626, -105.0931050119728 40.16313991872316, -105.0931050114934 40.1631399988786, -105.0931040000302 40.16325199822559, -105.0931039998199 40.16329599907725, -105.0931469291512 40.16390871444782, -105.0931479999207 40.16392399940396, -105.0931480029145 40.16392408767742, -105.0931569991541 40.16423199918421, -105.0931259993862 40.16516199880555, -105.0931289999454 40.16569099842605, -105.0931319995954 40.16601699884203, -105.093122999789 40.1669069989264, -105.0931289996238 40.16735399928291, -105.0931369998561 40.16781299868737, -105.0931339988095 40.16872599950739, -105.0931369991391 40.16900499892864, -105.0931479994263 40.17023599850143, -105.0931500001353 40.17054199825319, -105.093151000261 40.17065999832266, -105.0931330003842 40.17149199908522, -105.0931459999594 40.17231399916508, -105.0930759995535 40.17368299823816, -105.093035999663 40.17395399970057, -105.093035412355 40.17395404356559))</t>
         </is>
       </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>Altona MS</t>
-        </is>
-      </c>
+      <c r="H78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4375,11 +4359,7 @@
           <t>POLYGON ((-105.1023829530066 40.18125894705506, -105.1023831548078 40.18140800978896, -105.102370035092 40.18248900592155, -105.1023460249624 40.18414699542499, -105.1023359709285 40.18488705328424, -105.102324014524 40.18558510414968, -105.102314050903 40.18661587375054, -105.1022961545613 40.18759500754209, -105.1022951231635 40.18764908370499, -105.1022919348154 40.18813304226678, -105.1022929712663 40.18856787832284, -105.1031670440105 40.18857088157077, -105.1035181760235 40.18857208617342, -105.1046560755281 40.18857104075413, -105.1051969341203 40.18856904580717, -105.1057839557793 40.18856912679325, -105.106394960974 40.18856901265301, -105.1067500432291 40.18856802423286, -105.1069608759509 40.18856709474983, -105.1075808282699 40.18856700385626, -105.1080901776704 40.18856708418473, -105.1102081396324 40.18856189061061, -105.111460935844 40.18856089171691, -105.1117581070876 40.18856554113695, -105.1120540599835 40.18855794243968, -105.1120313601333 40.18760194311961, -105.112017894645 40.18707819066701, -105.112011570436 40.18673288206929, -105.1120085237062 40.186557607745, -105.1119319115066 40.18487960280919, -105.1119049061916 40.18402300359683, -105.1119118919206 40.18367686408679, -105.1119091664257 40.18315088404788, -105.1119081200098 40.18251894680662, -105.1118759946224 40.18181388411318, -105.1118629926047 40.18127002597253, -105.1115040224316 40.18126909494015, -105.1113569308159 40.18126805117004, -105.1112559916314 40.18126990755782, -105.1101640174649 40.18126520655875, -105.1089940736708 40.18126612354689, -105.1086240113595 40.18126487136174, -105.1084361110251 40.18126505829095, -105.1080911123929 40.18126196732355, -105.1072020949942 40.18126004898254, -105.106833109551 40.18125797063896, -105.106641973712 40.18126088969616, -105.1059451380013 40.18126098709274, -105.1052980584674 40.18125987759827, -105.1051319899099 40.18126013369076, -105.1047898365833 40.18126006333194, -105.1044011718303 40.18125708676741, -105.1036499481707 40.18125506224674, -105.1033940415842 40.18125610659184, -105.1027139937316 40.18126200709273, -105.1023829530066 40.18125894705506))</t>
         </is>
       </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>Longs Peak MS</t>
-        </is>
-      </c>
+      <c r="H94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4543,11 +4523,7 @@
           <t>POLYGON ((-105.0551857428336 40.19115277071814, -105.0552111773586 40.19115247588264, -105.0576711777204 40.19105147542044, -105.0599381776194 40.19154047538977, -105.0599451784452 40.19310447585676, -105.0593371782352 40.19309847586848, -105.0593451786143 40.19487747591219, -105.0599531783856 40.19487547541794, -105.0599607462004 40.19697811055131, -105.0599628313483 40.19812507551509, -105.0599654497826 40.19956479210923, -105.0599659789192 40.19985581559262, -105.059967664644 40.20078266614567, -105.059968926204 40.2014763253382, -105.0599701793699 40.20216547762988, -105.0602041798525 40.20216247700513, -105.0604371797873 40.20261947653857, -105.0604711807169 40.20272847758034, -105.0604696887987 40.20325998334323, -105.0604691803505 40.2035581312503, -105.0604691803914 40.20358828730515, -105.0605809999359 40.20358599860956, -105.0625290002004 40.20354499890966, -105.0647029999319 40.20349699885044, -105.0647501006766 40.20349602781442, -105.0647339491228 40.20337651726427, -105.0647313741987 40.20266464448074, -105.0647303790163 40.20099722600703, -105.0647362886098 40.20007406548243, -105.0647251582375 40.20007486118185, -105.0647365324077 40.19910003526667, -105.0647365332339 40.19909770441809, -105.064562850699 40.19806721120871, -105.0645385435449 40.19782321419675, -105.0645757570088 40.1971347874193, -105.0645758289882 40.1971334511428, -105.0645220075083 40.19679514516783, -105.0642860933617 40.19647762079072, -105.0638133563912 40.19618043809251, -105.0646926527958 40.19618265905708, -105.0639941019674 40.19573944112544, -105.0632898897123 40.19531381132088, -105.0632053551679 40.19517051471762, -105.0630363648705 40.19487200885944, -105.0629597916534 40.19469895531674, -105.0628134193528 40.19450776646138, -105.0627135803031 40.19432866794923, -105.0626076206911 40.19389338013623, -105.0624336669717 40.19315996562867, -105.0622520623238 40.19240865041179, -105.0621761075427 40.19214028124743, -105.0621311110377 40.19188990154627, -105.0621325686364 40.19166352775939, -105.0621312059593 40.19066864203916, -105.0621129654896 40.18988220023222, -105.0621158423633 40.18943540829499, -105.0621179136866 40.18911371844126, -105.0621190158081 40.18894255062722, -105.0625048190455 40.18897514439156, -105.0633638095203 40.18897514555042, -105.0641869916493 40.18894930200723, -105.0640045704488 40.18875033664372, -105.0635401820393 40.18815007432843, -105.0631167943398 40.18756256584666, -105.063108661064 40.18754993426116, -105.0630597388427 40.18749304870389, -105.0622351951782 40.18669611553849, -105.0614424718392 40.18606310096347, -105.0612086079817 40.18538810152727, -105.0610479441212 40.18482678180195, -105.0610956824389 40.18379374470699, -105.0611256911425 40.18296224313866, -105.0609142053907 40.18264013476896, -105.0602107919676 40.18217755251773, -105.0599001379389 40.18194956648689, -105.059747225974 40.18174422809434, -105.0563433097719 40.18182116446065, -105.0563426497601 40.18182117903999, -105.0563435646631 40.18183609266326, -105.0563475109136 40.18206710151329, -105.0563500596562 40.18221623312483, -105.0558656311479 40.18222843305814, -105.0554415540536 40.18223911220016, -105.0553171302694 40.18224224525912, -105.0553029537267 40.18224260232314, -105.0553029531036 40.18224233843291, -105.0552122394415 40.18224293424132, -105.0551953437782 40.18224286923797, -105.0551907707022 40.18769647581839, -105.0551896265968 40.18906734845638, -105.0551896237061 40.18907048357343, -105.0551895553035 40.18914970721488, -105.0551895524011 40.1891528441331, -105.0551895204548 40.18923708718096, -105.0551895198951 40.1892402250088, -105.0551857428336 40.19115277071814))</t>
         </is>
       </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t>Timberline K-8</t>
-        </is>
-      </c>
+      <c r="H98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -5509,11 +5485,7 @@
           <t>POLYGON ((-105.2068465057981 40.07117836077267, -105.2068798224365 40.07280181856465, -105.2068677753563 40.07325874343877, -105.2068647486335 40.07396214178695, -105.2068623764414 40.07451341961843, -105.2076420782932 40.07371766177889, -105.2082801606808 40.07302997161467, -105.2086245150866 40.07265908095091, -105.2099806192159 40.07132523758062, -105.2107244253088 40.07057602937812, -105.2112000554906 40.07019030381962, -105.2138871567176 40.06781106466761, -105.2161601606601 40.065676155581, -105.2161515695624 40.06476845457101, -105.2161489168033 40.06403186699564, -105.2161370889706 40.06326895154256, -105.2161351423245 40.06185481826265, -105.2160151985019 40.06185644695927, -105.2144889285572 40.06184333056139, -105.2116771982488 40.06182044730468, -105.2070381967239 40.06179344782172, -105.2068437684325 40.06179232904368, -105.2068438304768 40.06178308493803, -105.2068520652456 40.06169608423045, -105.2068749843029 40.06085309603117, -105.2068741762046 40.05938002791319, -105.2068748975684 40.0589608656869, -105.2068740084848 40.05834961512206, -105.2055541963941 40.05838544689875, -105.2052551959982 40.05847144768208, -105.2048171966658 40.05844444708361, -105.2043011952846 40.05848944735493, -105.2036141957108 40.05861644723085, -105.2030841948025 40.05879544709134, -105.2029191954679 40.05892644793907, -105.2025611961079 40.05994444774891, -105.2022581955147 40.06021544819658, -105.2020791960017 40.06027244767436, -105.2020971959404 40.06055644730947, -105.2039251968715 40.06102844726419, -105.2039191966671 40.06188244736903, -105.2023031957252 40.06217144785335, -105.2012341952632 40.06256244833814, -105.2010431953765 40.06269044755282, -105.2008701954203 40.06280544810341, -105.2004271948154 40.0631064479396, -105.1994881955361 40.06370844772376, -105.197510194433 40.06410844816937, -105.1975131946994 40.06384744877385, -105.1962251942363 40.0631234489768, -105.1960821947275 40.06189544761963, -105.1944631938403 40.06188444842264, -105.1939423130284 40.06188444891134, -105.1939389409759 40.06188596206637, -105.1935278372535 40.06188410371627, -105.1930531938404 40.06188344841224, -105.1928031939953 40.06197244919012, -105.192830194072 40.06206044878067, -105.1928621939255 40.06214444837541, -105.1928981932525 40.06221544871938, -105.1932001627259 40.06253903928965, -105.195066194525 40.06429244893643, -105.1950261937514 40.06432744874969, -105.1950591935295 40.06435544887151, -105.1950961944753 40.06438544818828, -105.1951361943555 40.06441744945245, -105.1951891945079 40.06445744948024, -105.1952181943264 40.06447744843081, -105.1952991946379 40.06453244880927, -105.1953261940917 40.06454944869287, -105.1954081943274 40.06459844880609, -105.1954221947172 40.06460744901683, -105.1954341946791 40.06461344928788, -105.1954481948594 40.06462144887348, -105.1954631949272 40.06462944929453, -105.1954741938401 40.0646354487212, -105.1954861952043 40.06464244871119, -105.1955071952751 40.06465344790787, -105.1955191940804 40.06465944816699, -105.1955361941598 40.06466844907239, -105.1955621953032 40.06468144828445, -105.1958335281126 40.06482122755254, -105.1961561946336 40.06498744839866, -105.1961811946941 40.06500444822031, -105.1962161953141 40.06502844808715, -105.1962471945175 40.0650494481572, -105.1962861947403 40.06507844902631, -105.1963061946974 40.06509244910959, -105.1963351948621 40.0651164493617, -105.1964601945655 40.06521144902592, -105.196613194153 40.06534144843442, -105.1967121942066 40.06543344785908, -105.1967491951159 40.06548244853415, -105.1967551952459 40.06549044945493, -105.1967811954029 40.06553144866818, -105.197500195574 40.06553044795643, -105.1993447543905 40.06554629272709, -105.2003585210558 40.0655549887631, -105.2022371955249 40.06554144896795, -105.2022461967158 40.06719644869614, -105.202495195546 40.06738144820481, -105.2026291967245 40.06751244885115, -105.2024761975983 40.06763844798303, -105.2023491962878 40.06777944851839, -105.2022321959824 40.06797144872966, -105.2021841960138 40.06808744821939, -105.2021581970034 40.06820744840584, -105.2021606973751 40.06883412167546, -105.2021571971997 40.06915744908764, -105.2008557060834 40.06916006349055, -105.1982481955772 40.06916644960438, -105.1983431964843 40.06969344951722, -105.1981921953054 40.0700514489731, -105.1978608565895 40.07054974585753, -105.1976471349798 40.070854867217, -105.1974891959825 40.07108844907243, -105.1974111953331 40.07173844977702, -105.1971151965505 40.07180144923354, -105.1959639747934 40.07179589531189, -105.1959629613449 40.07179313125406, -105.1955317416101 40.07179076427918, -105.1955325357656 40.0721290328372, -105.19555338647 40.07215351162139, -105.195571161459 40.0721891665423, -105.195575276256 40.07222722619021, -105.1955696351996 40.07225420104457, -105.1955552225853 40.07228173548236, -105.1955329102784 40.07230570863143, -105.1956497600617 40.07230497294984, -105.1958715408196 40.07265610430982, -105.195948214593 40.07277500006112, -105.1965590232563 40.07277292288894, -105.1967158901643 40.07277306047437, -105.1968731121383 40.07277402287241, -105.1969338538223 40.07277500556847, -105.1970328286375 40.07277608949424, -105.1971160825409 40.07277713118252, -105.1977160136586 40.07278309635792, -105.1979078919024 40.07278497129465, -105.1982398337714 40.07278913325598, -105.1998038607809 40.07279101579683, -105.2011680960696 40.07280306606555, -105.2021660596678 40.07281690086156, -105.2030440636358 40.07280708357413, -105.2032059353273 40.07280695141796, -105.2036409100057 40.07278308778325, -105.2038469064714 40.07274298737001, -105.2038830407287 40.07273292346781, -105.2040609420013 40.07266200516737, -105.2042239527948 40.07256387047889, -105.2045168221222 40.07234912431174, -105.2052689409496 40.0716189076843, -105.205479003384 40.07146406586098, -105.2056899679546 40.07134793401426, -105.2058299486888 40.07128597501093, -105.2060310188561 40.07122691751993, -105.2062419806407 40.0711939631236, -105.2063513217104 40.07118051817727, -105.2067702438353 40.07117795720276, -105.2068465057981 40.07117836077267))</t>
         </is>
       </c>
-      <c r="H121" t="inlineStr">
-        <is>
-          <t>Niwot HS</t>
-        </is>
-      </c>
+      <c r="H121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -6097,11 +6069,7 @@
           <t>POLYGON ((-105.2936404423018 40.04090982706559, -105.2936404333365 40.04090969195224, -105.2936393298994 40.04089176076243, -105.2936387602875 40.04088251278208, -105.2936382144575 40.04088243885319, -105.2936381907138 40.04087325219269, -105.2936381107935 40.04084275698107, -105.2936375293797 40.04061951931827, -105.2936362147382 40.04011443848095, -105.2934722142269 40.04010743878002, -105.2934792144789 40.03920443815797, -105.2923682131695 40.03918943861687, -105.2923892136016 40.03902243843871, -105.2924912138074 40.03896743828266, -105.2926092133786 40.0388264377026, -105.2927262144654 40.03861943834501, -105.292842214139 40.03837543840261, -105.2929572138373 40.03793343784105, -105.2929242137023 40.03785143845414, -105.2921662137698 40.03784743828271, -105.292166213115 40.03765743823374, -105.2929242141904 40.03765843834879, -105.2927792134548 40.03731343830118, -105.2932632137346 40.03730943865403, -105.2932582145944 40.03688043786936, -105.2916252132727 40.03688043864178, -105.2916242139543 40.03633843870183, -105.2930502139936 40.03635143785036, -105.2930342143154 40.03628543748766, -105.2929422134349 40.03619843809624, -105.292908213494 40.03617043802443, -105.2927832141158 40.03600443825045, -105.2927602138006 40.03597043795142, -105.2927107603088 40.03587813792029, -105.2926582136129 40.03576543800347, -105.2926232139659 40.0355924378065, -105.2925802137358 40.03543343821553, -105.2926902132874 40.03525443823721, -105.2926532134305 40.03511543756299, -105.2926922137881 40.03505743828392, -105.2927552137461 40.03499443757188, -105.2931342134192 40.03501543737434, -105.2932612136337 40.03502943777404, -105.2933812135632 40.03506143848394, -105.2934642135779 40.03506843745255, -105.293634213987 40.0348184377084, -105.2936462145961 40.03479243761252, -105.2936532138585 40.0347724377023, -105.2936592133786 40.03474943774147, -105.2936612144225 40.03473943780755, -105.2936652146541 40.03472043765701, -105.2936672133564 40.03469843746568, -105.2936672134586 40.03467943736553, -105.2936672134593 40.03466743801314, -105.2936652138936 40.03464443725404, -105.293662213805 40.0346264378129, -105.2936581157056 40.03460848684401, -105.2936542131837 40.03459443783817, -105.2936502137531 40.0345814379154, -105.2936462131523 40.03456843799037, -105.2936422133352 40.03455943695012, -105.2935046256782 40.03432954495042, -105.2933842142322 40.03413143774353, -105.2930712139342 40.03413743794434, -105.2930142135916 40.03410643800208, -105.2929952137423 40.03410643813415, -105.2929572138224 40.03408143815955, -105.2929102131477 40.03405643732565, -105.2928912131919 40.03404143802341, -105.2928792139851 40.03402643777797, -105.2928672138293 40.03400943808766, -105.2928562133356 40.0339904380472, -105.2928432126227 40.03397843786441, -105.2928422125705 40.03392543824812, -105.2928442131984 40.03390943819936, -105.2928502132125 40.03389443694749, -105.2928602128196 40.03387843775223, -105.2928772133286 40.03385543686772, -105.2928832130675 40.03383743735128, -105.2928852132439 40.03382543798608, -105.2928972826058 40.03380499689747, -105.2929052133355 40.03379043772514, -105.2929162131264 40.03378343780931, -105.292924213406 40.03377143750584, -105.292933213333 40.03375743685223, -105.2930112141034 40.03362143735369, -105.293291955493 40.03362143728865, -105.2937372138235 40.0336214372065, -105.2937382974607 40.03337909957001, -105.2937386793353 40.03329355655762, -105.2937395508468 40.03309847291506, -105.2937402132035 40.03295043792892, -105.2932286416031 40.03294919515979, -105.2931052137653 40.03294843796873, -105.2927092126049 40.03294843766469, -105.2927108121817 40.03286705423627, -105.292710907085 40.03286705440682, -105.2927122130598 40.03278743752472, -105.2936812128586 40.03278843795151, -105.2936722139328 40.03195643683105, -105.2933122135404 40.03195643722582, -105.2933122133834 40.03167943790211, -105.2936742141418 40.03167843776409, -105.2936732131968 40.03155043743585, -105.2932162129589 40.03154943719254, -105.2932342129986 40.03110243735086, -105.2932282125647 40.0310404366715, -105.293669213941 40.03104043735713, -105.2936642128336 40.03048443747013, -105.2936648818336 40.03047785401582, -105.2936537748646 40.03047788728623, -105.2927552572933 40.03049408413858, -105.29275521762 40.0304882505582, -105.2927385970148 40.03048906550561, -105.2926902128227 40.03049143643388, -105.292694024948 40.03033512199099, -105.2926953162127 40.03015092069578, -105.2926952125016 40.02997043747474, -105.2927355065977 40.02996954708772, -105.2928733794138 40.02996650196004, -105.293193212992 40.02995943740156, -105.2932232128183 40.0299614365863, -105.2932232133512 40.02983612015983, -105.2931884875867 40.02976646198516, -105.2931867492964 40.02966709736802, -105.2936473388391 40.02965363342965, -105.2936571602725 40.02965404007967, -105.293657096737 40.02964638804434, -105.2936542127414 40.02932343683928, -105.2933562129823 40.02932143711671, -105.2930897958375 40.02932328771823, -105.29278021285 40.02932543663955, -105.2927792132976 40.02925843639324, -105.2926812130856 40.02925543766246, -105.2926814065824 40.02924882814005, -105.2926819728648 40.02922943366055, -105.2926912123074 40.02891343650078, -105.2927623809299 40.0289131834094, -105.2927622187183 40.02890295353519, -105.2932416180685 40.02890518641989, -105.2932459804773 40.02805555882141, -105.2932121680632 40.02797051286821, -105.2931062443818 40.02797125870275, -105.2927482126114 40.0279784372106, -105.2926652124506 40.02798243734529, -105.2926662131555 40.02781943678586, -105.2926862126045 40.02765543642518, -105.2926882122127 40.02760543682441, -105.2926782129605 40.02736543611802, -105.2927526221468 40.0273611710597, -105.2928406316727 40.0273612309844, -105.2936104824806 40.02736175091879, -105.2936342486239 40.02736138454571, -105.293635212304 40.02716843638694, -105.2932082126097 40.02716843631173, -105.2932082128545 40.02696443724676, -105.2936352122566 40.02695443650428, -105.2936362122575 40.02682843733329, -105.2936314855515 40.02575744316506, -105.2936332128447 40.02541943670018, -105.2936339345848 40.02541515269726, -105.2926069291672 40.02543973575167, -105.2925031180585 40.02550902431486, -105.2920939363481 40.025498130862, -105.2915040127181 40.02550612476494, -105.2902481507636 40.02550796560364, -105.290043906236 40.02550594671673, -105.2887301598848 40.02552001896971, -105.2867490705732 40.02551994347327, -105.2856660543705 40.0255160131922, -105.2856812109885 40.02583443661324, -105.2856822111836 40.02592843665887, -105.2856742107215 40.02601043682525, -105.2855892107703 40.02642143748587, -105.2855692118289 40.02663843724292, -105.2855712105374 40.02672743692585, -105.2855754584629 40.02732638721953, -105.2855862117171 40.02922543814994, -105.2855863693517 40.02924870043505, -105.2855895839882 40.02975199420325, -105.2855932655471 40.03029421670868, -105.2856075598998 40.03111985202749, -105.2856121682715 40.03181337185057, -105.2856187194815 40.03279928309118, -105.2856191603849 40.03286696954467, -105.2856190537651 40.03286696934653, -105.2856233092233 40.03353419031163, -105.2856302124652 40.03499243870875, -105.2840522108804 40.03500343762658, -105.2824672114959 40.03498943845764, -105.282092223959 40.03498258560737, -105.2820922571864 40.03498831830537, -105.282084254758 40.03633731870206, -105.2820832571337 40.03638731727795, -105.2820839552159 40.03641671759907, -105.2820842547273 40.03642931825196, -105.2820972563 40.03729531910635, -105.2820932567946 40.03789431907661, -105.2820892579222 40.03830031885973, -105.2820822583888 40.03910131882655, -105.2820971543631 40.04091685759044, -105.2834189457056 40.04091203595226, -105.2849108458764 40.04090192430674, -105.2875159710775 40.04090702642674, -105.2878070718198 40.04090289503355, -105.2895539205841 40.04091295761805, -105.2904721577454 40.04092204125421, -105.2907728790686 40.04092505749229, -105.2908289544505 40.04092488447498, -105.2910829027924 40.04092287413435, -105.2912833009954 40.04092752663995, -105.2913789966629 40.04092093945307, -105.2917750974063 40.04091808576007, -105.2920969046858 40.04091701973583, -105.29268691454 40.04092412030541, -105.2930040630487 40.04092798433868, -105.2934190202191 40.04094986543068, -105.2936419909393 40.04097306619047, -105.2936404423018 40.04090982706559))</t>
         </is>
       </c>
-      <c r="H135" t="inlineStr">
-        <is>
-          <t>Centennial MS</t>
-        </is>
-      </c>
+      <c r="H135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -6559,11 +6527,7 @@
           <t>POLYGON ((-105.2810182375564 40.02092314129024, -105.2810232518009 40.02093831867468, -105.2813222531418 40.02180131874344, -105.2814522517319 40.02218931788916, -105.2816952524114 40.02294531788972, -105.2817882518133 40.02320731847269, -105.2819012528731 40.02352531873172, -105.2819872512269 40.02381131814664, -105.282030253746 40.02400831769852, -105.2820462506693 40.02416731908562, -105.2820552528565 40.02447831817484, -105.2820799576935 40.02551691771405, -105.2832522926848 40.02551476930772, -105.283568919774 40.02551402008966, -105.2856660543705 40.0255160131922, -105.2856570833245 40.024507963209, -105.2856500166217 40.02368906050599, -105.2856359777445 40.02327094245604, -105.2856281572593 40.02314602207673, -105.2855958483006 40.02297411245853, -105.285527898361 40.02278099918674, -105.2854569165297 40.02264388269615, -105.2851988391675 40.02227801733283, -105.2849598351697 40.0219788954425, -105.2849019229106 40.02188709849514, -105.2848640990607 40.02176596516206, -105.2848648315332 40.02074201109222, -105.2848861179262 40.02055894665072, -105.2849060840865 40.0204549406858, -105.2848988256668 40.02037888518526, -105.284697939107 40.01977100051715, -105.2844501492575 40.0190919268021, -105.284370977069 40.0188370251274, -105.2842460118721 40.01849803489817, -105.2840818920156 40.01812191122571, -105.280344103938 40.01889429097838, -105.2803492507365 40.01890931823954, -105.2806882501358 40.01992431817114, -105.2810182375564 40.02092314129024))</t>
         </is>
       </c>
-      <c r="H146" t="inlineStr">
-        <is>
-          <t>Casey MS</t>
-        </is>
-      </c>
+      <c r="H146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -6729,7 +6693,7 @@
       </c>
       <c r="H150" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -7275,7 +7239,7 @@
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -7317,7 +7281,7 @@
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -7359,7 +7323,7 @@
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -7401,7 +7365,7 @@
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -7443,7 +7407,7 @@
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -7569,7 +7533,7 @@
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -7611,7 +7575,7 @@
       </c>
       <c r="H171" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -7653,7 +7617,7 @@
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -7693,11 +7657,7 @@
           <t>POLYGON ((-105.2861390115304 39.9722881143455, -105.2858238862138 39.97236126581304, -105.27937173981 39.97062142832051, -105.2725517491279 39.97264797001431, -105.271852448133 39.97308048041847, -105.2715141300797 39.97329796337442, -105.2710101713048 39.97334763678315, -105.270307086264 39.97305969060716, -105.2697051344663 39.97289908688346, -105.2692628275347 39.97275407844554, -105.2691738497955 39.97268801552585, -105.2690799989563 39.97258598049818, -105.2690168630316 39.97247494815974, -105.2689518921809 39.97237900979596, -105.2685800812342 39.97206997752857, -105.2685508772606 39.97205399709568, -105.2684250963644 39.97200405616698, -105.2682871089833 39.97197605214665, -105.2678989563334 39.97196209453039, -105.2678150881506 39.97196796449851, -105.2676519270121 39.97199810756532, -105.2674990387551 39.97204995801228, -105.2672269835133 39.97220506197835, -105.2675241635705 39.97252987079597, -105.2675699456847 39.97260188768651, -105.2676559560471 39.97301493963212, -105.2676558232941 39.97305392063711, -105.2676291675686 39.97312798814713, -105.2675718637409 39.97319101215554, -105.2666550309857 39.97366490295155, -105.2667058624657 39.97372100771231, -105.2667850117981 39.97384387860475, -105.2668418659355 39.97401694200342, -105.2668598632439 39.97418004298486, -105.2668451742927 39.97430190077704, -105.2667868299745 39.97445990631218, -105.266692839123 39.97460795677274, -105.2665689187773 39.9747430446541, -105.2664161606558 39.97485913137701, -105.2660540573271 39.97504809120751, -105.2657899058223 39.97518289262955, -105.2653280294155 39.97543506074108, -105.2649458519276 39.97564895769812, -105.2645848340075 39.97583105123501, -105.2638469416451 39.97623912559444, -105.2637739724697 39.97629003692276, -105.263615040984 39.9764349327568, -105.2633100577322 39.97681698813182, -105.2630501760598 39.97715713335895, -105.2628789145055 39.97735800467315, -105.2627520289152 39.97752108281585, -105.26252984924 39.9776900043216, -105.2623861695196 39.97775696645165, -105.2620860198477 39.97787493928896, -105.2615248868786 39.97803190413939, -105.2614059907024 39.97805197236678, -105.2611229553935 39.97807087721965, -105.2610451726245 39.97806906869406, -105.2601148835307 39.97807592132791, -105.2601128299923 39.97876111940365, -105.2601148541277 39.97909905757952, -105.2601240925484 39.97971894376179, -105.2601270663233 39.97988805426846, -105.2601323605739 39.9802193019425, -105.2599182938995 39.98021663796225, -105.2596720231951 39.98021969945855, -105.2594349816054 39.98024065229194, -105.2571982901938 39.98073639001605, -105.2562962594057 39.98090963595508, -105.2563429162402 39.98103886783078, -105.2565239845004 39.98149797393191, -105.2566190534311 39.98165712142143, -105.2567530779354 39.98179988076132, -105.256964863671 39.98195186270966, -105.2572230666266 39.9820970781437, -105.2580081412259 39.98250090116355, -105.2585298309313 39.98190601192692, -105.2587659545189 39.98203909986017, -105.2590951262364 39.98219791177391, -105.2594090755475 39.98232292541489, -105.2595830614137 39.98236803476654, -105.2598249010107 39.98239901077235, -105.2609279514417 39.98239691129109, -105.2618568300338 39.98240212864589, -105.2620281769223 39.98238601133514, -105.2622488849338 39.98233705323542, -105.2624050298437 39.98227999986478, -105.2625501634418 39.98220810062183, -105.2632858671283 39.98173194873376, -105.2636771671341 39.98208907864245, -105.2638610800784 39.98225691251253, -105.2644248927018 39.98277910578437, -105.264593914942 39.98292000547517, -105.2647808344368 39.98304501876047, -105.2653939206792 39.9833559267931, -105.2658890858176 39.98361004180648, -105.266313014888 39.98382502725105, -105.2671729209081 39.98428302002201, -105.2672730197861 39.98433592936551, -105.267683104764 39.98453194102219, -105.2679329289423 39.98463209445797, -105.2682309574687 39.9847241095941, -105.2685961061897 39.98480802222888, -105.2689670763001 39.98485900393208, -105.2692050571009 39.98487402981937, -105.2693230565022 39.98487477127614, -105.2693219715217 39.98568827537257, -105.2770692361139 39.98569787181271, -105.2821720691177 39.98569760737838, -105.2857057924208 39.98570468543087, -105.2862482059948 39.98525743155678, -105.2862071928632 39.98015902991641, -105.2861390115304 39.9722881143455))</t>
         </is>
       </c>
-      <c r="H173" t="inlineStr">
-        <is>
-          <t>Southern Hills MS</t>
-        </is>
-      </c>
+      <c r="H173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -7737,7 +7697,7 @@
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -7777,11 +7737,7 @@
           <t>POLYGON ((-105.245800143718 39.98094801864188, -105.2458591469235 39.98091493167031, -105.2459760636716 39.98085397183197, -105.2462461766525 39.98076397524878, -105.2465098781437 39.98067011993611, -105.2466978596759 39.98059504023666, -105.2469939547208 39.98042603675346, -105.2474948699503 39.98016304674198, -105.2482510874011 39.97975896003506, -105.2489968741238 39.97937488524389, -105.2496579462505 39.97902795654765, -105.2500300959376 39.9788420898406, -105.2500740536243 39.97882406757441, -105.2501190742881 39.97880796779358, -105.2501651609402 39.97879296910547, -105.2502119576847 39.97877907073762, -105.2502591032779 39.97876709330425, -105.2503069611447 39.97875594149448, -105.2503558798193 39.97874698866123, -105.2504051496909 39.97873995766609, -105.2504540584652 39.97873402466791, -105.2505029630528 39.97872891393846, -105.2506028915245 39.9787250123996, -105.2511381731693 39.97871793375031, -105.2520448639634 39.97872702547376, -105.2529308837927 39.97872892806342, -105.2534379337529 39.97873303370792, -105.2538251064159 39.97873193926058, -105.2546219021326 39.97873803075372, -105.2548084360336 39.97873894737987, -105.2556071116555 39.97874286908414, -105.2565470129442 39.97874513280774, -105.2574351597284 39.97875112306168, -105.2587978821324 39.97876194364169, -105.2601128299923 39.97876111940365, -105.2601148835307 39.97807592132791, -105.2601158412143 39.97770202615754, -105.2601159707622 39.97746209543652, -105.2601151665028 39.97708188388466, -105.2601068763516 39.97629399305483, -105.260105851442 39.97567192797527, -105.2601010269371 39.97511601350899, -105.2581178634619 39.9751069276835, -105.2574420856145 39.9750969972116, -105.2565468246362 39.97509812957833, -105.255609828812 39.97509587190684, -105.25472492212 39.97509509007728, -105.2538379091741 39.97508496345969, -105.2529390662315 39.97508990325123, -105.252047017541 39.9750910075517, -105.2507499800561 39.9750920530555, -105.2504421226539 39.97507107259827, -105.2502709701032 39.97503803420135, -105.2501091656749 39.97498607322357, -105.2500069235402 39.97494110512169, -105.249689947461 39.97478009681639, -105.2491308613379 39.9753498844948, -105.2485418287389 39.97590999502591, -105.2482839415636 39.97617407001634, -105.2482201068636 39.97626095285669, -105.2481321091086 39.9764169631363, -105.2481198770704 39.97644411369523, -105.2480588565181 39.97663806625191, -105.2480388532614 39.97683705034323, -105.245967834937 39.97683497498167, -105.2459671126042 39.97645393922107, -105.2459720164586 39.9756161130714, -105.2451691589491 39.97561900799606, -105.2446071695026 39.97561803880048, -105.2440379798706 39.97563407057132, -105.2425921489947 39.97563194856655, -105.2424318460008 39.9756560225469, -105.242267879168 39.97570507050918, -105.2420848579998 39.97579195809596, -105.2419621656047 39.97587211837142, -105.2417741744749 39.9756691010777, -105.2415438868199 39.97542288863698, -105.2415029964935 39.97538491354085, -105.2414428800109 39.97533591360214, -105.2413428299869 39.97527886402315, -105.241233839971 39.97522700908468, -105.2411971215205 39.97531202783664, -105.2411318317776 39.97540412010915, -105.2410670165164 39.97546491831289, -105.2409581733426 39.97556212833344, -105.2409141414532 39.97559991366145, -105.2414479703547 39.97615811412556, -105.2428560147591 39.97766810735965, -105.245800143718 39.98094801864188))</t>
         </is>
       </c>
-      <c r="H175" t="inlineStr">
-        <is>
-          <t>Southern Hills MS</t>
-        </is>
-      </c>
+      <c r="H175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -7821,7 +7777,7 @@
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -7863,7 +7819,7 @@
       </c>
       <c r="H177" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -7905,7 +7861,7 @@
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -8157,7 +8113,7 @@
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>Fairview HS</t>
         </is>
       </c>
     </row>
@@ -8578,6 +8534,160 @@
       <c r="H194" t="inlineStr">
         <is>
           <t>Lyons Middle Senior</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr"/>
+      <c r="B195" t="inlineStr"/>
+      <c r="C195" t="inlineStr"/>
+      <c r="D195" t="inlineStr"/>
+      <c r="E195" t="inlineStr"/>
+      <c r="F195" t="inlineStr"/>
+      <c r="G195" t="inlineStr"/>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>Casey MS</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr"/>
+      <c r="B196" t="inlineStr"/>
+      <c r="C196" t="inlineStr"/>
+      <c r="D196" t="inlineStr"/>
+      <c r="E196" t="inlineStr"/>
+      <c r="F196" t="inlineStr"/>
+      <c r="G196" t="inlineStr"/>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>Centennial MS</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr"/>
+      <c r="B197" t="inlineStr"/>
+      <c r="C197" t="inlineStr"/>
+      <c r="D197" t="inlineStr"/>
+      <c r="E197" t="inlineStr"/>
+      <c r="F197" t="inlineStr"/>
+      <c r="G197" t="inlineStr"/>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>Fairview HS</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr"/>
+      <c r="B198" t="inlineStr"/>
+      <c r="C198" t="inlineStr"/>
+      <c r="D198" t="inlineStr"/>
+      <c r="E198" t="inlineStr"/>
+      <c r="F198" t="inlineStr"/>
+      <c r="G198" t="inlineStr"/>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>Fairview HS</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr"/>
+      <c r="B199" t="inlineStr"/>
+      <c r="C199" t="inlineStr"/>
+      <c r="D199" t="inlineStr"/>
+      <c r="E199" t="inlineStr"/>
+      <c r="F199" t="inlineStr"/>
+      <c r="G199" t="inlineStr"/>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>Niwot HS</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr"/>
+      <c r="B200" t="inlineStr"/>
+      <c r="C200" t="inlineStr"/>
+      <c r="D200" t="inlineStr"/>
+      <c r="E200" t="inlineStr"/>
+      <c r="F200" t="inlineStr"/>
+      <c r="G200" t="inlineStr"/>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>Centaurus HS</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr"/>
+      <c r="B201" t="inlineStr"/>
+      <c r="C201" t="inlineStr"/>
+      <c r="D201" t="inlineStr"/>
+      <c r="E201" t="inlineStr"/>
+      <c r="F201" t="inlineStr"/>
+      <c r="G201" t="inlineStr"/>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>Centaurus HS</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr"/>
+      <c r="B202" t="inlineStr"/>
+      <c r="C202" t="inlineStr"/>
+      <c r="D202" t="inlineStr"/>
+      <c r="E202" t="inlineStr"/>
+      <c r="F202" t="inlineStr"/>
+      <c r="G202" t="inlineStr"/>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>Altona MS</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr"/>
+      <c r="B203" t="inlineStr"/>
+      <c r="C203" t="inlineStr"/>
+      <c r="D203" t="inlineStr"/>
+      <c r="E203" t="inlineStr"/>
+      <c r="F203" t="inlineStr"/>
+      <c r="G203" t="inlineStr"/>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>Longs Peak MS</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr"/>
+      <c r="B204" t="inlineStr"/>
+      <c r="C204" t="inlineStr"/>
+      <c r="D204" t="inlineStr"/>
+      <c r="E204" t="inlineStr"/>
+      <c r="F204" t="inlineStr"/>
+      <c r="G204" t="inlineStr"/>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>Timberline K-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr"/>
+      <c r="B205" t="inlineStr"/>
+      <c r="C205" t="inlineStr"/>
+      <c r="D205" t="inlineStr"/>
+      <c r="E205" t="inlineStr"/>
+      <c r="F205" t="inlineStr"/>
+      <c r="G205" t="inlineStr"/>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>Louisville MS</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Upgrade Conda env for Geopandas to Conda Forge - upgrades to Python 3.12 - upgrades many packages
</commit_message>
<xml_diff>
--- a/data/pct_supersite.xlsx
+++ b/data/pct_supersite.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H205"/>
+  <dimension ref="A1:H194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,7 +508,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0551857428336 40.19115277071814, -105.0551776917097 40.19522915038146, -105.0551776862514 40.19523231880929, -105.0551753942906 40.19639223054278, -105.0551753876223 40.19639540436918, -105.0551741138158 40.19735908950151, -105.0551741094728 40.19736226693898, -105.0551708746955 40.19981423720408, -105.0551708702638 40.19981742814952, -105.0551698743182 40.20057201079945, -105.055169869857 40.20057520624766, -105.0551698371555 40.20059995386577, -105.0551687234147 40.20144399367533, -105.0551673600189 40.20247699891858, -105.055166559143 40.20308397822347, -105.0551659441694 40.2035505108879, -105.055165939419 40.20355375046467, -105.0551658011341 40.20366106365725, -105.0551657962894 40.20366431764384, -105.0551658037605 40.20367628174822, -105.0551658058408 40.20367704099404, -105.0551658094086 40.20367990683798, -105.0551933208667 40.20367993430043, -105.0557612194496 40.20367601713887, -105.0557639998678 40.20367599809817, -105.056911999972 40.20367299893432, -105.058538999233 40.20362899881254, -105.0594407995711 40.20360935166872, -105.0594569996611 40.2036089990881, -105.0594589803057 40.20360895889921, -105.0604691803914 40.20358828730515, -105.0604691803505 40.2035581312503, -105.0604696887987 40.20325998334323, -105.0604711807169 40.20272847758034, -105.0604371797873 40.20261947653857, -105.0602041798525 40.20216247700513, -105.0599701793699 40.20216547762988, -105.059968926204 40.2014763253382, -105.059967664644 40.20078266614567, -105.0599659789192 40.19985581559262, -105.0599654497826 40.19956479210923, -105.0599628313483 40.19812507551509, -105.0599607462004 40.19697811055131, -105.0599531783856 40.19487547541794, -105.0593451786143 40.19487747591219, -105.0593371782352 40.19309847586848, -105.0599451784452 40.19310447585676, -105.0599381776194 40.19154047538977, -105.0576711777204 40.19105147542044, -105.0552111773586 40.19115247588264, -105.0551857428336 40.19115277071814))</t>
+          <t>POLYGON ((-105.05518574283364 40.19115277071814, -105.05517769170969 40.195229150381465, -105.0551776862514 40.19523231880929, -105.05517539429064 40.196392230542784, -105.05517538762234 40.196395404369184, -105.05517411381584 40.19735908950151, -105.05517410947282 40.19736226693898, -105.05517087469549 40.19981423720408, -105.05517087026377 40.19981742814952, -105.05516987431824 40.200572010799455, -105.05516986985695 40.200575206247656, -105.0551698371555 40.20059995386577, -105.05516872341471 40.201443993675326, -105.0551673600189 40.20247699891858, -105.05516655914298 40.20308397822347, -105.05516594416939 40.2035505108879, -105.05516593941897 40.20355375046467, -105.05516580113411 40.20366106365725, -105.05516579628939 40.20366431764384, -105.05516580376054 40.203676281748216, -105.05516580584083 40.20367704099404, -105.0551658094086 40.203679906837976, -105.05519332086666 40.20367993430043, -105.05576121944962 40.20367601713887, -105.05576399986776 40.20367599809817, -105.05691199997196 40.203672998934316, -105.05853899923298 40.20362899881254, -105.05944079957108 40.20360935166872, -105.05945699966105 40.2036089990881, -105.05945898030575 40.20360895889921, -105.06046918039142 40.20358828730515, -105.06046918035045 40.2035581312503, -105.06046968879875 40.20325998334323, -105.06047118071693 40.20272847758034, -105.0604371797873 40.202619476538565, -105.06020417985249 40.20216247700513, -105.05997017936994 40.202165477629876, -105.05996892620396 40.2014763253382, -105.05996766464402 40.20078266614567, -105.05996597891917 40.19985581559262, -105.05996544978255 40.19956479210923, -105.05996283134832 40.19812507551509, -105.05996074620042 40.19697811055131, -105.05995317838557 40.19487547541794, -105.0593451786143 40.194877475912186, -105.05933717823515 40.19309847586848, -105.05994517844516 40.19310447585676, -105.05993817761936 40.19154047538977, -105.05767117772044 40.19105147542044, -105.05521117735856 40.19115247588264, -105.05518574283364 40.19115277071814))</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -550,7 +550,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1691971726547 39.92869943197082, -105.1720714920114 39.92870144219746, -105.1754132357649 39.92870368835112, -105.1754136393685 39.92870368858787, -105.1784019212843 39.92870168376908, -105.1818511117197 39.92869648384348, -105.1838441764116 39.92869343178848, -105.1841991763519 39.92873643054561, -105.1843711756133 39.92868243090511, -105.1846711757492 39.92865043161049, -105.1848971762652 39.92868243096175, -105.1851551757211 39.92870443083596, -105.1853591757001 39.92871443082796, -105.185584175611 39.92863943112477, -105.1857881765031 39.92869343037078, -105.1860781767717 39.92871443107489, -105.1862427122102 39.92871305375947, -105.1874398749427 39.92870302575108, -105.188280750955 39.92869597460466, -105.1891882146993 39.92868835848437, -105.1900135071195 39.92868142556227, -105.1912021775201 39.92867143016532, -105.1921605878346 39.92866908889513, -105.1952731788288 39.9286614295662, -105.1953454862046 39.92714404290943, -105.1954277266185 39.92535293082255, -105.1954701680578 39.92442856826072, -105.1954828953945 39.92415135493398, -105.1955126848871 39.9235025188834, -105.1955539541311 39.92260363188283, -105.1955832718303 39.92176253388807, -105.1956074363542 39.92104863795893, -105.1956271775804 39.92046542890528, -105.1956491770346 39.92026642822356, -105.1957021779222 39.92016442965017, -105.1958741782275 39.91996042930643, -105.1960031773458 39.91985842861604, -105.1960461779453 39.91979442941913, -105.1963542841982 39.91947358440687, -105.1969171547176 39.91888743134161, -105.1971382584971 39.91865717884937, -105.1975931774295 39.91818342841723, -105.1977971773725 39.91800542846681, -105.1980761776685 39.9178604287125, -105.1988809443973 39.91750583145522, -105.199981771958 39.9170207684681, -105.2005472795797 39.91677157902036, -105.2013773094024 39.91640582131284, -105.2019980528428 39.91613227988852, -105.2026927027816 39.91582616438962, -105.2029610455153 39.91570919533338, -105.2032861789647 39.91558342752357, -105.2034951787843 39.91545442818257, -105.2036994329652 39.91536577400033, -105.2039238798093 39.91526835479848, -105.2044351788381 39.9150464284585, -105.2046181793619 39.91493942746109, -105.2047771484222 39.9148745542603, -105.2051264319463 39.91473201341331, -105.2055840142236 39.91454527467528, -105.206223179592 39.91428442723124, -105.2062611795562 39.91424142750945, -105.2062749820281 39.91414793981343, -105.2032744790532 39.91416684927634, -105.2006351177575 39.91416696934041, -105.1991893697619 39.91416701068361, -105.1985745597549 39.91416702150446, -105.1971047644128 39.91416703407202, -105.1953160550247 39.91416702303262, -105.1938763305775 39.91416699469512, -105.1933546555779 39.91416710270681, -105.1926978672329 39.91416724236024, -105.1921136011874 39.91416735873496, -105.1907538888507 39.91416762414558, -105.184478826679 39.91416864003449, -105.183940205586 39.91416757726816, -105.1797462276226 39.91415918540865, -105.1750099583544 39.91414955744559, -105.1703876457997 39.91414592693626, -105.1698987794962 39.91414553623513, -105.1672381230998 39.91414337611825, -105.1667719578876 39.91414299090538, -105.1660586296656 39.91414239888842, -105.1660551691404 39.91414543039225, -105.1667811694029 39.91414643017314, -105.1664291702388 39.91446243005227, -105.166191382003 39.91467703189569, -105.165771169777 39.91505643053332, -105.1655443536664 39.91525113571893, -105.1654411081812 39.91533976457623, -105.1653261706187 39.91543843057572, -105.1652391701635 39.91551743064041, -105.1651911705359 39.91556343026098, -105.1651441694907 39.91561043069991, -105.1650981707705 39.91565743043201, -105.1650101693641 39.91575343103027, -105.1649671701462 39.91580243080151, -105.1648851691561 39.91590143085672, -105.1648461695037 39.91595242998492, -105.1647701698895 39.91605543015623, -105.1647351700435 39.91610742981835, -105.1647001699047 39.91616043100622, -105.1646341694698 39.91626743032371, -105.1646031703354 39.91632143116104, -105.1645731700432 39.91637543129664, -105.1645451695898 39.91643043068115, -105.1644911707665 39.91654143049509, -105.164466170124 39.91659743022988, -105.1644431695573 39.91665343128377, -105.1644201698922 39.91671043117081, -105.1644039955596 39.91676568834629, -105.1643791695969 39.91682443108952, -105.1643431692571 39.91693943089195, -105.1643181695924 39.91703943068446, -105.1643011700438 39.91711143056493, -105.1642831691156 39.91720843082771, -105.1642691698713 39.9172944312483, -105.164252170015 39.91746043060891, -105.1642461697306 39.91757743084622, -105.1642451696164 39.91763643035888, -105.1642451698137 39.9176944303499, -105.1642424012036 39.91775341659991, -105.1642501701213 39.91781243087021, -105.1642551707236 39.91787043012771, -105.1642601699189 39.91792943091778, -105.1642761702455 39.91804643044339, -105.1642884593234 39.91812177339535, -105.164296170029 39.91816243017999, -105.1643053411744 39.91820675962112, -105.1643221692171 39.9182784311875, -105.1643371707714 39.91833643166945, -105.164353170338 39.91839343171948, -105.1643861694348 39.91849843079937, -105.1643321704804 39.91850343061419, -105.1643381704867 39.9185204310016, -105.164309169988 39.91852643134861, -105.1643624542901 39.91869085135099, -105.1645974878803 39.9194160806231, -105.1647712351076 39.91995219355358, -105.1648787705816 39.92028399905023, -105.1649289453365 39.92043881225101, -105.1650144136964 39.92070252454433, -105.16518049081 39.92121495046698, -105.1652441708609 39.9214114314059, -105.1653237098382 39.92165438665059, -105.1653951749806 39.92187267534758, -105.1654869016675 39.92215285243409, -105.1655303409743 39.92228553721576, -105.1656411242788 39.92262398563496, -105.1657268548612 39.92288591118818, -105.1657275634698 39.92230633689709, -105.1657281978904 39.9217877867605, -105.1664399270526 39.92147694665487, -105.1664402288849 39.92140295359366, -105.1664467117113 39.91980299921306, -105.166447182215 39.91968681418613, -105.1657361994478 39.91968510580809, -105.1657362185154 39.91968073314587, -105.1657441987671 39.91786472559452, -105.1658011410363 39.91786477827342, -105.1703991191808 39.91786890709702, -105.1723779797716 39.91787062869179, -105.1727429112322 39.91787094127734, -105.1747177665097 39.91787271395971, -105.1750614612326 39.91787301775404, -105.175109560094 39.92148483573595, -105.1751139608899 39.92179674478729, -105.1751604661924 39.92509409736032, -105.1720534350199 39.92507720338283, -105.1720532452068 39.92516347726848, -105.1714361169425 39.92559896103811, -105.1709545337192 39.92602504583957, -105.1704456617958 39.92612806410983, -105.1691867517787 39.92638291988158, -105.1691855501184 39.92670357827446, -105.1691857771099 39.92718979236645, -105.1691864470017 39.92863672319584, -105.169197172132 39.92863411235809, -105.1691971726547 39.92869943197082))</t>
+          <t>POLYGON ((-105.16919717265475 39.92869943197082, -105.17207149201138 39.92870144219746, -105.17541323576492 39.92870368835112, -105.17541363936846 39.928703688587866, -105.17840192128428 39.928701683769084, -105.1818511117197 39.92869648384348, -105.18384417641157 39.92869343178848, -105.18419917635188 39.92873643054561, -105.18437117561326 39.928682430905106, -105.18467117574924 39.92865043161049, -105.18489717626518 39.92868243096175, -105.18515517572106 39.928704430835964, -105.18535917570011 39.92871443082796, -105.18558417561098 39.92863943112477, -105.1857881765031 39.92869343037078, -105.18607817677173 39.92871443107489, -105.18624271221022 39.92871305375947, -105.18743987494265 39.928703025751076, -105.18828075095502 39.92869597460466, -105.18918821469929 39.928688358484365, -105.19001350711949 39.92868142556227, -105.1912021775201 39.928671430165316, -105.19216058783456 39.928669088895134, -105.1952731788288 39.9286614295662, -105.1953454862046 39.92714404290943, -105.19542772661853 39.92535293082255, -105.19547016805777 39.92442856826072, -105.19548289539446 39.92415135493398, -105.19551268488709 39.923502518883396, -105.19555395413113 39.92260363188283, -105.19558327183032 39.92176253388807, -105.19560743635417 39.921048637958926, -105.19562717758036 39.92046542890528, -105.19564917703458 39.92026642822356, -105.19570217792217 39.92016442965017, -105.19587417822746 39.91996042930643, -105.19600317734584 39.91985842861604, -105.1960461779453 39.919794429419134, -105.19635428419821 39.919473584406866, -105.19691715471758 39.91888743134161, -105.19713825849709 39.91865717884937, -105.19759317742951 39.91818342841723, -105.1977971773725 39.91800542846681, -105.19807617766847 39.9178604287125, -105.1988809443973 39.917505831455216, -105.19998177195798 39.9170207684681, -105.20054727957974 39.91677157902036, -105.20137730940245 39.916405821312836, -105.2019980528428 39.916132279888515, -105.20269270278163 39.91582616438962, -105.20296104551534 39.915709195333385, -105.20328617896469 39.91558342752357, -105.20349517878434 39.91545442818257, -105.20369943296522 39.91536577400033, -105.20392387980932 39.91526835479848, -105.20443517883814 39.9150464284585, -105.2046181793619 39.914939427461086, -105.20477714842221 39.9148745542603, -105.20512643194631 39.91473201341331, -105.20558401422359 39.914545274675284, -105.20622317959203 39.914284427231244, -105.20626117955617 39.914241427509445, -105.20627498202815 39.914147939813425, -105.20327447905323 39.91416684927634, -105.20063511775746 39.91416696934041, -105.19918936976191 39.914167010683606, -105.19857455975492 39.91416702150446, -105.19710476441277 39.91416703407202, -105.19531605502466 39.91416702303262, -105.19387633057747 39.91416699469512, -105.19335465557788 39.91416710270681, -105.19269786723292 39.914167242360236, -105.19211360118737 39.91416735873496, -105.19075388885071 39.91416762414558, -105.18447882667904 39.91416864003449, -105.18394020558601 39.91416757726816, -105.17974622762259 39.91415918540865, -105.17500995835444 39.91414955744559, -105.1703876457997 39.91414592693626, -105.16989877949622 39.914145536235125, -105.16723812309985 39.91414337611825, -105.1667719578876 39.914142990905376, -105.16605862966559 39.91414239888842, -105.16605516914044 39.914145430392246, -105.16678116940285 39.91414643017314, -105.16642917023879 39.91446243005227, -105.166191382003 39.91467703189569, -105.16577116977697 39.91505643053332, -105.16554435366639 39.915251135718925, -105.16544110818116 39.91533976457623, -105.16532617061874 39.91543843057572, -105.16523917016352 39.91551743064041, -105.16519117053592 39.91556343026098, -105.16514416949074 39.915610430699914, -105.16509817077055 39.91565743043201, -105.1650101693641 39.91575343103027, -105.16496717014616 39.915802430801506, -105.16488516915607 39.91590143085672, -105.16484616950375 39.91595242998492, -105.16477016988952 39.916055430156234, -105.16473517004353 39.916107429818354, -105.16470016990468 39.91616043100622, -105.1646341694698 39.916267430323714, -105.16460317033541 39.91632143116104, -105.16457317004323 39.916375431296636, -105.16454516958977 39.916430430681146, -105.16449117076647 39.916541430495094, -105.16446617012404 39.916597430229885, -105.1644431695573 39.91665343128377, -105.1644201698922 39.916710431170806, -105.16440399555958 39.91676568834629, -105.16437916959688 39.916824431089516, -105.16434316925707 39.91693943089195, -105.16431816959236 39.91703943068446, -105.16430117004379 39.91711143056493, -105.1642831691156 39.917208430827706, -105.16426916987132 39.9172944312483, -105.16425217001498 39.91746043060891, -105.1642461697306 39.91757743084622, -105.16424516961645 39.917636430358876, -105.16424516981368 39.9176944303499, -105.16424240120362 39.91775341659991, -105.16425017012135 39.91781243087021, -105.16425517072365 39.917870430127714, -105.16426016991892 39.91792943091778, -105.16427617024551 39.91804643044339, -105.16428845932342 39.91812177339535, -105.16429617002902 39.91816243017999, -105.16430534117443 39.91820675962112, -105.16432216921706 39.918278431187495, -105.16433717077138 39.91833643166945, -105.16435317033803 39.91839343171948, -105.16438616943478 39.918498430799374, -105.1643321704804 39.918503430614194, -105.16433817048674 39.918520431001596, -105.16430916998797 39.91852643134861, -105.16436245429009 39.91869085135099, -105.16459748788026 39.9194160806231, -105.1647712351076 39.919952193553584, -105.16487877058155 39.920283999050234, -105.16492894533647 39.920438812251014, -105.16501441369637 39.92070252454433, -105.16518049080997 39.92121495046698, -105.16524417086094 39.9214114314059, -105.16532370983818 39.92165438665059, -105.16539517498063 39.92187267534758, -105.16548690166752 39.92215285243409, -105.16553034097433 39.922285537215764, -105.16564112427876 39.92262398563496, -105.16572685486118 39.92288591118818, -105.16572756346983 39.922306336897094, -105.16572819789037 39.9217877867605, -105.16643992705262 39.92147694665487, -105.16644022888494 39.921402953593656, -105.1664467117113 39.91980299921306, -105.16644718221501 39.91968681418613, -105.16573619944784 39.91968510580809, -105.16573621851538 39.919680733145874, -105.16574419876713 39.91786472559452, -105.16580114103631 39.91786477827342, -105.17039911918077 39.917868907097024, -105.17237797977157 39.91787062869179, -105.17274291123223 39.91787094127734, -105.17471776650967 39.91787271395971, -105.17506146123259 39.91787301775404, -105.17510956009404 39.92148483573595, -105.17511396088993 39.92179674478729, -105.1751604661924 39.925094097360315, -105.17205343501988 39.92507720338283, -105.17205324520683 39.92516347726848, -105.17143611694254 39.92559896103811, -105.17095453371917 39.92602504583957, -105.17044566179578 39.926128064109825, -105.16918675177874 39.926382919881576, -105.16918555011837 39.926703578274456, -105.1691857771099 39.92718979236645, -105.16918644700166 39.92863672319584, -105.16919717213199 39.92863411235809, -105.16919717265475 39.92869943197082))</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -592,7 +592,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1846878292357 39.9626284939408, -105.1845921801246 39.96264443594031, -105.1842001793857 39.96258943629537, -105.1841021800759 39.96259043491916, -105.183756179454 39.96352043583736, -105.184684179543 39.96329443567719, -105.1846878292357 39.9626284939408))</t>
+          <t>POLYGON ((-105.18468782923568 39.9626284939408, -105.18459218012461 39.962644435940305, -105.18420017938566 39.962589436295374, -105.18410218007588 39.96259043491916, -105.18375617945398 39.96352043583736, -105.18468417954304 39.96329443567719, -105.18468782923568 39.9626284939408))</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -634,7 +634,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1543926683685 39.92920502459549, -105.1584225394937 39.92924921683296, -105.1592581712754 39.92926956379147, -105.159808177506 39.92926407705372, -105.1601519120273 39.92923292102617, -105.1604121448398 39.92918722070032, -105.1607375215015 39.9291131147585, -105.1611512880181 39.92900352248355, -105.1615000714133 39.92889016393721, -105.161753602932 39.92883367977832, -105.1621020483118 39.92878823466037, -105.1625711373537 39.9287574391029, -105.1635322820768 39.92874595284867, -105.1642865869104 39.92873746663779, -105.1657570205717 39.92871886091139, -105.1658309152665 39.92871792608083, -105.1662548834643 39.92871805655115, -105.1662549969533 39.928718054178, -105.1662549995615 39.92871799924519, -105.1666546602336 39.92871548911919, -105.1674080147692 39.92870738861864, -105.1684020970337 39.92870328012041, -105.1689792892025 39.92870089102008, -105.1691971726547 39.92869943197082, -105.1691864470017 39.92863672319584, -105.1691857771099 39.92718979236645, -105.1691855501184 39.92670357827446, -105.1691867517787 39.92638291988158, -105.1704456617958 39.92612806410983, -105.1709545337192 39.92602504583957, -105.1714361169425 39.92559896103811, -105.1720532452068 39.92516347726848, -105.1720534350199 39.92507720338283, -105.1751604661924 39.92509409736032, -105.1751139608899 39.92179674478729, -105.175109560094 39.92148483573595, -105.1750614612326 39.91787301775404, -105.1747177665097 39.91787271395971, -105.1727429112322 39.91787094127734, -105.1723779797716 39.91787062869179, -105.1703991191808 39.91786890709702, -105.1658011410363 39.91786477827342, -105.1657441987671 39.91786472559452, -105.1657362185154 39.91968073314587, -105.1657361994478 39.91968510580809, -105.166447182215 39.91968681418613, -105.1664467117113 39.91980299921306, -105.1664402288849 39.92140295359366, -105.1664399270526 39.92147694665487, -105.1657281978904 39.9217877867605, -105.1657275634698 39.92230633689709, -105.1657268548612 39.92288591118818, -105.1656411242788 39.92262398563496, -105.1655561676404 39.92236443280233, -105.1655303409743 39.92228553721576, -105.1654869016675 39.92215285243409, -105.1653951749806 39.92187267534758, -105.1653237110079 39.92165438665396, -105.1652441708609 39.9214114314059, -105.16518049081 39.92121495046698, -105.1650144136964 39.92070252454433, -105.1649289453365 39.92043881225101, -105.1648787705816 39.92028399905023, -105.1647712351076 39.91995219355358, -105.1645974878803 39.9194160806231, -105.1643624542901 39.91869085135099, -105.164309169988 39.91852643134861, -105.1643381704867 39.9185204310016, -105.1643321704804 39.91850343061419, -105.1643861694348 39.91849843079937, -105.164353170338 39.91839343171948, -105.1643371707714 39.91833643166945, -105.1643221692171 39.9182784311875, -105.1643053411744 39.91820675962112, -105.164296170029 39.91816243017999, -105.1642884593234 39.91812177339535, -105.1642761702455 39.91804643044339, -105.1642601699189 39.91792943091778, -105.1642551707236 39.91787043012771, -105.1642501701213 39.91781243087021, -105.1642424012036 39.91775341659991, -105.1642451698137 39.9176944303499, -105.1642451696164 39.91763643035888, -105.1642461697306 39.91757743084622, -105.164252170015 39.91746043060891, -105.1642691698713 39.9172944312483, -105.1642831691156 39.91720843082771, -105.1643011700438 39.91711143056493, -105.1643181695924 39.91703943068446, -105.1643431692571 39.91693943089195, -105.1643791695969 39.91682443108952, -105.1644039955596 39.91676568834629, -105.1644201698922 39.91671043117081, -105.1644431695573 39.91665343128377, -105.164466170124 39.91659743022988, -105.1644911707665 39.91654143049509, -105.1645451695898 39.91643043068115, -105.1645731700432 39.91637543129664, -105.1646031703354 39.91632143116104, -105.1646341694698 39.91626743032371, -105.1647001699047 39.91616043100622, -105.1647351700435 39.91610742981835, -105.1647701698895 39.91605543015623, -105.1648461695037 39.91595242998492, -105.1648851691561 39.91590143085672, -105.1649671701462 39.91580243080151, -105.1650101693641 39.91575343103027, -105.1650981707705 39.91565743043201, -105.1651441694907 39.91561043069991, -105.1651911705359 39.91556343026098, -105.1652391701635 39.91551743064041, -105.1653261706187 39.91543843057572, -105.1654411093463 39.91533976548027, -105.1655443548316 39.91525113662293, -105.165771169777 39.91505643053332, -105.166191382003 39.91467703189569, -105.1664291702388 39.91446243005227, -105.1667811694029 39.91414643017314, -105.1660551691404 39.91414543039225, -105.1660586296656 39.91414239888842, -105.1660433311038 39.91414238604561, -105.1660414667389 39.91414238424149, -105.1660335028282 39.91414237825769, -105.1657674166974 39.91414214035058, -105.1656197775234 39.91414007793439, -105.1653843869967 39.91413671650596, -105.1597894853714 39.91405668205347, -105.1597872521927 39.91406027900977, -105.1595944786778 39.91437078041713, -105.1596578648334 39.91446825382197, -105.1596293633845 39.91449664855583, -105.1596237810907 39.91450221346633, -105.1595164293762 39.91460915970136, -105.1593720303506 39.91474801753947, -105.159224524582 39.91488492237188, -105.1590739649175 39.91501983021065, -105.1589203925095 39.91515269703326, -105.1587638578233 39.91528348785139, -105.1586044078573 39.9154121595606, -105.158442087245 39.91553867445327, -105.1581913877433 39.91572520461699, -105.1581090454066 39.91578507585127, -105.1579384216276 39.91590488966813, -105.1577651350117 39.91602239142268, -105.1575892371669 39.91613755333574, -105.1572338884087 39.91636116034464, -105.1575302839714 39.91655621347035, -105.1577746378509 39.91671702287918, -105.1579275072425 39.91681762361618, -105.1581491025685 39.91696344873351, -105.1583274686104 39.91708082921885, -105.1585666038691 39.91723878705952, -105.1603055531215 39.91837485627751, -105.1600253028527 39.91870189133563, -105.1598269566003 39.91901895595584, -105.1595950980057 39.91949992110294, -105.1594397843317 39.92000938757063, -105.1593531241248 39.92051422485057, -105.1593363328675 39.92097861282231, -105.159392660749 39.92127867495055, -105.1594518515067 39.92151119309244, -105.1595331459662 39.92176394508856, -105.1595441708892 39.9218411185521, -105.159549137059 39.92213212748413, -105.1595000443468 39.92239607289664, -105.1593928517688 39.92272792847135, -105.1593489329071 39.92295510244214, -105.1593240716457 39.92314994043188, -105.1593181288922 39.92341209226864, -105.1593410913043 39.92366911296291, -105.1593930067307 39.92391194467338, -105.1594896552691 39.92417074226947, -105.1593649354347 39.92420125178063, -105.1583669577626 39.92438215168665, -105.1553914786326 39.92587910701046, -105.1529676659906 39.92757344066692, -105.1528602268732 39.92765236531067, -105.152811943482 39.92759395590548, -105.1527150220277 39.92751103240507, -105.1525650276937 39.92741696785791, -105.1522728951571 39.92729694388894, -105.1518008886623 39.92713903944904, -105.1509951643673 39.926906002276, -105.1501920333945 39.92665512248843, -105.1499354224894 39.9266075614999, -105.1496798081671 39.92658790550655, -105.1494517080693 39.92659703411626, -105.1492417950238 39.92661623843878, -105.1490713052404 39.92664910577311, -105.1487484862316 39.92670132388253, -105.1485005912732 39.92674490274334, -105.1482007498478 39.92681495141585, -105.1480060316116 39.92687642658183, -105.1477736234155 39.92698659579152, -105.1476407261165 39.92707044000966, -105.1475480861019 39.92716769475399, -105.1474552458694 39.92730389707974, -105.1474091926363 39.92740354325586, -105.1473666150558 39.92750859322428, -105.1473592734381 39.92757329688838, -105.1473588973077 39.92764611433476, -105.147350596778 39.92789690372945, -105.1473353612929 39.92823691226646, -105.1473540173529 39.92881527871196, -105.1473559810769 39.92887606955925, -105.1488042084431 39.92888071244524, -105.1499603189246 39.92887708230292, -105.1502156221988 39.92888858119842, -105.1505451015723 39.92892175208359, -105.15086059695 39.92896560292694, -105.1516954582233 39.92913613299276, -105.1519553136435 39.92916551454322, -105.1522663875301 39.92916645411064, -105.1543926683685 39.92920502459549))</t>
+          <t>POLYGON ((-105.15439266836849 39.92920502459549, -105.15842253949369 39.929249216832964, -105.15925817127537 39.92926956379147, -105.15980817750602 39.929264077053716, -105.16015191202733 39.92923292102617, -105.16041214483981 39.92918722070032, -105.16073752150152 39.9291131147585, -105.16115128801812 39.92900352248355, -105.16150007141333 39.92889016393721, -105.16175360293202 39.92883367977832, -105.16210204831177 39.92878823466037, -105.16257113735374 39.928757439102895, -105.16353228207683 39.92874595284867, -105.16428658691042 39.92873746663779, -105.16575702057173 39.92871886091139, -105.16583091526645 39.92871792608083, -105.16625488346429 39.92871805655115, -105.16625499695328 39.928718054178, -105.16625499956153 39.92871799924519, -105.16665466023362 39.92871548911919, -105.16740801476922 39.92870738861864, -105.16840209703366 39.92870328012041, -105.16897928920247 39.92870089102008, -105.16919717265475 39.92869943197082, -105.16918644700166 39.92863672319584, -105.1691857771099 39.92718979236645, -105.16918555011837 39.926703578274456, -105.16918675177874 39.926382919881576, -105.17044566179578 39.926128064109825, -105.17095453371917 39.92602504583957, -105.17143611694254 39.92559896103811, -105.17205324520683 39.92516347726848, -105.17205343501988 39.92507720338283, -105.1751604661924 39.925094097360315, -105.17511396088993 39.92179674478729, -105.17510956009404 39.92148483573595, -105.17506146123259 39.91787301775404, -105.17471776650967 39.91787271395971, -105.17274291123223 39.91787094127734, -105.17237797977157 39.91787062869179, -105.17039911918077 39.917868907097024, -105.16580114103631 39.91786477827342, -105.16574419876713 39.91786472559452, -105.16573621851538 39.919680733145874, -105.16573619944784 39.91968510580809, -105.16644718221501 39.91968681418613, -105.1664467117113 39.91980299921306, -105.16644022888494 39.921402953593656, -105.16643992705262 39.92147694665487, -105.16572819789037 39.9217877867605, -105.16572756346983 39.922306336897094, -105.16572685486118 39.92288591118818, -105.16564112427876 39.92262398563496, -105.16555616764043 39.92236443280233, -105.16553034097433 39.922285537215764, -105.16548690166752 39.92215285243409, -105.16539517498063 39.92187267534758, -105.1653237110079 39.92165438665396, -105.16524417086094 39.9214114314059, -105.16518049080997 39.92121495046698, -105.16501441369637 39.92070252454433, -105.16492894533647 39.920438812251014, -105.16487877058155 39.920283999050234, -105.1647712351076 39.919952193553584, -105.16459748788026 39.9194160806231, -105.16436245429009 39.91869085135099, -105.16430916998797 39.91852643134861, -105.16433817048674 39.918520431001596, -105.1643321704804 39.918503430614194, -105.16438616943478 39.918498430799374, -105.16435317033803 39.91839343171948, -105.16433717077138 39.91833643166945, -105.16432216921706 39.918278431187495, -105.16430534117443 39.91820675962112, -105.16429617002902 39.91816243017999, -105.16428845932342 39.91812177339535, -105.16427617024551 39.91804643044339, -105.16426016991892 39.91792943091778, -105.16425517072365 39.917870430127714, -105.16425017012135 39.91781243087021, -105.16424240120362 39.91775341659991, -105.16424516981368 39.9176944303499, -105.16424516961645 39.917636430358876, -105.1642461697306 39.91757743084622, -105.16425217001498 39.91746043060891, -105.16426916987132 39.9172944312483, -105.1642831691156 39.917208430827706, -105.16430117004379 39.91711143056493, -105.16431816959236 39.91703943068446, -105.16434316925707 39.91693943089195, -105.16437916959688 39.916824431089516, -105.16440399555958 39.91676568834629, -105.1644201698922 39.916710431170806, -105.1644431695573 39.91665343128377, -105.16446617012404 39.916597430229885, -105.16449117076647 39.916541430495094, -105.16454516958977 39.916430430681146, -105.16457317004323 39.916375431296636, -105.16460317033541 39.91632143116104, -105.1646341694698 39.916267430323714, -105.16470016990468 39.91616043100622, -105.16473517004353 39.916107429818354, -105.16477016988952 39.916055430156234, -105.16484616950375 39.91595242998492, -105.16488516915607 39.91590143085672, -105.16496717014616 39.915802430801506, -105.1650101693641 39.91575343103027, -105.16509817077055 39.91565743043201, -105.16514416949074 39.915610430699914, -105.16519117053592 39.91556343026098, -105.16523917016352 39.91551743064041, -105.16532617061874 39.91543843057572, -105.16544110934635 39.91533976548027, -105.16554435483158 39.915251136622935, -105.16577116977697 39.91505643053332, -105.166191382003 39.91467703189569, -105.16642917023879 39.91446243005227, -105.16678116940285 39.91414643017314, -105.16605516914044 39.914145430392246, -105.16605862966559 39.91414239888842, -105.1660433311038 39.91414238604561, -105.16604146673893 39.914142384241494, -105.16603350282823 39.91414237825769, -105.16576741669736 39.91414214035058, -105.16561977752337 39.91414007793439, -105.16538438699666 39.914136716505965, -105.15978948537136 39.91405668205347, -105.1597872521927 39.91406027900977, -105.15959447867782 39.91437078041713, -105.15965786483343 39.91446825382197, -105.15962936338445 39.914496648555826, -105.1596237810907 39.91450221346633, -105.15951642937621 39.91460915970136, -105.1593720303506 39.91474801753947, -105.15922452458202 39.91488492237188, -105.15907396491754 39.91501983021065, -105.15892039250949 39.915152697033264, -105.15876385782332 39.91528348785139, -105.15860440785733 39.9154121595606, -105.15844208724498 39.915538674453266, -105.15819138774329 39.91572520461699, -105.1581090454066 39.91578507585127, -105.15793842162762 39.91590488966813, -105.15776513501174 39.91602239142268, -105.15758923716692 39.916137553335744, -105.15723388840868 39.91636116034464, -105.15753028397137 39.91655621347035, -105.1577746378509 39.916717022879176, -105.15792750724249 39.91681762361618, -105.1581491025685 39.91696344873351, -105.15832746861042 39.917080829218854, -105.1585666038691 39.91723878705952, -105.16030555312153 39.91837485627751, -105.16002530285272 39.91870189133563, -105.15982695660026 39.91901895595584, -105.15959509800572 39.91949992110294, -105.15943978433165 39.92000938757063, -105.15935312412476 39.92051422485057, -105.15933633286753 39.92097861282231, -105.15939266074905 39.92127867495055, -105.15945185150672 39.921511193092435, -105.1595331459662 39.921763945088564, -105.15954417088922 39.9218411185521, -105.15954913705899 39.922132127484126, -105.1595000443468 39.92239607289664, -105.15939285176877 39.92272792847135, -105.1593489329071 39.92295510244214, -105.15932407164566 39.92314994043188, -105.15931812889222 39.92341209226864, -105.15934109130431 39.92366911296291, -105.15939300673071 39.92391194467338, -105.15948965526913 39.92417074226947, -105.15936493543467 39.92420125178063, -105.15836695776257 39.92438215168665, -105.15539147863262 39.92587910701046, -105.15296766599057 39.92757344066692, -105.1528602268732 39.92765236531067, -105.15281194348198 39.92759395590548, -105.15271502202766 39.92751103240507, -105.15256502769371 39.92741696785791, -105.15227289515714 39.92729694388894, -105.15180088866228 39.92713903944904, -105.15099516436734 39.926906002276, -105.15019203339449 39.92665512248843, -105.14993542248942 39.9266075614999, -105.14967980816715 39.92658790550655, -105.14945170806935 39.92659703411626, -105.14924179502383 39.926616238438775, -105.14907130524044 39.92664910577311, -105.14874848623158 39.92670132388253, -105.14850059127323 39.92674490274334, -105.14820074984783 39.92681495141585, -105.14800603161157 39.92687642658183, -105.14777362341553 39.92698659579152, -105.14764072611653 39.92707044000966, -105.1475480861019 39.92716769475399, -105.14745524586935 39.92730389707974, -105.1474091926363 39.927403543255856, -105.14736661505584 39.92750859322428, -105.14735927343807 39.92757329688838, -105.14735889730771 39.92764611433476, -105.14735059677795 39.92789690372945, -105.14733536129295 39.928236912266456, -105.1473540173529 39.92881527871196, -105.14735598107694 39.92887606955925, -105.14880420844312 39.92888071244524, -105.14996031892461 39.92887708230292, -105.15021562219884 39.92888858119842, -105.15054510157229 39.92892175208359, -105.15086059694998 39.92896560292694, -105.15169545822333 39.92913613299276, -105.15195531364348 39.92916551454322, -105.15226638753013 39.92916645411064, -105.15439266836849 39.92920502459549))</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1470184689167 39.92887114754381, -105.1473559810769 39.92887606955925, -105.1473540173529 39.92881527871196, -105.1473353612929 39.92823691226646, -105.147350596778 39.92789690372945, -105.1473588973077 39.92764611433476, -105.1473592734381 39.92757329688838, -105.1473666150558 39.92750859322428, -105.1474091926363 39.92740354325586, -105.1474552458694 39.92730389707974, -105.1475480861019 39.92716769475399, -105.1476407261165 39.92707044000966, -105.1477736234155 39.92698659579152, -105.1480060316116 39.92687642658183, -105.1482007498478 39.92681495141585, -105.1485005912732 39.92674490274334, -105.1487484862316 39.92670132388253, -105.1490713052404 39.92664910577311, -105.1492417950238 39.92661623843878, -105.1494517080693 39.92659703411626, -105.1496798081671 39.92658790550655, -105.1499354224894 39.9266075614999, -105.1501920333945 39.92665512248843, -105.1509951643673 39.926906002276, -105.1518008886623 39.92713903944904, -105.1522728951571 39.92729694388894, -105.1525650276937 39.92741696785791, -105.1527150220277 39.92751103240507, -105.152811943482 39.92759395590548, -105.1528602268732 39.92765236531067, -105.1529676659906 39.92757344066692, -105.1553914786326 39.92587910701046, -105.1583669577626 39.92438215168665, -105.1593649354347 39.92420125178063, -105.1594896552691 39.92417074226947, -105.1593930067307 39.92391194467338, -105.1593410913043 39.92366911296291, -105.1593181288922 39.92341209226864, -105.1593240716457 39.92314994043188, -105.1593489329071 39.92295510244214, -105.1593928517688 39.92272792847135, -105.1595000443468 39.92239607289664, -105.159549137059 39.92213212748413, -105.1595441708892 39.9218411185521, -105.1595331459662 39.92176394508856, -105.1594518515067 39.92151119309244, -105.159392660749 39.92127867495055, -105.1593363328675 39.92097861282231, -105.1593531241248 39.92051422485057, -105.1594397843317 39.92000938757063, -105.1595950980057 39.91949992110294, -105.1598269566003 39.91901895595584, -105.1600253028527 39.91870189133563, -105.1603055531215 39.91837485627751, -105.1585666038691 39.91723878705952, -105.1583274686104 39.91708082921885, -105.1581491025685 39.91696344873351, -105.1579275072425 39.91681762361618, -105.1577746378509 39.91671702287918, -105.1575302839714 39.91655621347035, -105.1572338884087 39.91636116034464, -105.1575892371669 39.91613755333574, -105.1577651350117 39.91602239142268, -105.1579384216276 39.91590488966813, -105.1581090454066 39.91578507585127, -105.1581913877433 39.91572520461699, -105.158442087245 39.91553867445327, -105.1586044078573 39.9154121595606, -105.1587638578233 39.91528348785139, -105.1589203925095 39.91515269703326, -105.1590739649175 39.91501983021065, -105.159224524582 39.91488492237188, -105.1593720303506 39.91474801753947, -105.1595164293762 39.91460915970136, -105.1596237810907 39.91450221346633, -105.1596293633845 39.91449664855583, -105.1596578648334 39.91446825382197, -105.1595944786778 39.91437078041713, -105.1597894853714 39.91405668205347, -105.156420131756 39.91405356845262, -105.1560293437166 39.91405351953847, -105.1550121913589 39.91405339401757, -105.1532334610398 39.91405315098152, -105.1511818705786 39.9140528369392, -105.147676653323 39.91405221810871, -105.1473391472332 39.91405215140002, -105.1471032891195 39.91405210433869, -105.1470531994023 39.91775944655548, -105.1470470425149 39.92145044388781, -105.147046321183 39.92186965993315, -105.147038645905 39.92502944310596, -105.1470393599495 39.92524137222502, -105.1470244855684 39.92746831055086, -105.1470238512916 39.92761587682738, -105.1470188937999 39.92877200297731, -105.1470187184292 39.92881293486509, -105.1470184689167 39.92887114754381))</t>
+          <t>POLYGON ((-105.14701846891668 39.92887114754381, -105.14735598107694 39.92887606955925, -105.1473540173529 39.92881527871196, -105.14733536129295 39.928236912266456, -105.14735059677795 39.92789690372945, -105.14735889730771 39.92764611433476, -105.14735927343807 39.92757329688838, -105.14736661505584 39.92750859322428, -105.1474091926363 39.927403543255856, -105.14745524586935 39.92730389707974, -105.1475480861019 39.92716769475399, -105.14764072611653 39.92707044000966, -105.14777362341553 39.92698659579152, -105.14800603161157 39.92687642658183, -105.14820074984783 39.92681495141585, -105.14850059127323 39.92674490274334, -105.14874848623158 39.92670132388253, -105.14907130524044 39.92664910577311, -105.14924179502383 39.926616238438775, -105.14945170806935 39.92659703411626, -105.14967980816715 39.92658790550655, -105.14993542248942 39.9266075614999, -105.15019203339449 39.92665512248843, -105.15099516436734 39.926906002276, -105.15180088866228 39.92713903944904, -105.15227289515714 39.92729694388894, -105.15256502769371 39.92741696785791, -105.15271502202766 39.92751103240507, -105.15281194348198 39.92759395590548, -105.1528602268732 39.92765236531067, -105.15296766599057 39.92757344066692, -105.15539147863262 39.92587910701046, -105.15836695776257 39.92438215168665, -105.15936493543467 39.92420125178063, -105.15948965526913 39.92417074226947, -105.15939300673071 39.92391194467338, -105.15934109130431 39.92366911296291, -105.15931812889222 39.92341209226864, -105.15932407164566 39.92314994043188, -105.1593489329071 39.92295510244214, -105.15939285176877 39.92272792847135, -105.1595000443468 39.92239607289664, -105.15954913705899 39.922132127484126, -105.15954417088922 39.9218411185521, -105.1595331459662 39.921763945088564, -105.15945185150672 39.921511193092435, -105.15939266074905 39.92127867495055, -105.15933633286753 39.92097861282231, -105.15935312412476 39.92051422485057, -105.15943978433165 39.92000938757063, -105.15959509800572 39.91949992110294, -105.15982695660026 39.91901895595584, -105.16002530285272 39.91870189133563, -105.16030555312153 39.91837485627751, -105.1585666038691 39.91723878705952, -105.15832746861042 39.917080829218854, -105.1581491025685 39.91696344873351, -105.15792750724249 39.91681762361618, -105.1577746378509 39.916717022879176, -105.15753028397137 39.91655621347035, -105.15723388840868 39.91636116034464, -105.15758923716692 39.916137553335744, -105.15776513501174 39.91602239142268, -105.15793842162762 39.91590488966813, -105.1581090454066 39.91578507585127, -105.15819138774329 39.91572520461699, -105.15844208724498 39.915538674453266, -105.15860440785733 39.9154121595606, -105.15876385782332 39.91528348785139, -105.15892039250949 39.915152697033264, -105.15907396491754 39.91501983021065, -105.15922452458202 39.91488492237188, -105.1593720303506 39.91474801753947, -105.15951642937621 39.91460915970136, -105.1596237810907 39.91450221346633, -105.15962936338445 39.914496648555826, -105.15965786483343 39.91446825382197, -105.15959447867782 39.91437078041713, -105.15978948537136 39.91405668205347, -105.15642013175595 39.91405356845262, -105.1560293437166 39.91405351953847, -105.15501219135895 39.91405339401757, -105.15323346103978 39.91405315098152, -105.15118187057861 39.9140528369392, -105.14767665332297 39.914052218108715, -105.14733914723315 39.91405215140002, -105.1471032891195 39.91405210433869, -105.14705319940227 39.91775944655548, -105.14704704251487 39.921450443887814, -105.14704632118296 39.92186965993315, -105.14703864590498 39.92502944310596, -105.14703935994947 39.92524137222502, -105.14702448556838 39.92746831055086, -105.14702385129164 39.92761587682738, -105.14701889379992 39.92877200297731, -105.14701871842918 39.92881293486509, -105.14701846891668 39.92887114754381))</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -718,7 +718,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1470184689167 39.92887114754381, -105.1436712912503 39.92889157348318, -105.1435958776075 39.92889181480177, -105.1435950820782 39.92889181774414, -105.1423066729647 39.92889593602464, -105.1391145604889 39.92890607867842, -105.1386248219273 39.92890763964525, -105.138619806365 39.92890769866385, -105.1376618506932 39.92891071719205, -105.1376612209119 39.92893150972372, -105.1376599462519 39.92897351444855, -105.1376407559584 39.92953592366019, -105.1376321063676 39.92984063493733, -105.1376238948989 39.93013023535828, -105.1376029272597 39.93086976333272, -105.1376034417805 39.93096545410189, -105.137605376672 39.93128768051638, -105.1376081834016 39.93175509745066, -105.1376017361011 39.93244089603266, -105.1375976976845 39.93286861358298, -105.1375954953071 39.9331018756593, -105.137586602701 39.93404371593252, -105.1375702679211 39.93577373335888, -105.1375669599118 39.93612418884327, -105.1439189795436 39.93611367046935, -105.1440164747856 39.93611446356771, -105.1442484505646 39.9361164015211, -105.1449619332645 39.93611399050048, -105.1450238629434 39.93606888524504, -105.1451144448477 39.93599694473017, -105.1451494551524 39.93595295254981, -105.1451762486899 39.93591523518277, -105.1452010134529 39.9358743619442, -105.1452237716626 39.93582560712774, -105.1452509919021 39.9357059902176, -105.1452801413981 39.93560843016036, -105.1453363564666 39.93542117809809, -105.1453570529653 39.93537556652313, -105.1453981922486 39.93533316839468, -105.1454650981695 39.9352938946994, -105.1457440526855 39.93520910173404, -105.1457990692858 39.93519005438458, -105.1457381055787 39.93499449790574, -105.1456793939515 39.93467618621654, -105.1456296173628 39.93442581733552, -105.1456026666607 39.93425058347665, -105.1455897208455 39.9340610946816, -105.1455906116229 39.93388952030274, -105.1456005666682 39.9337608687663, -105.1456108359693 39.93357145139034, -105.1456349984811 39.93338922531228, -105.1456496513171 39.93324986402978, -105.1457114410977 39.93297481700465, -105.1458009969508 39.93271772807628, -105.1458839993473 39.93249807388542, -105.1459388721907 39.93236894253652, -105.1459939602941 39.93221788879237, -105.146115958527 39.93197162260368, -105.1471407192517 39.9304413008367, -105.1472110480887 39.93030925934641, -105.147286055663 39.9301700826792, -105.1473379956629 39.93000224019443, -105.1473716775894 39.92977357407104, -105.1473554323961 39.92932313619318, -105.1473580132078 39.92893901860379, -105.1473559810769 39.92887606955925, -105.1470184689167 39.92887114754381))</t>
+          <t>POLYGON ((-105.14701846891668 39.92887114754381, -105.14367129125034 39.928891573483185, -105.14359587760754 39.92889181480177, -105.14359508207822 39.92889181774414, -105.1423066729647 39.92889593602464, -105.13911456048892 39.92890607867842, -105.1386248219273 39.928907639645246, -105.13861980636503 39.92890769866385, -105.1376618506932 39.928910717192046, -105.13766122091185 39.92893150972372, -105.13765994625194 39.92897351444855, -105.13764075595837 39.92953592366019, -105.13763210636765 39.92984063493733, -105.13762389489885 39.930130235358284, -105.13760292725966 39.930869763332716, -105.13760344178047 39.93096545410189, -105.13760537667198 39.931287680516384, -105.13760818340158 39.93175509745066, -105.13760173610106 39.93244089603266, -105.13759769768453 39.932868613582976, -105.13759549530711 39.9331018756593, -105.13758660270099 39.934043715932525, -105.13757026792113 39.93577373335888, -105.13756695991184 39.93612418884327, -105.14391897954364 39.936113670469354, -105.14401647478557 39.936114463567705, -105.14424845056456 39.9361164015211, -105.1449619332645 39.93611399050048, -105.14502386294343 39.936068885245035, -105.14511444484768 39.93599694473017, -105.14514945515238 39.93595295254981, -105.14517624868995 39.93591523518277, -105.14520101345293 39.9358743619442, -105.14522377166257 39.93582560712774, -105.14525099190207 39.9357059902176, -105.14528014139809 39.93560843016036, -105.14533635646657 39.93542117809809, -105.14535705296534 39.935375566523135, -105.14539819224865 39.935333168394685, -105.14546509816947 39.9352938946994, -105.14574405268552 39.93520910173404, -105.14579906928584 39.935190054384584, -105.14573810557869 39.93499449790574, -105.14567939395153 39.93467618621654, -105.14562961736283 39.93442581733552, -105.14560266666066 39.934250583476654, -105.14558972084548 39.9340610946816, -105.14559061162288 39.93388952030274, -105.1456005666682 39.9337608687663, -105.14561083596931 39.933571451390335, -105.1456349984811 39.933389225312276, -105.14564965131714 39.933249864029776, -105.14571144109769 39.93297481700465, -105.14580099695084 39.932717728076284, -105.14588399934732 39.93249807388542, -105.14593887219068 39.93236894253652, -105.14599396029406 39.932217888792366, -105.14611595852696 39.931971622603676, -105.14714071925168 39.9304413008367, -105.14721104808872 39.93030925934641, -105.14728605566299 39.930170082679204, -105.14733799566288 39.930002240194426, -105.14737167758945 39.92977357407104, -105.14735543239611 39.92932313619318, -105.14735801320775 39.92893901860379, -105.14735598107694 39.92887606955925, -105.14701846891668 39.92887114754381))</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -760,7 +760,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1477488371468 39.93764394966898, -105.1481608339255 39.93791157511409, -105.1487222428795 39.9381847876604, -105.1492773244566 39.93841898582257, -105.1496342695291 39.93853803083237, -105.1499646111669 39.93862564635383, -105.150579251275 39.93875078777978, -105.1515351773747 39.93887650126569, -105.153016730735 39.93907372224082, -105.153615332423 39.93915773704804, -105.1538472753946 39.93920490299118, -105.154102382476 39.93926286130255, -105.1543713842128 39.93932801019039, -105.1546912666086 39.93943263026893, -105.1551653197302 39.93962160409981, -105.1555092002975 39.93978185915769, -105.1555450745614 39.93974703246373, -105.1562040953381 39.93897594602319, -105.156290847027 39.93888698533789, -105.156429935 39.93874492365819, -105.1565611470148 39.93860887726743, -105.1580819375469 39.93723090699732, -105.1583431615177 39.93698186639371, -105.1584521736139 39.93686194950827, -105.1586781359882 39.93653209437913, -105.1587851218764 39.93631800967754, -105.1588401572359 39.93615208613267, -105.1588821147656 39.93582003817583, -105.1588829666984 39.93557791215292, -105.1588520752734 39.93533706472737, -105.1588146629055 39.93520570766016, -105.1560554738131 39.93164964151831, -105.159808177506 39.92926407705372, -105.1592581712754 39.92926956379147, -105.1584225394937 39.92924921683296, -105.1543926683685 39.92920502459549, -105.1522663875301 39.92916645411064, -105.1519553136435 39.92916551454322, -105.1516954582233 39.92913613299276, -105.15086059695 39.92896560292694, -105.1505451015723 39.92892175208359, -105.1502156221988 39.92888858119842, -105.1499603189246 39.92887708230292, -105.1488042084431 39.92888071244524, -105.1473559810769 39.92887606955925, -105.1473580132078 39.92893901860379, -105.1473554323961 39.92932313619318, -105.1473716775894 39.92977357407104, -105.1473379956629 39.93000224019443, -105.147286055663 39.9301700826792, -105.1472110480887 39.93030925934641, -105.1471407192517 39.9304413008367, -105.146115958527 39.93197162260368, -105.1459939602941 39.93221788879237, -105.1459388721907 39.93236894253652, -105.1458839993473 39.93249807388542, -105.1458009969508 39.93271772807628, -105.1457114410977 39.93297481700465, -105.1456496513171 39.93324986402978, -105.1456349984811 39.93338922531228, -105.1456108359693 39.93357145139034, -105.1456005666682 39.9337608687663, -105.1455906116229 39.93388952030274, -105.1455897208455 39.9340610946816, -105.1456026666607 39.93425058347665, -105.1456296173628 39.93442581733552, -105.1456793939515 39.93467618621654, -105.1457381055787 39.93499449790574, -105.1457990692858 39.93519005438458, -105.1458982291993 39.93545610241225, -105.1459715766644 39.9356386282458, -105.1460884237871 39.93588093045062, -105.146540121278 39.93652930366475, -105.1468724672683 39.93691279552667, -105.1472375781706 39.93724634415188, -105.1477488371468 39.93764394966898))</t>
+          <t>POLYGON ((-105.14774883714679 39.93764394966898, -105.14816083392554 39.937911575114086, -105.14872224287951 39.9381847876604, -105.14927732445656 39.93841898582257, -105.14963426952914 39.93853803083237, -105.14996461116688 39.93862564635383, -105.15057925127502 39.93875078777978, -105.15153517737465 39.93887650126569, -105.15301673073502 39.93907372224082, -105.15361533242303 39.93915773704804, -105.15384727539463 39.93920490299118, -105.154102382476 39.939262861302545, -105.15437138421281 39.939328010190394, -105.15469126660862 39.93943263026893, -105.15516531973016 39.93962160409981, -105.1555092002975 39.93978185915769, -105.15554507456137 39.93974703246373, -105.15620409533811 39.93897594602319, -105.15629084702697 39.938886985337895, -105.15642993500002 39.93874492365819, -105.15656114701483 39.93860887726743, -105.15808193754688 39.93723090699732, -105.15834316151775 39.93698186639371, -105.15845217361392 39.93686194950827, -105.15867813598817 39.93653209437913, -105.15878512187642 39.93631800967754, -105.15884015723587 39.93615208613267, -105.15888211476562 39.93582003817583, -105.1588829666984 39.93557791215292, -105.15885207527337 39.93533706472737, -105.15881466290546 39.93520570766016, -105.15605547381307 39.93164964151831, -105.15980817750602 39.929264077053716, -105.15925817127537 39.92926956379147, -105.15842253949369 39.929249216832964, -105.15439266836849 39.92920502459549, -105.15226638753013 39.92916645411064, -105.15195531364348 39.92916551454322, -105.15169545822333 39.92913613299276, -105.15086059694998 39.92896560292694, -105.15054510157229 39.92892175208359, -105.15021562219884 39.92888858119842, -105.14996031892461 39.92887708230292, -105.14880420844312 39.92888071244524, -105.14735598107694 39.92887606955925, -105.14735801320775 39.92893901860379, -105.14735543239611 39.92932313619318, -105.14737167758945 39.92977357407104, -105.14733799566288 39.930002240194426, -105.14728605566299 39.930170082679204, -105.14721104808872 39.93030925934641, -105.14714071925168 39.9304413008367, -105.14611595852696 39.931971622603676, -105.14599396029406 39.932217888792366, -105.14593887219068 39.93236894253652, -105.14588399934732 39.93249807388542, -105.14580099695084 39.932717728076284, -105.14571144109769 39.93297481700465, -105.14564965131714 39.933249864029776, -105.1456349984811 39.933389225312276, -105.14561083596931 39.933571451390335, -105.1456005666682 39.9337608687663, -105.14559061162288 39.93388952030274, -105.14558972084548 39.9340610946816, -105.14560266666066 39.934250583476654, -105.14562961736283 39.93442581733552, -105.14567939395153 39.93467618621654, -105.14573810557869 39.93499449790574, -105.14579906928584 39.935190054384584, -105.14589822919928 39.93545610241225, -105.14597157666435 39.935638628245805, -105.14608842378708 39.935880930450615, -105.14654012127802 39.93652930366475, -105.14687246726825 39.936912795526666, -105.14723757817065 39.93724634415188, -105.14774883714679 39.93764394966898))</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -802,7 +802,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1587851218764 39.93631800967754, -105.1586781359882 39.93653209437913, -105.1584521736139 39.93686194950827, -105.1583431615177 39.93698186639371, -105.1580819375469 39.93723090699732, -105.1565611470148 39.93860887726743, -105.156429935 39.93874492365819, -105.156290847027 39.93888698533789, -105.1562040953381 39.93897594602319, -105.1555450745614 39.93974703246373, -105.1555092002975 39.93978185915769, -105.1560922753161 39.940163787752, -105.1566372808513 39.9406067890523, -105.1570812822657 39.94104079033195, -105.1573832849974 39.94145079192295, -105.1578252915845 39.94220679424946, -105.1580602931684 39.94261279598288, -105.1585962997493 39.94358079987696, -105.1589627797873 39.94421017317883, -105.1590713055986 39.94436680235875, -105.1592766572467 39.94459357402653, -105.159518308048 39.94479480357361, -105.1597439684961 39.94494168271444, -105.1599477326538 39.94505666831378, -105.1601873107974 39.94515480424463, -105.160520323111 39.94526370683572, -105.16074979636 39.94530954194396, -105.1609447840726 39.94534199305829, -105.1611304724021 39.94535683738516, -105.1613593181915 39.94534980422551, -105.1615903683127 39.94532959320887, -105.1630884467118 39.94512594021865, -105.1636862002967 39.94505334437473, -105.1636320801801 39.94482103827956, -105.1635750285351 39.9446009797892, -105.1634948490132 39.94429794785718, -105.1633550865634 39.94378198668555, -105.1633021722153 39.94359103958861, -105.1631980133074 39.94323303212497, -105.1628769198138 39.94231601326964, -105.1626888242614 39.94169504212864, -105.1626649967702 39.94160904746479, -105.1626440231492 39.94152306025195, -105.1626248393608 39.94143598127076, -105.1626088627851 39.94134891077801, -105.1625960967277 39.94126212438719, -105.1625858278116 39.94117507060656, -105.1625769906578 39.94108692311173, -105.1625731407585 39.94099988812983, -105.1625718746753 39.94082309269349, -105.1625790263986 39.94074707079799, -105.1625879731143 39.94066913214759, -105.1626008311626 39.94059312786391, -105.1626140503101 39.94051602582904, -105.162630123188 39.94043893214972, -105.1626490443607 39.9403629447151, -105.1626701055143 39.94028696354345, -105.162718992763 39.94013694300597, -105.162746822912 39.94006208044461, -105.1627829034754 39.93997790757243, -105.1628200508432 39.93989401251284, -105.1628600477878 39.93981094898524, -105.1629011086264 39.93972898736373, -105.1629471673523 39.93964594154362, -105.1629928582588 39.93956509134216, -105.1630421124366 39.93948507474977, -105.1630931496289 39.93940506425146, -105.1632019791923 39.93924890425799, -105.1632629575522 39.93917798160172, -105.1633249999631 39.93910788522759, -105.1633898917043 39.93903889505227, -105.1634558449628 39.93897100674868, -105.1635239351863 39.93890394695319, -105.163594868139 39.93883909303319, -105.1636668717177 39.938773966593, -105.1637410043112 39.93871104303593, -105.1642599884158 39.93825794789033, -105.1644648816942 39.93807406597744, -105.1646640902998 39.93788604932791, -105.1647608452607 39.93779107157614, -105.1648568970293 39.93769389588451, -105.1649088775099 39.93763886807371, -105.1649590854191 39.93758191397288, -105.1650071467542 39.93752605061351, -105.1650548619299 39.93746799131537, -105.1651151284636 39.93739596680214, -105.1651711298179 39.93732091084251, -105.1652249909484 39.93724612243673, -105.1652781438186 39.93716996024013, -105.1653791026839 39.93701706993694, -105.1654700989026 39.93686003278812, -105.1655129231004 39.93678109527023, -105.1655539695186 39.93670105376755, -105.1655838624477 39.93664101959121, -105.1656091263775 39.93657987496384, -105.1656351002727 39.93651900619267, -105.1656571511606 39.93645812602905, -105.1656781405316 39.93639587107268, -105.1657049704915 39.93630590529387, -105.1657300509366 39.93620907139002, -105.1658739997193 39.93621399863118, -105.1659871752904 39.9362624329908, -105.1659873030505 39.93626023394562, -105.1660033259753 39.93598576505014, -105.166003329776 39.93598570561753, -105.1660326082687 39.93546115149928, -105.1660503453821 39.93509378069637, -105.1660647969186 39.93392020542746, -105.166056515896 39.93295616617159, -105.1660467016499 39.93181341576487, -105.1660381193122 39.93081421993796, -105.166031494597 39.93004289540448, -105.1660261074718 39.92941559118069, -105.1660201718075 39.92872443199441, -105.1658309152665 39.92871792608083, -105.1657570205717 39.92871886091139, -105.1642865869104 39.92873746663779, -105.1635322820768 39.92874595284867, -105.1625711373537 39.9287574391029, -105.1621020483118 39.92878823466037, -105.161753602932 39.92883367977832, -105.1615000714133 39.92889016393721, -105.1611512880181 39.92900352248355, -105.1607375215015 39.9291131147585, -105.1604121448398 39.92918722070032, -105.1601519120273 39.92923292102617, -105.159808177506 39.92926407705372, -105.1560554738131 39.93164964151831, -105.1588146629055 39.93520570766016, -105.1588520752734 39.93533706472737, -105.1588829666984 39.93557791215292, -105.1588821147656 39.93582003817583, -105.1588401572359 39.93615208613267, -105.1587851218764 39.93631800967754))</t>
+          <t>POLYGON ((-105.15878512187642 39.93631800967754, -105.15867813598817 39.93653209437913, -105.15845217361392 39.93686194950827, -105.15834316151775 39.93698186639371, -105.15808193754688 39.93723090699732, -105.15656114701483 39.93860887726743, -105.15642993500002 39.93874492365819, -105.15629084702697 39.938886985337895, -105.15620409533811 39.93897594602319, -105.15554507456137 39.93974703246373, -105.1555092002975 39.93978185915769, -105.1560922753161 39.940163787752, -105.15663728085129 39.940606789052296, -105.15708128226574 39.94104079033195, -105.15738328499737 39.94145079192295, -105.1578252915845 39.94220679424946, -105.15806029316842 39.94261279598288, -105.15859629974929 39.94358079987696, -105.15896277978726 39.94421017317883, -105.15907130559862 39.94436680235875, -105.1592766572467 39.94459357402653, -105.15951830804804 39.94479480357361, -105.15974396849614 39.94494168271444, -105.15994773265383 39.945056668313775, -105.16018731079738 39.94515480424463, -105.160520323111 39.94526370683572, -105.16074979636004 39.945309541943956, -105.16094478407264 39.945341993058285, -105.16113047240214 39.945356837385155, -105.16135931819154 39.945349804225515, -105.16159036831274 39.945329593208875, -105.1630884467118 39.945125940218645, -105.16368620029668 39.945053344374735, -105.1636320801801 39.944821038279564, -105.16357502853508 39.9446009797892, -105.16349484901325 39.94429794785718, -105.16335508656337 39.94378198668555, -105.1633021722153 39.94359103958861, -105.16319801330741 39.943233032124965, -105.1628769198138 39.94231601326964, -105.16268882426142 39.941695042128636, -105.1626649967702 39.941609047464794, -105.1626440231492 39.941523060251946, -105.16262483936079 39.94143598127076, -105.16260886278506 39.94134891077801, -105.16259609672771 39.94126212438719, -105.16258582781163 39.94117507060656, -105.16257699065784 39.941086923111726, -105.16257314075852 39.94099988812983, -105.16257187467531 39.94082309269349, -105.16257902639856 39.94074707079799, -105.16258797311431 39.94066913214759, -105.16260083116256 39.94059312786391, -105.16261405031008 39.94051602582904, -105.16263012318804 39.94043893214972, -105.16264904436072 39.9403629447151, -105.16267010551428 39.94028696354345, -105.16271899276299 39.94013694300597, -105.16274682291196 39.94006208044461, -105.1627829034754 39.93997790757243, -105.1628200508432 39.93989401251284, -105.16286004778785 39.93981094898524, -105.16290110862637 39.93972898736373, -105.16294716735233 39.939645941543624, -105.16299285825883 39.93956509134216, -105.16304211243657 39.93948507474977, -105.16309314962889 39.93940506425146, -105.16320197919231 39.939248904257994, -105.16326295755219 39.93917798160172, -105.16332499996312 39.939107885227585, -105.16338989170434 39.93903889505227, -105.16345584496278 39.93897100674868, -105.1635239351863 39.93890394695319, -105.163594868139 39.93883909303319, -105.1636668717177 39.938773966593, -105.16374100431125 39.93871104303593, -105.16425998841576 39.93825794789033, -105.16446488169423 39.93807406597744, -105.16466409029975 39.937886049327915, -105.16476084526066 39.93779107157614, -105.16485689702925 39.93769389588451, -105.16490887750993 39.937638868073705, -105.16495908541913 39.93758191397288, -105.16500714675422 39.937526050613506, -105.1650548619299 39.937467991315366, -105.16511512846355 39.93739596680214, -105.16517112981792 39.93732091084251, -105.16522499094845 39.93724612243673, -105.16527814381863 39.937169960240126, -105.16537910268387 39.93701706993694, -105.16547009890257 39.93686003278812, -105.16551292310038 39.936781095270234, -105.16555396951864 39.93670105376755, -105.16558386244768 39.936641019591214, -105.16560912637749 39.93657987496384, -105.16563510027267 39.93651900619267, -105.16565715116059 39.93645812602905, -105.16567814053157 39.93639587107268, -105.16570497049152 39.93630590529387, -105.16573005093659 39.936209071390024, -105.16587399971932 39.93621399863118, -105.16598717529035 39.9362624329908, -105.16598730305047 39.93626023394562, -105.16600332597527 39.93598576505014, -105.16600332977605 39.935985705617526, -105.16603260826868 39.935461151499275, -105.16605034538208 39.93509378069637, -105.16606479691863 39.93392020542746, -105.16605651589599 39.93295616617159, -105.16604670164995 39.93181341576487, -105.16603811931222 39.93081421993796, -105.166031494597 39.93004289540448, -105.16602610747184 39.92941559118069, -105.1660201718075 39.92872443199441, -105.16583091526645 39.92871792608083, -105.16575702057173 39.92871886091139, -105.16428658691042 39.92873746663779, -105.16353228207683 39.92874595284867, -105.16257113735374 39.928757439102895, -105.16210204831177 39.92878823466037, -105.16175360293202 39.92883367977832, -105.16150007141333 39.92889016393721, -105.16115128801812 39.92900352248355, -105.16073752150152 39.9291131147585, -105.16041214483981 39.92918722070032, -105.16015191202733 39.92923292102617, -105.15980817750602 39.929264077053716, -105.15605547381307 39.93164964151831, -105.15881466290546 39.93520570766016, -105.15885207527337 39.93533706472737, -105.1588829666984 39.93557791215292, -105.15888211476562 39.93582003817583, -105.15884015723587 39.93615208613267, -105.15878512187642 39.93631800967754))</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -844,7 +844,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1566313947508 39.94696697503216, -105.1611199911071 39.94690008212007, -105.1636184553306 39.94688087687528, -105.1640603336121 39.94689480786831, -105.1636862002967 39.94505334437473, -105.1630884467118 39.94512594021865, -105.1615903683127 39.94532959320887, -105.1613593181915 39.94534980422551, -105.1611304724021 39.94535683738516, -105.1609447840726 39.94534199305829, -105.16074979636 39.94530954194396, -105.160520323111 39.94526370683572, -105.1601873107974 39.94515480424463, -105.1599477326538 39.94505666831378, -105.1597439684961 39.94494168271444, -105.159518308048 39.94479480357361, -105.1592766572467 39.94459357402653, -105.1590713055986 39.94436680235875, -105.1589627797873 39.94421017317883, -105.1585962997493 39.94358079987696, -105.1580602931684 39.94261279598288, -105.1578252915845 39.94220679424946, -105.1573832849974 39.94145079192295, -105.1570812822657 39.94104079033195, -105.1566372808513 39.9406067890523, -105.1560922753161 39.940163787752, -105.1555092002975 39.93978185915769, -105.1551653197302 39.93962160409981, -105.1546912666086 39.93943263026893, -105.1543713842128 39.93932801019039, -105.154102382476 39.93926286130255, -105.1538472753946 39.93920490299118, -105.153615332423 39.93915773704804, -105.153016730735 39.93907372224082, -105.1515351773747 39.93887650126569, -105.150579251275 39.93875078777978, -105.1499646111669 39.93862564635383, -105.1496342695291 39.93853803083237, -105.1492773244566 39.93841898582257, -105.1487222428795 39.9381847876604, -105.1481608339255 39.93791157511409, -105.1477488371468 39.93764394966898, -105.1472375781706 39.93724634415188, -105.1468724672683 39.93691279552667, -105.146540121278 39.93652930366475, -105.1460884237871 39.93588093045062, -105.1459715766644 39.9356386282458, -105.1458982291993 39.93545610241225, -105.1457990692858 39.93519005438458, -105.1457440526855 39.93520910173404, -105.1454650981695 39.9352938946994, -105.1453981922486 39.93533316839468, -105.1453570529653 39.93537556652313, -105.1453363564666 39.93542117809809, -105.1452801413981 39.93560843016036, -105.1452509919021 39.9357059902176, -105.1452237716626 39.93582560712774, -105.1452010134529 39.9358743619442, -105.1451762486899 39.93591523518277, -105.1451494551524 39.93595295254981, -105.1451144448477 39.93599694473017, -105.1450238629434 39.93606888524504, -105.1449619332645 39.93611399050048, -105.1442484505646 39.9361164015211, -105.1440164747856 39.93611446356771, -105.1439189795436 39.93611367046935, -105.1375669599118 39.93612418884327, -105.1375796290724 39.93717680439059, -105.1375804232843 39.93724229677402, -105.13758090158 39.93728200849577, -105.137587250081 39.93780781910959, -105.1375901359232 39.9380468199151, -105.1375934532797 39.93832156847123, -105.1376000835919 39.93887058729946, -105.1376002640181 39.93888552805745, -105.1376032162488 39.9391298924964, -105.1376082126364 39.93954372301226, -105.1376092642489 39.9396308257882, -105.1376101533659 39.93970445864476, -105.1376101662146 39.93970556469871, -105.1376101742235 39.93970626003536, -105.1376659994644 39.93973899908963, -105.1380069982713 39.93995099908016, -105.1400129996827 39.94124299866457, -105.1405889992587 39.94161999863454, -105.1409599991531 39.94185799904378, -105.141208999877 39.9420169995477, -105.1415170000054 39.9422179981579, -105.1429179998172 39.94312999953807, -105.1435829995349 39.94355199879121, -105.1436849993157 39.94361699895295, -105.1438049994702 39.94369699936311, -105.1444109992605 39.94408999827592, -105.1465979998178 39.94550799907834, -105.1469689981003 39.94574899894534, -105.1470224473384 39.94578389403245, -105.1479109994562 39.94636399921564, -105.1483709999483 39.94665999878806, -105.1487869967502 39.94692837327946, -105.1488331432633 39.9468859991199, -105.1493928596184 39.94688718322774, -105.1532378179738 39.94686842813926, -105.1535295268834 39.94686536897351, -105.1538449811731 39.94686205978073, -105.1541975052208 39.94685836112814, -105.1544700033438 39.94685549950776, -105.1566300792916 39.94683280321451, -105.1566313947508 39.94696697503216))</t>
+          <t>POLYGON ((-105.15663139475083 39.94696697503216, -105.16111999110713 39.946900082120074, -105.16361845533064 39.94688087687528, -105.16406033361208 39.94689480786831, -105.16368620029668 39.945053344374735, -105.1630884467118 39.945125940218645, -105.16159036831274 39.945329593208875, -105.16135931819154 39.945349804225515, -105.16113047240214 39.945356837385155, -105.16094478407264 39.945341993058285, -105.16074979636004 39.945309541943956, -105.160520323111 39.94526370683572, -105.16018731079738 39.94515480424463, -105.15994773265383 39.945056668313775, -105.15974396849614 39.94494168271444, -105.15951830804804 39.94479480357361, -105.1592766572467 39.94459357402653, -105.15907130559862 39.94436680235875, -105.15896277978726 39.94421017317883, -105.15859629974929 39.94358079987696, -105.15806029316842 39.94261279598288, -105.1578252915845 39.94220679424946, -105.15738328499737 39.94145079192295, -105.15708128226574 39.94104079033195, -105.15663728085129 39.940606789052296, -105.1560922753161 39.940163787752, -105.1555092002975 39.93978185915769, -105.15516531973016 39.93962160409981, -105.15469126660862 39.93943263026893, -105.15437138421281 39.939328010190394, -105.154102382476 39.939262861302545, -105.15384727539463 39.93920490299118, -105.15361533242303 39.93915773704804, -105.15301673073502 39.93907372224082, -105.15153517737465 39.93887650126569, -105.15057925127502 39.93875078777978, -105.14996461116688 39.93862564635383, -105.14963426952914 39.93853803083237, -105.14927732445656 39.93841898582257, -105.14872224287951 39.9381847876604, -105.14816083392554 39.937911575114086, -105.14774883714679 39.93764394966898, -105.14723757817065 39.93724634415188, -105.14687246726825 39.936912795526666, -105.14654012127802 39.93652930366475, -105.14608842378708 39.935880930450615, -105.14597157666435 39.935638628245805, -105.14589822919928 39.93545610241225, -105.14579906928584 39.935190054384584, -105.14574405268552 39.93520910173404, -105.14546509816947 39.9352938946994, -105.14539819224865 39.935333168394685, -105.14535705296534 39.935375566523135, -105.14533635646657 39.93542117809809, -105.14528014139809 39.93560843016036, -105.14525099190207 39.9357059902176, -105.14522377166257 39.93582560712774, -105.14520101345293 39.9358743619442, -105.14517624868995 39.93591523518277, -105.14514945515238 39.93595295254981, -105.14511444484768 39.93599694473017, -105.14502386294343 39.936068885245035, -105.1449619332645 39.93611399050048, -105.14424845056456 39.9361164015211, -105.14401647478557 39.936114463567705, -105.14391897954364 39.936113670469354, -105.13756695991184 39.93612418884327, -105.13757962907239 39.93717680439059, -105.13758042328428 39.93724229677402, -105.13758090157998 39.93728200849577, -105.13758725008098 39.93780781910959, -105.13759013592323 39.9380468199151, -105.13759345327975 39.93832156847123, -105.13760008359186 39.93887058729946, -105.13760026401813 39.938885528057455, -105.1376032162488 39.9391298924964, -105.13760821263644 39.93954372301226, -105.13760926424892 39.9396308257882, -105.13761015336587 39.93970445864476, -105.13761016621459 39.93970556469871, -105.13761017422354 39.93970626003536, -105.13766599946442 39.93973899908963, -105.13800699827127 39.93995099908016, -105.1400129996827 39.94124299866457, -105.14058899925865 39.941619998634536, -105.14095999915313 39.94185799904378, -105.14120899987702 39.942016999547704, -105.14151700000538 39.9422179981579, -105.1429179998172 39.943129999538066, -105.14358299953487 39.94355199879121, -105.14368499931568 39.943616998952955, -105.14380499947022 39.94369699936311, -105.14441099926047 39.94408999827592, -105.14659799981776 39.945507999078345, -105.14696899810028 39.94574899894534, -105.14702244733836 39.94578389403245, -105.14791099945617 39.94636399921564, -105.14837099994834 39.946659998788064, -105.14878699675018 39.946928373279455, -105.14883314326335 39.9468859991199, -105.14939285961843 39.946887183227744, -105.15323781797376 39.94686842813926, -105.15352952688337 39.94686536897351, -105.15384498117308 39.94686205978073, -105.15419750522078 39.946858361128136, -105.1544700033438 39.946855499507755, -105.15663007929156 39.94683280321451, -105.15663139475083 39.94696697503216))</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1777988506388 39.9622247658564, -105.1779603294206 39.96230169761951, -105.1780795667658 39.96212243842648, -105.1780617120378 39.96101742820876, -105.1780563504867 39.96064057285627, -105.1780562582363 39.96063407794388, -105.1760332411225 39.96066191903108, -105.1753197877496 39.96067107019252, -105.1752660781159 39.9606704126778, -105.1751530130947 39.96066902761821, -105.1751515536733 39.96066900909348, -105.1751673978478 39.95941085853762, -105.1752731802447 39.95941238698667, -105.1756586713841 39.95941795615627, -105.1767015637337 39.95943301604639, -105.1770275234974 39.95943772098945, -105.1770358705875 39.9584045834283, -105.1770363078439 39.95835052526509, -105.1770375221035 39.95820029775011, -105.1770375813809 39.95819321332797, -105.1753811772785 39.95817043580769, -105.1753791767883 39.95758643523679, -105.1786071533748 39.95766248214333, -105.178782063112 39.95766574209604, -105.1789897484092 39.957669611876, -105.1789848485213 39.95766031512748, -105.177648397834 39.95512435329022, -105.1776144429687 39.95506001242811, -105.1775799624868 39.95499299062175, -105.1775470406094 39.95492554265083, -105.1775156877714 39.95485768836055, -105.1774859155525 39.95478945300295, -105.1774577273785 39.95472085370143, -105.1774311360077 39.95465191391003, -105.1774061518873 39.95458265077165, -105.1773827784174 39.95451308681337, -105.1773610213213 39.95444324817128, -105.1773575396614 39.95443111644111, -105.1773408910587 39.95437314928622, -105.177322394536 39.95430281359553, -105.1773055304672 39.95423226451359, -105.177290313959 39.95416152369918, -105.1772767414146 39.95409060825552, -105.1772648208975 39.95401954432493, -105.1772552845585 39.95394743780206, -105.1772475047739 39.95387510202673, -105.1772414131593 39.9538026430856, -105.1772370166073 39.95373008711738, -105.1772416938306 39.95365372245707, -105.1772507335152 39.95357595507921, -105.1772613072263 39.95349823162613, -105.1772734159885 39.95342058182205, -105.177290609483 39.95332415578926, -105.1774078670555 39.95259250878293, -105.1774296504487 39.95249004043743, -105.1774426914856 39.95247925641739, -105.1776474058934 39.95230996305708, -105.1776425915952 39.95225318368962, -105.1776494915453 39.95224847092626, -105.1776503630244 39.95222278293825, -105.1776527450811 39.9521525489294, -105.1776542787933 39.95210731667019, -105.1777091771583 39.95048843468322, -105.1765421764602 39.95049343511674, -105.1765441762881 39.95029543509211, -105.1737901766914 39.9502784352506, -105.1732691751886 39.95049443510379, -105.171721175293 39.95049343486586, -105.171721175489 39.95026543539605, -105.1713521750109 39.95026343503369, -105.1710701754516 39.9496574351276, -105.1709821753827 39.94931543455208, -105.1708731754645 39.94899843388744, -105.1706751750825 39.94883443513947, -105.1705001743236 39.94877043461553, -105.1702541750417 39.94875143479771, -105.1703601751532 39.94872843443577, -105.1699691748952 39.94766043485847, -105.1696509264492 39.94772961758919, -105.1696508514793 39.94772963358609, -105.1685594742733 39.94796687370324, -105.1663871736281 39.94844043457117, -105.1657381741117 39.9485814352014, -105.1657421736448 39.94800015855595, -105.1657468007817 39.94732775484253, -105.165775173689 39.94320443381061, -105.1664695916308 39.9432063625764, -105.1683021747413 39.94321143381614, -105.1693041740566 39.94127343310699, -105.1693161728545 39.9392404329576, -105.1676961733447 39.939242433397, -105.1669986961005 39.93946070845881, -105.1664371723441 39.93963643311929, -105.1657621735393 39.94010243415755, -105.1657314686866 39.93778700123453, -105.1657309930949 39.93726410639616, -105.1657358633377 39.93725561378023, -105.1657790841984 39.93717594147653, -105.1658204732303 39.93709568651817, -105.1658600197634 39.93701487859802, -105.1658977131763 39.93693353750162, -105.1659335404815 39.93685168841169, -105.1659572086535 39.93679429393993, -105.1659674910183 39.93676935921954, -105.1659749417947 39.93647953441914, -105.1659871764604 39.93626243299418, -105.1659873018805 39.93626023394222, -105.1658916104535 39.93622118475289, -105.1658739997193 39.93621399863118, -105.1657300509366 39.93620907139002, -105.1657049704915 39.93630590529387, -105.1656781405316 39.93639587107268, -105.1656571511606 39.93645812602905, -105.1656351002727 39.93651900619267, -105.1656091263775 39.93657987496384, -105.1655838624477 39.93664101959121, -105.1655539695186 39.93670105376755, -105.1655129231004 39.93678109527023, -105.1654700989026 39.93686003278812, -105.1653791026839 39.93701706993694, -105.1652781438186 39.93716996024013, -105.1652249909484 39.93724612243673, -105.1651711298179 39.93732091084251, -105.1651151284636 39.93739596680214, -105.1650548619299 39.93746799131537, -105.1650071467542 39.93752605061351, -105.1649590854191 39.93758191397288, -105.1649088775099 39.93763886807371, -105.1648568970293 39.93769389588451, -105.1647608452607 39.93779107157614, -105.1646640902998 39.93788604932791, -105.1644648816942 39.93807406597744, -105.1642599884158 39.93825794789033, -105.1637410043112 39.93871104303593, -105.1636668717177 39.938773966593, -105.163594868139 39.93883909303319, -105.1635239351863 39.93890394695319, -105.1634558449628 39.93897100674868, -105.1633898917043 39.93903889505227, -105.1633249999631 39.93910788522759, -105.1632629575522 39.93917798160172, -105.1632019791923 39.93924890425799, -105.1630931496289 39.93940506425146, -105.1630421124366 39.93948507474977, -105.1629928582588 39.93956509134216, -105.1629471673523 39.93964594154362, -105.1629011086264 39.93972898736373, -105.1628600477878 39.93981094898524, -105.1628200508432 39.93989401251284, -105.1627829034754 39.93997790757243, -105.162746822912 39.94006208044461, -105.162718992763 39.94013694300597, -105.1626701055143 39.94028696354345, -105.1626490443607 39.9403629447151, -105.162630123188 39.94043893214972, -105.1626140503101 39.94051602582904, -105.1626008311626 39.94059312786391, -105.1625879731143 39.94066913214759, -105.1625790263986 39.94074707079799, -105.1625718746753 39.94082309269349, -105.1625731407585 39.94099988812983, -105.1625769906578 39.94108692311173, -105.1625858278116 39.94117507060656, -105.1625960967277 39.94126212438719, -105.1626088627851 39.94134891077801, -105.1626248393608 39.94143598127076, -105.1626440231492 39.94152306025195, -105.1626649967702 39.94160904746479, -105.1626888242614 39.94169504212864, -105.1628769198138 39.94231601326964, -105.1631980133074 39.94323303212497, -105.1633021722153 39.94359103958861, -105.1633550865634 39.94378198668555, -105.1634948490132 39.94429794785718, -105.1635750285351 39.9446009797892, -105.1636320801801 39.94482103827956, -105.1636862002967 39.94505334437473, -105.1640603336121 39.94689480786831, -105.1636184553306 39.94688087687528, -105.1611199911071 39.94690008212007, -105.1566313947508 39.94696697503216, -105.1566300792916 39.94683280321451, -105.1544700033438 39.94685549950776, -105.1541975052208 39.94685836112814, -105.1538449811731 39.94686205978073, -105.1535295268834 39.94686536897351, -105.1532378179738 39.94686842813926, -105.1493928596184 39.94688718322774, -105.1488331432633 39.9468859991199, -105.1487869967502 39.94692837327946, -105.1493769991665 39.94730899849206, -105.1502339997436 39.94785999905235, -105.1505859991704 39.94808599920534, -105.1510029999227 39.9483689989986, -105.1520270002295 39.94907999894239, -105.1526479997484 39.94953399844792, -105.1538259995572 39.95043899936822, -105.1543240000297 39.95082499846626, -105.1545469991415 39.95082499900798, -105.154634999516 39.95082499893148, -105.155603998905 39.95163699829544, -105.1564621234448 39.95235626096443, -105.1568089995898 39.95264699943566, -105.1594730000078 39.95466099895394, -105.1603829998639 39.95530799832515, -105.1604879993213 39.95538299862599, -105.1605708372656 39.95542490543037, -105.1605729992732 39.95542599889634, -105.160553485336 39.95544433019448, -105.160507601197 39.95548743481859, -105.1605070003541 39.955487998663, -105.1605739993225 39.95553199876508, -105.1609239990875 39.95574399904351, -105.1611820283237 39.95589271854974, -105.1612710001578 39.9559439989421, -105.1615179991773 39.95607999946219, -105.162090999951 39.95638499933245, -105.1623139998591 39.95649799874107, -105.1626729999983 39.95667199866357, -105.1629539988249 39.95680199904174, -105.163260000118 39.95693999941128, -105.1635449998441 39.95706699912397, -105.1640439992191 39.95727199887524, -105.1655459994386 39.95785699862255, -105.1657049993032 39.95791899851163, -105.1658829843055 39.95798883313223, -105.166280999977 39.95814499912188, -105.1663260779203 39.95809453148716, -105.1663729998672 39.95804199855646, -105.1663939993887 39.95801599875833, -105.1663429988309 39.95789999829524, -105.1661250002072 39.95739999859541, -105.1661089994848 39.95726499912967, -105.1660659997773 39.95698699837227, -105.1660599995567 39.9569419984156, -105.1661219997786 39.95695499897838, -105.1668249995467 39.95710599849211, -105.1672029990481 39.95741599921722, -105.1677549991503 39.95786999907147, -105.16867899997 39.95862899864169, -105.1718929991997 39.96004699882172, -105.1750629987647 39.96129699910314, -105.175195000182 39.96134899884276, -105.1777729991336 39.96222499799526, -105.1777779996259 39.96221599908061, -105.1777786369145 39.96221513532904, -105.1777988506388 39.9622247658564))</t>
+          <t>POLYGON ((-105.17779885063878 39.962224765856405, -105.17796032942059 39.96230169761951, -105.1780795667658 39.96212243842648, -105.17806171203779 39.961017428208756, -105.17805635048674 39.96064057285627, -105.1780562582363 39.96063407794388, -105.17603324112252 39.960661919031075, -105.17531978774957 39.96067107019252, -105.1752660781159 39.9606704126778, -105.17515301309466 39.96066902761821, -105.17515155367326 39.96066900909348, -105.17516739784779 39.959410858537616, -105.17527318024473 39.95941238698667, -105.17565867138414 39.959417956156265, -105.1767015637337 39.95943301604639, -105.1770275234974 39.95943772098945, -105.17703587058749 39.9584045834283, -105.17703630784392 39.95835052526509, -105.1770375221035 39.95820029775011, -105.17703758138086 39.95819321332797, -105.17538117727852 39.958170435807695, -105.17537917678827 39.95758643523679, -105.17860715337477 39.95766248214333, -105.17878206311204 39.95766574209604, -105.17898974840921 39.957669611876, -105.17898484852128 39.95766031512748, -105.17764839783405 39.955124353290216, -105.17761444296868 39.955060012428106, -105.17757996248685 39.954992990621754, -105.17754704060941 39.954925542650834, -105.17751568777136 39.954857688360555, -105.17748591555247 39.95478945300295, -105.17745772737848 39.95472085370143, -105.17743113600767 39.95465191391003, -105.17740615188734 39.95458265077165, -105.17738277841741 39.95451308681337, -105.17736102132127 39.95444324817128, -105.1773575396614 39.954431116441114, -105.17734089105869 39.95437314928622, -105.17732239453598 39.95430281359553, -105.17730553046717 39.95423226451359, -105.17729031395902 39.954161523699184, -105.17727674141463 39.95409060825552, -105.1772648208975 39.95401954432493, -105.17725528455851 39.953947437802064, -105.17724750477393 39.95387510202673, -105.17724141315925 39.9538026430856, -105.17723701660725 39.95373008711738, -105.17724169383058 39.95365372245707, -105.1772507335152 39.95357595507921, -105.17726130722629 39.95349823162613, -105.17727341598847 39.95342058182205, -105.17729060948304 39.95332415578926, -105.17740786705552 39.952592508782935, -105.17742965044866 39.95249004043743, -105.17744269148557 39.95247925641739, -105.17764740589335 39.95230996305708, -105.1776425915952 39.95225318368962, -105.17764949154531 39.952248470926264, -105.17765036302441 39.95222278293825, -105.17765274508112 39.952152548929405, -105.17765427879333 39.952107316670194, -105.1777091771583 39.950488434683216, -105.17654217646017 39.95049343511674, -105.1765441762881 39.95029543509211, -105.17379017669141 39.950278435250596, -105.1732691751886 39.95049443510379, -105.17172117529299 39.95049343486586, -105.17172117548903 39.95026543539605, -105.1713521750109 39.95026343503369, -105.1710701754516 39.9496574351276, -105.17098217538266 39.94931543455208, -105.17087317546446 39.94899843388744, -105.17067517508251 39.948834435139474, -105.17050017432359 39.94877043461553, -105.17025417504168 39.94875143479771, -105.1703601751532 39.94872843443577, -105.16996917489516 39.94766043485847, -105.16965092644924 39.94772961758919, -105.16965085147935 39.947729633586086, -105.16855947427327 39.94796687370324, -105.1663871736281 39.94844043457117, -105.16573817411167 39.948581435201405, -105.16574217364477 39.94800015855595, -105.16574680078169 39.947327754842526, -105.16577517368896 39.943204433810614, -105.16646959163076 39.943206362576404, -105.16830217474134 39.94321143381614, -105.1693041740566 39.94127343310699, -105.16931617285451 39.9392404329576, -105.16769617334474 39.939242433397, -105.16699869610046 39.93946070845881, -105.16643717234412 39.93963643311929, -105.16576217353935 39.94010243415755, -105.16573146868664 39.937787001234526, -105.16573099309491 39.937264106396164, -105.16573586333769 39.93725561378023, -105.1657790841984 39.937175941476525, -105.16582047323028 39.93709568651817, -105.1658600197634 39.93701487859802, -105.1658977131763 39.93693353750162, -105.1659335404815 39.93685168841169, -105.16595720865354 39.93679429393993, -105.16596749101828 39.93676935921954, -105.1659749417947 39.93647953441914, -105.16598717646038 39.936262432994184, -105.16598730188049 39.93626023394222, -105.16589161045346 39.93622118475289, -105.16587399971932 39.93621399863118, -105.16573005093659 39.936209071390024, -105.16570497049152 39.93630590529387, -105.16567814053157 39.93639587107268, -105.16565715116059 39.93645812602905, -105.16563510027267 39.93651900619267, -105.16560912637749 39.93657987496384, -105.16558386244768 39.936641019591214, -105.16555396951864 39.93670105376755, -105.16551292310038 39.936781095270234, -105.16547009890257 39.93686003278812, -105.16537910268387 39.93701706993694, -105.16527814381863 39.937169960240126, -105.16522499094845 39.93724612243673, -105.16517112981792 39.93732091084251, -105.16511512846355 39.93739596680214, -105.1650548619299 39.937467991315366, -105.16500714675422 39.937526050613506, -105.16495908541913 39.93758191397288, -105.16490887750993 39.937638868073705, -105.16485689702925 39.93769389588451, -105.16476084526066 39.93779107157614, -105.16466409029975 39.937886049327915, -105.16446488169423 39.93807406597744, -105.16425998841576 39.93825794789033, -105.16374100431125 39.93871104303593, -105.1636668717177 39.938773966593, -105.163594868139 39.93883909303319, -105.1635239351863 39.93890394695319, -105.16345584496278 39.93897100674868, -105.16338989170434 39.93903889505227, -105.16332499996312 39.939107885227585, -105.16326295755219 39.93917798160172, -105.16320197919231 39.939248904257994, -105.16309314962889 39.93940506425146, -105.16304211243657 39.93948507474977, -105.16299285825883 39.93956509134216, -105.16294716735233 39.939645941543624, -105.16290110862637 39.93972898736373, -105.16286004778785 39.93981094898524, -105.1628200508432 39.93989401251284, -105.1627829034754 39.93997790757243, -105.16274682291196 39.94006208044461, -105.16271899276299 39.94013694300597, -105.16267010551428 39.94028696354345, -105.16264904436072 39.9403629447151, -105.16263012318804 39.94043893214972, -105.16261405031008 39.94051602582904, -105.16260083116256 39.94059312786391, -105.16258797311431 39.94066913214759, -105.16257902639856 39.94074707079799, -105.16257187467531 39.94082309269349, -105.16257314075852 39.94099988812983, -105.16257699065784 39.941086923111726, -105.16258582781163 39.94117507060656, -105.16259609672771 39.94126212438719, -105.16260886278506 39.94134891077801, -105.16262483936079 39.94143598127076, -105.1626440231492 39.941523060251946, -105.1626649967702 39.941609047464794, -105.16268882426142 39.941695042128636, -105.1628769198138 39.94231601326964, -105.16319801330741 39.943233032124965, -105.1633021722153 39.94359103958861, -105.16335508656337 39.94378198668555, -105.16349484901325 39.94429794785718, -105.16357502853508 39.9446009797892, -105.1636320801801 39.944821038279564, -105.16368620029668 39.945053344374735, -105.16406033361208 39.94689480786831, -105.16361845533064 39.94688087687528, -105.16111999110713 39.946900082120074, -105.15663139475083 39.94696697503216, -105.15663007929156 39.94683280321451, -105.1544700033438 39.946855499507755, -105.15419750522078 39.946858361128136, -105.15384498117308 39.94686205978073, -105.15352952688337 39.94686536897351, -105.15323781797376 39.94686842813926, -105.14939285961843 39.946887183227744, -105.14883314326335 39.9468859991199, -105.14878699675018 39.946928373279455, -105.14937699916646 39.94730899849206, -105.15023399974363 39.94785999905235, -105.1505859991704 39.94808599920534, -105.15100299992268 39.948368998998596, -105.15202700022954 39.949079998942395, -105.1526479997484 39.94953399844792, -105.15382599955721 39.950438999368224, -105.15432400002966 39.95082499846626, -105.1545469991415 39.95082499900798, -105.15463499951605 39.95082499893148, -105.15560399890504 39.95163699829544, -105.15646212344481 39.95235626096443, -105.15680899958977 39.952646999435665, -105.15947300000778 39.95466099895394, -105.16038299986391 39.95530799832515, -105.16048799932132 39.955382998625986, -105.16057083726557 39.95542490543037, -105.16057299927321 39.95542599889634, -105.16055348533597 39.95544433019448, -105.16050760119697 39.95548743481859, -105.16050700035407 39.955487998663, -105.16057399932254 39.95553199876508, -105.16092399908746 39.955743999043506, -105.1611820283237 39.95589271854974, -105.16127100015778 39.9559439989421, -105.16151799917733 39.95607999946219, -105.16209099995102 39.95638499933245, -105.16231399985905 39.95649799874107, -105.16267299999834 39.95667199866357, -105.16295399882495 39.95680199904174, -105.16326000011804 39.95693999941128, -105.16354499984406 39.957066999123974, -105.16404399921912 39.957271998875235, -105.16554599943859 39.957856998622546, -105.16570499930324 39.95791899851163, -105.1658829843055 39.957988833132234, -105.16628099997698 39.95814499912188, -105.16632607792026 39.958094531487156, -105.16637299986718 39.95804199855646, -105.16639399938875 39.958015998758334, -105.16634299883087 39.95789999829524, -105.16612500020719 39.95739999859541, -105.16610899948478 39.95726499912967, -105.16606599977727 39.95698699837227, -105.16605999955671 39.9569419984156, -105.1661219997786 39.956954998978375, -105.16682499954673 39.95710599849211, -105.16720299904809 39.95741599921722, -105.16775499915033 39.95786999907147, -105.16867899997003 39.958628998641686, -105.17189299919968 39.96004699882172, -105.17506299876474 39.96129699910314, -105.175195000182 39.96134899884276, -105.17777299913361 39.96222499799526, -105.17777799962595 39.962215999080605, -105.17777863691451 39.96221513532904, -105.17779885063878 39.962224765856405))</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -928,7 +928,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.132714663984 39.97135212374958, -105.1327146054549 39.97135212356304, -105.1327145579161 39.97119025763981, -105.1327142628682 39.97019653200053, -105.1327193515535 39.96995687077294, -105.1327228337507 39.96986689598629, -105.1327195315171 39.96947027243025, -105.1327151412824 39.9691659558876, -105.1327180592421 39.9688889724552, -105.1327290874463 39.9688288876109, -105.1327739804785 39.96877412640302, -105.1328169240748 39.96875010571533, -105.1328771385485 39.96873773783532, -105.1328978978705 39.96873783278408, -105.1329729052466 39.96873797441319, -105.1334221039853 39.96873693358972, -105.1339458879853 39.96873310802705, -105.134616987672 39.9687360608628, -105.1348970597835 39.96873694847295, -105.1356806657604 39.96874485295404, -105.1409718570907 39.9687743257597, -105.1411484834786 39.96875700316673, -105.1413437296394 39.96873258971108, -105.1415438644826 39.96866172247041, -105.1416835511761 39.96860139021794, -105.1418093763021 39.96852671673524, -105.1419173381126 39.96842892711096, -105.1420433384291 39.96830892639375, -105.1420743382712 39.9682629259876, -105.1421503383544 39.96812792517319, -105.1422074729856 39.96791313929997, -105.1422113366961 39.96770492316075, -105.1421767761853 39.96667984017955, -105.1421934114149 39.96616516356316, -105.1422267360074 39.96601156303456, -105.1422784346384 39.96589733965961, -105.1424003203377 39.96568682201359, -105.1425217921166 39.96555494231168, -105.1427083187379 39.96541969037425, -105.1428993207166 39.96531662179055, -105.1431599644167 39.96522091709688, -105.1432607766169 39.96519209645445, -105.143508784869 39.96517236669215, -105.1447703368318 39.96518290919838, -105.1458193408466 39.96518290820572, -105.1463623431024 39.9651829077625, -105.1464993430814 39.96518190774901, -105.1468023445748 39.96518190732379, -105.1468843448076 39.9651819073298, -105.148694400112 39.96520942180835, -105.1473873390943 39.9631518974572, -105.1472833384483 39.96300889746738, -105.1469435569407 39.96253178409309, -105.146964829352 39.96118358125917, -105.1471433292461 39.9610888885334, -105.1474233292882 39.9608348874724, -105.1474783292935 39.96067388704216, -105.1475413289239 39.96058288607245, -105.1477023298843 39.96053988550928, -105.1479113299665 39.96052988568547, -105.1481633309252 39.96050288531993, -105.148442331826 39.96043888478479, -105.1485519832549 39.9603747977174, -105.1486360896811 39.96027854212333, -105.1487807857528 39.96014315192021, -105.1488280260406 39.95998959277168, -105.1488102555673 39.95983225986645, -105.1488898824022 39.95970382063977, -105.1489322573949 39.95959314057911, -105.1489191124549 39.95943939649989, -105.1489150752814 39.9593214255841, -105.1489295982557 39.95920708593706, -105.1489624985801 39.95913212151229, -105.1489630686094 39.9590213131738, -105.1491123870097 39.95888951135321, -105.1492801913796 39.9587756383149, -105.1493875746369 39.95866872974738, -105.1495089481525 39.95855114036917, -105.14957663923 39.95845433338604, -105.1496074453243 39.95836556608734, -105.1496680490963 39.95832285639452, -105.1498075423503 39.95829468443688, -105.1499234796544 39.95833078124081, -105.1500673796851 39.95834909104068, -105.1501787648453 39.95836730195432, -105.1503599521743 39.95836070242881, -105.1504946719067 39.95835753730839, -105.1510067595082 39.95813389543042, -105.1511141390507 39.95802698524815, -105.1512631405784 39.95795594635907, -105.1514817763424 39.95789226645639, -105.1517236373106 39.95782865724059, -105.1520305612702 39.95775809457165, -105.1521993358148 39.95775386844422, -105.1524063363067 39.95768886822943, -105.1526193367725 39.95766986805643, -105.152762336867 39.95764386738736, -105.1528813375599 39.95762886696753, -105.1531233379393 39.95756386642059, -105.153231338895 39.95755286658486, -105.1534343395124 39.95747686623236, -105.1535573391292 39.9574168657316, -105.1536263393625 39.9573298649078, -105.153743633434 39.95701975793894, -105.1537623376568 39.9569568633737, -105.1537952697089 39.95691267774466, -105.1538790755611 39.95687361027492, -105.1539693380937 39.95684286262208, -105.1540583390035 39.9568058623279, -105.1541954630687 39.95676732486336, -105.1543069734991 39.95676051091827, -105.1544416174925 39.95677163805132, -105.1545530567024 39.95677912074012, -105.1546411983074 39.95680083238248, -105.1547015985866 39.95679743867733, -105.1547480456136 39.95679757785513, -105.1548456401288 39.95678714697017, -105.1549572589689 39.95675888529122, -105.1550644145168 39.956694864728, -105.1551993655313 39.95664522612983, -105.1553156290344 39.95661697800303, -105.1554364472436 39.95660661518612, -105.1555340594246 39.95659260905028, -105.1556595935678 39.95656796301251, -105.1558313434274 39.95644585841386, -105.1560333438127 39.95633185794351, -105.1561273445217 39.95625685770177, -105.156216344759 39.95622285764431, -105.1563643445258 39.95621085739178, -105.1565023450971 39.956184856996, -105.1565713451126 39.95615085648439, -105.1566163457147 39.9560978561319, -105.1566903449367 39.95593085549667, -105.1567443440113 39.95587785488445, -105.1568973448171 39.95573785436316, -105.157045344928 39.95563985366856, -105.1573523454056 39.95551485287092, -105.1575053456166 39.95549185275024, -105.1577993479427 39.95551485189716, -105.1580433482104 39.95544885175151, -105.158151348373 39.95544185164904, -105.1582673485683 39.95541785178789, -105.1584013489657 39.95539185076902, -105.1584773487649 39.9553558505898, -105.1585573490083 39.95530785100657, -105.1585993486792 39.95524535072974, -105.1586223493838 39.95516784949032, -105.158646349241 39.95512151586125, -105.1588352249162 39.95521334278688, -105.1597388118858 39.95581121070809, -105.1599753885531 39.9559715043019, -105.1603146271586 39.95566066292508, -105.1611396467652 39.95615130950625, -105.1611820283237 39.95589271854974, -105.1609239990875 39.95574399904351, -105.1605739993225 39.95553199876508, -105.1605070003541 39.955487998663, -105.160507601197 39.95548743481859, -105.160553485336 39.95544433019448, -105.1605729992732 39.95542599889634, -105.1605708372656 39.95542490543037, -105.1604879993213 39.95538299862599, -105.1603829998639 39.95530799832515, -105.1594730000078 39.95466099895394, -105.1568089995898 39.95264699943566, -105.1564621234448 39.95235626096443, -105.155603998905 39.95163699829544, -105.154634999516 39.95082499893148, -105.1545469991415 39.95082499900798, -105.1543240000297 39.95082499846626, -105.1538259995572 39.95043899936822, -105.1526479997484 39.94953399844792, -105.1520270002295 39.94907999894239, -105.1510029999227 39.9483689989986, -105.1505859991704 39.94808599920534, -105.1502339997436 39.94785999905235, -105.1493769991665 39.94730899849206, -105.1487869967502 39.94692837327946, -105.1483709999483 39.94665999878806, -105.1479109994562 39.94636399921564, -105.1470224473384 39.94578389403245, -105.1469689981003 39.94574899894534, -105.1465979998178 39.94550799907834, -105.1444109992605 39.94408999827592, -105.1438049994702 39.94369699936311, -105.1436849993157 39.94361699895295, -105.1435829995349 39.94355199879121, -105.1429179998172 39.94312999953807, -105.1415170000054 39.9422179981579, -105.141208999877 39.9420169995477, -105.1409599991531 39.94185799904378, -105.1405889992587 39.94161999863454, -105.1400129996827 39.94124299866457, -105.1380069982713 39.93995099908016, -105.1376659994644 39.93973899908963, -105.1376101742235 39.93970626003536, -105.1376106683007 39.93974719309715, -105.13757654182 39.9397486123599, -105.1370090029643 39.93974203840741, -105.1364432759128 39.93974592316794, -105.1309208893939 39.93966636177272, -105.1305578104314 39.93965950845269, -105.129260217686 39.93962179633774, -105.1281533050244 39.93958961368488, -105.1280999834125 39.93958806354111, -105.1281027487722 39.93982376694078, -105.1281160435918 39.94095694729186, -105.1281166731066 39.94131881581806, -105.1281179815044 39.94209470227083, -105.1281188559567 39.9426128500413, -105.128119170051 39.94275986892613, -105.1281189566972 39.94321673837639, -105.1281202734379 39.94328281974127, -105.1280154169606 39.94328510754713, -105.1280107097569 39.9438364185598, -105.1279857222323 39.94676288303474, -105.1279608891086 39.94967093417858, -105.1279535055246 39.95053550276305, -105.127953497769 39.95054658538529, -105.1279522914871 39.95238450217838, -105.1279511266712 39.9541802399316, -105.1280631665933 39.95781743936814, -105.1152851635068 39.95784843935154, -105.1152741627195 39.96032944007523, -105.1145691634786 39.96033344011676, -105.1145961633331 39.95785343948453, -105.1093269879348 39.95789786884638, -105.1093269988958 39.95789799857891, -105.1081605804928 39.95790194404009, -105.108159162151 39.95790844019832, -105.1081481615724 39.95847244081943, -105.1078871611286 39.95851244033037, -105.1079021614665 39.95931444023918, -105.1093821626999 39.95928944047934, -105.1093741622733 39.95969644064292, -105.1092751638475 39.97241644265112, -105.1092231749659 39.97382200756769, -105.1092199916418 39.97462689328338, -105.1092260671889 39.97499889140114, -105.1092339554898 39.97511696238349, -105.1092758343959 39.97528099404412, -105.1092904101518 39.97530904500583, -105.1092964823203 39.97532071473902, -105.1092491642645 39.97610344217862, -105.1108412041789 39.97609179069381, -105.1108470594524 39.97608530949304, -105.1117668377299 39.9760899171973, -105.1123831027614 39.97608512830671, -105.1133790200561 39.97608188493721, -105.1133870040023 39.97608190631396, -105.1132631646667 39.97570744192655, -105.113406165381 39.97567644266403, -105.1135711643946 39.97554144292338, -105.1140021644149 39.97552144240487, -105.114358165628 39.97545244199855, -105.1158010195454 39.97481841383456, -105.1171265636503 39.97423590742287, -105.1171981652229 39.97420444199783, -105.118018165306 39.97395344192811, -105.1182721659632 39.97381044163679, -105.1186161666875 39.97368444138921, -105.1186181657589 39.97287744155079, -105.1194881869002 39.97287256612985, -105.1203420443671 39.97286990956984, -105.1206801658403 39.97287044195357, -105.1209041446044 39.97286348814555, -105.1211677547576 39.97285530417747, -105.1212921660192 39.9728514412086, -105.1214051667389 39.9728474415511, -105.1217242765111 39.97281619705816, -105.1229011674566 39.97270644080103, -105.1241911675568 39.97273944124998, -105.1242581672639 39.97274644167108, -105.1244201369517 39.97276780367894, -105.1245523833219 39.97278895695491, -105.1246601669836 39.97280844165002, -105.1247921674847 39.97283644067091, -105.1248531668425 39.97285044186012, -105.1249011680386 39.97286244087732, -105.1249497653521 39.97287524610411, -105.1250681668962 39.972906441131, -105.1251781675552 39.97293944155944, -105.1252489123642 39.97296264565752, -105.1253031669845 39.97298044167606, -105.1254030021113 39.97301706732278, -105.1254721676893 39.97304244124539, -105.125568498434 39.97308157000424, -105.1256304425993 39.97260260723626, -105.1256339410851 39.97236269794815, -105.1256813227789 39.96875778727393, -105.1260857937713 39.96875972803437, -105.1269735298878 39.96876419450597, -105.127061221905 39.9687646845617, -105.1274844113412 39.96876705475879, -105.1275570164911 39.96876746234612, -105.1280108127828 39.96877000157099, -105.1283536248506 39.96877385278868, -105.1284532215353 39.96877325434858, -105.128553963989 39.9690911268271, -105.1288680870524 39.97011308536674, -105.1289943503059 39.97052774621444, -105.1291247538012 39.97093561123375, -105.1292770345935 39.97141508682, -105.1293981153291 39.97178608088523, -105.1295809285128 39.97234769805092, -105.1296648708499 39.97234691583657, -105.1296709720262 39.97234693273894, -105.1298094143496 39.97234732795977, -105.1301103864602 39.97234818710459, -105.1301840582684 39.97234839379923, -105.1306659725923 39.97234976349554, -105.1307176733622 39.97234991204898, -105.1309714865439 39.97235173645367, -105.1313794898227 39.97235471554273, -105.1314539558249 39.9723552617133, -105.1316832172676 39.97235693758834, -105.1319873907501 39.97235915665501, -105.1322020387081 39.97236225831516, -105.1326031913209 39.97237094391207, -105.1326092883675 39.97237107593023, -105.1326240548662 39.97237145444323, -105.1327149078208 39.97237232493223, -105.1327149084221 39.97237221325229, -105.1327153345106 39.97237221641146, -105.132714663984 39.97135212374958))</t>
+          <t>POLYGON ((-105.13271466398398 39.971352123749575, -105.13271460545486 39.97135212356304, -105.13271455791606 39.97119025763981, -105.1327142628682 39.97019653200053, -105.1327193515535 39.96995687077294, -105.13272283375075 39.969866895986286, -105.13271953151714 39.96947027243025, -105.13271514128239 39.9691659558876, -105.13271805924214 39.968888972455204, -105.13272908744628 39.968828887610904, -105.13277398047853 39.96877412640302, -105.13281692407482 39.96875010571533, -105.13287713854848 39.96873773783532, -105.13289789787048 39.96873783278408, -105.13297290524663 39.968737974413195, -105.13342210398528 39.96873693358972, -105.1339458879853 39.96873310802705, -105.134616987672 39.968736060862796, -105.13489705978346 39.96873694847295, -105.13568066576039 39.96874485295404, -105.14097185709069 39.9687743257597, -105.14114848347856 39.96875700316673, -105.14134372963943 39.96873258971108, -105.14154386448264 39.96866172247041, -105.1416835511761 39.96860139021794, -105.1418093763021 39.96852671673524, -105.14191733811258 39.968428927110956, -105.14204333842906 39.96830892639375, -105.14207433827117 39.968262925987595, -105.14215033835444 39.96812792517319, -105.14220747298562 39.967913139299974, -105.14221133669608 39.96770492316075, -105.14217677618532 39.96667984017955, -105.14219341141487 39.96616516356316, -105.14222673600742 39.96601156303456, -105.14227843463836 39.965897339659605, -105.14240032033774 39.96568682201359, -105.14252179211657 39.96555494231168, -105.14270831873786 39.96541969037425, -105.14289932071657 39.96531662179055, -105.14315996441672 39.96522091709688, -105.14326077661686 39.96519209645445, -105.14350878486904 39.96517236669215, -105.14477033683178 39.96518290919838, -105.14581934084656 39.96518290820572, -105.14636234310242 39.965182907762504, -105.1464993430814 39.96518190774901, -105.14680234457477 39.96518190732379, -105.14688434480763 39.9651819073298, -105.14869440011198 39.965209421808346, -105.14738733909425 39.9631518974572, -105.14728333844832 39.96300889746738, -105.14694355694073 39.96253178409309, -105.14696482935197 39.96118358125917, -105.14714332924608 39.9610888885334, -105.14742332928822 39.9608348874724, -105.14747832929355 39.960673887042155, -105.14754132892394 39.96058288607245, -105.14770232988428 39.960539885509284, -105.14791132996652 39.960529885685474, -105.14816333092517 39.960502885319926, -105.148442331826 39.960438884784786, -105.14855198325488 39.9603747977174, -105.14863608968113 39.96027854212333, -105.14878078575276 39.960143151920214, -105.14882802604059 39.959989592771684, -105.14881025556731 39.959832259866445, -105.14888988240219 39.95970382063977, -105.14893225739489 39.95959314057911, -105.1489191124549 39.95943939649989, -105.14891507528137 39.9593214255841, -105.14892959825569 39.95920708593706, -105.14896249858015 39.95913212151229, -105.14896306860943 39.9590213131738, -105.14911238700965 39.95888951135321, -105.1492801913796 39.9587756383149, -105.14938757463689 39.95866872974738, -105.14950894815253 39.958551140369174, -105.14957663922996 39.95845433338604, -105.14960744532426 39.95836556608734, -105.14966804909628 39.95832285639452, -105.1498075423503 39.95829468443688, -105.1499234796544 39.95833078124081, -105.15006737968514 39.95834909104068, -105.15017876484532 39.95836730195432, -105.15035995217428 39.95836070242881, -105.15049467190673 39.958357537308395, -105.15100675950825 39.95813389543042, -105.15111413905069 39.958026985248146, -105.15126314057838 39.95795594635907, -105.15148177634237 39.95789226645639, -105.15172363731062 39.95782865724059, -105.15203056127018 39.95775809457165, -105.15219933581484 39.95775386844422, -105.15240633630674 39.95768886822943, -105.15261933677253 39.95766986805643, -105.15276233686697 39.95764386738736, -105.15288133755988 39.95762886696753, -105.15312333793932 39.957563866420585, -105.15323133889504 39.957552866584855, -105.15343433951236 39.95747686623236, -105.15355733912922 39.957416865731595, -105.15362633936248 39.9573298649078, -105.15374363343398 39.95701975793894, -105.15376233765683 39.9569568633737, -105.15379526970891 39.95691267774466, -105.15387907556105 39.95687361027492, -105.15396933809366 39.956842862622075, -105.15405833900346 39.9568058623279, -105.15419546306869 39.956767324863364, -105.15430697349913 39.95676051091827, -105.15444161749252 39.95677163805132, -105.15455305670235 39.95677912074012, -105.15464119830736 39.956800832382484, -105.15470159858656 39.956797438677334, -105.15474804561359 39.956797577855134, -105.15484564012878 39.95678714697017, -105.15495725896889 39.956758885291215, -105.15506441451677 39.956694864728, -105.15519936553133 39.95664522612983, -105.1553156290344 39.95661697800303, -105.15543644724357 39.95660661518612, -105.15553405942464 39.956592609050276, -105.15565959356785 39.95656796301251, -105.15583134342742 39.956445858413865, -105.15603334381272 39.95633185794351, -105.15612734452172 39.95625685770177, -105.15621634475905 39.95622285764431, -105.1563643445258 39.95621085739178, -105.15650234509707 39.956184856995996, -105.15657134511264 39.95615085648439, -105.15661634571471 39.9560978561319, -105.15669034493668 39.95593085549667, -105.15674434401129 39.95587785488445, -105.15689734481711 39.95573785436316, -105.15704534492801 39.955639853668565, -105.15735234540561 39.95551485287092, -105.15750534561661 39.95549185275024, -105.15779934794274 39.955514851897156, -105.15804334821037 39.95544885175151, -105.15815134837301 39.95544185164904, -105.15826734856834 39.955417851787885, -105.15840134896565 39.95539185076902, -105.15847734876488 39.9553558505898, -105.15855734900829 39.95530785100657, -105.15859934867916 39.95524535072974, -105.15862234938382 39.95516784949032, -105.15864634924095 39.95512151586125, -105.15883522491622 39.955213342786884, -105.15973881188577 39.95581121070809, -105.15997538855308 39.9559715043019, -105.16031462715864 39.955660662925084, -105.16113964676515 39.956151309506254, -105.1611820283237 39.95589271854974, -105.16092399908746 39.955743999043506, -105.16057399932254 39.95553199876508, -105.16050700035407 39.955487998663, -105.16050760119697 39.95548743481859, -105.16055348533597 39.95544433019448, -105.16057299927321 39.95542599889634, -105.16057083726557 39.95542490543037, -105.16048799932132 39.955382998625986, -105.16038299986391 39.95530799832515, -105.15947300000778 39.95466099895394, -105.15680899958977 39.952646999435665, -105.15646212344481 39.95235626096443, -105.15560399890504 39.95163699829544, -105.15463499951605 39.95082499893148, -105.1545469991415 39.95082499900798, -105.15432400002966 39.95082499846626, -105.15382599955721 39.950438999368224, -105.1526479997484 39.94953399844792, -105.15202700022954 39.949079998942395, -105.15100299992268 39.948368998998596, -105.1505859991704 39.94808599920534, -105.15023399974363 39.94785999905235, -105.14937699916646 39.94730899849206, -105.14878699675018 39.946928373279455, -105.14837099994834 39.946659998788064, -105.14791099945617 39.94636399921564, -105.14702244733836 39.94578389403245, -105.14696899810028 39.94574899894534, -105.14659799981776 39.945507999078345, -105.14441099926047 39.94408999827592, -105.14380499947022 39.94369699936311, -105.14368499931568 39.943616998952955, -105.14358299953487 39.94355199879121, -105.1429179998172 39.943129999538066, -105.14151700000538 39.9422179981579, -105.14120899987702 39.942016999547704, -105.14095999915313 39.94185799904378, -105.14058899925865 39.941619998634536, -105.1400129996827 39.94124299866457, -105.13800699827127 39.93995099908016, -105.13766599946442 39.93973899908963, -105.13761017422354 39.93970626003536, -105.13761066830068 39.939747193097155, -105.13757654182001 39.9397486123599, -105.13700900296429 39.93974203840741, -105.13644327591278 39.93974592316794, -105.13092088939388 39.939666361772716, -105.13055781043143 39.93965950845269, -105.12926021768598 39.93962179633774, -105.12815330502438 39.93958961368488, -105.12809998341253 39.93958806354111, -105.12810274877225 39.939823766940776, -105.12811604359183 39.94095694729186, -105.12811667310663 39.94131881581806, -105.1281179815044 39.94209470227083, -105.12811885595674 39.9426128500413, -105.12811917005104 39.94275986892613, -105.12811895669716 39.94321673837639, -105.12812027343794 39.94328281974127, -105.12801541696062 39.94328510754713, -105.12801070975691 39.943836418559805, -105.12798572223228 39.946762883034744, -105.12796088910865 39.94967093417858, -105.12795350552462 39.95053550276305, -105.12795349776896 39.95054658538529, -105.12795229148715 39.95238450217838, -105.12795112667123 39.9541802399316, -105.12806316659325 39.95781743936814, -105.11528516350681 39.95784843935154, -105.1152741627195 39.960329440075235, -105.11456916347859 39.96033344011676, -105.11459616333309 39.95785343948453, -105.10932698793475 39.95789786884638, -105.10932699889575 39.95789799857891, -105.10816058049275 39.95790194404009, -105.10815916215097 39.95790844019832, -105.10814816157236 39.95847244081943, -105.1078871611286 39.95851244033037, -105.10790216146646 39.959314440239176, -105.10938216269992 39.95928944047934, -105.10937416227326 39.959696440642915, -105.10927516384749 39.972416442651124, -105.10922317496588 39.97382200756769, -105.10921999164184 39.97462689328338, -105.10922606718886 39.974998891401135, -105.10923395548977 39.97511696238349, -105.10927583439593 39.97528099404412, -105.10929041015177 39.97530904500583, -105.10929648232026 39.97532071473902, -105.10924916426448 39.97610344217862, -105.11084120417891 39.976091790693815, -105.11084705945237 39.97608530949304, -105.11176683772987 39.9760899171973, -105.11238310276143 39.976085128306714, -105.11337902005612 39.97608188493721, -105.1133870040023 39.97608190631396, -105.1132631646667 39.97570744192655, -105.11340616538101 39.97567644266403, -105.11357116439456 39.97554144292338, -105.11400216441494 39.97552144240487, -105.11435816562796 39.97545244199855, -105.11580101954537 39.97481841383456, -105.11712656365034 39.974235907422866, -105.11719816522287 39.974204441997834, -105.11801816530597 39.97395344192811, -105.1182721659632 39.97381044163679, -105.11861616668753 39.97368444138921, -105.11861816575893 39.97287744155079, -105.11948818690017 39.97287256612985, -105.12034204436713 39.972869909569845, -105.12068016584033 39.972870441953575, -105.12090414460438 39.97286348814555, -105.12116775475764 39.97285530417747, -105.12129216601923 39.9728514412086, -105.12140516673887 39.972847441551096, -105.12172427651106 39.97281619705816, -105.12290116745665 39.972706440801026, -105.1241911675568 39.97273944124998, -105.12425816726389 39.972746441671084, -105.12442013695171 39.97276780367894, -105.12455238332191 39.972788956954915, -105.12466016698356 39.97280844165002, -105.12479216748471 39.97283644067091, -105.1248531668425 39.972850441860125, -105.12490116803862 39.97286244087732, -105.12494976535206 39.97287524610411, -105.1250681668962 39.972906441131, -105.12517816755525 39.97293944155944, -105.12524891236417 39.972962645657525, -105.1253031669845 39.972980441676064, -105.12540300211128 39.97301706732278, -105.12547216768927 39.97304244124539, -105.12556849843396 39.97308157000424, -105.12563044259932 39.97260260723626, -105.12563394108514 39.97236269794815, -105.1256813227789 39.96875778727393, -105.12608579377134 39.96875972803437, -105.12697352988779 39.96876419450597, -105.127061221905 39.9687646845617, -105.12748441134124 39.96876705475879, -105.12755701649105 39.96876746234612, -105.12801081278276 39.96877000157099, -105.1283536248506 39.96877385278868, -105.1284532215353 39.96877325434858, -105.12855396398898 39.9690911268271, -105.12886808705242 39.97011308536674, -105.12899435030594 39.970527746214444, -105.12912475380116 39.97093561123375, -105.12927703459351 39.97141508682, -105.12939811532907 39.97178608088523, -105.12958092851277 39.97234769805092, -105.1296648708499 39.97234691583657, -105.12967097202625 39.97234693273894, -105.1298094143496 39.972347327959774, -105.1301103864602 39.972348187104586, -105.13018405826844 39.97234839379923, -105.13066597259227 39.97234976349554, -105.13071767336216 39.97234991204898, -105.13097148654386 39.97235173645367, -105.13137948982275 39.97235471554273, -105.13145395582487 39.972355261713304, -105.13168321726762 39.97235693758834, -105.13198739075007 39.97235915665501, -105.13220203870807 39.97236225831516, -105.13260319132092 39.97237094391207, -105.13260928836748 39.97237107593023, -105.13262405486618 39.97237145444323, -105.13271490782084 39.97237232493223, -105.13271490842207 39.97237221325229, -105.13271533451059 39.972372216411465, -105.13271466398398 39.971352123749575))</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -970,7 +970,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1469435569407 39.96253178409309, -105.1472833384483 39.96300889746738, -105.1473873390943 39.9631518974572, -105.148694400112 39.96520942180835, -105.1491546814992 39.96520549842712, -105.1499591002229 39.96520089786635, -105.1528301109463 39.96518103268608, -105.1554532690506 39.96514994269476, -105.1563762083814 39.9651309339529, -105.1580453725514 39.96512093089092, -105.1583707543674 39.96511069713443, -105.1585646253969 39.9650952948947, -105.1587585229728 39.96507456680651, -105.1589524603611 39.96504584965834, -105.1591741481606 39.96500389980679, -105.1593023204964 39.96497765080175, -105.1596004190962 39.96488000674642, -105.1600663952859 39.96469988937269, -105.1606614234813 39.96446507215775, -105.1610773868694 39.96432516649111, -105.161389229453 39.96424619829306, -105.16169407117 39.9641831855031, -105.1620542665501 39.96412299749996, -105.1623984016815 39.96409488425228, -105.1626480901568 39.96407354029382, -105.1633384051544 39.9640808828587, -105.1641930794864 39.96408398179263, -105.164483696346 39.96409814183401, -105.1647484114118 39.96413788198119, -105.1649780902026 39.96419277954295, -105.1653133155886 39.96428428971744, -105.1655931600189 39.96437830147045, -105.1658954174411 39.96449888213142, -105.1658948481799 39.96259403227716, -105.1658790077759 39.96191819436262, -105.1658690419163 39.96169103439433, -105.1658632077242 39.96100519839205, -105.1658572573323 39.96030582959796, -105.1658540832327 39.95993247886946, -105.1658491420113 39.95935187665621, -105.1658796374968 39.95890351659605, -105.1658829843055 39.95798883313223, -105.1657049993032 39.95791899851163, -105.1655459994386 39.95785699862255, -105.1640439992191 39.95727199887524, -105.1635449998441 39.95706699912397, -105.163260000118 39.95693999941128, -105.1629539988249 39.95680199904174, -105.1626729999983 39.95667199866357, -105.1623139998591 39.95649799874107, -105.162090999951 39.95638499933245, -105.1615179991773 39.95607999946219, -105.1612710001578 39.9559439989421, -105.1611820283237 39.95589271854974, -105.1611396467652 39.95615130950625, -105.1603146271586 39.95566066292508, -105.1599753885531 39.9559715043019, -105.1597388118858 39.95581121070809, -105.1588352249162 39.95521334278688, -105.158646349241 39.95512151586125, -105.1586223493838 39.95516784949032, -105.1585993486792 39.95524535072974, -105.1585573490083 39.95530785100657, -105.1584773487649 39.9553558505898, -105.1584013489657 39.95539185076902, -105.1582673485683 39.95541785178789, -105.158151348373 39.95544185164904, -105.1580433482104 39.95544885175151, -105.1577993479427 39.95551485189716, -105.1575053456166 39.95549185275024, -105.1573523454056 39.95551485287092, -105.157045344928 39.95563985366856, -105.1568973448171 39.95573785436316, -105.1567443440113 39.95587785488445, -105.1566903449367 39.95593085549667, -105.1566163457147 39.9560978561319, -105.1565713451126 39.95615085648439, -105.1565023450971 39.956184856996, -105.1563643445258 39.95621085739178, -105.156216344759 39.95622285764431, -105.1561273445217 39.95625685770177, -105.1560333438127 39.95633185794351, -105.1558313434274 39.95644585841386, -105.1556595935678 39.95656796301251, -105.1555340594246 39.95659260905028, -105.1554364472436 39.95660661518612, -105.1553156290344 39.95661697800303, -105.1551993655313 39.95664522612983, -105.1550644145168 39.956694864728, -105.1549572589689 39.95675888529122, -105.1548456401288 39.95678714697017, -105.1547480456136 39.95679757785513, -105.1547015985866 39.95679743867733, -105.1546411983074 39.95680083238248, -105.1545530567024 39.95677912074012, -105.1544416174925 39.95677163805132, -105.1543069734991 39.95676051091827, -105.1541954630687 39.95676732486336, -105.1540583390035 39.9568058623279, -105.1539693380937 39.95684286262208, -105.1538790755611 39.95687361027492, -105.1537952697089 39.95691267774466, -105.1537623376568 39.9569568633737, -105.153743633434 39.95701975793894, -105.1536263393625 39.9573298649078, -105.1535573391292 39.9574168657316, -105.1534343395124 39.95747686623236, -105.153231338895 39.95755286658486, -105.1531233379393 39.95756386642059, -105.1528813375599 39.95762886696753, -105.152762336867 39.95764386738736, -105.1526193367725 39.95766986805643, -105.1524063363067 39.95768886822943, -105.1521993358148 39.95775386844422, -105.1520305612702 39.95775809457165, -105.1517236373106 39.95782865724059, -105.1514817763424 39.95789226645639, -105.1512631405784 39.95795594635907, -105.1511141390507 39.95802698524815, -105.1510067595082 39.95813389543042, -105.1504946719067 39.95835753730839, -105.1503599521743 39.95836070242881, -105.1501787648453 39.95836730195432, -105.1500673796851 39.95834909104068, -105.1499234796544 39.95833078124081, -105.1498075423503 39.95829468443688, -105.1496680490963 39.95832285639452, -105.1496074453243 39.95836556608734, -105.14957663923 39.95845433338604, -105.1495089481525 39.95855114036917, -105.1493875746369 39.95866872974738, -105.1492801913796 39.9587756383149, -105.1491123870097 39.95888951135321, -105.1489630686094 39.9590213131738, -105.1489624985801 39.95913212151229, -105.1489295982557 39.95920708593706, -105.1489150752814 39.9593214255841, -105.1489191124549 39.95943939649989, -105.1489322573949 39.95959314057911, -105.1488898824022 39.95970382063977, -105.1488102555673 39.95983225986645, -105.1488280260406 39.95998959277168, -105.1487807857528 39.96014315192021, -105.1486360896811 39.96027854212333, -105.1485519832549 39.9603747977174, -105.148442331826 39.96043888478479, -105.1481633309252 39.96050288531993, -105.1479113299665 39.96052988568547, -105.1477023298843 39.96053988550928, -105.1475413289239 39.96058288607245, -105.1474783292935 39.96067388704216, -105.1474233292882 39.9608348874724, -105.1471433292461 39.9610888885334, -105.146964829352 39.96118358125917, -105.1469435569407 39.96253178409309))</t>
+          <t>POLYGON ((-105.14694355694073 39.96253178409309, -105.14728333844832 39.96300889746738, -105.14738733909425 39.9631518974572, -105.14869440011198 39.965209421808346, -105.14915468149916 39.96520549842712, -105.14995910022286 39.965200897866346, -105.15283011094628 39.96518103268608, -105.15545326905064 39.96514994269476, -105.1563762083814 39.9651309339529, -105.15804537255138 39.96512093089092, -105.15837075436744 39.96511069713443, -105.15856462539693 39.9650952948947, -105.1587585229728 39.965074566806514, -105.1589524603611 39.96504584965834, -105.15917414816059 39.96500389980679, -105.15930232049637 39.96497765080175, -105.15960041909622 39.96488000674642, -105.16006639528587 39.96469988937269, -105.16066142348126 39.96446507215775, -105.16107738686935 39.964325166491115, -105.161389229453 39.96424619829306, -105.16169407117 39.964183185503096, -105.16205426655006 39.964122997499956, -105.16239840168153 39.96409488425228, -105.16264809015685 39.964073540293825, -105.16333840515442 39.9640808828587, -105.16419307948638 39.964083981792626, -105.16448369634598 39.96409814183401, -105.16474841141184 39.964137881981195, -105.1649780902026 39.96419277954295, -105.16531331558865 39.96428428971744, -105.16559316001887 39.964378301470454, -105.16589541744115 39.96449888213142, -105.16589484817989 39.96259403227716, -105.16587900777587 39.96191819436262, -105.16586904191627 39.96169103439433, -105.16586320772421 39.96100519839205, -105.16585725733235 39.96030582959796, -105.16585408323267 39.95993247886946, -105.1658491420113 39.959351876656214, -105.16587963749681 39.958903516596045, -105.1658829843055 39.957988833132234, -105.16570499930324 39.95791899851163, -105.16554599943859 39.957856998622546, -105.16404399921912 39.957271998875235, -105.16354499984406 39.957066999123974, -105.16326000011804 39.95693999941128, -105.16295399882495 39.95680199904174, -105.16267299999834 39.95667199866357, -105.16231399985905 39.95649799874107, -105.16209099995102 39.95638499933245, -105.16151799917733 39.95607999946219, -105.16127100015778 39.9559439989421, -105.1611820283237 39.95589271854974, -105.16113964676515 39.956151309506254, -105.16031462715864 39.955660662925084, -105.15997538855308 39.9559715043019, -105.15973881188577 39.95581121070809, -105.15883522491622 39.955213342786884, -105.15864634924095 39.95512151586125, -105.15862234938382 39.95516784949032, -105.15859934867916 39.95524535072974, -105.15855734900829 39.95530785100657, -105.15847734876488 39.9553558505898, -105.15840134896565 39.95539185076902, -105.15826734856834 39.955417851787885, -105.15815134837301 39.95544185164904, -105.15804334821037 39.95544885175151, -105.15779934794274 39.955514851897156, -105.15750534561661 39.95549185275024, -105.15735234540561 39.95551485287092, -105.15704534492801 39.955639853668565, -105.15689734481711 39.95573785436316, -105.15674434401129 39.95587785488445, -105.15669034493668 39.95593085549667, -105.15661634571471 39.9560978561319, -105.15657134511264 39.95615085648439, -105.15650234509707 39.956184856995996, -105.1563643445258 39.95621085739178, -105.15621634475905 39.95622285764431, -105.15612734452172 39.95625685770177, -105.15603334381272 39.95633185794351, -105.15583134342742 39.956445858413865, -105.15565959356785 39.95656796301251, -105.15553405942464 39.956592609050276, -105.15543644724357 39.95660661518612, -105.1553156290344 39.95661697800303, -105.15519936553133 39.95664522612983, -105.15506441451677 39.956694864728, -105.15495725896889 39.956758885291215, -105.15484564012878 39.95678714697017, -105.15474804561359 39.956797577855134, -105.15470159858656 39.956797438677334, -105.15464119830736 39.956800832382484, -105.15455305670235 39.95677912074012, -105.15444161749252 39.95677163805132, -105.15430697349913 39.95676051091827, -105.15419546306869 39.956767324863364, -105.15405833900346 39.9568058623279, -105.15396933809366 39.956842862622075, -105.15387907556105 39.95687361027492, -105.15379526970891 39.95691267774466, -105.15376233765683 39.9569568633737, -105.15374363343398 39.95701975793894, -105.15362633936248 39.9573298649078, -105.15355733912922 39.957416865731595, -105.15343433951236 39.95747686623236, -105.15323133889504 39.957552866584855, -105.15312333793932 39.957563866420585, -105.15288133755988 39.95762886696753, -105.15276233686697 39.95764386738736, -105.15261933677253 39.95766986805643, -105.15240633630674 39.95768886822943, -105.15219933581484 39.95775386844422, -105.15203056127018 39.95775809457165, -105.15172363731062 39.95782865724059, -105.15148177634237 39.95789226645639, -105.15126314057838 39.95795594635907, -105.15111413905069 39.958026985248146, -105.15100675950825 39.95813389543042, -105.15049467190673 39.958357537308395, -105.15035995217428 39.95836070242881, -105.15017876484532 39.95836730195432, -105.15006737968514 39.95834909104068, -105.1499234796544 39.95833078124081, -105.1498075423503 39.95829468443688, -105.14966804909628 39.95832285639452, -105.14960744532426 39.95836556608734, -105.14957663922996 39.95845433338604, -105.14950894815253 39.958551140369174, -105.14938757463689 39.95866872974738, -105.1492801913796 39.9587756383149, -105.14911238700965 39.95888951135321, -105.14896306860943 39.9590213131738, -105.14896249858015 39.95913212151229, -105.14892959825569 39.95920708593706, -105.14891507528137 39.9593214255841, -105.1489191124549 39.95943939649989, -105.14893225739489 39.95959314057911, -105.14888988240219 39.95970382063977, -105.14881025556731 39.959832259866445, -105.14882802604059 39.959989592771684, -105.14878078575276 39.960143151920214, -105.14863608968113 39.96027854212333, -105.14855198325488 39.9603747977174, -105.148442331826 39.960438884784786, -105.14816333092517 39.960502885319926, -105.14791132996652 39.960529885685474, -105.14770232988428 39.960539885509284, -105.14754132892394 39.96058288607245, -105.14747832929355 39.960673887042155, -105.14742332928822 39.9608348874724, -105.14714332924608 39.9610888885334, -105.14696482935197 39.96118358125917, -105.14694355694073 39.96253178409309))</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1012,7 +1012,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1511840458521 39.97762806941142, -105.1503649180572 39.97797809023514, -105.1504028475811 39.97802706963947, -105.1505558997787 39.97824193563466, -105.1506618817289 39.97838088993017, -105.1508070352091 39.97853588555293, -105.1510139320686 39.97868887123922, -105.1512419852102 39.97882188090264, -105.1514890587039 39.97893408385762, -105.1516928440833 39.97899811433265, -105.1519758743095 39.9790568933244, -105.1521720292124 39.97907807448019, -105.1525968273794 39.97911696440125, -105.1546161157948 39.97927209810255, -105.1549860097431 39.97930203055521, -105.155197887842 39.97931886110557, -105.1552770308644 39.97933392266862, -105.155458033647 39.979387995404, -105.1556128761117 39.97946395135801, -105.1557479917776 39.97955988874499, -105.1558980182553 39.97945903783057, -105.156023870116 39.97933999693076, -105.1561128433848 39.97910389984132, -105.1561968984269 39.97892296596781, -105.1563260121182 39.97872295083356, -105.156485026981 39.97853702451009, -105.1566929394302 39.9783490478104, -105.1568391167868 39.97823198766081, -105.1569161223485 39.97817511693055, -105.1570940838718 39.97805293534529, -105.1575379103652 39.97785495259414, -105.1577030738282 39.97779394982241, -105.1580100081515 39.97771113208039, -105.1583250364957 39.97765112328229, -105.1585060459044 39.97763189385436, -105.1589089590516 39.9776221060531, -105.1590099389456 39.97762295333611, -105.1597729990135 39.97766391584672, -105.159924944536 39.97767699238972, -105.160191846309 39.97767887746299, -105.1604571169876 39.97765001132789, -105.1607118328299 39.97759091532916, -105.1612810554912 39.97743199485603, -105.1615300344844 39.97737809680851, -105.1617588644038 39.97735790479039, -105.1620400653798 39.97735406243233, -105.162320075189 39.97737492366687, -105.1625211587942 39.97740900359284, -105.1626900249334 39.97746412824674, -105.1628509077528 39.97754613107234, -105.1629831715816 39.97764287573666, -105.1630970814578 39.97777113558509, -105.1633348417548 39.97803811539852, -105.163456094038 39.97812494352087, -105.1636401340146 39.97821497466567, -105.1637919096834 39.97826291009962, -105.1638721328699 39.97827604690609, -105.1641139846472 39.97829294847602, -105.1644808270593 39.97828989908837, -105.1650300462948 39.97827996626899, -105.1652778920959 39.97823895876851, -105.165331838292 39.97822593878153, -105.1656070754674 39.97820203074534, -105.165639904273 39.97820212598116, -105.1657440951674 39.97820297757695, -105.1658379434426 39.978202974992, -105.1658350282252 39.97862794311265, -105.1660539287566 39.97862565398879, -105.1679504485915 39.97863091778471, -105.1688872339223 39.97863350366777, -105.1698279435228 39.97863609678081, -105.1705561331186 39.97863809480832, -105.1707601398161 39.97863865429652, -105.1713767703544 39.97863884954739, -105.1736004540525 39.97863952981174, -105.1737145515828 39.97863956374063, -105.1746315779191 39.97863985840293, -105.1749131590959 39.97863994859521, -105.1753102988506 39.97864007456597, -105.1753077055884 39.97815307154284, -105.1753071625874 39.97807062647465, -105.1753066251767 39.97798897490134, -105.1753039309026 39.97757977851963, -105.1752998415047 39.97695824622881, -105.1752957663743 39.97633889713853, -105.1752921682676 39.97579225049291, -105.1752921268262 39.97576430925468, -105.1752933364211 39.97554706487885, -105.1752932053162 39.97554706270822, -105.1752952276789 39.97514060311426, -105.1752970387502 39.97477164542337, -105.1752987049537 39.97441934769093, -105.1752986424906 39.97332390459598, -105.1752986400875 39.97327644619253, -105.1752986321791 39.97312339547399, -105.1752993592102 39.97299154292094, -105.1753000521294 39.97286562741104, -105.1753029543753 39.97233821445883, -105.1753040182588 39.97230874160383, -105.1753349979691 39.97230887841319, -105.1754036449972 39.97230917804725, -105.1761817574226 39.97231257916473, -105.1775629965025 39.97231860602722, -105.1782463742659 39.97232158132549, -105.1792927120879 39.97232533345959, -105.1797370086139 39.9723251692939, -105.1802034669848 39.97232431015902, -105.1807346165126 39.97232332753696, -105.181313336771 39.97232225425414, -105.1818888682263 39.97232118367459, -105.1824693614918 39.97231969607867, -105.1825779238971 39.97232006357458, -105.1826878500371 39.97232043832547, -105.1827443502702 39.97231958783131, -105.1827049815247 39.96884194995791, -105.1826965883272 39.96810050650755, -105.1834828991021 39.96810018023088, -105.1843769878934 39.96809980246061, -105.184378790729 39.9663747723468, -105.1845014339616 39.96523026465304, -105.1836529999933 39.96489799860698, -105.182328924705 39.96438302610748, -105.1823765858315 39.96435856048586, -105.1829501799709 39.96406143557106, -105.1831431795536 39.96390943620628, -105.183359179438 39.96390543564833, -105.1846811801298 39.96359143505422, -105.1846831809932 39.96346543564761, -105.1850871806001 39.96337543512138, -105.1852101802556 39.96334743554963, -105.1859091799674 39.96319543556243, -105.1867561809799 39.96303243590308, -105.1875491802892 39.96290443543483, -105.1882881813402 39.96279743543808, -105.1892731804752 39.96267043497246, -105.1892811813567 39.96148043493095, -105.1889071811083 39.96174843466853, -105.188260316038 39.96197615552799, -105.1877131813326 39.96209643507789, -105.1876121808403 39.9621674358669, -105.1872551801046 39.96227843565087, -105.187073180655 39.96230143525784, -105.1867361810641 39.96239743503643, -105.1862821800566 39.96244943611252, -105.1852781797714 39.96245943558378, -105.1851691808371 39.96256443568562, -105.1846881802595 39.96256443553224, -105.184684179543 39.96329443567719, -105.183756179454 39.96352043583736, -105.183681180111 39.96353243572506, -105.1835581803465 39.96355343554686, -105.1833721791185 39.96357743607462, -105.1832471796654 39.96358943518963, -105.1831221800468 39.96359843587509, -105.1829971802545 39.96360343569754, -105.1828711795887 39.96360543613775, -105.182745178819 39.96360443634497, -105.1826201798852 39.9636004354759, -105.1824941789573 39.96359343521812, -105.1823521786804 39.96357643573872, -105.1822441795616 39.96356843645984, -105.1821201788212 39.96355143678812, -105.1820251788167 39.96353643541125, -105.1818761791532 39.9635074363657, -105.1815991793696 39.96344043598965, -105.1815181794293 39.96341743539393, -105.1814281797796 39.9633894364229, -105.1813451795762 39.96336143602115, -105.1812645330557 39.96333272334351, -105.1811751798336 39.96329843665993, -105.1811201784924 39.96327643628931, -105.1810651795186 39.96325343616735, -105.1810111789803 39.96322943544858, -105.1809571796388 39.96320443587675, -105.1809041787385 39.96317943634221, -105.1808511790458 39.96315343615423, -105.180799178964 39.96312643537638, -105.1807481784856 39.96309843581128, -105.1806971792238 39.96307043532614, -105.1806471783964 39.96304143605229, -105.1805491783552 39.96298243605077, -105.1805011791406 39.96295143559319, -105.1804541783631 39.96292043608274, -105.1804071788043 39.96288743619242, -105.1803891795854 39.96287543542729, -105.1800231788606 39.96283243551652, -105.1791101784401 39.96248843618227, -105.1790331792207 39.9626014355022, -105.1780361786519 39.96221443573692, -105.1780248042583 39.96220476780362, -105.1779603294206 39.96230169761951, -105.1777988506388 39.9622247658564, -105.1777786369145 39.96221513532904, -105.1777779996259 39.96221599908061, -105.1777729991336 39.96222499799526, -105.175195000182 39.96134899884276, -105.1750629987647 39.96129699910314, -105.1718929991997 39.96004699882172, -105.16867899997 39.95862899864169, -105.1677549991503 39.95786999907147, -105.1672029990481 39.95741599921722, -105.1668249995467 39.95710599849211, -105.1661219997786 39.95695499897838, -105.1660599995567 39.9569419984156, -105.1660659997773 39.95698699837227, -105.1661089994848 39.95726499912967, -105.1661250002072 39.95739999859541, -105.1663429988309 39.95789999829524, -105.1663939993887 39.95801599875833, -105.1663729998672 39.95804199855646, -105.1663260779203 39.95809453148716, -105.166280999977 39.95814499912188, -105.1658829843055 39.95798883313223, -105.1658796374968 39.95890351659605, -105.1658491420113 39.95935187665621, -105.1658540832327 39.95993247886946, -105.1658572573323 39.96030582959796, -105.1658632077242 39.96100519839205, -105.1658690419163 39.96169103439433, -105.1658790077759 39.96191819436262, -105.1658948481799 39.96259403227716, -105.1658954174411 39.96449888213142, -105.1659093981826 39.9647605444362, -105.1657134604707 39.96502846372699, -105.1657337016853 39.96587189904916, -105.1659096570623 39.96587234083293, -105.1659176730908 39.96628989535596, -105.1659271352761 39.96678289958627, -105.1659328385439 39.9671163032743, -105.1659271946471 39.96736485266955, -105.1659173739074 39.96779730547408, -105.1659167013721 39.9678268415455, -105.1659173507963 39.96852063654418, -105.1659765753193 39.96870010874206, -105.1659717583129 39.96959747823431, -105.1659715425365 39.96964872511244, -105.1659682676887 39.97043932947262, -105.1661945786645 39.97070261644534, -105.1662930670842 39.9708759461761, -105.1659397850224 39.97109272097257, -105.1657812165369 39.97121736908545, -105.1656783276281 39.97135647557006, -105.1654495110187 39.9715953031206, -105.1652580859233 39.97178777022467, -105.165015469692 39.97199796091019, -105.1645654451613 39.97232091807293, -105.162966444379 39.97350192482068, -105.1625194429483 39.97376992644322, -105.1616924407705 39.97405292884947, -105.1608564390357 39.97426193043724, -105.1605892002895 39.97434552290812, -105.160370437352 39.97444093195681, -105.1598574370196 39.97471893324816, -105.1594534353477 39.97493993463027, -105.1589844345162 39.97513493662397, -105.1576284311342 39.9755679397703, -105.1553614253813 39.97627694524857, -105.1539069600931 39.97673105134181, -105.1527122301567 39.97711140868529, -105.1511840458521 39.97762806941142))</t>
+          <t>POLYGON ((-105.15118404585209 39.97762806941142, -105.15036491805724 39.97797809023514, -105.15040284758113 39.97802706963947, -105.15055589977874 39.978241935634664, -105.15066188172887 39.97838088993017, -105.15080703520906 39.97853588555293, -105.15101393206855 39.97868887123922, -105.15124198521019 39.97882188090264, -105.15148905870387 39.978934083857624, -105.15169284408326 39.97899811433265, -105.15197587430947 39.9790568933244, -105.1521720292124 39.979078074480185, -105.1525968273794 39.97911696440125, -105.15461611579481 39.97927209810255, -105.1549860097431 39.97930203055521, -105.15519788784195 39.97931886110557, -105.15527703086438 39.97933392266862, -105.15545803364702 39.979387995404, -105.15561287611168 39.979463951358014, -105.15574799177763 39.979559888744994, -105.1558980182553 39.979459037830566, -105.15602387011602 39.97933999693076, -105.15611284338485 39.97910389984132, -105.15619689842694 39.97892296596781, -105.15632601211819 39.97872295083356, -105.15648502698096 39.97853702451009, -105.15669293943022 39.9783490478104, -105.15683911678676 39.978231987660806, -105.1569161223485 39.97817511693055, -105.1570940838718 39.97805293534529, -105.15753791036516 39.97785495259414, -105.15770307382823 39.97779394982241, -105.15801000815148 39.97771113208039, -105.15832503649568 39.97765112328229, -105.1585060459044 39.97763189385436, -105.15890895905163 39.977622106053104, -105.15900993894557 39.97762295333611, -105.15977299901351 39.97766391584672, -105.15992494453604 39.97767699238972, -105.16019184630896 39.97767887746299, -105.16045711698757 39.97765001132789, -105.16071183282988 39.97759091532916, -105.16128105549124 39.977431994856026, -105.16153003448439 39.977378096808515, -105.16175886440382 39.97735790479039, -105.16204006537984 39.977354062432326, -105.16232007518902 39.97737492366687, -105.16252115879416 39.97740900359284, -105.16269002493335 39.97746412824674, -105.16285090775283 39.977546131072344, -105.16298317158157 39.97764287573666, -105.16309708145783 39.97777113558509, -105.16333484175478 39.97803811539852, -105.16345609403798 39.978124943520875, -105.16364013401457 39.97821497466567, -105.16379190968343 39.97826291009962, -105.16387213286986 39.97827604690609, -105.16411398464723 39.978292948476025, -105.16448082705932 39.978289899088374, -105.16503004629483 39.978279966268985, -105.16527789209587 39.978238958768515, -105.16533183829205 39.97822593878153, -105.16560707546739 39.978202030745344, -105.16563990427296 39.97820212598116, -105.16574409516735 39.97820297757695, -105.1658379434426 39.978202974992, -105.16583502822523 39.97862794311265, -105.1660539287566 39.978625653988786, -105.16795044859154 39.97863091778471, -105.16888723392226 39.97863350366777, -105.16982794352282 39.97863609678081, -105.1705561331186 39.97863809480832, -105.1707601398161 39.97863865429652, -105.17137677035437 39.978638849547394, -105.17360045405252 39.978639529811744, -105.17371455158282 39.97863956374063, -105.17463157791911 39.97863985840293, -105.17491315909594 39.97863994859521, -105.17531029885065 39.978640074565966, -105.17530770558837 39.97815307154284, -105.17530716258736 39.978070626474654, -105.17530662517672 39.977988974901336, -105.17530393090259 39.977579778519626, -105.1752998415047 39.97695824622881, -105.17529576637435 39.97633889713853, -105.17529216826763 39.97579225049291, -105.17529212682622 39.97576430925468, -105.17529333642108 39.975547064878846, -105.17529320531615 39.97554706270822, -105.17529522767889 39.97514060311426, -105.17529703875019 39.97477164542337, -105.17529870495368 39.97441934769093, -105.17529864249056 39.97332390459598, -105.17529864008753 39.97327644619253, -105.17529863217905 39.97312339547399, -105.17529935921023 39.97299154292094, -105.1753000521294 39.97286562741104, -105.17530295437525 39.97233821445883, -105.17530401825883 39.972308741603825, -105.17533499796909 39.97230887841319, -105.17540364499725 39.972309178047254, -105.17618175742264 39.97231257916473, -105.17756299650247 39.97231860602722, -105.17824637426594 39.97232158132549, -105.17929271208794 39.972325333459594, -105.17973700861394 39.9723251692939, -105.18020346698484 39.972324310159024, -105.18073461651261 39.97232332753696, -105.18131333677096 39.972322254254145, -105.18188886822627 39.972321183674595, -105.18246936149183 39.97231969607867, -105.18257792389707 39.97232006357458, -105.18268785003706 39.97232043832547, -105.18274435027017 39.972319587831315, -105.18270498152465 39.96884194995791, -105.18269658832716 39.968100506507554, -105.18348289910209 39.96810018023088, -105.18437698789344 39.96809980246061, -105.18437879072897 39.9663747723468, -105.18450143396159 39.965230264653044, -105.18365299999328 39.96489799860698, -105.18232892470502 39.964383026107484, -105.18237658583149 39.96435856048586, -105.18295017997087 39.96406143557106, -105.18314317955361 39.96390943620628, -105.18335917943803 39.96390543564833, -105.18468118012977 39.96359143505422, -105.1846831809932 39.96346543564761, -105.18508718060008 39.96337543512138, -105.18521018025564 39.96334743554963, -105.18590917996742 39.963195435562426, -105.18675618097987 39.96303243590308, -105.18754918028917 39.96290443543483, -105.18828818134021 39.962797435438084, -105.18927318047518 39.96267043497246, -105.1892811813567 39.96148043493095, -105.18890718110833 39.96174843466853, -105.18826031603797 39.96197615552799, -105.18771318133258 39.96209643507789, -105.18761218084032 39.962167435866895, -105.18725518010456 39.96227843565087, -105.18707318065496 39.96230143525784, -105.1867361810641 39.96239743503643, -105.18628218005655 39.96244943611252, -105.18527817977143 39.96245943558378, -105.18516918083706 39.96256443568562, -105.18468818025946 39.96256443553224, -105.18468417954304 39.96329443567719, -105.18375617945398 39.96352043583736, -105.18368118011101 39.963532435725064, -105.1835581803465 39.963553435546864, -105.18337217911846 39.963577436074615, -105.18324717966541 39.96358943518963, -105.18312218004684 39.96359843587509, -105.1829971802545 39.96360343569754, -105.18287117958873 39.96360543613775, -105.18274517881902 39.96360443634497, -105.1826201798852 39.963600435475904, -105.18249417895733 39.96359343521812, -105.18235217868045 39.963576435738716, -105.18224417956161 39.96356843645984, -105.18212017882117 39.96355143678812, -105.1820251788167 39.96353643541125, -105.18187617915322 39.9635074363657, -105.18159917936961 39.963440435989654, -105.1815181794293 39.96341743539393, -105.18142817977963 39.9633894364229, -105.1813451795762 39.96336143602115, -105.18126453305565 39.963332723343505, -105.18117517983359 39.96329843665993, -105.18112017849242 39.963276436289306, -105.18106517951861 39.96325343616735, -105.1810111789803 39.96322943544858, -105.18095717963881 39.96320443587675, -105.18090417873846 39.96317943634221, -105.18085117904582 39.96315343615423, -105.18079917896395 39.96312643537638, -105.18074817848563 39.963098435811276, -105.18069717922376 39.96307043532614, -105.18064717839636 39.963041436052286, -105.18054917835521 39.96298243605077, -105.18050117914056 39.96295143559319, -105.18045417836309 39.96292043608274, -105.18040717880433 39.962887436192425, -105.18038917958538 39.962875435427286, -105.18002317886062 39.96283243551652, -105.17911017844007 39.96248843618227, -105.17903317922068 39.9626014355022, -105.17803617865185 39.96221443573692, -105.17802480425831 39.96220476780362, -105.17796032942059 39.96230169761951, -105.17779885063878 39.962224765856405, -105.17777863691451 39.96221513532904, -105.17777799962595 39.962215999080605, -105.17777299913361 39.96222499799526, -105.175195000182 39.96134899884276, -105.17506299876474 39.96129699910314, -105.17189299919968 39.96004699882172, -105.16867899997003 39.958628998641686, -105.16775499915033 39.95786999907147, -105.16720299904809 39.95741599921722, -105.16682499954673 39.95710599849211, -105.1661219997786 39.956954998978375, -105.16605999955671 39.9569419984156, -105.16606599977727 39.95698699837227, -105.16610899948478 39.95726499912967, -105.16612500020719 39.95739999859541, -105.16634299883087 39.95789999829524, -105.16639399938875 39.958015998758334, -105.16637299986718 39.95804199855646, -105.16632607792026 39.958094531487156, -105.16628099997698 39.95814499912188, -105.1658829843055 39.957988833132234, -105.16587963749681 39.958903516596045, -105.1658491420113 39.959351876656214, -105.16585408323267 39.95993247886946, -105.16585725733235 39.96030582959796, -105.16586320772421 39.96100519839205, -105.16586904191627 39.96169103439433, -105.16587900777587 39.96191819436262, -105.16589484817989 39.96259403227716, -105.16589541744115 39.96449888213142, -105.1659093981826 39.9647605444362, -105.16571346047074 39.965028463726995, -105.1657337016853 39.965871899049155, -105.16590965706231 39.96587234083293, -105.1659176730908 39.966289895355956, -105.1659271352761 39.96678289958627, -105.1659328385439 39.967116303274295, -105.16592719464714 39.967364852669554, -105.16591737390743 39.96779730547408, -105.16591670137207 39.9678268415455, -105.16591735079628 39.96852063654418, -105.1659765753193 39.96870010874206, -105.16597175831293 39.96959747823431, -105.16597154253645 39.96964872511244, -105.16596826768873 39.97043932947262, -105.16619457866447 39.97070261644534, -105.16629306708415 39.9708759461761, -105.16593978502245 39.97109272097257, -105.1657812165369 39.97121736908545, -105.16567832762807 39.97135647557006, -105.16544951101874 39.9715953031206, -105.16525808592333 39.971787770224665, -105.16501546969201 39.97199796091019, -105.16456544516134 39.97232091807293, -105.16296644437902 39.97350192482068, -105.16251944294834 39.97376992644322, -105.16169244077052 39.974052928849474, -105.16085643903571 39.97426193043724, -105.16058920028946 39.974345522908116, -105.16037043735196 39.974440931956806, -105.15985743701962 39.97471893324816, -105.15945343534766 39.97493993463027, -105.15898443451623 39.97513493662397, -105.15762843113424 39.9755679397703, -105.15536142538129 39.97627694524857, -105.15390696009314 39.97673105134181, -105.1527122301567 39.97711140868529, -105.15118404585209 39.97762806941142))</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1054,7 +1054,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.156329421909 39.97232839907968, -105.1563198480149 39.97435582372207, -105.1563197008376 39.9743906166452, -105.1599104579264 39.97444804360306, -105.160370437352 39.97444093195681, -105.1605892002895 39.97434552290812, -105.1608564390357 39.97426193043724, -105.1616924407705 39.97405292884947, -105.1625194429483 39.97376992644322, -105.162966444379 39.97350192482068, -105.1645654451613 39.97232091807293, -105.165015469692 39.97199796091019, -105.1652580859233 39.97178777022467, -105.1654495110187 39.9715953031206, -105.1656783276281 39.97135647557006, -105.1657812165369 39.97121736908545, -105.1659397850224 39.97109272097257, -105.1662930670842 39.9708759461761, -105.1661945786645 39.97070261644534, -105.1659682676887 39.97043932947262, -105.1659715425365 39.96964872511244, -105.1659717583129 39.96959747823431, -105.1659765753193 39.96870010874206, -105.1659173507963 39.96852063654418, -105.1659167013721 39.9678268415455, -105.1659173739074 39.96779730547408, -105.1659271946471 39.96736485266955, -105.1659328385439 39.9671163032743, -105.1659271352761 39.96678289958627, -105.1659176730908 39.96628989535596, -105.1659096570623 39.96587234083293, -105.1657337016853 39.96587189904916, -105.1657134604707 39.96502846372699, -105.1659093981826 39.9647605444362, -105.1658954174411 39.96449888213142, -105.1655931600189 39.96437830147045, -105.1653133155886 39.96428428971744, -105.1649780902026 39.96419277954295, -105.1647484114118 39.96413788198119, -105.164483696346 39.96409814183401, -105.1641930794864 39.96408398179263, -105.1633384051544 39.9640808828587, -105.1626480901568 39.96407354029382, -105.1623984016815 39.96409488425228, -105.1620542665501 39.96412299749996, -105.16169407117 39.9641831855031, -105.161389229453 39.96424619829306, -105.1610773868694 39.96432516649111, -105.1606614234813 39.96446507215775, -105.1600663952859 39.96469988937269, -105.1596004190962 39.96488000674642, -105.1593023204964 39.96497765080175, -105.1591741481606 39.96500389980679, -105.1589524603611 39.96504584965834, -105.1587585229728 39.96507456680651, -105.1585646253969 39.9650952948947, -105.1583707543674 39.96511069713443, -105.1580453725514 39.96512093089092, -105.1563762083814 39.9651309339529, -105.1563836773766 39.96527525633939, -105.156377543934 39.96595602878138, -105.1563773619482 39.96848953887152, -105.1563687453229 39.968684342056, -105.1563417103309 39.97039592247952, -105.1563362950712 39.97192301121288, -105.1563315315155 39.97205484452347, -105.156329421909 39.97232839907968))</t>
+          <t>POLYGON ((-105.15632942190896 39.97232839907968, -105.15631984801487 39.97435582372207, -105.1563197008376 39.9743906166452, -105.15991045792636 39.97444804360306, -105.16037043735196 39.974440931956806, -105.16058920028946 39.974345522908116, -105.16085643903571 39.97426193043724, -105.16169244077052 39.974052928849474, -105.16251944294834 39.97376992644322, -105.16296644437902 39.97350192482068, -105.16456544516134 39.97232091807293, -105.16501546969201 39.97199796091019, -105.16525808592333 39.971787770224665, -105.16544951101874 39.9715953031206, -105.16567832762807 39.97135647557006, -105.1657812165369 39.97121736908545, -105.16593978502245 39.97109272097257, -105.16629306708415 39.9708759461761, -105.16619457866447 39.97070261644534, -105.16596826768873 39.97043932947262, -105.16597154253645 39.96964872511244, -105.16597175831293 39.96959747823431, -105.1659765753193 39.96870010874206, -105.16591735079628 39.96852063654418, -105.16591670137207 39.9678268415455, -105.16591737390743 39.96779730547408, -105.16592719464714 39.967364852669554, -105.1659328385439 39.967116303274295, -105.1659271352761 39.96678289958627, -105.1659176730908 39.966289895355956, -105.16590965706231 39.96587234083293, -105.1657337016853 39.965871899049155, -105.16571346047074 39.965028463726995, -105.1659093981826 39.9647605444362, -105.16589541744115 39.96449888213142, -105.16559316001887 39.964378301470454, -105.16531331558865 39.96428428971744, -105.1649780902026 39.96419277954295, -105.16474841141184 39.964137881981195, -105.16448369634598 39.96409814183401, -105.16419307948638 39.964083981792626, -105.16333840515442 39.9640808828587, -105.16264809015685 39.964073540293825, -105.16239840168153 39.96409488425228, -105.16205426655006 39.964122997499956, -105.16169407117 39.964183185503096, -105.161389229453 39.96424619829306, -105.16107738686935 39.964325166491115, -105.16066142348126 39.96446507215775, -105.16006639528587 39.96469988937269, -105.15960041909622 39.96488000674642, -105.15930232049637 39.96497765080175, -105.15917414816059 39.96500389980679, -105.1589524603611 39.96504584965834, -105.1587585229728 39.965074566806514, -105.15856462539693 39.9650952948947, -105.15837075436744 39.96511069713443, -105.15804537255138 39.96512093089092, -105.1563762083814 39.9651309339529, -105.15638367737664 39.96527525633939, -105.156377543934 39.96595602878138, -105.15637736194819 39.968489538871516, -105.15636874532292 39.968684342056, -105.15634171033089 39.97039592247952, -105.15633629507123 39.97192301121288, -105.15633153151552 39.97205484452347, -105.15632942190896 39.97232839907968))</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1410811029379 39.97296808587065, -105.1417619400029 39.97336688798534, -105.1418319160097 39.9732910627605, -105.1419560546458 39.97316105094687, -105.1420910811044 39.97306401444264, -105.1422749751233 39.97296987557731, -105.1424511686638 39.97291496958876, -105.142636862039 39.9728858966902, -105.144084080593 39.97288488450913, -105.1445468599055 39.97288494008312, -105.1446010684806 39.97289004827322, -105.1448099658239 39.97292692938436, -105.1449681239247 39.97297792838406, -105.1452688264766 39.97306313261024, -105.1454121659785 39.97308196696445, -105.1457010775136 39.97310207193204, -105.1465748957557 39.97309679385843, -105.1468497224026 39.97296655428324, -105.1469267424887 39.97293720268624, -105.147006415429 39.97293902018367, -105.1470063742493 39.97290218127869, -105.1472916414865 39.97290504238159, -105.1474597910268 39.97291467962244, -105.1474557445568 39.97244657193539, -105.1468334106985 39.9724625167936, -105.1468560320575 39.9714791368918, -105.1472646481268 39.97130401562464, -105.1476998983715 39.97106622807066, -105.1477953625288 39.97102502014906, -105.1478101108981 39.97104111407433, -105.1479050518321 39.97110399460654, -105.1481300736089 39.97119609789256, -105.1483559645197 39.97125800517019, -105.148577051611 39.97128311171325, -105.1493549002968 39.97127806936677, -105.1501908928033 39.97127594257257, -105.1510529931602 39.9712568699012, -105.1510711338833 39.97204013385311, -105.1510754606821 39.97238251194248, -105.1511906189166 39.97238369993654, -105.1543608103686 39.97235038931903, -105.1560722927011 39.97232993234917, -105.156329421909 39.97232839907968, -105.1563315315155 39.97205484452347, -105.1563362950712 39.97192301121288, -105.1563417103309 39.97039592247952, -105.1563687453229 39.968684342056, -105.1563773619482 39.96848953887152, -105.156377543934 39.96595602878138, -105.1563836773766 39.96527525633939, -105.1563762083814 39.9651309339529, -105.1554532690506 39.96514994269476, -105.1528301109463 39.96518103268608, -105.1499591002229 39.96520089786635, -105.1491546814992 39.96520549842712, -105.148694400112 39.96520942180835, -105.1468843448076 39.9651819073298, -105.1468023445748 39.96518190732379, -105.1464993430814 39.96518190774901, -105.1463623431024 39.9651829077625, -105.1458193408466 39.96518290820572, -105.1447703368318 39.96518290919838, -105.143508784869 39.96517236669215, -105.1432607766169 39.96519209645445, -105.1431599644167 39.96522091709688, -105.1428993207166 39.96531662179055, -105.1427083187379 39.96541969037425, -105.1425217921166 39.96555494231168, -105.1424003203377 39.96568682201359, -105.1422784346384 39.96589733965961, -105.1422267360074 39.96601156303456, -105.1421934114149 39.96616516356316, -105.1421767761853 39.96667984017955, -105.1422113366961 39.96770492316075, -105.1422074729856 39.96791313929997, -105.1421503383544 39.96812792517319, -105.1420743382712 39.9682629259876, -105.1420433384291 39.96830892639375, -105.1419173381126 39.96842892711096, -105.1418093763021 39.96852671673524, -105.1416835511761 39.96860139021794, -105.1415438644826 39.96866172247041, -105.1413437296394 39.96873258971108, -105.1411484834786 39.96875700316673, -105.1409718570907 39.9687743257597, -105.1356806657604 39.96874485295404, -105.1348970597835 39.96873694847295, -105.134616987672 39.9687360608628, -105.1339458879853 39.96873310802705, -105.1334221039853 39.96873693358972, -105.1329729052466 39.96873797441319, -105.1328978978705 39.96873783278408, -105.1328771385485 39.96873773783532, -105.1328169240748 39.96875010571533, -105.1327739804785 39.96877412640302, -105.1327290874463 39.9688288876109, -105.1327180592421 39.9688889724552, -105.1327151412824 39.9691659558876, -105.1327195315171 39.96947027243025, -105.1327228337507 39.96986689598629, -105.1327193515535 39.96995687077294, -105.1327142628682 39.97019653200053, -105.1327146054549 39.97135212356304, -105.132714663984 39.97135212374958, -105.1327153345106 39.97237221641146, -105.1327149084221 39.97237221325229, -105.1327149078208 39.97237232493223, -105.1327149233977 39.97242314113262, -105.1327159959923 39.9725200663986, -105.1327180335489 39.97273804347041, -105.1338669384731 39.97274087488337, -105.1345680324247 39.97274694397268, -105.1346706681118 39.97274871400992, -105.1349190988446 39.97275299757594, -105.1351970196934 39.97275909331277, -105.1354970791385 39.97276196468327, -105.135705093256 39.97276289706459, -105.1359709084177 39.97276401074883, -105.1362520681869 39.97276489844887, -105.1365910243183 39.97276706652148, -105.1369710084886 39.97276991043685, -105.1380078803221 39.97277207382956, -105.1381528713102 39.97274809692661, -105.1382669161346 39.97270590414211, -105.1383459977635 39.97266305213679, -105.1384459984396 39.97257798962455, -105.1386620274633 39.97227806644061, -105.138897872462 39.97234606329846, -105.1391438457741 39.97238801187403, -105.1393960276398 39.97240307573568, -105.1396229824941 39.97239802138446, -105.1398498385006 39.97241190715587, -105.1401471596422 39.97246005385595, -105.1402821154131 39.9725120847603, -105.1405330473047 39.97262899065191, -105.1406529380903 39.97269607279399, -105.1410811029379 39.97296808587065))</t>
+          <t>POLYGON ((-105.14108110293786 39.972968085870654, -105.14176194000291 39.973366887985335, -105.14183191600975 39.973291062760495, -105.14195605464582 39.97316105094687, -105.14209108110437 39.97306401444264, -105.14227497512331 39.972969875577306, -105.14245116866384 39.97291496958876, -105.14263686203896 39.9728858966902, -105.14408408059302 39.972884884509135, -105.14454685990553 39.97288494008312, -105.14460106848055 39.97289004827322, -105.14480996582388 39.972926929384364, -105.14496812392468 39.97297792838406, -105.14526882647655 39.973063132610235, -105.14541216597846 39.97308196696445, -105.14570107751364 39.97310207193204, -105.14657489575569 39.97309679385843, -105.14684972240256 39.97296655428324, -105.14692674248867 39.97293720268624, -105.147006415429 39.972939020183674, -105.14700637424934 39.97290218127869, -105.14729164148649 39.97290504238159, -105.14745979102679 39.97291467962244, -105.14745574455684 39.97244657193539, -105.14683341069852 39.9724625167936, -105.1468560320575 39.9714791368918, -105.14726464812685 39.97130401562464, -105.14769989837153 39.97106622807066, -105.14779536252881 39.971025020149064, -105.14781011089808 39.97104111407433, -105.14790505183214 39.971103994606544, -105.1481300736089 39.97119609789256, -105.14835596451965 39.97125800517019, -105.14857705161103 39.97128311171325, -105.14935490029683 39.97127806936677, -105.15019089280328 39.971275942572575, -105.15105299316022 39.971256869901204, -105.1510711338833 39.97204013385311, -105.15107546068208 39.97238251194248, -105.15119061891656 39.97238369993654, -105.15436081036864 39.972350389319026, -105.15607229270108 39.97232993234917, -105.15632942190896 39.97232839907968, -105.15633153151552 39.97205484452347, -105.15633629507123 39.97192301121288, -105.15634171033089 39.97039592247952, -105.15636874532292 39.968684342056, -105.15637736194819 39.968489538871516, -105.156377543934 39.96595602878138, -105.15638367737664 39.96527525633939, -105.1563762083814 39.9651309339529, -105.15545326905064 39.96514994269476, -105.15283011094628 39.96518103268608, -105.14995910022286 39.965200897866346, -105.14915468149916 39.96520549842712, -105.14869440011198 39.965209421808346, -105.14688434480763 39.9651819073298, -105.14680234457477 39.96518190732379, -105.1464993430814 39.96518190774901, -105.14636234310242 39.965182907762504, -105.14581934084656 39.96518290820572, -105.14477033683178 39.96518290919838, -105.14350878486904 39.96517236669215, -105.14326077661686 39.96519209645445, -105.14315996441672 39.96522091709688, -105.14289932071657 39.96531662179055, -105.14270831873786 39.96541969037425, -105.14252179211657 39.96555494231168, -105.14240032033774 39.96568682201359, -105.14227843463836 39.965897339659605, -105.14222673600742 39.96601156303456, -105.14219341141487 39.96616516356316, -105.14217677618532 39.96667984017955, -105.14221133669608 39.96770492316075, -105.14220747298562 39.967913139299974, -105.14215033835444 39.96812792517319, -105.14207433827117 39.968262925987595, -105.14204333842906 39.96830892639375, -105.14191733811258 39.968428927110956, -105.1418093763021 39.96852671673524, -105.1416835511761 39.96860139021794, -105.14154386448264 39.96866172247041, -105.14134372963943 39.96873258971108, -105.14114848347856 39.96875700316673, -105.14097185709069 39.9687743257597, -105.13568066576039 39.96874485295404, -105.13489705978346 39.96873694847295, -105.134616987672 39.968736060862796, -105.1339458879853 39.96873310802705, -105.13342210398528 39.96873693358972, -105.13297290524663 39.968737974413195, -105.13289789787048 39.96873783278408, -105.13287713854848 39.96873773783532, -105.13281692407482 39.96875010571533, -105.13277398047853 39.96877412640302, -105.13272908744628 39.968828887610904, -105.13271805924214 39.968888972455204, -105.13271514128239 39.9691659558876, -105.13271953151714 39.96947027243025, -105.13272283375075 39.969866895986286, -105.1327193515535 39.96995687077294, -105.1327142628682 39.97019653200053, -105.13271460545486 39.97135212356304, -105.13271466398398 39.971352123749575, -105.13271533451059 39.972372216411465, -105.13271490842207 39.97237221325229, -105.13271490782084 39.97237232493223, -105.13271492339774 39.97242314113262, -105.1327159959923 39.9725200663986, -105.13271803354893 39.972738043470414, -105.13386693847312 39.97274087488337, -105.13456803242472 39.97274694397268, -105.1346706681118 39.97274871400992, -105.13491909884459 39.97275299757594, -105.13519701969336 39.972759093312774, -105.13549707913852 39.97276196468327, -105.13570509325596 39.97276289706459, -105.13597090841772 39.97276401074883, -105.1362520681869 39.97276489844887, -105.13659102431832 39.972767066521484, -105.13697100848864 39.972769910436845, -105.13800788032212 39.97277207382956, -105.13815287131024 39.97274809692661, -105.13826691613455 39.97270590414211, -105.13834599776351 39.97266305213679, -105.13844599843965 39.97257798962455, -105.13866202746328 39.97227806644061, -105.13889787246198 39.97234606329846, -105.13914384577414 39.97238801187403, -105.13939602763979 39.972403075735684, -105.13962298249407 39.97239802138446, -105.13984983850062 39.972411907155866, -105.14014715964223 39.972460053855954, -105.14028211541309 39.9725120847603, -105.14053304730466 39.97262899065191, -105.14065293809031 39.97269607279399, -105.14108110293786 39.972968085870654))</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1327149078208 39.97237232493223, -105.1326240548662 39.97237145444323, -105.1326092883675 39.97237107593023, -105.1326031913209 39.97237094391207, -105.1322020387081 39.97236225831516, -105.1319873907501 39.97235915665501, -105.1316832172676 39.97235693758834, -105.1314539558249 39.9723552617133, -105.1313794898227 39.97235471554273, -105.1309714865439 39.97235173645367, -105.1307176733622 39.97234991204898, -105.1306659725923 39.97234976349554, -105.1301840582684 39.97234839379923, -105.1301103864602 39.97234818710459, -105.1298094143496 39.97234732795977, -105.1296709720262 39.97234693273894, -105.1296648708499 39.97234691583657, -105.1295809285128 39.97234769805092, -105.1293981153291 39.97178608088523, -105.1292770345935 39.97141508682, -105.1291247538012 39.97093561123375, -105.1289943503059 39.97052774621444, -105.1288680870524 39.97011308536674, -105.128553963989 39.9690911268271, -105.1284532215353 39.96877325434858, -105.1283536248506 39.96877385278868, -105.1280108127828 39.96877000157099, -105.1275570164911 39.96876746234612, -105.1274844113412 39.96876705475879, -105.127061221905 39.9687646845617, -105.1269735298878 39.96876419450597, -105.1260857937713 39.96875972803437, -105.1256813227789 39.96875778727393, -105.1256339410851 39.97236269794815, -105.1256304425993 39.97260260723626, -105.125568498434 39.97308157000424, -105.1259336601506 39.97325526013939, -105.1265094311803 39.97363524625856, -105.1269897690644 39.97410774900974, -105.1274121598896 39.97481223461234, -105.1275745938115 39.97544829877226, -105.1276644462961 39.97603262125949, -105.1276525381961 39.97673399347658, -105.1276466084615 39.97708321067033, -105.1273435143957 39.97735082326365, -105.1278751389853 39.97724196051531, -105.1285810424273 39.97709407394184, -105.1288189364574 39.97704899579355, -105.1290571708148 39.97700693726274, -105.1292929066513 39.97696487020448, -105.1295311225317 39.97692610525043, -105.1295918539046 39.97691312287947, -105.1296518574046 39.97690288425013, -105.129713999398 39.97689292626037, -105.1297750609442 39.97688488677507, -105.1298379006302 39.97687795087256, -105.1299589906039 39.976864768547, -105.1300746618064 39.97685388159796, -105.130198828228 39.97684589219254, -105.1307808317385 39.97684309169715, -105.1321378796018 39.97683809725402, -105.1333829314064 39.97682394561945, -105.1345908763852 39.97680911350178, -105.1357531011968 39.97680290928571, -105.13678106013 39.97680764835362, -105.1367811807096 39.97680764873362, -105.1367812462675 39.97680764894022, -105.1367812813878 39.97680764905088, -105.1402610924567 39.97681258380209, -105.1402610830722 39.97681347542572, -105.1409831119745 39.97681055059026, -105.1409958621201 39.97603391013515, -105.1433054578167 39.97603468882662, -105.1433047175067 39.97601730831056, -105.146288028921 39.97468729729214, -105.1464875196881 39.97431430316958, -105.1468277049785 39.973816196973, -105.1474597910268 39.97291467962244, -105.1472916414865 39.97290504238159, -105.1470063742493 39.97290218127869, -105.147006415429 39.97293902018367, -105.1469267424887 39.97293720268624, -105.1468497224026 39.97296655428324, -105.1465748957557 39.97309679385843, -105.1457010775136 39.97310207193204, -105.1454121659785 39.97308196696445, -105.1452688264766 39.97306313261024, -105.1449681239247 39.97297792838406, -105.1448099658239 39.97292692938436, -105.1446010684806 39.97289004827322, -105.1445468599055 39.97288494008312, -105.144084080593 39.97288488450913, -105.142636862039 39.9728858966902, -105.1424511686638 39.97291496958876, -105.1422749751233 39.97296987557731, -105.1420910811044 39.97306401444264, -105.1419560546458 39.97316105094687, -105.1418319160097 39.9732910627605, -105.1417619400029 39.97336688798534, -105.1410811029379 39.97296808587065, -105.1406529380903 39.97269607279399, -105.1405330473047 39.97262899065191, -105.1402821154131 39.9725120847603, -105.1401471596422 39.97246005385595, -105.1398498385006 39.97241190715587, -105.1396229824941 39.97239802138446, -105.1393960276398 39.97240307573568, -105.1391438457741 39.97238801187403, -105.138897872462 39.97234606329846, -105.1386620274633 39.97227806644061, -105.1384459984396 39.97257798962455, -105.1383459977635 39.97266305213679, -105.1382669161346 39.97270590414211, -105.1381528713102 39.97274809692661, -105.1380078803221 39.97277207382956, -105.1369710084886 39.97276991043685, -105.1365910243183 39.97276706652148, -105.1362520681869 39.97276489844887, -105.1359709084177 39.97276401074883, -105.135705093256 39.97276289706459, -105.1354970791385 39.97276196468327, -105.1351970196934 39.97275909331277, -105.1349190988446 39.97275299757594, -105.1346706681118 39.97274871400992, -105.1345680324247 39.97274694397268, -105.1338669384731 39.97274087488337, -105.1327180335489 39.97273804347041, -105.1327159959923 39.9725200663986, -105.1327149233977 39.97242314113262, -105.1327149078208 39.97237232493223))</t>
+          <t>POLYGON ((-105.13271490782084 39.97237232493223, -105.13262405486618 39.97237145444323, -105.13260928836748 39.97237107593023, -105.13260319132092 39.97237094391207, -105.13220203870807 39.97236225831516, -105.13198739075007 39.97235915665501, -105.13168321726762 39.97235693758834, -105.13145395582487 39.972355261713304, -105.13137948982275 39.97235471554273, -105.13097148654386 39.97235173645367, -105.13071767336216 39.97234991204898, -105.13066597259227 39.97234976349554, -105.13018405826844 39.97234839379923, -105.1301103864602 39.972348187104586, -105.1298094143496 39.972347327959774, -105.12967097202625 39.97234693273894, -105.1296648708499 39.97234691583657, -105.12958092851277 39.97234769805092, -105.12939811532907 39.97178608088523, -105.12927703459351 39.97141508682, -105.12912475380116 39.97093561123375, -105.12899435030594 39.970527746214444, -105.12886808705242 39.97011308536674, -105.12855396398898 39.9690911268271, -105.1284532215353 39.96877325434858, -105.1283536248506 39.96877385278868, -105.12801081278276 39.96877000157099, -105.12755701649105 39.96876746234612, -105.12748441134124 39.96876705475879, -105.127061221905 39.9687646845617, -105.12697352988779 39.96876419450597, -105.12608579377134 39.96875972803437, -105.1256813227789 39.96875778727393, -105.12563394108514 39.97236269794815, -105.12563044259932 39.97260260723626, -105.12556849843396 39.97308157000424, -105.12593366015055 39.97325526013939, -105.12650943118032 39.97363524625856, -105.12698976906441 39.97410774900974, -105.12741215988962 39.97481223461234, -105.12757459381146 39.975448298772264, -105.12766444629614 39.97603262125949, -105.12765253819613 39.97673399347658, -105.12764660846148 39.97708321067033, -105.12734351439568 39.97735082326365, -105.12787513898526 39.977241960515315, -105.12858104242734 39.977094073941835, -105.12881893645745 39.97704899579355, -105.12905717081482 39.97700693726274, -105.1292929066513 39.976964870204476, -105.12953112253166 39.976926105250435, -105.12959185390464 39.976913122879466, -105.12965185740464 39.97690288425013, -105.12971399939796 39.97689292626037, -105.12977506094421 39.976884886775075, -105.12983790063018 39.97687795087256, -105.12995899060385 39.976864768547, -105.13007466180638 39.97685388159796, -105.13019882822799 39.976845892192536, -105.13078083173855 39.97684309169715, -105.13213787960184 39.97683809725402, -105.13338293140637 39.97682394561945, -105.13459087638523 39.97680911350178, -105.13575310119678 39.97680290928571, -105.13678106013002 39.97680764835362, -105.13678118070965 39.97680764873362, -105.1367812462675 39.976807648940216, -105.13678128138777 39.976807649050876, -105.14026109245668 39.97681258380209, -105.14026108307223 39.97681347542572, -105.14098311197453 39.97681055059026, -105.14099586212012 39.97603391013515, -105.14330545781672 39.97603468882662, -105.1433047175067 39.97601730831056, -105.14628802892103 39.974687297292135, -105.1464875196881 39.97431430316958, -105.14682770497846 39.973816196973004, -105.14745979102679 39.97291467962244, -105.14729164148649 39.97290504238159, -105.14700637424934 39.97290218127869, -105.147006415429 39.972939020183674, -105.14692674248867 39.97293720268624, -105.14684972240256 39.97296655428324, -105.14657489575569 39.97309679385843, -105.14570107751364 39.97310207193204, -105.14541216597846 39.97308196696445, -105.14526882647655 39.973063132610235, -105.14496812392468 39.97297792838406, -105.14480996582388 39.972926929384364, -105.14460106848055 39.97289004827322, -105.14454685990553 39.97288494008312, -105.14408408059302 39.972884884509135, -105.14263686203896 39.9728858966902, -105.14245116866384 39.97291496958876, -105.14227497512331 39.972969875577306, -105.14209108110437 39.97306401444264, -105.14195605464582 39.97316105094687, -105.14183191600975 39.973291062760495, -105.14176194000291 39.973366887985335, -105.14108110293786 39.972968085870654, -105.14065293809031 39.97269607279399, -105.14053304730466 39.97262899065191, -105.14028211541309 39.9725120847603, -105.14014715964223 39.972460053855954, -105.13984983850062 39.972411907155866, -105.13962298249407 39.97239802138446, -105.13939602763979 39.972403075735684, -105.13914384577414 39.97238801187403, -105.13889787246198 39.97234606329846, -105.13866202746328 39.97227806644061, -105.13844599843965 39.97257798962455, -105.13834599776351 39.97266305213679, -105.13826691613455 39.97270590414211, -105.13815287131024 39.97274809692661, -105.13800788032212 39.97277207382956, -105.13697100848864 39.972769910436845, -105.13659102431832 39.972767066521484, -105.1362520681869 39.97276489844887, -105.13597090841772 39.97276401074883, -105.13570509325596 39.97276289706459, -105.13549707913852 39.97276196468327, -105.13519701969336 39.972759093312774, -105.13491909884459 39.97275299757594, -105.1346706681118 39.97274871400992, -105.13456803242472 39.97274694397268, -105.13386693847312 39.97274087488337, -105.13271803354893 39.972738043470414, -105.1327159959923 39.9725200663986, -105.13271492339774 39.97242314113262, -105.13271490782084 39.97237232493223))</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1432885288381 39.97773242539142, -105.1443578909704 39.97771813279025, -105.1454398517117 39.97770993676632, -105.1455568987575 39.97770892415254, -105.1457797399434 39.97772494111891, -105.1463556201261 39.97772664370834, -105.1467964654496 39.97773046055833, -105.1467929027271 39.97812756649449, -105.1467766786365 39.9792879899573, -105.1467793224256 39.97967051067013, -105.1467799769283 39.97970215462984, -105.1468361234154 39.97978109470943, -105.1468879846528 39.97982709894254, -105.1475184832175 39.97946322695857, -105.148333500575 39.9789977880094, -105.1489677979379 39.9786628128497, -105.1497484075909 39.97826089699517, -105.1503649180572 39.97797809023514, -105.1511840458521 39.97762806941142, -105.1527122301567 39.97711140868529, -105.1539069600931 39.97673105134181, -105.1553614253813 39.97627694524857, -105.1576284311342 39.9755679397703, -105.1589844345162 39.97513493662397, -105.1594534353477 39.97493993463027, -105.1598574370196 39.97471893324816, -105.160370437352 39.97444093195681, -105.1599104579264 39.97444804360306, -105.1563197008376 39.9743906166452, -105.1563198480149 39.97435582372207, -105.156329421909 39.97232839907968, -105.1560722927011 39.97232993234917, -105.1543608103686 39.97235038931903, -105.1511906189166 39.97238369993654, -105.1510754606821 39.97238251194248, -105.1510711338833 39.97204013385311, -105.1510529931602 39.9712568699012, -105.1501908928033 39.97127594257257, -105.1493549002968 39.97127806936677, -105.148577051611 39.97128311171325, -105.1483559645197 39.97125800517019, -105.1481300736089 39.97119609789256, -105.1479050518321 39.97110399460654, -105.1478101108981 39.97104111407433, -105.1477953625288 39.97102502014906, -105.1476998983715 39.97106622807066, -105.1472646481268 39.97130401562464, -105.1468560320575 39.9714791368918, -105.1468334106985 39.9724625167936, -105.1474557445568 39.97244657193539, -105.1474597910268 39.97291467962244, -105.1468277049785 39.973816196973, -105.1464875196881 39.97431430316958, -105.146288028921 39.97468729729214, -105.1433047175067 39.97601730831056, -105.1433054578167 39.97603468882662, -105.1433105828532 39.97615496704697, -105.1433117063147 39.97673384507582, -105.1433036870691 39.9771906058965, -105.1432943712138 39.977650378093, -105.1432885288381 39.97773242539142))</t>
+          <t>POLYGON ((-105.14328852883806 39.97773242539142, -105.14435789097041 39.97771813279025, -105.14543985171171 39.97770993676632, -105.14555689875752 39.97770892415254, -105.14577973994338 39.977724941118915, -105.14635562012606 39.97772664370834, -105.14679646544958 39.977730460558334, -105.14679290272714 39.978127566494486, -105.14677667863653 39.9792879899573, -105.14677932242559 39.979670510670125, -105.14677997692831 39.97970215462984, -105.14683612341538 39.97978109470943, -105.1468879846528 39.979827098942536, -105.14751848321748 39.97946322695857, -105.148333500575 39.9789977880094, -105.14896779793789 39.9786628128497, -105.14974840759088 39.978260896995174, -105.15036491805724 39.97797809023514, -105.15118404585209 39.97762806941142, -105.1527122301567 39.97711140868529, -105.15390696009314 39.97673105134181, -105.15536142538129 39.97627694524857, -105.15762843113424 39.9755679397703, -105.15898443451623 39.97513493662397, -105.15945343534766 39.97493993463027, -105.15985743701962 39.97471893324816, -105.16037043735196 39.974440931956806, -105.15991045792636 39.97444804360306, -105.1563197008376 39.9743906166452, -105.15631984801487 39.97435582372207, -105.15632942190896 39.97232839907968, -105.15607229270108 39.97232993234917, -105.15436081036864 39.972350389319026, -105.15119061891656 39.97238369993654, -105.15107546068208 39.97238251194248, -105.1510711338833 39.97204013385311, -105.15105299316022 39.971256869901204, -105.15019089280328 39.971275942572575, -105.14935490029683 39.97127806936677, -105.14857705161103 39.97128311171325, -105.14835596451965 39.97125800517019, -105.1481300736089 39.97119609789256, -105.14790505183214 39.971103994606544, -105.14781011089808 39.97104111407433, -105.14779536252881 39.971025020149064, -105.14769989837153 39.97106622807066, -105.14726464812685 39.97130401562464, -105.1468560320575 39.9714791368918, -105.14683341069852 39.9724625167936, -105.14745574455684 39.97244657193539, -105.14745979102679 39.97291467962244, -105.14682770497846 39.973816196973004, -105.1464875196881 39.97431430316958, -105.14628802892103 39.974687297292135, -105.1433047175067 39.97601730831056, -105.14330545781672 39.97603468882662, -105.14331058285325 39.976154967046966, -105.14331170631475 39.97673384507582, -105.14330368706908 39.977190605896496, -105.14329437121383 39.977650378092996, -105.14328852883806 39.97773242539142))</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.166057391659 39.98000036044625, -105.1660560052696 39.98000040596588, -105.166056001947 39.98000036722793, -105.1660546877398 39.97987039392753, -105.1660513282059 39.97953810432843, -105.1660524971388 39.97915319426635, -105.1660527537385 39.97906729471996, -105.1660529846982 39.97899093757391, -105.1660539287566 39.97862565398879, -105.1658350282252 39.97862794311265, -105.1658379434426 39.978202974992, -105.1657440951674 39.97820297757695, -105.165639904273 39.97820212598116, -105.1656070754674 39.97820203074534, -105.165331838292 39.97822593878153, -105.1652778920959 39.97823895876851, -105.1650300462948 39.97827996626899, -105.1644808270593 39.97828989908837, -105.1641139846472 39.97829294847602, -105.1638721328699 39.97827604690609, -105.1637919096834 39.97826291009962, -105.1636401340146 39.97821497466567, -105.163456094038 39.97812494352087, -105.1633348417548 39.97803811539852, -105.1630970814578 39.97777113558509, -105.1629831715816 39.97764287573666, -105.1628509077528 39.97754613107234, -105.1626900249334 39.97746412824674, -105.1625211587942 39.97740900359284, -105.162320075189 39.97737492366687, -105.1620400653798 39.97735406243233, -105.1617588644038 39.97735790479039, -105.1615300344844 39.97737809680851, -105.1612810554912 39.97743199485603, -105.1607118328299 39.97759091532916, -105.1604571169876 39.97765001132789, -105.160191846309 39.97767887746299, -105.159924944536 39.97767699238972, -105.1597729990135 39.97766391584672, -105.1590099389456 39.97762295333611, -105.1589089590516 39.9776221060531, -105.1585060459044 39.97763189385436, -105.1583250364957 39.97765112328229, -105.1580100081515 39.97771113208039, -105.1577030738282 39.97779394982241, -105.1575379103652 39.97785495259414, -105.1570940838718 39.97805293534529, -105.1569161223485 39.97817511693055, -105.1568391167868 39.97823198766081, -105.1566929394302 39.9783490478104, -105.156485026981 39.97853702451009, -105.1563260121182 39.97872295083356, -105.1561968984269 39.97892296596781, -105.1561128433848 39.97910389984132, -105.156023870116 39.97933999693076, -105.1558980182553 39.97945903783057, -105.1557479917776 39.97955988874499, -105.1556128761117 39.97946395135801, -105.155458033647 39.979387995404, -105.1552770308644 39.97933392266862, -105.155197887842 39.97931886110557, -105.1549860097431 39.97930203055521, -105.1546161157948 39.97927209810255, -105.1525968273794 39.97911696440125, -105.1521720292124 39.97907807448019, -105.1519758743095 39.9790568933244, -105.1516928440833 39.97899811433265, -105.1514890587039 39.97893408385762, -105.1512419852102 39.97882188090264, -105.1510139320686 39.97868887123922, -105.1508070352091 39.97853588555293, -105.1506618817289 39.97838088993017, -105.1505558997787 39.97824193563466, -105.1504028475811 39.97802706963947, -105.1503649180572 39.97797809023514, -105.1497484075909 39.97826089699517, -105.1489677979379 39.9786628128497, -105.148333500575 39.9789977880094, -105.1475184832175 39.97946322695857, -105.1468879846528 39.97982709894254, -105.1464240452805 39.98008176384018, -105.1457566642355 39.98047476361054, -105.1455056956341 39.98064918734519, -105.1452546542914 39.98083735166556, -105.145003255205 39.98109421840952, -105.1447852378586 39.98137690039386, -105.1448400473045 39.9814050698708, -105.145155149327 39.98154192904205, -105.1454828518837 39.98165796143559, -105.1456310739417 39.98170206584106, -105.1459379881031 39.98176697286765, -105.1462529347776 39.98179703921972, -105.1467528265832 39.98180900367372, -105.1468042627624 39.98181279634973, -105.1468081054982 39.981912698399, -105.1468064120832 39.98218933688447, -105.1468041462498 39.98256024646881, -105.1467999228885 39.98291327827012, -105.1468001093051 39.9832646177242, -105.1467999600195 39.9833149307671, -105.1467991011445 39.98360336229756, -105.1467984523332 39.98382182769259, -105.1467978359181 39.98402906106782, -105.1467979231119 39.98423359101629, -105.1467993259979 39.98444428729881, -105.1467988922919 39.98464789066697, -105.1467987389826 39.98506280471422, -105.1467990272064 39.98514077741453, -105.1467968881911 39.98590616402691, -105.1473611102601 39.98610692973283, -105.1475190255502 39.98614480803915, -105.1484356133935 39.98636238526203, -105.1485830601631 39.98648523702375, -105.148701617686 39.98652304325331, -105.1486668298643 39.98662199615023, -105.1486448966827 39.98679213212387, -105.1486480228316 39.9868780671644, -105.1486449052872 39.98692911868827, -105.1544729774459 39.98688990858965, -105.1600758682569 39.98684699487811, -105.1636131392401 39.98682915798647, -105.1640844117053 39.98682677377659, -105.1642373985336 39.98682599908209, -105.1652483903585 39.98682087571383, -105.165249938283 39.98682086759958, -105.1654436915867 39.98681856417538, -105.165974893996 39.98681224725572, -105.1659751117827 39.98681224608544, -105.165974894609 39.98681212206605, -105.1659816707675 39.98040380617206, -105.166065785029 39.98040377608608, -105.1660576266512 39.98001166799104, -105.1660575821633 39.98001166786214, -105.1660575394011 39.98000748868384, -105.166057391659 39.98000036044625))</t>
+          <t>POLYGON ((-105.16605739165898 39.980000360446255, -105.1660560052696 39.98000040596588, -105.16605600194698 39.98000036722793, -105.16605468773977 39.97987039392753, -105.16605132820585 39.979538104328434, -105.16605249713876 39.979153194266345, -105.16605275373851 39.97906729471996, -105.16605298469823 39.97899093757391, -105.1660539287566 39.978625653988786, -105.16583502822523 39.97862794311265, -105.1658379434426 39.978202974992, -105.16574409516735 39.97820297757695, -105.16563990427296 39.97820212598116, -105.16560707546739 39.978202030745344, -105.16533183829205 39.97822593878153, -105.16527789209587 39.978238958768515, -105.16503004629483 39.978279966268985, -105.16448082705932 39.978289899088374, -105.16411398464723 39.978292948476025, -105.16387213286986 39.97827604690609, -105.16379190968343 39.97826291009962, -105.16364013401457 39.97821497466567, -105.16345609403798 39.978124943520875, -105.16333484175478 39.97803811539852, -105.16309708145783 39.97777113558509, -105.16298317158157 39.97764287573666, -105.16285090775283 39.977546131072344, -105.16269002493335 39.97746412824674, -105.16252115879416 39.97740900359284, -105.16232007518902 39.97737492366687, -105.16204006537984 39.977354062432326, -105.16175886440382 39.97735790479039, -105.16153003448439 39.977378096808515, -105.16128105549124 39.977431994856026, -105.16071183282988 39.97759091532916, -105.16045711698757 39.97765001132789, -105.16019184630896 39.97767887746299, -105.15992494453604 39.97767699238972, -105.15977299901351 39.97766391584672, -105.15900993894557 39.97762295333611, -105.15890895905163 39.977622106053104, -105.1585060459044 39.97763189385436, -105.15832503649568 39.97765112328229, -105.15801000815148 39.97771113208039, -105.15770307382823 39.97779394982241, -105.15753791036516 39.97785495259414, -105.1570940838718 39.97805293534529, -105.1569161223485 39.97817511693055, -105.15683911678676 39.978231987660806, -105.15669293943022 39.9783490478104, -105.15648502698096 39.97853702451009, -105.15632601211819 39.97872295083356, -105.15619689842694 39.97892296596781, -105.15611284338485 39.97910389984132, -105.15602387011602 39.97933999693076, -105.1558980182553 39.979459037830566, -105.15574799177763 39.979559888744994, -105.15561287611168 39.979463951358014, -105.15545803364702 39.979387995404, -105.15527703086438 39.97933392266862, -105.15519788784195 39.97931886110557, -105.1549860097431 39.97930203055521, -105.15461611579481 39.97927209810255, -105.1525968273794 39.97911696440125, -105.1521720292124 39.979078074480185, -105.15197587430947 39.9790568933244, -105.15169284408326 39.97899811433265, -105.15148905870387 39.978934083857624, -105.15124198521019 39.97882188090264, -105.15101393206855 39.97868887123922, -105.15080703520906 39.97853588555293, -105.15066188172887 39.97838088993017, -105.15055589977874 39.978241935634664, -105.15040284758113 39.97802706963947, -105.15036491805724 39.97797809023514, -105.14974840759088 39.978260896995174, -105.14896779793789 39.9786628128497, -105.148333500575 39.9789977880094, -105.14751848321748 39.97946322695857, -105.1468879846528 39.979827098942536, -105.14642404528053 39.980081763840175, -105.14575666423549 39.980474763610545, -105.1455056956341 39.98064918734519, -105.14525465429142 39.980837351665556, -105.14500325520497 39.98109421840952, -105.14478523785858 39.98137690039386, -105.14484004730447 39.9814050698708, -105.14515514932701 39.981541929042045, -105.14548285188374 39.98165796143559, -105.1456310739417 39.981702065841056, -105.1459379881031 39.981766972867646, -105.14625293477762 39.98179703921972, -105.14675282658315 39.98180900367372, -105.14680426276236 39.98181279634973, -105.1468081054982 39.981912698399, -105.14680641208321 39.98218933688447, -105.14680414624985 39.98256024646881, -105.14679992288848 39.98291327827012, -105.14680010930508 39.983264617724195, -105.14679996001954 39.9833149307671, -105.14679910114454 39.98360336229756, -105.1467984523332 39.98382182769259, -105.14679783591812 39.984029061067815, -105.14679792311188 39.98423359101629, -105.14679932599793 39.98444428729881, -105.14679889229194 39.98464789066697, -105.14679873898258 39.98506280471422, -105.14679902720638 39.98514077741453, -105.14679688819109 39.98590616402691, -105.14736111026015 39.98610692973283, -105.14751902555021 39.98614480803915, -105.14843561339349 39.986362385262034, -105.14858306016312 39.98648523702375, -105.148701617686 39.98652304325331, -105.14866682986434 39.98662199615023, -105.14864489668268 39.986792132123874, -105.14864802283162 39.9868780671644, -105.14864490528718 39.986929118688266, -105.15447297744593 39.98688990858965, -105.16007586825687 39.986846994878114, -105.1636131392401 39.98682915798647, -105.1640844117053 39.98682677377659, -105.16423739853357 39.98682599908209, -105.16524839035853 39.98682087571383, -105.16524993828304 39.98682086759958, -105.16544369158672 39.98681856417538, -105.16597489399598 39.98681224725572, -105.16597511178274 39.986812246085435, -105.16597489460902 39.98681212206605, -105.16598167076747 39.98040380617206, -105.16606578502898 39.98040377608608, -105.16605762665115 39.98001166799104, -105.16605758216333 39.980011667862144, -105.16605753940114 39.98000748868384, -105.16605739165898 39.980000360446255))</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1432885288381 39.97773242539142, -105.1420770432057 39.97776765748668, -105.1409456587332 39.97776151773809, -105.1409293598499 39.97880895007127, -105.1404369659418 39.97880899577163, -105.1403200008789 39.97879408159125, -105.1399528897068 39.9787119508487, -105.1398623998234 39.97870544999949, -105.1391939833452 39.9786950285204, -105.1368970054142 39.97868457762276, -105.1368547160319 39.97965870039376, -105.1368509912206 39.9799669411584, -105.136862070902 39.98029887266666, -105.1368601054013 39.98066809809995, -105.1368619200536 39.98166791044249, -105.1368710296304 39.98263809867464, -105.1368658968665 39.98320002809678, -105.1368760662072 39.98363599987925, -105.1368760086788 39.9839149131145, -105.1369150197316 39.98402786426627, -105.136991932848 39.98412693492242, -105.137043097014 39.98416909736873, -105.1371601067108 39.98424413577549, -105.1373158899584 39.9843429050377, -105.1378400755192 39.98468907677978, -105.1379600767696 39.98480612599635, -105.1380169493754 39.98491611294507, -105.1380459539424 39.98503205218287, -105.1380488539903 39.98515806618041, -105.1380518736492 39.9856651169243, -105.1380419916548 39.98611502626242, -105.1380400266357 39.98688889589904, -105.1380400749165 39.98694709482201, -105.1421841164575 39.98696003216568, -105.1443771337807 39.98696407309227, -105.1463303467963 39.98696016489203, -105.1486449052872 39.98692911868827, -105.1486480228316 39.9868780671644, -105.1486448966827 39.98679213212387, -105.1486668298643 39.98662199615023, -105.148701617686 39.98652304325331, -105.1485830601631 39.98648523702375, -105.1484356133935 39.98636238526203, -105.1475190255502 39.98614480803915, -105.1473611102601 39.98610692973283, -105.1467968881911 39.98590616402691, -105.1467990272064 39.98514077741453, -105.1467987389826 39.98506280471422, -105.1467988922919 39.98464789066697, -105.1467993259979 39.98444428729881, -105.1467979231119 39.98423359101629, -105.1467978359181 39.98402906106782, -105.1467984523332 39.98382182769259, -105.1467991011445 39.98360336229756, -105.1467999600195 39.9833149307671, -105.1468001093051 39.9832646177242, -105.1467999228885 39.98291327827012, -105.1468041462498 39.98256024646881, -105.1468064120832 39.98218933688447, -105.1468081054982 39.981912698399, -105.1468042627624 39.98181279634973, -105.1467528265832 39.98180900367372, -105.1462529347776 39.98179703921972, -105.1459379881031 39.98176697286765, -105.1456310739417 39.98170206584106, -105.1454828518837 39.98165796143559, -105.145155149327 39.98154192904205, -105.1448400473045 39.9814050698708, -105.1447852378586 39.98137690039386, -105.145003255205 39.98109421840952, -105.1452546542914 39.98083735166556, -105.1455056956341 39.98064918734519, -105.1457566642355 39.98047476361054, -105.1464240452805 39.98008176384018, -105.1468879846528 39.97982709894254, -105.1468361234154 39.97978109470943, -105.1467799769283 39.97970215462984, -105.1467793224256 39.97967051067013, -105.1467766786365 39.9792879899573, -105.1467929027271 39.97812756649449, -105.1467964654496 39.97773046055833, -105.1463556201261 39.97772664370834, -105.1457797399434 39.97772494111891, -105.1455568987575 39.97770892415254, -105.1454398517117 39.97770993676632, -105.1443578909704 39.97771813279025, -105.1432885288381 39.97773242539142))</t>
+          <t>POLYGON ((-105.14328852883806 39.97773242539142, -105.14207704320569 39.97776765748668, -105.14094565873317 39.97776151773809, -105.14092935984995 39.97880895007127, -105.14043696594179 39.97880899577163, -105.14032000087889 39.978794081591246, -105.13995288970679 39.9787119508487, -105.13986239982341 39.97870544999949, -105.13919398334521 39.9786950285204, -105.13689700541417 39.97868457762276, -105.13685471603189 39.979658700393756, -105.13685099122064 39.9799669411584, -105.13686207090196 39.98029887266666, -105.13686010540134 39.98066809809995, -105.13686192005358 39.98166791044249, -105.13687102963041 39.98263809867464, -105.13686589686654 39.98320002809678, -105.13687606620718 39.983635999879255, -105.13687600867881 39.9839149131145, -105.1369150197316 39.98402786426627, -105.13699193284798 39.98412693492242, -105.137043097014 39.984169097368735, -105.13716010671078 39.98424413577549, -105.13731588995836 39.9843429050377, -105.13784007551922 39.98468907677978, -105.13796007676959 39.98480612599635, -105.1380169493754 39.98491611294507, -105.1380459539424 39.98503205218287, -105.13804885399031 39.98515806618041, -105.13805187364925 39.9856651169243, -105.13804199165476 39.98611502626242, -105.13804002663572 39.986888895899035, -105.13804007491647 39.986947094822014, -105.1421841164575 39.98696003216568, -105.14437713378065 39.98696407309227, -105.14633034679633 39.986960164892025, -105.14864490528718 39.986929118688266, -105.14864802283162 39.9868780671644, -105.14864489668268 39.986792132123874, -105.14866682986434 39.98662199615023, -105.148701617686 39.98652304325331, -105.14858306016312 39.98648523702375, -105.14843561339349 39.986362385262034, -105.14751902555021 39.98614480803915, -105.14736111026015 39.98610692973283, -105.14679688819109 39.98590616402691, -105.14679902720638 39.98514077741453, -105.14679873898258 39.98506280471422, -105.14679889229194 39.98464789066697, -105.14679932599793 39.98444428729881, -105.14679792311188 39.98423359101629, -105.14679783591812 39.984029061067815, -105.1467984523332 39.98382182769259, -105.14679910114454 39.98360336229756, -105.14679996001954 39.9833149307671, -105.14680010930508 39.983264617724195, -105.14679992288848 39.98291327827012, -105.14680414624985 39.98256024646881, -105.14680641208321 39.98218933688447, -105.1468081054982 39.981912698399, -105.14680426276236 39.98181279634973, -105.14675282658315 39.98180900367372, -105.14625293477762 39.98179703921972, -105.1459379881031 39.981766972867646, -105.1456310739417 39.981702065841056, -105.14548285188374 39.98165796143559, -105.14515514932701 39.981541929042045, -105.14484004730447 39.9814050698708, -105.14478523785858 39.98137690039386, -105.14500325520497 39.98109421840952, -105.14525465429142 39.980837351665556, -105.1455056956341 39.98064918734519, -105.14575666423549 39.980474763610545, -105.14642404528053 39.980081763840175, -105.1468879846528 39.979827098942536, -105.14683612341538 39.97978109470943, -105.14677997692831 39.97970215462984, -105.14677932242559 39.979670510670125, -105.14677667863653 39.9792879899573, -105.14679290272714 39.978127566494486, -105.14679646544958 39.977730460558334, -105.14635562012606 39.97772664370834, -105.14577973994338 39.977724941118915, -105.14555689875752 39.97770892415254, -105.14543985171171 39.97770993676632, -105.14435789097041 39.97771813279025, -105.14328852883806 39.97773242539142))</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1306,10 +1306,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1278491696992 39.98669844549102, -105.1278929800003 39.98688710210271, -105.1278529946731 39.98947786494407, -105.1278595500547 39.99060939569144, -105.1280717529826 39.99060563213883, -105.1282287101203 39.990606162723, -105.1307358058815 39.99061460499159, -105.1307415269931 39.98829279039961, -105.131057485362 39.98813023334419, -105.131771009591 39.98813583993596, -105.1311695131819 39.98706498517915, -105.1311069093307 39.98692138552279, -105.1319496864446 39.9869269236389, -105.1333510646578 39.98693611959428, -105.1349481206317 39.98693405035077, -105.1358909917806 39.98693593439277, -105.1380400749165 39.98694709482201, -105.1380400266357 39.98688889589904, -105.1380419916548 39.98611502626242, -105.1380518736492 39.9856651169243, -105.1380488539903 39.98515806618041, -105.1380459539424 39.98503205218287, -105.1380169493754 39.98491611294507, -105.1379600767696 39.98480612599635, -105.1378400755192 39.98468907677978, -105.1373158899584 39.9843429050377, -105.1371601067108 39.98424413577549, -105.137043097014 39.98416909736873, -105.136991932848 39.98412693492242, -105.1369150197316 39.98402786426627, -105.1368760086788 39.9839149131145, -105.1368760662072 39.98363599987925, -105.1368658968665 39.98320002809678, -105.1368710296304 39.98263809867464, -105.1368619200536 39.98166791044249, -105.1368601054013 39.98066809809995, -105.136862070902 39.98029887266666, -105.1368509912206 39.9799669411584, -105.1368547160319 39.97965870039376, -105.1368970054142 39.97868457762276, -105.1391939833452 39.9786950285204, -105.1398623998234 39.97870544999949, -105.1399528897068 39.9787119508487, -105.1403200008789 39.97879408159125, -105.1404369659418 39.97880899577163, -105.1409293598499 39.97880895007127, -105.1409456587332 39.97776151773809, -105.1420770432057 39.97776765748668, -105.1432885288381 39.97773242539142, -105.1432943712138 39.977650378093, -105.1433036870691 39.9771906058965, -105.1433117063147 39.97673384507582, -105.1433105828532 39.97615496704697, -105.1433054578167 39.97603468882662, -105.1409958621201 39.97603391013515, -105.1409831119745 39.97681055059026, -105.1402610830722 39.97681347542572, -105.1402610924567 39.97681258380209, -105.1367812813878 39.97680764905088, -105.1367812462675 39.97680764894022, -105.1367811807096 39.97680764873362, -105.13678106013 39.97680764835362, -105.1357531011968 39.97680290928571, -105.1345908763852 39.97680911350178, -105.1333829314064 39.97682394561945, -105.1321378796018 39.97683809725402, -105.1307808317385 39.97684309169715, -105.130198828228 39.97684589219254, -105.1300746618064 39.97685388159796, -105.1299589906039 39.976864768547, -105.1298379006302 39.97687795087256, -105.1297750609442 39.97688488677507, -105.129713999398 39.97689292626037, -105.1296518574046 39.97690288425013, -105.1295918539046 39.97691312287947, -105.1295311225317 39.97692610525043, -105.1292929066513 39.97696487020448, -105.1290571708148 39.97700693726274, -105.1288189364574 39.97704899579355, -105.1285810424273 39.97709407394184, -105.1278751389853 39.97724196051531, -105.1273435143957 39.97735082326365, -105.1271320977502 39.97739411515896, -105.1251821045501 39.97776690536398, -105.1220440922178 39.97834907560969, -105.1218390971384 39.97837997317655, -105.1212738234645 39.9784519641494, -105.1209279925593 39.97846208286956, -105.1206690055671 39.97844805327635, -105.1204351430655 39.97840802722106, -105.120213921188 39.9783408640164, -105.1199982265585 39.97824241435777, -105.1201190479548 39.97979700902974, -105.120230166672 39.98108244243971, -105.1219081678686 39.98099644262695, -105.1225391670139 39.98073944211418, -105.1232421681502 39.98033144190374, -105.1235891680376 39.98066744275177, -105.1243405817918 39.98021614971381, -105.1255771679067 39.97947344233817, -105.1253541688852 39.97925444189506, -105.1255304415947 39.97914450912447, -105.1260051674357 39.97884844174765, -105.1262311691111 39.97870844220219, -105.1271081689285 39.97816144152506, -105.1276701687788 39.97808644191434, -105.1276742985784 39.97835509150174, -105.1276812036791 39.97880423869458, -105.1276880805791 39.97925149078886, -105.12769489113 39.97973687298536, -105.1276979486562 39.98011536714193, -105.1276992570783 39.98027720192252, -105.1277006654453 39.98045161563807, -105.1277022727454 39.98065050362139, -105.1277031693758 39.98076144258219, -105.1275471685854 39.9807554418902, -105.1274521692765 39.98074644262105, -105.1273271684002 39.98072644199087, -105.1273066551089 39.98072157695184, -105.127214375739 39.98069969063391, -105.1271711685487 39.98068944278467, -105.127139392241 39.98068334791111, -105.1270981684207 39.98067544186095, -105.1269711680979 39.98065844167844, -105.1268901681804 39.98065044284952, -105.1267971687024 39.98065044260115, -105.1266971688295 39.98065244248855, -105.1266091684414 39.98065844226225, -105.1264991677584 39.98067244239655, -105.126331169116 39.98070644271509, -105.1261481677718 39.9807394421338, -105.1259671694033 39.98075344203813, -105.1258431687578 39.98075244156166, -105.1256331685554 39.98073244235897, -105.1254741692224 39.98069944174981, -105.1253301685872 39.98066944203719, -105.1250891674626 39.98064744247992, -105.12468924775 39.98064430008328, -105.1239441684502 39.98063844197828, -105.1239481684561 39.98099044193104, -105.123848168531 39.98109744278342, -105.1237131684662 39.98127144197014, -105.1236411680837 39.98141344271861, -105.123586168347 39.98161144252593, -105.1235830349789 39.98201442443881, -105.1235781685477 39.98264044277064, -105.1236691677244 39.98278344313378, -105.123744168235 39.98286744302084, -105.1238561683382 39.98296444303244, -105.1240021678686 39.98305844296069, -105.1242251688294 39.98315444282675, -105.1249263230647 39.98314996424318, -105.1258921445311 39.98314315953377, -105.1268441685182 39.98313644257139, -105.1268601685777 39.98365144197767, -105.1278411686021 39.98365144210749, -105.1278251690041 39.98379744319919, -105.1278173436443 39.98417719271642, -105.1278081691162 39.98462244192449, -105.1278341691096 39.98513544239999, -105.1278368922283 39.98539987307798, -105.127841169928 39.98581544210798, -105.1278438505662 39.98611127501945, -105.1278491696992 39.98669844549102))</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
+          <t>POLYGON ((-105.12784916969922 39.986698445491015, -105.12789298000034 39.98688710210271, -105.12785299467315 39.98947786494407, -105.12785955005472 39.990609395691436, -105.1280717529826 39.99060563213883, -105.12822871012031 39.990606162723005, -105.13073580588154 39.99061460499159, -105.13074152699315 39.98829279039961, -105.131057485362 39.988130233344194, -105.13177100959103 39.988135839935964, -105.1311695131819 39.98706498517915, -105.13110690933073 39.98692138552279, -105.13194968644457 39.986926923638904, -105.13335106465783 39.98693611959428, -105.13494812063175 39.98693405035077, -105.13589099178058 39.98693593439277, -105.13804007491647 39.986947094822014, -105.13804002663572 39.986888895899035, -105.13804199165476 39.98611502626242, -105.13805187364925 39.9856651169243, -105.13804885399031 39.98515806618041, -105.1380459539424 39.98503205218287, -105.1380169493754 39.98491611294507, -105.13796007676959 39.98480612599635, -105.13784007551922 39.98468907677978, -105.13731588995836 39.9843429050377, -105.13716010671078 39.98424413577549, -105.137043097014 39.984169097368735, -105.13699193284798 39.98412693492242, -105.1369150197316 39.98402786426627, -105.13687600867881 39.9839149131145, -105.13687606620718 39.983635999879255, -105.13686589686654 39.98320002809678, -105.13687102963041 39.98263809867464, -105.13686192005358 39.98166791044249, -105.13686010540134 39.98066809809995, -105.13686207090196 39.98029887266666, -105.13685099122064 39.9799669411584, -105.13685471603189 39.979658700393756, -105.13689700541417 39.97868457762276, -105.13919398334521 39.9786950285204, -105.13986239982341 39.97870544999949, -105.13995288970679 39.9787119508487, -105.14032000087889 39.978794081591246, -105.14043696594179 39.97880899577163, -105.14092935984995 39.97880895007127, -105.14094565873317 39.97776151773809, -105.14207704320569 39.97776765748668, -105.14328852883806 39.97773242539142, -105.14329437121383 39.977650378092996, -105.14330368706908 39.977190605896496, -105.14331170631475 39.97673384507582, -105.14331058285325 39.976154967046966, -105.14330545781672 39.97603468882662, -105.14099586212012 39.97603391013515, -105.14098311197453 39.97681055059026, -105.14026108307223 39.97681347542572, -105.14026109245668 39.97681258380209, -105.13678128138777 39.976807649050876, -105.1367812462675 39.976807648940216, -105.13678118070965 39.97680764873362, -105.13678106013002 39.97680764835362, -105.13575310119678 39.97680290928571, -105.13459087638523 39.97680911350178, -105.13338293140637 39.97682394561945, -105.13213787960184 39.97683809725402, -105.13078083173855 39.97684309169715, -105.13019882822799 39.976845892192536, -105.13007466180638 39.97685388159796, -105.12995899060385 39.976864768547, -105.12983790063018 39.97687795087256, -105.12977506094421 39.976884886775075, -105.12971399939796 39.97689292626037, -105.12965185740464 39.97690288425013, -105.12959185390464 39.976913122879466, -105.12953112253166 39.976926105250435, -105.1292929066513 39.976964870204476, -105.12905717081482 39.97700693726274, -105.12881893645745 39.97704899579355, -105.12858104242734 39.977094073941835, -105.12787513898526 39.977241960515315, -105.12734351439568 39.97735082326365, -105.12713209775025 39.97739411515896, -105.12518210455008 39.97776690536398, -105.12204409221776 39.97834907560969, -105.12183909713839 39.97837997317655, -105.1212738234645 39.9784519641494, -105.12092799255929 39.978462082869555, -105.12066900556705 39.978448053276345, -105.12043514306552 39.978408027221064, -105.120213921188 39.978340864016396, -105.11999822655854 39.97824241435777, -105.12011904795484 39.97979700902974, -105.12023016667196 39.98108244243971, -105.12190816786861 39.980996442626946, -105.12253916701391 39.98073944211418, -105.12324216815017 39.98033144190374, -105.12358916803758 39.980667442751766, -105.12434058179181 39.98021614971381, -105.12557716790668 39.97947344233817, -105.12535416888515 39.97925444189506, -105.12553044159466 39.97914450912447, -105.12600516743572 39.97884844174765, -105.1262311691111 39.97870844220219, -105.12710816892852 39.97816144152506, -105.12767016877879 39.978086441914336, -105.12767429857837 39.97835509150174, -105.1276812036791 39.97880423869458, -105.12768808057913 39.97925149078886, -105.12769489113002 39.97973687298536, -105.12769794865618 39.98011536714193, -105.12769925707835 39.98027720192252, -105.12770066544532 39.98045161563807, -105.12770227274538 39.98065050362139, -105.12770316937583 39.980761442582185, -105.12754716858537 39.980755441890196, -105.12745216927647 39.980746442621054, -105.12732716840023 39.98072644199087, -105.1273066551089 39.98072157695184, -105.12721437573896 39.980699690633905, -105.12717116854866 39.98068944278467, -105.127139392241 39.98068334791111, -105.12709816842069 39.980675441860946, -105.1269711680979 39.980658441678436, -105.1268901681804 39.980650442849516, -105.12679716870242 39.98065044260115, -105.12669716882947 39.98065244248855, -105.1266091684414 39.980658442262246, -105.1264991677584 39.98067244239655, -105.12633116911601 39.98070644271509, -105.12614816777177 39.9807394421338, -105.12596716940325 39.98075344203813, -105.1258431687578 39.98075244156166, -105.12563316855537 39.98073244235897, -105.12547416922237 39.98069944174981, -105.12533016858723 39.98066944203719, -105.12508916746263 39.98064744247992, -105.12468924774997 39.980644300083284, -105.12394416845024 39.98063844197828, -105.12394816845612 39.98099044193104, -105.12384816853096 39.981097442783415, -105.12371316846621 39.98127144197014, -105.12364116808365 39.98141344271861, -105.123586168347 39.98161144252593, -105.12358303497885 39.98201442443881, -105.12357816854767 39.982640442770645, -105.12366916772436 39.98278344313378, -105.12374416823499 39.98286744302084, -105.12385616833825 39.98296444303244, -105.12400216786861 39.98305844296069, -105.12422516882944 39.98315444282675, -105.12492632306473 39.983149964243175, -105.12589214453108 39.98314315953377, -105.12684416851818 39.98313644257139, -105.12686016857774 39.98365144197767, -105.1278411686021 39.983651442107494, -105.12782516900411 39.98379744319919, -105.12781734364428 39.98417719271642, -105.12780816911615 39.984622441924486, -105.12783416910956 39.98513544239999, -105.12783689222834 39.98539987307798, -105.127841169928 39.985815442107985, -105.12784385056624 39.98611127501945, -105.12784916969922 39.986698445491015))</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Louisville MS</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1344,7 +1348,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.122814800146 39.9941474397444, -105.1232589140897 39.9941456611968, -105.1232577328613 39.99406674611331, -105.1277274031719 39.99403166429317, -105.1279510944342 39.99413186772644, -105.130985314058 39.99412962806004, -105.1373254730912 39.99414433762385, -105.1373344848354 39.99415560978961, -105.1373171675768 39.99412687745504, -105.137238682844 39.99402892802352, -105.137074025071 39.99382251842898, -105.1369478356576 39.99366484366936, -105.1366846484058 39.99334350090711, -105.1363601032011 39.99293808389312, -105.1362092993563 39.9927488742651, -105.1360892608934 39.99260074961433, -105.1359338287744 39.99240842764129, -105.1357523239725 39.99216717136393, -105.1355853380476 39.99196337403938, -105.1354053211107 39.99173403761317, -105.1352268226642 39.99151066265726, -105.1350337149407 39.99126770047961, -105.1348936768962 39.99109449003459, -105.1347274599285 39.99089260055993, -105.1345659104594 39.9906871500192, -105.1344186234449 39.99050843549372, -105.1342816803595 39.99033642476832, -105.1341170481164 39.9901285815575, -105.1339768844758 39.98995084195541, -105.1338799556239 39.98982780950551, -105.1337830079288 39.98970835162631, -105.1336506897271 39.98954112200693, -105.1335091236261 39.98936552183038, -105.1333279086329 39.98913117329037, -105.1332093986706 39.98898900736968, -105.133052472283 39.98878952811079, -105.1328912098864 39.98859003392314, -105.1328035729189 39.98846822260197, -105.1327035629912 39.98834279617489, -105.1326097496832 39.98821738940678, -105.1325421026776 39.98812304593438, -105.1324468372132 39.98797976262467, -105.1323501027325 39.98782169923754, -105.1322764196897 39.98769754795746, -105.1321829035977 39.98751733397457, -105.1320788415059 39.98728227664778, -105.1320229031967 39.98714245361968, -105.1319838670466 39.98702794530658, -105.1319663894916 39.9869762907518, -105.1319496864446 39.9869269236389, -105.1311069093307 39.98692138552279, -105.1311695131819 39.98706498517915, -105.131771009591 39.98813583993596, -105.131057485362 39.98813023334419, -105.1307415269931 39.98829279039961, -105.1307358058815 39.99061460499159, -105.1282287101203 39.990606162723, -105.1280717529826 39.99060563213883, -105.1278595500547 39.99060939569144, -105.1278529946731 39.98947786494407, -105.1278929788344 39.98688710119829, -105.127849169714 39.9866984427891, -105.1252729795815 39.9867354607854, -105.1230647672254 39.98677086630205, -105.1211532829889 39.9867767735869, -105.1185851681232 39.98678444408168, -105.1186071665135 39.98330244358745, -105.1174133094992 39.98331547110325, -105.1173974168023 39.9851484639417, -105.1173718857854 39.98689901321579, -105.1173699922748 39.98694351032786, -105.1185703104926 39.98693549769058, -105.118575976712 39.98710775588565, -105.1185474045477 39.99235909652852, -105.1185472892864 39.99238619608135, -105.1189229397637 39.99238378801977, -105.1199496728335 39.99237720607682, -105.1204839651552 39.99237377836661, -105.121007043891 39.9923704175954, -105.1222303531299 39.99236784607286, -105.1223383484516 39.99236705245885, -105.1223389573864 39.99236704634767, -105.1223232452224 39.99378812123183, -105.1223849223714 39.99378832326342, -105.1225145804866 39.99383477964317, -105.1226719071595 39.99394172642054, -105.122814800146 39.9941474397444))</t>
+          <t>POLYGON ((-105.12281480014596 39.994147439744395, -105.1232589140897 39.9941456611968, -105.12325773286126 39.99406674611331, -105.12772740317189 39.994031664293175, -105.12795109443424 39.99413186772644, -105.13098531405798 39.994129628060044, -105.1373254730912 39.99414433762385, -105.13733448483536 39.99415560978961, -105.13731716757682 39.99412687745504, -105.13723868284397 39.99402892802352, -105.13707402507096 39.99382251842898, -105.13694783565762 39.99366484366936, -105.13668464840583 39.99334350090711, -105.13636010320106 39.99293808389312, -105.13620929935627 39.9927488742651, -105.13608926089341 39.992600749614326, -105.13593382877438 39.99240842764129, -105.13575232397254 39.99216717136393, -105.13558533804756 39.99196337403938, -105.1354053211107 39.99173403761317, -105.1352268226642 39.99151066265726, -105.13503371494068 39.99126770047961, -105.1348936768962 39.99109449003459, -105.13472745992847 39.99089260055993, -105.13456591045943 39.9906871500192, -105.13441862344494 39.99050843549372, -105.13428168035952 39.990336424768316, -105.13411704811641 39.9901285815575, -105.13397688447584 39.989950841955405, -105.13387995562393 39.98982780950551, -105.13378300792884 39.989708351626305, -105.13365068972713 39.989541122006926, -105.13350912362614 39.98936552183038, -105.13332790863292 39.989131173290374, -105.13320939867059 39.98898900736968, -105.13305247228296 39.98878952811079, -105.13289120988635 39.98859003392314, -105.13280357291886 39.98846822260197, -105.13270356299121 39.98834279617489, -105.13260974968317 39.988217389406785, -105.13254210267756 39.98812304593438, -105.13244683721317 39.98797976262467, -105.13235010273253 39.987821699237536, -105.1322764196897 39.98769754795746, -105.13218290359771 39.98751733397457, -105.13207884150593 39.98728227664778, -105.13202290319668 39.987142453619676, -105.13198386704664 39.98702794530658, -105.13196638949155 39.9869762907518, -105.13194968644457 39.986926923638904, -105.13110690933073 39.98692138552279, -105.1311695131819 39.98706498517915, -105.13177100959103 39.988135839935964, -105.131057485362 39.988130233344194, -105.13074152699315 39.98829279039961, -105.13073580588154 39.99061460499159, -105.12822871012031 39.990606162723005, -105.1280717529826 39.99060563213883, -105.12785955005472 39.990609395691436, -105.12785299467315 39.98947786494407, -105.12789297883441 39.98688710119829, -105.12784916971395 39.9866984427891, -105.12527297958147 39.986735460785404, -105.12306476722542 39.98677086630205, -105.12115328298886 39.9867767735869, -105.1185851681232 39.98678444408168, -105.11860716651354 39.983302443587455, -105.11741330949921 39.983315471103246, -105.11739741680232 39.9851484639417, -105.11737188578539 39.98689901321579, -105.11736999227477 39.98694351032786, -105.11857031049257 39.98693549769058, -105.11857597671197 39.987107755885646, -105.11854740454771 39.992359096528524, -105.11854728928638 39.99238619608135, -105.1189229397637 39.99238378801977, -105.11994967283347 39.992377206076824, -105.12048396515519 39.992373778366606, -105.12100704389098 39.992370417595396, -105.12223035312992 39.99236784607286, -105.12233834845158 39.992367052458846, -105.12233895738636 39.992367046347674, -105.12232324522239 39.99378812123183, -105.12238492237144 39.993788323263416, -105.12251458048662 39.993834779643166, -105.12267190715949 39.99394172642054, -105.12281480014596 39.994147439744395))</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1386,7 +1390,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1373344848354 39.99415560978961, -105.1405141950552 39.99813279982534, -105.1407003492131 39.99804212814589, -105.1412987486078 39.99773918448757, -105.1415483564617 39.99743752080339, -105.1418815666315 39.99705442482142, -105.1422639133758 39.99651569716553, -105.1442614765063 39.99492166747812, -105.1443011561806 39.99478265717581, -105.145432872713 39.99479210016541, -105.1459611770951 39.99455926085398, -105.1464615829938 39.99416230126948, -105.1464417042601 39.99416206738315, -105.144391560983 39.99414172076281, -105.1420251518719 39.99413754337094, -105.1420251150731 39.99409011730622, -105.1420196366719 39.99328214605311, -105.1420443856928 39.99194516432361, -105.1420481770373 39.99174975307309, -105.1420734313855 39.99063712851107, -105.1420783450416 39.98928484211632, -105.1415918589478 39.98910192904754, -105.1413589869341 39.98899990595528, -105.1412199367258 39.98890586154172, -105.1411048925439 39.98879404785005, -105.1410390000473 39.98870105504957, -105.1408521197491 39.98840508760531, -105.1407751612244 39.98831288337433, -105.140741088259 39.98827708949863, -105.1406048747112 39.98818689627998, -105.1404471198639 39.98812106878106, -105.1400201332226 39.98801404484783, -105.1392598453997 39.98783405292181, -105.1389948690339 39.98779808513689, -105.1380318297478 39.98776102489464, -105.1380390475004 39.98700611356928, -105.1380400749165 39.98694709482201, -105.1358909917806 39.98693593439277, -105.1349481206317 39.98693405035077, -105.1333510646578 39.98693611959428, -105.1319496864446 39.9869269236389, -105.1319663894916 39.9869762907518, -105.1319838670466 39.98702794530658, -105.1320229031967 39.98714245361968, -105.1320788415059 39.98728227664778, -105.1321829035977 39.98751733397457, -105.1322764196897 39.98769754795746, -105.1323501027325 39.98782169923754, -105.1324468372132 39.98797976262467, -105.1325421026776 39.98812304593438, -105.1326097496832 39.98821738940678, -105.1327035629912 39.98834279617489, -105.1328035729189 39.98846822260197, -105.1328912098864 39.98859003392314, -105.133052472283 39.98878952811079, -105.1332093986706 39.98898900736968, -105.1333279086329 39.98913117329037, -105.1335091236261 39.98936552183038, -105.1336506897271 39.98954112200693, -105.1337830079288 39.98970835162631, -105.1338799556239 39.98982780950551, -105.1339768844758 39.98995084195541, -105.1341170481164 39.9901285815575, -105.1342816803595 39.99033642476832, -105.1344186234449 39.99050843549372, -105.1345659104594 39.9906871500192, -105.1347274599285 39.99089260055993, -105.1348936768962 39.99109449003459, -105.1350337149407 39.99126770047961, -105.1352268226642 39.99151066265726, -105.1354053211107 39.99173403761317, -105.1355853380476 39.99196337403938, -105.1357523239725 39.99216717136393, -105.1359338287744 39.99240842764129, -105.1360892608934 39.99260074961433, -105.1362092993563 39.9927488742651, -105.1363601032011 39.99293808389312, -105.1366846484058 39.99334350090711, -105.1369478356576 39.99366484366936, -105.137074025071 39.99382251842898, -105.137238682844 39.99402892802352, -105.1373171675768 39.99412687745504, -105.1373344848354 39.99415560978961))</t>
+          <t>POLYGON ((-105.13733448483536 39.99415560978961, -105.1405141950552 39.99813279982534, -105.14070034921306 39.99804212814589, -105.14129874860778 39.99773918448757, -105.14154835646167 39.997437520803395, -105.14188156663147 39.99705442482142, -105.14226391337579 39.99651569716553, -105.14426147650629 39.994921667478124, -105.14430115618062 39.99478265717581, -105.145432872713 39.994792100165405, -105.14596117709509 39.994559260853976, -105.14646158299378 39.994162301269476, -105.1464417042601 39.99416206738315, -105.14439156098304 39.99414172076281, -105.14202515187186 39.99413754337094, -105.14202511507307 39.99409011730622, -105.1420196366719 39.99328214605311, -105.1420443856928 39.99194516432361, -105.14204817703734 39.99174975307309, -105.14207343138551 39.99063712851107, -105.14207834504158 39.98928484211632, -105.14159185894778 39.989101929047536, -105.14135898693414 39.98899990595528, -105.14121993672583 39.988905861541724, -105.14110489254391 39.98879404785005, -105.14103900004729 39.988701055049575, -105.14085211974908 39.98840508760531, -105.14077516122435 39.98831288337433, -105.14074108825902 39.98827708949863, -105.14060487471124 39.98818689627998, -105.14044711986395 39.98812106878106, -105.14002013322259 39.98801404484783, -105.13925984539972 39.98783405292181, -105.13899486903388 39.98779808513689, -105.13803182974779 39.98776102489464, -105.13803904750041 39.98700611356928, -105.13804007491647 39.986947094822014, -105.13589099178058 39.98693593439277, -105.13494812063175 39.98693405035077, -105.13335106465783 39.98693611959428, -105.13194968644457 39.986926923638904, -105.13196638949155 39.9869762907518, -105.13198386704664 39.98702794530658, -105.13202290319668 39.987142453619676, -105.13207884150593 39.98728227664778, -105.13218290359771 39.98751733397457, -105.1322764196897 39.98769754795746, -105.13235010273253 39.987821699237536, -105.13244683721317 39.98797976262467, -105.13254210267756 39.98812304593438, -105.13260974968317 39.988217389406785, -105.13270356299121 39.98834279617489, -105.13280357291886 39.98846822260197, -105.13289120988635 39.98859003392314, -105.13305247228296 39.98878952811079, -105.13320939867059 39.98898900736968, -105.13332790863292 39.989131173290374, -105.13350912362614 39.98936552183038, -105.13365068972713 39.989541122006926, -105.13378300792884 39.989708351626305, -105.13387995562393 39.98982780950551, -105.13397688447584 39.989950841955405, -105.13411704811641 39.9901285815575, -105.13428168035952 39.990336424768316, -105.13441862344494 39.99050843549372, -105.13456591045943 39.9906871500192, -105.13472745992847 39.99089260055993, -105.1348936768962 39.99109449003459, -105.13503371494068 39.99126770047961, -105.1352268226642 39.99151066265726, -105.1354053211107 39.99173403761317, -105.13558533804756 39.99196337403938, -105.13575232397254 39.99216717136393, -105.13593382877438 39.99240842764129, -105.13608926089341 39.992600749614326, -105.13620929935627 39.9927488742651, -105.13636010320106 39.99293808389312, -105.13668464840583 39.99334350090711, -105.13694783565762 39.99366484366936, -105.13707402507096 39.99382251842898, -105.13723868284397 39.99402892802352, -105.13731716757682 39.99412687745504, -105.13733448483536 39.99415560978961))</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1428,7 +1432,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1464417042601 39.99416206738315, -105.1464615829938 39.99416230126948, -105.1466363980306 39.99416436382368, -105.146790174619 39.9941694428106, -105.1467891751321 39.99400744202379, -105.1489619720619 39.99399513205215, -105.1511885403603 39.99398043009678, -105.1527391763146 39.99397744204157, -105.1527289655441 39.99412802825835, -105.1548798542597 39.99410483914303, -105.1548904876865 39.99260044586263, -105.1548905001314 39.99259868061086, -105.1548910742555 39.99251738266482, -105.1548927785468 39.99227636637016, -105.1550702284904 39.99239786295302, -105.1560127966663 39.99270667940952, -105.1561716319405 39.99274373072714, -105.156359603665 39.99274076059307, -105.1570945121236 39.99246391068015, -105.1576955197453 39.99206442405352, -105.158249423521 39.99149224398947, -105.1585727934224 39.99093128003249, -105.1582367037443 39.99049132434087, -105.1582351763826 39.99048931494893, -105.1598894223283 39.99048544917379, -105.1603292951578 39.99048441784612, -105.1644396301791 39.99047469439939, -105.165293913414 39.9904726547182, -105.165280121269 39.98963940654668, -105.1652800904351 39.98963757722175, -105.1630484245457 39.98939258460942, -105.1629316619924 39.98939933324853, -105.1629369535138 39.98923604238151, -105.1629411450479 39.9891100499324, -105.1629701445979 39.98894706885007, -105.1630340843738 39.98879105290501, -105.1631318802227 39.98864501967785, -105.1632068468137 39.98856892148969, -105.1633738472757 39.98842912912709, -105.1636180300277 39.98827007062972, -105.1638820078671 39.98807702897645, -105.1639629797611 39.98801302742708, -105.1640557053296 39.98791588344694, -105.164152903713 39.98795517594412, -105.1652129168158 39.98840770990265, -105.1652600612412 39.9884278360004, -105.16525834624 39.98830990071465, -105.1652418264078 39.98717422250558, -105.1652483903585 39.98682087571383, -105.1642373985336 39.98682599908209, -105.1640844117053 39.98682677377659, -105.1636131392401 39.98682915798647, -105.1600758682569 39.98684699487811, -105.1544729774459 39.98688990858965, -105.1486449052872 39.98692911868827, -105.1463303467963 39.98696016489203, -105.1443771337807 39.98696407309227, -105.1421841164575 39.98696003216568, -105.1380400749165 39.98694709482201, -105.1380390475004 39.98700611356928, -105.1380318297478 39.98776102489464, -105.1389948690339 39.98779808513689, -105.1392598453997 39.98783405292181, -105.1400201332226 39.98801404484783, -105.1404471198639 39.98812106878106, -105.1406048747112 39.98818689627998, -105.140741088259 39.98827708949863, -105.1407751612244 39.98831288337433, -105.1408521197491 39.98840508760531, -105.1410390000473 39.98870105504957, -105.1411048925439 39.98879404785005, -105.1412199367258 39.98890586154172, -105.1413589869341 39.98899990595528, -105.1415918589478 39.98910192904754, -105.1420783450416 39.98928484211632, -105.1420734313855 39.99063712851107, -105.1420481770373 39.99174975307309, -105.1420443856928 39.99194516432361, -105.1420196366719 39.99328214605311, -105.1420251150731 39.99409011730622, -105.1420251518719 39.99413754337094, -105.144391560983 39.99414172076281, -105.1464417042601 39.99416206738315))</t>
+          <t>POLYGON ((-105.1464417042601 39.99416206738315, -105.14646158299378 39.994162301269476, -105.1466363980306 39.99416436382368, -105.14679017461899 39.9941694428106, -105.14678917513206 39.994007442023786, -105.14896197206194 39.99399513205215, -105.15118854036027 39.99398043009678, -105.15273917631464 39.99397744204157, -105.15272896554406 39.99412802825835, -105.15487985425969 39.99410483914303, -105.15489048768646 39.99260044586263, -105.15489050013137 39.99259868061086, -105.1548910742555 39.99251738266482, -105.15489277854675 39.992276366370156, -105.15507022849043 39.99239786295302, -105.15601279666635 39.992706679409515, -105.15617163194054 39.99274373072714, -105.15635960366501 39.99274076059307, -105.1570945121236 39.99246391068015, -105.1576955197453 39.99206442405352, -105.15824942352096 39.99149224398947, -105.15857279342244 39.99093128003249, -105.15823670374425 39.99049132434087, -105.15823517638263 39.99048931494893, -105.15988942232826 39.99048544917379, -105.16032929515781 39.99048441784612, -105.16443963017906 39.99047469439939, -105.16529391341399 39.990472654718204, -105.16528012126903 39.98963940654668, -105.16528009043512 39.98963757722175, -105.16304842454566 39.98939258460942, -105.16293166199242 39.98939933324853, -105.1629369535138 39.989236042381506, -105.16294114504788 39.9891100499324, -105.16297014459795 39.988947068850074, -105.1630340843738 39.98879105290501, -105.16313188022269 39.988645019677854, -105.16320684681372 39.988568921489694, -105.16337384727566 39.98842912912709, -105.1636180300277 39.988270070629724, -105.16388200786707 39.98807702897645, -105.16396297976111 39.98801302742708, -105.1640557053296 39.98791588344694, -105.16415290371303 39.98795517594412, -105.16521291681579 39.98840770990265, -105.16526006124123 39.9884278360004, -105.16525834624004 39.98830990071465, -105.16524182640784 39.98717422250558, -105.16524839035853 39.98682087571383, -105.16423739853357 39.98682599908209, -105.1640844117053 39.98682677377659, -105.1636131392401 39.98682915798647, -105.16007586825687 39.986846994878114, -105.15447297744593 39.98688990858965, -105.14864490528718 39.986929118688266, -105.14633034679633 39.986960164892025, -105.14437713378065 39.98696407309227, -105.1421841164575 39.98696003216568, -105.13804007491647 39.986947094822014, -105.13803904750041 39.98700611356928, -105.13803182974779 39.98776102489464, -105.13899486903388 39.98779808513689, -105.13925984539972 39.98783405292181, -105.14002013322259 39.98801404484783, -105.14044711986395 39.98812106878106, -105.14060487471124 39.98818689627998, -105.14074108825902 39.98827708949863, -105.14077516122435 39.98831288337433, -105.14085211974908 39.98840508760531, -105.14103900004729 39.988701055049575, -105.14110489254391 39.98879404785005, -105.14121993672583 39.988905861541724, -105.14135898693414 39.98899990595528, -105.14159185894778 39.989101929047536, -105.14207834504158 39.98928484211632, -105.14207343138551 39.99063712851107, -105.14204817703734 39.99174975307309, -105.1420443856928 39.99194516432361, -105.1420196366719 39.99328214605311, -105.14202511507307 39.99409011730622, -105.14202515187186 39.99413754337094, -105.14439156098304 39.99414172076281, -105.1464417042601 39.99416206738315))</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1470,7 +1474,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON (((-105.0528281835631 39.98653346176652, -105.057580642476 39.98649541493525, -105.0623500000977 39.98645786501839, -105.0634606537379 39.98647581498217, -105.0634909949253 39.98647646216797, -105.0670338384547 39.98653575957677, -105.0670371933367 39.98633703838531, -105.0670383169087 39.98633729479067, -105.0670400578877 39.98623419443279, -105.0670935888734 39.98306391759739, -105.0704747521287 39.9830759158628, -105.0709660816366 39.98308237411967, -105.0717146023103 39.9830922080333, -105.0717552482085 39.98309274272643, -105.0718117048491 39.98309269216385, -105.0718160675592 39.98243292109945, -105.0718328878368 39.98140187753952, -105.0718501168945 39.98058990350253, -105.0718568404095 39.98014410421328, -105.0718668765302 39.9794736037379, -105.0719256017096 39.97947406682838, -105.072615305267 39.97948638758501, -105.0732085340372 39.97949698163314, -105.0737704031381 39.9795008692249, -105.0740721520792 39.9795029564586, -105.0743940604178 39.97950518038726, -105.0757716939829 39.97952383912966, -105.0761908360338 39.97952951234009, -105.079294460449 39.97957148382346, -105.0834853211123 39.97962377507007, -105.0835085716659 39.97962404552135, -105.0903270877842 39.9797032929451, -105.0904860571139 39.97970281937673, -105.0904860309043 39.97970621027422, -105.0906909442718 39.97970782075467, -105.0952100830245 39.97971518827352, -105.0951916295389 39.97607892625242, -105.09057003187 39.97607998460246, -105.0904542693785 39.97608297782843, -105.0904417425443 39.97584710582651, -105.0904193253848 39.97563881566658, -105.0903689920018 39.97550995382825, -105.0902914261388 39.9752737605607, -105.0902418876107 39.97501264559047, -105.090192863608 39.97466574347093, -105.09020081638 39.97411529796517, -105.090215942638 39.97240347779733, -105.0903030782694 39.97240400643749, -105.0909639507684 39.97239290149737, -105.0911648255174 39.9723941636361, -105.0912461536423 39.97239802052451, -105.0913521083569 39.97240086766923, -105.091422029526 39.97240303667677, -105.0936430785647 39.97241500683583, -105.0943081662019 39.97241487935375, -105.0946450026706 39.97241304460964, -105.0950421100944 39.97241608789733, -105.0953327932177 39.97241727370804, -105.0953437698846 39.97241731765187, -105.0953442665838 39.9725246251522, -105.0953453933799 39.97327727257912, -105.0959485841525 39.97327529347321, -105.0959485145728 39.97252466095966, -105.0959494027172 39.97241976308735, -105.095958529845 39.97241979958787, -105.0968671338764 39.97242303532938, -105.0974380772597 39.97241405009566, -105.0975640093021 39.97241206530735, -105.0975654791955 39.97243912451826, -105.0975682202136 39.97252892556443, -105.097555653059 39.97609100741533, -105.1045601154635 39.97610235688621, -105.1045682620514 39.97377105019996, -105.1054698415779 39.97377082908722, -105.105473750072 39.97254757141797, -105.1054728138778 39.97241715154041, -105.1062811423174 39.97241796939557, -105.1084309638869 39.97240690009586, -105.1092651591187 39.97241000593239, -105.1092319271565 39.97335287654287, -105.1092231749659 39.97382200756769, -105.1092751638475 39.97241644265112, -105.1093741622733 39.95969644064292, -105.1093821626999 39.95928944047934, -105.1079021614665 39.95931444023918, -105.1078871611286 39.95851244033037, -105.1081481615724 39.95847244081943, -105.108159162151 39.95790844019832, -105.1081605804928 39.95790194404009, -105.1093269988958 39.95789799857891, -105.1093269891051 39.95789786885034, -105.1145961633331 39.95785343948453, -105.114596161064 39.95785363401997, -105.1145691634786 39.96033344011676, -105.1152741627195 39.96032944007523, -105.1152851630498 39.95784852040962, -105.1152851635068 39.95784843935154, -105.1153011708886 39.95784840182763, -105.1280631665933 39.95781743936814, -105.1279511266712 39.9541802399316, -105.1275969938948 39.95418130612799, -105.123917995392 39.95417275040911, -105.122915947411 39.9541704003749, -105.1221412534314 39.95416857667849, -105.1219282161555 39.95416609003437, -105.1219274612313 39.95416420247147, -105.1219274219854 39.9541641041705, -105.1218596147571 39.95399464274431, -105.1218595928261 39.95399458773195, -105.1218588428563 39.95399265154909, -105.1212409789274 39.95239711023925, -105.1212402116839 39.95239512986274, -105.1211425524197 39.95214293317645, -105.1208344622029 39.95231849365693, -105.1202915592579 39.95263547808772, -105.1195382450427 39.95307531282278, -105.1191493047299 39.95329831619954, -105.1187553437 39.95351607060863, -105.1187141847171 39.9535379997394, -105.1186784815315 39.9535570152557, -105.1186187238068 39.95358884322316, -105.1183565051931 39.95372850081748, -105.117952905488 39.95393554051217, -105.1175446702312 39.95413712341077, -105.1171319226882 39.95433319133069, -105.1168183436197 39.95447639359539, -105.116714786145 39.9545236833886, -105.1163333293274 39.95469102504197, -105.116313361281 39.95469978414111, -105.1162933932295 39.95470854323679, -105.1159620331638 39.95484806240092, -105.1158678660671 39.95488770999074, -105.1154383419312 39.95506113542697, -105.1150049476127 39.95522876318281, -105.1145677688295 39.95539055747477, -105.1141270308449 39.95554643435185, -105.1140082423906 39.95558653116191, -105.1136828193298 39.95569636794119, -105.1133266682007 39.95581051213452, -105.1131700219747 39.95586071435858, -105.1126929847616 39.95600929462459, -105.1116536337618 39.9563330070136, -105.1096858334962 39.95694394506538, -105.1096858339151 39.95694203025841, -105.1096858341623 39.95694198702748, -105.1096858348311 39.95694166549327, -105.1096858834961 39.95675247881106, -105.1096858833603 39.95675209332704, -105.1096858849444 39.95675017942472, -105.1096859488912 39.95650205073775, -105.1096859492947 39.95650013863272, -105.1096860642593 39.95606241165259, -105.1096860656454 39.9560578723183, -105.1097953395361 39.95602384071586, -105.1116617064129 39.95544256909836, -105.1116618529628 39.95544252365849, -105.1117767887673 39.95540672865434, -105.1117769341467 39.95540668321035, -105.1127687274608 39.95509777442294, -105.1127688540783 39.95509773521934, -105.1131990914742 39.95496035760923, -105.1131991758889 39.95496033087274, -105.1133510467449 39.95490942808447, -105.11335113234 39.95490939955047, -105.1136263172395 39.95481716172755, -105.1136263582815 39.95481714745462, -105.114012933914 39.95468134876749, -105.1140129761261 39.9546813344983, -105.1140502299476 39.95466824747247, -105.114470783806 39.95451362643593, -105.1148876386112 39.95435342811378, -105.1148876796628 39.95435341203906, -105.1153007919514 39.95418765163744, -105.1153008740644 39.95418761768639, -105.1157101228989 39.95401635248451, -105.1157102437373 39.95401629974841, -105.1159825492359 39.95389755732932, -105.1159827099648 39.95389748671265, -105.1161155012183 39.95383957709619, -105.1161156596115 39.95383950557092, -105.116334950052 39.95373994901936, -105.1163351483355 39.95373985961334, -105.1165168095012 39.95365738096457, -105.1165170078045 39.95365728795569, -105.1169139209715 39.95346982135294, -105.1169141533329 39.95346970684071, -105.1171975662708 39.95333055615466, -105.1171978373564 39.95333042285662, -105.1173067147139 39.95327695464484, -105.117306984649 39.95327681774006, -105.1176446054035 39.95310459353603, -105.1176950733087 39.95307884083901, -105.1176953784864 39.95307867973241, -105.1180788781805 39.95287553813031, -105.1180792150897 39.95287535280995, -105.1184580166002 39.95266710653517, -105.1184583840751 39.95266689609635, -105.1186783405708 39.952541095606, -105.1186787479589 39.95254086278207, -105.1188915068743 39.95241917390688, -105.1188919107704 39.95241893746794, -105.1205118309458 39.95147311368525, -105.1205122547498 39.95147287280292, -105.1208145917061 39.95129598108178, -105.1208145432466 39.9512958566309, -105.1205322612619 39.95056686151733, -105.1205159574603 39.95052896648702, -105.1205159176727 39.95052896635597, -105.1204972471613 39.95052883010491, -105.120148872229 39.95052627615362, -105.1186763655381 39.95051759418457, -105.1163054180666 39.95053456487648, -105.1154455703091 39.95054103085187, -105.1140142902583 39.95055178123432, -105.1116931313675 39.95057001988807, -105.1094369900144 39.95058967151289, -105.1094369786246 39.95058777647951, -105.1094363338094 39.95048410258741, -105.1094328410816 39.94991861852341, -105.1094328507301 39.94991672806453, -105.1094361068799 39.94924734204911, -105.1094360954028 39.94924546232647, -105.1094235269228 39.94715448261204, -105.1094235249433 39.9471544195589, -105.1094234744751 39.94715260545215, -105.1094187052575 39.94697912515855, -105.1094186985288 39.94697723374308, -105.1094099375368 39.9443619741967, -105.1094099306489 39.94436011070076, -105.1094093143913 39.94417601301638, -105.1094093074983 39.94417415042114, -105.1094088564013 39.94403971046976, -105.1094088495082 39.94403784787448, -105.1094065693434 39.94335667470221, -105.1094331579206 39.94335669819747, -105.1094342847429 39.94335669931566, -105.1099356478872 39.94335744415169, -105.1099367758796 39.94335744526892, -105.1100939092638 39.94335767276832, -105.1100950384264 39.94335767388797, -105.1113682413915 39.94335951176833, -105.1113693752345 39.94335951289126, -105.1115086222681 39.94335971324735, -105.1115097327091 39.94335971429, -105.1117277916897 39.94335836258531, -105.1117289010016 39.94335835641672, -105.1139797592105 39.94334428565912, -105.1139808884187 39.94334427863482, -105.1185561841228 39.94332791779106, -105.1185577375591 39.9432111717849, -105.1185786931275 39.94163553556272, -105.1185787173852 39.94163370729682, -105.1186017016353 39.93990465320577, -105.1186017200063 39.93990283122475, -105.1186032935058 39.93973953897395, -105.1186032568698 39.9397377195128, -105.1186017162192 39.93965976470523, -105.1186016797191 39.93965792092657, -105.1185971028635 39.93942645961974, -105.1185970663537 39.93942461764238, -105.1185948615821 39.93931056474968, -105.1185948788888 39.93930872385114, -105.1185957683928 39.93921277192599, -105.1185957855938 39.93921094994099, -105.1185965403389 39.93912927308293, -105.1185965575348 39.9391274519986, -105.1185988473492 39.93887951686656, -105.1185988645399 39.93887769668284, -105.1185991667161 39.93884455687426, -105.1185991792267 39.93884273667501, -105.1186179804826 39.93603959378159, -105.1186179894219 39.93603778437812, -105.1186184037774 39.93567568026551, -105.1186175723289 39.93567414007994, -105.1182587942474 39.93500805834684, -105.1182594976906 39.93500675201376, -105.1186732794773 39.93423877115278, -105.118673946249 39.93423753404684, -105.1187153808925 39.93415893428716, -105.1187155377534 39.93415766216859, -105.1187356803395 39.93399418722844, -105.1187358911118 39.93399247936708, -105.1187555828143 39.93382885792241, -105.1187554050253 39.93382717399349, -105.1187496800574 39.93377277206956, -105.1187426310094 39.93370658508118, -105.1187423547122 39.93370473330269, -105.1186310511322 39.93297192257087, -105.1186305278242 39.93297156507604, -105.1144418766246 39.9301116330937, -105.1144411075297 39.93011005976095, -105.1144409722058 39.93010978460534, -105.1142675329075 39.92975529512095, -105.1142666296578 39.9297534484365, -105.1140585185026 39.92932809442664, -105.1137262203602 39.92864847858181, -105.1137255080341 39.92864659560585, -105.1137050251862 39.92859566099454, -105.113704554754 39.92859527303179, -105.1134254430625 39.92836563900499, -105.1127892552828 39.92784224790676, -105.1118443320229 39.92708224169476, -105.1117548190385 39.92701045155007, -105.1109611901158 39.92646588786492, -105.110533010465 39.92620741090535, -105.1102888127801 39.92606301804486, -105.1097181218421 39.92570515554632, -105.1093983533093 39.92550463644266, -105.1093970325059 39.92591051920145, -105.1093963927524 39.92610719247062, -105.1093961314852 39.9261876173348, -105.1093961302332 39.92618804064294, -105.1108909641212 39.9270703063674, -105.1108928284495 39.92707140337049, -105.1109472591628 39.92710996005612, -105.1109489916877 39.92711119441476, -105.11100184127 39.92714905852634, -105.1110035830733 39.92715030732615, -105.1110555422339 39.92718882769187, -105.1110572395243 39.92719008714854, -105.1110572686417 39.92719010976344, -105.1111083231939 39.92722931245594, -105.1111100062535 39.92723060608901, -105.1111100307173 39.9272306241849, -105.111160165556 39.92727049114104, -105.1111618506854 39.92727183251554, -105.1112110529834 39.92731235648804, -105.111212659834 39.92731368048491, -105.1112127180535 39.92731372841661, -105.1112609750245 39.92735489495286, -105.1112626165257 39.92735629742379, -105.1113099106939 39.9273980938567, -105.1113115286313 39.92739952596935, -105.1113578471896 39.927441941449, -105.1113594310861 39.92744339416132, -105.1114047705602 39.92748642237255, -105.1114063367063 39.92748791105097, -105.1114505828162 39.92753148766221, -105.1114521207296 39.9275330041653, -105.1114952746698 39.92757712467863, -105.1114967564333 39.92757864099171, -105.1114967808562 39.92757866629268, -105.1115389009839 39.92762335432344, -105.1115403777728 39.9276249228577, -105.1115814571705 39.92767016037045, -105.1115828952545 39.92767174678695, -105.1116229245829 39.92771753014858, -105.1116243367531 39.92771914800042, -105.111663293943 39.92776544921718, -105.111664672062 39.92776708947031, -105.1117025524685 39.92781390222298, -105.1117038953714 39.92781556397286, -105.1117406873717 39.92786287471342, -105.1117419938938 39.92786455705546, -105.1117776870397 39.92791235133907, -105.1117789525426 39.92791404705239, -105.1118135410398 39.92796231495335, -105.1118147748001 39.92796403847989, -105.111848236553 39.92801275650742, -105.1118494304382 39.92801449791246, -105.1118817643469 39.92806365345461, -105.1118829195319 39.92806541184156, -105.1119141116025 39.92811499674616, -105.1119151561972 39.92811665928968, -105.1119152257527 39.92811677120648, -105.1119452737562 39.92816676565235, -105.1119463480464 39.92816855528933, -105.1119762689248 39.92822075322429, -105.1120049849938 39.9282733442855, -105.1120324811199 39.92832631491299, -105.1120587550635 39.92837964708677, -105.1120837940408 39.92843332545336, -105.1120967981585 39.92846279035226, -105.112107214614 39.92848647687905, -105.1121075772735 39.92848730040697, -105.1122038636647 39.92861595039223, -105.112204645089 39.92861698878723, -105.1122051443685 39.9286176515559, -105.1131118570121 39.93037915497996, -105.113233333253 39.93062041135646, -105.1132659917676 39.93068783125076, -105.1132844999339 39.93072888441935, -105.1133020484817 39.93077020005903, -105.1133186421806 39.93081176197423, -105.113334278771 39.93085355574722, -105.113348960637 39.93089557328036, -105.1133626703306 39.93093779650227, -105.1133754137557 39.93098021552567, -105.1133871804378 39.93102282040854, -105.1133979751567 39.93106559315386, -105.1134077827836 39.93110851930052, -105.113416610382 39.93115159076657, -105.1134244521873 39.93119479222157, -105.1134313012498 39.93123811103305, -105.113437162339 39.9312815310053, -105.113442030799 39.93132504761954, -105.1134459032609 39.93136863564597, -105.1134487762438 39.931412289669, -105.1134506592019 39.93145599260789, -105.1134515416603 39.9314997345202, -105.1134514272185 39.93154349920609, -105.113450314771 39.93158727495323, -105.1134482067322 39.93163104825973, -105.1134451020171 39.93167480381061, -105.1134409983348 39.93171853259142, -105.1134359028049 39.93176221661275, -105.113429811982 39.93180584415427, -105.1134227329501 39.9318494035309, -105.113414662279 39.93189288032042, -105.1134056070834 39.93193625743383, -105.1133955662373 39.93197952676115, -105.1133845491696 39.93202267572452, -105.1133725489611 39.9320656862871, -105.113359577355 39.93210855038208, -105.1133456344566 39.93215124909558, -105.1133307273246 39.93219377524553, -105.1133148583837 39.93223611352849, -105.1132980335634 39.93227824955331, -105.1132802564333 39.93232017252367, -105.1132615340774 39.93236187075425, -105.1132418736157 39.9324033262552, -105.1132212762678 39.9324445300235, -105.1131997491178 39.9324854703738, -105.1131773051049 39.93252613473981, -105.1131539431397 39.93256650870666, -105.1131296761662 39.93260657880734, -105.1131045065741 39.93264633604267, -105.113078446138 39.93268576694161, -105.1130514984277 39.93272486070767, -105.113023677573 39.93276360117568, -105.1129949918083 39.93280198026674, -105.1129654411784 39.93283998987437, -105.112935043359 39.93287760754068, -105.1129038065386 39.93291483329256, -105.1128717343385 39.93295164732695, -105.1128388431675 39.93298804429421, -105.1128051389664 39.93302400800174, -105.1127706323048 39.93305953127903, -105.1127353419725 39.93309460157923, -105.112699266845 39.93312921079185, -105.1126624222279 39.93316334185509, -105.1126248198305 39.93319699300623, -105.1125864726237 39.93323014627482, -105.1125473923425 39.93326279539504, -105.1125075872323 39.93329493048649, -105.1124670725634 39.93332654079186, -105.1124258612613 39.93335761644661, -105.1123839627366 39.93338814847505, -105.1123413922496 39.93341812792112, -105.112298162726 39.93344754492023, -105.1122542835765 39.93347639049676, -105.1122097787322 39.93350518891695, -105.1108825455564 39.93434273300105, -105.1097777212305 39.93505856392756, -105.1092370249853 39.93540888430044, -105.109236684834 39.93553881744052, -105.109237555661 39.93614271109521, -105.1092309617087 39.93614452157765, -105.1091476096643 39.93614433425925, -105.109037945844 39.93614408640219, -105.1086808361625 39.93614327640896, -105.1081492163309 39.93614206184396, -105.1046341365572 39.93611220688962, -105.099991742204 39.93605491013817, -105.0951422560202 39.93606933899665, -105.0950355885139 39.93607365200723, -105.09476502367 39.93607269419247, -105.0945908398346 39.93607115000719, -105.0944119399563 39.93606956913881, -105.0942317090223 39.936068511994, -105.0941950319923 39.93606829722803, -105.0940532611034 39.93606746625473, -105.0938741497766 39.9360664242047, -105.0936100881903 39.93606736899439, -105.0933812509434 39.93606530861484, -105.0924035059316 39.93606276275314, -105.0918615391184 39.93606134993986, -105.0910157459438 39.93605931468678, -105.0908557345987 39.93605890767786, -105.0908493310474 39.93733416590344, -105.090845184441 39.93815985715184, -105.0908424959132 39.93869504775551, -105.0909012831155 39.93869845210159, -105.0909023057667 39.93869844672675, -105.0909009129949 39.93899798932196, -105.0908992109706 39.93920895855562, -105.0908988896852 39.93924889918723, -105.0909386654367 39.93925538111568, -105.0909388888204 39.93925539722021, -105.0909399203652 39.93925547113504, -105.0909447678353 39.94006555055373, -105.0909032136222 39.94006601094053, -105.0909043710449 39.94131892761472, -105.0909044712291 39.9414271563125, -105.0910619178891 39.94143530162019, -105.0910619951027 39.94143530369561, -105.0910630538564 39.94143533357321, -105.0910588121924 39.94240422444584, -105.0910515015407 39.94328985775073, -105.0908401727396 39.94329100598443, -105.0906429394402 39.94329094929207, -105.0905381523252 39.94329137849177, -105.0905070988288 39.94329150589123, -105.089837629017 39.94329425448934, -105.0860388355787 39.94332055103774, -105.0821871148648 39.94335411398962, -105.0812630425988 39.9433621325146, -105.0767360412157 39.94334022196765, -105.076617719676 39.94333941431218, -105.0766014550372 39.94499877740917, -105.0765867743723 39.9464964353545, -105.076573762168 39.94765414067553, -105.0765585879308 39.94919947316338, -105.076548242864 39.95054710934591, -105.076103921084 39.95054268882134, -105.0753572740584 39.95053202794011, -105.0745735205932 39.95052068211166, -105.074243983681 39.95048048858849, -105.0720227034047 39.95021855966071, -105.0718823803634 39.9502020119051, -105.071880156866 39.95049172946248, -105.0718814336875 39.95058499173008, -105.0719811965841 39.95763613716662, -105.0719822955386 39.95771376408718, -105.0719823361877 39.95771661303881, -105.0742030621761 39.95772626543882, -105.07420410847 39.95772626840448, -105.0753793466463 39.95772928122915, -105.0753803964513 39.95772928419706, -105.0765556299548 39.95773230031829, -105.0765567090186 39.95773230338303, -105.0796267977524 39.9577626764316, -105.0796278873055 39.95776268671114, -105.079707513408 39.95776347343922, -105.0797086205163 39.95776348378201, -105.0811915867279 39.95778588334476, -105.0811926774133 39.95778589991825, -105.0827430961593 39.95779841380289, -105.0827441915763 39.95779842227282, -105.0830905532878 39.95780121430522, -105.0830916557268 39.9578012227973, -105.0830912914456 39.9578828783425, -105.0830914379236 39.95791388241516, -105.0830917470141 39.95796309669239, -105.0830905175779 39.95814383200661, -105.0830896020937 39.9582756696281, -105.083089599058 39.95827597494203, -105.0831265976219 39.95829352042862, -105.0831284436178 39.95829423682988, -105.0831677422527 39.95830886707035, -105.0831695767604 39.9583095483035, -105.0832092320398 39.95832365923636, -105.0832110480427 39.95832430437537, -105.0832510541473 39.95833789057515, -105.0832528481451 39.9583384978061, -105.0832931933815 39.95835155742886, -105.0832949770394 39.95835213309849, -105.083335634549 39.95836465613951, -105.0833374008502 39.95836519932185, -105.0833783706378 39.95837718488006, -105.0833801172471 39.95837769466598, -105.0834213876632 39.95838913369234, -105.0834230736785 39.95838960002673, -105.0834231134047 39.95838961097829, -105.0834646692338 39.95840050341751, -105.0834663110015 39.95840093266411, -105.0834663694259 39.95840094818657, -105.0835082013262 39.95841129040186, -105.0835097976648 39.95841168435775, -105.0835098782986 39.95841170446378, -105.0835519734337 39.95842149010389, -105.0835535208322 39.95842184875641, -105.0835536225104 39.95842187254114, -105.0835959715385 39.95843109796932, -105.083597505047 39.95843143135245, -105.0835975938788 39.95843145058738, -105.0836401827601 39.95844011485198, -105.0836417643307 39.95844043579893, -105.0836845965917 39.95844853621046, -105.0836861011444 39.95844881995132, -105.0836861584315 39.9584488300656, -105.0837291908175 39.95845635836152, -105.0837307130412 39.95845662325169, -105.0837739607767 39.95846357768551, -105.0837754562364 39.95846381725983, -105.0838188865613 39.95847019591163, -105.083820295618 39.9584704018488, -105.0838203494051 39.95847041014899, -105.083837605523 39.958472716926, -105.0838390743395 39.95847291137007, -105.0838639576698 39.95847620759785, -105.0838653855513 39.95847639739046, -105.0839091600622 39.95848161179256, -105.0839105506463 39.95848177623136, -105.0839544773578 39.95848640753589, -105.0839557534282 39.95848654183878, -105.0839558329632 39.95848655023193, -105.0839998978684 39.95849059208348, -105.0840011529878 39.95849070739629, -105.0840012149839 39.9584907130241, -105.0840454063616 39.95849416808221, -105.084046681476 39.95849426725479, -105.0840909911929 39.95849712558269, -105.0840921470791 39.95849720000647, -105.0840922289767 39.9584972048054, -105.0841366382675 39.95849947263985, -105.0841378188191 39.95849953274163, -105.0841823300452 39.95850120648842, -105.0841834837884 39.95850124847972, -105.084228056008 39.95850232438844, -105.0842290811161 39.95850234880245, -105.0842291677117 39.95850235091626, -105.0842738021159 39.95850282538841, -105.0842748694392 39.95850283644447, -105.0842768016851 39.9585028461176, -105.0843195519606 39.95850271303195, -105.0843205760685 39.95850270952104, -105.0843652950352 39.95850198277773, -105.0843662724055 39.95850196648848, -105.0844110125797 39.95850063996208, -105.084411946718 39.95850061180795, -105.0844566952575 39.95849868004812, -105.0844575826417 39.95849864181768, -105.0845023278417 39.95849610478225, -105.0845031673014 39.95849605647136, -105.0845478892426 39.95849291769114, -105.0845486842725 39.95849286201446, -105.0845933771403 39.95848911516397, -105.0845941253996 39.95848905211304, -105.0846387715935 39.95848470433415, -105.0846394730714 39.95848463571034, -105.0846840621009 39.95847967976002, -105.0846847144455 39.95847960735617, -105.084702105477 39.95847744359641, -105.0847027555357 39.95847736217756, -105.0847292287157 39.95847404947573, -105.0847298330974 39.95847397329614, -105.0847742609255 39.95846780984096, -105.0847748173279 39.95846773258756, -105.0848191434705 39.95846096800619, -105.0848196530585 39.9584608905839, -105.084863865833 39.95845352123168, -105.08486432509 39.95845344452852, -105.0849084092641 39.95844547305273, -105.0849088216957 39.95844539798203, -105.0849527690538 39.95843682795595, -105.0849531323029 39.95843675721125, -105.0849969218048 39.95842758405593, -105.0849972405584 39.95842751675351, -105.0850408592745 39.95841774942916, -105.0850411288291 39.95841768915476, -105.0850845674009 39.95840732672732, -105.0850847889214 39.95840727438583, -105.0851280286276 39.95839631588745, -105.0851282032845 39.95839627148312, -105.0851712382503 39.95838472049549, -105.0851713683735 39.95838468583803, -105.0851743486054 39.95838384363866, -105.0851744799152 39.95838380628351, -105.0852141728226 39.95837254677202, -105.0852142572362 39.95837252275794, -105.0852568276513 39.95835979650178, -105.0852568616573 39.95835978581623, -105.0853101451451 39.95834291902096, -105.0853102002613 39.95834290120607, -105.0858421626544 39.95817871226845, -105.0858422212814 39.95817869446593, -105.085944214198 39.95814721264614, -105.085944272825 39.95814719484354, -105.0864089196698 39.95800377927178, -105.0864090392693 39.95800374277388, -105.0876435368176 39.95801568769421, -105.087644656805 39.95801569800683, -105.0879119632444 39.95801828447654, -105.0879130844023 39.95801829479073, -105.0879358702931 39.9580185149788, -105.0879369926213 39.95801852529694, -105.0880433829552 39.95801955328184, -105.0880445006021 39.9580195635822, -105.0880454746665 39.95803347060461, -105.0881558248172 39.95803753346706, -105.088156924958 39.9580375355978, -105.0886128489525 39.9580386337409, -105.0886129648172 39.95803863415455, -105.0886136635223 39.95803863574837, -105.0886139490879 39.95803863676791, -105.0886669710434 39.95803876480815, -105.088667006154 39.95803876493348, -105.0886681074652 39.95803876706348, -105.0886676791558 39.95810768699305, -105.0886662517168 39.95824081254283, -105.0886640890448 39.95844581560196, -105.088625575105 39.95844758571651, -105.0881544918518 39.95844611011514, -105.088040376847 39.95844732158841, -105.0880382211008 39.95885810821171, -105.0880380735751 39.95888622819314, -105.0880333812514 39.95978094919757, -105.0879262449088 39.95978400035138, -105.08747407241 39.95978207714827, -105.0874111940689 39.96005124220132, -105.0872096218029 39.96007571814968, -105.0871191644284 39.96008593633609, -105.0870446975825 39.96009434918611, -105.0863498292124 39.96017287246411, -105.0859393187197 39.96023012947124, -105.08581766119 39.96024710027866, -105.0857839598441 39.9602517994901, -105.0854661723567 39.96029612401237, -105.0850658527888 39.96035196090204, -105.0850096380202 39.96035979868915, -105.0847427531886 39.96039702446389, -105.0847392436433 39.96039751348618, -105.0847357340925 39.96039800340896, -105.0847322268825 39.96039849334009, -105.0847287173152 39.96039898596462, -105.0847252042421 39.96039947767574, -105.0847217017135 39.96039996762343, -105.084718187448 39.96040046293266, -105.0847146790509 39.96040095556098, -105.0847111706537 39.96040144818916, -105.0847076657566 39.96040194263121, -105.0847041550022 39.96040243795269, -105.0847006442421 39.96040293417474, -105.0846971358338 39.96040342860376, -105.0846936321015 39.96040392395023, -105.0846901236711 39.96040442198164, -105.0846866093832 39.96040492089254, -105.0846831091674 39.96040541535069, -105.0846795960389 39.96040591606685, -105.0846760887787 39.96040641410207, -105.0846725838647 39.96040691124497, -105.0846690754121 39.9604074128783, -105.0846655681353 39.96040791361514, -105.0846620596881 39.96040841434764, -105.084658553587 39.96040891418785, -105.0846550486509 39.96040941493276, -105.0846515390111 39.96040991926331, -105.0846480352453 39.96041042001222, -105.0846445279518 39.96041092345035, -105.0846410230044 39.96041142599616, -105.0846375180461 39.96041193034313, -105.0846340072247 39.9604124364702, -105.0846305022718 39.9604129399163, -105.0846269961319 39.96041344606006, -105.0846234911624 39.96041395220792, -105.0846199861873 39.96041445925627, -105.0846164765197 39.96041496808895, -105.0846129774075 39.96041547335694, -105.0846094677397 39.96041598218939, -105.0846059651107 39.96041648834515, -105.0846024612894 39.96041699809916, -105.0845989527754 39.96041750963744, -105.0845954524706 39.96041801850324, -105.0845919427861 39.96041853003707, -105.0845884389701 39.96041903889005, -105.0845849386486 39.96041955045742, -105.0845814336346 39.96042006380912, -105.0845779274502 39.96042057715649, -105.0845744247878 39.96042108871516, -105.0845709185977 39.96042160296298, -105.0845674159353 39.96042211452143, -105.0845639132453 39.96042263058297, -105.0845604058738 39.96042314662753, -105.0845569031947 39.96042366088757, -105.0845534028563 39.96042417515598, -105.0845498989903 39.9604246921135, -105.0845463951242 39.96042520907093, -105.0845428912471 39.96042572782954, -105.0845393908921 39.96042624479943, -105.084535885839 39.96042676445424, -105.084532385484 39.96042728142393, -105.0845288827715 39.96042780108701, -105.0845253812295 39.96042832075415, -105.084521877341 39.96042884131344, -105.0845183769638 39.96042936188523, -105.0845148742347 39.9604298842498, -105.0845113679944 39.96043040660159, -105.0845078687929 39.96043092627666, -105.0845043707397 39.96043144955845, -105.0845008668181 39.96043197552092, -105.0844973664296 39.9604324978934, -105.084493861343 39.9604330229508, -105.08449036446 39.96043354623639, -105.0844868605436 39.96043407129777, -105.0844833613033 39.96043459727665, -105.0844798585408 39.96043512504401, -105.0844763604763 39.96043565012621, -105.0844728588786 39.96043617879819, -105.0844693537751 39.9604367065568, -105.0844658615568 39.96043723256042, -105.0844623576018 39.9604377639256, -105.0844588583501 39.96043829170497, -105.0844553579115 39.96043882218198, -105.0844518598192 39.96043935176664, -105.0844483605509 39.96043988224761, -105.0844448577714 39.96044041271587, -105.0844413596679 39.96044094410149, -105.0844378592126 39.96044147727986, -105.0844343622794 39.96044200866955, -105.0844308618186 39.96044254274836, -105.0844273637038 39.96044307593485, -105.0844238655837 39.96044361002188, -105.0844203651116 39.96044414590168, -105.0844168669913 39.96044467998852, -105.08441336886 39.96044521587651, -105.084409871899 39.96044575176866, -105.0844063749324 39.9604462885613, -105.0844028744492 39.96044682624184, -105.084399377488 39.96044736213367, -105.0843958758232 39.96044790161103, -105.0843923823731 39.96044843751532, -105.0843888830491 39.96044897700094, -105.0843853907528 39.96044951561112, -105.0843818890714 39.96045005779001, -105.0843783956046 39.96045059639577, -105.0843748950935 39.9604511385787, -105.0843714004397 39.96045167988194, -105.0843679010934 39.9604522229695, -105.0843644052637 39.96045276516899, -105.0843609117802 39.96045330647613, -105.0843574100874 39.9604538504556, -105.0843539166038 39.96045439176255, -105.0843504219278 39.96045493666776, -105.0843469248999 39.9604554833657, -105.0843434325701 39.96045602737846, -105.0843399355421 39.9604565740762, -105.084336433827 39.96045712165759, -105.084332941497 39.96045766567005, -105.0843294456338 39.9604582132723, -105.084325955617 39.96045876179622, -105.0843224562315 39.96045931118692, -105.0843189638848 39.96045985790089, -105.0843154691753 39.9604604082089, -105.084311972114 39.96046096030963, -105.0843084762395 39.96046150971257, -105.0843049838761 39.96046205912804, -105.0843014903368 39.96046260943984, -105.0842979956051 39.9604631633499, -105.0842944985435 39.96046371545011, -105.084291009691 39.96046426487781, -105.0842875137723 39.96046482148525, -105.0842840190458 39.96046537449425, -105.0842805290064 39.96046592661936, -105.0842770330929 39.96046648232583, -105.0842735418555 39.96046703894973, -105.0842700471124 39.96046759466021, -105.084266553545 39.96046814947415, -105.0842630623074 39.96046870609777, -105.0842595687235 39.96046926361346, -105.0842560774913 39.96046981933619, -105.0842525827315 39.96047037774804, -105.0842490903123 39.96047093616829, -105.0842456002338 39.96047149459685, -105.0842421054573 39.96047205571033, -105.0842386165491 39.96047261414292, -105.0842351229429 39.96047317526042, -105.0842316316773 39.96047373638628, -105.0842281427526 39.96047429752046, -105.0842246467834 39.96047486223177, -105.0842211601992 39.96047542337421, -105.0842176677466 39.96047598719733, -105.0842141752939 39.96047655102036, -105.0842106840116 39.96047711484754, -105.0842071938996 39.96047767867879, -105.0842037049579 39.96047824251414, -105.084200213659 39.9604788090429, -105.08419672354</t>
+          <t>MULTIPOLYGON (((-105.05282818356312 39.98653346176652, -105.05758064247598 39.98649541493525, -105.06235000009765 39.98645786501839, -105.06346065373788 39.98647581498217, -105.06349099492526 39.98647646216797, -105.06703383845469 39.986535759576775, -105.06703719333667 39.98633703838531, -105.06703831690874 39.98633729479067, -105.06704005788771 39.98623419443279, -105.06709358887338 39.98306391759739, -105.07047475212875 39.9830759158628, -105.07096608163656 39.98308237411967, -105.07171460231034 39.9830922080333, -105.0717552482085 39.983092742726434, -105.07181170484914 39.98309269216385, -105.07181606755924 39.98243292109945, -105.07183288783676 39.98140187753952, -105.07185011689448 39.98058990350253, -105.0718568404095 39.98014410421328, -105.07186687653018 39.9794736037379, -105.07192560170961 39.97947406682838, -105.07261530526698 39.979486387585006, -105.07320853403718 39.97949698163314, -105.07377040313808 39.9795008692249, -105.07407215207915 39.9795029564586, -105.07439406041776 39.979505180387264, -105.07577169398292 39.97952383912966, -105.07619083603376 39.97952951234009, -105.07929446044902 39.97957148382346, -105.0834853211123 39.979623775070074, -105.08350857166586 39.97962404552135, -105.09032708778417 39.9797032929451, -105.09048605711386 39.979702819376726, -105.09048603090432 39.979706210274216, -105.09069094427178 39.97970782075467, -105.0952100830245 39.97971518827352, -105.09519162953886 39.97607892625242, -105.09057003187004 39.976079984602464, -105.09045426937853 39.97608297782843, -105.09044174254427 39.97584710582651, -105.09041932538481 39.975638815666585, -105.09036899200183 39.97550995382825, -105.09029142613885 39.975273760560704, -105.09024188761072 39.975012645590475, -105.090192863608 39.97466574347093, -105.09020081638 39.97411529796517, -105.090215942638 39.97240347779733, -105.09030307826939 39.972404006437486, -105.09096395076844 39.97239290149737, -105.09116482551741 39.9723941636361, -105.0912461536423 39.97239802052451, -105.0913521083569 39.97240086766923, -105.09142202952599 39.97240303667677, -105.09364307856468 39.97241500683583, -105.09430816620187 39.97241487935375, -105.09464500267062 39.97241304460964, -105.0950421100944 39.97241608789733, -105.09533279321772 39.97241727370804, -105.09534376988462 39.972417317651875, -105.09534426658375 39.972524625152204, -105.09534539337994 39.97327727257912, -105.09594858415254 39.973275293473215, -105.09594851457278 39.97252466095966, -105.09594940271718 39.97241976308735, -105.09595852984498 39.97241979958787, -105.09686713387642 39.972423035329385, -105.0974380772597 39.97241405009566, -105.09756400930208 39.972412065307346, -105.09756547919547 39.97243912451826, -105.09756822021363 39.97252892556443, -105.09755565305896 39.97609100741533, -105.10456011546347 39.97610235688621, -105.10456826205139 39.97377105019996, -105.1054698415779 39.97377082908722, -105.105473750072 39.97254757141797, -105.10547281387781 39.97241715154041, -105.10628114231736 39.97241796939557, -105.1084309638869 39.97240690009586, -105.10926515911866 39.97241000593239, -105.10923192715646 39.97335287654287, -105.10922317496588 39.97382200756769, -105.10927516384749 39.972416442651124, -105.10937416227326 39.959696440642915, -105.10938216269992 39.95928944047934, -105.10790216146646 39.959314440239176, -105.1078871611286 39.95851244033037, -105.10814816157236 39.95847244081943, -105.10815916215097 39.95790844019832, -105.10816058049275 39.95790194404009, -105.10932699889575 39.95789799857891, -105.1093269891051 39.95789786885034, -105.11459616333309 39.95785343948453, -105.11459616106403 39.95785363401997, -105.11456916347859 39.96033344011676, -105.1152741627195 39.960329440075235, -105.11528516304983 39.95784852040962, -105.11528516350681 39.95784843935154, -105.1153011708886 39.95784840182763, -105.12806316659325 39.95781743936814, -105.12795112667123 39.9541802399316, -105.12759699389478 39.95418130612799, -105.12391799539202 39.95417275040911, -105.12291594741103 39.9541704003749, -105.12214125343137 39.95416857667849, -105.12192821615547 39.95416609003437, -105.12192746123134 39.954164202471475, -105.12192742198542 39.9541641041705, -105.12185961475706 39.95399464274431, -105.12185959282607 39.95399458773195, -105.12185884285634 39.953992651549086, -105.1212409789274 39.952397110239254, -105.12124021168391 39.95239512986274, -105.12114255241967 39.95214293317645, -105.12083446220286 39.952318493656925, -105.12029155925786 39.95263547808772, -105.11953824504275 39.953075312822776, -105.11914930472986 39.953298316199536, -105.11875534370003 39.95351607060863, -105.11871418471706 39.953537999739396, -105.11867848153149 39.953557015255704, -105.11861872380682 39.95358884322316, -105.11835650519312 39.95372850081748, -105.11795290548802 39.95393554051217, -105.1175446702312 39.95413712341077, -105.11713192268822 39.95433319133069, -105.11681834361968 39.954476393595385, -105.11671478614501 39.9545236833886, -105.11633332932739 39.95469102504197, -105.11631336128096 39.95469978414111, -105.11629339322947 39.95470854323679, -105.11596203316375 39.95484806240092, -105.11586786606709 39.954887709990736, -105.11543834193118 39.955061135426966, -105.11500494761273 39.95522876318281, -105.11456776882949 39.95539055747477, -105.11412703084486 39.955546434351845, -105.11400824239063 39.955586531161906, -105.11368281932975 39.95569636794119, -105.1133266682007 39.95581051213452, -105.11317002197465 39.95586071435858, -105.11269298476161 39.95600929462459, -105.11165363376176 39.9563330070136, -105.10968583349619 39.956943945065376, -105.10968583391507 39.95694203025841, -105.10968583416233 39.956941987027484, -105.10968583483108 39.95694166549327, -105.10968588349614 39.95675247881106, -105.10968588336033 39.95675209332704, -105.10968588494437 39.956750179424716, -105.10968594889121 39.956502050737754, -105.10968594929469 39.95650013863272, -105.10968606425932 39.95606241165259, -105.10968606564536 39.956057872318304, -105.10979533953609 39.956023840715865, -105.1116617064129 39.95544256909836, -105.11166185296281 39.95544252365849, -105.11177678876732 39.95540672865434, -105.11177693414672 39.95540668321035, -105.11276872746079 39.95509777442294, -105.11276885407825 39.95509773521934, -105.11319909147424 39.95496035760923, -105.11319917588894 39.954960330872744, -105.11335104674485 39.95490942808447, -105.11335113233997 39.954909399550466, -105.11362631723951 39.95481716172755, -105.11362635828154 39.95481714745462, -105.11401293391395 39.95468134876749, -105.11401297612609 39.9546813344983, -105.11405022994758 39.95466824747247, -105.11447078380596 39.95451362643593, -105.11488763861115 39.95435342811378, -105.11488767966276 39.95435341203906, -105.11530079195144 39.95418765163744, -105.11530087406443 39.95418761768639, -105.11571012289888 39.95401635248451, -105.11571024373734 39.95401629974841, -105.11598254923587 39.95389755732932, -105.11598270996484 39.95389748671265, -105.11611550121827 39.95383957709619, -105.1161156596115 39.95383950557092, -105.11633495005195 39.95373994901936, -105.11633514833547 39.953739859613336, -105.11651680950125 39.95365738096457, -105.11651700780448 39.95365728795569, -105.1169139209715 39.95346982135294, -105.11691415333294 39.953469706840714, -105.11719756627078 39.95333055615466, -105.1171978373564 39.953330422856624, -105.11730671471388 39.95327695464484, -105.11730698464898 39.95327681774006, -105.11764460540348 39.953104593536025, -105.11769507330867 39.95307884083901, -105.11769537848645 39.953078679732414, -105.11807887818048 39.95287553813031, -105.1180792150897 39.95287535280995, -105.11845801660016 39.95266710653517, -105.11845838407508 39.95266689609635, -105.11867834057075 39.952541095606, -105.11867874795891 39.952540862782065, -105.11889150687433 39.95241917390688, -105.11889191077039 39.95241893746794, -105.12051183094582 39.951473113685246, -105.12051225474977 39.95147287280292, -105.12081459170605 39.95129598108178, -105.12081454324664 39.9512958566309, -105.12053226126186 39.95056686151733, -105.12051595746031 39.95052896648702, -105.12051591767269 39.95052896635597, -105.12049724716132 39.95052883010491, -105.12014887222897 39.95052627615362, -105.11867636553808 39.950517594184575, -105.11630541806657 39.95053456487648, -105.11544557030915 39.95054103085187, -105.11401429025831 39.950551781234324, -105.11169313136747 39.95057001988807, -105.10943699001442 39.950589671512894, -105.10943697862461 39.95058777647951, -105.10943633380936 39.95048410258741, -105.10943284108157 39.94991861852341, -105.10943285073009 39.94991672806453, -105.1094361068799 39.949247342049105, -105.10943609540278 39.949245462326466, -105.10942352692282 39.947154482612035, -105.10942352494331 39.9471544195589, -105.10942347447511 39.94715260545215, -105.10941870525751 39.94697912515855, -105.10941869852884 39.94697723374308, -105.10940993753678 39.944361974196696, -105.10940993064888 39.944360110700764, -105.10940931439131 39.94417601301638, -105.1094093074983 39.94417415042114, -105.10940885640127 39.94403971046976, -105.10940884950823 39.94403784787448, -105.10940656934343 39.94335667470221, -105.10943315792059 39.94335669819747, -105.10943428474289 39.94335669931566, -105.10993564788716 39.94335744415169, -105.1099367758796 39.943357445268916, -105.11009390926382 39.94335767276832, -105.11009503842642 39.943357673887974, -105.11136824139152 39.94335951176833, -105.1113693752345 39.94335951289126, -105.11150862226808 39.943359713247354, -105.11150973270905 39.943359714290004, -105.11172779168966 39.943358362585315, -105.11172890100157 39.943358356416724, -105.11397975921047 39.94334428565912, -105.11398088841871 39.94334427863482, -105.11855618412275 39.94332791779106, -105.11855773755909 39.943211171784895, -105.11857869312752 39.941635535562725, -105.11857871738516 39.941633707296816, -105.11860170163527 39.939904653205765, -105.11860172000627 39.93990283122475, -105.11860329350581 39.93973953897395, -105.11860325686982 39.9397377195128, -105.11860171621919 39.939659764705226, -105.11860167971913 39.93965792092657, -105.11859710286353 39.93942645961974, -105.11859706635366 39.93942461764238, -105.11859486158205 39.93931056474968, -105.11859487888876 39.93930872385114, -105.11859576839282 39.93921277192599, -105.11859578559378 39.93921094994099, -105.11859654033891 39.939129273082926, -105.1185965575348 39.9391274519986, -105.11859884734919 39.93887951686656, -105.11859886453993 39.93887769668284, -105.11859916671611 39.93884455687426, -105.11859917922668 39.93884273667501, -105.11861798048264 39.936039593781594, -105.11861798942189 39.936037784378115, -105.11861840377736 39.93567568026551, -105.11861757232887 39.93567414007994, -105.1182587942474 39.93500805834684, -105.11825949769062 39.93500675201376, -105.11867327947735 39.93423877115278, -105.11867394624905 39.934237534046844, -105.11871538089252 39.93415893428716, -105.11871553775345 39.93415766216859, -105.11873568033954 39.93399418722844, -105.1187358911118 39.93399247936708, -105.11875558281426 39.93382885792241, -105.1187554050253 39.933827173993485, -105.1187496800574 39.93377277206956, -105.11874263100938 39.933706585081175, -105.11874235471217 39.93370473330269, -105.1186310511322 39.93297192257087, -105.11863052782422 39.93297156507604, -105.11444187662464 39.9301116330937, -105.11444110752966 39.93011005976095, -105.11444097220584 39.93010978460534, -105.1142675329075 39.92975529512095, -105.11426662965783 39.9297534484365, -105.11405851850257 39.92932809442664, -105.11372622036018 39.928648478581806, -105.1137255080341 39.92864659560585, -105.11370502518622 39.92859566099454, -105.113704554754 39.92859527303179, -105.11342544306254 39.928365639004994, -105.11278925528282 39.92784224790676, -105.11184433202287 39.92708224169476, -105.11175481903848 39.92701045155007, -105.11096119011577 39.92646588786492, -105.11053301046505 39.92620741090535, -105.11028881278011 39.926063018044864, -105.10971812184209 39.92570515554632, -105.10939835330933 39.92550463644266, -105.10939703250588 39.92591051920145, -105.10939639275243 39.926107192470624, -105.10939613148517 39.926187617334804, -105.10939613023315 39.92618804064294, -105.11089096412121 39.9270703063674, -105.1108928284495 39.92707140337049, -105.1109472591628 39.92710996005612, -105.11094899168774 39.92711119441476, -105.11100184126995 39.92714905852634, -105.11100358307333 39.92715030732615, -105.11105554223388 39.92718882769187, -105.11105723952434 39.92719008714854, -105.11105726864167 39.927190109763444, -105.1111083231939 39.92722931245594, -105.11111000625351 39.92723060608901, -105.11111003071726 39.9272306241849, -105.11116016555597 39.927270491141044, -105.11116185068539 39.92727183251554, -105.11121105298342 39.927312356488045, -105.11121265983401 39.927313680484914, -105.11121271805345 39.92731372841661, -105.11126097502452 39.927354894952856, -105.11126261652569 39.92735629742379, -105.11130991069386 39.9273980938567, -105.11131152863133 39.92739952596935, -105.11135784718955 39.927441941449, -105.11135943108611 39.92744339416132, -105.11140477056018 39.927486422372546, -105.11140633670627 39.92748791105097, -105.11145058281625 39.927531487662215, -105.11145212072955 39.927533004165305, -105.11149527466982 39.92757712467863, -105.11149675643327 39.92757864099171, -105.11149678085623 39.92757866629268, -105.11153890098393 39.92762335432344, -105.11154037777284 39.9276249228577, -105.11158145717052 39.92767016037045, -105.11158289525449 39.92767174678695, -105.11162292458286 39.92771753014858, -105.11162433675311 39.92771914800042, -105.11166329394297 39.927765449217176, -105.11166467206196 39.927767089470315, -105.1117025524685 39.92781390222298, -105.11170389537139 39.927815563972864, -105.1117406873717 39.92786287471342, -105.11174199389379 39.927864557055464, -105.11177768703973 39.927912351339074, -105.11177895254258 39.92791404705239, -105.11181354103977 39.92796231495335, -105.11181477480007 39.927964038479885, -105.111848236553 39.92801275650742, -105.11184943043821 39.92801449791246, -105.1118817643469 39.928063653454615, -105.1118829195319 39.92806541184156, -105.1119141116025 39.92811499674616, -105.11191515619717 39.92811665928968, -105.11191522575268 39.92811677120648, -105.11194527375616 39.92816676565235, -105.11194634804639 39.92816855528933, -105.11197626892476 39.928220753224295, -105.11200498499379 39.9282733442855, -105.11203248111991 39.928326314912994, -105.11205875506353 39.92837964708677, -105.11208379404083 39.92843332545336, -105.1120967981585 39.928462790352256, -105.11210721461401 39.92848647687905, -105.1121075772735 39.92848730040697, -105.11220386366466 39.928615950392235, -105.112204645089 39.92861698878723, -105.11220514436852 39.928617651555896, -105.11311185701206 39.93037915497996, -105.11323333325305 39.93062041135646, -105.11326599176763 39.930687831250765, -105.11328449993394 39.930728884419345, -105.11330204848167 39.93077020005903, -105.11331864218059 39.93081176197423, -105.11333427877096 39.93085355574722, -105.11334896063697 39.93089557328036, -105.11336267033056 39.93093779650227, -105.1133754137557 39.93098021552567, -105.11338718043777 39.931022820408536, -105.11339797515667 39.93106559315386, -105.11340778278355 39.93110851930052, -105.11341661038198 39.93115159076657, -105.11342445218732 39.93119479222157, -105.11343130124985 39.931238111033046, -105.11343716233904 39.931281531005304, -105.11344203079899 39.93132504761954, -105.1134459032609 39.931368635645974, -105.11344877624384 39.931412289669, -105.11345065920192 39.93145599260789, -105.11345154166025 39.9314997345202, -105.11345142721848 39.931543499206086, -105.113450314771 39.93158727495323, -105.11344820673222 39.93163104825973, -105.11344510201705 39.93167480381061, -105.11344099833475 39.93171853259142, -105.11343590280485 39.93176221661275, -105.11342981198197 39.93180584415427, -105.11342273295006 39.9318494035309, -105.11341466227896 39.93189288032042, -105.11340560708335 39.931936257433826, -105.11339556623729 39.93197952676115, -105.11338454916958 39.93202267572452, -105.11337254896111 39.9320656862871, -105.11335957735497 39.93210855038208, -105.1133456344566 39.932151249095575, -105.11333072732457 39.93219377524553, -105.11331485838367 39.93223611352849, -105.11329803356344 39.93227824955331, -105.11328025643331 39.932320172523674, -105.11326153407741 39.93236187075425, -105.11324187361573 39.932403326255205, -105.11322127626775 39.9324445300235, -105.1131997491178 39.9324854703738, -105.11317730510494 39.93252613473981, -105.11315394313968 39.932566508706664, -105.11312967616615 39.932606578807345, -105.1131045065741 39.932646336042666, -105.11307844613805 39.93268576694161, -105.11305149842772 39.932724860707665, -105.11302367757303 39.93276360117568, -105.11299499180829 39.93280198026674, -105.11296544117845 39.932839989874374, -105.11293504335902 39.932877607540675, -105.11290380653861 39.932914833292564, -105.11287173433848 39.932951647326945, -105.11283884316747 39.93298804429421, -105.11280513896635 39.933024008001745, -105.11277063230482 39.93305953127903, -105.11273534197245 39.933094601579235, -105.11269926684498 39.933129210791854, -105.11266242222794 39.933163341855085, -105.11262481983047 39.93319699300623, -105.11258647262373 39.93323014627482, -105.11254739234246 39.933262795395045, -105.11250758723226 39.93329493048649, -105.1124670725634 39.93332654079186, -105.11242586126134 39.933357616446614, -105.11238396273663 39.933388148475046, -105.11234139224962 39.93341812792112, -105.11229816272599 39.93344754492023, -105.1122542835765 39.933476390496764, -105.11220977873216 39.933505188916946, -105.11088254555642 39.934342733001046, -105.10977772123046 39.935058563927555, -105.10923702498535 39.93540888430044, -105.10923668483399 39.93553881744052, -105.10923755566098 39.936142711095215, -105.10923096170869 39.936144521577646, -105.1091476096643 39.936144334259254, -105.10903794584395 39.93614408640219, -105.10868083616255 39.936143276408956, -105.10814921633094 39.93614206184396, -105.10463413655724 39.93611220688962, -105.09999174220404 39.936054910138175, -105.09514225602024 39.936069338996646, -105.0950355885139 39.93607365200723, -105.09476502367005 39.93607269419247, -105.09459083983457 39.936071150007194, -105.09441193995632 39.93606956913881, -105.09423170902234 39.936068511994, -105.09419503199229 39.93606829722803, -105.09405326110337 39.936067466254734, -105.09387414977664 39.9360664242047, -105.09361008819027 39.936067368994394, -105.09338125094337 39.93606530861484, -105.09240350593156 39.93606276275314, -105.09186153911837 39.93606134993986, -105.09101574594376 39.93605931468678, -105.09085573459869 39.93605890767786, -105.09084933104744 39.937334165903444, -105.09084518444097 39.93815985715184, -105.0908424959132 39.93869504775551, -105.09090128311554 39.93869845210159, -105.09090230576669 39.93869844672675, -105.09090091299491 39.93899798932196, -105.0908992109706 39.93920895855562, -105.09089888968522 39.93924889918723, -105.09093866543665 39.93925538111568, -105.09093888882045 39.93925539722021, -105.09093992036517 39.93925547113504, -105.09094476783531 39.940065550553726, -105.09090321362216 39.940066010940534, -105.09090437104491 39.941318927614724, -105.09090447122907 39.9414271563125, -105.09106191788906 39.94143530162019, -105.09106199510268 39.941435303695606, -105.0910630538564 39.94143533357321, -105.0910588121924 39.94240422444584, -105.09105150154073 39.943289857750734, -105.09084017273963 39.943291005984435, -105.09064293944019 39.94329094929207, -105.0905381523252 39.94329137849177, -105.0905070988288 39.94329150589123, -105.08983762901697 39.94329425448934, -105.08603883557872 39.943320551037736, -105.08218711486477 39.94335411398962, -105.0812630425988 39.9433621325146, -105.0767360412157 39.94334022196765, -105.07661771967601 39.943339414312184, -105.07660145503716 39.94499877740917, -105.07658677437226 39.9464964353545, -105.07657376216802 39.94765414067553, -105.07655858793079 39.949199473163375, -105.07654824286396 39.95054710934591, -105.07610392108398 39.950542688821336, -105.07535727405836 39.95053202794011, -105.0745735205932 39.95052068211166, -105.07424398368101 39.95048048858849, -105.07202270340467 39.95021855966071, -105.07188238036339 39.9502020119051, -105.07188015686602 39.95049172946248, -105.07188143368751 39.95058499173008, -105.07198119658413 39.957636137166624, -105.07198229553856 39.95771376408718, -105.07198233618772 39.95771661303881, -105.07420306217612 39.957726265438815, -105.07420410847003 39.95772626840448, -105.07537934664629 39.95772928122915, -105.07538039645134 39.95772928419706, -105.07655562995483 39.95773230031829, -105.07655670901862 39.95773230338303, -105.07962679775243 39.9577626764316, -105.07962788730552 39.95776268671114, -105.07970751340797 39.95776347343922, -105.07970862051631 39.95776348378201, -105.08119158672785 39.957785883344755, -105.08119267741326 39.95778589991825, -105.08274309615933 39.95779841380289, -105.08274419157625 39.95779842227282, -105.0830905532878 39.95780121430522, -105.08309165572685 39.9578012227973, -105.08309129144561 39.9578828783425, -105.08309143792356 39.95791388241516, -105.08309174701412 39.95796309669239, -105.08309051757786 39.95814383200661, -105.08308960209372 39.9582756696281, -105.08308959905796 39.95827597494203, -105.08312659762191 39.95829352042862, -105.08312844361778 39.95829423682988, -105.08316774225267 39.95830886707035, -105.08316957676038 39.958309548303504, -105.08320923203983 39.958323659236356, -105.08321104804271 39.958324304375374, -105.08325105414725 39.95833789057515, -105.08325284814514 39.958338497806096, -105.08329319338146 39.958351557428855, -105.0832949770394 39.958352133098494, -105.08333563454902 39.95836465613951, -105.08333740085024 39.95836519932185, -105.08337837063785 39.958377184880064, -105.08338011724715 39.958377694665984, -105.08342138766321 39.958389133692336, -105.08342307367853 39.95838960002673, -105.08342311340468 39.958389610978294, -105.08346466923376 39.958400503417515, -105.08346631100146 39.95840093266411, -105.08346636942586 39.95840094818657, -105.08350820132617 39.95841129040186, -105.08350979766483 39.95841168435775, -105.08350987829856 39.958411704463785, -105.08355197343367 39.95842149010389, -105.08355352083221 39.95842184875641, -105.08355362251038 39.958421872541145, -105.08359597153846 39.95843109796932, -105.08359750504702 39.95843143135245, -105.08359759387879 39.95843145058738, -105.08364018276009 39.95844011485198, -105.08364176433072 39.958440435798934, -105.08368459659174 39.95844853621046, -105.08368610114441 39.95844881995132, -105.08368615843146 39.9584488300656, -105.08372919081746 39.958456358361516, -105.08373071304122 39.95845662325169, -105.0837739607767 39.958463577685514, -105.08377545623642 39.958463817259826, -105.08381888656132 39.95847019591163, -105.08382029561803 39.9584704018488, -105.08382034940509 39.95847041014899, -105.08383760552302 39.958472716925996, -105.08383907433954 39.958472911370066, -105.08386395766976 39.95847620759785, -105.08386538555133 39.958476397390456, -105.08390916006216 39.958481611792564, -105.08391055064631 39.95848177623136, -105.08395447735782 39.95848640753589, -105.08395575342821 39.95848654183878, -105.08395583296316 39.95848655023193, -105.08399989786838 39.95849059208348, -105.08400115298781 39.95849070739629, -105.08400121498387 39.958490713024105, -105.08404540636155 39.95849416808221, -105.08404668147602 39.958494267254785, -105.08409099119287 39.95849712558269, -105.08409214707908 39.95849720000647, -105.08409222897674 39.9584972048054, -105.08413663826745 39.95849947263985, -105.08413781881913 39.95849953274163, -105.08418233004518 39.95850120648842, -105.08418348378844 39.95850124847972, -105.08422805600803 39.95850232438844, -105.08422908111606 39.958502348802455, -105.0842291677117 39.958502350916255, -105.08427380211587 39.95850282538841, -105.08427486943923 39.95850283644447, -105.08427680168515 39.9585028461176, -105.08431955196065 39.958502713031955, -105.08432057606852 39.958502709521035, -105.08436529503523 39.958501982777726, -105.08436627240553 39.95850196648848, -105.08441101257975 39.958500639962075, -105.08441194671802 39.95850061180795, -105.08445669525753 39.95849868004812, -105.08445758264173 39.958498641817684, -105.08450232784169 39.95849610478225, -105.0845031673014 39.95849605647136, -105.08454788924257 39.95849291769114, -105.08454868427253 39.95849286201446, -105.08459337714025 39.95848911516397, -105.08459412539965 39.958489052113045, -105.08463877159355 39.95848470433415, -105.08463947307139 39.95848463571034, -105.08468406210092 39.95847967976002, -105.08468471444553 39.958479607356175, -105.08470210547705 39.95847744359641, -105.08470275553569 39.95847736217756, -105.08472922871567 39.958474049475726, -105.08472983309741 39.95847397329614, -105.08477426092547 39.95846780984096, -105.08477481732787 39.958467732587565, -105.08481914347053 39.958460968006186, -105.08481965305849 39.9584608905839, -105.08486386583297 39.95845352123168, -105.08486432509001 39.958453444528516, -105.08490840926406 39.958445473052734, -105.08490882169568 39.95844539798203, -105.08495276905376 39.95843682795595, -105.08495313230289 39.958436757211246, -105.08499692180484 39.958427584055926, -105.08499724055841 39.95842751675351, -105.08504085927449 39.95841774942916, -105.08504112882912 39.958417689154764, -105.08508456740086 39.95840732672732, -105.08508478892142 39.95840727438583, -105.08512802862755 39.95839631588745, -105.08512820328454 39.95839627148312, -105.0851712382503 39.95838472049549, -105.08517136837347 39.95838468583803, -105.08517434860536 39.95838384363866, -105.08517447991524 39.958383806283514, -105.08521417282265 39.95837254677202, -105.08521425723616 39.95837252275794, -105.0852568276513 39.95835979650178, -105.0852568616573 39.958359785816235, -105.08531014514506 39.958342919020964, -105.08531020026126 39.958342901206066, -105.08584216265436 39.95817871226845, -105.08584222128135 39.95817869446593, -105.08594421419804 39.95814721264614, -105.08594427282497 39.95814719484354, -105.08640891966976 39.95800377927178, -105.08640903926931 39.958003742773876, -105.08764353681755 39.95801568769421, -105.08764465680503 39.958015698006825, -105.0879119632444 39.958018284476545, -105.08791308440235 39.95801829479073, -105.0879358702931 39.958018514978804, -105.08793699262132 39.95801852529694, -105.0880433829552 39.95801955328184, -105.08804450060208 39.9580195635822, -105.0880454746665 39.95803347060461, -105.08815582481716 39.95803753346706, -105.08815692495803 39.958037535597796, -105.08861284895245 39.9580386337409, -105.08861296481724 39.958038634154555, -105.08861366352227 39.95803863574837, -105.08861394908794 39.95803863676791, -105.08866697104342 39.95803876480815, -105.08866700615397 39.95803876493348, -105.08866810746521 39.95803876706348, -105.08866767915576 39.958107686993046, -105.08866625171684 39.95824081254283, -105.08866408904484 39.958445815601955, -105.08862557510496 39.958447585716506, -105.08815449185182 39.95844611011514, -105.08804037684705 39.95844732158841, -105.08803822110079 39.958858108211714, -105.08803807357513 39.958886228193144, -105.08803338125136 39.959780949197565, -105.08792624490883 39.95978400035138, -105.08747407241 39.95978207714827, -105.08741119406886 39.960051242201324, -105.08720962180288 39.96007571814968, -105.08711916442843 39.96008593633609, -105.08704469758246 39.960094349186114, -105.08634982921242 39.960172872464106, -105.08593931871971 39.96023012947124, -105.08581766119005 39.96024710027866, -105.08578395984408 39.9602517994901, -105.08546617235673 39.960296124012366, -105.08506585278884 39.96035196090204, -105.08500963802015 39.960359798689154, -105.08474275318855 39.960397024463894, -105.08473924364331 39.96039751348618, -105.08473573409255 39.96039800340896, -105.08473222688248 39.96039849334009, -105.08472871731517 39.96039898596462, -105.08472520424212 39.96039947767574, -105.0847217017135 39.96039996762343, -105.08471818744799 39.96040046293266, -105.08471467905086 39.96040095556098, -105.08471117065368 39.96040144818916, -105.08470766575664 39.96040194263121, -105.08470415500216 39.960402437952695, -105.08470064424209 39.960402934174745, -105.08469713583379 39.96040342860376, -105.08469363210146 39.96040392395023, -105.08469012367108 39.960404421981636, -105.08468660938323 39.96040492089254, -105.0846831091674 39.960405415350685, -105.08467959603888 39.960405916066854, -105.08467608877866 39.960406414102074, -105.08467258386467 39.960406911244974, -105.08466907541207 39.960407412878304, -105.0846655681353 39.960407913615136, -105.08466205968807 39.96040841434764, -105.08465855358702 39.96040891418785, -105.08465504865086 39.960409414932755, -105.08465153901115 39.96040991926331, -105.08464803524532 39.96041042001222, -105.08464452795175 39.96041092345035, -105.08464102300442 39.960411425996156, -105.08463751804608 39.96041193034313, -105.08463400722472 39.9604124364702, -105.0846305022718 39.9604129399163, -105.08462699613192 39.96041344606006, -105.0846234911624 39.960413952207915, -105.08461998618733 39.96041445925627, -105.08461647651971 39.96041496808895, -105.0846129774075 39.96041547335694, -105.08460946773972 39.96041598218939, -105.08460596511074 39.96041648834515, -105.08460246128935 39.96041699809916, -105.08459895277538 39.96041750963744, -105.08459545247061 39.96041801850324, -105.08459194278612 39.960418530037074, -105.08458843897006 39.96041903889005, -105.08458493864862 39.960419550457424, -105.08458143363461 39.96042006380912, -105.08457792745017 39.96042057715649, -105.08457442478777 39.96042108871516, -105.08457091859775 39.96042160296298, -105.0845674159353 39.96042211452143, -105.08456391324533 39.96042263058297, -105.08456040587379 39.960423146627534, -105.08455690319468 39.96042366088757, -105.08455340285633 39.96042417515598, -105.08454989899035 39.9604246921135, -105.08454639512424 39.96042520907093, -105.08454289124712 39.960425727829545, -105.0845393908921 39.96042624479943, -105.08453588583903 39.96042676445424, -105.08453238548395 39.96042728142393, -105.08452888277152 39.96042780108701, -105.08452538122945 39.960428320754154, -105.08452187734105 39.960428841313444, -105.08451837696383 39.96042936188523, -105.08451487423473 39.9604298842498, -105.08451136799444 39.96043040660159, -105.08450786879293 39.96043092627666, -105.08450437073972 39.96043144955845, -105.08450086681815 39.96043197552092, -105.08449736642959 39.9604324978934, -105.08449386134296 39.960433022950795, -105.08449036445998 39.96043354623639, -105.08448686054362 39.96043407129777, -105.08448336130334 39.96043459727665, -105.08447985854079 39.96043512504401, -105.08447636047626 39.960435650126215, -105.08447285887856 39.96043617879819, -105.08446935377509 39.9604367065568, -105.08446586155684 39.96043723256042, -105.08446235760177 39.9604377639256, -105.08445885835008 39.960438291704975, -105.08445535791151 39.96043882218198, -105.08445185981917 39.96043935176664, -105.08444836055092 39.96043988224761, -105.08444485777137 39.96044041271587, -105.0844413596679 39.96044094410149, -105.08443785921261 39.96044147727986, -105.08443436227941 39.960442008669546, -105.08443086181856 39.96044254274836, -105.08442736370384 39.96044307593485, -105.08442386558366 39.96044361002188, -105.08442036511163 39.960444145901675, -105.08441686699132 39.96044467998852, -105.08441336885998 39.96044521587651, -105.08440987189897 39.96044575176866, -105.08440637493241 39.9604462885613, -105.08440287444915 39.96044682624184, -105.08439937748803 39.96044736213367, -105.08439587582323 39.960447901611026, -105.08439238237312 39.960448437515325, -105.0843888830491 39.96044897700094, -105.08438539075281 39.96044951561112, -105.0843818890714 39.96045005779001, -105.08437839560462 39.960450596395766, -105.08437489509348 39.9604511385787, -105.08437140043974 39.96045167988194, -105.08436790109343 39.9604522229695, -105.08436440526367 39.96045276516899, -105.08436091178017 39.960453306476126, -105.08435741008739 39.9604538504556, -105.08435391660376 39.96045439176255, -105.08435042192775 39.96045493666776, -105.08434692489992 39.9604554833657, -105.08434343257005 39.96045602737846, -105.0843399355421 39.960456574076204, -105.08433643382705 39.96045712165759, -105.084332941497 39.96045766567005, -105.08432944563383 39.960458213272304, -105.08432595561705 39.96045876179622, -105.08432245623155 39.960459311186916, -105.08431896388483 39.96045985790089, -105.08431546917534 39.960460408208895, -105.08431197211404 39.96046096030963, -105.08430847623954 39.960461509712566, -105.08430498387612 39.96046205912804, -105.0843014903368 39.96046260943984</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1512,7 +1516,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0559701557746 40.00568045011807, -105.0561221547891 40.00567145049642, -105.0561661556522 40.00563345075564, -105.0561531550697 40.0055424501676, -105.056107155146 40.00544945007372, -105.0571341561924 40.00545445010541, -105.0604611556923 40.00038144912251, -105.0640551537651 40.00037580618888, -105.0678619251848 40.00037085969463, -105.0744775635209 40.00036260693889, -105.0744770000605 40.00022899907422, -105.0744769994021 40.00005999822572, -105.0744790001136 39.99814399960752, -105.0744799999501 39.99791599833095, -105.0744720000795 39.99760599830033, -105.0744300017446 39.99733099854296, -105.0743510006399 39.99705999889498, -105.0742349999409 39.99679799885913, -105.0740829997001 39.99654599904907, -105.0739000001836 39.99630199852007, -105.0736860016148 39.9960719991295, -105.0733690015316 39.9957939984819, -105.0726170002045 39.99513499887867, -105.0723899995719 39.99489399859032, -105.0721960003037 39.99463699847043, -105.0720660003175 39.99442399870839, -105.0720359997661 39.99436699888737, -105.0719159993805 39.99409699899344, -105.0718799993343 39.99397799875175, -105.0718370192644 39.99383006495202, -105.0745450086098 39.99387001187085, -105.0758477384717 39.99390275861118, -105.0767412374697 39.99392255236432, -105.0767427244234 39.99392258574381, -105.0782446319749 39.99395584100868, -105.0783021140238 39.99395711315582, -105.0784748461619 39.99395994064453, -105.0784780588218 39.99396002894687, -105.079199983667 39.99397988502232, -105.0797780687563 39.99400011124025, -105.0804078235278 39.99403397578976, -105.0811001375908 39.99411006473294, -105.0811160663361 39.99384109073499, -105.0811151734891 39.99328902385216, -105.0811158889356 39.991952104357, -105.0811289517245 39.99133612493978, -105.0811314706972 39.99054232569287, -105.0811310648665 39.99044100165043, -105.0810032135734 39.99044053704765, -105.0806826117772 39.99043222283221, -105.0801900463319 39.99042685546382, -105.0795302550174 39.99041015292351, -105.0782662806757 39.99040196122129, -105.0782701483692 39.98977643642316, -105.0782773372099 39.98936539461084, -105.0782797903372 39.98896863345706, -105.078291626234 39.98855760861304, -105.0782988357461 39.98814299210392, -105.0783014433929 39.98772121019498, -105.0783111951955 39.98689553384761, -105.0782995407455 39.98677634180367, -105.0795759197414 39.98679312590777, -105.0800022714316 39.98680162144831, -105.0806001148401 39.98680553363357, -105.0812159749153 39.98681471489445, -105.0823341689822 39.98686196199735, -105.0823330669949 39.9868562577193, -105.0858280409819 39.98687167128099, -105.0905288265568 39.98692812962798, -105.0905269565108 39.98688310164826, -105.0905160203686 39.98513792585213, -105.0905020718375 39.98419187321576, -105.0905019035476 39.9835659626409, -105.0905040799873 39.98326289787578, -105.0905039957234 39.98291417235387, -105.0905041197469 39.98191268877581, -105.0905035131034 39.98129446275688, -105.0905034317418 39.98121888616951, -105.0904855034348 39.97977515944299, -105.0904860309043 39.97970621027422, -105.0904860571139 39.97970281937673, -105.0903270877842 39.9797032929451, -105.0835085716659 39.97962404552135, -105.0834853211123 39.97962377507007, -105.079294460449 39.97957148382346, -105.0761908360338 39.97952951234009, -105.0757716939829 39.97952383912966, -105.0743940604178 39.97950518038726, -105.0740721520792 39.9795029564586, -105.0737704031381 39.9795008692249, -105.0732085340372 39.97949698163314, -105.072615305267 39.97948638758501, -105.0719256017096 39.97947406682838, -105.0718668765302 39.9794736037379, -105.0718568404095 39.98014410421328, -105.0718501168945 39.98058990350253, -105.0718328878368 39.98140187753952, -105.0718160675592 39.98243292109945, -105.0718117048491 39.98309269216385, -105.0717552482085 39.98309274272643, -105.0717146023103 39.9830922080333, -105.0709660816366 39.98308237411967, -105.0704747521287 39.9830759158628, -105.0670935888734 39.98306391759739, -105.0670400578877 39.98623419443279, -105.0670383169087 39.98633729479067, -105.0670371933367 39.98633703838531, -105.0670338384547 39.98653575957677, -105.0634909949253 39.98647646216797, -105.0634606537379 39.98647581498217, -105.0623500000977 39.98645786501839, -105.057580642476 39.98649541493525, -105.0528281835631 39.98653346176652, -105.0528281825257 39.98653558462474, -105.0528294585598 39.98661866671064, -105.0528295848461 39.98668834697705, -105.0528304499507 39.98732437495488, -105.0528348717868 39.9905809484678, -105.0528390825118 39.99368010602634, -105.0528393044056 39.99384272774888, -105.0528394349737 39.99393997815403, -105.0528283593103 39.99690249635807, -105.0528200519861 39.99912227758396, -105.0528167871464 39.9999946998671, -105.0528157911476 40.00026000119946, -105.0528157886235 40.00026074333486, -105.0554312871795 40.0002650169132, -105.0554323634255 40.00026501655961, -105.055634433771 40.0002650128381, -105.0556344759296 40.00026501300059, -105.0556355545178 40.00026501265413, -105.0556326108461 40.00046785188778, -105.0556266371632 40.0007685128878, -105.0555647273613 40.00388346806245, -105.055531007058 40.00563956685976, -105.0555401553612 40.00564045054492, -105.0555902120115 40.00566690495083, -105.0556471557209 40.00567245091049, -105.0557201558533 40.00567145055776, -105.0558361548308 40.00567645117783, -105.0559061543596 40.00567545085779, -105.0559701557746 40.00568045011807))</t>
+          <t>POLYGON ((-105.05597015577457 40.00568045011807, -105.0561221547891 40.00567145049642, -105.05616615565222 40.00563345075564, -105.05615315506971 40.0055424501676, -105.05610715514595 40.00544945007372, -105.05713415619238 40.00545445010541, -105.06046115569234 40.000381449122514, -105.06405515376512 40.000375806188885, -105.06786192518477 40.00037085969463, -105.07447756352092 40.000362606938886, -105.0744770000605 40.000228999074224, -105.0744769994021 40.00005999822572, -105.07447900011357 39.99814399960752, -105.07447999995014 39.99791599833095, -105.0744720000795 39.99760599830033, -105.07443000174464 39.99733099854296, -105.07435100063994 39.997059998894976, -105.07423499994091 39.99679799885913, -105.07408299970014 39.99654599904907, -105.07390000018356 39.996301998520075, -105.07368600161479 39.9960719991295, -105.0733690015316 39.9957939984819, -105.07261700020454 39.99513499887867, -105.07238999957193 39.99489399859032, -105.07219600030372 39.994636998470426, -105.07206600031748 39.99442399870839, -105.07203599976614 39.99436699888737, -105.07191599938052 39.99409699899344, -105.07187999933433 39.993977998751745, -105.07183701926438 39.99383006495202, -105.07454500860979 39.993870011870854, -105.07584773847165 39.993902758611185, -105.07674123746973 39.993922552364324, -105.07674272442344 39.99392258574381, -105.07824463197487 39.993955841008685, -105.07830211402381 39.993957113155815, -105.07847484616191 39.99395994064453, -105.07847805882183 39.993960028946866, -105.079199983667 39.99397988502232, -105.07977806875631 39.994000111240254, -105.08040782352784 39.99403397578976, -105.0811001375908 39.994110064732936, -105.08111606633608 39.99384109073499, -105.08111517348912 39.993289023852164, -105.08111588893556 39.991952104357, -105.08112895172451 39.99133612493978, -105.08113147069722 39.99054232569287, -105.08113106486645 39.99044100165043, -105.08100321357342 39.99044053704765, -105.08068261177723 39.99043222283221, -105.08019004633188 39.99042685546382, -105.07953025501742 39.99041015292351, -105.07826628067572 39.990401961221295, -105.07827014836919 39.989776436423156, -105.07827733720985 39.98936539461084, -105.07827979033719 39.988968633457056, -105.07829162623398 39.988557608613036, -105.07829883574611 39.98814299210392, -105.07830144339289 39.987721210194984, -105.0783111951955 39.98689553384761, -105.07829954074549 39.98677634180367, -105.07957591974144 39.986793125907774, -105.08000227143157 39.986801621448315, -105.08060011484007 39.98680553363357, -105.0812159749153 39.98681471489445, -105.08233416898223 39.98686196199735, -105.08233306699488 39.986856257719296, -105.08582804098191 39.986871671280994, -105.09052882655683 39.98692812962798, -105.09052695651083 39.98688310164826, -105.0905160203686 39.98513792585213, -105.09050207183748 39.984191873215764, -105.09050190354759 39.9835659626409, -105.09050407998734 39.98326289787578, -105.09050399572335 39.98291417235387, -105.09050411974688 39.981912688775815, -105.09050351310337 39.98129446275688, -105.0905034317418 39.981218886169515, -105.09048550343476 39.97977515944299, -105.09048603090432 39.979706210274216, -105.09048605711386 39.979702819376726, -105.09032708778417 39.9797032929451, -105.08350857166586 39.97962404552135, -105.0834853211123 39.979623775070074, -105.07929446044902 39.97957148382346, -105.07619083603376 39.97952951234009, -105.07577169398292 39.97952383912966, -105.07439406041776 39.979505180387264, -105.07407215207915 39.9795029564586, -105.07377040313808 39.9795008692249, -105.07320853403718 39.97949698163314, -105.07261530526698 39.979486387585006, -105.07192560170961 39.97947406682838, -105.07186687653018 39.9794736037379, -105.0718568404095 39.98014410421328, -105.07185011689448 39.98058990350253, -105.07183288783676 39.98140187753952, -105.07181606755924 39.98243292109945, -105.07181170484914 39.98309269216385, -105.0717552482085 39.983092742726434, -105.07171460231034 39.9830922080333, -105.07096608163656 39.98308237411967, -105.07047475212875 39.9830759158628, -105.06709358887338 39.98306391759739, -105.06704005788771 39.98623419443279, -105.06703831690874 39.98633729479067, -105.06703719333667 39.98633703838531, -105.06703383845469 39.986535759576775, -105.06349099492526 39.98647646216797, -105.06346065373788 39.98647581498217, -105.06235000009765 39.98645786501839, -105.05758064247598 39.98649541493525, -105.05282818356312 39.98653346176652, -105.0528281825257 39.98653558462474, -105.05282945855984 39.98661866671064, -105.05282958484612 39.986688346977054, -105.05283044995075 39.98732437495488, -105.05283487178679 39.9905809484678, -105.05283908251178 39.99368010602634, -105.05283930440564 39.99384272774888, -105.05283943497368 39.99393997815403, -105.05282835931031 39.99690249635807, -105.0528200519861 39.999122277583965, -105.05281678714636 39.9999946998671, -105.05281579114761 40.00026000119946, -105.05281578862346 40.00026074333486, -105.05543128717946 40.000265016913204, -105.05543236342551 40.00026501655961, -105.055634433771 40.0002650128381, -105.05563447592964 40.000265013000586, -105.05563555451785 40.00026501265413, -105.0556326108461 40.000467851887784, -105.05562663716323 40.000768512887795, -105.05556472736133 40.00388346806245, -105.05553100705797 40.005639566859756, -105.05554015536124 40.00564045054492, -105.05559021201147 40.00566690495083, -105.05564715572095 40.00567245091049, -105.05572015585328 40.00567145055776, -105.05583615483084 40.005676451177834, -105.05590615435958 40.00567545085779, -105.05597015577457 40.00568045011807))</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1554,7 +1558,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1092964823203 39.97532071473902, -105.1092904101518 39.97530904500583, -105.1092758320701 39.97528099133424, -105.1092339554898 39.97511696238349, -105.1092260671889 39.97499889140114, -105.1092199916418 39.97462689328338, -105.1092231749814 39.97382200486576, -105.1092319271565 39.97335287654287, -105.1092651591187 39.97241000593239, -105.1084309638869 39.97240690009586, -105.1062811423174 39.97241796939557, -105.1054728138778 39.97241715154041, -105.105473750072 39.97254757141797, -105.1054698415779 39.97377082908722, -105.1045682620514 39.97377105019996, -105.1045601154635 39.97610235688621, -105.097555653059 39.97609100741533, -105.0975682202136 39.97252892556443, -105.0975654791955 39.97243912451826, -105.0975640093021 39.97241206530735, -105.0974380772597 39.97241405009566, -105.0968671338764 39.97242303532938, -105.095958529845 39.97241979958787, -105.0959494027172 39.97241976308735, -105.0959485145728 39.97252466095966, -105.0959485841525 39.97327529347321, -105.0953453933799 39.97327727257912, -105.0953442665838 39.9725246251522, -105.0953437698846 39.97241731765187, -105.0953327932177 39.97241727370804, -105.0950421100944 39.97241608789733, -105.0946450026706 39.97241304460964, -105.0943081662019 39.97241487935375, -105.0936430785647 39.97241500683583, -105.091422029526 39.97240303667677, -105.0913521083569 39.97240086766923, -105.0912461536423 39.97239802052451, -105.0911648255174 39.9723941636361, -105.0909639507684 39.97239290149737, -105.0903030782694 39.97240400643749, -105.090215942638 39.97240347779733, -105.09020081638 39.97411529796517, -105.090192863608 39.97466574347093, -105.0902418876107 39.97501264559047, -105.0902914261388 39.9752737605607, -105.0903689920018 39.97550995382825, -105.0904193253848 39.97563881566658, -105.0904417425443 39.97584710582651, -105.0904542693785 39.97608297782843, -105.09057003187 39.97607998460246, -105.0951916295389 39.97607892625242, -105.0952100830245 39.97971518827352, -105.0906909442718 39.97970782075467, -105.0904860309043 39.97970621027422, -105.0904855034348 39.97977515944299, -105.0905034317418 39.98121888616951, -105.0905035131034 39.98129446275688, -105.0905041197469 39.98191268877581, -105.0905039957234 39.98291417235387, -105.0905040799873 39.98326289787578, -105.0905019035476 39.9835659626409, -105.0905020718375 39.98419187321576, -105.0905160203686 39.98513792585213, -105.0905269565108 39.98688310164826, -105.0905288265568 39.98692812962798, -105.0927489637514 39.9869329743509, -105.0943223346905 39.98694808340338, -105.0963929897977 39.98694990812138, -105.098331016714 39.98698412932367, -105.098434505815 39.98698684960066, -105.0985320536637 39.98698941399471, -105.1014498374917 39.98698013024322, -105.103439024915 39.98699303012703, -105.1062505998226 39.98700731608795, -105.1078061103663 39.98700797037096, -105.1078060590639 39.98695498706369, -105.1078220583742 39.98653090532559, -105.1078050868355 39.9862549537617, -105.1077691785012 39.98604509665183, -105.1076760619038 39.98572990356753, -105.1076159278525 39.98557486819453, -105.1074641115097 39.98528994713687, -105.107278854246 39.98492502517655, -105.1072209426614 39.98475599728788, -105.1071971366225 39.98461398831283, -105.1071878991829 39.9844209678387, -105.1072079188933 39.9842288711616, -105.1073091654765 39.98381304076367, -105.1073759754432 39.98355192370965, -105.1074541166158 39.98324390187725, -105.1074760223592 39.98315805076438, -105.1075081575968 39.98303105628209, -105.1076315724385 39.98246858705549, -105.1077270577214 39.98213713482575, -105.1078259452344 39.98175808246668, -105.1079229285001 39.98152397044463, -105.1079849679163 39.98140888248692, -105.1080241473747 39.98135987658505, -105.1082001068512 39.98116803426773, -105.1084030895306 39.98099303037341, -105.1086481178667 39.98082887503443, -105.1086971431693 39.98080488305403, -105.1095481361159 39.98038500504651, -105.1096519135303 39.9803340215819, -105.1100210818607 39.98011400588797, -105.1104370634613 39.9797568874656, -105.1106279420174 39.979574974821, -105.1109720115203 39.97918686477371, -105.1109053486704 39.97906594403207, -105.1117843009302 39.97806382540433, -105.1139118935617 39.97724541987482, -105.1139224334814 39.97724106355832, -105.1139225010929 39.97722270381748, -105.1139263929838 39.97616781171246, -105.1139267909006 39.97613287191204, -105.113926640384 39.97608334227244, -105.1138089882512 39.97608305170019, -105.1133790200561 39.97608188493721, -105.1123831027614 39.97608512830671, -105.1117668377299 39.9760899171973, -105.1108470594524 39.97608530949304, -105.1108412041789 39.97609179069381, -105.1092491642645 39.97610344217862, -105.1092964823203 39.97532071473902))</t>
+          <t>POLYGON ((-105.10929648232026 39.97532071473902, -105.10929041015177 39.97530904500583, -105.1092758320701 39.97528099133424, -105.10923395548977 39.97511696238349, -105.10922606718886 39.974998891401135, -105.10921999164184 39.97462689328338, -105.10922317498135 39.97382200486576, -105.10923192715646 39.97335287654287, -105.10926515911866 39.97241000593239, -105.1084309638869 39.97240690009586, -105.10628114231736 39.97241796939557, -105.10547281387781 39.97241715154041, -105.105473750072 39.97254757141797, -105.1054698415779 39.97377082908722, -105.10456826205139 39.97377105019996, -105.10456011546347 39.97610235688621, -105.09755565305896 39.97609100741533, -105.09756822021363 39.97252892556443, -105.09756547919547 39.97243912451826, -105.09756400930208 39.972412065307346, -105.0974380772597 39.97241405009566, -105.09686713387642 39.972423035329385, -105.09595852984498 39.97241979958787, -105.09594940271718 39.97241976308735, -105.09594851457278 39.97252466095966, -105.09594858415254 39.973275293473215, -105.09534539337994 39.97327727257912, -105.09534426658375 39.972524625152204, -105.09534376988462 39.972417317651875, -105.09533279321772 39.97241727370804, -105.0950421100944 39.97241608789733, -105.09464500267062 39.97241304460964, -105.09430816620187 39.97241487935375, -105.09364307856468 39.97241500683583, -105.09142202952599 39.97240303667677, -105.0913521083569 39.97240086766923, -105.0912461536423 39.97239802052451, -105.09116482551741 39.9723941636361, -105.09096395076844 39.97239290149737, -105.09030307826939 39.972404006437486, -105.090215942638 39.97240347779733, -105.09020081638 39.97411529796517, -105.090192863608 39.97466574347093, -105.09024188761072 39.975012645590475, -105.09029142613885 39.975273760560704, -105.09036899200183 39.97550995382825, -105.09041932538481 39.975638815666585, -105.09044174254427 39.97584710582651, -105.09045426937853 39.97608297782843, -105.09057003187004 39.976079984602464, -105.09519162953886 39.97607892625242, -105.0952100830245 39.97971518827352, -105.09069094427178 39.97970782075467, -105.09048603090432 39.979706210274216, -105.09048550343476 39.97977515944299, -105.0905034317418 39.981218886169515, -105.09050351310337 39.98129446275688, -105.09050411974688 39.981912688775815, -105.09050399572335 39.98291417235387, -105.09050407998734 39.98326289787578, -105.09050190354759 39.9835659626409, -105.09050207183748 39.984191873215764, -105.0905160203686 39.98513792585213, -105.09052695651083 39.98688310164826, -105.09052882655683 39.98692812962798, -105.09274896375145 39.9869329743509, -105.09432233469055 39.986948083403384, -105.09639298979774 39.98694990812138, -105.09833101671397 39.98698412932367, -105.09843450581504 39.98698684960066, -105.09853205366373 39.98698941399471, -105.10144983749169 39.98698013024322, -105.10343902491498 39.98699303012703, -105.10625059982263 39.987007316087954, -105.10780611036631 39.98700797037096, -105.10780605906393 39.98695498706369, -105.10782205837418 39.986530905325594, -105.10780508683546 39.9862549537617, -105.10776917850124 39.98604509665183, -105.10767606190376 39.98572990356753, -105.10761592785252 39.985574868194526, -105.10746411150966 39.98528994713687, -105.10727885424596 39.98492502517655, -105.10722094266141 39.98475599728788, -105.10719713662247 39.98461398831283, -105.10718789918289 39.9844209678387, -105.1072079188933 39.984228871161605, -105.10730916547654 39.98381304076367, -105.1073759754432 39.983551923709655, -105.1074541166158 39.98324390187725, -105.10747602235918 39.98315805076438, -105.10750815759684 39.983031056282094, -105.10763157243852 39.982468587055486, -105.10772705772139 39.98213713482575, -105.1078259452344 39.981758082466676, -105.10792292850014 39.98152397044463, -105.10798496791634 39.98140888248692, -105.10802414737475 39.98135987658505, -105.10820010685119 39.98116803426773, -105.10840308953055 39.98099303037341, -105.10864811786665 39.98082887503443, -105.10869714316932 39.98080488305403, -105.10954813611588 39.980385005046514, -105.10965191353031 39.9803340215819, -105.11002108186068 39.98011400588797, -105.11043706346129 39.9797568874656, -105.1106279420174 39.979574974821, -105.1109720115203 39.97918686477371, -105.11090534867039 39.97906594403207, -105.11178430093021 39.97806382540433, -105.11391189356168 39.97724541987482, -105.11392243348138 39.97724106355832, -105.11392250109286 39.97722270381748, -105.11392639298379 39.976167811712465, -105.11392679090056 39.97613287191204, -105.11392664038401 39.97608334227244, -105.1138089882512 39.97608305170019, -105.11337902005612 39.97608188493721, -105.11238310276143 39.976085128306714, -105.11176683772987 39.9760899171973, -105.11084705945237 39.97608530949304, -105.11084120417891 39.976091790693815, -105.10924916426448 39.97610344217862, -105.10929648232026 39.97532071473902))</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1596,7 +1600,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1073759754432 39.98355192370965, -105.1073091654765 39.98381304076367, -105.1072079188933 39.9842288711616, -105.1071878991829 39.9844209678387, -105.1071971366225 39.98461398831283, -105.1072209426614 39.98475599728788, -105.107278854246 39.98492502517655, -105.1074641115097 39.98528994713687, -105.1076159278525 39.98557486819453, -105.1076760619038 39.98572990356753, -105.1077691785012 39.98604509665183, -105.1078050868355 39.9862549537617, -105.1078220583742 39.98653090532559, -105.1078060590639 39.98695498706369, -105.1078061103663 39.98700797037096, -105.1091016110865 39.98701312174199, -105.1137151610658 39.98698207706551, -105.1157364703514 39.98696958815421, -105.1173699922748 39.98694351032786, -105.1173718857854 39.98689901321579, -105.1173974168023 39.9851484639417, -105.1174133094992 39.98331547110325, -105.1186071665135 39.98330244358745, -105.1185851681232 39.98678444408168, -105.1211532829889 39.9867767735869, -105.1230647672254 39.98677086630205, -105.1252729795815 39.9867354607854, -105.1278491696992 39.98669844549102, -105.1278438505662 39.98611127501945, -105.127841169928 39.98581544210798, -105.1278368922283 39.98539987307798, -105.1278341691096 39.98513544239999, -105.1278081691162 39.98462244192449, -105.1278173436443 39.98417719271642, -105.1278251690041 39.98379744319919, -105.1278411686021 39.98365144210749, -105.1268601685777 39.98365144197767, -105.1268441685182 39.98313644257139, -105.1258921445311 39.98314315953377, -105.1249263230647 39.98314996424318, -105.1242251688294 39.98315444282675, -105.1240021678686 39.98305844296069, -105.1238561683382 39.98296444303244, -105.123744168235 39.98286744302084, -105.1236691677244 39.98278344313378, -105.1235781685477 39.98264044277064, -105.1235830349789 39.98201442443881, -105.123586168347 39.98161144252593, -105.1236411680837 39.98141344271861, -105.1237131684662 39.98127144197014, -105.123848168531 39.98109744278342, -105.1239481684561 39.98099044193104, -105.1239441684502 39.98063844197828, -105.12468924775 39.98064430008328, -105.1250891674626 39.98064744247992, -105.1253301685872 39.98066944203719, -105.1254741692224 39.98069944174981, -105.1256331685554 39.98073244235897, -105.1258431687578 39.98075244156166, -105.1259671694033 39.98075344203813, -105.1261481677718 39.9807394421338, -105.126331169116 39.98070644271509, -105.1264991677584 39.98067244239655, -105.1266091684414 39.98065844226225, -105.1266971688295 39.98065244248855, -105.1267971687024 39.98065044260115, -105.1268901681804 39.98065044284952, -105.1269711680979 39.98065844167844, -105.1270981684207 39.98067544186095, -105.127139392241 39.98068334791111, -105.1271711685487 39.98068944278467, -105.127214375739 39.98069969063391, -105.1273066551089 39.98072157695184, -105.1273271684002 39.98072644199087, -105.1274521692765 39.98074644262105, -105.1275471685854 39.9807554418902, -105.1277031693758 39.98076144258219, -105.1277022727454 39.98065050362139, -105.1277006654453 39.98045161563807, -105.1276992570783 39.98027720192252, -105.1276979486562 39.98011536714193, -105.12769489113 39.97973687298536, -105.1276880805791 39.97925149078886, -105.1276812036791 39.97880423869458, -105.1276742985784 39.97835509150174, -105.1276701687788 39.97808644191434, -105.1271081689285 39.97816144152506, -105.1262311691111 39.97870844220219, -105.1260051674357 39.97884844174765, -105.1255304415947 39.97914450912447, -105.1253541688852 39.97925444189506, -105.1255771679067 39.97947344233817, -105.1243405817918 39.98021614971381, -105.1235891680376 39.98066744275177, -105.1232421681502 39.98033144190374, -105.1225391670139 39.98073944211418, -105.1219081678686 39.98099644262695, -105.120230166672 39.98108244243971, -105.1201190479548 39.97979700902974, -105.1199982265585 39.97824241435777, -105.120213921188 39.9783408640164, -105.1204351430655 39.97840802722106, -105.1206690055671 39.97844805327635, -105.1209279925593 39.97846208286956, -105.1212738234645 39.9784519641494, -105.1218390971384 39.97837997317655, -105.1220440922178 39.97834907560969, -105.1251821045501 39.97776690536398, -105.1271320977502 39.97739411515896, -105.1273435143957 39.97735082326365, -105.1276466084615 39.97708321067033, -105.1276525381961 39.97673399347658, -105.1276644462961 39.97603262125949, -105.1275745938115 39.97544829877226, -105.1274121598896 39.97481223461234, -105.1269897690644 39.97410774900974, -105.1265094311803 39.97363524625856, -105.1259336601506 39.97325526013939, -105.125568498434 39.97308157000424, -105.1254721676893 39.97304244124539, -105.1254030021113 39.97301706732278, -105.1253031669845 39.97298044167606, -105.1252489123642 39.97296264565752, -105.1251781675552 39.97293944155944, -105.1250681668962 39.972906441131, -105.1249497653521 39.97287524610411, -105.1249011680386 39.97286244087732, -105.1248531668425 39.97285044186012, -105.1247921674847 39.97283644067091, -105.1246601669836 39.97280844165002, -105.1245523833219 39.97278895695491, -105.1244201369517 39.97276780367894, -105.1242581672639 39.97274644167108, -105.1241911675568 39.97273944124998, -105.1229011674566 39.97270644080103, -105.1217242765111 39.97281619705816, -105.1214051667389 39.9728474415511, -105.1212921660192 39.9728514412086, -105.1211677547576 39.97285530417747, -105.1209041446044 39.97286348814555, -105.1206801658403 39.97287044195357, -105.1203420443671 39.97286990956984, -105.1194881869002 39.97287256612985, -105.1186181657589 39.97287744155079, -105.1186161666875 39.97368444138921, -105.1182721659632 39.97381044163679, -105.118018165306 39.97395344192811, -105.1171981652229 39.97420444199783, -105.1171265636503 39.97423590742287, -105.1158010195454 39.97481841383456, -105.114358165628 39.97545244199855, -105.1140021644149 39.97552144240487, -105.1135711643946 39.97554144292338, -105.113406165381 39.97567644266403, -105.1132631646667 39.97570744192655, -105.1133870040023 39.97608190631396, -105.1138089882512 39.97608305170019, -105.113926640384 39.97608334227244, -105.1139267909006 39.97613287191204, -105.1139263929838 39.97616781171246, -105.1139225010929 39.97722270381748, -105.1139224334814 39.97724106355832, -105.1139118935617 39.97724541987482, -105.1117843009302 39.97806382540433, -105.1109053486704 39.97906594403207, -105.1109720115203 39.97918686477371, -105.1106279420174 39.979574974821, -105.1104370634613 39.9797568874656, -105.1100210818607 39.98011400588797, -105.1096519135303 39.9803340215819, -105.1095481361159 39.98038500504651, -105.1086971431693 39.98080488305403, -105.1086481178667 39.98082887503443, -105.1084030895306 39.98099303037341, -105.1082001068512 39.98116803426773, -105.1080241473747 39.98135987658505, -105.1079849679163 39.98140888248692, -105.1079229285001 39.98152397044463, -105.1078259452344 39.98175808246668, -105.1077270577214 39.98213713482575, -105.1076315724385 39.98246858705549, -105.1075081575968 39.98303105628209, -105.1074760223592 39.98315805076438, -105.1074541166158 39.98324390187725, -105.1073759754432 39.98355192370965))</t>
+          <t>POLYGON ((-105.1073759754432 39.983551923709655, -105.10730916547654 39.98381304076367, -105.1072079188933 39.984228871161605, -105.10718789918289 39.9844209678387, -105.10719713662247 39.98461398831283, -105.10722094266141 39.98475599728788, -105.10727885424596 39.98492502517655, -105.10746411150966 39.98528994713687, -105.10761592785252 39.985574868194526, -105.10767606190376 39.98572990356753, -105.10776917850124 39.98604509665183, -105.10780508683546 39.9862549537617, -105.10782205837418 39.986530905325594, -105.10780605906393 39.98695498706369, -105.10780611036631 39.98700797037096, -105.10910161108649 39.98701312174199, -105.11371516106578 39.98698207706551, -105.11573647035142 39.98696958815421, -105.11736999227477 39.98694351032786, -105.11737188578539 39.98689901321579, -105.11739741680232 39.9851484639417, -105.11741330949921 39.983315471103246, -105.11860716651354 39.983302443587455, -105.1185851681232 39.98678444408168, -105.12115328298886 39.9867767735869, -105.12306476722542 39.98677086630205, -105.12527297958147 39.986735460785404, -105.12784916969922 39.986698445491015, -105.12784385056624 39.98611127501945, -105.127841169928 39.985815442107985, -105.12783689222834 39.98539987307798, -105.12783416910956 39.98513544239999, -105.12780816911615 39.984622441924486, -105.12781734364428 39.98417719271642, -105.12782516900411 39.98379744319919, -105.1278411686021 39.983651442107494, -105.12686016857774 39.98365144197767, -105.12684416851818 39.98313644257139, -105.12589214453108 39.98314315953377, -105.12492632306473 39.983149964243175, -105.12422516882944 39.98315444282675, -105.12400216786861 39.98305844296069, -105.12385616833825 39.98296444303244, -105.12374416823499 39.98286744302084, -105.12366916772436 39.98278344313378, -105.12357816854767 39.982640442770645, -105.12358303497885 39.98201442443881, -105.123586168347 39.98161144252593, -105.12364116808365 39.98141344271861, -105.12371316846621 39.98127144197014, -105.12384816853096 39.981097442783415, -105.12394816845612 39.98099044193104, -105.12394416845024 39.98063844197828, -105.12468924774997 39.980644300083284, -105.12508916746263 39.98064744247992, -105.12533016858723 39.98066944203719, -105.12547416922237 39.98069944174981, -105.12563316855537 39.98073244235897, -105.1258431687578 39.98075244156166, -105.12596716940325 39.98075344203813, -105.12614816777177 39.9807394421338, -105.12633116911601 39.98070644271509, -105.1264991677584 39.98067244239655, -105.1266091684414 39.980658442262246, -105.12669716882947 39.98065244248855, -105.12679716870242 39.98065044260115, -105.1268901681804 39.980650442849516, -105.1269711680979 39.980658441678436, -105.12709816842069 39.980675441860946, -105.127139392241 39.98068334791111, -105.12717116854866 39.98068944278467, -105.12721437573896 39.980699690633905, -105.1273066551089 39.98072157695184, -105.12732716840023 39.98072644199087, -105.12745216927647 39.980746442621054, -105.12754716858537 39.980755441890196, -105.12770316937583 39.980761442582185, -105.12770227274538 39.98065050362139, -105.12770066544532 39.98045161563807, -105.12769925707835 39.98027720192252, -105.12769794865618 39.98011536714193, -105.12769489113002 39.97973687298536, -105.12768808057913 39.97925149078886, -105.1276812036791 39.97880423869458, -105.12767429857837 39.97835509150174, -105.12767016877879 39.978086441914336, -105.12710816892852 39.97816144152506, -105.1262311691111 39.97870844220219, -105.12600516743572 39.97884844174765, -105.12553044159466 39.97914450912447, -105.12535416888515 39.97925444189506, -105.12557716790668 39.97947344233817, -105.12434058179181 39.98021614971381, -105.12358916803758 39.980667442751766, -105.12324216815017 39.98033144190374, -105.12253916701391 39.98073944211418, -105.12190816786861 39.980996442626946, -105.12023016667196 39.98108244243971, -105.12011904795484 39.97979700902974, -105.11999822655854 39.97824241435777, -105.120213921188 39.978340864016396, -105.12043514306552 39.978408027221064, -105.12066900556705 39.978448053276345, -105.12092799255929 39.978462082869555, -105.1212738234645 39.9784519641494, -105.12183909713839 39.97837997317655, -105.12204409221776 39.97834907560969, -105.12518210455008 39.97776690536398, -105.12713209775025 39.97739411515896, -105.12734351439568 39.97735082326365, -105.12764660846148 39.97708321067033, -105.12765253819613 39.97673399347658, -105.12766444629614 39.97603262125949, -105.12757459381146 39.975448298772264, -105.12741215988962 39.97481223461234, -105.12698976906441 39.97410774900974, -105.12650943118032 39.97363524625856, -105.12593366015055 39.97325526013939, -105.12556849843396 39.97308157000424, -105.12547216768927 39.97304244124539, -105.12540300211128 39.97301706732278, -105.1253031669845 39.972980441676064, -105.12524891236417 39.972962645657525, -105.12517816755525 39.97293944155944, -105.1250681668962 39.972906441131, -105.12494976535206 39.97287524610411, -105.12490116803862 39.97286244087732, -105.1248531668425 39.972850441860125, -105.12479216748471 39.97283644067091, -105.12466016698356 39.97280844165002, -105.12455238332191 39.972788956954915, -105.12442013695171 39.97276780367894, -105.12425816726389 39.972746441671084, -105.1241911675568 39.97273944124998, -105.12290116745665 39.972706440801026, -105.12172427651106 39.97281619705816, -105.12140516673887 39.972847441551096, -105.12129216601923 39.9728514412086, -105.12116775475764 39.97285530417747, -105.12090414460438 39.97286348814555, -105.12068016584033 39.972870441953575, -105.12034204436713 39.972869909569845, -105.11948818690017 39.97287256612985, -105.11861816575893 39.97287744155079, -105.11861616668753 39.97368444138921, -105.1182721659632 39.97381044163679, -105.11801816530597 39.97395344192811, -105.11719816522287 39.974204441997834, -105.11712656365034 39.974235907422866, -105.11580101954537 39.97481841383456, -105.11435816562796 39.97545244199855, -105.11400216441494 39.97552144240487, -105.11357116439456 39.97554144292338, -105.11340616538101 39.97567644266403, -105.1132631646667 39.97570744192655, -105.1133870040023 39.97608190631396, -105.1138089882512 39.97608305170019, -105.11392664038401 39.97608334227244, -105.11392679090056 39.97613287191204, -105.11392639298379 39.976167811712465, -105.11392250109286 39.97722270381748, -105.11392243348138 39.97724106355832, -105.11391189356168 39.97724541987482, -105.11178430093021 39.97806382540433, -105.11090534867039 39.97906594403207, -105.1109720115203 39.97918686477371, -105.1106279420174 39.979574974821, -105.11043706346129 39.9797568874656, -105.11002108186068 39.98011400588797, -105.10965191353031 39.9803340215819, -105.10954813611588 39.980385005046514, -105.10869714316932 39.98080488305403, -105.10864811786665 39.98082887503443, -105.10840308953055 39.98099303037341, -105.10820010685119 39.98116803426773, -105.10802414737475 39.98135987658505, -105.10798496791634 39.98140888248692, -105.10792292850014 39.98152397044463, -105.1078259452344 39.981758082466676, -105.10772705772139 39.98213713482575, -105.10763157243852 39.982468587055486, -105.10750815759684 39.983031056282094, -105.10747602235918 39.98315805076438, -105.1074541166158 39.98324390187725, -105.1073759754432 39.983551923709655))</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1638,7 +1642,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1074268767083 39.99417800868869, -105.1074179133983 39.99449505084446, -105.1074219793821 39.9948428831692, -105.1074118466262 39.99536306685848, -105.1074071554426 39.9963019144348, -105.1073710079347 39.99644289583818, -105.1072999251899 39.99657607111498, -105.1071950160415 39.99669513035742, -105.1070971302669 39.99677193739147, -105.1068751336015 39.99689306868019, -105.1065620076894 39.99703310417146, -105.1060899401119 39.99725303107669, -105.1060208900468 39.99728107134368, -105.1056769263536 39.99744488274133, -105.1055848806782 39.99749892268895, -105.1054220962793 39.99762601885258, -105.1053211663243 39.9977349323769, -105.1052358470442 39.99786009672034, -105.1051798392762 39.99797794895188, -105.1051379051814 39.99813098857716, -105.1051068977895 39.99830794929273, -105.105104998287 39.99863599531165, -105.1051140678082 39.99941209919503, -105.105125942928 40.00019699675529, -105.1053192989058 40.00019710578297, -105.1067553062359 40.00019910416006, -105.1076403102274 40.00019910286098, -105.1080413119849 40.00019910224839, -105.1092652724153 40.00020694295018, -105.1092663179089 40.00010213861572, -105.109237767345 39.99740700430097, -105.1144575601929 39.997370068387, -105.1147403634717 39.99736788392994, -105.1147423330233 39.99719108125619, -105.1147423325333 39.99684808060402, -105.1171730685706 39.99447212761837, -105.1172719606722 39.99440410043128, -105.1181990168995 39.99399786252945, -105.1181048759368 39.99385507456891, -105.1180370301155 39.99379692572312, -105.1179979121066 39.99377350597219, -105.1180669999796 39.99372004658021, -105.118216385493 39.99356413201255, -105.1183169872036 39.99344651479904, -105.1183824196342 39.99333575309119, -105.1184119771252 39.99326403416953, -105.1184374443334 39.99316489464574, -105.1184463683575 39.99308807454024, -105.1184579818192 39.99235779818542, -105.1185474045477 39.99235909652852, -105.118575976712 39.98710775588565, -105.1185703104926 39.98693549769058, -105.1173699922748 39.98694351032786, -105.1157364703514 39.98696958815421, -105.1137151610658 39.98698207706551, -105.1091016110865 39.98701312174199, -105.1078061103663 39.98700797037096, -105.1078040387233 39.98705792564128, -105.107799154696 39.98747298633479, -105.1078290710654 39.98773196213229, -105.1078389484039 39.98781407738738, -105.107897111169 39.98800204843946, -105.1079888729067 39.98818107397756, -105.1081121061065 39.9883489508796, -105.1082650458444 39.98850210553319, -105.1085589326976 39.98872189753453, -105.1088750448076 39.98892501821378, -105.1097618919571 39.98949189078966, -105.1093708360158 39.98984799412505, -105.1091749499771 39.99002604363177, -105.1088879912164 39.99027708136278, -105.1085750480045 39.99057799335898, -105.1083611633228 39.99078205987701, -105.1082500316964 39.99092992368484, -105.1081468301556 39.99112613023217, -105.1080530770463 39.99147912142979, -105.1078720733517 39.99217112403288, -105.1075879366984 39.99323200703812, -105.1074619818677 39.9937218730101, -105.1074268767083 39.99417800868869))</t>
+          <t>POLYGON ((-105.10742687670829 39.994178008688685, -105.10741791339828 39.99449505084446, -105.10742197938205 39.9948428831692, -105.10741184662622 39.99536306685848, -105.10740715544259 39.996301914434795, -105.10737100793472 39.99644289583818, -105.10729992518993 39.99657607111498, -105.10719501604149 39.99669513035742, -105.1070971302669 39.99677193739147, -105.10687513360152 39.996893068680194, -105.10656200768943 39.997033104171464, -105.1060899401119 39.99725303107669, -105.10602089004684 39.99728107134368, -105.1056769263536 39.997444882741334, -105.10558488067818 39.99749892268895, -105.10542209627931 39.99762601885258, -105.10532116632427 39.9977349323769, -105.10523584704421 39.997860096720345, -105.10517983927622 39.99797794895188, -105.10513790518138 39.99813098857716, -105.10510689778953 39.99830794929273, -105.10510499828705 39.99863599531165, -105.10511406780824 39.99941209919503, -105.10512594292797 40.000196996755285, -105.1053192989058 40.00019710578297, -105.10675530623585 40.00019910416006, -105.10764031022741 40.00019910286098, -105.10804131198492 40.000199102248395, -105.10926527241534 40.00020694295018, -105.10926631790886 40.00010213861572, -105.10923776734505 39.99740700430097, -105.11445756019292 39.997370068387, -105.11474036347168 39.99736788392994, -105.11474233302329 39.99719108125619, -105.1147423325333 39.99684808060402, -105.1171730685706 39.99447212761837, -105.11727196067218 39.99440410043128, -105.11819901689945 39.993997862529454, -105.11810487593678 39.99385507456891, -105.11803703011549 39.993796925723125, -105.1179979121066 39.99377350597219, -105.1180669999796 39.993720046580215, -105.11821638549301 39.99356413201255, -105.11831698720356 39.99344651479904, -105.11838241963416 39.99333575309119, -105.11841197712522 39.99326403416953, -105.11843744433341 39.993164894645744, -105.11844636835751 39.99308807454024, -105.11845798181916 39.99235779818542, -105.11854740454771 39.992359096528524, -105.11857597671197 39.987107755885646, -105.11857031049257 39.98693549769058, -105.11736999227477 39.98694351032786, -105.11573647035142 39.98696958815421, -105.11371516106578 39.98698207706551, -105.10910161108649 39.98701312174199, -105.10780611036631 39.98700797037096, -105.10780403872334 39.98705792564128, -105.10779915469604 39.98747298633479, -105.10782907106541 39.987731962132294, -105.10783894840387 39.987814077387384, -105.10789711116895 39.98800204843946, -105.10798887290672 39.98818107397756, -105.10811210610653 39.9883489508796, -105.10826504584439 39.98850210553319, -105.10855893269759 39.98872189753453, -105.10887504480758 39.988925018213784, -105.1097618919571 39.98949189078966, -105.10937083601584 39.98984799412505, -105.10917494997712 39.99002604363177, -105.1088879912164 39.990277081362784, -105.10857504800451 39.990577993358976, -105.10836116332281 39.99078205987701, -105.1082500316964 39.99092992368484, -105.10814683015563 39.99112613023217, -105.10805307704632 39.99147912142979, -105.10787207335174 39.99217112403288, -105.10758793669844 39.993232007038124, -105.1074619818677 39.9937218730101, -105.10742687670829 39.994178008688685))</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1680,7 +1684,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.098434505815 39.98698684960066, -105.098425233536 39.98869406335574, -105.0984987870677 39.98920331965681, -105.0985802450703 39.989575351782, -105.098713325453 39.98986177474411, -105.0990142408286 39.99036007002557, -105.1001392495099 39.99155507360361, -105.1012642592493 39.9927900777523, -105.1025611164681 39.99417822593036, -105.1026372271915 39.99417730301308, -105.1033309075516 39.99417002861044, -105.104424177499 39.99416609782019, -105.1046989999438 39.99416704044547, -105.1053089814462 39.99416611039474, -105.1067419641112 39.99417512506341, -105.107193848588 39.99417090134831, -105.1074268767083 39.99417800868869, -105.1074619818677 39.9937218730101, -105.1075879366984 39.99323200703812, -105.1078720733517 39.99217112403288, -105.1080530770463 39.99147912142979, -105.1081468301556 39.99112613023217, -105.1082500316964 39.99092992368484, -105.1083611633228 39.99078205987701, -105.1085750480045 39.99057799335898, -105.1088879912164 39.99027708136278, -105.1091749499771 39.99002604363177, -105.1093708360158 39.98984799412505, -105.1097618919571 39.98949189078966, -105.1088750448076 39.98892501821378, -105.1085589326976 39.98872189753453, -105.1082650458444 39.98850210553319, -105.1081121061065 39.9883489508796, -105.1079888729067 39.98818107397756, -105.107897111169 39.98800204843946, -105.1078389484039 39.98781407738738, -105.1078290710654 39.98773196213229, -105.107799154696 39.98747298633479, -105.1078040387233 39.98705792564128, -105.1078061103663 39.98700797037096, -105.1062505998226 39.98700731608795, -105.103439024915 39.98699303012703, -105.1014498374917 39.98698013024322, -105.0985320536637 39.98698941399471, -105.098434505815 39.98698684960066))</t>
+          <t>POLYGON ((-105.09843450581504 39.98698684960066, -105.09842523353602 39.98869406335574, -105.09849878706765 39.98920331965681, -105.09858024507025 39.989575351782, -105.098713325453 39.98986177474411, -105.09901424082855 39.99036007002557, -105.1001392495099 39.991555073603614, -105.10126425924932 39.9927900777523, -105.10256111646811 39.99417822593036, -105.10263722719145 39.99417730301308, -105.10333090755162 39.99417002861044, -105.10442417749903 39.99416609782019, -105.10469899994379 39.99416704044547, -105.10530898144616 39.99416611039474, -105.10674196411115 39.99417512506341, -105.107193848588 39.99417090134831, -105.10742687670829 39.994178008688685, -105.1074619818677 39.9937218730101, -105.10758793669844 39.993232007038124, -105.10787207335174 39.99217112403288, -105.10805307704632 39.99147912142979, -105.10814683015563 39.99112613023217, -105.1082500316964 39.99092992368484, -105.10836116332281 39.99078205987701, -105.10857504800451 39.990577993358976, -105.1088879912164 39.990277081362784, -105.10917494997712 39.99002604363177, -105.10937083601584 39.98984799412505, -105.1097618919571 39.98949189078966, -105.10887504480758 39.988925018213784, -105.10855893269759 39.98872189753453, -105.10826504584439 39.98850210553319, -105.10811210610653 39.9883489508796, -105.10798887290672 39.98818107397756, -105.10789711116895 39.98800204843946, -105.10783894840387 39.987814077387384, -105.10782907106541 39.987731962132294, -105.10779915469604 39.98747298633479, -105.10780403872334 39.98705792564128, -105.10780611036631 39.98700797037096, -105.10625059982263 39.987007316087954, -105.10343902491498 39.98699303012703, -105.10144983749169 39.98698013024322, -105.09853205366373 39.98698941399471, -105.09843450581504 39.98698684960066))</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1722,7 +1726,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0904550880611 39.9942759955102, -105.0904620045996 39.9952640236598, -105.0904500399845 39.99624594571998, -105.0904530895482 39.99722407790484, -105.0904520874176 39.99822305849236, -105.0904590209923 39.9987328701514, -105.0904668755554 39.9992080952137, -105.0904878248934 40.00023707619584, -105.0915058762835 40.00023300128316, -105.0923201075038 40.00022902009626, -105.0933631213459 40.00022913486146, -105.093588321395 40.00022915970511, -105.0951118364204 40.00022787647301, -105.09594211683 40.00022612187422, -105.0969290964702 40.0002249100984, -105.0982809135926 40.0002180976596, -105.098275854867 39.99968303789096, -105.098281055877 39.9994060635949, -105.098263058895 39.99918912838726, -105.0981563886066 39.99913843951978, -105.0981134865098 39.99733154522283, -105.0981183667658 39.99669115896096, -105.0970409247304 39.99668868803055, -105.0970504895929 39.99435746963948, -105.0970438108035 39.99426619863205, -105.0973530112771 39.99426405545619, -105.0975261479318 39.99425889487533, -105.0982650973134 39.99423786405374, -105.09917317366 39.99422592605629, -105.1003939180896 39.99421286835806, -105.101003853483 39.99421992275619, -105.1014679323252 39.99420587984281, -105.1020419939718 39.99418288121557, -105.102476886653 39.99417924779587, -105.1025611164681 39.99417822593036, -105.1012642592493 39.9927900777523, -105.1001392495099 39.99155507360361, -105.0990142408286 39.99036007002557, -105.098713325453 39.98986177474411, -105.0985802450703 39.989575351782, -105.0984987870677 39.98920331965681, -105.098425233536 39.98869406335574, -105.098434505815 39.98698684960066, -105.098331016714 39.98698412932367, -105.0963929897977 39.98694990812138, -105.0943223346905 39.98694808340338, -105.0927489637514 39.9869329743509, -105.0905288265568 39.98692812962798, -105.0905299979112 39.98697095931441, -105.0905369086479 39.98718703259705, -105.0905101352913 39.98849613268706, -105.0905070331811 39.98931007940942, -105.0904842921616 39.99003529887713, -105.0904758608932 39.99075697368887, -105.0904801281333 39.99135407366492, -105.0904901335344 39.99230313157403, -105.0904632968407 39.99338437814676, -105.0904550880611 39.9942759955102))</t>
+          <t>POLYGON ((-105.09045508806108 39.9942759955102, -105.09046200459964 39.9952640236598, -105.09045003998446 39.996245945719984, -105.09045308954823 39.99722407790484, -105.09045208741762 39.99822305849236, -105.09045902099231 39.9987328701514, -105.09046687555544 39.999208095213696, -105.0904878248934 40.000237076195845, -105.09150587628349 40.00023300128316, -105.09232010750375 40.000229020096256, -105.09336312134589 40.00022913486146, -105.09358832139499 40.00022915970511, -105.09511183642041 40.000227876473005, -105.09594211683003 40.00022612187422, -105.09692909647025 40.0002249100984, -105.09828091359265 40.0002180976596, -105.09827585486701 39.99968303789096, -105.09828105587698 39.999406063594904, -105.09826305889496 39.99918912838726, -105.09815638860663 39.999138439519776, -105.09811348650983 39.997331545222835, -105.09811836676585 39.99669115896096, -105.09704092473036 39.99668868803055, -105.09705048959292 39.99435746963948, -105.09704381080347 39.994266198632054, -105.09735301127714 39.99426405545619, -105.09752614793179 39.99425889487533, -105.09826509731344 39.99423786405374, -105.09917317365996 39.99422592605629, -105.10039391808957 39.99421286835806, -105.10100385348302 39.994219922756194, -105.10146793232522 39.99420587984281, -105.10204199397182 39.99418288121557, -105.10247688665297 39.99417924779587, -105.10256111646811 39.99417822593036, -105.10126425924932 39.9927900777523, -105.1001392495099 39.991555073603614, -105.09901424082855 39.99036007002557, -105.098713325453 39.98986177474411, -105.09858024507025 39.989575351782, -105.09849878706765 39.98920331965681, -105.09842523353602 39.98869406335574, -105.09843450581504 39.98698684960066, -105.09833101671397 39.98698412932367, -105.09639298979774 39.98694990812138, -105.09432233469055 39.986948083403384, -105.09274896375145 39.9869329743509, -105.09052882655683 39.98692812962798, -105.0905299979112 39.986970959314405, -105.09053690864789 39.98718703259705, -105.0905101352913 39.98849613268706, -105.09050703318113 39.98931007940942, -105.09048429216159 39.99003529887713, -105.09047586089318 39.99075697368887, -105.09048012813331 39.99135407366492, -105.09049013353439 39.99230313157403, -105.09046329684065 39.993384378146764, -105.09045508806108 39.9942759955102))</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1764,7 +1768,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0811001375908 39.99411006473294, -105.0813647840702 39.99412394688741, -105.0816370503526 39.99415099672483, -105.0834328869529 39.99424013055927, -105.0842338934564 39.99428612129016, -105.0855008770419 39.99435903992745, -105.0865630752016 39.99441803287974, -105.0870830185183 39.99443307291057, -105.0876038274055 39.99442313297462, -105.0880441061664 39.99439094036055, -105.0890169501104 39.99429311425293, -105.089320019476 39.99428595858863, -105.0904550880611 39.9942759955102, -105.0904632968407 39.99338437814676, -105.0904901335344 39.99230313157403, -105.0904801281333 39.99135407366492, -105.0904758608932 39.99075697368887, -105.0904842921616 39.99003529887713, -105.0905070331811 39.98931007940942, -105.0905101352913 39.98849613268706, -105.0905369086479 39.98718703259705, -105.0905299979112 39.98697095931441, -105.0905288265568 39.98692812962798, -105.0858280409819 39.98687167128099, -105.0823330669949 39.9868562577193, -105.0823341689822 39.98686196199735, -105.0812159749153 39.98681471489445, -105.0806001148401 39.98680553363357, -105.0800022714316 39.98680162144831, -105.0795759197414 39.98679312590777, -105.0782995407455 39.98677634180367, -105.0783111951955 39.98689553384761, -105.0783014433929 39.98772121019498, -105.0782988357461 39.98814299210392, -105.078291626234 39.98855760861304, -105.0782797903372 39.98896863345706, -105.0782773372099 39.98936539461084, -105.0782701483692 39.98977643642316, -105.0782662806757 39.99040196122129, -105.0795302550174 39.99041015292351, -105.0801900463319 39.99042685546382, -105.0806826117772 39.99043222283221, -105.0810032135734 39.99044053704765, -105.0811310648665 39.99044100165043, -105.0811314706972 39.99054232569287, -105.0811289517245 39.99133612493978, -105.0811158889356 39.991952104357, -105.0811151734891 39.99328902385216, -105.0811160663361 39.99384109073499, -105.0811001375908 39.99411006473294))</t>
+          <t>POLYGON ((-105.0811001375908 39.994110064732936, -105.08136478407019 39.99412394688741, -105.08163705035263 39.994150996724834, -105.08343288695295 39.99424013055927, -105.08423389345637 39.99428612129016, -105.08550087704187 39.99435903992745, -105.0865630752016 39.994418032879736, -105.08708301851829 39.99443307291057, -105.0876038274055 39.99442313297462, -105.08804410616644 39.994390940360546, -105.08901695011045 39.994293114252926, -105.08932001947596 39.994285958588634, -105.09045508806108 39.9942759955102, -105.09046329684065 39.993384378146764, -105.09049013353439 39.99230313157403, -105.09048012813331 39.99135407366492, -105.09047586089318 39.99075697368887, -105.09048429216159 39.99003529887713, -105.09050703318113 39.98931007940942, -105.0905101352913 39.98849613268706, -105.09053690864789 39.98718703259705, -105.0905299979112 39.986970959314405, -105.09052882655683 39.98692812962798, -105.08582804098191 39.986871671280994, -105.08233306699488 39.986856257719296, -105.08233416898223 39.98686196199735, -105.0812159749153 39.98681471489445, -105.08060011484007 39.98680553363357, -105.08000227143157 39.986801621448315, -105.07957591974144 39.986793125907774, -105.07829954074549 39.98677634180367, -105.0783111951955 39.98689553384761, -105.07830144339289 39.987721210194984, -105.07829883574611 39.98814299210392, -105.07829162623398 39.988557608613036, -105.07827979033719 39.988968633457056, -105.07827733720985 39.98936539461084, -105.07827014836919 39.989776436423156, -105.07826628067572 39.990401961221295, -105.07953025501742 39.99041015292351, -105.08019004633188 39.99042685546382, -105.08068261177723 39.99043222283221, -105.08100321357342 39.99044053704765, -105.08113106486645 39.99044100165043, -105.08113147069722 39.99054232569287, -105.08112895172451 39.99133612493978, -105.08111588893556 39.991952104357, -105.08111517348912 39.993289023852164, -105.08111606633608 39.99384109073499, -105.0811001375908 39.994110064732936))</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1806,7 +1810,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0782446319749 39.99395584100868, -105.0782568099038 39.99398431131635, -105.0783884189876 39.99439614161719, -105.0784401529231 39.99460865978737, -105.0785002577784 39.99507371599493, -105.0785556619938 39.99540533108009, -105.0786034096311 39.99581916647913, -105.0786936977909 39.99631169581173, -105.0788908713218 39.9969457823338, -105.0790215348869 39.99723800868806, -105.079128532958 39.9974821604017, -105.0792963350588 39.99788470248784, -105.0794746962881 39.99831402703181, -105.0796419087898 39.99870953135873, -105.0798632216472 39.99921029820563, -105.0799004811676 39.99937982296505, -105.0798767032428 40.00013093747118, -105.0798843206321 40.00022951007099, -105.0799145302103 40.00022934273726, -105.0826975562436 40.00021386648334, -105.0827135121339 40.00021392423083, -105.0828379787892 40.00021434670388, -105.0839528968833 40.00021203449376, -105.0842138295373 40.000211876937, -105.0854960002848 40.00021210184526, -105.0867839089919 40.00020793964026, -105.0880621232142 40.00021306285356, -105.0893631222864 40.0002281350852, -105.0904878248934 40.00023707619584, -105.0904668755554 39.9992080952137, -105.0904590209923 39.9987328701514, -105.0904520874176 39.99822305849236, -105.0904530895482 39.99722407790484, -105.0904500399845 39.99624594571998, -105.0904620045996 39.9952640236598, -105.0904550880611 39.9942759955102, -105.089320019476 39.99428595858863, -105.0890169501104 39.99429311425293, -105.0880441061664 39.99439094036055, -105.0876038274055 39.99442313297462, -105.0870830185183 39.99443307291057, -105.0865630752016 39.99441803287974, -105.0855008770419 39.99435903992745, -105.0842338934564 39.99428612129016, -105.0834328869529 39.99424013055927, -105.0816370503526 39.99415099672483, -105.0813647840702 39.99412394688741, -105.0811001375908 39.99411006473294, -105.0804078235278 39.99403397578976, -105.0797780687563 39.99400011124025, -105.079199983667 39.99397988502232, -105.0784780588218 39.99396002894687, -105.0784748461619 39.99395994064453, -105.0783021140238 39.99395711315582, -105.0782446319749 39.99395584100868))</t>
+          <t>POLYGON ((-105.07824463197487 39.993955841008685, -105.07825680990382 39.99398431131635, -105.07838841898756 39.99439614161719, -105.07844015292308 39.99460865978737, -105.07850025777842 39.99507371599493, -105.07855566199378 39.995405331080086, -105.07860340963109 39.99581916647913, -105.07869369779085 39.996311695811734, -105.07889087132179 39.996945782333796, -105.07902153488686 39.997238008688065, -105.07912853295802 39.9974821604017, -105.07929633505876 39.99788470248784, -105.07947469628807 39.99831402703181, -105.07964190878982 39.99870953135873, -105.07986322164723 39.99921029820563, -105.07990048116756 39.99937982296505, -105.07987670324276 40.00013093747118, -105.07988432063206 40.00022951007099, -105.07991453021035 40.00022934273726, -105.08269755624364 40.000213866483335, -105.0827135121339 40.00021392423083, -105.0828379787892 40.000214346703885, -105.08395289688328 40.000212034493764, -105.08421382953733 40.000211876937, -105.08549600028483 40.00021210184526, -105.08678390899193 40.000207939640255, -105.08806212321424 40.00021306285356, -105.08936312228641 40.0002281350852, -105.0904878248934 40.000237076195845, -105.09046687555544 39.999208095213696, -105.09045902099231 39.9987328701514, -105.09045208741762 39.99822305849236, -105.09045308954823 39.99722407790484, -105.09045003998446 39.996245945719984, -105.09046200459964 39.9952640236598, -105.09045508806108 39.9942759955102, -105.08932001947596 39.994285958588634, -105.08901695011045 39.994293114252926, -105.08804410616644 39.994390940360546, -105.0876038274055 39.99442313297462, -105.08708301851829 39.99443307291057, -105.0865630752016 39.994418032879736, -105.08550087704187 39.99435903992745, -105.08423389345637 39.99428612129016, -105.08343288695295 39.99424013055927, -105.08163705035263 39.994150996724834, -105.08136478407019 39.99412394688741, -105.0811001375908 39.994110064732936, -105.08040782352784 39.99403397578976, -105.07977806875631 39.994000111240254, -105.079199983667 39.99397988502232, -105.07847805882183 39.993960028946866, -105.07847484616191 39.99395994064453, -105.07830211402381 39.993957113155815, -105.07824463197487 39.993955841008685))</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1848,10 +1852,14 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0744840001105 40.00754717649394, -105.0744840004529 40.00754899853014, -105.0744840014802 40.00754920928831, -105.0744959994806 40.00913899920532, -105.0744850002892 40.01025499937742, -105.0744939996588 40.01117199953493, -105.0744939994117 40.01312199935634, -105.0744879997328 40.01486699832747, -105.0750330000281 40.01486599880874, -105.0776729999707 40.01487699919728, -105.0778080003735 40.01487099884424, -105.0780740000252 40.01483699883885, -105.0785220001667 40.0147389989032, -105.0787519998548 40.01470499815898, -105.0790640003765 40.0146869983785, -105.0798880004663 40.01470099918091, -105.0827519996697 40.0147379995101, -105.083827279062 40.01474776707985, -105.0838636006166 40.01474809629242, -105.0838678605798 40.01474813508104, -105.0839630017275 40.01474899892437, -105.084275999784 40.01475199921421, -105.084343261355 40.01475098794224, -105.0844090000323 40.01474999906352, -105.0863749999974 40.01472599885857, -105.0865649991523 40.01472399889266, -105.0905288819658 40.01468199225995, -105.0905289991035 40.0146819917752, -105.0905557415763 40.01468189398261, -105.0924409249201 40.01467444931598, -105.0932924249816 40.01467107691634, -105.0933139431195 40.01248606893635, -105.0933140887827 40.01198287150529, -105.0933129151652 40.01122189458499, -105.0933126135376 40.01105094940586, -105.0933099689575 40.0108779091348, -105.0933099762549 40.01069699925051, -105.0933091657515 40.01035411921701, -105.093309443264 40.01025378320853, -105.0933088726542 40.01016387563778, -105.0933051569746 40.00994891221197, -105.0933161589406 40.00948089214382, -105.0932939057928 40.00908193347691, -105.0932830467683 40.00826903791486, -105.0932839692943 40.00739606304989, -105.0932938828004 40.00699090412751, -105.0932959870564 40.00538111757357, -105.0932939383563 40.00512608058885, -105.0933018889842 40.00385287724529, -105.0933040871278 40.00360389412218, -105.093300989612 40.00340513019348, -105.0933119971037 40.00293601104079, -105.0933390080789 40.00214126804693, -105.0931508052644 40.00213842182832, -105.0903574852876 40.00212367809764, -105.0882204212901 40.00211118790698, -105.08822934821 40.00271429971438, -105.0858460122409 40.00271024910187, -105.0840693395224 40.00271148340227, -105.0839257284982 40.00271103102219, -105.0838931675961 40.00576387712228, -105.0838750855414 40.00747700408438, -105.0834530015145 40.00748030588483, -105.0785867684244 40.00751825042298, -105.0751311968962 40.00754507131038, -105.0744840001105 40.00754717649394))</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr"/>
+          <t>POLYGON ((-105.07448400011053 40.007547176493944, -105.07448400045293 40.00754899853014, -105.07448400148016 40.007549209288314, -105.07449599948062 40.00913899920532, -105.07448500028922 40.01025499937742, -105.07449399965881 40.01117199953493, -105.07449399941167 40.01312199935634, -105.07448799973284 40.01486699832747, -105.07503300002809 40.01486599880874, -105.07767299997074 40.01487699919728, -105.07780800037347 40.01487099884424, -105.07807400002524 40.014836998838845, -105.07852200016674 40.0147389989032, -105.07875199985482 40.014704998158976, -105.07906400037653 40.0146869983785, -105.07988800046628 40.01470099918091, -105.08275199966967 40.014737999510096, -105.08382727906202 40.014747767079854, -105.08386360061655 40.01474809629242, -105.08386786057979 40.014748135081035, -105.08396300172747 40.01474899892437, -105.08427599978398 40.014751999214205, -105.08434326135499 40.014750987942236, -105.08440900003225 40.01474999906352, -105.0863749999974 40.014725998858566, -105.0865649991523 40.01472399889266, -105.09052888196575 40.01468199225995, -105.09052899910351 40.0146819917752, -105.09055574157632 40.01468189398261, -105.09244092492013 40.01467444931598, -105.09329242498157 40.01467107691634, -105.09331394311954 40.01248606893635, -105.09331408878269 40.01198287150529, -105.0933129151652 40.01122189458499, -105.09331261353765 40.01105094940586, -105.09330996895748 40.0108779091348, -105.09330997625493 40.010696999250506, -105.0933091657515 40.01035411921701, -105.09330944326403 40.01025378320853, -105.09330887265418 40.01016387563778, -105.09330515697457 40.009948912211975, -105.09331615894057 40.00948089214382, -105.09329390579282 40.009081933476914, -105.0932830467683 40.008269037914864, -105.0932839692943 40.00739606304989, -105.09329388280035 40.00699090412751, -105.09329598705642 40.00538111757357, -105.09329393835633 40.00512608058885, -105.09330188898419 40.003852877245286, -105.09330408712778 40.00360389412218, -105.09330098961199 40.00340513019348, -105.09331199710367 40.00293601104079, -105.0933390080789 40.00214126804693, -105.0931508052644 40.00213842182832, -105.0903574852876 40.00212367809764, -105.08822042129007 40.002111187906976, -105.08822934821 40.00271429971438, -105.08584601224086 40.00271024910187, -105.08406933952236 40.002711483402265, -105.08392572849819 40.002711031022194, -105.0838931675961 40.00576387712228, -105.08387508554138 40.00747700408438, -105.08345300151446 40.007480305884826, -105.07858676842436 40.00751825042298, -105.0751311968962 40.00754507131038, -105.07448400011053 40.007547176493944))</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Centaurus HS</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1886,7 +1894,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0968210984977 40.01464899904126, -105.0968081659261 40.01339944902477, -105.0977161660674 40.01340144824596, -105.097693165477 40.01108044794793, -105.1029281665798 40.01109144817353, -105.1029321674492 40.01426744896852, -105.1029350211734 40.01499712229778, -105.1032709245142 40.01491293018051, -105.1034218352742 40.01487089764663, -105.1037299656432 40.0148068969059, -105.1039339914919 40.01477904602595, -105.104085101401 40.01476391866188, -105.1044218596395 40.01474997564399, -105.1045118307443 40.01475000951929, -105.1048549288133 40.01475091000491, -105.1059210138599 40.01475098945919, -105.1074929904923 40.01475388076332, -105.10756828865 40.01475361643449, -105.1075681349589 40.01462218923842, -105.1075026571879 40.01077491615019, -105.1029187339748 40.01076626095388, -105.1029199096802 40.01038596654633, -105.1029211524815 40.00986602708125, -105.1029131134702 40.00830397399917, -105.1029119999167 40.00745295413691, -105.102904985609 40.00651187053455, -105.102902070423 40.00609294163367, -105.1028968524552 40.00416907780282, -105.1028969979259 40.00414409672911, -105.1028968882406 40.00397910915716, -105.1028969891118 40.00383910388316, -105.1028931003117 40.00346491715381, -105.1028828890649 40.00227593018461, -105.1028839584027 40.00160198420788, -105.1028850353084 40.00123303111563, -105.1028662911329 40.00021572247173, -105.1026611629879 40.00020198051732, -105.1024880132352 40.00020687411115, -105.1017151521594 40.0002171089322, -105.1011147656632 40.00022834788566, -105.1005860007567 40.00024244015062, -105.1004571078078 40.00024213047868, -105.0998539486272 40.00022686216714, -105.0982809135926 40.0002180976596, -105.0969290964702 40.0002249100984, -105.09594211683 40.00022612187422, -105.0951118364204 40.00022787647301, -105.093588321395 40.00022915970511, -105.0933631213459 40.00022913486146, -105.0923201075038 40.00022902009626, -105.0915058762835 40.00023300128316, -105.0904878248934 40.00023707619584, -105.0893631222864 40.0002281350852, -105.0880621232142 40.00021306285356, -105.0867839089919 40.00020793964026, -105.0854960002848 40.00021210184526, -105.0842138295373 40.000211876937, -105.0839528968833 40.00021203449376, -105.0828379787892 40.00021434670388, -105.0827135121339 40.00021392423083, -105.0826975562436 40.00021386648334, -105.0799145302103 40.00022934273726, -105.0798843206321 40.00022951007099, -105.0798767032428 40.00013093747118, -105.0799004811676 39.99937982296505, -105.0798632216472 39.99921029820563, -105.0796419087898 39.99870953135873, -105.0794746962881 39.99831402703181, -105.0792963350588 39.99788470248784, -105.079128532958 39.9974821604017, -105.0790215348869 39.99723800868806, -105.0788908713218 39.9969457823338, -105.0786936977909 39.99631169581173, -105.0786034096311 39.99581916647913, -105.0785556619938 39.99540533108009, -105.0785002577784 39.99507371599493, -105.0784401529231 39.99460865978737, -105.0783884189876 39.99439614161719, -105.0782568099038 39.99398431131635, -105.0782446319749 39.99395584100868, -105.0767427244234 39.99392258574381, -105.0767412374697 39.99392255236432, -105.0758477384717 39.99390275861118, -105.0745450086098 39.99387001187085, -105.0718370192644 39.99383006495202, -105.0718799993343 39.99397799875175, -105.0719159993805 39.99409699899344, -105.0720359997661 39.99436699888737, -105.0720660003175 39.99442399870839, -105.0721960003037 39.99463699847043, -105.0723899995719 39.99489399859032, -105.0726170002045 39.99513499887867, -105.0733690015316 39.9957939984819, -105.0736860016148 39.9960719991295, -105.0739000001836 39.99630199852007, -105.0740829997001 39.99654599904907, -105.0742349999409 39.99679799885913, -105.0743510006399 39.99705999889498, -105.0744300017446 39.99733099854296, -105.0744720000795 39.99760599830033, -105.0744799999501 39.99791599833095, -105.0744790001136 39.99814399960752, -105.0744769994021 40.00005999822572, -105.0744770000605 40.00022899907422, -105.074477999321 40.00046599897158, -105.0744799997885 40.0007489983894, -105.0744820000614 40.00248399837474, -105.074475000093 40.00379499887224, -105.0744809997915 40.00389299933561, -105.0744759999931 40.00412799915949, -105.0744768152457 40.00418672611349, -105.0744770006211 40.00419999892615, -105.074476815134 40.00421095567354, -105.0744759988608 40.00425899837897, -105.0744770000379 40.00485699808893, -105.0744799998352 40.00548099818882, -105.0744800693377 40.00549913954058, -105.0744829989317 40.00626690809695, -105.0744829995353 40.0062669990658, -105.0744834354184 40.00666768629058, -105.0744840001084 40.00718699899353, -105.0744840001105 40.00754717649394, -105.0751311968962 40.00754507131038, -105.0785867684244 40.00751825042298, -105.0834530015145 40.00748030588483, -105.0838750855414 40.00747700408438, -105.0838931675961 40.00576387712228, -105.0839257284982 40.00271103102219, -105.0840693395224 40.00271148340227, -105.0858460122409 40.00271024910187, -105.08822934821 40.00271429971438, -105.0882204212901 40.00211118790698, -105.0903574852876 40.00212367809764, -105.0931508052644 40.00213842182832, -105.0933390080789 40.00214126804693, -105.0933119971037 40.00293601104079, -105.093300989612 40.00340513019348, -105.0933040871278 40.00360389412218, -105.0933018889842 40.00385287724529, -105.0932939383563 40.00512608058885, -105.0932959870564 40.00538111757357, -105.0932938828004 40.00699090412751, -105.0932839692943 40.00739606304989, -105.0932830467683 40.00826903791486, -105.0932939057928 40.00908193347691, -105.0933161589406 40.00948089214382, -105.0933051569746 40.00994891221197, -105.0933088726542 40.01016387563778, -105.093309443264 40.01025378320853, -105.0933091657515 40.01035411921701, -105.0933099762549 40.01069699925051, -105.0933099689575 40.0108779091348, -105.0933126135376 40.01105094940586, -105.0933129151652 40.01122189458499, -105.0933140887827 40.01198287150529, -105.0933139431195 40.01248606893635, -105.0932924249816 40.01467107691634, -105.0933119998438 40.01467099914053, -105.0940020010792 40.01467199918716, -105.0968210984977 40.01464899904126))</t>
+          <t>POLYGON ((-105.0968210984977 40.014648999041256, -105.09680816592609 40.01339944902477, -105.09771616606744 40.013401448245965, -105.09769316547703 40.01108044794793, -105.10292816657982 40.01109144817353, -105.10293216744923 40.01426744896852, -105.1029350211734 40.01499712229778, -105.10327092451425 40.01491293018051, -105.1034218352742 40.01487089764663, -105.10372996564324 40.0148068969059, -105.10393399149194 40.01477904602595, -105.10408510140103 40.01476391866188, -105.10442185963949 40.014749975643994, -105.10451183074434 40.01475000951929, -105.10485492881331 40.014750910004906, -105.10592101385987 40.014750989459195, -105.10749299049229 40.014753880763315, -105.10756828865004 40.01475361643449, -105.10756813495888 40.014622189238416, -105.1075026571879 40.01077491615019, -105.10291873397485 40.01076626095388, -105.10291990968022 40.01038596654633, -105.10292115248147 40.00986602708125, -105.10291311347017 40.00830397399917, -105.10291199991674 40.00745295413691, -105.10290498560897 40.006511870534545, -105.10290207042296 40.00609294163367, -105.10289685245523 40.00416907780282, -105.10289699792587 40.004144096729114, -105.1028968882406 40.003979109157164, -105.1028969891118 40.00383910388316, -105.10289310031172 40.00346491715381, -105.1028828890649 40.00227593018461, -105.10288395840271 40.00160198420788, -105.10288503530845 40.00123303111563, -105.10286629113293 40.00021572247173, -105.10266116298794 40.000201980517325, -105.10248801323519 40.00020687411115, -105.10171515215941 40.000217108932205, -105.10111476566317 40.00022834788566, -105.10058600075669 40.00024244015062, -105.10045710780777 40.000242130478675, -105.09985394862723 40.00022686216714, -105.09828091359265 40.0002180976596, -105.09692909647025 40.0002249100984, -105.09594211683003 40.00022612187422, -105.09511183642041 40.000227876473005, -105.09358832139499 40.00022915970511, -105.09336312134589 40.00022913486146, -105.09232010750375 40.000229020096256, -105.09150587628349 40.00023300128316, -105.0904878248934 40.000237076195845, -105.08936312228641 40.0002281350852, -105.08806212321424 40.00021306285356, -105.08678390899193 40.000207939640255, -105.08549600028483 40.00021210184526, -105.08421382953733 40.000211876937, -105.08395289688328 40.000212034493764, -105.0828379787892 40.000214346703885, -105.0827135121339 40.00021392423083, -105.08269755624364 40.000213866483335, -105.07991453021035 40.00022934273726, -105.07988432063206 40.00022951007099, -105.07987670324276 40.00013093747118, -105.07990048116756 39.99937982296505, -105.07986322164723 39.99921029820563, -105.07964190878982 39.99870953135873, -105.07947469628807 39.99831402703181, -105.07929633505876 39.99788470248784, -105.07912853295802 39.9974821604017, -105.07902153488686 39.997238008688065, -105.07889087132179 39.996945782333796, -105.07869369779085 39.996311695811734, -105.07860340963109 39.99581916647913, -105.07855566199378 39.995405331080086, -105.07850025777842 39.99507371599493, -105.07844015292308 39.99460865978737, -105.07838841898756 39.99439614161719, -105.07825680990382 39.99398431131635, -105.07824463197487 39.993955841008685, -105.07674272442344 39.99392258574381, -105.07674123746973 39.993922552364324, -105.07584773847165 39.993902758611185, -105.07454500860979 39.993870011870854, -105.07183701926438 39.99383006495202, -105.07187999933433 39.993977998751745, -105.07191599938052 39.99409699899344, -105.07203599976614 39.99436699888737, -105.07206600031748 39.99442399870839, -105.07219600030372 39.994636998470426, -105.07238999957193 39.99489399859032, -105.07261700020454 39.99513499887867, -105.0733690015316 39.9957939984819, -105.07368600161479 39.9960719991295, -105.07390000018356 39.996301998520075, -105.07408299970014 39.99654599904907, -105.07423499994091 39.99679799885913, -105.07435100063994 39.997059998894976, -105.07443000174464 39.99733099854296, -105.0744720000795 39.99760599830033, -105.07447999995014 39.99791599833095, -105.07447900011357 39.99814399960752, -105.0744769994021 40.00005999822572, -105.0744770000605 40.000228999074224, -105.07447799932103 40.000465998971585, -105.0744799997885 40.0007489983894, -105.07448200006138 40.002483998374736, -105.07447500009303 40.003794998872245, -105.07448099979149 40.00389299933561, -105.07447599999306 40.004127999159486, -105.07447681524569 40.00418672611349, -105.07447700062106 40.004199998926154, -105.07447681513396 40.00421095567354, -105.07447599886085 40.00425899837897, -105.07447700003787 40.004856998088925, -105.07447999983516 40.005480998188816, -105.07448006933765 40.005499139540575, -105.0744829989317 40.00626690809695, -105.07448299953529 40.0062669990658, -105.07448343541839 40.00666768629058, -105.07448400010841 40.00718699899353, -105.07448400011053 40.007547176493944, -105.0751311968962 40.00754507131038, -105.07858676842436 40.00751825042298, -105.08345300151446 40.007480305884826, -105.08387508554138 40.00747700408438, -105.0838931675961 40.00576387712228, -105.08392572849819 40.002711031022194, -105.08406933952236 40.002711483402265, -105.08584601224086 40.00271024910187, -105.08822934821 40.00271429971438, -105.08822042129007 40.002111187906976, -105.0903574852876 40.00212367809764, -105.0931508052644 40.00213842182832, -105.0933390080789 40.00214126804693, -105.09331199710367 40.00293601104079, -105.09330098961199 40.00340513019348, -105.09330408712778 40.00360389412218, -105.09330188898419 40.003852877245286, -105.09329393835633 40.00512608058885, -105.09329598705642 40.00538111757357, -105.09329388280035 40.00699090412751, -105.0932839692943 40.00739606304989, -105.0932830467683 40.008269037914864, -105.09329390579282 40.009081933476914, -105.09331615894057 40.00948089214382, -105.09330515697457 40.009948912211975, -105.09330887265418 40.01016387563778, -105.09330944326403 40.01025378320853, -105.0933091657515 40.01035411921701, -105.09330997625493 40.010696999250506, -105.09330996895748 40.0108779091348, -105.09331261353765 40.01105094940586, -105.0933129151652 40.01122189458499, -105.09331408878269 40.01198287150529, -105.09331394311954 40.01248606893635, -105.09329242498157 40.01467107691634, -105.09331199984379 40.01467099914053, -105.0940020010792 40.01467199918716, -105.0968210984977 40.014648999041256))</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1928,7 +1936,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0982809135926 40.0002180976596, -105.0998539486272 40.00022686216714, -105.1004571078078 40.00024213047868, -105.1005860007567 40.00024244015062, -105.1011147656632 40.00022834788566, -105.1017151521594 40.0002171089322, -105.1024880132352 40.00020687411115, -105.1026611629879 40.00020198051732, -105.1028662911329 40.00021572247173, -105.103607154678 40.0001898632859, -105.1040901046762 40.00019097321382, -105.105125942928 40.00019699675529, -105.1051140678082 39.99941209919503, -105.105104998287 39.99863599531165, -105.1051068977895 39.99830794929273, -105.1051379051814 39.99813098857716, -105.1051798392762 39.99797794895188, -105.1052358470442 39.99786009672034, -105.1053211663243 39.9977349323769, -105.1054220962793 39.99762601885258, -105.1055848806782 39.99749892268895, -105.1056769263536 39.99744488274133, -105.1060208900468 39.99728107134368, -105.1060899401119 39.99725303107669, -105.1065620076894 39.99703310417146, -105.1068751336015 39.99689306868019, -105.1070971302669 39.99677193739147, -105.1071950160415 39.99669513035742, -105.1072999251899 39.99657607111498, -105.1073710079347 39.99644289583818, -105.1074071554426 39.9963019144348, -105.1074118466262 39.99536306685848, -105.1074219793821 39.9948428831692, -105.1074179133983 39.99449505084446, -105.1074268767083 39.99417800868869, -105.107193848588 39.99417090134831, -105.1067419641112 39.99417512506341, -105.1053089814462 39.99416611039474, -105.1046989999438 39.99416704044547, -105.104424177499 39.99416609782019, -105.1033309075516 39.99417002861044, -105.1026372271915 39.99417730301308, -105.1025611164681 39.99417822593036, -105.102476886653 39.99417924779587, -105.1020419939718 39.99418288121557, -105.1014679323252 39.99420587984281, -105.101003853483 39.99421992275619, -105.1003939180896 39.99421286835806, -105.09917317366 39.99422592605629, -105.0982650973134 39.99423786405374, -105.0975261479318 39.99425889487533, -105.0973530112771 39.99426405545619, -105.0970438108035 39.99426619863205, -105.0970504895929 39.99435746963948, -105.0970409247304 39.99668868803055, -105.0981183667658 39.99669115896096, -105.0981134865098 39.99733154522283, -105.0981563886066 39.99913843951978, -105.098263058895 39.99918912838726, -105.098281055877 39.9994060635949, -105.098275854867 39.99968303789096, -105.0982809135926 40.0002180976596))</t>
+          <t>POLYGON ((-105.09828091359265 40.0002180976596, -105.09985394862723 40.00022686216714, -105.10045710780777 40.000242130478675, -105.10058600075669 40.00024244015062, -105.10111476566317 40.00022834788566, -105.10171515215941 40.000217108932205, -105.10248801323519 40.00020687411115, -105.10266116298794 40.000201980517325, -105.10286629113293 40.00021572247173, -105.10360715467802 40.0001898632859, -105.10409010467622 40.00019097321382, -105.10512594292797 40.000196996755285, -105.10511406780824 39.99941209919503, -105.10510499828705 39.99863599531165, -105.10510689778953 39.99830794929273, -105.10513790518138 39.99813098857716, -105.10517983927622 39.99797794895188, -105.10523584704421 39.997860096720345, -105.10532116632427 39.9977349323769, -105.10542209627931 39.99762601885258, -105.10558488067818 39.99749892268895, -105.1056769263536 39.997444882741334, -105.10602089004684 39.99728107134368, -105.1060899401119 39.99725303107669, -105.10656200768943 39.997033104171464, -105.10687513360152 39.996893068680194, -105.1070971302669 39.99677193739147, -105.10719501604149 39.99669513035742, -105.10729992518993 39.99657607111498, -105.10737100793472 39.99644289583818, -105.10740715544259 39.996301914434795, -105.10741184662622 39.99536306685848, -105.10742197938205 39.9948428831692, -105.10741791339828 39.99449505084446, -105.10742687670829 39.994178008688685, -105.107193848588 39.99417090134831, -105.10674196411115 39.99417512506341, -105.10530898144616 39.99416611039474, -105.10469899994379 39.99416704044547, -105.10442417749903 39.99416609782019, -105.10333090755162 39.99417002861044, -105.10263722719145 39.99417730301308, -105.10256111646811 39.99417822593036, -105.10247688665297 39.99417924779587, -105.10204199397182 39.99418288121557, -105.10146793232522 39.99420587984281, -105.10100385348302 39.994219922756194, -105.10039391808957 39.99421286835806, -105.09917317365996 39.99422592605629, -105.09826509731344 39.99423786405374, -105.09752614793179 39.99425889487533, -105.09735301127714 39.99426405545619, -105.09704381080347 39.994266198632054, -105.09705048959292 39.99435746963948, -105.09704092473036 39.99668868803055, -105.09811836676585 39.99669115896096, -105.09811348650983 39.997331545222835, -105.09815638860663 39.999138439519776, -105.09826305889496 39.99918912838726, -105.09828105587698 39.999406063594904, -105.09827585486701 39.99968303789096, -105.09828091359265 40.0002180976596))</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1970,7 +1978,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1028662911329 40.00021572247173, -105.1028850353084 40.00123303111563, -105.1028839584027 40.00160198420788, -105.1028828890649 40.00227593018461, -105.1028931003117 40.00346491715381, -105.1028969891118 40.00383910388316, -105.1028968882406 40.00397910915716, -105.1028969979259 40.00414409672911, -105.1028968524552 40.00416907780282, -105.102902070423 40.00609294163367, -105.102904985609 40.00651187053455, -105.1029119999167 40.00745295413691, -105.1029131134702 40.00830397399917, -105.1029211524815 40.00986602708125, -105.1029199096802 40.01038596654633, -105.1029187339748 40.01076626095388, -105.1075026571879 40.01077491615019, -105.1075681349589 40.01462218923842, -105.10756828865 40.01475361643449, -105.1080486438543 40.01475192657379, -105.1105560664339 40.01473943407785, -105.1105601717934 40.01435618301711, -105.1118169210616 40.01363272390126, -105.1120551899672 40.01316817480327, -105.1133852018378 40.01249016979386, -105.1133509829044 40.01201286862782, -105.1136931479484 40.01180305609206, -105.1138475779678 40.01162389750351, -105.1142013247205 40.01121349713745, -105.1142366021811 40.01110200384621, -105.1142021579376 40.01090890468547, -105.1141717798238 40.01085855805781, -105.1139400367938 40.01047445261041, -105.1139748795943 40.01016354509047, -105.1138816269313 40.00996120182681, -105.1137354716539 40.00984934691608, -105.1134671916322 40.00971973315597, -105.1126167071906 40.00944957839319, -105.1123818862575 40.00933650518886, -105.1123850954861 40.0092367825163, -105.1125460955506 40.009118545706, -105.1135527848292 40.00915992609273, -105.1138595621785 40.00904999000269, -105.1139182214054 40.00874268377794, -105.1140548223516 40.00872057596153, -105.1143214105558 40.00881271895139, -105.1145438842861 40.00876316467217, -105.114690116975 40.00858194204327, -105.1149006847169 40.00846983893248, -105.115439060473 40.00840796360136, -105.116862273694 40.00845912278751, -105.1180058771873 40.00874783898299, -105.1181222934217 40.00879838850203, -105.1185405381531 40.00890644040241, -105.1187095139158 40.00890792962496, -105.1189986310474 40.00883908245553, -105.1190870064322 40.0087948143735, -105.1193165119794 40.00867985395175, -105.1196441700197 40.00809229319403, -105.1196943148284 40.00795817051018, -105.1195936883294 40.00762459431621, -105.119540466071 40.00744816089534, -105.1197580464724 40.00744815083699, -105.1196526706213 40.00716149139468, -105.1194215525195 40.0070419771017, -105.1192726232592 40.00696496198054, -105.1192454207034 40.00695089665385, -105.1192404971615 40.00694707781889, -105.1192390085427 40.00694456186928, -105.1192382918508 40.00694181880084, -105.119238394275 40.00693899737787, -105.1192393044043 40.00693625337662, -105.1192409757474 40.00693373255002, -105.1192433185294 40.00693157150168, -105.1192459938729 40.00693005101848, -105.1193197250956 40.00689420959378, -105.1194060086062 40.00682009016207, -105.1192301331914 40.00668445678808, -105.1190329886974 40.00582317381761, -105.1190369363567 40.00583079922135, -105.1195333961401 40.00583735955976, -105.1195327169743 40.00576134809078, -105.1213307250641 40.0053580770317, -105.1214496535599 40.00533079571107, -105.1215377044217 40.00538187734463, -105.1215941830349 40.00533747112853, -105.121636499543 40.00532262664415, -105.1217993195672 40.00526550337217, -105.1218971879952 40.00524509838811, -105.1221650240661 40.00518777490752, -105.1224421350409 40.0051425824149, -105.1226924750917 40.0050751058488, -105.1230748528706 40.00489650674073, -105.1231029045344 40.00485631831071, -105.1230188523702 40.00459895975199, -105.1231447079403 40.00415326086031, -105.1231304599729 40.00382534596935, -105.1232110077422 40.00372316836474, -105.1232036365329 40.00356334052815, -105.1244795338295 40.00275100502883, -105.124836392481 40.0020944593464, -105.1252510719455 40.00190993453685, -105.1255673805286 40.00186449358997, -105.126031309827 40.0016728350766, -105.1268634316468 40.0010890935762, -105.1272287212306 40.00074701903485, -105.1278863996462 40.00019607993971, -105.1249943870176 40.00018608330566, -105.1243803841114 40.00018608413534, -105.1227223770928 40.00019008632776, -105.1220613732507 40.0001900867268, -105.1211533696423 40.00019008802158, -105.1198903638917 40.00018108926099, -105.118486358255 40.0001810905321, -105.1179783559487 40.00018109093085, -105.1176593547601 40.00018109182523, -105.1172943527015 40.00019009165216, -105.1167513496874 40.00019009295482, -105.1159253461369 40.00019009324066, -105.1153463435339 40.00019009409569, -105.1150783428394 40.00019209442387, -105.1147383414262 40.00019209458394, -105.112839332849 40.00020409717904, -105.1106733234379 40.00020809977608, -105.1097053190127 40.0002081010155, -105.1094463176448 40.00020810124028, -105.1092652724153 40.00020694295018, -105.1080413119849 40.00019910224839, -105.1076403102274 40.00019910286098, -105.1067553062359 40.00019910416006, -105.1053192989058 40.00019710578297, -105.105125942928 40.00019699675529, -105.1040901046762 40.00019097321382, -105.103607154678 40.0001898632859, -105.1028662911329 40.00021572247173))</t>
+          <t>POLYGON ((-105.10286629113293 40.00021572247173, -105.10288503530845 40.00123303111563, -105.10288395840271 40.00160198420788, -105.1028828890649 40.00227593018461, -105.10289310031172 40.00346491715381, -105.1028969891118 40.00383910388316, -105.1028968882406 40.003979109157164, -105.10289699792587 40.004144096729114, -105.10289685245523 40.00416907780282, -105.10290207042296 40.00609294163367, -105.10290498560897 40.006511870534545, -105.10291199991674 40.00745295413691, -105.10291311347017 40.00830397399917, -105.10292115248147 40.00986602708125, -105.10291990968022 40.01038596654633, -105.10291873397485 40.01076626095388, -105.1075026571879 40.01077491615019, -105.10756813495888 40.014622189238416, -105.10756828865004 40.01475361643449, -105.10804864385432 40.014751926573794, -105.11055606643392 40.014739434077846, -105.11056017179338 40.01435618301711, -105.1118169210616 40.01363272390126, -105.11205518996721 40.01316817480327, -105.11338520183779 40.01249016979386, -105.11335098290442 40.01201286862782, -105.1136931479484 40.011803056092056, -105.11384757796782 40.01162389750351, -105.11420132472048 40.011213497137454, -105.11423660218112 40.01110200384621, -105.11420215793761 40.01090890468547, -105.11417177982383 40.01085855805781, -105.11394003679385 40.01047445261041, -105.11397487959427 40.01016354509047, -105.11388162693126 40.00996120182681, -105.11373547165385 40.009849346916084, -105.11346719163221 40.00971973315597, -105.1126167071906 40.009449578393195, -105.11238188625752 40.00933650518886, -105.11238509548609 40.009236782516304, -105.1125460955506 40.009118545705995, -105.11355278482921 40.00915992609273, -105.11385956217846 40.009049990002694, -105.11391822140544 40.00874268377794, -105.11405482235156 40.00872057596153, -105.11432141055585 40.00881271895139, -105.11454388428615 40.00876316467217, -105.11469011697498 40.00858194204327, -105.1149006847169 40.00846983893248, -105.11543906047298 40.008407963601364, -105.11686227369401 40.008459122787514, -105.11800587718733 40.00874783898299, -105.11812229342168 40.00879838850203, -105.11854053815308 40.008906440402406, -105.1187095139158 40.00890792962496, -105.11899863104738 40.00883908245553, -105.11908700643215 40.0087948143735, -105.1193165119794 40.008679853951755, -105.11964417001971 40.008092293194025, -105.11969431482844 40.00795817051018, -105.11959368832939 40.00762459431621, -105.119540466071 40.007448160895336, -105.11975804647237 40.007448150836986, -105.11965267062126 40.00716149139468, -105.11942155251948 40.0070419771017, -105.11927262325922 40.006964961980536, -105.11924542070335 40.00695089665385, -105.11924049716151 40.006947077818886, -105.11923900854266 40.00694456186928, -105.11923829185083 40.00694181880084, -105.11923839427497 40.006938997377866, -105.11923930440426 40.00693625337662, -105.11924097574743 40.006933732550024, -105.11924331852944 40.00693157150168, -105.11924599387287 40.00693005101848, -105.11931972509558 40.00689420959378, -105.11940600860623 40.00682009016207, -105.11923013319144 40.00668445678808, -105.11903298869737 40.00582317381761, -105.11903693635668 40.00583079922135, -105.1195333961401 40.00583735955976, -105.11953271697426 40.00576134809078, -105.1213307250641 40.0053580770317, -105.12144965355988 40.005330795711075, -105.1215377044217 40.00538187734463, -105.12159418303489 40.00533747112853, -105.12163649954297 40.00532262664415, -105.12179931956717 40.00526550337217, -105.12189718799517 40.00524509838811, -105.12216502406613 40.00518777490752, -105.12244213504086 40.0051425824149, -105.12269247509171 40.0050751058488, -105.12307485287063 40.00489650674073, -105.12310290453439 40.004856318310715, -105.1230188523702 40.004598959751995, -105.12314470794028 40.00415326086031, -105.12313045997294 40.00382534596935, -105.1232110077422 40.00372316836474, -105.12320363653289 40.00356334052815, -105.1244795338295 40.002751005028834, -105.12483639248099 40.0020944593464, -105.12525107194548 40.00190993453685, -105.12556738052864 40.00186449358997, -105.12603130982697 40.001672835076604, -105.12686343164678 40.001089093576205, -105.12722872123057 40.000747019034854, -105.12788639964619 40.000196079939705, -105.12499438701764 40.000186083305664, -105.12438038411136 40.00018608413534, -105.12272237709283 40.00019008632776, -105.12206137325067 40.000190086726796, -105.12115336964231 40.000190088021576, -105.11989036389167 40.00018108926099, -105.11848635825496 40.000181090532095, -105.11797835594867 40.00018109093085, -105.11765935476015 40.00018109182523, -105.11729435270146 40.00019009165216, -105.11675134968743 40.00019009295482, -105.11592534613695 40.00019009324066, -105.11534634353389 40.00019009409569, -105.11507834283935 40.000192094423866, -105.11473834142616 40.000192094583944, -105.11283933284896 40.000204097179044, -105.11067332343787 40.00020809977608, -105.10970531901273 40.000208101015495, -105.10944631764484 40.00020810124028, -105.10926527241534 40.00020694295018, -105.10804131198492 40.000199102248395, -105.10764031022741 40.00019910286098, -105.10675530623585 40.00019910416006, -105.1053192989058 40.00019710578297, -105.10512594292797 40.000196996755285, -105.10409010467622 40.00019097321382, -105.10360715467802 40.0001898632859, -105.10286629113293 40.00021572247173))</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2012,7 +2020,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1092652724153 40.00020694295018, -105.1094463176448 40.00020810124028, -105.1097053190127 40.0002081010155, -105.1106733234379 40.00020809977608, -105.112839332849 40.00020409717904, -105.1147383414262 40.00019209458394, -105.1150783428394 40.00019209442387, -105.1153463435339 40.00019009409569, -105.1159253461369 40.00019009324066, -105.1167513496874 40.00019009295482, -105.1172943527015 40.00019009165216, -105.1176593547601 40.00018109182523, -105.1179783559487 40.00018109093085, -105.118486358255 40.0001810905321, -105.1198903638917 40.00018108926099, -105.1211533696423 40.00019008802158, -105.1220613732507 40.0001900867268, -105.1227223770928 40.00019008632776, -105.1243803841114 40.00018608413534, -105.1249943870176 40.00018608330566, -105.1278863996462 40.00019607993971, -105.1281614002314 40.00019307989155, -105.1284524015447 40.00019307950447, -105.1302618979046 40.00020779027882, -105.1310556496412 40.00019967631347, -105.1310199000001 40.00000111003435, -105.1309530171901 39.99976206309216, -105.1308618342599 39.99952787931828, -105.130825874301 39.99944513331248, -105.1306979651387 39.99920396788463, -105.1306010059876 39.99904800375236, -105.1304929772026 39.99889310286233, -105.1303351563433 39.9987050988637, -105.1302219428106 39.99858504466381, -105.1301019410162 39.9984660664744, -105.1290031309847 39.99750802562184, -105.1287950428024 39.9973099756827, -105.1287410996148 39.99725297585866, -105.1286219097554 39.9971169780709, -105.1285559440074 39.99703907658157, -105.1284588462749 39.99691001280862, -105.1283130497574 39.99667894551565, -105.1281848229492 39.99643310985479, -105.1280571000947 39.99609503653452, -105.1279878358992 39.99583703830547, -105.1279541047636 39.99541196996041, -105.1279508746169 39.99430289398319, -105.1279510944342 39.99413186772644, -105.1277274031719 39.99403166429317, -105.1232577328613 39.99406674611331, -105.1232589140897 39.9941456611968, -105.122814800146 39.9941474397444, -105.1226719071595 39.99394172642054, -105.1225145804866 39.99383477964317, -105.1223849223714 39.99378832326342, -105.1223232452224 39.99378812123183, -105.1223389573864 39.99236704634767, -105.1223383484516 39.99236705245885, -105.1222303531299 39.99236784607286, -105.121007043891 39.9923704175954, -105.1204839651552 39.99237377836661, -105.1199496728335 39.99237720607682, -105.1189229397637 39.99238378801977, -105.1185472892864 39.99238619608135, -105.1185474045477 39.99235909652852, -105.1184579818192 39.99235779818542, -105.1184463683575 39.99308807454024, -105.1184374443334 39.99316489464574, -105.1184119771252 39.99326403416953, -105.1183824196342 39.99333575309119, -105.1183169872036 39.99344651479904, -105.118216385493 39.99356413201255, -105.1180669999796 39.99372004658021, -105.1179979121066 39.99377350597219, -105.1180370301155 39.99379692572312, -105.1181048759368 39.99385507456891, -105.1181990168995 39.99399786252945, -105.1172719606722 39.99440410043128, -105.1171730685706 39.99447212761837, -105.1147423325333 39.99684808060402, -105.1147423330233 39.99719108125619, -105.1147403634717 39.99736788392994, -105.1144575601929 39.997370068387, -105.109237767345 39.99740700430097, -105.1092663179089 40.00010213861572, -105.1092652724153 40.00020694295018))</t>
+          <t>POLYGON ((-105.10926527241534 40.00020694295018, -105.10944631764484 40.00020810124028, -105.10970531901273 40.000208101015495, -105.11067332343787 40.00020809977608, -105.11283933284896 40.000204097179044, -105.11473834142616 40.000192094583944, -105.11507834283935 40.000192094423866, -105.11534634353389 40.00019009409569, -105.11592534613695 40.00019009324066, -105.11675134968743 40.00019009295482, -105.11729435270146 40.00019009165216, -105.11765935476015 40.00018109182523, -105.11797835594867 40.00018109093085, -105.11848635825496 40.000181090532095, -105.11989036389167 40.00018108926099, -105.12115336964231 40.000190088021576, -105.12206137325067 40.000190086726796, -105.12272237709283 40.00019008632776, -105.12438038411136 40.00018608413534, -105.12499438701764 40.000186083305664, -105.12788639964619 40.000196079939705, -105.12816140023142 40.000193079891545, -105.12845240154472 40.00019307950447, -105.13026189790463 40.00020779027882, -105.1310556496412 40.00019967631347, -105.13101990000008 40.000001110034354, -105.13095301719011 39.999762063092156, -105.13086183425986 39.99952787931828, -105.13082587430098 39.999445133312484, -105.1306979651387 39.999203967884625, -105.13060100598761 39.999048003752364, -105.13049297720265 39.99889310286233, -105.13033515634329 39.9987050988637, -105.13022194281065 39.99858504466381, -105.13010194101615 39.9984660664744, -105.12900313098474 39.99750802562184, -105.1287950428024 39.997309975682704, -105.12874109961479 39.99725297585866, -105.1286219097554 39.9971169780709, -105.12855594400737 39.997039076581565, -105.12845884627488 39.99691001280862, -105.12831304975744 39.996678945515654, -105.12818482294917 39.99643310985479, -105.12805710009474 39.99609503653452, -105.12798783589918 39.995837038305474, -105.12795410476359 39.99541196996041, -105.1279508746169 39.99430289398319, -105.12795109443424 39.99413186772644, -105.12772740317189 39.994031664293175, -105.12325773286126 39.99406674611331, -105.1232589140897 39.9941456611968, -105.12281480014596 39.994147439744395, -105.12267190715949 39.99394172642054, -105.12251458048662 39.993834779643166, -105.12238492237144 39.993788323263416, -105.12232324522239 39.99378812123183, -105.12233895738636 39.992367046347674, -105.12233834845158 39.992367052458846, -105.12223035312992 39.99236784607286, -105.12100704389098 39.992370417595396, -105.12048396515519 39.992373778366606, -105.11994967283347 39.992377206076824, -105.1189229397637 39.99238378801977, -105.11854728928638 39.99238619608135, -105.11854740454771 39.992359096528524, -105.11845798181916 39.99235779818542, -105.11844636835751 39.99308807454024, -105.11843744433341 39.993164894645744, -105.11841197712522 39.99326403416953, -105.11838241963416 39.99333575309119, -105.11831698720356 39.99344651479904, -105.11821638549301 39.99356413201255, -105.1180669999796 39.993720046580215, -105.1179979121066 39.99377350597219, -105.11803703011549 39.993796925723125, -105.11810487593678 39.99385507456891, -105.11819901689945 39.993997862529454, -105.11727196067218 39.99440410043128, -105.1171730685706 39.99447212761837, -105.1147423325333 39.99684808060402, -105.11474233302329 39.99719108125619, -105.11474036347168 39.99736788392994, -105.11445756019292 39.997370068387, -105.10923776734505 39.99740700430097, -105.10926631790886 40.00010213861572, -105.10926527241534 40.00020694295018))</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2054,7 +2062,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1537707329934 40.000125192599, -105.1537709990355 40.00012399912667, -105.1538145028673 40.00012399915835, -105.1539019988791 40.00012399883708, -105.1550500005115 40.00012499920634, -105.156588390307 40.00012897627218, -105.1568362961492 40.00012961529795, -105.1568367408974 40.00012757393174, -105.1568459364061 40.00004260990784, -105.1568526260754 39.99995385836775, -105.157040634938 39.99799156637739, -105.1570808518021 39.99757180685464, -105.1570990085866 39.9974216510589, -105.1571164998218 39.99727085921636, -105.1571750076949 39.99676647874302, -105.1572403745552 39.99617565911632, -105.1572405990433 39.99617363150352, -105.1565059962698 39.99617247919943, -105.1562106152407 39.99617225447206, -105.155460491504 39.99617391781758, -105.1545751648555 39.99617619263377, -105.1539519884817 39.99617947834857, -105.1527344190078 39.99618588769861, -105.1527329270777 39.99618589581407, -105.1527319606385 39.99568069342332, -105.152730749748 39.99504526780311, -105.1527303188908 39.9948198724531, -105.1527298717996 39.99458662691797, -105.1527298679238 39.99458462834716, -105.1527297013948 39.9944982043476, -105.1527294447671 39.99436232136527, -105.1527291642861 39.99422330402094, -105.1527289655441 39.99412802825835, -105.1527391763146 39.99397744204157, -105.1511885403603 39.99398043009678, -105.1489619720619 39.99399513205215, -105.1467891751321 39.99400744202379, -105.146790174619 39.9941694428106, -105.1466363980306 39.99416436382368, -105.1465101961338 39.99416287454163, -105.1464615829938 39.99416230126948, -105.1459611770951 39.99455926085398, -105.145432872713 39.99479210016541, -105.1443011561806 39.99478265717581, -105.1442614765063 39.99492166747812, -105.1422639133758 39.99651569716553, -105.1418815666315 39.99705442482142, -105.1415483564617 39.99743752080339, -105.1412987486078 39.99773918448757, -105.1407003492131 39.99804212814589, -105.1405141950552 39.99813279982534, -105.1373344848354 39.99415560978961, -105.1373254730912 39.99414433762385, -105.130985314058 39.99412962806004, -105.1279510944342 39.99413186772644, -105.1279508746169 39.99430289398319, -105.1279541047636 39.99541196996041, -105.1279878358992 39.99583703830547, -105.1280571000947 39.99609503653452, -105.1281848229492 39.99643310985479, -105.1283130497574 39.99667894551565, -105.1284588462749 39.99691001280862, -105.1285559440074 39.99703907658157, -105.1286219097554 39.9971169780709, -105.1287410996148 39.99725297585866, -105.1287950428024 39.9973099756827, -105.1290031309847 39.99750802562184, -105.1301019410162 39.9984660664744, -105.1302219428106 39.99858504466381, -105.1303351563433 39.9987050988637, -105.1304929772026 39.99889310286233, -105.1306010059876 39.99904800375236, -105.1306979651387 39.99920396788463, -105.130825874301 39.99944513331248, -105.1308618342599 39.99952787931828, -105.1309530171901 39.99976206309216, -105.1310199000001 40.00000111003435, -105.1310556496412 40.00019967631347, -105.1310749033248 40.00039110612163, -105.1310950875115 40.00061902365207, -105.1310980615045 40.00072911608232, -105.131103063404 40.00086007783933, -105.1311040366654 40.00107612986969, -105.1311086818536 40.0013477354128, -105.1310948532135 40.00217994944209, -105.1310944311785 40.0023664283858, -105.131093056197 40.00297413289702, -105.1310878320044 40.00360990666242, -105.1310844505609 40.00509939167827, -105.1310873461379 40.00565936943882, -105.1310941022362 40.00641004040492, -105.1310878876888 40.00656896854314, -105.1310850732638 40.00695713206541, -105.1310838449696 40.0070521123623, -105.1310812050261 40.0072279023247, -105.1310799403458 40.00731207101194, -105.1310783415883 40.00740538300349, -105.1312534875319 40.00740314937847, -105.1312832577426 40.00740312838888, -105.1312832797619 40.00740100560996, -105.1312846278433 40.00740100451655, -105.1312935033927 40.0074009977704, -105.1341532742665 40.00739890930889, -105.1352314904021 40.00739810368863, -105.1352364821891 40.00739524908467, -105.1352393859926 40.00739365149774, -105.1352423002596 40.00739206835435, -105.1352452227105 40.00739048793876, -105.1352481509593 40.00738891834928, -105.1352510862016 40.00738735508647, -105.1352540284179 40.00738580175289, -105.1352569823076 40.00738425566137, -105.1352599396577 40.00738271948803, -105.1352629028349 40.00738118873692, -105.1352658741379 40.00737967152132, -105.1352688524633 40.00737815522849, -105.1352718377627 40.00737664886486, -105.1352748300459 40.00737515062921, -105.1352778304647 40.00737366412773, -105.1352808355393 40.0073721830448, -105.1352838464216 40.00737071098678, -105.1352868666396 40.00736924526279, -105.135289895003 40.00736778947173, -105.1352929268364 40.00736634179746, -105.1352959656584 40.00736490135053, -105.1352990137873 40.00736347264144, -105.1353020700854 40.00736204936203, -105.135305126345 40.0073606332877, -105.1353081895787 40.00735922714261, -105.1353112632951 40.00735783183841, -105.135314340501 40.00735644104851, -105.135317425857 40.00735505929084, -105.1353205170111 40.00735368835932, -105.1353236163394 40.00735232195684, -105.1353267214561 40.0073509681818, -105.1353298312142 40.00734962252728, -105.1353329491368 40.00734828320308, -105.1353360716767 40.0073469565026, -105.1353391988867 40.00734563251877, -105.1353423365797 40.00734431937593, -105.1353454777428 40.00734301434984, -105.1353486235328 40.0073417201462, -105.1353517774874 40.00734043227291, -105.1353549384305 40.00733915162687, -105.1353581004821 40.00733788269282, -105.1353612706934 40.00733662098969, -105.1353644455413 40.00733536830775, -105.1353676297153 40.00733412376111, -105.1353708173401 40.00733289093387, -105.1353740131392 40.00733166263565, -105.1353772100516 40.00733044514874, -105.1353804151141 40.00732923669405, -105.1353836271604 40.00732803636732, -105.1353868426767 40.0073268441574, -105.1353900651913 40.00732565737344, -105.1353932911278 40.00732448771268, -105.1353965217443 40.00732331896733, -105.1353997616435 40.007322166463, -105.1354030026946 40.00732101756492, -105.1354062565613 40.00731988131641, -105.1354095045527 40.0073187486519, -105.1354127665357 40.00731762774004, -105.1354160272801 40.00731651943344, -105.1354192973746 40.00731541475887, -105.1354225721009 40.00731432000612, -105.1354258526205 40.00731323698013, -105.135427728691 40.00731262145808, -105.1354291354535 40.00731215936529, -105.1354324252654 40.00731109077897, -105.1354341517882 40.00731040633411, -105.1356722521112 40.00730740311281, -105.13974885825 40.00725594913141, -105.1398428922491 40.00725476218737, -105.1398447187669 40.00725686822421, -105.1399362728994 40.00736244634241, -105.1405243015636 40.00736530590967, -105.1405236235035 40.00722199126245, -105.1405235952953 40.00721578925072, -105.1405233594408 40.00716677296265, -105.1405233533581 40.00716526074064, -105.140523180474 40.00712851609968, -105.1405231402594 40.0071210369189, -105.140523033826 40.00709723672683, -105.1405227731292 40.00704226881942, -105.1405227300227 40.00703333867119, -105.1405213135668 40.00673438548746, -105.1405204679228 40.00655532323205, -105.1405197450146 40.00640230115203, -105.1405189063033 40.00622503572305, -105.1405180110712 40.00603560944315, -105.1405171003353 40.0058433487435, -105.1405159169233 40.00559328571963, -105.1405152394761 40.0054507501174, -105.1405147282165 40.00534222924821, -105.1405138435483 40.00515546892974, -105.1405129177941 40.00496006307164, -105.1405119956253 40.00476531109808, -105.1405117178504 40.0047060325794, -105.140510985685 40.00455144149755, -105.1405095938914 40.00425738248826, -105.1405095795938 40.00425431840782, -105.1405086488789 40.00405785874783, -105.1405083861383 40.00400217209295, -105.1405083759637 40.00400010325159, -105.1405082039836 40.0039638566653, -105.1405073285334 40.00377868691076, -105.1414141544557 40.00377504835109, -105.141509603522 40.00377466514739, -105.1415175843889 40.00365291029514, -105.1414905848927 40.00358891121111, -105.1414825826895 40.00347591238927, -105.1414825701238 40.00249991777957, -105.141499568217 40.00238291850106, -105.1415115688388 40.00233991970254, -105.1415255674581 40.00230091972836, -105.1415915660002 40.00217492028406, -105.1417900173021 40.00198145342109, -105.14179056115 40.00198092282215, -105.1413045598964 40.00160192301993, -105.1408455558642 40.00122292597722, -105.1407508565735 40.00112723061763, -105.1407505560302 40.00112692615965, -105.1406575531707 40.0009829265404, -105.1406015518538 40.00081292761907, -105.1405755504105 40.00063393005045, -105.1405885450742 40.00027393090059, -105.1405914290438 40.00022490629105, -105.1405990316423 40.00013293952663, -105.149532503279 40.00012599868626, -105.1495325033061 40.00012394248593, -105.1496865034817 40.00012394214083, -105.1512284955127 40.0001169433975, -105.1512644961406 40.00011694331047, -105.1515154957292 40.00011694385289, -105.1515160075409 40.0001189979974, -105.1515363523692 40.00020070855813, -105.1515373454481 40.00020071065877, -105.1516755779333 40.00020098063606, -105.1517734538989 40.00041189854682, -105.1526815171395 40.00062425548496, -105.1531903592538 40.00041976453732, -105.1532393860764 40.0003995175149, -105.1534616395557 40.00019996334979, -105.1535166308957 40.00019969810031, -105.1535781771506 40.00013044327525, -105.1537707329934 40.000125192599))</t>
+          <t>POLYGON ((-105.15377073299338 40.000125192599, -105.15377099903554 40.00012399912667, -105.15381450286732 40.00012399915835, -105.15390199887914 40.00012399883708, -105.1550500005115 40.000124999206335, -105.15658839030704 40.00012897627218, -105.1568362961492 40.00012961529795, -105.15683674089738 40.00012757393174, -105.15684593640609 40.000042609907844, -105.15685262607542 39.999953858367746, -105.15704063493796 39.997991566377394, -105.15708085180212 39.997571806854644, -105.15709900858657 39.9974216510589, -105.15711649982177 39.997270859216364, -105.15717500769495 39.99676647874302, -105.15724037455517 39.99617565911632, -105.15724059904332 39.996173631503524, -105.15650599626977 39.99617247919943, -105.15621061524074 39.99617225447206, -105.15546049150397 39.99617391781758, -105.15457516485553 39.99617619263377, -105.15395198848165 39.99617947834857, -105.15273441900779 39.99618588769861, -105.15273292707768 39.996185895814065, -105.15273196063852 39.99568069342332, -105.15273074974802 39.99504526780311, -105.15273031889083 39.9948198724531, -105.15272987179958 39.99458662691797, -105.15272986792377 39.994584628347155, -105.15272970139479 39.9944982043476, -105.15272944476715 39.994362321365266, -105.15272916428606 39.99422330402094, -105.15272896554406 39.99412802825835, -105.15273917631464 39.99397744204157, -105.15118854036027 39.99398043009678, -105.14896197206194 39.99399513205215, -105.14678917513206 39.994007442023786, -105.14679017461899 39.9941694428106, -105.1466363980306 39.99416436382368, -105.14651019613379 39.99416287454163, -105.14646158299378 39.994162301269476, -105.14596117709509 39.994559260853976, -105.145432872713 39.994792100165405, -105.14430115618062 39.99478265717581, -105.14426147650629 39.994921667478124, -105.14226391337579 39.99651569716553, -105.14188156663147 39.99705442482142, -105.14154835646167 39.997437520803395, -105.14129874860778 39.99773918448757, -105.14070034921306 39.99804212814589, -105.1405141950552 39.99813279982534, -105.13733448483536 39.99415560978961, -105.1373254730912 39.99414433762385, -105.13098531405798 39.994129628060044, -105.12795109443424 39.99413186772644, -105.1279508746169 39.99430289398319, -105.12795410476359 39.99541196996041, -105.12798783589918 39.995837038305474, -105.12805710009474 39.99609503653452, -105.12818482294917 39.99643310985479, -105.12831304975744 39.996678945515654, -105.12845884627488 39.99691001280862, -105.12855594400737 39.997039076581565, -105.1286219097554 39.9971169780709, -105.12874109961479 39.99725297585866, -105.1287950428024 39.997309975682704, -105.12900313098474 39.99750802562184, -105.13010194101615 39.9984660664744, -105.13022194281065 39.99858504466381, -105.13033515634329 39.9987050988637, -105.13049297720265 39.99889310286233, -105.13060100598761 39.999048003752364, -105.1306979651387 39.999203967884625, -105.13082587430098 39.999445133312484, -105.13086183425986 39.99952787931828, -105.13095301719011 39.999762063092156, -105.13101990000008 40.000001110034354, -105.1310556496412 40.00019967631347, -105.13107490332477 40.000391106121626, -105.13109508751147 40.00061902365207, -105.13109806150453 40.00072911608232, -105.13110306340398 40.000860077839334, -105.13110403666545 40.001076129869695, -105.1311086818536 40.0013477354128, -105.13109485321345 40.00217994944209, -105.1310944311785 40.0023664283858, -105.13109305619696 40.00297413289702, -105.13108783200435 40.00360990666242, -105.13108445056093 40.00509939167827, -105.13108734613792 40.00565936943882, -105.13109410223623 40.00641004040492, -105.13108788768884 40.00656896854314, -105.13108507326379 40.00695713206541, -105.1310838449696 40.007052112362295, -105.13108120502608 40.0072279023247, -105.13107994034577 40.00731207101194, -105.13107834158829 40.00740538300349, -105.13125348753188 40.00740314937847, -105.1312832577426 40.00740312838888, -105.13128327976194 40.00740100560996, -105.13128462784326 40.00740100451655, -105.13129350339274 40.007400997770404, -105.13415327426647 40.00739890930889, -105.13523149040209 40.00739810368863, -105.13523648218913 40.007395249084674, -105.13523938599256 40.00739365149774, -105.1352423002596 40.00739206835435, -105.13524522271045 40.00739048793876, -105.13524815095934 40.00738891834928, -105.13525108620158 40.00738735508647, -105.1352540284179 40.00738580175289, -105.13525698230758 40.00738425566137, -105.13525993965773 40.00738271948803, -105.13526290283485 40.00738118873692, -105.13526587413794 40.00737967152132, -105.1352688524633 40.00737815522849, -105.13527183776274 40.007376648864856, -105.13527483004592 40.00737515062921, -105.13527783046473 40.00737366412773, -105.1352808355393 40.0073721830448, -105.1352838464216 40.007370710986784, -105.13528686663963 40.007369245262794, -105.13528989500296 40.00736778947173, -105.13529292683639 40.00736634179746, -105.13529596565837 40.00736490135053, -105.13529901378726 40.00736347264144, -105.13530207008544 40.00736204936203, -105.13530512634496 40.007360633287696, -105.13530818957865 40.00735922714261, -105.1353112632951 40.00735783183841, -105.13531434050101 40.00735644104851, -105.13531742585704 40.007355059290845, -105.1353205170111 40.00735368835932, -105.13532361633942 40.007352321956844, -105.13532672145614 40.0073509681818, -105.1353298312142 40.00734962252728, -105.1353329491368 40.00734828320308, -105.13533607167668 40.0073469565026, -105.13533919888674 40.00734563251877, -105.13534233657974 40.00734431937593, -105.13534547774285 40.007343014349836, -105.1353486235328 40.0073417201462, -105.13535177748739 40.00734043227291, -105.1353549384305 40.00733915162687, -105.1353581004821 40.00733788269282, -105.13536127069344 40.00733662098969, -105.1353644455413 40.00733536830775, -105.13536762971528 40.00733412376111, -105.13537081734013 40.00733289093387, -105.13537401313924 40.00733166263565, -105.13537721005157 40.00733044514874, -105.13538041511407 40.007329236694055, -105.13538362716035 40.00732803636732, -105.1353868426767 40.0073268441574, -105.13539006519126 40.00732565737344, -105.13539329112781 40.00732448771268, -105.13539652174428 40.00732331896733, -105.13539976164354 40.007322166463, -105.13540300269459 40.00732101756492, -105.13540625656131 40.00731988131641, -105.13540950455268 40.007318748651905, -105.13541276653572 40.007317627740036, -105.13541602728006 40.00731651943344, -105.13541929737464 40.00731541475887, -105.13542257210094 40.00731432000612, -105.1354258526205 40.00731323698013, -105.135427728691 40.007312621458084, -105.13542913545349 40.00731215936529, -105.13543242526539 40.00731109077897, -105.1354341517882 40.00731040633411, -105.13567225211118 40.00730740311281, -105.13974885824997 40.007255949131405, -105.13984289224915 40.007254762187365, -105.1398447187669 40.00725686822421, -105.13993627289945 40.00736244634241, -105.14052430156362 40.007365305909666, -105.14052362350347 40.007221991262455, -105.14052359529526 40.00721578925072, -105.14052335944076 40.00716677296265, -105.14052335335812 40.00716526074064, -105.14052318047405 40.00712851609968, -105.14052314025936 40.007121036918896, -105.14052303382604 40.00709723672683, -105.14052277312916 40.00704226881942, -105.1405227300227 40.00703333867119, -105.14052131356677 40.00673438548746, -105.14052046792277 40.00655532323205, -105.14051974501459 40.00640230115203, -105.14051890630327 40.00622503572305, -105.14051801107122 40.00603560944315, -105.14051710033527 40.0058433487435, -105.14051591692329 40.00559328571963, -105.14051523947612 40.0054507501174, -105.14051472821647 40.00534222924821, -105.14051384354828 40.005155468929736, -105.14051291779414 40.00496006307164, -105.14051199562529 40.00476531109808, -105.14051171785037 40.0047060325794, -105.14051098568495 40.004551441497554, -105.14050959389135 40.004257382488255, -105.14050957959384 40.00425431840782, -105.14050864887894 40.00405785874783, -105.14050838613834 40.00400217209295, -105.14050837596368 40.00400010325159, -105.14050820398356 40.0039638566653, -105.1405073285334 40.00377868691076, -105.14141415445575 40.00377504835109, -105.14150960352195 40.00377466514739, -105.14151758438891 40.00365291029514, -105.14149058489267 40.00358891121111, -105.1414825826895 40.00347591238927, -105.14148257012384 40.002499917779566, -105.14149956821704 40.00238291850106, -105.1415115688388 40.00233991970254, -105.14152556745809 40.00230091972836, -105.14159156600022 40.00217492028406, -105.14179001730211 40.00198145342109, -105.14179056115002 40.00198092282215, -105.14130455989637 40.001601923019926, -105.14084555586425 40.001222925977224, -105.14075085657349 40.00112723061763, -105.1407505560302 40.00112692615965, -105.14065755317074 40.000982926540395, -105.14060155185382 40.000812927619066, -105.14057555041046 40.00063393005045, -105.14058854507417 40.00027393090059, -105.14059142904382 40.000224906291045, -105.1405990316423 40.00013293952663, -105.14953250327905 40.00012599868626, -105.14953250330608 40.00012394248593, -105.14968650348173 40.00012394214083, -105.15122849551267 40.0001169433975, -105.15126449614058 40.000116943310466, -105.15151549572916 40.00011694385289, -105.1515160075409 40.0001189979974, -105.15153635236916 40.000200708558125, -105.15153734544808 40.00020071065877, -105.15167557793335 40.00020098063606, -105.15177345389893 40.000411898546815, -105.1526815171395 40.00062425548496, -105.15319035925384 40.00041976453732, -105.15323938607644 40.0003995175149, -105.15346163955572 40.000199963349786, -105.15351663089567 40.00019969810031, -105.15357817715062 40.00013044327525, -105.15377073299338 40.000125192599))</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2096,7 +2104,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1278863996462 40.00019607993971, -105.1272287212306 40.00074701903485, -105.1268634316468 40.0010890935762, -105.126031309827 40.0016728350766, -105.1255673805286 40.00186449358997, -105.1252510719455 40.00190993453685, -105.124836392481 40.0020944593464, -105.1244795338295 40.00275100502883, -105.1232036365329 40.00356334052815, -105.1232110077422 40.00372316836474, -105.1231304599729 40.00382534596935, -105.1231447079403 40.00415326086031, -105.1230188523702 40.00459895975199, -105.1231029045344 40.00485631831071, -105.1230748528706 40.00489650674073, -105.1226924750917 40.0050751058488, -105.1224421350409 40.0051425824149, -105.1221650240661 40.00518777490752, -105.1218971879952 40.00524509838811, -105.1217993195672 40.00526550337217, -105.121636499543 40.00532262664415, -105.1215941830349 40.00533747112853, -105.1215377044217 40.00538187734463, -105.1214496535599 40.00533079571107, -105.1213307250641 40.0053580770317, -105.1195327169743 40.00576134809078, -105.1195333961401 40.00583735955976, -105.1190369363567 40.00583079922135, -105.1190329886974 40.00582317381761, -105.1192301331914 40.00668445678808, -105.1194060086062 40.00682009016207, -105.1193197250956 40.00689420959378, -105.1192459938729 40.00693005101848, -105.1192433185294 40.00693157150168, -105.1192409757474 40.00693373255002, -105.1192393044043 40.00693625337662, -105.119238394275 40.00693899737787, -105.1192382918508 40.00694181880084, -105.1192390085427 40.00694456186928, -105.1192404971615 40.00694707781889, -105.1192454207034 40.00695089665385, -105.1192726232592 40.00696496198054, -105.1194215525195 40.0070419771017, -105.1196526706213 40.00716149139468, -105.1197580464724 40.00744815083699, -105.119540466071 40.00744816089534, -105.1195936883294 40.00762459431621, -105.1196943148284 40.00795817051018, -105.1196441700197 40.00809229319403, -105.1193165119794 40.00867985395175, -105.1190870064322 40.0087948143735, -105.1189986310474 40.00883908245553, -105.1187095139158 40.00890792962496, -105.1185405381531 40.00890644040241, -105.1181222934217 40.00879838850203, -105.1180058771873 40.00874783898299, -105.116862273694 40.00845912278751, -105.115439060473 40.00840796360136, -105.1149006847169 40.00846983893248, -105.114690116975 40.00858194204327, -105.1145438842861 40.00876316467217, -105.1143214105558 40.00881271895139, -105.1140548223516 40.00872057596153, -105.1139182214054 40.00874268377794, -105.1138595621785 40.00904999000269, -105.1135527848292 40.00915992609273, -105.1125460955506 40.009118545706, -105.1123850954861 40.0092367825163, -105.1123818862575 40.00933650518886, -105.1126167071906 40.00944957839319, -105.1134671916322 40.00971973315597, -105.1137354716539 40.00984934691608, -105.1138816269313 40.00996120182681, -105.1139748795943 40.01016354509047, -105.1139400367938 40.01047445261041, -105.1141717798238 40.01085855805781, -105.1142021579376 40.01090890468547, -105.1142366021811 40.01110200384621, -105.1142013247205 40.01121349713745, -105.1138475779678 40.01162389750351, -105.1136931479484 40.01180305609206, -105.1133509829044 40.01201286862782, -105.1133852018378 40.01249016979386, -105.1120551899672 40.01316817480327, -105.1118169210616 40.01363272390126, -105.1105601717934 40.01435618301711, -105.1105560664339 40.01473943407785, -105.1122469451198 40.01473097961565, -105.1146619125952 40.01472507426003, -105.1156980975397 40.01470903980398, -105.1161868294974 40.01471588399428, -105.1170672978585 40.0147089289058, -105.1181791141706 40.01470300707963, -105.1188578336503 40.01470113439711, -105.1195301011676 40.01470390183892, -105.1214918766175 40.014719966371, -105.1218310758678 40.01471586345145, -105.1218710675092 40.01471489668231, -105.1219249777837 40.01471507343112, -105.1219788956684 40.01471387757833, -105.1224409110659 40.01470990067528, -105.1247659160872 40.01470211478069, -105.1251979466517 40.01469693136669, -105.125677823302 40.01469107754211, -105.1279621437234 40.01468007705167, -105.1293080595201 40.0146940193177, -105.1311049552121 40.0146981347173, -105.1327730822116 40.01468012434484, -105.1340880509 40.01467304856543, -105.1357511197931 40.0146659589759, -105.135810672579 40.01466588316285, -105.1358106759398 40.01466371889595, -105.1358098300447 40.01441792346685, -105.1358084176293 40.01416174617611, -105.1358072921032 40.01389725402277, -105.135806156309 40.01363183505427, -105.1358343250365 40.01363171595667, -105.1358204177624 40.01350958353772, -105.1358050604791 40.01337472476187, -105.1358050413 40.01337020160395, -105.1358050213227 40.01336538933267, -105.135803927714 40.01310830335805, -105.1358026199699 40.01280227681977, -105.1358015338484 40.01254773971242, -105.1357996656098 40.01210916173971, -105.1356620779171 40.01210995833265, -105.1356610401132 40.01210996406044, -105.1324447468638 40.01212852478138, -105.1313466466419 40.01213865468601, -105.131257730989 40.01213947371401, -105.1312570076791 40.01207374506328, -105.1312569842205 40.01207158521304, -105.1311700055415 40.01207226986423, -105.1310979697797 40.0120728383325, -105.1310967316625 40.01207284788168, -105.131091726775 40.01172384982907, -105.1310997144627 40.01070685621357, -105.1311008088521 40.01070634634, -105.1310909392437 40.00956811928324, -105.1310700786464 40.00794700646802, -105.1310778532248 40.0074339520929, -105.1310783415883 40.00740538300349, -105.1310799403458 40.00731207101194, -105.1310812050261 40.0072279023247, -105.1310838449696 40.0070521123623, -105.1310850732638 40.00695713206541, -105.1310878876888 40.00656896854314, -105.1310941022362 40.00641004040492, -105.1310873461379 40.00565936943882, -105.1310844505609 40.00509939167827, -105.1310878320044 40.00360990666242, -105.131093056197 40.00297413289702, -105.1310944311785 40.0023664283858, -105.1310948532135 40.00217994944209, -105.1311086818536 40.0013477354128, -105.1311040366654 40.00107612986969, -105.131103063404 40.00086007783933, -105.1310980615045 40.00072911608232, -105.1310950875115 40.00061902365207, -105.1310749033248 40.00039110612163, -105.1310556496412 40.00019967631347, -105.1302618979046 40.00020779027882, -105.1284524015447 40.00019307950447, -105.1281614002314 40.00019307989155, -105.1278863996462 40.00019607993971))</t>
+          <t>POLYGON ((-105.12788639964619 40.000196079939705, -105.12722872123057 40.000747019034854, -105.12686343164678 40.001089093576205, -105.12603130982697 40.001672835076604, -105.12556738052864 40.00186449358997, -105.12525107194548 40.00190993453685, -105.12483639248099 40.0020944593464, -105.1244795338295 40.002751005028834, -105.12320363653289 40.00356334052815, -105.1232110077422 40.00372316836474, -105.12313045997294 40.00382534596935, -105.12314470794028 40.00415326086031, -105.1230188523702 40.004598959751995, -105.12310290453439 40.004856318310715, -105.12307485287063 40.00489650674073, -105.12269247509171 40.0050751058488, -105.12244213504086 40.0051425824149, -105.12216502406613 40.00518777490752, -105.12189718799517 40.00524509838811, -105.12179931956717 40.00526550337217, -105.12163649954297 40.00532262664415, -105.12159418303489 40.00533747112853, -105.1215377044217 40.00538187734463, -105.12144965355988 40.005330795711075, -105.1213307250641 40.0053580770317, -105.11953271697426 40.00576134809078, -105.1195333961401 40.00583735955976, -105.11903693635668 40.00583079922135, -105.11903298869737 40.00582317381761, -105.11923013319144 40.00668445678808, -105.11940600860623 40.00682009016207, -105.11931972509558 40.00689420959378, -105.11924599387287 40.00693005101848, -105.11924331852944 40.00693157150168, -105.11924097574743 40.006933732550024, -105.11923930440426 40.00693625337662, -105.11923839427497 40.006938997377866, -105.11923829185083 40.00694181880084, -105.11923900854266 40.00694456186928, -105.11924049716151 40.006947077818886, -105.11924542070335 40.00695089665385, -105.11927262325922 40.006964961980536, -105.11942155251948 40.0070419771017, -105.11965267062126 40.00716149139468, -105.11975804647237 40.007448150836986, -105.119540466071 40.007448160895336, -105.11959368832939 40.00762459431621, -105.11969431482844 40.00795817051018, -105.11964417001971 40.008092293194025, -105.1193165119794 40.008679853951755, -105.11908700643215 40.0087948143735, -105.11899863104738 40.00883908245553, -105.1187095139158 40.00890792962496, -105.11854053815308 40.008906440402406, -105.11812229342168 40.00879838850203, -105.11800587718733 40.00874783898299, -105.11686227369401 40.008459122787514, -105.11543906047298 40.008407963601364, -105.1149006847169 40.00846983893248, -105.11469011697498 40.00858194204327, -105.11454388428615 40.00876316467217, -105.11432141055585 40.00881271895139, -105.11405482235156 40.00872057596153, -105.11391822140544 40.00874268377794, -105.11385956217846 40.009049990002694, -105.11355278482921 40.00915992609273, -105.1125460955506 40.009118545705995, -105.11238509548609 40.009236782516304, -105.11238188625752 40.00933650518886, -105.1126167071906 40.009449578393195, -105.11346719163221 40.00971973315597, -105.11373547165385 40.009849346916084, -105.11388162693126 40.00996120182681, -105.11397487959427 40.01016354509047, -105.11394003679385 40.01047445261041, -105.11417177982383 40.01085855805781, -105.11420215793761 40.01090890468547, -105.11423660218112 40.01110200384621, -105.11420132472048 40.011213497137454, -105.11384757796782 40.01162389750351, -105.1136931479484 40.011803056092056, -105.11335098290442 40.01201286862782, -105.11338520183779 40.01249016979386, -105.11205518996721 40.01316817480327, -105.1118169210616 40.01363272390126, -105.11056017179338 40.01435618301711, -105.11055606643392 40.014739434077846, -105.11224694511981 40.01473097961565, -105.11466191259521 40.01472507426003, -105.11569809753966 40.014709039803975, -105.11618682949737 40.01471588399428, -105.11706729785851 40.014708928905804, -105.11817911417056 40.01470300707963, -105.11885783365025 40.014701134397114, -105.11953010116764 40.01470390183892, -105.12149187661747 40.014719966371, -105.12183107586785 40.01471586345145, -105.12187106750919 40.01471489668231, -105.12192497778368 40.01471507343112, -105.12197889566836 40.01471387757833, -105.12244091106588 40.01470990067528, -105.12476591608718 40.01470211478069, -105.12519794665165 40.01469693136669, -105.12567782330197 40.01469107754211, -105.12796214372338 40.01468007705167, -105.12930805952014 40.0146940193177, -105.13110495521214 40.0146981347173, -105.13277308221161 40.01468012434484, -105.13408805089999 40.014673048565434, -105.13575111979314 40.014665958975904, -105.13581067257898 40.01466588316285, -105.13581067593978 40.01466371889595, -105.13580983004466 40.01441792346685, -105.13580841762929 40.014161746176114, -105.1358072921032 40.013897254022766, -105.135806156309 40.01363183505427, -105.13583432503647 40.01363171595667, -105.13582041776242 40.01350958353772, -105.1358050604791 40.01337472476187, -105.13580504130005 40.013370201603955, -105.13580502132265 40.01336538933267, -105.13580392771401 40.013108303358045, -105.13580261996987 40.01280227681977, -105.13580153384838 40.012547739712424, -105.13579966560978 40.01210916173971, -105.13566207791715 40.01210995833265, -105.13566104011323 40.012109964060436, -105.1324447468638 40.01212852478138, -105.13134664664189 40.01213865468601, -105.131257730989 40.01213947371401, -105.13125700767907 40.01207374506328, -105.13125698422046 40.01207158521304, -105.13117000554146 40.012072269864234, -105.13109796977967 40.0120728383325, -105.13109673166252 40.012072847881676, -105.13109172677497 40.01172384982907, -105.1310997144627 40.010706856213574, -105.13110080885212 40.01070634634, -105.1310909392437 40.009568119283244, -105.13107007864642 40.007947006468015, -105.13107785322475 40.0074339520929, -105.13107834158829 40.00740538300349, -105.13107994034577 40.00731207101194, -105.13108120502608 40.0072279023247, -105.1310838449696 40.007052112362295, -105.13108507326379 40.00695713206541, -105.13108788768884 40.00656896854314, -105.13109410223623 40.00641004040492, -105.13108734613792 40.00565936943882, -105.13108445056093 40.00509939167827, -105.13108783200435 40.00360990666242, -105.13109305619696 40.00297413289702, -105.1310944311785 40.0023664283858, -105.13109485321345 40.00217994944209, -105.1311086818536 40.0013477354128, -105.13110403666545 40.001076129869695, -105.13110306340398 40.000860077839334, -105.13109806150453 40.00072911608232, -105.13109508751147 40.00061902365207, -105.13107490332477 40.000391106121626, -105.1310556496412 40.00019967631347, -105.13026189790463 40.00020779027882, -105.12845240154472 40.00019307950447, -105.12816140023142 40.000193079891545, -105.12788639964619 40.000196079939705))</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2138,7 +2146,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1123371190536 40.04651893042601, -105.1123366900865 40.04658012665188, -105.1123366731379 40.04658248811084, -105.1123354147434 40.04676250668771, -105.1123309979452 40.04739433331647, -105.112330888596 40.04741005387065, -105.1123302681899 40.04749872120584, -105.1123296974318 40.0475803086633, -105.1123229001954 40.04855248897933, -105.1123218378891 40.04870461761656, -105.112392173119 40.04869545288748, -105.1127817580233 40.04864540026167, -105.1141782671779 40.04846883077132, -105.1151371742824 40.04834545259219, -105.1159511368379 40.04820936852636, -105.1180384926233 40.04779473006271, -105.1220411513055 40.04703446196407, -105.1244748378258 40.0465721293676, -105.1281644085359 40.04587100599928, -105.1311570490046 40.04532707446116, -105.1311570037658 40.04527134096249, -105.1311569094684 40.04515495007782, -105.1311610113387 40.04406704094007, -105.1311559623812 40.04321793513203, -105.1311510917365 40.04081806645879, -105.1311550651878 40.04047987090068, -105.1311590894281 40.0401320664122, -105.131145064082 40.0398198926297, -105.1311201440057 40.03927708677072, -105.1310990889926 40.03834996598214, -105.1310650469673 40.03738107533779, -105.1310490163915 40.03658189669205, -105.1310000230925 40.02794393773443, -105.1309969825158 40.02794400096061, -105.1309957951422 40.02789410985726, -105.1309909037535 40.02611376122235, -105.1309978878637 40.02485876942394, -105.1310068742717 40.02376277574164, -105.1310048639694 40.0229017810233, -105.1310018638014 40.02277278218614, -105.130998857059 40.02229978498944, -105.131000855409 40.02215978531176, -105.1310015904696 40.02216011730349, -105.131001914456 40.02212688053156, -105.1310111497333 40.02141013649386, -105.1310251261564 40.02021299758439, -105.1310359638921 40.01933209591846, -105.1310380626037 40.01914213441396, -105.131042960859 40.01876495883627, -105.1310575495072 40.01831992727238, -105.1311777798524 40.01832048835271, -105.1311777986908 40.01831830522199, -105.1312431051194 40.01831823124324, -105.1317155406373 40.01831768913188, -105.1320616319306 40.01831728968089, -105.1345297826865 40.01831441593423, -105.1345339076398 40.01830035084866, -105.1355935115999 40.01829732614752, -105.1357992116425 40.01829673750202, -105.1358069737647 40.01716072833008, -105.1358083466995 40.01623507505892, -105.1358091438079 40.01569681831801, -105.1358099276981 40.01516827058219, -105.1358103602851 40.01487676008018, -105.135810672579 40.01466588316285, -105.1357511197931 40.0146659589759, -105.1340880509 40.01467304856543, -105.1327730822116 40.01468012434484, -105.1311049552121 40.0146981347173, -105.1293080595201 40.0146940193177, -105.1279621437234 40.01468007705167, -105.125677823302 40.01469107754211, -105.1251979466517 40.01469693136669, -105.1247659160872 40.01470211478069, -105.1224409110659 40.01470990067528, -105.1219788956684 40.01471387757833, -105.1219249777837 40.01471507343112, -105.1218710675092 40.01471489668231, -105.1218310758678 40.01471586345145, -105.1214918766175 40.014719966371, -105.1195301011676 40.01470390183892, -105.1188578336503 40.01470113439711, -105.1181791141706 40.01470300707963, -105.1170672978585 40.0147089289058, -105.1161868294974 40.01471588399428, -105.1156980975397 40.01470903980398, -105.1146619125952 40.01472507426003, -105.1122469451198 40.01473097961565, -105.1105560664339 40.01473943407785, -105.1080486438543 40.01475192657379, -105.10756828865 40.01475361643449, -105.1074929904923 40.01475388076332, -105.1059210138599 40.01475098945919, -105.1048549288133 40.01475091000491, -105.1045118307443 40.01475000951929, -105.1044218596395 40.01474997564399, -105.104085101401 40.01476391866188, -105.1039339914919 40.01477904602595, -105.1037299656432 40.0148068969059, -105.1034218352742 40.01487089764663, -105.1032709245142 40.01491293018051, -105.1029350211734 40.01499712229778, -105.1029381666813 40.01697244858164, -105.1029531677396 40.0182424491116, -105.1029258020212 40.01922928731726, -105.1028801685531 40.02039944897465, -105.1028411684982 40.02101744933578, -105.1027191685341 40.0229774492492, -105.1026901679704 40.02391744893649, -105.102681714784 40.02523098211869, -105.1026813585937 40.02624327690542, -105.1026851686352 40.02731645051675, -105.1026703866881 40.0282598185744, -105.1026821685567 40.02903745095252, -105.1027065698951 40.02953569354239, -105.1025462936187 40.0295350594423, -105.1025509999655 40.02982099987915, -105.1026589993872 40.0325789998223, -105.1028159251721 40.03659410284713, -105.1028159996535 40.03659599988478, -105.1028159808093 40.03659641862485, -105.1026950932294 40.03923308897296, -105.1026695167741 40.03979091557985, -105.102684106142 40.03979099374556, -105.1026843791355 40.04070640471347, -105.1026843795041 40.04070875362413, -105.1026844241735 40.04085566869285, -105.1026853227765 40.04386122510869, -105.1026792879808 40.04699933304118, -105.1026468422424 40.04711176082813, -105.1026531716483 40.0476534526228, -105.1030171704752 40.04768345267631, -105.1033391709822 40.04790545288033, -105.1037471714223 40.0480454529342, -105.1041869090785 40.04810254797782, -105.1051951720775 40.0482334531068, -105.1056231709406 40.0481744531596, -105.1064479966728 40.0482222769794, -105.1072881721325 40.04830245271919, -105.1075741724027 40.04816445209948, -105.1084266880845 40.04775137397073, -105.109125173029 40.04741245282467, -105.1096111728036 40.0474164516294, -105.1100331727537 40.04752645257917, -105.1103231729248 40.04751845193728, -105.1107256413342 40.047267544397, -105.1111171727025 40.04702345167325, -105.1111851729639 40.04692845194887, -105.1112241729621 40.04694545172396, -105.111576173255 40.04658445258669, -105.1116441732981 40.04653845179544, -105.1117501733669 40.04650145208792, -105.1118461736203 40.04649345213979, -105.1123371190536 40.04651893042601))</t>
+          <t>POLYGON ((-105.11233711905356 40.04651893042601, -105.11233669008645 40.04658012665188, -105.1123366731379 40.04658248811084, -105.11233541474337 40.04676250668771, -105.11233099794522 40.04739433331647, -105.11233088859603 40.04741005387065, -105.11233026818994 40.04749872120584, -105.11232969743182 40.0475803086633, -105.11232290019544 40.04855248897933, -105.1123218378891 40.048704617616565, -105.11239217311903 40.04869545288748, -105.11278175802333 40.04864540026167, -105.11417826717788 40.04846883077132, -105.11513717428244 40.04834545259219, -105.1159511368379 40.04820936852636, -105.1180384926233 40.04779473006271, -105.12204115130554 40.04703446196407, -105.12447483782576 40.046572129367604, -105.12816440853591 40.04587100599928, -105.1311570490046 40.045327074461156, -105.13115700376582 40.045271340962486, -105.13115690946843 40.045154950077816, -105.13116101133868 40.04406704094007, -105.13115596238119 40.04321793513203, -105.1311510917365 40.04081806645879, -105.13115506518781 40.04047987090068, -105.13115908942807 40.0401320664122, -105.13114506408198 40.0398198926297, -105.1311201440057 40.03927708677072, -105.13109908899263 40.03834996598214, -105.1310650469673 40.03738107533779, -105.13104901639146 40.03658189669205, -105.13100002309253 40.027943937734435, -105.13099698251575 40.02794400096061, -105.13099579514224 40.027894109857264, -105.13099090375351 40.02611376122235, -105.13099788786366 40.024858769423936, -105.13100687427173 40.023762775741645, -105.13100486396942 40.0229017810233, -105.13100186380144 40.02277278218614, -105.13099885705896 40.02229978498944, -105.13100085540904 40.02215978531176, -105.13100159046962 40.02216011730349, -105.13100191445596 40.02212688053156, -105.13101114973331 40.021410136493856, -105.13102512615643 40.02021299758439, -105.13103596389206 40.01933209591846, -105.13103806260374 40.01914213441396, -105.13104296085905 40.01876495883627, -105.13105754950722 40.01831992727238, -105.13117777985237 40.018320488352714, -105.13117779869077 40.01831830522199, -105.1312431051194 40.01831823124324, -105.13171554063727 40.018317689131884, -105.13206163193061 40.018317289680894, -105.1345297826865 40.01831441593423, -105.13453390763979 40.01830035084866, -105.13559351159988 40.01829732614752, -105.13579921164248 40.01829673750202, -105.1358069737647 40.017160728330076, -105.13580834669948 40.016235075058916, -105.13580914380788 40.01569681831801, -105.13580992769808 40.015168270582194, -105.13581036028515 40.01487676008018, -105.13581067257898 40.01466588316285, -105.13575111979314 40.014665958975904, -105.13408805089999 40.014673048565434, -105.13277308221161 40.01468012434484, -105.13110495521214 40.0146981347173, -105.12930805952014 40.0146940193177, -105.12796214372338 40.01468007705167, -105.12567782330197 40.01469107754211, -105.12519794665165 40.01469693136669, -105.12476591608718 40.01470211478069, -105.12244091106588 40.01470990067528, -105.12197889566836 40.01471387757833, -105.12192497778368 40.01471507343112, -105.12187106750919 40.01471489668231, -105.12183107586785 40.01471586345145, -105.12149187661747 40.014719966371, -105.11953010116764 40.01470390183892, -105.11885783365025 40.014701134397114, -105.11817911417056 40.01470300707963, -105.11706729785851 40.014708928905804, -105.11618682949737 40.01471588399428, -105.11569809753966 40.014709039803975, -105.11466191259521 40.01472507426003, -105.11224694511981 40.01473097961565, -105.11055606643392 40.014739434077846, -105.10804864385432 40.014751926573794, -105.10756828865004 40.01475361643449, -105.10749299049229 40.014753880763315, -105.10592101385987 40.014750989459195, -105.10485492881331 40.014750910004906, -105.10451183074434 40.01475000951929, -105.10442185963949 40.014749975643994, -105.10408510140103 40.01476391866188, -105.10393399149194 40.01477904602595, -105.10372996564324 40.0148068969059, -105.1034218352742 40.01487089764663, -105.10327092451425 40.01491293018051, -105.1029350211734 40.01499712229778, -105.10293816668126 40.01697244858164, -105.10295316773959 40.0182424491116, -105.10292580202116 40.01922928731726, -105.10288016855306 40.02039944897465, -105.10284116849823 40.02101744933578, -105.1027191685341 40.022977449249204, -105.1026901679704 40.023917448936494, -105.10268171478404 40.02523098211869, -105.10268135859371 40.02624327690542, -105.10268516863519 40.02731645051675, -105.10267038668809 40.028259818574405, -105.1026821685567 40.029037450952515, -105.10270656989513 40.029535693542385, -105.10254629361869 40.0295350594423, -105.10255099996546 40.02982099987915, -105.10265899938722 40.0325789998223, -105.10281592517207 40.036594102847125, -105.10281599965352 40.03659599988478, -105.10281598080928 40.03659641862485, -105.10269509322943 40.03923308897296, -105.10266951677411 40.03979091557985, -105.102684106142 40.03979099374556, -105.1026843791355 40.04070640471347, -105.1026843795041 40.04070875362413, -105.1026844241735 40.04085566869285, -105.10268532277654 40.043861225108685, -105.10267928798083 40.04699933304118, -105.10264684224236 40.04711176082813, -105.1026531716483 40.047653452622804, -105.10301717047521 40.04768345267631, -105.10333917098221 40.04790545288033, -105.10374717142233 40.048045452934204, -105.10418690907845 40.04810254797782, -105.10519517207746 40.0482334531068, -105.10562317094062 40.0481744531596, -105.10644799667284 40.0482222769794, -105.10728817213253 40.04830245271919, -105.10757417240269 40.048164452099485, -105.1084266880845 40.047751373970726, -105.109125173029 40.047412452824666, -105.10961117280355 40.047416451629395, -105.1100331727537 40.04752645257917, -105.11032317292475 40.04751845193728, -105.11072564133424 40.047267544397, -105.11111717270255 40.047023451673255, -105.11118517296391 40.04692845194887, -105.11122417296212 40.046945451723964, -105.11157617325505 40.04658445258669, -105.11164417329809 40.04653845179544, -105.11175017336687 40.046501452087924, -105.11184617362032 40.04649345213979, -105.11233711905356 40.04651893042601))</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2180,7 +2188,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.055531007058 40.00563956685976, -105.0554948489156 40.00752250682681, -105.0554920362152 40.00777826834898, -105.0554887295674 40.00808087222916, -105.0554881852632 40.00812897442378, -105.055488010625 40.00814642135131, -105.0554879813757 40.00814947087598, -105.0554871758176 40.00854380587615, -105.055478575345 40.00901219736176, -105.0554783834164 40.00902816353494, -105.0554777210193 40.00908880877136, -105.0554763115184 40.00921806165778, -105.0554720783693 40.0096054501175, -105.0554725655142 40.00972422301597, -105.0554222037575 40.01418812084223, -105.055416567316 40.01468733327196, -105.0554156695371 40.01476968888103, -105.0554144707321 40.01485168306485, -105.0553212996101 40.02118039422834, -105.0553161721816 40.02152862889884, -105.0553096519419 40.02197149228508, -105.0553704800526 40.02900128894915, -105.0553731474197 40.02930921737802, -105.0553734970732 40.02935099038166, -105.0572990048041 40.02937898721802, -105.0572986143669 40.02932960170075, -105.0590285319982 40.0293478789069, -105.0635752689524 40.02939578802361, -105.0638602058847 40.02939878502951, -105.0649744767153 40.02941049880896, -105.0744113186602 40.02947762086787, -105.0745327172269 40.02945595305492, -105.0745328849534 40.02945592305122, -105.0754018587228 40.02943386962981, -105.0768122923012 40.02942074147485, -105.078005091435 40.02938687123739, -105.0839197303368 40.02931609609333, -105.0931518258988 40.02918620709578, -105.0932781041408 40.02918798359186, -105.093278115994 40.02918422969531, -105.0932811432405 40.02804004205014, -105.0932859305596 40.02747701672733, -105.0932721215243 40.02673905599428, -105.0932701551091 40.0249738796151, -105.0932859333844 40.02448391547184, -105.0932512581774 40.02403870358864, -105.0932461330376 40.02397289158463, -105.0931978680358 40.02392303299272, -105.0930819863873 40.02383505149371, -105.0929940508606 40.02379109266099, -105.0921908756633 40.02357110983468, -105.0917461574974 40.02341909884239, -105.091267170976 40.02320602169296, -105.0909089889242 40.02303399974662, -105.090862035699 40.0230039097498, -105.090748044287 40.02283989095658, -105.0907148656797 40.02259709640494, -105.0907239101849 40.02239892435168, -105.0907700896878 40.02220088405854, -105.0908431657576 40.0220102966353, -105.0838758179136 40.02203417364419, -105.0838785948523 40.02013841703303, -105.0838803806291 40.01891959045461, -105.0838837425258 40.01662393031971, -105.083827279062 40.01474776707985, -105.0827519996697 40.0147379995101, -105.0798880004663 40.01470099918091, -105.0790640003765 40.0146869983785, -105.0787519998548 40.01470499815898, -105.0785220001667 40.0147389989032, -105.0780740000252 40.01483699883885, -105.0778080003735 40.01487099884424, -105.0776729999707 40.01487699919728, -105.0750330000281 40.01486599880874, -105.0744879997328 40.01486699832747, -105.0744939994117 40.01312199935634, -105.0744939996588 40.01117199953493, -105.0744850002892 40.01025499937742, -105.0744959994806 40.00913899920532, -105.0744840014802 40.00754920928831, -105.0744840004529 40.00754899853014, -105.0744840001105 40.00754717649394, -105.0744840001084 40.00718699899353, -105.0744834354184 40.00666768629058, -105.0744829995353 40.0062669990658, -105.0744829989317 40.00626690809695, -105.0744800693377 40.00549913954058, -105.0744799998352 40.00548099818882, -105.0744770000379 40.00485699808893, -105.0744759988608 40.00425899837897, -105.074476815134 40.00421095567354, -105.0744770006211 40.00419999892615, -105.0744768152457 40.00418672611349, -105.0744759999931 40.00412799915949, -105.0744809997915 40.00389299933561, -105.074475000093 40.00379499887224, -105.0744820000614 40.00248399837474, -105.0744799997885 40.0007489983894, -105.074477999321 40.00046599897158, -105.0744775635209 40.00036260693889, -105.0678619251848 40.00037085969463, -105.0640551537651 40.00037580618888, -105.0604611556923 40.00038144912251, -105.0571341561924 40.00545445010541, -105.056107155146 40.00544945007372, -105.0561531550697 40.0055424501676, -105.0561661556522 40.00563345075564, -105.0561221547891 40.00567145049642, -105.0559701557746 40.00568045011807, -105.0559061543596 40.00567545085779, -105.0558361548308 40.00567645117783, -105.0557201558533 40.00567145055776, -105.0556471557209 40.00567245091049, -105.0555902120115 40.00566690495083, -105.0555401553612 40.00564045054492, -105.055531007058 40.00563956685976))</t>
+          <t>POLYGON ((-105.05553100705797 40.005639566859756, -105.0554948489156 40.00752250682681, -105.05549203621517 40.00777826834898, -105.05548872956737 40.00808087222916, -105.05548818526317 40.008128974423784, -105.055488010625 40.00814642135131, -105.05548798137572 40.008149470875985, -105.05548717581763 40.00854380587615, -105.05547857534498 40.009012197361756, -105.05547838341639 40.00902816353494, -105.05547772101929 40.00908880877136, -105.05547631151839 40.009218061657776, -105.05547207836933 40.009605450117505, -105.05547256551421 40.00972422301597, -105.05542220375753 40.014188120842235, -105.05541656731597 40.01468733327196, -105.05541566953706 40.01476968888103, -105.05541447073212 40.01485168306485, -105.05532129961013 40.02118039422834, -105.05531617218165 40.02152862889884, -105.05530965194194 40.02197149228508, -105.0553704800526 40.02900128894915, -105.05537314741967 40.02930921737802, -105.05537349707322 40.02935099038166, -105.05729900480414 40.029378987218024, -105.05729861436693 40.02932960170075, -105.05902853199824 40.029347878906904, -105.06357526895243 40.029395788023606, -105.06386020588465 40.02939878502951, -105.0649744767153 40.029410498808964, -105.07441131866024 40.02947762086787, -105.07453271722687 40.02945595305492, -105.07453288495337 40.02945592305122, -105.07540185872278 40.029433869629806, -105.07681229230116 40.02942074147485, -105.07800509143505 40.029386871237385, -105.08391973033685 40.02931609609333, -105.09315182589883 40.029186207095776, -105.09327810414077 40.02918798359186, -105.09327811599397 40.02918422969531, -105.09328114324053 40.028040042050144, -105.09328593055957 40.02747701672733, -105.09327212152434 40.026739055994284, -105.09327015510911 40.0249738796151, -105.09328593338437 40.02448391547184, -105.09325125817739 40.02403870358864, -105.0932461330376 40.02397289158463, -105.09319786803577 40.02392303299272, -105.09308198638732 40.023835051493705, -105.09299405086063 40.02379109266099, -105.0921908756633 40.023571109834684, -105.09174615749735 40.02341909884239, -105.09126717097601 40.023206021692964, -105.09090898892418 40.02303399974662, -105.09086203569902 40.0230039097498, -105.09074804428701 40.02283989095658, -105.09071486567966 40.02259709640494, -105.09072391018492 40.022398924351684, -105.09077008968781 40.02220088405854, -105.09084316575763 40.0220102966353, -105.08387581791361 40.022034173644194, -105.08387859485227 40.02013841703303, -105.08388038062908 40.01891959045461, -105.08388374252584 40.01662393031971, -105.08382727906202 40.014747767079854, -105.08275199966967 40.014737999510096, -105.07988800046628 40.01470099918091, -105.07906400037653 40.0146869983785, -105.07875199985482 40.014704998158976, -105.07852200016674 40.0147389989032, -105.07807400002524 40.014836998838845, -105.07780800037347 40.01487099884424, -105.07767299997074 40.01487699919728, -105.07503300002809 40.01486599880874, -105.07448799973284 40.01486699832747, -105.07449399941167 40.01312199935634, -105.07449399965881 40.01117199953493, -105.07448500028922 40.01025499937742, -105.07449599948062 40.00913899920532, -105.07448400148016 40.007549209288314, -105.07448400045293 40.00754899853014, -105.07448400011053 40.007547176493944, -105.07448400010841 40.00718699899353, -105.07448343541839 40.00666768629058, -105.07448299953529 40.0062669990658, -105.0744829989317 40.00626690809695, -105.07448006933765 40.005499139540575, -105.07447999983516 40.005480998188816, -105.07447700003787 40.004856998088925, -105.07447599886085 40.00425899837897, -105.07447681513396 40.00421095567354, -105.07447700062106 40.004199998926154, -105.07447681524569 40.00418672611349, -105.07447599999306 40.004127999159486, -105.07448099979149 40.00389299933561, -105.07447500009303 40.003794998872245, -105.07448200006138 40.002483998374736, -105.0744799997885 40.0007489983894, -105.07447799932103 40.000465998971585, -105.07447756352092 40.000362606938886, -105.06786192518477 40.00037085969463, -105.06405515376512 40.000375806188885, -105.06046115569234 40.000381449122514, -105.05713415619238 40.00545445010541, -105.05610715514595 40.00544945007372, -105.05615315506971 40.0055424501676, -105.05616615565222 40.00563345075564, -105.0561221547891 40.00567145049642, -105.05597015577457 40.00568045011807, -105.05590615435958 40.00567545085779, -105.05583615483084 40.005676451177834, -105.05572015585328 40.00567145055776, -105.05564715572095 40.00567245091049, -105.05559021201147 40.00566690495083, -105.05554015536124 40.00564045054492, -105.05553100705797 40.005639566859756))</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2222,7 +2230,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1001890666374 40.0365861357637, -105.1006730215405 40.03658834247638, -105.10169116661 40.03659297910841, -105.1024390289422 40.03659198951182, -105.1025598020035 40.0365934089866, -105.1028149509367 40.0365964060725, -105.1028150546037 40.03659409894916, -105.1028159251721 40.03659410284713, -105.1026589993872 40.0325789998223, -105.1025509999655 40.02982099987915, -105.1025462936187 40.0295350594423, -105.1027065698951 40.02953569354239, -105.1026821685567 40.02903745095252, -105.1026703866881 40.0282598185744, -105.1026851686352 40.02731645051675, -105.1026813585937 40.02624327690542, -105.102681714784 40.02523098211869, -105.1026901679704 40.02391744893649, -105.1027191685341 40.0229774492492, -105.1028411684982 40.02101744933578, -105.1028801685531 40.02039944897465, -105.1029258020212 40.01922928731726, -105.1029531677396 40.0182424491116, -105.1029381666813 40.01697244858164, -105.1029350211734 40.01499712229778, -105.1029321674492 40.01426744896852, -105.1029281665798 40.01109144817353, -105.097693165477 40.01108044794793, -105.0977161660674 40.01340144824596, -105.0968081659261 40.01339944902477, -105.0968210984977 40.01464899904126, -105.0940020010792 40.01467199918716, -105.0933119998438 40.01467099914053, -105.0932924249816 40.01467107691634, -105.0924409249201 40.01467444931598, -105.0905557415763 40.01468189398261, -105.0905289991035 40.0146819917752, -105.0905288819658 40.01468199225995, -105.0865649991523 40.01472399889266, -105.0863749999974 40.01472599885857, -105.0844090000323 40.01474999906352, -105.084343261355 40.01475098794224, -105.084275999784 40.01475199921421, -105.0839630017275 40.01474899892437, -105.0838678605798 40.01474813508104, -105.0838636006166 40.01474809629242, -105.083827279062 40.01474776707985, -105.0838837425258 40.01662393031971, -105.0838803806291 40.01891959045461, -105.0838785948523 40.02013841703303, -105.0838758179136 40.02203417364419, -105.0908431657576 40.0220102966353, -105.0907700896878 40.02220088405854, -105.0907239101849 40.02239892435168, -105.0907148656797 40.02259709640494, -105.090748044287 40.02283989095658, -105.090862035699 40.0230039097498, -105.0909089889242 40.02303399974662, -105.091267170976 40.02320602169296, -105.0917461574974 40.02341909884239, -105.0921908756633 40.02357110983468, -105.0929940508606 40.02379109266099, -105.0930819863873 40.02383505149371, -105.0931978680358 40.02392303299272, -105.0932461330376 40.02397289158463, -105.0932512581774 40.02403870358864, -105.0932859333844 40.02448391547184, -105.0932701551091 40.0249738796151, -105.0932721215243 40.02673905599428, -105.0932859305596 40.02747701672733, -105.0932811432405 40.02804004205014, -105.093278115994 40.02918422969531, -105.0932781041408 40.02918798359186, -105.0932771569118 40.02954604904288, -105.0932771587994 40.02954828538074, -105.0932799187763 40.03315298656989, -105.0932660793007 40.03445498903162, -105.0932498805525 40.03465588098658, -105.0932661500697 40.03641808697719, -105.0932659649652 40.03644910672872, -105.0943030451334 40.03645907211912, -105.0948858479327 40.03646798320575, -105.0967000918928 40.03647406617456, -105.0974501522911 40.03652390280385, -105.0980398279309 40.0365789418307, -105.0981459030162 40.03657793878254, -105.0982648439792 40.03657588254173, -105.1001890666374 40.0365861357637))</t>
+          <t>POLYGON ((-105.10018906663741 40.0365861357637, -105.10067302154054 40.03658834247638, -105.10169116661 40.03659297910841, -105.10243902894221 40.03659198951182, -105.10255980200348 40.036593408986604, -105.10281495093672 40.0365964060725, -105.10281505460367 40.03659409894916, -105.10281592517207 40.036594102847125, -105.10265899938722 40.0325789998223, -105.10255099996546 40.02982099987915, -105.10254629361869 40.0295350594423, -105.10270656989513 40.029535693542385, -105.1026821685567 40.029037450952515, -105.10267038668809 40.028259818574405, -105.10268516863519 40.02731645051675, -105.10268135859371 40.02624327690542, -105.10268171478404 40.02523098211869, -105.1026901679704 40.023917448936494, -105.1027191685341 40.022977449249204, -105.10284116849823 40.02101744933578, -105.10288016855306 40.02039944897465, -105.10292580202116 40.01922928731726, -105.10295316773959 40.0182424491116, -105.10293816668126 40.01697244858164, -105.1029350211734 40.01499712229778, -105.10293216744923 40.01426744896852, -105.10292816657982 40.01109144817353, -105.09769316547703 40.01108044794793, -105.09771616606744 40.013401448245965, -105.09680816592609 40.01339944902477, -105.0968210984977 40.014648999041256, -105.0940020010792 40.01467199918716, -105.09331199984379 40.01467099914053, -105.09329242498157 40.01467107691634, -105.09244092492013 40.01467444931598, -105.09055574157632 40.01468189398261, -105.09052899910351 40.0146819917752, -105.09052888196575 40.01468199225995, -105.0865649991523 40.01472399889266, -105.0863749999974 40.014725998858566, -105.08440900003225 40.01474999906352, -105.08434326135499 40.014750987942236, -105.08427599978398 40.014751999214205, -105.08396300172747 40.01474899892437, -105.08386786057979 40.014748135081035, -105.08386360061655 40.01474809629242, -105.08382727906202 40.014747767079854, -105.08388374252584 40.01662393031971, -105.08388038062908 40.01891959045461, -105.08387859485227 40.02013841703303, -105.08387581791361 40.022034173644194, -105.09084316575763 40.0220102966353, -105.09077008968781 40.02220088405854, -105.09072391018492 40.022398924351684, -105.09071486567966 40.02259709640494, -105.09074804428701 40.02283989095658, -105.09086203569902 40.0230039097498, -105.09090898892418 40.02303399974662, -105.09126717097601 40.023206021692964, -105.09174615749735 40.02341909884239, -105.0921908756633 40.023571109834684, -105.09299405086063 40.02379109266099, -105.09308198638732 40.023835051493705, -105.09319786803577 40.02392303299272, -105.0932461330376 40.02397289158463, -105.09325125817739 40.02403870358864, -105.09328593338437 40.02448391547184, -105.09327015510911 40.0249738796151, -105.09327212152434 40.026739055994284, -105.09328593055957 40.02747701672733, -105.09328114324053 40.028040042050144, -105.09327811599397 40.02918422969531, -105.09327810414077 40.02918798359186, -105.0932771569118 40.02954604904288, -105.09327715879944 40.02954828538074, -105.09327991877633 40.03315298656989, -105.09326607930068 40.03445498903162, -105.09324988055253 40.03465588098658, -105.09326615006967 40.03641808697719, -105.09326596496518 40.036449106728725, -105.09430304513344 40.03645907211912, -105.09488584793274 40.03646798320575, -105.09670009189284 40.036474066174556, -105.09745015229113 40.03652390280385, -105.09803982793088 40.036578941830705, -105.09814590301619 40.036577938782536, -105.09826484397915 40.03657588254173, -105.10018906663741 40.0365861357637))</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2264,7 +2272,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0745197458059 40.0367801358539, -105.0745289562424 40.03678022026028, -105.0764070677692 40.03673899785905, -105.077231076108 40.03670201426075, -105.0778698489772 40.03669412284164, -105.079774076906 40.03664589626428, -105.0799669395501 40.03664495133486, -105.0804430035852 40.03664613519665, -105.0818698528698 40.0366359423162, -105.0821451783561 40.0366410577063, -105.0834706824193 40.0366170265913, -105.0841350419274 40.0366048733181, -105.0845868696259 40.03659799090407, -105.0860072257907 40.03656461893113, -105.0871331521834 40.03656293390402, -105.08791402058 40.03653570070365, -105.088113979198 40.03653641480377, -105.0900346795452 40.03651466058861, -105.09075211339 40.03649704222295, -105.0912858161849 40.03647978094377, -105.0917974218741 40.03646729444759, -105.0925322369786 40.03645559339146, -105.0932659649652 40.03644910672872, -105.0932661500697 40.03641808697719, -105.0932498805525 40.03465588098658, -105.0932660793007 40.03445498903162, -105.0932799187763 40.03315298656989, -105.0932771587994 40.02954828538074, -105.0932771569118 40.02954604904288, -105.0932781041408 40.02918798359186, -105.0931518258988 40.02918620709578, -105.0839197303368 40.02931609609333, -105.078005091435 40.02938687123739, -105.0768122923012 40.02942074147485, -105.0754018587228 40.02943386962981, -105.0745328849534 40.02945592305122, -105.0745327172269 40.02945595305492, -105.0745324669392 40.02959422652986, -105.07453211158 40.02971216726446, -105.0745312391551 40.0300017372458, -105.0745303026692 40.03031264446549, -105.0745295272226 40.03056996853651, -105.0745284945585 40.03091298833388, -105.0745274924888 40.03124528590179, -105.0745265235287 40.0315670215677, -105.0745254894941 40.03191006834344, -105.0745244895618 40.03224220646752, -105.0745233901277 40.03260680211014, -105.0745256901408 40.03304603155402, -105.0745296723356 40.03343238597822, -105.0745325576077 40.03371235248387, -105.0745360980917 40.03405591861951, -105.0745454496656 40.03435658084311, -105.0745529364156 40.03467594643446, -105.0745465685537 40.03504025955956, -105.0745416880214 40.03531945703482, -105.0745375689464 40.03555512314, -105.0745317567318 40.03588764597963, -105.0745257085542 40.03627372821985, -105.0745221593776 40.03657406448868, -105.0745197458059 40.0367801358539))</t>
+          <t>POLYGON ((-105.07451974580589 40.0367801358539, -105.07452895624245 40.03678022026028, -105.07640706776922 40.03673899785905, -105.07723107610796 40.036702014260754, -105.07786984897723 40.03669412284164, -105.07977407690598 40.036645896264275, -105.07996693955012 40.03664495133486, -105.08044300358516 40.036646135196655, -105.0818698528698 40.0366359423162, -105.08214517835614 40.0366410577063, -105.08347068241932 40.0366170265913, -105.08413504192741 40.0366048733181, -105.08458686962594 40.03659799090407, -105.08600722579071 40.03656461893113, -105.08713315218343 40.03656293390402, -105.08791402057996 40.036535700703645, -105.08811397919803 40.03653641480377, -105.09003467954523 40.03651466058861, -105.09075211339 40.036497042222955, -105.0912858161849 40.03647978094377, -105.09179742187409 40.03646729444759, -105.09253223697863 40.03645559339146, -105.09326596496518 40.036449106728725, -105.09326615006967 40.03641808697719, -105.09324988055253 40.03465588098658, -105.09326607930068 40.03445498903162, -105.09327991877633 40.03315298656989, -105.09327715879944 40.02954828538074, -105.0932771569118 40.02954604904288, -105.09327810414077 40.02918798359186, -105.09315182589883 40.029186207095776, -105.08391973033685 40.02931609609333, -105.07800509143505 40.029386871237385, -105.07681229230116 40.02942074147485, -105.07540185872278 40.029433869629806, -105.07453288495337 40.02945592305122, -105.07453271722687 40.02945595305492, -105.07453246693922 40.02959422652986, -105.07453211157996 40.02971216726446, -105.07453123915508 40.030001737245804, -105.07453030266916 40.03031264446549, -105.07452952722255 40.03056996853651, -105.07452849455848 40.03091298833388, -105.07452749248881 40.03124528590179, -105.07452652352866 40.031567021567696, -105.07452548949415 40.031910068343436, -105.07452448956182 40.032242206467515, -105.07452339012772 40.032606802110145, -105.07452569014079 40.03304603155402, -105.07452967233564 40.033432385978216, -105.07453255760765 40.03371235248387, -105.07453609809168 40.03405591861951, -105.07454544966558 40.03435658084311, -105.07455293641564 40.03467594643446, -105.07454656855371 40.03504025955956, -105.07454168802136 40.03531945703482, -105.07453756894638 40.03555512314, -105.07453175673176 40.03588764597963, -105.07452570855419 40.03627372821985, -105.07452215937758 40.03657406448868, -105.07451974580589 40.0367801358539))</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2306,7 +2314,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0554342598844 40.03667252329386, -105.0567282309792 40.03667744940823, -105.0579080811921 40.03668606045213, -105.0584791103931 40.03669291454876, -105.0592820070989 40.03668692582659, -105.0603999597087 40.03670010692939, -105.0614763062396 40.03665985144334, -105.0745197458059 40.0367801358539, -105.0745221593776 40.03657406448868, -105.0745257085542 40.03627372821985, -105.0745317567318 40.03588764597963, -105.0745375689464 40.03555512314, -105.0745416880214 40.03531945703482, -105.0745465685537 40.03504025955956, -105.0745529364156 40.03467594643446, -105.0745454496656 40.03435658084311, -105.0745360980917 40.03405591861951, -105.0745325576077 40.03371235248387, -105.0745296723356 40.03343238597822, -105.0745256901408 40.03304603155402, -105.0745233901277 40.03260680211014, -105.0745244895618 40.03224220646752, -105.0745254894941 40.03191006834344, -105.0745265235287 40.0315670215677, -105.0745274924888 40.03124528590179, -105.0745284945585 40.03091298833388, -105.0745295272226 40.03056996853651, -105.0745303026692 40.03031264446549, -105.0745312391551 40.0300017372458, -105.07453211158 40.02971216726446, -105.0745324669392 40.02959422652986, -105.0745327172269 40.02945595305492, -105.0744113186602 40.02947762086787, -105.0649744767153 40.02941049880896, -105.0638602058847 40.02939878502951, -105.0635752689524 40.02939578802361, -105.0590285319982 40.0293478789069, -105.0572986143669 40.02932960170075, -105.0572990048041 40.02937898721802, -105.0553734970732 40.02935099038166, -105.0553898967095 40.03131800400271, -105.0553916639802 40.0315298997633, -105.0553923068964 40.03160700942662, -105.0554056000837 40.03320149646342, -105.0554208607084 40.03503174441796, -105.0554302318307 40.03615562906905, -105.0554331606792 40.03650690784292, -105.0554338426251 40.03658900636015, -105.0554342598844 40.03667252329386))</t>
+          <t>POLYGON ((-105.05543425988436 40.03667252329386, -105.05672823097918 40.03667744940823, -105.05790808119205 40.03668606045213, -105.05847911039305 40.03669291454876, -105.05928200709886 40.036686925826594, -105.06039995970866 40.03670010692939, -105.0614763062396 40.03665985144334, -105.07451974580589 40.0367801358539, -105.07452215937758 40.03657406448868, -105.07452570855419 40.03627372821985, -105.07453175673176 40.03588764597963, -105.07453756894638 40.03555512314, -105.07454168802136 40.03531945703482, -105.07454656855371 40.03504025955956, -105.07455293641564 40.03467594643446, -105.07454544966558 40.03435658084311, -105.07453609809168 40.03405591861951, -105.07453255760765 40.03371235248387, -105.07452967233564 40.033432385978216, -105.07452569014079 40.03304603155402, -105.07452339012772 40.032606802110145, -105.07452448956182 40.032242206467515, -105.07452548949415 40.031910068343436, -105.07452652352866 40.031567021567696, -105.07452749248881 40.03124528590179, -105.07452849455848 40.03091298833388, -105.07452952722255 40.03056996853651, -105.07453030266916 40.03031264446549, -105.07453123915508 40.030001737245804, -105.07453211157996 40.02971216726446, -105.07453246693922 40.02959422652986, -105.07453271722687 40.02945595305492, -105.07441131866024 40.02947762086787, -105.0649744767153 40.029410498808964, -105.06386020588465 40.02939878502951, -105.06357526895243 40.029395788023606, -105.05902853199824 40.029347878906904, -105.05729861436693 40.02932960170075, -105.05729900480414 40.029378987218024, -105.05537349707322 40.02935099038166, -105.0553898967095 40.03131800400271, -105.05539166398023 40.0315298997633, -105.05539230689637 40.031607009426615, -105.05540560008372 40.03320149646342, -105.05542086070835 40.03503174441796, -105.05543023183073 40.03615562906905, -105.05543316067919 40.03650690784292, -105.0554338426251 40.036589006360146, -105.05543425988436 40.03667252329386))</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2348,7 +2356,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0744558810239 40.05863659313462, -105.0745146859398 40.05863727920769, -105.0756287845519 40.0586107647075, -105.0756894991879 40.05860931995065, -105.0759345299473 40.0586034873418, -105.0792274048168 40.05851918430813, -105.0840087530437 40.05839659701924, -105.0841732933825 40.05839318572592, -105.0841917016195 40.0583944643371, -105.0851360604096 40.0583835004576, -105.0851349998694 40.05767599920211, -105.0851289998757 40.05597599831112, -105.0851359967967 40.05478460759633, -105.0851360005034 40.05478399876696, -105.0854325985144 40.05477981029983, -105.0854899993208 40.0547789996671, -105.0857284081495 40.05477400606802, -105.0870649999386 40.05474599856022, -105.0879790002037 40.05472799853271, -105.0880729992952 40.05472499900154, -105.0884069999753 40.05471499928784, -105.0884071497086 40.05468594109873, -105.0885508936923 40.05468309608522, -105.0885914901302 40.0516029994436, -105.0848306182493 40.05167911626123, -105.0825789135272 40.05166890577286, -105.0818424752722 40.05166555662806, -105.0792302994018 40.05165453321396, -105.0768864024621 40.05164378804999, -105.0768804516109 40.05210105696608, -105.0768805121942 40.05253864336154, -105.0758088773955 40.05253489796397, -105.0758025133187 40.05203938252086, -105.0745544422358 40.05204327532577, -105.0745550182547 40.05163282615113, -105.0744476312415 40.05163232838198, -105.0744476835939 40.05135782403028, -105.0745140122514 40.04769642058474, -105.0745140737896 40.04768787808877, -105.0745140591466 40.04763297404017, -105.0745150628084 40.04735790836305, -105.0745161416358 40.04712786405292, -105.0745168938871 40.04689287663231, -105.0745178991544 40.04678911214037, -105.0745068748686 40.04643795967877, -105.074513026078 40.04499510219038, -105.0745219961443 40.04372986972937, -105.0745238487455 40.0434331192556, -105.0745251445191 40.04334006189931, -105.0745310116858 40.0429151249635, -105.0745328736032 40.04238805228886, -105.0745060347882 40.04125198658492, -105.0745151680207 40.03841594639277, -105.0745110993422 40.03752291552019, -105.0745289562424 40.03678022026028, -105.0745197458059 40.0367801358539, -105.0614763062396 40.03665985144334, -105.0603999597087 40.03670010692939, -105.0592820070989 40.03668692582659, -105.0584791103931 40.03669291454876, -105.0579080811921 40.03668606045213, -105.0567282309792 40.03667744940823, -105.0554342598844 40.03667252329386, -105.0554415609123 40.03816398170832, -105.0554471109753 40.03929767112174, -105.0554558612454 40.04108497102352, -105.0554628576467 40.04251422452845, -105.0554694939043 40.04386956126768, -105.0554691137273 40.04415188527337, -105.0554665087686 40.04601063733477, -105.0554656988988 40.04658897680252, -105.0554654855536 40.04674097808282, -105.0554639797832 40.04781621901886, -105.0554635752588 40.04802681178261, -105.0554617276261 40.04898736880429, -105.0554575802229 40.05114448977547, -105.0554564529153 40.05147054475928, -105.0554825561433 40.05147059848782, -105.0557649381428 40.05147513640274, -105.0561671024448 40.05147989575173, -105.0566950867909 40.05147808230976, -105.0578509647604 40.05149212546669, -105.059021243916 40.05152182856352, -105.0596536702594 40.05154569021519, -105.060527571388 40.05159428800574, -105.0612066207599 40.051637394604, -105.0616823649435 40.05166033756993, -105.0626766229397 40.05173809362753, -105.0640450641673 40.05184511903973, -105.0647501782283 40.05190790061582, -105.0648729526629 40.05192510956043, -105.0648949233701 40.05195291910809, -105.0649101686027 40.05197109509274, -105.0649241510404 40.05201891411187, -105.0649189226959 40.05255805324911, -105.0649221367494 40.0529500804111, -105.0649150734545 40.05428010555752, -105.064950873571 40.05443589368472, -105.0650249526216 40.05458304109962, -105.0651359206932 40.05471605299295, -105.0652400306826 40.05480401695475, -105.0653799385941 40.05488003696146, -105.0654551193627 40.0549110666868, -105.0656419499437 40.0549680466717, -105.0658660782917 40.05500210719094, -105.0663018740834 40.05500786371755, -105.0678552463241 40.05500820379884, -105.0689669641412 40.05500878798364, -105.0727921552727 40.05501505383305, -105.0744698815867 40.05499407560352, -105.0744559393871 40.05625407243888, -105.0744520799825 40.05767305298166, -105.0744531690238 40.05789898721773, -105.0744595602976 40.05850596309622, -105.0744549994243 40.05850599851571, -105.0744558810239 40.05863659313462))</t>
+          <t>POLYGON ((-105.07445588102387 40.05863659313462, -105.07451468593976 40.05863727920769, -105.07562878455187 40.0586107647075, -105.07568949918789 40.05860931995065, -105.07593452994729 40.0586034873418, -105.0792274048168 40.05851918430813, -105.0840087530437 40.05839659701924, -105.08417329338248 40.05839318572592, -105.08419170161949 40.0583944643371, -105.08513606040961 40.0583835004576, -105.0851349998694 40.05767599920211, -105.08512899987574 40.05597599831112, -105.0851359967967 40.05478460759633, -105.0851360005034 40.054783998766965, -105.08543259851439 40.054779810299834, -105.08548999932077 40.0547789996671, -105.0857284081495 40.05477400606802, -105.08706499993858 40.05474599856022, -105.08797900020372 40.05472799853271, -105.08807299929515 40.054724999001536, -105.0884069999753 40.05471499928784, -105.0884071497086 40.05468594109873, -105.08855089369231 40.05468309608522, -105.08859149013016 40.0516029994436, -105.08483061824931 40.05167911626123, -105.08257891352724 40.051668905772864, -105.0818424752722 40.05166555662806, -105.07923029940176 40.05165453321396, -105.07688640246205 40.05164378804999, -105.07688045161093 40.05210105696608, -105.07688051219424 40.052538643361544, -105.07580887739553 40.05253489796397, -105.07580251331868 40.05203938252086, -105.07455444223584 40.052043275325765, -105.07455501825471 40.051632826151135, -105.07444763124147 40.05163232838198, -105.07444768359392 40.05135782403028, -105.07451401225136 40.047696420584735, -105.07451407378959 40.04768787808877, -105.07451405914664 40.04763297404017, -105.07451506280836 40.04735790836305, -105.07451614163583 40.04712786405292, -105.0745168938871 40.046892876632306, -105.07451789915444 40.04678911214037, -105.07450687486865 40.04643795967877, -105.074513026078 40.04499510219038, -105.0745219961443 40.04372986972937, -105.07452384874549 40.043433119255596, -105.07452514451909 40.043340061899315, -105.07453101168578 40.0429151249635, -105.07453287360319 40.042388052288864, -105.07450603478816 40.04125198658492, -105.07451516802074 40.038415946392774, -105.07451109934225 40.037522915520185, -105.07452895624245 40.03678022026028, -105.07451974580589 40.0367801358539, -105.0614763062396 40.03665985144334, -105.06039995970866 40.03670010692939, -105.05928200709886 40.036686925826594, -105.05847911039305 40.03669291454876, -105.05790808119205 40.03668606045213, -105.05672823097918 40.03667744940823, -105.05543425988436 40.03667252329386, -105.05544156091233 40.038163981708315, -105.05544711097534 40.03929767112174, -105.05545586124539 40.041084971023515, -105.0554628576467 40.04251422452845, -105.05546949390434 40.04386956126768, -105.05546911372734 40.044151885273365, -105.05546650876856 40.04601063733477, -105.05546569889884 40.04658897680252, -105.05546548555358 40.04674097808282, -105.05546397978316 40.047816219018856, -105.05546357525881 40.04802681178261, -105.05546172762607 40.04898736880429, -105.05545758022286 40.05114448977547, -105.05545645291525 40.05147054475928, -105.05548255614333 40.051470598487825, -105.05576493814283 40.051475136402736, -105.05616710244476 40.05147989575173, -105.05669508679087 40.051478082309764, -105.05785096476042 40.051492125466694, -105.05902124391599 40.051521828563516, -105.05965367025941 40.05154569021519, -105.06052757138796 40.05159428800574, -105.06120662075986 40.051637394604, -105.06168236494352 40.05166033756993, -105.06267662293969 40.05173809362753, -105.06404506416733 40.05184511903973, -105.06475017822834 40.051907900615824, -105.06487295266287 40.05192510956043, -105.06489492337013 40.05195291910809, -105.06491016860267 40.05197109509274, -105.0649241510404 40.05201891411187, -105.0649189226959 40.052558053249115, -105.06492213674942 40.0529500804111, -105.06491507345453 40.054280105557524, -105.064950873571 40.05443589368472, -105.06502495262156 40.05458304109962, -105.06513592069322 40.05471605299295, -105.0652400306826 40.05480401695475, -105.06537993859413 40.05488003696146, -105.06545511936268 40.0549110666868, -105.06564194994372 40.0549680466717, -105.0658660782917 40.055002107190944, -105.0663018740834 40.05500786371755, -105.06785524632411 40.05500820379884, -105.06896696414115 40.05500878798364, -105.07279215527268 40.05501505383305, -105.0744698815867 40.054994075603524, -105.07445593938705 40.056254072438875, -105.07445207998246 40.057673052981656, -105.07445316902376 40.05789898721773, -105.07445956029761 40.05850596309622, -105.07445499942432 40.05850599851571, -105.07445588102387 40.05863659313462))</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2390,7 +2398,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0758088773955 40.05253489796397, -105.0768805121942 40.05253864336154, -105.0768804516109 40.05210105696608, -105.0768864024621 40.05164378804999, -105.0792302994018 40.05165453321396, -105.0818424752722 40.05166555662806, -105.0825789135272 40.05166890577286, -105.0848306182493 40.05167911626123, -105.0885914901302 40.0516029994436, -105.0885990423906 40.05160299935086, -105.0897789997489 40.05160299875137, -105.0899995756501 40.05159123299453, -105.0900900219845 40.051586407994, -105.0904266303785 40.05157358999863, -105.0907760893881 40.05155550903792, -105.0911249907122 40.051532678592, -105.0914732310975 40.05150510640654, -105.0918207002382 40.05147280380604, -105.0921672901947 40.05143577852198, -105.0925163645043 40.0513944180138, -105.0932005084189 40.05131239020253, -105.0942217990759 40.05117248402676, -105.0943080600169 40.05116066723405, -105.0951703956968 40.0510425272284, -105.0954614821845 40.05100639971867, -105.0977544186944 40.0507217967189, -105.0977558540278 40.05082807537017, -105.097820349445 40.05082178845365, -105.0978899997922 40.05081499888719, -105.0978909739147 40.05092757690758, -105.097891999113 40.05104599855178, -105.09792980189 40.05104626267937, -105.0979703985353 40.05104654643616, -105.0979804876369 40.05104661671356, -105.0979807008552 40.05106073521769, -105.0993629758621 40.05105626527324, -105.0995544225072 40.051055642804, -105.1023431361151 40.05104657071399, -105.1024438386238 40.05104624222915, -105.1026720190462 40.05104549616681, -105.1026732264753 40.05008443806988, -105.1026737105639 40.04980603301352, -105.1026756993881 40.04866973800066, -105.1026752844997 40.04866833515337, -105.1026544039104 40.04765355413717, -105.1026531716483 40.0476534526228, -105.1026515547724 40.04751510558266, -105.1026468422424 40.04711176082813, -105.1026792879808 40.04699933304118, -105.1026853227765 40.04386122510869, -105.1026844241735 40.04085566869285, -105.1026843795041 40.04070875362413, -105.1026843791355 40.04070640471347, -105.102684106142 40.03979099374556, -105.1026695167741 40.03979091557985, -105.1026950932294 40.03923308897296, -105.1028159808093 40.03659641862485, -105.1028159996535 40.03659599988478, -105.1028159251721 40.03659410284713, -105.1028150546037 40.03659409894916, -105.1028149509367 40.0365964060725, -105.1025598020035 40.0365934089866, -105.1024390289422 40.03659198951182, -105.10169116661 40.03659297910841, -105.1006730215405 40.03658834247638, -105.1001890666374 40.0365861357637, -105.0982648439792 40.03657588254173, -105.0981459030162 40.03657793878254, -105.0980398279309 40.0365789418307, -105.0974501522911 40.03652390280385, -105.0967000918928 40.03647406617456, -105.0948858479327 40.03646798320575, -105.0943030451334 40.03645907211912, -105.0932659649652 40.03644910672872, -105.0925322369786 40.03645559339146, -105.0917974218741 40.03646729444759, -105.0912858161849 40.03647978094377, -105.09075211339 40.03649704222295, -105.0900346795452 40.03651466058861, -105.088113979198 40.03653641480377, -105.08791402058 40.03653570070365, -105.0871331521834 40.03656293390402, -105.0860072257907 40.03656461893113, -105.0845868696259 40.03659799090407, -105.0841350419274 40.0366048733181, -105.0834706824193 40.0366170265913, -105.0821451783561 40.0366410577063, -105.0818698528698 40.0366359423162, -105.0804430035852 40.03664613519665, -105.0799669395501 40.03664495133486, -105.079774076906 40.03664589626428, -105.0778698489772 40.03669412284164, -105.077231076108 40.03670201426075, -105.0764070677692 40.03673899785905, -105.0745289562424 40.03678022026028, -105.0745110993422 40.03752291552019, -105.0745151680207 40.03841594639277, -105.0745060347882 40.04125198658492, -105.0745328736032 40.04238805228886, -105.0745310116858 40.0429151249635, -105.0745251445191 40.04334006189931, -105.0745238487455 40.0434331192556, -105.0745219961443 40.04372986972937, -105.074513026078 40.04499510219038, -105.0745068748686 40.04643795967877, -105.0745178991544 40.04678911214037, -105.0745168938871 40.04689287663231, -105.0745161416358 40.04712786405292, -105.0745150628084 40.04735790836305, -105.0745140591466 40.04763297404017, -105.0745140737896 40.04768787808877, -105.0745140122514 40.04769642058474, -105.0744476835939 40.05135782403028, -105.0744476312415 40.05163232838198, -105.0745550182547 40.05163282615113, -105.0745544422358 40.05204327532577, -105.0758025133187 40.05203938252086, -105.0758088773955 40.05253489796397))</t>
+          <t>POLYGON ((-105.07580887739553 40.05253489796397, -105.07688051219424 40.052538643361544, -105.07688045161093 40.05210105696608, -105.07688640246205 40.05164378804999, -105.07923029940176 40.05165453321396, -105.0818424752722 40.05166555662806, -105.08257891352724 40.051668905772864, -105.08483061824931 40.05167911626123, -105.08859149013016 40.0516029994436, -105.08859904239058 40.051602999350855, -105.08977899974894 40.05160299875137, -105.08999957565014 40.05159123299453, -105.09009002198454 40.051586407994, -105.09042663037854 40.05157358999863, -105.09077608938813 40.05155550903792, -105.09112499071216 40.051532678592004, -105.09147323109747 40.051505106406545, -105.09182070023823 40.05147280380604, -105.0921672901947 40.05143577852198, -105.09251636450432 40.0513944180138, -105.09320050841886 40.05131239020253, -105.09422179907592 40.051172484026765, -105.09430806001693 40.05116066723405, -105.09517039569678 40.051042527228404, -105.0954614821845 40.051006399718666, -105.09775441869442 40.050721796718896, -105.09775585402784 40.05082807537017, -105.09782034944497 40.050821788453646, -105.09788999979219 40.05081499888719, -105.09789097391474 40.05092757690758, -105.09789199911299 40.05104599855178, -105.09792980189005 40.05104626267937, -105.09797039853531 40.05104654643616, -105.09798048763695 40.051046616713556, -105.09798070085525 40.05106073521769, -105.09936297586215 40.05105626527324, -105.09955442250721 40.051055642804, -105.10234313611514 40.051046570713986, -105.10244383862376 40.05104624222915, -105.10267201904621 40.05104549616681, -105.10267322647528 40.05008443806988, -105.10267371056392 40.049806033013525, -105.1026756993881 40.04866973800066, -105.10267528449968 40.048668335153366, -105.10265440391039 40.04765355413717, -105.1026531716483 40.047653452622804, -105.10265155477236 40.04751510558266, -105.10264684224236 40.04711176082813, -105.10267928798083 40.04699933304118, -105.10268532277654 40.043861225108685, -105.1026844241735 40.04085566869285, -105.1026843795041 40.04070875362413, -105.1026843791355 40.04070640471347, -105.102684106142 40.03979099374556, -105.10266951677411 40.03979091557985, -105.10269509322943 40.03923308897296, -105.10281598080928 40.03659641862485, -105.10281599965352 40.03659599988478, -105.10281592517207 40.036594102847125, -105.10281505460367 40.03659409894916, -105.10281495093672 40.0365964060725, -105.10255980200348 40.036593408986604, -105.10243902894221 40.03659198951182, -105.10169116661 40.03659297910841, -105.10067302154054 40.03658834247638, -105.10018906663741 40.0365861357637, -105.09826484397915 40.03657588254173, -105.09814590301619 40.036577938782536, -105.09803982793088 40.036578941830705, -105.09745015229113 40.03652390280385, -105.09670009189284 40.036474066174556, -105.09488584793274 40.03646798320575, -105.09430304513344 40.03645907211912, -105.09326596496518 40.036449106728725, -105.09253223697863 40.03645559339146, -105.09179742187409 40.03646729444759, -105.0912858161849 40.03647978094377, -105.09075211339 40.036497042222955, -105.09003467954523 40.03651466058861, -105.08811397919803 40.03653641480377, -105.08791402057996 40.036535700703645, -105.08713315218343 40.03656293390402, -105.08600722579071 40.03656461893113, -105.08458686962594 40.03659799090407, -105.08413504192741 40.0366048733181, -105.08347068241932 40.0366170265913, -105.08214517835614 40.0366410577063, -105.0818698528698 40.0366359423162, -105.08044300358516 40.036646135196655, -105.07996693955012 40.03664495133486, -105.07977407690598 40.036645896264275, -105.07786984897723 40.03669412284164, -105.07723107610796 40.036702014260754, -105.07640706776922 40.03673899785905, -105.07452895624245 40.03678022026028, -105.07451109934225 40.037522915520185, -105.07451516802074 40.038415946392774, -105.07450603478816 40.04125198658492, -105.07453287360319 40.042388052288864, -105.07453101168578 40.0429151249635, -105.07452514451909 40.043340061899315, -105.07452384874549 40.043433119255596, -105.0745219961443 40.04372986972937, -105.074513026078 40.04499510219038, -105.07450687486865 40.04643795967877, -105.07451789915444 40.04678911214037, -105.0745168938871 40.046892876632306, -105.07451614163583 40.04712786405292, -105.07451506280836 40.04735790836305, -105.07451405914664 40.04763297404017, -105.07451407378959 40.04768787808877, -105.07451401225136 40.047696420584735, -105.07444768359392 40.05135782403028, -105.07444763124147 40.05163232838198, -105.07455501825471 40.051632826151135, -105.07455444223584 40.052043275325765, -105.07580251331868 40.05203938252086, -105.07580887739553 40.05253489796397))</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2432,7 +2440,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0554511248211 40.06936354972414, -105.055644999382 40.06936499880712, -105.0572127089671 40.06937197487099, -105.0572179993606 40.06937199876948, -105.0592120002484 40.06940499902917, -105.0593426560375 40.06940674894576, -105.0596331223491 40.06941063787821, -105.0601829990579 40.06941799889565, -105.0603636327102 40.06941982370994, -105.0605789991055 40.06942199934052, -105.0616579986632 40.06943599866338, -105.0619449997488 40.06943899948466, -105.0626028841051 40.06944299951855, -105.0626029989926 40.06944299905324, -105.0649630001291 40.06946799883155, -105.0689249998753 40.0695029995014, -105.0697552004102 40.06950419234072, -105.0697548215246 40.06944946988995, -105.0697544681871 40.06939552840116, -105.0697422175754 40.06752208694817, -105.0697254481382 40.06588984691014, -105.07101418206 40.0658938571426, -105.0712136929241 40.06589447335874, -105.0713346284021 40.06589484424511, -105.0723920732313 40.06589810049037, -105.0736190076878 40.06590186255607, -105.0737394461666 40.06590223088772, -105.0744094543165 40.06590427752417, -105.0744091050698 40.06577459463895, -105.07440818319 40.06450199465363, -105.0744109995861 40.06450299936188, -105.0744899995075 40.06454499905961, -105.0744800018876 40.06401401023398, -105.0744820017798 40.06375103912782, -105.0744819996887 40.06375099859063, -105.074458999274 40.06216599871489, -105.0744577994122 40.06210286921108, -105.0744539992241 40.06190299903914, -105.074454050825 40.06181835300561, -105.0744559985365 40.05865399872508, -105.0744558810239 40.05863659313462, -105.0744549994243 40.05850599851571, -105.0744595602976 40.05850596309622, -105.0744531690238 40.05789898721773, -105.0744520799825 40.05767305298166, -105.0744559393871 40.05625407243888, -105.0744698815867 40.05499407560352, -105.0727921552727 40.05501505383305, -105.0689669641412 40.05500878798364, -105.0678552463241 40.05500820379884, -105.0663018740834 40.05500786371755, -105.0658660782917 40.05500210719094, -105.0656419499437 40.0549680466717, -105.0654551193627 40.0549110666868, -105.0653799385941 40.05488003696146, -105.0652400306826 40.05480401695475, -105.0651359206932 40.05471605299295, -105.0650249526216 40.05458304109962, -105.064950873571 40.05443589368472, -105.0649150734545 40.05428010555752, -105.0649221367494 40.0529500804111, -105.0649189226959 40.05255805324911, -105.0649241510404 40.05201891411187, -105.0649101686027 40.05197109509274, -105.0648949233701 40.05195291910809, -105.0648729526629 40.05192510956043, -105.0647501782283 40.05190790061582, -105.0640450641673 40.05184511903973, -105.0626766229397 40.05173809362753, -105.0616823649435 40.05166033756993, -105.0612066207599 40.051637394604, -105.060527571388 40.05159428800574, -105.0596536702594 40.05154569021519, -105.059021243916 40.05152182856352, -105.0578509647604 40.05149212546669, -105.0566950867909 40.05147808230976, -105.0561671024448 40.05147989575173, -105.0557649381428 40.05147513640274, -105.0554825561433 40.05147059848782, -105.0554564529153 40.05147054475928, -105.0554563122968 40.05151114401765, -105.0554542737668 40.05209778695296, -105.0554580642362 40.05842399669204, -105.0554693891445 40.06582907619643, -105.0554511248211 40.06936354972414))</t>
+          <t>POLYGON ((-105.0554511248211 40.06936354972414, -105.05564499938197 40.06936499880712, -105.05721270896711 40.06937197487099, -105.05721799936057 40.069371998769476, -105.05921200024844 40.069404999029175, -105.05934265603747 40.06940674894576, -105.05963312234911 40.069410637878214, -105.06018299905793 40.06941799889565, -105.06036363271022 40.06941982370994, -105.06057899910549 40.06942199934052, -105.0616579986632 40.06943599866338, -105.06194499974877 40.06943899948466, -105.06260288410506 40.06944299951855, -105.0626029989926 40.06944299905324, -105.0649630001291 40.06946799883155, -105.06892499987532 40.0695029995014, -105.06975520041023 40.069504192340716, -105.06975482152461 40.06944946988995, -105.06975446818713 40.06939552840116, -105.06974221757535 40.067522086948166, -105.06972544813823 40.06588984691014, -105.07101418205995 40.0658938571426, -105.07121369292412 40.06589447335874, -105.07133462840213 40.065894844245115, -105.07239207323133 40.065898100490365, -105.07361900768781 40.065901862556075, -105.07373944616663 40.065902230887716, -105.07440945431648 40.06590427752417, -105.07440910506983 40.065774594638945, -105.07440818318999 40.06450199465363, -105.07441099958606 40.06450299936188, -105.0744899995075 40.06454499905961, -105.07448000188757 40.064014010233976, -105.07448200177983 40.063751039127816, -105.07448199968866 40.063750998590635, -105.07445899927404 40.06216599871489, -105.07445779941216 40.06210286921108, -105.07445399922415 40.06190299903914, -105.07445405082501 40.061818353005606, -105.07445599853646 40.05865399872508, -105.07445588102387 40.05863659313462, -105.07445499942432 40.05850599851571, -105.07445956029761 40.05850596309622, -105.07445316902376 40.05789898721773, -105.07445207998246 40.057673052981656, -105.07445593938705 40.056254072438875, -105.0744698815867 40.054994075603524, -105.07279215527268 40.05501505383305, -105.06896696414115 40.05500878798364, -105.06785524632411 40.05500820379884, -105.0663018740834 40.05500786371755, -105.0658660782917 40.055002107190944, -105.06564194994372 40.0549680466717, -105.06545511936268 40.0549110666868, -105.06537993859413 40.05488003696146, -105.0652400306826 40.05480401695475, -105.06513592069322 40.05471605299295, -105.06502495262156 40.05458304109962, -105.064950873571 40.05443589368472, -105.06491507345453 40.054280105557524, -105.06492213674942 40.0529500804111, -105.0649189226959 40.052558053249115, -105.0649241510404 40.05201891411187, -105.06491016860267 40.05197109509274, -105.06489492337013 40.05195291910809, -105.06487295266287 40.05192510956043, -105.06475017822834 40.051907900615824, -105.06404506416733 40.05184511903973, -105.06267662293969 40.05173809362753, -105.06168236494352 40.05166033756993, -105.06120662075986 40.051637394604, -105.06052757138796 40.05159428800574, -105.05965367025941 40.05154569021519, -105.05902124391599 40.051521828563516, -105.05785096476042 40.051492125466694, -105.05669508679087 40.051478082309764, -105.05616710244476 40.05147989575173, -105.05576493814283 40.051475136402736, -105.05548255614333 40.051470598487825, -105.05545645291525 40.05147054475928, -105.05545631229676 40.051511144017645, -105.05545427376683 40.052097786952956, -105.05545806423616 40.05842399669204, -105.05546938914453 40.06582907619643, -105.0554511248211 40.06936354972414))</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2474,7 +2482,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1026752844997 40.04866833515337, -105.1026756993881 40.04866973800066, -105.1026756688101 40.04868704307379, -105.1026737105639 40.04980603301352, -105.1026732264753 40.05008443806988, -105.1026720190462 40.05104549616681, -105.1024438386238 40.05104624222915, -105.1023431361151 40.05104657071399, -105.0995544225072 40.051055642804, -105.0993629758621 40.05105626527324, -105.0979807008552 40.05106073521769, -105.0979804876369 40.05104661671356, -105.0979703985353 40.05104654643616, -105.09792980189 40.05104626267937, -105.097891999113 40.05104599855178, -105.0978909739147 40.05092757690758, -105.0978899997922 40.05081499888719, -105.097820349445 40.05082178845365, -105.0977558540278 40.05082807537017, -105.0977544186944 40.0507217967189, -105.0954614821845 40.05100639971867, -105.0951703956968 40.0510425272284, -105.0943080600169 40.05116066723405, -105.0942217990759 40.05117248402676, -105.0932005084189 40.05131239020253, -105.0925163645043 40.0513944180138, -105.0921672901947 40.05143577852198, -105.0918207002382 40.05147280380604, -105.0914732310975 40.05150510640654, -105.0911249907122 40.051532678592, -105.0907760893881 40.05155550903792, -105.0904266303785 40.05157358999863, -105.0900900219845 40.051586407994, -105.0899995756501 40.05159123299453, -105.0897789997489 40.05160299875137, -105.0885990423906 40.05160299935086, -105.0885914901302 40.0516029994436, -105.0885508936923 40.05468309608522, -105.0884071497086 40.05468594109873, -105.0884069999753 40.05471499928784, -105.0880729992952 40.05472499900154, -105.0879790002037 40.05472799853271, -105.0870649999386 40.05474599856022, -105.0857284081495 40.05477400606802, -105.0854899993208 40.0547789996671, -105.0854325985144 40.05477981029983, -105.0851360005034 40.05478399876696, -105.0851359967967 40.05478460759633, -105.0851289998757 40.05597599831112, -105.0851349998694 40.05767599920211, -105.0851360604096 40.0583835004576, -105.0841917016195 40.0583944643371, -105.0841732933825 40.05839318572592, -105.0840087530437 40.05839659701924, -105.0792274048168 40.05851918430813, -105.0759345299473 40.0586034873418, -105.0756894991879 40.05860931995065, -105.0756287845519 40.0586107647075, -105.0745146859398 40.05863727920769, -105.0744558810239 40.05863659313462, -105.0744559985365 40.05865399872508, -105.074454050825 40.06181835300561, -105.0744539992241 40.06190299903914, -105.0744577994122 40.06210286921108, -105.074458999274 40.06216599871489, -105.0744819996887 40.06375099859063, -105.0744820017798 40.06375103912782, -105.0744800018876 40.06401401023398, -105.0744899995075 40.06454499905961, -105.0744109995861 40.06450299936188, -105.07440818319 40.06450199465363, -105.0744091050698 40.06577459463895, -105.0744094543165 40.06590427752417, -105.0737394461666 40.06590223088772, -105.0736190076878 40.06590186255607, -105.0723920732313 40.06589810049037, -105.0713346284021 40.06589484424511, -105.0712136929241 40.06589447335874, -105.07101418206 40.0658938571426, -105.0697254481382 40.06588984691014, -105.0697422175754 40.06752208694817, -105.0697544681871 40.06939552840116, -105.0697548215246 40.06944946988995, -105.0697552004102 40.06950419234072, -105.0689249998753 40.0695029995014, -105.0649630001291 40.06946799883155, -105.0626029989926 40.06944299905324, -105.0626028841051 40.06944299951855, -105.0619449997488 40.06943899948466, -105.0616579986632 40.06943599866338, -105.0605789991055 40.06942199934052, -105.0603636327102 40.06941982370994, -105.0601829990579 40.06941799889565, -105.0596331223491 40.06941063787821, -105.0593426560375 40.06940674894576, -105.0592120002484 40.06940499902917, -105.0572179993606 40.06937199876948, -105.0572127089671 40.06937197487099, -105.055644999382 40.06936499880712, -105.0554511248211 40.06936354972414, -105.0554510471109 40.06937851290341, -105.0554524783247 40.07097781636424, -105.0554543197811 40.07301208584704, -105.0554454483656 40.07616858804563, -105.0554393436516 40.07833891985845, -105.0554359155676 40.07955726421665, -105.0554338942331 40.0802760293785, -105.0554120967009 40.08737439782387, -105.0554116626656 40.08751615800497, -105.0554115838102 40.0876056618749, -105.0554235981428 40.09475507605646, -105.0554241217421 40.09570511636053, -105.0554258013926 40.0987667225997, -105.0554275083234 40.10188004134116, -105.0554275553799 40.10196193683294, -105.0554275913097 40.10204463836374, -105.0554283485588 40.10374754276933, -105.0554291707098 40.1055942872819, -105.0554303061645 40.10813983466713, -105.0554307971221 40.10923987562791, -105.0554270937738 40.11409009148291, -105.0554253132042 40.11642002734557, -105.0554252479113 40.11650224198018, -105.0554247936661 40.11658455689023, -105.0554021173245 40.12057908303889, -105.0554011703724 40.12074599216336, -105.0553838251001 40.1238012151376, -105.055364943468 40.13045509249489, -105.0553632754563 40.13104290372788, -105.0553733597693 40.13819028553863, -105.055373432471 40.13824238373312, -105.0553734627153 40.13826344007112, -105.055393108424 40.1382658753683, -105.0570841697421 40.13820687462603, -105.0623920537045 40.13814787912667, -105.0630970281733 40.13814387787887, -105.0644970736709 40.13812287925889, -105.0646163718572 40.1381387740668, -105.0647026837377 40.13816640688852, -105.0647902892207 40.13821288423826, -105.0648822428967 40.13829711858007, -105.0649247890964 40.13837338792121, -105.0649496601588 40.13851303311695, -105.0649012584268 40.13969700518675, -105.0649223983107 40.13978009284535, -105.0649318121612 40.13979936609553, -105.064944699213 40.13982145163131, -105.0650172912994 40.139897965545, -105.0651172543858 40.13995483397098, -105.0652349113323 40.13998458559128, -105.0728341139191 40.13987189343821, -105.0737770801883 40.13984989482434, -105.0742440761428 40.13984499868648, -105.0742413915201 40.13481684621029, -105.0745131984398 40.13479486487819, -105.0762711360049 40.13472286783558, -105.077656234461 40.13468386293215, -105.0799831751011 40.13457186759719, -105.0831630652203 40.13445687173049, -105.0832755753651 40.13446682896835, -105.0846750309919 40.13445787330612, -105.0879403055598 40.13442385884984, -105.0887041365292 40.13437587163286, -105.0899250393446 40.13434187663415, -105.0905391301851 40.13433687298826, -105.0920430472559 40.13429687652557, -105.0927490541487 40.13428987731798, -105.0930212415033 40.13428686643668, -105.0932020045514 40.13427787787717, -105.0940880142722 40.13427987836944, -105.0944050049201 40.13427896522876, -105.0944350199997 40.134278878763, -105.094924071347 40.13427687757695, -105.0960260840791 40.13426087793793, -105.100395113552 40.13418487869186, -105.1024960005596 40.13413300172339, -105.1025130341002 40.13316287731691, -105.1025130798614 40.13316287747433, -105.1025159988629 40.13273999857439, -105.1025160356038 40.13273712294061, -105.1025179999277 40.13258299867876, -105.1025180390099 40.13258012395364, -105.1025200434061 40.13243179457795, -105.1025208956859 40.13236863345693, -105.1025208985428 40.13236854610418, -105.1025210001115 40.13236099904633, -105.1025210274599 40.13235812428076, -105.1025240000488 40.13204399934031, -105.1025240042946 40.13204387506588, -105.1025240297279 40.13204112728457, -105.1025760197128 40.13028913563045, -105.1025799998919 40.12972199930932, -105.102580007196 40.12971914068536, -105.1026009987942 40.12899914491633, -105.1026199748849 40.12780915094283, -105.102613011494 40.1269980044177, -105.1026129788531 40.12699515466171, -105.1026079666242 40.12563116308593, -105.1025933159556 40.12434282390554, -105.1025929997185 40.12431499915309, -105.1025929516966 40.12431217185932, -105.1026069423613 40.12339617624002, -105.1025936013678 40.12274330220411, -105.1025909997468 40.12261599858662, -105.1025909364169 40.1226131811466, -105.1025999247444 40.12158918688989, -105.102589913081 40.12030619389375, -105.1025908978088 40.11877820311115, -105.1025998826839 40.11735921063693, -105.1025918715604 40.11623621837558, -105.1025978687041 40.11595521996043, -105.1026248568706 40.11476822632236, -105.1026358474677 40.11387523166452, -105.1026848320188 40.11217024101816, -105.1027597898385 40.10796526554306, -105.1028087714702 40.10606527686117, -105.1028667414235 40.10313529354308, -105.1028797383626 40.10274829614033, -105.1028947333134 40.10234929813812, -105.1029217180384 40.10077430727056, -105.1029277018902 40.09914531659737, -105.10292669628 40.09859731941704, -105.1029186627907 40.09518334037977, -105.1029176620542 40.09506434040284, -105.1029096529556 40.09419034488765, -105.1028736401172 40.09295735208356, -105.1028446249253 40.09147236144211, -105.1028516136799 40.09036036716439, -105.1028616097687 40.08986237079274, -105.1028735849614 40.087470384517, -105.1028245622727 40.08517239756888, -105.1027735541582 40.08443040191825, -105.1026675453045 40.08346740788972, -105.1026095363755 40.08263041244874, -105.1025615037952 40.07935443077139, -105.1025374854621 40.07766444120318, -105.1025254783728 40.07687944590899, -105.1024964654179 40.07555245356421, -105.1024954463695 40.07365746393571, -105.102470438583 40.07289646909179, -105.1024994253575 40.07160047635688, -105.1025594126134 40.07030448299344, -105.1026054059957 40.06957348809928, -105.102645401495 40.06906149046338, -105.1027803791896 40.06693450274735, -105.1028123634834 40.06542651197705, -105.1028163580333 40.06485551625902, -105.1028123562107 40.06463451646805, -105.1028003500522 40.06390752115306, -105.1027003303502 40.06197953228403, -105.1026813262938 40.06166753369345, -105.1026613204671 40.06104253748129, -105.1026613075969 40.05979754436118, -105.1026703003016 40.05912354872488, -105.1026712996146 40.05898654924477, -105.1026792934692 40.05839155274374, -105.1026842588058 40.05482757360987, -105.1026850856534 40.05469400586137, -105.1030127220029 40.05470170556622, -105.1075213440146 40.05474778494823, -105.1091184618087 40.05475687891815, -105.1091217152768 40.05475689714407, -105.1091259965851 40.05475692155351, -105.1091983627627 40.05475733508034, -105.1093298053343 40.05475796929817, -105.1093501079484 40.05475806865417, -105.1094268000201 40.05475849848371, -105.112295331825 40.05478317236675, -105.1123010373814 40.05261792365371, -105.1123014585939 40.05245819411288, -105.1123014745322 40.05245209673996, -105.1123014812907 40.05244946685348, -105.1123050016747 40.05111258405419, -105.1123209305204 40.04883466002885, -105.1123229001954 40.04855248897933, -105.1123296974318 40.0475803086633, -105.1123302681899 40.04749872120584, -105.112330888596 40.04741005387065, -105.1123309979452 40.04739433331647, -105.1123354147434 40.04676250668771, -105.1123366731379 40.04658248811084, -105.1123366900865 40.04658012665188, -105.1123371190536 40.04651893042601, -105.1118461736203 40.04649345213979, -105.1117501733669 40.04650145208792, -105.1116441732981 40.04653845179544, -105.111576173255 40.04658445258669, -105.1112241729621 40.04694545172396, -105.1111851729639 40.04692845194887, -105.1111171727025 40.04702345167325, -105.1107256413342 40.047267544397, -105.1103231729248 40.04751845193728, -105.1100331727537 40.04752645257917, -105.1096111728036 40.0474164516294, -105.109125173029 40.04741245282467, -105.1084266880845 40.04775137397073, -105.1075741724027 40.04816445209948, -105.1072881721325 40.04830245271919, -105.1064479966728 40.0482222769794, -105.1056231709406 40.0481744531596, -105.1051951720775 40.0482334531068, -105.1041869090785 40.04810254797782, -105.1037471714223 40.0480454529342, -105.1033391709822 40.04790545288033, -105.1030171704752 40.04768345267631, -105.1026544039104 40.04765355413717, -105.1026752844997 40.04866833515337))</t>
+          <t>POLYGON ((-105.10267528449968 40.048668335153366, -105.1026756993881 40.04866973800066, -105.10267566881006 40.04868704307379, -105.10267371056392 40.049806033013525, -105.10267322647528 40.05008443806988, -105.10267201904621 40.05104549616681, -105.10244383862376 40.05104624222915, -105.10234313611514 40.051046570713986, -105.09955442250721 40.051055642804, -105.09936297586215 40.05105626527324, -105.09798070085525 40.05106073521769, -105.09798048763695 40.051046616713556, -105.09797039853531 40.05104654643616, -105.09792980189005 40.05104626267937, -105.09789199911299 40.05104599855178, -105.09789097391474 40.05092757690758, -105.09788999979219 40.05081499888719, -105.09782034944497 40.050821788453646, -105.09775585402784 40.05082807537017, -105.09775441869442 40.050721796718896, -105.0954614821845 40.051006399718666, -105.09517039569678 40.051042527228404, -105.09430806001693 40.05116066723405, -105.09422179907592 40.051172484026765, -105.09320050841886 40.05131239020253, -105.09251636450432 40.0513944180138, -105.0921672901947 40.05143577852198, -105.09182070023823 40.05147280380604, -105.09147323109747 40.051505106406545, -105.09112499071216 40.051532678592004, -105.09077608938813 40.05155550903792, -105.09042663037854 40.05157358999863, -105.09009002198454 40.051586407994, -105.08999957565014 40.05159123299453, -105.08977899974894 40.05160299875137, -105.08859904239058 40.051602999350855, -105.08859149013016 40.0516029994436, -105.08855089369231 40.05468309608522, -105.0884071497086 40.05468594109873, -105.0884069999753 40.05471499928784, -105.08807299929515 40.054724999001536, -105.08797900020372 40.05472799853271, -105.08706499993858 40.05474599856022, -105.0857284081495 40.05477400606802, -105.08548999932077 40.0547789996671, -105.08543259851439 40.054779810299834, -105.0851360005034 40.054783998766965, -105.0851359967967 40.05478460759633, -105.08512899987574 40.05597599831112, -105.0851349998694 40.05767599920211, -105.08513606040961 40.0583835004576, -105.08419170161949 40.0583944643371, -105.08417329338248 40.05839318572592, -105.0840087530437 40.05839659701924, -105.0792274048168 40.05851918430813, -105.07593452994729 40.0586034873418, -105.07568949918789 40.05860931995065, -105.07562878455187 40.0586107647075, -105.07451468593976 40.05863727920769, -105.07445588102387 40.05863659313462, -105.07445599853646 40.05865399872508, -105.07445405082501 40.061818353005606, -105.07445399922415 40.06190299903914, -105.07445779941216 40.06210286921108, -105.07445899927404 40.06216599871489, -105.07448199968866 40.063750998590635, -105.07448200177983 40.063751039127816, -105.07448000188757 40.064014010233976, -105.0744899995075 40.06454499905961, -105.07441099958606 40.06450299936188, -105.07440818318999 40.06450199465363, -105.07440910506983 40.065774594638945, -105.07440945431648 40.06590427752417, -105.07373944616663 40.065902230887716, -105.07361900768781 40.065901862556075, -105.07239207323133 40.065898100490365, -105.07133462840213 40.065894844245115, -105.07121369292412 40.06589447335874, -105.07101418205995 40.0658938571426, -105.06972544813823 40.06588984691014, -105.06974221757535 40.067522086948166, -105.06975446818713 40.06939552840116, -105.06975482152461 40.06944946988995, -105.06975520041023 40.069504192340716, -105.06892499987532 40.0695029995014, -105.0649630001291 40.06946799883155, -105.0626029989926 40.06944299905324, -105.06260288410506 40.06944299951855, -105.06194499974877 40.06943899948466, -105.0616579986632 40.06943599866338, -105.06057899910549 40.06942199934052, -105.06036363271022 40.06941982370994, -105.06018299905793 40.06941799889565, -105.05963312234911 40.069410637878214, -105.05934265603747 40.06940674894576, -105.05921200024844 40.069404999029175, -105.05721799936057 40.069371998769476, -105.05721270896711 40.06937197487099, -105.05564499938197 40.06936499880712, -105.0554511248211 40.06936354972414, -105.05545104711094 40.069378512903405, -105.05545247832467 40.07097781636424, -105.05545431978108 40.07301208584704, -105.05544544836563 40.07616858804563, -105.05543934365164 40.07833891985845, -105.0554359155676 40.079557264216646, -105.05543389423313 40.0802760293785, -105.05541209670088 40.08737439782387, -105.05541166266563 40.08751615800497, -105.05541158381016 40.087605661874896, -105.05542359814284 40.09475507605646, -105.05542412174208 40.095705116360534, -105.05542580139259 40.0987667225997, -105.0554275083234 40.10188004134116, -105.05542755537985 40.101961936832936, -105.05542759130974 40.102044638363736, -105.0554283485588 40.10374754276933, -105.05542917070981 40.105594287281896, -105.05543030616454 40.10813983466713, -105.05543079712206 40.109239875627914, -105.05542709377382 40.11409009148291, -105.05542531320415 40.11642002734557, -105.05542524791129 40.11650224198018, -105.05542479366609 40.11658455689023, -105.0554021173245 40.12057908303889, -105.05540117037238 40.12074599216336, -105.05538382510011 40.123801215137604, -105.05536494346798 40.13045509249489, -105.05536327545626 40.13104290372788, -105.05537335976935 40.138190285538634, -105.055373432471 40.13824238373312, -105.05537346271525 40.13826344007112, -105.05539310842397 40.138265875368305, -105.05708416974208 40.13820687462603, -105.06239205370451 40.13814787912667, -105.06309702817332 40.13814387787887, -105.06449707367086 40.13812287925889, -105.06461637185723 40.1381387740668, -105.06470268373766 40.138166406888516, -105.06479028922067 40.138212884238264, -105.06488224289666 40.13829711858007, -105.06492478909641 40.138373387921206, -105.06494966015882 40.13851303311695, -105.06490125842684 40.139697005186754, -105.06492239831067 40.13978009284535, -105.06493181216116 40.13979936609553, -105.06494469921302 40.13982145163131, -105.06501729129936 40.139897965545, -105.06511725438575 40.139954833970975, -105.06523491133225 40.13998458559128, -105.07283411391913 40.13987189343821, -105.07377708018825 40.139849894824344, -105.07424407614279 40.13984499868648, -105.07424139152015 40.13481684621029, -105.0745131984398 40.13479486487819, -105.07627113600489 40.134722867835585, -105.07765623446096 40.13468386293215, -105.07998317510113 40.13457186759719, -105.08316306522026 40.13445687173049, -105.08327557536505 40.13446682896835, -105.0846750309919 40.13445787330612, -105.0879403055598 40.134423858849836, -105.0887041365292 40.134375871632855, -105.08992503934465 40.134341876634146, -105.09053913018508 40.13433687298826, -105.0920430472559 40.13429687652557, -105.09274905414868 40.134289877317975, -105.0930212415033 40.13428686643668, -105.09320200455142 40.134277877877174, -105.09408801427219 40.13427987836944, -105.09440500492015 40.13427896522876, -105.09443501999968 40.134278878763, -105.09492407134704 40.13427687757695, -105.09602608407914 40.134260877937926, -105.10039511355204 40.13418487869186, -105.10249600055958 40.13413300172339, -105.10251303410024 40.133162877316906, -105.10251307986141 40.133162877474334, -105.10251599886288 40.13273999857439, -105.1025160356038 40.13273712294061, -105.10251799992771 40.132582998678764, -105.10251803900992 40.13258012395364, -105.10252004340607 40.13243179457795, -105.10252089568591 40.13236863345693, -105.1025208985428 40.13236854610418, -105.10252100011147 40.132360999046334, -105.10252102745994 40.132358124280756, -105.10252400004879 40.13204399934031, -105.10252400429462 40.132043875065875, -105.10252402972787 40.132041127284566, -105.1025760197128 40.13028913563045, -105.10257999989194 40.12972199930932, -105.102580007196 40.12971914068536, -105.10260099879417 40.12899914491633, -105.10261997488487 40.12780915094283, -105.10261301149396 40.1269980044177, -105.10261297885306 40.12699515466171, -105.10260796662425 40.125631163085934, -105.10259331595564 40.12434282390554, -105.10259299971851 40.12431499915309, -105.10259295169656 40.124312171859316, -105.1026069423613 40.12339617624002, -105.10259360136781 40.122743302204114, -105.10259099974677 40.122615998586625, -105.10259093641686 40.122613181146605, -105.10259992474438 40.12158918688989, -105.10258991308096 40.12030619389375, -105.10259089780884 40.11877820311115, -105.10259988268386 40.117359210636934, -105.10259187156043 40.11623621837558, -105.1025978687041 40.11595521996043, -105.10262485687056 40.11476822632236, -105.10263584746771 40.113875231664515, -105.10268483201882 40.11217024101816, -105.10275978983849 40.10796526554306, -105.10280877147022 40.10606527686117, -105.10286674142345 40.103135293543076, -105.10287973836265 40.10274829614033, -105.1028947333134 40.102349298138115, -105.10292171803842 40.10077430727056, -105.10292770189017 40.099145316597365, -105.10292669628002 40.09859731941704, -105.1029186627907 40.09518334037977, -105.10291766205424 40.095064340402836, -105.10290965295565 40.09419034488765, -105.10287364011715 40.09295735208356, -105.10284462492532 40.091472361442115, -105.10285161367986 40.090360367164386, -105.10286160976871 40.089862370792744, -105.10287358496144 40.087470384517, -105.10282456227274 40.08517239756888, -105.10277355415825 40.084430401918254, -105.10266754530453 40.08346740788972, -105.10260953637551 40.082630412448744, -105.10256150379522 40.07935443077139, -105.10253748546211 40.07766444120318, -105.10252547837284 40.076879445908986, -105.1024964654179 40.075552453564214, -105.10249544636947 40.07365746393571, -105.102470438583 40.072896469091795, -105.10249942535748 40.071600476356885, -105.10255941261345 40.07030448299344, -105.10260540599575 40.06957348809928, -105.10264540149498 40.06906149046338, -105.1027803791896 40.06693450274735, -105.10281236348342 40.06542651197705, -105.10281635803327 40.064855516259016, -105.10281235621075 40.064634516468054, -105.1028003500522 40.06390752115306, -105.10270033035025 40.06197953228403, -105.10268132629379 40.06166753369345, -105.1026613204671 40.06104253748129, -105.10266130759686 40.05979754436118, -105.10267030030157 40.05912354872488, -105.10267129961463 40.05898654924477, -105.10267929346921 40.05839155274374, -105.10268425880584 40.05482757360987, -105.10268508565343 40.05469400586137, -105.10301272200289 40.05470170556622, -105.1075213440146 40.05474778494823, -105.10911846180872 40.05475687891815, -105.1091217152768 40.054756897144074, -105.10912599658513 40.05475692155351, -105.1091983627627 40.05475733508034, -105.10932980533427 40.054757969298166, -105.10935010794844 40.05475806865417, -105.10942680002015 40.054758498483714, -105.11229533182497 40.054783172366754, -105.11230103738139 40.052617923653706, -105.11230145859389 40.05245819411288, -105.1123014745322 40.052452096739955, -105.11230148129066 40.05244946685348, -105.11230500167467 40.05111258405419, -105.11232093052038 40.04883466002885, -105.11232290019544 40.04855248897933, -105.11232969743182 40.0475803086633, -105.11233026818994 40.04749872120584, -105.11233088859603 40.04741005387065, -105.11233099794522 40.04739433331647, -105.11233541474337 40.04676250668771, -105.1123366731379 40.04658248811084, -105.11233669008645 40.04658012665188, -105.11233711905356 40.04651893042601, -105.11184617362032 40.04649345213979, -105.11175017336687 40.046501452087924, -105.11164417329809 40.04653845179544, -105.11157617325505 40.04658445258669, -105.11122417296212 40.046945451723964, -105.11118517296391 40.04692845194887, -105.11111717270255 40.047023451673255, -105.11072564133424 40.047267544397, -105.11032317292475 40.04751845193728, -105.1100331727537 40.04752645257917, -105.10961117280355 40.047416451629395, -105.109125173029 40.047412452824666, -105.1084266880845 40.047751373970726, -105.10757417240269 40.048164452099485, -105.10728817213253 40.04830245271919, -105.10644799667284 40.0482222769794, -105.10562317094062 40.0481744531596, -105.10519517207746 40.0482334531068, -105.10418690907845 40.04810254797782, -105.10374717142233 40.048045452934204, -105.10333917098221 40.04790545288033, -105.10301717047521 40.04768345267631, -105.10265440391039 40.04765355413717, -105.10267528449968 40.048668335153366))</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2516,7 +2524,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1025160356038 40.13273712294061, -105.1025159988629 40.13273999857439, -105.1025130798614 40.13316287747433, -105.1041803847008 40.13315484466681, -105.1044939964566 40.13312987928641, -105.1055759631424 40.13312799972009, -105.1055759857053 40.13312511863367, -105.1055770144187 40.13300287849541, -105.1085152097078 40.13299386796137, -105.1086315304633 40.13298881317525, -105.1087220040101 40.13297863883014, -105.1088964020049 40.13293936322003, -105.1089796055062 40.13291013523579, -105.1090587413161 40.13287489693305, -105.1091328252846 40.13283461228306, -105.1092018368701 40.13278836166751, -105.1092647735506 40.13273806278027, -105.1093205768746 40.13268270513078, -105.1093585944797 40.13263279385802, -105.1093701834689 40.13263246468068, -105.1096519310758 40.13263086368207, -105.1098582235746 40.1326323161728, -105.1103350195741 40.13263517546018, -105.110591834876 40.13263671418122, -105.1109074261621 40.13263860431368, -105.111021497991 40.13263928746463, -105.1115905511339 40.13264209640875, -105.1119701840193 40.13263846362696, -105.1119769681384 40.13240697386129, -105.1119826842302 40.13221195301501, -105.1119871837674 40.13205846401782, -105.1121931826917 40.1319974642461, -105.1122250359624 40.13198450641528, -105.1122248807698 40.13196726034626, -105.1126460873139 40.13184417366759, -105.1130752163228 40.13171876581113, -105.1134884683498 40.13159766957149, -105.1138787565874 40.13160434794801, -105.1142691989206 40.13161076343259, -105.1146592764502 40.13161717097666, -105.1150500767831 40.13162358771766, -105.1152464520673 40.13162554514241, -105.1155191846595 40.13164146329787, -105.1167491843696 40.13166446387874, -105.1167582823744 40.13069277850736, -105.1190737172402 40.13069586675535, -105.1190789667365 40.13069587415787, -105.1190837455796 40.13069590702754, -105.1196690057948 40.13069987439082, -105.1214287020073 40.13069788718315, -105.1214388421045 40.13069787537972, -105.1214389852497 40.1306978758488, -105.125637981124 40.13071087844324, -105.1295199780874 40.13072688132058, -105.129739962766 40.13072788110647, -105.1308018207651 40.13073588184478, -105.131019817435 40.13074388165322, -105.1310483145869 40.12882902900039, -105.1310573131 40.12712102857881, -105.1310553132711 40.12555802887955, -105.1310483121341 40.12350602835088, -105.1310413121898 40.12134002807184, -105.131030312504 40.11993502837323, -105.1310243109556 40.11903302886184, -105.1310173108496 40.11649802904655, -105.1310173105552 40.11642102922118, -105.1310173486831 40.11641334503174, -105.1310183122412 40.11621802952327, -105.1310553120431 40.11535402919674, -105.1311303117171 40.114313029054, -105.1311973097867 40.11310902852121, -105.1312113114617 40.11250802867715, -105.1312403110973 40.11140002800153, -105.1312733098291 40.11046202797889, -105.1312713110947 40.10989302815075, -105.1313063115642 40.10894602876141, -105.1313783109039 40.10663902806576, -105.1314603103063 40.10285102851227, -105.1314613102898 40.1017110280084, -105.1314743099729 40.09982802847355, -105.1314753089459 40.09960702888224, -105.13149630911 40.09849502893818, -105.1315033084531 40.09835802848521, -105.1315413093822 40.09489902827075, -105.1315353089882 40.09441602918015, -105.1315713090677 40.09267102844738, -105.131565308569 40.09121302826923, -105.1315573093293 40.09073602900505, -105.1315123076631 40.08860202899108, -105.1315023083889 40.0879120286511, -105.1314686920482 40.08736528489368, -105.1314681373808 40.08736529032833, -105.1314680581192 40.08735891798165, -105.1314231385745 40.08373028926654, -105.1314141381591 40.08325728973681, -105.1314061367591 40.0827892910741, -105.131364137045 40.08008229048873, -105.1313161362929 40.07558629064913, -105.1313121353605 40.07453929131646, -105.1313291354456 40.07367829108345, -105.1312771363536 40.07281128908546, -105.1312769801043 40.07280485163446, -105.1312471358889 40.07157529118987, -105.131250135106 40.07142728958371, -105.1312561355187 40.07114629121654, -105.1312571353166 40.07052429035368, -105.1312471352586 40.06877329065517, -105.1312421349654 40.06840629078298, -105.1312311345578 40.06758328902276, -105.1312181355008 40.06555429029728, -105.1312261348082 40.06486429056906, -105.1312161352539 40.06423529025914, -105.131220135557 40.06361729016729, -105.131234134076 40.06223529081105, -105.1312291345053 40.06187129073018, -105.1312251347958 40.06072029049393, -105.1312141343774 40.06023929086055, -105.1312201340746 40.06002129004976, -105.131228134939 40.05974929071716, -105.1312141338369 40.05887029037866, -105.1312131325501 40.05874928993782, -105.1312051349296 40.05727829088557, -105.131207134803 40.05564929051275, -105.1312061330529 40.05519229072108, -105.1312051341252 40.0549272902714, -105.1312151333568 40.05463829014283, -105.1312059997651 40.05463199871355, -105.1312034302793 40.05463055486094, -105.1312141679244 40.05437597462971, -105.131216169747 40.05413797270889, -105.1312209170923 40.05372291390245, -105.131211005441 40.05265005956795, -105.1312107819624 40.05257722664825, -105.131205846102 40.05096312075745, -105.1311931055019 40.05054498601775, -105.1311891001171 40.04930496819956, -105.1311841143478 40.04824612972813, -105.1311790599092 40.04779398012801, -105.1311759744774 40.04744011431053, -105.1311661736642 40.04661103317486, -105.1311558744463 40.04547805719804, -105.1311570490046 40.04532707446116, -105.1281644085359 40.04587100599928, -105.1244748378258 40.0465721293676, -105.1220411513055 40.04703446196407, -105.1180384926233 40.04779473006271, -105.1159511368379 40.04820936852636, -105.1151371742824 40.04834545259219, -105.1141782671779 40.04846883077132, -105.1127817580233 40.04864540026167, -105.112392173119 40.04869545288748, -105.1123218378891 40.04870461761656, -105.1123209305204 40.04883466002885, -105.1123050016747 40.05111258405419, -105.1123014812907 40.05244946685348, -105.1123014745322 40.05245209673996, -105.1123014585939 40.05245819411288, -105.1123010373814 40.05261792365371, -105.112295331825 40.05478317236675, -105.1094268000201 40.05475849848371, -105.1093501079484 40.05475806865417, -105.1093298053343 40.05475796929817, -105.1091983627627 40.05475733508034, -105.1091259965851 40.05475692155351, -105.1091217152768 40.05475689714407, -105.1091184618087 40.05475687891815, -105.1075213440146 40.05474778494823, -105.1030127220029 40.05470170556622, -105.1026850856534 40.05469400586137, -105.1026842588058 40.05482757360987, -105.1026792934692 40.05839155274374, -105.1026712996146 40.05898654924477, -105.1026703003016 40.05912354872488, -105.1026613075969 40.05979754436118, -105.1026613204671 40.06104253748129, -105.1026813262938 40.06166753369345, -105.1027003303502 40.06197953228403, -105.1028003500522 40.06390752115306, -105.1028123562107 40.06463451646805, -105.1028163580333 40.06485551625902, -105.1028123634834 40.06542651197705, -105.1027803791896 40.06693450274735, -105.102645401495 40.06906149046338, -105.1026054059957 40.06957348809928, -105.1025594126134 40.07030448299344, -105.1024994253575 40.07160047635688, -105.102470438583 40.07289646909179, -105.1024954463695 40.07365746393571, -105.1024964654179 40.07555245356421, -105.1025254783728 40.07687944590899, -105.1025374854621 40.07766444120318, -105.1025615037952 40.07935443077139, -105.1026095363755 40.08263041244874, -105.1026675453045 40.08346740788972, -105.1027735541582 40.08443040191825, -105.1028245622727 40.08517239756888, -105.1028735849614 40.087470384517, -105.1028616097687 40.08986237079274, -105.1028516136799 40.09036036716439, -105.1028446249253 40.09147236144211, -105.1028736401172 40.09295735208356, -105.1029096529556 40.09419034488765, -105.1029176620542 40.09506434040284, -105.1029186627907 40.09518334037977, -105.10292669628 40.09859731941704, -105.1029277018902 40.09914531659737, -105.1029217180384 40.10077430727056, -105.1028947333134 40.10234929813812, -105.1028797383626 40.10274829614033, -105.1028667414235 40.10313529354308, -105.1028087714702 40.10606527686117, -105.1027597898385 40.10796526554306, -105.1026848320188 40.11217024101816, -105.1026358474677 40.11387523166452, -105.1026248568706 40.11476822632236, -105.1025978687041 40.11595521996043, -105.1025918715604 40.11623621837558, -105.1025998826839 40.11735921063693, -105.1025908978088 40.11877820311115, -105.102589913081 40.12030619389375, -105.1025999247444 40.12158918688989, -105.1025909364169 40.1226131811466, -105.1025909997468 40.12261599858662, -105.1025936013678 40.12274330220411, -105.1026069423613 40.12339617624002, -105.1025929516966 40.12431217185932, -105.1025929997185 40.12431499915309, -105.1025933159556 40.12434282390554, -105.1026079666242 40.12563116308593, -105.1026129788531 40.12699515466171, -105.102613011494 40.1269980044177, -105.1026199748849 40.12780915094283, -105.1026009987942 40.12899914491633, -105.102580007196 40.12971914068536, -105.1025799998919 40.12972199930932, -105.1025760197128 40.13028913563045, -105.1025240297279 40.13204112728457, -105.1025240042946 40.13204387506588, -105.1025240000488 40.13204399934031, -105.1025210274599 40.13235812428076, -105.1025210001115 40.13236099904633, -105.1025208985428 40.13236854610418, -105.1025208956859 40.13236863345693, -105.1025200434061 40.13243179457795, -105.1025180390099 40.13258012395364, -105.1025179999277 40.13258299867876, -105.1025160356038 40.13273712294061))</t>
+          <t>POLYGON ((-105.1025160356038 40.13273712294061, -105.10251599886288 40.13273999857439, -105.10251307986141 40.133162877474334, -105.10418038470081 40.133154844666805, -105.10449399645664 40.133129879286415, -105.10557596314243 40.13312799972009, -105.10557598570526 40.13312511863367, -105.10557701441869 40.13300287849541, -105.10851520970782 40.13299386796137, -105.10863153046331 40.13298881317525, -105.10872200401013 40.13297863883014, -105.10889640200492 40.132939363220025, -105.10897960550622 40.13291013523579, -105.10905874131613 40.13287489693305, -105.10913282528465 40.13283461228306, -105.10920183687014 40.13278836166751, -105.10926477355065 40.13273806278027, -105.1093205768746 40.132682705130776, -105.1093585944797 40.13263279385802, -105.10937018346885 40.13263246468068, -105.10965193107583 40.13263086368207, -105.10985822357458 40.132632316172796, -105.11033501957412 40.13263517546018, -105.11059183487598 40.132636714181224, -105.11090742616213 40.13263860431368, -105.11102149799099 40.13263928746463, -105.11159055113394 40.13264209640875, -105.11197018401934 40.13263846362696, -105.11197696813835 40.132406973861286, -105.11198268423017 40.13221195301501, -105.11198718376741 40.13205846401782, -105.1121931826917 40.1319974642461, -105.11222503596242 40.13198450641528, -105.11222488076984 40.13196726034626, -105.11264608731393 40.13184417366759, -105.11307521632277 40.13171876581113, -105.11348846834984 40.13159766957149, -105.11387875658743 40.13160434794801, -105.11426919892061 40.13161076343259, -105.11465927645017 40.13161717097666, -105.1150500767831 40.131623587717655, -105.11524645206731 40.131625545142406, -105.11551918465949 40.13164146329787, -105.11674918436962 40.131664463878735, -105.11675828237443 40.13069277850736, -105.11907371724016 40.130695866755346, -105.11907896673645 40.130695874157865, -105.1190837455796 40.130695907027544, -105.11966900579479 40.13069987439082, -105.12142870200725 40.13069788718315, -105.12143884210452 40.130697875379724, -105.12143898524974 40.1306978758488, -105.12563798112399 40.13071087844324, -105.12951997808737 40.130726881320584, -105.12973996276604 40.13072788110647, -105.13080182076511 40.13073588184478, -105.13101981743496 40.130743881653224, -105.13104831458692 40.12882902900039, -105.13105731309996 40.12712102857881, -105.13105531327106 40.125558028879546, -105.13104831213407 40.12350602835088, -105.1310413121898 40.12134002807184, -105.13103031250398 40.11993502837323, -105.13102431095558 40.119033028861836, -105.13101731084956 40.11649802904655, -105.13101731055518 40.11642102922118, -105.13101734868309 40.11641334503174, -105.13101831224118 40.116218029523274, -105.13105531204309 40.11535402919674, -105.13113031171706 40.114313029053996, -105.13119730978674 40.11310902852121, -105.1312113114617 40.11250802867715, -105.13124031109733 40.111400028001526, -105.13127330982914 40.11046202797889, -105.13127131109465 40.10989302815075, -105.13130631156417 40.10894602876141, -105.13137831090386 40.106639028065764, -105.13146031030627 40.10285102851227, -105.13146131028984 40.101711028008395, -105.13147430997293 40.09982802847355, -105.13147530894588 40.09960702888224, -105.13149630910998 40.09849502893818, -105.13150330845312 40.09835802848521, -105.13154130938224 40.09489902827075, -105.13153530898825 40.094416029180145, -105.13157130906771 40.092671028447384, -105.13156530856897 40.09121302826923, -105.13155730932927 40.09073602900505, -105.13151230766312 40.08860202899108, -105.13150230838892 40.0879120286511, -105.13146869204817 40.08736528489368, -105.13146813738082 40.08736529032833, -105.13146805811917 40.087358917981646, -105.13142313857455 40.08373028926654, -105.13141413815906 40.083257289736814, -105.1314061367591 40.0827892910741, -105.13136413704501 40.080082290488726, -105.13131613629291 40.07558629064913, -105.1313121353605 40.074539291316455, -105.13132913544558 40.07367829108345, -105.13127713635365 40.07281128908546, -105.13127698010429 40.07280485163446, -105.13124713588887 40.07157529118987, -105.13125013510601 40.07142728958371, -105.13125613551865 40.071146291216536, -105.1312571353166 40.07052429035368, -105.13124713525865 40.068773290655166, -105.13124213496536 40.06840629078298, -105.13123113455781 40.06758328902276, -105.13121813550079 40.06555429029728, -105.13122613480824 40.06486429056906, -105.13121613525388 40.06423529025914, -105.13122013555704 40.06361729016729, -105.13123413407604 40.062235290811046, -105.13122913450528 40.06187129073018, -105.13122513479581 40.060720290493926, -105.13121413437736 40.06023929086055, -105.13122013407462 40.06002129004976, -105.13122813493895 40.059749290717164, -105.1312141338369 40.058870290378664, -105.13121313255013 40.05874928993782, -105.13120513492963 40.05727829088557, -105.13120713480302 40.055649290512754, -105.13120613305291 40.05519229072108, -105.13120513412518 40.0549272902714, -105.13121513335679 40.05463829014283, -105.13120599976514 40.05463199871355, -105.13120343027933 40.05463055486094, -105.13121416792443 40.054375974629714, -105.131216169747 40.054137972708894, -105.13122091709235 40.053722913902455, -105.13121100544105 40.052650059567945, -105.13121078196237 40.05257722664825, -105.13120584610205 40.05096312075745, -105.13119310550192 40.050544986017755, -105.13118910011711 40.04930496819956, -105.13118411434779 40.048246129728135, -105.13117905990921 40.04779398012801, -105.13117597447743 40.047440114310525, -105.13116617366418 40.046611033174855, -105.13115587444632 40.04547805719804, -105.1311570490046 40.045327074461156, -105.12816440853591 40.04587100599928, -105.12447483782576 40.046572129367604, -105.12204115130554 40.04703446196407, -105.1180384926233 40.04779473006271, -105.1159511368379 40.04820936852636, -105.11513717428244 40.04834545259219, -105.11417826717788 40.04846883077132, -105.11278175802333 40.04864540026167, -105.11239217311903 40.04869545288748, -105.1123218378891 40.048704617616565, -105.11232093052038 40.04883466002885, -105.11230500167467 40.05111258405419, -105.11230148129066 40.05244946685348, -105.1123014745322 40.052452096739955, -105.11230145859389 40.05245819411288, -105.11230103738139 40.052617923653706, -105.11229533182497 40.054783172366754, -105.10942680002015 40.054758498483714, -105.10935010794844 40.05475806865417, -105.10932980533427 40.054757969298166, -105.1091983627627 40.05475733508034, -105.10912599658513 40.05475692155351, -105.1091217152768 40.054756897144074, -105.10911846180872 40.05475687891815, -105.1075213440146 40.05474778494823, -105.10301272200289 40.05470170556622, -105.10268508565343 40.05469400586137, -105.10268425880584 40.05482757360987, -105.10267929346921 40.05839155274374, -105.10267129961463 40.05898654924477, -105.10267030030157 40.05912354872488, -105.10266130759686 40.05979754436118, -105.1026613204671 40.06104253748129, -105.10268132629379 40.06166753369345, -105.10270033035025 40.06197953228403, -105.1028003500522 40.06390752115306, -105.10281235621075 40.064634516468054, -105.10281635803327 40.064855516259016, -105.10281236348342 40.06542651197705, -105.1027803791896 40.06693450274735, -105.10264540149498 40.06906149046338, -105.10260540599575 40.06957348809928, -105.10255941261345 40.07030448299344, -105.10249942535748 40.071600476356885, -105.102470438583 40.072896469091795, -105.10249544636947 40.07365746393571, -105.1024964654179 40.075552453564214, -105.10252547837284 40.076879445908986, -105.10253748546211 40.07766444120318, -105.10256150379522 40.07935443077139, -105.10260953637551 40.082630412448744, -105.10266754530453 40.08346740788972, -105.10277355415825 40.084430401918254, -105.10282456227274 40.08517239756888, -105.10287358496144 40.087470384517, -105.10286160976871 40.089862370792744, -105.10285161367986 40.090360367164386, -105.10284462492532 40.091472361442115, -105.10287364011715 40.09295735208356, -105.10290965295565 40.09419034488765, -105.10291766205424 40.095064340402836, -105.1029186627907 40.09518334037977, -105.10292669628002 40.09859731941704, -105.10292770189017 40.099145316597365, -105.10292171803842 40.10077430727056, -105.1028947333134 40.102349298138115, -105.10287973836265 40.10274829614033, -105.10286674142345 40.103135293543076, -105.10280877147022 40.10606527686117, -105.10275978983849 40.10796526554306, -105.10268483201882 40.11217024101816, -105.10263584746771 40.113875231664515, -105.10262485687056 40.11476822632236, -105.1025978687041 40.11595521996043, -105.10259187156043 40.11623621837558, -105.10259988268386 40.117359210636934, -105.10259089780884 40.11877820311115, -105.10258991308096 40.12030619389375, -105.10259992474438 40.12158918688989, -105.10259093641686 40.122613181146605, -105.10259099974677 40.122615998586625, -105.10259360136781 40.122743302204114, -105.1026069423613 40.12339617624002, -105.10259295169656 40.124312171859316, -105.10259299971851 40.12431499915309, -105.10259331595564 40.12434282390554, -105.10260796662425 40.125631163085934, -105.10261297885306 40.12699515466171, -105.10261301149396 40.1269980044177, -105.10261997488487 40.12780915094283, -105.10260099879417 40.12899914491633, -105.102580007196 40.12971914068536, -105.10257999989194 40.12972199930932, -105.1025760197128 40.13028913563045, -105.10252402972787 40.132041127284566, -105.10252400429462 40.132043875065875, -105.10252400004879 40.13204399934031, -105.10252102745994 40.132358124280756, -105.10252100011147 40.132360999046334, -105.1025208985428 40.13236854610418, -105.10252089568591 40.13236863345693, -105.10252004340607 40.13243179457795, -105.10251803900992 40.13258012395364, -105.10251799992771 40.132582998678764, -105.1025160356038 40.13273712294061))</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2558,7 +2566,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.174943929118 40.00016597541908, -105.1755389603882 40.00016710290019, -105.176907147349 40.00016792502332, -105.1781569577279 40.00014094854438, -105.1793810524402 40.00011690691521, -105.1801420832138 40.00011407962215, -105.1811590475376 40.00011113122423, -105.1840981545727 40.00011510349158, -105.1906400392679 40.00010099696486, -105.1908131549582 40.00010201071742, -105.193474990138 40.00010170190278, -105.1934732468954 39.99998381946754, -105.1934576319139 39.99892492757701, -105.1964298760536 39.99604846059979, -105.1990257041367 39.99355631287658, -105.2029582688417 39.99342377712174, -105.2033772696824 39.99340858016221, -105.2125093588739 39.99318486329975, -105.2126539990297 39.99178199891079, -105.2126889998817 39.99139699911375, -105.2127249983793 39.99099299884455, -105.2127899996551 39.99032999898677, -105.2128229998723 39.98972899884425, -105.2128209981865 39.98794399929118, -105.212820998313 39.98749399914585, -105.212819999065 39.9874409984555, -105.2128199983129 39.98714499875833, -105.2128409991863 39.98614399888426, -105.2128408265147 39.98613467486216, -105.2128393984281 39.98605755172515, -105.212838999747 39.98603599893198, -105.2128335385606 39.98575351525029, -105.2128209987258 39.98510499896647, -105.2128219705335 39.98490281397867, -105.2128239999816 39.98447999876575, -105.2128279999043 39.98376599906238, -105.2128298606279 39.98346834759489, -105.212830000377 39.98344599815635, -105.2128303968119 39.98311209701794, -105.21283300067 39.9809199993889, -105.2128330007686 39.98049724201171, -105.212833000599 39.98012599947322, -105.2128395034223 39.98012199063935, -105.2128301877808 39.97808843595108, -105.2149131886728 39.97773343595954, -105.2160471505688 39.97825984715396, -105.2161149998271 39.9782349994438, -105.216200462426 39.97812263862686, -105.214956998355 39.97754499902697, -105.2135299983809 39.97688599922395, -105.2133739976538 39.97681299863746, -105.2131699989533 39.97671799874688, -105.2128311259303 39.97656205643337, -105.21283099974 39.97656199847693, -105.2101649988539 39.97532799912825, -105.2096699996618 39.9751049989255, -105.2093549990471 39.97496399882614, -105.2090049985782 39.97480699849135, -105.2087029993851 39.97467099834954, -105.2070459994989 39.9739889990676, -105.2048370000834 39.97313299845037, -105.2041369988925 39.97286199893107, -105.2034419994515 39.97259099900295, -105.2027290000227 39.97231199833313, -105.2014580003957 39.9718209988399, -105.1994079998071 39.97102099847267, -105.1989119987643 39.97083099883623, -105.1983979997043 39.9706339986794, -105.194591998727 39.96914999847615, -105.1918849995989 39.96810099902086, -105.1911419992523 39.96781299893013, -105.1901129992968 39.96740799898152, -105.1892829988523 39.96708899899218, -105.1886569997244 39.96684799823526, -105.1878959996133 39.96655099935374, -105.1847509988542 39.96532799810699, -105.1845030591753 39.96523090136483, -105.1845014339616 39.96523026465304, -105.184378790729 39.9663747723468, -105.1843769878934 39.96809980246061, -105.1834828991021 39.96810018023088, -105.1826965883272 39.96810050650755, -105.1827049815247 39.96884194995791, -105.1827443502702 39.97231958783131, -105.1826878500371 39.97232043832547, -105.1825779238971 39.97232006357458, -105.1824693614918 39.97231969607867, -105.1818888682263 39.97232118367459, -105.181313336771 39.97232225425414, -105.1807346165126 39.97232332753696, -105.1802034669848 39.97232431015902, -105.1797370086139 39.9723251692939, -105.1792927120879 39.97232533345959, -105.1782463742659 39.97232158132549, -105.1775629965025 39.97231860602722, -105.1761817574226 39.97231257916473, -105.1754036449972 39.97230917804725, -105.1753349979691 39.97230887841319, -105.1753040182588 39.97230874160383, -105.1753029543753 39.97233821445883, -105.1753000521294 39.97286562741104, -105.1752993592102 39.97299154292094, -105.1752986321791 39.97312339547399, -105.1752986400875 39.97327644619253, -105.1752986424906 39.97332390459598, -105.1752987049537 39.97441934769093, -105.1752970387502 39.97477164542337, -105.1752952276789 39.97514060311426, -105.1752932053162 39.97554706270822, -105.1752933364211 39.97554706487885, -105.1752921268262 39.97576430925468, -105.1752921682676 39.97579225049291, -105.1752957663743 39.97633889713853, -105.1752998415047 39.97695824622881, -105.1753039309026 39.97757977851963, -105.1753066251767 39.97798897490134, -105.1753071625874 39.97807062647465, -105.1753077055884 39.97815307154284, -105.1753102988506 39.97864007456597, -105.1749131590959 39.97863994859521, -105.1746315779191 39.97863985840293, -105.1737145515828 39.97863956374063, -105.1736004540525 39.97863952981174, -105.1713767703544 39.97863884954739, -105.1707601398161 39.97863865429652, -105.1705561331186 39.97863809480832, -105.1698279435228 39.97863609678081, -105.1688872339223 39.97863350366777, -105.1679504485915 39.97863091778471, -105.1660539287566 39.97862565398879, -105.1660529846982 39.97899093757391, -105.1660527537385 39.97906729471996, -105.1660524971388 39.97915319426635, -105.1660513282059 39.97953810432843, -105.166056001947 39.98000036722793, -105.1660560052696 39.98000040596588, -105.166057391659 39.98000036044625, -105.1660575394011 39.98000748868384, -105.1660575821633 39.98001166786214, -105.1660576266512 39.98001166799104, -105.166065785029 39.98040377608608, -105.1659816707675 39.98040380617206, -105.165974894609 39.98681212206605, -105.1659751117827 39.98681224608544, -105.165974893996 39.98681224725572, -105.1654436915867 39.98681856417538, -105.165249938283 39.98682086759958, -105.1652483903585 39.98682087571383, -105.1652418264078 39.98717422250558, -105.16525834624 39.98830990071465, -105.1652635700362 39.98855007082879, -105.166015041699 39.98853805963923, -105.1660804282237 39.99047413845548, -105.1661011979201 39.99226524125937, -105.1661144516633 39.99299008623935, -105.1661344118897 39.99408141175241, -105.1661076621722 39.99433846647752, -105.1660231465483 39.99515061432765, -105.1659122328651 39.99618293581459, -105.1658730304246 39.99656131156476, -105.1658367798869 39.99690524121675, -105.1657887406089 39.99735372905148, -105.1657802058163 39.9974419470633, -105.1657328518576 39.99789118618674, -105.1655696121921 39.99937187250002, -105.1654798192196 40.00004424309991, -105.1654647813974 40.00012800196317, -105.1678868478647 40.00012802026858, -105.1687138966328 40.00012902694554, -105.1695448773694 40.00012894105895, -105.1710501696939 40.00012198994988, -105.1714810047041 40.00012294450879, -105.1724918970514 40.00012087845364, -105.174943929118 40.00016597541908))</t>
+          <t>POLYGON ((-105.174943929118 40.00016597541908, -105.17553896038821 40.000167102900186, -105.17690714734904 40.00016792502332, -105.17815695772794 40.000140948544384, -105.1793810524402 40.00011690691521, -105.18014208321378 40.00011407962215, -105.18115904753758 40.00011113122423, -105.18409815457268 40.00011510349158, -105.19064003926789 40.00010099696486, -105.19081315495824 40.00010201071742, -105.19347499013801 40.00010170190278, -105.19347324689535 39.99998381946754, -105.19345763191394 39.99892492757701, -105.19642987605361 39.99604846059979, -105.19902570413672 39.993556312876585, -105.20295826884174 39.99342377712174, -105.20337726968239 39.99340858016221, -105.21250935887393 39.99318486329975, -105.21265399902974 39.99178199891079, -105.21268899988175 39.991396999113746, -105.21272499837931 39.99099299884455, -105.2127899996551 39.990329998986766, -105.2128229998723 39.98972899884425, -105.2128209981865 39.98794399929118, -105.212820998313 39.987493999145855, -105.21281999906496 39.987440998455504, -105.21281999831294 39.98714499875833, -105.21284099918626 39.98614399888426, -105.21284082651475 39.98613467486216, -105.21283939842807 39.986057551725146, -105.21283899974702 39.98603599893198, -105.21283353856064 39.98575351525029, -105.2128209987258 39.98510499896647, -105.21282197053348 39.98490281397867, -105.21282399998162 39.98447999876575, -105.21282799990433 39.983765999062385, -105.21282986062786 39.983468347594886, -105.21283000037698 39.98344599815635, -105.21283039681194 39.98311209701794, -105.21283300067002 39.9809199993889, -105.21283300076855 39.98049724201171, -105.21283300059898 39.980125999473216, -105.21283950342234 39.980121990639354, -105.21283018778081 39.97808843595108, -105.21491318867275 39.97773343595954, -105.21604715056883 39.97825984715396, -105.21611499982714 39.9782349994438, -105.21620046242603 39.978122638626864, -105.21495699835502 39.97754499902697, -105.21352999838092 39.97688599922395, -105.21337399765382 39.97681299863746, -105.21316999895335 39.97671799874688, -105.21283112593028 39.976562056433366, -105.21283099974 39.97656199847693, -105.21016499885391 39.97532799912825, -105.20966999966176 39.975104998925495, -105.20935499904714 39.97496399882614, -105.20900499857824 39.97480699849135, -105.2087029993851 39.97467099834954, -105.20704599949893 39.9739889990676, -105.20483700008339 39.97313299845037, -105.20413699889251 39.972861998931066, -105.2034419994515 39.97259099900295, -105.2027290000227 39.97231199833313, -105.20145800039566 39.971820998839895, -105.19940799980714 39.971020998472675, -105.1989119987643 39.970830998836234, -105.19839799970426 39.9706339986794, -105.19459199872699 39.969149998476155, -105.1918849995989 39.968100999020855, -105.19114199925232 39.96781299893013, -105.19011299929684 39.96740799898152, -105.18928299885233 39.96708899899218, -105.18865699972436 39.96684799823526, -105.18789599961327 39.966550999353736, -105.18475099885423 39.96532799810699, -105.1845030591753 39.96523090136483, -105.18450143396159 39.965230264653044, -105.18437879072897 39.9663747723468, -105.18437698789344 39.96809980246061, -105.18348289910209 39.96810018023088, -105.18269658832716 39.968100506507554, -105.18270498152465 39.96884194995791, -105.18274435027017 39.972319587831315, -105.18268785003706 39.97232043832547, -105.18257792389707 39.97232006357458, -105.18246936149183 39.97231969607867, -105.18188886822627 39.972321183674595, -105.18131333677096 39.972322254254145, -105.18073461651261 39.97232332753696, -105.18020346698484 39.972324310159024, -105.17973700861394 39.9723251692939, -105.17929271208794 39.972325333459594, -105.17824637426594 39.97232158132549, -105.17756299650247 39.97231860602722, -105.17618175742264 39.97231257916473, -105.17540364499725 39.972309178047254, -105.17533499796909 39.97230887841319, -105.17530401825883 39.972308741603825, -105.17530295437525 39.97233821445883, -105.1753000521294 39.97286562741104, -105.17529935921023 39.97299154292094, -105.17529863217905 39.97312339547399, -105.17529864008753 39.97327644619253, -105.17529864249056 39.97332390459598, -105.17529870495368 39.97441934769093, -105.17529703875019 39.97477164542337, -105.17529522767889 39.97514060311426, -105.17529320531615 39.97554706270822, -105.17529333642108 39.975547064878846, -105.17529212682622 39.97576430925468, -105.17529216826763 39.97579225049291, -105.17529576637435 39.97633889713853, -105.1752998415047 39.97695824622881, -105.17530393090259 39.977579778519626, -105.17530662517672 39.977988974901336, -105.17530716258736 39.978070626474654, -105.17530770558837 39.97815307154284, -105.17531029885065 39.978640074565966, -105.17491315909594 39.97863994859521, -105.17463157791911 39.97863985840293, -105.17371455158282 39.97863956374063, -105.17360045405252 39.978639529811744, -105.17137677035437 39.978638849547394, -105.1707601398161 39.97863865429652, -105.1705561331186 39.97863809480832, -105.16982794352282 39.97863609678081, -105.16888723392226 39.97863350366777, -105.16795044859154 39.97863091778471, -105.1660539287566 39.978625653988786, -105.16605298469823 39.97899093757391, -105.16605275373851 39.97906729471996, -105.16605249713876 39.979153194266345, -105.16605132820585 39.979538104328434, -105.16605600194698 39.98000036722793, -105.1660560052696 39.98000040596588, -105.16605739165898 39.980000360446255, -105.16605753940114 39.98000748868384, -105.16605758216333 39.980011667862144, -105.16605762665115 39.98001166799104, -105.16606578502898 39.98040377608608, -105.16598167076747 39.98040380617206, -105.16597489460902 39.98681212206605, -105.16597511178274 39.986812246085435, -105.16597489399598 39.98681224725572, -105.16544369158672 39.98681856417538, -105.16524993828304 39.98682086759958, -105.16524839035853 39.98682087571383, -105.16524182640784 39.98717422250558, -105.16525834624004 39.98830990071465, -105.16526357003622 39.98855007082879, -105.16601504169904 39.988538059639225, -105.16608042822367 39.990474138455475, -105.16610119792009 39.99226524125937, -105.16611445166329 39.992990086239345, -105.16613441188971 39.99408141175241, -105.16610766217217 39.99433846647752, -105.16602314654831 39.99515061432765, -105.16591223286507 39.996182935814595, -105.16587303042463 39.99656131156476, -105.1658367798869 39.99690524121675, -105.16578874060889 39.99735372905148, -105.16578020581626 39.9974419470633, -105.16573285185758 39.99789118618674, -105.16556961219206 39.99937187250002, -105.1654798192196 40.00004424309991, -105.16546478139743 40.00012800196317, -105.1678868478647 40.00012802026858, -105.16871389663281 40.00012902694554, -105.1695448773694 40.000128941058954, -105.17105016969391 40.00012198994988, -105.17148100470412 40.00012294450879, -105.17249189705142 40.00012087845364, -105.174943929118 40.00016597541908))</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -2600,10 +2608,14 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1782688488585 40.01463291530548, -105.1782689995687 40.01463299858616, -105.179412999948 40.01461999874561, -105.1808354543097 40.01462562931187, -105.1827040007133 40.01463299831895, -105.1834549992717 40.0146349225061, -105.1838739999368 40.01463599886635, -105.1841701799736 40.01463570346134, -105.1858630004019 40.01463399899924, -105.1864974973728 40.01463462047163, -105.1868859994811 40.01463499863746, -105.1879306387029 40.01464043574966, -105.1880389993641 40.01464099911838, -105.1886723010191 40.01463892504425, -105.1895639999455 40.01463599872144, -105.1942429993284 40.01465399917136, -105.1943553939693 40.01465460062421, -105.1951779999087 40.01465899884218, -105.1966359998847 40.01466699895634, -105.1967699330014 40.01466790959612, -105.1967830001021 40.0146679988932, -105.1983059994697 40.01466299922393, -105.1988599995382 40.01467899903977, -105.2006159994158 40.01467999898198, -105.2009300000826 40.01468399931195, -105.201182717144 40.01468616479592, -105.2012799993588 40.01468699864344, -105.2020565681202 40.01468240032865, -105.2020579655673 40.01468239223043, -105.2027989994621 40.01467799882614, -105.2028090273656 40.01467798954275, -105.2027581900902 40.01266844174256, -105.2038051899005 40.01281044069496, -105.2043981908388 40.01288544030034, -105.2045691898613 40.01294644116913, -105.2048331905392 40.01297844102542, -105.2050351910883 40.01296044132123, -105.2050398702081 40.01392145197964, -105.2050431900852 40.0146034419073, -105.2069742231526 40.01462497172324, -105.2078121909381 40.01462344028587, -105.2078361910397 40.01348944102689, -105.2075011914237 40.01348844053171, -105.2074681901274 40.01104044140051, -105.2098111911977 40.01104044022411, -105.2098292659196 40.01246736656677, -105.2098311921049 40.01261944051893, -105.2101881770135 40.0126180919686, -105.2101880793582 40.01262205279892, -105.2121356176559 40.01262468172177, -105.2130646768166 40.01262642336378, -105.213064157268 40.01258789120162, -105.2130592574697 40.01222416348261, -105.2130589996108 40.01220499962974, -105.2130529986013 40.01186999911342, -105.2130460006044 40.01138699885649, -105.2130454473815 40.01133281594282, -105.2130440003177 40.01119099898076, -105.2130312388504 40.01016524665692, -105.2130280004494 40.00990499912331, -105.2130180708937 40.00983143781237, -105.2130060003659 40.00974199894547, -105.2129829999123 40.00961299956395, -105.2129829986977 40.0095865752715, -105.2129829998411 40.0095709993631, -105.2130219997471 40.00935599951865, -105.2130219996678 40.00906603303326, -105.2130219999797 40.00890899948654, -105.2130189997407 40.00870099855842, -105.2130112852478 40.00853642174128, -105.213003999585 40.0083809993364, -105.2129869521706 40.00829726722127, -105.2129700000606 40.00821399827627, -105.2129235378465 40.00809508272722, -105.2128859992807 40.00799899844429, -105.2126530118967 40.00758899420312, -105.2126529828366 40.00758894189271, -105.2125739999607 40.00741399830913, -105.2125429989301 40.00731899837689, -105.2125049987698 40.00709399945863, -105.2125054826385 40.00647891950867, -105.2125059976708 40.00582199879766, -105.2125107894076 40.00369755140002, -105.2110311909939 40.00371343942365, -105.21103119153 40.00352344002083, -105.2111551901976 40.00343643944229, -105.2111711906653 40.00325443919979, -105.2111441915764 40.00300243863417, -105.2117761908399 40.0030044389501, -105.2117791909032 40.00354043954807, -105.2125117588774 40.00352564947486, -105.2125161427577 40.00307331652181, -105.2125269999105 40.00195299848955, -105.212566988398 40.00156499793533, -105.2125669991999 40.00156493581707, -105.2125852425582 40.00147525356017, -105.2127399996955 40.00071399866724, -105.2127818519077 40.00052534458408, -105.2128050001144 40.00042099923211, -105.2128159972606 40.00024511251258, -105.2128159836817 40.00024499989686, -105.2127969995393 40.00008999943838, -105.2127928656112 40.00007553362977, -105.2127829993984 40.00004099865892, -105.2127459994442 39.99984399810055, -105.2127392146961 39.99881852246104, -105.2127389991961 39.99878599927126, -105.2127455277946 39.99746149416151, -105.2127469993367 39.99716299909484, -105.2127440001071 39.99692699925155, -105.2127449818323 39.99692495901152, -105.2126844006306 39.99661445128344, -105.2126006533221 39.99626870887596, -105.2125139076481 39.9958991302809, -105.2124961767938 39.99569533982743, -105.2124925687887 39.99544869177733, -105.2124983315102 39.99518419448454, -105.2124740351865 39.99470038739478, -105.2124601767598 39.99431311694229, -105.2124779991473 39.99348899860376, -105.2125093588739 39.99318486329975, -105.2033772696824 39.99340858016221, -105.2029582688417 39.99342377712174, -105.1990257041367 39.99355631287658, -105.1964298760536 39.99604846059979, -105.1934576319139 39.99892492757701, -105.1934732468954 39.99998381946754, -105.193474990138 40.00010170190278, -105.1908131549582 40.00010201071742, -105.1906400392679 40.00010099696486, -105.1840981545727 40.00011510349158, -105.1811590475376 40.00011113122423, -105.1801420832138 40.00011407962215, -105.1793810524402 40.00011690691521, -105.1781569577279 40.00014094854438, -105.1781831559926 40.00056488123449, -105.1781969902901 40.00081006671814, -105.1782380691662 40.00148495285106, -105.1782610216749 40.00532089112599, -105.1782459979963 40.00585698788481, -105.1782109170462 40.00640702843349, -105.1781838615073 40.00729886938524, -105.1781999993325 40.00796407729013, -105.1782029610038 40.0085468924531, -105.1782108321747 40.00884586714735, -105.1782329229247 40.00968705887914, -105.1782201536082 40.01239296866031, -105.1782518670392 40.01369208709981, -105.1782688488585 40.01463291530548))</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr"/>
+          <t>POLYGON ((-105.17826884885845 40.014632915305484, -105.17826899956872 40.01463299858616, -105.17941299994798 40.01461999874561, -105.18083545430966 40.01462562931187, -105.18270400071329 40.01463299831895, -105.18345499927167 40.014634922506104, -105.18387399993684 40.014635998866346, -105.18417017997363 40.01463570346134, -105.18586300040191 40.014633998999244, -105.18649749737284 40.014634620471625, -105.18688599948108 40.01463499863746, -105.18793063870288 40.01464043574966, -105.18803899936414 40.014640999118384, -105.18867230101914 40.01463892504425, -105.18956399994552 40.01463599872144, -105.19424299932842 40.01465399917136, -105.19435539396932 40.01465460062421, -105.1951779999087 40.01465899884218, -105.19663599988468 40.01466699895634, -105.19676993300136 40.01466790959612, -105.1967830001021 40.014667998893195, -105.19830599946968 40.01466299922393, -105.19885999953817 40.014678999039766, -105.20061599941579 40.01467999898198, -105.2009300000826 40.01468399931195, -105.20118271714404 40.01468616479592, -105.20127999935877 40.01468699864344, -105.20205656812023 40.014682400328645, -105.20205796556735 40.01468239223043, -105.20279899946215 40.014677998826144, -105.20280902736565 40.014677989542754, -105.20275819009024 40.012668441742555, -105.20380518990045 40.01281044069496, -105.20439819083882 40.012885440300344, -105.20456918986132 40.012946441169134, -105.2048331905392 40.01297844102542, -105.20503519108834 40.01296044132123, -105.20503987020814 40.01392145197964, -105.20504319008523 40.0146034419073, -105.20697422315263 40.01462497172324, -105.20781219093811 40.014623440285874, -105.20783619103973 40.01348944102689, -105.20750119142375 40.01348844053171, -105.20746819012743 40.01104044140051, -105.20981119119767 40.011040440224114, -105.20982926591964 40.012467366566774, -105.20983119210486 40.01261944051893, -105.21018817701355 40.0126180919686, -105.21018807935823 40.01262205279892, -105.21213561765589 40.012624681721775, -105.21306467681661 40.012626423363784, -105.213064157268 40.01258789120162, -105.21305925746974 40.01222416348261, -105.21305899961078 40.01220499962974, -105.21305299860126 40.01186999911342, -105.21304600060444 40.01138699885649, -105.21304544738146 40.01133281594282, -105.21304400031774 40.01119099898076, -105.21303123885042 40.010165246656925, -105.21302800044937 40.009904999123314, -105.21301807089367 40.00983143781237, -105.2130060003659 40.00974199894547, -105.2129829999123 40.00961299956395, -105.21298299869767 40.0095865752715, -105.21298299984113 40.0095709993631, -105.2130219997471 40.009355999518654, -105.21302199966782 40.009066033033264, -105.21302199997974 40.008908999486536, -105.21301899974073 40.00870099855842, -105.21301128524784 40.00853642174128, -105.21300399958496 40.0083809993364, -105.2129869521706 40.008297267221266, -105.2129700000606 40.00821399827627, -105.21292353784645 40.00809508272722, -105.21288599928072 40.00799899844429, -105.21265301189669 40.00758899420312, -105.2126529828366 40.00758894189271, -105.21257399996067 40.00741399830913, -105.21254299893013 40.00731899837689, -105.21250499876983 40.00709399945863, -105.21250548263852 40.006478919508666, -105.21250599767083 40.00582199879766, -105.21251078940765 40.003697551400016, -105.21103119099389 40.00371343942365, -105.21103119153004 40.00352344002083, -105.21115519019756 40.00343643944229, -105.21117119066528 40.00325443919979, -105.21114419157635 40.00300243863417, -105.21177619083987 40.0030044389501, -105.2117791909032 40.00354043954807, -105.21251175887738 40.00352564947486, -105.21251614275768 40.003073316521814, -105.21252699991051 40.00195299848955, -105.21256698839802 40.001564997935326, -105.21256699919985 40.00156493581707, -105.21258524255825 40.001475253560166, -105.21273999969553 40.000713998667244, -105.21278185190766 40.000525344584084, -105.2128050001144 40.000420999232105, -105.21281599726058 40.00024511251258, -105.21281598368172 40.00024499989686, -105.21279699953932 40.00008999943838, -105.2127928656112 40.00007553362977, -105.21278299939843 40.00004099865892, -105.2127459994442 39.99984399810055, -105.21273921469607 39.99881852246104, -105.2127389991961 39.99878599927126, -105.21274552779455 39.997461494161506, -105.21274699933667 39.99716299909484, -105.21274400010705 39.99692699925155, -105.21274498183229 39.996924959011515, -105.21268440063064 39.99661445128344, -105.2126006533221 39.99626870887596, -105.21251390764806 39.995899130280904, -105.21249617679379 39.99569533982743, -105.2124925687887 39.99544869177733, -105.21249833151022 39.99518419448454, -105.21247403518655 39.99470038739478, -105.2124601767598 39.99431311694229, -105.2124779991473 39.99348899860376, -105.21250935887393 39.99318486329975, -105.20337726968239 39.99340858016221, -105.20295826884174 39.99342377712174, -105.19902570413672 39.993556312876585, -105.19642987605361 39.99604846059979, -105.19345763191394 39.99892492757701, -105.19347324689535 39.99998381946754, -105.19347499013801 40.00010170190278, -105.19081315495824 40.00010201071742, -105.19064003926789 40.00010099696486, -105.18409815457268 40.00011510349158, -105.18115904753758 40.00011113122423, -105.18014208321378 40.00011407962215, -105.1793810524402 40.00011690691521, -105.17815695772794 40.000140948544384, -105.17818315599263 40.00056488123449, -105.1781969902901 40.00081006671814, -105.17823806916618 40.00148495285106, -105.17826102167494 40.00532089112599, -105.17824599799634 40.00585698788481, -105.17821091704616 40.00640702843349, -105.17818386150726 40.00729886938524, -105.1781999993325 40.007964077290126, -105.17820296100382 40.008546892453104, -105.17821083217468 40.00884586714735, -105.1782329229247 40.009687058879145, -105.17822015360817 40.012392968660315, -105.1782518670392 40.01369208709981, -105.17826884885845 40.014632915305484))</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Centaurus HS</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2638,7 +2650,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.131216169747 40.05413797270889, -105.1312141679244 40.05437597462971, -105.1312034302793 40.05463055486094, -105.1312059997651 40.05463199871355, -105.1312151333568 40.05463829014283, -105.1313101329301 40.05456629110776, -105.1317031328973 40.05436329066021, -105.1319961338741 40.05425829067238, -105.1325041341113 40.05415429008961, -105.1329041339726 40.05411629033144, -105.1333401327132 40.05411628953848, -105.133690132606 40.05404529037242, -105.1340761340211 40.05386929093724, -105.1344121329457 40.05377628997379, -105.1349341339898 40.05378229096474, -105.1352131341163 40.05372229007944, -105.1360851348651 40.05334828960167, -105.1366211339717 40.05321729100668, -105.1369211341096 40.05319528942255, -105.1371141330145 40.05320128964343, -105.1374791331605 40.053074290269, -105.1380581339729 40.0527892905053, -105.1382651345308 40.0526522901612, -105.1385441337409 40.05252628951144, -105.138766134054 40.05234528973559, -105.1391951326456 40.05215229000667, -105.1394881334066 40.05209229106099, -105.1397811330371 40.05213129111328, -105.1404101340526 40.05226828965515, -105.1405531334419 40.05226829027612, -105.1406461339316 40.05230128984537, -105.1411321330766 40.05226928997327, -105.1412101335628 40.05224128986859, -105.1414601343164 40.05222528959065, -105.1418181357289 40.05218128953825, -105.1422181337478 40.05218728953625, -105.1428901343515 40.05228028849469, -105.1435331350977 40.05235728932603, -105.14388313487 40.05233028948903, -105.1442621341128 40.05224828958868, -105.1443591344388 40.05221428814447, -105.1460351344894 40.05162229008017, -105.1462421358811 40.05158428960294, -105.146507134829 40.05162828892156, -105.1467096475382 40.05174079629727, -105.1467141338478 40.05174329043003, -105.1475214657036 40.05240284117516, -105.1477619994002 40.05248499915338, -105.1480409998483 40.05248499847494, -105.1491200004597 40.05241399877543, -105.149419999981 40.05241999931873, -105.1495849996936 40.05249099906354, -105.1495927840303 40.0524967076198, -105.1495941346949 40.05249728903948, -105.1497291342438 40.05259628881397, -105.1499441353162 40.05288728991736, -105.1500709278685 40.05298027054587, -105.1503129996857 40.05305099857401, -105.1505920000701 40.05305099892555, -105.1505987666178 40.05305728885442, -105.1506011352395 40.05305728882134, -105.1506660946248 40.05311767337918, -105.1508419991454 40.05315599894361, -105.1511639996712 40.05311799890815, -105.1514139993553 40.05303499916442, -105.1516930001067 40.05285399910237, -105.1520634530785 40.05256504639421, -105.1520642591071 40.0525644174675, -105.1520530348799 40.05218408774775, -105.1520482361644 40.05202146772876, -105.1520712442313 40.05201190102868, -105.1521876377263 40.05195702483574, -105.1523709083099 40.05192184554181, -105.1526102549068 40.05192063987319, -105.15267013907 40.05191182082855, -105.1527184816784 40.05188986072653, -105.1528089772994 40.05183494919256, -105.152836948917 40.05178229025947, -105.1527996939401 40.0517351334993, -105.1528329969947 40.05168682004388, -105.1529012724015 40.05161217584052, -105.1529783703864 40.05155730943326, -105.1531397555849 40.05143984165882, -105.1532347199211 40.05138383001786, -105.1533116082054 40.05136846626508, -105.1534287685995 40.05133659738699, -105.1535204189365 40.05131571000074, -105.1535861239172 40.05130360977193, -105.1536317958948 40.05128052536217, -105.153703493422 40.05123331131377, -105.1537447568463 40.05119928871704, -105.1537747601148 40.05118391274718, -105.1538618324175 40.05110049708283, -105.1539418604768 40.05108179820791, -105.1541395682197 40.05110146049368, -105.1542393670629 40.051143104026, -105.1543122705736 40.05120343378905, -105.1543524386634 40.0512901004921, -105.1544126177785 40.05130870358548, -105.1544498855746 40.05131259703548, -105.1544755440843 40.05131527765732, -105.1545269491046 40.05130536228518, -105.1546185274299 40.05130207615829, -105.1546944698589 40.0513009857922, -105.1547816445631 40.05128785033533, -105.1548545492162 40.05127033098574, -105.1549462249694 40.05125056835962, -105.155047563932 40.05126268791455, -105.1551721161439 40.05127806416193, -105.1552922383388 40.05128579671553, -105.1554265831195 40.05130777039776, -105.1555756460016 40.05133523860343, -105.155747305266 40.05139785533414, -105.1559449171125 40.051452809891, -105.1560672076075 40.05148776040432, -105.156182259442 40.05151215429144, -105.1563698698731 40.05150490630326, -105.1564951449201 40.05150537027536, -105.1566557219626 40.05152101697655, -105.156851779706 40.05152988258859, -105.1569577263993 40.05151454247685, -105.1570661436412 40.05154087557591, -105.157190994115 40.05158591350226, -105.157298495359 40.05160449895396, -105.1574342921437 40.05158897145586, -105.1575282456326 40.05158931609547, -105.1575908832443 40.05158954611878, -105.1575919391772 40.05158955015285, -105.1576639618218 40.05158981519088, -105.1577685196039 40.05155814409517, -105.1578831959852 40.05153560939884, -105.1580062850491 40.05148732646475, -105.1580990127872 40.05143575882849, -105.1581693302335 40.05139953848941, -105.1582751446963 40.0513216564015, -105.1584092219116 40.05122068951568, -105.1585395127557 40.05116145649118, -105.1587239578759 40.05108137939627, -105.1588224049339 40.05104736108841, -105.1588728812464 40.05103129138426, -105.1593482686524 40.05103662897318, -105.1595130289511 40.05103847795551, -105.1595497573073 40.0510384773496, -105.1595874136325 40.05105893417739, -105.1596549405419 40.05111494767892, -105.1597265106609 40.05116466489707, -105.1597935154553 40.05123422078098, -105.159876657559 40.05128822670264, -105.1599624177394 40.05135426038001, -105.1600339312413 40.05141495168196, -105.1600768884722 40.05147705390013, -105.1601396905426 40.05158504873061, -105.1601740137286 40.05167799262278, -105.1601936833895 40.05188593181764, -105.160194346883 40.05189295255178, -105.1601953579844 40.05189936276693, -105.160201266795 40.05193680045235, -105.1602342926047 40.05202203722605, -105.1602561397624 40.05220183654168, -105.1602218951422 40.05227028792482, -105.1601749235323 40.05238603017087, -105.1601642242853 40.05244927305546, -105.1601535180372 40.05250545570828, -105.1601009883901 40.05258598317823, -105.1600485362148 40.05265048645484, -105.1600586416582 40.05271452735239, -105.1600897153273 40.05275437456363, -105.1601311367479 40.05281017486806, -105.1601621305672 40.05286605072398, -105.1601932854801 40.05288986654357, -105.1602311089501 40.05292335067315, -105.1603040995684 40.05295659877761, -105.1603624839046 40.05296697322286, -105.1603981176738 40.05297751575439, -105.1604596628149 40.05298015204612, -105.1606098666646 40.05297498286759, -105.1607036947628 40.05297429690353, -105.1608079517161 40.05297353524253, -105.1608240356948 40.05297341770119, -105.1608279643923 40.05297338871971, -105.160891354474 40.05297292385619, -105.1610268077163 40.05298796284046, -105.1611730028394 40.05293880593047, -105.1612775409593 40.05288193857015, -105.1613716102433 40.05283316157037, -105.1614865311916 40.05278423221279, -105.1615911051033 40.05271934887317, -105.1616540197808 40.05264675530231, -105.1617273198083 40.05258210256712, -105.1618022051694 40.05247829679478, -105.1619047081888 40.05240805722977, -105.1619520472971 40.05230765616699, -105.1620291104283 40.0522398322612, -105.1622773176912 40.05211314107409, -105.1625770852535 40.05202319452241, -105.162727133867 40.05198972996543, -105.1628557406417 40.05196199555888, -105.1629758668792 40.05193543590796, -105.1630999311205 40.051924238339, -105.1632498597902 40.05191494894872, -105.1633658337125 40.05191585656047, -105.1634372860497 40.05189972807043, -105.1634941191975 40.05186291666683, -105.1635797130987 40.0517840142715, -105.1636657356831 40.05170844907624, -105.1637070317691 40.05165640548891, -105.1637524313982 40.05158787030133, -105.1638339316571 40.05152331397849, -105.1639326605231 40.05144388037487, -105.1640410996069 40.05139593472637, -105.1641309913249 40.05134884735053, -105.1642694282163 40.05131773912331, -105.1643867503607 40.05131644664036, -105.1644822108131 40.05131651800511, -105.1645678403559 40.05132000210335, -105.1647220812559 40.0513403043466, -105.1648608305505 40.05142553350745, -105.1649212127349 40.05148304796267, -105.1649453974719 40.05155411656848, -105.1649468807872 40.05161450597241, -105.164935389596 40.05168266274925, -105.1649253408261 40.05173109043365, -105.1649357829235 40.05187367951304, -105.1649515280593 40.0519371797482, -105.1649669596101 40.05195100002284, -105.1650579994036 40.05195099953081, -105.1653113904446 40.05201382030101, -105.1653173844367 40.05201229577091, -105.1654030527817 40.05200806347592, -105.1655088629726 40.05199043827383, -105.1655799060003 40.05196663732222, -105.165648750986 40.05193625429996, -105.1657559025758 40.05191750514264, -105.1659058511208 40.05190384239806, -105.1660201575936 40.05188173626777, -105.1660501816832 40.05185395159862, -105.1660856138928 40.0518140823167, -105.1661313790737 40.05176088895957, -105.1662384021501 40.05167736591554, -105.1663239373181 40.05160952042499, -105.1664011403114 40.05151207338047, -105.1664736601505 40.05146078375623, -105.1666408738178 40.05138324620814, -105.1666993909921 40.05136613985114, -105.1668981002619 40.05132446858931, -105.1670995030762 40.05127835733884, -105.1671464633991 40.05126049418936, -105.1672094394409 40.0512376803974, -105.1673022957037 40.05122237770144, -105.167427709391 40.05120897908306, -105.1675050332762 40.05117737289109, -105.1676261415118 40.05113215513653, -105.1676963712698 40.05109189923789, -105.1677831638122 40.05104046255979, -105.1677931005396 40.05103765951979, -105.1689099714373 40.05103750031685, -105.1689467501823 40.05103749776507, -105.1689875652156 40.05103748966823, -105.1689960014125 40.05103741479722, -105.1711336761778 40.05103113964618, -105.171347248249 40.0510305133593, -105.1713527073654 40.05103049558405, -105.1716427702465 40.05102964076442, -105.1716459099946 40.05102963168614, -105.1723984922067 40.05102741077957, -105.1724016811853 40.05102740001921, -105.1726165283522 40.05102676779798, -105.1726983997368 40.05102652451531, -105.1728325803302 40.05102612868573, -105.1736898899024 40.05102358741136, -105.174428782014 40.05102139560601, -105.1753060140316 40.05101878505296, -105.1755701079732 40.05101799679088, -105.1755736157177 40.05101798773977, -105.1755771234751 40.05101797598657, -105.175580085081 40.05101796720103, -105.1755841471719 40.05101795700623, -105.1761905990056 40.05101614793633, -105.176194113803 40.0510161343829, -105.1761979860374 40.05101612363364, -105.1762011363404 40.05101611265975, -105.1762046476006 40.05101610359928, -105.1762081530053 40.05101609362164, -105.1780338616441 40.05101062691166, -105.1782826872876 40.05101600343033, -105.178285099815 40.05095033556441, -105.1782909993724 40.05078899852872, -105.1783619916895 40.05013707172179, -105.1783619978893 40.05013699968696, -105.1783889994008 40.0494039987319, -105.1783889921711 40.04940279904402, -105.1783850000171 40.04872299868529, -105.1783823374743 40.04787297522466, -105.1783819997574 40.04776499876323, -105.1783700003943 40.04545199887659, -105.1783569989513 40.04397399911803, -105.1783593807407 40.04381992401295, -105.1783670002116 40.04332699857592, -105.1783709996006 40.04307199909479, -105.1783800001195 40.04215799916332, -105.1783800027096 40.04215794693271, -105.1783870000278 40.04106199875608, -105.1783899999625 40.04087199920473, -105.1783900004663 40.04081899851942, -105.1783920002899 40.04072099871122, -105.1784048433664 40.03966053615192, -105.1784199995207 40.03840899927504, -105.1784249996421 40.03670199816679, -105.1784399998176 40.03537799842891, -105.1784889999836 40.03472599927464, -105.178490000368 40.03469499888762, -105.178531999708 40.03353499925799, -105.1785369999334 40.03339099877271, -105.1785399991614 40.03279999949025, -105.1785309996551 40.03216499864769, -105.1784769999151 40.03169499900179, -105.1784589989599 40.03107899928678, -105.1784620001129 40.03036699889137, -105.1784680003464 40.02915899894963, -105.1785019999882 40.0272379988253, -105.1785159996695 40.0261089991069, -105.1785169994261 40.02605499869539, -105.1784799995173 40.02439999821404, -105.1784639995815 40.02391999874165, -105.1784449993586 40.02333599866598, -105.1784189992241 40.02213199938647, -105.1784120001571 40.02177899910858, -105.1783799991943 40.02048599914978, -105.1783460002359 40.01914399873556, -105.1783049994997 40.01838899907003, -105.1782029988481 40.01737399931093, -105.1781489999591 40.01684399893904, -105.1781320000762 40.01633599939375, -105.1781410003895 40.01595099914135, -105.1782570004259 40.01483999953051, -105.1782689995687 40.01463299858616, -105.1782688488585 40.01463291530548, -105.1782518670392 40.01369208709981, -105.1782201536082 40.01239296866031, -105.1782329229247 40.00968705887914, -105.1782108321747 40.00884586714735, -105.1782029610038 40.0085468924531, -105.1781999993325 40.00796407729013, -105.1781838615073 40.00729886938524, -105.1782109170462 40.00640702843349, -105.1782459979963 40.00585698788481, -105.1782610216749 40.00532089112599, -105.1782380691662 40.00148495285106, -105.1781969902901 40.00081006671814, -105.1781831559926 40.00056488123449, -105.1781569577279 40.00014094854438, -105.176907147349 40.00016792502332, -105.1755389603882 40.00016710290019, -105.174943929118 40.00016597541908, -105.1724918970514 40.00012087845364, -105.1714810047041 40.00012294450879, -105.1710501696939 40.00012198994988, -105.1695448773694 40.00012894105895, -105.1687138966328 40.00012902694554, -105.1678868478647 40.00012802026858, -105.1654647813974 40.00012800196317, -105.1654798192196 40.00004424309991, -105.1655696121921 39.99937187250002, -105.1657328518576 39.99789118618674, -105.1657802058163 39.9974419470633, -105.1657887406089 39.99735372905148, -105.1658367798869 39.99690524121675, -105.1658730304246 39.99656131156476, -105.1659122328651 39.99618293581459, -105.1660231465483 39.99515061432765, -105.1661076621722 39.99433846647752, -105.1661344118897 39.99408141175241, -105.1661144516633 39.99299008623935, -105.1661011979201 39.99226524125937, -105.1660804282237 39.99047413845548, -105.166015041699 39.98853805963923, -105.1652635700362 39.98855007082879, -105.1652600612412 39.9884278360004, -105.1652129168158 39.98840770990265, -105.164152903713 39.98795517594412, -105.1640557053296 39.98791588344694, -105.1639629797611 39.98801302742708, -105.1638820078671 39.98807702897645, -105.1636180300277 39.98827007062972, -105.1633738472757 39.98842912912709, -105.1632068468137 39.98856892148969, -105.1631318802227 39.98864501967785, -105.1630340843738 39.98879105290501, -105.1629701445979 39.98894706885007, -105.1629411450479 39.9891100499324, -105.1629369535138 39.98923604238151, -105.1629316619924 39.98939933324853, -105.1630484245457 39.98939258460942, -105.1652800904351 39.98963757722175, -105.165280121269 39.98963940654668, -105.165293913414 39.9904726547182, -105.1644396301791 39.99047469439939, -105.1603292951578 39.99048441784612, -105.1598894223283 39.99048544917379, -105.1582351763826 39.99048931494893, -105.1582367037443 39.99049132434087, -105.1585727934224 39.99093128003249, -105.158249423521 39.99149224398947, -105.1576955197453 39.99206442405352, -105.1570945121236 39.99246391068015, -105.156359603665 39.99274076059307, -105.1561716319405 39.99274373072714, -105.1560127966663 39.99270667940952, -105.1550702284904 39.99239786295302, -105.1548927785468 39.99227636637016, -105.1548910742555 39.99251738266482, -105.1548905001314 39.99259868061086, -105.1548904876865 39.99260044586263, -105.1548798542597 39.99410483914303, -105.1527289655441 39.99412802825835, -105.1527291642998 39.994223301319, -105.1527294447671 39.99436232136527, -105.1527297013948 39.9944982043476, -105.1527298679238 39.99458462834716, -105.1527298717996 39.99458662691797, -105.1527303188908 39.9948198724531, -105.152730749748 39.99504526780311, -105.1527319606385 39.99568069342332, -105.1527329270777 39.99618589581407, -105.1527344190078 39.99618588769861, -105.1539519884817 39.99617947834857, -105.1545751648555 39.99617619263377, -105.155460491504 39.99617391781758, -105.1562106152407 39.99617225447206, -105.1565059962698 39.99617247919943, -105.1572405990433 39.99617363150352, -105.1572403745552 39.99617565911632, -105.1571750076949 39.99676647874302, -105.1571164998218 39.99727085921636, -105.1570990085866 39.9974216510589, -105.1570808518021 39.99757180685464, -105.157040634938 39.99799156637739, -105.1568526260754 39.99995385836775, -105.1568459364061 40.00004260990784, -105.1568367408974 40.00012757393174, -105.1568362961492 40.00012961529795, -105.156588390307 40.00012897627218, -105.1550500005115 40.00012499920634, -105.1539019988791 40.00012399883708, -105.1537709990355 40.00012399912667, -105.1537707329934 40.000125192599, -105.1535781771506 40.00013044327525, -105.1535166309048 40.00019969629903, -105.1534616395557 40.00019996334979, -105.1532393860764 40.0003995175149, -105.1531903592538 40.00041976453732, -105.1526815171395 40.00062425548496, -105.1517734538989 40.00041189854682, -105.1516755779333 40.00020098063606, -105.1515373454481 40.00020071065877, -105.1515363523692 40.00020070855813, -105.1515160075409 40.0001189979974, -105.1515154957292 40.00011694385289, -105.1512644961406 40.00011694331047, -105.1512284955127 40.0001169433975, -105.1496865034817 40.00012394214083, -105.1495325033061 40.00012394248593, -105.149532503279 40.00012599868626, -105.1405990316423 40.00013293952663, -105.1405914290438 40.00022490629105, -105.1405885450742 40.00027393090059, -105.1405755504105 40.00063393005045, -105.1406015518538 40.00081292761907, -105.1406575531707 40.0009829265404, -105.1407505560302 40.00112692615965, -105.1407508565735 40.00112723061763, -105.1408455558642 40.00122292597722, -105.1413045598964 40.00160192301993, -105.14179056115 40.00198092282215, -105.1417900173021 40.00198145342109, -105.1415915660002 40.00217492028406, -105.1415255674581 40.00230091972836, -105.1415115688388 40.00233991970254, -105.141499568217 40.00238291850106, -105.1414825701238 40.00249991777957, -105.1414825826895 40.00347591238927, -105.1414905848927 40.00358891121111, -105.1415175843889 40.00365291029514, -105.141509603522 40.00377466514739, -105.1414141544557 40.00377504835109, -105.1405073285334 40.00377868691076, -105.1405082039836 40.0039638566653, -105.1405083759637 40.00400010325159, -105.1405083861383 40.00400217209295, -105.1405086488789 40.00405785874783, -105.1405095795938 40.00425431840782, -105.1405095938914 40.00425738248826, -105.140510985685 40.00455144149755, -105.1405117178504 40.0047060325794, -105.1405119956253 40.00476531109808, -105.1405129177941 40.00496006307164, -105.1405138435483 40.00515546892974, -105.1405147282165 40.00534222924821, -105.1405152394761 40.0054507501174, -105.1405159169233 40.00559328571963, -105.1405171003353 40.0058433487435, -105.1405180110712 40.00603560944315, -105.1405189063033 40.00622503572305, -105.1405197450146 40.00640230115203, -105.1405204679228 40.00655532323205, -105.1405213135668 40.00673438548746, -105.1405227300227 40.00703333867119, -105.1405227731292 40.00704226881942, -105.140523033826 40.00709723672683, -105.1405231402594 40.0071210369189, -105.140523180474 40.00712851609968, -105.1405233533581 40.00716526074064, -105.1405233594408 40.00716677296265, -105.1405235952953 40.00721578925072, -105.1405236235035 40.00722199126245, -105.1405243015636 40.00736530590967, -105.1399362728994 40.00736244634241, -105.1398447187669 40.00725686822421, -105.1398428922491 40.00725476218737, -105.13974885825 40.00725594913141, -105.1356722521112 40.00730740311281, -105.1354341517882 40.00731040633411, -105.1354324252654 40.00731109077897, -105.1354291354535 40.00731215936529, -105.135427728691 40.00731262145808, -105.1354258526205 40.00731323698013, -105.1354225721009 40.00731432000612, -105.1354192973746 40.00731541475887, -105.1354160272801 40.00731651943344, -105.1354127665357 40.00731762774004, -105.1354095045527 40.0073187486519, -105.1354062565613 40.00731988131641, -105.1354030026946 40.00732101756492, -105.1353997616435 40.007322166463, -105.1353965217443 40.00732331896733, -105.1353932911278 40.00732448771268, -105.1353900651913 40.00732565737344, -105.1353868426767 40.0073268441574, -105.1353836271604 40.00732803636732, -105.1353804151141 40.00732923669405, -105.1353772100516 40.00733044514874, -105.1353740131392 40.00733166263565, -105.1353708173401 40.00733289093387, -105.1353676297153 40.00733412376111, -105.1353644455413 40.00733536830775, -105.1353612706934 40.00733662098969, -105.1353581004821 40.00733788269282, -105.1353549384305 40.00733915162687, -105.1353517774874 40.00734043227291, -105.1353486235328 40.0073417201462, -105.1353454777428 40.00734301434984, -105.1353423365797 40.00734431937593, -105.1353391988867 40.00734563251877, -105.1353360716767 40.0073469565026, -105.1353329491368 40.00734828320308, -105.1353298312142 40.00734962252728, -105.1353267214561 40.0073509681818, -105.1353236163394 40.00735232195684, -105.1353205170111 40.00735368835932, -105.135317425857 40.00735505929084, -105.135314340501 40.00735644104851, -105.1353112632951 40.00735783183841, -105.1353081895787 40.00735922714261, -105.135305126345 40.0073606332877, -105.1353020700854 40.00736204936203, -105.1352990137873 40.00736347264144, -105.1352959656584 40.00736490135053, -105.1352929268364 40.00736634179746, -105.135289895003 40.00736778947173, -105.1352868666396 40.00736924526279, -105.1352838464216 40.00737071098678, -105.1352808355393 40.0073721830448, -105.1352778304647 40.00737366412773, -105.1352748300459 40.00737515062921, -105.1352718377627 40.00737664886486, -105.1352688524633 40.00737815522849, -105.1352658741379 40.00737967152132, -105.1352629028349 40.00738118873692, -105.1352599396577 40.00738271948803, -105.1352569823076 40.00738425566137, -105.1352540284179 40.00738580175289, -105.1352510862016 40.00738735508647, -105.1352481509593 40.00738891834928, -105.1352452227105 40.00739048793876, -105.1352423002596 40.00739206835435, -105.1352393859926 40.00739365149774, -105.1352364821891 40.00739524908467, -105.1352314904021 40.00739810368863, -105.1341532742665 40.00739890930889, -105.1312935033927 40.0074009977704, -105.1312846278433 40.00740100451655, -105.1312832797619 40.00740100560996, -105.1312832577426 40.00740312838888, -105.1312534875319 40.00740314937847, -105.1310783415883 40.00740538300349, -105.1310778532248 40.0074339520929, -105.1310700786464 40.00794700646802, -105.1310909392437 40.00956811928324, -105.1311008088521 40.01070634634, -105.1310997144627 40.01070685621357, -105.131091726775 40.01172384982907, -105.1310967316625 40.01207284788168, -105.1310979697797 40.0120728383325, -105.1311700055415 40.01207226986423, -105.1312569842205 40.01207158521304, -105.1312570076791 40.01207374506328, -105.131257730989 40.01213947371401, -105.1313466466419 40.01213865468601, -105.1324447468638 40.01212852478138, -105.1356610401132 40.01210996406044, -105.1356620779171 40.01210995833265, -105.1357996656098 40.01210916173971, -105.1358015338484 40.01254773971242, -105.1358026199699 40.01280227681977, -105.135803927714 40.01310830335805, -105.1358050213227 40.01336538933267, -105.1358050413 40.01337020160395, -105.1358050604791 40.01337472476187, -105.1358204177624 40.01350958353772, -105.1358343250365 40.01363171595667, -105.135806156309 40.01363183505427, -105.1358072921032 40.01389725402277, -105.1358084176293 40.01416174617611, -105.1358098300447 40.01441792346685, -105.1358106759398 40.01466371889595, -105.135810672579 40.01466588316285, -105.1358103602851 40.01487676008018, -105.1358099276981 40.01516827058219, -105.1358091438079 40.01569681831801, -105.1358083466995 40.01623507505892, -105.1358069737647 40.01716072833008, -105.1357992116425 40.01829673750202, -105.1355935115999 40.01829732614752, -105.1345339076398 40.01830035084866, -105.1345297826865 40.01831441593423, -105.1320616319306 40.01831728968089, -105.1317155406373 40.01831768913188, -105.1312431051194 40.01831823124324, -105.1311777986908 40.01831830522199, -105.1311777798524 40.01832048835271, -105.1310575495072 40.01831992727238, -105.131042960859 40.01876495883627, -105.1310380626037 40.01914213441396, -105.1310359638921 40.01933209591846, -105.1310251261564 40.02021299758439, -105.1310111497333 40.02141013649386, -105.131001914456 40.02212688053156, -105.1310015904696 40.02216011730349, -105.131000855409 40.02215978531176, -105.130998857059 40.02229978498944, -105.1310018638014 40.02277278218614, -105.1310048639694 40.0229017810233, -105.1310068742717 40.02376277574164, -105.1309978878637 40.02485876942394, -105.1309909037535 40.02611376122235, -105.1309957951422 40.02789410985726, -105.1309969825158 40.02794400096061, -105.1310000230925 40.02794393773443, -105.1310490163915 40.03658189669205, -105.1310650469673 40.03738107533779, -105.1310990889926 40.03834996598214, -105.1311201440057 40.03927708677072, -105.131145064082 40.0398198926297, -105.1311590894281 40.0401320664122, -105.1311550651878 40.04047987090068, -105.1311510917365 40.04081806645879, -105.1311559623812 40.04321793513203, -105.1311610113387 40.04406704094007, -105.1311569094684 40.04515495007782, -105.1311570037658 40.04527134096249, -105.1311570490046 40.04532707446116, -105.1311558744463 40.04547805719804, -105.1311661736642 40.04661103317486, -105.1311759744774 40.04744011431053, -105.1311790599092 40.04779398012801, -105.1311841143478 40.04824612972813, -105.1311891001171 40.04930496819956, -105.1311931055019 40.05054498601775, -105.131205846102 40.05096312075745, -105.1312107819624 40.05257722664825, -105.131211005441 40.05265005956795, -105.1312209170923 40.05372291390245, -105.131216169747 40.05413797270889))</t>
+          <t>POLYGON ((-105.131216169747 40.054137972708894, -105.13121416792443 40.054375974629714, -105.13120343027933 40.05463055486094, -105.13120599976514 40.05463199871355, -105.13121513335679 40.05463829014283, -105.13131013293014 40.05456629110776, -105.13170313289729 40.054363290660206, -105.13199613387408 40.05425829067238, -105.13250413411133 40.05415429008961, -105.1329041339726 40.054116290331436, -105.13334013271316 40.05411628953848, -105.13369013260602 40.05404529037242, -105.13407613402109 40.053869290937236, -105.13441213294574 40.05377628997379, -105.13493413398982 40.05378229096474, -105.13521313411631 40.05372229007944, -105.13608513486506 40.053348289601665, -105.13662113397173 40.05321729100668, -105.13692113410956 40.05319528942255, -105.13711413301452 40.05320128964343, -105.13747913316054 40.053074290268995, -105.13805813397289 40.0527892905053, -105.13826513453076 40.0526522901612, -105.13854413374094 40.05252628951144, -105.138766134054 40.05234528973559, -105.13919513264561 40.052152290006674, -105.13948813340659 40.05209229106099, -105.13978113303708 40.052131291113284, -105.14041013405257 40.052268289655146, -105.14055313344193 40.052268290276125, -105.14064613393161 40.052301289845374, -105.14113213307658 40.052269289973275, -105.14121013356277 40.05224128986859, -105.14146013431638 40.05222528959065, -105.14181813572887 40.05218128953825, -105.14221813374778 40.05218728953625, -105.1428901343515 40.05228028849469, -105.14353313509766 40.052357289326025, -105.14388313486997 40.052330289489035, -105.14426213411276 40.052248289588675, -105.14435913443882 40.05221428814447, -105.14603513448941 40.05162229008017, -105.14624213588111 40.05158428960294, -105.14650713482904 40.05162828892156, -105.14670964753824 40.051740796297274, -105.14671413384782 40.051743290430025, -105.14752146570363 40.05240284117516, -105.14776199940019 40.05248499915338, -105.1480409998483 40.05248499847494, -105.14912000045967 40.05241399877543, -105.14941999998102 40.05241999931873, -105.1495849996936 40.052490999063544, -105.14959278403029 40.052496707619795, -105.14959413469492 40.05249728903948, -105.14972913424377 40.052596288813966, -105.14994413531618 40.052887289917365, -105.15007092786853 40.052980270545866, -105.15031299968574 40.05305099857401, -105.15059200007013 40.05305099892555, -105.15059876661776 40.05305728885442, -105.15060113523947 40.05305728882134, -105.15066609462482 40.053117673379184, -105.15084199914541 40.05315599894361, -105.15116399967118 40.05311799890815, -105.15141399935528 40.05303499916442, -105.15169300010675 40.052853999102375, -105.1520634530785 40.05256504639421, -105.15206425910714 40.0525644174675, -105.15205303487993 40.052184087747754, -105.15204823616442 40.05202146772876, -105.15207124423127 40.05201190102868, -105.15218763772631 40.05195702483574, -105.15237090830992 40.05192184554181, -105.15261025490679 40.05192063987319, -105.15267013907 40.05191182082855, -105.15271848167838 40.051889860726526, -105.15280897729937 40.05183494919256, -105.15283694891697 40.05178229025947, -105.15279969394011 40.0517351334993, -105.15283299699472 40.05168682004388, -105.15290127240151 40.05161217584052, -105.15297837038636 40.05155730943326, -105.15313975558492 40.05143984165882, -105.1532347199211 40.05138383001786, -105.15331160820543 40.05136846626508, -105.15342876859948 40.05133659738699, -105.15352041893651 40.05131571000074, -105.15358612391715 40.05130360977193, -105.1536317958948 40.051280525362166, -105.15370349342199 40.051233311313766, -105.15374475684631 40.05119928871704, -105.15377476011477 40.05118391274718, -105.15386183241749 40.05110049708283, -105.15394186047676 40.05108179820791, -105.15413956821975 40.05110146049368, -105.15423936706293 40.051143104025996, -105.15431227057358 40.05120343378905, -105.15435243866337 40.0512901004921, -105.15441261777848 40.051308703585484, -105.15444988557458 40.051312597035476, -105.15447554408435 40.05131527765732, -105.1545269491046 40.051305362285184, -105.15461852742989 40.05130207615829, -105.15469446985885 40.0513009857922, -105.15478164456307 40.05128785033533, -105.15485454921618 40.051270330985744, -105.15494622496944 40.05125056835962, -105.15504756393197 40.05126268791455, -105.15517211614386 40.051278064161934, -105.1552922383388 40.051285796715526, -105.15542658311952 40.051307770397756, -105.15557564600164 40.05133523860343, -105.155747305266 40.05139785533414, -105.15594491711255 40.051452809890996, -105.15606720760749 40.05148776040432, -105.15618225944198 40.05151215429144, -105.15636986987309 40.051504906303265, -105.15649514492009 40.05150537027536, -105.15665572196258 40.05152101697655, -105.156851779706 40.05152988258859, -105.15695772639931 40.05151454247685, -105.15706614364125 40.05154087557591, -105.15719099411497 40.05158591350226, -105.15729849535903 40.05160449895396, -105.15743429214369 40.051588971455864, -105.15752824563263 40.05158931609547, -105.15759088324425 40.05158954611878, -105.15759193917715 40.051589550152855, -105.1576639618218 40.05158981519088, -105.15776851960395 40.051558144095175, -105.15788319598524 40.05153560939884, -105.15800628504907 40.05148732646475, -105.15809901278716 40.05143575882849, -105.15816933023348 40.051399538489406, -105.1582751446963 40.0513216564015, -105.15840922191157 40.05122068951568, -105.15853951275574 40.05116145649118, -105.15872395787588 40.05108137939627, -105.1588224049339 40.051047361088415, -105.15887288124637 40.05103129138426, -105.15934826865238 40.05103662897318, -105.15951302895108 40.05103847795551, -105.15954975730733 40.0510384773496, -105.15958741363254 40.05105893417739, -105.15965494054187 40.05111494767892, -105.15972651066092 40.05116466489707, -105.15979351545529 40.05123422078098, -105.15987665755898 40.05128822670264, -105.15996241773941 40.05135426038001, -105.16003393124133 40.05141495168196, -105.16007688847216 40.05147705390013, -105.16013969054255 40.05158504873061, -105.16017401372865 40.05167799262278, -105.16019368338945 40.051885931817644, -105.160194346883 40.05189295255178, -105.16019535798439 40.05189936276693, -105.16020126679499 40.051936800452346, -105.16023429260466 40.052022037226045, -105.16025613976238 40.05220183654168, -105.1602218951422 40.05227028792482, -105.16017492353228 40.052386030170865, -105.16016422428534 40.05244927305546, -105.16015351803719 40.05250545570828, -105.16010098839008 40.05258598317823, -105.16004853621476 40.052650486454844, -105.16005864165815 40.052714527352386, -105.16008971532732 40.052754374563634, -105.16013113674794 40.05281017486806, -105.16016213056723 40.05286605072398, -105.1601932854801 40.05288986654357, -105.16023110895006 40.05292335067315, -105.16030409956835 40.05295659877761, -105.16036248390458 40.05296697322286, -105.16039811767375 40.052977515754385, -105.16045966281487 40.052980152046125, -105.16060986666464 40.05297498286759, -105.16070369476283 40.05297429690353, -105.16080795171605 40.05297353524253, -105.1608240356948 40.05297341770119, -105.16082796439227 40.05297338871971, -105.16089135447405 40.05297292385619, -105.1610268077163 40.05298796284046, -105.16117300283939 40.05293880593047, -105.16127754095929 40.05288193857015, -105.1613716102433 40.05283316157037, -105.16148653119157 40.05278423221279, -105.16159110510327 40.05271934887317, -105.16165401978081 40.05264675530231, -105.16172731980828 40.05258210256712, -105.16180220516941 40.05247829679478, -105.16190470818879 40.05240805722977, -105.16195204729715 40.05230765616699, -105.16202911042834 40.0522398322612, -105.16227731769125 40.05211314107409, -105.16257708525347 40.05202319452241, -105.16272713386697 40.051989729965435, -105.16285574064172 40.051961995558884, -105.16297586687922 40.05193543590796, -105.16309993112051 40.051924238339, -105.16324985979016 40.05191494894872, -105.16336583371255 40.05191585656047, -105.16343728604966 40.05189972807043, -105.16349411919751 40.051862916666835, -105.16357971309866 40.0517840142715, -105.1636657356831 40.05170844907624, -105.16370703176909 40.05165640548891, -105.16375243139824 40.051587870301326, -105.16383393165714 40.051523313978485, -105.16393266052312 40.05144388037487, -105.16404109960692 40.051395934726365, -105.1641309913249 40.05134884735053, -105.16426942821634 40.05131773912331, -105.16438675036066 40.05131644664036, -105.16448221081306 40.05131651800511, -105.16456784035591 40.051320002103346, -105.16472208125589 40.0513403043466, -105.16486083055051 40.05142553350745, -105.16492121273487 40.05148304796267, -105.16494539747187 40.051554116568475, -105.16494688078716 40.05161450597241, -105.16493538959601 40.05168266274925, -105.16492534082607 40.05173109043365, -105.1649357829235 40.051873679513044, -105.16495152805932 40.0519371797482, -105.16496695961008 40.05195100002284, -105.16505799940357 40.05195099953081, -105.16531139044459 40.052013820301006, -105.16531738443669 40.05201229577091, -105.1654030527817 40.05200806347592, -105.16550886297264 40.051990438273826, -105.16557990600035 40.05196663732222, -105.16564875098595 40.05193625429996, -105.16575590257582 40.05191750514264, -105.16590585112084 40.05190384239806, -105.16602015759356 40.051881736267774, -105.16605018168318 40.05185395159862, -105.16608561389279 40.051814082316696, -105.16613137907372 40.05176088895957, -105.16623840215007 40.05167736591554, -105.16632393731811 40.05160952042499, -105.16640114031144 40.05151207338047, -105.16647366015052 40.051460783756234, -105.16664087381784 40.05138324620814, -105.16669939099206 40.05136613985114, -105.16689810026186 40.05132446858931, -105.16709950307616 40.051278357338845, -105.16714646339913 40.05126049418936, -105.16720943944088 40.0512376803974, -105.16730229570373 40.05122237770144, -105.16742770939105 40.051208979083064, -105.16750503327624 40.05117737289109, -105.1676261415118 40.05113215513653, -105.16769637126981 40.05109189923789, -105.16778316381217 40.05104046255979, -105.16779310053964 40.051037659519785, -105.16890997143729 40.05103750031685, -105.1689467501823 40.05103749776507, -105.16898756521562 40.05103748966823, -105.16899600141247 40.05103741479722, -105.17113367617777 40.051031139646184, -105.17134724824902 40.0510305133593, -105.17135270736543 40.05103049558405, -105.17164277024654 40.05102964076442, -105.17164590999464 40.05102963168614, -105.1723984922067 40.05102741077957, -105.17240168118529 40.05102740001921, -105.17261652835224 40.05102676779798, -105.17269839973677 40.051026524515315, -105.1728325803302 40.051026128685734, -105.17368988990238 40.051023587411365, -105.17442878201399 40.05102139560601, -105.17530601403156 40.05101878505296, -105.17557010797324 40.051017996790875, -105.1755736157177 40.05101798773977, -105.17557712347508 40.05101797598657, -105.17558008508098 40.051017967201034, -105.17558414717193 40.05101795700623, -105.17619059900558 40.05101614793633, -105.17619411380304 40.0510161343829, -105.17619798603742 40.051016123633644, -105.17620113634044 40.05101611265975, -105.17620464760058 40.05101610359928, -105.17620815300526 40.05101609362164, -105.17803386164407 40.05101062691166, -105.17828268728758 40.05101600343033, -105.17828509981497 40.05095033556441, -105.17829099937236 40.050788998528716, -105.17836199168954 40.05013707172179, -105.17836199788928 40.050136999686956, -105.17838899940075 40.0494039987319, -105.17838899217111 40.04940279904402, -105.17838500001709 40.04872299868529, -105.17838233747429 40.047872975224664, -105.17838199975745 40.047764998763235, -105.17837000039427 40.04545199887659, -105.17835699895134 40.04397399911803, -105.17835938074074 40.04381992401295, -105.17836700021161 40.04332699857592, -105.17837099960056 40.04307199909479, -105.17838000011953 40.04215799916332, -105.17838000270959 40.04215794693271, -105.17838700002783 40.041061998756085, -105.17838999996249 40.040871999204725, -105.17839000046631 40.04081899851942, -105.17839200028992 40.04072099871122, -105.17840484336635 40.03966053615192, -105.17841999952066 40.03840899927504, -105.17842499964212 40.03670199816679, -105.17843999981758 40.03537799842891, -105.17848899998363 40.03472599927464, -105.17849000036797 40.03469499888762, -105.17853199970799 40.033534999257995, -105.17853699993337 40.03339099877271, -105.17853999916144 40.03279999949025, -105.17853099965508 40.03216499864769, -105.17847699991513 40.03169499900179, -105.17845899895991 40.031078999286784, -105.17846200011294 40.03036699889137, -105.17846800034636 40.02915899894963, -105.17850199998819 40.0272379988253, -105.17851599966946 40.0261089991069, -105.17851699942607 40.026054998695386, -105.17847999951732 40.02439999821404, -105.17846399958147 40.02391999874165, -105.17844499935862 40.023335998665985, -105.17841899922409 40.02213199938647, -105.17841200015711 40.02177899910858, -105.17837999919433 40.020485999149784, -105.17834600023595 40.01914399873556, -105.17830499949972 40.01838899907003, -105.17820299884812 40.01737399931093, -105.17814899995913 40.016843998939045, -105.17813200007618 40.016335999393746, -105.17814100038952 40.01595099914135, -105.17825700042589 40.01483999953051, -105.17826899956872 40.01463299858616, -105.17826884885845 40.014632915305484, -105.1782518670392 40.01369208709981, -105.17822015360817 40.012392968660315, -105.1782329229247 40.009687058879145, -105.17821083217468 40.00884586714735, -105.17820296100382 40.008546892453104, -105.1781999993325 40.007964077290126, -105.17818386150726 40.00729886938524, -105.17821091704616 40.00640702843349, -105.17824599799634 40.00585698788481, -105.17826102167494 40.00532089112599, -105.17823806916618 40.00148495285106, -105.1781969902901 40.00081006671814, -105.17818315599263 40.00056488123449, -105.17815695772794 40.000140948544384, -105.17690714734904 40.00016792502332, -105.17553896038821 40.000167102900186, -105.174943929118 40.00016597541908, -105.17249189705142 40.00012087845364, -105.17148100470412 40.00012294450879, -105.17105016969391 40.00012198994988, -105.1695448773694 40.000128941058954, -105.16871389663281 40.00012902694554, -105.1678868478647 40.00012802026858, -105.16546478139743 40.00012800196317, -105.1654798192196 40.00004424309991, -105.16556961219206 39.99937187250002, -105.16573285185758 39.99789118618674, -105.16578020581626 39.9974419470633, -105.16578874060889 39.99735372905148, -105.1658367798869 39.99690524121675, -105.16587303042463 39.99656131156476, -105.16591223286507 39.996182935814595, -105.16602314654831 39.99515061432765, -105.16610766217217 39.99433846647752, -105.16613441188971 39.99408141175241, -105.16611445166329 39.992990086239345, -105.16610119792009 39.99226524125937, -105.16608042822367 39.990474138455475, -105.16601504169904 39.988538059639225, -105.16526357003622 39.98855007082879, -105.16526006124123 39.9884278360004, -105.16521291681579 39.98840770990265, -105.16415290371303 39.98795517594412, -105.1640557053296 39.98791588344694, -105.16396297976111 39.98801302742708, -105.16388200786707 39.98807702897645, -105.1636180300277 39.988270070629724, -105.16337384727566 39.98842912912709, -105.16320684681372 39.988568921489694, -105.16313188022269 39.988645019677854, -105.1630340843738 39.98879105290501, -105.16297014459795 39.988947068850074, -105.16294114504788 39.9891100499324, -105.1629369535138 39.989236042381506, -105.16293166199242 39.98939933324853, -105.16304842454566 39.98939258460942, -105.16528009043512 39.98963757722175, -105.16528012126903 39.98963940654668, -105.16529391341399 39.990472654718204, -105.16443963017906 39.99047469439939, -105.16032929515781 39.99048441784612, -105.15988942232826 39.99048544917379, -105.15823517638263 39.99048931494893, -105.15823670374425 39.99049132434087, -105.15857279342244 39.99093128003249, -105.15824942352096 39.99149224398947, -105.1576955197453 39.99206442405352, -105.1570945121236 39.99246391068015, -105.15635960366501 39.99274076059307, -105.15617163194054 39.99274373072714, -105.15601279666635 39.992706679409515, -105.15507022849043 39.99239786295302, -105.15489277854675 39.992276366370156, -105.1548910742555 39.99251738266482, -105.15489050013137 39.99259868061086, -105.15489048768646 39.99260044586263, -105.15487985425969 39.99410483914303, -105.15272896554406 39.99412802825835, -105.15272916429981 39.994223301318996, -105.15272944476715 39.994362321365266, -105.15272970139479 39.9944982043476, -105.15272986792377 39.994584628347155, -105.15272987179958 39.99458662691797, -105.15273031889083 39.9948198724531, -105.15273074974802 39.99504526780311, -105.15273196063852 39.99568069342332, -105.15273292707768 39.996185895814065, -105.15273441900779 39.99618588769861, -105.15395198848165 39.99617947834857, -105.15457516485553 39.99617619263377, -105.15546049150397 39.99617391781758, -105.15621061524074 39.99617225447206, -105.15650599626977 39.99617247919943, -105.15724059904332 39.996173631503524, -105.15724037455517 39.99617565911632, -105.15717500769495 39.99676647874302, -105.15711649982177 39.997270859216364, -105.15709900858657 39.9974216510589, -105.15708085180212 39.997571806854644, -105.15704063493796 39.997991566377394, -105.15685262607542 39.999953858367746, -105.15684593640609 40.000042609907844, -105.15683674089738 40.00012757393174, -105.1568362961492 40.00012961529795, -105.15658839030704 40.00012897627218, -105.1550500005115 40.000124999206335, -105.15390199887914 40.00012399883708, -105.15377099903554 40.00012399912667, -105.15377073299338 40.000125192599, -105.15357817715062 40.00013044327525, -105.1535166309048 40.00019969629903, -105.15346163955572 40.000199963349786, -105.15323938607644 40.0003995175149, -105.15319035925384 40.00041976453732, -105.1526815171395 40.00062425548496, -105.15177345389893 40.000411898546815, -105.15167557793335 40.00020098063606, -105.15153734544808 40.00020071065877, -105.15153635236916 40.000200708558125, -105.1515160075409 40.0001189979974, -105.15151549572916 40.00011694385289, -105.15126449614058 40.000116943310466, -105.15122849551267 40.0001169433975, -105.14968650348173 40.00012394214083, -105.14953250330608 40.00012394248593, -105.14953250327905 40.00012599868626, -105.1405990316423 40.00013293952663, -105.14059142904382 40.000224906291045, -105.14058854507417 40.00027393090059, -105.14057555041046 40.00063393005045, -105.14060155185382 40.000812927619066, -105.14065755317074 40.000982926540395, -105.1407505560302 40.00112692615965, -105.14075085657349 40.00112723061763, -105.14084555586425 40.001222925977224, -105.14130455989637 40.001601923019926, -105.14179056115002 40.00198092282215, -105.14179001730211 40.00198145342109, -105.14159156600022 40.00217492028406, -105.14152556745809 40.00230091972836, -105.1415115688388 40.00233991970254, -105.14149956821704 40.00238291850106, -105.14148257012384 40.002499917779566, -105.1414825826895 40.00347591238927, -105.14149058489267 40.00358891121111, -105.14151758438891 40.00365291029514, -105.14150960352195 40.00377466514739, -105.14141415445575 40.00377504835109, -105.1405073285334 40.00377868691076, -105.14050820398356 40.0039638566653, -105.14050837596368 40.00400010325159, -105.14050838613834 40.00400217209295, -105.14050864887894 40.00405785874783, -105.14050957959384 40.00425431840782, -105.14050959389135 40.004257382488255, -105.14051098568495 40.004551441497554, -105.14051171785037 40.0047060325794, -105.14051199562529 40.00476531109808, -105.14051291779414 40.00496006307164, -105.14051384354828 40.005155468929736, -105.14051472821647 40.00534222924821, -105.14051523947612 40.0054507501174, -105.14051591692329 40.00559328571963, -105.14051710033527 40.0058433487435, -105.14051801107122 40.00603560944315, -105.14051890630327 40.00622503572305, -105.14051974501459 40.00640230115203, -105.14052046792277 40.00655532323205, -105.14052131356677 40.00673438548746, -105.1405227300227 40.00703333867119, -105.14052277312916 40.00704226881942, -105.14052303382604 40.00709723672683, -105.14052314025936 40.007121036918896, -105.14052318047405 40.00712851609968, -105.14052335335812 40.00716526074064, -105.14052335944076 40.00716677296265, -105.14052359529526 40.00721578925072, -105.14052362350347 40.007221991262455, -105.14052430156362 40.007365305909666, -105.13993627289945 40.00736244634241, -105.1398447187669 40.00725686822421, -105.13984289224915 40.007254762187365, -105.13974885824997 40.007255949131405, -105.13567225211118 40.00730740311281, -105.1354341517882 40.00731040633411, -105.13543242526539 40.00731109077897, -105.13542913545349 40.00731215936529, -105.135427728691 40.007312621458084, -105.1354258526205 40.00731323698013, -105.13542257210094 40.00731432000612, -105.13541929737464 40.00731541475887, -105.13541602728006 40.00731651943344, -105.13541276653572 40.007317627740036, -105.13540950455268 40.007318748651905, -105.13540625656131 40.00731988131641, -105.13540300269459 40.00732101756492, -105.13539976164354 40.007322166463, -105.13539652174428 40.00732331896733, -105.13539329112781 40.00732448771268, -105.13539006519126 40.00732565737344, -105.1353868426767 40.0073268441574, -105.13538362716035 40.00732803636732, -105.13538041511407 40.007329236694055, -105.13537721005157 40.00733044514874, -105.13537401313924 40.00733166263565, -105.13537081734013 40.00733289093387, -105.13536762971528 40.00733412376111, -105.1353644455413 40.00733536830775, -105.13536127069344 40.00733662098969, -105.1353581004821 40.00733788269282, -105.1353549384305 40.00733915162687, -105.13535177748739 40.00734043227291, -105.1353486235328 40.0073417201462, -105.13534547774285 40.007343014349836, -105.13534233657974 40.00734431937593, -105.13533919888674 40.00734563251877, -105.13533607167668 40.0073469565026, -105.1353329491368 40.00734828320308, -105.1353298312142 40.00734962252728, -105.13532672145614 40.0073509681818, -105.13532361633942 40.007352321956844, -105.1353205170111 40.00735368835932, -105.13531742585704 40.007355059290845, -105.13531434050101 40.00735644104851, -105.1353112632951 40.00735783183841, -105.13530818957865 40.00735922714261, -105.13530512634496 40.007360633287696, -105.13530207008544 40.00736204936203, -105.13529901378726 40.00736347264144, -105.13529596565837 40.00736490135053, -105.13529292683639 40.00736634179746, -105.13528989500296 40.00736778947173, -105.13528686663963 40.007369245262794, -105.1352838464216 40.007370710986784, -105.1352808355393 40.0073721830448, -105.13527783046473 40.00737366412773, -105.13527483004592 40.00737515062921, -105.13527183776274 40.007376648864856, -105.1352688524633 40.00737815522849, -105.13526587413794 40.00737967152132, -105.13526290283485 40.00738118873692, -105.13525993965773 40.00738271948803, -105.13525698230758 40.00738425566137, -105.1352540284179 40.00738580175289, -105.13525108620158 40.00738735508647, -105.13524815095934 40.00738891834928, -105.13524522271045 40.00739048793876, -105.1352423002596 40.00739206835435, -105.13523938599256 40.00739365149774, -105.13523648218913 40.007395249084674, -105.13523149040209 40.00739810368863, -105.13415327426647 40.00739890930889, -105.13129350339274 40.007400997770404, -105.13128462784326 40.00740100451655, -105.13128327976194 40.00740100560996, -105.1312832577426 40.00740312838888, -105.13125348753188 40.00740314937847, -105.13107834158829 40.00740538300349, -105.13107785322475 40.0074339520929, -105.13107007864642 40.007947006468015, -105.1310909392437 40.009568119283244, -105.13110080885212 40.01070634634, -105.1310997144627 40.010706856213574, -105.13109172677497 40.01172384982907, -105.13109673166252 40.012072847881676, -105.13109796977967 40.0120728383325, -105.13117000554146 40.012072269864234, -105.13125698422046 40.01207158521304, -105.13125700767907 40.01207374506328, -105.131257730989 40.01213947371401, -105.13134664664189 40.01213865468601, -105.1324447468638 40.01212852478138, -105.13566104011323 40.012109964060436, -105.13566207791715 40.01210995833265, -105.13579966560978 40.01210916173971, -105.13580153384838 40.012547739712424, -105.13580261996987 40.01280227681977, -105.13580392771401 40.013108303358045, -105.13580502132265 40.01336538933267, -105.13580504130005 40.013370201603955, -105.1358050604791 40.01337472476187, -105.13582041776242 40.01350958353772, -105.13583432503647 40.01363171595667, -105.135806156309 40.01363183505427, -105.1358072921032 40.013897254022766, -105.13580841762929 40.014161746176114, -105.13580983004466 40.01441792346685, -105.13581067593978 40.01466371889595, -105.13581067257898 40.01466588316285, -105.13581036028515 40.01487676008018, -105.13580992769808 40.015168270582194, -105.13580914380788 40.01569681831801, -105.13580834669948 40.016235075058916, -105.1358069737647 40.017160728330076, -105.13579921164248 40.01829673750202, -105.13559351159988 40.01829732614752, -105.13453390763979 40.01830035084866, -105.1345297826865 40.01831441593423, -105.13206163193061 40.018317289680894, -105.13171554063727 40.018317689131884, -105.1312431051194 40.01831823124324, -105.13117779869077 40.01831830522199, -105.13117777985237 40.018320488352714, -105.13105754950722 40.01831992727238, -105.13104296085905 40.01876495883627, -105.13103806260374 40.01914213441396, -105.13103596389206 40.01933209591846, -105.13102512615643 40.02021299758439, -105.13101114973331 40.021410136493856, -105.13100191445596 40.02212688053156, -105.13100159046962 40.02216011730349, -105.13100085540904 40.02215978531176, -105.13099885705896 40.02229978498944, -105.13100186380144 40.02277278218614, -105.13100486396942 40.0229017810233, -105.13100687427173 40.023762775741645, -105.13099788786366 40.024858769423936, -105.13099090375351 40.02611376122235, -105.13099579514224 40.027894109857264, -105.13099698251575 40.02794400096061, -105.13100002309253 40.027943937734435, -105.13104901639146 40.03658189669205, -105.1310650469673 40.03738107533779, -105.13109908899263 40.03834996598214, -105.1311201440057 40.03927708677072, -105.13114506408198 40.0398198926297, -105.13115908942807 40.0401320664122, -105.13115506518781 40.04047987090068, -105.1311510917365 40.04081806645879, -105.13115596238119 40.04321793513203, -105.13116101133868 40.04406704094007, -105.13115690946843 40.045154950077816, -105.13115700376582 40.045271340962486, -105.1311570490046 40.045327074461156, -105.13115587444632 40.04547805719804, -105.13116617366418 40.046611033174855, -105.13117597447743 40.047440114310525, -105.13117905990921 40.04779398012801, -105.13118411434779 40.048246129728135, -105.13118910011711 40.04930496819956, -105.13119310550192 40.050544986017755, -105.13120584610205 40.05096312075745, -105.13121078196237 40.05257722664825, -105.13121100544105 40.052650059567945, -105.13122091709235 40.053722913902455, -105.131216169747 40.054137972708894))</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -2680,7 +2692,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1782826872876 40.05101600343033, -105.1782648264534 40.05150006269764, -105.1782644506778 40.05154440521416, -105.1782639989751 40.05158099921608, -105.178263560529 40.05164953755293, -105.1782629098679 40.05172628563411, -105.17826281953 40.0517369797149, -105.1782599831768 40.05207187265444, -105.1783150298185 40.05289695593319, -105.1792791044592 40.05291391396824, -105.1808499194844 40.05297097716174, -105.1810900318997 40.05295901299321, -105.181634137556 40.05287212018803, -105.1820808364559 40.05275997603398, -105.183032859544 40.05252595895561, -105.1834799100499 40.05241408505804, -105.1837449660089 40.0523379457604, -105.1841109799606 40.05221404245921, -105.1845948610465 40.05201606556757, -105.1855890330141 40.05150489254471, -105.1859561437452 40.05133787312688, -105.1860739219509 40.05128301523376, -105.1865891528303 40.05110103698697, -105.186761844639 40.05106691731628, -105.1871139097341 40.05102202758273, -105.1874701141536 40.05100899230384, -105.1876408543125 40.05101110192317, -105.1898231403873 40.05099996834632, -105.190541176169 40.05099311224429, -105.193556072647 40.05099511879222, -105.1953150594626 40.05098303108169, -105.1970779129768 40.05098492732375, -105.1986618884415 40.05096711334441, -105.2003868673473 40.0509710568036, -105.2021501393274 40.05095887602959, -105.2041148441928 40.05095487116898, -105.2043788313958 40.0509539005148, -105.2044870718699 40.05095307988262, -105.2045610150865 40.05095299453317, -105.205092923763 40.05094996364262, -105.2068754960821 40.0509590891893, -105.2081978387787 40.05095099446869, -105.2090240797686 40.05095088430189, -105.2129851315648 40.05097810021972, -105.2142720767539 40.05100298094995, -105.2161281134339 40.05101689547124, -105.2181329590166 40.05098090728932, -105.2185580170287 40.05098798369225, -105.2195420594132 40.05100904745145, -105.2208558434475 40.05102293925202, -105.2239610583144 40.0510389198197, -105.2255020750835 40.0510420466769, -105.2313310609188 40.05105906073936, -105.2322589673265 40.05109498290111, -105.2328579827825 40.05110405832345, -105.233742911622 40.05109392331027, -105.234254046906 40.05108806575161, -105.234505146494 40.05109413413817, -105.2345658693909 40.0510950970329, -105.2348829780416 40.05109024293931, -105.2348717728759 40.04950637015926, -105.2366521446513 40.04810295900571, -105.236973906076 40.04784509661621, -105.2373031389998 40.04755756582615, -105.2379150718361 40.04702313301646, -105.238130844994 40.04683008772683, -105.2383869376615 40.04655505184557, -105.2385538760367 40.04633499171325, -105.2389010418821 40.04578207368654, -105.2390160894422 40.04558687675885, -105.2393799143466 40.04497195457869, -105.240272135138 40.04347893719775, -105.2405720149029 40.04304889223569, -105.2414939075501 40.04153506926259, -105.242137900229 40.04049086907413, -105.2422833566422 40.04025801664534, -105.2423570942121 40.04013997459672, -105.242371581746 40.0401394431425, -105.2425142025077 40.03991144219246, -105.24264120286 40.03971844241541, -105.2428152033527 40.03950244199812, -105.2430092033677 40.03929644165687, -105.2431468286627 40.03917225845748, -105.2432242029855 40.03910244206068, -105.2433064056922 40.03903892199388, -105.2434222030257 40.03894944238947, -105.2435522027756 40.03885844241933, -105.2437532031555 40.03873044189604, -105.2437872024745 40.03871244225677, -105.2438006785438 40.03859655127737, -105.2437996973181 40.03858015455958, -105.2425780966287 40.03862463649937, -105.2425769492914 40.03862654872201, -105.2385454852443 40.03864375463035, -105.2398934198544 40.03772339791855, -105.2404672015227 40.03726344178768, -105.241018201577 40.03650844155181, -105.2409032015566 40.03652344124953, -105.2396062009134 40.03652244116942, -105.2394381522089 40.03651262561413, -105.2391190094183 40.03621631438021, -105.2382342008113 40.03540544098632, -105.2378882000602 40.03516344213855, -105.237397200161 40.0349504419565, -105.2370662006303 40.03487744228755, -105.2367342003588 40.03483044207642, -105.2362041999249 40.03484844131424, -105.2359922007589 40.0349134417673, -105.2357952003409 40.03500344132726, -105.2356341995921 40.0350774410321, -105.2348572000809 40.03552544198848, -105.2348322862713 40.0361973792786, -105.2348242002542 40.03641544158987, -105.2348286362072 40.03708139570391, -105.2348372005173 40.03836744194803, -105.2338002012012 40.03945344235616, -105.2336891999156 40.04015244226186, -105.2335462006925 40.04015244262079, -105.2328302880019 40.04015369964417, -105.2314588703982 40.04015761180696, -105.2298354739006 40.04016222201453, -105.2286399728214 40.0401628702557, -105.2276746826273 40.0401621385647, -105.2258593874601 40.04016074121972, -105.22407704741 40.04015412622703, -105.223497505316 40.04015150481216, -105.2210591982608 40.04014044384326, -105.2209821983598 40.04014844366193, -105.220913197136 40.04017644371963, -105.2208591976603 40.04021944344885, -105.2208581977847 40.04005444358192, -105.2184331975993 40.04005444361138, -105.218441197225 40.03832844367185, -105.2207161974315 40.03835144348213, -105.2207471963628 40.0375574432325, -105.2207291969135 40.03650744297263, -105.2227401974629 40.03650644306278, -105.2227395470943 40.03558613982754, -105.2227431977602 40.03464544348129, -105.222917197469 40.03452644327425, -105.2232891976821 40.03439244202391, -105.2236111982574 40.03421344303411, -105.2241681975645 40.03399244230303, -105.2245743280957 40.03386447092257, -105.2250371980086 40.03374044312552, -105.2255911987063 40.03359744281072, -105.225982197759 40.03347944212604, -105.2259859825384 40.03291451209868, -105.2259870021577 40.0322697246056, -105.2259891973577 40.0312724419347, -105.2259891978973 40.03071444140571, -105.2259871977661 40.03029944157155, -105.2259931976188 40.02985144192847, -105.2259941979395 40.02962444223154, -105.2259961973092 40.0293284414642, -105.2253951967717 40.02932644126568, -105.225394197129 40.02923344208104, -105.2253944375382 40.02922698588036, -105.2253876759348 40.02922707245764, -105.2253838715813 40.02922712104237, -105.2250902606939 40.02922118797638, -105.2243452592167 40.02922218854747, -105.2242922587597 40.02922218887095, -105.2240485290634 40.0292221896779, -105.2240448012386 40.02921896182992, -105.2234171967727 40.02858844157902, -105.2231341967773 40.02873844263139, -105.2227491964695 40.02893444274527, -105.2221531959837 40.02913544191373, -105.2220471963629 40.0291604417221, -105.2217758048782 40.02920913506678, -105.2216681962193 40.02922844212854, -105.2215368541062 40.02924212396792, -105.221524196698 40.02924344258807, -105.2213741961431 40.02925244173912, -105.2209515721532 40.02925336013067, -105.22047383285 40.0292534418192, -105.2199463053364 40.02925557303384, -105.2191025662913 40.02925881640458, -105.2185102178733 40.02926210714222, -105.2184761957898 40.02926244201551, -105.2180831955133 40.02926644208032, -105.2178571961912 40.02928944246727, -105.2177341859115 40.02931463718165, -105.2176198784911 40.0293380499647, -105.2175251954509 40.02935744244781, -105.2173882346814 40.02940610874885, -105.2172628810816 40.02945581657214, -105.2171013733368 40.02953197961455, -105.2170861959579 40.02953944212074, -105.2169183296271 40.02964944212096, -105.216714195362 40.02978944179781, -105.216393195045 40.030018442685, -105.2163231954602 40.03000344222524, -105.2162281958708 40.02996544241743, -105.2161731957375 40.02993344293114, -105.2160821948466 40.029843442886, -105.2160431949233 40.02976544318457, -105.2160301953674 40.0296674427522, -105.2160241944471 40.02958644314366, -105.2160111955 40.02941744250101, -105.2159851951632 40.0292884429292, -105.2159541953328 40.02928944287671, -105.2158601952949 40.02929244290664, -105.2154397747579 40.02930063641094, -105.2142271952085 40.02931444306602, -105.2132951941631 40.02931044250712, -105.2121779687597 40.02931370359353, -105.2116561945448 40.0293154428859, -105.2115561934457 40.02929544246373, -105.2114661938733 40.02925644249451, -105.2113901939955 40.02920244289452, -105.2113691942612 40.02918144297956, -105.21132119374 40.02911044242671, -105.2112971941228 40.02903344233737, -105.2113005886311 40.02886265923356, -105.2113071938985 40.02853044222877, -105.2113161932457 40.02663444274262, -105.2112871930142 40.02556744269105, -105.2112831926451 40.02472144241093, -105.2112831927006 40.02414744200545, -105.2112661927701 40.02380644202619, -105.2112281926976 40.02354844225731, -105.2111681958693 40.02340961220849, -105.2111421929906 40.02334944202191, -105.2110908591813 40.02325882755933, -105.2110271929919 40.02314644131605, -105.2109292903985 40.02301884637291, -105.2109051937388 40.02298744145597, -105.2108295770383 40.02291528432966, -105.2107433476153 40.02283715262609, -105.2106593493525 40.0227561515699, -105.2104213509922 40.02261115079264, -105.210131353124 40.02246915041668, -105.2096453553682 40.02228714891598, -105.2092683557341 40.02218214859246, -105.2089568292927 40.02211259715015, -105.2085064200148 40.02197920421263, -105.2081351092813 40.0218317118302, -105.2077919256969 40.02163067272885, -105.2073173661939 40.02133714445619, -105.2072853658604 40.02131414432528, -105.2071853679822 40.02123014325992, -105.2069473712818 40.02099014246873, -105.2067823753913 40.02074214075176, -105.2066866789568 40.02047579851763, -105.2066508805403 40.02015162089645, -105.2066396306025 40.01988469898361, -105.2066282588804 40.01964637159548, -105.2066417223345 40.0193985748575, -105.2066873211797 40.01744464479255, -105.2067009491717 40.01715872104394, -105.2066918318187 40.01639614326426, -105.2067183070375 40.01600540075746, -105.2067098058444 40.0150998456722, -105.2067203549632 40.0147049988613, -105.2066710004365 40.01470499853, -105.206367999478 40.01470099950867, -105.2055099991169 40.01468499841905, -105.2052452071275 40.01468054190908, -105.2052129998992 40.0146799993535, -105.2048625378809 40.01467753585545, -105.2046439989874 40.01467599916017, -105.2045197317803 40.01467615277912, -105.2038309998592 40.01467699888822, -105.2027989994621 40.01467799882614, -105.2020579655673 40.01468239223043, -105.2020565681202 40.01468240032865, -105.2012799993588 40.01468699864344, -105.201182717144 40.01468616479592, -105.2009300000826 40.01468399931195, -105.2006159994158 40.01467999898198, -105.1988599995382 40.01467899903977, -105.1983059994697 40.01466299922393, -105.1967830001021 40.0146679988932, -105.1967699330014 40.01466790959612, -105.1966359998847 40.01466699895634, -105.1951779999087 40.01465899884218, -105.1943553939693 40.01465460062421, -105.1942429993284 40.01465399917136, -105.1895639999455 40.01463599872144, -105.1886723010191 40.01463892504425, -105.1880389993641 40.01464099911838, -105.1879306387029 40.01464043574966, -105.1868859994811 40.01463499863746, -105.1864974973728 40.01463462047163, -105.1858630004019 40.01463399899924, -105.1841701799736 40.01463570346134, -105.1838739999368 40.01463599886635, -105.1834549992717 40.0146349225061, -105.1827040007133 40.01463299831895, -105.1808354543097 40.01462562931187, -105.179412999948 40.01461999874561, -105.1782689995687 40.01463299858616, -105.1782570004259 40.01483999953051, -105.1781410003895 40.01595099914135, -105.1781320000762 40.01633599939375, -105.1781489999591 40.01684399893904, -105.1782029988481 40.01737399931093, -105.1783049994997 40.01838899907003, -105.1783460002359 40.01914399873556, -105.1783799991943 40.02048599914978, -105.1784120001571 40.02177899910858, -105.1784189992241 40.02213199938647, -105.1784449993586 40.02333599866598, -105.1784639995815 40.02391999874165, -105.1784799995173 40.02439999821404, -105.1785169994261 40.02605499869539, -105.1785159996695 40.0261089991069, -105.1785019999882 40.0272379988253, -105.1784680003464 40.02915899894963, -105.1784620001129 40.03036699889137, -105.1784589989599 40.03107899928678, -105.1784769999151 40.03169499900179, -105.1785309996551 40.03216499864769, -105.1785399991614 40.03279999949025, -105.1785369999334 40.03339099877271, -105.178531999708 40.03353499925799, -105.178490000368 40.03469499888762, -105.1784889999836 40.03472599927464, -105.1784399998176 40.03537799842891, -105.1784249996421 40.03670199816679, -105.1784199995207 40.03840899927504, -105.1784048433664 40.03966053615192, -105.1783920002899 40.04072099871122, -105.1783900004663 40.04081899851942, -105.1783899999625 40.04087199920473, -105.1783870000278 40.04106199875608, -105.1783800027096 40.04215794693271, -105.1783800001195 40.04215799916332, -105.1783709996006 40.04307199909479, -105.1783670002116 40.04332699857592, -105.1783593807407 40.04381992401295, -105.1783569989513 40.04397399911803, -105.1783700003943 40.04545199887659, -105.1783819997574 40.04776499876323, -105.1783823374743 40.04787297522466, -105.1783850000171 40.04872299868529, -105.1783889921711 40.04940279904402, -105.1783889994008 40.0494039987319, -105.1783619978893 40.05013699968696, -105.1783619916895 40.05013707172179, -105.1782909993724 40.05078899852872, -105.178285099815 40.05095033556441, -105.1782826872876 40.05101600343033))</t>
+          <t>POLYGON ((-105.17828268728758 40.05101600343033, -105.17826482645339 40.05150006269764, -105.17826445067783 40.05154440521416, -105.1782639989751 40.05158099921608, -105.17826356052903 40.05164953755293, -105.17826290986788 40.05172628563411, -105.17826281953003 40.0517369797149, -105.1782599831768 40.052071872654444, -105.1783150298185 40.05289695593319, -105.17927910445918 40.05291391396824, -105.18084991948444 40.05297097716174, -105.18109003189973 40.05295901299321, -105.18163413755602 40.05287212018803, -105.18208083645591 40.052759976033975, -105.18303285954396 40.05252595895561, -105.18347991004987 40.05241408505804, -105.18374496600886 40.0523379457604, -105.18411097996065 40.052214042459205, -105.18459486104653 40.05201606556757, -105.18558903301408 40.05150489254471, -105.18595614374524 40.05133787312688, -105.18607392195088 40.05128301523376, -105.1865891528303 40.05110103698697, -105.18676184463898 40.051066917316284, -105.18711390973405 40.051022027582725, -105.18747011415358 40.05100899230384, -105.18764085431249 40.05101110192317, -105.18982314038726 40.050999968346325, -105.19054117616905 40.050993112244285, -105.19355607264703 40.05099511879222, -105.19531505946262 40.050983031081685, -105.19707791297684 40.050984927323746, -105.19866188844146 40.050967113344406, -105.20038686734733 40.0509710568036, -105.20215013932743 40.05095887602959, -105.20411484419279 40.050954871168976, -105.20437883139577 40.0509539005148, -105.20448707186988 40.050953079882625, -105.20456101508651 40.05095299453317, -105.20509292376302 40.05094996364262, -105.20687549608213 40.0509590891893, -105.20819783877867 40.050950994468685, -105.20902407976862 40.05095088430189, -105.21298513156485 40.05097810021972, -105.21427207675386 40.051002980949946, -105.21612811343392 40.051016895471236, -105.21813295901661 40.05098090728932, -105.21855801702871 40.05098798369225, -105.21954205941316 40.05100904745145, -105.22085584344752 40.05102293925202, -105.22396105831439 40.051038919819696, -105.2255020750835 40.051042046676905, -105.23133106091885 40.051059060739355, -105.23225896732653 40.05109498290111, -105.23285798278255 40.05110405832345, -105.233742911622 40.05109392331027, -105.23425404690599 40.051088065751614, -105.23450514649396 40.05109413413817, -105.23456586939088 40.0510950970329, -105.23488297804161 40.05109024293931, -105.23487177287592 40.04950637015926, -105.23665214465126 40.04810295900571, -105.23697390607605 40.04784509661621, -105.23730313899979 40.04755756582615, -105.23791507183613 40.04702313301646, -105.23813084499396 40.04683008772683, -105.23838693766153 40.046555051845566, -105.23855387603672 40.04633499171325, -105.23890104188214 40.04578207368654, -105.23901608944219 40.045586876758854, -105.23937991434661 40.04497195457869, -105.24027213513796 40.043478937197754, -105.24057201490292 40.04304889223569, -105.24149390755007 40.041535069262586, -105.24213790022903 40.040490869074134, -105.24228335664218 40.04025801664534, -105.24235709421208 40.04013997459672, -105.24237158174604 40.0401394431425, -105.24251420250768 40.039911442192455, -105.24264120285997 40.039718442415406, -105.24281520335269 40.03950244199812, -105.24300920336769 40.03929644165687, -105.24314682866274 40.039172258457484, -105.24322420298553 40.03910244206068, -105.24330640569224 40.03903892199388, -105.24342220302569 40.038949442389466, -105.24355220277559 40.038858442419325, -105.24375320315555 40.038730441896035, -105.24378720247454 40.038712442256774, -105.24380067854382 40.038596551277365, -105.24379969731814 40.038580154559575, -105.24257809662866 40.03862463649937, -105.24257694929143 40.03862654872201, -105.23854548524427 40.03864375463035, -105.23989341985435 40.037723397918555, -105.24046720152272 40.03726344178768, -105.24101820157696 40.03650844155181, -105.24090320155658 40.03652344124953, -105.23960620091343 40.036522441169424, -105.23943815220889 40.03651262561413, -105.23911900941827 40.03621631438021, -105.2382342008113 40.035405440986324, -105.2378882000602 40.03516344213855, -105.23739720016104 40.034950441956504, -105.23706620063027 40.03487744228755, -105.2367342003588 40.03483044207642, -105.23620419992491 40.03484844131424, -105.23599220075887 40.0349134417673, -105.23579520034092 40.03500344132726, -105.23563419959214 40.0350774410321, -105.23485720008091 40.03552544198848, -105.23483228627128 40.036197379278605, -105.23482420025421 40.03641544158987, -105.23482863620723 40.03708139570391, -105.23483720051732 40.038367441948026, -105.23380020120116 40.039453442356155, -105.23368919991559 40.040152442261856, -105.23354620069246 40.04015244262079, -105.2328302880019 40.04015369964417, -105.2314588703982 40.04015761180696, -105.22983547390062 40.04016222201453, -105.22863997282141 40.0401628702557, -105.22767468262725 40.040162138564696, -105.22585938746009 40.040160741219715, -105.22407704741003 40.04015412622703, -105.22349750531596 40.04015150481216, -105.22105919826082 40.040140443843256, -105.2209821983598 40.040148443661934, -105.220913197136 40.04017644371963, -105.22085919766035 40.04021944344885, -105.2208581977847 40.040054443581916, -105.21843319759925 40.04005444361138, -105.21844119722505 40.03832844367185, -105.2207161974315 40.03835144348213, -105.22074719636284 40.0375574432325, -105.22072919691348 40.036507442972635, -105.22274019746293 40.03650644306278, -105.22273954709433 40.035586139827544, -105.22274319776018 40.03464544348129, -105.22291719746897 40.03452644327425, -105.22328919768213 40.034392442023915, -105.22361119825736 40.03421344303411, -105.22416819756447 40.03399244230303, -105.22457432809568 40.03386447092257, -105.22503719800864 40.03374044312552, -105.22559119870633 40.03359744281072, -105.22598219775895 40.033479442126044, -105.22598598253838 40.03291451209868, -105.2259870021577 40.0322697246056, -105.2259891973577 40.031272441934696, -105.2259891978973 40.03071444140571, -105.22598719776606 40.03029944157155, -105.22599319761879 40.02985144192847, -105.22599419793946 40.029624442231544, -105.22599619730916 40.0293284414642, -105.22539519677166 40.02932644126568, -105.22539419712899 40.02923344208104, -105.22539443753824 40.02922698588036, -105.2253876759348 40.029227072457644, -105.22538387158134 40.029227121042375, -105.2250902606939 40.029221187976376, -105.2243452592167 40.02922218854747, -105.22429225875968 40.029222188870946, -105.22404852906344 40.029222189677895, -105.22404480123862 40.02921896182992, -105.22341719677267 40.02858844157902, -105.22313419677728 40.028738442631386, -105.2227491964695 40.028934442745275, -105.22215319598371 40.02913544191373, -105.22204719636294 40.0291604417221, -105.22177580487825 40.02920913506678, -105.22166819621934 40.02922844212854, -105.22153685410616 40.02924212396792, -105.22152419669797 40.02924344258807, -105.22137419614309 40.02925244173912, -105.22095157215317 40.029253360130674, -105.22047383285002 40.0292534418192, -105.21994630533635 40.029255573033836, -105.21910256629131 40.02925881640458, -105.21851021787334 40.02926210714222, -105.21847619578985 40.02926244201551, -105.2180831955133 40.02926644208032, -105.21785719619116 40.029289442467274, -105.21773418591154 40.02931463718165, -105.21761987849106 40.0293380499647, -105.2175251954509 40.02935744244781, -105.21738823468142 40.02940610874885, -105.21726288108155 40.02945581657214, -105.2171013733368 40.02953197961455, -105.21708619595795 40.02953944212074, -105.21691832962706 40.02964944212096, -105.21671419536204 40.02978944179781, -105.21639319504503 40.030018442685, -105.21632319546022 40.03000344222524, -105.2162281958708 40.029965442417435, -105.21617319573753 40.02993344293114, -105.21608219484663 40.029843442886, -105.21604319492326 40.029765443184566, -105.21603019536744 40.0296674427522, -105.21602419444714 40.02958644314366, -105.21601119549997 40.029417442501014, -105.21598519516317 40.0292884429292, -105.21595419533278 40.02928944287671, -105.21586019529485 40.029292442906645, -105.21543977475791 40.029300636410944, -105.21422719520845 40.02931444306602, -105.21329519416307 40.029310442507125, -105.21217796875966 40.02931370359353, -105.21165619454476 40.029315442885895, -105.21155619344569 40.029295442463734, -105.21146619387335 40.029256442494514, -105.21139019399551 40.02920244289452, -105.21136919426115 40.029181442979564, -105.21132119373996 40.02911044242671, -105.21129719412276 40.029033442337365, -105.21130058863108 40.02886265923356, -105.21130719389852 40.02853044222877, -105.2113161932457 40.02663444274262, -105.21128719301419 40.02556744269105, -105.21128319264511 40.02472144241093, -105.21128319270062 40.02414744200545, -105.21126619277014 40.02380644202619, -105.21122819269765 40.02354844225731, -105.21116819586933 40.02340961220849, -105.21114219299055 40.02334944202191, -105.21109085918125 40.02325882755933, -105.2110271929919 40.02314644131605, -105.21092929039852 40.02301884637291, -105.21090519373878 40.022987441455975, -105.21082957703833 40.022915284329656, -105.21074334761526 40.02283715262609, -105.21065934935245 40.0227561515699, -105.21042135099223 40.02261115079264, -105.21013135312397 40.022469150416676, -105.20964535536818 40.02228714891598, -105.20926835573408 40.022182148592464, -105.20895682929275 40.02211259715015, -105.20850642001483 40.02197920421263, -105.20813510928129 40.021831711830195, -105.20779192569692 40.021630672728854, -105.2073173661939 40.02133714445619, -105.20728536586044 40.02131414432528, -105.20718536798223 40.02123014325992, -105.20694737128179 40.02099014246873, -105.2067823753913 40.02074214075176, -105.20668667895676 40.02047579851763, -105.2066508805403 40.02015162089645, -105.20663963060254 40.01988469898361, -105.20662825888037 40.019646371595485, -105.20664172233452 40.019398574857505, -105.20668732117969 40.01744464479255, -105.20670094917168 40.01715872104394, -105.20669183181872 40.01639614326426, -105.20671830703753 40.016005400757464, -105.20670980584435 40.0150998456722, -105.20672035496321 40.0147049988613, -105.20667100043647 40.01470499853, -105.20636799947805 40.01470099950867, -105.20550999911694 40.01468499841905, -105.20524520712755 40.01468054190908, -105.20521299989923 40.0146799993535, -105.20486253788094 40.014677535855455, -105.20464399898744 40.01467599916017, -105.20451973178025 40.01467615277912, -105.20383099985916 40.01467699888822, -105.20279899946215 40.014677998826144, -105.20205796556735 40.01468239223043, -105.20205656812023 40.014682400328645, -105.20127999935877 40.01468699864344, -105.20118271714404 40.01468616479592, -105.2009300000826 40.01468399931195, -105.20061599941579 40.01467999898198, -105.19885999953817 40.014678999039766, -105.19830599946968 40.01466299922393, -105.1967830001021 40.014667998893195, -105.19676993300136 40.01466790959612, -105.19663599988468 40.01466699895634, -105.1951779999087 40.01465899884218, -105.19435539396932 40.01465460062421, -105.19424299932842 40.01465399917136, -105.18956399994552 40.01463599872144, -105.18867230101914 40.01463892504425, -105.18803899936414 40.014640999118384, -105.18793063870288 40.01464043574966, -105.18688599948108 40.01463499863746, -105.18649749737284 40.014634620471625, -105.18586300040191 40.014633998999244, -105.18417017997363 40.01463570346134, -105.18387399993684 40.014635998866346, -105.18345499927167 40.014634922506104, -105.18270400071329 40.01463299831895, -105.18083545430966 40.01462562931187, -105.17941299994798 40.01461999874561, -105.17826899956872 40.01463299858616, -105.17825700042589 40.01483999953051, -105.17814100038952 40.01595099914135, -105.17813200007618 40.016335999393746, -105.17814899995913 40.016843998939045, -105.17820299884812 40.01737399931093, -105.17830499949972 40.01838899907003, -105.17834600023595 40.01914399873556, -105.17837999919433 40.020485999149784, -105.17841200015711 40.02177899910858, -105.17841899922409 40.02213199938647, -105.17844499935862 40.023335998665985, -105.17846399958147 40.02391999874165, -105.17847999951732 40.02439999821404, -105.17851699942607 40.026054998695386, -105.17851599966946 40.0261089991069, -105.17850199998819 40.0272379988253, -105.17846800034636 40.02915899894963, -105.17846200011294 40.03036699889137, -105.17845899895991 40.031078999286784, -105.17847699991513 40.03169499900179, -105.17853099965508 40.03216499864769, -105.17853999916144 40.03279999949025, -105.17853699993337 40.03339099877271, -105.17853199970799 40.033534999257995, -105.17849000036797 40.03469499888762, -105.17848899998363 40.03472599927464, -105.17843999981758 40.03537799842891, -105.17842499964212 40.03670199816679, -105.17841999952066 40.03840899927504, -105.17840484336635 40.03966053615192, -105.17839200028992 40.04072099871122, -105.17839000046631 40.04081899851942, -105.17838999996249 40.040871999204725, -105.17838700002783 40.041061998756085, -105.17838000270959 40.04215794693271, -105.17838000011953 40.04215799916332, -105.17837099960056 40.04307199909479, -105.17836700021161 40.04332699857592, -105.17835938074074 40.04381992401295, -105.17835699895134 40.04397399911803, -105.17837000039427 40.04545199887659, -105.17838199975745 40.047764998763235, -105.17838233747429 40.047872975224664, -105.17838500001709 40.04872299868529, -105.17838899217111 40.04940279904402, -105.17838899940075 40.0494039987319, -105.17836199788928 40.050136999686956, -105.17836199168954 40.05013707172179, -105.17829099937236 40.050788998528716, -105.17828509981497 40.05095033556441, -105.17828268728758 40.05101600343033))</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -2722,7 +2734,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1960821947275 40.06189544761963, -105.1962251942363 40.0631234489768, -105.1975131946994 40.06384744877385, -105.197510194433 40.06410844816937, -105.1994881955361 40.06370844772376, -105.2004271948154 40.0631064479396, -105.2008701954203 40.06280544810341, -105.2010431953765 40.06269044755282, -105.2012341952632 40.06256244833814, -105.2023031957252 40.06217144785335, -105.2039191966671 40.06188244736903, -105.2039251968715 40.06102844726419, -105.2020971959404 40.06055644730947, -105.2020791960017 40.06027244767436, -105.2022581955147 40.06021544819658, -105.2025611961079 40.05994444774891, -105.2029191954679 40.05892644793907, -105.2030841948025 40.05879544709134, -105.2036141957108 40.05861644723085, -105.2043011952846 40.05848944735493, -105.2048171966658 40.05844444708361, -105.2052551959982 40.05847144768208, -105.2055541963941 40.05838544689875, -105.2068740084848 40.05834961512206, -105.2068748975684 40.0589608656869, -105.2068741762046 40.05938002791319, -105.2068749843029 40.06085309603117, -105.2068520652456 40.06169608423045, -105.2068438304768 40.06178308493803, -105.2068437684325 40.06179232904368, -105.2070381967239 40.06179344782172, -105.2116771982488 40.06182044730468, -105.2144889285572 40.06184333056139, -105.2160151985019 40.06185644695927, -105.2161351423245 40.06185481826265, -105.2161351368842 40.06185105984153, -105.2161370248116 40.06165505807027, -105.2161389050824 40.0607749575591, -105.2161151623542 40.05918488788823, -105.2159997620123 40.0591844562415, -105.2159321990569 40.05825844688626, -105.212820197039 40.05823044648699, -105.2128581978988 40.05759144654688, -105.2130431979704 40.05758444664818, -105.213117197296 40.05756744624475, -105.2131981981032 40.05754944636183, -105.2133621975794 40.05750044691125, -105.213604197271 40.05742944613198, -105.2139361978653 40.05733944632712, -105.2142531979739 40.05728144632609, -105.2143381982444 40.0572654468832, -105.2147491987564 40.05722544618729, -105.2150271981241 40.05721844599338, -105.2160991982986 40.05722244647633, -105.2160881989679 40.05694944610164, -105.2160381978682 40.05677044599801, -105.2159241988464 40.05654844624868, -105.215927198784 40.05607344660881, -105.2159399253224 40.05548742980623, -105.2159491981005 40.05506044566964, -105.2159731984142 40.05462644657686, -105.2178801587147 40.05464468834945, -105.2199480798594 40.05465482055129, -105.22080819831 40.05466444502937, -105.2207951986344 40.0557584459232, -105.2215101992092 40.05551444592377, -105.2226751991902 40.05523444591667, -105.2234611993335 40.05515144511462, -105.2238901992559 40.05506344591768, -105.2242669549185 40.05496813582263, -105.2244915600372 40.05491131624516, -105.2245622003918 40.05489344487475, -105.2247629796722 40.05483727490623, -105.2248982008678 40.05479944495026, -105.2250889657715 40.0547790063182, -105.2252621999629 40.05476044491763, -105.2255182005121 40.05476544570443, -105.2255172002856 40.05374544531903, -105.2255144818426 40.05233267196999, -105.2255131993988 40.05166644490966, -105.2255121997152 40.05104844465996, -105.2255132508242 40.05104207956713, -105.2255020750835 40.0510420466769, -105.2239610583144 40.0510389198197, -105.2208558434475 40.05102293925202, -105.2195420594132 40.05100904745145, -105.2185580170287 40.05098798369225, -105.2181329590166 40.05098090728932, -105.2161281134339 40.05101689547124, -105.2142720767539 40.05100298094995, -105.2129851315648 40.05097810021972, -105.2090240797686 40.05095088430189, -105.2081978387787 40.05095099446869, -105.2068754960821 40.0509590891893, -105.205092923763 40.05094996364262, -105.2045610150865 40.05095299453317, -105.2044870718699 40.05095307988262, -105.2043788313958 40.0509539005148, -105.2041148441928 40.05095487116898, -105.2021501393274 40.05095887602959, -105.2003868673473 40.0509710568036, -105.1986618884415 40.05096711334441, -105.1970779129768 40.05098492732375, -105.1953150594626 40.05098303108169, -105.193556072647 40.05099511879222, -105.190541176169 40.05099311224429, -105.1898231403873 40.05099996834632, -105.1876408543125 40.05101110192317, -105.1874701141536 40.05100899230384, -105.1874830192246 40.05107710836387, -105.1875660074355 40.05128596709104, -105.1875879525897 40.05140791340108, -105.1875778656828 40.05181609530394, -105.1875600554017 40.0526621148755, -105.187572844066 40.05314502800933, -105.1875631799087 40.05431802100534, -105.1875728747385 40.05438502954205, -105.1876240915529 40.05451199601824, -105.187716097916 40.05462507225001, -105.187806868407 40.05469586942515, -105.1890060523925 40.05525610584433, -105.1899970110951 40.05573204335349, -105.1901521703863 40.05578489233883, -105.1902560228349 40.05580795669995, -105.1904249215761 40.05582488102775, -105.1915640832911 40.05576396818461, -105.1918738386621 40.05575793274691, -105.191969912644 40.05576313110993, -105.1920598386544 40.05578505787751, -105.1921418331136 40.0558228860117, -105.1922069688011 40.05587604142063, -105.1922860284396 40.05600994299636, -105.1923229025104 40.05615086969796, -105.1923349934261 40.05742906057168, -105.1923378644477 40.05798002742052, -105.1923260857593 40.05876896275024, -105.1923369278518 40.05976988664435, -105.1923121153621 40.0606760066349, -105.1923271715966 40.06161407709632, -105.1923190191863 40.06175790262779, -105.1923131275911 40.06195499140038, -105.1923279987251 40.06206401506077, -105.1923691540231 40.06220687413975, -105.1924478996872 40.0623330885058, -105.1927811391311 40.0626719079231, -105.1932001627259 40.06253903928965, -105.1928981932525 40.06221544871938, -105.1928621939255 40.06214444837541, -105.192830194072 40.06206044878067, -105.1928031939953 40.06197244919012, -105.1930531938404 40.06188344841224, -105.1935278372535 40.06188410371627, -105.1939389409759 40.06188596206637, -105.1939423130284 40.06188444891134, -105.1944631938403 40.06188444842264, -105.1960821947275 40.06189544761963))</t>
+          <t>POLYGON ((-105.19608219472745 40.061895447619634, -105.19622519423635 40.0631234489768, -105.19751319469937 40.06384744877385, -105.197510194433 40.06410844816937, -105.1994881955361 40.06370844772376, -105.20042719481545 40.0631064479396, -105.20087019542031 40.06280544810341, -105.20104319537651 40.06269044755282, -105.2012341952632 40.06256244833814, -105.20230319572521 40.06217144785335, -105.20391919666712 40.06188244736903, -105.20392519687151 40.061028447264185, -105.20209719594037 40.060556447309466, -105.2020791960017 40.06027244767436, -105.20225819551469 40.06021544819658, -105.20256119610794 40.05994444774891, -105.20291919546786 40.05892644793907, -105.20308419480254 40.05879544709134, -105.20361419571084 40.058616447230854, -105.20430119528456 40.05848944735493, -105.20481719666584 40.05844444708361, -105.20525519599822 40.05847144768208, -105.20555419639409 40.058385446898754, -105.20687400848476 40.05834961512206, -105.20687489756837 40.0589608656869, -105.20687417620464 40.05938002791319, -105.20687498430289 40.060853096031174, -105.20685206524557 40.06169608423045, -105.20684383047684 40.06178308493803, -105.2068437684325 40.061792329043676, -105.20703819672389 40.06179344782172, -105.2116771982488 40.061820447304676, -105.21448892855722 40.061843330561395, -105.21601519850194 40.06185644695927, -105.21613514232453 40.06185481826265, -105.21613513688418 40.06185105984153, -105.2161370248116 40.061655058070265, -105.21613890508245 40.060774957559104, -105.21611516235417 40.05918488788823, -105.21599976201229 40.0591844562415, -105.21593219905685 40.05825844688626, -105.21282019703902 40.05823044648699, -105.21285819789883 40.05759144654688, -105.21304319797039 40.05758444664818, -105.213117197296 40.057567446244754, -105.21319819810316 40.057549446361826, -105.21336219757937 40.05750044691125, -105.21360419727095 40.057429446131984, -105.2139361978653 40.05733944632712, -105.21425319797387 40.05728144632609, -105.21433819824436 40.0572654468832, -105.21474919875641 40.05722544618729, -105.21502719812406 40.05721844599338, -105.21609919829862 40.05722244647633, -105.2160881989679 40.05694944610164, -105.21603819786819 40.05677044599801, -105.21592419884637 40.05654844624868, -105.21592719878397 40.056073446608806, -105.21593992532243 40.05548742980623, -105.21594919810053 40.05506044566964, -105.21597319841416 40.05462644657686, -105.21788015871469 40.05464468834945, -105.21994807985942 40.05465482055129, -105.22080819830997 40.054664445029374, -105.22079519863445 40.0557584459232, -105.22151019920918 40.05551444592377, -105.2226751991902 40.055234445916675, -105.22346119933347 40.055151445114625, -105.22389019925588 40.05506344591768, -105.22426695491855 40.05496813582263, -105.22449156003717 40.05491131624516, -105.22456220039183 40.05489344487475, -105.22476297967225 40.054837274906234, -105.22489820086776 40.054799444950255, -105.22508896577155 40.0547790063182, -105.22526219996293 40.05476044491763, -105.22551820051213 40.054765445704426, -105.2255172002856 40.05374544531903, -105.22551448184258 40.052332671969985, -105.22551319939883 40.051666444909664, -105.22551219971524 40.05104844465996, -105.2255132508242 40.05104207956713, -105.2255020750835 40.051042046676905, -105.22396105831439 40.051038919819696, -105.22085584344752 40.05102293925202, -105.21954205941316 40.05100904745145, -105.21855801702871 40.05098798369225, -105.21813295901661 40.05098090728932, -105.21612811343392 40.051016895471236, -105.21427207675386 40.051002980949946, -105.21298513156485 40.05097810021972, -105.20902407976862 40.05095088430189, -105.20819783877867 40.050950994468685, -105.20687549608213 40.0509590891893, -105.20509292376302 40.05094996364262, -105.20456101508651 40.05095299453317, -105.20448707186988 40.050953079882625, -105.20437883139577 40.0509539005148, -105.20411484419279 40.050954871168976, -105.20215013932743 40.05095887602959, -105.20038686734733 40.0509710568036, -105.19866188844146 40.050967113344406, -105.19707791297684 40.050984927323746, -105.19531505946262 40.050983031081685, -105.19355607264703 40.05099511879222, -105.19054117616905 40.050993112244285, -105.18982314038726 40.050999968346325, -105.18764085431249 40.05101110192317, -105.18747011415358 40.05100899230384, -105.18748301922463 40.05107710836387, -105.18756600743554 40.05128596709104, -105.18758795258968 40.05140791340108, -105.18757786568275 40.05181609530394, -105.18756005540168 40.052662114875496, -105.18757284406598 40.053145028009325, -105.1875631799087 40.054318021005344, -105.1875728747385 40.05438502954205, -105.18762409155286 40.05451199601824, -105.18771609791604 40.05462507225001, -105.18780686840704 40.054695869425146, -105.18900605239251 40.05525610584433, -105.18999701109513 40.05573204335349, -105.19015217038631 40.05578489233883, -105.19025602283494 40.05580795669995, -105.19042492157611 40.055824881027746, -105.19156408329107 40.055763968184614, -105.19187383866208 40.05575793274691, -105.19196991264398 40.055763131109934, -105.19205983865436 40.05578505787751, -105.19214183311357 40.0558228860117, -105.19220696880112 40.05587604142063, -105.19228602843958 40.05600994299636, -105.19232290251036 40.05615086969796, -105.19233499342606 40.05742906057168, -105.1923378644477 40.05798002742052, -105.19232608575933 40.058768962750236, -105.19233692785184 40.05976988664435, -105.19231211536213 40.0606760066349, -105.19232717159663 40.061614077096316, -105.19231901918627 40.06175790262779, -105.19231312759109 40.06195499140038, -105.19232799872515 40.06206401506077, -105.1923691540231 40.062206874139754, -105.19244789968718 40.0623330885058, -105.1927811391311 40.0626719079231, -105.19320016272589 40.06253903928965, -105.19289819325246 40.06221544871938, -105.19286219392555 40.062144448375406, -105.192830194072 40.06206044878067, -105.19280319399527 40.06197244919012, -105.19305319384037 40.06188344841224, -105.19352783725346 40.06188410371627, -105.19393894097588 40.06188596206637, -105.19394231302836 40.061884448911336, -105.1944631938403 40.06188444842264, -105.19608219472745 40.061895447619634))</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -2764,7 +2776,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1784389978209 40.06250902945073, -105.1793061843293 40.06251039500064, -105.1804101034247 40.06250709331072, -105.1807809107792 40.06250189337818, -105.1808792950956 40.06248642751207, -105.1809818361483 40.06245838376665, -105.1812240041372 40.06235518637328, -105.1812404473227 40.0623426416048, -105.1814415779459 40.06225506745857, -105.1817535568669 40.06211429107486, -105.1820142414536 40.06199575457967, -105.182648259628 40.06244855791299, -105.1829217252438 40.06260732591054, -105.1832576233965 40.06272744841069, -105.1839352461995 40.06283133001712, -105.1845896211293 40.062857448644, -105.1853016220106 40.06277944797684, -105.1859546228259 40.06267644696645, -105.1859053468927 40.06119793928947, -105.1886851148256 40.06029994091084, -105.1923596162155 40.06287144706564, -105.1927811391311 40.0626719079231, -105.1924478996872 40.0623330885058, -105.1923691540231 40.06220687413975, -105.1923279987251 40.06206401506077, -105.1923131275911 40.06195499140038, -105.1923190191863 40.06175790262779, -105.1923271715966 40.06161407709632, -105.1923121153621 40.0606760066349, -105.1923369278518 40.05976988664435, -105.1923260857593 40.05876896275024, -105.1923378644477 40.05798002742052, -105.1923349934261 40.05742906057168, -105.1923229025104 40.05615086969796, -105.1922860284396 40.05600994299636, -105.1922069688011 40.05587604142063, -105.1921418331136 40.0558228860117, -105.1920598386544 40.05578505787751, -105.191969912644 40.05576313110993, -105.1918738386621 40.05575793274691, -105.1915640832911 40.05576396818461, -105.1904249215761 40.05582488102775, -105.1902560228349 40.05580795669995, -105.1901521703863 40.05578489233883, -105.1899970110951 40.05573204335349, -105.1890060523925 40.05525610584433, -105.187806868407 40.05469586942515, -105.187716097916 40.05462507225001, -105.1876240915529 40.05451199601824, -105.1875728747385 40.05438502954205, -105.1875631799087 40.05431802100534, -105.187572844066 40.05314502800933, -105.1875600554017 40.0526621148755, -105.1875778656828 40.05181609530394, -105.1875879525897 40.05140791340108, -105.1875660074355 40.05128596709104, -105.1874830192246 40.05107710836387, -105.1874701141536 40.05100899230384, -105.1871139097341 40.05102202758273, -105.186761844639 40.05106691731628, -105.1865891528303 40.05110103698697, -105.1860739219509 40.05128301523376, -105.1859561437452 40.05133787312688, -105.1855890330141 40.05150489254471, -105.1845948610465 40.05201606556757, -105.1841109799606 40.05221404245921, -105.1837449660089 40.0523379457604, -105.1834799100499 40.05241408505804, -105.183032859544 40.05252595895561, -105.1820808364559 40.05275997603398, -105.181634137556 40.05287212018803, -105.1810900318997 40.05295901299321, -105.1808499194844 40.05297097716174, -105.1792791044592 40.05291391396824, -105.1783150298185 40.05289695593319, -105.1783188115135 40.05354129855904, -105.1783261176787 40.0547859519297, -105.1783680552524 40.05642110313737, -105.1783599732862 40.05677109239733, -105.1783591501339 40.0570969437221, -105.1783769328844 40.05900599693569, -105.1783991261733 40.06088898368674, -105.1784389978209 40.06250902945073))</t>
+          <t>POLYGON ((-105.1784389978209 40.06250902945073, -105.17930618432933 40.062510395000636, -105.1804101034247 40.06250709331072, -105.18078091077925 40.062501893378176, -105.18087929509562 40.06248642751207, -105.18098183614832 40.06245838376665, -105.18122400413722 40.06235518637328, -105.1812404473227 40.0623426416048, -105.18144157794586 40.06225506745857, -105.1817535568669 40.06211429107486, -105.18201424145363 40.06199575457967, -105.18264825962801 40.062448557912994, -105.18292172524383 40.06260732591054, -105.18325762339646 40.06272744841069, -105.18393524619951 40.06283133001712, -105.18458962112933 40.062857448643996, -105.18530162201056 40.06277944797684, -105.1859546228259 40.06267644696645, -105.18590534689268 40.06119793928947, -105.18868511482556 40.060299940910845, -105.19235961621548 40.06287144706564, -105.1927811391311 40.0626719079231, -105.19244789968718 40.0623330885058, -105.1923691540231 40.062206874139754, -105.19232799872515 40.06206401506077, -105.19231312759109 40.06195499140038, -105.19231901918627 40.06175790262779, -105.19232717159663 40.061614077096316, -105.19231211536213 40.0606760066349, -105.19233692785184 40.05976988664435, -105.19232608575933 40.058768962750236, -105.1923378644477 40.05798002742052, -105.19233499342606 40.05742906057168, -105.19232290251036 40.05615086969796, -105.19228602843958 40.05600994299636, -105.19220696880112 40.05587604142063, -105.19214183311357 40.0558228860117, -105.19205983865436 40.05578505787751, -105.19196991264398 40.055763131109934, -105.19187383866208 40.05575793274691, -105.19156408329107 40.055763968184614, -105.19042492157611 40.055824881027746, -105.19025602283494 40.05580795669995, -105.19015217038631 40.05578489233883, -105.18999701109513 40.05573204335349, -105.18900605239251 40.05525610584433, -105.18780686840704 40.054695869425146, -105.18771609791604 40.05462507225001, -105.18762409155286 40.05451199601824, -105.1875728747385 40.05438502954205, -105.1875631799087 40.054318021005344, -105.18757284406598 40.053145028009325, -105.18756005540168 40.052662114875496, -105.18757786568275 40.05181609530394, -105.18758795258968 40.05140791340108, -105.18756600743554 40.05128596709104, -105.18748301922463 40.05107710836387, -105.18747011415358 40.05100899230384, -105.18711390973405 40.051022027582725, -105.18676184463898 40.051066917316284, -105.1865891528303 40.05110103698697, -105.18607392195088 40.05128301523376, -105.18595614374524 40.05133787312688, -105.18558903301408 40.05150489254471, -105.18459486104653 40.05201606556757, -105.18411097996065 40.052214042459205, -105.18374496600886 40.0523379457604, -105.18347991004987 40.05241408505804, -105.18303285954396 40.05252595895561, -105.18208083645591 40.052759976033975, -105.18163413755602 40.05287212018803, -105.18109003189973 40.05295901299321, -105.18084991948444 40.05297097716174, -105.17927910445918 40.05291391396824, -105.1783150298185 40.05289695593319, -105.17831881151353 40.05354129855904, -105.17832611767871 40.0547859519297, -105.17836805525243 40.056421103137374, -105.17835997328619 40.05677109239733, -105.17835915013391 40.0570969437221, -105.17837693288443 40.05900599693569, -105.17839912617335 40.06088898368674, -105.1784389978209 40.06250902945073))</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -2806,7 +2818,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1312151333568 40.05463829014283, -105.1312051341252 40.0549272902714, -105.1312061330529 40.05519229072108, -105.131207134803 40.05564929051275, -105.1312051349296 40.05727829088557, -105.1312131325501 40.05874928993782, -105.1312141338369 40.05887029037866, -105.131228134939 40.05974929071716, -105.1312201340746 40.06002129004976, -105.1312141343774 40.06023929086055, -105.1312251347958 40.06072029049393, -105.1312291345053 40.06187129073018, -105.131234134076 40.06223529081105, -105.131220135557 40.06361729016729, -105.1312161352539 40.06423529025914, -105.1312261348082 40.06486429056906, -105.1312181355008 40.06555429029728, -105.1312311345578 40.06758328902276, -105.1312421349654 40.06840629078298, -105.1312471352586 40.06877329065517, -105.1312571353166 40.07052429035368, -105.1312561355187 40.07114629121654, -105.131250135106 40.07142728958371, -105.1312471358889 40.07157529118987, -105.1312769801043 40.07280485163446, -105.1312771363536 40.07281128908546, -105.1313291354456 40.07367829108345, -105.1313121353605 40.07453929131646, -105.1313161362929 40.07558629064913, -105.131364137045 40.08008229048873, -105.1314061367591 40.0827892910741, -105.1314141381591 40.08325728973681, -105.1314231385745 40.08373028926654, -105.1314680581192 40.08735891798165, -105.1314681373808 40.08736529032833, -105.1314686920482 40.08736528489368, -105.1349071383346 40.08733428902195, -105.1373061386617 40.08732428977066, -105.1382631386586 40.08732328982324, -105.1409871387648 40.08731128953013, -105.1420031391563 40.08730728976931, -105.1422081395893 40.08730028957377, -105.1443011396943 40.08730228806577, -105.146593138654 40.08730128957986, -105.1490541379685 40.08730928858999, -105.1497181388009 40.08731828785967, -105.1500315862041 40.08732238622535, -105.1500284624822 40.0871466566247, -105.1500291083445 40.08709170551144, -105.1500427118692 40.08593392692988, -105.1500582070947 40.08461508818777, -105.1500890297157 40.08199147048771, -105.1501631871213 40.07267877556609, -105.1504709850217 40.07267797250206, -105.1515658922463 40.0726689296074, -105.1530480376165 40.07268108133522, -105.154548143014 40.0726748738095, -105.1556951124087 40.07268708580514, -105.1578201323059 40.07269203249005, -105.159760010841 40.07270600258341, -105.1611550631462 40.07269912567766, -105.1639618314581 40.07271199840581, -105.1656459493443 40.07270810421043, -105.16913782298 40.07270004808169, -105.1723069106384 40.07271595167755, -105.1734149911134 40.07271607235776, -105.1743461234318 40.07273105648155, -105.1772851292169 40.0727390372715, -105.178142065461 40.07272688001402, -105.1784958444745 40.07272210092214, -105.1785009334851 40.07240092923784, -105.1785170121184 40.0705839359631, -105.1785168294514 40.07054687553875, -105.1785070374569 40.06989596523194, -105.1784949589715 40.06912398591355, -105.1784878891469 40.06774505925052, -105.1784838531813 40.06747949598464, -105.1784698949102 40.06656101062823, -105.1784791200518 40.06543907893126, -105.1784670297129 40.06489687116308, -105.1784478642381 40.06326429697376, -105.1784389978209 40.06250902945073, -105.1783991261733 40.06088898368674, -105.1783769328844 40.05900599693569, -105.1783591501339 40.0570969437221, -105.1783599732862 40.05677109239733, -105.1783680552524 40.05642110313737, -105.1783261176787 40.0547859519297, -105.1783188115135 40.05354129855904, -105.1783150298185 40.05289695593319, -105.1782599831768 40.05207187265444, -105.17826281953 40.0517369797149, -105.1782629098679 40.05172628563411, -105.178263560529 40.05164953755293, -105.1782639989751 40.05158099921608, -105.1782644506778 40.05154440521416, -105.1782648264534 40.05150006269764, -105.1782826872876 40.05101600343033, -105.1780338616441 40.05101062691166, -105.1762081530053 40.05101609362164, -105.1762046476006 40.05101610359928, -105.1762011363404 40.05101611265975, -105.1761979860374 40.05101612363364, -105.176194113803 40.0510161343829, -105.1761905990056 40.05101614793633, -105.1755841471719 40.05101795700623, -105.175580085081 40.05101796720103, -105.1755771234751 40.05101797598657, -105.1755736157177 40.05101798773977, -105.1755701079732 40.05101799679088, -105.1753060140316 40.05101878505296, -105.174428782014 40.05102139560601, -105.1736898899024 40.05102358741136, -105.1728325803302 40.05102612868573, -105.1726983997368 40.05102652451531, -105.1726165283522 40.05102676779798, -105.1724016811853 40.05102740001921, -105.1723984922067 40.05102741077957, -105.1716459099946 40.05102963168614, -105.1716427702465 40.05102964076442, -105.1713527073654 40.05103049558405, -105.171347248249 40.0510305133593, -105.1711336761778 40.05103113964618, -105.1689960014125 40.05103741479722, -105.1689875652156 40.05103748966823, -105.1689467501823 40.05103749776507, -105.1689099714373 40.05103750031685, -105.1677931005396 40.05103765951979, -105.1677831638122 40.05104046255979, -105.1676963712698 40.05109189923789, -105.1676261415118 40.05113215513653, -105.1675050332762 40.05117737289109, -105.167427709391 40.05120897908306, -105.1673022957037 40.05122237770144, -105.1672094394409 40.0512376803974, -105.1671464633991 40.05126049418936, -105.1670995030762 40.05127835733884, -105.1668981002619 40.05132446858931, -105.1666993909921 40.05136613985114, -105.1666408738178 40.05138324620814, -105.1664736601505 40.05146078375623, -105.1664011403114 40.05151207338047, -105.1663239373181 40.05160952042499, -105.1662384021501 40.05167736591554, -105.1661313790737 40.05176088895957, -105.1660856138928 40.0518140823167, -105.1660501816832 40.05185395159862, -105.1660201575936 40.05188173626777, -105.1659058511208 40.05190384239806, -105.1657559025758 40.05191750514264, -105.165648750986 40.05193625429996, -105.1655799060003 40.05196663732222, -105.1655088629726 40.05199043827383, -105.1654030527817 40.05200806347592, -105.1653173844367 40.05201229577091, -105.1653113904446 40.05201382030101, -105.1650579994036 40.05195099953081, -105.1649669596101 40.05195100002284, -105.1649515280593 40.0519371797482, -105.1649357829235 40.05187367951304, -105.1649253408261 40.05173109043365, -105.164935389596 40.05168266274925, -105.1649468807872 40.05161450597241, -105.1649453974719 40.05155411656848, -105.1649212127349 40.05148304796267, -105.1648608305505 40.05142553350745, -105.1647220812559 40.0513403043466, -105.1645678403559 40.05132000210335, -105.1644822108131 40.05131651800511, -105.1643867503607 40.05131644664036, -105.1642694282163 40.05131773912331, -105.1641309913249 40.05134884735053, -105.1640410996069 40.05139593472637, -105.1639326605231 40.05144388037487, -105.1638339316571 40.05152331397849, -105.1637524313982 40.05158787030133, -105.1637070317691 40.05165640548891, -105.1636657356831 40.05170844907624, -105.1635797130987 40.0517840142715, -105.1634941191975 40.05186291666683, -105.1634372860497 40.05189972807043, -105.1633658337125 40.05191585656047, -105.1632498597902 40.05191494894872, -105.1630999311205 40.051924238339, -105.1629758668792 40.05193543590796, -105.1628557406417 40.05196199555888, -105.162727133867 40.05198972996543, -105.1625770852535 40.05202319452241, -105.1622773176912 40.05211314107409, -105.1620291104283 40.0522398322612, -105.1619520472971 40.05230765616699, -105.1619047081888 40.05240805722977, -105.1618022051694 40.05247829679478, -105.1617273198083 40.05258210256712, -105.1616540197808 40.05264675530231, -105.1615911051033 40.05271934887317, -105.1614865311916 40.05278423221279, -105.1613716102433 40.05283316157037, -105.1612775409593 40.05288193857015, -105.1611730028394 40.05293880593047, -105.1610268077163 40.05298796284046, -105.160891354474 40.05297292385619, -105.1608279643923 40.05297338871971, -105.1608240356948 40.05297341770119, -105.1608079517161 40.05297353524253, -105.1607036947628 40.05297429690353, -105.1606098666646 40.05297498286759, -105.1604596628149 40.05298015204612, -105.1603981176738 40.05297751575439, -105.1603624839046 40.05296697322286, -105.1603040995684 40.05295659877761, -105.1602311089501 40.05292335067315, -105.1601932854801 40.05288986654357, -105.1601621305672 40.05286605072398, -105.1601311367479 40.05281017486806, -105.1600897153273 40.05275437456363, -105.1600586416582 40.05271452735239, -105.1600485362148 40.05265048645484, -105.1601009883901 40.05258598317823, -105.1601535180372 40.05250545570828, -105.1601642242853 40.05244927305546, -105.1601749235323 40.05238603017087, -105.1602218951422 40.05227028792482, -105.1602561397624 40.05220183654168, -105.1602342926047 40.05202203722605, -105.160201266795 40.05193680045235, -105.1601953579844 40.05189936276693, -105.160194346883 40.05189295255178, -105.1601936833895 40.05188593181764, -105.1601740137286 40.05167799262278, -105.1601396905426 40.05158504873061, -105.1600768884722 40.05147705390013, -105.1600339312413 40.05141495168196, -105.1599624177394 40.05135426038001, -105.159876657559 40.05128822670264, -105.1597935154553 40.05123422078098, -105.1597265106609 40.05116466489707, -105.1596549405419 40.05111494767892, -105.1595874136325 40.05105893417739, -105.1595497573073 40.0510384773496, -105.1595130289511 40.05103847795551, -105.1593482686524 40.05103662897318, -105.1588728812464 40.05103129138426, -105.1588224049339 40.05104736108841, -105.1587239578759 40.05108137939627, -105.1585395127557 40.05116145649118, -105.1584092219116 40.05122068951568, -105.1582751446963 40.0513216564015, -105.1581693302335 40.05139953848941, -105.1580990127872 40.05143575882849, -105.1580062850491 40.05148732646475, -105.1578831959852 40.05153560939884, -105.1577685196039 40.05155814409517, -105.1576639618218 40.05158981519088, -105.1575919391772 40.05158955015285, -105.1575908832443 40.05158954611878, -105.1575282456326 40.05158931609547, -105.1574342921437 40.05158897145586, -105.157298495359 40.05160449895396, -105.157190994115 40.05158591350226, -105.1570661436412 40.05154087557591, -105.1569577263993 40.05151454247685, -105.156851779706 40.05152988258859, -105.1566557219626 40.05152101697655, -105.1564951449201 40.05150537027536, -105.1563698698731 40.05150490630326, -105.156182259442 40.05151215429144, -105.1560672076075 40.05148776040432, -105.1559449171125 40.051452809891, -105.155747305266 40.05139785533414, -105.1555756460016 40.05133523860343, -105.1554265831195 40.05130777039776, -105.1552922383388 40.05128579671553, -105.1551721161439 40.05127806416193, -105.155047563932 40.05126268791455, -105.1549462249694 40.05125056835962, -105.1548545492162 40.05127033098574, -105.1547816445631 40.05128785033533, -105.1546944698589 40.0513009857922, -105.1546185274299 40.05130207615829, -105.1545269491046 40.05130536228518, -105.1544755440843 40.05131527765732, -105.1544498855746 40.05131259703548, -105.1544126177785 40.05130870358548, -105.1543524386634 40.0512901004921, -105.1543122705736 40.05120343378905, -105.1542393670629 40.051143104026, -105.1541395682197 40.05110146049368, -105.1539418604768 40.05108179820791, -105.1538618324175 40.05110049708283, -105.1537747601148 40.05118391274718, -105.1537447568463 40.05119928871704, -105.153703493422 40.05123331131377, -105.1536317958948 40.05128052536217, -105.1535861239172 40.05130360977193, -105.1535204189365 40.05131571000074, -105.1534287685995 40.05133659738699, -105.1533116082054 40.05136846626508, -105.1532347199211 40.05138383001786, -105.1531397555849 40.05143984165882, -105.1529783703864 40.05155730943326, -105.1529012724015 40.05161217584052, -105.1528329969947 40.05168682004388, -105.1527996939401 40.0517351334993, -105.152836948917 40.05178229025947, -105.1528089772994 40.05183494919256, -105.1527184816784 40.05188986072653, -105.15267013907 40.05191182082855, -105.1526102549068 40.05192063987319, -105.1523709083099 40.05192184554181, -105.1521876377263 40.05195702483574, -105.1520712442313 40.05201190102868, -105.1520482361644 40.05202146772876, -105.1520530348799 40.05218408774775, -105.1520642591071 40.0525644174675, -105.1520634530785 40.05256504639421, -105.1516930001067 40.05285399910237, -105.1514139993553 40.05303499916442, -105.1511639996712 40.05311799890815, -105.1508419991454 40.05315599894361, -105.1506660946248 40.05311767337918, -105.1506011352395 40.05305728882134, -105.1505987666178 40.05305728885442, -105.1505920000701 40.05305099892555, -105.1503129996857 40.05305099857401, -105.1500709278685 40.05298027054587, -105.1499441353162 40.05288728991736, -105.1497291342438 40.05259628881397, -105.1495941346949 40.05249728903948, -105.1495927840303 40.0524967076198, -105.1495849996936 40.05249099906354, -105.149419999981 40.05241999931873, -105.1491200004597 40.05241399877543, -105.1480409998483 40.05248499847494, -105.1477619994002 40.05248499915338, -105.1475214657036 40.05240284117516, -105.1467141338478 40.05174329043003, -105.1467096475382 40.05174079629727, -105.146507134829 40.05162828892156, -105.1462421358811 40.05158428960294, -105.1460351344894 40.05162229008017, -105.1443591344388 40.05221428814447, -105.1442621341128 40.05224828958868, -105.14388313487 40.05233028948903, -105.1435331350977 40.05235728932603, -105.1428901343515 40.05228028849469, -105.1422181337478 40.05218728953625, -105.1418181357289 40.05218128953825, -105.1414601343164 40.05222528959065, -105.1412101335628 40.05224128986859, -105.1411321330766 40.05226928997327, -105.1406461339316 40.05230128984537, -105.1405531334419 40.05226829027612, -105.1404101340526 40.05226828965515, -105.1397811330371 40.05213129111328, -105.1394881334066 40.05209229106099, -105.1391951326456 40.05215229000667, -105.138766134054 40.05234528973559, -105.1385441337409 40.05252628951144, -105.1382651345308 40.0526522901612, -105.1380581339729 40.0527892905053, -105.1374791331605 40.053074290269, -105.1371141330145 40.05320128964343, -105.1369211341096 40.05319528942255, -105.1366211339717 40.05321729100668, -105.1360851348651 40.05334828960167, -105.1352131341163 40.05372229007944, -105.1349341339898 40.05378229096474, -105.1344121329457 40.05377628997379, -105.1340761340211 40.05386929093724, -105.133690132606 40.05404529037242, -105.1333401327132 40.05411628953848, -105.1329041339726 40.05411629033144, -105.1325041341113 40.05415429008961, -105.1319961338741 40.05425829067238, -105.1317031328973 40.05436329066021, -105.1313101329301 40.05456629110776, -105.1312151333568 40.05463829014283))</t>
+          <t>POLYGON ((-105.13121513335679 40.05463829014283, -105.13120513412518 40.0549272902714, -105.13120613305291 40.05519229072108, -105.13120713480302 40.055649290512754, -105.13120513492963 40.05727829088557, -105.13121313255013 40.05874928993782, -105.1312141338369 40.058870290378664, -105.13122813493895 40.059749290717164, -105.13122013407462 40.06002129004976, -105.13121413437736 40.06023929086055, -105.13122513479581 40.060720290493926, -105.13122913450528 40.06187129073018, -105.13123413407604 40.062235290811046, -105.13122013555704 40.06361729016729, -105.13121613525388 40.06423529025914, -105.13122613480824 40.06486429056906, -105.13121813550079 40.06555429029728, -105.13123113455781 40.06758328902276, -105.13124213496536 40.06840629078298, -105.13124713525865 40.068773290655166, -105.1312571353166 40.07052429035368, -105.13125613551865 40.071146291216536, -105.13125013510601 40.07142728958371, -105.13124713588887 40.07157529118987, -105.13127698010429 40.07280485163446, -105.13127713635365 40.07281128908546, -105.13132913544558 40.07367829108345, -105.1313121353605 40.074539291316455, -105.13131613629291 40.07558629064913, -105.13136413704501 40.080082290488726, -105.1314061367591 40.0827892910741, -105.13141413815906 40.083257289736814, -105.13142313857455 40.08373028926654, -105.13146805811917 40.087358917981646, -105.13146813738082 40.08736529032833, -105.13146869204817 40.08736528489368, -105.13490713833464 40.087334289021946, -105.13730613866171 40.087324289770656, -105.13826313865856 40.08732328982324, -105.14098713876481 40.087311289530135, -105.14200313915634 40.08730728976931, -105.14220813958934 40.08730028957377, -105.14430113969432 40.08730228806577, -105.14659313865397 40.08730128957986, -105.14905413796853 40.08730928858999, -105.14971813880092 40.08731828785967, -105.15003158620414 40.087322386225345, -105.15002846248223 40.087146656624704, -105.15002910834453 40.08709170551144, -105.15004271186916 40.085933926929876, -105.15005820709473 40.084615088187775, -105.1500890297157 40.081991470487715, -105.15016318712127 40.07267877556609, -105.15047098502167 40.07267797250206, -105.15156589224627 40.072668929607396, -105.1530480376165 40.07268108133522, -105.15454814301404 40.0726748738095, -105.15569511240872 40.072687085805136, -105.15782013230594 40.072692032490046, -105.15976001084104 40.07270600258341, -105.16115506314621 40.07269912567766, -105.1639618314581 40.072711998405815, -105.16564594934432 40.072708104210434, -105.16913782298003 40.072700048081686, -105.17230691063841 40.07271595167755, -105.17341499111339 40.072716072357764, -105.17434612343179 40.07273105648155, -105.17728512921693 40.072739037271496, -105.17814206546103 40.072726880014024, -105.17849584447447 40.072722100922135, -105.17850093348505 40.07240092923784, -105.17851701211839 40.0705839359631, -105.17851682945137 40.07054687553875, -105.17850703745694 40.069895965231936, -105.17849495897146 40.06912398591355, -105.17848788914692 40.06774505925052, -105.1784838531813 40.067479495984635, -105.17846989491015 40.066561010628234, -105.17847912005185 40.065439078931256, -105.17846702971286 40.06489687116308, -105.17844786423808 40.06326429697376, -105.1784389978209 40.06250902945073, -105.17839912617335 40.06088898368674, -105.17837693288443 40.05900599693569, -105.17835915013391 40.0570969437221, -105.17835997328619 40.05677109239733, -105.17836805525243 40.056421103137374, -105.17832611767871 40.0547859519297, -105.17831881151353 40.05354129855904, -105.1783150298185 40.05289695593319, -105.1782599831768 40.052071872654444, -105.17826281953003 40.0517369797149, -105.17826290986788 40.05172628563411, -105.17826356052903 40.05164953755293, -105.1782639989751 40.05158099921608, -105.17826445067783 40.05154440521416, -105.17826482645339 40.05150006269764, -105.17828268728758 40.05101600343033, -105.17803386164407 40.05101062691166, -105.17620815300526 40.05101609362164, -105.17620464760058 40.05101610359928, -105.17620113634044 40.05101611265975, -105.17619798603742 40.051016123633644, -105.17619411380304 40.0510161343829, -105.17619059900558 40.05101614793633, -105.17558414717193 40.05101795700623, -105.17558008508098 40.051017967201034, -105.17557712347508 40.05101797598657, -105.1755736157177 40.05101798773977, -105.17557010797324 40.051017996790875, -105.17530601403156 40.05101878505296, -105.17442878201399 40.05102139560601, -105.17368988990238 40.051023587411365, -105.1728325803302 40.051026128685734, -105.17269839973677 40.051026524515315, -105.17261652835224 40.05102676779798, -105.17240168118529 40.05102740001921, -105.1723984922067 40.05102741077957, -105.17164590999464 40.05102963168614, -105.17164277024654 40.05102964076442, -105.17135270736543 40.05103049558405, -105.17134724824902 40.0510305133593, -105.17113367617777 40.051031139646184, -105.16899600141247 40.05103741479722, -105.16898756521562 40.05103748966823, -105.1689467501823 40.05103749776507, -105.16890997143729 40.05103750031685, -105.16779310053964 40.051037659519785, -105.16778316381217 40.05104046255979, -105.16769637126981 40.05109189923789, -105.1676261415118 40.05113215513653, -105.16750503327624 40.05117737289109, -105.16742770939105 40.051208979083064, -105.16730229570373 40.05122237770144, -105.16720943944088 40.0512376803974, -105.16714646339913 40.05126049418936, -105.16709950307616 40.051278357338845, -105.16689810026186 40.05132446858931, -105.16669939099206 40.05136613985114, -105.16664087381784 40.05138324620814, -105.16647366015052 40.051460783756234, -105.16640114031144 40.05151207338047, -105.16632393731811 40.05160952042499, -105.16623840215007 40.05167736591554, -105.16613137907372 40.05176088895957, -105.16608561389279 40.051814082316696, -105.16605018168318 40.05185395159862, -105.16602015759356 40.051881736267774, -105.16590585112084 40.05190384239806, -105.16575590257582 40.05191750514264, -105.16564875098595 40.05193625429996, -105.16557990600035 40.05196663732222, -105.16550886297264 40.051990438273826, -105.1654030527817 40.05200806347592, -105.16531738443669 40.05201229577091, -105.16531139044459 40.052013820301006, -105.16505799940357 40.05195099953081, -105.16496695961008 40.05195100002284, -105.16495152805932 40.0519371797482, -105.1649357829235 40.051873679513044, -105.16492534082607 40.05173109043365, -105.16493538959601 40.05168266274925, -105.16494688078716 40.05161450597241, -105.16494539747187 40.051554116568475, -105.16492121273487 40.05148304796267, -105.16486083055051 40.05142553350745, -105.16472208125589 40.0513403043466, -105.16456784035591 40.051320002103346, -105.16448221081306 40.05131651800511, -105.16438675036066 40.05131644664036, -105.16426942821634 40.05131773912331, -105.1641309913249 40.05134884735053, -105.16404109960692 40.051395934726365, -105.16393266052312 40.05144388037487, -105.16383393165714 40.051523313978485, -105.16375243139824 40.051587870301326, -105.16370703176909 40.05165640548891, -105.1636657356831 40.05170844907624, -105.16357971309866 40.0517840142715, -105.16349411919751 40.051862916666835, -105.16343728604966 40.05189972807043, -105.16336583371255 40.05191585656047, -105.16324985979016 40.05191494894872, -105.16309993112051 40.051924238339, -105.16297586687922 40.05193543590796, -105.16285574064172 40.051961995558884, -105.16272713386697 40.051989729965435, -105.16257708525347 40.05202319452241, -105.16227731769125 40.05211314107409, -105.16202911042834 40.0522398322612, -105.16195204729715 40.05230765616699, -105.16190470818879 40.05240805722977, -105.16180220516941 40.05247829679478, -105.16172731980828 40.05258210256712, -105.16165401978081 40.05264675530231, -105.16159110510327 40.05271934887317, -105.16148653119157 40.05278423221279, -105.1613716102433 40.05283316157037, -105.16127754095929 40.05288193857015, -105.16117300283939 40.05293880593047, -105.1610268077163 40.05298796284046, -105.16089135447405 40.05297292385619, -105.16082796439227 40.05297338871971, -105.1608240356948 40.05297341770119, -105.16080795171605 40.05297353524253, -105.16070369476283 40.05297429690353, -105.16060986666464 40.05297498286759, -105.16045966281487 40.052980152046125, -105.16039811767375 40.052977515754385, -105.16036248390458 40.05296697322286, -105.16030409956835 40.05295659877761, -105.16023110895006 40.05292335067315, -105.1601932854801 40.05288986654357, -105.16016213056723 40.05286605072398, -105.16013113674794 40.05281017486806, -105.16008971532732 40.052754374563634, -105.16005864165815 40.052714527352386, -105.16004853621476 40.052650486454844, -105.16010098839008 40.05258598317823, -105.16015351803719 40.05250545570828, -105.16016422428534 40.05244927305546, -105.16017492353228 40.052386030170865, -105.1602218951422 40.05227028792482, -105.16025613976238 40.05220183654168, -105.16023429260466 40.052022037226045, -105.16020126679499 40.051936800452346, -105.16019535798439 40.05189936276693, -105.160194346883 40.05189295255178, -105.16019368338945 40.051885931817644, -105.16017401372865 40.05167799262278, -105.16013969054255 40.05158504873061, -105.16007688847216 40.05147705390013, -105.16003393124133 40.05141495168196, -105.15996241773941 40.05135426038001, -105.15987665755898 40.05128822670264, -105.15979351545529 40.05123422078098, -105.15972651066092 40.05116466489707, -105.15965494054187 40.05111494767892, -105.15958741363254 40.05105893417739, -105.15954975730733 40.0510384773496, -105.15951302895108 40.05103847795551, -105.15934826865238 40.05103662897318, -105.15887288124637 40.05103129138426, -105.1588224049339 40.051047361088415, -105.15872395787588 40.05108137939627, -105.15853951275574 40.05116145649118, -105.15840922191157 40.05122068951568, -105.1582751446963 40.0513216564015, -105.15816933023348 40.051399538489406, -105.15809901278716 40.05143575882849, -105.15800628504907 40.05148732646475, -105.15788319598524 40.05153560939884, -105.15776851960395 40.051558144095175, -105.1576639618218 40.05158981519088, -105.15759193917715 40.051589550152855, -105.15759088324425 40.05158954611878, -105.15752824563263 40.05158931609547, -105.15743429214369 40.051588971455864, -105.15729849535903 40.05160449895396, -105.15719099411497 40.05158591350226, -105.15706614364125 40.05154087557591, -105.15695772639931 40.05151454247685, -105.156851779706 40.05152988258859, -105.15665572196258 40.05152101697655, -105.15649514492009 40.05150537027536, -105.15636986987309 40.051504906303265, -105.15618225944198 40.05151215429144, -105.15606720760749 40.05148776040432, -105.15594491711255 40.051452809890996, -105.155747305266 40.05139785533414, -105.15557564600164 40.05133523860343, -105.15542658311952 40.051307770397756, -105.1552922383388 40.051285796715526, -105.15517211614386 40.051278064161934, -105.15504756393197 40.05126268791455, -105.15494622496944 40.05125056835962, -105.15485454921618 40.051270330985744, -105.15478164456307 40.05128785033533, -105.15469446985885 40.0513009857922, -105.15461852742989 40.05130207615829, -105.1545269491046 40.051305362285184, -105.15447554408435 40.05131527765732, -105.15444988557458 40.051312597035476, -105.15441261777848 40.051308703585484, -105.15435243866337 40.0512901004921, -105.15431227057358 40.05120343378905, -105.15423936706293 40.051143104025996, -105.15413956821975 40.05110146049368, -105.15394186047676 40.05108179820791, -105.15386183241749 40.05110049708283, -105.15377476011477 40.05118391274718, -105.15374475684631 40.05119928871704, -105.15370349342199 40.051233311313766, -105.1536317958948 40.051280525362166, -105.15358612391715 40.05130360977193, -105.15352041893651 40.05131571000074, -105.15342876859948 40.05133659738699, -105.15331160820543 40.05136846626508, -105.1532347199211 40.05138383001786, -105.15313975558492 40.05143984165882, -105.15297837038636 40.05155730943326, -105.15290127240151 40.05161217584052, -105.15283299699472 40.05168682004388, -105.15279969394011 40.0517351334993, -105.15283694891697 40.05178229025947, -105.15280897729937 40.05183494919256, -105.15271848167838 40.051889860726526, -105.15267013907 40.05191182082855, -105.15261025490679 40.05192063987319, -105.15237090830992 40.05192184554181, -105.15218763772631 40.05195702483574, -105.15207124423127 40.05201190102868, -105.15204823616442 40.05202146772876, -105.15205303487993 40.052184087747754, -105.15206425910714 40.0525644174675, -105.1520634530785 40.05256504639421, -105.15169300010675 40.052853999102375, -105.15141399935528 40.05303499916442, -105.15116399967118 40.05311799890815, -105.15084199914541 40.05315599894361, -105.15066609462482 40.053117673379184, -105.15060113523947 40.05305728882134, -105.15059876661776 40.05305728885442, -105.15059200007013 40.05305099892555, -105.15031299968574 40.05305099857401, -105.15007092786853 40.052980270545866, -105.14994413531618 40.052887289917365, -105.14972913424377 40.052596288813966, -105.14959413469492 40.05249728903948, -105.14959278403029 40.052496707619795, -105.1495849996936 40.052490999063544, -105.14941999998102 40.05241999931873, -105.14912000045967 40.05241399877543, -105.1480409998483 40.05248499847494, -105.14776199940019 40.05248499915338, -105.14752146570363 40.05240284117516, -105.14671413384782 40.051743290430025, -105.14670964753824 40.051740796297274, -105.14650713482904 40.05162828892156, -105.14624213588111 40.05158428960294, -105.14603513448941 40.05162229008017, -105.14435913443882 40.05221428814447, -105.14426213411276 40.052248289588675, -105.14388313486997 40.052330289489035, -105.14353313509766 40.052357289326025, -105.1428901343515 40.05228028849469, -105.14221813374778 40.05218728953625, -105.14181813572887 40.05218128953825, -105.14146013431638 40.05222528959065, -105.14121013356277 40.05224128986859, -105.14113213307658 40.052269289973275, -105.14064613393161 40.052301289845374, -105.14055313344193 40.052268290276125, -105.14041013405257 40.052268289655146, -105.13978113303708 40.052131291113284, -105.13948813340659 40.05209229106099, -105.13919513264561 40.052152290006674, -105.138766134054 40.05234528973559, -105.13854413374094 40.05252628951144, -105.13826513453076 40.0526522901612, -105.13805813397289 40.0527892905053, -105.13747913316054 40.053074290268995, -105.13711413301452 40.05320128964343, -105.13692113410956 40.05319528942255, -105.13662113397173 40.05321729100668, -105.13608513486506 40.053348289601665, -105.13521313411631 40.05372229007944, -105.13493413398982 40.05378229096474, -105.13441213294574 40.05377628997379, -105.13407613402109 40.053869290937236, -105.13369013260602 40.05404529037242, -105.13334013271316 40.05411628953848, -105.1329041339726 40.054116290331436, -105.13250413411133 40.05415429008961, -105.13199613387408 40.05425829067238, -105.13170313289729 40.054363290660206, -105.13131013293014 40.05456629110776, -105.13121513335679 40.05463829014283))</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -2848,7 +2860,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1880841936159 40.07263945058795, -105.1893946744375 40.07264673391924, -105.1917239390811 40.07265964144332, -105.1938520922997 40.07267139500048, -105.1938518906687 40.07277208786569, -105.1940641417293 40.07277292533653, -105.194183128132 40.07277406474559, -105.1942781733234 40.07277486502355, -105.1948670366262 40.07277889370809, -105.1955909649218 40.07278409976774, -105.1959218927785 40.07277508923514, -105.195948214593 40.07277500006112, -105.1958715408196 40.07265610430982, -105.1956497600617 40.07230497294984, -105.1955329102784 40.07230570863143, -105.1955552225853 40.07228173548236, -105.1955696351996 40.07225420104457, -105.195575276256 40.07222722619021, -105.195571161459 40.0721891665423, -105.19555338647 40.07215351162139, -105.1955325357656 40.0721290328372, -105.1955317416101 40.07179076427918, -105.1959629613449 40.07179313125406, -105.1959639747934 40.07179589531189, -105.1971151965505 40.07180144923354, -105.1974111953331 40.07173844977702, -105.1974891959825 40.07108844907243, -105.1976471349798 40.070854867217, -105.1978608565895 40.07054974585753, -105.1981921953054 40.0700514489731, -105.1983431964843 40.06969344951722, -105.1982481955772 40.06916644960438, -105.2008557060834 40.06916006349055, -105.2021571971997 40.06915744908764, -105.2021606973751 40.06883412167546, -105.2021581970034 40.06820744840584, -105.2021841960138 40.06808744821939, -105.2022321959824 40.06797144872966, -105.2023491962878 40.06777944851839, -105.2024761975983 40.06763844798303, -105.2026291967245 40.06751244885115, -105.202495195546 40.06738144820481, -105.2022461967158 40.06719644869614, -105.2022371955249 40.06554144896795, -105.2003585210558 40.0655549887631, -105.1993447543905 40.06554629272709, -105.197500195574 40.06553044795643, -105.1967811954029 40.06553144866818, -105.1967551952459 40.06549044945493, -105.1967491951159 40.06548244853415, -105.1967121942066 40.06543344785908, -105.196613194153 40.06534144843442, -105.1964601945655 40.06521144902592, -105.1963351948621 40.0651164493617, -105.1963061946974 40.06509244910959, -105.1962861947403 40.06507844902631, -105.1962471945175 40.0650494481572, -105.1962161953141 40.06502844808715, -105.1961811946941 40.06500444822031, -105.1961561946336 40.06498744839866, -105.1958335281126 40.06482122755254, -105.1955621953032 40.06468144828445, -105.1955361941598 40.06466844907239, -105.1955191940804 40.06465944816699, -105.1955071952751 40.06465344790787, -105.1954861952043 40.06464244871119, -105.1954741938401 40.0646354487212, -105.1954631949272 40.06462944929453, -105.1954481948594 40.06462144887348, -105.1954341946791 40.06461344928788, -105.1954221947172 40.06460744901683, -105.1954081943274 40.06459844880609, -105.1953261940917 40.06454944869287, -105.1952991946379 40.06453244880927, -105.1952181943264 40.06447744843081, -105.1951891945079 40.06445744948024, -105.1951361943555 40.06441744945245, -105.1950961944753 40.06438544818828, -105.1950591935295 40.06435544887151, -105.1950261937514 40.06432744874969, -105.195066194525 40.06429244893643, -105.1932001627259 40.06253903928965, -105.1927811391311 40.0626719079231, -105.1923596162155 40.06287144706564, -105.1886851148256 40.06029994091084, -105.1859053468927 40.06119793928947, -105.1859546228259 40.06267644696645, -105.1853016220106 40.06277944797684, -105.1845896211293 40.062857448644, -105.1839352461995 40.06283133001712, -105.1832576233965 40.06272744841069, -105.1829217252438 40.06260732591054, -105.182648259628 40.06244855791299, -105.1820142414536 40.06199575457967, -105.1817535568669 40.06211429107486, -105.1814415779459 40.06225506745857, -105.1812404473227 40.0623426416048, -105.1812240041372 40.06235518637328, -105.1809818361483 40.06245838376665, -105.1808792950956 40.06248642751207, -105.1807809107792 40.06250189337818, -105.1804101034247 40.06250709331072, -105.1793061843293 40.06251039500064, -105.1784389978209 40.06250902945073, -105.1784478642381 40.06326429697376, -105.1784670297129 40.06489687116308, -105.1784791200518 40.06543907893126, -105.1784698949102 40.06656101062823, -105.1784838531813 40.06747949598464, -105.1784878891469 40.06774505925052, -105.1784949589715 40.06912398591355, -105.1784950725557 40.06913121664342, -105.1785051917741 40.06913045045798, -105.1792591686312 40.06913657318423, -105.1812891923216 40.06915245055091, -105.181286191659 40.06800644970687, -105.1812873206927 40.06800015368258, -105.181714937013 40.06800107072923, -105.1823828306993 40.06798204711436, -105.1825171400026 40.06799010278778, -105.1827810018886 40.06803008491246, -105.1829580021636 40.06807806249881, -105.1831270176412 40.06815292118763, -105.1831601619173 40.06817113054244, -105.183740034292 40.06856390986091, -105.1838490101667 40.06846881885282, -105.1837501921285 40.06857045028935, -105.1833961920323 40.06889744939709, -105.1832611922969 40.06912044991955, -105.1839211916622 40.06912445053024, -105.185800786321 40.06912764169806, -105.1880671940498 40.06913144933019, -105.1880706438702 40.07136436642797, -105.1880841936159 40.07263945058795))</t>
+          <t>POLYGON ((-105.18808419361588 40.07263945058795, -105.18939467443747 40.07264673391924, -105.19172393908114 40.072659641443316, -105.19385209229966 40.07267139500048, -105.19385189066865 40.072772087865694, -105.19406414172929 40.07277292533653, -105.19418312813204 40.07277406474559, -105.19427817332344 40.07277486502355, -105.19486703662623 40.07277889370809, -105.19559096492179 40.07278409976774, -105.19592189277849 40.072775089235144, -105.19594821459299 40.07277500006112, -105.19587154081958 40.07265610430982, -105.19564976006166 40.07230497294984, -105.19553291027836 40.072305708631426, -105.19555522258528 40.072281735482356, -105.19556963519956 40.07225420104457, -105.19557527625595 40.072227226190215, -105.19557116145899 40.0721891665423, -105.19555338647001 40.072153511621394, -105.19553253576561 40.0721290328372, -105.1955317416101 40.07179076427918, -105.19596296134492 40.07179313125406, -105.19596397479337 40.07179589531189, -105.19711519655048 40.07180144923354, -105.19741119533312 40.07173844977702, -105.19748919598247 40.071088449072434, -105.1976471349798 40.070854867217, -105.19786085658947 40.07054974585753, -105.19819219530544 40.0700514489731, -105.19834319648426 40.06969344951722, -105.1982481955772 40.06916644960438, -105.20085570608342 40.06916006349055, -105.20215719719974 40.06915744908764, -105.20216069737508 40.06883412167546, -105.2021581970034 40.068207448405836, -105.2021841960138 40.068087448219394, -105.20223219598242 40.06797144872966, -105.20234919628778 40.067779448518394, -105.2024761975983 40.06763844798303, -105.20262919672446 40.06751244885115, -105.20249519554599 40.06738144820481, -105.20224619671583 40.06719644869614, -105.20223719552489 40.06554144896795, -105.20035852105578 40.065554988763104, -105.19934475439051 40.06554629272709, -105.197500195574 40.06553044795643, -105.19678119540292 40.06553144866818, -105.19675519524594 40.065490449454934, -105.19674919511594 40.06548244853415, -105.1967121942066 40.06543344785908, -105.19661319415297 40.06534144843442, -105.1964601945655 40.06521144902592, -105.19633519486206 40.065116449361696, -105.19630619469736 40.065092449109585, -105.1962861947403 40.06507844902631, -105.19624719451745 40.0650494481572, -105.19621619531407 40.065028448087155, -105.19618119469408 40.06500444822031, -105.1961561946336 40.06498744839866, -105.19583352811263 40.06482122755254, -105.19556219530322 40.064681448284446, -105.19553619415981 40.06466844907239, -105.19551919408043 40.064659448166985, -105.1955071952751 40.064653447907865, -105.19548619520427 40.06464244871119, -105.1954741938401 40.0646354487212, -105.19546319492719 40.06462944929453, -105.19544819485938 40.06462144887348, -105.19543419467907 40.06461344928788, -105.19542219471717 40.064607449016826, -105.19540819432744 40.06459844880609, -105.19532619409173 40.06454944869287, -105.19529919463793 40.064532448809274, -105.19521819432644 40.064477448430814, -105.19518919450789 40.06445744948024, -105.19513619435548 40.06441744945245, -105.19509619447527 40.064385448188276, -105.19505919352953 40.06435544887151, -105.1950261937514 40.06432744874969, -105.19506619452498 40.06429244893643, -105.19320016272589 40.06253903928965, -105.1927811391311 40.0626719079231, -105.19235961621548 40.06287144706564, -105.18868511482556 40.060299940910845, -105.18590534689268 40.06119793928947, -105.1859546228259 40.06267644696645, -105.18530162201056 40.06277944797684, -105.18458962112933 40.062857448643996, -105.18393524619951 40.06283133001712, -105.18325762339646 40.06272744841069, -105.18292172524383 40.06260732591054, -105.18264825962801 40.062448557912994, -105.18201424145363 40.06199575457967, -105.1817535568669 40.06211429107486, -105.18144157794586 40.06225506745857, -105.1812404473227 40.0623426416048, -105.18122400413722 40.06235518637328, -105.18098183614832 40.06245838376665, -105.18087929509562 40.06248642751207, -105.18078091077925 40.062501893378176, -105.1804101034247 40.06250709331072, -105.17930618432933 40.062510395000636, -105.1784389978209 40.06250902945073, -105.17844786423808 40.06326429697376, -105.17846702971286 40.06489687116308, -105.17847912005185 40.065439078931256, -105.17846989491015 40.066561010628234, -105.1784838531813 40.067479495984635, -105.17848788914692 40.06774505925052, -105.17849495897146 40.06912398591355, -105.17849507255573 40.06913121664342, -105.17850519177411 40.069130450457976, -105.17925916863116 40.06913657318423, -105.18128919232159 40.06915245055091, -105.18128619165903 40.06800644970687, -105.18128732069269 40.068000153682576, -105.181714937013 40.06800107072923, -105.1823828306993 40.067982047114356, -105.18251714000264 40.06799010278778, -105.1827810018886 40.068030084912465, -105.18295800216363 40.06807806249881, -105.18312701764117 40.068152921187625, -105.18316016191731 40.06817113054244, -105.18374003429201 40.06856390986091, -105.18384901016671 40.06846881885282, -105.18375019212854 40.06857045028935, -105.18339619203232 40.06889744939709, -105.18326119229694 40.069120449919545, -105.18392119166224 40.06912445053024, -105.18580078632104 40.06912764169806, -105.18806719404984 40.06913144933019, -105.18807064387016 40.07136436642797, -105.18808419361588 40.07263945058795))</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -2890,7 +2902,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1547910443339 40.10160295281706, -105.1594304890262 40.10160443093669, -105.1614744733263 40.10160415291411, -105.1624462852989 40.10160759494413, -105.1627463884044 40.10160727756193, -105.162745878241 40.10149052707892, -105.1627744971364 40.10144969519414, -105.1628003334446 40.10125337388077, -105.1628328288079 40.10114708801201, -105.1629114325541 40.10105457433082, -105.1629403482016 40.1009537331956, -105.1630261902674 40.10083396358396, -105.1631727536655 40.10064617859581, -105.1633012463015 40.10052107796384, -105.1634618268533 40.10037152088923, -105.1636007588962 40.10029009387689, -105.1636825346362 40.10027396553426, -105.1638246000031 40.1002771072795, -105.1640911875274 40.10023969478414, -105.1642014326381 40.10021273845721, -105.1642869891572 40.10015024909485, -105.1643909381817 40.09995961059775, -105.164394973355 40.09986142393318, -105.1643390429973 40.09967850396548, -105.1643751267407 40.09956404480679, -105.1644680692662 40.09944429475246, -105.1645642939285 40.09937910902314, -105.1648670799139 40.0992026860207, -105.1650522630877 40.09910502493955, -105.1651770897275 40.09900173334665, -105.1652910858499 40.09893387138398, -105.1653340980059 40.09885489136187, -105.1653171162074 40.09869663455474, -105.1653317923612 40.09860120674662, -105.1654284036489 40.09845691671995, -105.165453709729 40.09836697491093, -105.1654576092707 40.09829606568717, -105.1654582390793 40.09816786405847, -105.165490675229 40.09807248767891, -105.1655654783973 40.0980290608214, -105.1656722619646 40.09798299935861, -105.1658324577136 40.09790981449991, -105.166095414537 40.0978860253817, -105.16632643203 40.09785668815526, -105.1665253086471 40.09786271790858, -105.1666603591826 40.0978467413104, -105.1667668614243 40.0978579600548, -105.166851998958 40.09788002749483, -105.1670507835059 40.0979051506871, -105.1672853384415 40.09787854890141, -105.1674487236722 40.09787901957451, -105.1675477578299 40.09785733257959, -105.1675946027945 40.09782761281062, -105.1676267295847 40.09779497309102, -105.1676589217346 40.09774869415765, -105.1676666652484 40.09761778583655, -105.1678129561249 40.0974818200669, -105.1679561463537 40.09725310290229, -105.1681872051748 40.097076277577, -105.1684049635546 40.09698980339898, -105.1685651694304 40.09695104110424, -105.1687814685314 40.09698815687596, -105.1689552419898 40.09704320919361, -105.1690670901817 40.09719097558062, -105.1690463028637 40.0960826305675, -105.1690438651976 40.09505598433667, -105.169054853203 40.09462073046497, -105.1690858737971 40.09447885489597, -105.1691079352005 40.09433736433639, -105.1690904074871 40.09427371581661, -105.1690612714555 40.09414797944284, -105.1690669033671 40.09382399952331, -105.1690676294168 40.09341829161983, -105.1690910864483 40.09327912691391, -105.1691336287767 40.09300289877228, -105.1690753833012 40.09260401984817, -105.1690650509102 40.09237159263287, -105.1690649575054 40.09145107771945, -105.1690614344188 40.09014968437621, -105.1690618914051 40.08854734181894, -105.1690508854828 40.08742081434125, -105.1690488848439 40.08721476831359, -105.1690662178607 40.08709728796521, -105.1690791421419 40.08709728808531, -105.1699591416146 40.08707228785719, -105.1701781411211 40.08706628765196, -105.1713191414329 40.08705928692613, -105.1725011418384 40.08704528692955, -105.1757431417456 40.08702028738892, -105.1760791423071 40.08701728667786, -105.1771691416208 40.08698528660337, -105.178761141561 40.08696128581556, -105.1808461424632 40.08694828645896, -105.1821951420464 40.0869462851299, -105.1835361420234 40.08691628641589, -105.1846341422089 40.08690228587696, -105.1852421427044 40.08689828635889, -105.1853451439115 40.08690028647014, -105.1857791432559 40.08694228585087, -105.1862071424008 40.08700528569321, -105.1865131428577 40.08705628575504, -105.1867131424599 40.08710228521863, -105.1869111415545 40.0871572862816, -105.1872751430461 40.08727928560096, -105.1877881430586 40.08746028560382, -105.187901142137 40.0875002862527, -105.1879091430847 40.08750328542086, -105.1879129845044 40.08750456571757, -105.1879120318739 40.087501088446, -105.1879288796204 40.08725901393426, -105.1879367177722 40.08684890384132, -105.1879580266744 40.08573387104014, -105.1879828820664 40.08420899185455, -105.1879849016488 40.08337803203136, -105.1880101273988 40.08153800596429, -105.1880109830068 40.08142902449755, -105.1880128391563 40.08125800461307, -105.1880401421608 40.07904189470351, -105.1880519079191 40.07733113014445, -105.1880671719961 40.07641702604863, -105.188070113258 40.07624298911882, -105.1880708562545 40.07619876208987, -105.1880801936184 40.07619945109983, -105.188192193863 40.07618545050101, -105.1882921938901 40.07615545069577, -105.1885141942192 40.07610945042958, -105.188729194604 40.07604045081974, -105.1889631943489 40.07592345061921, -105.18910319508 40.0759064506717, -105.1893281944698 40.07585345077683, -105.1896741947545 40.07570145051615, -105.1899641949593 40.07566445030815, -105.1902241265108 40.07560863429631, -105.1907511950104 40.07549545089397, -105.1907521948045 40.07546245021675, -105.1907541950898 40.07543245047793, -105.1907571945497 40.07540445015314, -105.1907621941908 40.07536145038617, -105.190767194877 40.07532545046012, -105.1907751946438 40.07528244972295, -105.1907811943645 40.07525545084962, -105.1907921949662 40.07520944998442, -105.1908011950725 40.07517645092222, -105.1908111950647 40.07514245121535, -105.1908181943892 40.07512045091352, -105.1908321947982 40.07508045099295, -105.1908421948001 40.07505445084159, -105.1910911942501 40.07506045112101, -105.1914101946249 40.07502445075971, -105.1919231953974 40.0750234505873, -105.1921041958643 40.07508645023321, -105.1924521950065 40.07516645038263, -105.1929101955311 40.07545545029699, -105.1930686556212 40.07551448774536, -105.1935500196004 40.07569382935834, -105.1942621963568 40.07595945108564, -105.1945641953128 40.0754304506349, -105.1944611949431 40.07540045034644, -105.1944861950927 40.07535544988587, -105.1944961955827 40.07523545057487, -105.1942701949712 40.07470545027712, -105.1941301947049 40.07448244993503, -105.1939661962362 40.07404145051328, -105.1939091944498 40.07392045037489, -105.1938671953461 40.07375044969388, -105.1938631961004 40.07289745028993, -105.1926061727062 40.07290183614763, -105.1910141758257 40.07290737187865, -105.1891170700742 40.07291393943083, -105.1880889785409 40.07291738748686, -105.186579245816 40.07290802007324, -105.1853123095948 40.07290014352606, -105.1835708587782 40.07288929420034, -105.1829851934239 40.07288645145971, -105.1814644385908 40.0729143637982, -105.1801665604356 40.07291007946497, -105.1784741913036 40.07290045107155, -105.1784681917568 40.07272945154712, -105.1784700126258 40.07272244957001, -105.178142065461 40.07272688001402, -105.1772851292169 40.0727390372715, -105.1743461234318 40.07273105648155, -105.1734149911134 40.07271607235776, -105.1723069106384 40.07271595167755, -105.16913782298 40.07270004808169, -105.1656459493443 40.07270810421043, -105.1639618314581 40.07271199840581, -105.1611550631462 40.07269912567766, -105.159760010841 40.07270600258341, -105.1578201323059 40.07269203249005, -105.1556951124087 40.07268708580514, -105.154548143014 40.0726748738095, -105.1530480376165 40.07268108133522, -105.1515658922463 40.0726689296074, -105.1504709850217 40.07267797250206, -105.1501631871213 40.07267877556609, -105.1500890297157 40.08199147048771, -105.1500582070947 40.08461508818777, -105.1500427118692 40.08593392692988, -105.1500291083445 40.08709170551144, -105.1500284624822 40.0871466566247, -105.1500315862041 40.08732238622535, -105.1503301391773 40.08732628912127, -105.1505482607425 40.08732532748923, -105.1505590916493 40.08775506776752, -105.1505388737468 40.08793399243624, -105.1504380319817 40.08836193466365, -105.1502919166002 40.08890586204939, -105.1502730612071 40.08902796527107, -105.1502670294704 40.08908889026885, -105.1502418931692 40.08973805003863, -105.1502290998738 40.08986291678186, -105.1502271176818 40.09024888266667, -105.1502481463396 40.09067801875981, -105.1502920639366 40.090826116572, -105.1503509251028 40.09091798442525, -105.1504550752855 40.09103002878979, -105.1505850491047 40.09112513076602, -105.1509691325867 40.09129402290613, -105.1517160942745 40.09158589547712, -105.1517909045741 40.09163498487955, -105.1519211509103 40.09174710660227, -105.1520220070036 40.09187506125325, -105.1521509879569 40.09216506676574, -105.1522459778917 40.09246210647947, -105.1523218826696 40.09257708391691, -105.1524239456605 40.09267896267339, -105.1525261515865 40.09275311622527, -105.1527571187147 40.09288091231203, -105.1528060367679 40.09289094223133, -105.153005001525 40.09291597223615, -105.1532069735748 40.09291191280226, -105.1541520415113 40.09277007650465, -105.1542489372922 40.09276405226741, -105.1544429903503 40.09277094765564, -105.1545309238994 40.09277011290997, -105.1547048938937 40.09279012334013, -105.1548679838794 40.09284112289536, -105.1553178420634 40.09315404401035, -105.1551540911595 40.09330399112451, -105.155019925391 40.09346994805548, -105.1549189245638 40.09365110331297, -105.1548118297138 40.09390608435718, -105.1547759486652 40.09407398207865, -105.1547684123273 40.09436209381196, -105.1547597804309 40.09612820611819, -105.154758895776 40.09630987935132, -105.1547571609056 40.09707495511488, -105.154756106325 40.09770606877903, -105.1547554099797 40.09863594701231, -105.1547549925367 40.09919504942512, -105.1547441136172 40.09953208943183, -105.1547570382219 40.09999005930496, -105.1547921010463 40.10075991187671, -105.1547910443339 40.10160295281706))</t>
+          <t>POLYGON ((-105.1547910443339 40.10160295281706, -105.15943048902622 40.10160443093669, -105.16147447332631 40.101604152914106, -105.16244628529887 40.101607594944134, -105.1627463884044 40.101607277561925, -105.16274587824098 40.10149052707892, -105.16277449713643 40.10144969519414, -105.16280033344457 40.101253373880766, -105.16283282880786 40.101147088012006, -105.16291143255413 40.101054574330824, -105.16294034820156 40.100953733195595, -105.16302619026744 40.10083396358396, -105.16317275366546 40.10064617859581, -105.16330124630154 40.10052107796384, -105.16346182685328 40.100371520889226, -105.16360075889624 40.10029009387689, -105.16368253463615 40.100273965534264, -105.16382460000307 40.1002771072795, -105.16409118752742 40.100239694784136, -105.1642014326381 40.10021273845721, -105.16428698915718 40.10015024909485, -105.16439093818171 40.09995961059775, -105.16439497335499 40.099861423933184, -105.16433904299731 40.09967850396548, -105.16437512674068 40.09956404480679, -105.1644680692662 40.09944429475246, -105.1645642939285 40.09937910902314, -105.1648670799139 40.099202686020696, -105.1650522630877 40.09910502493955, -105.16517708972745 40.09900173334665, -105.16529108584986 40.09893387138398, -105.16533409800586 40.09885489136187, -105.16531711620739 40.09869663455474, -105.16533179236121 40.09860120674662, -105.16542840364889 40.09845691671995, -105.16545370972898 40.09836697491093, -105.16545760927073 40.098296065687165, -105.1654582390793 40.09816786405847, -105.16549067522898 40.098072487678905, -105.16556547839726 40.098029060821396, -105.16567226196464 40.09798299935861, -105.16583245771358 40.097909814499914, -105.166095414537 40.097886025381705, -105.16632643203002 40.09785668815526, -105.16652530864712 40.09786271790858, -105.16666035918263 40.0978467413104, -105.1667668614243 40.097857960054796, -105.16685199895795 40.09788002749483, -105.1670507835059 40.0979051506871, -105.16728533844152 40.09787854890141, -105.16744872367217 40.097879019574506, -105.16754775782991 40.09785733257959, -105.16759460279451 40.09782761281062, -105.16762672958473 40.09779497309102, -105.1676589217346 40.09774869415765, -105.1676666652484 40.097617785836555, -105.16781295612493 40.0974818200669, -105.16795614635373 40.097253102902286, -105.16818720517479 40.097076277576996, -105.16840496355456 40.09698980339898, -105.16856516943041 40.09695104110424, -105.16878146853138 40.09698815687596, -105.16895524198985 40.09704320919361, -105.16906709018166 40.09719097558062, -105.16904630286368 40.0960826305675, -105.1690438651976 40.095055984336675, -105.16905485320302 40.09462073046497, -105.16908587379714 40.094478854895975, -105.16910793520046 40.09433736433639, -105.16909040748709 40.09427371581661, -105.16906127145552 40.094147979442845, -105.16906690336705 40.09382399952331, -105.16906762941682 40.093418291619834, -105.16909108644835 40.093279126913906, -105.16913362877666 40.09300289877228, -105.16907538330122 40.092604019848174, -105.16906505091019 40.092371592632865, -105.16906495750537 40.09145107771945, -105.16906143441878 40.090149684376215, -105.16906189140508 40.088547341818945, -105.16905088548285 40.08742081434125, -105.1690488848439 40.087214768313586, -105.16906621786075 40.08709728796521, -105.16907914214185 40.08709728808531, -105.16995914161461 40.08707228785719, -105.17017814112107 40.087066287651965, -105.17131914143293 40.087059286926134, -105.17250114183837 40.08704528692955, -105.17574314174557 40.087020287388924, -105.17607914230706 40.08701728667786, -105.17716914162082 40.086985286603365, -105.17876114156095 40.08696128581556, -105.1808461424632 40.08694828645896, -105.18219514204638 40.0869462851299, -105.1835361420234 40.086916286415885, -105.18463414220894 40.08690228587696, -105.18524214270438 40.08689828635889, -105.18534514391155 40.08690028647014, -105.1857791432559 40.086942285850874, -105.18620714240082 40.08700528569321, -105.18651314285769 40.08705628575504, -105.1867131424599 40.08710228521863, -105.18691114155452 40.087157286281595, -105.18727514304611 40.087279285600964, -105.18778814305864 40.08746028560382, -105.18790114213695 40.0875002862527, -105.18790914308472 40.08750328542086, -105.18791298450441 40.087504565717566, -105.18791203187388 40.087501088446, -105.1879288796204 40.087259013934265, -105.1879367177722 40.08684890384132, -105.18795802667437 40.08573387104014, -105.18798288206645 40.08420899185455, -105.18798490164883 40.08337803203136, -105.1880101273988 40.08153800596429, -105.18801098300685 40.08142902449755, -105.18801283915626 40.08125800461307, -105.18804014216083 40.079041894703515, -105.18805190791906 40.07733113014445, -105.1880671719961 40.07641702604863, -105.188070113258 40.076242989118825, -105.18807085625447 40.076198762089874, -105.1880801936184 40.07619945109983, -105.18819219386302 40.07618545050101, -105.18829219389012 40.076155450695765, -105.18851419421918 40.07610945042958, -105.188729194604 40.07604045081974, -105.18896319434891 40.075923450619214, -105.18910319508004 40.075906450671695, -105.18932819446984 40.075853450776826, -105.18967419475453 40.07570145051615, -105.18996419495933 40.075664450308146, -105.19022412651081 40.07560863429631, -105.19075119501042 40.075495450893975, -105.19075219480449 40.075462450216754, -105.19075419508978 40.075432450477926, -105.1907571945497 40.075404450153144, -105.19076219419077 40.07536145038617, -105.19076719487695 40.07532545046012, -105.19077519464376 40.07528244972295, -105.19078119436448 40.075255450849625, -105.19079219496625 40.07520944998442, -105.19080119507251 40.07517645092222, -105.19081119506471 40.07514245121535, -105.19081819438921 40.075120450913516, -105.1908321947982 40.07508045099295, -105.19084219480007 40.07505445084159, -105.19109119425013 40.07506045112101, -105.19141019462492 40.07502445075971, -105.19192319539738 40.0750234505873, -105.1921041958643 40.07508645023321, -105.19245219500647 40.07516645038263, -105.19291019553113 40.075455450296985, -105.19306865562119 40.07551448774536, -105.1935500196004 40.075693829358336, -105.19426219635677 40.075959451085645, -105.19456419531275 40.075430450634904, -105.19446119494306 40.075400450346436, -105.19448619509271 40.07535544988587, -105.19449619558274 40.07523545057487, -105.19427019497124 40.07470545027712, -105.19413019470491 40.074482449935026, -105.19396619623618 40.074041450513285, -105.19390919444979 40.073920450374885, -105.19386719534614 40.07375044969388, -105.19386319610042 40.07289745028993, -105.19260617270622 40.07290183614763, -105.19101417582573 40.07290737187865, -105.18911707007419 40.072913939430826, -105.18808897854088 40.07291738748686, -105.18657924581603 40.07290802007324, -105.18531230959479 40.072900143526056, -105.1835708587782 40.07288929420034, -105.18298519342392 40.07288645145971, -105.18146443859081 40.072914363798205, -105.18016656043561 40.07291007946497, -105.17847419130362 40.072900451071554, -105.17846819175679 40.07272945154712, -105.1784700126258 40.07272244957001, -105.17814206546103 40.072726880014024, -105.17728512921693 40.072739037271496, -105.17434612343179 40.07273105648155, -105.17341499111339 40.072716072357764, -105.17230691063841 40.07271595167755, -105.16913782298003 40.072700048081686, -105.16564594934432 40.072708104210434, -105.1639618314581 40.072711998405815, -105.16115506314621 40.07269912567766, -105.15976001084104 40.07270600258341, -105.15782013230594 40.072692032490046, -105.15569511240872 40.072687085805136, -105.15454814301404 40.0726748738095, -105.1530480376165 40.07268108133522, -105.15156589224627 40.072668929607396, -105.15047098502167 40.07267797250206, -105.15016318712127 40.07267877556609, -105.1500890297157 40.081991470487715, -105.15005820709473 40.084615088187775, -105.15004271186916 40.085933926929876, -105.15002910834453 40.08709170551144, -105.15002846248223 40.087146656624704, -105.15003158620414 40.087322386225345, -105.1503301391773 40.08732628912127, -105.15054826074254 40.08732532748923, -105.15055909164926 40.087755067767525, -105.1505388737468 40.08793399243624, -105.15043803198166 40.088361934663645, -105.15029191660018 40.088905862049394, -105.1502730612071 40.08902796527107, -105.15026702947037 40.089088890268854, -105.15024189316918 40.08973805003863, -105.1502290998738 40.08986291678186, -105.15022711768182 40.09024888266667, -105.15024814633956 40.09067801875981, -105.15029206393665 40.090826116572, -105.15035092510281 40.09091798442525, -105.15045507528546 40.09103002878979, -105.15058504910466 40.09112513076602, -105.1509691325867 40.09129402290613, -105.15171609427455 40.09158589547712, -105.15179090457409 40.09163498487955, -105.15192115091034 40.09174710660227, -105.15202200700361 40.09187506125325, -105.1521509879569 40.092165066765745, -105.15224597789172 40.092462106479466, -105.15232188266958 40.09257708391691, -105.15242394566049 40.09267896267339, -105.1525261515865 40.09275311622527, -105.15275711871475 40.092880912312026, -105.15280603676786 40.09289094223133, -105.15300500152499 40.09291597223615, -105.15320697357481 40.092911912802265, -105.15415204151131 40.09277007650465, -105.1542489372922 40.09276405226741, -105.15444299035028 40.09277094765564, -105.15453092389943 40.092770112909975, -105.15470489389374 40.09279012334013, -105.1548679838794 40.09284112289536, -105.15531784206338 40.093154044010355, -105.15515409115949 40.093303991124515, -105.15501992539099 40.09346994805548, -105.15491892456382 40.09365110331297, -105.15481182971382 40.09390608435718, -105.15477594866518 40.09407398207865, -105.15476841232726 40.09436209381196, -105.15475978043091 40.096128206118195, -105.15475889577603 40.09630987935132, -105.15475716090556 40.09707495511488, -105.15475610632501 40.09770606877903, -105.15475540997969 40.09863594701231, -105.15475499253671 40.09919504942512, -105.15474411361718 40.099532089431825, -105.15475703822187 40.09999005930496, -105.15479210104625 40.100759911876715, -105.1547910443339 40.10160295281706))</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -2932,7 +2944,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1594304890262 40.10160443093669, -105.1594219558605 40.10315811995677, -105.1594495599439 40.10886022285561, -105.1594520114176 40.10922888777313, -105.1594718259507 40.11205812132699, -105.159467921669 40.11419687283805, -105.1594566443818 40.11609286922273, -105.1594641412873 40.11689641328065, -105.1614528663692 40.11528080007928, -105.1674439177613 40.11003576716704, -105.1685799278165 40.10901976085416, -105.1688417643584 40.10884061707407, -105.1763019499671 40.1023029683946, -105.1770289540793 40.10167497796913, -105.1842254973132 40.09480566330672, -105.1842981568986 40.09474644455597, -105.1847691909817 40.09436254127205, -105.1842313087119 40.09437102454378, -105.1842268610857 40.09437092141485, -105.1837133098082 40.09435902413936, -105.1836459240365 40.09435811360667, -105.1877841432244 40.09059128547788, -105.1878801447803 40.09031128629881, -105.187895143864 40.09008128635119, -105.1880331435849 40.08791628622662, -105.1880329532884 40.08791559131351, -105.1879211426858 40.08750728610932, -105.1879129845044 40.08750456571757, -105.1879091430847 40.08750328542086, -105.187901142137 40.0875002862527, -105.1877881430586 40.08746028560382, -105.1872751430461 40.08727928560096, -105.1869111415545 40.0871572862816, -105.1867131424599 40.08710228521863, -105.1865131428577 40.08705628575504, -105.1862071424008 40.08700528569321, -105.1857791432559 40.08694228585087, -105.1853451439115 40.08690028647014, -105.1852421427044 40.08689828635889, -105.1846341422089 40.08690228587696, -105.1835361420234 40.08691628641589, -105.1821951420464 40.0869462851299, -105.1808461424632 40.08694828645896, -105.178761141561 40.08696128581556, -105.1771691416208 40.08698528660337, -105.1760791423071 40.08701728667786, -105.1757431417456 40.08702028738892, -105.1725011418384 40.08704528692955, -105.1713191414329 40.08705928692613, -105.1701781411211 40.08706628765196, -105.1699591416146 40.08707228785719, -105.1690791421419 40.08709728808531, -105.1690662178607 40.08709728796521, -105.1690488848439 40.08721476831359, -105.1690508854828 40.08742081434125, -105.1690618914051 40.08854734181894, -105.1690614344188 40.09014968437621, -105.1690649575054 40.09145107771945, -105.1690650509102 40.09237159263287, -105.1690753833012 40.09260401984817, -105.1691336287767 40.09300289877228, -105.1690910864483 40.09327912691391, -105.1690676294168 40.09341829161983, -105.1690669033671 40.09382399952331, -105.1690612714555 40.09414797944284, -105.1690904074871 40.09427371581661, -105.1691079352005 40.09433736433639, -105.1690858737971 40.09447885489597, -105.169054853203 40.09462073046497, -105.1690438651976 40.09505598433667, -105.1690463028637 40.0960826305675, -105.1690670901817 40.09719097558062, -105.1689552419898 40.09704320919361, -105.1687814685314 40.09698815687596, -105.1685651694304 40.09695104110424, -105.1684049635546 40.09698980339898, -105.1681872051748 40.097076277577, -105.1679561463537 40.09725310290229, -105.1678129561249 40.0974818200669, -105.1676666652484 40.09761778583655, -105.1676589217346 40.09774869415765, -105.1676267295847 40.09779497309102, -105.1675946027945 40.09782761281062, -105.1675477578299 40.09785733257959, -105.1674487236722 40.09787901957451, -105.1672853384415 40.09787854890141, -105.1670507835059 40.0979051506871, -105.166851998958 40.09788002749483, -105.1667668614243 40.0978579600548, -105.1666603591826 40.0978467413104, -105.1665253086471 40.09786271790858, -105.16632643203 40.09785668815526, -105.166095414537 40.0978860253817, -105.1658324577136 40.09790981449991, -105.1656722619646 40.09798299935861, -105.1655654783973 40.0980290608214, -105.165490675229 40.09807248767891, -105.1654582390793 40.09816786405847, -105.1654576092707 40.09829606568717, -105.165453709729 40.09836697491093, -105.1654284036489 40.09845691671995, -105.1653317923612 40.09860120674662, -105.1653171162074 40.09869663455474, -105.1653340980059 40.09885489136187, -105.1652910858499 40.09893387138398, -105.1651770897275 40.09900173334665, -105.1650522630877 40.09910502493955, -105.1648670799139 40.0992026860207, -105.1645642939285 40.09937910902314, -105.1644680692662 40.09944429475246, -105.1643751267407 40.09956404480679, -105.1643390429973 40.09967850396548, -105.164394973355 40.09986142393318, -105.1643909381817 40.09995961059775, -105.1642869891572 40.10015024909485, -105.1642014326381 40.10021273845721, -105.1640911875274 40.10023969478414, -105.1638246000031 40.1002771072795, -105.1636825346362 40.10027396553426, -105.1636007588962 40.10029009387689, -105.1634618268533 40.10037152088923, -105.1633012463015 40.10052107796384, -105.1631727536655 40.10064617859581, -105.1630261902674 40.10083396358396, -105.1629403482016 40.1009537331956, -105.1629114325541 40.10105457433082, -105.1628328288079 40.10114708801201, -105.1628003334446 40.10125337388077, -105.1627744971364 40.10144969519414, -105.162745878241 40.10149052707892, -105.1627463884044 40.10160727756193, -105.1624462852989 40.10160759494413, -105.1614744733263 40.10160415291411, -105.1594304890262 40.10160443093669))</t>
+          <t>POLYGON ((-105.15943048902622 40.10160443093669, -105.15942195586052 40.103158119956774, -105.15944955994391 40.10886022285561, -105.1594520114176 40.10922888777313, -105.15947182595067 40.11205812132699, -105.15946792166899 40.11419687283805, -105.15945664438176 40.11609286922273, -105.15946414128727 40.11689641328065, -105.16145286636917 40.115280800079276, -105.16744391776132 40.11003576716704, -105.16857992781651 40.10901976085416, -105.16884176435845 40.108840617074065, -105.17630194996711 40.1023029683946, -105.17702895407928 40.101674977969125, -105.18422549731315 40.094805663306715, -105.1842981568986 40.094746444555966, -105.18476919098173 40.09436254127205, -105.18423130871186 40.09437102454378, -105.18422686108573 40.09437092141485, -105.1837133098082 40.09435902413936, -105.18364592403653 40.09435811360667, -105.18778414322443 40.09059128547788, -105.18788014478031 40.090311286298814, -105.18789514386395 40.09008128635119, -105.1880331435849 40.08791628622662, -105.18803295328843 40.08791559131351, -105.1879211426858 40.08750728610932, -105.18791298450441 40.087504565717566, -105.18790914308472 40.08750328542086, -105.18790114213695 40.0875002862527, -105.18778814305864 40.08746028560382, -105.18727514304611 40.087279285600964, -105.18691114155452 40.087157286281595, -105.1867131424599 40.08710228521863, -105.18651314285769 40.08705628575504, -105.18620714240082 40.08700528569321, -105.1857791432559 40.086942285850874, -105.18534514391155 40.08690028647014, -105.18524214270438 40.08689828635889, -105.18463414220894 40.08690228587696, -105.1835361420234 40.086916286415885, -105.18219514204638 40.0869462851299, -105.1808461424632 40.08694828645896, -105.17876114156095 40.08696128581556, -105.17716914162082 40.086985286603365, -105.17607914230706 40.08701728667786, -105.17574314174557 40.087020287388924, -105.17250114183837 40.08704528692955, -105.17131914143293 40.087059286926134, -105.17017814112107 40.087066287651965, -105.16995914161461 40.08707228785719, -105.16907914214185 40.08709728808531, -105.16906621786075 40.08709728796521, -105.1690488848439 40.087214768313586, -105.16905088548285 40.08742081434125, -105.16906189140508 40.088547341818945, -105.16906143441878 40.090149684376215, -105.16906495750537 40.09145107771945, -105.16906505091019 40.092371592632865, -105.16907538330122 40.092604019848174, -105.16913362877666 40.09300289877228, -105.16909108644835 40.093279126913906, -105.16906762941682 40.093418291619834, -105.16906690336705 40.09382399952331, -105.16906127145552 40.094147979442845, -105.16909040748709 40.09427371581661, -105.16910793520046 40.09433736433639, -105.16908587379714 40.094478854895975, -105.16905485320302 40.09462073046497, -105.1690438651976 40.095055984336675, -105.16904630286368 40.0960826305675, -105.16906709018166 40.09719097558062, -105.16895524198985 40.09704320919361, -105.16878146853138 40.09698815687596, -105.16856516943041 40.09695104110424, -105.16840496355456 40.09698980339898, -105.16818720517479 40.097076277576996, -105.16795614635373 40.097253102902286, -105.16781295612493 40.0974818200669, -105.1676666652484 40.097617785836555, -105.1676589217346 40.09774869415765, -105.16762672958473 40.09779497309102, -105.16759460279451 40.09782761281062, -105.16754775782991 40.09785733257959, -105.16744872367217 40.097879019574506, -105.16728533844152 40.09787854890141, -105.1670507835059 40.0979051506871, -105.16685199895795 40.09788002749483, -105.1667668614243 40.097857960054796, -105.16666035918263 40.0978467413104, -105.16652530864712 40.09786271790858, -105.16632643203002 40.09785668815526, -105.166095414537 40.097886025381705, -105.16583245771358 40.097909814499914, -105.16567226196464 40.09798299935861, -105.16556547839726 40.098029060821396, -105.16549067522898 40.098072487678905, -105.1654582390793 40.09816786405847, -105.16545760927073 40.098296065687165, -105.16545370972898 40.09836697491093, -105.16542840364889 40.09845691671995, -105.16533179236121 40.09860120674662, -105.16531711620739 40.09869663455474, -105.16533409800586 40.09885489136187, -105.16529108584986 40.09893387138398, -105.16517708972745 40.09900173334665, -105.1650522630877 40.09910502493955, -105.1648670799139 40.099202686020696, -105.1645642939285 40.09937910902314, -105.1644680692662 40.09944429475246, -105.16437512674068 40.09956404480679, -105.16433904299731 40.09967850396548, -105.16439497335499 40.099861423933184, -105.16439093818171 40.09995961059775, -105.16428698915718 40.10015024909485, -105.1642014326381 40.10021273845721, -105.16409118752742 40.100239694784136, -105.16382460000307 40.1002771072795, -105.16368253463615 40.100273965534264, -105.16360075889624 40.10029009387689, -105.16346182685328 40.100371520889226, -105.16330124630154 40.10052107796384, -105.16317275366546 40.10064617859581, -105.16302619026744 40.10083396358396, -105.16294034820156 40.100953733195595, -105.16291143255413 40.101054574330824, -105.16283282880786 40.101147088012006, -105.16280033344457 40.101253373880766, -105.16277449713643 40.10144969519414, -105.16274587824098 40.10149052707892, -105.1627463884044 40.101607277561925, -105.16244628529887 40.101607594944134, -105.16147447332631 40.101604152914106, -105.15943048902622 40.10160443093669))</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -2974,7 +2986,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1310181860247 40.11642745992815, -105.1311001857065 40.11641745990186, -105.1311361855693 40.11640146052148, -105.1311941855785 40.11632246004667, -105.1312731862733 40.11603745969056, -105.1313421735774 40.11588122329221, -105.1313536700491 40.11585518628547, -105.1314091855054 40.11572946035969, -105.1314881866388 40.11547746041233, -105.1315867964692 40.11541012927728, -105.1316741852191 40.11535046009578, -105.1317241867259 40.115191460073, -105.1318891858139 40.11515346003952, -105.1322901860955 40.11511545933612, -105.1322751860538 40.11537845966455, -105.1323321866405 40.11548845960182, -105.1323543636915 40.11550215156709, -105.1324471863394 40.11555946059213, -105.1326261859337 40.11553245951755, -105.1327901954493 40.11544179157702, -105.1330331862589 40.1153074606795, -105.1331191859966 40.11521445939096, -105.1331411856992 40.11488445961638, -105.133234186949 40.1147304599069, -105.1333340990247 40.11463557074746, -105.1334131856659 40.11456046023817, -105.1335362178282 40.11456046070084, -105.1336711859251 40.11456046016362, -105.1338501858913 40.11461045973502, -105.1342361863052 40.11481945914035, -105.134329186555 40.11493445989868, -105.1344361864871 40.11494046008041, -105.1346221871356 40.11477045999761, -105.1346861864186 40.1145994604477, -105.1347221866439 40.11440245982309, -105.1350148427649 40.11403187214655, -105.1350602254513 40.11397440482906, -105.1350801857764 40.1139464596064, -105.135182139388 40.11393135543081, -105.1352747246668 40.11399622867296, -105.1353697140693 40.11414098052226, -105.1354881867362 40.1143364596393, -105.1356101869878 40.11439745989412, -105.1357101866312 40.1143694590412, -105.1357961873731 40.11427645936892, -105.1357961869385 40.11416645986762, -105.1357461861792 40.11397446007563, -105.135839187088 40.11381545968592, -105.135989187307 40.11374945946562, -105.1360886500456 40.11374159503977, -105.1362041868162 40.11373245991339, -105.1363067782619 40.11374563253825, -105.1364611865636 40.11376545914218, -105.136647186488 40.11372745988353, -105.1367132737641 40.1136867910588, -105.1367901873759 40.11363945994061, -105.1368346130924 40.11357172155405, -105.1368911870444 40.11348545902928, -105.136926249788 40.11333338529389, -105.1369771870886 40.1131124602168, -105.1369701872679 40.11299745903131, -105.1369049964273 40.11285831592468, -105.1368341870956 40.11272245868071, -105.1367911864023 40.11260145944513, -105.1366771874476 40.11241445906841, -105.1367061863406 40.11229345931134, -105.1368491873511 40.11220045890114, -105.1369921868139 40.11221745873338, -105.1371491860115 40.11229945967833, -105.1373141862809 40.11240445921667, -105.1373815568126 40.11239409447652, -105.137381607722 40.11239400637307, -105.1374571875025 40.11238245959723, -105.1375501870297 40.11229945883865, -105.1375851861427 40.11219045989127, -105.1375783082322 40.11213281406475, -105.1375641863439 40.11201445996381, -105.1375291873222 40.1118764593884, -105.1375931871308 40.11181145885294, -105.1378641325305 40.11172992844479, -105.1379221864662 40.11171245960098, -105.1380043977404 40.11165544251909, -105.1381346354642 40.11156511596145, -105.1383520505958 40.11141634734895, -105.1385021871975 40.1113174589991, -105.1385885373203 40.11121663711587, -105.1386811865493 40.11110845948276, -105.1387881878956 40.11089445929716, -105.1388881875843 40.1108174596417, -105.1391321875739 40.11077945940796, -105.1392166376191 40.11076175266201, -105.1392452612604 40.11075575100678, -105.139318187819 40.11074045974925, -105.1393678994795 40.11072429438088, -105.1395584243935 40.11066233928282, -105.1396041866986 40.11064745841755, -105.139761662953 40.11061060263292, -105.139933186621 40.11057045894069, -105.1401831872421 40.11054845896744, -105.1402242919559 40.11052569800182, -105.1402249272183 40.11052579274737, -105.1403254691414 40.11047119351303, -105.1404621873911 40.11037345868738, -105.1406051874184 40.11035645826706, -105.1406771869243 40.11047245857907, -105.1407334051194 40.11062448513666, -105.1407481874379 40.11066445856965, -105.140834187162 40.11075245890581, -105.1409411875114 40.11075745877094, -105.1411311766261 40.1106291019769, -105.1413141878553 40.1105054587965, -105.1413481734702 40.11044279920952, -105.1413941070261 40.11035810907864, -105.1414421879518 40.11026945914983, -105.1414707361548 40.11017746660836, -105.1414781867133 40.11015345869473, -105.1415522170272 40.11016179340662, -105.1416291874734 40.11017045872525, -105.1416791872043 40.11020345863564, -105.1417791876447 40.11018145895183, -105.1418291878365 40.11010445836963, -105.1418291876094 40.11005455446081, -105.1418291868519 40.10988545812238, -105.1418336763905 40.10988134348353, -105.1419011880146 40.10981945778273, -105.1419941874593 40.10979745872118, -105.1420791878335 40.10989045903131, -105.1420893355731 40.10999193837458, -105.142101188436 40.11011045872333, -105.142126431106 40.11012005767923, -105.1421721882141 40.11013745854567, -105.1423603463296 40.11012042383983, -105.142415188456 40.11011545817529, -105.1424617281768 40.1101221067335, -105.1425371920236 40.11013288780438, -105.1425655734614 40.11013694209405, -105.1425889933667 40.11014028752435, -105.1426306946563 40.11014624465503, -105.142676579207 40.11015280013385, -105.142723188132 40.11015945870771, -105.1428108591608 40.11016490951189, -105.1429161884725 40.11017145869828, -105.1429648250731 40.11017641491812, -105.1429648182534 40.11017771543015, -105.1429664300369 40.11017657839365, -105.1430731876633 40.11018745855665, -105.1431521881496 40.11013245795137, -105.1431796482247 40.11002829750333, -105.1432101875002 40.10991245887465, -105.1433101881548 40.10983045861817, -105.1433261756351 40.10975684233937, -105.143353188753 40.10963245825586, -105.1433382934257 40.10957753407826, -105.143311550045 40.10947891718003, -105.1432891876009 40.10939645879092, -105.1432609860456 40.10935610828796, -105.1432241877329 40.10930345901374, -105.1432328627724 40.10926008276815, -105.143246187286 40.10919345809153, -105.1433391874849 40.10910545859052, -105.1434139958149 40.10909877173545, -105.1435181878683 40.10908945828713, -105.1436391882093 40.10914945901379, -105.1437251880138 40.10919945804216, -105.1438211598157 40.10919242101242, -105.1438751876574 40.10918845906782, -105.1439693495291 40.10914216706989, -105.1440541880079 40.10910045846919, -105.144096572717 40.10909719816408, -105.144123205141 40.10909515020784, -105.1441548387739 40.1090927168681, -105.1441971870977 40.10908945911586, -105.1442691886938 40.10915545782236, -105.144345777039 40.10927439618445, -105.1443541882314 40.10928745804113, -105.1444693672245 40.10929912209676, -105.1444797799127 40.10930245231871, -105.1444972586797 40.10930194682363, -105.1446208477053 40.10929837426536, -105.1447756584748 40.10929241273082, -105.1448795350452 40.10928805784319, -105.1450518589718 40.10928083304527, -105.145156188375 40.1092764585858, -105.1452858210533 40.10929371331622, -105.1454491885845 40.10931545852137, -105.1456711885987 40.10930945796668, -105.1457684551437 40.10927877952781, -105.1459173643046 40.10923181175473, -105.1459501886296 40.1092214585894, -105.14603607745 40.10920312262454, -105.1461281887017 40.10918345829599, -105.1462641887339 40.10909045812184, -105.1463979289381 40.10907882875447, -105.1465861886723 40.10906245846613, -105.1466952183154 40.10908102655211, -105.146815189195 40.10910145810936, -105.1469201518979 40.10911105121482, -105.1470011879937 40.10911845817668, -105.1470486443322 40.10911952728623, -105.1471561250959 40.10912194792165, -105.1472231888622 40.10912345873804, -105.1472670149087 40.10914467042698, -105.1473230421344 40.10917178706982, -105.1474308225596 40.10922395285124, -105.1474731885267 40.10924445749985, -105.1475425064825 40.10924445742264, -105.1476126056347 40.10924445788622, -105.1476639806363 40.10924445792431, -105.1477521893066 40.10924445771168, -105.1478568619915 40.10927209172333, -105.1480021884751 40.109310458268, -105.1481495371838 40.10931457831904, -105.1483626110154 40.10932053569708, -105.1484881807936 40.10932404681184, -105.1486101887807 40.10932745778867, -105.148681535631 40.10935141047885, -105.1486906073675 40.10935551079681, -105.1487742892276 40.10938470218268, -105.1488282710606 40.10942647438896, -105.1489321887245 40.1095144583186, -105.1489961900791 40.10967345746549, -105.1490951105112 40.10978119433448, -105.1491636738781 40.10981642606204, -105.1492181885192 40.10984345882783, -105.1493760472449 40.1098539470783, -105.1495327897234 40.10986436057436, -105.1498051887075 40.10988245858211, -105.1499037995298 40.10983605366251, -105.1500261889393 40.10977845814232, -105.1500616825502 40.10974049989558, -105.1500969366913 40.10970279759637, -105.1501310738441 40.10966628976156, -105.1501701894573 40.10962445796797, -105.150213190036 40.10948145755771, -105.150192927634 40.10942765734119, -105.1501841896918 40.10940445815319, -105.1501460270222 40.10937066109187, -105.150113914031 40.10934222227647, -105.150035810524 40.10927305377975, -105.1499481896146 40.10919545785707, -105.1499411886424 40.10911345803316, -105.1500271894042 40.10901445758356, -105.1501361731898 40.10894852276716, -105.1501628272604 40.1089323972873, -105.1501829687099 40.10892021131422, -105.1501990355049 40.1089104906731, -105.150216358927 40.10890001008798, -105.1502271897408 40.1088934573679, -105.1502991895659 40.10876745797281, -105.1503701892914 40.10874045812216, -105.1505561895843 40.10874045817922, -105.1507351896093 40.10865745754312, -105.1509501898016 40.10867945738578, -105.1510291895926 40.10873445721234, -105.1511498943537 40.108892914989, -105.1512721889252 40.10905345792743, -105.151443190266 40.10915745838717, -105.1515425217955 40.10915797339747, -105.1516361903776 40.10915845863114, -105.152058189739 40.10899345806407, -105.152168642065 40.10888557367066, -105.1521720437602 40.10888555509551, -105.1521871900507 40.10886745719991, -105.1522441899349 40.10883445806299, -105.1522521895131 40.10872445833751, -105.1522161898024 40.10867445774499, -105.1519151896514 40.1086254581982, -105.1518011892207 40.10854845784844, -105.1518081899357 40.10844445794176, -105.1520521905081 40.10809245803009, -105.1521161891182 40.10785645730169, -105.1522381891769 40.1078014575306, -105.1526961899649 40.10774645807478, -105.1530101897713 40.1076424577811, -105.1531681905297 40.10752745787505, -105.1532041904084 40.10742245698562, -105.1531971895655 40.10730745767818, -105.1530821895656 40.10724745707277, -105.1527891896304 40.10716445739909, -105.1527461895664 40.10708745705721, -105.1528251898034 40.10689545706076, -105.1528251894787 40.1068184572149, -105.1529611896807 40.10678045703483, -105.1532181895994 40.10680245729557, -105.1534041890178 40.10683545695765, -105.153533190452 40.10679645699769, -105.1536831893247 40.10669845729011, -105.1538481902248 40.10664345777509, -105.1543781900811 40.10669245702027, -105.1546631906193 40.10667645674386, -105.1549851905804 40.10658345749179, -105.1551071895624 40.106484457227, -105.1551781906975 40.10638545677693, -105.155372190027 40.10630845692795, -105.1557151895679 40.10621545706669, -105.1564161904518 40.10613345690832, -105.1565797245652 40.10604856929712, -105.1569951900118 40.10582045723518, -105.157138190582 40.10579245659894, -105.157239191129 40.10571045628147, -105.157253190884 40.10562845707536, -105.1571241900853 40.10546345672344, -105.1571241898577 40.1053754563856, -105.1572321903226 40.10529845652795, -105.1576681914213 40.10507845747404, -105.1580761909817 40.10495245717316, -105.1581892413284 40.10490396872007, -105.1584981900914 40.10477145654381, -105.1587201908592 40.10476045668218, -105.1588991905787 40.10458445709242, -105.1589061910858 40.10450845692532, -105.1588201907179 40.10434845704976, -105.1588411915942 40.10426645671227, -105.1590781918603 40.10400245670831, -105.1594259918098 40.10399197542836, -105.1594259842159 40.10399044520795, -105.1594219558605 40.10315811995677, -105.1594304890262 40.10160443093669, -105.1547910443339 40.10160295281706, -105.1547921010463 40.10075991187671, -105.1547570382219 40.09999005930496, -105.1547441136172 40.09953208943183, -105.1547549925367 40.09919504942512, -105.1547554099797 40.09863594701231, -105.154756106325 40.09770606877903, -105.1547571609056 40.09707495511488, -105.154758895776 40.09630987935132, -105.1547597804309 40.09612820611819, -105.1547684123273 40.09436209381196, -105.1547759486652 40.09407398207865, -105.1548118297138 40.09390608435718, -105.1549189245638 40.09365110331297, -105.155019925391 40.09346994805548, -105.1551540911595 40.09330399112451, -105.1553178420634 40.09315404401035, -105.1548679838794 40.09284112289536, -105.1547048938937 40.09279012334013, -105.1545309238994 40.09277011290997, -105.1544429903503 40.09277094765564, -105.1542489372922 40.09276405226741, -105.1541520415113 40.09277007650465, -105.1532069735748 40.09291191280226, -105.153005001525 40.09291597223615, -105.1528060367679 40.09289094223133, -105.1527571187147 40.09288091231203, -105.1525261515865 40.09275311622527, -105.1524239456605 40.09267896267339, -105.1523218826696 40.09257708391691, -105.1522459778917 40.09246210647947, -105.1521509879569 40.09216506676574, -105.1520220070036 40.09187506125325, -105.1519211509103 40.09174710660227, -105.1517909045741 40.09163498487955, -105.1517160942745 40.09158589547712, -105.1509691325867 40.09129402290613, -105.1505850491047 40.09112513076602, -105.1504550752855 40.09103002878979, -105.1503509251028 40.09091798442525, -105.1502920639366 40.090826116572, -105.1502481463396 40.09067801875981, -105.1502271176818 40.09024888266667, -105.1502290998738 40.08986291678186, -105.1502418931692 40.08973805003863, -105.1502670294704 40.08908889026885, -105.1502730612071 40.08902796527107, -105.1502919166002 40.08890586204939, -105.1504380319817 40.08836193466365, -105.1505388737468 40.08793399243624, -105.1505590916493 40.08775506776752, -105.1505482607425 40.08732532748923, -105.1503301391773 40.08732628912127, -105.1500315862041 40.08732238622535, -105.1497181388009 40.08731828785967, -105.1490541379685 40.08730928858999, -105.146593138654 40.08730128957986, -105.1443011396943 40.08730228806577, -105.1422081395893 40.08730028957377, -105.1420031391563 40.08730728976931, -105.1409871387648 40.08731128953013, -105.1382631386586 40.08732328982324, -105.1373061386617 40.08732428977066, -105.1349071383346 40.08733428902195, -105.1314691798739 40.08736528014637, -105.1314686920482 40.08736528489368, -105.1315023083889 40.0879120286511, -105.1315123076631 40.08860202899108, -105.1315573093293 40.09073602900505, -105.131565308569 40.09121302826923, -105.1315713090677 40.09267102844738, -105.1315353089882 40.09441602918015, -105.1315413093822 40.09489902827075, -105.1315033084531 40.09835802848521, -105.13149630911 40.09849502893818, -105.1314753089459 40.09960702888224, -105.1314743099729 40.09982802847355, -105.1314613102898 40.1017110280084, -105.1314603103063 40.10285102851227, -105.1313783109039 40.10663902806576, -105.1313063115642 40.10894602876141, -105.1312713110947 40.10989302815075, -105.1312733098291 40.11046202797889, -105.1312403110973 40.11140002800153, -105.1312113114617 40.11250802867715, -105.1311973097867 40.11310902852121, -105.1311303117171 40.114313029054, -105.1310553120431 40.11535402919674, -105.1310183122412 40.11621802952327, -105.1310173486831 40.11641334503174, -105.131018259415 40.11641262021929, -105.1310181860247 40.11642745992815))</t>
+          <t>POLYGON ((-105.13101818602466 40.116427459928154, -105.13110018570654 40.11641745990186, -105.13113618556928 40.11640146052148, -105.1311941855785 40.116322460046675, -105.13127318627333 40.11603745969056, -105.13134217357741 40.115881223292206, -105.13135367004905 40.115855186285465, -105.13140918550543 40.11572946035969, -105.13148818663885 40.11547746041233, -105.13158679646924 40.11541012927728, -105.13167418521913 40.115350460095776, -105.13172418672588 40.115191460073, -105.13188918581388 40.115153460039515, -105.13229018609555 40.115115459336124, -105.1322751860538 40.11537845966455, -105.13233218664047 40.11548845960182, -105.13235436369149 40.11550215156709, -105.1324471863394 40.11555946059213, -105.13262618593367 40.115532459517546, -105.13279019544932 40.11544179157702, -105.1330331862589 40.115307460679496, -105.1331191859966 40.11521445939096, -105.13314118569923 40.11488445961638, -105.13323418694895 40.1147304599069, -105.13333409902465 40.11463557074746, -105.13341318566592 40.114560460238174, -105.13353621782824 40.11456046070084, -105.13367118592514 40.11456046016362, -105.13385018589126 40.11461045973502, -105.13423618630522 40.11481945914035, -105.13432918655498 40.11493445989868, -105.13443618648708 40.11494046008041, -105.13462218713558 40.11477045999761, -105.13468618641862 40.1145994604477, -105.13472218664393 40.11440245982309, -105.13501484276493 40.11403187214655, -105.13506022545131 40.11397440482906, -105.13508018577642 40.1139464596064, -105.13518213938798 40.113931355430815, -105.13527472466679 40.11399622867296, -105.13536971406927 40.11414098052226, -105.13548818673618 40.114336459639304, -105.13561018698785 40.11439745989412, -105.13571018663121 40.1143694590412, -105.13579618737309 40.114276459368924, -105.13579618693852 40.11416645986762, -105.13574618617922 40.11397446007563, -105.13583918708804 40.113815459685924, -105.13598918730703 40.11374945946562, -105.13608865004555 40.11374159503977, -105.13620418681622 40.11373245991339, -105.13630677826191 40.113745632538254, -105.13646118656362 40.11376545914218, -105.13664718648805 40.11372745988353, -105.13671327376406 40.113686791058804, -105.13679018737588 40.113639459940615, -105.13683461309236 40.113571721554045, -105.13689118704438 40.11348545902928, -105.13692624978802 40.11333338529389, -105.13697718708858 40.113112460216804, -105.13697018726795 40.112997459031305, -105.13690499642728 40.112858315924676, -105.13683418709557 40.112722458680715, -105.13679118640235 40.11260145944513, -105.13667718744762 40.11241445906841, -105.13670618634059 40.11229345931134, -105.1368491873511 40.112200458901135, -105.13699218681394 40.11221745873338, -105.13714918601148 40.11229945967833, -105.13731418628093 40.11240445921667, -105.13738155681257 40.11239409447652, -105.13738160772198 40.112394006373066, -105.13745718750249 40.11238245959723, -105.13755018702972 40.11229945883865, -105.13758518614266 40.11219045989127, -105.13757830823218 40.11213281406475, -105.1375641863439 40.11201445996381, -105.13752918732217 40.1118764593884, -105.13759318713076 40.11181145885294, -105.13786413253045 40.11172992844479, -105.1379221864662 40.11171245960098, -105.13800439774043 40.111655442519094, -105.13813463546417 40.11156511596145, -105.13835205059576 40.11141634734895, -105.1385021871975 40.111317458999096, -105.1385885373203 40.111216637115874, -105.13868118654932 40.11110845948276, -105.13878818789559 40.110894459297164, -105.13888818758431 40.1108174596417, -105.1391321875739 40.11077945940796, -105.13921663761907 40.11076175266201, -105.13924526126036 40.110755751006785, -105.13931818781897 40.11074045974925, -105.1393678994795 40.11072429438088, -105.13955842439347 40.11066233928282, -105.13960418669859 40.11064745841755, -105.13976166295305 40.11061060263292, -105.13993318662101 40.11057045894069, -105.1401831872421 40.11054845896744, -105.14022429195595 40.11052569800182, -105.14022492721833 40.110525792747374, -105.1403254691414 40.11047119351303, -105.14046218739112 40.110373458687384, -105.14060518741837 40.11035645826706, -105.14067718692428 40.110472458579075, -105.14073340511936 40.11062448513666, -105.14074818743785 40.11066445856965, -105.14083418716199 40.110752458905814, -105.14094118751137 40.11075745877094, -105.14113117662608 40.1106291019769, -105.1413141878553 40.110505458796496, -105.14134817347019 40.11044279920952, -105.14139410702606 40.11035810907864, -105.14144218795181 40.110269459149826, -105.1414707361548 40.11017746660836, -105.14147818671329 40.110153458694725, -105.14155221702717 40.11016179340662, -105.14162918747343 40.11017045872525, -105.14167918720432 40.11020345863564, -105.1417791876447 40.11018145895183, -105.14182918783652 40.11010445836963, -105.1418291876094 40.11005455446081, -105.14182918685188 40.10988545812238, -105.1418336763905 40.10988134348353, -105.14190118801461 40.10981945778273, -105.1419941874593 40.10979745872118, -105.14207918783355 40.10989045903131, -105.14208933557312 40.109991938374584, -105.14210118843596 40.11011045872333, -105.14212643110595 40.11012005767923, -105.14217218821408 40.11013745854567, -105.14236034632955 40.11012042383983, -105.14241518845598 40.110115458175294, -105.14246172817677 40.1101221067335, -105.14253719202358 40.110132887804376, -105.14256557346143 40.11013694209405, -105.14258899336666 40.11014028752435, -105.14263069465633 40.11014624465503, -105.14267657920696 40.11015280013385, -105.14272318813195 40.110159458707706, -105.14281085916079 40.110164909511894, -105.14291618847248 40.110171458698275, -105.14296482507312 40.110176414918115, -105.1429648182534 40.110177715430154, -105.14296643003689 40.11017657839365, -105.14307318766335 40.11018745855665, -105.14315218814961 40.110132457951366, -105.14317964822474 40.110028297503334, -105.14321018750016 40.10991245887465, -105.1433101881548 40.10983045861817, -105.14332617563505 40.10975684233937, -105.14335318875304 40.10963245825586, -105.14333829342567 40.10957753407826, -105.14331155004504 40.109478917180034, -105.14328918760094 40.10939645879092, -105.14326098604556 40.10935610828796, -105.14322418773291 40.10930345901374, -105.14323286277241 40.10926008276815, -105.14324618728601 40.109193458091525, -105.14333918748494 40.10910545859052, -105.1434139958149 40.10909877173545, -105.14351818786825 40.10908945828713, -105.14363918820928 40.109149459013786, -105.14372518801385 40.10919945804216, -105.14382115981567 40.10919242101242, -105.14387518765736 40.109188459067816, -105.14396934952912 40.10914216706989, -105.14405418800791 40.10910045846919, -105.14409657271696 40.10909719816408, -105.14412320514096 40.109095150207835, -105.14415483877394 40.109092716868105, -105.1441971870977 40.109089459115864, -105.14426918869377 40.10915545782236, -105.14434577703895 40.109274396184446, -105.1443541882314 40.10928745804113, -105.1444693672245 40.10929912209676, -105.1444797799127 40.10930245231871, -105.14449725867966 40.109301946823635, -105.14462084770527 40.10929837426536, -105.14477565847484 40.109292412730824, -105.14487953504525 40.10928805784319, -105.14505185897177 40.10928083304527, -105.14515618837504 40.109276458585796, -105.14528582105332 40.10929371331622, -105.14544918858455 40.109315458521365, -105.14567118859874 40.10930945796668, -105.14576845514371 40.10927877952781, -105.1459173643046 40.109231811754725, -105.14595018862956 40.1092214585894, -105.14603607745003 40.109203122624535, -105.14612818870168 40.10918345829599, -105.14626418873392 40.10909045812184, -105.14639792893813 40.10907882875447, -105.1465861886723 40.109062458466134, -105.14669521831539 40.10908102655211, -105.14681518919504 40.10910145810936, -105.14692015189793 40.10911105121482, -105.1470011879937 40.10911845817668, -105.14704864433224 40.10911952728623, -105.14715612509589 40.10912194792165, -105.1472231888622 40.10912345873804, -105.14726701490875 40.10914467042698, -105.14732304213442 40.10917178706982, -105.1474308225596 40.10922395285124, -105.1474731885267 40.10924445749985, -105.14754250648251 40.10924445742264, -105.14761260563466 40.10924445788622, -105.14766398063628 40.10924445792431, -105.1477521893066 40.10924445771168, -105.14785686199149 40.109272091723334, -105.14800218847513 40.109310458268, -105.14814953718376 40.10931457831904, -105.14836261101539 40.10932053569708, -105.14848818079363 40.10932404681184, -105.14861018878065 40.109327457788666, -105.14868153563097 40.10935141047885, -105.14869060736753 40.10935551079681, -105.14877428922763 40.10938470218268, -105.14882827106062 40.10942647438896, -105.1489321887245 40.1095144583186, -105.14899619007909 40.10967345746549, -105.14909511051121 40.10978119433448, -105.1491636738781 40.10981642606204, -105.14921818851924 40.10984345882783, -105.14937604724486 40.1098539470783, -105.14953278972337 40.109864360574356, -105.14980518870746 40.109882458582106, -105.14990379952984 40.109836053662505, -105.15002618893935 40.10977845814232, -105.15006168255023 40.10974049989558, -105.15009693669128 40.10970279759637, -105.15013107384414 40.109666289761556, -105.15017018945728 40.10962445796797, -105.15021319003601 40.10948145755771, -105.15019292763395 40.10942765734119, -105.15018418969179 40.109404458153186, -105.15014602702216 40.109370661091866, -105.150113914031 40.10934222227647, -105.15003581052405 40.109273053779745, -105.14994818961456 40.10919545785707, -105.14994118864236 40.10911345803316, -105.15002718940416 40.109014457583555, -105.15013617318976 40.108948522767164, -105.15016282726036 40.108932397287305, -105.1501829687099 40.10892021131422, -105.15019903550494 40.1089104906731, -105.15021635892704 40.10890001008798, -105.15022718974079 40.1088934573679, -105.15029918956587 40.10876745797281, -105.15037018929142 40.10874045812216, -105.15055618958428 40.10874045817922, -105.15073518960934 40.108657457543124, -105.15095018980156 40.10867945738578, -105.1510291895926 40.108734457212336, -105.15114989435367 40.108892914989, -105.1512721889252 40.10905345792743, -105.15144319026602 40.109157458387166, -105.1515425217955 40.10915797339747, -105.15163619037757 40.10915845863114, -105.15205818973901 40.10899345806407, -105.15216864206499 40.10888557367066, -105.15217204376017 40.10888555509551, -105.15218719005071 40.10886745719991, -105.15224418993486 40.108834458062994, -105.15225218951315 40.108724458337505, -105.1522161898024 40.10867445774499, -105.15191518965136 40.1086254581982, -105.15180118922069 40.108548457848435, -105.1518081899357 40.108444457941765, -105.15205219050809 40.10809245803009, -105.15211618911823 40.10785645730169, -105.1522381891769 40.1078014575306, -105.15269618996487 40.10774645807478, -105.15301018977131 40.107642457781104, -105.15316819052967 40.10752745787505, -105.15320419040842 40.107422456985624, -105.15319718956553 40.10730745767818, -105.15308218956555 40.10724745707277, -105.15278918963043 40.107164457399094, -105.15274618956637 40.10708745705721, -105.15282518980344 40.10689545706076, -105.15282518947866 40.1068184572149, -105.15296118968074 40.10678045703483, -105.15321818959941 40.10680245729557, -105.15340418901778 40.10683545695765, -105.15353319045201 40.106796456997685, -105.15368318932471 40.106698457290115, -105.15384819022479 40.10664345777509, -105.15437819008106 40.10669245702027, -105.15466319061927 40.10667645674386, -105.15498519058043 40.106583457491794, -105.1551071895624 40.106484457227, -105.15517819069753 40.10638545677693, -105.15537219002702 40.10630845692795, -105.15571518956787 40.10621545706669, -105.15641619045178 40.10613345690832, -105.15657972456523 40.106048569297116, -105.15699519001176 40.105820457235176, -105.15713819058196 40.10579245659894, -105.15723919112895 40.10571045628147, -105.157253190884 40.10562845707536, -105.15712419008531 40.10546345672344, -105.15712418985767 40.1053754563856, -105.15723219032265 40.10529845652795, -105.1576681914213 40.10507845747404, -105.15807619098169 40.10495245717316, -105.15818924132842 40.104903968720066, -105.15849819009142 40.10477145654381, -105.15872019085924 40.10476045668218, -105.15889919057865 40.10458445709242, -105.15890619108582 40.104508456925316, -105.15882019071795 40.10434845704976, -105.1588411915942 40.104266456712274, -105.1590781918603 40.10400245670831, -105.15942599180975 40.103991975428364, -105.15942598421591 40.10399044520795, -105.15942195586052 40.103158119956774, -105.15943048902622 40.10160443093669, -105.1547910443339 40.10160295281706, -105.15479210104625 40.100759911876715, -105.15475703822187 40.09999005930496, -105.15474411361718 40.099532089431825, -105.15475499253671 40.09919504942512, -105.15475540997969 40.09863594701231, -105.15475610632501 40.09770606877903, -105.15475716090556 40.09707495511488, -105.15475889577603 40.09630987935132, -105.15475978043091 40.096128206118195, -105.15476841232726 40.09436209381196, -105.15477594866518 40.09407398207865, -105.15481182971382 40.09390608435718, -105.15491892456382 40.09365110331297, -105.15501992539099 40.09346994805548, -105.15515409115949 40.093303991124515, -105.15531784206338 40.093154044010355, -105.1548679838794 40.09284112289536, -105.15470489389374 40.09279012334013, -105.15453092389943 40.092770112909975, -105.15444299035028 40.09277094765564, -105.1542489372922 40.09276405226741, -105.15415204151131 40.09277007650465, -105.15320697357481 40.092911912802265, -105.15300500152499 40.09291597223615, -105.15280603676786 40.09289094223133, -105.15275711871475 40.092880912312026, -105.1525261515865 40.09275311622527, -105.15242394566049 40.09267896267339, -105.15232188266958 40.09257708391691, -105.15224597789172 40.092462106479466, -105.1521509879569 40.092165066765745, -105.15202200700361 40.09187506125325, -105.15192115091034 40.09174710660227, -105.15179090457409 40.09163498487955, -105.15171609427455 40.09158589547712, -105.1509691325867 40.09129402290613, -105.15058504910466 40.09112513076602, -105.15045507528546 40.09103002878979, -105.15035092510281 40.09091798442525, -105.15029206393665 40.090826116572, -105.15024814633956 40.09067801875981, -105.15022711768182 40.09024888266667, -105.1502290998738 40.08986291678186, -105.15024189316918 40.08973805003863, -105.15026702947037 40.089088890268854, -105.1502730612071 40.08902796527107, -105.15029191660018 40.088905862049394, -105.15043803198166 40.088361934663645, -105.1505388737468 40.08793399243624, -105.15055909164926 40.087755067767525, -105.15054826074254 40.08732532748923, -105.1503301391773 40.08732628912127, -105.15003158620414 40.087322386225345, -105.14971813880092 40.08731828785967, -105.14905413796853 40.08730928858999, -105.14659313865397 40.08730128957986, -105.14430113969432 40.08730228806577, -105.14220813958934 40.08730028957377, -105.14200313915634 40.08730728976931, -105.14098713876481 40.087311289530135, -105.13826313865856 40.08732328982324, -105.13730613866171 40.087324289770656, -105.13490713833464 40.087334289021946, -105.13146917987386 40.08736528014637, -105.13146869204817 40.08736528489368, -105.13150230838892 40.0879120286511, -105.13151230766312 40.08860202899108, -105.13155730932927 40.09073602900505, -105.13156530856897 40.09121302826923, -105.13157130906771 40.092671028447384, -105.13153530898825 40.094416029180145, -105.13154130938224 40.09489902827075, -105.13150330845312 40.09835802848521, -105.13149630910998 40.09849502893818, -105.13147530894588 40.09960702888224, -105.13147430997293 40.09982802847355, -105.13146131028984 40.101711028008395, -105.13146031030627 40.10285102851227, -105.13137831090386 40.106639028065764, -105.13130631156417 40.10894602876141, -105.13127131109465 40.10989302815075, -105.13127330982914 40.11046202797889, -105.13124031109733 40.111400028001526, -105.1312113114617 40.11250802867715, -105.13119730978674 40.11310902852121, -105.13113031171706 40.114313029053996, -105.13105531204309 40.11535402919674, -105.13101831224118 40.116218029523274, -105.13101734868309 40.11641334503174, -105.13101825941496 40.116412620219286, -105.13101818602466 40.116427459928154))</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -3016,7 +3028,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0694111630307 40.16090422372054, -105.0694629539653 40.16092000499503, -105.0705369421375 40.16129000865394, -105.0719189271613 40.16175401236442, -105.0730759142553 40.16213901527696, -105.0739259058449 40.16241901849396, -105.0744968993014 40.16262302002178, -105.0756918859996 40.16302902328239, -105.0775498655427 40.16357702807103, -105.0787978532788 40.16380003091128, -105.0795948459216 40.16388103180415, -105.0802848402826 40.16392203294821, -105.0807888352324 40.1639220337433, -105.0813998304982 40.16392203444205, -105.0829128177578 40.16392203457659, -105.083609519032 40.16392308127849, -105.0881761464068 40.16392102833853, -105.0881693626968 40.16382478228903, -105.0881650625537 40.16356494168014, -105.0881668740553 40.16350208512876, -105.0881648387267 40.16306998948579, -105.0881598089886 40.16280928973737, -105.0881623938254 40.1623954782369, -105.0886809584908 40.16239212456986, -105.089468094328 40.16239711982808, -105.0909838252546 40.16238410086513, -105.0917190936679 40.16238697525812, -105.0925199158311 40.16237689791628, -105.0931070011848 40.1623778683723, -105.0931070642517 40.16237164155648, -105.0931129997678 40.16178000016573, -105.0931149989175 40.16163199930823, -105.0931069993422 40.16131200006891, -105.0931069998108 40.1613119217147, -105.0930749990154 40.16110699945172, -105.0930749994591 40.16106100006206, -105.093074999123 40.16093800027746, -105.0930969990843 40.16066999982127, -105.0930949991611 40.1604880000312, -105.0931024819559 40.16045158549526, -105.0931099998072 40.16041499996014, -105.0931679955306 40.16027501197318, -105.0933151831979 40.16027514992445, -105.0941529994326 40.16027600012808, -105.0942474912358 40.16027599866759, -105.0943463028096 40.16027599968295, -105.0944589999225 40.16027599890212, -105.0946219991399 40.16027500002095, -105.0948714164467 40.16027221347903, -105.0951589994661 40.16026899899504, -105.095906860969 40.16024372245906, -105.0960168884854 40.16023999747829, -105.0960170000153 40.16023999516622, -105.0960982895062 40.16023918860394, -105.0967180002406 40.1602330001241, -105.0998739874729 40.16022399957189, -105.1010630001934 40.16022199906198, -105.1010699280626 40.16022203558438, -105.1010700959203 40.16022203616376, -105.101072318054 40.16022203122495, -105.1024143180025 40.16022903062637, -105.1025380465539 40.16023089182191, -105.1025308525397 40.15833903828675, -105.1025300254877 40.15811310850285, -105.1025330984857 40.15783201429117, -105.1025348528603 40.15734804860777, -105.1025273195647 40.15708198833205, -105.1025349607258 40.15616598225654, -105.1025389095845 40.15597987361276, -105.1025408535364 40.15589203525391, -105.1025510586691 40.15536993918337, -105.1025500235287 40.15524091410313, -105.1025509828481 40.15513797217847, -105.1025491274585 40.15484313600666, -105.102548967894 40.15474787901242, -105.1025521426915 40.1535918999715, -105.1025509038905 40.15331408529797, -105.1025269148411 40.15245998279159, -105.1025241155214 40.15238805053694, -105.1025230471926 40.15232600608753, -105.1025218377547 40.15228811819185, -105.1025211214181 40.15222689904034, -105.1025180890108 40.15145988949109, -105.1025050362951 40.14879511117771, -105.1025010726383 40.14800394189388, -105.1025001051187 40.14700606985371, -105.102502929779 40.14639994742078, -105.1025001325828 40.14589894492562, -105.1024981568708 40.14513495817679, -105.1023439541302 40.14513991701689, -105.1022109134351 40.14513506664392, -105.1015230045419 40.14514010867565, -105.0990280016897 40.14515976042167, -105.0990280139276 40.14516186616938, -105.0989499689927 40.14516302193299, -105.0986779613497 40.14516704726665, -105.098092228735 40.14516666229105, -105.097606796941 40.14516634178373, -105.0968736807809 40.14517072225551, -105.0965041099488 40.1451729276964, -105.0930050175926 40.14519860354697, -105.0930001352231 40.14519863948767, -105.0929935040886 40.14519869358574, -105.093029978758 40.14305370096206, -105.0930299956357 40.14304440276907, -105.0930284442628 40.14304439100033, -105.093045987539 40.14181003041903, -105.0930491917959 40.14158465180761, -105.093049477186 40.14156459725995, -105.0930791148364 40.13795822815074, -105.0981402379528 40.13794363574316, -105.0982528459573 40.13794331765722, -105.0996625321596 40.13792759514475, -105.0997720158061 40.1379263713126, -105.1009877654586 40.13791166467198, -105.1021479210987 40.13789982771293, -105.1021475120736 40.13792643765014, -105.1023785623185 40.13790392707252, -105.1024538827684 40.13544014837245, -105.102489941688 40.13437620457013, -105.1024959974291 40.13413313590875, -105.1024960005596 40.13413300172339, -105.100395113552 40.13418487869186, -105.0960260840791 40.13426087793793, -105.094924071347 40.13427687757695, -105.0944350199997 40.134278878763, -105.0944050049201 40.13427896522876, -105.0940880142722 40.13427987836944, -105.0932020045514 40.13427787787717, -105.0930212415033 40.13428686643668, -105.0927490541487 40.13428987731798, -105.0920430472559 40.13429687652557, -105.0905391301851 40.13433687298826, -105.0899250393446 40.13434187663415, -105.0887041365292 40.13437587163286, -105.0879403055598 40.13442385884984, -105.0846750309919 40.13445787330612, -105.0832755753651 40.13446682896835, -105.0831630652203 40.13445687173049, -105.0799831751011 40.13457186759719, -105.077656234461 40.13468386293215, -105.0762711360049 40.13472286783558, -105.0745131984398 40.13479486487819, -105.0742413915201 40.13481684621029, -105.0742440761428 40.13984499868648, -105.0737770801883 40.13984989482434, -105.0728341139191 40.13987189343821, -105.0652349113323 40.13998458559128, -105.0651172543858 40.13995483397098, -105.0650172912994 40.139897965545, -105.064944699213 40.13982145163131, -105.0649318121612 40.13979936609553, -105.0649223983107 40.13978009284535, -105.0649012584268 40.13969700518675, -105.0649496601588 40.13851303311695, -105.0649247890964 40.13837338792121, -105.0648822428967 40.13829711858007, -105.0647902892207 40.13821288423826, -105.0647026837377 40.13816640688852, -105.0646163718572 40.1381387740668, -105.0644970736709 40.13812287925889, -105.0630970281733 40.13814387787887, -105.0623920537045 40.13814787912667, -105.0570841697421 40.13820687462603, -105.055393108424 40.1382658753683, -105.0553734627153 40.13826344007112, -105.0553735349496 40.13831543018563, -105.0553581629 40.14497257258469, -105.0553568117257 40.14555727121959, -105.0553554845123 40.14607040548283, -105.055348545721 40.14875222591935, -105.0553462127781 40.14965381974552, -105.055340783666 40.15175194196998, -105.0553386499967 40.15257631307534, -105.0553379947871 40.15282923958088, -105.0553382659259 40.15546513428482, -105.0553382920939 40.15571473362403, -105.0553383718875 40.15647913976149, -105.0553387559006 40.1601157733564, -105.0553382965441 40.16019791122213, -105.0553377713311 40.16028796999728, -105.0580710513005 40.16025799056519, -105.0606010313516 40.16022699272562, -105.062539016009 40.16009099355082, -105.0634333444827 40.15986251985857, -105.064296309749 40.15959008850385, -105.064919505624 40.15935175545492, -105.0662970046367 40.1588843247345, -105.066765552507 40.15964313063317, -105.067322977026 40.16013699897744, -105.0678959694674 40.1604240008717, -105.0687409608614 40.16070000328342, -105.0694111630307 40.16090422372054))</t>
+          <t>POLYGON ((-105.06941116303074 40.160904223720536, -105.06946295396526 40.16092000499503, -105.07053694213745 40.16129000865394, -105.0719189271613 40.16175401236442, -105.07307591425534 40.16213901527696, -105.07392590584493 40.16241901849396, -105.07449689930137 40.16262302002178, -105.07569188599962 40.16302902328239, -105.07754986554265 40.16357702807103, -105.07879785327876 40.16380003091128, -105.07959484592165 40.16388103180415, -105.08028484028256 40.16392203294821, -105.08078883523244 40.1639220337433, -105.08139983049817 40.16392203444205, -105.08291281775779 40.16392203457659, -105.083609519032 40.16392308127849, -105.08817614640682 40.16392102833853, -105.08816936269676 40.16382478228903, -105.08816506255374 40.163564941680136, -105.08816687405532 40.16350208512876, -105.08816483872667 40.16306998948579, -105.08815980898855 40.162809289737375, -105.08816239382541 40.162395478236895, -105.08868095849083 40.162392124569855, -105.08946809432798 40.16239711982808, -105.09098382525458 40.162384100865125, -105.09171909366789 40.16238697525812, -105.09251991583112 40.16237689791628, -105.09310700118482 40.162377868372296, -105.09310706425171 40.162371641556476, -105.09311299976775 40.16178000016573, -105.0931149989175 40.16163199930823, -105.09310699934221 40.16131200006891, -105.09310699981081 40.1613119217147, -105.09307499901536 40.16110699945172, -105.0930749994591 40.16106100006206, -105.09307499912298 40.16093800027746, -105.09309699908425 40.16066999982127, -105.09309499916112 40.1604880000312, -105.09310248195592 40.16045158549526, -105.09310999980721 40.16041499996014, -105.0931679955306 40.16027501197318, -105.09331518319786 40.16027514992445, -105.09415299943264 40.16027600012808, -105.09424749123583 40.16027599866759, -105.09434630280961 40.16027599968295, -105.09445899992254 40.16027599890212, -105.09462199913989 40.16027500002095, -105.09487141644672 40.16027221347903, -105.09515899946608 40.160268998995036, -105.09590686096895 40.16024372245906, -105.09601688848535 40.16023999747829, -105.09601700001525 40.16023999516622, -105.0960982895062 40.16023918860394, -105.09671800024059 40.1602330001241, -105.09987398747286 40.16022399957189, -105.10106300019336 40.16022199906198, -105.10106992806263 40.160222035584376, -105.10107009592029 40.16022203616376, -105.10107231805398 40.16022203122495, -105.10241431800253 40.16022903062637, -105.10253804655386 40.16023089182191, -105.10253085253969 40.158339038286755, -105.10253002548765 40.158113108502846, -105.10253309848568 40.157832014291166, -105.10253485286032 40.15734804860777, -105.10252731956473 40.15708198833205, -105.10253496072579 40.15616598225654, -105.10253890958454 40.15597987361276, -105.10254085353641 40.155892035253906, -105.10255105866906 40.155369939183366, -105.10255002352865 40.15524091410313, -105.10255098284809 40.15513797217847, -105.10254912745849 40.15484313600666, -105.10254896789401 40.15474787901242, -105.1025521426915 40.153591899971495, -105.10255090389055 40.15331408529797, -105.10252691484109 40.15245998279159, -105.1025241155214 40.15238805053694, -105.1025230471926 40.152326006087534, -105.10252183775468 40.152288118191855, -105.10252112141806 40.15222689904034, -105.10251808901076 40.151459889491086, -105.1025050362951 40.148795111177705, -105.10250107263828 40.14800394189388, -105.10250010511871 40.14700606985371, -105.10250292977904 40.146399947420775, -105.10250013258276 40.14589894492562, -105.10249815687077 40.14513495817679, -105.1023439541302 40.14513991701689, -105.10221091343509 40.145135066643924, -105.10152300454192 40.145140108675655, -105.09902800168969 40.14515976042167, -105.09902801392755 40.14516186616938, -105.0989499689927 40.145163021932994, -105.09867796134972 40.145167047266646, -105.09809222873498 40.14516666229105, -105.09760679694095 40.14516634178373, -105.09687368078094 40.145170722255514, -105.0965041099488 40.1451729276964, -105.09300501759257 40.145198603546966, -105.09300013522305 40.14519863948767, -105.09299350408857 40.14519869358574, -105.09302997875801 40.143053700962064, -105.09302999563572 40.14304440276907, -105.09302844426283 40.14304439100033, -105.09304598753899 40.14181003041903, -105.09304919179591 40.14158465180761, -105.09304947718599 40.14156459725995, -105.09307911483643 40.13795822815074, -105.09814023795285 40.137943635743156, -105.09825284595735 40.137943317657225, -105.09966253215963 40.137927595144745, -105.09977201580614 40.137926371312595, -105.10098776545858 40.13791166467198, -105.10214792109869 40.13789982771293, -105.10214751207361 40.13792643765014, -105.10237856231855 40.13790392707252, -105.10245388276844 40.13544014837245, -105.10248994168802 40.13437620457013, -105.10249599742907 40.13413313590875, -105.10249600055958 40.13413300172339, -105.10039511355204 40.13418487869186, -105.09602608407914 40.134260877937926, -105.09492407134704 40.13427687757695, -105.09443501999968 40.134278878763, -105.09440500492015 40.13427896522876, -105.09408801427219 40.13427987836944, -105.09320200455142 40.134277877877174, -105.0930212415033 40.13428686643668, -105.09274905414868 40.134289877317975, -105.0920430472559 40.13429687652557, -105.09053913018508 40.13433687298826, -105.08992503934465 40.134341876634146, -105.0887041365292 40.134375871632855, -105.0879403055598 40.134423858849836, -105.0846750309919 40.13445787330612, -105.08327557536505 40.13446682896835, -105.08316306522026 40.13445687173049, -105.07998317510113 40.13457186759719, -105.07765623446096 40.13468386293215, -105.07627113600489 40.134722867835585, -105.0745131984398 40.13479486487819, -105.07424139152015 40.13481684621029, -105.07424407614279 40.13984499868648, -105.07377708018825 40.139849894824344, -105.07283411391913 40.13987189343821, -105.06523491133225 40.13998458559128, -105.06511725438575 40.139954833970975, -105.06501729129936 40.139897965545, -105.06494469921302 40.13982145163131, -105.06493181216116 40.13979936609553, -105.06492239831067 40.13978009284535, -105.06490125842684 40.139697005186754, -105.06494966015882 40.13851303311695, -105.06492478909641 40.138373387921206, -105.06488224289666 40.13829711858007, -105.06479028922067 40.138212884238264, -105.06470268373766 40.138166406888516, -105.06461637185723 40.1381387740668, -105.06449707367086 40.13812287925889, -105.06309702817332 40.13814387787887, -105.06239205370451 40.13814787912667, -105.05708416974208 40.13820687462603, -105.05539310842397 40.138265875368305, -105.05537346271525 40.13826344007112, -105.05537353494962 40.13831543018563, -105.05535816290005 40.14497257258469, -105.05535681172572 40.145557271219594, -105.0553554845123 40.14607040548283, -105.05534854572102 40.148752225919345, -105.05534621277815 40.149653819745524, -105.055340783666 40.15175194196998, -105.05533864999673 40.15257631307534, -105.05533799478707 40.15282923958088, -105.05533826592585 40.15546513428482, -105.05533829209388 40.15571473362403, -105.05533837188753 40.15647913976149, -105.05533875590058 40.1601157733564, -105.05533829654408 40.160197911222134, -105.05533777133105 40.160287969997285, -105.05807105130047 40.16025799056519, -105.06060103135162 40.16022699272562, -105.06253901600904 40.16009099355082, -105.06343334448275 40.15986251985857, -105.06429630974895 40.15959008850385, -105.06491950562399 40.15935175545492, -105.06629700463674 40.1588843247345, -105.06676555250696 40.15964313063317, -105.06732297702601 40.160136998977435, -105.0678959694674 40.1604240008717, -105.0687409608614 40.160700003283424, -105.06941116303074 40.160904223720536))</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -3058,7 +3070,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1023785623185 40.13790392707252, -105.1021475120736 40.13792643765014, -105.1021479210987 40.13789982771293, -105.1009877654586 40.13791166467198, -105.0997720158061 40.1379263713126, -105.0996625321596 40.13792759514475, -105.0982528459573 40.13794331765722, -105.0981402379528 40.13794363574316, -105.0930791148364 40.13795822815074, -105.093049477186 40.14156459725995, -105.0930491917959 40.14158465180761, -105.093045987539 40.14181003041903, -105.0930284442628 40.14304439100033, -105.0930299956357 40.14304440276907, -105.093029978758 40.14305370096206, -105.0929935040886 40.14519869358574, -105.0930001352231 40.14519863948767, -105.0930050175926 40.14519860354697, -105.0965041099488 40.1451729276964, -105.0968736807809 40.14517072225551, -105.097606796941 40.14516634178373, -105.098092228735 40.14516666229105, -105.0986779613497 40.14516704726665, -105.0989499689927 40.14516302193299, -105.0990280139276 40.14516186616938, -105.0990280016897 40.14515976042167, -105.1015230045419 40.14514010867565, -105.1022109134351 40.14513506664392, -105.1023439541302 40.14513991701689, -105.1024981568708 40.14513495817679, -105.1024978851669 40.14505891499658, -105.1024858520981 40.14350593317315, -105.1024841527631 40.14275594762682, -105.1024810405372 40.14212509703757, -105.1024760872819 40.14162600789496, -105.1024748909418 40.14109591255694, -105.1024740861529 40.1410500642974, -105.10248484046 40.14080111460713, -105.1024840663346 40.14050490896979, -105.1024620834747 40.13998187873563, -105.1023858746459 40.13876111274642, -105.1023738441738 40.13849396630643, -105.1023699939893 40.13826519835369, -105.1023689318634 40.13823288407544, -105.1023752778215 40.13801137617609, -105.1023785623185 40.13790392707252))</t>
+          <t>POLYGON ((-105.10237856231855 40.13790392707252, -105.10214751207361 40.13792643765014, -105.10214792109869 40.13789982771293, -105.10098776545858 40.13791166467198, -105.09977201580614 40.137926371312595, -105.09966253215963 40.137927595144745, -105.09825284595735 40.137943317657225, -105.09814023795285 40.137943635743156, -105.09307911483643 40.13795822815074, -105.09304947718599 40.14156459725995, -105.09304919179591 40.14158465180761, -105.09304598753899 40.14181003041903, -105.09302844426283 40.14304439100033, -105.09302999563572 40.14304440276907, -105.09302997875801 40.143053700962064, -105.09299350408857 40.14519869358574, -105.09300013522305 40.14519863948767, -105.09300501759257 40.145198603546966, -105.0965041099488 40.1451729276964, -105.09687368078094 40.145170722255514, -105.09760679694095 40.14516634178373, -105.09809222873498 40.14516666229105, -105.09867796134972 40.145167047266646, -105.0989499689927 40.145163021932994, -105.09902801392755 40.14516186616938, -105.09902800168969 40.14515976042167, -105.10152300454192 40.145140108675655, -105.10221091343509 40.145135066643924, -105.1023439541302 40.14513991701689, -105.10249815687077 40.14513495817679, -105.1024978851669 40.14505891499658, -105.10248585209811 40.14350593317315, -105.10248415276305 40.14275594762682, -105.10248104053717 40.14212509703757, -105.10247608728189 40.14162600789496, -105.1024748909418 40.14109591255694, -105.1024740861529 40.1410500642974, -105.10248484046004 40.14080111460713, -105.10248406633464 40.14050490896979, -105.10246208347475 40.13998187873563, -105.10238587464595 40.138761112746415, -105.10237384417375 40.13849396630643, -105.10236999398934 40.138265198353686, -105.10236893186335 40.13823288407544, -105.10237527782145 40.13801137617609, -105.10237856231855 40.13790392707252))</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -3100,7 +3112,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1024981568708 40.14513495817679, -105.1025001325828 40.14589894492562, -105.102502929779 40.14639994742078, -105.1025001051187 40.14700606985371, -105.1027896623851 40.14680212506761, -105.103097277509 40.14655653548774, -105.1032734493735 40.14644982251246, -105.1032931256744 40.14613706866657, -105.1033239976599 40.14594537180952, -105.1033781591728 40.1457986582683, -105.1035694298707 40.1456584188717, -105.1037377706737 40.14553499119413, -105.1041052205383 40.14536990728234, -105.1042286659116 40.14533691899432, -105.1042410057594 40.14520402266659, -105.1043439248778 40.14520086261507, -105.1044871661829 40.14517390139294, -105.1046167067099 40.14513060227208, -105.1047560762105 40.1450840177562, -105.1048608113467 40.14504900859458, -105.1049990293322 40.14500280892646, -105.1051659901088 40.14494700107727, -105.1053782970942 40.1448743635278, -105.1056838215419 40.14478594833889, -105.1058998209801 40.14470394763508, -105.1060476780228 40.14465520375037, -105.1067939256991 40.14439089125828, -105.1070510249035 40.14428305730459, -105.1071470935328 40.14424797156938, -105.1079030226773 40.14392111893775, -105.1082699579036 40.1437469469786, -105.108417879155 40.14365191711192, -105.1084469854705 40.14362895567095, -105.109161980491 40.14307795071951, -105.1095840635151 40.14276697772822, -105.1102731505028 40.14230207715557, -105.1103920126454 40.14222094634746, -105.11066983058 40.14205305535067, -105.1108640824602 40.14192386303387, -105.1110718385429 40.14181008893544, -105.11129310243 40.1417109098067, -105.1113486218073 40.14168839314541, -105.111914063396 40.14145906879407, -105.1118408160296 40.14135893235024, -105.1118008162135 40.14127193177784, -105.1117835285537 40.14120268263837, -105.1117628186357 40.1411279316719, -105.1117588196545 40.14101493067353, -105.1117749312176 40.14089309708596, -105.1118561705442 40.14075995496132, -105.1119998637142 40.14065774078199, -105.1125598222135 40.14028292737444, -105.1127738473876 40.14009513471218, -105.1128369225726 40.13988506646543, -105.112821162624 40.13976312771756, -105.1127638668591 40.13964901145435, -105.1125981540443 40.13947907904089, -105.1119741665393 40.13888512691707, -105.1123358415979 40.13859691635773, -105.1129148435082 40.1381329148556, -105.1132657026752 40.13781976323562, -105.1131408606045 40.13782501213419, -105.1119888677549 40.13787495353632, -105.1114349101069 40.13792387823695, -105.1108038685421 40.13794206824723, -105.1102219402103 40.13794092967218, -105.1091628387754 40.1379458619553, -105.108666034557 40.13794500347248, -105.108056921774 40.13794403750942, -105.1075200236577 40.13794907779817, -105.1067370455531 40.13795410143008, -105.1062229991387 40.13796607638333, -105.1060709416614 40.13797406821882, -105.1058158452907 40.13798692398434, -105.1056139162883 40.13800486109454, -105.105411106619 40.13802287680309, -105.1047938387192 40.13807100314683, -105.1023699939893 40.13826519835369, -105.1023738441738 40.13849396630643, -105.1023858746459 40.13876111274642, -105.1024620834747 40.13998187873563, -105.1024840663346 40.14050490896979, -105.10248484046 40.14080111460713, -105.1024740861529 40.1410500642974, -105.1024748909418 40.14109591255694, -105.1024760872819 40.14162600789496, -105.1024810405372 40.14212509703757, -105.1024841527631 40.14275594762682, -105.1024858520981 40.14350593317315, -105.1024978851669 40.14505891499658, -105.1024981568708 40.14513495817679))</t>
+          <t>POLYGON ((-105.10249815687077 40.14513495817679, -105.10250013258276 40.14589894492562, -105.10250292977904 40.146399947420775, -105.10250010511871 40.14700606985371, -105.10278966238515 40.14680212506761, -105.10309727750897 40.14655653548774, -105.1032734493735 40.14644982251246, -105.10329312567441 40.14613706866657, -105.10332399765994 40.14594537180952, -105.10337815917278 40.145798658268305, -105.10356942987075 40.145658418871704, -105.10373777067375 40.14553499119413, -105.1041052205383 40.145369907282344, -105.10422866591159 40.14533691899432, -105.10424100575939 40.14520402266659, -105.10434392487782 40.14520086261507, -105.10448716618295 40.145173901392944, -105.10461670670995 40.14513060227208, -105.10475607621049 40.1450840177562, -105.10486081134673 40.145049008594576, -105.10499902933219 40.145002808926456, -105.10516599010879 40.14494700107727, -105.10537829709425 40.1448743635278, -105.10568382154187 40.14478594833889, -105.10589982098013 40.14470394763508, -105.10604767802278 40.144655203750375, -105.10679392569911 40.144390891258276, -105.10705102490346 40.14428305730459, -105.10714709353277 40.144247971569385, -105.1079030226773 40.14392111893775, -105.10826995790363 40.1437469469786, -105.108417879155 40.143651917111924, -105.10844698547054 40.14362895567095, -105.10916198049098 40.14307795071951, -105.10958406351513 40.14276697772822, -105.11027315050282 40.14230207715557, -105.11039201264539 40.142220946347464, -105.11066983058001 40.142053055350665, -105.11086408246017 40.141923863033874, -105.11107183854291 40.141810088935436, -105.11129310242995 40.141710909806704, -105.11134862180728 40.14168839314541, -105.11191406339604 40.14145906879407, -105.11184081602963 40.141358932350236, -105.11180081621352 40.14127193177784, -105.11178352855369 40.14120268263837, -105.1117628186357 40.141127931671896, -105.11175881965453 40.141014930673535, -105.11177493121764 40.14089309708596, -105.11185617054421 40.14075995496132, -105.11199986371425 40.14065774078199, -105.1125598222135 40.14028292737444, -105.11277384738763 40.14009513471218, -105.11283692257261 40.13988506646543, -105.11282116262402 40.139763127717565, -105.11276386685908 40.139649011454345, -105.11259815404428 40.13947907904089, -105.11197416653927 40.13888512691707, -105.1123358415979 40.13859691635773, -105.11291484350821 40.138132914855596, -105.11326570267524 40.13781976323562, -105.11314086060446 40.13782501213419, -105.11198886775489 40.13787495353632, -105.11143491010694 40.13792387823695, -105.1108038685421 40.13794206824723, -105.11022194021031 40.137940929672176, -105.10916283877545 40.1379458619553, -105.10866603455696 40.13794500347248, -105.10805692177395 40.13794403750942, -105.1075200236577 40.13794907779817, -105.10673704555313 40.137954101430076, -105.10622299913865 40.13796607638333, -105.10607094166144 40.137974068218824, -105.10581584529066 40.13798692398434, -105.10561391628828 40.13800486109454, -105.105411106619 40.13802287680309, -105.1047938387192 40.13807100314683, -105.10236999398934 40.138265198353686, -105.10237384417375 40.13849396630643, -105.10238587464595 40.138761112746415, -105.10246208347475 40.13998187873563, -105.10248406633464 40.14050490896979, -105.10248484046004 40.14080111460713, -105.1024740861529 40.1410500642974, -105.1024748909418 40.14109591255694, -105.10247608728189 40.14162600789496, -105.10248104053717 40.14212509703757, -105.10248415276305 40.14275594762682, -105.10248585209811 40.14350593317315, -105.1024978851669 40.14505891499658, -105.10249815687077 40.14513495817679))</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -3142,7 +3154,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1093585944797 40.13263279385802, -105.1093205768746 40.13268270513078, -105.1092647735506 40.13273806278027, -105.1092018368701 40.13278836166751, -105.1091328252846 40.13283461228306, -105.1090587413161 40.13287489693305, -105.1089796055062 40.13291013523579, -105.1088964020049 40.13293936322003, -105.1087220040101 40.13297863883014, -105.1086315304633 40.13298881317525, -105.1085152097078 40.13299386796137, -105.1055770144187 40.13300287849541, -105.1055759857053 40.13312511863367, -105.1055759631424 40.13312799972009, -105.1044939964566 40.13312987928641, -105.1041803847008 40.13315484466681, -105.1025130798614 40.13316287747433, -105.1025130341002 40.13316287731691, -105.1024960005596 40.13413300172339, -105.1024959974291 40.13413313590875, -105.102489941688 40.13437620457013, -105.1024538827684 40.13544014837245, -105.1023785623185 40.13790392707252, -105.1023752778215 40.13801137617609, -105.1023689318634 40.13823288407544, -105.1023699939893 40.13826519835369, -105.1047938387192 40.13807100314683, -105.105411106619 40.13802287680309, -105.1056139162883 40.13800486109454, -105.1058158452907 40.13798692398434, -105.1060709416614 40.13797406821882, -105.1062229991387 40.13796607638333, -105.1067370455531 40.13795410143008, -105.1075200236577 40.13794907779817, -105.108056921774 40.13794403750942, -105.108666034557 40.13794500347248, -105.1091628387754 40.1379458619553, -105.1102219402103 40.13794092967218, -105.1108038685421 40.13794206824723, -105.1114349101069 40.13792387823695, -105.1119888677549 40.13787495353632, -105.1131408606045 40.13782501213419, -105.1132657026752 40.13781976323562, -105.1133909369859 40.13781404447786, -105.1140931460601 40.13779690126499, -105.1143270696734 40.13779603509296, -105.1151238749654 40.13781186951335, -105.1153910575788 40.13781193606512, -105.1163031792091 40.13780206622556, -105.1172280717856 40.13781089914383, -105.1181829755937 40.13782586265843, -105.1184898474704 40.13782797427399, -105.119842842414 40.13784286624009, -105.1201221062495 40.1378569612092, -105.1204010352615 40.13786693756008, -105.1206799823645 40.13787389253752, -105.1214760632031 40.13789187653235, -105.1214610678309 40.13390007780051, -105.1214538947259 40.13229605177493, -105.1214388421045 40.13069787537972, -105.1214287020073 40.13069788718315, -105.1196690057948 40.13069987439082, -105.1190837455796 40.13069590702754, -105.1190789667365 40.13069587415787, -105.1190737172402 40.13069586675535, -105.1167582823744 40.13069277850736, -105.1167491843696 40.13166446387874, -105.1155191846595 40.13164146329787, -105.1152464520673 40.13162554514241, -105.1150500767831 40.13162358771766, -105.1146592764502 40.13161717097666, -105.1142691989206 40.13161076343259, -105.1138787565874 40.13160434794801, -105.1134884683498 40.13159766957149, -105.1130752163228 40.13171876581113, -105.1126460873139 40.13184417366759, -105.1123102126654 40.13194232418207, -105.1122248807698 40.13196726034626, -105.1122250359624 40.13198450641528, -105.1121931826917 40.1319974642461, -105.1119871837674 40.13205846401782, -105.1119826842302 40.13221195301501, -105.1119769681384 40.13240697386129, -105.1119701840193 40.13263846362696, -105.1115905511339 40.13264209640875, -105.111021497991 40.13263928746463, -105.1109074261621 40.13263860431368, -105.110591834876 40.13263671418122, -105.1103350195741 40.13263517546018, -105.1098582235746 40.1326323161728, -105.1096519310758 40.13263086368207, -105.1093701834689 40.13263246468068, -105.1093585944797 40.13263279385802))</t>
+          <t>POLYGON ((-105.1093585944797 40.13263279385802, -105.1093205768746 40.132682705130776, -105.10926477355065 40.13273806278027, -105.10920183687014 40.13278836166751, -105.10913282528465 40.13283461228306, -105.10905874131613 40.13287489693305, -105.10897960550622 40.13291013523579, -105.10889640200492 40.132939363220025, -105.10872200401013 40.13297863883014, -105.10863153046331 40.13298881317525, -105.10851520970782 40.13299386796137, -105.10557701441869 40.13300287849541, -105.10557598570526 40.13312511863367, -105.10557596314243 40.13312799972009, -105.10449399645664 40.133129879286415, -105.10418038470081 40.133154844666805, -105.10251307986141 40.133162877474334, -105.10251303410024 40.133162877316906, -105.10249600055958 40.13413300172339, -105.10249599742907 40.13413313590875, -105.10248994168802 40.13437620457013, -105.10245388276844 40.13544014837245, -105.10237856231855 40.13790392707252, -105.10237527782145 40.13801137617609, -105.10236893186335 40.13823288407544, -105.10236999398934 40.138265198353686, -105.1047938387192 40.13807100314683, -105.105411106619 40.13802287680309, -105.10561391628828 40.13800486109454, -105.10581584529066 40.13798692398434, -105.10607094166144 40.137974068218824, -105.10622299913865 40.13796607638333, -105.10673704555313 40.137954101430076, -105.1075200236577 40.13794907779817, -105.10805692177395 40.13794403750942, -105.10866603455696 40.13794500347248, -105.10916283877545 40.1379458619553, -105.11022194021031 40.137940929672176, -105.1108038685421 40.13794206824723, -105.11143491010694 40.13792387823695, -105.11198886775489 40.13787495353632, -105.11314086060446 40.13782501213419, -105.11326570267524 40.13781976323562, -105.1133909369859 40.137814044477864, -105.11409314606009 40.13779690126499, -105.11432706967338 40.13779603509296, -105.11512387496536 40.13781186951335, -105.11539105757885 40.13781193606512, -105.11630317920908 40.13780206622556, -105.11722807178558 40.13781089914383, -105.1181829755937 40.13782586265843, -105.11848984747044 40.13782797427399, -105.11984284241402 40.137842866240085, -105.12012210624953 40.1378569612092, -105.12040103526145 40.13786693756008, -105.12067998236445 40.13787389253752, -105.12147606320309 40.13789187653235, -105.12146106783091 40.13390007780051, -105.12145389472587 40.13229605177493, -105.12143884210452 40.130697875379724, -105.12142870200725 40.13069788718315, -105.11966900579479 40.13069987439082, -105.1190837455796 40.130695907027544, -105.11907896673645 40.130695874157865, -105.11907371724016 40.130695866755346, -105.11675828237443 40.13069277850736, -105.11674918436962 40.131664463878735, -105.11551918465949 40.13164146329787, -105.11524645206731 40.131625545142406, -105.1150500767831 40.131623587717655, -105.11465927645017 40.13161717097666, -105.11426919892061 40.13161076343259, -105.11387875658743 40.13160434794801, -105.11348846834984 40.13159766957149, -105.11307521632277 40.13171876581113, -105.11264608731393 40.13184417366759, -105.11231021266543 40.13194232418207, -105.11222488076984 40.13196726034626, -105.11222503596242 40.13198450641528, -105.1121931826917 40.1319974642461, -105.11198718376741 40.13205846401782, -105.11198268423017 40.13221195301501, -105.11197696813835 40.132406973861286, -105.11197018401934 40.13263846362696, -105.11159055113394 40.13264209640875, -105.11102149799099 40.13263928746463, -105.11090742616213 40.13263860431368, -105.11059183487598 40.132636714181224, -105.11033501957412 40.13263517546018, -105.10985822357458 40.132632316172796, -105.10965193107583 40.13263086368207, -105.10937018346885 40.13263246468068, -105.1093585944797 40.13263279385802))</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -3184,7 +3196,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1214760632031 40.13789187653235, -105.1308880005306 40.13793399959673, -105.1308880033281 40.13793413290086, -105.1308973195819 40.13793389877544, -105.1309083153879 40.13760103000428, -105.1309613147293 40.13428302934808, -105.1309633151163 40.13416902954575, -105.1309663158803 40.13407590265542, -105.1309568622919 40.13407299670184, -105.1309708325789 40.13358999631841, -105.1309879188726 40.13259022536034, -105.130988858237 40.13253599608295, -105.1310003956401 40.13199844572109, -105.1310098430939 40.13155699817882, -105.131019817435 40.13074388165322, -105.1308018207651 40.13073588184478, -105.129739962766 40.13072788110647, -105.1295199780874 40.13072688132058, -105.125637981124 40.13071087844324, -105.1214389852497 40.1306978758488, -105.1214388421045 40.13069787537972, -105.1214538947259 40.13229605177493, -105.1214610678309 40.13390007780051, -105.1214760632031 40.13789187653235))</t>
+          <t>POLYGON ((-105.12147606320309 40.13789187653235, -105.13088800053063 40.13793399959673, -105.13088800332805 40.13793413290086, -105.13089731958193 40.137933898775444, -105.13090831538794 40.137601030004284, -105.1309613147293 40.13428302934808, -105.13096331511632 40.13416902954575, -105.13096631588034 40.13407590265542, -105.13095686229188 40.13407299670184, -105.13097083257887 40.133589996318406, -105.13098791887256 40.13259022536034, -105.13098885823698 40.13253599608295, -105.13100039564006 40.131998445721095, -105.13100984309389 40.13155699817882, -105.13101981743496 40.130743881653224, -105.13080182076511 40.13073588184478, -105.12973996276604 40.13072788110647, -105.12951997808737 40.130726881320584, -105.12563798112399 40.13071087844324, -105.12143898524974 40.1306978758488, -105.12143884210452 40.130697875379724, -105.12145389472587 40.13229605177493, -105.12146106783091 40.13390007780051, -105.12147606320309 40.13789187653235))</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -3226,7 +3238,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1307838281008 40.14408406823397, -105.1342608923332 40.14412010763965, -105.1364291795246 40.14414397092094, -105.1403029875258 40.14417201661489, -105.1403039064428 40.14487807514858, -105.1402998507262 40.14524260909443, -105.1409069457254 40.14524570513932, -105.142750445879 40.14525141953902, -105.1437970848807 40.14525465077416, -105.1438027736181 40.14518642667634, -105.1438416939682 40.14432211683176, -105.1438437148945 40.14411087928234, -105.1437948536189 40.14403344277093, -105.1438040968366 40.14334059201494, -105.1447821331934 40.1432909504777, -105.1465770584305 40.14329508206774, -105.1476290272116 40.14323186273604, -105.1483019035963 40.14322403006873, -105.1495319555793 40.14324012078783, -105.1498348825798 40.14324558926504, -105.1498349038207 40.1432448823255, -105.1498180030151 40.14312294543797, -105.1498050538428 40.14299800157078, -105.1497938776427 40.14287608292592, -105.1497859249596 40.14275307526516, -105.1497801255132 40.1426289762457, -105.149776114543 40.14250488264477, -105.1497759486375 40.14225891591448, -105.149786951589 40.14165007201457, -105.1497978801225 40.14042988002099, -105.1497999356095 40.14023909780055, -105.1498010231064 40.13981909107122, -105.1498061257537 40.13889700636557, -105.149807177543 40.13862304222842, -105.1498081394624 40.13843609968689, -105.1498098482598 40.13824311969565, -105.149815764785 40.13794141607789, -105.1498199786094 40.13745611129382, -105.1498198856968 40.13733504933415, -105.1498129742711 40.13714890698322, -105.149814008592 40.13666987899488, -105.1498249439201 40.1360739361236, -105.1498261476252 40.13556196666508, -105.1498528474846 40.13512021381311, -105.1498600254167 40.134747029857, -105.1498670034918 40.13450300648549, -105.1498685752776 40.13448395904759, -105.1498753453663 40.13440193369182, -105.1498796782463 40.13406899981911, -105.1496318083555 40.13407168791918, -105.1455886884994 40.1340649989241, -105.1455887080084 40.13376199738765, -105.1456168014993 40.12884799589443, -105.1456487281823 40.12675200170747, -105.1456423360221 40.12643537867292, -105.1456327957312 40.12596286157071, -105.1451267445326 40.1263892194086, -105.1448846966432 40.12662004649052, -105.1447137065043 40.12678007314066, -105.1446938377278 40.12679883459163, -105.1443716376531 40.12710336772473, -105.1433827002903 40.12803805788978, -105.1416416731433 40.12976299450775, -105.1414536901801 40.12994403235987, -105.1412255205253 40.13022372772332, -105.1410715897065 40.13039683245281, -105.1409685953441 40.13051183984713, -105.1405674928146 40.13101869438201, -105.1404134914445 40.13123248008579, -105.1404134075242 40.13123259600766, -105.1402873438578 40.13141953294432, -105.1400313152862 40.13181050557099, -105.1399113154917 40.13199350715775, -105.1396172542842 40.13246945491051, -105.1394061770989 40.13283739637802, -105.1388641599894 40.13379438525001, -105.1387601569389 40.13397838399309, -105.1387142130814 40.13405542457127, -105.1383481339877 40.1340678960071, -105.136218990986 40.13406390604963, -105.1355969920545 40.13406290499365, -105.1351949880881 40.13406190558131, -105.131264018241 40.13407590214059, -105.1309663158803 40.13407590265542, -105.1309633151163 40.13416902954575, -105.1309613147293 40.13428302934808, -105.1309083153879 40.13760103000428, -105.1308973195819 40.13793389877544, -105.1308973153534 40.13793402935524, -105.1308863138307 40.13833002958336, -105.1308793142346 40.13849702881259, -105.1308803139455 40.13859202915448, -105.1308803144594 40.13869102876136, -105.1308769439179 40.13869433055886, -105.1308748979951 40.13959340728248, -105.1308738036668 40.13966968195346, -105.1308540934902 40.14082413527648, -105.1308516911788 40.14119194657553, -105.1308480583487 40.14160703767477, -105.1308490491988 40.14182006539099, -105.1308250256407 40.14268800923669, -105.1308196679674 40.14306795796484, -105.1307991588671 40.14349994692689, -105.1307838281008 40.14408406823397))</t>
+          <t>POLYGON ((-105.13078382810082 40.144084068233965, -105.13426089233324 40.14412010763965, -105.13642917952457 40.14414397092094, -105.14030298752581 40.14417201661489, -105.14030390644282 40.144878075148576, -105.1402998507262 40.14524260909443, -105.14090694572539 40.14524570513932, -105.14275044587899 40.14525141953902, -105.14379708488073 40.145254650774156, -105.14380277361813 40.14518642667634, -105.14384169396823 40.14432211683176, -105.14384371489446 40.144110879282344, -105.14379485361894 40.144033442770926, -105.14380409683658 40.143340592014944, -105.14478213319342 40.1432909504777, -105.14657705843045 40.143295082067745, -105.1476290272116 40.14323186273604, -105.1483019035963 40.14322403006873, -105.14953195557932 40.14324012078783, -105.14983488257978 40.14324558926504, -105.14983490382068 40.143244882325504, -105.14981800301507 40.143122945437966, -105.14980505384283 40.14299800157078, -105.14979387764272 40.14287608292592, -105.1497859249596 40.14275307526516, -105.14978012551325 40.142628976245696, -105.149776114543 40.142504882644765, -105.14977594863747 40.14225891591448, -105.14978695158904 40.14165007201457, -105.14979788012253 40.14042988002099, -105.1497999356095 40.14023909780055, -105.14980102310638 40.139819091071224, -105.14980612575371 40.138897006365575, -105.14980717754304 40.138623042228424, -105.1498081394624 40.13843609968689, -105.14980984825979 40.13824311969565, -105.14981576478498 40.13794141607789, -105.14981997860944 40.13745611129382, -105.14981988569683 40.13733504933415, -105.14981297427106 40.13714890698322, -105.14981400859199 40.13666987899488, -105.1498249439201 40.1360739361236, -105.14982614762522 40.13556196666508, -105.14985284748457 40.13512021381311, -105.14986002541671 40.134747029857, -105.14986700349179 40.13450300648549, -105.14986857527758 40.13448395904759, -105.14987534536627 40.13440193369182, -105.14987967824634 40.13406899981911, -105.14963180835552 40.13407168791918, -105.14558868849944 40.134064998924096, -105.14558870800842 40.13376199738765, -105.14561680149934 40.12884799589443, -105.14564872818227 40.12675200170747, -105.14564233602215 40.12643537867292, -105.14563279573125 40.12596286157071, -105.14512674453258 40.1263892194086, -105.14488469664316 40.126620046490515, -105.14471370650433 40.12678007314066, -105.14469383772784 40.126798834591625, -105.14437163765314 40.12710336772473, -105.14338270029026 40.12803805788978, -105.14164167314328 40.12976299450775, -105.14145369018013 40.12994403235987, -105.14122552052527 40.13022372772332, -105.14107158970647 40.13039683245281, -105.1409685953441 40.13051183984713, -105.14056749281461 40.13101869438201, -105.14041349144453 40.13123248008579, -105.14041340752419 40.13123259600766, -105.14028734385782 40.13141953294432, -105.14003131528621 40.13181050557099, -105.13991131549166 40.13199350715775, -105.13961725428423 40.132469454910506, -105.13940617709889 40.13283739637802, -105.13886415998937 40.13379438525001, -105.13876015693886 40.13397838399309, -105.13871421308136 40.134055424571265, -105.13834813398768 40.134067896007096, -105.13621899098595 40.134063906049626, -105.13559699205447 40.13406290499365, -105.13519498808807 40.134061905581305, -105.13126401824097 40.134075902140594, -105.13096631588034 40.13407590265542, -105.13096331511632 40.13416902954575, -105.1309613147293 40.13428302934808, -105.13090831538794 40.137601030004284, -105.13089731958193 40.137933898775444, -105.13089731535335 40.13793402935524, -105.13088631383067 40.13833002958336, -105.13087931423458 40.138497028812594, -105.13088031394553 40.13859202915448, -105.13088031445943 40.138691028761365, -105.13087694391785 40.138694330558856, -105.13087489799513 40.13959340728248, -105.1308738036668 40.13966968195346, -105.13085409349023 40.14082413527648, -105.13085169117876 40.14119194657553, -105.13084805834866 40.141607037674774, -105.13084904919876 40.141820065390995, -105.13082502564075 40.14268800923669, -105.13081966796736 40.14306795796484, -105.13079915886713 40.14349994692689, -105.13078382810082 40.144084068233965))</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -3268,7 +3280,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1651737208989 40.13809354823222, -105.1651786863176 40.1384400314556, -105.1651834468346 40.13877235868039, -105.1651882225575 40.1391056595273, -105.1651929227027 40.13942427697685, -105.1652132108072 40.13959086442447, -105.1652673115459 40.13976711914741, -105.165325318486 40.13988623673776, -105.1654302838812 40.14004103861132, -105.1654873590649 40.14010749740176, -105.1655521459996 40.14017312918123, -105.1657164112696 40.14030681665903, -105.1658690317878 40.14041243595285, -105.1662816750196 40.14069790434522, -105.166550523917 40.14088389028058, -105.1666848917594 40.14097058285963, -105.1669889958632 40.14073702366179, -105.1674183082148 40.14052163973111, -105.1676808053344 40.140429730724, -105.168063932312 40.14035299410429, -105.1685828137058 40.1403117959339, -105.1688937247929 40.14030939369401, -105.1690963244106 40.14030802512433, -105.1695892062839 40.14026575996809, -105.1697436335394 40.14022590227972, -105.1698922171966 40.14017405906508, -105.1700333115879 40.14011006082929, -105.1701655510882 40.14003552305471, -105.170400900026 40.13985240616859, -105.1706277844607 40.13965158597978, -105.1708600988039 40.13944463123175, -105.1712118985003 40.13912936270009, -105.1715649078606 40.13881467384258, -105.1718903105261 40.13852744262318, -105.1720274571306 40.1384063822998, -105.1722596489909 40.13821553865855, -105.1723868773267 40.13813299543261, -105.172466481085 40.13807733091087, -105.1725961726703 40.13801538580748, -105.1727258183717 40.1379631772656, -105.172885851678 40.13792273774178, -105.1729406791253 40.13791035873074, -105.1730573728468 40.13791017924589, -105.1730616583728 40.13791017245951, -105.1730894544393 40.13791012952569, -105.1730891493124 40.13790818057446, -105.1783750656559 40.13792076736095, -105.1783856925215 40.13792375374909, -105.1783857569761 40.13792377194132, -105.178390832764 40.13742799644631, -105.1783940230415 40.13644990497878, -105.1783948972642 40.13528101768208, -105.1783961618531 40.13508913406532, -105.1783958547979 40.13492689429661, -105.1783991093832 40.13408688368758, -105.1784048791175 40.13377395099028, -105.1783991396833 40.1337020124477, -105.1783999480014 40.13330396605977, -105.1784131673081 40.13194404858856, -105.1784180942343 40.13105298307757, -105.1784189256439 40.1310280042764, -105.1784229738302 40.13100413231251, -105.178427016947 40.13098108442205, -105.1784339246554 40.13095694572148, -105.178444049129 40.13093391475787, -105.1784548908681 40.13091006260262, -105.1784840588681 40.13086786763377, -105.1785020389263 40.13084705429363, -105.1785641690483 40.13079204933064, -105.1785684592082 40.13078897836895, -105.1785511991025 40.13076045923802, -105.1784921990268 40.13071445866245, -105.1783901991411 40.13068445895293, -105.1763945382965 40.13068560471505, -105.168948196977 40.1306634594016, -105.1689124571838 40.13066294718519, -105.1689125986237 40.1306329048518, -105.1689281965424 40.13055845919673, -105.1690031954348 40.12720745836092, -105.1689921957212 40.12714645870656, -105.1689571957668 40.12709045909411, -105.168898196283 40.12704245954604, -105.1688701962396 40.1270274592329, -105.1687951961079 40.12700445884948, -105.1687057057889 40.12700441568506, -105.1667741949328 40.12700345879298, -105.1667081954379 40.12699345858284, -105.166642195758 40.12696145922249, -105.1665921947485 40.12690745915487, -105.1665751958297 40.1268584592293, -105.1665941954893 40.12633345884351, -105.1658119066372 40.12652845903283, -105.1653700089539 40.12664755526463, -105.1648051947436 40.12681345989837, -105.1644421950803 40.12692945902451, -105.1636321946816 40.12720345937235, -105.1633531947814 40.12731345908721, -105.1629311946616 40.12746646007216, -105.1628381942516 40.1275384598923, -105.1627731945469 40.12760446023837, -105.1627091942639 40.12764845894845, -105.1625441952281 40.1276864588521, -105.1620093210164 40.12797305594989, -105.1604831934606 40.12878445990846, -105.1603761943632 40.1288334601072, -105.1602477556501 40.1288630990707, -105.1601261845107 40.12889596708893, -105.1599321943844 40.1289494599988, -105.1598101948547 40.12896045970615, -105.159667193892 40.12894945954594, -105.159567194188 40.1289214593066, -105.1594881935436 40.12887746060884, -105.1594381937382 40.12879546005235, -105.1593311935832 40.1284274605238, -105.1593241941156 40.12833945963551, -105.1593311943713 40.12824045994564, -105.1593961948648 40.12808645966798, -105.1594101940028 40.12802046036595, -105.1593961945012 40.12792145999537, -105.1593099156614 40.12782736753463, -105.1593321942806 40.12776146020572, -105.159295194393 40.12773946004652, -105.1591931935459 40.12775345958096, -105.1590381943059 40.12775145938977, -105.1587271935286 40.12775946009889, -105.1583881937712 40.12771545958289, -105.1581221932529 40.12766346026724, -105.1578931932202 40.12765245913534, -105.1576939255081 40.12766480027194, -105.1574571934914 40.12767945991541, -105.1572911938164 40.12771146007818, -105.1571021940422 40.12773645947969, -105.1568041930755 40.12776145992218, -105.1565956562976 40.12772766228106, -105.1565141933392 40.12771445982453, -105.1563391925392 40.1276614597395, -105.1559481928024 40.12743746043777, -105.1557801926516 40.12740145928399, -105.1556931920723 40.12731245959085, -105.15561919262 40.12719845979632, -105.1555921921127 40.12707946011266, -105.1556001924722 40.12702245971152, -105.1555461931968 40.12695945989714, -105.155437192927 40.12695445958236, -105.1552101930545 40.12692646033931, -105.1550255475185 40.12692646026373, -105.1549821926101 40.12692646047514, -105.1548092204482 40.12693493214863, -105.154300191837 40.12695046002028, -105.1527758874465 40.12694600356159, -105.1513948839501 40.12694194872075, -105.1508891916811 40.12694046027134, -105.1503821911598 40.12695246089658, -105.1501191918396 40.1269784605735, -105.1498021911529 40.12714446046252, -105.1493501918869 40.12752346094415, -105.1490791919685 40.12769346043497, -105.1489711913174 40.12773246071522, -105.1488141912797 40.12775946127093, -105.1486281913429 40.12777546030672, -105.1484921909401 40.12776446038666, -105.1483701909708 40.12775946068273, -105.148131047267 40.12775946111901, -105.1480411907711 40.12775946117674, -105.1479051910319 40.12776446140642, -105.1478051914117 40.1277864601138, -105.1476831913874 40.12780346061299, -105.1474471915002 40.12785746102228, -105.1473611912454 40.12789646119431, -105.1471681902714 40.12801146050332, -105.1469681918037 40.12816546030267, -105.1467601907007 40.12837346040647, -105.1466521909948 40.12851646037345, -105.1465091905153 40.1286324608168, -105.1463811910671 40.1286814612758, -105.1462091902176 40.1287254615651, -105.1459941909125 40.12876946043333, -105.1457651912196 40.12883446131615, -105.1456271903526 40.12885446106298, -105.1456167644999 40.12885442637793, -105.1455887080084 40.13376199738765, -105.1455886884994 40.1340649989241, -105.1496318083555 40.13407168791918, -105.1498796782463 40.13406899981911, -105.1498753453663 40.13440193369182, -105.1498685752776 40.13448395904759, -105.1498670034918 40.13450300648549, -105.1498600254167 40.134747029857, -105.1498528474846 40.13512021381311, -105.1498261476252 40.13556196666508, -105.1498249439201 40.1360739361236, -105.149814008592 40.13666987899488, -105.1498129742711 40.13714890698322, -105.1503191707842 40.13715837302616, -105.1507431046308 40.13725134436186, -105.1510724448465 40.13742605361374, -105.1514033148078 40.13763760641476, -105.151637130646 40.1377693929659, -105.1518946254916 40.13786586504331, -105.152150057365 40.13792551837336, -105.1526632313863 40.1379476509616, -105.1530713796339 40.1379351829944, -105.1536736820492 40.13791678139307, -105.1536495667924 40.13793002960441, -105.155268701542 40.13792138674664, -105.1557802404645 40.13792963792211, -105.1567409085716 40.13792156678671, -105.1578722149581 40.13791205130461, -105.1587047159848 40.13790527114151, -105.1592891232496 40.13790050869093, -105.1593307595289 40.13795994325748, -105.1633370163746 40.13791990694669, -105.1651711002737 40.13791065718695, -105.1651737208989 40.13809354823222))</t>
+          <t>POLYGON ((-105.16517372089888 40.13809354823222, -105.16517868631759 40.1384400314556, -105.16518344683463 40.13877235868039, -105.16518822255753 40.139105659527296, -105.1651929227027 40.13942427697685, -105.16521321080721 40.13959086442447, -105.16526731154586 40.139767119147415, -105.16532531848597 40.13988623673776, -105.16543028388116 40.14004103861132, -105.16548735906485 40.140107497401765, -105.16555214599961 40.14017312918123, -105.16571641126957 40.14030681665903, -105.16586903178778 40.140412435952854, -105.16628167501958 40.14069790434522, -105.16655052391704 40.140883890280584, -105.16668489175936 40.14097058285963, -105.1669889958632 40.14073702366179, -105.16741830821476 40.140521639731105, -105.16768080533437 40.140429730724, -105.16806393231201 40.14035299410429, -105.16858281370583 40.140311795933904, -105.16889372479292 40.14030939369401, -105.16909632441063 40.14030802512433, -105.16958920628393 40.14026575996809, -105.16974363353935 40.140225902279724, -105.16989221719656 40.14017405906508, -105.17003331158791 40.14011006082929, -105.1701655510882 40.14003552305471, -105.17040090002595 40.139852406168586, -105.17062778446072 40.139651585979784, -105.17086009880386 40.139444631231754, -105.17121189850032 40.13912936270009, -105.17156490786058 40.13881467384258, -105.1718903105261 40.13852744262318, -105.17202745713062 40.1384063822998, -105.17225964899092 40.13821553865855, -105.17238687732667 40.13813299543261, -105.17246648108498 40.138077330910875, -105.1725961726703 40.138015385807485, -105.17272581837172 40.137963177265604, -105.17288585167798 40.13792273774178, -105.1729406791253 40.13791035873074, -105.17305737284677 40.137910179245885, -105.17306165837277 40.137910172459506, -105.17308945443934 40.137910129525686, -105.17308914931239 40.137908180574456, -105.17837506565593 40.137920767360946, -105.17838569252147 40.137923753749085, -105.17838575697611 40.137923771941324, -105.17839083276404 40.137427996446306, -105.17839402304146 40.13644990497878, -105.17839489726424 40.135281017682075, -105.17839616185312 40.13508913406532, -105.17839585479788 40.13492689429661, -105.17839910938315 40.13408688368758, -105.17840487911754 40.13377395099028, -105.17839913968335 40.1337020124477, -105.17839994800136 40.13330396605977, -105.17841316730812 40.13194404858856, -105.17841809423427 40.131052983077566, -105.17841892564394 40.1310280042764, -105.1784229738302 40.13100413231251, -105.17842701694698 40.130981084422054, -105.1784339246554 40.13095694572148, -105.17844404912896 40.13093391475787, -105.17845489086814 40.13091006260262, -105.1784840588681 40.13086786763377, -105.17850203892633 40.13084705429363, -105.17856416904833 40.13079204933064, -105.17856845920818 40.130788978368955, -105.17855119910251 40.13076045923802, -105.1784921990268 40.130714458662446, -105.17839019914108 40.130684458952935, -105.17639453829649 40.13068560471505, -105.16894819697697 40.1306634594016, -105.16891245718378 40.13066294718519, -105.16891259862375 40.1306329048518, -105.16892819654235 40.130558459196735, -105.16900319543478 40.12720745836092, -105.16899219572122 40.127146458706555, -105.16895719576684 40.127090459094106, -105.16889819628297 40.12704245954604, -105.16887019623955 40.1270274592329, -105.16879519610792 40.127004458849484, -105.16870570578885 40.127004415685064, -105.16677419493276 40.127003458792984, -105.16670819543795 40.12699345858284, -105.16664219575804 40.12696145922249, -105.16659219474849 40.12690745915487, -105.16657519582972 40.1268584592293, -105.16659419548927 40.12633345884351, -105.16581190663724 40.126528459032826, -105.16537000895394 40.12664755526463, -105.1648051947436 40.126813459898365, -105.16444219508034 40.12692945902451, -105.16363219468157 40.12720345937235, -105.16335319478137 40.12731345908721, -105.1629311946616 40.127466460072164, -105.16283819425159 40.1275384598923, -105.16277319454686 40.12760446023837, -105.16270919426387 40.12764845894845, -105.16254419522811 40.1276864588521, -105.1620093210164 40.127973055949894, -105.16048319346062 40.12878445990846, -105.16037619436318 40.1288334601072, -105.16024775565006 40.1288630990707, -105.16012618451066 40.12889596708893, -105.15993219438444 40.1289494599988, -105.15981019485466 40.12896045970615, -105.15966719389199 40.12894945954594, -105.15956719418796 40.1289214593066, -105.15948819354355 40.12887746060884, -105.15943819373818 40.12879546005235, -105.15933119358321 40.128427460523795, -105.15932419411557 40.128339459635505, -105.15933119437133 40.12824045994564, -105.15939619486478 40.12808645966798, -105.15941019400277 40.128020460365946, -105.15939619450118 40.12792145999537, -105.15930991566137 40.12782736753463, -105.15933219428058 40.12776146020572, -105.15929519439304 40.12773946004652, -105.15919319354586 40.12775345958096, -105.15903819430594 40.12775145938977, -105.15872719352858 40.127759460098886, -105.15838819377116 40.12771545958289, -105.15812219325285 40.127663460267236, -105.1578931932202 40.12765245913534, -105.15769392550806 40.127664800271944, -105.15745719349138 40.127679459915406, -105.15729119381645 40.12771146007818, -105.15710219404221 40.127736459479685, -105.15680419307546 40.12776145992218, -105.15659565629761 40.12772766228106, -105.15651419333918 40.12771445982453, -105.15633919253925 40.1276614597395, -105.15594819280243 40.12743746043777, -105.15578019265165 40.127401459283995, -105.15569319207229 40.127312459590854, -105.15561919262002 40.12719845979632, -105.15559219211266 40.12707946011266, -105.15560019247224 40.12702245971152, -105.15554619319677 40.126959459897144, -105.15543719292698 40.12695445958236, -105.15521019305447 40.126926460339305, -105.15502554751848 40.126926460263725, -105.15498219261008 40.12692646047514, -105.1548092204482 40.12693493214863, -105.15430019183701 40.12695046002028, -105.15277588744652 40.12694600356159, -105.15139488395013 40.12694194872075, -105.1508891916811 40.12694046027134, -105.1503821911598 40.12695246089658, -105.15011919183956 40.126978460573504, -105.14980219115287 40.12714446046252, -105.14935019188688 40.127523460944154, -105.14907919196847 40.12769346043497, -105.14897119131737 40.127732460715215, -105.14881419127971 40.127759461270934, -105.14862819134288 40.127775460306715, -105.14849219094015 40.127764460386665, -105.1483701909708 40.12775946068273, -105.14813104726704 40.12775946111901, -105.14804119077108 40.12775946117674, -105.1479051910319 40.12776446140642, -105.14780519141166 40.127786460113796, -105.14768319138743 40.12780346061299, -105.14744719150019 40.12785746102228, -105.14736119124542 40.12789646119431, -105.14716819027137 40.12801146050332, -105.14696819180368 40.12816546030267, -105.1467601907007 40.12837346040647, -105.14665219099479 40.128516460373454, -105.14650919051532 40.1286324608168, -105.14638119106708 40.128681461275804, -105.14620919021763 40.1287254615651, -105.14599419091246 40.128769460433325, -105.14576519121955 40.128834461316146, -105.14562719035258 40.12885446106298, -105.14561676449995 40.128854426377934, -105.14558870800842 40.13376199738765, -105.14558868849944 40.134064998924096, -105.14963180835552 40.13407168791918, -105.14987967824634 40.13406899981911, -105.14987534536627 40.13440193369182, -105.14986857527758 40.13448395904759, -105.14986700349179 40.13450300648549, -105.14986002541671 40.134747029857, -105.14985284748457 40.13512021381311, -105.14982614762522 40.13556196666508, -105.1498249439201 40.1360739361236, -105.14981400859199 40.13666987899488, -105.14981297427106 40.13714890698322, -105.15031917078419 40.13715837302616, -105.15074310463076 40.13725134436186, -105.15107244484652 40.13742605361374, -105.15140331480775 40.13763760641476, -105.15163713064597 40.1377693929659, -105.15189462549161 40.13786586504331, -105.15215005736496 40.13792551837336, -105.15266323138633 40.1379476509616, -105.1530713796339 40.137935182994404, -105.15367368204925 40.137916781393066, -105.15364956679244 40.137930029604405, -105.15526870154196 40.13792138674664, -105.1557802404645 40.13792963792211, -105.15674090857163 40.13792156678671, -105.15787221495815 40.13791205130461, -105.1587047159848 40.137905271141506, -105.15928912324958 40.137900508690926, -105.15933075952893 40.13795994325748, -105.16333701637463 40.13791990694669, -105.16517110027371 40.13791065718695, -105.16517372089888 40.13809354823222))</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -3310,7 +3322,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1498349038207 40.1432448823255, -105.150186104229 40.14325692674986, -105.1505759365282 40.14326908694103, -105.1517970320264 40.14335787309525, -105.1524478848306 40.14339002936889, -105.1526081194201 40.14339298169327, -105.153773043639 40.14341487112591, -105.1544159877143 40.14345495338198, -105.1549171006202 40.14353111966914, -105.1557741435631 40.14367505161148, -105.1559639727837 40.14369702973576, -105.1562071196229 40.14371504756664, -105.1563931109972 40.1437180721734, -105.156705029212 40.14371790054443, -105.1573059000603 40.14366093807035, -105.1574229490422 40.14364508892761, -105.1576609971429 40.14361010744357, -105.1577720212397 40.1435829847798, -105.1579138418921 40.14354909030219, -105.1588479936346 40.14329710124521, -105.1591234964964 40.14322434274879, -105.1592119001119 40.1432009959051, -105.1594265702752 40.14316237349377, -105.159846160942 40.14311803973713, -105.1602571584037 40.14311787637087, -105.1605738963089 40.14315504276812, -105.1608751394325 40.14321494904825, -105.1610651328073 40.14327589993582, -105.1616030480891 40.14343312723048, -105.1619913300557 40.14352762602385, -105.1623054935046 40.14355772630975, -105.1626169388502 40.1435661303607, -105.163241063002 40.14352202466333, -105.1636174823973 40.14344760145708, -105.1641436103766 40.14326981787581, -105.1645518287281 40.14306462267481, -105.1649219364783 40.14281116543131, -105.1652389731235 40.14251870949103, -105.1655277855063 40.14220409895851, -105.1657382797755 40.14197304422079, -105.1666197252302 40.14102063172989, -105.1666848917594 40.14097058285963, -105.166550523917 40.14088389028058, -105.1662816750196 40.14069790434522, -105.1658690317878 40.14041243595285, -105.1657164112696 40.14030681665903, -105.1655521459996 40.14017312918123, -105.1654873590649 40.14010749740176, -105.1654302838812 40.14004103861132, -105.165325318486 40.13988623673776, -105.1652673115459 40.13976711914741, -105.1652132108072 40.13959086442447, -105.1651929227027 40.13942427697685, -105.1651882225575 40.1391056595273, -105.1651834468346 40.13877235868039, -105.1651786863176 40.1384400314556, -105.1651737208989 40.13809354823222, -105.1651711002737 40.13791065718695, -105.1633370163746 40.13791990694669, -105.1593307595289 40.13795994325748, -105.1592891232496 40.13790050869093, -105.1587047159848 40.13790527114151, -105.1578722149581 40.13791205130461, -105.1567409085716 40.13792156678671, -105.1557802404645 40.13792963792211, -105.155268701542 40.13792138674664, -105.1536495667924 40.13793002960441, -105.1536736820492 40.13791678139307, -105.1530713796339 40.1379351829944, -105.1526632313863 40.1379476509616, -105.152150057365 40.13792551837336, -105.1518946254916 40.13786586504331, -105.151637130646 40.1377693929659, -105.1514033148078 40.13763760641476, -105.1510724448465 40.13742605361374, -105.1507431046308 40.13725134436186, -105.1503191707842 40.13715837302616, -105.1498129742711 40.13714890698322, -105.1498198856968 40.13733504933415, -105.1498199786094 40.13745611129382, -105.149815764785 40.13794141607789, -105.1498098482598 40.13824311969565, -105.1498081394624 40.13843609968689, -105.149807177543 40.13862304222842, -105.1498061257537 40.13889700636557, -105.1498010231064 40.13981909107122, -105.1497999356095 40.14023909780055, -105.1497978801225 40.14042988002099, -105.149786951589 40.14165007201457, -105.1497759486375 40.14225891591448, -105.149776114543 40.14250488264477, -105.1497801255132 40.1426289762457, -105.1497859249596 40.14275307526516, -105.1497938776427 40.14287608292592, -105.1498050538428 40.14299800157078, -105.1498180030151 40.14312294543797, -105.1498349038207 40.1432448823255))</t>
+          <t>POLYGON ((-105.14983490382068 40.143244882325504, -105.15018610422901 40.14325692674986, -105.1505759365282 40.14326908694103, -105.15179703202637 40.14335787309525, -105.15244788483061 40.14339002936889, -105.15260811942008 40.14339298169327, -105.15377304363902 40.143414871125906, -105.15441598771432 40.14345495338198, -105.15491710062015 40.14353111966914, -105.15577414356305 40.14367505161148, -105.15596397278371 40.14369702973576, -105.15620711962293 40.14371504756664, -105.1563931109972 40.1437180721734, -105.15670502921203 40.14371790054443, -105.15730590006034 40.143660938070354, -105.1574229490422 40.143645088927606, -105.1576609971429 40.14361010744357, -105.15777202123968 40.1435829847798, -105.15791384189214 40.143549090302194, -105.15884799363457 40.14329710124521, -105.15912349649638 40.14322434274879, -105.15921190011194 40.143200995905104, -105.15942657027517 40.143162373493766, -105.15984616094197 40.143118039737125, -105.16025715840371 40.14311787637087, -105.16057389630893 40.14315504276812, -105.1608751394325 40.14321494904825, -105.16106513280734 40.143275899935816, -105.16160304808906 40.14343312723048, -105.1619913300557 40.143527626023854, -105.16230549350456 40.14355772630975, -105.16261693885016 40.1435661303607, -105.16324106300199 40.14352202466333, -105.16361748239733 40.14344760145708, -105.16414361037658 40.14326981787581, -105.16455182872807 40.14306462267481, -105.16492193647828 40.14281116543131, -105.16523897312354 40.14251870949103, -105.16552778550634 40.14220409895851, -105.16573827977548 40.14197304422079, -105.16661972523019 40.141020631729894, -105.16668489175936 40.14097058285963, -105.16655052391704 40.140883890280584, -105.16628167501958 40.14069790434522, -105.16586903178778 40.140412435952854, -105.16571641126957 40.14030681665903, -105.16555214599961 40.14017312918123, -105.16548735906485 40.140107497401765, -105.16543028388116 40.14004103861132, -105.16532531848597 40.13988623673776, -105.16526731154586 40.139767119147415, -105.16521321080721 40.13959086442447, -105.1651929227027 40.13942427697685, -105.16518822255753 40.139105659527296, -105.16518344683463 40.13877235868039, -105.16517868631759 40.1384400314556, -105.16517372089888 40.13809354823222, -105.16517110027371 40.13791065718695, -105.16333701637463 40.13791990694669, -105.15933075952893 40.13795994325748, -105.15928912324958 40.137900508690926, -105.1587047159848 40.137905271141506, -105.15787221495815 40.13791205130461, -105.15674090857163 40.13792156678671, -105.1557802404645 40.13792963792211, -105.15526870154196 40.13792138674664, -105.15364956679244 40.137930029604405, -105.15367368204925 40.137916781393066, -105.1530713796339 40.137935182994404, -105.15266323138633 40.1379476509616, -105.15215005736496 40.13792551837336, -105.15189462549161 40.13786586504331, -105.15163713064597 40.1377693929659, -105.15140331480775 40.13763760641476, -105.15107244484652 40.13742605361374, -105.15074310463076 40.13725134436186, -105.15031917078419 40.13715837302616, -105.14981297427106 40.13714890698322, -105.14981988569683 40.13733504933415, -105.14981997860944 40.13745611129382, -105.14981576478498 40.13794141607789, -105.14980984825979 40.13824311969565, -105.1498081394624 40.13843609968689, -105.14980717754304 40.138623042228424, -105.14980612575371 40.138897006365575, -105.14980102310638 40.139819091071224, -105.1497999356095 40.14023909780055, -105.14979788012253 40.14042988002099, -105.14978695158904 40.14165007201457, -105.14977594863747 40.14225891591448, -105.149776114543 40.142504882644765, -105.14978012551325 40.142628976245696, -105.1497859249596 40.14275307526516, -105.14979387764272 40.14287608292592, -105.14980505384283 40.14299800157078, -105.14981800301507 40.143122945437966, -105.14983490382068 40.143244882325504))</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -3352,7 +3364,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1526054812183 40.14785108866048, -105.1530461006681 40.1478594437918, -105.1534450751366 40.14777326084277, -105.1536176075861 40.14743299265101, -105.1539602690666 40.14722430411358, -105.1545300792188 40.14712989087602, -105.1550768482382 40.1470878341806, -105.1554527332914 40.14706274153117, -105.1560213916252 40.1471955069432, -105.1564198731371 40.14720543049145, -105.1568300936406 40.14714548246869, -105.1572976851163 40.14699832205635, -105.1581416401855 40.14672994156258, -105.1588370408193 40.14656597354273, -105.1594982794621 40.14640189978035, -105.1602044051932 40.14636902544356, -105.1612286938062 40.14646815301536, -105.162081930237 40.14661919860736, -105.1628556829655 40.14672631591058, -105.1638566902905 40.1469302084362, -105.1641221599461 40.14693968778932, -105.1734022512444 40.14696631970439, -105.1744325006828 40.14741195665381, -105.1746285858786 40.14768047738642, -105.1752051140806 40.14776365501274, -105.175811175027 40.1480216737566, -105.177477287678 40.14885354254437, -105.1783060114801 40.1492065285213, -105.1783316896897 40.14922173345824, -105.1783322539086 40.14912099754154, -105.1783342685619 40.14786827670135, -105.1783342828933 40.1478649966097, -105.1783343699196 40.1478468345418, -105.1783402810778 40.14660499955411, -105.178337307856 40.14535299840424, -105.1783373495214 40.14522699350773, -105.1783483399981 40.14435999722787, -105.1783507230336 40.14416221146657, -105.1783513876863 40.14416088307052, -105.178355161728 40.14414850346271, -105.1783547608992 40.14414764583766, -105.1783493436875 40.14413299714823, -105.1783533903674 40.14336199241301, -105.1783713737261 40.14226699561438, -105.1783763779464 40.14133799839369, -105.1783763784656 40.14133788851696, -105.178379409163 40.13975199673494, -105.1783808185894 40.13938497043898, -105.1783856925215 40.13792375374909, -105.1783750656559 40.13792076736095, -105.1730891493124 40.13790818057446, -105.1730894544393 40.13791012952569, -105.1730616583728 40.13791017245951, -105.1730573728468 40.13791017924589, -105.1729406791253 40.13791035873074, -105.172885851678 40.13792273774178, -105.1727258183717 40.1379631772656, -105.1725961726703 40.13801538580748, -105.172466481085 40.13807733091087, -105.1723868773267 40.13813299543261, -105.1722596489909 40.13821553865855, -105.1720274571306 40.1384063822998, -105.1718903105261 40.13852744262318, -105.1715649078606 40.13881467384258, -105.1712118985003 40.13912936270009, -105.1708600988039 40.13944463123175, -105.1706277844607 40.13965158597978, -105.170400900026 40.13985240616859, -105.1701655510882 40.14003552305471, -105.1700333115879 40.14011006082929, -105.1698922171966 40.14017405906508, -105.1697436335394 40.14022590227972, -105.1695892062839 40.14026575996809, -105.1690963244106 40.14030802512433, -105.1688937247929 40.14030939369401, -105.1685828137058 40.1403117959339, -105.168063932312 40.14035299410429, -105.1676808053344 40.140429730724, -105.1674183082148 40.14052163973111, -105.1669889958632 40.14073702366179, -105.1666848917594 40.14097058285963, -105.1666197252302 40.14102063172989, -105.1657382797755 40.14197304422079, -105.1655277855063 40.14220409895851, -105.1652389731235 40.14251870949103, -105.1649219364783 40.14281116543131, -105.1645518287281 40.14306462267481, -105.1641436103766 40.14326981787581, -105.1636174823973 40.14344760145708, -105.163241063002 40.14352202466333, -105.1626169388502 40.1435661303607, -105.1623054935046 40.14355772630975, -105.1619913300557 40.14352762602385, -105.1616030480891 40.14343312723048, -105.1610651328073 40.14327589993582, -105.1608751394325 40.14321494904825, -105.1605738963089 40.14315504276812, -105.1602571584037 40.14311787637087, -105.159846160942 40.14311803973713, -105.1594265702752 40.14316237349377, -105.1592119001119 40.1432009959051, -105.1591234964964 40.14322434274879, -105.1588479936346 40.14329710124521, -105.1579138418921 40.14354909030219, -105.1577720212397 40.1435829847798, -105.1576609971429 40.14361010744357, -105.1574229490422 40.14364508892761, -105.1573059000603 40.14366093807035, -105.156705029212 40.14371790054443, -105.1563931109972 40.1437180721734, -105.1562071196229 40.14371504756664, -105.1559639727837 40.14369702973576, -105.1557741435631 40.14367505161148, -105.1549171006202 40.14353111966914, -105.1544159877143 40.14345495338198, -105.153773043639 40.14341487112591, -105.1526081194201 40.14339298169327, -105.1524478848306 40.14339002936889, -105.1517970320264 40.14335787309525, -105.1505759365282 40.14326908694103, -105.150186104229 40.14325692674986, -105.1498349038207 40.1432448823255, -105.1498770736336 40.14346105428401, -105.1499019296383 40.14356599493146, -105.1499598340936 40.14378303770945, -105.1500651590963 40.14409987378166, -105.1501831558417 40.14438710078105, -105.1502418727191 40.14451602706418, -105.1502910696387 40.14461802143452, -105.1503449175444 40.14472002985641, -105.1504728950902 40.14494497133565, -105.150580035526 40.14511796549188, -105.1506968531819 40.14529431126436, -105.1508819242063 40.14553998559051, -105.1518030131312 40.14673306701286, -105.1518840306267 40.14683899958022, -105.1524551649044 40.14763791331065, -105.1526054812183 40.14785108866048))</t>
+          <t>POLYGON ((-105.15260548121832 40.14785108866048, -105.15304610066815 40.1478594437918, -105.15344507513664 40.14777326084277, -105.15361760758613 40.147432992651005, -105.1539602690666 40.14722430411358, -105.15453007921884 40.147129890876016, -105.15507684823818 40.1470878341806, -105.15545273329136 40.147062741531165, -105.15602139162522 40.1471955069432, -105.15641987313708 40.14720543049145, -105.15683009364056 40.14714548246869, -105.15729768511629 40.146998322056355, -105.15814164018552 40.146729941562576, -105.15883704081925 40.14656597354273, -105.15949827946207 40.14640189978035, -105.1602044051932 40.14636902544356, -105.16122869380615 40.146468153015356, -105.16208193023698 40.14661919860736, -105.16285568296549 40.14672631591058, -105.16385669029046 40.146930208436196, -105.1641221599461 40.14693968778932, -105.17340225124443 40.14696631970439, -105.17443250068277 40.147411956653805, -105.17462858587864 40.147680477386416, -105.17520511408061 40.14776365501274, -105.17581117502695 40.1480216737566, -105.17747728767799 40.148853542544366, -105.17830601148013 40.149206528521304, -105.17833168968971 40.14922173345824, -105.1783322539086 40.14912099754154, -105.17833426856191 40.147868276701345, -105.17833428289335 40.1478649966097, -105.17833436991964 40.147846834541795, -105.1783402810778 40.14660499955411, -105.17833730785604 40.14535299840424, -105.17833734952136 40.14522699350773, -105.1783483399981 40.14435999722787, -105.17835072303357 40.14416221146657, -105.17835138768633 40.14416088307052, -105.17835516172805 40.14414850346271, -105.17835476089924 40.144147645837656, -105.17834934368746 40.144132997148226, -105.1783533903674 40.143361992413006, -105.1783713737261 40.14226699561438, -105.17837637794638 40.141337998393695, -105.17837637846564 40.141337888516965, -105.17837940916303 40.139751996734944, -105.17838081858942 40.139384970438975, -105.17838569252147 40.137923753749085, -105.17837506565593 40.137920767360946, -105.17308914931239 40.137908180574456, -105.17308945443934 40.137910129525686, -105.17306165837277 40.137910172459506, -105.17305737284677 40.137910179245885, -105.1729406791253 40.13791035873074, -105.17288585167798 40.13792273774178, -105.17272581837172 40.137963177265604, -105.1725961726703 40.138015385807485, -105.17246648108498 40.138077330910875, -105.17238687732667 40.13813299543261, -105.17225964899092 40.13821553865855, -105.17202745713062 40.1384063822998, -105.1718903105261 40.13852744262318, -105.17156490786058 40.13881467384258, -105.17121189850032 40.13912936270009, -105.17086009880386 40.139444631231754, -105.17062778446072 40.139651585979784, -105.17040090002595 40.139852406168586, -105.1701655510882 40.14003552305471, -105.17003331158791 40.14011006082929, -105.16989221719656 40.14017405906508, -105.16974363353935 40.140225902279724, -105.16958920628393 40.14026575996809, -105.16909632441063 40.14030802512433, -105.16889372479292 40.14030939369401, -105.16858281370583 40.140311795933904, -105.16806393231201 40.14035299410429, -105.16768080533437 40.140429730724, -105.16741830821476 40.140521639731105, -105.1669889958632 40.14073702366179, -105.16668489175936 40.14097058285963, -105.16661972523019 40.141020631729894, -105.16573827977548 40.14197304422079, -105.16552778550634 40.14220409895851, -105.16523897312354 40.14251870949103, -105.16492193647828 40.14281116543131, -105.16455182872807 40.14306462267481, -105.16414361037658 40.14326981787581, -105.16361748239733 40.14344760145708, -105.16324106300199 40.14352202466333, -105.16261693885016 40.1435661303607, -105.16230549350456 40.14355772630975, -105.1619913300557 40.143527626023854, -105.16160304808906 40.14343312723048, -105.16106513280734 40.143275899935816, -105.1608751394325 40.14321494904825, -105.16057389630893 40.14315504276812, -105.16025715840371 40.14311787637087, -105.15984616094197 40.143118039737125, -105.15942657027517 40.143162373493766, -105.15921190011194 40.143200995905104, -105.15912349649638 40.14322434274879, -105.15884799363457 40.14329710124521, -105.15791384189214 40.143549090302194, -105.15777202123968 40.1435829847798, -105.1576609971429 40.14361010744357, -105.1574229490422 40.143645088927606, -105.15730590006034 40.143660938070354, -105.15670502921203 40.14371790054443, -105.1563931109972 40.1437180721734, -105.15620711962293 40.14371504756664, -105.15596397278371 40.14369702973576, -105.15577414356305 40.14367505161148, -105.15491710062015 40.14353111966914, -105.15441598771432 40.14345495338198, -105.15377304363902 40.143414871125906, -105.15260811942008 40.14339298169327, -105.15244788483061 40.14339002936889, -105.15179703202637 40.14335787309525, -105.1505759365282 40.14326908694103, -105.15018610422901 40.14325692674986, -105.14983490382068 40.143244882325504, -105.14987707363363 40.14346105428401, -105.14990192963835 40.14356599493146, -105.14995983409355 40.143783037709454, -105.15006515909629 40.14409987378166, -105.15018315584167 40.14438710078105, -105.15024187271909 40.14451602706418, -105.15029106963871 40.144618021434525, -105.15034491754442 40.14472002985641, -105.15047289509023 40.144944971335654, -105.15058003552605 40.14511796549188, -105.15069685318191 40.14529431126436, -105.15088192420632 40.14553998559051, -105.15180301313121 40.14673306701286, -105.15188403062668 40.14683899958022, -105.15245516490444 40.147637913310646, -105.15260548121832 40.14785108866048))</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -3394,7 +3406,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1782538706628 40.16695343985297, -105.1782579902131 40.16641899487397, -105.1782655161564 40.1650051485672, -105.178274033215 40.16340399540454, -105.1782749234563 40.16315591889484, -105.178284679339 40.16043600372073, -105.1782850786808 40.16032399691657, -105.1782851194905 40.16030891223458, -105.1782860862953 40.15995699669625, -105.1782862950887 40.15989422276495, -105.1782870964684 40.15965399674796, -105.178294217315 40.15818577184383, -105.1782951121814 40.15799899804473, -105.1782960843966 40.15719956301125, -105.1782960854515 40.15719884340366, -105.1782960871354 40.15719749425114, -105.1782971626988 40.15633399335119, -105.1783005822134 40.15597644463524, -105.1783011802659 40.1559149983927, -105.1783012893748 40.15590656871396, -105.1783291792601 40.15375999780937, -105.1783301522852 40.15303800468062, -105.1783233146343 40.15242367651192, -105.1783232044195 40.15240999729076, -105.1783262111119 40.15130500003102, -105.1783252470594 40.15034799549664, -105.1783316896897 40.14922173345824, -105.1783060114801 40.1492065285213, -105.177477287678 40.14885354254437, -105.175811175027 40.1480216737566, -105.1752051140806 40.14776365501274, -105.1746285858786 40.14768047738642, -105.1744325006828 40.14741195665381, -105.1734022512444 40.14696631970439, -105.1641221599461 40.14693968778932, -105.1638566902905 40.1469302084362, -105.1628556829655 40.14672631591058, -105.162081930237 40.14661919860736, -105.1612286938062 40.14646815301536, -105.1602044051932 40.14636902544356, -105.1594982794621 40.14640189978035, -105.1588370408193 40.14656597354273, -105.1581416401855 40.14672994156258, -105.1572976851163 40.14699832205635, -105.1568300936406 40.14714548246869, -105.1564198731371 40.14720543049145, -105.1560213916252 40.1471955069432, -105.1554527332914 40.14706274153117, -105.1550768482382 40.1470878341806, -105.1545300792188 40.14712989087602, -105.1539602690666 40.14722430411358, -105.1536176075861 40.14743299265101, -105.1534450751366 40.14777326084277, -105.1530461006681 40.1478594437918, -105.1526054812183 40.14785108866048, -105.1528500909462 40.1481991128168, -105.152970155993 40.14836500679122, -105.153516171437 40.14911387833198, -105.1536529206088 40.14930590055002, -105.1537200387882 40.14940300616207, -105.1539059797718 40.14970003979097, -105.1539619990861 40.14979903307982, -105.1541221488244 40.1501031275813, -105.1541688479994 40.15020593589973, -105.154259008105 40.15041511202504, -105.1543398797804 40.15062206452643, -105.1543888892721 40.15076303710305, -105.1544500739712 40.15097212729577, -105.1544679088951 40.1510528879393, -105.1544850111905 40.15113694093213, -105.1544978464772 40.15121604024894, -105.154509940763 40.15130007826262, -105.1545198884175 40.15138410985629, -105.1545269704766 40.15146895696729, -105.1545350860712 40.15163204311543, -105.1545328653188 40.15171713710714, -105.1545361802424 40.15254398638052, -105.154647999395 40.16705899872255, -105.1546488353165 40.16705898771062, -105.1546488300367 40.16705586518081, -105.1551078351645 40.16704986397507, -105.1562688454048 40.16703286263721, -105.1572978539927 40.16702986225165, -105.1593498721462 40.16705286010649, -105.1595208740774 40.16707385977891, -105.1596798760458 40.16712085952145, -105.1598118775726 40.1671618596847, -105.1599118790576 40.16721485751804, -105.1602088846895 40.16741385793949, -105.161120902206 40.16807485153609, -105.1622709235831 40.1688868436568, -105.1631259398792 40.16948983996239, -105.1635209475333 40.16973283788921, -105.1637179519749 40.16985083726004, -105.1638209526211 40.16989583642651, -105.1640679558686 40.16999983608142, -105.1642169582605 40.17006083511097, -105.1642709600386 40.17007883540592, -105.1650199693466 40.17032183177924, -105.1664129896231 40.17079382714124, -105.1665174951051 40.17073080935722, -105.1665201919034 40.17073175740313, -105.1668849048761 40.17085999075397, -105.1668943955052 40.17084829540469, -105.1668985520034 40.17084317464879, -105.1668896186171 40.17084009214113, -105.1669304607418 40.17078976692029, -105.1669332093008 40.17078637943621, -105.1670240178124 40.17067447924944, -105.167026766362 40.17067109176306, -105.167035661948 40.17067421828263, -105.1677465944088 40.16979815123889, -105.1677518350548 40.16979169341922, -105.1687231045455 40.16859477217606, -105.1687256438738 40.1685916425322, -105.1687255340658 40.16858670852341, -105.1728195198593 40.17056786550766, -105.1728205681745 40.1705683728318, -105.1729529231051 40.17063241614367, -105.1733576954174 40.17082828027013, -105.1733657812711 40.17083213172842, -105.1734768197971 40.17088453830642, -105.1734768239046 40.17088245964705, -105.1734766984293 40.17058819044085, -105.1734767013714 40.17058610997677, -105.1734854970979 40.16912908258862, -105.1734876717343 40.1687689579743, -105.1734888774345 40.16876895687698, -105.1735104074165 40.16876894654175, -105.1735112021403 40.16875746475598, -105.1735772011636 40.16694246349251, -105.1782538706628 40.16695343985297))</t>
+          <t>POLYGON ((-105.17825387066277 40.166953439852975, -105.17825799021314 40.16641899487397, -105.1782655161564 40.165005148567204, -105.17827403321505 40.163403995404536, -105.17827492345634 40.163155918894844, -105.17828467933904 40.16043600372073, -105.1782850786808 40.16032399691657, -105.1782851194905 40.160308912234576, -105.17828608629526 40.15995699669625, -105.17828629508872 40.159894222764954, -105.17828709646844 40.15965399674796, -105.17829421731496 40.158185771843826, -105.17829511218137 40.157998998044725, -105.17829608439656 40.15719956301125, -105.17829608545148 40.15719884340366, -105.17829608713544 40.15719749425114, -105.17829716269877 40.15633399335119, -105.17830058221338 40.155976444635236, -105.1783011802659 40.1559149983927, -105.1783012893748 40.15590656871396, -105.17832917926015 40.153759997809374, -105.17833015228523 40.153038004680624, -105.17832331463428 40.15242367651192, -105.17832320441953 40.15240999729076, -105.17832621111188 40.151305000031016, -105.17832524705936 40.15034799549664, -105.17833168968971 40.14922173345824, -105.17830601148013 40.149206528521304, -105.17747728767799 40.148853542544366, -105.17581117502695 40.1480216737566, -105.17520511408061 40.14776365501274, -105.17462858587864 40.147680477386416, -105.17443250068277 40.147411956653805, -105.17340225124443 40.14696631970439, -105.1641221599461 40.14693968778932, -105.16385669029046 40.146930208436196, -105.16285568296549 40.14672631591058, -105.16208193023698 40.14661919860736, -105.16122869380615 40.146468153015356, -105.1602044051932 40.14636902544356, -105.15949827946207 40.14640189978035, -105.15883704081925 40.14656597354273, -105.15814164018552 40.146729941562576, -105.15729768511629 40.146998322056355, -105.15683009364056 40.14714548246869, -105.15641987313708 40.14720543049145, -105.15602139162522 40.1471955069432, -105.15545273329136 40.147062741531165, -105.15507684823818 40.1470878341806, -105.15453007921884 40.147129890876016, -105.1539602690666 40.14722430411358, -105.15361760758613 40.147432992651005, -105.15344507513664 40.14777326084277, -105.15304610066815 40.1478594437918, -105.15260548121832 40.14785108866048, -105.15285009094617 40.1481991128168, -105.15297015599302 40.148365006791224, -105.15351617143698 40.14911387833198, -105.15365292060878 40.14930590055002, -105.15372003878824 40.149403006162075, -105.15390597977176 40.14970003979097, -105.15396199908606 40.14979903307982, -105.15412214882443 40.150103127581296, -105.15416884799939 40.150205935899734, -105.15425900810499 40.15041511202504, -105.15433987978037 40.15062206452643, -105.15438888927213 40.150763037103054, -105.15445007397118 40.150972127295766, -105.15446790889514 40.1510528879393, -105.15448501119052 40.15113694093213, -105.15449784647717 40.15121604024894, -105.154509940763 40.15130007826262, -105.15451988841751 40.151384109856295, -105.15452697047661 40.151468956967285, -105.15453508607119 40.15163204311543, -105.15453286531883 40.15171713710714, -105.15453618024242 40.15254398638052, -105.15464799939501 40.16705899872255, -105.15464883531652 40.16705898771062, -105.15464883003673 40.167055865180814, -105.15510783516454 40.16704986397507, -105.15626884540481 40.167032862637214, -105.15729785399269 40.167029862251646, -105.15934987214617 40.16705286010649, -105.15952087407739 40.16707385977891, -105.15967987604576 40.167120859521454, -105.15981187757257 40.167161859684704, -105.15991187905757 40.16721485751804, -105.16020888468945 40.16741385793949, -105.16112090220598 40.16807485153609, -105.1622709235831 40.1688868436568, -105.16312593987924 40.16948983996239, -105.16352094753327 40.169732837889214, -105.16371795197493 40.169850837260036, -105.16382095262105 40.16989583642651, -105.16406795586859 40.169999836081416, -105.16421695826051 40.17006083511097, -105.16427096003862 40.17007883540592, -105.16501996934656 40.17032183177924, -105.16641298962311 40.17079382714124, -105.1665174951051 40.170730809357224, -105.16652019190344 40.17073175740313, -105.16688490487608 40.17085999075397, -105.16689439550517 40.17084829540469, -105.16689855200339 40.17084317464879, -105.16688961861706 40.170840092141134, -105.16693046074175 40.170789766920294, -105.16693320930081 40.17078637943621, -105.16702401781235 40.17067447924944, -105.16702676636204 40.17067109176306, -105.16703566194798 40.17067421828263, -105.16774659440881 40.16979815123889, -105.16775183505476 40.16979169341922, -105.16872310454552 40.168594772176064, -105.16872564387377 40.1685916425322, -105.16872553406576 40.16858670852341, -105.17281951985935 40.170567865507664, -105.1728205681745 40.1705683728318, -105.17295292310514 40.17063241614367, -105.1733576954174 40.17082828027013, -105.17336578127112 40.17083213172842, -105.1734768197971 40.170884538306424, -105.17347682390464 40.170882459647046, -105.17347669842927 40.17058819044085, -105.17347670137138 40.17058610997677, -105.17348549709789 40.16912908258862, -105.17348767173426 40.1687689579743, -105.17348887743452 40.16876895687698, -105.17351040741647 40.168768946541746, -105.17351120214029 40.16875746475598, -105.17357720116361 40.16694246349251, -105.17825387066277 40.166953439852975))</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -3436,7 +3448,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1471472878128 40.17412208832916, -105.1538401553576 40.17416747340352, -105.1538534119111 40.17702152067658, -105.1546629131087 40.17736968103145, -105.1546620818144 40.17647724158829, -105.1546599342045 40.17417298750612, -105.1546589995688 40.17417299912417, -105.1546569996872 40.17249899848197, -105.1546569998319 40.17225799859407, -105.1546530002739 40.17018099915842, -105.154647999395 40.16705899872255, -105.1545361802424 40.15254398638052, -105.1545328653188 40.15171713710714, -105.1545350860712 40.15163204311543, -105.1545269704766 40.15146895696729, -105.1545198884175 40.15138410985629, -105.154509940763 40.15130007826262, -105.1544978464772 40.15121604024894, -105.1544850111905 40.15113694093213, -105.1544679088951 40.1510528879393, -105.1544500739712 40.15097212729577, -105.1543888892721 40.15076303710305, -105.1543398797804 40.15062206452643, -105.154259008105 40.15041511202504, -105.1541688479994 40.15020593589973, -105.1541221488244 40.1501031275813, -105.1539619990861 40.14979903307982, -105.1539059797718 40.14970003979097, -105.1537200387882 40.14940300616207, -105.1536529206088 40.14930590055002, -105.153516171437 40.14911387833198, -105.152970155993 40.14836500679122, -105.1528500909462 40.1481991128168, -105.1526054812183 40.14785108866048, -105.1524551649044 40.14763791331065, -105.1518840306267 40.14683899958022, -105.1518030131312 40.14673306701286, -105.1508819242063 40.14553998559051, -105.1506968531819 40.14529431126436, -105.150580035526 40.14511796549188, -105.1504728950902 40.14494497133565, -105.1503449175444 40.14472002985641, -105.1502910696387 40.14461802143452, -105.1502418727191 40.14451602706418, -105.1501831558417 40.14438710078105, -105.1500651590963 40.14409987378166, -105.1499598340936 40.14378303770945, -105.1499019296383 40.14356599493146, -105.1498770736336 40.14346105428401, -105.1498349038207 40.1432448823255, -105.1498348825798 40.14324558926504, -105.1495319555793 40.14324012078783, -105.1483019035963 40.14322403006873, -105.1476290272116 40.14323186273604, -105.1465770584305 40.14329508206774, -105.1447821331934 40.1432909504777, -105.1438040968366 40.14334059201494, -105.1437948536189 40.14403344277093, -105.1438437148945 40.14411087928234, -105.1438416939682 40.14432211683176, -105.1438027736181 40.14518642667634, -105.1437970848807 40.14525465077416, -105.142750445879 40.14525141953902, -105.1409069457254 40.14524570513932, -105.1402998507262 40.14524260909443, -105.1403039064428 40.14487807514858, -105.1403029875258 40.14417201661489, -105.1364291795246 40.14414397092094, -105.1342608923332 40.14412010763965, -105.1307838281008 40.14408406823397, -105.1307706181843 40.14524627362162, -105.1307729608928 40.14602102086895, -105.1307720001907 40.14619808137281, -105.1307658734509 40.14838211269672, -105.130768171165 40.14861792972759, -105.13076413403 40.14929597231239, -105.1307559901569 40.14960999290478, -105.1307521629572 40.1499199086414, -105.1307489090925 40.15005798014178, -105.1307410602994 40.15018587951855, -105.130738284654 40.15026891162164, -105.130737051567 40.15052901211791, -105.1307039956057 40.15167610960546, -105.1306961733624 40.15179906721498, -105.1306731437359 40.15241693007437, -105.1306839956621 40.1531200000652, -105.1306709238675 40.15421006123214, -105.1306689779113 40.15437092124854, -105.1306649581363 40.15471597557438, -105.1306608851026 40.15625709456641, -105.1306530671956 40.15717010964009, -105.130653033185 40.15743995864469, -105.1306308693006 40.15849100944353, -105.130625151603 40.15967607572149, -105.130654096629 40.16086893953873, -105.1306731679469 40.16223306885373, -105.1306670700193 40.1629610647313, -105.1306711654045 40.16332700698624, -105.1307381013153 40.16462082086606, -105.1307639196129 40.1650918902609, -105.1308120310599 40.16591888439482, -105.1308126707608 40.1659723349019, -105.130813006224 40.16600288927486, -105.1308159542148 40.16611901906788, -105.1308149506016 40.16617199689249, -105.1308250336257 40.1664240343811, -105.1308271425553 40.16649706227742, -105.1308239029101 40.16696208098051, -105.1308241373161 40.16698486700984, -105.1308239570611 40.16701808292218, -105.1308240275999 40.16707106507126, -105.1471472878128 40.17412208832916))</t>
+          <t>POLYGON ((-105.14714728781279 40.174122088329156, -105.15384015535763 40.17416747340352, -105.15385341191113 40.17702152067658, -105.15466291310872 40.17736968103145, -105.15466208181435 40.17647724158829, -105.15465993420452 40.17417298750612, -105.15465899956884 40.174172999124174, -105.15465699968722 40.17249899848197, -105.15465699983194 40.17225799859407, -105.15465300027391 40.17018099915842, -105.15464799939501 40.16705899872255, -105.15453618024242 40.15254398638052, -105.15453286531883 40.15171713710714, -105.15453508607119 40.15163204311543, -105.15452697047661 40.151468956967285, -105.15451988841751 40.151384109856295, -105.154509940763 40.15130007826262, -105.15449784647717 40.15121604024894, -105.15448501119052 40.15113694093213, -105.15446790889514 40.1510528879393, -105.15445007397118 40.150972127295766, -105.15438888927213 40.150763037103054, -105.15433987978037 40.15062206452643, -105.15425900810499 40.15041511202504, -105.15416884799939 40.150205935899734, -105.15412214882443 40.150103127581296, -105.15396199908606 40.14979903307982, -105.15390597977176 40.14970003979097, -105.15372003878824 40.149403006162075, -105.15365292060878 40.14930590055002, -105.15351617143698 40.14911387833198, -105.15297015599302 40.148365006791224, -105.15285009094617 40.1481991128168, -105.15260548121832 40.14785108866048, -105.15245516490444 40.147637913310646, -105.15188403062668 40.14683899958022, -105.15180301313121 40.14673306701286, -105.15088192420632 40.14553998559051, -105.15069685318191 40.14529431126436, -105.15058003552605 40.14511796549188, -105.15047289509023 40.144944971335654, -105.15034491754442 40.14472002985641, -105.15029106963871 40.144618021434525, -105.15024187271909 40.14451602706418, -105.15018315584167 40.14438710078105, -105.15006515909629 40.14409987378166, -105.14995983409355 40.143783037709454, -105.14990192963835 40.14356599493146, -105.14987707363363 40.14346105428401, -105.14983490382068 40.143244882325504, -105.14983488257978 40.14324558926504, -105.14953195557932 40.14324012078783, -105.1483019035963 40.14322403006873, -105.1476290272116 40.14323186273604, -105.14657705843045 40.143295082067745, -105.14478213319342 40.1432909504777, -105.14380409683658 40.143340592014944, -105.14379485361894 40.144033442770926, -105.14384371489446 40.144110879282344, -105.14384169396823 40.14432211683176, -105.14380277361813 40.14518642667634, -105.14379708488073 40.145254650774156, -105.14275044587899 40.14525141953902, -105.14090694572539 40.14524570513932, -105.1402998507262 40.14524260909443, -105.14030390644282 40.144878075148576, -105.14030298752581 40.14417201661489, -105.13642917952457 40.14414397092094, -105.13426089233324 40.14412010763965, -105.13078382810082 40.144084068233965, -105.13077061818426 40.145246273621616, -105.13077296089278 40.14602102086895, -105.1307720001907 40.14619808137281, -105.13076587345093 40.14838211269672, -105.13076817116502 40.14861792972759, -105.13076413402999 40.149295972312395, -105.13075599015693 40.14960999290478, -105.13075216295717 40.1499199086414, -105.1307489090925 40.15005798014178, -105.1307410602994 40.15018587951855, -105.13073828465399 40.15026891162164, -105.13073705156695 40.15052901211791, -105.13070399560574 40.15167610960546, -105.13069617336244 40.15179906721498, -105.13067314373593 40.152416930074374, -105.13068399566212 40.1531200000652, -105.13067092386753 40.15421006123214, -105.13066897791134 40.15437092124854, -105.13066495813634 40.154715975574376, -105.1306608851026 40.15625709456641, -105.13065306719562 40.15717010964009, -105.13065303318498 40.157439958644694, -105.13063086930057 40.15849100944353, -105.13062515160298 40.159676075721485, -105.13065409662904 40.16086893953873, -105.13067316794692 40.16223306885373, -105.13066707001934 40.1629610647313, -105.13067116540445 40.16332700698624, -105.13073810131534 40.16462082086606, -105.1307639196129 40.165091890260896, -105.13081203105992 40.16591888439482, -105.13081267076079 40.1659723349019, -105.13081300622405 40.16600288927486, -105.13081595421475 40.16611901906788, -105.13081495060159 40.166171996892494, -105.13082503362571 40.1664240343811, -105.1308271425553 40.16649706227742, -105.13082390291014 40.16696208098051, -105.13082413731605 40.16698486700984, -105.1308239570611 40.16701808292218, -105.13082402759993 40.16707106507126, -105.14714728781279 40.174122088329156))</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
@@ -3478,7 +3490,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.116570983888 40.17038692899581, -105.1178158853752 40.17039407161238, -105.1189430393077 40.17040410635464, -105.1201371329569 40.17040995858668, -105.1213079395277 40.17042093779713, -105.121525052716 40.17030992094868, -105.1216010718557 40.17028189425179, -105.1217538294875 40.17022502077831, -105.1220218780124 40.17009193377212, -105.1222858991367 40.16997503008646, -105.1227099792626 40.16977492039106, -105.12286693377 40.16973507943386, -105.1230330395367 40.16972299339648, -105.1231979098613 40.16974000185597, -105.1236068909988 40.16987502346031, -105.1237131288848 40.16994701792339, -105.1237881252106 40.17003894983811, -105.1238240450009 40.17014393179502, -105.1238589814622 40.17036201103702, -105.1239140607193 40.17043191685794, -105.1239768248647 40.17047110252382, -105.1240518509146 40.17049303305797, -105.1241330608343 40.17049686548875, -105.1242368732107 40.17049006543995, -105.1247628040899 40.17050266266191, -105.1251120458792 40.1705110252873, -105.1257700895006 40.17051700061796, -105.1258720702785 40.1705178801278, -105.1265029177806 40.17052403795397, -105.1278590524257 40.17054186296041, -105.1290921320947 40.17055186590388, -105.1292932296001 40.17054751516088, -105.1307328951028 40.17054394185323, -105.1307919383922 40.17054413045692, -105.1308520529194 40.17054487184136, -105.1308380730325 40.1698239502182, -105.1308381211171 40.16968312372387, -105.1308328523583 40.16953294692157, -105.130826950711 40.16923590355137, -105.130825096449 40.16911593337741, -105.1308268264415 40.16899487857084, -105.130829023898 40.16878789975995, -105.130829951995 40.16861687941822, -105.1308339090772 40.16841512361963, -105.1308248690956 40.16770711920258, -105.1308251696132 40.16745401704761, -105.1308240275999 40.16707106507126, -105.1308239570611 40.16701808292218, -105.1308241373161 40.16698486700984, -105.1308239029101 40.16696208098051, -105.1308271425553 40.16649706227742, -105.1308250336257 40.1664240343811, -105.1308149506016 40.16617199689249, -105.1308159542148 40.16611901906788, -105.130813006224 40.16600288927486, -105.1308126707608 40.1659723349019, -105.1308120310599 40.16591888439482, -105.1307639196129 40.1650918902609, -105.1307381013153 40.16462082086606, -105.1306711654045 40.16332700698624, -105.1306670700193 40.1629610647313, -105.1306731679469 40.16223306885373, -105.130654096629 40.16086893953873, -105.130625151603 40.15967607572149, -105.1306308693006 40.15849100944353, -105.130653033185 40.15743995864469, -105.1306530671956 40.15717010964009, -105.1306608851026 40.15625709456641, -105.1306649581363 40.15471597557438, -105.1306689779113 40.15437092124854, -105.1306709238675 40.15421006123214, -105.1306839956621 40.1531200000652, -105.1306731437359 40.15241693007437, -105.1306961733624 40.15179906721498, -105.1307039956057 40.15167610960546, -105.130737051567 40.15052901211791, -105.130738284654 40.15026891162164, -105.1307410602994 40.15018587951855, -105.1307489090925 40.15005798014178, -105.1307521629572 40.1499199086414, -105.1307559901569 40.14960999290478, -105.13076413403 40.14929597231239, -105.130768171165 40.14861792972759, -105.1307658734509 40.14838211269672, -105.1307720001907 40.14619808137281, -105.1307729608928 40.14602102086895, -105.1307706181843 40.14524627362162, -105.1307838281008 40.14408406823397, -105.1307991588671 40.14349994692689, -105.1308196679674 40.14306795796484, -105.1308250256407 40.14268800923669, -105.1308490491988 40.14182006539099, -105.1308480583487 40.14160703767477, -105.1308516911788 40.14119194657553, -105.1308540934902 40.14082413527648, -105.1308738036668 40.13966968195346, -105.1308748979951 40.13959340728248, -105.1308769439179 40.13869433055886, -105.1303923142009 40.13916902875051, -105.1303313154118 40.13922902808567, -105.1247883151495 40.14478902902466, -105.1243203153778 40.14526002966053, -105.1219613160375 40.14750802952513, -105.1214713155419 40.14797502969255, -105.1214643159671 40.14822102985509, -105.1214633158546 40.14837802926677, -105.1214593168065 40.1485880297608, -105.1212533161005 40.14879703059298, -105.1208303159887 40.14919902937343, -105.1201383165571 40.14990102921602, -105.1198893170867 40.15014302898289, -105.1196193162772 40.15040603050766, -105.1191113168914 40.1508870293791, -105.1187093166785 40.15128002911514, -105.1186593166722 40.15133602907218, -105.1185163167286 40.15147502962919, -105.1183783160733 40.15159102880732, -105.1182913165957 40.15165502930292, -105.1181203168223 40.15176802990709, -105.1180673167806 40.15179502982453, -105.1180609815329 40.15179809088321, -105.1182028332557 40.15194705840466, -105.1183070978197 40.15204595469579, -105.1183438054582 40.15207946904088, -105.1183971615081 40.15212818354858, -105.1184530983278 40.15217925452586, -105.1185569580286 40.15227407924778, -105.1185979210221 40.152306058452, -105.1184100399258 40.15238093001999, -105.1183699045664 40.15239287599296, -105.1181098361258 40.15239009487254, -105.1179191567963 40.15239001397271, -105.117506960274 40.15240210146893, -105.1174328341978 40.15241503338955, -105.1173059253008 40.1524621040393, -105.1172200976211 40.15252001746637, -105.1166951371468 40.15305303542566, -105.1166700602342 40.15420207679241, -105.1166568381386 40.15604101638774, -105.1166160349168 40.15693305837366, -105.1166100273826 40.15774505678377, -105.1166159241907 40.15815904714898, -105.1167730976391 40.15826690417002, -105.1169598643474 40.15839297726098, -105.1170558268282 40.15844298275286, -105.1172780401464 40.15850109239538, -105.1173569140303 40.15853594269353, -105.1174591409044 40.15861698847455, -105.1175149031218 40.15868991962917, -105.1175369714868 40.15877399457021, -105.1170668668149 40.15876996742648, -105.1166568464329 40.15876998071828, -105.1165298328746 40.15877010874338, -105.1164088961616 40.15877107998472, -105.1155992023579 40.15877635047435, -105.1144260887028 40.1587661282411, -105.1120558549978 40.15875188276502, -105.1119470882641 40.15875206700218, -105.1119398694822 40.15970406397353, -105.111922147322 40.1614309849511, -105.1119199845855 40.16162204059638, -105.1119180988292 40.1618270976319, -105.1124691605463 40.16188110459242, -105.1128541752237 40.1619400431437, -105.1144081317069 40.16218708707287, -105.1152900204082 40.16233002871216, -105.1161798614204 40.16245898955479, -105.1166030728205 40.16253478804553, -105.1165972617726 40.16319765565999, -105.1165970657052 40.16325098554722, -105.1165841379701 40.16417218994248, -105.1165760565016 40.16499226566529, -105.1165748537872 40.16504069631765, -105.1172139845696 40.16505066564728, -105.1172139417619 40.16506098594407, -105.1172158396557 40.16529597741587, -105.1171978432182 40.165569061323, -105.1172010077831 40.16634210758333, -105.1171939036757 40.16677801553631, -105.1165898987154 40.1667771114352, -105.1165908282008 40.16724708567887, -105.1165920008793 40.16729293305302, -105.1165821468334 40.16783506950146, -105.1165761090586 40.16858886896271, -105.1165759788454 40.16873902862955, -105.1165718372282 40.16909286551239, -105.1165708265899 40.16977997472073, -105.116570983888 40.17038692899581))</t>
+          <t>POLYGON ((-105.11657098388795 40.17038692899581, -105.11781588537522 40.17039407161238, -105.11894303930771 40.17040410635464, -105.12013713295688 40.17040995858668, -105.12130793952765 40.17042093779713, -105.12152505271601 40.17030992094868, -105.1216010718557 40.170281894251794, -105.12175382948746 40.17022502077831, -105.12202187801238 40.17009193377212, -105.12228589913668 40.16997503008646, -105.1227099792626 40.16977492039106, -105.12286693377001 40.169735079433856, -105.12303303953671 40.16972299339648, -105.12319790986133 40.16974000185597, -105.12360689099884 40.16987502346031, -105.12371312888476 40.16994701792339, -105.12378812521057 40.17003894983811, -105.12382404500092 40.17014393179502, -105.12385898146225 40.17036201103702, -105.12391406071934 40.17043191685794, -105.12397682486474 40.17047110252382, -105.12405185091457 40.170493033057966, -105.12413306083432 40.17049686548875, -105.12423687321073 40.17049006543995, -105.12476280408994 40.17050266266191, -105.12511204587916 40.170511025287304, -105.12577008950062 40.17051700061796, -105.12587207027855 40.1705178801278, -105.12650291778061 40.170524037953975, -105.1278590524257 40.17054186296041, -105.12909213209471 40.17055186590388, -105.12929322960005 40.170547515160884, -105.13073289510278 40.170543941853225, -105.13079193839218 40.17054413045692, -105.1308520529194 40.17054487184136, -105.13083807303255 40.1698239502182, -105.13083812111708 40.16968312372387, -105.1308328523583 40.16953294692157, -105.13082695071097 40.16923590355137, -105.13082509644899 40.169115933377405, -105.1308268264415 40.16899487857084, -105.13082902389796 40.16878789975995, -105.13082995199497 40.168616879418224, -105.13083390907721 40.16841512361963, -105.13082486909565 40.16770711920258, -105.1308251696132 40.16745401704761, -105.13082402759993 40.16707106507126, -105.1308239570611 40.16701808292218, -105.13082413731605 40.16698486700984, -105.13082390291014 40.16696208098051, -105.1308271425553 40.16649706227742, -105.13082503362571 40.1664240343811, -105.13081495060159 40.166171996892494, -105.13081595421475 40.16611901906788, -105.13081300622405 40.16600288927486, -105.13081267076079 40.1659723349019, -105.13081203105992 40.16591888439482, -105.1307639196129 40.165091890260896, -105.13073810131534 40.16462082086606, -105.13067116540445 40.16332700698624, -105.13066707001934 40.1629610647313, -105.13067316794692 40.16223306885373, -105.13065409662904 40.16086893953873, -105.13062515160298 40.159676075721485, -105.13063086930057 40.15849100944353, -105.13065303318498 40.157439958644694, -105.13065306719562 40.15717010964009, -105.1306608851026 40.15625709456641, -105.13066495813634 40.154715975574376, -105.13066897791134 40.15437092124854, -105.13067092386753 40.15421006123214, -105.13068399566212 40.1531200000652, -105.13067314373593 40.152416930074374, -105.13069617336244 40.15179906721498, -105.13070399560574 40.15167610960546, -105.13073705156695 40.15052901211791, -105.13073828465399 40.15026891162164, -105.1307410602994 40.15018587951855, -105.1307489090925 40.15005798014178, -105.13075216295717 40.1499199086414, -105.13075599015693 40.14960999290478, -105.13076413402999 40.149295972312395, -105.13076817116502 40.14861792972759, -105.13076587345093 40.14838211269672, -105.1307720001907 40.14619808137281, -105.13077296089278 40.14602102086895, -105.13077061818426 40.145246273621616, -105.13078382810082 40.144084068233965, -105.13079915886713 40.14349994692689, -105.13081966796736 40.14306795796484, -105.13082502564075 40.14268800923669, -105.13084904919876 40.141820065390995, -105.13084805834866 40.141607037674774, -105.13085169117876 40.14119194657553, -105.13085409349023 40.14082413527648, -105.1308738036668 40.13966968195346, -105.13087489799513 40.13959340728248, -105.13087694391785 40.138694330558856, -105.13039231420086 40.13916902875051, -105.1303313154118 40.13922902808567, -105.12478831514953 40.144789029024665, -105.12432031537783 40.145260029660534, -105.12196131603747 40.147508029525135, -105.12147131554194 40.14797502969255, -105.12146431596709 40.14822102985509, -105.12146331585461 40.148378029266766, -105.12145931680647 40.1485880297608, -105.12125331610045 40.14879703059298, -105.1208303159887 40.149199029373435, -105.12013831655707 40.149901029216025, -105.11988931708672 40.15014302898289, -105.11961931627718 40.15040603050766, -105.11911131689145 40.1508870293791, -105.11870931667852 40.151280029115135, -105.11865931667215 40.15133602907218, -105.11851631672864 40.15147502962919, -105.11837831607326 40.151591028807324, -105.11829131659566 40.15165502930292, -105.11812031682226 40.15176802990709, -105.11806731678058 40.15179502982453, -105.11806098153292 40.15179809088321, -105.11820283325568 40.15194705840466, -105.11830709781968 40.15204595469579, -105.11834380545822 40.15207946904088, -105.11839716150807 40.15212818354858, -105.11845309832782 40.15217925452586, -105.11855695802862 40.15227407924778, -105.11859792102206 40.152306058452, -105.1184100399258 40.152380930019994, -105.11836990456644 40.15239287599296, -105.11810983612575 40.15239009487254, -105.11791915679635 40.152390013972706, -105.11750696027399 40.15240210146893, -105.11743283419779 40.15241503338955, -105.11730592530077 40.1524621040393, -105.1172200976211 40.15252001746637, -105.1166951371468 40.15305303542566, -105.11667006023423 40.15420207679241, -105.11665683813858 40.15604101638774, -105.11661603491685 40.15693305837366, -105.11661002738259 40.15774505678377, -105.11661592419067 40.15815904714898, -105.11677309763905 40.15826690417002, -105.11695986434736 40.15839297726098, -105.11705582682825 40.15844298275286, -105.11727804014639 40.158501092395376, -105.11735691403027 40.158535942693526, -105.11745914090439 40.15861698847455, -105.11751490312183 40.15868991962917, -105.1175369714868 40.15877399457021, -105.11706686681494 40.15876996742648, -105.11665684643289 40.15876998071828, -105.11652983287456 40.15877010874338, -105.11640889616157 40.158771079984724, -105.11559920235794 40.158776350474355, -105.11442608870276 40.158766128241105, -105.11205585499783 40.158751882765024, -105.1119470882641 40.15875206700218, -105.11193986948223 40.15970406397353, -105.11192214732199 40.1614309849511, -105.1119199845855 40.16162204059638, -105.11191809882915 40.1618270976319, -105.11246916054628 40.161881104592425, -105.11285417522373 40.1619400431437, -105.11440813170687 40.162187087072866, -105.11529002040822 40.16233002871216, -105.11617986142043 40.16245898955479, -105.11660307282054 40.16253478804553, -105.11659726177261 40.16319765565999, -105.11659706570515 40.163250985547215, -105.11658413797008 40.164172189942484, -105.11657605650164 40.16499226566529, -105.11657485378718 40.165040696317654, -105.11721398456963 40.16505066564728, -105.1172139417619 40.165060985944066, -105.11721583965567 40.165295977415866, -105.11719784321824 40.165569061323005, -105.11720100778314 40.166342107583326, -105.1171939036757 40.16677801553631, -105.11658989871539 40.1667771114352, -105.11659082820076 40.16724708567887, -105.11659200087932 40.16729293305302, -105.11658214683338 40.16783506950146, -105.11657610905856 40.16858886896271, -105.11657597884539 40.168739028629545, -105.1165718372282 40.16909286551239, -105.11657082658994 40.169779974720726, -105.11657098388795 40.17038692899581))</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -3520,7 +3532,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.111914063396 40.14145906879407, -105.1119990902711 40.14158401244808, -105.1120890445636 40.14169793699239, -105.1124091545411 40.14214208108856, -105.1126628483858 40.14250392147972, -105.1127390863524 40.14262112108667, -105.1127798633632 40.14274698668299, -105.1127950949235 40.14327603066909, -105.1127931209043 40.14368587804928, -105.1127839663049 40.14378604574785, -105.1127408575495 40.14394402272607, -105.1126838230354 40.14403497126058, -105.1125719440864 40.1441460498956, -105.11240786854 40.14425201241458, -105.1122721256333 40.1443448924646, -105.1121071451179 40.14448406724551, -105.1120641736526 40.14455502336704, -105.1120071470319 40.14470691361935, -105.1119931259656 40.14478208466217, -105.1119941641746 40.1450390353672, -105.1119929840249 40.14549692472122, -105.1119936796568 40.14619063122835, -105.111994034971 40.14688104107174, -105.1119819719483 40.1486829267191, -105.111970201264 40.15061702541113, -105.111964885932 40.15155199513816, -105.1119648264145 40.15162705807939, -105.1119630291551 40.15219310487264, -105.1119630286397 40.15225596880479, -105.111963031645 40.15231800956109, -105.1138379798012 40.15232099564363, -105.1155611697305 40.15233689853603, -105.1159511562896 40.15232995978926, -105.1163498803985 40.15229587185886, -105.1168350531517 40.15222089096753, -105.117098960966 40.1521630366401, -105.1170990396997 40.15216301978879, -105.1171067626289 40.15216074423739, -105.1171083166701 40.15216303071296, -105.1174373163797 40.15206603050657, -105.1176343172161 40.15199203009031, -105.1178293167799 40.15191002952171, -105.1180609815329 40.15179809088321, -105.1180673167806 40.15179502982453, -105.1181203168223 40.15176802990709, -105.1182913165957 40.15165502930292, -105.1183783160733 40.15159102880732, -105.1185163167286 40.15147502962919, -105.1186593166722 40.15133602907218, -105.1187093166785 40.15128002911514, -105.1191113168914 40.1508870293791, -105.1196193162772 40.15040603050766, -105.1198893170867 40.15014302898289, -105.1201383165571 40.14990102921602, -105.1208303159887 40.14919902937343, -105.1212533161005 40.14879703059298, -105.1214593168065 40.1485880297608, -105.1214633158546 40.14837802926677, -105.1214643159671 40.14822102985509, -105.1214713155419 40.14797502969255, -105.1219613160375 40.14750802952513, -105.1243203153778 40.14526002966053, -105.1247883151495 40.14478902902466, -105.1303313154118 40.13922902808567, -105.1303923142009 40.13916902875051, -105.1308769439179 40.13869433055886, -105.1308803144594 40.13869102876136, -105.1308803139455 40.13859202915448, -105.1308793142346 40.13849702881259, -105.1308863138307 40.13833002958336, -105.1308973153534 40.13793402935524, -105.1308973195819 40.13793389877544, -105.1308880033281 40.13793413290086, -105.1308880005306 40.13793399959673, -105.1214760632031 40.13789187653235, -105.1206799823645 40.13787389253752, -105.1204010352615 40.13786693756008, -105.1201221062495 40.1378569612092, -105.119842842414 40.13784286624009, -105.1184898474704 40.13782797427399, -105.1181829755937 40.13782586265843, -105.1172280717856 40.13781089914383, -105.1163031792091 40.13780206622556, -105.1153910575788 40.13781193606512, -105.1151238749654 40.13781186951335, -105.1143270696734 40.13779603509296, -105.1140931460601 40.13779690126499, -105.1133909369859 40.13781404447786, -105.1132657026752 40.13781976323562, -105.1129148435082 40.1381329148556, -105.1123358415979 40.13859691635773, -105.1119741665393 40.13888512691707, -105.1125981540443 40.13947907904089, -105.1127638668591 40.13964901145435, -105.112821162624 40.13976312771756, -105.1128369225726 40.13988506646543, -105.1127738473876 40.14009513471218, -105.1125598222135 40.14028292737444, -105.1119998637142 40.14065774078199, -105.1118561705442 40.14075995496132, -105.1117749312176 40.14089309708596, -105.1117588196545 40.14101493067353, -105.1117628186357 40.1411279316719, -105.1117835285537 40.14120268263837, -105.1118008162135 40.14127193177784, -105.1118408160296 40.14135893235024, -105.111914063396 40.14145906879407))</t>
+          <t>POLYGON ((-105.11191406339604 40.14145906879407, -105.11199909027106 40.14158401244808, -105.1120890445636 40.14169793699239, -105.11240915454108 40.14214208108856, -105.11266284838575 40.142503921479715, -105.11273908635239 40.14262112108667, -105.11277986336322 40.142746986682994, -105.11279509492347 40.143276030669085, -105.11279312090427 40.14368587804928, -105.11278396630487 40.14378604574785, -105.11274085754948 40.143944022726075, -105.11268382303544 40.14403497126058, -105.11257194408641 40.1441460498956, -105.11240786854 40.144252012414576, -105.11227212563333 40.1443448924646, -105.11210714511788 40.14448406724551, -105.11206417365264 40.14455502336704, -105.11200714703187 40.14470691361935, -105.1119931259656 40.14478208466217, -105.11199416417462 40.145039035367205, -105.11199298402494 40.14549692472122, -105.11199367965678 40.14619063122835, -105.11199403497098 40.14688104107174, -105.11198197194828 40.148682926719104, -105.11197020126396 40.15061702541113, -105.11196488593201 40.15155199513816, -105.11196482641452 40.15162705807939, -105.11196302915513 40.15219310487264, -105.11196302863969 40.15225596880479, -105.11196303164496 40.15231800956109, -105.11383797980122 40.15232099564363, -105.11556116973053 40.15233689853603, -105.1159511562896 40.152329959789256, -105.1163498803985 40.15229587185886, -105.11683505315172 40.15222089096753, -105.11709896096602 40.152163036640104, -105.11709903969965 40.15216301978879, -105.11710676262885 40.15216074423739, -105.1171083166701 40.15216303071296, -105.11743731637968 40.15206603050657, -105.11763431721609 40.15199203009031, -105.1178293167799 40.15191002952171, -105.11806098153292 40.15179809088321, -105.11806731678058 40.15179502982453, -105.11812031682226 40.15176802990709, -105.11829131659566 40.15165502930292, -105.11837831607326 40.151591028807324, -105.11851631672864 40.15147502962919, -105.11865931667215 40.15133602907218, -105.11870931667852 40.151280029115135, -105.11911131689145 40.1508870293791, -105.11961931627718 40.15040603050766, -105.11988931708672 40.15014302898289, -105.12013831655707 40.149901029216025, -105.1208303159887 40.149199029373435, -105.12125331610045 40.14879703059298, -105.12145931680647 40.1485880297608, -105.12146331585461 40.148378029266766, -105.12146431596709 40.14822102985509, -105.12147131554194 40.14797502969255, -105.12196131603747 40.147508029525135, -105.12432031537783 40.145260029660534, -105.12478831514953 40.144789029024665, -105.1303313154118 40.13922902808567, -105.13039231420086 40.13916902875051, -105.13087694391785 40.138694330558856, -105.13088031445943 40.138691028761365, -105.13088031394553 40.13859202915448, -105.13087931423458 40.138497028812594, -105.13088631383067 40.13833002958336, -105.13089731535335 40.13793402935524, -105.13089731958193 40.137933898775444, -105.13088800332805 40.13793413290086, -105.13088800053063 40.13793399959673, -105.12147606320309 40.13789187653235, -105.12067998236445 40.13787389253752, -105.12040103526145 40.13786693756008, -105.12012210624953 40.1378569612092, -105.11984284241402 40.137842866240085, -105.11848984747044 40.13782797427399, -105.1181829755937 40.13782586265843, -105.11722807178558 40.13781089914383, -105.11630317920908 40.13780206622556, -105.11539105757885 40.13781193606512, -105.11512387496536 40.13781186951335, -105.11432706967338 40.13779603509296, -105.11409314606009 40.13779690126499, -105.1133909369859 40.137814044477864, -105.11326570267524 40.13781976323562, -105.11291484350821 40.138132914855596, -105.1123358415979 40.13859691635773, -105.11197416653927 40.13888512691707, -105.11259815404428 40.13947907904089, -105.11276386685908 40.139649011454345, -105.11282116262402 40.139763127717565, -105.11283692257261 40.13988506646543, -105.11277384738763 40.14009513471218, -105.1125598222135 40.14028292737444, -105.11199986371425 40.14065774078199, -105.11185617054421 40.14075995496132, -105.11177493121764 40.14089309708596, -105.11175881965453 40.141014930673535, -105.1117628186357 40.141127931671896, -105.11178352855369 40.14120268263837, -105.11180081621352 40.14127193177784, -105.11184081602963 40.141358932350236, -105.11191406339604 40.14145906879407))</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -3562,7 +3574,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1051399989076 40.16020108764328, -105.1051400004159 40.16025199911635, -105.1051410002289 40.16030099923575, -105.1051503173048 40.16030096622104, -105.1068299991866 40.16029499859334, -105.1073450001184 40.16022799895545, -105.1077819997477 40.16013699863746, -105.1082079998631 40.16001999929222, -105.108461998888 40.15992999885013, -105.1086199994601 40.15987499865997, -105.1090149994251 40.15970599910182, -105.1093910002993 40.15951199882478, -105.1097429994652 40.15929699888233, -105.1100720003185 40.15905999866217, -105.1103729990311 40.15880299892639, -105.1104429993529 40.15873099894289, -105.1106439998662 40.15852399914743, -105.1130460729817 40.15615723779523, -105.1131817329908 40.15603004308861, -105.1131833166732 40.1560310309896, -105.1171083166701 40.15216303071296, -105.1171067626289 40.15216074423739, -105.1170990396997 40.15216301978879, -105.117098960966 40.1521630366401, -105.1168350531517 40.15222089096753, -105.1163498803985 40.15229587185886, -105.1159511562896 40.15232995978926, -105.1155611697305 40.15233689853603, -105.1138379798012 40.15232099564363, -105.111963031645 40.15231800956109, -105.1119630286397 40.15225596880479, -105.1119630291551 40.15219310487264, -105.1119648264145 40.15162705807939, -105.111964885932 40.15155199513816, -105.111970201264 40.15061702541113, -105.1119819719483 40.1486829267191, -105.111994034971 40.14688104107174, -105.1119936796568 40.14619063122835, -105.1119929840249 40.14549692472122, -105.1119941641746 40.1450390353672, -105.1119931259656 40.14478208466217, -105.1120071470319 40.14470691361935, -105.1120641736526 40.14455502336704, -105.1121071451179 40.14448406724551, -105.1122721256333 40.1443448924646, -105.11240786854 40.14425201241458, -105.1125719440864 40.1441460498956, -105.1126838230354 40.14403497126058, -105.1127408575495 40.14394402272607, -105.1127839663049 40.14378604574785, -105.1127931209043 40.14368587804928, -105.1127950949235 40.14327603066909, -105.1127798633632 40.14274698668299, -105.1127390863524 40.14262112108667, -105.1126628483858 40.14250392147972, -105.1124091545411 40.14214208108856, -105.1120890445636 40.14169793699239, -105.1119990902711 40.14158401244808, -105.111914063396 40.14145906879407, -105.1113486218073 40.14168839314541, -105.11129310243 40.1417109098067, -105.1110718385429 40.14181008893544, -105.1108640824602 40.14192386303387, -105.11066983058 40.14205305535067, -105.1103920126454 40.14222094634746, -105.1102731505028 40.14230207715557, -105.1095840635151 40.14276697772822, -105.109161980491 40.14307795071951, -105.1084469854705 40.14362895567095, -105.108417879155 40.14365191711192, -105.1082699579036 40.1437469469786, -105.1079030226773 40.14392111893775, -105.1071470935328 40.14424797156938, -105.1070510249035 40.14428305730459, -105.1067939256991 40.14439089125828, -105.1060476780228 40.14465520375037, -105.1058998209801 40.14470394763508, -105.1056838215419 40.14478594833889, -105.1053782970942 40.1448743635278, -105.1051659901088 40.14494700107727, -105.1049990293322 40.14500280892646, -105.1048608113467 40.14504900859458, -105.1047560762105 40.1450840177562, -105.1046167067099 40.14513060227208, -105.1044871661829 40.14517390139294, -105.1043439248778 40.14520086261507, -105.1042410057594 40.14520402266659, -105.1042286659116 40.14533691899432, -105.1041052205383 40.14536990728234, -105.1037377706737 40.14553499119413, -105.1035694298707 40.1456584188717, -105.1033781591728 40.1457986582683, -105.1033239976599 40.14594537180952, -105.1032931256744 40.14613706866657, -105.1032734493735 40.14644982251246, -105.103097277509 40.14655653548774, -105.1027896623851 40.14680212506761, -105.1025001051187 40.14700606985371, -105.1025010726383 40.14800394189388, -105.1025050362951 40.14879511117771, -105.1025180890108 40.15145988949109, -105.1025211214181 40.15222689904034, -105.1025218377547 40.15228811819185, -105.1025230471926 40.15232600608753, -105.1025241155214 40.15238805053694, -105.1025269148411 40.15245998279159, -105.1025509038905 40.15331408529797, -105.1025521426915 40.1535918999715, -105.102548967894 40.15474787901242, -105.1025491274585 40.15484313600666, -105.1025509828481 40.15513797217847, -105.1025500235287 40.15524091410313, -105.1025510586691 40.15536993918337, -105.1025408535364 40.15589203525391, -105.1025389095845 40.15597987361276, -105.1025349607258 40.15616598225654, -105.1025273195647 40.15708198833205, -105.1025348528603 40.15734804860777, -105.1025330984857 40.15783201429117, -105.1025300254877 40.15811310850285, -105.1025308525397 40.15833903828675, -105.1025380465539 40.16023089182191, -105.1025414551247 40.16023094317227, -105.1037689994997 40.16021099846859, -105.1049759993214 40.16020199886749, -105.1051399994199 40.16020099938218, -105.1051399989076 40.16020108764328))</t>
+          <t>POLYGON ((-105.10513999890763 40.16020108764328, -105.10514000041587 40.16025199911635, -105.1051410002289 40.16030099923575, -105.10515031730476 40.16030096622104, -105.1068299991866 40.16029499859334, -105.10734500011841 40.16022799895545, -105.1077819997477 40.16013699863746, -105.10820799986311 40.160019999292224, -105.108461998888 40.15992999885013, -105.10861999946009 40.159874998659966, -105.10901499942511 40.159705999101824, -105.10939100029927 40.159511998824776, -105.10974299946521 40.159296998882326, -105.11007200031845 40.159059998662165, -105.1103729990311 40.15880299892639, -105.11044299935288 40.158730998942886, -105.1106439998662 40.15852399914743, -105.1130460729817 40.156157237795234, -105.11318173299078 40.156030043088606, -105.11318331667317 40.1560310309896, -105.1171083166701 40.15216303071296, -105.11710676262885 40.15216074423739, -105.11709903969965 40.15216301978879, -105.11709896096602 40.152163036640104, -105.11683505315172 40.15222089096753, -105.1163498803985 40.15229587185886, -105.1159511562896 40.152329959789256, -105.11556116973053 40.15233689853603, -105.11383797980122 40.15232099564363, -105.11196303164496 40.15231800956109, -105.11196302863969 40.15225596880479, -105.11196302915513 40.15219310487264, -105.11196482641452 40.15162705807939, -105.11196488593201 40.15155199513816, -105.11197020126396 40.15061702541113, -105.11198197194828 40.148682926719104, -105.11199403497098 40.14688104107174, -105.11199367965678 40.14619063122835, -105.11199298402494 40.14549692472122, -105.11199416417462 40.145039035367205, -105.1119931259656 40.14478208466217, -105.11200714703187 40.14470691361935, -105.11206417365264 40.14455502336704, -105.11210714511788 40.14448406724551, -105.11227212563333 40.1443448924646, -105.11240786854 40.144252012414576, -105.11257194408641 40.1441460498956, -105.11268382303544 40.14403497126058, -105.11274085754948 40.143944022726075, -105.11278396630487 40.14378604574785, -105.11279312090427 40.14368587804928, -105.11279509492347 40.143276030669085, -105.11277986336322 40.142746986682994, -105.11273908635239 40.14262112108667, -105.11266284838575 40.142503921479715, -105.11240915454108 40.14214208108856, -105.1120890445636 40.14169793699239, -105.11199909027106 40.14158401244808, -105.11191406339604 40.14145906879407, -105.11134862180728 40.14168839314541, -105.11129310242995 40.141710909806704, -105.11107183854291 40.141810088935436, -105.11086408246017 40.141923863033874, -105.11066983058001 40.142053055350665, -105.11039201264539 40.142220946347464, -105.11027315050282 40.14230207715557, -105.10958406351513 40.14276697772822, -105.10916198049098 40.14307795071951, -105.10844698547054 40.14362895567095, -105.108417879155 40.143651917111924, -105.10826995790363 40.1437469469786, -105.1079030226773 40.14392111893775, -105.10714709353277 40.144247971569385, -105.10705102490346 40.14428305730459, -105.10679392569911 40.144390891258276, -105.10604767802278 40.144655203750375, -105.10589982098013 40.14470394763508, -105.10568382154187 40.14478594833889, -105.10537829709425 40.1448743635278, -105.10516599010879 40.14494700107727, -105.10499902933219 40.145002808926456, -105.10486081134673 40.145049008594576, -105.10475607621049 40.1450840177562, -105.10461670670995 40.14513060227208, -105.10448716618295 40.145173901392944, -105.10434392487782 40.14520086261507, -105.10424100575939 40.14520402266659, -105.10422866591159 40.14533691899432, -105.1041052205383 40.145369907282344, -105.10373777067375 40.14553499119413, -105.10356942987075 40.145658418871704, -105.10337815917278 40.145798658268305, -105.10332399765994 40.14594537180952, -105.10329312567441 40.14613706866657, -105.1032734493735 40.14644982251246, -105.10309727750897 40.14655653548774, -105.10278966238515 40.14680212506761, -105.10250010511871 40.14700606985371, -105.10250107263828 40.14800394189388, -105.1025050362951 40.148795111177705, -105.10251808901076 40.151459889491086, -105.10252112141806 40.15222689904034, -105.10252183775468 40.152288118191855, -105.1025230471926 40.152326006087534, -105.1025241155214 40.15238805053694, -105.10252691484109 40.15245998279159, -105.10255090389055 40.15331408529797, -105.1025521426915 40.153591899971495, -105.10254896789401 40.15474787901242, -105.10254912745849 40.15484313600666, -105.10255098284809 40.15513797217847, -105.10255002352865 40.15524091410313, -105.10255105866906 40.155369939183366, -105.10254085353641 40.155892035253906, -105.10253890958454 40.15597987361276, -105.10253496072579 40.15616598225654, -105.10252731956473 40.15708198833205, -105.10253485286032 40.15734804860777, -105.10253309848568 40.157832014291166, -105.10253002548765 40.158113108502846, -105.10253085253969 40.158339038286755, -105.10253804655386 40.16023089182191, -105.1025414551247 40.16023094317227, -105.10376899949974 40.160210998468585, -105.10497599932141 40.160201998867485, -105.10513999941988 40.16020099938218, -105.10513999890763 40.16020108764328))</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -3604,7 +3616,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.113046069445 40.15615724048531, -105.1106439998662 40.15852399914743, -105.1104429993529 40.15873099894289, -105.1103729990311 40.15880299892639, -105.1100720003185 40.15905999866217, -105.1097429994652 40.15929699888233, -105.1093910002993 40.15951199882478, -105.1090149994251 40.15970599910182, -105.1086199994601 40.15987499865997, -105.108461998888 40.15992999885013, -105.1082079998631 40.16001999929222, -105.1077819997477 40.16013699863746, -105.1073450001184 40.16022799895545, -105.1068299991866 40.16029499859334, -105.1051503173048 40.16030096622104, -105.1051410002289 40.16030099923575, -105.1051400004159 40.16025199911635, -105.1051399989076 40.16020108764328, -105.1051399994199 40.16020099938218, -105.1049759993214 40.16020199886749, -105.1037689994997 40.16021099846859, -105.1025414551247 40.16023094317227, -105.1025380465539 40.16023089182191, -105.1025380471068 40.16023099809953, -105.1025380469332 40.16023102782011, -105.1025371099835 40.16033012490647, -105.1025209099907 40.16157198012871, -105.1025169988298 40.16187393466532, -105.1025181698239 40.1638169634628, -105.1025170800547 40.16388092145418, -105.1025160379682 40.1639369188412, -105.1031840415855 40.16394195935164, -105.103677080317 40.16394612238616, -105.1038330922279 40.16394500997102, -105.1045090132611 40.1639421091939, -105.1047079567183 40.16394196567863, -105.1051648822849 40.1639418802194, -105.1065950219932 40.1639470315879, -105.1066651357448 40.16395001536953, -105.1067341690429 40.16395409331374, -105.1068471620639 40.16396710560917, -105.1069429762893 40.16398088256068, -105.1070108843633 40.1639940160608, -105.1070780652923 40.16400906811618, -105.1082731704586 40.16425497387738, -105.1085479413354 40.16432206318458, -105.1089738343674 40.16443001641591, -105.1100030937519 40.16470910805382, -105.1100988467301 40.16473386278766, -105.1102310199266 40.16477191754039, -105.110289962224 40.16478886190662, -105.1103839012256 40.16481800271197, -105.1104778281293 40.16484906536721, -105.1105710354952 40.16488094870694, -105.1116081561806 40.16522703402034, -105.1116631630715 40.16524396445848, -105.1117160178029 40.1652619855213, -105.1117688604256 40.16528192758562, -105.1118570363875 40.16531791071103, -105.1119209135053 40.16534804808578, -105.1119701511368 40.16537291976826, -105.1120639554807 40.16542594103517, -105.112108879061 40.16545409272166, -105.1125519077741 40.16569687827598, -105.1130901738581 40.16599296203069, -105.1131540349894 40.16602611761037, -105.1132200511067 40.16605790778953, -105.1132850099166 40.16608694924108, -105.113351041756 40.16611599424528, -105.1134188736415 40.16614312416581, -105.1134881502598 40.16616806221542, -105.1135581469168 40.16619190474991, -105.1140391409941 40.16636700585848, -105.114257998739 40.16645311086631, -105.1142990589053 40.16646889471472, -105.1143858335447 40.16649993030593, -105.1144751196768 40.16652987542733, -105.1145640645576 40.1665570750903, -105.114654084047 40.16658400357179, -105.1148070054376 40.16662404329671, -105.1148838304701 40.16664296596607, -105.1149620986271 40.16665997232576, -105.1152809105213 40.16672499648895, -105.1153770639367 40.16674288528087, -105.1154478567137 40.16675300355626, -105.1155039946341 40.16676005319269, -105.115560862259 40.16676490856722, -105.1156180914168 40.16676894283142, -105.1156739004071 40.16677104947827, -105.1157329357246 40.16677206984441, -105.1160449488657 40.16677392990827, -105.1164929344271 40.16677596656673, -105.1165898987154 40.1667771114352, -105.1171939036757 40.16677801553631, -105.1172010077831 40.16634210758333, -105.1171978432182 40.165569061323, -105.1172158396557 40.16529597741587, -105.1172139417619 40.16506098594407, -105.1172139845696 40.16505066564728, -105.1165748537872 40.16504069631765, -105.1165760565016 40.16499226566529, -105.1165841379701 40.16417218994248, -105.1165970657052 40.16325098554722, -105.1165972617726 40.16319765565999, -105.1166030728205 40.16253478804553, -105.1161798614204 40.16245898955479, -105.1152900204082 40.16233002871216, -105.1144081317069 40.16218708707287, -105.1128541752237 40.1619400431437, -105.1124691605463 40.16188110459242, -105.1119180988292 40.1618270976319, -105.1119199845855 40.16162204059638, -105.111922147322 40.1614309849511, -105.1119398694822 40.15970406397353, -105.1119470882641 40.15875206700218, -105.1120558549978 40.15875188276502, -105.1144260887028 40.1587661282411, -105.1155992023579 40.15877635047435, -105.1164088961616 40.15877107998472, -105.1165298328746 40.15877010874338, -105.1166568464329 40.15876998071828, -105.1170668668149 40.15876996742648, -105.1175369714868 40.15877399457021, -105.1175149031218 40.15868991962917, -105.1174591409044 40.15861698847455, -105.1173569140303 40.15853594269353, -105.1172780401464 40.15850109239538, -105.1170558268282 40.15844298275286, -105.1169598643474 40.15839297726098, -105.1167730976391 40.15826690417002, -105.1166159241907 40.15815904714898, -105.1166100273826 40.15774505678377, -105.1166160349168 40.15693305837366, -105.1166568381386 40.15604101638774, -105.1166700602342 40.15420207679241, -105.1166951371468 40.15305303542566, -105.1172200976211 40.15252001746637, -105.1173059253008 40.1524621040393, -105.1174328341978 40.15241503338955, -105.117506960274 40.15240210146893, -105.1179191567963 40.15239001397271, -105.1181098361258 40.15239009487254, -105.1183699045664 40.15239287599296, -105.1184100399258 40.15238093001999, -105.1185979210221 40.152306058452, -105.1185569580286 40.15227407924778, -105.1184530983278 40.15217925452586, -105.1183971615081 40.15212818354858, -105.1183438054582 40.15207946904088, -105.1183070978197 40.15204595469579, -105.1182028332557 40.15194705840466, -105.1180609815329 40.15179809088321, -105.1178293167799 40.15191002952171, -105.1176343172161 40.15199203009031, -105.1174373163797 40.15206603050657, -105.1171083166701 40.15216303071296, -105.1132350662543 40.15598003692975, -105.1131833166732 40.1560310309896, -105.1131817329908 40.15603004308861, -105.113046069445 40.15615724048531))</t>
+          <t>POLYGON ((-105.11304606944503 40.15615724048531, -105.1106439998662 40.15852399914743, -105.11044299935288 40.158730998942886, -105.1103729990311 40.15880299892639, -105.11007200031845 40.159059998662165, -105.10974299946521 40.159296998882326, -105.10939100029927 40.159511998824776, -105.10901499942511 40.159705999101824, -105.10861999946009 40.159874998659966, -105.108461998888 40.15992999885013, -105.10820799986311 40.160019999292224, -105.1077819997477 40.16013699863746, -105.10734500011841 40.16022799895545, -105.1068299991866 40.16029499859334, -105.10515031730476 40.16030096622104, -105.1051410002289 40.16030099923575, -105.10514000041587 40.16025199911635, -105.10513999890763 40.16020108764328, -105.10513999941988 40.16020099938218, -105.10497599932141 40.160201998867485, -105.10376899949974 40.160210998468585, -105.1025414551247 40.16023094317227, -105.10253804655386 40.16023089182191, -105.10253804710682 40.16023099809953, -105.1025380469332 40.16023102782011, -105.10253710998349 40.160330124906466, -105.1025209099907 40.161571980128706, -105.10251699882977 40.16187393466532, -105.10251816982392 40.1638169634628, -105.10251708005468 40.16388092145418, -105.10251603796816 40.1639369188412, -105.10318404158555 40.16394195935164, -105.10367708031696 40.16394612238616, -105.10383309222794 40.16394500997102, -105.10450901326105 40.163942109193904, -105.10470795671833 40.16394196567863, -105.10516488228494 40.1639418802194, -105.10659502199316 40.163947031587895, -105.10666513574483 40.16395001536953, -105.10673416904294 40.16395409331374, -105.10684716206393 40.163967105609174, -105.10694297628926 40.16398088256068, -105.1070108843633 40.163994016060805, -105.10707806529231 40.16400906811618, -105.10827317045857 40.16425497387738, -105.10854794133543 40.164322063184585, -105.10897383436743 40.164430016415906, -105.11000309375193 40.16470910805382, -105.11009884673012 40.16473386278766, -105.11023101992657 40.164771917540385, -105.11028996222399 40.164788861906615, -105.11038390122556 40.16481800271197, -105.11047782812933 40.16484906536721, -105.11057103549523 40.164880948706944, -105.11160815618057 40.16522703402034, -105.11166316307148 40.16524396445848, -105.1117160178029 40.165261985521305, -105.11176886042561 40.16528192758562, -105.11185703638748 40.16531791071103, -105.11192091350534 40.165348048085775, -105.11197015113677 40.16537291976826, -105.1120639554807 40.165425941035174, -105.11210887906095 40.16545409272166, -105.1125519077741 40.16569687827598, -105.11309017385805 40.16599296203069, -105.11315403498939 40.16602611761037, -105.1132200511067 40.16605790778953, -105.11328500991664 40.16608694924108, -105.11335104175605 40.16611599424528, -105.11341887364155 40.16614312416581, -105.11348815025977 40.16616806221542, -105.11355814691676 40.16619190474991, -105.11403914099411 40.16636700585848, -105.11425799873903 40.16645311086631, -105.1142990589053 40.16646889471472, -105.11438583354474 40.16649993030593, -105.11447511967678 40.16652987542733, -105.11456406455758 40.166557075090296, -105.11465408404699 40.16658400357179, -105.11480700543758 40.16662404329671, -105.11488383047015 40.16664296596607, -105.11496209862712 40.16665997232576, -105.1152809105213 40.16672499648895, -105.11537706393668 40.16674288528087, -105.11544785671374 40.16675300355626, -105.11550399463411 40.16676005319269, -105.115560862259 40.16676490856722, -105.11561809141685 40.166768942831425, -105.11567390040715 40.16677104947827, -105.11573293572462 40.166772069844406, -105.11604494886569 40.166773929908274, -105.11649293442713 40.16677596656673, -105.11658989871539 40.1667771114352, -105.1171939036757 40.16677801553631, -105.11720100778314 40.166342107583326, -105.11719784321824 40.165569061323005, -105.11721583965567 40.165295977415866, -105.1172139417619 40.165060985944066, -105.11721398456963 40.16505066564728, -105.11657485378718 40.165040696317654, -105.11657605650164 40.16499226566529, -105.11658413797008 40.164172189942484, -105.11659706570515 40.163250985547215, -105.11659726177261 40.16319765565999, -105.11660307282054 40.16253478804553, -105.11617986142043 40.16245898955479, -105.11529002040822 40.16233002871216, -105.11440813170687 40.162187087072866, -105.11285417522373 40.1619400431437, -105.11246916054628 40.161881104592425, -105.11191809882915 40.1618270976319, -105.1119199845855 40.16162204059638, -105.11192214732199 40.1614309849511, -105.11193986948223 40.15970406397353, -105.1119470882641 40.15875206700218, -105.11205585499783 40.158751882765024, -105.11442608870276 40.158766128241105, -105.11559920235794 40.158776350474355, -105.11640889616157 40.158771079984724, -105.11652983287456 40.15877010874338, -105.11665684643289 40.15876998071828, -105.11706686681494 40.15876996742648, -105.1175369714868 40.15877399457021, -105.11751490312183 40.15868991962917, -105.11745914090439 40.15861698847455, -105.11735691403027 40.158535942693526, -105.11727804014639 40.158501092395376, -105.11705582682825 40.15844298275286, -105.11695986434736 40.15839297726098, -105.11677309763905 40.15826690417002, -105.11661592419067 40.15815904714898, -105.11661002738259 40.15774505678377, -105.11661603491685 40.15693305837366, -105.11665683813858 40.15604101638774, -105.11667006023423 40.15420207679241, -105.1166951371468 40.15305303542566, -105.1172200976211 40.15252001746637, -105.11730592530077 40.1524621040393, -105.11743283419779 40.15241503338955, -105.11750696027399 40.15240210146893, -105.11791915679635 40.152390013972706, -105.11810983612575 40.15239009487254, -105.11836990456644 40.15239287599296, -105.1184100399258 40.152380930019994, -105.11859792102206 40.152306058452, -105.11855695802862 40.15227407924778, -105.11845309832782 40.15217925452586, -105.11839716150807 40.15212818354858, -105.11834380545822 40.15207946904088, -105.11830709781968 40.15204595469579, -105.11820283325568 40.15194705840466, -105.11806098153292 40.15179809088321, -105.1178293167799 40.15191002952171, -105.11763431721609 40.15199203009031, -105.11743731637968 40.15206603050657, -105.1171083166701 40.15216303071296, -105.1132350662543 40.15598003692975, -105.11318331667317 40.1560310309896, -105.11318173299078 40.156030043088606, -105.11304606944503 40.15615724048531))</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -3646,7 +3658,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1129648650939 40.17399302530533, -105.1135388728523 40.17399412254758, -105.1141211221343 40.17399304779159, -105.1152698530993 40.17399495472824, -105.1160359994517 40.17400189448648, -105.116518036311 40.17400294520597, -105.1165319571477 40.1733109383496, -105.1165419082626 40.17262495703965, -105.1165530540567 40.17159995367778, -105.1165560403185 40.17132407516121, -105.1165658865861 40.17059307302266, -105.116570983888 40.17038692899581, -105.1165708265899 40.16977997472073, -105.1165718372282 40.16909286551239, -105.1165759788454 40.16873902862955, -105.1165761090586 40.16858886896271, -105.1165821468334 40.16783506950146, -105.1165920008793 40.16729293305302, -105.1165908282008 40.16724708567887, -105.1165898987154 40.1667771114352, -105.1164929344271 40.16677596656673, -105.1160449488657 40.16677392990827, -105.1157329357246 40.16677206984441, -105.1156739004071 40.16677104947827, -105.1156180914168 40.16676894283142, -105.115560862259 40.16676490856722, -105.1155039946341 40.16676005319269, -105.1154478567137 40.16675300355626, -105.1153770639367 40.16674288528087, -105.1152809105213 40.16672499648895, -105.1149620986271 40.16665997232576, -105.1148838304701 40.16664296596607, -105.1148070054376 40.16662404329671, -105.114654084047 40.16658400357179, -105.1145640645576 40.1665570750903, -105.1144751196768 40.16652987542733, -105.1143858335447 40.16649993030593, -105.1142990589053 40.16646889471472, -105.114257998739 40.16645311086631, -105.1140391409941 40.16636700585848, -105.1135581469168 40.16619190474991, -105.1134881502598 40.16616806221542, -105.1134188736415 40.16614312416581, -105.113351041756 40.16611599424528, -105.1132850099166 40.16608694924108, -105.1132200511067 40.16605790778953, -105.1131540349894 40.16602611761037, -105.1130901738581 40.16599296203069, -105.1125519077741 40.16569687827598, -105.112108879061 40.16545409272166, -105.1120639554807 40.16542594103517, -105.1119701511368 40.16537291976826, -105.1119209135053 40.16534804808578, -105.1118570363875 40.16531791071103, -105.1117688604256 40.16528192758562, -105.1117160178029 40.1652619855213, -105.1116631630715 40.16524396445848, -105.1116081561806 40.16522703402034, -105.1105710354952 40.16488094870694, -105.1104778281293 40.16484906536721, -105.1103839012256 40.16481800271197, -105.110289962224 40.16478886190662, -105.1102310199266 40.16477191754039, -105.1100988467301 40.16473386278766, -105.1100030937519 40.16470910805382, -105.1089738343674 40.16443001641591, -105.1085479413354 40.16432206318458, -105.1082731704586 40.16425497387738, -105.1070780652923 40.16400906811618, -105.1070108843633 40.1639940160608, -105.1069429762893 40.16398088256068, -105.1068471620639 40.16396710560917, -105.1067341690429 40.16395409331374, -105.1066651357448 40.16395001536953, -105.1065950219932 40.1639470315879, -105.1051648822849 40.1639418802194, -105.1047079567183 40.16394196567863, -105.1045090132611 40.1639421091939, -105.1038330922279 40.16394500997102, -105.103677080317 40.16394612238616, -105.1031840415855 40.16394195935164, -105.1025160379682 40.1639369188412, -105.1025141437187 40.1657308741228, -105.1025060264547 40.16736503926331, -105.1025081247895 40.16902696535896, -105.1025021205653 40.17066690196754, -105.1024978523519 40.17231590278406, -105.102497972706 40.17264610216935, -105.1024980637468 40.17289211231032, -105.1024899190531 40.17355092136356, -105.1024948495252 40.17393196664215, -105.1031539808862 40.17394109419757, -105.1037841434783 40.17394709886039, -105.104960093369 40.17394508381765, -105.1055809814998 40.17394610608032, -105.1061850487927 40.17394706770438, -105.1068388827713 40.17394407772057, -105.1071749152855 40.17394412134063, -105.1074021595161 40.17394407015826, -105.1078341011998 40.17394388906459, -105.1083290304438 40.17394309660612, -105.1085748492892 40.17394887014564, -105.1092240015637 40.17395106642266, -105.1098341136038 40.17395889228536, -105.1101958776593 40.17396505455947, -105.1104410147507 40.17396505683724, -105.1110468951035 40.17396188144068, -105.1117388825559 40.17398287436851, -105.1129648650939 40.17399302530533))</t>
+          <t>POLYGON ((-105.11296486509387 40.17399302530533, -105.11353887285227 40.173994122547576, -105.11412112213432 40.17399304779159, -105.1152698530993 40.17399495472824, -105.11603599945174 40.17400189448648, -105.11651803631102 40.17400294520597, -105.11653195714767 40.1733109383496, -105.11654190826259 40.17262495703965, -105.11655305405665 40.17159995367778, -105.1165560403185 40.17132407516121, -105.11656588658606 40.17059307302266, -105.11657098388795 40.17038692899581, -105.11657082658994 40.169779974720726, -105.1165718372282 40.16909286551239, -105.11657597884539 40.168739028629545, -105.11657610905856 40.16858886896271, -105.11658214683338 40.16783506950146, -105.11659200087932 40.16729293305302, -105.11659082820076 40.16724708567887, -105.11658989871539 40.1667771114352, -105.11649293442713 40.16677596656673, -105.11604494886569 40.166773929908274, -105.11573293572462 40.166772069844406, -105.11567390040715 40.16677104947827, -105.11561809141685 40.166768942831425, -105.115560862259 40.16676490856722, -105.11550399463411 40.16676005319269, -105.11544785671374 40.16675300355626, -105.11537706393668 40.16674288528087, -105.1152809105213 40.16672499648895, -105.11496209862712 40.16665997232576, -105.11488383047015 40.16664296596607, -105.11480700543758 40.16662404329671, -105.11465408404699 40.16658400357179, -105.11456406455758 40.166557075090296, -105.11447511967678 40.16652987542733, -105.11438583354474 40.16649993030593, -105.1142990589053 40.16646889471472, -105.11425799873903 40.16645311086631, -105.11403914099411 40.16636700585848, -105.11355814691676 40.16619190474991, -105.11348815025977 40.16616806221542, -105.11341887364155 40.16614312416581, -105.11335104175605 40.16611599424528, -105.11328500991664 40.16608694924108, -105.1132200511067 40.16605790778953, -105.11315403498939 40.16602611761037, -105.11309017385805 40.16599296203069, -105.1125519077741 40.16569687827598, -105.11210887906095 40.16545409272166, -105.1120639554807 40.165425941035174, -105.11197015113677 40.16537291976826, -105.11192091350534 40.165348048085775, -105.11185703638748 40.16531791071103, -105.11176886042561 40.16528192758562, -105.1117160178029 40.165261985521305, -105.11166316307148 40.16524396445848, -105.11160815618057 40.16522703402034, -105.11057103549523 40.164880948706944, -105.11047782812933 40.16484906536721, -105.11038390122556 40.16481800271197, -105.11028996222399 40.164788861906615, -105.11023101992657 40.164771917540385, -105.11009884673012 40.16473386278766, -105.11000309375193 40.16470910805382, -105.10897383436743 40.164430016415906, -105.10854794133543 40.164322063184585, -105.10827317045857 40.16425497387738, -105.10707806529231 40.16400906811618, -105.1070108843633 40.163994016060805, -105.10694297628926 40.16398088256068, -105.10684716206393 40.163967105609174, -105.10673416904294 40.16395409331374, -105.10666513574483 40.16395001536953, -105.10659502199316 40.163947031587895, -105.10516488228494 40.1639418802194, -105.10470795671833 40.16394196567863, -105.10450901326105 40.163942109193904, -105.10383309222794 40.16394500997102, -105.10367708031696 40.16394612238616, -105.10318404158555 40.16394195935164, -105.10251603796816 40.1639369188412, -105.10251414371872 40.1657308741228, -105.10250602645473 40.16736503926331, -105.10250812478945 40.16902696535896, -105.10250212056526 40.170666901967536, -105.10249785235186 40.17231590278406, -105.10249797270599 40.172646102169345, -105.1024980637468 40.17289211231032, -105.1024899190531 40.17355092136356, -105.10249484952516 40.17393196664215, -105.10315398088623 40.17394109419757, -105.10378414347832 40.17394709886039, -105.10496009336902 40.17394508381765, -105.10558098149984 40.173946106080315, -105.10618504879267 40.173947067704376, -105.10683888277134 40.17394407772057, -105.10717491528548 40.17394412134063, -105.10740215951606 40.17394407015826, -105.10783410119977 40.17394388906459, -105.10832903044376 40.17394309660612, -105.1085748492892 40.173948870145644, -105.10922400156372 40.17395106642266, -105.10983411360375 40.173958892285356, -105.11019587765927 40.173965054559474, -105.11044101475073 40.17396505683724, -105.11104689510346 40.17396188144068, -105.11173888255588 40.173982874368505, -105.11296486509387 40.17399302530533))</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -3688,10 +3700,14 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.093035412355 40.17395404356559, -105.0930355022931 40.17396373747397, -105.0930905495083 40.1739629603663, -105.0933063695626 40.17394767675843, -105.0947811388498 40.17392604651604, -105.0950699350661 40.17392596063161, -105.0955101015059 40.1739269531794, -105.0957541527641 40.17392890476933, -105.0963270854283 40.17393008282001, -105.0964931512326 40.17392709427654, -105.0974990948966 40.17392895400177, -105.0977370735687 40.17392895919532, -105.0979528772734 40.17392696481058, -105.0981518434555 40.1739279313386, -105.0989699184054 40.17392802714794, -105.0998391512321 40.17393103942207, -105.1001161310761 40.17393199790583, -105.101211927436 40.17392892050625, -105.1023799809039 40.17393102219533, -105.1024508498185 40.17392907018132, -105.1024948495252 40.17393196664215, -105.1024899190531 40.17355092136356, -105.1024980637468 40.17289211231032, -105.102497972706 40.17264610216935, -105.1024978523519 40.17231590278406, -105.1025021205653 40.17066690196754, -105.1025081247895 40.16902696535896, -105.1025060264547 40.16736503926331, -105.1025141437187 40.1657308741228, -105.1025160379682 40.1639369188412, -105.1025170800547 40.16388092145418, -105.1025181698239 40.1638169634628, -105.1025169988298 40.16187393466532, -105.1025209099907 40.16157198012871, -105.1025371099835 40.16033012490647, -105.1025380469332 40.16023102782011, -105.1025380471068 40.16023099809953, -105.1025380465539 40.16023089182191, -105.1024143180025 40.16022903062637, -105.101072318054 40.16022203122495, -105.1010700959203 40.16022203616376, -105.1010699280626 40.16022203558438, -105.1010630001934 40.16022199906198, -105.0998739874729 40.16022399957189, -105.0967180002406 40.1602330001241, -105.0960982895062 40.16023918860394, -105.0960170000153 40.16023999516622, -105.0960168884854 40.16023999747829, -105.095906860969 40.16024372245906, -105.0951589994661 40.16026899899504, -105.0948714164467 40.16027221347903, -105.0946219991399 40.16027500002095, -105.0944589999225 40.16027599890212, -105.0943463028096 40.16027599968295, -105.0942474912358 40.16027599866759, -105.0941529994326 40.16027600012808, -105.0933151831979 40.16027514992445, -105.0931679955306 40.16027501197318, -105.0931099998072 40.16041499996014, -105.0931024819559 40.16045158549526, -105.0930949991611 40.1604880000312, -105.0930969990843 40.16066999982127, -105.093074999123 40.16093800027746, -105.0930749994591 40.16106100006206, -105.0930749990154 40.16110699945172, -105.0931069998108 40.1613119217147, -105.0931069993422 40.16131200006891, -105.0931149989175 40.16163199930823, -105.0931129997678 40.16178000016573, -105.0931070642517 40.16237164155648, -105.0931070011848 40.1623778683723, -105.0931070004038 40.1623779989626, -105.0931050119728 40.16313991872316, -105.0931050114934 40.1631399988786, -105.0931040000302 40.16325199822559, -105.0931039998199 40.16329599907725, -105.0931469291512 40.16390871444782, -105.0931479999207 40.16392399940396, -105.0931480029145 40.16392408767742, -105.0931569991541 40.16423199918421, -105.0931259993862 40.16516199880555, -105.0931289999454 40.16569099842605, -105.0931319995954 40.16601699884203, -105.093122999789 40.1669069989264, -105.0931289996238 40.16735399928291, -105.0931369998561 40.16781299868737, -105.0931339988095 40.16872599950739, -105.0931369991391 40.16900499892864, -105.0931479994263 40.17023599850143, -105.0931500001353 40.17054199825319, -105.093151000261 40.17065999832266, -105.0931330003842 40.17149199908522, -105.0931459999594 40.17231399916508, -105.0930759995535 40.17368299823816, -105.093035999663 40.17395399970057, -105.093035412355 40.17395404356559))</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr"/>
+          <t>POLYGON ((-105.09303541235504 40.17395404356559, -105.09303550229312 40.17396373747397, -105.09309054950829 40.173962960366296, -105.0933063695626 40.17394767675843, -105.09478113884975 40.17392604651604, -105.09506993506612 40.17392596063161, -105.09551010150588 40.173926953179404, -105.09575415276406 40.17392890476933, -105.09632708542826 40.17393008282001, -105.0964931512326 40.173927094276536, -105.09749909489656 40.173928954001774, -105.09773707356871 40.173928959195315, -105.09795287727341 40.173926964810576, -105.09815184345548 40.1739279313386, -105.09896991840537 40.17392802714794, -105.0998391512321 40.17393103942207, -105.10011613107612 40.17393199790583, -105.10121192743595 40.17392892050625, -105.10237998090392 40.173931022195326, -105.10245084981848 40.173929070181316, -105.10249484952516 40.17393196664215, -105.1024899190531 40.17355092136356, -105.1024980637468 40.17289211231032, -105.10249797270599 40.172646102169345, -105.10249785235186 40.17231590278406, -105.10250212056526 40.170666901967536, -105.10250812478945 40.16902696535896, -105.10250602645473 40.16736503926331, -105.10251414371872 40.1657308741228, -105.10251603796816 40.1639369188412, -105.10251708005468 40.16388092145418, -105.10251816982392 40.1638169634628, -105.10251699882977 40.16187393466532, -105.1025209099907 40.161571980128706, -105.10253710998349 40.160330124906466, -105.1025380469332 40.16023102782011, -105.10253804710682 40.16023099809953, -105.10253804655386 40.16023089182191, -105.10241431800253 40.16022903062637, -105.10107231805398 40.16022203122495, -105.10107009592029 40.16022203616376, -105.10106992806263 40.160222035584376, -105.10106300019336 40.16022199906198, -105.09987398747286 40.16022399957189, -105.09671800024059 40.1602330001241, -105.0960982895062 40.16023918860394, -105.09601700001525 40.16023999516622, -105.09601688848535 40.16023999747829, -105.09590686096895 40.16024372245906, -105.09515899946608 40.160268998995036, -105.09487141644672 40.16027221347903, -105.09462199913989 40.16027500002095, -105.09445899992254 40.16027599890212, -105.09434630280961 40.16027599968295, -105.09424749123583 40.16027599866759, -105.09415299943264 40.16027600012808, -105.09331518319786 40.16027514992445, -105.0931679955306 40.16027501197318, -105.09310999980721 40.16041499996014, -105.09310248195592 40.16045158549526, -105.09309499916112 40.1604880000312, -105.09309699908425 40.16066999982127, -105.09307499912298 40.16093800027746, -105.0930749994591 40.16106100006206, -105.09307499901536 40.16110699945172, -105.09310699981081 40.1613119217147, -105.09310699934221 40.16131200006891, -105.0931149989175 40.16163199930823, -105.09311299976775 40.16178000016573, -105.09310706425171 40.162371641556476, -105.09310700118482 40.162377868372296, -105.09310700040379 40.1623779989626, -105.09310501197284 40.16313991872316, -105.09310501149345 40.1631399988786, -105.09310400003017 40.16325199822559, -105.09310399981993 40.16329599907725, -105.0931469291512 40.16390871444782, -105.09314799992066 40.16392399940396, -105.09314800291452 40.163924087677415, -105.09315699915409 40.16423199918421, -105.09312599938616 40.16516199880555, -105.0931289999454 40.16569099842605, -105.09313199959539 40.16601699884203, -105.093122999789 40.1669069989264, -105.0931289996238 40.16735399928291, -105.09313699985609 40.16781299868737, -105.09313399880948 40.16872599950739, -105.09313699913912 40.16900499892864, -105.09314799942635 40.17023599850143, -105.09315000013525 40.170541998253185, -105.09315100026096 40.170659998322655, -105.09313300038424 40.17149199908522, -105.09314599995942 40.17231399916508, -105.09307599955353 40.173682998238164, -105.09303599966297 40.17395399970057, -105.09303541235504 40.17395404356559))</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Altona MS</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3726,7 +3742,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0830771760332 40.1739901157939, -105.0830771458684 40.17399043991578, -105.088302814376 40.1739809907825, -105.0883029993709 40.17397700160376, -105.0883031426125 40.17397700121329, -105.0883123178483 40.17397704920117, -105.0888742073944 40.17397999371771, -105.0892635502055 40.17397922794395, -105.0898870002667 40.17397799833534, -105.0899358508228 40.17397797709733, -105.0920959995587 40.17397699788575, -105.0920961416262 40.17397699748644, -105.0920962144237 40.17397699684266, -105.0928349994319 40.17396899906539, -105.0928751701174 40.17396600181887, -105.093035412355 40.17395404356559, -105.093035999663 40.17395399970057, -105.0930759995535 40.17368299823816, -105.0931459999594 40.17231399916508, -105.0931330003842 40.17149199908522, -105.093151000261 40.17065999832266, -105.0931500001353 40.17054199825319, -105.0931479994263 40.17023599850143, -105.0931369991391 40.16900499892864, -105.0931339988095 40.16872599950739, -105.0931369998561 40.16781299868737, -105.0931289996238 40.16735399928291, -105.093122999789 40.1669069989264, -105.0931319995954 40.16601699884203, -105.0931289999454 40.16569099842605, -105.0931259993862 40.16516199880555, -105.0931569991541 40.16423199918421, -105.0931480029145 40.16392408767742, -105.0931479999207 40.16392399940396, -105.0931469291512 40.16390871444782, -105.0931039998199 40.16329599907725, -105.0931040000302 40.16325199822559, -105.0931050114934 40.1631399988786, -105.0931050119728 40.16313991872316, -105.0931070004038 40.1623779989626, -105.0931070011848 40.1623778683723, -105.0925199158311 40.16237689791628, -105.0917190936679 40.16238697525812, -105.0909838252546 40.16238410086513, -105.089468094328 40.16239711982808, -105.0886809584908 40.16239212456986, -105.0881623938254 40.1623954782369, -105.0881598089886 40.16280928973737, -105.0881648387267 40.16306998948579, -105.0881668740553 40.16350208512876, -105.0881650625537 40.16356494168014, -105.0881693626968 40.16382478228903, -105.0881761464068 40.16392102833853, -105.083609519032 40.16392308127849, -105.0836161082395 40.16399500687811, -105.0836141587786 40.16413802271901, -105.0836030415373 40.16460987586909, -105.0836106635436 40.16484891209912, -105.0836300593452 40.16545713053579, -105.0836269525403 40.16549692411329, -105.0836220561698 40.16553698593949, -105.083613938554 40.16557703616078, -105.0835959221352 40.16565603140108, -105.0835711141966 40.16573390518737, -105.0835558587693 40.16577090983481, -105.0835398631979 40.16581202954788, -105.0835210296103 40.16584902129782, -105.0835000500647 40.16588600531175, -105.0834769351456 40.1659210605575, -105.0834260412004 40.16599307439358, -105.0833268254032 40.1661261315451, -105.0832439014171 40.16622795275293, -105.0832150677106 40.16626188854235, -105.0831919525168 40.16629694372924, -105.0831681144781 40.16633309328626, -105.0831478259643 40.16637392366613, -105.0831339771326 40.16641505106289, -105.0831190490881 40.16645699775201, -105.0831080505025 40.16650005739481, -105.0830950003841 40.16658593425269, -105.0830878765151 40.16693097503487, -105.0830959771383 40.16724395293009, -105.0830960976557 40.16792502758191, -105.0830930531922 40.16830494684462, -105.0830910643746 40.16868788974446, -105.0830899607455 40.16886796812796, -105.0830891382825 40.16941095828075, -105.0830898739331 40.16975794923593, -105.0830908276374 40.17077009335227, -105.0830780316235 40.17151508279193, -105.083075148123 40.17192712109441, -105.083080876397 40.17274410150467, -105.0830810478255 40.17329999660924, -105.0830759771914 40.17348500237775, -105.0830749017534 40.17371888591792, -105.0830771760332 40.1739901157939))</t>
+          <t>POLYGON ((-105.08307717603323 40.1739901157939, -105.0830771458684 40.17399043991578, -105.08830281437605 40.173980990782496, -105.08830299937091 40.17397700160376, -105.08830314261247 40.17397700121329, -105.08831231784832 40.17397704920117, -105.0888742073944 40.17397999371771, -105.08926355020547 40.17397922794395, -105.08988700026669 40.17397799833534, -105.08993585082284 40.17397797709733, -105.09209599955867 40.17397699788575, -105.09209614162616 40.17397699748644, -105.09209621442366 40.17397699684266, -105.09283499943187 40.173968999065394, -105.09287517011735 40.17396600181887, -105.09303541235504 40.17395404356559, -105.09303599966297 40.17395399970057, -105.09307599955353 40.173682998238164, -105.09314599995942 40.17231399916508, -105.09313300038424 40.17149199908522, -105.09315100026096 40.170659998322655, -105.09315000013525 40.170541998253185, -105.09314799942635 40.17023599850143, -105.09313699913912 40.16900499892864, -105.09313399880948 40.16872599950739, -105.09313699985609 40.16781299868737, -105.0931289996238 40.16735399928291, -105.093122999789 40.1669069989264, -105.09313199959539 40.16601699884203, -105.0931289999454 40.16569099842605, -105.09312599938616 40.16516199880555, -105.09315699915409 40.16423199918421, -105.09314800291452 40.163924087677415, -105.09314799992066 40.16392399940396, -105.0931469291512 40.16390871444782, -105.09310399981993 40.16329599907725, -105.09310400003017 40.16325199822559, -105.09310501149345 40.1631399988786, -105.09310501197284 40.16313991872316, -105.09310700040379 40.1623779989626, -105.09310700118482 40.162377868372296, -105.09251991583112 40.16237689791628, -105.09171909366789 40.16238697525812, -105.09098382525458 40.162384100865125, -105.08946809432798 40.16239711982808, -105.08868095849083 40.162392124569855, -105.08816239382541 40.162395478236895, -105.08815980898855 40.162809289737375, -105.08816483872667 40.16306998948579, -105.08816687405532 40.16350208512876, -105.08816506255374 40.163564941680136, -105.08816936269676 40.16382478228903, -105.08817614640682 40.16392102833853, -105.083609519032 40.16392308127849, -105.08361610823951 40.16399500687811, -105.08361415877863 40.16413802271901, -105.08360304153727 40.16460987586909, -105.08361066354364 40.164848912099124, -105.08363005934517 40.16545713053579, -105.08362695254029 40.16549692411329, -105.08362205616976 40.16553698593949, -105.08361393855401 40.165577036160784, -105.08359592213525 40.165656031401085, -105.08357111419664 40.165733905187366, -105.08355585876932 40.16577090983481, -105.08353986319791 40.16581202954788, -105.08352102961028 40.165849021297824, -105.08350005006473 40.16588600531175, -105.08347693514555 40.1659210605575, -105.08342604120041 40.16599307439358, -105.08332682540323 40.1661261315451, -105.08324390141712 40.16622795275293, -105.0832150677106 40.16626188854235, -105.08319195251681 40.166296943729236, -105.08316811447813 40.16633309328626, -105.08314782596429 40.16637392366613, -105.08313397713256 40.16641505106289, -105.08311904908807 40.166456997752015, -105.0831080505025 40.16650005739481, -105.08309500038412 40.16658593425269, -105.08308787651507 40.16693097503487, -105.08309597713834 40.167243952930086, -105.08309609765571 40.16792502758191, -105.08309305319224 40.16830494684462, -105.08309106437456 40.16868788974446, -105.08308996074547 40.16886796812796, -105.08308913828246 40.16941095828075, -105.08308987393313 40.16975794923593, -105.08309082763743 40.170770093352274, -105.08307803162349 40.17151508279193, -105.08307514812302 40.171927121094406, -105.08308087639703 40.17274410150467, -105.08308104782546 40.17329999660924, -105.08307597719143 40.173485002377745, -105.08307490175343 40.17371888591792, -105.08307717603323 40.1739901157939))</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -3768,7 +3784,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0742231786078 40.16392547155616, -105.0742215999097 40.16416458903731, -105.0742090610333 40.16507712783093, -105.0741958388199 40.1669369918969, -105.0741638490064 40.16707413190915, -105.0741380236129 40.16776993589061, -105.0741261470178 40.16858108777058, -105.0741240911042 40.17022405894838, -105.0741420367103 40.17175894537512, -105.0741348956377 40.17409999127664, -105.0750621597752 40.17409407028626, -105.076705975677 40.17407100247446, -105.0768720438574 40.17406804212276, -105.0774139014207 40.17405986681544, -105.0775441759869 40.17405787252455, -105.0784149087419 40.17405007076083, -105.0790899520972 40.17403194202814, -105.0793730489725 40.17402803066916, -105.0805848880472 40.17400992414674, -105.081386942714 40.1739969089824, -105.0817029589484 40.1739931120255, -105.0830771760332 40.1739901157939, -105.0830749017534 40.17371888591792, -105.0830759771914 40.17348500237775, -105.0830810478255 40.17329999660924, -105.083080876397 40.17274410150467, -105.083075148123 40.17192712109441, -105.0830780316235 40.17151508279193, -105.0830908276374 40.17077009335227, -105.0830898739331 40.16975794923593, -105.0830891382825 40.16941095828075, -105.0830899607455 40.16886796812796, -105.0830910643746 40.16868788974446, -105.0830930531922 40.16830494684462, -105.0830960976557 40.16792502758191, -105.0830959771383 40.16724395293009, -105.0830878765151 40.16693097503487, -105.0830950003841 40.16658593425269, -105.0831080505025 40.16650005739481, -105.0831190490881 40.16645699775201, -105.0831339771326 40.16641505106289, -105.0831478259643 40.16637392366613, -105.0831681144781 40.16633309328626, -105.0831919525168 40.16629694372924, -105.0832150677106 40.16626188854235, -105.0832439014171 40.16622795275293, -105.0833268254032 40.1661261315451, -105.0834260412004 40.16599307439358, -105.0834769351456 40.1659210605575, -105.0835000500647 40.16588600531175, -105.0835210296103 40.16584902129782, -105.0835398631979 40.16581202954788, -105.0835558587693 40.16577090983481, -105.0835711141966 40.16573390518737, -105.0835959221352 40.16565603140108, -105.083613938554 40.16557703616078, -105.0836220561698 40.16553698593949, -105.0836269525403 40.16549692411329, -105.0836300593452 40.16545713053579, -105.0836106635436 40.16484891209912, -105.0836030415373 40.16460987586909, -105.0836141587786 40.16413802271901, -105.0836161082395 40.16399500687811, -105.083609519032 40.16392308127849, -105.0829128177578 40.16392203457659, -105.0813998304982 40.16392203444205, -105.0807888352324 40.1639220337433, -105.0802848402826 40.16392203294821, -105.0795948459216 40.16388103180415, -105.0787978532788 40.16380003091128, -105.0775498655427 40.16357702807103, -105.0756918859996 40.16302902328239, -105.0744968993014 40.16262302002178, -105.0739259058449 40.16241901849396, -105.0738611778402 40.16249747081726, -105.0737631785805 40.16272347069402, -105.0737421773876 40.16283947077967, -105.073754178833 40.16295347066195, -105.0738071777814 40.16305847119569, -105.0739731785512 40.1632404708329, -105.0740821782435 40.16340247036388, -105.0741431786743 40.16353047110911, -105.0742051785918 40.1637754707742, -105.0742231786078 40.16392547155616))</t>
+          <t>POLYGON ((-105.07422317860775 40.16392547155616, -105.07422159990975 40.164164589037306, -105.07420906103332 40.16507712783093, -105.0741958388199 40.1669369918969, -105.07416384900642 40.16707413190915, -105.07413802361292 40.16776993589061, -105.07412614701776 40.16858108777058, -105.07412409110422 40.17022405894838, -105.07414203671033 40.171758945375124, -105.07413489563774 40.17409999127664, -105.07506215977516 40.17409407028626, -105.07670597567699 40.174071002474456, -105.07687204385743 40.174068042122755, -105.07741390142073 40.17405986681544, -105.07754417598686 40.17405787252455, -105.07841490874192 40.174050070760835, -105.07908995209725 40.17403194202814, -105.07937304897254 40.174028030669156, -105.08058488804723 40.174009924146745, -105.08138694271403 40.1739969089824, -105.08170295894837 40.1739931120255, -105.08307717603323 40.1739901157939, -105.08307490175343 40.17371888591792, -105.08307597719143 40.173485002377745, -105.08308104782546 40.17329999660924, -105.08308087639703 40.17274410150467, -105.08307514812302 40.171927121094406, -105.08307803162349 40.17151508279193, -105.08309082763743 40.170770093352274, -105.08308987393313 40.16975794923593, -105.08308913828246 40.16941095828075, -105.08308996074547 40.16886796812796, -105.08309106437456 40.16868788974446, -105.08309305319224 40.16830494684462, -105.08309609765571 40.16792502758191, -105.08309597713834 40.167243952930086, -105.08308787651507 40.16693097503487, -105.08309500038412 40.16658593425269, -105.0831080505025 40.16650005739481, -105.08311904908807 40.166456997752015, -105.08313397713256 40.16641505106289, -105.08314782596429 40.16637392366613, -105.08316811447813 40.16633309328626, -105.08319195251681 40.166296943729236, -105.0832150677106 40.16626188854235, -105.08324390141712 40.16622795275293, -105.08332682540323 40.1661261315451, -105.08342604120041 40.16599307439358, -105.08347693514555 40.1659210605575, -105.08350005006473 40.16588600531175, -105.08352102961028 40.165849021297824, -105.08353986319791 40.16581202954788, -105.08355585876932 40.16577090983481, -105.08357111419664 40.165733905187366, -105.08359592213525 40.165656031401085, -105.08361393855401 40.165577036160784, -105.08362205616976 40.16553698593949, -105.08362695254029 40.16549692411329, -105.08363005934517 40.16545713053579, -105.08361066354364 40.164848912099124, -105.08360304153727 40.16460987586909, -105.08361415877863 40.16413802271901, -105.08361610823951 40.16399500687811, -105.083609519032 40.16392308127849, -105.08291281775779 40.16392203457659, -105.08139983049817 40.16392203444205, -105.08078883523244 40.1639220337433, -105.08028484028256 40.16392203294821, -105.07959484592165 40.16388103180415, -105.07879785327876 40.16380003091128, -105.07754986554265 40.16357702807103, -105.07569188599962 40.16302902328239, -105.07449689930137 40.16262302002178, -105.07392590584493 40.16241901849396, -105.07386117784016 40.162497470817264, -105.07376317858052 40.16272347069402, -105.07374217738763 40.162839470779666, -105.07375417883298 40.16295347066195, -105.07380717778136 40.16305847119569, -105.07397317855124 40.1632404708329, -105.07408217824351 40.16340247036388, -105.07414317867435 40.163530471109105, -105.07420517859181 40.1637754707742, -105.07422317860775 40.16392547155616))</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -3810,7 +3826,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0670660565744 40.17763371171144, -105.0670663900754 40.177730367958, -105.0670932333527 40.18157908311534, -105.0681970778381 40.1815609933296, -105.0705671335802 40.18150201555372, -105.071855079057 40.1814689097076, -105.0736709800798 40.18142812870585, -105.0741588784485 40.18141592642099, -105.074182886726 40.18032508999734, -105.0741650450267 40.17871608683249, -105.0741679464936 40.17762379964213, -105.0741689057888 40.17724195131272, -105.0741588320919 40.17679308076072, -105.0741524295275 40.17570984374514, -105.074151011784 40.17546988524433, -105.0741348956377 40.17409999127664, -105.0741420367103 40.17175894537512, -105.0741240911042 40.17022405894838, -105.0741261470178 40.16858108777058, -105.0741380236129 40.16776993589061, -105.0741584163987 40.16722051667698, -105.0741638490064 40.16707413190915, -105.0741958388199 40.1669369918969, -105.0742090610333 40.16507712783093, -105.0742215999097 40.16416458903731, -105.0742231786078 40.16392547155616, -105.0742051785918 40.1637754707742, -105.0741431786743 40.16353047110911, -105.0740821782435 40.16340247036388, -105.0739731785512 40.1632404708329, -105.0738071777814 40.16305847119569, -105.073754178833 40.16295347066195, -105.0737421773876 40.16283947077967, -105.0737631785805 40.16272347069402, -105.0738611778402 40.16249747081726, -105.0739259058449 40.16241901849396, -105.0730759142553 40.16213901527696, -105.0719189271613 40.16175401236442, -105.0705369421375 40.16129000865394, -105.0694629539653 40.16092000499503, -105.0694111630307 40.16090422372054, -105.0689725401897 40.16113013534599, -105.0684992704832 40.16135539178723, -105.0689887855424 40.1618894461977, -105.0690794916851 40.1619889533341, -105.0692646761394 40.16219209918427, -105.0693539608267 40.1622900444892, -105.0694449513376 40.16238986040845, -105.0695365017366 40.16249028447161, -105.0696730762008 40.16262018933153, -105.0697765395714 40.16271473582595, -105.0699787471539 40.16289951940838, -105.0701550066105 40.16305681397562, -105.0703804641565 40.16323529954771, -105.0711107510569 40.16381343696385, -105.0716009565898 40.16400079816211, -105.0716063693274 40.16433043272091, -105.0716146066078 40.16498277526175, -105.0710065092227 40.1648152438267, -105.0700625038011 40.16454979057855, -105.0696307602086 40.16454426598023, -105.0689869716922 40.16455176868926, -105.0686456338963 40.16455287570224, -105.0684789369425 40.16475923917578, -105.0682378207239 40.16505772046782, -105.0680545246087 40.16528489551064, -105.0680270215794 40.16543056534422, -105.0679624680124 40.16577246289581, -105.0679475088123 40.16585168964777, -105.0680775020221 40.16608425757718, -105.0682505460679 40.16639383349164, -105.068431855338 40.16671819881601, -105.0685881730954 40.16699784732862, -105.0685888605255 40.16705920435815, -105.0685909942695 40.16751728354365, -105.0686323263576 40.16760712016501, -105.0687296043239 40.16781962045806, -105.0688340700417 40.16805157342573, -105.0689685835843 40.16818978871847, -105.0690924732613 40.16831925413381, -105.0692236861258 40.16845846733594, -105.0690669467599 40.16870070883218, -105.0689954745381 40.16881117180088, -105.069001375795 40.16925225627143, -105.0691851660852 40.16949232218418, -105.0693083248916 40.16954815441962, -105.0694904125201 40.1696307011031, -105.069593849699 40.16967759275655, -105.069770804172 40.16980021285955, -105.0699965925169 40.16995667405463, -105.0700839003286 40.17001717250243, -105.0701130518095 40.17012801034537, -105.070130222646 40.1701932959897, -105.0700903919518 40.17038641030021, -105.0700654619531 40.17050725216793, -105.0700490748938 40.17058729610622, -105.0701873071285 40.17085983825155, -105.0703213021316 40.17112402272167, -105.0704140291814 40.17115210803604, -105.0706892573018 40.17123797281743, -105.0708035182736 40.17127361762239, -105.0709274429077 40.17147883318172, -105.0709656546354 40.17154231984762, -105.0711494002002 40.17166902037516, -105.0713919649312 40.17183679362187, -105.0715316809831 40.17193354874935, -105.0715257345117 40.17197993947205, -105.0715024987211 40.17216110206002, -105.071493494646 40.17223903902581, -105.0714151828517 40.172324112408, -105.0712322250403 40.17252357899062, -105.0711711597935 40.17259038091576, -105.0709653184227 40.17265834146566, -105.0708027271205 40.17271196641693, -105.0706089644674 40.1727774133586, -105.0704758464944 40.17286042088165, -105.0702143999142 40.1730234451326, -105.0701781533955 40.17325428528496, -105.0702866310458 40.173576234709, -105.0702945408748 40.17360039409835, -105.07033336786 40.1737189889846, -105.0703699476555 40.17383072432401, -105.0704526828224 40.17398700036528, -105.0704676384679 40.17401525411931, -105.0705337647592 40.17417980111477, -105.0682879316216 40.17423889546469, -105.0679761762959 40.1742478872944, -105.067719899077 40.17425488999454, -105.0674951080714 40.17426310871814, -105.0648471501122 40.17433607520882, -105.0648456787189 40.17433611380135, -105.0648251809503 40.17521009306972, -105.0648232919619 40.17529063303029, -105.0648230964495 40.17529898664483, -105.0648193538381 40.17552207135812, -105.0648015744186 40.17658180266726, -105.0647999073873 40.17663002753556, -105.0647640413511 40.1768099757366, -105.0645142074258 40.17729412114653, -105.0644352911514 40.17744601058907, -105.0644334584831 40.17745551625659, -105.0645251580844 40.17747706551972, -105.0648269026477 40.17755689531555, -105.0649588454808 40.17757496072856, -105.066045045976 40.17757108247091, -105.0669959168821 40.17757492265862, -105.0670664737271 40.17756559058409, -105.0670660565744 40.17763371171144))</t>
+          <t>POLYGON ((-105.06706605657438 40.177633711711444, -105.06706639007544 40.177730367958, -105.06709323335268 40.18157908311534, -105.06819707783808 40.181560993329605, -105.07056713358017 40.18150201555372, -105.07185507905702 40.181468909707604, -105.07367098007978 40.18142812870585, -105.0741588784485 40.18141592642099, -105.07418288672598 40.18032508999734, -105.07416504502673 40.17871608683249, -105.07416794649365 40.17762379964213, -105.07416890578881 40.177241951312716, -105.07415883209191 40.176793080760724, -105.07415242952753 40.17570984374514, -105.07415101178397 40.17546988524433, -105.07413489563774 40.17409999127664, -105.07414203671033 40.171758945375124, -105.07412409110422 40.17022405894838, -105.07412614701776 40.16858108777058, -105.07413802361292 40.16776993589061, -105.07415841639869 40.16722051667698, -105.07416384900642 40.16707413190915, -105.0741958388199 40.1669369918969, -105.07420906103332 40.16507712783093, -105.07422159990975 40.164164589037306, -105.07422317860775 40.16392547155616, -105.07420517859181 40.1637754707742, -105.07414317867435 40.163530471109105, -105.07408217824351 40.16340247036388, -105.07397317855124 40.1632404708329, -105.07380717778136 40.16305847119569, -105.07375417883298 40.16295347066195, -105.07374217738763 40.162839470779666, -105.07376317858052 40.16272347069402, -105.07386117784016 40.162497470817264, -105.07392590584493 40.16241901849396, -105.07307591425534 40.16213901527696, -105.0719189271613 40.16175401236442, -105.07053694213745 40.16129000865394, -105.06946295396526 40.16092000499503, -105.06941116303074 40.160904223720536, -105.06897254018966 40.16113013534599, -105.06849927048319 40.16135539178723, -105.06898878554237 40.161889446197705, -105.06907949168506 40.1619889533341, -105.06926467613941 40.16219209918427, -105.06935396082675 40.1622900444892, -105.06944495133762 40.16238986040845, -105.06953650173658 40.16249028447161, -105.06967307620077 40.162620189331534, -105.06977653957138 40.16271473582595, -105.06997874715387 40.162899519408384, -105.07015500661055 40.16305681397562, -105.07038046415646 40.16323529954771, -105.07111075105688 40.16381343696385, -105.07160095658983 40.164000798162114, -105.07160636932743 40.16433043272091, -105.07161460660781 40.16498277526175, -105.07100650922266 40.1648152438267, -105.07006250380113 40.16454979057855, -105.06963076020858 40.16454426598023, -105.06898697169218 40.16455176868926, -105.06864563389628 40.16455287570224, -105.06847893694253 40.16475923917578, -105.06823782072385 40.16505772046782, -105.0680545246087 40.165284895510645, -105.0680270215794 40.165430565344224, -105.06796246801244 40.16577246289581, -105.06794750881227 40.16585168964777, -105.06807750202213 40.166084257577175, -105.06825054606789 40.16639383349164, -105.06843185533805 40.166718198816014, -105.06858817309545 40.16699784732862, -105.06858886052551 40.16705920435815, -105.06859099426948 40.167517283543646, -105.06863232635763 40.16760712016501, -105.06872960432388 40.16781962045806, -105.06883407004166 40.16805157342573, -105.06896858358427 40.16818978871847, -105.06909247326125 40.16831925413381, -105.06922368612577 40.16845846733594, -105.06906694675986 40.168700708832176, -105.06899547453807 40.16881117180088, -105.06900137579503 40.16925225627143, -105.06918516608525 40.16949232218418, -105.0693083248916 40.16954815441962, -105.0694904125201 40.1696307011031, -105.069593849699 40.16967759275655, -105.06977080417197 40.16980021285955, -105.06999659251692 40.16995667405463, -105.07008390032863 40.170017172502426, -105.07011305180946 40.170128010345366, -105.07013022264597 40.1701932959897, -105.07009039195178 40.17038641030021, -105.07006546195315 40.17050725216793, -105.0700490748938 40.17058729610622, -105.07018730712852 40.17085983825155, -105.07032130213159 40.17112402272167, -105.0704140291814 40.17115210803604, -105.07068925730182 40.17123797281743, -105.07080351827359 40.17127361762239, -105.07092744290775 40.171478833181716, -105.07096565463536 40.17154231984762, -105.07114940020016 40.171669020375155, -105.07139196493121 40.17183679362187, -105.0715316809831 40.17193354874935, -105.07152573451172 40.171979939472045, -105.07150249872113 40.172161102060016, -105.071493494646 40.17223903902581, -105.07141518285165 40.172324112408, -105.07123222504028 40.17252357899062, -105.07117115979351 40.17259038091576, -105.07096531842268 40.172658341465656, -105.07080272712045 40.17271196641693, -105.07060896446737 40.1727774133586, -105.07047584649442 40.172860420881655, -105.07021439991418 40.1730234451326, -105.07017815339547 40.17325428528496, -105.07028663104585 40.173576234709, -105.07029454087483 40.17360039409835, -105.07033336786003 40.1737189889846, -105.07036994765555 40.17383072432401, -105.07045268282239 40.17398700036528, -105.07046763846789 40.17401525411931, -105.07053376475923 40.17417980111477, -105.06828793162155 40.17423889546469, -105.0679761762959 40.1742478872944, -105.067719899077 40.17425488999454, -105.06749510807141 40.174263108718144, -105.06484715011224 40.17433607520882, -105.06484567871885 40.17433611380135, -105.06482518095028 40.17521009306972, -105.06482329196194 40.17529063303029, -105.06482309644953 40.17529898664483, -105.06481935383808 40.17552207135812, -105.06480157441857 40.17658180266726, -105.06479990738731 40.17663002753556, -105.06476404135105 40.1768099757366, -105.06451420742577 40.17729412114653, -105.06443529115141 40.17744601058907, -105.06443345848308 40.17745551625659, -105.0645251580844 40.177477065519724, -105.06482690264772 40.177556895315554, -105.06495884548076 40.17757496072856, -105.06604504597603 40.177571082470905, -105.0669959168821 40.17757492265862, -105.06706647372714 40.177565590584095, -105.06706605657438 40.177633711711444))</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -3852,7 +3868,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0682879304474 40.17423889546031, -105.0705337647592 40.17417980111477, -105.0704676384679 40.17401525411931, -105.0704526828224 40.17398700036528, -105.0703699476555 40.17383072432401, -105.07033336786 40.1737189889846, -105.0702945408748 40.17360039409835, -105.0702866310458 40.173576234709, -105.0701781533955 40.17325428528496, -105.0702143999142 40.1730234451326, -105.0704758464944 40.17286042088165, -105.0706089644674 40.1727774133586, -105.0708027271205 40.17271196641693, -105.0709653184227 40.17265834146566, -105.0711711597935 40.17259038091576, -105.0712322250403 40.17252357899062, -105.0714151828517 40.172324112408, -105.071493494646 40.17223903902581, -105.0715024987211 40.17216110206002, -105.0715257345117 40.17197993947205, -105.0715316809831 40.17193354874935, -105.0713919649312 40.17183679362187, -105.0711494002002 40.17166902037516, -105.0709656546354 40.17154231984762, -105.0709274429077 40.17147883318172, -105.0708035182736 40.17127361762239, -105.0706892573018 40.17123797281743, -105.0704140291814 40.17115210803604, -105.0703213021316 40.17112402272167, -105.0701873071285 40.17085983825155, -105.0700490748938 40.17058729610622, -105.0700654619531 40.17050725216793, -105.0700903919518 40.17038641030021, -105.070130222646 40.1701932959897, -105.0701130518095 40.17012801034537, -105.0700839003286 40.17001717250243, -105.0699965925169 40.16995667405463, -105.069770804172 40.16980021285955, -105.069593849699 40.16967759275655, -105.0694904125201 40.1696307011031, -105.0693083248916 40.16954815441962, -105.0691851660852 40.16949232218418, -105.069001375795 40.16925225627143, -105.0689954745381 40.16881117180088, -105.0690669467599 40.16870070883218, -105.0692236861258 40.16845846733594, -105.0690924732613 40.16831925413381, -105.0689685835843 40.16818978871847, -105.0688340700417 40.16805157342573, -105.0687296043239 40.16781962045806, -105.0686323263576 40.16760712016501, -105.0685909942695 40.16751728354365, -105.0685888605255 40.16705920435815, -105.0685881730954 40.16699784732862, -105.068431855338 40.16671819881601, -105.0682505460679 40.16639383349164, -105.0680775020221 40.16608425757718, -105.0679475088123 40.16585168964777, -105.0679624680124 40.16577246289581, -105.0680270215794 40.16543056534422, -105.0680545246087 40.16528489551064, -105.0682378207239 40.16505772046782, -105.0684789369425 40.16475923917578, -105.0686456338963 40.16455287570224, -105.0689869716922 40.16455176868926, -105.0696307602086 40.16454426598023, -105.0700625038011 40.16454979057855, -105.0710065092227 40.1648152438267, -105.0716146066078 40.16498277526175, -105.0716063693274 40.16433043272091, -105.0716009565898 40.16400079816211, -105.0711107510569 40.16381343696385, -105.0703804641565 40.16323529954771, -105.0701550066105 40.16305681397562, -105.0699787471539 40.16289951940838, -105.0697765395714 40.16271473582595, -105.0696730762008 40.16262018933153, -105.0695365017366 40.16249028447161, -105.0694449513376 40.16238986040845, -105.0693539608267 40.1622900444892, -105.0692646761394 40.16219209918427, -105.0690794916851 40.1619889533341, -105.0689887855424 40.1618894461977, -105.0684992704832 40.16135539178723, -105.0689725401897 40.16113013534599, -105.0694111630307 40.16090422372054, -105.0687409608614 40.16070000328342, -105.0678959694674 40.1604240008717, -105.067322977026 40.16013699897744, -105.066765552507 40.15964313063317, -105.0662970046367 40.1588843247345, -105.064919505624 40.15935175545492, -105.064296309749 40.15959008850385, -105.0634333444827 40.15986251985857, -105.062539016009 40.16009099355082, -105.0606010313516 40.16022699272562, -105.0580710513005 40.16025799056519, -105.0553377713311 40.16028796999728, -105.0553376788475 40.16030391644374, -105.0553372380196 40.16037944725436, -105.0553368567356 40.16044496943694, -105.0553334854068 40.16102383273662, -105.0552966362117 40.16734916580195, -105.0552963083236 40.16740327517449, -105.0552760273123 40.17074210973164, -105.0552661885532 40.1723617576026, -105.0552661709637 40.17236480711001, -105.0552600297223 40.17337558245075, -105.0552600120969 40.17337863736143, -105.0552583760022 40.17364790868083, -105.0552583571967 40.17365096448745, -105.0552531555569 40.17450722459085, -105.0552531367156 40.17451028580081, -105.0552526542794 40.17458963771727, -105.0552526354381 40.17459269892721, -105.0552520195328 40.17467199268808, -105.0552519959952 40.1746750538799, -105.0552514076745 40.17474994901017, -105.0552513829568 40.17475301109806, -105.0552414762126 40.17601476607788, -105.0552302810579 40.17744046057113, -105.05523025625 40.17744353616711, -105.0551970875692 40.18166723030277, -105.0551970626169 40.18167032751156, -105.0551956991301 40.18184398208187, -105.0551956753519 40.18184707929512, -105.0551953462757 40.18223997368663, -105.0551953437782 40.18224286923797, -105.0552122394415 40.18224293424132, -105.0553029531036 40.18224233843291, -105.0553029537267 40.18224260232314, -105.0553171302694 40.18224224525912, -105.0554415540536 40.18223911220016, -105.0558656311479 40.18222843305814, -105.0563500596562 40.18221623312483, -105.0563475109136 40.18206710151329, -105.0563435646631 40.18183609266326, -105.0563426497601 40.18182117903999, -105.0563433097719 40.18182116446065, -105.059747225974 40.18174422809434, -105.0601897983534 40.18173421777126, -105.0597216533793 40.18141975678429, -105.0596885581266 40.18140630485958, -105.059826470133 40.18115851431644, -105.059840829938 40.18109097138242, -105.0598551995451 40.18102336093536, -105.0599031409281 40.18078827800947, -105.0596008853944 40.18066543418264, -105.0596208859462 40.18063637913681, -105.0596019956903 40.18062869946323, -105.059764907116 40.1803920478598, -105.0598394236868 40.18023540209372, -105.0597911097008 40.17990489630286, -105.0597920607357 40.17976956508435, -105.0597926998086 40.178807614259, -105.0600016657531 40.1788079711668, -105.0600122636052 40.17686582156504, -105.0600181192359 40.17674127431975, -105.0599075570974 40.17657074028857, -105.0598840870326 40.17646461930363, -105.0598964787459 40.17578559439733, -105.0599042822537 40.17541989242346, -105.0599338941769 40.17527841706814, -105.0599492665999 40.17511385088302, -105.0599189820093 40.17445629318946, -105.0603291131787 40.17444305988593, -105.0608598872117 40.17443409681316, -105.061864881507 40.17441787099343, -105.0644569935728 40.17434888012696, -105.0645800655635 40.17434311222554, -105.0648456787189 40.17433611380135, -105.0648471501122 40.17433607520882, -105.0674951080714 40.17426310871814, -105.067719899077 40.17425488999454, -105.0679761762959 40.1742478872944, -105.0682879304474 40.17423889546031))</t>
+          <t>POLYGON ((-105.06828793044744 40.17423889546031, -105.07053376475923 40.17417980111477, -105.07046763846789 40.17401525411931, -105.07045268282239 40.17398700036528, -105.07036994765555 40.17383072432401, -105.07033336786003 40.1737189889846, -105.07029454087483 40.17360039409835, -105.07028663104585 40.173576234709, -105.07017815339547 40.17325428528496, -105.07021439991418 40.1730234451326, -105.07047584649442 40.172860420881655, -105.07060896446737 40.1727774133586, -105.07080272712045 40.17271196641693, -105.07096531842268 40.172658341465656, -105.07117115979351 40.17259038091576, -105.07123222504028 40.17252357899062, -105.07141518285165 40.172324112408, -105.071493494646 40.17223903902581, -105.07150249872113 40.172161102060016, -105.07152573451172 40.171979939472045, -105.0715316809831 40.17193354874935, -105.07139196493121 40.17183679362187, -105.07114940020016 40.171669020375155, -105.07096565463536 40.17154231984762, -105.07092744290775 40.171478833181716, -105.07080351827359 40.17127361762239, -105.07068925730182 40.17123797281743, -105.0704140291814 40.17115210803604, -105.07032130213159 40.17112402272167, -105.07018730712852 40.17085983825155, -105.0700490748938 40.17058729610622, -105.07006546195315 40.17050725216793, -105.07009039195178 40.17038641030021, -105.07013022264597 40.1701932959897, -105.07011305180946 40.170128010345366, -105.07008390032863 40.170017172502426, -105.06999659251692 40.16995667405463, -105.06977080417197 40.16980021285955, -105.069593849699 40.16967759275655, -105.0694904125201 40.1696307011031, -105.0693083248916 40.16954815441962, -105.06918516608525 40.16949232218418, -105.06900137579503 40.16925225627143, -105.06899547453807 40.16881117180088, -105.06906694675986 40.168700708832176, -105.06922368612577 40.16845846733594, -105.06909247326125 40.16831925413381, -105.06896858358427 40.16818978871847, -105.06883407004166 40.16805157342573, -105.06872960432388 40.16781962045806, -105.06863232635763 40.16760712016501, -105.06859099426948 40.167517283543646, -105.06858886052551 40.16705920435815, -105.06858817309545 40.16699784732862, -105.06843185533805 40.166718198816014, -105.06825054606789 40.16639383349164, -105.06807750202213 40.166084257577175, -105.06794750881227 40.16585168964777, -105.06796246801244 40.16577246289581, -105.0680270215794 40.165430565344224, -105.0680545246087 40.165284895510645, -105.06823782072385 40.16505772046782, -105.06847893694253 40.16475923917578, -105.06864563389628 40.16455287570224, -105.06898697169218 40.16455176868926, -105.06963076020858 40.16454426598023, -105.07006250380113 40.16454979057855, -105.07100650922266 40.1648152438267, -105.07161460660781 40.16498277526175, -105.07160636932743 40.16433043272091, -105.07160095658983 40.164000798162114, -105.07111075105688 40.16381343696385, -105.07038046415646 40.16323529954771, -105.07015500661055 40.16305681397562, -105.06997874715387 40.162899519408384, -105.06977653957138 40.16271473582595, -105.06967307620077 40.162620189331534, -105.06953650173658 40.16249028447161, -105.06944495133762 40.16238986040845, -105.06935396082675 40.1622900444892, -105.06926467613941 40.16219209918427, -105.06907949168506 40.1619889533341, -105.06898878554237 40.161889446197705, -105.06849927048319 40.16135539178723, -105.06897254018966 40.16113013534599, -105.06941116303074 40.160904223720536, -105.0687409608614 40.160700003283424, -105.0678959694674 40.1604240008717, -105.06732297702601 40.160136998977435, -105.06676555250696 40.15964313063317, -105.06629700463674 40.1588843247345, -105.06491950562399 40.15935175545492, -105.06429630974895 40.15959008850385, -105.06343334448275 40.15986251985857, -105.06253901600904 40.16009099355082, -105.06060103135162 40.16022699272562, -105.05807105130047 40.16025799056519, -105.05533777133105 40.160287969997285, -105.05533767884754 40.16030391644374, -105.05533723801958 40.160379447254364, -105.05533685673561 40.160444969436945, -105.05533348540678 40.16102383273662, -105.05529663621171 40.16734916580195, -105.0552963083236 40.167403275174486, -105.05527602731226 40.17074210973164, -105.05526618855318 40.1723617576026, -105.05526617096366 40.172364807110014, -105.0552600297223 40.173375582450745, -105.05526001209694 40.17337863736143, -105.05525837600217 40.17364790868083, -105.05525835719672 40.17365096448745, -105.05525315555691 40.17450722459085, -105.05525313671565 40.174510285800814, -105.05525265427937 40.17458963771727, -105.05525263543805 40.174592698927206, -105.05525201953284 40.17467199268808, -105.05525199599519 40.1746750538799, -105.05525140767448 40.17474994901017, -105.05525138295677 40.17475301109806, -105.05524147621263 40.17601476607788, -105.05523028105787 40.17744046057113, -105.05523025624996 40.17744353616711, -105.0551970875692 40.18166723030277, -105.05519706261687 40.18167032751156, -105.05519569913012 40.18184398208187, -105.05519567535185 40.18184707929512, -105.05519534627571 40.18223997368663, -105.05519534377817 40.18224286923797, -105.05521223944152 40.182242934241316, -105.05530295310362 40.18224233843291, -105.05530295372668 40.182242602323136, -105.05531713026943 40.18224224525912, -105.05544155405357 40.182239112200165, -105.05586563114791 40.18222843305814, -105.05635005965624 40.182216233124834, -105.05634751091362 40.18206710151329, -105.05634356466312 40.18183609266326, -105.05634264976005 40.18182117903999, -105.0563433097719 40.18182116446065, -105.05974722597395 40.18174422809434, -105.06018979835343 40.181734217771265, -105.05972165337928 40.181419756784294, -105.05968855812664 40.18140630485958, -105.05982647013296 40.18115851431644, -105.05984082993798 40.18109097138242, -105.05985519954511 40.181023360935356, -105.05990314092813 40.18078827800947, -105.05960088539442 40.18066543418264, -105.05962088594617 40.180636379136814, -105.05960199569029 40.18062869946323, -105.05976490711602 40.180392047859804, -105.05983942368682 40.18023540209372, -105.05979110970084 40.17990489630286, -105.05979206073573 40.17976956508435, -105.05979269980864 40.178807614259, -105.0600016657531 40.1788079711668, -105.06001226360516 40.176865821565045, -105.06001811923592 40.176741274319745, -105.05990755709738 40.17657074028857, -105.05988408703263 40.17646461930363, -105.05989647874587 40.17578559439733, -105.05990428225367 40.175419892423456, -105.05993389417688 40.17527841706814, -105.05994926659994 40.17511385088302, -105.05991898200926 40.174456293189465, -105.0603291131787 40.17444305988593, -105.06085988721166 40.17443409681316, -105.06186488150705 40.17441787099343, -105.06445699357285 40.17434888012696, -105.06458006556346 40.174343112225536, -105.06484567871885 40.17433611380135, -105.06484715011224 40.17433607520882, -105.06749510807141 40.174263108718144, -105.067719899077 40.17425488999454, -105.0679761762959 40.1742478872944, -105.06828793044744 40.17423889546031))</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
@@ -3894,7 +3910,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0648456787189 40.17433611380135, -105.0645800655635 40.17434311222554, -105.0644569935728 40.17434888012696, -105.061864881507 40.17441787099343, -105.0608598872117 40.17443409681316, -105.0603291131787 40.17444305988593, -105.0599189820093 40.17445629318946, -105.0599492665999 40.17511385088302, -105.0599338941769 40.17527841706814, -105.0599042822537 40.17541989242346, -105.0598964787459 40.17578559439733, -105.0598840870326 40.17646461930363, -105.0599075570974 40.17657074028857, -105.0600181192359 40.17674127431975, -105.0600122636052 40.17686582156504, -105.0600016657531 40.1788079711668, -105.0597926998086 40.178807614259, -105.0597920607357 40.17976956508435, -105.0597911097008 40.17990489630286, -105.0598394236868 40.18023540209372, -105.059764907116 40.1803920478598, -105.0596019956903 40.18062869946323, -105.0596208859462 40.18063637913681, -105.0596008853944 40.18066543418264, -105.0599031409281 40.18078827800947, -105.0598551995451 40.18102336093536, -105.059840829938 40.18109097138242, -105.059826470133 40.18115851431644, -105.0596885581266 40.18140630485958, -105.0597216533793 40.18141975678429, -105.0601897983534 40.18173421777126, -105.0640804191193 40.1816461432256, -105.064327931285 40.18164053757673, -105.0647003861965 40.18163209925449, -105.0647829616283 40.18163038730162, -105.0649311500239 40.18162506478151, -105.0655768798686 40.18161404104264, -105.0666149759152 40.18158691732067, -105.0670932333527 40.18157908311534, -105.0670663900754 40.177730367958, -105.0670660565744 40.17763371171144, -105.0670664737271 40.17756559058409, -105.0669959168821 40.17757492265862, -105.066045045976 40.17757108247091, -105.0649588454808 40.17757496072856, -105.0648269026477 40.17755689531555, -105.0645251580844 40.17747706551972, -105.0644334584831 40.17745551625659, -105.0644352911514 40.17744601058907, -105.0645142074258 40.17729412114653, -105.0647640413511 40.1768099757366, -105.0647999073873 40.17663002753556, -105.0648015744186 40.17658180266726, -105.0648193538381 40.17552207135812, -105.0648230964495 40.17529898664483, -105.0648232919619 40.17529063303029, -105.0648251809503 40.17521009306972, -105.0648456787189 40.17433611380135))</t>
+          <t>POLYGON ((-105.06484567871885 40.17433611380135, -105.06458006556346 40.174343112225536, -105.06445699357285 40.17434888012696, -105.06186488150705 40.17441787099343, -105.06085988721166 40.17443409681316, -105.0603291131787 40.17444305988593, -105.05991898200926 40.174456293189465, -105.05994926659994 40.17511385088302, -105.05993389417688 40.17527841706814, -105.05990428225367 40.175419892423456, -105.05989647874587 40.17578559439733, -105.05988408703263 40.17646461930363, -105.05990755709738 40.17657074028857, -105.06001811923592 40.176741274319745, -105.06001226360516 40.176865821565045, -105.0600016657531 40.1788079711668, -105.05979269980864 40.178807614259, -105.05979206073573 40.17976956508435, -105.05979110970084 40.17990489630286, -105.05983942368682 40.18023540209372, -105.05976490711602 40.180392047859804, -105.05960199569029 40.18062869946323, -105.05962088594617 40.180636379136814, -105.05960088539442 40.18066543418264, -105.05990314092813 40.18078827800947, -105.05985519954511 40.181023360935356, -105.05984082993798 40.18109097138242, -105.05982647013296 40.18115851431644, -105.05968855812664 40.18140630485958, -105.05972165337928 40.181419756784294, -105.06018979835343 40.181734217771265, -105.06408041911926 40.1816461432256, -105.064327931285 40.181640537576726, -105.06470038619652 40.18163209925449, -105.0647829616283 40.18163038730162, -105.06493115002391 40.18162506478151, -105.06557687986863 40.18161404104264, -105.06661497591523 40.181586917320665, -105.06709323335268 40.18157908311534, -105.06706639007544 40.177730367958, -105.06706605657438 40.177633711711444, -105.06706647372714 40.177565590584095, -105.0669959168821 40.17757492265862, -105.06604504597603 40.177571082470905, -105.06495884548076 40.17757496072856, -105.06482690264772 40.177556895315554, -105.0645251580844 40.177477065519724, -105.06443345848308 40.17745551625659, -105.06443529115141 40.17744601058907, -105.06451420742577 40.17729412114653, -105.06476404135105 40.1768099757366, -105.06479990738731 40.17663002753556, -105.06480157441857 40.17658180266726, -105.06481935383808 40.17552207135812, -105.06482309644953 40.17529898664483, -105.06482329196194 40.17529063303029, -105.06482518095028 40.17521009306972, -105.06484567871885 40.17433611380135))</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -3936,7 +3952,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0741588784485 40.18141592642099, -105.0741590040985 40.18141592508253, -105.0741589989394 40.18141599891602, -105.0742213953465 40.18141533169408, -105.0743460002694 40.18141399915928, -105.0748488307096 40.18140972683914, -105.0749491062686 40.18140887518751, -105.0749512998315 40.1814088562331, -105.074994614442 40.18140848769917, -105.0750794787078 40.18140776661161, -105.0751256104216 40.18140737415841, -105.0751725711776 40.18140697482621, -105.0752857084997 40.18140603775041, -105.07528732196 40.18140602476426, -105.0752889683034 40.18140601099832, -105.0753716177243 40.18140533109495, -105.0754426945701 40.18140475183662, -105.0754427615047 40.18140475118179, -105.0754793720476 40.18140445241381, -105.0754801423805 40.18140444533542, -105.0754802879918 40.18140444406882, -105.0754809843561 40.18140443581816, -105.0754817065584 40.1814044267618, -105.0754823594775 40.18140441835159, -105.0754828890952 40.18140441128996, -105.0754833764362 40.18140440497369, -105.0754838896094 40.18140439875229, -105.0754843640343 40.1814043923886, -105.0754847668221 40.18140438756314, -105.0754851766551 40.18140438276357, -105.0754857884719 40.18140437510305, -105.0754862699419 40.18140436876526, -105.0754867044386 40.18140436315555, -105.0754870813941 40.18140435823524, -105.0754876110117 40.18140435117355, -105.0754881864285 40.18140434337942, -105.0754889755653 40.18140433366811, -105.0754896977676 40.18140432461163, -105.0754902191659 40.18140431751977, -105.0754909178842 40.1814043083771, -105.0754918162324 40.18140429726549, -105.0754928555007 40.18140428396937, -105.0754939617036 40.18140427001845, -105.0754949175929 40.18140425821746, -105.0754958335596 40.18140424626989, -105.0754992743014 40.18140420216343, -105.07567141702 40.1814020043033, -105.0757328277791 40.18140122006803, -105.0757847958733 40.18140055696272, -105.0760438342818 40.18139724985279, -105.0761605000241 40.18139576015877, -105.0767199990883 40.18137999893392, -105.0767260138254 40.18138012633025, -105.0767293198357 40.18138003305935, -105.0771488379866 40.18138893907403, -105.0783319997978 40.18137399852338, -105.0783919311324 40.18137356773583, -105.0784709995856 40.18137299864745, -105.0789949582022 40.1813679774565, -105.0790969992628 40.18136699894468, -105.0791404726563 40.18136676813425, -105.0794739995876 40.18136499888473, -105.0800087806139 40.18136153274529, -105.0800909992445 40.18136099921094, -105.0804579995503 40.18135599921748, -105.0809140000496 40.18134999857968, -105.080939139291 40.18134974656282, -105.0814130000746 40.18134499934133, -105.081720788544 40.18134121835852, -105.0820477158421 40.18133720223299, -105.0822269997535 40.18133499881429, -105.0830779995653 40.18132199897433, -105.0830780465165 40.18132200184557, -105.0830780437171 40.18132188385164, -105.0830671110233 40.18001103243297, -105.0830661325881 40.17946995861438, -105.0830660404303 40.17930991634611, -105.0830638265291 40.1786200504606, -105.0830620459956 40.17791810757945, -105.0830610125146 40.17721095080906, -105.0830670926721 40.17651095809577, -105.0830628233633 40.17592292983689, -105.0830620150246 40.17576288399911, -105.0830678587874 40.17533493508519, -105.0830668929726 40.17496708024814, -105.083060890151 40.17466207194415, -105.0830668337051 40.17410098249666, -105.0830771760332 40.1739901157939, -105.0817029589484 40.1739931120255, -105.081386942714 40.1739969089824, -105.0805848880472 40.17400992414674, -105.0793730489725 40.17402803066916, -105.0790899520972 40.17403194202814, -105.0784149087419 40.17405007076083, -105.0775441759869 40.17405787252455, -105.0774139014207 40.17405986681544, -105.0768720438574 40.17406804212276, -105.076705975677 40.17407100247446, -105.0750621597752 40.17409407028626, -105.0741348956377 40.17409999127664, -105.074151011784 40.17546988524433, -105.0741524295275 40.17570984374514, -105.0741588320919 40.17679308076072, -105.0741689057888 40.17724195131272, -105.0741679464936 40.17762379964213, -105.0741650450267 40.17871608683249, -105.074182886726 40.18032508999734, -105.0741588784485 40.18141592642099))</t>
+          <t>POLYGON ((-105.0741588784485 40.18141592642099, -105.0741590040985 40.18141592508253, -105.07415899893937 40.181415998916016, -105.07422139534653 40.18141533169408, -105.07434600026936 40.18141399915928, -105.07484883070958 40.18140972683914, -105.07494910626858 40.181408875187515, -105.07495129983145 40.1814088562331, -105.07499461444203 40.18140848769917, -105.07507947870778 40.181407766611606, -105.0751256104216 40.18140737415841, -105.07517257117757 40.18140697482621, -105.07528570849966 40.181406037750406, -105.07528732196002 40.181406024764264, -105.07528896830341 40.181406010998316, -105.07537161772426 40.18140533109495, -105.07544269457006 40.181404751836624, -105.07544276150472 40.181404751181795, -105.0754793720476 40.18140445241381, -105.0754801423805 40.181404445335424, -105.07548028799177 40.18140444406882, -105.07548098435613 40.18140443581816, -105.07548170655839 40.1814044267618, -105.07548235947755 40.18140441835159, -105.0754828890952 40.18140441128996, -105.07548337643617 40.18140440497369, -105.07548388960943 40.181404398752285, -105.0754843640343 40.1814043923886, -105.07548476682211 40.18140438756314, -105.0754851766551 40.181404382763574, -105.07548578847187 40.18140437510305, -105.0754862699419 40.18140436876526, -105.07548670443857 40.18140436315555, -105.0754870813941 40.18140435823524, -105.0754876110117 40.181404351173555, -105.07548818642847 40.18140434337942, -105.07548897556535 40.18140433366811, -105.07548969776762 40.181404324611634, -105.07549021916586 40.18140431751977, -105.0754909178842 40.181404308377104, -105.0754918162324 40.18140429726549, -105.07549285550066 40.18140428396937, -105.07549396170357 40.18140427001845, -105.07549491759286 40.18140425821746, -105.07549583355956 40.18140424626989, -105.07549927430142 40.18140420216343, -105.07567141702002 40.1814020043033, -105.07573282777906 40.181401220068025, -105.07578479587326 40.18140055696272, -105.07604383428185 40.18139724985279, -105.07616050002407 40.18139576015877, -105.07671999908833 40.18137999893392, -105.07672601382544 40.181380126330254, -105.07672931983566 40.18138003305935, -105.0771488379866 40.18138893907403, -105.07833199979777 40.18137399852338, -105.0783919311324 40.18137356773583, -105.07847099958559 40.181372998647454, -105.07899495820217 40.1813679774565, -105.07909699926284 40.18136699894468, -105.07914047265628 40.181366768134254, -105.07947399958759 40.18136499888473, -105.08000878061385 40.181361532745285, -105.08009099924446 40.18136099921094, -105.08045799955026 40.18135599921748, -105.08091400004963 40.18134999857968, -105.08093913929105 40.18134974656282, -105.08141300007463 40.181344999341334, -105.08172078854405 40.18134121835852, -105.08204771584212 40.18133720223299, -105.08222699975353 40.181334998814286, -105.0830779995653 40.181321998974326, -105.08307804651646 40.18132200184557, -105.0830780437171 40.18132188385164, -105.08306711102331 40.180011032432965, -105.08306613258806 40.179469958614376, -105.08306604043034 40.17930991634611, -105.08306382652911 40.1786200504606, -105.08306204599559 40.17791810757945, -105.08306101251462 40.177210950809055, -105.08306709267207 40.17651095809577, -105.08306282336332 40.175922929836894, -105.08306201502462 40.17576288399911, -105.08306785878742 40.17533493508519, -105.0830668929726 40.17496708024814, -105.08306089015099 40.17466207194415, -105.0830668337051 40.17410098249666, -105.08307717603323 40.1739901157939, -105.08170295894837 40.1739931120255, -105.08138694271403 40.1739969089824, -105.08058488804723 40.174009924146745, -105.07937304897254 40.174028030669156, -105.07908995209725 40.17403194202814, -105.07841490874192 40.174050070760835, -105.07754417598686 40.17405787252455, -105.07741390142073 40.17405986681544, -105.07687204385743 40.174068042122755, -105.07670597567699 40.174071002474456, -105.07506215977516 40.17409407028626, -105.07413489563774 40.17409999127664, -105.07415101178397 40.17546988524433, -105.07415242952753 40.17570984374514, -105.07415883209191 40.176793080760724, -105.07416890578881 40.177241951312716, -105.07416794649365 40.17762379964213, -105.07416504502673 40.17871608683249, -105.07418288672598 40.18032508999734, -105.0741588784485 40.18141592642099))</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -3978,7 +3994,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0882981163367 40.18491807621724, -105.0887011128427 40.18492198101348, -105.0902899786259 40.18491307348874, -105.0911719576278 40.18490301835476, -105.0916490612702 40.18490388126406, -105.0918319813998 40.1849001347693, -105.0925499726852 40.18489992217005, -105.0928220041592 40.1848981353862, -105.0928751029819 40.18487691059035, -105.0929398690146 40.18487988378341, -105.0930311203723 40.1848829501716, -105.0933180959382 40.18489603843726, -105.0935220751613 40.18490197135755, -105.0941109333502 40.18488894183066, -105.094774519132 40.18490090548593, -105.0952350801125 40.18490304026881, -105.0954820988939 40.18489402209389, -105.095652117363 40.18489296956173, -105.096631019945 40.18489501639142, -105.0976560704005 40.18490105856144, -105.0976590764801 40.1845140024562, -105.097663170104 40.18418487289025, -105.0976589090309 40.18369512313647, -105.0976589570384 40.18344504022772, -105.0976649289801 40.18310109352984, -105.0976661129391 40.18302203686868, -105.0976719805968 40.18275605179154, -105.0976819842619 40.18142798182426, -105.0976810945381 40.18139695801594, -105.0976820282116 40.18123911525603, -105.0979779776586 40.18124508567654, -105.0984779720444 40.18124407812935, -105.0995441092706 40.18125299249242, -105.0996289322149 40.18125301158086, -105.0998909045749 40.1812550164052, -105.1001410733742 40.18125588193266, -105.1004688931724 40.18125893725914, -105.1011120077466 40.18126500100817, -105.1019341080188 40.18126508942446, -105.1023829530066 40.18125894705506, -105.1023970324222 40.18093204823994, -105.102413175028 40.18019091209275, -105.1024151073728 40.17943188442915, -105.1024348285392 40.17795588288692, -105.1024359298053 40.17764513457093, -105.102446985836 40.17691688312216, -105.1024459726393 40.17647792955385, -105.1024538771325 40.17579907983215, -105.1024659300747 40.1745939986924, -105.1024928436826 40.1739690192746, -105.1024948495252 40.17393196664215, -105.1024508498185 40.17392907018132, -105.1023799809039 40.17393102219533, -105.101211927436 40.17392892050625, -105.1001161310761 40.17393199790583, -105.0998391512321 40.17393103942207, -105.0989699184054 40.17392802714794, -105.0981518434555 40.1739279313386, -105.0979528772734 40.17392696481058, -105.0977370735687 40.17392895919532, -105.0974990948966 40.17392895400177, -105.0964931512326 40.17392709427654, -105.0963270854283 40.17393008282001, -105.0957541527641 40.17392890476933, -105.0955101015059 40.1739269531794, -105.0950699350661 40.17392596063161, -105.0947811388498 40.17392604651604, -105.0933063695626 40.17394767675843, -105.0930905495083 40.1739629603663, -105.0930355022931 40.17396373747397, -105.093035412355 40.17395404356559, -105.0928751701174 40.17396600181887, -105.0928349994319 40.17396899906539, -105.0920962144237 40.17397699684266, -105.0920961416262 40.17397699748644, -105.0920959995587 40.17397699788575, -105.0899358508228 40.17397797709733, -105.0898870002667 40.17397799833534, -105.0892635502055 40.17397922794395, -105.0888742073944 40.17397999371771, -105.0883123178483 40.17397704920117, -105.0883031426125 40.17397700121329, -105.0883029993709 40.17397700160376, -105.088302814376 40.1739809907825, -105.0830771458684 40.17399043991578, -105.0830668337051 40.17410098249666, -105.083060890151 40.17466207194415, -105.0830668929726 40.17496708024814, -105.0830678587874 40.17533493508519, -105.0830620150246 40.17576288399911, -105.0830628233633 40.17592292983689, -105.0830670926721 40.17651095809577, -105.0830610125146 40.17721095080906, -105.0830620459956 40.17791810757945, -105.0830638265291 40.1786200504606, -105.0830660404303 40.17930991634611, -105.0830661325881 40.17946995861438, -105.0830671110233 40.18001103243297, -105.0830780437171 40.18132188385164, -105.083318930598 40.18131891107805, -105.0840949994594 40.18130899845324, -105.0841204628213 40.18130854336619, -105.084150999356 40.18130799844511, -105.0845753067049 40.18130415518736, -105.0850339993664 40.18129999879005, -105.0856240002148 40.18129601317868, -105.08592199969 40.18129399891361, -105.0864130162753 40.18128845234943, -105.0877799994275 40.18127299902209, -105.0881015683002 40.18126505230806, -105.088305942072 40.18126000087282, -105.088294918421 40.18195796533448, -105.0882920205831 40.1821410568142, -105.0882910177791 40.18236588166063, -105.0882910647159 40.18266907847092, -105.0882910657439 40.18267530999828, -105.0882910888346 40.18282706780983, -105.0882911592627 40.18305189555398, -105.0882901155294 40.183519940556, -105.0882911213452 40.18388587384965, -105.0882931276252 40.18420486757227, -105.0882949212177 40.18455899895611, -105.0882981163367 40.18491807621724))</t>
+          <t>POLYGON ((-105.0882981163367 40.18491807621724, -105.08870111284273 40.18492198101348, -105.09028997862589 40.184913073488744, -105.09117195762782 40.18490301835476, -105.09164906127016 40.18490388126406, -105.09183198139984 40.1849001347693, -105.09254997268522 40.18489992217005, -105.09282200415919 40.1848981353862, -105.09287510298186 40.18487691059035, -105.0929398690146 40.18487988378341, -105.09303112037227 40.1848829501716, -105.09331809593819 40.18489603843726, -105.09352207516133 40.184901971357554, -105.09411093335024 40.184888941830664, -105.09477451913202 40.184900905485925, -105.09523508011253 40.184903040268814, -105.09548209889392 40.18489402209389, -105.09565211736299 40.18489296956173, -105.09663101994502 40.18489501639142, -105.09765607040052 40.18490105856144, -105.09765907648014 40.184514002456204, -105.097663170104 40.18418487289025, -105.09765890903093 40.183695123136474, -105.09765895703838 40.183445040227724, -105.0976649289801 40.183101093529835, -105.09766611293907 40.18302203686868, -105.09767198059677 40.182756051791536, -105.09768198426192 40.18142798182426, -105.09768109453806 40.18139695801594, -105.09768202821158 40.18123911525603, -105.09797797765857 40.18124508567654, -105.0984779720444 40.18124407812935, -105.09954410927057 40.18125299249242, -105.09962893221488 40.18125301158086, -105.09989090457488 40.1812550164052, -105.10014107337417 40.18125588193266, -105.10046889317243 40.181258937259145, -105.10111200774664 40.18126500100817, -105.10193410801878 40.18126508942446, -105.10238295300661 40.18125894705506, -105.10239703242222 40.18093204823994, -105.10241317502798 40.18019091209275, -105.10241510737283 40.17943188442915, -105.10243482853916 40.17795588288692, -105.10243592980534 40.17764513457093, -105.10244698583598 40.17691688312216, -105.1024459726393 40.176477929553855, -105.1024538771325 40.175799079832146, -105.10246593007467 40.1745939986924, -105.10249284368261 40.1739690192746, -105.10249484952516 40.17393196664215, -105.10245084981848 40.173929070181316, -105.10237998090392 40.173931022195326, -105.10121192743595 40.17392892050625, -105.10011613107612 40.17393199790583, -105.0998391512321 40.17393103942207, -105.09896991840537 40.17392802714794, -105.09815184345548 40.1739279313386, -105.09795287727341 40.173926964810576, -105.09773707356871 40.173928959195315, -105.09749909489656 40.173928954001774, -105.0964931512326 40.173927094276536, -105.09632708542826 40.17393008282001, -105.09575415276406 40.17392890476933, -105.09551010150588 40.173926953179404, -105.09506993506612 40.17392596063161, -105.09478113884975 40.17392604651604, -105.0933063695626 40.17394767675843, -105.09309054950829 40.173962960366296, -105.09303550229312 40.17396373747397, -105.09303541235504 40.17395404356559, -105.09287517011735 40.17396600181887, -105.09283499943187 40.173968999065394, -105.09209621442366 40.17397699684266, -105.09209614162616 40.17397699748644, -105.09209599955867 40.17397699788575, -105.08993585082284 40.17397797709733, -105.08988700026669 40.17397799833534, -105.08926355020547 40.17397922794395, -105.0888742073944 40.17397999371771, -105.08831231784832 40.17397704920117, -105.08830314261247 40.17397700121329, -105.08830299937091 40.17397700160376, -105.08830281437605 40.173980990782496, -105.0830771458684 40.17399043991578, -105.0830668337051 40.17410098249666, -105.08306089015099 40.17466207194415, -105.0830668929726 40.17496708024814, -105.08306785878742 40.17533493508519, -105.08306201502462 40.17576288399911, -105.08306282336332 40.175922929836894, -105.08306709267207 40.17651095809577, -105.08306101251462 40.177210950809055, -105.08306204599559 40.17791810757945, -105.08306382652911 40.1786200504606, -105.08306604043034 40.17930991634611, -105.08306613258806 40.179469958614376, -105.08306711102331 40.180011032432965, -105.0830780437171 40.18132188385164, -105.08331893059803 40.18131891107805, -105.08409499945935 40.18130899845324, -105.08412046282133 40.181308543366185, -105.084150999356 40.181307998445114, -105.08457530670486 40.181304155187355, -105.08503399936636 40.181299998790045, -105.08562400021484 40.18129601317868, -105.08592199968996 40.18129399891361, -105.08641301627534 40.181288452349435, -105.08777999942754 40.18127299902209, -105.08810156830025 40.181265052308056, -105.08830594207201 40.18126000087282, -105.08829491842096 40.181957965334476, -105.08829202058307 40.1821410568142, -105.08829101777913 40.18236588166063, -105.08829106471588 40.18266907847092, -105.0882910657439 40.18267530999828, -105.08829108883464 40.18282706780983, -105.08829115926271 40.18305189555398, -105.08829011552938 40.183519940555996, -105.08829112134516 40.18388587384965, -105.08829312762524 40.18420486757227, -105.08829492121768 40.18455899895611, -105.0882981163367 40.18491807621724))</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -4020,7 +4036,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1120540599835 40.18855794243968, -105.1125329666713 40.18856092088617, -105.1125820027335 40.18856108520247, -105.1133670179578 40.18855190824585, -105.1134489979368 40.18854998659783, -105.1145858430134 40.18854499691239, -105.1146671019506 40.18854389517986, -105.1158580022557 40.18853797614679, -105.1167671242837 40.18854593391976, -105.1167491721246 40.18747609020114, -105.1167379495575 40.18718094924454, -105.1167259507816 40.18670599882897, -105.116720178492 40.18646001468655, -105.116716841756 40.1861629787624, -105.1166988685117 40.18547800407755, -105.1166981727474 40.18528391975315, -105.1166869917791 40.18491795447697, -105.1166749597231 40.18444904255475, -105.1166659838771 40.18420002786293, -105.1166618862477 40.18403805076851, -105.1166529128777 40.18372507366393, -105.1166478295378 40.18348403258791, -105.1166471363139 40.18322598670356, -105.116629956247 40.18284490311632, -105.1166100944872 40.18205093918248, -105.1166031416664 40.1816970661943, -105.116596113968 40.18129295713768, -105.1165861302571 40.18058796920991, -105.1165821338566 40.18028104811957, -105.1165549603175 40.17945109801703, -105.1165310198988 40.17811111064275, -105.1165261549901 40.1776411241069, -105.1165360006526 40.17671988341143, -105.1165338821993 40.17582605437854, -105.1165261743185 40.17489528498265, -105.116518036311 40.17400294520597, -105.1160359994517 40.17400189448648, -105.1152698530993 40.17399495472824, -105.1141211221343 40.17399304779159, -105.1135388728523 40.17399412254758, -105.1129648650939 40.17399302530533, -105.1117388825559 40.17398287436851, -105.1110468951035 40.17396188144068, -105.1104410147507 40.17396505683724, -105.1101958776593 40.17396505455947, -105.1098341136038 40.17395889228536, -105.1092240015637 40.17395106642266, -105.1085748492892 40.17394887014564, -105.1083290304438 40.17394309660612, -105.1078341011998 40.17394388906459, -105.1074021595161 40.17394407015826, -105.1071749152855 40.17394412134063, -105.1068388827713 40.17394407772057, -105.1061850487927 40.17394706770438, -105.1055809814998 40.17394610608032, -105.104960093369 40.17394508381765, -105.1037841434783 40.17394709886039, -105.1031539808862 40.17394109419757, -105.1024948495252 40.17393196664215, -105.1024928436826 40.1739690192746, -105.1024659300747 40.1745939986924, -105.1024538771325 40.17579907983215, -105.1024459726393 40.17647792955385, -105.102446985836 40.17691688312216, -105.1024359298053 40.17764513457093, -105.1024348285392 40.17795588288692, -105.1024151073728 40.17943188442915, -105.102413175028 40.18019091209275, -105.1023970324222 40.18093204823994, -105.1023829530066 40.18125894705506, -105.1027139937316 40.18126200709273, -105.1033940415842 40.18125610659184, -105.1036499481707 40.18125506224674, -105.1044011718303 40.18125708676741, -105.1047898365833 40.18126006333194, -105.1051319899099 40.18126013369076, -105.1052980584674 40.18125987759827, -105.1059451380013 40.18126098709274, -105.106641973712 40.18126088969616, -105.106833109551 40.18125797063896, -105.1072020949942 40.18126004898254, -105.1080911123929 40.18126196732355, -105.1084361110251 40.18126505829095, -105.1086240113595 40.18126487136174, -105.1089940736708 40.18126612354689, -105.1101640174649 40.18126520655875, -105.1112559916314 40.18126990755782, -105.1113569308159 40.18126805117004, -105.1115040224316 40.18126909494015, -105.1118629926047 40.18127002597253, -105.1118759946224 40.18181388411318, -105.1119081200098 40.18251894680662, -105.1119091664257 40.18315088404788, -105.1119118919206 40.18367686408679, -105.1119049061916 40.18402300359683, -105.1119319115066 40.18487960280919, -105.1120085237062 40.186557607745, -105.112011570436 40.18673288206929, -105.112017894645 40.18707819066701, -105.1120313601333 40.18760194311961, -105.1120540599835 40.18855794243968))</t>
+          <t>POLYGON ((-105.11205405998355 40.18855794243968, -105.1125329666713 40.18856092088617, -105.11258200273355 40.18856108520247, -105.11336701795776 40.18855190824585, -105.1134489979368 40.18854998659783, -105.11458584301336 40.18854499691239, -105.11466710195064 40.18854389517986, -105.1158580022557 40.18853797614679, -105.11676712428374 40.188545933919755, -105.11674917212461 40.18747609020114, -105.11673794955749 40.187180949244535, -105.11672595078159 40.18670599882897, -105.11672017849202 40.186460014686546, -105.11671684175599 40.1861629787624, -105.11669886851168 40.185478004077545, -105.11669817274743 40.185283919753154, -105.11668699177908 40.18491795447697, -105.11667495972313 40.18444904255475, -105.11666598387714 40.18420002786293, -105.1166618862477 40.18403805076851, -105.11665291287771 40.18372507366393, -105.11664782953784 40.18348403258791, -105.11664713631386 40.18322598670356, -105.11662995624701 40.18284490311632, -105.11661009448719 40.18205093918248, -105.11660314166639 40.1816970661943, -105.11659611396803 40.18129295713768, -105.11658613025709 40.18058796920991, -105.11658213385661 40.18028104811957, -105.11655496031747 40.17945109801703, -105.11653101989876 40.17811111064275, -105.11652615499011 40.1776411241069, -105.11653600065256 40.17671988341143, -105.11653388219928 40.17582605437854, -105.11652617431852 40.174895284982654, -105.11651803631102 40.17400294520597, -105.11603599945174 40.17400189448648, -105.1152698530993 40.17399495472824, -105.11412112213432 40.17399304779159, -105.11353887285227 40.173994122547576, -105.11296486509387 40.17399302530533, -105.11173888255588 40.173982874368505, -105.11104689510346 40.17396188144068, -105.11044101475073 40.17396505683724, -105.11019587765927 40.173965054559474, -105.10983411360375 40.173958892285356, -105.10922400156372 40.17395106642266, -105.1085748492892 40.173948870145644, -105.10832903044376 40.17394309660612, -105.10783410119977 40.17394388906459, -105.10740215951606 40.17394407015826, -105.10717491528548 40.17394412134063, -105.10683888277134 40.17394407772057, -105.10618504879267 40.173947067704376, -105.10558098149984 40.173946106080315, -105.10496009336902 40.17394508381765, -105.10378414347832 40.17394709886039, -105.10315398088623 40.17394109419757, -105.10249484952516 40.17393196664215, -105.10249284368261 40.1739690192746, -105.10246593007467 40.1745939986924, -105.1024538771325 40.175799079832146, -105.1024459726393 40.176477929553855, -105.10244698583598 40.17691688312216, -105.10243592980534 40.17764513457093, -105.10243482853916 40.17795588288692, -105.10241510737283 40.17943188442915, -105.10241317502798 40.18019091209275, -105.10239703242222 40.18093204823994, -105.10238295300661 40.18125894705506, -105.1027139937316 40.18126200709273, -105.10339404158417 40.18125610659184, -105.10364994817074 40.18125506224674, -105.1044011718303 40.18125708676741, -105.10478983658334 40.18126006333194, -105.10513198990989 40.18126013369076, -105.10529805846741 40.181259877598265, -105.10594513800126 40.18126098709274, -105.10664197371197 40.18126088969616, -105.106833109551 40.18125797063896, -105.10720209499424 40.181260048982544, -105.1080911123929 40.18126196732355, -105.10843611102514 40.18126505829095, -105.10862401135945 40.18126487136174, -105.10899407367083 40.18126612354689, -105.11016401746487 40.18126520655875, -105.1112559916314 40.18126990755782, -105.11135693081592 40.181268051170036, -105.11150402243163 40.18126909494015, -105.11186299260471 40.18127002597253, -105.11187599462237 40.181813884113176, -105.11190812000976 40.18251894680662, -105.11190916642572 40.18315088404788, -105.11191189192058 40.18367686408679, -105.11190490619155 40.184023003596835, -105.11193191150662 40.18487960280919, -105.11200852370617 40.186557607745, -105.11201157043604 40.186732882069286, -105.11201789464505 40.18707819066701, -105.11203136013326 40.18760194311961, -105.11205405998355 40.18855794243968))</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -4062,7 +4078,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1165261549901 40.1776411241069, -105.1174219417209 40.17763997436666, -105.1178120334309 40.17763989210152, -105.1184218537746 40.17764190656982, -105.1187718795563 40.17763894366483, -105.1190359860411 40.17764091218946, -105.1192561066179 40.17763697116306, -105.1197460479765 40.1776369364914, -105.1208880553671 40.17763602013243, -105.1213210764438 40.17763908664261, -105.1216109398022 40.17764305561492, -105.1218231639748 40.17764292597858, -105.1219530749401 40.17764307709177, -105.1222751700047 40.1776430311781, -105.1225399855552 40.17764609279298, -105.1227468366854 40.17764704269614, -105.1232170949696 40.17764692907965, -105.1236998500359 40.1776520698262, -105.1241858485652 40.17765310228246, -105.1244660551103 40.17765593392282, -105.124667896276 40.1776568641137, -105.1251499519391 40.17765897759355, -105.1256219770149 40.17766297764157, -105.1257790871407 40.17766293693992, -105.1261230023669 40.1776648738, -105.1263949802122 40.17766712566281, -105.1266308316704 40.17766596567792, -105.1271150244153 40.17766999892689, -105.1276038868331 40.17767102625083, -105.1278268473479 40.17767092017744, -105.1280870065147 40.17767505197183, -105.1286180993395 40.17767593526457, -105.1288968991793 40.17767408543865, -105.1291538710248 40.17767189112629, -105.1295700601191 40.17767706849542, -105.1298259304175 40.1776800838546, -105.1302199323399 40.17768491404231, -105.1303620005069 40.17768701475256, -105.1307810922348 40.17768506038569, -105.1309088561322 40.17768491898182, -105.1309089894072 40.17686906099571, -105.130907895079 40.17667497536176, -105.1309108852502 40.17618991643079, -105.1309011192309 40.1758791343955, -105.1309030890619 40.17558211464502, -105.1308961355192 40.17475305743081, -105.130896930049 40.17421089176275, -105.1308928914898 40.17403189495574, -105.1308978484933 40.17384386824337, -105.1308981571233 40.1736550034996, -105.1308928515666 40.17318199632658, -105.130890136097 40.17308892735598, -105.1308980849702 40.1728770261307, -105.1308830569357 40.17234908671396, -105.1308731301453 40.17200206767621, -105.1308640602036 40.17169513068922, -105.1308610970434 40.17144997901022, -105.1308601753751 40.17135609075753, -105.1308571509205 40.17105603681589, -105.130858089966 40.17094897815058, -105.1308520529194 40.17054487184136, -105.1307919383922 40.17054413045692, -105.1307328951028 40.17054394185323, -105.1292932296001 40.17054751516088, -105.1290921320947 40.17055186590388, -105.1278590524257 40.17054186296041, -105.1265029177806 40.17052403795397, -105.1258720702785 40.1705178801278, -105.1257700895006 40.17051700061796, -105.1251120458792 40.1705110252873, -105.1247628040899 40.17050266266191, -105.1242368732107 40.17049006543995, -105.1241330608343 40.17049686548875, -105.1240518509146 40.17049303305797, -105.1239768248647 40.17047110252382, -105.1239140607193 40.17043191685794, -105.1238589814622 40.17036201103702, -105.1238240450009 40.17014393179502, -105.1237881252106 40.17003894983811, -105.1237131288848 40.16994701792339, -105.1236068909988 40.16987502346031, -105.1231979098613 40.16974000185597, -105.1230330395367 40.16972299339648, -105.12286693377 40.16973507943386, -105.1227099792626 40.16977492039106, -105.1222858991367 40.16997503008646, -105.1220218780124 40.17009193377212, -105.1217538294875 40.17022502077831, -105.1216010718557 40.17028189425179, -105.121525052716 40.17030992094868, -105.1213079395277 40.17042093779713, -105.1201371329569 40.17040995858668, -105.1189430393077 40.17040410635464, -105.1178158853752 40.17039407161238, -105.116570983888 40.17038692899581, -105.1165658865861 40.17059307302266, -105.1165560403185 40.17132407516121, -105.1165530540567 40.17159995367778, -105.1165419082626 40.17262495703965, -105.1165319571477 40.1733109383496, -105.116518036311 40.17400294520597, -105.1165261743185 40.17489528498265, -105.1165338821993 40.17582605437854, -105.1165360006526 40.17671988341143, -105.1165261549901 40.1776411241069))</t>
+          <t>POLYGON ((-105.11652615499011 40.1776411241069, -105.11742194172093 40.177639974366656, -105.11781203343088 40.177639892101524, -105.11842185377465 40.17764190656982, -105.11877187955628 40.17763894366483, -105.11903598604107 40.17764091218946, -105.11925610661794 40.17763697116306, -105.11974604797648 40.177636936491396, -105.12088805536713 40.17763602013243, -105.1213210764438 40.177639086642614, -105.12161093980218 40.17764305561492, -105.12182316397481 40.17764292597858, -105.12195307494012 40.17764307709177, -105.12227517000467 40.1776430311781, -105.12253998555525 40.177646092792976, -105.12274683668544 40.177647042696144, -105.12321709496963 40.17764692907965, -105.12369985003595 40.1776520698262, -105.12418584856518 40.17765310228246, -105.12446605511033 40.17765593392282, -105.124667896276 40.1776568641137, -105.12514995193905 40.17765897759355, -105.1256219770149 40.177662977641575, -105.12577908714074 40.17766293693992, -105.12612300236688 40.1776648738, -105.12639498021224 40.177667125662815, -105.12663083167037 40.17766596567792, -105.12711502441535 40.177669998926895, -105.12760388683311 40.177671026250835, -105.12782684734793 40.17767092017744, -105.12808700651469 40.17767505197183, -105.12861809933955 40.177675935264574, -105.12889689917931 40.17767408543865, -105.1291538710248 40.17767189112629, -105.12957006011906 40.17767706849542, -105.12982593041752 40.177680083854604, -105.13021993233986 40.17768491404231, -105.13036200050692 40.177687014752564, -105.13078109223483 40.17768506038569, -105.13090885613224 40.17768491898182, -105.13090898940719 40.176869060995706, -105.13090789507902 40.17667497536176, -105.1309108852502 40.17618991643079, -105.1309011192309 40.1758791343955, -105.13090308906192 40.17558211464502, -105.13089613551918 40.174753057430806, -105.130896930049 40.17421089176275, -105.13089289148976 40.17403189495574, -105.13089784849328 40.17384386824337, -105.13089815712326 40.1736550034996, -105.1308928515666 40.17318199632658, -105.13089013609704 40.17308892735598, -105.13089808497016 40.1728770261307, -105.13088305693566 40.17234908671396, -105.1308731301453 40.17200206767621, -105.13086406020362 40.171695130689216, -105.13086109704335 40.17144997901022, -105.13086017537508 40.17135609075753, -105.1308571509205 40.17105603681589, -105.130858089966 40.17094897815058, -105.1308520529194 40.17054487184136, -105.13079193839218 40.17054413045692, -105.13073289510278 40.170543941853225, -105.12929322960005 40.170547515160884, -105.12909213209471 40.17055186590388, -105.1278590524257 40.17054186296041, -105.12650291778061 40.170524037953975, -105.12587207027855 40.1705178801278, -105.12577008950062 40.17051700061796, -105.12511204587916 40.170511025287304, -105.12476280408994 40.17050266266191, -105.12423687321073 40.17049006543995, -105.12413306083432 40.17049686548875, -105.12405185091457 40.170493033057966, -105.12397682486474 40.17047110252382, -105.12391406071934 40.17043191685794, -105.12385898146225 40.17036201103702, -105.12382404500092 40.17014393179502, -105.12378812521057 40.17003894983811, -105.12371312888476 40.16994701792339, -105.12360689099884 40.16987502346031, -105.12319790986133 40.16974000185597, -105.12303303953671 40.16972299339648, -105.12286693377001 40.169735079433856, -105.1227099792626 40.16977492039106, -105.12228589913668 40.16997503008646, -105.12202187801238 40.17009193377212, -105.12175382948746 40.17022502077831, -105.1216010718557 40.170281894251794, -105.12152505271601 40.17030992094868, -105.12130793952765 40.17042093779713, -105.12013713295688 40.17040995858668, -105.11894303930771 40.17040410635464, -105.11781588537522 40.17039407161238, -105.11657098388795 40.17038692899581, -105.11656588658606 40.17059307302266, -105.1165560403185 40.17132407516121, -105.11655305405665 40.17159995367778, -105.11654190826259 40.17262495703965, -105.11653195714767 40.1733109383496, -105.11651803631102 40.17400294520597, -105.11652617431852 40.174895284982654, -105.11653388219928 40.17582605437854, -105.11653600065256 40.17671988341143, -105.11652615499011 40.1776411241069))</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -4104,7 +4120,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1309088561322 40.17768491898182, -105.1309031473364 40.17900092566963, -105.1308910444444 40.1812969306925, -105.1310488305122 40.1812400601295, -105.1311270103189 40.18121093710647, -105.13120484353 40.18117989006359, -105.1312819648703 40.1811480184159, -105.1313580144205 40.1811158677041, -105.1314110967712 40.18109489988948, -105.1314720576864 40.18107313218118, -105.1315330096338 40.18105301257906, -105.1315821232844 40.18103807081247, -105.1316068563493 40.18103101207436, -105.1316581071536 40.18101799904638, -105.1317308526495 40.18100093675281, -105.131778860317 40.1809920301551, -105.1318748524613 40.18097806074758, -105.1319228321764 40.1809740957999, -105.1320320248758 40.18096812992588, -105.132141888408 40.18097012681933, -105.1326050058594 40.18097105009712, -105.1330101172125 40.18097700389311, -105.1334528284318 40.18097895687249, -105.1339610569703 40.18097699879955, -105.1344309520948 40.18098205393646, -105.1346728983831 40.18098089768213, -105.1350969557553 40.18099102084687, -105.1354809875879 40.18099003658985, -105.1359709530833 40.18098993315579, -105.1364530720413 40.18098486207412, -105.1374658786663 40.18099408219389, -105.1374508438165 40.17971891338569, -105.1374501325315 40.17924811815468, -105.1374200054615 40.1791258647816, -105.1374058496366 40.17909589849825, -105.1373461721418 40.17901198352556, -105.1366349501433 40.17842695566897, -105.1363121757919 40.17815197386796, -105.136278848435 40.17809312311183, -105.1362371272728 40.17799800966988, -105.1362218892418 40.17770203462756, -105.1362249268315 40.17713407217776, -105.1362290297834 40.17696910261856, -105.1362520696783 40.17687693807623, -105.1363079727668 40.17679613129526, -105.1363881062587 40.17673489321179, -105.1365610830145 40.17664512117685, -105.1367830366418 40.17656511168438, -105.136930878063 40.17649090780505, -105.1370548571764 40.17639494235723, -105.1371280764355 40.1762881106674, -105.1371648396174 40.17617210589435, -105.1371708332454 40.17598792530425, -105.1371650156462 40.17526703176821, -105.1371698726245 40.17469193726257, -105.1371821150771 40.17407404143466, -105.1471472878128 40.17412208832916, -105.1308240275999 40.16707106507126, -105.1308251696132 40.16745401704761, -105.1308248690956 40.16770711920258, -105.1308339090772 40.16841512361963, -105.130829951995 40.16861687941822, -105.130829023898 40.16878789975995, -105.1308268264415 40.16899487857084, -105.130825096449 40.16911593337741, -105.130826950711 40.16923590355137, -105.1308328523583 40.16953294692157, -105.1308381211171 40.16968312372387, -105.1308380730325 40.1698239502182, -105.1308520529194 40.17054487184136, -105.130858089966 40.17094897815058, -105.1308571509205 40.17105603681589, -105.1308601753751 40.17135609075753, -105.1308610970434 40.17144997901022, -105.1308640602036 40.17169513068922, -105.1308731301453 40.17200206767621, -105.1308830569357 40.17234908671396, -105.1308980849702 40.1728770261307, -105.130890136097 40.17308892735598, -105.1308928515666 40.17318199632658, -105.1308981571233 40.1736550034996, -105.1308978484933 40.17384386824337, -105.1308928914898 40.17403189495574, -105.130896930049 40.17421089176275, -105.1308961355192 40.17475305743081, -105.1309030890619 40.17558211464502, -105.1309011192309 40.1758791343955, -105.1309108852502 40.17618991643079, -105.130907895079 40.17667497536176, -105.1309089894072 40.17686906099571, -105.1309088561322 40.17768491898182))</t>
+          <t>POLYGON ((-105.13090885613224 40.17768491898182, -105.13090314733635 40.179000925669634, -105.13089104444444 40.1812969306925, -105.13104883051216 40.181240060129504, -105.13112701031886 40.18121093710647, -105.13120484353004 40.18117989006359, -105.13128196487033 40.1811480184159, -105.13135801442051 40.1811158677041, -105.13141109677117 40.18109489988948, -105.13147205768638 40.181073132181176, -105.13153300963383 40.181053012579056, -105.13158212328445 40.18103807081247, -105.13160685634934 40.181031012074364, -105.13165810715357 40.181017999046375, -105.13173085264951 40.18100093675281, -105.13177886031704 40.180992030155096, -105.13187485246134 40.180978060747584, -105.13192283217644 40.180974095799904, -105.13203202487576 40.18096812992588, -105.13214188840804 40.180970126819325, -105.1326050058594 40.18097105009712, -105.13301011721245 40.18097700389311, -105.13345282843183 40.180978956872494, -105.1339610569703 40.18097699879955, -105.13443095209482 40.18098205393646, -105.13467289838307 40.18098089768213, -105.13509695575529 40.18099102084687, -105.13548098758793 40.18099003658985, -105.13597095308332 40.180989933155786, -105.13645307204129 40.18098486207412, -105.13746587866632 40.18099408219389, -105.13745084381652 40.17971891338569, -105.13745013253146 40.17924811815468, -105.13742000546154 40.179125864781604, -105.13740584963655 40.179095898498254, -105.13734617214182 40.17901198352556, -105.13663495014329 40.17842695566897, -105.13631217579193 40.17815197386796, -105.136278848435 40.17809312311183, -105.13623712727279 40.177998009669885, -105.13622188924182 40.177702034627565, -105.13622492683153 40.177134072177765, -105.13622902978338 40.176969102618564, -105.13625206967829 40.17687693807623, -105.13630797276683 40.17679613129526, -105.13638810625869 40.176734893211794, -105.1365610830145 40.176645121176854, -105.13678303664183 40.17656511168438, -105.13693087806303 40.176490907805054, -105.13705485717638 40.17639494235723, -105.13712807643549 40.1762881106674, -105.13716483961744 40.176172105894345, -105.13717083324545 40.17598792530425, -105.13716501564623 40.17526703176821, -105.1371698726245 40.17469193726257, -105.13718211507712 40.174074041434665, -105.14714728781279 40.174122088329156, -105.13082402759993 40.16707106507126, -105.1308251696132 40.16745401704761, -105.13082486909565 40.16770711920258, -105.13083390907721 40.16841512361963, -105.13082995199497 40.168616879418224, -105.13082902389796 40.16878789975995, -105.1308268264415 40.16899487857084, -105.13082509644899 40.169115933377405, -105.13082695071097 40.16923590355137, -105.1308328523583 40.16953294692157, -105.13083812111708 40.16968312372387, -105.13083807303255 40.1698239502182, -105.1308520529194 40.17054487184136, -105.130858089966 40.17094897815058, -105.1308571509205 40.17105603681589, -105.13086017537508 40.17135609075753, -105.13086109704335 40.17144997901022, -105.13086406020362 40.171695130689216, -105.1308731301453 40.17200206767621, -105.13088305693566 40.17234908671396, -105.13089808497016 40.1728770261307, -105.13089013609704 40.17308892735598, -105.1308928515666 40.17318199632658, -105.13089815712326 40.1736550034996, -105.13089784849328 40.17384386824337, -105.13089289148976 40.17403189495574, -105.130896930049 40.17421089176275, -105.13089613551918 40.174753057430806, -105.13090308906192 40.17558211464502, -105.1309011192309 40.1758791343955, -105.1309108852502 40.17618991643079, -105.13090789507902 40.17667497536176, -105.13090898940719 40.176869060995706, -105.13090885613224 40.17768491898182))</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
@@ -4146,7 +4162,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1405401452844 40.18101191718048, -105.1413021021828 40.1810132066264, -105.1423573659127 40.18101052813203, -105.1425719316643 40.18101409985752, -105.1430908768405 40.18101597689952, -105.143395112158 40.18101197393602, -105.1435990883817 40.18101699534053, -105.1442490343259 40.18101707610546, -105.1446430721145 40.18101911203982, -105.1450120519175 40.18102189197308, -105.1456931508489 40.18101903953585, -105.146606091477 40.18103089331234, -105.1466429495136 40.18103210385007, -105.1467148395546 40.18104110747008, -105.1467509471205 40.18104890474046, -105.1467870475715 40.18105807364797, -105.1468188485585 40.18106805349251, -105.1468531296272 40.18108298179864, -105.1468849161317 40.18109598141652, -105.1469448708388 40.18112910712441, -105.1476560227444 40.1814738708766, -105.1479519577899 40.18162191216626, -105.1483889400588 40.18183297150602, -105.1488219468181 40.18205197693125, -105.1490050866868 40.18214202486052, -105.149425077922 40.18231789122009, -105.1495920495657 40.18235106440956, -105.1496800636416 40.18235709611336, -105.1497638248641 40.18235487944441, -105.1497837703873 40.18235282607152, -105.1498071522691 40.18235089298177, -105.150461083381 40.18234408710372, -105.1510441395029 40.18233898468227, -105.1514900809613 40.18234087921265, -105.152052029506 40.18233406171446, -105.1529890653381 40.1823269962545, -105.1540219743234 40.18232899315603, -105.1543419168035 40.18232447880018, -105.1546641045306 40.18231993243897, -105.1547749998258 40.18231999974654, -105.1547761624487 40.18231997349721, -105.1547760472109 40.18231676688708, -105.154772043574 40.18204276868759, -105.154734010364 40.17971278356963, -105.1546629770468 40.17743779821491, -105.1546629131087 40.17736968103145, -105.1538534119111 40.17702152067658, -105.1538401553576 40.17416747340352, -105.1471472878128 40.17412208832916, -105.1371821150771 40.17407404143466, -105.1371698726245 40.17469193726257, -105.1371650156462 40.17526703176821, -105.1371708332454 40.17598792530425, -105.1371648396174 40.17617210589435, -105.1371280764355 40.1762881106674, -105.1370548571764 40.17639494235723, -105.136930878063 40.17649090780505, -105.1367830366418 40.17656511168438, -105.1365610830145 40.17664512117685, -105.1363881062587 40.17673489321179, -105.1363079727668 40.17679613129526, -105.1362520696783 40.17687693807623, -105.1362290297834 40.17696910261856, -105.1362249268315 40.17713407217776, -105.1362218892418 40.17770203462756, -105.1362371272728 40.17799800966988, -105.136278848435 40.17809312311183, -105.1363121757919 40.17815197386796, -105.1366349501433 40.17842695566897, -105.1373461721418 40.17901198352556, -105.1374058496366 40.17909589849825, -105.1374200054615 40.1791258647816, -105.1374501325315 40.17924811815468, -105.1374508438165 40.17971891338569, -105.1374658786663 40.18099408219389, -105.1377940672133 40.18099511087775, -105.1389342101846 40.18100321744779, -105.1405401452844 40.18101191718048))</t>
+          <t>POLYGON ((-105.1405401452844 40.181011917180484, -105.14130210218279 40.1810132066264, -105.14235736591272 40.18101052813203, -105.14257193166426 40.18101409985752, -105.1430908768405 40.18101597689952, -105.14339511215802 40.181011973936016, -105.14359908838172 40.181016995340535, -105.14424903432591 40.181017076105455, -105.14464307211446 40.18101911203982, -105.14501205191752 40.18102189197308, -105.14569315084894 40.18101903953585, -105.14660609147701 40.18103089331234, -105.14664294951363 40.18103210385007, -105.14671483955456 40.18104110747008, -105.14675094712052 40.181048904740464, -105.14678704757154 40.181058073647975, -105.1468188485585 40.18106805349251, -105.14685312962723 40.18108298179864, -105.14688491613171 40.18109598141652, -105.14694487083881 40.181129107124406, -105.14765602274439 40.1814738708766, -105.14795195778987 40.181621912166264, -105.14838894005884 40.18183297150602, -105.14882194681812 40.18205197693125, -105.14900508668684 40.18214202486052, -105.149425077922 40.182317891220094, -105.1495920495657 40.18235106440956, -105.14968006364164 40.182357096113364, -105.14976382486408 40.18235487944441, -105.14978377038734 40.182352826071515, -105.14980715226915 40.182350892981766, -105.15046108338099 40.18234408710372, -105.15104413950291 40.182338984682275, -105.1514900809613 40.182340879212646, -105.15205202950598 40.18233406171446, -105.15298906533808 40.1823269962545, -105.15402197432338 40.182328993156034, -105.1543419168035 40.18232447880018, -105.1546641045306 40.18231993243897, -105.15477499982585 40.18231999974654, -105.15477616244868 40.18231997349721, -105.1547760472109 40.182316766887084, -105.15477204357396 40.182042768687595, -105.154734010364 40.179712783569634, -105.15466297704683 40.17743779821491, -105.15466291310872 40.17736968103145, -105.15385341191113 40.17702152067658, -105.15384015535763 40.17416747340352, -105.14714728781279 40.174122088329156, -105.13718211507712 40.174074041434665, -105.1371698726245 40.17469193726257, -105.13716501564623 40.17526703176821, -105.13717083324545 40.17598792530425, -105.13716483961744 40.176172105894345, -105.13712807643549 40.1762881106674, -105.13705485717638 40.17639494235723, -105.13693087806303 40.176490907805054, -105.13678303664183 40.17656511168438, -105.1365610830145 40.176645121176854, -105.13638810625869 40.176734893211794, -105.13630797276683 40.17679613129526, -105.13625206967829 40.17687693807623, -105.13622902978338 40.176969102618564, -105.13622492683153 40.177134072177765, -105.13622188924182 40.177702034627565, -105.13623712727279 40.177998009669885, -105.136278848435 40.17809312311183, -105.13631217579193 40.17815197386796, -105.13663495014329 40.17842695566897, -105.13734617214182 40.17901198352556, -105.13740584963655 40.179095898498254, -105.13742000546154 40.179125864781604, -105.13745013253146 40.17924811815468, -105.13745084381652 40.17971891338569, -105.13746587866632 40.18099408219389, -105.13779406721329 40.18099511087775, -105.13893421018457 40.18100321744779, -105.1405401452844 40.181011917180484))</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -4188,7 +4204,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1548391576341 40.18279499875759, -105.1547920001525 40.18279499845895, -105.1547749998258 40.18231999974654, -105.1546641045306 40.18231993243897, -105.1543419168035 40.18232447880018, -105.1540219743234 40.18232899315603, -105.1529890653381 40.1823269962545, -105.152052029506 40.18233406171446, -105.1514900809613 40.18234087921265, -105.1510441395029 40.18233898468227, -105.150461083381 40.18234408710372, -105.1498071522691 40.18235089298177, -105.1497837703873 40.18235282607152, -105.1497638248641 40.18235487944441, -105.1496800636416 40.18235709611336, -105.1495920495657 40.18235106440956, -105.149425077922 40.18231789122009, -105.1490050866868 40.18214202486052, -105.1488219468181 40.18205197693125, -105.1483889400588 40.18183297150602, -105.1479519577899 40.18162191216626, -105.1476560227444 40.1814738708766, -105.1469448708388 40.18112910712441, -105.1468849161317 40.18109598141652, -105.1468531296272 40.18108298179864, -105.1468188485585 40.18106805349251, -105.1467870475715 40.18105807364797, -105.1467509471205 40.18104890474046, -105.1467148395546 40.18104110747008, -105.1466429495136 40.18103210385007, -105.146606091477 40.18103089331234, -105.1456931508489 40.18101903953585, -105.1450120519175 40.18102189197308, -105.1446430721145 40.18101911203982, -105.1442490343259 40.18101707610546, -105.1435990883817 40.18101699534053, -105.143395112158 40.18101197393602, -105.1430908768405 40.18101597689952, -105.1425719316643 40.18101409985752, -105.1423573659127 40.18101052813203, -105.1413021021828 40.1810132066264, -105.1405401452844 40.18101191718048, -105.1405331492857 40.18125209538468, -105.1405448299654 40.18144591190818, -105.1405369547856 40.18175090081714, -105.1405351182005 40.18196309512832, -105.1405480352217 40.18243090819281, -105.1405469198001 40.1831160931675, -105.1405549520951 40.18457598748516, -105.1405499407048 40.18559195046055, -105.1411838501522 40.18558705667058, -105.1421778420108 40.18557997984929, -105.1427991722154 40.18558492095656, -105.143180039099 40.18557813629327, -105.1433229083853 40.185567047181, -105.1434608562389 40.18553892338728, -105.1436329945333 40.18547494330328, -105.1438099169543 40.18538599674668, -105.1439618997615 40.18527501200008, -105.1445681553766 40.18467102363869, -105.1447638346391 40.18448495549296, -105.1455759136412 40.18497306383122, -105.146354126635 40.18543690593991, -105.1465411469029 40.18553904801176, -105.1473779389415 40.1860288663483, -105.1475689822392 40.18611509756006, -105.1477029506709 40.18616409427499, -105.1479840590923 40.18620695166086, -105.1481271732022 40.18621809316517, -105.1484761105867 40.18622601744052, -105.1492338322608 40.18622804402173, -105.149422086174 40.1862310863429, -105.149767435774 40.18623386221527, -105.1502070059285 40.18623401219416, -105.1503790560849 40.18625594521194, -105.1505470758935 40.18629598298839, -105.1507049815138 40.18635410806133, -105.150754973536 40.18637704427427, -105.1508920796487 40.18644306698239, -105.1510561674728 40.18655199530703, -105.1512549275952 40.18674008851822, -105.1512841145291 40.18677202034032, -105.1513771482871 40.18691697006431, -105.1514418613204 40.1870708929312, -105.1514629316738 40.18715001697894, -105.1514729168124 40.18729691198585, -105.1514618466591 40.18813002987395, -105.1514639163036 40.18863404452328, -105.15211893606 40.1886360171759, -105.1531178909332 40.18864697919484, -105.1545576450007 40.18865252803892, -105.1547139138904 40.18865312900746, -105.1548369993615 40.18865397295026, -105.154841999169 40.18754899881291, -105.1548431080552 40.18754893457554, -105.1548431219606 40.18754573195616, -105.1550295159042 40.18753491771105, -105.1550295936307 40.18753811519997, -105.1550332835498 40.18768878906563, -105.1556639597298 40.18766202520918, -105.156950659277 40.18760411594983, -105.158125901028 40.18755334084461, -105.1584590925243 40.18753745755789, -105.1584640423004 40.18753722180259, -105.1584638890017 40.18733882211959, -105.1584638862964 40.18733561945109, -105.1584622689358 40.18524309810573, -105.1584622286077 40.18523943690133, -105.158429101739 40.18522127318123, -105.1580737797326 40.18500654159926, -105.1575644515808 40.1847899325708, -105.1568855688112 40.18450120863788, -105.1563442888084 40.18427100243236, -105.1561902006576 40.18420546794748, -105.1548751995001 40.18420846777963, -105.1548391987841 40.18280146725144, -105.1548391576341 40.18279499875759))</t>
+          <t>POLYGON ((-105.15483915763413 40.18279499875759, -105.15479200015248 40.18279499845895, -105.15477499982585 40.18231999974654, -105.1546641045306 40.18231993243897, -105.1543419168035 40.18232447880018, -105.15402197432338 40.182328993156034, -105.15298906533808 40.1823269962545, -105.15205202950598 40.18233406171446, -105.1514900809613 40.182340879212646, -105.15104413950291 40.182338984682275, -105.15046108338099 40.18234408710372, -105.14980715226915 40.182350892981766, -105.14978377038734 40.182352826071515, -105.14976382486408 40.18235487944441, -105.14968006364164 40.182357096113364, -105.1495920495657 40.18235106440956, -105.149425077922 40.182317891220094, -105.14900508668684 40.18214202486052, -105.14882194681812 40.18205197693125, -105.14838894005884 40.18183297150602, -105.14795195778987 40.181621912166264, -105.14765602274439 40.1814738708766, -105.14694487083881 40.181129107124406, -105.14688491613171 40.18109598141652, -105.14685312962723 40.18108298179864, -105.1468188485585 40.18106805349251, -105.14678704757154 40.181058073647975, -105.14675094712052 40.181048904740464, -105.14671483955456 40.18104110747008, -105.14664294951363 40.18103210385007, -105.14660609147701 40.18103089331234, -105.14569315084894 40.18101903953585, -105.14501205191752 40.18102189197308, -105.14464307211446 40.18101911203982, -105.14424903432591 40.181017076105455, -105.14359908838172 40.181016995340535, -105.14339511215802 40.181011973936016, -105.1430908768405 40.18101597689952, -105.14257193166426 40.18101409985752, -105.14235736591272 40.18101052813203, -105.14130210218279 40.1810132066264, -105.1405401452844 40.181011917180484, -105.14053314928573 40.18125209538468, -105.14054482996538 40.181445911908185, -105.14053695478557 40.18175090081714, -105.14053511820046 40.181963095128324, -105.1405480352217 40.182430908192806, -105.14054691980013 40.1831160931675, -105.14055495209506 40.18457598748516, -105.14054994070476 40.18559195046055, -105.14118385015217 40.185587056670585, -105.14217784201082 40.185579979849294, -105.14279917221542 40.185584920956565, -105.143180039099 40.18557813629327, -105.14332290838526 40.185567047180996, -105.14346085623893 40.18553892338728, -105.14363299453328 40.185474943303284, -105.14380991695432 40.18538599674668, -105.1439618997615 40.185275012000076, -105.1445681553766 40.18467102363869, -105.14476383463905 40.184484955492955, -105.14557591364118 40.184973063831215, -105.14635412663502 40.18543690593991, -105.14654114690289 40.18553904801176, -105.14737793894153 40.1860288663483, -105.14756898223924 40.18611509756006, -105.14770295067086 40.18616409427499, -105.14798405909232 40.18620695166086, -105.14812717320221 40.186218093165174, -105.14847611058669 40.18622601744052, -105.1492338322608 40.18622804402173, -105.14942208617396 40.1862310863429, -105.14976743577402 40.18623386221527, -105.15020700592852 40.18623401219416, -105.15037905608492 40.18625594521194, -105.15054707589354 40.18629598298839, -105.15070498151384 40.18635410806133, -105.15075497353604 40.186377044274266, -105.1508920796487 40.18644306698239, -105.15105616747283 40.186551995307035, -105.15125492759519 40.18674008851822, -105.15128411452908 40.18677202034032, -105.15137714828711 40.18691697006431, -105.15144186132042 40.187070892931196, -105.15146293167382 40.18715001697894, -105.15147291681242 40.187296911985854, -105.15146184665912 40.188130029873946, -105.1514639163036 40.188634044523276, -105.15211893606003 40.188636017175895, -105.15311789093317 40.188646979194836, -105.1545576450007 40.188652528038915, -105.15471391389042 40.18865312900746, -105.15483699936152 40.18865397295026, -105.15484199916904 40.18754899881291, -105.1548431080552 40.18754893457554, -105.1548431219606 40.187545731956156, -105.15502951590416 40.18753491771105, -105.15502959363067 40.18753811519997, -105.15503328354981 40.18768878906563, -105.15566395972985 40.18766202520918, -105.15695065927703 40.18760411594983, -105.15812590102801 40.18755334084461, -105.15845909252428 40.18753745755789, -105.15846404230035 40.187537221802586, -105.15846388900172 40.187338822119585, -105.15846388629636 40.18733561945109, -105.15846226893584 40.18524309810573, -105.15846222860773 40.185239436901334, -105.15842910173899 40.18522127318123, -105.15807377973265 40.185006541599265, -105.15756445158078 40.1847899325708, -105.15688556881125 40.184501208637876, -105.15634428880844 40.18427100243236, -105.15619020065765 40.18420546794748, -105.15487519950011 40.18420846777963, -105.15483919878406 40.18280146725144, -105.15483915763413 40.18279499875759))</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
@@ -4230,7 +4246,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1309021056735 40.18314994122324, -105.1308979191687 40.1841851230857, -105.1309039419183 40.18465813085619, -105.1309051019469 40.18497190483541, -105.1309110183405 40.18513498587469, -105.1309118354979 40.18564393849361, -105.1309191252318 40.18634507253613, -105.1309188689071 40.186986063103, -105.1309220276749 40.18759110388334, -105.1309130611667 40.18812198620383, -105.1309169704838 40.1885889481708, -105.1318741020108 40.18858897966873, -105.1324877712597 40.18858819304007, -105.1329919645237 40.18858594522387, -105.1332378739106 40.18858507826119, -105.1336301658559 40.18858687135872, -105.1337998285665 40.18858713414526, -105.1339970425581 40.18858913116373, -105.1344490936186 40.18859413046857, -105.134910837415 40.18859394212554, -105.1395980233061 40.18860096041269, -105.1405798463564 40.18860209558213, -105.1405770053055 40.18778513128763, -105.1405741264152 40.18704310963169, -105.1405721409861 40.18633513022635, -105.1405499407048 40.18559195046055, -105.1405549520951 40.18457598748516, -105.1405469198001 40.1831160931675, -105.1405480352217 40.18243090819281, -105.1405351182005 40.18196309512832, -105.1405369547856 40.18175090081714, -105.1405448299654 40.18144591190818, -105.1405331492857 40.18125209538468, -105.1405401452844 40.18101191718048, -105.1389342101846 40.18100321744779, -105.1377940672133 40.18099511087775, -105.1374658786663 40.18099408219389, -105.1364530720413 40.18098486207412, -105.1359709530833 40.18098993315579, -105.1354809875879 40.18099003658985, -105.1350969557553 40.18099102084687, -105.1346728983831 40.18098089768213, -105.1344309520948 40.18098205393646, -105.1339610569703 40.18097699879955, -105.1334528284318 40.18097895687249, -105.1330101172125 40.18097700389311, -105.1326050058594 40.18097105009712, -105.132141888408 40.18097012681933, -105.1320320248758 40.18096812992588, -105.1319228321764 40.1809740957999, -105.1318748524613 40.18097806074758, -105.131778860317 40.1809920301551, -105.1317308526495 40.18100093675281, -105.1316581071536 40.18101799904638, -105.1316068563493 40.18103101207436, -105.1315821232844 40.18103807081247, -105.1315330096338 40.18105301257906, -105.1314720576864 40.18107313218118, -105.1314110967712 40.18109489988948, -105.1313580144205 40.1811158677041, -105.1312819648703 40.1811480184159, -105.13120484353 40.18117989006359, -105.1311270103189 40.18121093710647, -105.1310488305122 40.1812400601295, -105.1308910444444 40.1812969306925, -105.1308898627142 40.181442199769, -105.1309021056735 40.18314994122324))</t>
+          <t>POLYGON ((-105.13090210567347 40.18314994122324, -105.13089791916875 40.1841851230857, -105.13090394191835 40.18465813085619, -105.1309051019469 40.18497190483541, -105.1309110183405 40.18513498587469, -105.13091183549793 40.185643938493605, -105.13091912523178 40.18634507253613, -105.13091886890706 40.186986063103, -105.13092202767487 40.18759110388334, -105.13091306116665 40.18812198620383, -105.13091697048377 40.188588948170796, -105.13187410201084 40.18858897966873, -105.1324877712597 40.18858819304007, -105.13299196452373 40.18858594522387, -105.13323787391064 40.18858507826119, -105.1336301658559 40.188586871358716, -105.13379982856648 40.18858713414526, -105.13399704255812 40.18858913116373, -105.13444909361857 40.188594130468566, -105.13491083741502 40.188593942125536, -105.1395980233061 40.18860096041269, -105.14057984635642 40.18860209558213, -105.14057700530546 40.18778513128763, -105.14057412641525 40.187043109631695, -105.14057214098612 40.186335130226354, -105.14054994070476 40.18559195046055, -105.14055495209506 40.18457598748516, -105.14054691980013 40.1831160931675, -105.1405480352217 40.182430908192806, -105.14053511820046 40.181963095128324, -105.14053695478557 40.18175090081714, -105.14054482996538 40.181445911908185, -105.14053314928573 40.18125209538468, -105.1405401452844 40.181011917180484, -105.13893421018457 40.18100321744779, -105.13779406721329 40.18099511087775, -105.13746587866632 40.18099408219389, -105.13645307204129 40.18098486207412, -105.13597095308332 40.180989933155786, -105.13548098758793 40.18099003658985, -105.13509695575529 40.18099102084687, -105.13467289838307 40.18098089768213, -105.13443095209482 40.18098205393646, -105.1339610569703 40.18097699879955, -105.13345282843183 40.180978956872494, -105.13301011721245 40.18097700389311, -105.1326050058594 40.18097105009712, -105.13214188840804 40.180970126819325, -105.13203202487576 40.18096812992588, -105.13192283217644 40.180974095799904, -105.13187485246134 40.180978060747584, -105.13177886031704 40.180992030155096, -105.13173085264951 40.18100093675281, -105.13165810715357 40.181017999046375, -105.13160685634934 40.181031012074364, -105.13158212328445 40.18103807081247, -105.13153300963383 40.181053012579056, -105.13147205768638 40.181073132181176, -105.13141109677117 40.18109489988948, -105.13135801442051 40.1811158677041, -105.13128196487033 40.1811480184159, -105.13120484353004 40.18117989006359, -105.13112701031886 40.18121093710647, -105.13104883051216 40.181240060129504, -105.13089104444444 40.1812969306925, -105.13088986271421 40.181442199769, -105.13090210567347 40.18314994122324))</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -4272,7 +4288,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1165261549901 40.1776411241069, -105.1165310198988 40.17811111064275, -105.1165549603175 40.17945109801703, -105.1165821338566 40.18028104811957, -105.1165861302571 40.18058796920991, -105.116596113968 40.18129295713768, -105.1166031416664 40.1816970661943, -105.1166100944872 40.18205093918248, -105.116629956247 40.18284490311632, -105.1166471363139 40.18322598670356, -105.1166478295378 40.18348403258791, -105.1181399756025 40.18348293184021, -105.1182788792666 40.18347707616869, -105.1184319165658 40.18343997341372, -105.1185679120891 40.18337810703469, -105.1186818533886 40.18329201084904, -105.1187659737543 40.18322613010817, -105.1188951651607 40.18316506409089, -105.1190338779328 40.18312901119844, -105.1191810413247 40.18311796606829, -105.1202389777537 40.18312693626036, -105.1207500518038 40.18313108523442, -105.1213760298617 40.18313286226297, -105.1218470014979 40.18313989398624, -105.1225431386271 40.18313997219258, -105.1228259009038 40.1831378760785, -105.1237968864134 40.18314296078427, -105.1247918415252 40.18315003708833, -105.1257549650661 40.18315288497893, -105.1267130933322 40.18315296267368, -105.1276948495358 40.18315201064156, -105.1285731595809 40.18315291373522, -105.1287188346433 40.1831520090774, -105.1292048515975 40.18315686338585, -105.1296851475755 40.18316087324337, -105.1301998238924 40.18316087336503, -105.1306411163663 40.18316310812266, -105.1307861094221 40.18315588431248, -105.1308469695733 40.18315305881777, -105.1309021056735 40.18314994122324, -105.1308898627142 40.181442199769, -105.1308910444444 40.1812969306925, -105.1309031473364 40.17900092566963, -105.1309088561322 40.17768491898182, -105.1307810922348 40.17768506038569, -105.1303620005069 40.17768701475256, -105.1302199323399 40.17768491404231, -105.1298259304175 40.1776800838546, -105.1295700601191 40.17767706849542, -105.1291538710248 40.17767189112629, -105.1288968991793 40.17767408543865, -105.1286180993395 40.17767593526457, -105.1280870065147 40.17767505197183, -105.1278268473479 40.17767092017744, -105.1276038868331 40.17767102625083, -105.1271150244153 40.17766999892689, -105.1266308316704 40.17766596567792, -105.1263949802122 40.17766712566281, -105.1261230023669 40.1776648738, -105.1257790871407 40.17766293693992, -105.1256219770149 40.17766297764157, -105.1251499519391 40.17765897759355, -105.124667896276 40.1776568641137, -105.1244660551103 40.17765593392282, -105.1241858485652 40.17765310228246, -105.1236998500359 40.1776520698262, -105.1232170949696 40.17764692907965, -105.1227468366854 40.17764704269614, -105.1225399855552 40.17764609279298, -105.1222751700047 40.1776430311781, -105.1219530749401 40.17764307709177, -105.1218231639748 40.17764292597858, -105.1216109398022 40.17764305561492, -105.1213210764438 40.17763908664261, -105.1208880553671 40.17763602013243, -105.1197460479765 40.1776369364914, -105.1192561066179 40.17763697116306, -105.1190359860411 40.17764091218946, -105.1187718795563 40.17763894366483, -105.1184218537746 40.17764190656982, -105.1178120334309 40.17763989210152, -105.1174219417209 40.17763997436666, -105.1165261549901 40.1776411241069))</t>
+          <t>POLYGON ((-105.11652615499011 40.1776411241069, -105.11653101989876 40.17811111064275, -105.11655496031747 40.17945109801703, -105.11658213385661 40.18028104811957, -105.11658613025709 40.18058796920991, -105.11659611396803 40.18129295713768, -105.11660314166639 40.1816970661943, -105.11661009448719 40.18205093918248, -105.11662995624701 40.18284490311632, -105.11664713631386 40.18322598670356, -105.11664782953784 40.18348403258791, -105.11813997560255 40.18348293184021, -105.11827887926658 40.183477076168685, -105.1184319165658 40.18343997341372, -105.11856791208909 40.18337810703469, -105.11868185338861 40.183292010849044, -105.11876597375434 40.183226130108174, -105.11889516516072 40.183165064090886, -105.11903387793285 40.18312901119844, -105.11918104132468 40.18311796606829, -105.1202389777537 40.18312693626036, -105.12075005180378 40.18313108523442, -105.12137602986171 40.18313286226297, -105.12184700149787 40.18313989398624, -105.12254313862705 40.183139972192585, -105.12282590090378 40.1831378760785, -105.12379688641344 40.183142960784274, -105.12479184152518 40.18315003708833, -105.12575496506611 40.18315288497893, -105.12671309333221 40.18315296267368, -105.12769484953579 40.183152010641564, -105.12857315958087 40.18315291373522, -105.12871883464332 40.183152009077396, -105.12920485159746 40.183156863385854, -105.12968514757546 40.183160873243374, -105.13019982389235 40.183160873365026, -105.13064111636626 40.18316310812266, -105.13078610942213 40.183155884312484, -105.13084696957328 40.18315305881777, -105.13090210567347 40.18314994122324, -105.13088986271421 40.181442199769, -105.13089104444444 40.1812969306925, -105.13090314733635 40.179000925669634, -105.13090885613224 40.17768491898182, -105.13078109223483 40.17768506038569, -105.13036200050692 40.177687014752564, -105.13021993233986 40.17768491404231, -105.12982593041752 40.177680083854604, -105.12957006011906 40.17767706849542, -105.1291538710248 40.17767189112629, -105.12889689917931 40.17767408543865, -105.12861809933955 40.177675935264574, -105.12808700651469 40.17767505197183, -105.12782684734793 40.17767092017744, -105.12760388683311 40.177671026250835, -105.12711502441535 40.177669998926895, -105.12663083167037 40.17766596567792, -105.12639498021224 40.177667125662815, -105.12612300236688 40.1776648738, -105.12577908714074 40.17766293693992, -105.1256219770149 40.177662977641575, -105.12514995193905 40.17765897759355, -105.124667896276 40.1776568641137, -105.12446605511033 40.17765593392282, -105.12418584856518 40.17765310228246, -105.12369985003595 40.1776520698262, -105.12321709496963 40.17764692907965, -105.12274683668544 40.177647042696144, -105.12253998555525 40.177646092792976, -105.12227517000467 40.1776430311781, -105.12195307494012 40.17764307709177, -105.12182316397481 40.17764292597858, -105.12161093980218 40.17764305561492, -105.1213210764438 40.177639086642614, -105.12088805536713 40.17763602013243, -105.11974604797648 40.177636936491396, -105.11925610661794 40.17763697116306, -105.11903598604107 40.17764091218946, -105.11877187955628 40.17763894366483, -105.11842185377465 40.17764190656982, -105.11781203343088 40.177639892101524, -105.11742194172093 40.177639974366656, -105.11652615499011 40.1776411241069))</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
@@ -4314,7 +4330,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1167671242837 40.18854593391976, -105.1172141737779 40.18854906207515, -105.1174969479037 40.18854890001953, -105.1179300587332 40.18854813537448, -105.1183019485997 40.18854991306068, -105.1186970917979 40.1885539619918, -105.1190850825382 40.1885568881324, -105.1194899230949 40.18855492662844, -105.121360830748 40.18856299055086, -105.1256918879809 40.18856611215961, -105.1288573477865 40.18857997484698, -105.1309169704838 40.1885889481708, -105.1309130611667 40.18812198620383, -105.1309220276749 40.18759110388334, -105.1309188689071 40.186986063103, -105.1309191252318 40.18634507253613, -105.1309118354979 40.18564393849361, -105.1309110183405 40.18513498587469, -105.1309051019469 40.18497190483541, -105.1309039419183 40.18465813085619, -105.1308979191687 40.1841851230857, -105.1309021056735 40.18314994122324, -105.1308469695733 40.18315305881777, -105.1307861094221 40.18315588431248, -105.1306411163663 40.18316310812266, -105.1301998238924 40.18316087336503, -105.1296851475755 40.18316087324337, -105.1292048515975 40.18315686338585, -105.1287188346433 40.1831520090774, -105.1285731595809 40.18315291373522, -105.1276948495358 40.18315201064156, -105.1267130933322 40.18315296267368, -105.1257549650661 40.18315288497893, -105.1247918415252 40.18315003708833, -105.1237968864134 40.18314296078427, -105.1228259009038 40.1831378760785, -105.1225431386271 40.18313997219258, -105.1218470014979 40.18313989398624, -105.1213760298617 40.18313286226297, -105.1207500518038 40.18313108523442, -105.1202389777537 40.18312693626036, -105.1191810413247 40.18311796606829, -105.1190338779328 40.18312901119844, -105.1188951651607 40.18316506409089, -105.1187659737543 40.18322613010817, -105.1186818533886 40.18329201084904, -105.1185679120891 40.18337810703469, -105.1184319165658 40.18343997341372, -105.1182788792666 40.18347707616869, -105.1181399756025 40.18348293184021, -105.1166478295378 40.18348403258791, -105.1166529128777 40.18372507366393, -105.1166618862477 40.18403805076851, -105.1166659838771 40.18420002786293, -105.1166749597231 40.18444904255475, -105.1166869917791 40.18491795447697, -105.1166981727474 40.18528391975315, -105.1166988685117 40.18547800407755, -105.116716841756 40.1861629787624, -105.116720178492 40.18646001468655, -105.1167259507816 40.18670599882897, -105.1167379495575 40.18718094924454, -105.1167491721246 40.18747609020114, -105.1167671242837 40.18854593391976))</t>
+          <t>POLYGON ((-105.11676712428374 40.188545933919755, -105.11721417377788 40.18854906207515, -105.1174969479037 40.18854890001953, -105.11793005873315 40.18854813537448, -105.11830194859972 40.18854991306068, -105.1186970917979 40.1885539619918, -105.11908508253823 40.188556888132396, -105.11948992309487 40.18855492662844, -105.12136083074796 40.188562990550864, -105.12569188798088 40.18856611215961, -105.1288573477865 40.18857997484698, -105.13091697048377 40.188588948170796, -105.13091306116665 40.18812198620383, -105.13092202767487 40.18759110388334, -105.13091886890706 40.186986063103, -105.13091912523178 40.18634507253613, -105.13091183549793 40.185643938493605, -105.1309110183405 40.18513498587469, -105.1309051019469 40.18497190483541, -105.13090394191835 40.18465813085619, -105.13089791916875 40.1841851230857, -105.13090210567347 40.18314994122324, -105.13084696957328 40.18315305881777, -105.13078610942213 40.183155884312484, -105.13064111636626 40.18316310812266, -105.13019982389235 40.183160873365026, -105.12968514757546 40.183160873243374, -105.12920485159746 40.183156863385854, -105.12871883464332 40.183152009077396, -105.12857315958087 40.18315291373522, -105.12769484953579 40.183152010641564, -105.12671309333221 40.18315296267368, -105.12575496506611 40.18315288497893, -105.12479184152518 40.18315003708833, -105.12379688641344 40.183142960784274, -105.12282590090378 40.1831378760785, -105.12254313862705 40.183139972192585, -105.12184700149787 40.18313989398624, -105.12137602986171 40.18313286226297, -105.12075005180378 40.18313108523442, -105.1202389777537 40.18312693626036, -105.11918104132468 40.18311796606829, -105.11903387793285 40.18312901119844, -105.11889516516072 40.183165064090886, -105.11876597375434 40.183226130108174, -105.11868185338861 40.183292010849044, -105.11856791208909 40.18337810703469, -105.1184319165658 40.18343997341372, -105.11827887926658 40.183477076168685, -105.11813997560255 40.18348293184021, -105.11664782953784 40.18348403258791, -105.11665291287771 40.18372507366393, -105.1166618862477 40.18403805076851, -105.11666598387714 40.18420002786293, -105.11667495972313 40.18444904255475, -105.11668699177908 40.18491795447697, -105.11669817274743 40.185283919753154, -105.11669886851168 40.185478004077545, -105.11671684175599 40.1861629787624, -105.11672017849202 40.186460014686546, -105.11672595078159 40.18670599882897, -105.11673794955749 40.187180949244535, -105.11674917212461 40.18747609020114, -105.11676712428374 40.188545933919755))</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -4356,10 +4372,14 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1023829530066 40.18125894705506, -105.1023831548078 40.18140800978896, -105.102370035092 40.18248900592155, -105.1023460249624 40.18414699542499, -105.1023359709285 40.18488705328424, -105.102324014524 40.18558510414968, -105.102314050903 40.18661587375054, -105.1022961545613 40.18759500754209, -105.1022951231635 40.18764908370499, -105.1022919348154 40.18813304226678, -105.1022929712663 40.18856787832284, -105.1031670440105 40.18857088157077, -105.1035181760235 40.18857208617342, -105.1046560755281 40.18857104075413, -105.1051969341203 40.18856904580717, -105.1057839557793 40.18856912679325, -105.106394960974 40.18856901265301, -105.1067500432291 40.18856802423286, -105.1069608759509 40.18856709474983, -105.1075808282699 40.18856700385626, -105.1080901776704 40.18856708418473, -105.1102081396324 40.18856189061061, -105.111460935844 40.18856089171691, -105.1117581070876 40.18856554113695, -105.1120540599835 40.18855794243968, -105.1120313601333 40.18760194311961, -105.112017894645 40.18707819066701, -105.112011570436 40.18673288206929, -105.1120085237062 40.186557607745, -105.1119319115066 40.18487960280919, -105.1119049061916 40.18402300359683, -105.1119118919206 40.18367686408679, -105.1119091664257 40.18315088404788, -105.1119081200098 40.18251894680662, -105.1118759946224 40.18181388411318, -105.1118629926047 40.18127002597253, -105.1115040224316 40.18126909494015, -105.1113569308159 40.18126805117004, -105.1112559916314 40.18126990755782, -105.1101640174649 40.18126520655875, -105.1089940736708 40.18126612354689, -105.1086240113595 40.18126487136174, -105.1084361110251 40.18126505829095, -105.1080911123929 40.18126196732355, -105.1072020949942 40.18126004898254, -105.106833109551 40.18125797063896, -105.106641973712 40.18126088969616, -105.1059451380013 40.18126098709274, -105.1052980584674 40.18125987759827, -105.1051319899099 40.18126013369076, -105.1047898365833 40.18126006333194, -105.1044011718303 40.18125708676741, -105.1036499481707 40.18125506224674, -105.1033940415842 40.18125610659184, -105.1027139937316 40.18126200709273, -105.1023829530066 40.18125894705506))</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr"/>
+          <t>POLYGON ((-105.10238295300661 40.18125894705506, -105.10238315480781 40.18140800978896, -105.10237003509204 40.18248900592155, -105.10234602496243 40.18414699542499, -105.10233597092846 40.18488705328424, -105.10232401452396 40.18558510414968, -105.10231405090299 40.18661587375054, -105.1022961545613 40.187595007542086, -105.10229512316351 40.18764908370499, -105.10229193481537 40.18813304226678, -105.1022929712663 40.188567878322836, -105.10316704401049 40.18857088157077, -105.10351817602353 40.18857208617342, -105.10465607552808 40.188571040754134, -105.10519693412031 40.18856904580717, -105.10578395577929 40.18856912679325, -105.10639496097401 40.18856901265301, -105.10675004322914 40.18856802423286, -105.1069608759509 40.18856709474983, -105.10758082826989 40.188567003856264, -105.10809017767042 40.188567084184726, -105.11020813963242 40.188561890610615, -105.11146093584401 40.18856089171691, -105.11175810708758 40.18856554113695, -105.11205405998355 40.18855794243968, -105.11203136013326 40.18760194311961, -105.11201789464505 40.18707819066701, -105.11201157043604 40.186732882069286, -105.11200852370617 40.186557607745, -105.11193191150662 40.18487960280919, -105.11190490619155 40.184023003596835, -105.11191189192058 40.18367686408679, -105.11190916642572 40.18315088404788, -105.11190812000976 40.18251894680662, -105.11187599462237 40.181813884113176, -105.11186299260471 40.18127002597253, -105.11150402243163 40.18126909494015, -105.11135693081592 40.181268051170036, -105.1112559916314 40.18126990755782, -105.11016401746487 40.18126520655875, -105.10899407367083 40.18126612354689, -105.10862401135945 40.18126487136174, -105.10843611102514 40.18126505829095, -105.1080911123929 40.18126196732355, -105.10720209499424 40.181260048982544, -105.106833109551 40.18125797063896, -105.10664197371197 40.18126088969616, -105.10594513800126 40.18126098709274, -105.10529805846741 40.181259877598265, -105.10513198990989 40.18126013369076, -105.10478983658334 40.18126006333194, -105.1044011718303 40.18125708676741, -105.10364994817074 40.18125506224674, -105.10339404158417 40.18125610659184, -105.1027139937316 40.18126200709273, -105.10238295300661 40.18125894705506))</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Longs Peak MS</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4394,7 +4414,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0882981163367 40.18491807621724, -105.0882949675341 40.18526093467713, -105.0882970333903 40.18562906740542, -105.0883031109046 40.18598513502888, -105.0883060825807 40.1863219755426, -105.0883030954296 40.18663793242343, -105.0883008736399 40.18700495102672, -105.0882981267758 40.18757703146103, -105.0882981174619 40.18781503600134, -105.0882961422876 40.18849610088071, -105.0882951376611 40.18860288421402, -105.0892150876339 40.18859599888286, -105.0905810015349 40.18859398078645, -105.091522093662 40.18858303424472, -105.0925408347064 40.1885759229387, -105.0930503658067 40.1885802518252, -105.0931478712857 40.18858108041262, -105.093651870293 40.18857791098326, -105.0939400119303 40.18857810009743, -105.0943032647279 40.18857649050751, -105.0944039097845 40.18857604474166, -105.0946659350194 40.18857488223757, -105.0956509796097 40.1885761355268, -105.0965920413584 40.18857008941826, -105.0976301211599 40.18856107878358, -105.0985989901536 40.18857405442757, -105.0992658626611 40.18856895540347, -105.0995568688824 40.18856886575384, -105.1004760702672 40.18856710473342, -105.1006454886887 40.18856718836553, -105.1008698157056 40.18856729739159, -105.1010960533666 40.18856740807102, -105.1013414703393 40.18856752769821, -105.1016386463216 40.18856767203621, -105.1018591320755 40.18856777761645, -105.1022260358258 40.18856792185923, -105.1022929712663 40.18856787832284, -105.1022919348154 40.18813304226678, -105.1022951231635 40.18764908370499, -105.1022961545613 40.18759500754209, -105.102314050903 40.18661587375054, -105.102324014524 40.18558510414968, -105.1023359709285 40.18488705328424, -105.1023460249624 40.18414699542499, -105.102370035092 40.18248900592155, -105.1023831548078 40.18140800978896, -105.1023829530066 40.18125894705506, -105.1019341080188 40.18126508942446, -105.1011120077466 40.18126500100817, -105.1004688931724 40.18125893725914, -105.1001410733742 40.18125588193266, -105.0998909045749 40.1812550164052, -105.0996289322149 40.18125301158086, -105.0995441092706 40.18125299249242, -105.0984779720444 40.18124407812935, -105.0979779776586 40.18124508567654, -105.0976820282116 40.18123911525603, -105.0976810945381 40.18139695801594, -105.0976819842619 40.18142798182426, -105.0976719805968 40.18275605179154, -105.0976661129391 40.18302203686868, -105.0976649289801 40.18310109352984, -105.0976589570384 40.18344504022772, -105.0976589090309 40.18369512313647, -105.097663170104 40.18418487289025, -105.0976590764801 40.1845140024562, -105.0976560704005 40.18490105856144, -105.096631019945 40.18489501639142, -105.095652117363 40.18489296956173, -105.0954820988939 40.18489402209389, -105.0952350801125 40.18490304026881, -105.094774519132 40.18490090548593, -105.0941109333502 40.18488894183066, -105.0935220751613 40.18490197135755, -105.0933180959382 40.18489603843726, -105.0930311203723 40.1848829501716, -105.0929398690146 40.18487988378341, -105.0928751029819 40.18487691059035, -105.0928220041592 40.1848981353862, -105.0925499726852 40.18489992217005, -105.0918319813998 40.1849001347693, -105.0916490612702 40.18490388126406, -105.0911719576278 40.18490301835476, -105.0902899786259 40.18491307348874, -105.0887011128427 40.18492198101348, -105.0882981163367 40.18491807621724))</t>
+          <t>POLYGON ((-105.0882981163367 40.18491807621724, -105.08829496753414 40.18526093467713, -105.08829703339032 40.185629067405415, -105.08830311090462 40.18598513502888, -105.08830608258073 40.186321975542604, -105.08830309542958 40.18663793242343, -105.08830087363992 40.187004951026715, -105.08829812677577 40.18757703146103, -105.08829811746186 40.18781503600134, -105.08829614228765 40.188496100880705, -105.08829513766112 40.18860288421402, -105.08921508763389 40.18859599888286, -105.09058100153493 40.18859398078645, -105.09152209366201 40.18858303424472, -105.09254083470643 40.1885759229387, -105.09305036580668 40.1885802518252, -105.09314787128572 40.18858108041262, -105.09365187029303 40.188577910983255, -105.09394001193029 40.18857810009743, -105.0943032647279 40.18857649050751, -105.09440390978452 40.18857604474166, -105.09466593501938 40.188574882237575, -105.09565097960967 40.1885761355268, -105.09659204135845 40.188570089418256, -105.09763012115991 40.18856107878358, -105.09859899015365 40.18857405442757, -105.0992658626611 40.18856895540347, -105.09955686888244 40.18856886575384, -105.10047607026725 40.188567104733416, -105.10064548868866 40.18856718836553, -105.1008698157056 40.188567297391586, -105.10109605336665 40.188567408071016, -105.10134147033934 40.18856752769821, -105.10163864632163 40.18856767203621, -105.10185913207549 40.18856777761645, -105.10222603582581 40.18856792185923, -105.1022929712663 40.188567878322836, -105.10229193481537 40.18813304226678, -105.10229512316351 40.18764908370499, -105.1022961545613 40.187595007542086, -105.10231405090299 40.18661587375054, -105.10232401452396 40.18558510414968, -105.10233597092846 40.18488705328424, -105.10234602496243 40.18414699542499, -105.10237003509204 40.18248900592155, -105.10238315480781 40.18140800978896, -105.10238295300661 40.18125894705506, -105.10193410801878 40.18126508942446, -105.10111200774664 40.18126500100817, -105.10046889317243 40.181258937259145, -105.10014107337417 40.18125588193266, -105.09989090457488 40.1812550164052, -105.09962893221488 40.18125301158086, -105.09954410927057 40.18125299249242, -105.0984779720444 40.18124407812935, -105.09797797765857 40.18124508567654, -105.09768202821158 40.18123911525603, -105.09768109453806 40.18139695801594, -105.09768198426192 40.18142798182426, -105.09767198059677 40.182756051791536, -105.09766611293907 40.18302203686868, -105.0976649289801 40.183101093529835, -105.09765895703838 40.183445040227724, -105.09765890903093 40.183695123136474, -105.097663170104 40.18418487289025, -105.09765907648014 40.184514002456204, -105.09765607040052 40.18490105856144, -105.09663101994502 40.18489501639142, -105.09565211736299 40.18489296956173, -105.09548209889392 40.18489402209389, -105.09523508011253 40.184903040268814, -105.09477451913202 40.184900905485925, -105.09411093335024 40.184888941830664, -105.09352207516133 40.184901971357554, -105.09331809593819 40.18489603843726, -105.09303112037227 40.1848829501716, -105.0929398690146 40.18487988378341, -105.09287510298186 40.18487691059035, -105.09282200415919 40.1848981353862, -105.09254997268522 40.18489992217005, -105.09183198139984 40.1849001347693, -105.09164906127016 40.18490388126406, -105.09117195762782 40.18490301835476, -105.09028997862589 40.184913073488744, -105.08870111284273 40.18492198101348, -105.0882981163367 40.18491807621724))</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
@@ -4436,7 +4456,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0741589989394 40.18141599891602, -105.0741819992327 40.18232099821282, -105.0741979989235 40.1834589986692, -105.0742039991643 40.18429199826076, -105.074197000263 40.18869199904079, -105.074197000453 40.18874392269232, -105.0753352826321 40.18872998637555, -105.0776511302102 40.18870504443171, -105.0778161408352 40.18870509857946, -105.0785510892 40.18868993637176, -105.0792469265356 40.18869000018054, -105.0807080918733 40.1886821309134, -105.0808020163372 40.18868208690873, -105.0828160158762 40.1886809719122, -105.0830850002736 40.18865311719252, -105.0834201577121 40.1886329134413, -105.0840608966072 40.18862890672658, -105.0850019534098 40.18862405280476, -105.0850681792846 40.18862291791372, -105.086419060216 40.18862089503253, -105.0882951376611 40.18860288421402, -105.0882961422876 40.18849610088071, -105.0882981174619 40.18781503600134, -105.0882981267758 40.18757703146103, -105.0883008736399 40.18700495102672, -105.0883030954296 40.18663793242343, -105.0883060825807 40.1863219755426, -105.0883031109046 40.18598513502888, -105.0882970333903 40.18562906740542, -105.0882949675341 40.18526093467713, -105.0882981163367 40.18491807621724, -105.0882949212177 40.18455899895611, -105.0882931276252 40.18420486757227, -105.0882911213452 40.18388587384965, -105.0882901155294 40.183519940556, -105.0882911592627 40.18305189555398, -105.0882910888346 40.18282706780983, -105.0882910657439 40.18267530999828, -105.0882910647159 40.18266907847092, -105.0882910177791 40.18236588166063, -105.0882920205831 40.1821410568142, -105.088294918421 40.18195796533448, -105.088305942072 40.18126000087282, -105.0881015683002 40.18126505230806, -105.0877799994275 40.18127299902209, -105.0864130162753 40.18128845234943, -105.08592199969 40.18129399891361, -105.0856240002148 40.18129601317868, -105.0850339993664 40.18129999879005, -105.0845753067049 40.18130415518736, -105.084150999356 40.18130799844511, -105.0841204628213 40.18130854336619, -105.0840949994594 40.18130899845324, -105.083318930598 40.18131891107805, -105.0830780437171 40.18132188385164, -105.0830780465165 40.18132200184557, -105.0830779995653 40.18132199897433, -105.0822269997535 40.18133499881429, -105.0820477158421 40.18133720223299, -105.081720788544 40.18134121835852, -105.0814130000746 40.18134499934133, -105.080939139291 40.18134974656282, -105.0809140000496 40.18134999857968, -105.0804579995503 40.18135599921748, -105.0800909992445 40.18136099921094, -105.0800087806139 40.18136153274529, -105.0794739995876 40.18136499888473, -105.0791404726563 40.18136676813425, -105.0790969992628 40.18136699894468, -105.0789949582022 40.1813679774565, -105.0784709995856 40.18137299864745, -105.0783919311324 40.18137356773583, -105.0783319997978 40.18137399852338, -105.0771488379866 40.18138893907403, -105.0767293198357 40.18138003305935, -105.0767260138254 40.18138012633025, -105.0767199990883 40.18137999893392, -105.0761605000241 40.18139576015877, -105.0760438342818 40.18139724985279, -105.0757847958733 40.18140055696272, -105.0757328277791 40.18140122006803, -105.07567141702 40.1814020043033, -105.0754992743014 40.18140420216343, -105.0754958335596 40.18140424626989, -105.0754949175929 40.18140425821746, -105.0754939617036 40.18140427001845, -105.0754928555007 40.18140428396937, -105.0754918162324 40.18140429726549, -105.0754909178842 40.1814043083771, -105.0754902191659 40.18140431751977, -105.0754896977676 40.18140432461163, -105.0754889755653 40.18140433366811, -105.0754881864285 40.18140434337942, -105.0754876110117 40.18140435117355, -105.0754870813941 40.18140435823524, -105.0754867044386 40.18140436315555, -105.0754862699419 40.18140436876526, -105.0754857884719 40.18140437510305, -105.0754851766551 40.18140438276357, -105.0754847668221 40.18140438756314, -105.0754843640343 40.1814043923886, -105.0754838896094 40.18140439875229, -105.0754833764362 40.18140440497369, -105.0754828890952 40.18140441128996, -105.0754823594775 40.18140441835159, -105.0754817065584 40.1814044267618, -105.0754809843561 40.18140443581816, -105.0754802879918 40.18140444406882, -105.0754801423805 40.18140444533542, -105.0754793720476 40.18140445241381, -105.0754427615047 40.18140475118179, -105.0754426945701 40.18140475183662, -105.0753716177243 40.18140533109495, -105.0752889683034 40.18140601099832, -105.07528732196 40.18140602476426, -105.0752857084997 40.18140603775041, -105.0751725711776 40.18140697482621, -105.0751256104216 40.18140737415841, -105.0750794787078 40.18140776661161, -105.074994614442 40.18140848769917, -105.0749512998315 40.1814088562331, -105.0749491062686 40.18140887518751, -105.0748488307096 40.18140972683914, -105.0743460002694 40.18141399915928, -105.0742213953465 40.18141533169408, -105.0741589989394 40.18141599891602))</t>
+          <t>POLYGON ((-105.07415899893937 40.181415998916016, -105.07418199923268 40.182320998212816, -105.07419799892354 40.183458998669195, -105.07420399916433 40.18429199826076, -105.07419700026296 40.18869199904079, -105.07419700045295 40.18874392269232, -105.07533528263208 40.18872998637555, -105.07765113021019 40.188705044431714, -105.07781614083518 40.18870509857946, -105.07855108920002 40.18868993637176, -105.07924692653562 40.18869000018054, -105.08070809187328 40.1886821309134, -105.08080201633722 40.18868208690873, -105.0828160158762 40.1886809719122, -105.08308500027364 40.188653117192516, -105.08342015771214 40.188632913441296, -105.08406089660723 40.18862890672658, -105.08500195340982 40.18862405280476, -105.08506817928458 40.18862291791372, -105.08641906021597 40.18862089503253, -105.08829513766112 40.18860288421402, -105.08829614228765 40.188496100880705, -105.08829811746186 40.18781503600134, -105.08829812677577 40.18757703146103, -105.08830087363992 40.187004951026715, -105.08830309542958 40.18663793242343, -105.08830608258073 40.186321975542604, -105.08830311090462 40.18598513502888, -105.08829703339032 40.185629067405415, -105.08829496753414 40.18526093467713, -105.0882981163367 40.18491807621724, -105.08829492121768 40.18455899895611, -105.08829312762524 40.18420486757227, -105.08829112134516 40.18388587384965, -105.08829011552938 40.183519940555996, -105.08829115926271 40.18305189555398, -105.08829108883464 40.18282706780983, -105.0882910657439 40.18267530999828, -105.08829106471588 40.18266907847092, -105.08829101777913 40.18236588166063, -105.08829202058307 40.1821410568142, -105.08829491842096 40.181957965334476, -105.08830594207201 40.18126000087282, -105.08810156830025 40.181265052308056, -105.08777999942754 40.18127299902209, -105.08641301627534 40.181288452349435, -105.08592199968996 40.18129399891361, -105.08562400021484 40.18129601317868, -105.08503399936636 40.181299998790045, -105.08457530670486 40.181304155187355, -105.084150999356 40.181307998445114, -105.08412046282133 40.181308543366185, -105.08409499945935 40.18130899845324, -105.08331893059803 40.18131891107805, -105.0830780437171 40.18132188385164, -105.08307804651646 40.18132200184557, -105.0830779995653 40.181321998974326, -105.08222699975353 40.181334998814286, -105.08204771584212 40.18133720223299, -105.08172078854405 40.18134121835852, -105.08141300007463 40.181344999341334, -105.08093913929105 40.18134974656282, -105.08091400004963 40.18134999857968, -105.08045799955026 40.18135599921748, -105.08009099924446 40.18136099921094, -105.08000878061385 40.181361532745285, -105.07947399958759 40.18136499888473, -105.07914047265628 40.181366768134254, -105.07909699926284 40.18136699894468, -105.07899495820217 40.1813679774565, -105.07847099958559 40.181372998647454, -105.0783919311324 40.18137356773583, -105.07833199979777 40.18137399852338, -105.0771488379866 40.18138893907403, -105.07672931983566 40.18138003305935, -105.07672601382544 40.181380126330254, -105.07671999908833 40.18137999893392, -105.07616050002407 40.18139576015877, -105.07604383428185 40.18139724985279, -105.07578479587326 40.18140055696272, -105.07573282777906 40.181401220068025, -105.07567141702002 40.1814020043033, -105.07549927430142 40.18140420216343, -105.07549583355956 40.18140424626989, -105.07549491759286 40.18140425821746, -105.07549396170357 40.18140427001845, -105.07549285550066 40.18140428396937, -105.0754918162324 40.18140429726549, -105.0754909178842 40.181404308377104, -105.07549021916586 40.18140431751977, -105.07548969776762 40.181404324611634, -105.07548897556535 40.18140433366811, -105.07548818642847 40.18140434337942, -105.0754876110117 40.181404351173555, -105.0754870813941 40.18140435823524, -105.07548670443857 40.18140436315555, -105.0754862699419 40.18140436876526, -105.07548578847187 40.18140437510305, -105.0754851766551 40.181404382763574, -105.07548476682211 40.18140438756314, -105.0754843640343 40.1814043923886, -105.07548388960943 40.181404398752285, -105.07548337643617 40.18140440497369, -105.0754828890952 40.18140441128996, -105.07548235947755 40.18140441835159, -105.07548170655839 40.1814044267618, -105.07548098435613 40.18140443581816, -105.07548028799177 40.18140444406882, -105.0754801423805 40.181404445335424, -105.0754793720476 40.18140445241381, -105.07544276150472 40.181404751181795, -105.07544269457006 40.181404751836624, -105.07537161772426 40.18140533109495, -105.07528896830341 40.181406010998316, -105.07528732196002 40.181406024764264, -105.07528570849966 40.181406037750406, -105.07517257117757 40.18140697482621, -105.0751256104216 40.18140737415841, -105.07507947870778 40.181407766611606, -105.07499461444203 40.18140848769917, -105.07495129983145 40.1814088562331, -105.07494910626858 40.181408875187515, -105.07484883070958 40.18140972683914, -105.07434600026936 40.18141399915928, -105.07422139534653 40.18141533169408, -105.07415899893937 40.181415998916016))</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -4478,7 +4498,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.059747225974 40.18174422809434, -105.0599001379389 40.18194956648689, -105.0602107919676 40.18217755251773, -105.0609142053907 40.18264013476896, -105.0611256911425 40.18296224313866, -105.0610956824389 40.18379374470699, -105.0610479441212 40.18482678180195, -105.0612086079817 40.18538810152727, -105.0614424718392 40.18606310096347, -105.0622351951782 40.18669611553849, -105.0630597388427 40.18749304870389, -105.063108661064 40.18754993426116, -105.0631167943398 40.18756256584666, -105.0635401820393 40.18815007432843, -105.0640045704488 40.18875033664372, -105.0641869916493 40.18894930200723, -105.0651997902578 40.18891749747873, -105.0654836260324 40.18890612936462, -105.0660593651484 40.18888963844063, -105.0667321623178 40.18886696164368, -105.0684881182713 40.18882795956538, -105.0712696953714 40.18877960887091, -105.0723715024337 40.18876381652939, -105.0741305895364 40.18874473545243, -105.074197000453 40.18874392269232, -105.074197000263 40.18869199904079, -105.0742039991643 40.18429199826076, -105.0741979989235 40.1834589986692, -105.0741819992327 40.18232099821282, -105.0741589989394 40.18141599891602, -105.0741590040985 40.18141592508253, -105.0741588784485 40.18141592642099, -105.0736709800798 40.18142812870585, -105.071855079057 40.1814689097076, -105.0705671335802 40.18150201555372, -105.0681970778381 40.1815609933296, -105.0670932333527 40.18157908311534, -105.0666149759152 40.18158691732067, -105.0655768798686 40.18161404104264, -105.0649311500239 40.18162506478151, -105.0647829616283 40.18163038730162, -105.0647003861965 40.18163209925449, -105.064327931285 40.18164053757673, -105.0640804191193 40.1816461432256, -105.0601897983534 40.18173421777126, -105.059747225974 40.18174422809434))</t>
+          <t>POLYGON ((-105.05974722597395 40.18174422809434, -105.05990013793887 40.18194956648689, -105.06021079196762 40.18217755251773, -105.0609142053907 40.18264013476896, -105.06112569114245 40.18296224313866, -105.06109568243895 40.18379374470699, -105.06104794412117 40.184826781801945, -105.0612086079817 40.185388101527266, -105.06144247183923 40.18606310096347, -105.06223519517822 40.18669611553849, -105.0630597388427 40.187493048703885, -105.06310866106398 40.18754993426116, -105.06311679433985 40.18756256584666, -105.06354018203929 40.18815007432843, -105.0640045704488 40.18875033664372, -105.06418699164927 40.18894930200723, -105.06519979025778 40.188917497478734, -105.0654836260324 40.18890612936462, -105.06605936514839 40.18888963844063, -105.06673216231783 40.18886696164368, -105.06848811827135 40.18882795956538, -105.07126969537143 40.18877960887091, -105.07237150243368 40.18876381652939, -105.07413058953642 40.18874473545243, -105.07419700045295 40.18874392269232, -105.07419700026296 40.18869199904079, -105.07420399916433 40.18429199826076, -105.07419799892354 40.183458998669195, -105.07418199923268 40.182320998212816, -105.07415899893937 40.181415998916016, -105.0741590040985 40.18141592508253, -105.0741588784485 40.18141592642099, -105.07367098007978 40.18142812870585, -105.07185507905702 40.181468909707604, -105.07056713358017 40.18150201555372, -105.06819707783808 40.181560993329605, -105.06709323335268 40.18157908311534, -105.06661497591523 40.181586917320665, -105.06557687986863 40.18161404104264, -105.06493115002391 40.18162506478151, -105.0647829616283 40.18163038730162, -105.06470038619652 40.18163209925449, -105.064327931285 40.181640537576726, -105.06408041911926 40.1816461432256, -105.06018979835343 40.181734217771265, -105.05974722597395 40.18174422809434))</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
@@ -4520,10 +4540,14 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0551857428336 40.19115277071814, -105.0552111773586 40.19115247588264, -105.0576711777204 40.19105147542044, -105.0599381776194 40.19154047538977, -105.0599451784452 40.19310447585676, -105.0593371782352 40.19309847586848, -105.0593451786143 40.19487747591219, -105.0599531783856 40.19487547541794, -105.0599607462004 40.19697811055131, -105.0599628313483 40.19812507551509, -105.0599654497826 40.19956479210923, -105.0599659789192 40.19985581559262, -105.059967664644 40.20078266614567, -105.059968926204 40.2014763253382, -105.0599701793699 40.20216547762988, -105.0602041798525 40.20216247700513, -105.0604371797873 40.20261947653857, -105.0604711807169 40.20272847758034, -105.0604696887987 40.20325998334323, -105.0604691803505 40.2035581312503, -105.0604691803914 40.20358828730515, -105.0605809999359 40.20358599860956, -105.0625290002004 40.20354499890966, -105.0647029999319 40.20349699885044, -105.0647501006766 40.20349602781442, -105.0647339491228 40.20337651726427, -105.0647313741987 40.20266464448074, -105.0647303790163 40.20099722600703, -105.0647362886098 40.20007406548243, -105.0647251582375 40.20007486118185, -105.0647365324077 40.19910003526667, -105.0647365332339 40.19909770441809, -105.064562850699 40.19806721120871, -105.0645385435449 40.19782321419675, -105.0645757570088 40.1971347874193, -105.0645758289882 40.1971334511428, -105.0645220075083 40.19679514516783, -105.0642860933617 40.19647762079072, -105.0638133563912 40.19618043809251, -105.0646926527958 40.19618265905708, -105.0639941019674 40.19573944112544, -105.0632898897123 40.19531381132088, -105.0632053551679 40.19517051471762, -105.0630363648705 40.19487200885944, -105.0629597916534 40.19469895531674, -105.0628134193528 40.19450776646138, -105.0627135803031 40.19432866794923, -105.0626076206911 40.19389338013623, -105.0624336669717 40.19315996562867, -105.0622520623238 40.19240865041179, -105.0621761075427 40.19214028124743, -105.0621311110377 40.19188990154627, -105.0621325686364 40.19166352775939, -105.0621312059593 40.19066864203916, -105.0621129654896 40.18988220023222, -105.0621158423633 40.18943540829499, -105.0621179136866 40.18911371844126, -105.0621190158081 40.18894255062722, -105.0625048190455 40.18897514439156, -105.0633638095203 40.18897514555042, -105.0641869916493 40.18894930200723, -105.0640045704488 40.18875033664372, -105.0635401820393 40.18815007432843, -105.0631167943398 40.18756256584666, -105.063108661064 40.18754993426116, -105.0630597388427 40.18749304870389, -105.0622351951782 40.18669611553849, -105.0614424718392 40.18606310096347, -105.0612086079817 40.18538810152727, -105.0610479441212 40.18482678180195, -105.0610956824389 40.18379374470699, -105.0611256911425 40.18296224313866, -105.0609142053907 40.18264013476896, -105.0602107919676 40.18217755251773, -105.0599001379389 40.18194956648689, -105.059747225974 40.18174422809434, -105.0563433097719 40.18182116446065, -105.0563426497601 40.18182117903999, -105.0563435646631 40.18183609266326, -105.0563475109136 40.18206710151329, -105.0563500596562 40.18221623312483, -105.0558656311479 40.18222843305814, -105.0554415540536 40.18223911220016, -105.0553171302694 40.18224224525912, -105.0553029537267 40.18224260232314, -105.0553029531036 40.18224233843291, -105.0552122394415 40.18224293424132, -105.0551953437782 40.18224286923797, -105.0551907707022 40.18769647581839, -105.0551896265968 40.18906734845638, -105.0551896237061 40.18907048357343, -105.0551895553035 40.18914970721488, -105.0551895524011 40.1891528441331, -105.0551895204548 40.18923708718096, -105.0551895198951 40.1892402250088, -105.0551857428336 40.19115277071814))</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr"/>
+          <t>POLYGON ((-105.05518574283364 40.19115277071814, -105.05521117735856 40.19115247588264, -105.05767117772044 40.19105147542044, -105.05993817761936 40.19154047538977, -105.05994517844516 40.19310447585676, -105.05933717823515 40.19309847586848, -105.0593451786143 40.194877475912186, -105.05995317838557 40.19487547541794, -105.05996074620042 40.19697811055131, -105.05996283134832 40.19812507551509, -105.05996544978255 40.19956479210923, -105.05996597891917 40.19985581559262, -105.05996766464402 40.20078266614567, -105.05996892620396 40.2014763253382, -105.05997017936994 40.202165477629876, -105.06020417985249 40.20216247700513, -105.0604371797873 40.202619476538565, -105.06047118071693 40.20272847758034, -105.06046968879875 40.20325998334323, -105.06046918035045 40.2035581312503, -105.06046918039142 40.20358828730515, -105.06058099993591 40.20358599860956, -105.06252900020037 40.20354499890966, -105.06470299993185 40.20349699885044, -105.06475010067658 40.20349602781442, -105.06473394912284 40.203376517264275, -105.06473137419869 40.20266464448074, -105.06473037901632 40.20099722600703, -105.06473628860981 40.20007406548243, -105.06472515823751 40.200074861181854, -105.06473653240775 40.19910003526667, -105.06473653323386 40.19909770441809, -105.06456285069898 40.19806721120871, -105.06453854354486 40.197823214196745, -105.06457575700881 40.1971347874193, -105.06457582898823 40.1971334511428, -105.06452200750834 40.19679514516783, -105.06428609336166 40.196477620790716, -105.06381335639115 40.19618043809251, -105.06469265279577 40.19618265905708, -105.06399410196742 40.19573944112544, -105.06328988971231 40.19531381132088, -105.0632053551679 40.195170514717624, -105.06303636487053 40.19487200885944, -105.06295979165343 40.19469895531674, -105.06281341935285 40.194507766461385, -105.06271358030307 40.19432866794923, -105.06260762069114 40.19389338013623, -105.06243366697167 40.19315996562867, -105.06225206232376 40.19240865041179, -105.06217610754268 40.19214028124743, -105.06213111103769 40.19188990154627, -105.06213256863641 40.19166352775939, -105.06213120595926 40.190668642039164, -105.06211296548958 40.18988220023222, -105.06211584236327 40.18943540829499, -105.0621179136866 40.18911371844126, -105.06211901580812 40.18894255062722, -105.06250481904551 40.188975144391556, -105.06336380952025 40.188975145550415, -105.06418699164927 40.18894930200723, -105.0640045704488 40.18875033664372, -105.06354018203929 40.18815007432843, -105.06311679433985 40.18756256584666, -105.06310866106398 40.18754993426116, -105.0630597388427 40.187493048703885, -105.06223519517822 40.18669611553849, -105.06144247183923 40.18606310096347, -105.0612086079817 40.185388101527266, -105.06104794412117 40.184826781801945, -105.06109568243895 40.18379374470699, -105.06112569114245 40.18296224313866, -105.0609142053907 40.18264013476896, -105.06021079196762 40.18217755251773, -105.05990013793887 40.18194956648689, -105.05974722597395 40.18174422809434, -105.0563433097719 40.18182116446065, -105.05634264976005 40.18182117903999, -105.05634356466312 40.18183609266326, -105.05634751091362 40.18206710151329, -105.05635005965624 40.182216233124834, -105.05586563114791 40.18222843305814, -105.05544155405357 40.182239112200165, -105.05531713026943 40.18224224525912, -105.05530295372668 40.182242602323136, -105.05530295310362 40.18224233843291, -105.05521223944152 40.182242934241316, -105.05519534377817 40.18224286923797, -105.05519077070223 40.18769647581839, -105.05518962659677 40.18906734845638, -105.05518962370611 40.18907048357343, -105.05518955530353 40.18914970721488, -105.05518955240115 40.189152844133105, -105.05518952045476 40.18923708718096, -105.0551895198951 40.189240225008795, -105.05518574283364 40.19115277071814))</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>Timberline K-8</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4558,7 +4582,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0647339491228 40.20337651726427, -105.0647501006766 40.20349602781442, -105.0647763071737 40.20349548788953, -105.0647999996946 40.20349499884104, -105.0649459997082 40.20349199875547, -105.0650095092602 40.20349053724983, -105.0662489993874 40.20346199884766, -105.067296999437 40.20343799958135, -105.0690749998827 40.2033999992119, -105.074014699015 40.20330567887017, -105.0740449135742 40.20330506064477, -105.0741613829337 40.20330267867917, -105.074174153481 40.20330244200157, -105.0741711838814 40.20330247609904, -105.0741712712824 40.20329264686716, -105.0741714903699 40.20326779279068, -105.0741735880171 40.20303094825258, -105.0741760932321 40.2027479664625, -105.0741819087761 40.20209113330615, -105.0741876627714 40.20144129690684, -105.0741918663698 40.20078168731853, -105.0741944486666 40.20036070732497, -105.0741975998984 40.19984661967961, -105.074199127075 40.19948139601922, -105.0741989123659 40.19907360358597, -105.0741986932105 40.19865770627052, -105.0741983171571 40.19794219855124, -105.074198183371 40.19768747513977, -105.0741931830242 40.197637475825, -105.0741931829567 40.19745124190834, -105.0741931823814 40.19692335905753, -105.0741931821864 40.1964505573902, -105.0741932934809 40.1959239402651, -105.0741934852469 40.19582692062273, -105.0741833857628 40.19582695548362, -105.0741833528728 40.19582695626313, -105.0741846979554 40.19519860032454, -105.0741849993988 40.19506099831302, -105.0741866277237 40.19350533427544, -105.0741868342215 40.19330843383593, -105.0741869991224 40.19315099831903, -105.0741848767469 40.19186178209335, -105.0741831076248 40.19078680189006, -105.0741829994041 40.19072099901145, -105.0741969996016 40.18953799820169, -105.074197000453 40.18874392269232, -105.0741305895364 40.18874473545243, -105.0723715024337 40.18876381652939, -105.0712696953714 40.18877960887091, -105.0684881182713 40.18882795956538, -105.0667321623178 40.18886696164368, -105.0660593651484 40.18888963844063, -105.0654836260324 40.18890612936462, -105.0651997902578 40.18891749747873, -105.0641869916493 40.18894930200723, -105.0633638095203 40.18897514555042, -105.0625048190455 40.18897514439156, -105.0621190158081 40.18894255062722, -105.0621179136866 40.18911371844126, -105.0621158423633 40.18943540829499, -105.0621129654896 40.18988220023222, -105.0621312059593 40.19066864203916, -105.0621325686364 40.19166352775939, -105.0621311110377 40.19188990154627, -105.0621761075427 40.19214028124743, -105.0622520623238 40.19240865041179, -105.0624336669717 40.19315996562867, -105.0626076206911 40.19389338013623, -105.0627135803031 40.19432866794923, -105.0628134193528 40.19450776646138, -105.0629597916534 40.19469895531674, -105.0630363648705 40.19487200885944, -105.0632053551679 40.19517051471762, -105.0632898897123 40.19531381132088, -105.0639941019674 40.19573944112544, -105.0646926527958 40.19618265905708, -105.0638133563912 40.19618043809251, -105.0642860933617 40.19647762079072, -105.0645220075083 40.19679514516783, -105.0645758289882 40.1971334511428, -105.0645757570088 40.1971347874193, -105.0645385435449 40.19782321419675, -105.064562850699 40.19806721120871, -105.0647365332339 40.19909770441809, -105.0647365324077 40.19910003526667, -105.0647251582375 40.20007486118185, -105.0647362886098 40.20007406548243, -105.0647303790163 40.20099722600703, -105.0647313741987 40.20266464448074, -105.0647339491228 40.20337651726427))</t>
+          <t>POLYGON ((-105.06473394912284 40.203376517264275, -105.06475010067658 40.20349602781442, -105.06477630717366 40.20349548788953, -105.06479999969461 40.203494998841045, -105.06494599970824 40.20349199875547, -105.06500950926018 40.20349053724983, -105.0662489993874 40.20346199884766, -105.06729699943696 40.203437999581354, -105.06907499988272 40.2033999992119, -105.07401469901501 40.203305678870166, -105.0740449135742 40.203305060644766, -105.07416138293372 40.20330267867917, -105.07417415348101 40.20330244200157, -105.07417118388136 40.20330247609904, -105.07417127128235 40.20329264686716, -105.07417149036995 40.203267792790676, -105.07417358801709 40.203030948252575, -105.07417609323211 40.202747966462496, -105.07418190877611 40.20209113330615, -105.07418766277144 40.20144129690684, -105.07419186636979 40.20078168731853, -105.07419444866659 40.20036070732497, -105.0741975998984 40.19984661967961, -105.07419912707498 40.19948139601922, -105.07419891236592 40.19907360358597, -105.07419869321048 40.198657706270524, -105.07419831715706 40.19794219855124, -105.074198183371 40.19768747513977, -105.07419318302424 40.197637475825005, -105.07419318295668 40.19745124190834, -105.07419318238142 40.19692335905753, -105.0741931821864 40.1964505573902, -105.07419329348087 40.1959239402651, -105.07419348524694 40.19582692062273, -105.07418338576284 40.195826955483625, -105.07418335287282 40.19582695626313, -105.07418469795542 40.19519860032454, -105.07418499939884 40.19506099831302, -105.07418662772375 40.19350533427544, -105.07418683422146 40.19330843383593, -105.07418699912239 40.193150998319034, -105.07418487674687 40.19186178209335, -105.07418310762478 40.19078680189006, -105.0741829994041 40.190720999011454, -105.07419699960161 40.18953799820169, -105.07419700045295 40.18874392269232, -105.07413058953642 40.18874473545243, -105.07237150243368 40.18876381652939, -105.07126969537143 40.18877960887091, -105.06848811827135 40.18882795956538, -105.06673216231783 40.18886696164368, -105.06605936514839 40.18888963844063, -105.0654836260324 40.18890612936462, -105.06519979025778 40.188917497478734, -105.06418699164927 40.18894930200723, -105.06336380952025 40.188975145550415, -105.06250481904551 40.188975144391556, -105.06211901580812 40.18894255062722, -105.0621179136866 40.18911371844126, -105.06211584236327 40.18943540829499, -105.06211296548958 40.18988220023222, -105.06213120595926 40.190668642039164, -105.06213256863641 40.19166352775939, -105.06213111103769 40.19188990154627, -105.06217610754268 40.19214028124743, -105.06225206232376 40.19240865041179, -105.06243366697167 40.19315996562867, -105.06260762069114 40.19389338013623, -105.06271358030307 40.19432866794923, -105.06281341935285 40.194507766461385, -105.06295979165343 40.19469895531674, -105.06303636487053 40.19487200885944, -105.0632053551679 40.195170514717624, -105.06328988971231 40.19531381132088, -105.06399410196742 40.19573944112544, -105.06469265279577 40.19618265905708, -105.06381335639115 40.19618043809251, -105.06428609336166 40.196477620790716, -105.06452200750834 40.19679514516783, -105.06457582898823 40.1971334511428, -105.06457575700881 40.1971347874193, -105.06453854354486 40.197823214196745, -105.06456285069898 40.19806721120871, -105.06473653323386 40.19909770441809, -105.06473653240775 40.19910003526667, -105.06472515823751 40.200074861181854, -105.06473628860981 40.20007406548243, -105.06473037901632 40.20099722600703, -105.06473137419869 40.20266464448074, -105.06473394912284 40.203376517264275))</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -4600,7 +4624,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.074197000453 40.18874392269232, -105.0741969996016 40.18953799820169, -105.0741829994041 40.19072099901145, -105.0741831076248 40.19078680189006, -105.0741848767469 40.19186178209335, -105.0741869991224 40.19315099831903, -105.0741868342215 40.19330843383593, -105.0741866277237 40.19350533427544, -105.0741849993988 40.19506099831302, -105.0741846979554 40.19519860032454, -105.0741833211629 40.19582695614638, -105.0741833857628 40.19582695548362, -105.0860866501783 40.19578522125577, -105.0864171348487 40.19578640374956, -105.086511852989 40.19573006805931, -105.0863691492831 40.19564994852773, -105.0862408498609 40.19555587994729, -105.0860970978373 40.19541289181424, -105.0856561157612 40.19475906525103, -105.085164539641 40.19405220507761, -105.0846108330115 40.19347003621436, -105.0839140133439 40.19274500746122, -105.0838198935418 40.19262388145074, -105.0837278943623 40.19244895886795, -105.0836760421697 40.19226512124251, -105.0836707930744 40.19210275239081, -105.0836661096728 40.19195790388677, -105.0836579889063 40.19147198297522, -105.0836569850927 40.19116809046359, -105.0836591007846 40.19076401224247, -105.0836590748625 40.19070993241241, -105.0836319747668 40.19057587116042, -105.0833600845804 40.19002503843247, -105.0833160586309 40.18990793636564, -105.0831958823899 40.18936698223978, -105.0831681055887 40.18922687962414, -105.0831121703438 40.18900898727944, -105.0831049109525 40.18896696071855, -105.0830889958185 40.18881893919583, -105.0830848538614 40.18867699980355, -105.0830850002736 40.18865311719252, -105.0828160158762 40.1886809719122, -105.0808020163372 40.18868208690873, -105.0807080918733 40.1886821309134, -105.0792469265356 40.18869000018054, -105.0785510892 40.18868993637176, -105.0778161408352 40.18870509857946, -105.0776511302102 40.18870504443171, -105.0753352826321 40.18872998637555, -105.074197000453 40.18874392269232))</t>
+          <t>POLYGON ((-105.07419700045295 40.18874392269232, -105.07419699960161 40.18953799820169, -105.0741829994041 40.190720999011454, -105.07418310762478 40.19078680189006, -105.07418487674687 40.19186178209335, -105.07418699912239 40.193150998319034, -105.07418683422146 40.19330843383593, -105.07418662772375 40.19350533427544, -105.07418499939884 40.19506099831302, -105.07418469795542 40.19519860032454, -105.07418332116288 40.19582695614638, -105.07418338576284 40.195826955483625, -105.0860866501783 40.19578522125577, -105.08641713484873 40.19578640374956, -105.08651185298896 40.195730068059305, -105.08636914928312 40.19564994852773, -105.08624084986089 40.19555587994729, -105.08609709783727 40.19541289181424, -105.08565611576118 40.194759065251034, -105.08516453964101 40.19405220507761, -105.08461083301145 40.19347003621436, -105.08391401334387 40.19274500746122, -105.08381989354177 40.19262388145074, -105.08372789436226 40.19244895886795, -105.08367604216966 40.192265121242514, -105.08367079307445 40.19210275239081, -105.08366610967276 40.191957903886774, -105.08365798890631 40.191471982975216, -105.08365698509266 40.19116809046359, -105.0836591007846 40.19076401224247, -105.08365907486252 40.19070993241241, -105.08363197476682 40.19057587116042, -105.08336008458038 40.19002503843247, -105.08331605863091 40.18990793636564, -105.08319588238986 40.18936698223978, -105.08316810558865 40.189226879624144, -105.08311217034375 40.189008987279436, -105.08310491095251 40.18896696071855, -105.08308899581846 40.18881893919583, -105.08308485386137 40.188676999803555, -105.08308500027364 40.188653117192516, -105.0828160158762 40.1886809719122, -105.08080201633722 40.18868208690873, -105.08070809187328 40.1886821309134, -105.07924692653562 40.18869000018054, -105.07855108920002 40.18868993637176, -105.07781614083518 40.18870509857946, -105.07765113021019 40.188705044431714, -105.07533528263208 40.18872998637555, -105.07419700045295 40.18874392269232))</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -4642,7 +4666,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.086511852989 40.19573006805931, -105.0867218461393 40.19581207519037, -105.0868898415345 40.19585412732779, -105.0870629523426 40.19587890254427, -105.0872988309592 40.19588386235068, -105.0874972275109 40.19588263658899, -105.0880582329032 40.19587916782289, -105.0881840468208 40.19587839019044, -105.0892681643353 40.19586891298781, -105.0902370981357 40.1957691329993, -105.0910999059538 40.1957559910603, -105.0924638566949 40.19574708041702, -105.09306383352 40.19574606186691, -105.0930503658067 40.1885802518252, -105.0925408347064 40.1885759229387, -105.091522093662 40.18858303424472, -105.0905810015349 40.18859398078645, -105.0892150876339 40.18859599888286, -105.0882951376611 40.18860288421402, -105.086419060216 40.18862089503253, -105.0850681792846 40.18862291791372, -105.0850019534098 40.18862405280476, -105.0840608966072 40.18862890672658, -105.0834201577121 40.1886329134413, -105.0830850002736 40.18865311719252, -105.0830848538614 40.18867699980355, -105.0830889958185 40.18881893919583, -105.0831049109525 40.18896696071855, -105.0831121703438 40.18900898727944, -105.0831681055887 40.18922687962414, -105.0831958823899 40.18936698223978, -105.0833160586309 40.18990793636564, -105.0833600845804 40.19002503843247, -105.0836319747668 40.19057587116042, -105.0836590748625 40.19070993241241, -105.0836591007846 40.19076401224247, -105.0836569850927 40.19116809046359, -105.0836579889063 40.19147198297522, -105.0836661096728 40.19195790388677, -105.0836707930744 40.19210275239081, -105.0836760421697 40.19226512124251, -105.0837278943623 40.19244895886795, -105.0838198935418 40.19262388145074, -105.0839140133439 40.19274500746122, -105.0846108330115 40.19347003621436, -105.085164539641 40.19405220507761, -105.0856561157612 40.19475906525103, -105.0860970978373 40.19541289181424, -105.0862408498609 40.19555587994729, -105.0863691492831 40.19564994852773, -105.086511852989 40.19573006805931))</t>
+          <t>POLYGON ((-105.08651185298896 40.195730068059305, -105.08672184613931 40.19581207519037, -105.08688984153449 40.19585412732779, -105.08706295234258 40.195878902544266, -105.08729883095923 40.195883862350684, -105.08749722751094 40.19588263658899, -105.08805823290322 40.19587916782289, -105.08818404682084 40.19587839019044, -105.08926816433527 40.195868912987805, -105.09023709813569 40.195769132999295, -105.09109990595384 40.1957559910603, -105.09246385669488 40.19574708041702, -105.09306383351996 40.19574606186691, -105.09305036580668 40.1885802518252, -105.09254083470643 40.1885759229387, -105.09152209366201 40.18858303424472, -105.09058100153493 40.18859398078645, -105.08921508763389 40.18859599888286, -105.08829513766112 40.18860288421402, -105.08641906021597 40.18862089503253, -105.08506817928458 40.18862291791372, -105.08500195340982 40.18862405280476, -105.08406089660723 40.18862890672658, -105.08342015771214 40.188632913441296, -105.08308500027364 40.188653117192516, -105.08308485386137 40.188676999803555, -105.08308899581846 40.18881893919583, -105.08310491095251 40.18896696071855, -105.08311217034375 40.189008987279436, -105.08316810558865 40.189226879624144, -105.08319588238986 40.18936698223978, -105.08331605863091 40.18990793636564, -105.08336008458038 40.19002503843247, -105.08363197476682 40.19057587116042, -105.08365907486252 40.19070993241241, -105.0836591007846 40.19076401224247, -105.08365698509266 40.19116809046359, -105.08365798890631 40.191471982975216, -105.08366610967276 40.191957903886774, -105.08367079307445 40.19210275239081, -105.08367604216966 40.192265121242514, -105.08372789436226 40.19244895886795, -105.08381989354177 40.19262388145074, -105.08391401334387 40.19274500746122, -105.08461083301145 40.19347003621436, -105.08516453964101 40.19405220507761, -105.08565611576118 40.194759065251034, -105.08609709783727 40.19541289181424, -105.08624084986089 40.19555587994729, -105.08636914928312 40.19564994852773, -105.08651185298896 40.195730068059305))</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -4684,7 +4708,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.09306383352 40.19574606186691, -105.0930949795306 40.19574600935555, -105.0933991408409 40.1957660205662, -105.0937480333861 40.19578893417904, -105.0942998324741 40.19582298908553, -105.0944211395721 40.19583110066097, -105.0949888953552 40.19583089576602, -105.0955698757631 40.19583402616591, -105.096581827718 40.19584305219868, -105.0976751063603 40.19584109619835, -105.0999060366127 40.19584005096787, -105.1006950211054 40.19584003390204, -105.1015878906684 40.19582801449134, -105.1022181387225 40.19585406733855, -105.1022979448688 40.19585791106639, -105.1023788304601 40.19586093436818, -105.1023809230087 40.19574811518007, -105.1023868541003 40.19503988820251, -105.1023850650994 40.1948559566662, -105.1023748592168 40.19451991641212, -105.1023501276933 40.19385193690373, -105.1023401095519 40.19238187512373, -105.1023480324539 40.19219001707661, -105.1023450792598 40.19183807835071, -105.1023359238445 40.19064912338679, -105.1023129456827 40.18974287047573, -105.102305841591 40.18899891023079, -105.1022938744325 40.18859697923833, -105.1022929712663 40.18856787832284, -105.1022260358258 40.18856792185923, -105.1018591320755 40.18856777761645, -105.1016386463216 40.18856767203621, -105.1013414703393 40.18856752769821, -105.1010960533666 40.18856740807102, -105.1008698157056 40.18856729739159, -105.1006454886887 40.18856718836553, -105.1004760702672 40.18856710473342, -105.0995568688824 40.18856886575384, -105.0992658626611 40.18856895540347, -105.0985989901536 40.18857405442757, -105.0976301211599 40.18856107878358, -105.0965920413584 40.18857008941826, -105.0956509796097 40.1885761355268, -105.0946659350194 40.18857488223757, -105.0944039097845 40.18857604474166, -105.0943032647279 40.18857649050751, -105.0939400119303 40.18857810009743, -105.093651870293 40.18857791098326, -105.0931478712857 40.18858108041262, -105.0930503658067 40.1885802518252, -105.09306383352 40.19574606186691))</t>
+          <t>POLYGON ((-105.09306383351996 40.19574606186691, -105.09309497953063 40.195746009355545, -105.09339914084086 40.1957660205662, -105.09374803338606 40.19578893417904, -105.09429983247412 40.195822989085535, -105.09442113957206 40.195831100660975, -105.09498889535517 40.19583089576602, -105.09556987576313 40.19583402616591, -105.09658182771803 40.19584305219868, -105.09767510636028 40.19584109619835, -105.09990603661265 40.19584005096787, -105.10069502110537 40.195840033902044, -105.10158789066844 40.19582801449134, -105.10221813872249 40.19585406733855, -105.10229794486881 40.19585791106639, -105.10237883046007 40.19586093436818, -105.10238092300867 40.195748115180066, -105.10238685410033 40.19503988820251, -105.10238506509936 40.1948559566662, -105.10237485921675 40.19451991641212, -105.10235012769333 40.193851936903734, -105.10234010955186 40.19238187512373, -105.10234803245389 40.19219001707661, -105.10234507925982 40.191838078350706, -105.10233592384446 40.19064912338679, -105.1023129456827 40.18974287047573, -105.10230584159098 40.18899891023079, -105.10229387443255 40.188596979238326, -105.1022929712663 40.188567878322836, -105.10222603582581 40.18856792185923, -105.10185913207549 40.18856777761645, -105.10163864632163 40.18856767203621, -105.10134147033934 40.18856752769821, -105.10109605336665 40.188567408071016, -105.1008698157056 40.188567297391586, -105.10064548868866 40.18856718836553, -105.10047607026725 40.188567104733416, -105.09955686888244 40.18856886575384, -105.0992658626611 40.18856895540347, -105.09859899015365 40.18857405442757, -105.09763012115991 40.18856107878358, -105.09659204135845 40.188570089418256, -105.09565097960967 40.1885761355268, -105.09466593501938 40.188574882237575, -105.09440390978452 40.18857604474166, -105.0943032647279 40.18857649050751, -105.09394001193029 40.18857810009743, -105.09365187029303 40.188577910983255, -105.09314787128572 40.18858108041262, -105.09305036580668 40.1885802518252, -105.09306383351996 40.19574606186691))</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
@@ -4726,7 +4750,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1023480324539 40.19219001707661, -105.1048453489194 40.19218432049806, -105.1059229963339 40.19218606010607, -105.1065980674279 40.19219302506354, -105.1068051588693 40.19222200496674, -105.1069888555251 40.1922728652199, -105.1071770321067 40.19235393786226, -105.1077561498077 40.19267488967569, -105.1080720417897 40.19283188541718, -105.1081381084471 40.19285901135972, -105.1084081410572 40.19296094791824, -105.1087690678741 40.19306813230949, -105.1090740328479 40.1931339492639, -105.1093841120682 40.19318193926935, -105.1095688341273 40.19319899075646, -105.1096989545908 40.19321100232427, -105.1102461680016 40.1932309662153, -105.111723928605 40.1932291578423, -105.1122980561094 40.19322496265376, -105.1132889302573 40.19322004532617, -105.1139461768446 40.19321592716982, -105.1147551471709 40.19322109568412, -105.1166809681976 40.19322612331362, -105.1166861053213 40.1925689529913, -105.1166981026633 40.19228212466017, -105.1167018435294 40.19193597372305, -105.1167068843998 40.19148606110486, -105.1167070286926 40.19127001861614, -105.1167131784508 40.19106799642823, -105.1167148355026 40.19090109679001, -105.116718167382 40.19081793041203, -105.1167230820158 40.19058104045865, -105.1167349755193 40.19012209095266, -105.116760120845 40.18921709887078, -105.1167670206291 40.18900904033057, -105.1167671242837 40.18854593391976, -105.1158580022557 40.18853797614679, -105.1146671019506 40.18854389517986, -105.1145858430134 40.18854499691239, -105.1134489979368 40.18854998659783, -105.1133670179578 40.18855190824585, -105.1125820027335 40.18856108520247, -105.1125329666713 40.18856092088617, -105.1120540599835 40.18855794243968, -105.1117581070876 40.18856554113695, -105.111460935844 40.18856089171691, -105.1102081396324 40.18856189061061, -105.1080901776704 40.18856708418473, -105.1075808282699 40.18856700385626, -105.1069608759509 40.18856709474983, -105.1067500432291 40.18856802423286, -105.106394960974 40.18856901265301, -105.1057839557793 40.18856912679325, -105.1051969341203 40.18856904580717, -105.1046560755281 40.18857104075413, -105.1035181760235 40.18857208617342, -105.1031670440105 40.18857088157077, -105.1022929712663 40.18856787832284, -105.1022938744325 40.18859697923833, -105.102305841591 40.18899891023079, -105.1023129456827 40.18974287047573, -105.1023359238445 40.19064912338679, -105.1023450792598 40.19183807835071, -105.1023480324539 40.19219001707661))</t>
+          <t>POLYGON ((-105.10234803245389 40.19219001707661, -105.10484534891944 40.192184320498065, -105.10592299633394 40.19218606010607, -105.10659806742791 40.19219302506354, -105.1068051588693 40.19222200496674, -105.10698885552506 40.1922728652199, -105.10717703210675 40.192353937862265, -105.10775614980767 40.192674889675686, -105.10807204178971 40.19283188541718, -105.10813810844714 40.192859011359715, -105.10840814105715 40.192960947918245, -105.10876906787412 40.19306813230949, -105.10907403284793 40.1931339492639, -105.10938411206821 40.19318193926935, -105.10956883412727 40.193198990756464, -105.10969895459078 40.19321100232427, -105.11024616800164 40.1932309662153, -105.11172392860504 40.1932291578423, -105.11229805610941 40.19322496265376, -105.11328893025734 40.19322004532617, -105.11394617684462 40.19321592716982, -105.11475514717092 40.193221095684116, -105.1166809681976 40.19322612331362, -105.11668610532125 40.1925689529913, -105.11669810266332 40.19228212466017, -105.1167018435294 40.19193597372305, -105.11670688439978 40.19148606110486, -105.1167070286926 40.191270018616144, -105.1167131784508 40.19106799642823, -105.11671483550258 40.19090109679001, -105.11671816738198 40.19081793041203, -105.1167230820158 40.19058104045865, -105.11673497551928 40.190122090952656, -105.116760120845 40.189217098870785, -105.11676702062908 40.18900904033057, -105.11676712428374 40.188545933919755, -105.1158580022557 40.18853797614679, -105.11466710195064 40.18854389517986, -105.11458584301336 40.18854499691239, -105.1134489979368 40.18854998659783, -105.11336701795776 40.18855190824585, -105.11258200273355 40.18856108520247, -105.1125329666713 40.18856092088617, -105.11205405998355 40.18855794243968, -105.11175810708758 40.18856554113695, -105.11146093584401 40.18856089171691, -105.11020813963242 40.188561890610615, -105.10809017767042 40.188567084184726, -105.10758082826989 40.188567003856264, -105.1069608759509 40.18856709474983, -105.10675004322914 40.18856802423286, -105.10639496097401 40.18856901265301, -105.10578395577929 40.18856912679325, -105.10519693412031 40.18856904580717, -105.10465607552808 40.188571040754134, -105.10351817602353 40.18857208617342, -105.10316704401049 40.18857088157077, -105.1022929712663 40.188567878322836, -105.10229387443255 40.188596979238326, -105.10230584159098 40.18899891023079, -105.1023129456827 40.18974287047573, -105.10233592384446 40.19064912338679, -105.10234507925982 40.191838078350706, -105.10234803245389 40.19219001707661))</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
@@ -4768,7 +4792,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.125718068953 40.19610107083675, -105.1261540832188 40.19610193189156, -105.1267601314409 40.19610388963849, -105.1275960252971 40.19610191756082, -105.1284459067967 40.19609504349872, -105.1293050405962 40.19609807552655, -105.1301501480823 40.19611313473412, -105.1306419632079 40.19612211894584, -105.1308460028724 40.19612386837532, -105.1309118755788 40.1961229807733, -105.1309143668815 40.19582627612956, -105.1309068952795 40.19506196744772, -105.1309159646022 40.19339102690551, -105.1309241714 40.19306602798519, -105.130927931161 40.19290105697731, -105.130938058077 40.19248602396898, -105.1309351053868 40.19177694371588, -105.1309290385914 40.19131189615173, -105.1309189078632 40.19073812877721, -105.1309210102063 40.19008698709673, -105.1309218016256 40.18977065007875, -105.130921928735 40.1897199644653, -105.1309229040069 40.18960604336813, -105.1309280418581 40.18905510978355, -105.1309169704838 40.1885889481708, -105.1288573477865 40.18857997484698, -105.1256918879809 40.18856611215961, -105.121360830748 40.18856299055086, -105.1194899230949 40.18855492662844, -105.1190850825382 40.1885568881324, -105.1186970917979 40.1885539619918, -105.1183019485997 40.18854991306068, -105.1179300587332 40.18854813537448, -105.1174969479037 40.18854890001953, -105.1172141737779 40.18854906207515, -105.1167671242837 40.18854593391976, -105.1167670206291 40.18900904033057, -105.116760120845 40.18921709887078, -105.1167349755193 40.19012209095266, -105.1167230820158 40.19058104045865, -105.116718167382 40.19081793041203, -105.1167148355026 40.19090109679001, -105.1167131784508 40.19106799642823, -105.1167070286926 40.19127001861614, -105.1167068843998 40.19148606110486, -105.1167018435294 40.19193597372305, -105.1166981026633 40.19228212466017, -105.1166861053213 40.1925689529913, -105.1166809681976 40.19322612331362, -105.1166770285451 40.19392502492807, -105.1166778838765 40.19459896050941, -105.1166729592587 40.19528193635994, -105.1166738359791 40.19569810347589, -105.1184608325745 40.19570291563901, -105.1193890683886 40.19570295481263, -105.1199198436 40.1957219946514, -105.1207269104129 40.19575292005293, -105.1210021402629 40.19576288105466, -105.1213803209356 40.19577337127161, -105.1219490189156 40.19582231088875, -105.1229019987192 40.19589880009727, -105.1237576535158 40.19596722385328, -105.1245997948084 40.1960523429243, -105.1247440565115 40.19609187444581, -105.125718068953 40.19610107083675))</t>
+          <t>POLYGON ((-105.12571806895298 40.19610107083675, -105.12615408321882 40.19610193189156, -105.12676013144088 40.196103889638486, -105.12759602529707 40.196101917560824, -105.12844590679666 40.19609504349872, -105.12930504059624 40.19609807552655, -105.13015014808231 40.19611313473412, -105.13064196320786 40.19612211894584, -105.13084600287245 40.196123868375324, -105.13091187557878 40.196122980773296, -105.13091436688147 40.19582627612956, -105.13090689527945 40.19506196744772, -105.13091596460222 40.19339102690551, -105.13092417140001 40.19306602798519, -105.13092793116098 40.192901056977306, -105.13093805807702 40.19248602396898, -105.13093510538684 40.19177694371588, -105.13092903859138 40.19131189615173, -105.13091890786323 40.190738128777205, -105.13092101020634 40.19008698709673, -105.13092180162565 40.18977065007875, -105.13092192873505 40.1897199644653, -105.13092290400688 40.18960604336813, -105.13092804185807 40.18905510978355, -105.13091697048377 40.188588948170796, -105.1288573477865 40.18857997484698, -105.12569188798088 40.18856611215961, -105.12136083074796 40.188562990550864, -105.11948992309487 40.18855492662844, -105.11908508253823 40.188556888132396, -105.1186970917979 40.1885539619918, -105.11830194859972 40.18854991306068, -105.11793005873315 40.18854813537448, -105.1174969479037 40.18854890001953, -105.11721417377788 40.18854906207515, -105.11676712428374 40.188545933919755, -105.11676702062908 40.18900904033057, -105.116760120845 40.189217098870785, -105.11673497551928 40.190122090952656, -105.1167230820158 40.19058104045865, -105.11671816738198 40.19081793041203, -105.11671483550258 40.19090109679001, -105.1167131784508 40.19106799642823, -105.1167070286926 40.191270018616144, -105.11670688439978 40.19148606110486, -105.1167018435294 40.19193597372305, -105.11669810266332 40.19228212466017, -105.11668610532125 40.1925689529913, -105.1166809681976 40.19322612331362, -105.11667702854506 40.19392502492807, -105.11667788387655 40.19459896050941, -105.11667295925871 40.19528193635994, -105.11667383597906 40.19569810347589, -105.11846083257448 40.19570291563901, -105.11938906838859 40.19570295481263, -105.11991984359999 40.1957219946514, -105.12072691041293 40.195752920052925, -105.12100214026289 40.19576288105466, -105.12138032093561 40.19577337127161, -105.1219490189156 40.19582231088875, -105.1229019987192 40.19589880009727, -105.12375765351578 40.19596722385328, -105.12459979480842 40.1960523429243, -105.12474405651152 40.196091874445806, -105.12571806895298 40.19610107083675))</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
@@ -4810,7 +4834,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1309169704838 40.1885889481708, -105.1309280418581 40.18905510978355, -105.1309229040069 40.18960604336813, -105.130921928735 40.1897199644653, -105.1309218016256 40.18977065007875, -105.1309210102063 40.19008698709673, -105.1309189078632 40.19073812877721, -105.1309290385914 40.19131189615173, -105.1309351053868 40.19177694371588, -105.130938058077 40.19248602396898, -105.130927931161 40.19290105697731, -105.1309241714 40.19306602798519, -105.1309159646022 40.19339102690551, -105.1309068952795 40.19506196744772, -105.1309143668815 40.19582627612956, -105.1309118755788 40.1961229807733, -105.131428863541 40.19611090406575, -105.131612962076 40.19609309792698, -105.1323279809317 40.19593588095032, -105.1324450826828 40.1959280178147, -105.1332540925827 40.19593195905006, -105.1348288727205 40.19592596231499, -105.1350301269854 40.19591287200842, -105.1352240019548 40.19587395396812, -105.1354079776137 40.19581194452213, -105.1355888803089 40.19572192524484, -105.1358369116012 40.19559697881763, -105.13602885285 40.19551797416268, -105.136236034898 40.19546701789125, -105.1364520129437 40.19544491193961, -105.1366678295033 40.19545300248294, -105.1368781329192 40.19548797729049, -105.1370768360099 40.19555009198046, -105.137260019817 40.19563604069402, -105.1373920121044 40.1957221032935, -105.1374988457707 40.1958270281356, -105.1375698904066 40.19579595645354, -105.1376941713428 40.19571701074948, -105.1377931598583 40.19561492762381, -105.1378440929554 40.19552888914305, -105.1378820027869 40.19540108431987, -105.1378798473228 40.19526793844083, -105.1378531631223 40.19517012782561, -105.1378230709578 40.19510689543214, -105.1376100574661 40.19484187083497, -105.1375454390307 40.19470839136561, -105.1375355616143 40.19454672605157, -105.1375923408581 40.19430395938474, -105.1376931509601 40.19402737308724, -105.1378172716755 40.1937425963769, -105.1379855382644 40.19340239572814, -105.1380299823671 40.19334054861462, -105.1381209562706 40.19321395361075, -105.1382048744235 40.19298307526579, -105.1382230760014 40.19292603371227, -105.1382309133731 40.19246212904983, -105.1382130616972 40.19211700809573, -105.1382100112756 40.19188311242785, -105.1381899159193 40.19135406015155, -105.1381931303606 40.19122093099875, -105.1382269980436 40.19104507341488, -105.1382800092054 40.19090386463147, -105.1383409875964 40.19081291641721, -105.1384888809863 40.19066706248092, -105.1386390933875 40.19055607922262, -105.1388418881127 40.19045212286864, -105.1390571245268 40.1903641264425, -105.1392741398997 40.19027805712356, -105.1397161515111 40.19008590298159, -105.1398931114001 40.18999311953126, -105.140055118217 40.18988491630473, -105.1402460544696 40.18972107600812, -105.1403249583222 40.18962386905537, -105.1403530843913 40.18958497521279, -105.1404669626501 40.18937203172319, -105.1405340864813 40.18920094393643, -105.1405498995005 40.18912110937249, -105.1405798463564 40.18860209558213, -105.1395980233061 40.18860096041269, -105.134910837415 40.18859394212554, -105.1344490936186 40.18859413046857, -105.1339970425581 40.18858913116373, -105.1337998285665 40.18858713414526, -105.1336301658559 40.18858687135872, -105.1332378739106 40.18858507826119, -105.1329919645237 40.18858594522387, -105.1324877712597 40.18858819304007, -105.1318741020108 40.18858897966873, -105.1309169704838 40.1885889481708))</t>
+          <t>POLYGON ((-105.13091697048377 40.188588948170796, -105.13092804185807 40.18905510978355, -105.13092290400688 40.18960604336813, -105.13092192873505 40.1897199644653, -105.13092180162565 40.18977065007875, -105.13092101020634 40.19008698709673, -105.13091890786323 40.190738128777205, -105.13092903859138 40.19131189615173, -105.13093510538684 40.19177694371588, -105.13093805807702 40.19248602396898, -105.13092793116098 40.192901056977306, -105.13092417140001 40.19306602798519, -105.13091596460222 40.19339102690551, -105.13090689527945 40.19506196744772, -105.13091436688147 40.19582627612956, -105.13091187557878 40.196122980773296, -105.13142886354099 40.19611090406575, -105.13161296207605 40.196093097926976, -105.13232798093173 40.195935880950316, -105.13244508268276 40.1959280178147, -105.13325409258266 40.19593195905006, -105.13482887272048 40.19592596231499, -105.1350301269854 40.19591287200842, -105.13522400195484 40.195873953968125, -105.13540797761367 40.195811944522134, -105.13558888030886 40.19572192524484, -105.13583691160122 40.19559697881763, -105.13602885285 40.19551797416268, -105.13623603489803 40.195467017891254, -105.13645201294366 40.19544491193961, -105.13666782950332 40.195453002482935, -105.13687813291924 40.19548797729049, -105.13707683600988 40.195550091980465, -105.13726001981696 40.19563604069402, -105.1373920121044 40.1957221032935, -105.13749884577068 40.1958270281356, -105.1375698904066 40.19579595645354, -105.13769417134282 40.195717010749476, -105.13779315985835 40.19561492762381, -105.13784409295539 40.19552888914305, -105.13788200278685 40.19540108431987, -105.13787984732282 40.19526793844083, -105.13785316312227 40.19517012782561, -105.13782307095784 40.19510689543214, -105.13761005746609 40.19484187083497, -105.13754543903072 40.19470839136561, -105.13753556161427 40.19454672605157, -105.13759234085808 40.19430395938474, -105.13769315096015 40.194027373087245, -105.13781727167549 40.1937425963769, -105.13798553826442 40.193402395728135, -105.13802998236713 40.19334054861462, -105.13812095627064 40.19321395361075, -105.13820487442351 40.192983075265786, -105.1382230760014 40.19292603371227, -105.13823091337305 40.19246212904983, -105.1382130616972 40.19211700809573, -105.13821001127562 40.191883112427846, -105.13818991591928 40.191354060151546, -105.13819313036059 40.191220930998746, -105.13822699804356 40.19104507341488, -105.13828000920537 40.19090386463147, -105.13834098759642 40.19081291641721, -105.13848888098627 40.19066706248092, -105.1386390933875 40.190556079222624, -105.13884188811272 40.19045212286864, -105.13905712452683 40.190364126442496, -105.13927413989974 40.19027805712356, -105.1397161515111 40.19008590298159, -105.1398931114001 40.18999311953126, -105.14005511821703 40.18988491630473, -105.14024605446957 40.18972107600812, -105.14032495832224 40.18962386905537, -105.14035308439134 40.18958497521279, -105.14046696265011 40.18937203172319, -105.14053408648128 40.18920094393643, -105.14054989950047 40.189121109372486, -105.14057984635642 40.18860209558213, -105.1395980233061 40.18860096041269, -105.13491083741502 40.188593942125536, -105.13444909361857 40.188594130468566, -105.13399704255812 40.18858913116373, -105.13379982856648 40.18858713414526, -105.1336301658559 40.188586871358716, -105.13323787391064 40.18858507826119, -105.13299196452373 40.18858594522387, -105.1324877712597 40.18858819304007, -105.13187410201084 40.18858897966873, -105.13091697048377 40.188588948170796))</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
@@ -4852,7 +4876,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1409040306353 40.19154572658073, -105.1409890318654 40.19152972594931, -105.1411226446519 40.19153998197216, -105.1417411975476 40.19152646954736, -105.1422191542082 40.19159290600409, -105.1430128227406 40.19170322191939, -105.1435901972262 40.19178347003211, -105.1446851981676 40.19186346973615, -105.1454650795996 40.19166871898251, -105.145540002091 40.19156738941043, -105.145556198577 40.19110246879873, -105.1458950200733 40.19099873057759, -105.146023039163 40.19095953422137, -105.1469560824025 40.19063072326936, -105.1475290858815 40.19047172415833, -105.1479800890678 40.19036772283105, -105.1484240929505 40.19029072383959, -105.1486820954207 40.19027472289796, -105.1489900989153 40.19026372220461, -105.1493191020164 40.19026372260259, -105.1496481067909 40.19028072156684, -105.1498131075271 40.19030272138396, -105.150400114481 40.19034672131698, -105.1510521225241 40.19039872026119, -105.151725130212 40.19045971848809, -105.1520301329908 40.190480717349, -105.1520391995797 40.1904813219414, -105.1520391995784 40.1904544685933, -105.1522062000076 40.19044046900569, -105.1523262006294 40.19040146942321, -105.1526282001168 40.19021446851695, -105.1527832001366 40.1899674691564, -105.154617200905 40.18989046922776, -105.1555431997794 40.19021346870296, -105.155531199946 40.18866546838077, -105.1555308853084 40.18865548209631, -105.1548381373372 40.18865072595334, -105.1548369993615 40.18865397295026, -105.1547139138904 40.18865312900746, -105.1545576450007 40.18865252803892, -105.1531178909332 40.18864697919484, -105.15211893606 40.1886360171759, -105.1514639163036 40.18863404452328, -105.1514618466591 40.18813002987395, -105.1514729168124 40.18729691198585, -105.1514629316738 40.18715001697894, -105.1514418613204 40.1870708929312, -105.1513771482871 40.18691697006431, -105.1512841145291 40.18677202034032, -105.1512549275952 40.18674008851822, -105.1510561674728 40.18655199530703, -105.1508920796487 40.18644306698239, -105.150754973536 40.18637704427427, -105.1507049815138 40.18635410806133, -105.1505470758935 40.18629598298839, -105.1503790560849 40.18625594521194, -105.1502070059285 40.18623401219416, -105.149767435774 40.18623386221527, -105.149422086174 40.1862310863429, -105.1492338322608 40.18622804402173, -105.1484761105867 40.18622601744052, -105.1481271732022 40.18621809316517, -105.1479840590923 40.18620695166086, -105.1477029506709 40.18616409427499, -105.1475689822392 40.18611509756006, -105.1473779389415 40.1860288663483, -105.1465411469029 40.18553904801176, -105.146354126635 40.18543690593991, -105.1455759136412 40.18497306383122, -105.1447638346391 40.18448495549296, -105.1445681553766 40.18467102363869, -105.1439618997615 40.18527501200008, -105.1438099169543 40.18538599674668, -105.1436329945333 40.18547494330328, -105.1434608562389 40.18553892338728, -105.1433229083853 40.185567047181, -105.143180039099 40.18557813629327, -105.1427991722154 40.18558492095656, -105.1421778420108 40.18557997984929, -105.1411838501522 40.18558705667058, -105.1405499407048 40.18559195046055, -105.1405721409861 40.18633513022635, -105.1405741264152 40.18704310963169, -105.1405770053055 40.18778513128763, -105.1405798463564 40.18860209558213, -105.1405498995005 40.18912110937249, -105.1405340864813 40.18920094393643, -105.1404669626501 40.18937203172319, -105.1403530843913 40.18958497521279, -105.1403249583222 40.18962386905537, -105.1402460544696 40.18972107600812, -105.140055118217 40.18988491630473, -105.1398931114001 40.18999311953126, -105.1397161515111 40.19008590298159, -105.1392741398997 40.19027805712356, -105.1390571245268 40.1903641264425, -105.1388418881127 40.19045212286864, -105.1386390933875 40.19055607922262, -105.1384888809863 40.19066706248092, -105.1383409875964 40.19081291641721, -105.1382800092054 40.19090386463147, -105.1382269980436 40.19104507341488, -105.1381931303606 40.19122093099875, -105.1381899159193 40.19135406015155, -105.1382100112756 40.19188311242785, -105.1393233110076 40.19185722614801, -105.1395731959861 40.1916054697542, -105.1405211966407 40.19155347041578, -105.1409040306353 40.19154572658073))</t>
+          <t>POLYGON ((-105.14090403063526 40.19154572658073, -105.14098903186539 40.19152972594931, -105.14112264465186 40.19153998197216, -105.14174119754756 40.191526469547355, -105.14221915420819 40.19159290600409, -105.14301282274063 40.19170322191939, -105.1435901972262 40.191783470032114, -105.14468519816758 40.19186346973615, -105.1454650795996 40.19166871898251, -105.145540002091 40.19156738941043, -105.145556198577 40.191102468798725, -105.14589502007333 40.19099873057759, -105.14602303916301 40.19095953422137, -105.1469560824025 40.19063072326936, -105.14752908588154 40.19047172415833, -105.14798008906776 40.19036772283105, -105.14842409295046 40.19029072383959, -105.14868209542068 40.19027472289796, -105.1489900989153 40.190263722204605, -105.14931910201645 40.19026372260259, -105.14964810679093 40.190280721566836, -105.1498131075271 40.19030272138396, -105.15040011448097 40.19034672131698, -105.15105212252408 40.190398720261186, -105.151725130212 40.19045971848809, -105.15203013299082 40.190480717349, -105.15203919957975 40.1904813219414, -105.15203919957837 40.1904544685933, -105.1522062000076 40.190440469005694, -105.15232620062943 40.19040146942321, -105.15262820011681 40.19021446851695, -105.1527832001366 40.1899674691564, -105.15461720090497 40.18989046922776, -105.15554319977937 40.19021346870296, -105.15553119994598 40.18866546838077, -105.15553088530844 40.18865548209631, -105.15483813733722 40.188650725953345, -105.15483699936152 40.18865397295026, -105.15471391389042 40.18865312900746, -105.1545576450007 40.188652528038915, -105.15311789093317 40.188646979194836, -105.15211893606003 40.188636017175895, -105.1514639163036 40.188634044523276, -105.15146184665912 40.188130029873946, -105.15147291681242 40.187296911985854, -105.15146293167382 40.18715001697894, -105.15144186132042 40.187070892931196, -105.15137714828711 40.18691697006431, -105.15128411452908 40.18677202034032, -105.15125492759519 40.18674008851822, -105.15105616747283 40.186551995307035, -105.1508920796487 40.18644306698239, -105.15075497353604 40.186377044274266, -105.15070498151384 40.18635410806133, -105.15054707589354 40.18629598298839, -105.15037905608492 40.18625594521194, -105.15020700592852 40.18623401219416, -105.14976743577402 40.18623386221527, -105.14942208617396 40.1862310863429, -105.1492338322608 40.18622804402173, -105.14847611058669 40.18622601744052, -105.14812717320221 40.186218093165174, -105.14798405909232 40.18620695166086, -105.14770295067086 40.18616409427499, -105.14756898223924 40.18611509756006, -105.14737793894153 40.1860288663483, -105.14654114690289 40.18553904801176, -105.14635412663502 40.18543690593991, -105.14557591364118 40.184973063831215, -105.14476383463905 40.184484955492955, -105.1445681553766 40.18467102363869, -105.1439618997615 40.185275012000076, -105.14380991695432 40.18538599674668, -105.14363299453328 40.185474943303284, -105.14346085623893 40.18553892338728, -105.14332290838526 40.185567047180996, -105.143180039099 40.18557813629327, -105.14279917221542 40.185584920956565, -105.14217784201082 40.185579979849294, -105.14118385015217 40.185587056670585, -105.14054994070476 40.18559195046055, -105.14057214098612 40.186335130226354, -105.14057412641525 40.187043109631695, -105.14057700530546 40.18778513128763, -105.14057984635642 40.18860209558213, -105.14054989950047 40.189121109372486, -105.14053408648128 40.18920094393643, -105.14046696265011 40.18937203172319, -105.14035308439134 40.18958497521279, -105.14032495832224 40.18962386905537, -105.14024605446957 40.18972107600812, -105.14005511821703 40.18988491630473, -105.1398931114001 40.18999311953126, -105.1397161515111 40.19008590298159, -105.13927413989974 40.19027805712356, -105.13905712452683 40.190364126442496, -105.13884188811272 40.19045212286864, -105.1386390933875 40.190556079222624, -105.13848888098627 40.19066706248092, -105.13834098759642 40.19081291641721, -105.13828000920537 40.19090386463147, -105.13822699804356 40.19104507341488, -105.13819313036059 40.191220930998746, -105.13818991591928 40.191354060151546, -105.13821001127562 40.191883112427846, -105.13932331100759 40.19185722614801, -105.13957319598613 40.1916054697542, -105.14052119664075 40.191553470415776, -105.14090403063526 40.19154572658073))</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -4894,7 +4918,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1470302534053 40.2032916430533, -105.1470359037472 40.20329266990918, -105.1470852547486 40.20330164222964, -105.1475372602013 40.20329864181809, -105.1480176142956 40.20329544312548, -105.1484382710454 40.20329264098557, -105.1491162779991 40.20329663915726, -105.1493042800662 40.20329663931438, -105.1494542823717 40.20329763897393, -105.149969901152 40.20329763904111, -105.149971287175 40.20329763873301, -105.1499712682566 40.20329697851118, -105.1499702876212 40.20326363768343, -105.1499682812303 40.20282264077071, -105.1499702753119 40.20243164381855, -105.1499662706908 40.20210364514212, -105.1499563688645 40.20041626554917, -105.1499562482724 40.20039565687276, -105.149964101196 40.20036601195144, -105.1499554011348 40.19980913608271, -105.1499982009238 40.19982447013613, -105.1499962832889 40.19959051377015, -105.1499949388271 40.19942660956755, -105.1499887946139 40.1987172693529, -105.1499829925106 40.19805283933351, -105.1499812003125 40.19784746942187, -105.1496263405455 40.19758894297775, -105.1489791994848 40.19711747053223, -105.1485730402104 40.19710161420416, -105.1483218563037 40.19709180819938, -105.1479411771563 40.19687668244443, -105.1476461753783 40.19693668305129, -105.1474821738625 40.19693668216285, -105.1473461715542 40.19692568232102, -105.1467441635402 40.19682668434852, -105.1461431546569 40.19669468522994, -105.1456841479397 40.19655668763392, -105.1452121412532 40.19636968980674, -105.1448041341312 40.19618269030496, -105.1443811252396 40.19591869385945, -105.1440091178666 40.1956336960499, -105.1438091135656 40.19546269709496, -105.1435081061389 40.19524369871329, -105.1434151044106 40.19515569999793, -105.1433361023987 40.19506770115726, -105.1433001014114 40.19499570050589, -105.1432721000626 40.19491870167863, -105.1432360974586 40.19477070269613, -105.1432220946501 40.19460570364041, -105.1431720931412 40.1944467052078, -105.1431220907786 40.19435370620326, -105.1430720899324 40.1942987058851, -105.1429930883901 40.19419970643524, -105.142943085833 40.19412270623425, -105.1428930830832 40.1940017072699, -105.142879089666 40.19388676729531, -105.1428790829269 40.19388670873322, -105.1429070803512 40.19380370978143, -105.1429570807157 40.19370571023295, -105.1430142317597 40.19356972952564, -105.1430150797219 40.19356771111762, -105.1430341800693 40.19346310723986, -105.1430131974055 40.19345646962464, -105.1420492687273 40.19332518604399, -105.1404581968998 40.19310846976347, -105.1396701978683 40.19287647006031, -105.1390461965723 40.19282347040903, -105.1388341967081 40.19234946940898, -105.1393233110076 40.19185722614801, -105.1382100112756 40.19188311242785, -105.1382130616972 40.19211700809573, -105.1382309133731 40.19246212904983, -105.1382230760014 40.19292603371227, -105.1382048744235 40.19298307526579, -105.1381209562706 40.19321395361075, -105.1380299823671 40.19334054861462, -105.1379855382644 40.19340239572814, -105.1378172716755 40.1937425963769, -105.1376931509601 40.19402737308724, -105.1375923408581 40.19430395938474, -105.1375355616143 40.19454672605157, -105.1375454390307 40.19470839136561, -105.1376100574661 40.19484187083497, -105.1378230709578 40.19510689543214, -105.1378531631223 40.19517012782561, -105.1378798473228 40.19526793844083, -105.1378820027869 40.19540108431987, -105.1378440929554 40.19552888914305, -105.1377931598583 40.19561492762381, -105.1376941713428 40.19571701074948, -105.1375698904066 40.19579595645354, -105.1374988457707 40.1958270281356, -105.1376181400221 40.19594489442792, -105.1377001136391 40.19607993766859, -105.1377206639153 40.1961466265489, -105.1377468677383 40.19624094931515, -105.13776701842 40.19642301551437, -105.1377710924904 40.19659899168622, -105.1378071124828 40.19682612762801, -105.1378789597274 40.19704788547751, -105.137936072563 40.19714606602628, -105.1380739869633 40.19733097124663, -105.1382420525373 40.19750087237632, -105.1394453893641 40.19842256765077, -105.1399121318047 40.19877186966814, -105.1400399284933 40.19884089591208, -105.1400455342284 40.19884360355745, -105.140226296475 40.1989407564562, -105.1404911599142 40.19901387053109, -105.1403763267011 40.19919447351365, -105.1403371709287 40.19936202470887, -105.1403519357383 40.199413130313, -105.1403870897853 40.19960292861641, -105.1403905422183 40.19999525761074, -105.140396928093 40.20072105474402, -105.140392213476 40.20239822849558, -105.1404739759176 40.20239912306182, -105.1405330393615 40.20240095392563, -105.1405577962932 40.20240111553534, -105.1405584412157 40.20247175608726, -105.1405587440789 40.20248623202258, -105.1405708942545 40.2031272043286, -105.1405727578465 40.20321128612159, -105.1405783310746 40.20327465404951, -105.1406181803717 40.20327465360264, -105.1414041879966 40.20328165160092, -105.1450462311085 40.20328364593188, -105.1470302534053 40.2032916430533))</t>
+          <t>POLYGON ((-105.14703025340529 40.2032916430533, -105.14703590374715 40.20329266990918, -105.14708525474862 40.20330164222964, -105.14753726020133 40.203298641818094, -105.14801761429563 40.203295443125484, -105.14843827104538 40.20329264098557, -105.14911627799906 40.20329663915726, -105.14930428006622 40.20329663931438, -105.14945428237165 40.20329763897393, -105.14996990115196 40.20329763904111, -105.14997128717502 40.20329763873301, -105.14997126825659 40.203296978511176, -105.14997028762116 40.203263637683435, -105.14996828123034 40.202822640770705, -105.14997027531189 40.20243164381855, -105.14996627069075 40.202103645142124, -105.14995636886445 40.200416265549165, -105.14995624827245 40.20039565687276, -105.149964101196 40.20036601195144, -105.1499554011348 40.199809136082706, -105.14999820092376 40.19982447013613, -105.14999628328891 40.19959051377015, -105.14999493882712 40.199426609567546, -105.14998879461386 40.1987172693529, -105.14998299251059 40.198052839333506, -105.1499812003125 40.19784746942187, -105.14962634054551 40.19758894297775, -105.14897919948483 40.19711747053223, -105.1485730402104 40.19710161420416, -105.14832185630365 40.19709180819938, -105.1479411771563 40.196876682444426, -105.14764617537826 40.19693668305129, -105.14748217386251 40.19693668216285, -105.14734617155419 40.19692568232102, -105.14674416354019 40.19682668434852, -105.14614315465687 40.19669468522994, -105.14568414793975 40.196556687633915, -105.14521214125323 40.19636968980674, -105.14480413413118 40.19618269030496, -105.14438112523962 40.19591869385945, -105.14400911786664 40.1956336960499, -105.14380911356557 40.19546269709496, -105.14350810613891 40.19524369871329, -105.14341510441056 40.195155699997926, -105.14333610239869 40.195067701157264, -105.14330010141141 40.19499570050589, -105.14327210006265 40.19491870167863, -105.14323609745858 40.194770702696125, -105.14322209465014 40.194605703640406, -105.14317209314122 40.194446705207795, -105.14312209077858 40.19435370620326, -105.1430720899324 40.194298705885096, -105.14299308839014 40.19419970643524, -105.14294308583304 40.194122706234246, -105.14289308308324 40.194001707269905, -105.14287908966598 40.19388676729531, -105.14287908292691 40.193886708733224, -105.1429070803512 40.19380370978143, -105.14295708071572 40.19370571023295, -105.14301423175972 40.19356972952564, -105.14301507972189 40.193567711117616, -105.14303418006925 40.19346310723986, -105.14301319740552 40.193456469624635, -105.1420492687273 40.19332518604399, -105.14045819689983 40.19310846976347, -105.13967019786826 40.19287647006031, -105.13904619657231 40.19282347040903, -105.1388341967081 40.19234946940898, -105.13932331100759 40.19185722614801, -105.13821001127562 40.191883112427846, -105.1382130616972 40.19211700809573, -105.13823091337305 40.19246212904983, -105.1382230760014 40.19292603371227, -105.13820487442351 40.192983075265786, -105.13812095627064 40.19321395361075, -105.13802998236713 40.19334054861462, -105.13798553826442 40.193402395728135, -105.13781727167549 40.1937425963769, -105.13769315096015 40.194027373087245, -105.13759234085808 40.19430395938474, -105.13753556161427 40.19454672605157, -105.13754543903072 40.19470839136561, -105.13761005746609 40.19484187083497, -105.13782307095784 40.19510689543214, -105.13785316312227 40.19517012782561, -105.13787984732282 40.19526793844083, -105.13788200278685 40.19540108431987, -105.13784409295539 40.19552888914305, -105.13779315985835 40.19561492762381, -105.13769417134282 40.195717010749476, -105.1375698904066 40.19579595645354, -105.13749884577068 40.1958270281356, -105.13761814002214 40.19594489442792, -105.13770011363913 40.19607993766859, -105.13772066391535 40.1961466265489, -105.1377468677383 40.19624094931515, -105.13776701842005 40.19642301551437, -105.1377710924904 40.19659899168622, -105.13780711248285 40.196826127628015, -105.13787895972736 40.19704788547751, -105.13793607256297 40.197146066026285, -105.13807398696332 40.19733097124663, -105.13824205253725 40.197500872376324, -105.13944538936408 40.19842256765077, -105.1399121318047 40.198771869668136, -105.14003992849331 40.198840895912085, -105.14004553422843 40.19884360355745, -105.14022629647499 40.198940756456196, -105.1404911599142 40.19901387053109, -105.1403763267011 40.19919447351365, -105.14033717092867 40.19936202470887, -105.14035193573827 40.199413130313, -105.14038708978526 40.199602928616414, -105.14039054221831 40.199995257610745, -105.140396928093 40.200721054744015, -105.14039221347596 40.20239822849558, -105.1404739759176 40.20239912306182, -105.14053303936153 40.202400953925626, -105.14055779629315 40.20240111553534, -105.14055844121573 40.20247175608726, -105.14055874407893 40.20248623202258, -105.14057089425447 40.203127204328595, -105.14057275784646 40.203211286121594, -105.14057833107458 40.20327465404951, -105.14061818037173 40.20327465360264, -105.14140418799663 40.203281651600925, -105.14504623110852 40.203283645931876, -105.14703025340529 40.2032916430533))</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
@@ -4936,7 +4960,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1309118755788 40.1961229807733, -105.1310861199447 40.20325177510741, -105.131103999586 40.2032519987591, -105.1311050050803 40.20325199115882, -105.1311050689144 40.20324866892156, -105.1338881012024 40.20322866366779, -105.1341401040008 40.20322766440542, -105.1354471192618 40.20324566162454, -105.1356161214376 40.2032486610788, -105.1370411375896 40.20324765828751, -105.1393501657596 40.20326465486743, -105.1404671774334 40.20327365378093, -105.1405431778102 40.20327465376817, -105.1405783310746 40.20327465404951, -105.1405727578465 40.20321128612159, -105.1405708942545 40.2031272043286, -105.1405587440789 40.20248623202258, -105.1405584412157 40.20247175608726, -105.1405577962932 40.20240111553534, -105.1405330393615 40.20240095392563, -105.1404739759176 40.20239912306182, -105.140392213476 40.20239822849558, -105.140396928093 40.20072105474402, -105.1403905422183 40.19999525761074, -105.1403870897853 40.19960292861641, -105.1403519357383 40.199413130313, -105.1403371709287 40.19936202470887, -105.1403763267011 40.19919447351365, -105.1404911599142 40.19901387053109, -105.140226296475 40.1989407564562, -105.1400455342284 40.19884360355745, -105.1400399284933 40.19884089591208, -105.1399121318047 40.19877186966814, -105.1394453893641 40.19842256765077, -105.1382420525373 40.19750087237632, -105.1380739869633 40.19733097124663, -105.137936072563 40.19714606602628, -105.1378789597274 40.19704788547751, -105.1378071124828 40.19682612762801, -105.1377710924904 40.19659899168622, -105.13776701842 40.19642301551437, -105.1377468677383 40.19624094931515, -105.1377206639153 40.1961466265489, -105.1377001136391 40.19607993766859, -105.1376181400221 40.19594489442792, -105.1374988457707 40.1958270281356, -105.1373920121044 40.1957221032935, -105.137260019817 40.19563604069402, -105.1370768360099 40.19555009198046, -105.1368781329192 40.19548797729049, -105.1366678295033 40.19545300248294, -105.1364520129437 40.19544491193961, -105.136236034898 40.19546701789125, -105.13602885285 40.19551797416268, -105.1358369116012 40.19559697881763, -105.1355888803089 40.19572192524484, -105.1354079776137 40.19581194452213, -105.1352240019548 40.19587395396812, -105.1350301269854 40.19591287200842, -105.1348288727205 40.19592596231499, -105.1332540925827 40.19593195905006, -105.1324450826828 40.1959280178147, -105.1323279809317 40.19593588095032, -105.131612962076 40.19609309792698, -105.131428863541 40.19611090406575, -105.1309118755788 40.1961229807733))</t>
+          <t>POLYGON ((-105.13091187557878 40.196122980773296, -105.13108611994468 40.20325177510741, -105.13110399958599 40.2032519987591, -105.13110500508029 40.203251991158815, -105.13110506891444 40.20324866892156, -105.13388810120243 40.20322866366779, -105.13414010400083 40.20322766440542, -105.13544711926178 40.203245661624536, -105.13561612143764 40.203248661078796, -105.13704113758965 40.20324765828751, -105.13935016575962 40.203264654867425, -105.1404671774334 40.20327365378093, -105.14054317781024 40.20327465376817, -105.14057833107458 40.20327465404951, -105.14057275784646 40.203211286121594, -105.14057089425447 40.203127204328595, -105.14055874407893 40.20248623202258, -105.14055844121573 40.20247175608726, -105.14055779629315 40.20240111553534, -105.14053303936153 40.202400953925626, -105.1404739759176 40.20239912306182, -105.14039221347596 40.20239822849558, -105.140396928093 40.200721054744015, -105.14039054221831 40.199995257610745, -105.14038708978526 40.199602928616414, -105.14035193573827 40.199413130313, -105.14033717092867 40.19936202470887, -105.1403763267011 40.19919447351365, -105.1404911599142 40.19901387053109, -105.14022629647499 40.198940756456196, -105.14004553422843 40.19884360355745, -105.14003992849331 40.198840895912085, -105.1399121318047 40.198771869668136, -105.13944538936408 40.19842256765077, -105.13824205253725 40.197500872376324, -105.13807398696332 40.19733097124663, -105.13793607256297 40.197146066026285, -105.13787895972736 40.19704788547751, -105.13780711248285 40.196826127628015, -105.1377710924904 40.19659899168622, -105.13776701842005 40.19642301551437, -105.1377468677383 40.19624094931515, -105.13772066391535 40.1961466265489, -105.13770011363913 40.19607993766859, -105.13761814002214 40.19594489442792, -105.13749884577068 40.1958270281356, -105.1373920121044 40.1957221032935, -105.13726001981696 40.19563604069402, -105.13707683600988 40.195550091980465, -105.13687813291924 40.19548797729049, -105.13666782950332 40.195453002482935, -105.13645201294366 40.19544491193961, -105.13623603489803 40.195467017891254, -105.13602885285 40.19551797416268, -105.13583691160122 40.19559697881763, -105.13558888030886 40.19572192524484, -105.13540797761367 40.195811944522134, -105.13522400195484 40.195873953968125, -105.1350301269854 40.19591287200842, -105.13482887272048 40.19592596231499, -105.13325409258266 40.19593195905006, -105.13244508268276 40.1959280178147, -105.13232798093173 40.195935880950316, -105.13161296207605 40.196093097926976, -105.13142886354099 40.19611090406575, -105.13091187557878 40.196122980773296))</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
@@ -4978,7 +5002,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1298610279341 40.20685338449566, -105.1308211106729 40.20685958736579, -105.13106209839 40.20686114262469, -105.1310621395053 40.20684793765957, -105.1311011281608 40.2068508539929, -105.1311061048515 40.20615965121866, -105.1311220944714 40.20525265550346, -105.1311260827941 40.20434866191943, -105.1311000733982 40.20350866707759, -105.1311050050803 40.20325199115882, -105.131103999586 40.2032519987591, -105.1310861199447 40.20325177510741, -105.1309118755788 40.1961229807733, -105.1308460028724 40.19612386837532, -105.1306419632079 40.19612211894584, -105.1301501480823 40.19611313473412, -105.1293050405962 40.19609807552655, -105.1284459067967 40.19609504349872, -105.1275960252971 40.19610191756082, -105.1267601314409 40.19610388963849, -105.1261540832188 40.19610193189156, -105.125718068953 40.19610107083675, -105.1257549140013 40.19753689975536, -105.125740947971 40.19786297739789, -105.125656148779 40.1982451010535, -105.1255230373638 40.19875389386889, -105.1253470801112 40.19917689997085, -105.1250798843046 40.19984996591862, -105.1249548453065 40.20025693941326, -105.1248879077508 40.20051504070054, -105.1248510188365 40.20077708153192, -105.1248318678293 40.20262587183821, -105.1248368677285 40.20320367234526, -105.1248379976579 40.20320367781203, -105.1263099548083 40.20320830748921, -105.1263099741148 40.20321163359582, -105.1263100144433 40.20321840109568, -105.1263311955124 40.20321847223759, -105.1263311477963 40.20324703121165, -105.1263311072719 40.20327150312825, -105.1263310707939 40.20329352893387, -105.1263310249341 40.20332110892354, -105.1263309880781 40.20334363097754, -105.1263307346595 40.20349575096746, -105.1263306224686 40.20356382598065, -105.1263302855891 40.2037661830984, -105.1263299823805 40.20394852101129, -105.1263296824622 40.20412961875567, -105.1263293100186 40.20435383414205, -105.1263288168892 40.20465044754024, -105.1263273198157 40.20555140862761, -105.126325383258 40.20671719607243, -105.1263252134739 40.20681968499972, -105.1263251952959 40.20683047273798, -105.1267617702789 40.20683330818028, -105.1298610279341 40.20685338449566))</t>
+          <t>POLYGON ((-105.12986102793406 40.20685338449566, -105.13082111067293 40.20685958736579, -105.13106209839 40.20686114262469, -105.13106213950535 40.206847937659575, -105.13110112816078 40.206850853992904, -105.13110610485151 40.206159651218655, -105.13112209447138 40.205252655503465, -105.13112608279408 40.20434866191943, -105.13110007339816 40.20350866707759, -105.13110500508029 40.203251991158815, -105.13110399958599 40.2032519987591, -105.13108611994468 40.20325177510741, -105.13091187557878 40.196122980773296, -105.13084600287245 40.196123868375324, -105.13064196320786 40.19612211894584, -105.13015014808231 40.19611313473412, -105.12930504059624 40.19609807552655, -105.12844590679666 40.19609504349872, -105.12759602529707 40.196101917560824, -105.12676013144088 40.196103889638486, -105.12615408321882 40.19610193189156, -105.12571806895298 40.19610107083675, -105.12575491400126 40.197536899755356, -105.125740947971 40.19786297739789, -105.125656148779 40.1982451010535, -105.12552303736383 40.19875389386889, -105.12534708011115 40.19917689997085, -105.12507988430461 40.199849965918624, -105.12495484530648 40.20025693941326, -105.12488790775082 40.200515040700544, -105.12485101883645 40.200777081531925, -105.12483186782929 40.20262587183821, -105.12483686772846 40.20320367234526, -105.12483799765788 40.20320367781203, -105.12630995480828 40.203208307489206, -105.12630997411478 40.20321163359582, -105.1263100144433 40.20321840109568, -105.12633119551245 40.20321847223759, -105.1263311477963 40.203247031211646, -105.12633110727187 40.20327150312825, -105.12633107079388 40.20329352893387, -105.12633102493409 40.20332110892354, -105.12633098807805 40.203343630977535, -105.12633073465946 40.20349575096746, -105.12633062246864 40.20356382598065, -105.12633028558909 40.2037661830984, -105.12632998238045 40.20394852101129, -105.12632968246217 40.204129618755665, -105.12632931001856 40.20435383414205, -105.12632881688923 40.20465044754024, -105.1263273198157 40.20555140862761, -105.12632538325799 40.206717196072425, -105.12632521347393 40.20681968499972, -105.12632519529588 40.206830472737984, -105.12676177027889 40.20683330818028, -105.12986102793406 40.20685338449566))</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
@@ -5020,7 +5044,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1155968517825 40.20318341103974, -105.1155957253303 40.2034586936532, -105.1155087349688 40.21041195368512, -105.1159557476378 40.21041252829438, -105.1159566603877 40.21041252952389, -105.1213741436619 40.21041936286073, -105.1214718525096 40.20679480657027, -105.1215591626463 40.20345390870822, -105.1215602059391 40.20318796272678, -105.1220259643586 40.20319068285817, -105.1225519696027 40.20318968180091, -105.1239909869865 40.20319968052207, -105.1248368677285 40.20320367234526, -105.1248318678293 40.20262587183821, -105.1248510188365 40.20077708153192, -105.1248879077508 40.20051504070054, -105.1249548453065 40.20025693941326, -105.1250798843046 40.19984996591862, -105.1253470801112 40.19917689997085, -105.1255230373638 40.19875389386889, -105.125656148779 40.1982451010535, -105.125740947971 40.19786297739789, -105.1257549140013 40.19753689975536, -105.125718068953 40.19610107083675, -105.1247440565115 40.19609187444581, -105.1245997948084 40.1960523429243, -105.1237576535158 40.19596722385328, -105.1229019987192 40.19589880009727, -105.1219490189156 40.19582231088875, -105.1213803209356 40.19577337127161, -105.1210021402629 40.19576288105466, -105.1207269104129 40.19575292005293, -105.1199198436 40.1957219946514, -105.1193890683886 40.19570295481263, -105.1184608325745 40.19570291563901, -105.1166738359791 40.19569810347589, -105.1166689912511 40.19585895275579, -105.1166649124307 40.19601102066565, -105.1166778948944 40.19662899557532, -105.1166999925712 40.1977260282077, -105.1167098646986 40.19838791484564, -105.116728009481 40.19955109206061, -105.1167509256992 40.20024898411357, -105.1167838592617 40.20126589365006, -105.1167719154655 40.20179703893213, -105.1167849682243 40.20253003542514, -105.1168181523576 40.2031851359515, -105.1165226114093 40.20318244513436, -105.1158670888695 40.20318373616588, -105.1155968517825 40.20318341103974))</t>
+          <t>POLYGON ((-105.11559685178248 40.20318341103974, -105.11559572533034 40.2034586936532, -105.11550873496881 40.210411953685124, -105.11595574763777 40.21041252829438, -105.11595666038768 40.210412529523886, -105.12137414366192 40.21041936286073, -105.12147185250961 40.20679480657027, -105.12155916264626 40.20345390870822, -105.12156020593909 40.20318796272678, -105.1220259643586 40.20319068285817, -105.12255196960265 40.20318968180091, -105.12399098698651 40.20319968052207, -105.12483686772846 40.20320367234526, -105.12483186782929 40.20262587183821, -105.12485101883645 40.200777081531925, -105.12488790775082 40.200515040700544, -105.12495484530648 40.20025693941326, -105.12507988430461 40.199849965918624, -105.12534708011115 40.19917689997085, -105.12552303736383 40.19875389386889, -105.125656148779 40.1982451010535, -105.125740947971 40.19786297739789, -105.12575491400126 40.197536899755356, -105.12571806895298 40.19610107083675, -105.12474405651152 40.196091874445806, -105.12459979480842 40.1960523429243, -105.12375765351578 40.19596722385328, -105.1229019987192 40.19589880009727, -105.1219490189156 40.19582231088875, -105.12138032093561 40.19577337127161, -105.12100214026289 40.19576288105466, -105.12072691041293 40.195752920052925, -105.11991984359999 40.1957219946514, -105.11938906838859 40.19570295481263, -105.11846083257448 40.19570291563901, -105.11667383597906 40.19569810347589, -105.11666899125107 40.19585895275579, -105.11666491243066 40.19601102066565, -105.11667789489442 40.19662899557532, -105.1166999925712 40.197726028207704, -105.11670986469858 40.19838791484564, -105.11672800948101 40.19955109206061, -105.11675092569922 40.20024898411357, -105.11678385926169 40.20126589365006, -105.11677191546553 40.201797038932135, -105.11678496822432 40.20253003542514, -105.11681815235761 40.2031851359515, -105.11652261140927 40.20318244513436, -105.11586708886955 40.20318373616588, -105.11559685178248 40.20318341103974))</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
@@ -5062,7 +5086,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.102421336487 40.20328529873123, -105.1024213646419 40.20328751439211, -105.1024214449243 40.20329367141449, -105.1025008330252 40.20329617878833, -105.1026765488442 40.20329664572056, -105.1030852803135 40.20329706845792, -105.1043405998986 40.20329835559978, -105.105123135279 40.20329915147183, -105.1052308076059 40.2032992596835, -105.1053409606589 40.20329937175753, -105.1053837709425 40.20329941517127, -105.1054421903556 40.20329947399756, -105.1064851728413 40.20325111772296, -105.1073079789816 40.20321240066425, -105.1077521907158 40.20319147334009, -105.1091350909051 40.20319674093735, -105.1098898104245 40.20319715386316, -105.1108060990517 40.2031948859403, -105.111056502299 40.20319290306869, -105.1125030266368 40.20318604347585, -105.1134346468925 40.20318708080785, -105.1151857766577 40.20318901124353, -105.1155357402171 40.20318939435722, -105.1155968269777 40.20318946052415, -105.1155968517825 40.20318341103974, -105.1158670888695 40.20318373616588, -105.1165226114093 40.20318244513436, -105.1168181523576 40.2031851359515, -105.1167849682243 40.20253003542514, -105.1167719154655 40.20179703893213, -105.1167838592617 40.20126589365006, -105.1167509256992 40.20024898411357, -105.116728009481 40.19955109206061, -105.1167098646986 40.19838791484564, -105.1166999925712 40.1977260282077, -105.1166778948944 40.19662899557532, -105.1166649124307 40.19601102066565, -105.1166689912511 40.19585895275579, -105.1166738359791 40.19569810347589, -105.1166729592587 40.19528193635994, -105.1166778838765 40.19459896050941, -105.1166770285451 40.19392502492807, -105.1166809681976 40.19322612331362, -105.1147551471709 40.19322109568412, -105.1139461768446 40.19321592716982, -105.1132889302573 40.19322004532617, -105.1122980561094 40.19322496265376, -105.111723928605 40.1932291578423, -105.1102461680016 40.1932309662153, -105.1096989545908 40.19321100232427, -105.1095688341273 40.19319899075646, -105.1093841120682 40.19318193926935, -105.1090740328479 40.1931339492639, -105.1087690678741 40.19306813230949, -105.1084081410572 40.19296094791824, -105.1081381084471 40.19285901135972, -105.1080720417897 40.19283188541718, -105.1077561498077 40.19267488967569, -105.1071770321067 40.19235393786226, -105.1069888555251 40.1922728652199, -105.1068051588693 40.19222200496674, -105.1065980674279 40.19219302506354, -105.1059229963339 40.19218606010607, -105.1048453489194 40.19218432049806, -105.1023480324539 40.19219001707661, -105.1023401095519 40.19238187512373, -105.1023501276933 40.19385193690373, -105.1023748592168 40.19451991641212, -105.1023850650994 40.1948559566662, -105.1023868541003 40.19503988820251, -105.1023809230087 40.19574811518007, -105.1023788304601 40.19586093436818, -105.1024139175533 40.19696213301737, -105.1024319782109 40.19815907813807, -105.1024859020631 40.19952909100861, -105.1024847271985 40.20065462381238, -105.1024006556609 40.20088934679336, -105.1024054437498 40.2013562575215, -105.102421336487 40.20328529873123))</t>
+          <t>POLYGON ((-105.102421336487 40.20328529873123, -105.10242136464194 40.20328751439211, -105.10242144492427 40.20329367141449, -105.10250083302522 40.20329617878833, -105.10267654884422 40.20329664572056, -105.10308528031346 40.20329706845792, -105.10434059989859 40.203298355599784, -105.10512313527902 40.20329915147183, -105.10523080760592 40.2032992596835, -105.10534096065894 40.20329937175753, -105.10538377094248 40.203299415171266, -105.10544219035563 40.20329947399756, -105.10648517284133 40.20325111772296, -105.10730797898162 40.20321240066425, -105.1077521907158 40.20319147334009, -105.10913509090508 40.20319674093735, -105.10988981042452 40.20319715386316, -105.1108060990517 40.2031948859403, -105.11105650229896 40.20319290306869, -105.11250302663682 40.203186043475846, -105.11343464689254 40.20318708080785, -105.11518577665774 40.20318901124353, -105.11553574021708 40.203189394357224, -105.11559682697765 40.20318946052415, -105.11559685178248 40.20318341103974, -105.11586708886955 40.20318373616588, -105.11652261140927 40.20318244513436, -105.11681815235761 40.2031851359515, -105.11678496822432 40.20253003542514, -105.11677191546553 40.201797038932135, -105.11678385926169 40.20126589365006, -105.11675092569922 40.20024898411357, -105.11672800948101 40.19955109206061, -105.11670986469858 40.19838791484564, -105.1166999925712 40.197726028207704, -105.11667789489442 40.19662899557532, -105.11666491243066 40.19601102066565, -105.11666899125107 40.19585895275579, -105.11667383597906 40.19569810347589, -105.11667295925871 40.19528193635994, -105.11667788387655 40.19459896050941, -105.11667702854506 40.19392502492807, -105.1166809681976 40.19322612331362, -105.11475514717092 40.193221095684116, -105.11394617684462 40.19321592716982, -105.11328893025734 40.19322004532617, -105.11229805610941 40.19322496265376, -105.11172392860504 40.1932291578423, -105.11024616800164 40.1932309662153, -105.10969895459078 40.19321100232427, -105.10956883412727 40.193198990756464, -105.10938411206821 40.19318193926935, -105.10907403284793 40.1931339492639, -105.10876906787412 40.19306813230949, -105.10840814105715 40.192960947918245, -105.10813810844714 40.192859011359715, -105.10807204178971 40.19283188541718, -105.10775614980767 40.192674889675686, -105.10717703210675 40.192353937862265, -105.10698885552506 40.1922728652199, -105.1068051588693 40.19222200496674, -105.10659806742791 40.19219302506354, -105.10592299633394 40.19218606010607, -105.10484534891944 40.192184320498065, -105.10234803245389 40.19219001707661, -105.10234010955186 40.19238187512373, -105.10235012769333 40.193851936903734, -105.10237485921675 40.19451991641212, -105.10238506509936 40.1948559566662, -105.10238685410033 40.19503988820251, -105.10238092300867 40.195748115180066, -105.10237883046007 40.19586093436818, -105.10241391755333 40.196962133017365, -105.10243197821094 40.19815907813807, -105.10248590206305 40.199529091008614, -105.10248472719852 40.20065462381238, -105.10240065566093 40.20088934679336, -105.10240544374977 40.201356257521496, -105.102421336487 40.20328529873123))</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
@@ -5104,7 +5128,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0930820960962 40.20317412349315, -105.0932201875574 40.20317547481145, -105.0932147345931 40.20427675894129, -105.0932105779957 40.2051159902964, -105.0932041876712 40.206406475457, -105.0932022136999 40.20678056108493, -105.0932545485407 40.20678031284936, -105.0954331146536 40.20678761374383, -105.0971599989639 40.20679337055231, -105.0971607119664 40.20679337303581, -105.0976247948587 40.20679491652393, -105.0976247893968 40.20679703029651, -105.0977981545344 40.20679786929404, -105.0978192638643 40.20995469549757, -105.0978192865362 40.20995801171471, -105.0978221643321 40.21038836945402, -105.1020764826853 40.210400971623, -105.1024751480868 40.2103992398415, -105.1024778062865 40.2099546758207, -105.102494799139 40.20914168066236, -105.102465788828 40.20820268604596, -105.1025047847938 40.20772268878633, -105.1025137811899 40.20727069089985, -105.1025437709455 40.20634669622018, -105.1025237636843 40.20571670054039, -105.1025237619839 40.20539370203086, -105.1025107003073 40.20422330641446, -105.1018961897053 40.20421247454206, -105.1018971891388 40.2032814736801, -105.1024151901731 40.20329347428748, -105.1024214449243 40.20329367141449, -105.1024213646525 40.20328751259089, -105.102421336487 40.20328529873123, -105.1024054437498 40.2013562575215, -105.1024006556609 40.20088934679336, -105.1024847271985 40.20065462381238, -105.1024859020631 40.19952909100861, -105.1024319782109 40.19815907813807, -105.1024139175533 40.19696213301737, -105.1023788304601 40.19586093436818, -105.1022979448688 40.19585791106639, -105.1022181387225 40.19585406733855, -105.1015878906684 40.19582801449134, -105.1006950211054 40.19584003390204, -105.0999060366127 40.19584005096787, -105.0976751063603 40.19584109619835, -105.096581827718 40.19584305219868, -105.0955698757631 40.19583402616591, -105.0949888953552 40.19583089576602, -105.0944211395721 40.19583110066097, -105.0942998324741 40.19582298908553, -105.0937480333861 40.19578893417904, -105.0933991408409 40.1957660205662, -105.0930949795306 40.19574600935555, -105.09306383352 40.19574606186691, -105.0930717738308 40.20016075298534, -105.0930821032523 40.20316429217297, -105.0930821150281 40.20316762366792, -105.0930820960962 40.20317412349315))</t>
+          <t>POLYGON ((-105.09308209609623 40.20317412349315, -105.0932201875574 40.203175474811445, -105.09321473459312 40.20427675894129, -105.09321057799566 40.2051159902964, -105.09320418767116 40.206406475457, -105.09320221369985 40.20678056108493, -105.09325454854073 40.20678031284936, -105.09543311465357 40.206787613743835, -105.09715999896386 40.20679337055231, -105.09716071196644 40.206793373035815, -105.09762479485875 40.206794916523926, -105.09762478939679 40.20679703029651, -105.09779815453437 40.20679786929404, -105.09781926386432 40.20995469549757, -105.09781928653622 40.20995801171471, -105.09782216433213 40.21038836945402, -105.10207648268533 40.210400971622995, -105.10247514808682 40.2103992398415, -105.10247780628652 40.2099546758207, -105.10249479913901 40.209141680662356, -105.102465788828 40.208202686045965, -105.10250478479384 40.207722688786326, -105.10251378118986 40.207270690899854, -105.10254377094547 40.20634669622018, -105.1025237636843 40.205716700540385, -105.10252376198393 40.20539370203086, -105.1025107003073 40.204223306414455, -105.1018961897053 40.20421247454206, -105.10189718913881 40.2032814736801, -105.10241519017313 40.203293474287484, -105.10242144492427 40.20329367141449, -105.10242136465246 40.20328751259089, -105.102421336487 40.20328529873123, -105.10240544374977 40.201356257521496, -105.10240065566093 40.20088934679336, -105.10248472719852 40.20065462381238, -105.10248590206305 40.199529091008614, -105.10243197821094 40.19815907813807, -105.10241391755333 40.196962133017365, -105.10237883046007 40.19586093436818, -105.10229794486881 40.19585791106639, -105.10221813872249 40.19585406733855, -105.10158789066844 40.19582801449134, -105.10069502110537 40.195840033902044, -105.09990603661265 40.19584005096787, -105.09767510636028 40.19584109619835, -105.09658182771803 40.19584305219868, -105.09556987576313 40.19583402616591, -105.09498889535517 40.19583089576602, -105.09442113957206 40.195831100660975, -105.09429983247412 40.195822989085535, -105.09374803338606 40.19578893417904, -105.09339914084086 40.1957660205662, -105.09309497953063 40.195746009355545, -105.09306383351996 40.19574606186691, -105.09307177383076 40.20016075298534, -105.09308210325229 40.20316429217297, -105.0930821150281 40.20316762366792, -105.09308209609623 40.20317412349315))</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
@@ -5146,7 +5170,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.0741712712824 40.20329264686716, -105.0741712519851 40.20329479031248, -105.0741711838814 40.20330247609904, -105.0747471835121 40.20329593233741, -105.0765138064435 40.20327584437361, -105.0776037795553 40.20327547689448, -105.0779601843807 40.2032754757722, -105.0783671987761 40.20327647585538, -105.0787342713654 40.20327551513552, -105.0790784538952 40.20326612103604, -105.0798893828385 40.20325404710055, -105.0806879610338 40.20324837306046, -105.0816501847357 40.20324047561559, -105.0822069163204 40.20323024316917, -105.0830682814023 40.2032196909061, -105.0835791856489 40.20321847582563, -105.0835981069327 40.20321967515504, -105.0837211863008 40.203227474651, -105.0856447171413 40.20320449486757, -105.0877735888691 40.20318643920209, -105.088853254461 40.20317763139809, -105.0897408380691 40.20317038385568, -105.0904716416836 40.20316441081984, -105.0908696894077 40.20316115529705, -105.0912832223234 40.20316093513956, -105.0914944937617 40.2031624183343, -105.0917522278974 40.20316422728517, -105.0919455217571 40.20316558314721, -105.0921975370513 40.20316735111282, -105.0926146724067 40.20317027581347, -105.0928657727666 40.20317203549725, -105.09300572348 40.20317301534985, -105.093005727191 40.20317337651804, -105.0930820960962 40.20317412349315, -105.0930821150281 40.20316762366792, -105.0930717738308 40.20016075298534, -105.09306383352 40.19574606186691, -105.0924638566949 40.19574708041702, -105.0910999059538 40.1957559910603, -105.0902370981357 40.1957691329993, -105.0892681643353 40.19586891298781, -105.0881840468208 40.19587839019044, -105.0880582329032 40.19587916782289, -105.0874972275109 40.19588263658899, -105.0872988309592 40.19588386235068, -105.0870629523426 40.19587890254427, -105.0868898415345 40.19585412732779, -105.0867218461393 40.19581207519037, -105.086511852989 40.19573006805931, -105.0864171348487 40.19578640374956, -105.0860866501783 40.19578522125577, -105.0741934852469 40.19582692062273, -105.0741932934809 40.1959239402651, -105.0741931821864 40.1964505573902, -105.0741931823814 40.19692335905753, -105.0741931829567 40.19745124190834, -105.0741931830242 40.197637475825, -105.074198183371 40.19768747513977, -105.0741983171571 40.19794219855124, -105.0741986932105 40.19865770627052, -105.0741989123659 40.19907360358597, -105.074199127075 40.19948139601922, -105.0741975998984 40.19984661967961, -105.0741944486666 40.20036070732497, -105.0741918663698 40.20078168731853, -105.0741876627714 40.20144129690684, -105.0741819087761 40.20209113330615, -105.0741760932321 40.2027479664625, -105.0741735880171 40.20303094825258, -105.0741714903699 40.20326779279068, -105.0741712712824 40.20329264686716))</t>
+          <t>POLYGON ((-105.07417127128235 40.20329264686716, -105.07417125198513 40.203294790312476, -105.07417118388136 40.20330247609904, -105.0747471835121 40.20329593233741, -105.07651380644354 40.20327584437361, -105.07760377955532 40.20327547689448, -105.0779601843807 40.2032754757722, -105.0783671987761 40.20327647585538, -105.07873427136538 40.203275515135516, -105.07907845389524 40.20326612103604, -105.07988938283849 40.20325404710055, -105.0806879610338 40.20324837306046, -105.08165018473568 40.203240475615594, -105.08220691632043 40.20323024316917, -105.08306828140232 40.2032196909061, -105.0835791856489 40.20321847582563, -105.0835981069327 40.20321967515504, -105.08372118630079 40.203227474651, -105.08564471714132 40.20320449486757, -105.08777358886908 40.203186439202085, -105.08885325446103 40.20317763139809, -105.08974083806913 40.20317038385568, -105.09047164168356 40.20316441081984, -105.09086968940765 40.203161155297046, -105.09128322232336 40.203160935139564, -105.09149449376167 40.2031624183343, -105.09175222789742 40.20316422728517, -105.09194552175714 40.20316558314721, -105.09219753705133 40.20316735111282, -105.09261467240674 40.20317027581347, -105.09286577276664 40.20317203549725, -105.09300572347999 40.20317301534985, -105.09300572719101 40.203173376518045, -105.09308209609623 40.20317412349315, -105.0930821150281 40.20316762366792, -105.09307177383076 40.20016075298534, -105.09306383351996 40.19574606186691, -105.09246385669488 40.19574708041702, -105.09109990595384 40.1957559910603, -105.09023709813569 40.195769132999295, -105.08926816433527 40.195868912987805, -105.08818404682084 40.19587839019044, -105.08805823290322 40.19587916782289, -105.08749722751094 40.19588263658899, -105.08729883095923 40.195883862350684, -105.08706295234258 40.195878902544266, -105.08688984153449 40.19585412732779, -105.08672184613931 40.19581207519037, -105.08651185298896 40.195730068059305, -105.08641713484873 40.19578640374956, -105.0860866501783 40.19578522125577, -105.07419348524694 40.19582692062273, -105.07419329348087 40.1959239402651, -105.0741931821864 40.1964505573902, -105.07419318238142 40.19692335905753, -105.07419318295668 40.19745124190834, -105.07419318302424 40.197637475825005, -105.074198183371 40.19768747513977, -105.07419831715706 40.19794219855124, -105.07419869321048 40.198657706270524, -105.07419891236592 40.19907360358597, -105.07419912707498 40.19948139601922, -105.0741975998984 40.19984661967961, -105.07419444866659 40.20036070732497, -105.07419186636979 40.20078168731853, -105.07418766277144 40.20144129690684, -105.07418190877611 40.20209113330615, -105.07417609323211 40.202747966462496, -105.07417358801709 40.203030948252575, -105.07417149036995 40.203267792790676, -105.07417127128235 40.20329264686716))</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
@@ -5188,7 +5212,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t xml:space="preserve">POLYGON ((-105.1310573131 40.12712102857881, -105.1310483145869 40.12882902900039, -105.131019817435 40.13074388165322, -105.1310197778048 40.1307470797142, -105.1310098430939 40.13155699817882, -105.1310003956401 40.13199844572109, -105.130988858237 40.13253599608295, -105.1309879188726 40.13259022536034, -105.1309708325789 40.13358999631841, -105.1309568622919 40.13407299670184, -105.1309663158803 40.13407590265542, -105.1309672909742 40.13407590306819, -105.131264018241 40.13407590214059, -105.1351949880881 40.13406190558131, -105.1355969920545 40.13406290499365, -105.136218990986 40.13406390604963, -105.1383481339877 40.1340678960071, -105.1387142130814 40.13405542457127, -105.1387601569389 40.13397838399309, -105.1388641599894 40.13379438525001, -105.1394061770989 40.13283739637802, -105.1396172542842 40.13246945491051, -105.1399113154917 40.13199350715775, -105.1400313152862 40.13181050557099, -105.1402873438578 40.13141953294432, -105.1404134075242 40.13123259600766, -105.1404134914445 40.13123248008579, -105.1405674928146 40.13101869438201, -105.1409685953441 40.13051183984713, -105.1410715897065 40.13039683245281, -105.1412255205253 40.13022372772332, -105.1414536901801 40.12994403235987, -105.1416416731433 40.12976299450775, -105.1433827002903 40.12803805788978, -105.1443716376531 40.12710336772473, -105.1446938377278 40.12679883459163, -105.1447137065043 40.12678007314066, -105.1448846966432 40.12662004649052, -105.1451267445326 40.1263892194086, -105.1456327957312 40.12596286157071, -105.1456330410493 40.12597501111281, -105.1456423360221 40.12643537867292, -105.1456487281823 40.12675200170747, -105.1456168014993 40.12884799589443, -105.1456167644999 40.12885442637793, -105.1456271903526 40.12885446106298, -105.1457651912196 40.12883446131615, -105.1459941909125 40.12876946043333, -105.1462091902176 40.1287254615651, -105.1463811910671 40.1286814612758, -105.1465091905153 40.1286324608168, -105.1466521909948 40.12851646037345, -105.1467601907007 40.12837346040647, -105.1469681918037 40.12816546030267, -105.1471681902714 40.12801146050332, -105.1473611912454 40.12789646119431, -105.1474471915002 40.12785746102228, -105.1476831913874 40.12780346061299, -105.1478051914117 40.1277864601138, -105.1479051910319 40.12776446140642, -105.1480411907711 40.12775946117674, -105.148131047267 40.12775946111901, -105.1483701909708 40.12775946068273, -105.1484921909401 40.12776446038666, -105.1486281913429 40.12777546030672, -105.1488141912797 40.12775946127093, -105.1489711913174 40.12773246071522, -105.1490791919685 40.12769346043497, -105.1493501918869 40.12752346094415, -105.1498021911529 40.12714446046252, -105.1501191918396 40.1269784605735, -105.1503821911598 40.12695246089658, -105.1508891916811 40.12694046027134, -105.1513948839501 40.12694194872075, -105.1527758874465 40.12694600356159, -105.154300191837 40.12695046002028, -105.1548092204482 40.12693493214863, -105.1549821926101 40.12692646047514, -105.1550255475185 40.12692646026373, -105.1552101930545 40.12692646033931, -105.155437192927 40.12695445958236, -105.1555461931968 40.12695945989714, -105.1556001924722 40.12702245971152, -105.1555921921127 40.12707946011266, -105.15561919262 40.12719845979632, -105.1556931920723 40.12731245959085, -105.1557801926516 40.12740145928399, -105.1559481928024 40.12743746043777, -105.1563391925392 40.1276614597395, -105.1565141933392 40.12771445982453, -105.1565956562976 40.12772766228106, -105.1568041930755 40.12776145992218, -105.1571021940422 40.12773645947969, -105.1572911938164 40.12771146007818, -105.1574571934914 40.12767945991541, -105.1576939255126 40.12766479937127, -105.1578931932202 40.12765245913534, -105.1581221932529 40.12766346026724, -105.1583881937712 40.12771545958289, -105.1587271935286 40.12775946009889, -105.1590381943059 40.12775145938977, -105.1591931935459 40.12775345958096, -105.159295194393 40.12773946004652, -105.1593321942806 40.12776146020572, -105.1593099156614 40.12782736753463, -105.1593961945012 40.12792145999537, -105.1594101940028 40.12802046036595, -105.1593961948648 40.12808645966798, -105.1593311943713 40.12824045994564, -105.1593241941156 40.12833945963551, -105.1593311935832 40.1284274605238, -105.1594381937382 40.12879546005235, -105.1594881935436 40.12887746060884, -105.159567194188 40.1289214593066, -105.159667193892 40.12894945954594, -105.1598101948547 40.12896045970615, -105.1599321943844 40.1289494599988, -105.1601261845107 40.12889596708893, -105.1601262984775 40.1288959359017, -105.1601263677961 40.12889591719213, -105.1602477556501 40.1288630990707, -105.1603761943632 40.1288334601072, -105.1604831934606 40.12878445990846, -105.1620093210164 40.12797305594989, -105.1625441952281 40.1276864588521, -105.1627091942639 40.12764845894845, -105.1627731945469 40.12760446023837, -105.1628381942516 40.1275384598923, -105.1629311946616 40.12746646007216, -105.1633531947814 40.12731345908721, -105.1636321946816 40.12720345937235, -105.1644421950803 40.12692945902451, -105.1648051947436 40.12681345989837, -105.1653700230551 40.12664755080224, -105.1658119066417 40.12652845813221, -105.1665941954893 40.12633345884351, -105.1665751958297 40.1268584592293, -105.1665921947485 40.12690745915487, -105.166642195758 40.12696145922249, -105.1667081954379 40.12699345858284, -105.1667741949328 40.12700345879298, -105.1687057057889 40.12700441568506, -105.1687951961079 40.12700445884948, -105.1688701962396 40.1270274592329, -105.168898196283 40.12704245954604, -105.1689571957668 40.12709045909411, -105.1689921957212 40.12714645870656, -105.1690031954348 40.12720745836092, -105.1689281965424 40.13055845919673, -105.1689125986237 40.1306329048518, -105.1689124571838 40.13066294718519, -105.168948196977 40.1306634594016, -105.1752578000951 40.13068225546467, -105.1763945382965 40.13068560471505, -105.1783901991411 40.13068445895293, -105.1784921990268 40.13071445866245, -105.1785511991025 40.13076045923802, -105.1785684592082 40.13078897836895, -105.1785878532218 40.13077509578964, -105.1786140298435 40.13076007024781, -105.1786409233555 40.13074504669434, -105.1786699537986 40.13073195014857, -105.1786989738613 40.13072105023332, -105.1787301308545 40.13071207822432, -105.1787619985094 40.13070393137015, -105.1787938557948 40.13069798024438, -105.1788260618697 40.13069395205027, -105.1788589733049 40.13069212247468, -105.179390857748 40.13067493221092, -105.1794409400691 40.13067205133859, -105.1794921051437 40.13066697768263, -105.1795411344228 40.1306599761087, -105.1795891003167 40.13065105049456, -105.1796381489549 40.1306399311966, -105.1796850542687 40.13062798274787, -105.1797309025309 40.130613011496, -105.1797921646224 40.13059012217381, -105.1798219014639 40.13057894926776, -105.1798659835888 40.13055903124307, -105.1799089996035 40.13053801326528, -105.1799491668903 40.13051396662497, -105.179986111736 40.13049100982777, -105.1800399263207 40.13045492244582, -105.1800611061436 40.13043796166708, -105.1800941478542 40.13040813023044, -105.1811020789361 40.12954289682526, -105.1821979074391 40.12861201174101, -105.1830460833783 40.12786710866829, -105.1830669241476 40.12784602776817, -105.1830859705434 40.12782604072552, -105.1831309202504 40.12777290813871, -105.1831730413934 40.12771290397964, -105.1831968384394 40.12767096868016, -105.1832091004453 40.12764904103971, -105.183219937338 40.127626010706, -105.1832289697533 40.12760599617817, -105.1832390909328 40.12758296478057, -105.1832459824323 40.12756212029277, -105.1832601269916 40.12751988381583, -105.1832648585161 40.1275020532588, -105.1832688806296 40.1274831219725, -105.1832758462969 40.12744608143081, -105.1832821037178 40.12740794106342, -105.1832829024345 40.12739009972265, -105.1832840642105 40.12737088679798, -105.1832849779852 40.12732806464935, -105.1832850801665 40.12730610366077, -105.183283047838 40.12728194015271, -105.1832799848832 40.12709498627165, -105.1832478926514 40.12523010851267, -105.1832409714686 40.12448889466591, -105.1832360345671 40.1240128697098, -105.1832359130578 40.12396208391974, -105.1832329468866 40.12389280643219, -105.1832291403212 40.12380394395832, -105.183221067644 40.12354093495674, -105.1832278861207 40.12245990722899, -105.183220100863 40.12198112826896, -105.183219146654 40.12034198721235, -105.1832159800522 40.11979294537188, -105.1832148517188 40.11919010373395, -105.1832149465275 40.11870887570952, -105.1832138712203 40.11840196312736, -105.1832139548464 40.11744867340824, -105.183214007166 40.1166821157796, -105.1832146405067 40.11659945281932, -105.1832251983621 40.11659945655838, -105.1835731974845 40.11659745726456, -105.1849951982924 40.1162704558458, -105.1857061993235 40.1159434560531, -105.1863231985656 40.11585645599057, -105.186961199186 40.11590745667103, -105.1882521991136 40.11590845641862, -105.1888961995428 40.11596845552688, -105.1890751996802 40.11591345608336, -105.1892902001129 40.11582045598477, -105.1897331998464 40.11569945564447, -105.1899691999933 40.115595455292, -105.1910672884513 40.11491336443155, -105.1929294323047 40.11376950151904, -105.1948762005162 40.11269545465779, -105.1950342005667 40.112552455237, -105.1951632004082 40.11230545465229, -105.1953772000967 40.11216245484896, -105.1960992007815 40.11183845533019, -105.1963212002698 40.11168945582439, -105.1964147575616 40.11159022926454, -105.196645267477 40.11135237595381, -105.1969652001717 40.11105245479959, -105.1974232003322 40.11090445495005, -105.1977522006899 40.11066845516529, -105.1978522003374 40.11065745427793, -105.1980452007163 40.11072845516461, -105.1984532000932 40.11072845482413, -105.1987392013178 40.1106684554918, -105.1991112014255 40.11049745450588, -105.1993252010489 40.11031145514585, -105.1994638415446 40.11011339692165, -105.1996332004896 40.10987145438538, -105.1997762011607 40.10978945421208, -105.1999912005688 40.1097504539375, -105.2002192006999 40.10978345477821, -105.2005202008154 40.10970645519306, -105.2006808951484 40.10965817306413, -105.2009562018202 40.10957545420762, -105.2010252009949 40.10954845501812, -105.2013932011598 40.10940445475436, -105.2017722018164 40.10934945455519, -105.2021362010449 40.10918445388587, -105.202637201805 40.10880545431794, -105.2027592025271 40.10877245356505, -105.2030522015386 40.10873445440709, -105.203467201412 40.10855845411498, -105.2039462014829 40.10825645418945, -105.2043612024549 40.10813545392831, -105.2053482014456 40.10804245319163, -105.2063492015955 40.10784445371826, -105.2067782023472 40.10770645370304, -105.2069132020766 40.10763045329955, -105.2069115877363 40.10714795702492, -105.206911345534 40.10707560856458, -105.2069113465304 40.10707537710157, -105.2069040254027 40.104888613966, -105.2068932014407 40.10165445272636, -105.2126932031439 40.1016784526342, -105.2147332041786 40.10167545220847, -105.2208973467528 40.10168463798286, -105.220897521504 40.10168463840524, -105.231321784621 40.10169942400351, -105.2313218866605 40.10169942334027, -105.2369722631745 40.10170266098098, -105.2400021278141 40.10171013062091, -105.2429157878592 40.10173100142723, -105.2447240484117 40.10174391773126, -105.2454653469939 40.10173884432958, -105.2460191671759 40.10173505168282, -105.2479743423216 40.1017442592829, -105.2479746695375 40.10174426089772, -105.2479747868204 40.10174426115367, -105.2479752031713 40.10174426296303, -105.2479753357009 40.10174426325229, -105.249079210917 40.10174845048177, -105.249174211575 40.10177944987593, -105.2492452117605 40.10183644999019, -105.2492812117193 40.10191044937188, -105.2493129935197 40.10492068256983, -105.2493130091904 40.10492216055918, -105.2493130142846 40.10492268834712, -105.2493152121548 40.10513744966269, -105.2493982119145 40.1052624508334, -105.2495202115298 40.10533244960861, -105.255947197307 40.10532240708149, -105.2574129970683 40.10532006648594, -105.2586230328064 40.10531812044614, -105.26893309262 40.10530965932736, -105.2768772177547 40.10530344828223, -105.2777142184087 40.10525844880024, -105.2780752184868 40.10515344824243, -105.2784082179298 40.10496344875099, -105.2787982178782 40.104725447886, -105.2791212185347 40.10456344796724, -105.2794542187262 40.10443044801278, -105.2797872183302 40.10431644794893, -105.2812152187992 40.10407744786803, -105.2817202189721 40.10311144774851, -105.2816932183892 40.10171144787009, -105.2819782232338 40.10075949547533, -105.2819774149438 40.10073831713714, -105.2819768350256 40.10072310238548, -105.2819761427939 40.10038105317948, -105.282012830953 40.09975193069047, -105.2820501495957 40.09926089139519, -105.2821051272783 40.09794304108583, -105.2821321056455 40.09710801302935, -105.2821221684136 40.09529810758003, -105.2821409624091 40.09422807602022, -105.2821341594649 40.09311407433201, -105.2821399488127 40.09152792746865, -105.282137898842 40.0899340794033, -105.2821441072337 40.08721088474018, -105.2821390907224 40.08703424902927, -105.2821481523551 40.0870342787379, -105.2821479765674 40.08702801532603, -105.2821421522846 40.08682127765446, -105.2821423153658 40.0868150166831, -105.282162143671 40.08608727764472, -105.2821621432272 40.08608704978086, -105.2821623079241 40.08608101577435, -105.2821423075853 40.08554501716329, -105.2821423070911 40.08263701682382, -105.2821403062932 40.0821320170198, -105.2821463073063 40.08169901632542, -105.2821593066155 40.08068901713151, -105.2821612415979 40.08051401375702, -105.2821622666328 40.08051098862354, -105.2822277607727 40.08031775722681, -105.2823021518433 40.08009827885829, -105.2823952780968 40.07991484894792, -105.2823919994679 40.07989699918794, -105.2823430660183 40.07999338222898, -105.2822150312255 40.07998773507623, -105.2822148038009 40.07998772474011, -105.2822036751846 40.07998723360745, -105.2822223466844 40.07989150774977, -105.2821342160606 40.0791254445771, -105.2821112161553 40.07666744386643, -105.2782532143109 40.07666244408787, -105.278372214492 40.07653744417692, -105.2783742148064 40.07579144511136, -105.2780202147794 40.07579044515734, -105.2779022152453 40.07603844420503, -105.2777612150901 40.07620044483633, -105.2776022148752 40.07633644500343, -105.2774795717141 40.0764360956394, -105.277414215237 40.07647944379102, -105.2774182151642 40.07662844439344, -105.2774232152314 40.07679644423713, -105.277462332525 40.07819215800942, -105.277486220627 40.07914765992864, -105.2775032146846 40.07989444554472, -105.2774442150245 40.07989344467622, -105.2774492150437 40.079994445459, -105.2760592152198 40.07997644544199, -105.2752370110651 40.07998199860944, -105.275236925476 40.07998199844278, -105.2752368011957 40.07998199820081, -105.2752366651909 40.079981997936, -105.2752365174616 40.07998199764835, -105.2752363556628 40.07998199733333, -105.2741904007602 40.07997698391911, -105.2738472151207 40.07997344533944, -105.2732488422515 40.07998423568615, -105.2722111865051 40.0800029400344, -105.271602868858 40.08001390036796, -105.270773469619 40.08002883906712, -105.269120467453 40.08006436083225, -105.2678107184368 40.08009626548748, -105.265906623877 40.08014227963445, -105.2635022120304 40.08020744623987, -105.263475212196 40.07824944591677, -105.2611378514393 40.07826119045901, -105.2610523420133 40.07826161962124, -105.2603639449122 40.0782650686866, -105.2552788447606 40.07829042246069, -105.2528020506824 40.07830197723486, -105.2528018115011 40.07830197852396, -105.2509912135285 40.07831039161324, -105.2509901360399 40.07831039739476, -105.2505104677892 40.07831279674013, -105.2479762077927 40.07832544680577, -105.2467352086361 40.07833144715077, -105.2453582656843 40.07833797915564, -105.2453581543005 40.07833797981056, -105.245048207299 40.07833944731037, -105.2446880583013 40.07833920790986, -105.2446880588089 40.07833844686491, -105.2435522068469 40.07833844725607, -105.2423652076105 40.07833744689923, -105.2422160069221 40.0783371534334, -105.2403432064991 40.07833344770941, -105.2384812068036 40.07833244791702, -105.2378132062725 40.07833444783447, -105.2370786377037 40.07845203165877, -105.2366591894632 40.0785191707074, -105.2352892054144 40.07873844737262, -105.2334432055741 40.07899144749057, -105.2299052044168 40.08008044876753, -105.2350032064051 40.08016044862552, -105.2350497203358 40.08268589163298, -105.2350776389745 40.08420165278985, -105.2350852057845 40.0846124484227, -105.2351382054217 40.08551144874158, -105.2351162069385 40.08560644881669, -105.2349272055709 40.08608544943124, -105.2347532059639 40.0863524487831, -105.2346296381483 40.08650825210744, -105.2344114016713 40.08671004247304, -105.2342874907976 40.08682176614175, -105.2342102060382 40.08689144861766, -105.2341742062996 40.08691344866173, -105.234116919408 40.08694927681879, -105.2340547143473 40.08698818193187, -105.2340141176357 40.08701357127359, -105.2338752055783 40.08710044895112, -105.2337498879304 40.08716518662143, -105.2336642062275 40.0872094484582, -105.233557508418 40.08725212883198, -105.2334842065225 40.08728144947539, -105.2335198087319 40.087300620841, -105.2335350154684 40.08731185997121, -105.2335182680553 40.08731887517195, -105.2334670391323 40.08733945284803, -105.2334153508784 40.08735934044687, -105.2333632162177 40.08737853169327, -105.2333106562827 40.0873970203308, -105.2332572252643 40.08741486387087, -105.2332115864704 40.0874290192368, -105.233160289808 40.08744409547717, -105.2331195646996 40.08745541432238, -105.2331086089517 40.08745846109794, -105.2330565603615 40.08747210532881, -105.2330041639691 40.08748502911613, -105.2329514268327 40.08749722707182, -105.232898377103 40.08750869745924, -105.2328450159892 40.08751943127434, -105.2327913728077 40.08752942858451, -105.232737453437 40.08753868580036, -105.2326832836757 40.08754720298132, -105.2326288764451 40.08755497475301, -105.2325748982646 40.08756217648359, -105.2325209052109 40.08756868375681, -105.2324667696581 40.08757444944327, -105.2324125138727 40.08757947719696, -105.2323581460858 40.0875837616329, -105.2323036897474 40.08758730370593, -105.2322491612788 40.08759010255342, -105.2321945759326 40.08759215640933, -105.232139950141 40.08759346170912, -105.2320852944376 40.08759402388102, -105.2320306369806 40.0875938393878, -105.2319759906559 40.08759291186197, -105.2319213672231 40.08759123322496, -105.2318667865754 40.08758881433079, -105.2318122651521 40.08758564981383, -105.2317578193674 40.08758174061293, -105.2317034632943 40.08757708676092, -105.2316492191852 40.08757169551478, -105.2315951034686 40.08756556421094, -105.2315411374752 40.08755923148525, -105.229337317657 40.08728913118895, -105.2283729549368 40.08717092525384, -105.2280258931392 40.08716865993154, -105.2272912108504 40.08716386193717, -105.2272444844378 40.08716355701311, -105.2272236163383 40.08716344466387, -105.2271977580158 40.08717057341977, -105.2271717266588 40.08717815928905, -105.2271459834793 40.08718610609185, -105.2271204311677 40.08719440999577, -105.2270950662131 40.08720306919137, -105.227069908556 40.08721208192462, -105.2270449570381 40.08722144459034, -105.2270202222304 40.08723115271041, -105.226995713506 40.08724120810847, -105.2269713781346 40.08725160165343, -105.2269462956309 40.08726233387031, -105.2269223132005 40.08727301824765, -105.2269214580284 40.08727339899931, -105.226896880574 40.08728479617606, -105.2268725621166 40.08729651999401, -105.2268485155578 40.08730856958332, -105.2268247444441 40.08732093774738, -105.2268012569799 40.08733362540633, -105.226778067272 40.08734662358735, -105.2267551729715 40.08735993318564, -105.2267325834878 40.08737354701852, -105.2267103070542 40.08738745880117, -105.2266883530404 40.08740167125784, -105.2266667226549 40.08741617538511, -105.2266454253037 40.08743096490092, -105.2266244715363 40.08744604073107, -105.2266038602236 40.08746139206541, -105.22658359957 40.0874770198241, -105.2265637001611 40.08749291592657, -105.2265441631842 40.08750907677334, -105.226524998038 40.0875254978835, -105.2265062070929 40.08754217295839, -105.2264878009205 40.08755909752002, -105.2264697795498 40.08757626436348, -105.2264521500162 40.08759367350561, -105.226434455812 40.08761141663134, -105.2264158800905 40.08762967283475, -105.2263977138776 40.0876481506639, -105.2263825065714 40.08766855838156, -105.2263789361496 40.08767231912204, -105.2263767305145 40.08767464926904, -105.2263745307277 40.0876769830324, -105.2263723344585 40.0876793168041, -105.2263701416961 40.08768165328597, -105.2263679524405 40.08768399247809, -105.2263657702201 40.0876863316868, -105.2263635879888 40.08768867359738, -105.2263614080953 40.08769101731477, -105.2263592363989 40.0876933637535, -105.2263570647023 40.08769571019219, -105.226354900023 40.08769806115065, -105.2263527353471 40.08770041120849, -105.2263505776958 40.08770276398484, -105.2263484247239 40.08770511947421, -105.2263462740824 40.08770747857164, -105.2263441269622 40.08770983677667, -105.2263419810035 40.08771219768641, -105.2263398455944 40.08771455952174, -105.2263377078255 40.08771692495404, -105.2263355759121 40.08771929220145, -105.226333448689 40.08772165945994, -105.2263313249726 40.08772402942868, -105.2263292047701 40.08772640030627, -105.2263270845495 40.0877287756871, -105.2263249737094 40.08773115109006, -105.226322866376 40.08773352920324, -105.2263207637256 40.08773590912882, -105.2263186598953 40.08773829085281, -105.2263165619241 40.08774067349134, -105.226314467456 40.08774305974064, -105.2263123800232 40.08774544600666, -105.2263102972735 40.08774783408501, -105.2263082145056 40.08775022666651, -105.2263061352625 40.08775261745505, -105.2263040642092 40.08775501276614, -105.2263019919905 40.08775740627321, -105.2262999267926 40.08775980339941, -105.2262978662741 40.08776220323865, -105.2262958045756 40.08776460487633, -105.2262937499053 40.08776700833194, -105.226291699918 40.08776941359987, -105.2262896569624 40.08777181978507, -105.2262876128304 40.08777422686813, -105.2262855745432 40.08777663846826, -105.2262835374175 40.08777905277302, -105.2262815085034 40.08778146619655, -105.2262794831069 40.0877838796284, -105.2262774576886 40.08778629846402, -105.2262754393057 40.08778871731626, -105.2262734244331 40.08779113797818, -105.2262714142507 40.0877935586511, -105.2262694052227 40.08779598382996, -105.2262674008741 40.08779841172184, -105.2262654059096 40.08780083873525, -105.2262634085889 40.08780326844501, -105.2262614183 40.08780569907206, -105.2262594326977 40.0878081306108, -105.226257445901 40.08781056755058, -105.2262554673158 40.08781300360911, -105.2262534898923 40.08781544237237, -105.2262515195077 40.08781788025156, -105.2262495549714 40.08782032174722, -105.2262475892516 40.08782276594194, -105.2262456270494 40.08782521014498, -105.2262436742169 40.08782765707216, -105.2262417237222 40.08783010580613, -105.2262397767451 40.08783255454839, -105.2262378332675 40.08783500780219, -105.2262358933076 40.08783746106425, -105.2262339568581 40.08783991613592, -105.226232023919 40.08784237301715, -105.2262300991841 40.08784483081848, -105.2262281732657 40.08784729131887, -105.2262262543791 40.08784975273657, -105.2262243401755 40.08785221596659, -105.226222428306 40.08785468190413, -105.2262205211268 40.08785714785272, -105.2262186162781 40.08785961740938, -105.2262167161233 40.08786208607652, -105.2262148218203 40.0878645574594, -105.2262129298625 40.08786702884783, -105.2262110437421 40.0878695065546, -105.2262091611538 40.08787198066713, -105.2262072808852 40.08787446108968, -105.2262054064867 40.08787693972477, -105.226203534426 40.08787942016669, -105.2262016682208 40.08788190242377, -105.2261998043462 40.08788438828893, -105.226197947507 40.08788687417072, -105.226196091833 40.08788936185654, -105.2261942361589 40.08789184954237, -105.2261923945412 40.08789434086405, -105.2261905517435 40.08789683398418, -105.2261887112837 40.08789932891115, -105.2261868778629 40.08790182295415, -105.2261850455965 40.08790432150305, -105.2261832203618 40.08790682096924, -105.2261813974722 40.08790932044101, -105.2261795792655 40.08791182172511, -105.2261777645729 40.08791432391816, -105.2261759557322 40.08791682882699, -105.2261741480568 40.08791933553987, -105.226172348582 40.08792184407345, -105.2261705502725 40.0879243544111, -105.2261687566533 40.08792686475982, -105.2261669688859 40.08792937782427, -105.2261651799496 40.08793188998534, -105.2261634015482 40.08793440667458, -105.2261616231395 40.08793692516508, -105.2261598505936 40.08793944366944, -105.2261580815545 40.08794196488402, -105.2261563172056 40.08794448610973, -105.2261545551981 40.08794700824161, -105.2261528013842 40.08794953399544, -105.2261510475738 40.08795205884863, -105.226149300777 40.08795458912228, -105.2261475563434 40.08795711489833, -105.2261458165711 40.08795964789051, -105.2261440803236 40.08796217908979, -105.2261423475865 40.08796471209865, -105.2261406218776 40.08796724692545, -105.2261388996683 40.08796978626372, -105.2261371809875 40.08797232290842, -105.2261354658207 40.08797486046209, -105.2261337541534 40.08797740252725, -105.2261320460038 40.0879799446007, -105.2261303460513 40.08798248939556, -105.2261286460914 40.08798503599166, -105.226126950829 40.08798758079754, -105.2261252602387 40.08799013011774, -105.2261235755077 40.08799268035245, -105.2261218943052 40.08799522789362, -105.2261202165914 40.08799778264812, -105.226118542406 40.08800033470907, -105.2261168764069 40.08800289219328, -105.2261152092496 40.08800544607216, -105.2261135491024 40.08800800627216, -105.2261118948289 40.0880105637841, -105.2261102405372 40.08801312579922, -105.2261085932736 40.08801568963229, -105.2261069495313 40.08801825257306, -105.2261053092994 40.08802081732343, -105.2261036725816 40.08802338298269, -105.2261020440572 40.08802595226398, -105.2261004178852 40.08802851974954, -105.2260987916986 40.08803109083762, -105.2260971760652 40.08803366195077, -105.2260955615934 40.08803623576855, -105.2260939506355 40.08803881049528, -105.2260923455334 40.08804138703718, -105.2260907451214 40.08804396359018, -105.2260891482163 40.08804654285341, -105.2260875536562 40.08804912212216, -105.2260859637863 40.08805170140207, -105.2260843809301 40.08805428610243, -105.2260827980811 40.08805686900151, -105.2260812222603 40.08805945371852, -105.2260796499462 40.0880620411458, -105.226078084664 40.08806462949036, -105.2260765193853 40.08806721693423, -105.2260749611275 40.0880698079974, -105.2260734087289 40.088072399975, -105.2260718574956 40.08807499375673, -105.2260703097799 40.08807758754672, -105.2260687690924 40.08808018315465, -105.2260672295774 40.08808277876541, -105.2260656970834 40.08808537799534, -105.2260641669416 40.08808797542954, -105.2260626414721 40.08809057737804, -105.2260611230379 40.08809317934323, -105.2260596034202 40.08809578400751, -105.2260580920141 40.08809838779062, -105.2260565841257 40.08810099158206, -105.2260550832546 40.0881035998933, -105.2260535823798 40.08810620910523, -105.2260520885404 40.08810881833376, -105.2260505993841 40.08811142937476, -105.2260491125655 40.08811404222255, -105.2260476280957 40.08811665417521, -105.226046152992 40.08811926975269, -105.2260446767192 40.08812188442674, -105.2260432086508 40.08812450002085, -105.2260417429166 40.08812711832244, -105.2260402865523 40.08812973934819, -105.2260388290152 40.08813236037112, -105.2260373773409 40.08813498140795, -105.226035930357 40.08813760245592, -105.2260344868726 40.08814022801536, -105.2260330445643 40.08814285267693, -105.2260316128055 40.08814547826421, -105.2260301833774 40.08814810745953, -105.2260289772142 40.08815032829153, -105.2260799511012 40.08815043483378, -105.2260951784236 40.08815046645809, -105.2259971464311 40.08825128178296, -105.225866596984 40.08846589835929, -105.2258660799562 40.08846674914248, -105.2258442047025 40.08817345056035, -105.2258472559384 40.08702564690012, -105.2258472562248 40.08702557574974, -105.2258422045073 40.08612344890279, -105.2246712037403 40.08611344976358, -105.2246852045713 40.08554044892636, -105.2230462031982 40.08603244956893, -105.2219812039535 40.08618344991433, -105.2211162029895 40.08627444986659, -105.2211262032423 40.08639345027048, -105.2191138039488 40.0864074176304, -105.2182432027494 40.08641344971119, -105.2182532019159 40.08714945059754, -105.2163692023297 40.08714545077098, -105.216360202134 40.08892145040806, -105.2163292022599 40.08892045018143, -105.2162802020392 40.08892045046189, -105.2159742024865 40.08892045011142, -105.2148588360544 40.08892679371123, -105.2148042021617 40.08892745043244, -105.2143002021996 40.08892245043239, -105.213437201397 40.08892445097817, -105.2114362013246 40.08891745132185, -105.2102906849293 40.08891722500127, -105.2102892648914 40.08891722413985, -105.2102871823232 40.08891722341717, -105.2102854292613 40.08891722262064, -105.2102848781325 40.08891722213826, -105.2093902465011 40.08891684883024, -105.208456199712 40.08891645102268, -105.2075245971012 40.08890693460845, -105.2069481319076 40.08890527106102, -105.2069438669998 40.08890529265857, -105.2069747075104 40.09435044215074, -105.2069082004758 40.09435075068787, -105.2067688747363 40.09435139755085, -105.206769231588 40.09440878489543, -105.2067696857456 40.09448197611559, -105.206084292794 40.09448027846468, -105.204067954345 40.09447526321931, -105.2020925487541 40.09447072187066, -105.2004028346573 40.09447194731246, -105.2000942419318 40.09447216840297, -105.20004901646 40.0944713051883, -105.1999431444402 40.09446928464906, -105.1961591443175 40.09444728514715, -105.1941921454042 40.0944432846204, -105.1914201445046 40.09443828540665, -105.1878551441828 40.09443028595678, -105.1878554742897 40.09442402015232, -105.1878581347478 40.09437345425398, -105.1878581437286 40.09437328585741, -105.1878579783739 40.09437328631103, -105.1878583084638 40.09436702410904, -105.1878489982433 40.09436703406432, -105.1869333094328 40.09436802324625, -105.1869288298045 40.09436799308698, -105.1864923089405 40.09436502536359, -105.1851823083869 40.09435602463465, -105.1851806430128 40.0943560507158, -105.1847691909817 40.09436254127205, -105.1847611298219 40.09436911199498, -105.1842981568986 40.09474644455597, -105.1842254973132 40.09480566330672, -105.1770289540793 40.10167497796913, -105.1763019499671 40.1023029683946, -105.1688417643584 40.10884061707407, -105.1685799278165 40.10901976085416, -105.1674439177613 40.11003576716704, -105.1614528663692 40.11528080007928, -105.1609821531084 40.11566321114483, -105.1594641412873 40.11689641328065, -105.1594566443818 40.11609286922273, -105.159467921669 40.11419687283805, -105.1594718259507 40.11205812132699, -105.1594520114176 40.10922888777313, -105.1594495599439 40.10886022285561, -105.1594259918098 40.10399197542836, -105.1590781918603 40.10400245670831, -105.1588411915942 40.10426645671227, -105.1588201907179 40.10434845704976, -105.1589061910858 40.10450845692532, -105.1588991905787 40.10458445709242, -105.1587201908592 40.10476045668218, -105.1584981900914 40.10477145654381, -105.1581892413284 40.10490396872007, -105.1580761909817 40.10495245717316, -105.1576681914213 40.10507845747404, -105.1572321903226 40.10529845652795, -105.1571241898577 40.1053754563856, -105.1571241900853 40.10546345672344, -105.157253190884 40.10562845707536, -105.157239191129 40.10571045628147, -105.157138190582 40.10579245659894, -105.1569951900118 40.10582045723518, -105.1565797245652 40.10604856929712, -105.1564161904518 40.10613345690832, -105.1557151895679 40.10621545706669, -105.155372190027 40.10630845692795, -105.1551781906975 40.10638545677693, -105.1551071895624 40.106484457227, -105.1549851905804 40.10658345749179, -105.1546631906193 40.10667645674386, -105.1543781900811 40.10669245702027, -105.1538481902248 40.10664345777509, -105.1536831893247 40.10669845729011, -105.153533190452 40.10679645699769, -105.1534041890178 40.10683545695765, -105.1532181895994 40.10680245729557, -105.1529611896807 40.10678045703483, -105.1528251894787 40.1068184572149, -105.1528251898034 40.10689545706076, -105.1527461895664 40.10708745705721, -105.1527891896304 40.10716445739909, -105.1530821895656 40.10724745707277, -105.1531971895655 40.10730745767818, -105.1532041904084 40.10742245698562, -105.1531681905297 40.10752745787505, -105.1530101897713 40.1076424577811, -105.1526961899649 40.10774645807478, -105.1522381891769 40.1078014575306, -105.1521161891182 40.10785645730169, -105.1520521905081 40.10809245803009, -105.1518081899357 40.10844445794176, -105.1518011892207 40.10854845784844, -105.1519151896514 40.1086254581982, -105.1522161898024 40.10867445774499, -105.1522521895131 40.10872445833751, -105.1522441899349 40.10883445806299, -105.1521871900507 40.10886745719991, -105.1521720437602 40.10888555509551, -105.152168642065 40.10888557367066, -105.152058189739 40.10899345806407, -105.1516361903776 40.10915845863114, -105.1515425217955 40.10915797339747, -105.151443190266 </t>
+          <t>POLYGON ((-105.13105731309996 40.12712102857881, -105.13104831458692 40.12882902900039, -105.13101981743496 40.130743881653224, -105.13101977780484 40.1307470797142, -105.13100984309389 40.13155699817882, -105.13100039564006 40.131998445721095, -105.13098885823698 40.13253599608295, -105.13098791887256 40.13259022536034, -105.13097083257887 40.133589996318406, -105.13095686229188 40.13407299670184, -105.13096631588034 40.13407590265542, -105.13096729097423 40.134075903068194, -105.13126401824097 40.134075902140594, -105.13519498808807 40.134061905581305, -105.13559699205447 40.13406290499365, -105.13621899098595 40.134063906049626, -105.13834813398768 40.134067896007096, -105.13871421308136 40.134055424571265, -105.13876015693886 40.13397838399309, -105.13886415998937 40.13379438525001, -105.13940617709889 40.13283739637802, -105.13961725428423 40.132469454910506, -105.13991131549166 40.13199350715775, -105.14003131528621 40.13181050557099, -105.14028734385782 40.13141953294432, -105.14041340752419 40.13123259600766, -105.14041349144453 40.13123248008579, -105.14056749281461 40.13101869438201, -105.1409685953441 40.13051183984713, -105.14107158970647 40.13039683245281, -105.14122552052527 40.13022372772332, -105.14145369018013 40.12994403235987, -105.14164167314328 40.12976299450775, -105.14338270029026 40.12803805788978, -105.14437163765314 40.12710336772473, -105.14469383772784 40.126798834591625, -105.14471370650433 40.12678007314066, -105.14488469664316 40.126620046490515, -105.14512674453258 40.1263892194086, -105.14563279573125 40.12596286157071, -105.14563304104932 40.125975011112814, -105.14564233602215 40.12643537867292, -105.14564872818227 40.12675200170747, -105.14561680149934 40.12884799589443, -105.14561676449995 40.128854426377934, -105.14562719035258 40.12885446106298, -105.14576519121955 40.128834461316146, -105.14599419091246 40.128769460433325, -105.14620919021763 40.1287254615651, -105.14638119106708 40.128681461275804, -105.14650919051532 40.1286324608168, -105.14665219099479 40.128516460373454, -105.1467601907007 40.12837346040647, -105.14696819180368 40.12816546030267, -105.14716819027137 40.12801146050332, -105.14736119124542 40.12789646119431, -105.14744719150019 40.12785746102228, -105.14768319138743 40.12780346061299, -105.14780519141166 40.127786460113796, -105.1479051910319 40.12776446140642, -105.14804119077108 40.12775946117674, -105.14813104726704 40.12775946111901, -105.1483701909708 40.12775946068273, -105.14849219094015 40.127764460386665, -105.14862819134288 40.127775460306715, -105.14881419127971 40.127759461270934, -105.14897119131737 40.127732460715215, -105.14907919196847 40.12769346043497, -105.14935019188688 40.127523460944154, -105.14980219115287 40.12714446046252, -105.15011919183956 40.126978460573504, -105.1503821911598 40.12695246089658, -105.1508891916811 40.12694046027134, -105.15139488395013 40.12694194872075, -105.15277588744652 40.12694600356159, -105.15430019183701 40.12695046002028, -105.1548092204482 40.12693493214863, -105.15498219261008 40.12692646047514, -105.15502554751848 40.126926460263725, -105.15521019305447 40.126926460339305, -105.15543719292698 40.12695445958236, -105.15554619319677 40.126959459897144, -105.15560019247224 40.12702245971152, -105.15559219211266 40.12707946011266, -105.15561919262002 40.12719845979632, -105.15569319207229 40.127312459590854, -105.15578019265165 40.127401459283995, -105.15594819280243 40.12743746043777, -105.15633919253925 40.1276614597395, -105.15651419333918 40.12771445982453, -105.15659565629761 40.12772766228106, -105.15680419307546 40.12776145992218, -105.15710219404221 40.127736459479685, -105.15729119381645 40.12771146007818, -105.15745719349138 40.127679459915406, -105.15769392551258 40.127664799371274, -105.1578931932202 40.12765245913534, -105.15812219325285 40.127663460267236, -105.15838819377116 40.12771545958289, -105.15872719352858 40.127759460098886, -105.15903819430594 40.12775145938977, -105.15919319354586 40.12775345958096, -105.15929519439304 40.12773946004652, -105.15933219428058 40.12776146020572, -105.15930991566137 40.12782736753463, -105.15939619450118 40.12792145999537, -105.15941019400277 40.128020460365946, -105.15939619486478 40.12808645966798, -105.15933119437133 40.12824045994564, -105.15932419411557 40.128339459635505, -105.15933119358321 40.128427460523795, -105.15943819373818 40.12879546005235, -105.15948819354355 40.12887746060884, -105.15956719418796 40.1289214593066, -105.15966719389199 40.12894945954594, -105.15981019485466 40.12896045970615, -105.15993219438444 40.1289494599988, -105.16012618451066 40.12889596708893, -105.16012629847745 40.1288959359017, -105.16012636779612 40.12889591719213, -105.16024775565006 40.1288630990707, -105.16037619436318 40.1288334601072, -105.16048319346062 40.12878445990846, -105.1620093210164 40.127973055949894, -105.16254419522811 40.1276864588521, -105.16270919426387 40.12764845894845, -105.16277319454686 40.12760446023837, -105.16283819425159 40.1275384598923, -105.1629311946616 40.127466460072164, -105.16335319478137 40.12731345908721, -105.16363219468157 40.12720345937235, -105.16444219508034 40.12692945902451, -105.1648051947436 40.126813459898365, -105.1653700230551 40.12664755080224, -105.16581190664166 40.126528458132206, -105.16659419548927 40.12633345884351, -105.16657519582972 40.1268584592293, -105.16659219474849 40.12690745915487, -105.16664219575804 40.12696145922249, -105.16670819543795 40.12699345858284, -105.16677419493276 40.127003458792984, -105.16870570578885 40.127004415685064, -105.16879519610792 40.127004458849484, -105.16887019623955 40.1270274592329, -105.16889819628297 40.12704245954604, -105.16895719576684 40.127090459094106, -105.16899219572122 40.127146458706555, -105.16900319543478 40.12720745836092, -105.16892819654235 40.130558459196735, -105.16891259862375 40.1306329048518, -105.16891245718378 40.13066294718519, -105.16894819697697 40.1306634594016, -105.17525780009512 40.13068225546467, -105.17639453829649 40.13068560471505, -105.17839019914108 40.130684458952935, -105.1784921990268 40.130714458662446, -105.17855119910251 40.13076045923802, -105.17856845920818 40.130788978368955, -105.1785878532218 40.13077509578964, -105.17861402984349 40.13076007024781, -105.17864092335547 40.130745046694344, -105.17866995379858 40.13073195014857, -105.1786989738613 40.13072105023332, -105.17873013085455 40.13071207822432, -105.17876199850942 40.13070393137015, -105.17879385579481 40.130697980244385, -105.17882606186974 40.130693952050265, -105.1788589733049 40.130692122474684, -105.17939085774799 40.13067493221092, -105.17944094006911 40.13067205133859, -105.17949210514372 40.13066697768263, -105.1795411344228 40.130659976108696, -105.17958910031675 40.13065105049456, -105.17963814895494 40.1306399311966, -105.17968505426869 40.130627982747875, -105.17973090253089 40.130613011496, -105.17979216462236 40.13059012217381, -105.17982190146394 40.130578949267765, -105.17986598358878 40.130559031243074, -105.1799089996035 40.13053801326528, -105.17994916689032 40.130513966624974, -105.179986111736 40.13049100982777, -105.18003992632066 40.13045492244582, -105.18006110614358 40.130437961667084, -105.18009414785423 40.130408130230435, -105.18110207893609 40.129542896825264, -105.18219790743906 40.128612011741005, -105.18304608337829 40.12786710866829, -105.18306692414764 40.12784602776817, -105.18308597054336 40.12782604072552, -105.18313092025036 40.12777290813871, -105.18317304139345 40.12771290397964, -105.18319683843944 40.127670968680164, -105.18320910044525 40.12764904103971, -105.18321993733795 40.127626010706, -105.18322896975332 40.12760599617817, -105.18323909093279 40.127582964780565, -105.18324598243231 40.127562120292765, -105.18326012699163 40.12751988381583, -105.1832648585161 40.1275020532588, -105.18326888062958 40.1274831219725, -105.18327584629688 40.12744608143081, -105.1832821037178 40.12740794106342, -105.18328290243448 40.127390099722646, -105.18328406421048 40.127370886797976, -105.18328497798515 40.127328064649355, -105.18328508016651 40.12730610366077, -105.18328304783802 40.12728194015271, -105.18327998488321 40.12709498627165, -105.18324789265142 40.125230108512675, -105.18324097146863 40.12448889466591, -105.18323603456712 40.1240128697098, -105.18323591305776 40.123962083919736, -105.18323294688659 40.12389280643219, -105.18322914032119 40.12380394395832, -105.183221067644 40.123540934956736, -105.18322788612069 40.12245990722899, -105.183220100863 40.12198112826896, -105.18321914665395 40.12034198721235, -105.18321598005215 40.11979294537188, -105.18321485171883 40.11919010373395, -105.18321494652749 40.118708875709515, -105.18321387122035 40.11840196312736, -105.18321395484635 40.11744867340824, -105.18321400716599 40.116682115779604, -105.1832146405067 40.11659945281932, -105.18322519836212 40.116599456558376, -105.18357319748455 40.11659745726456, -105.18499519829243 40.1162704558458, -105.1857061993235 40.115943456053095, -105.1863231985656 40.115856455990574, -105.186961199186 40.11590745667103, -105.1882521991136 40.115908456418616, -105.18889619954282 40.115968455526875, -105.18907519968022 40.11591345608336, -105.1892902001129 40.115820455984775, -105.18973319984643 40.115699455644474, -105.18996919999327 40.115595455291995, -105.19106728845128 40.11491336443155, -105.19292943230472 40.11376950151904, -105.1948762005162 40.11269545465779, -105.19503420056672 40.112552455237, -105.19516320040816 40.11230545465229, -105.19537720009669 40.112162454848956, -105.19609920078153 40.11183845533019, -105.19632120026978 40.11168945582439, -105.1964147575616 40.11159022926454, -105.19664526747701 40.11135237595381, -105.19696520017166 40.11105245479959, -105.19742320033224 40.110904454950045, -105.19775220068986 40.11066845516529, -105.19785220033737 40.110657454277934, -105.19804520071632 40.11072845516461, -105.19845320009317 40.11072845482413, -105.19873920131776 40.110668455491805, -105.19911120142554 40.110497454505875, -105.19932520104891 40.11031145514585, -105.1994638415446 40.11011339692165, -105.19963320048963 40.10987145438538, -105.19977620116069 40.109789454212084, -105.19999120056882 40.1097504539375, -105.20021920069989 40.10978345477821, -105.20052020081545 40.10970645519306, -105.20068089514842 40.109658173064126, -105.20095620182019 40.109575454207615, -105.20102520099488 40.10954845501812, -105.20139320115982 40.10940445475436, -105.2017722018164 40.109349454555186, -105.20213620104491 40.10918445388587, -105.20263720180502 40.10880545431794, -105.20275920252708 40.10877245356505, -105.2030522015386 40.10873445440709, -105.203467201412 40.108558454114984, -105.20394620148292 40.10825645418945, -105.20436120245495 40.108135453928305, -105.20534820144557 40.10804245319163, -105.20634920159554 40.10784445371826, -105.20677820234718 40.10770645370304, -105.20691320207663 40.10763045329955, -105.2069115877363 40.10714795702492, -105.20691134553404 40.10707560856458, -105.20691134653038 40.107075377101566, -105.2069040254027 40.104888613966, -105.20689320144066 40.10165445272636, -105.21269320314391 40.1016784526342, -105.21473320417856 40.10167545220847, -105.22089734675276 40.10168463798286, -105.22089752150396 40.10168463840524, -105.23132178462099 40.101699424003506, -105.23132188666052 40.10169942334027, -105.23697226317451 40.101702660980976, -105.24000212781411 40.10171013062091, -105.24291578785923 40.10173100142723, -105.24472404841167 40.101743917731255, -105.24546534699388 40.10173884432958, -105.24601916717593 40.101735051682816, -105.24797434232157 40.101744259282896, -105.2479746695375 40.10174426089772, -105.24797478682038 40.10174426115367, -105.24797520317126 40.10174426296303, -105.24797533570093 40.10174426325229, -105.24907921091696 40.10174845048177, -105.24917421157502 40.101779449875934, -105.24924521176052 40.10183644999019, -105.24928121171928 40.10191044937188, -105.24931299351972 40.10492068256983, -105.24931300919039 40.104922160559184, -105.24931301428464 40.104922688347116, -105.24931521215476 40.10513744966269, -105.24939821191451 40.1052624508334, -105.24952021152978 40.10533244960861, -105.255947197307 40.105322407081495, -105.2574129970683 40.105320066485945, -105.25862303280643 40.10531812044614, -105.26893309262 40.10530965932736, -105.27687721775466 40.10530344828223, -105.27771421840869 40.10525844880024, -105.27807521848682 40.10515344824243, -105.2784082179298 40.104963448750986, -105.2787982178782 40.104725447886, -105.27912121853468 40.104563447967244, -105.27945421872622 40.10443044801278, -105.27978721833017 40.10431644794893, -105.2812152187992 40.10407744786803, -105.28172021897208 40.10311144774851, -105.28169321838922 40.10171144787009, -105.28197822323375 40.10075949547533, -105.28197741494381 40.10073831713714, -105.28197683502565 40.10072310238548, -105.28197614279391 40.100381053179476, -105.28201283095298 40.099751930690466, -105.28205014959568 40.09926089139519, -105.28210512727827 40.09794304108583, -105.28213210564554 40.09710801302935, -105.28212216841357 40.09529810758003, -105.2821409624091 40.094228076020215, -105.2821341594649 40.09311407433201, -105.2821399488127 40.09152792746865, -105.282137898842 40.0899340794033, -105.28214410723375 40.08721088474018, -105.2821390907224 40.087034249029266, -105.28214815235506 40.0870342787379, -105.28214797656739 40.08702801532603, -105.28214215228456 40.08682127765446, -105.28214231536583 40.0868150166831, -105.282162143671 40.086087277644715, -105.28216214322723 40.086087049780865, -105.2821623079241 40.086081015774354, -105.2821423075853 40.08554501716329, -105.28214230709114 40.08263701682382, -105.28214030629316 40.082132017019795, -105.28214630730635 40.081699016325416, -105.2821593066155 40.08068901713151, -105.28216124159793 40.08051401375702, -105.28216226663278 40.080510988623544, -105.28222776077268 40.08031775722681, -105.28230215184334 40.08009827885829, -105.28239527809679 40.079914848947915, -105.28239199946788 40.07989699918794, -105.28234306601831 40.079993382228984, -105.28221503122555 40.07998773507623, -105.28221480380088 40.07998772474011, -105.28220367518465 40.07998723360745, -105.28222234668438 40.07989150774977, -105.28213421606061 40.0791254445771, -105.2821112161553 40.076667443866434, -105.27825321431087 40.076662444087866, -105.27837221449197 40.07653744417692, -105.27837421480645 40.07579144511136, -105.27802021477937 40.07579044515734, -105.27790221524532 40.076038444205025, -105.27776121509011 40.07620044483633, -105.2776022148752 40.076336445003435, -105.27747957171408 40.0764360956394, -105.27741421523704 40.076479443791015, -105.27741821516419 40.07662844439344, -105.27742321523138 40.076796444237125, -105.27746233252502 40.07819215800942, -105.27748622062703 40.079147659928644, -105.2775032146846 40.079894445544724, -105.27744421502449 40.07989344467622, -105.27744921504366 40.079994445459, -105.27605921521977 40.07997644544199, -105.27523701106514 40.07998199860944, -105.27523692547598 40.07998199844278, -105.27523680119573 40.079981998200815, -105.27523666519092 40.079981997936, -105.27523651746156 40.07998199764835, -105.27523635566277 40.07998199733333, -105.27419040076023 40.07997698391911, -105.27384721512072 40.07997344533944, -105.27324884225148 40.079984235686155, -105.27221118650507 40.0800029400344, -105.27160286885797 40.08001390036796, -105.27077346961903 40.08002883906712, -105.26912046745295 40.08006436083225, -105.26781071843679 40.08009626548748, -105.26590662387704 40.08014227963445, -105.26350221203036 40.08020744623987, -105.26347521219596 40.07824944591677, -105.26113785143929 40.07826119045901, -105.26105234201327 40.07826161962124, -105.26036394491224 40.0782650686866, -105.25527884476058 40.07829042246069, -105.25280205068242 40.07830197723486, -105.2528018115011 40.07830197852396, -105.25099121352854 40.07831039161324, -105.25099013603987 40.07831039739476, -105.25051046778918 40.07831279674013, -105.24797620779272 40.07832544680577, -105.24673520863611 40.078331447150774, -105.2453582656843 40.07833797915564, -105.24535815430046 40.07833797981056, -105.24504820729896 40.07833944731037, -105.24468805830135 40.07833920790986, -105.2446880588089 40.07833844686491, -105.2435522068469 40.07833844725607, -105.2423652076105 40.078337446899226, -105.24221600692208 40.078337153433395, -105.2403432064991 40.07833344770941, -105.2384812068036 40.07833244791702, -105.2378132062725 40.07833444783447, -105.23707863770375 40.07845203165877, -105.23665918946315 40.0785191707074, -105.23528920541436 40.07873844737262, -105.23344320557413 40.078991447490566, -105.22990520441682 40.080080448767525, -105.23500320640507 40.08016044862552, -105.23504972033575 40.082685891632984, -105.23507763897449 40.08420165278985, -105.23508520578451 40.084612448422696, -105.23513820542169 40.08551144874158, -105.23511620693853 40.08560644881669, -105.23492720557088 40.08608544943124, -105.23475320596388 40.086352448783096, -105.23462963814833 40.08650825210744, -105.23441140167128 40.086710042473044, -105.23428749079763 40.08682176614175, -105.2342102060382 40.086891448617656, -105.23417420629958 40.086913448661726, -105.23411691940804 40.086949276818785, -105.23405471434727 40.08698818193187, -105.23401411763574 40.08701357127359, -105.2338752055783 40.08710044895112, -105.23374988793036 40.08716518662143, -105.23366420622754 40.087209448458204, -105.23355750841804 40.087252128831985, -105.23348420652255 40.08728144947539, -105.2335198087319 40.087300620841, -105.23353501546842 40.08731185997121, -105.23351826805532 40.087318875171945, -105.23346703913232 40.087339452848035, -105.23341535087839 40.087359340446866, -105.23336321621771 40.08737853169327, -105.23331065628268 40.0873970203308, -105.23325722526434 40.08741486387087, -105.23321158647039 40.0874290192368, -105.23316028980796 40.08744409547717, -105.2331195646996 40.08745541432238, -105.23310860895167 40.08745846109794, -105.23305656036149 40.087472105328814, -105.23300416396908 40.08748502911613, -105.23295142683274 40.08749722707182, -105.23289837710301 40.08750869745924, -105.23284501598923 40.08751943127434, -105.23279137280774 40.08752942858451, -105.23273745343701 40.08753868580036, -105.2326832836757 40.08754720298132, -105.23262887644508 40.08755497475301, -105.23257489826456 40.087562176483594, -105.23252090521092 40.087568683756814, -105.23246676965806 40.08757444944327, -105.23241251387269 40.08757947719696, -105.2323581460858 40.0875837616329, -105.23230368974735 40.08758730370593, -105.2322491612788 40.08759010255342, -105.23219457593261 40.08759215640933, -105.23213995014099 40.08759346170912, -105.23208529443761 40.087594023881024, -105.23203063698061 40.0875938393878, -105.23197599065594 40.08759291186197, -105.23192136722312 40.087591233224956, -105.23186678657542 40.08758881433079, -105.23181226515209 40.08758564981383, -105.2317578193674 40.087581740612926, -105.23170346329434 40.087577086760916, -105.23164921918521 40.087571695514775, -105.23159510346865 40.08756556421094, -105.23154113747518 40.08755923148525, -105.229337317657 40.087289131188946, -105.2283729549368 40.08717092525384, -105.22802589313916 40.087168659931535, -105.22729121085041 40.08716386193717, -105.22724448443779 40.08716355701311, -105.22722361633834 40.08716344466387, -105.22719775801576 40.08717057341977, -105.22717172665875 40.087178159289046, -105.22714598347935 40.08718610609185, -105.22712043116775 40.087194409995774, -105.22709506621307 40.08720306919137, -105.227069908556 40.08721208192462, -105.22704495703813 40.08722144459034, -105.22702022223042 40.08723115271041, -105.22699571350596 40.087241208108466, -105.22697137813459 40.08725160165343, -105.22694629563092 40.087262333870314, -105.22692231320049 40.08727301824765, -105.22692145802843 40.08727339899931, -105.22689688057402 40.087284796176064, -105.22687256211657 40.087296519994005, -105.22684851555779 40.08730856958332, -105.22682474444414 40.08732093774738, -105.22680125697993 40.08733362540633, -105.22677806727201 40.08734662358735, -105.22675517297154 40.08735993318564, -105.22673258348783 40.087373547018515, -105.2267103070542 40.08738745880117, -105.22668835304036 40.087401671257844, -105.22666672265485 40.08741617538511, -105.22664542530366 40.08743096490092, -105.2266244715363 40.08744604073107, -105.22660386022363 40.087461392065414, -105.22658359956998 40.0874770198241, -105.22656370016112 40.08749291592657, -105.22654416318423 40.08750907677334, -105.226524998038 40.0875254978835, -105.22650620709292 40.08754217295839, -105.22648780092054 40.08755909752002, -105.22646977954976 40.087576264363484, -105.22645215001624 40.08759367350561, -105.22643445581203 40.08761141663134, -105.22641588009053 40.08762967283475, -105.22639771387756 40.087648150663895, -105.22638250657144 40.08766855838156, -105.22637893614962 40.08767231912204, -105.22637673051449 40.08767464926904, -105.22637453072771 40.0876769830324, -105.22637233445855 40.0876793168041, -105.22637014169614 40.08768165328597, -105.22636795244047 40.08768399247809, -105.22636577022014 40.0876863316868, -105.2263635879888 40.08768867359738, -105.22636140809533 40.08769101731477, -105.22635923639888 40.0876933637535, -105.22635706470228 40.08769571019219, -105.22635490002297 40.087698061150654, -105.22635273534713 40.08770041120849, -105.22635057769583 40.08770276398484, -105.22634842472385 40.08770511947421, -105.22634627408237 40.08770747857164, -105.2263441269622 40.087709836776675, -105.22634198100351 40.087712197686415, -105.22633984559444 40.08771455952174, -105.22633770782554 40.08771692495404, -105.22633557591215 40.08771929220145, -105.226333448689 40.087721659459945, -105.22633132497256 40.08772402942868, -105.22632920477012 40.08772640030627, -105.2263270845495 40.0877287756871, -105.22632497370938 40.08773115109006, -105.22632286637598 40.08773352920324, -105.2263207637256 40.08773590912882, -105.22631865989526 40.08773829085281, -105.22631656192405 40.08774067349134, -105.22631446745598 40.08774305974064, -105.22631238002324 40.087745446006664, -105.22631029727353 40.08774783408501, -105.22630821450556 40.08775022666651, -105.22630613526246 40.087752617455045, -105.2263040642092 40.08775501276614, -105.22630199199047 40.087757406273205, -105.22629992679262 40.08775980339941, -105.22629786627414 40.087762203238654, -105.22629580457564 40.08776460487633, -105.22629374990531 40.08776700833194, -105.22629169991798 40.087769413599865, -105.22628965696238 40.08777181978507, -105.22628761283043 40.08777422686813, -105.22628557454316 40.08777663846826, -105.2262835374175 40.087779052773016, -105.22628150850342 40.087781466196546, -105.22627948310692 40.0877838796284, -105.22627745768861 40.08778629846402, -105.22627543930565 40.087788717316265, -105.22627342443312 40.08779113797818, -105.22627141425073 40.0877935586511, -105.22626940522272 40.08779598382996, -105.22626740087406 40.08779841172184, -105.22626540590961 40.08780083873525, -105.2262634085889 40.08780326844501, -105.22626141830003 40.08780569907206, -105.22625943269774 40.0878081306108, -105.22625744590096 40.087810567550584, -105.22625546731582 40.087813003609114, -105.22625348989226 40.087815442372374, -105.22625151950771 40.08781788025156, -105.22624955497145 40.08782032174722, -105.22624758925161 40.087822765941944, -105.22624562704942 40.087825210144985, -105.2262436742169 40.08782765707216, -105.22624172372221 40.087830105806134, -105.22623977674515 40.08783255454839, -105.22623783326755 40.08783500780219, -105.22623589330765 40.08783746106425, -105.22623395685808 40.08783991613592, -105.22623202391895 40.087842373017146, -105.22623009918414 40.087844830818476, -105.22622817326574 40.087847291318866, -105.22622625437913 40.08784975273657, -105.22622434017549 40.08785221596659, -105.22622242830604 40.087854681904126, -105.2262205211268 40.087857147852716, -105.22621861627809 40.08785961740938, -105.22621671612326 40.08786208607652, -105.22621482182035 40.0878645574594, -105.2262129298625 40.08786702884783, -105.22621104374208 40.0878695065546, -105.22620916115385 40.08787198066713, -105.22620728088522 40.08787446108968, -105.22620540648671 40.08787693972477, -105.22620353442599 40.08787942016669, -105.22620166822081 40.087881902423774, -105.2261998043462 40.08788438828893, -105.226197947507 40.08788687417072, -105.226196091833 40.08788936185654, -105.22619423615886 40.087891849542366, -105.22619239454121 40.087894340864054, -105.22619055174354 40.08789683398418, -105.22618871128371 40.08789932891115, -105.22618687786292 40.08790182295415, -105.22618504559645 40.08790432150305, -105.22618322036178 40.087906820969245, -105.22618139747217 40.08790932044101, -105.22617957926549 40.087911821725115, -105.22617776457287 40.08791432391816, -105.22617595573219 40.08791682882699, -105.22617414805676 40.08791933553987, -105.22617234858203 40.08792184407345, -105.22617055027254 40.0879243544111, -105.22616875665327 40.08792686475982, -105.22616696888593 40.087929377824274, -105.22616517994956 40.08793188998534, -105.22616340154822 40.087934406674584, -105.22616162313946 40.08793692516508, -105.22615985059359 40.08793944366944, -105.22615808155446 40.08794196488402, -105.22615631720561 40.08794448610973, -105.22615455519815 40.087947008241606, -105.2261528013842 40.08794953399544, -105.22615104757375 40.08795205884863, -105.22614930077698 40.087954589122276, -105.2261475563434 40.08795711489833, -105.22614581657106 40.08795964789051, -105.22614408032358 40.087962179089786, -105.22614234758655 40.08796471209865, -105.22614062187763 40.08796724692545, -105.22613889966833 40.08796978626372, -105.22613718098748 40.08797232290842, -105.22613546582066 40.08797486046209, -105.22613375415338 40.08797740252725, -105.22613204600376 40.0879799446007, -105.22613034605126 40.087982489395564, -105.2261286460914 40.087985035991665, -105.22612695082901 40.08798758079754, -105.22612526023875 40.08799013011774, -105.22612357550771 40.08799268035245, -105.2261218943052 40.08799522789362, -105.22612021659137 40.08799778264812, -105.226118542406 40.08800033470907, -105.22611687640695 40.08800289219328, -105.22611520924964 40.08800544607216, -105.22611354910242 40.08800800627216, -105.22611189482893 40.088010563784096, -105.22611024053718 40.08801312579922, -105.2261085932736 40.08801568963229, -105.22610694953133 40.088018252573065, -105.22610530929944 40.088020817323425, -105.22610367258157 40.08802338298269, -105.22610204405721 40.08802595226398, -105.2261004178852 40.088028519749535, -105.22609879169858 40.088031090837625, -105.22609717606518 40.088033661950774, -105.22609556159335 40.08803623576855, -105.22609395063553 40.08803881049528, -105.22609234553337 40.08804138703718, -105.2260907451214 40.08804396359018, -105.22608914821626 40.088046542853405, -105.22608755365617 40.088049122122165, -105.2260859637863 40.088051701402065, -105.22608438093015 40.08805428610243, -105.22608279808112 40.08805686900151, -105.22608122226026 40.08805945371852, -105.22607964994621 40.0880620411458, -105.22607808466402 40.08806462949036, -105.22607651938526 40.088067216934235, -105.22607496112747 40.0880698079974, -105.22607340872892 40.088072399975005, -105.22607185749558 40.08807499375673, -105.22607030977991 40.08807758754672, -105.22606876909245 40.08808018315465, -105.22606722957744 40.08808277876541, -105.2260656970834 40.08808537799534, -105.22606416694163 40.088087975429545, -105.22606264147205 40.08809057737804, -105.22606112303788 40.08809317934323, -105.22605960342018 40.088095784007514, -105.2260580920141 40.08809838779062, -105.22605658412569 40.08810099158206, -105.2260550832546 40.0881035998933, -105.22605358237979 40.088106209105234, -105.22605208854043 40.08810881833376, -105.22605059938407 40.08811142937476, -105.22604911256549 40.08811404222255, -105.22604762809566 40.08811665417521, -105.22604615299197 40.08811926975269, -105.22604467671918 40.08812188442674, -105.22604320865081 40.088124500020854, -105.22604174291665 40.08812711832244, -105.2260402865523 40.08812973934819, -105.22603882901521 40.08813236037112, -105.22603737734094 40.088134981407954, -105.22603593035697 40.088137602455916, -105.22603448687256 40.088140228015355, -105.22603304456426 40.08814285267693, -105.22603161280553 40.08814547826421, -105.22603018337745 40.08814810745953, -105.22602897721418 40.088150328291526, -105.22607995110123 40.08815043483378, -105.22609517842363 40.08815046645809, -105.22599714643113 40.08825128178296, -105.22586659698402 40.08846589835929, -105.22586607995625 40.088466749142476, -105.22584420470254 40.088173450560355, -105.22584725593843 40.087025646900116, -105.22584725622484 40.08702557574974, -105.22584220450734 40.08612344890279, -105.22467120374027 40.08611344976358, -105.22468520457126 40.08554044892636, -105.22304620319824 40.08603244956893, -105.22198120395349 40.08618344991433, -105.22111620298946 40.08627444986659, -105.22112620324229 40.08639345027048, -105.21911380394884 40.0864074176304, -105.21824320274943 40.086413449711195, -105.21825320191593 40.087149450597536, -105.21636920232973 40.08714545077098, -105.21636020213397 40.08892145040806, -105.21632920225987 40.08892045018143, -105.21628020203916 40.08892045046189, -105.21597420248646 40.08892045011142, -105.21485883605443 40.08892679371123, -105.21480420216173 40.08892745043244, -105.21430020219961 40.08892245043239, -105.21343720139699 40.08892445097817, -105.21143620132462 40.088917451321855, -105.21029068492928 40.088917225001275, -105.21028926489139 40.08891722413985, -105.21028718232324 40.08891722341717, -105.2102854292613 40.08891722262064, -105.21028487813246 40.088917222138264, -105.20939024650113 40.08891684883024, -105.20845619971197 40.088916451022676, -105.2075245971012 40.08890693460845, -105.20694813190755 40.088905271061016, -105.20694386699977 40.088905292658566, -105.20697470751037 40.09435044215074, -105.20690820047578 40.094350750687866, -105.2067688747363 40.094351397550845, -105.20676923158804 40.09440878489543, -105.2067696857456 40.09448197611559, -105.20608429279402 40.09448027846468, -105.20406795434502 40.09447526321931, -105.20209254875405 40.094470721870664, -105.20040283465731 40.094471947312464, -105.20009424193184 40.09447216840297, -105.20004901645996 40.0944713051883, -105.19994314444023 40.09446928464906, -105.19615914431746 40.09444728514715, -105.19419214540423 40.094443284620404, -105.1914201445046 40.09443828540665, -105.18785514418282 40.09443028595678, -105.18785547428973 40.094424020152324, -105.18785813474778 40.09437345425398, -105.18785814372862 40.09437328585741, -105.1878579783739 40.094373286311026, -105.18785830846376 40.09436702410904, -105.18784899824328 40.09436703406432, -105.18693330943276 40.094368023246254, -105.18692882980451 40.09436799308698, -105.18649230894046 40.094365025363594, -105.18518230838691 40.09435602463465, -105.18518064301284 40.0943560507158, -105.18476919098173 40.09436254127205, -105.18476112982191 40.09436911199498, -105.1842981568986 40.094746444555966, -105.18422549731315 40.094805663306715, -105.17702895407928 40.101674977969125, -105.17630194996711 40.1023029683946, -105.16884176435845 40.108840617074065, -105.16857992781651 40.10901976085416, -105.16744391776132 40.11003576716704, -105.16145286636917 40.115280800079276, -105.16098215310839 40.115663211144835, -105.15946414128727 40.11689641328065, -105.15945664438176 40.11609286922273, -105.15946792166899 40.11419687283805, -105.15947182595067 40.11205812132699, -105.1594520114176 40.10922888777313, -105.15944955994391 40.10886022285561, -105.15942599180975 40.103991975428364, -105.1590781918603 40.10400245670831, -105.1588411915942 40.104266456712274, -105.15882019071795 40.10434845704976, -105.15890619108582 40.104508456925316, -105.15889919057865 40.10458445709242, -105.15872019085924 40.10476045668218, -105.15849819009142 40.10477145654381, -105.15818924132842 40.104903968720066, -105.15807619098169 40.10495245717316, -105.1576681914213 40.10507845747404, -105.15723219032265 40.10529845652795, -105.15712418985767 40.1053754563856, -105.15712419008531 40.10546345672344, -105.157253190884 40.10562845707536, -105.15723919112895 40.10571045628147, -105.15713819058196 40.10579245659894, -105.15699519001176 40.105820457235176, -105.15657972456523 40.106048569297116, -105.15641619045178 40.10613345690832, -105.15571518956787 40.10621545706669, -105.15537219002702 40.10630845692795, -105.15517819069753 40.10638545677693, -105.1551071895624 40.106484457227, -105.15498519058043 40.106583457491794, -105.15466319061927 40.10667645674386, -105.15437819008106 40.10669245702027, -105.15384819022479 40.10664345777509, -105.15368318932471 40.106698457290115, -105.15353319045201 40.106796456</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
@@ -5230,7 +5254,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2375256738388 40.21215340678842, -105.2375888474373 40.21217212200987, -105.2377480206275 40.21221503235984, -105.2379089947786 40.21225492766121, -105.2382531469907 40.21233394286283, -105.2385250718239 40.21238698984812, -105.2389598532161 40.21245605048926, -105.2391448655202 40.21248391907451, -105.2395378637989 40.21252100282268, -105.240173510697 40.21256054891217, -105.2408482261573 40.21254669878218, -105.2423982432625 40.21246822384897, -105.2474073989616 40.21216358484006, -105.247903562935 40.21215772257648, -105.2484720883204 40.21220687468774, -105.2489830403355 40.21228909895829, -105.2490570237534 40.2122288669131, -105.2490779310821 40.21209412592485, -105.2490779976944 40.21188192884601, -105.2490891004617 40.21168704868182, -105.2491009835694 40.2114748763219, -105.2491200218061 40.2098089020194, -105.2491280275432 40.20957997668, -105.2491321751882 40.20884401736242, -105.2491389223662 40.2081799869804, -105.2491333807267 40.20708123820636, -105.2491260963326 40.20563989481353, -105.2491801479699 40.20339134112944, -105.2491001417855 40.20209807572476, -105.2490920767794 40.20040294165154, -105.2490808384753 40.20005291412734, -105.2490950139939 40.19970403869323, -105.2491349610035 40.19935604322565, -105.2492060683551 40.19900399762389, -105.2492720560855 40.19868103844711, -105.2496240869759 40.19777206562981, -105.2501468398309 40.1963830630064, -105.2504429187537 40.19569192921944, -105.2506700671437 40.19505390214626, -105.2507571156221 40.19484189111984, -105.2509278441987 40.19426193885505, -105.2510480854168 40.19378289785566, -105.251128067233 40.19334906462623, -105.2511688587229 40.19306009015745, -105.2512250028661 40.19268412784863, -105.2512201714743 40.19263497988327, -105.2512620323328 40.19078100832103, -105.2512708366069 40.19042910076806, -105.2512728793419 40.19035992760917, -105.2513251593687 40.18996309454393, -105.2513631207729 40.18976195783753, -105.2514121452115 40.18956990345745, -105.2515640955329 40.18912798988486, -105.2516426020531 40.18896839177604, -105.2517701514606 40.18866999528589, -105.2519900848442 40.18823399108171, -105.2522378783861 40.18771486822919, -105.2523756349295 40.18726868919389, -105.2524306858087 40.18709861365252, -105.2524606485371 40.18691885300608, -105.2525121774577 40.18656573341248, -105.2525208785175 40.18647583827981, -105.2525354448402 40.18620143498161, -105.2525315881172 40.18583362634788, -105.25252934145 40.18530056583182, -105.2525274869419 40.18514736422271, -105.2525301556369 40.1844139431651, -105.2525387386828 40.18432283639816, -105.2525743946251 40.1840470074099, -105.2525871015199 40.18395590945979, -105.2526296788501 40.18376833747199, -105.2527498821734 40.18333912233531, -105.2529261180664 40.18280694304339, -105.253078039459 40.18236612398484, -105.2536550817977 40.18065905718701, -105.25399607556 40.17969212288935, -105.2541849888223 40.17931095061293, -105.2544031694233 40.1789509780611, -105.2545981255651 40.17867907468217, -105.2547901205846 40.17843406661363, -105.2548619788221 40.17835598276324, -105.2551550850433 40.17805793306881, -105.2556928485074 40.17759706368269, -105.2560998395208 40.17727509539263, -105.256597910034 40.1769019831392, -105.2571339000771 40.17653196732557, -105.257431974741 40.17634098240335, -105.2579258979518 40.17602303303983, -105.2583939445418 40.17573494924251, -105.2591858685164 40.17524192755577, -105.2594530698302 40.17507503079606, -105.2597788394861 40.17486134021356, -105.259922959592 40.17476800339525, -105.2600399027519 40.17468891115395, -105.2604919918168 40.17435411846151, -105.2609068910448 40.17400991380792, -105.2612528584729 40.17367736902041, -105.2620909815401 40.17280312307784, -105.2625181023224 40.17233595523951, -105.2629171714872 40.17190688544689, -105.2632979539897 40.17148711098977, -105.2634458414853 40.17132553280113, -105.2636880185539 40.17107202042472, -105.2645149025374 40.17017000768613, -105.2646969924993 40.16997794442383, -105.2648848620745 40.16976997030894, -105.2650239158626 40.16960499562783, -105.2653128738472 40.16924102830085, -105.2670169814966 40.16702008892292, -105.2674019019527 40.16652591484335, -105.2675319525281 40.16637409616335, -105.267672001252 40.16622806149554, -105.2678199086888 40.1660858863526, -105.2679738826939 40.16594811469322, -105.2684930394841 40.16553903173121, -105.2690879621946 40.16504911541169, -105.2692239839592 40.16492805261808, -105.2693550140677 40.16480203701695, -105.2695360148851 40.16460612085194, -105.2696765647454 40.16445430805851, -105.2697699267179 40.16432866903166, -105.2699209938069 40.16411297051584, -105.2699677086567 40.16403966533331, -105.2700942025796 40.16381552915902, -105.2701712615655 40.16366049756138, -105.2702622050297 40.16344048475487, -105.2703063148495 40.16332942592565, -105.2707200565537 40.16209085880443, -105.2709803253456 40.16122948468642, -105.2710548301344 40.16101992291283, -105.2711099679204 40.16087952757026, -105.2711760657257 40.16073076537894, -105.2712861215609 40.16051498378532, -105.2713878505979 40.16033693215146, -105.2715416293441 40.16012333346266, -105.2716459279216 40.15999352021721, -105.2717639621956 40.15984276360062, -105.271816077702 40.15978834202192, -105.2718956276797 40.15970251896657, -105.2719641835216 40.15963554698551, -105.2720272785671 40.15956646841252, -105.2720875916517 40.15951206197915, -105.2722970408633 40.15932307653537, -105.2723540731905 40.15928008986383, -105.2726151585096 40.15909503233883, -105.2731520029101 40.15872192448415, -105.2735568724613 40.15844106713092, -105.2738358838627 40.15824286475723, -105.2741450220795 40.15802193630074, -105.2742468856654 40.15794499676178, -105.2744588801126 40.15777987830076, -105.2746357770759 40.15761080747117, -105.2747344479813 40.15752711641187, -105.2748632858387 40.15741202752761, -105.2750305123632 40.15725926668, -105.2754225917291 40.15688255289814, -105.2758929495494 40.15644495979728, -105.2763959191594 40.15594704292194, -105.2766783327523 40.15567077309503, -105.2781341188324 40.15428111162556, -105.2785179368782 40.15391275991212, -105.2793160425854 40.15314803978234, -105.2794728569717 40.15300092477589, -105.280206041469 40.15228913282684, -105.280836947521 40.15167212428224, -105.2809808922424 40.1515200419104, -105.2811198405698 40.15136410597679, -105.2812509272502 40.15120513605844, -105.2813741570252 40.1510420334142, -105.2814298541274 40.15096500015037, -105.2815369705137 40.15080598366004, -105.2815880233071 40.15072702048, -105.281682976191 40.15056798085986, -105.2817290364374 40.15048406638984, -105.2817718698596 40.1504020677656, -105.2818528863331 40.15023806078776, -105.2819260558769 40.15006690229658, -105.2820759337992 40.1496241186037, -105.2821258875183 40.14944111154255, -105.2821458605589 40.14934808820088, -105.2822096587099 40.14892990318661, -105.2822448240156 40.14826998094643, -105.2822451208162 40.14784201323412, -105.2822360982994 40.14719606295897, -105.28224793464 40.14573292184287, -105.2822446240266 40.14535916374291, -105.2822411001326 40.14507407386814, -105.2822421489368 40.14497003421873, -105.2822531667241 40.14398591947473, -105.2822551592731 40.14347505101375, -105.2822708529094 40.14181206938772, -105.2822679484925 40.14104287330215, -105.2822709455559 40.14021796128176, -105.2822731345116 40.13942187166376, -105.2822689487237 40.13804709279694, -105.2822808526307 40.13667399035533, -105.2822871155677 40.13605798978642, -105.2822869464721 40.13488086839918, -105.2822721443784 40.13369411122954, -105.282278130057 40.13238193944374, -105.28227995875 40.13192213067715, -105.2823018622755 40.13100007518779, -105.2823158253697 40.13054797525448, -105.2823048796789 40.12994511718988, -105.2823079566542 40.1295421346564, -105.2823100945402 40.12932087953102, -105.2823240983905 40.12807295927798, -105.2823149319752 40.12680193517511, -105.2823230762417 40.12615601536589, -105.2823139370068 40.12565912601642, -105.2823120082232 40.12503212758082, -105.2823108265935 40.12473098201075, -105.2823129161732 40.12418909163625, -105.2823138398862 40.12412403384995, -105.2823120718964 40.12389398635925, -105.2823098954699 40.12368013430066, -105.2822998880501 40.12211290531759, -105.2823039641844 40.12106206847565, -105.2823001360619 40.11979901308963, -105.282302930207 40.11847804797252, -105.28230101788 40.11773410707254, -105.2822928495963 40.11704588145643, -105.2822928240271 40.11638292419469, -105.2822860850855 40.11569497494339, -105.2822921703681 40.1144629590239, -105.2822851112858 40.11342801985863, -105.2822329804653 40.1128470466918, -105.2821319186914 40.11202687618564, -105.2820480529635 40.1114200377739, -105.2820288722131 40.11126901713702, -105.282007019785 40.11112595402247, -105.281895999471 40.11033596102865, -105.2818530515338 40.11001497049595, -105.2818161192508 40.10960202947805, -105.28182207568 40.10885892394143, -105.2818538952916 40.10852407589721, -105.2820240687228 40.10696212396728, -105.2820620998125 40.10658501047332, -105.2821100589534 40.10623289769167, -105.2821429877803 40.10588597033826, -105.2821721304822 40.10538091547843, -105.2821711087647 40.10503008189505, -105.2821500312105 40.10435500626381, -105.2821380164751 40.10397587712918, -105.2820498498076 40.10248206645011, -105.2819991328603 40.10135096358122, -105.2819900265868 40.10106901821791, -105.2819782232338 40.10075949547533, -105.2816932183892 40.10171144787009, -105.2817202189721 40.10311144774851, -105.2812152187992 40.10407744786803, -105.2797872183302 40.10431644794893, -105.2794542187262 40.10443044801278, -105.2791212185347 40.10456344796724, -105.2787982178782 40.104725447886, -105.2784082179298 40.10496344875099, -105.2780752184868 40.10515344824243, -105.2777142184087 40.10525844880024, -105.2768772177547 40.10530344828223, -105.26893309262 40.10530965932736, -105.2586230328064 40.10531812044614, -105.2495202115298 40.10533244960861, -105.2493982119145 40.1052624508334, -105.2493152121548 40.10513744966269, -105.2493130142846 40.10492268834712, -105.2492812117193 40.10191044937188, -105.2492452117605 40.10183644999019, -105.249174211575 40.10177944987593, -105.249079210917 40.10174845048177, -105.2479753357009 40.10174426325229, -105.2460191671759 40.10173505168282, -105.2447240484117 40.10174391773126, -105.2400021278141 40.10171013062091, -105.2369722631745 40.10170266098098, -105.2313217846245 40.10169942310286, -105.2147332041786 40.10167545220847, -105.2126932031439 40.1016784526342, -105.2068932014407 40.10165445272636, -105.2069132020766 40.10763045329955, -105.2067782023472 40.10770645370304, -105.2063492015955 40.10784445371826, -105.2053482014456 40.10804245319163, -105.2043612024549 40.10813545392831, -105.2039462014829 40.10825645418945, -105.203467201412 40.10855845411498, -105.2030522015386 40.10873445440709, -105.2027592025271 40.10877245356505, -105.202637201805 40.10880545431794, -105.2021362010449 40.10918445388587, -105.2017722018164 40.10934945455519, -105.2013932011598 40.10940445475436, -105.2009562018202 40.10957545420762, -105.2006808951484 40.10965817306413, -105.2005202008154 40.10970645519306, -105.2002192006999 40.10978345477821, -105.1999912005688 40.1097504539375, -105.1997762011607 40.10978945421208, -105.1996332004896 40.10987145438538, -105.1994638415446 40.11011339692165, -105.1993252010489 40.11031145514585, -105.1991112014255 40.11049745450588, -105.1987392013178 40.1106684554918, -105.1984532000932 40.11072845482413, -105.1980452007163 40.11072845516461, -105.1978522003374 40.11065745427793, -105.1977522006899 40.11066845516529, -105.1974232003322 40.11090445495005, -105.1969652001717 40.11105245479959, -105.1966452380238 40.11135240469705, -105.1964147080669 40.11159028047116, -105.1963212002698 40.11168945582439, -105.1960992007815 40.11183845533019, -105.1953772000967 40.11216245484896, -105.1951632004082 40.11230545465229, -105.1950342005667 40.112552455237, -105.1948762005162 40.11269545465779, -105.1929294323047 40.11376950151904, -105.1910672884513 40.11491336443155, -105.1899691999933 40.115595455292, -105.1897331998464 40.11569945564447, -105.1892902001129 40.11582045598477, -105.1890751996802 40.11591345608336, -105.1888961995428 40.11596845552688, -105.1882521991136 40.11590845641862, -105.186961199186 40.11590745667103, -105.1863231985656 40.11585645599057, -105.1857061993235 40.1159434560531, -105.1849951982924 40.1162704558458, -105.1835731974845 40.11659745726456, -105.1832251983621 40.11659945655838, -105.1832146405067 40.11659945281932, -105.183214007166 40.1166821157796, -105.1832139548464 40.11744867340824, -105.1832138712203 40.11840196312736, -105.1832149465275 40.11870887570952, -105.1832148517188 40.11919010373395, -105.1832159800522 40.11979294537188, -105.183219146654 40.12034198721235, -105.183220100863 40.12198112826896, -105.1832278861207 40.12245990722899, -105.183221067644 40.12354093495674, -105.1832291403212 40.12380394395832, -105.1832329468866 40.12389280643219, -105.1832359130578 40.12396208391974, -105.1832360345671 40.1240128697098, -105.1832409714686 40.12448889466591, -105.1832478926514 40.12523010851267, -105.1832799848832 40.12709498627165, -105.183283047838 40.12728194015271, -105.1832850801665 40.12730610366077, -105.1832849779852 40.12732806464935, -105.1832840642105 40.12737088679798, -105.1832829024345 40.12739009972265, -105.1832821037178 40.12740794106342, -105.1832758462969 40.12744608143081, -105.1832688806296 40.1274831219725, -105.1832648585161 40.1275020532588, -105.1832601269916 40.12751988381583, -105.1832459824323 40.12756212029277, -105.1832390909328 40.12758296478057, -105.1832289697533 40.12760599617817, -105.183219937338 40.127626010706, -105.1832091004453 40.12764904103971, -105.1831968384394 40.12767096868016, -105.1831730413934 40.12771290397964, -105.1831309202504 40.12777290813871, -105.1830859705434 40.12782604072552, -105.1830669241476 40.12784602776817, -105.1830460833783 40.12786710866829, -105.1821979074391 40.12861201174101, -105.1811020789361 40.12954289682526, -105.1800941478542 40.13040813023044, -105.1800611061436 40.13043796166708, -105.1800399263207 40.13045492244582, -105.179986111736 40.13049100982777, -105.1799491668903 40.13051396662497, -105.1799089996035 40.13053801326528, -105.1798659835888 40.13055903124307, -105.1798219014639 40.13057894926776, -105.1797921646224 40.13059012217381, -105.1797309025309 40.130613011496, -105.1796850542687 40.13062798274787, -105.1796381489549 40.1306399311966, -105.1795891003167 40.13065105049456, -105.1795411344228 40.1306599761087, -105.1794921051437 40.13066697768263, -105.1794409400691 40.13067205133859, -105.179390857748 40.13067493221092, -105.1788589733049 40.13069212247468, -105.1788260618697 40.13069395205027, -105.1787938557948 40.13069798024438, -105.1787619985094 40.13070393137015, -105.1787301308545 40.13071207822432, -105.1786989738613 40.13072105023332, -105.1786699537986 40.13073195014857, -105.1786409233555 40.13074504669434, -105.1786140298435 40.13076007024781, -105.1785878532218 40.13077509578964, -105.1785641690483 40.13079204933064, -105.1785020389263 40.13084705429363, -105.1784840588681 40.13086786763377, -105.1784548908681 40.13091006260262, -105.178444049129 40.13093391475787, -105.1784339246554 40.13095694572148, -105.178427016947 40.13098108442205, -105.1784229738302 40.13100413231251, -105.1784189256439 40.1310280042764, -105.1784180942343 40.13105298307757, -105.1784131673081 40.13194404858856, -105.1783999480014 40.13330396605977, -105.1783991396833 40.1337020124477, -105.1784048791175 40.13377395099028, -105.1783991093832 40.13408688368758, -105.1783958547979 40.13492689429661, -105.1783961618531 40.13508913406532, -105.1783948972642 40.13528101768208, -105.1783940230415 40.13644990497878, -105.178390832764 40.13742799644631, -105.1783857569761 40.13792377194132, -105.1783856925215 40.13792375374909, -105.1783808185894 40.13938497043898, -105.178379409163 40.13975199673494, -105.1783763784656 40.14133788851696, -105.1783763779464 40.14133799839369, -105.1783713737261 40.14226699561438, -105.1783533903674 40.14336199241301, -105.1783493436875 40.14413299714823, -105.1783547608992 40.14414764583766, -105.178355161728 40.14414850346271, -105.1783513876863 40.14416088307052, -105.1783507230336 40.14416221146657, -105.1783483399981 40.14435999722787, -105.1783373495214 40.14522699350773, -105.178337307856 40.14535299840424, -105.1783402810778 40.14660499955411, -105.1783343699196 40.1478468345418, -105.1783342828933 40.1478649966097, -105.1783342685619 40.14786827670135, -105.1783322539086 40.14912099754154, -105.1783316896897 40.14922173345824, -105.1783252470594 40.15034799549664, -105.1783262111119 40.15130500003102, -105.1783232044195 40.15240999729076, -105.1783233146343 40.15242367651192, -105.1805269108048 40.15242303287242, -105.1810738976344 40.15242591632405, -105.1813111069034 40.15242108043596, -105.1815479915646 40.15240910559849, -105.1817820605489 40.15238806389035, -105.1818991075093 40.15237411100617, -105.1820401582139 40.15235308738404, -105.1821801553084 40.15232794206795, -105.1823190782533 40.15230306922523, -105.1824590841067 40.15227600253172, -105.182710112977 40.15222288694235, -105.1828730610242 40.15218600002028, -105.1837960656397 40.1519518970866, -105.1848938428551 40.1516740664099, -105.185371896122 40.15157407225121, -105.1858548713612 40.15149193386713, -105.1861809691329 40.15144999539257, -105.1864240035056 40.15142292895067, -105.1867460425639 40.15140788086975, -105.1879138398475 40.15143180934523, -105.1880670766908 40.15143204295714, -105.1885371158692 40.15143989897324, -105.1897880866419 40.15145287192772, -105.1900959985721 40.151475933974, -105.1901821651026 40.15148687092086, -105.1902690376092 40.15150000635485, -105.1903530437875 40.1515139572273, -105.1903607319016 40.15151567733403, -105.1903685580774 40.15151697721171, -105.190538671026 40.15155504178544, -105.1907855534298 40.15162515455555, -105.1915674105982 40.15190011247274, -105.1920345103337 40.15208391058577, -105.1923195534507 40.15218102474685, -105.1924195873322 40.15221093918417, -105.1926164532757 40.15226691445299, -105.1928106038957 40.15231163858869, -105.1930859740666 40.15235906840143, -105.1932719139723 40.15237905281442, -105.1933641729247 40.15238808249043, -105.1934589589035 40.1523919022945, -105.1936471026224 40.15239898939397, -105.1947339421019 40.15239912036138, -105.1962029102129 40.15238706996752, -105.1981951622453 40.15239887839329, -105.2003928214677 40.15239608689111, -105.2020348748597 40.15239895990317, -105.2020348288985 40.15240195080602, -105.2020503898697 40.15240197831892, -105.2020364487111 40.15329796080596, -105.2020315545417 40.15972599329237, -105.2020255745659 40.16223504358608, -105.2020374952001 40.16276176079394, -105.2027058313554 40.16275704228173, -105.2036568346699 40.16276607272876, -105.204275853226 40.1627610700721, -105.204402908596 40.16275288496949, -105.2047631678317 40.16276396317483, -105.2051190177064 40.16280193104347, -105.2054358230001 40.1628499557001, -105.2054430254445 40.16285171318667, -105.2054513405443 40.16285297365462, -105.2057594418307 40.16292815196992, -105.2060545441587 40.16303102252008, -105.2064695961106 40.16319706058182, -105.2075973484901 40.16370804603448, -105.2079663720258 40.16384596142348, -105.208471675034 40.16399492621811, -105.208893623721 40.16409073764115, -105.2092101207403 40.16414588869302, -105.2097719959188 40.16420302786118, -105.2102431262866 40.1642280930169, -105.210282876894 40.16421995723896, -105.2103348850135 40.16419098891262, -105.2103420726814 40.1641830452953, -105.2103480358364 40.16404305802597, -105.2103360596888 40.16366309970188, -105.2103399774529 40.16299494039553, -105.2103250511464 40.16271901622092, -105.2104577488688 40.16271186533191, -105.2114361647588 40.16273866730598, -105.2114551128682 40.16273858942343, -105.2114541918538 40.16265488641469, -105.2114481148706 40.16210100461468, -105.2114419251987 40.16153662826254, -105.2114357450743 40.1609733461614, -105.211445205626 40.16044074274905, -105.2114547518592 40.15990340125506, -105.2114574488354 40.1597515686144, -105.2114578971068 40.15970288667428, -105.2115128656631 40.15970204940688, -105.2129959093312 40.15969805573759, -105.2131941054505 40.15970211607535, -105.2133871679963 40.1597360861206, -105.2133888417895 40.15973666758005, -105.2134026840091 40.15973910300605, -105.2135523785454 40.15979108244539, -105.2137705244286 40.1599008801363, -105.2139196676629 40.1599989766702, -105.2161254215365 40.16163091588331, -105.2162534566525 40.16173005539297, -105.216346341859 40.16184997175485, -105.2163983841494 40.16198296504717, -105.2164085389799 40.16212189431283, -105.2163766429966 40.16316414840772, -105.216387570914 40.16346092516294, -105.216431672717 40.16352499570027, -105.2165033956429 40.16357211283747, -105.2165641148155 40.16359012498538, -105.2171229723248 40.16365794850347, -105.2187148516423 40.16374610977638, -105.2195718189001 40.16380646337711, -105.2204321459541 40.16385745212516, -105.2206711284977 40.1638702560757, -105.2214121380213 40.16387204453422, -105.221422562563 40.16387457162896, -105.2239583699097 40.16388294605247, -105.2239688546215 40.16386690553799, -105.2239736138655 40.1638596199467, -105.2239903532979 40.16383283986644, -105.2239967381509 40.16382214384298, -105.224006478519 40.1638058304559, -105.2240219812683 40.16377860250336, -105.2240368685532 40.16375116503207, -105.2240511192151 40.16372352519695, -105.2240647426128 40.16369569112624, -105.2240777304896 40.16366767270738, -105.2240900781249 40.16363947623385, -105.2241017796098 40.16361111159879, -105.2241128360789 40.16358258871198, -105.2241232416413 40.16355391296346, -105.224132990381 40.16352509604751, -105.2241420834434 40.16349614517214, -105.2241505172601 40.16346707203724, -105.2241582906471 40.16343787934208, -105.2241653964961 40.16340858328122, -105.2241718336194 40.16337918745454, -105.2241776054884 40.16334970447931, -105.2241827026874 40.16332014063767, -105.2241845717366 40.16330764065921, -105.2241871334015 40.16329050405493, -105.2241908870154 40.16326080731471, -105.2241939681854 40.16323106033524, -105.2241973377886 40.16318605095493, -105.2244350245367 40.16315723912725, -105.2244362919172 40.16316198219946, -105.2244505406456 40.16316025452517, -105.2245144242828 40.16339939613837, -105.2247082718298 40.16363382177953, -105.2249818257083 40.16381829563245, -105.2250694176052 40.16383585388203, -105.2256663557273 40.16406137494877, -105.2256678452306 40.16413216490754, -105.2256813243259 40.16477260883281, -105.2256817332005 40.16479202842404, -105.2256818750221 40.16479877993083, -105.2256824544149 40.16482453049973, -105.2256844243245 40.16491826169906, -105.2256687399535 40.16490737000433, -105.225622720551 40.1648754133671, -105.2255273023727 40.16482628226239, -105.2255231832839 40.16482913740503, -105.2254394076139 40.16488720419893, -105.2253676718974 40.16489314729116, -105.2252718835901 40.16493571068604, -105.2253115747242 40.16497248433775, -105.2252636187942 40.16500904877324, -105.2249923617757 40.16509398665386, -105.2248727425661 40.16511815425683, -105.2247611907744 40.16511788867045, -105.224616900968 40.16533150285289, -105.2242177806518 40.16550782979035, -105.2238574073118 40.16595322475723, -105.223744737093 40.16622804315812, -105.2233295249893 40.16644100787245, -105.2229617944719 40.16673355524715, -105.2225778264069 40.16709941839082, -105.2218992279499 40.16741566810365, -105.2218022828014 40.16773942785083, -105.2216584533702 40.16783689066961, -105.2216180871181 40.16796516832436, -105.2217120314581 40.16837497049304, -105.2216872504429 40.16858886861951, -105.2215353261218 40.16871687666976, -105.2210479242416 40.16903969442674, -105.2209834746498 40.1692107056338, -105.2209825970954 40.16942466038511, -105.2209958764451 40.17007267832358, -105.2209942464392 40.17075262017089, -105.2209490736238 40.17075454926682, -105.2209452379962 40.17104190494121, -105.2209180356501 40.17104304341818, -105.2209249631671 40.17173139885161, -105.219512780327 40.17280376660269, -105.2202794070359 40.173387901259, -105.2203808215655 40.17364716484659, -105.2202707784989 40.17381279293881, -105.2202205384567 40.1738884129844, -105.2201239077362 40.17409218918033, -105.2200646444332 40.17426452904852, -105.2200622293657 40.17426452049823, -105.2199974989101 40.17450224221455, -105.2198931450574 40.17468538125315, -105.2197173965499 40.17478887776263, -105.2196529129766 40.17496599973029, -105.2194693196962 40.17503891197926, -105.2193892751817 40.17512430056305, -105.2194203953364 40.17530776793799, -105.2195156725639 40.17539358200687, -105.2196648551878 40.17546273799122, -105.2199294170655 40.17555352473044, -105.2203508305605 40.17578684214399, -105.2203902489557 40.17589085907136, -105.2203499006629 40.17601302357969, -105.2202735353905 40.1761753142792, -105.2201016958975 40.17629362365332, -105.2200605406032 40.17661140311732, -105.2201717351685 40.17670336867613, -105.2207130981636 40.17683916514571, -105.2209343573538 40.17690254127866, -105.2209498823131 40.17690698826339, -105.2209504946826 40.17720104252477, -105.2209175212665 40.17730006248134, -105.2208566666041 40.17739105439566, -105.220836538589 40.17741214369109, -105.2202864008077 40.17777893666681, -105.220117488975 40.17786390172237, -105.2199974868583 40.17789106247914, -105.2195426020305 40.17789490160314, -105.2175685758577 40.17788213413407, -105.216856365463 40.17788807886922, -105.2164373552633 40.17787112952691, -105.2163563704421 40.17789591176385, -105.2162996166446 40.17794600901495, -105.2162775854453 40.17799399481255, -105.2162775095794 40.17809803506817, -105.2162777006156 40.17942503624364, -105.216273617755 40.18023209753913, -105.2163134477625 40.18029313762295, -105.2163764117413 40.18031928352345, -105.2166849032533 40.18035393351696, -105.2166895455905 40.18035572814999, -105.2167004241158 40.18035694995044, -105.2167654567252 40.18038209019546, -105.21681754217 40.18042202223454, -105.2168506187815 40.18047206505125, -105.2169225721429 40.18081208938658, -105.2170143693512 40.18128612529975, -105.2171034839595 40.18180297880132, -105.2170914202869 40.18186389070432, -105.2170475391566 40.18191594175241, -105.2169603850203 40.18195992434277, -105.2163825031335 40.18201396018677, -105.2163093738847 40.1820420561787, -105.2162565617191 40.18208996641057, -105.2162254934443 40.18215906787933, -105.2162394135021 40.18302601656777, -105.2162415586689 40.18336998753779, -105.2162474576582 40.18350012203573, -105.2162385578948 40.18494706245082, -105.2162274413648 40.18529511846879, -105.2160526679446 40.18840712538431, -105.216033405516 40.18881994646077, -105.213960586736 40.18881703375629, -105.2120463668134 40.18880706586764, -105.2106715156284 40.18880802608792, -105.2106335313511 40.18898609076457, -105.2103764342442 40.18993306751391, -105.2100266806441 40.19103408882624, -105.2098155691652 40.19177007906735, -105.2094995010301 40.1928580058869, -105.2091984259771 40.19395310690636, -105.2089045943898 40.19510999151015, -105.2087234233432 40.19578703355778, -105.2086683889593 40.1959321129289, -105.2086406928428 40.19596306273813, -105.2085663813553 40.19601201399413, -105.2084735664693 40.19603511362853, -105.2077883784565 40.19603914913586, -105.2068409687329 40.19602785289616, -105.2066462168588 40.19605606126178, -105.2065934459002 40.19614203326668, -105.206527519511 40.19646804000249, -105.2065626038541 40.1974629650888, -105.2065655638411 40.19818713874076, -105.2065583859549 40.19918689807859, -105.2065224613652 40.19921590544162, -105.2064985931352 40.20026695558668, -105.2064956698662 40.20119288167668, -105.2065113711813 40.20228301306435, -105.2065196370012 40.20302202312945, -105.2065364904466 40.20309892941081, -105.2065995211983 40.20317705162115, -105.2068616666747 40.20332512998329, -105.2070116247092 40.20341994212115, -105.2070843763297 40.20348600941636, -105.207198688632 40.20362794753153, -105.2078055144393 40.20488098724236, -105.2080324533654 40.20547588162022, -105.2081025518568 40.20565998188825, -105.2084465086051 40.20643689730729, -105.2085364254026 40.20675912839982, -105.2085486222509 40.20683712046804, -105.2085881819834 40.20693692902196, -105.2085893556908 40.20693989055246, -105.2093945645056 40.20694301537822, -105.2112200146598 40.20694785888084, -105.2112200355214 40.20694488324806, -105.2129239172751 40.20694692941765, -105.2199621309225 40.20695787201179, -105.2206720080944 40.20698402009077, -105.2216698920536 40.20706191673026, -105.222365973368 40.20713496297432, -105.2226039571625 40.20716188737166, -105.2230591107592 40.2072280379063, -105.2233811434875 40.20727712290655, -105.2244988414743 40.20747689105567, -105.2252869043162 40.20764896314754, -105.2254621852371 40.2076970623319, -105.2260648403674 40.20784708452415, -105.2269460153104 40.20810501482701, -105.2275589000377 40.2083041088891, -105.2278678296129 40.20840887609876, -105.2281760304196 40.20851693527186, -105.2287730572086 40.20874398709151, -105.2293639462556 40.20898501994377, -105.2302830739557 40.20933991590296, -105.2310638404985 40.20964589388696, -105.2324380127532 40.21019700803472, -105.2335340538425 40.21064287608376, -105.2343870825283 40.21097288085786, -105.2345150751825 40.21102203838161, -105.2358578961313 40.21154696105116, -105.2361328388671 40.21165107906058, -105.2366669525995 40.21186504393149, -105.2368178362817 40.21192111290259, -105.2369708710281 40.21197691277624, -105.2371249945898 40.21202887193505, -105.2374329106352 40.21212592518525, -105.2375256738388 40.21215340678842))</t>
+          <t>POLYGON ((-105.23752567383883 40.212153406788424, -105.23758884743732 40.21217212200987, -105.23774802062749 40.21221503235984, -105.23790899477856 40.212254927661206, -105.23825314699071 40.212333942862834, -105.2385250718239 40.21238698984812, -105.23895985321607 40.21245605048926, -105.23914486552019 40.212483919074515, -105.23953786379886 40.21252100282268, -105.240173510697 40.21256054891217, -105.24084822615734 40.212546698782184, -105.24239824326246 40.212468223848965, -105.24740739896158 40.212163584840056, -105.24790356293497 40.21215772257648, -105.24847208832041 40.21220687468774, -105.24898304033553 40.21228909895829, -105.24905702375341 40.2122288669131, -105.24907793108208 40.21209412592485, -105.2490779976944 40.21188192884601, -105.2490891004617 40.21168704868182, -105.24910098356943 40.2114748763219, -105.24912002180612 40.2098089020194, -105.2491280275432 40.20957997668, -105.24913217518815 40.20884401736242, -105.24913892236616 40.2081799869804, -105.24913338072672 40.20708123820636, -105.24912609633259 40.20563989481353, -105.2491801479699 40.20339134112944, -105.24910014178552 40.202098075724756, -105.24909207677945 40.20040294165154, -105.24908083847527 40.20005291412734, -105.24909501399388 40.19970403869323, -105.24913496100355 40.19935604322565, -105.24920606835512 40.19900399762389, -105.24927205608549 40.19868103844711, -105.24962408697591 40.19777206562981, -105.25014683983093 40.1963830630064, -105.25044291875372 40.195691929219436, -105.25067006714366 40.19505390214626, -105.25075711562205 40.19484189111984, -105.2509278441987 40.19426193885505, -105.25104808541684 40.19378289785566, -105.25112806723297 40.193349064626226, -105.25116885872289 40.193060090157445, -105.25122500286612 40.19268412784863, -105.25122017147434 40.19263497988327, -105.2512620323328 40.190781008321025, -105.25127083660695 40.190429100768064, -105.25127287934188 40.190359927609165, -105.2513251593687 40.18996309454393, -105.25136312077294 40.18976195783753, -105.25141214521155 40.189569903457446, -105.25156409553286 40.18912798988486, -105.25164260205308 40.18896839177604, -105.25177015146062 40.18866999528589, -105.25199008484422 40.18823399108171, -105.2522378783861 40.18771486822919, -105.25237563492948 40.18726868919389, -105.25243068580875 40.18709861365252, -105.25246064853708 40.186918853006084, -105.25251217745772 40.18656573341248, -105.2525208785175 40.18647583827981, -105.2525354448402 40.186201434981605, -105.25253158811724 40.18583362634788, -105.25252934144997 40.185300565831824, -105.25252748694194 40.185147364222715, -105.25253015563689 40.184413943165104, -105.25253873868276 40.18432283639816, -105.25257439462511 40.1840470074099, -105.25258710151986 40.18395590945979, -105.2526296788501 40.18376833747199, -105.25274988217338 40.18333912233531, -105.25292611806638 40.18280694304339, -105.25307803945898 40.18236612398484, -105.25365508179772 40.180659057187015, -105.25399607555995 40.17969212288935, -105.25418498882227 40.17931095061293, -105.25440316942334 40.178950978061096, -105.25459812556512 40.17867907468217, -105.25479012058462 40.17843406661363, -105.25486197882206 40.178355982763236, -105.25515508504331 40.17805793306881, -105.25569284850742 40.17759706368269, -105.25609983952084 40.17727509539263, -105.25659791003399 40.1769019831392, -105.25713390007712 40.17653196732557, -105.257431974741 40.176340982403346, -105.25792589795181 40.176023033039826, -105.25839394454181 40.17573494924251, -105.25918586851641 40.17524192755577, -105.25945306983019 40.17507503079606, -105.25977883948612 40.17486134021356, -105.25992295959198 40.17476800339525, -105.26003990275193 40.17468891115395, -105.26049199181676 40.17435411846151, -105.26090689104484 40.17400991380792, -105.26125285847287 40.17367736902041, -105.26209098154011 40.17280312307784, -105.26251810232243 40.17233595523951, -105.26291717148723 40.171906885446894, -105.26329795398969 40.17148711098977, -105.26344584148532 40.17132553280113, -105.26368801855388 40.17107202042472, -105.2645149025374 40.17017000768613, -105.26469699249932 40.16997794442383, -105.26488486207448 40.16976997030894, -105.26502391586264 40.16960499562783, -105.26531287384724 40.16924102830085, -105.2670169814966 40.16702008892292, -105.26740190195274 40.16652591484335, -105.26753195252806 40.166374096163345, -105.26767200125197 40.166228061495545, -105.26781990868882 40.1660858863526, -105.26797388269391 40.165948114693215, -105.26849303948407 40.16553903173121, -105.26908796219465 40.16504911541169, -105.26922398395921 40.16492805261808, -105.26935501406768 40.16480203701695, -105.26953601488509 40.164606120851936, -105.26967656474541 40.16445430805851, -105.26976992671794 40.16432866903166, -105.26992099380695 40.16411297051584, -105.26996770865674 40.164039665333306, -105.27009420257964 40.16381552915902, -105.27017126156548 40.16366049756138, -105.27026220502967 40.16344048475487, -105.27030631484952 40.16332942592565, -105.27072005655373 40.162090858804426, -105.27098032534559 40.161229484686416, -105.27105483013437 40.16101992291283, -105.2711099679204 40.16087952757026, -105.27117606572571 40.160730765378936, -105.27128612156093 40.16051498378532, -105.27138785059792 40.16033693215146, -105.27154162934409 40.160123333462664, -105.2716459279216 40.159993520217206, -105.27176396219562 40.15984276360062, -105.27181607770204 40.15978834202192, -105.27189562767965 40.15970251896657, -105.27196418352158 40.15963554698551, -105.27202727856711 40.15956646841252, -105.27208759165165 40.15951206197915, -105.27229704086332 40.15932307653537, -105.27235407319046 40.15928008986383, -105.27261515850964 40.15909503233883, -105.2731520029101 40.158721924484155, -105.27355687246131 40.15844106713092, -105.27383588386273 40.15824286475723, -105.27414502207954 40.15802193630074, -105.27424688566538 40.157944996761785, -105.2744588801126 40.15777987830076, -105.27463577707594 40.15761080747117, -105.27473444798133 40.15752711641187, -105.27486328583872 40.157412027527606, -105.2750305123632 40.15725926668, -105.27542259172907 40.15688255289814, -105.27589294954937 40.156444959797284, -105.27639591915941 40.15594704292194, -105.27667833275225 40.155670773095025, -105.27813411883237 40.154281111625565, -105.2785179368782 40.153912759912124, -105.2793160425854 40.15314803978234, -105.27947285697165 40.15300092477589, -105.28020604146903 40.15228913282684, -105.28083694752101 40.15167212428224, -105.28098089224238 40.1515200419104, -105.28111984056981 40.15136410597679, -105.28125092725021 40.15120513605844, -105.28137415702517 40.1510420334142, -105.28142985412744 40.15096500015037, -105.28153697051374 40.15080598366004, -105.28158802330708 40.15072702048, -105.28168297619095 40.15056798085986, -105.28172903643735 40.150484066389836, -105.28177186985958 40.150402067765604, -105.28185288633313 40.15023806078776, -105.28192605587692 40.15006690229658, -105.28207593379922 40.149624118603704, -105.28212588751835 40.14944111154255, -105.28214586055887 40.14934808820088, -105.28220965870989 40.14892990318661, -105.28224482401558 40.14826998094643, -105.28224512081617 40.14784201323412, -105.28223609829939 40.14719606295897, -105.28224793463998 40.14573292184287, -105.28224462402657 40.14535916374291, -105.28224110013257 40.14507407386814, -105.2822421489368 40.14497003421873, -105.28225316672409 40.14398591947473, -105.28225515927315 40.14347505101375, -105.28227085290936 40.14181206938772, -105.28226794849247 40.14104287330215, -105.28227094555592 40.140217961281756, -105.28227313451158 40.139421871663764, -105.28226894872374 40.13804709279694, -105.28228085263075 40.13667399035533, -105.28228711556771 40.136057989786416, -105.28228694647214 40.13488086839918, -105.2822721443784 40.133694111229545, -105.28227813005698 40.13238193944374, -105.28227995874995 40.131922130677154, -105.28230186227553 40.131000075187785, -105.2823158253697 40.13054797525448, -105.28230487967889 40.129945117189884, -105.28230795665418 40.1295421346564, -105.28231009454015 40.129320879531015, -105.28232409839048 40.12807295927798, -105.28231493197522 40.12680193517511, -105.28232307624171 40.12615601536589, -105.28231393700685 40.12565912601642, -105.28231200822316 40.12503212758082, -105.28231082659353 40.124730982010746, -105.2823129161732 40.124189091636254, -105.28231383988616 40.12412403384995, -105.2823120718964 40.12389398635925, -105.28230989546985 40.123680134300656, -105.28229988805006 40.12211290531759, -105.28230396418436 40.12106206847565, -105.28230013606188 40.11979901308963, -105.28230293020695 40.11847804797252, -105.28230101787997 40.11773410707254, -105.28229284959627 40.11704588145643, -105.28229282402707 40.11638292419469, -105.2822860850855 40.115694974943395, -105.28229217036812 40.114462959023896, -105.28228511128576 40.11342801985863, -105.28223298046527 40.1128470466918, -105.2821319186914 40.11202687618564, -105.28204805296349 40.111420037773904, -105.28202887221315 40.11126901713702, -105.28200701978501 40.11112595402247, -105.28189599947096 40.11033596102865, -105.28185305153379 40.11001497049595, -105.28181611925076 40.109602029478054, -105.28182207567998 40.108858923941426, -105.28185389529156 40.108524075897215, -105.28202406872283 40.10696212396728, -105.28206209981252 40.106585010473324, -105.28211005895342 40.10623289769167, -105.28214298778032 40.105885970338264, -105.28217213048217 40.10538091547843, -105.28217110876473 40.10503008189505, -105.28215003121048 40.10435500626381, -105.28213801647512 40.10397587712918, -105.28204984980758 40.102482066450115, -105.28199913286032 40.10135096358122, -105.28199002658675 40.101069018217906, -105.28197822323375 40.10075949547533, -105.28169321838922 40.10171144787009, -105.28172021897208 40.10311144774851, -105.2812152187992 40.10407744786803, -105.27978721833017 40.10431644794893, -105.27945421872622 40.10443044801278, -105.27912121853468 40.104563447967244, -105.2787982178782 40.104725447886, -105.2784082179298 40.104963448750986, -105.27807521848682 40.10515344824243, -105.27771421840869 40.10525844880024, -105.27687721775466 40.10530344828223, -105.26893309262 40.10530965932736, -105.25862303280643 40.10531812044614, -105.24952021152978 40.10533244960861, -105.24939821191451 40.1052624508334, -105.24931521215476 40.10513744966269, -105.24931301428464 40.104922688347116, -105.24928121171928 40.10191044937188, -105.24924521176052 40.10183644999019, -105.24917421157502 40.101779449875934, -105.24907921091696 40.10174845048177, -105.24797533570093 40.10174426325229, -105.24601916717593 40.101735051682816, -105.24472404841167 40.101743917731255, -105.24000212781411 40.10171013062091, -105.23697226317451 40.101702660980976, -105.23132178462454 40.101699423102865, -105.21473320417856 40.10167545220847, -105.21269320314391 40.1016784526342, -105.20689320144066 40.10165445272636, -105.20691320207663 40.10763045329955, -105.20677820234718 40.10770645370304, -105.20634920159554 40.10784445371826, -105.20534820144557 40.10804245319163, -105.20436120245495 40.108135453928305, -105.20394620148292 40.10825645418945, -105.203467201412 40.108558454114984, -105.2030522015386 40.10873445440709, -105.20275920252708 40.10877245356505, -105.20263720180502 40.10880545431794, -105.20213620104491 40.10918445388587, -105.2017722018164 40.109349454555186, -105.20139320115982 40.10940445475436, -105.20095620182019 40.109575454207615, -105.20068089514842 40.109658173064126, -105.20052020081545 40.10970645519306, -105.20021920069989 40.10978345477821, -105.19999120056882 40.1097504539375, -105.19977620116069 40.109789454212084, -105.19963320048963 40.10987145438538, -105.1994638415446 40.11011339692165, -105.19932520104891 40.11031145514585, -105.19911120142554 40.110497454505875, -105.19873920131776 40.110668455491805, -105.19845320009317 40.11072845482413, -105.19804520071632 40.11072845516461, -105.19785220033737 40.110657454277934, -105.19775220068986 40.11066845516529, -105.19742320033224 40.110904454950045, -105.19696520017166 40.11105245479959, -105.19664523802378 40.11135240469705, -105.19641470806688 40.111590280471155, -105.19632120026978 40.11168945582439, -105.19609920078153 40.11183845533019, -105.19537720009669 40.112162454848956, -105.19516320040816 40.11230545465229, -105.19503420056672 40.112552455237, -105.1948762005162 40.11269545465779, -105.19292943230472 40.11376950151904, -105.19106728845128 40.11491336443155, -105.18996919999327 40.115595455291995, -105.18973319984643 40.115699455644474, -105.1892902001129 40.115820455984775, -105.18907519968022 40.11591345608336, -105.18889619954282 40.115968455526875, -105.1882521991136 40.115908456418616, -105.186961199186 40.11590745667103, -105.1863231985656 40.115856455990574, -105.1857061993235 40.115943456053095, -105.18499519829243 40.1162704558458, -105.18357319748455 40.11659745726456, -105.18322519836212 40.116599456558376, -105.1832146405067 40.11659945281932, -105.18321400716599 40.116682115779604, -105.18321395484635 40.11744867340824, -105.18321387122035 40.11840196312736, -105.18321494652749 40.118708875709515, -105.18321485171883 40.11919010373395, -105.18321598005215 40.11979294537188, -105.18321914665395 40.12034198721235, -105.183220100863 40.12198112826896, -105.18322788612069 40.12245990722899, -105.183221067644 40.123540934956736, -105.18322914032119 40.12380394395832, -105.18323294688659 40.12389280643219, -105.18323591305776 40.123962083919736, -105.18323603456712 40.1240128697098, -105.18324097146863 40.12448889466591, -105.18324789265142 40.125230108512675, -105.18327998488321 40.12709498627165, -105.18328304783802 40.12728194015271, -105.18328508016651 40.12730610366077, -105.18328497798515 40.127328064649355, -105.18328406421048 40.127370886797976, -105.18328290243448 40.127390099722646, -105.1832821037178 40.12740794106342, -105.18327584629688 40.12744608143081, -105.18326888062958 40.1274831219725, -105.1832648585161 40.1275020532588, -105.18326012699163 40.12751988381583, -105.18324598243231 40.127562120292765, -105.18323909093279 40.127582964780565, -105.18322896975332 40.12760599617817, -105.18321993733795 40.127626010706, -105.18320910044525 40.12764904103971, -105.18319683843944 40.127670968680164, -105.18317304139345 40.12771290397964, -105.18313092025036 40.12777290813871, -105.18308597054336 40.12782604072552, -105.18306692414764 40.12784602776817, -105.18304608337829 40.12786710866829, -105.18219790743906 40.128612011741005, -105.18110207893609 40.129542896825264, -105.18009414785423 40.130408130230435, -105.18006110614358 40.130437961667084, -105.18003992632066 40.13045492244582, -105.179986111736 40.13049100982777, -105.17994916689032 40.130513966624974, -105.1799089996035 40.13053801326528, -105.17986598358878 40.130559031243074, -105.17982190146394 40.130578949267765, -105.17979216462236 40.13059012217381, -105.17973090253089 40.130613011496, -105.17968505426869 40.130627982747875, -105.17963814895494 40.1306399311966, -105.17958910031675 40.13065105049456, -105.1795411344228 40.130659976108696, -105.17949210514372 40.13066697768263, -105.17944094006911 40.13067205133859, -105.17939085774799 40.13067493221092, -105.1788589733049 40.130692122474684, -105.17882606186974 40.130693952050265, -105.17879385579481 40.130697980244385, -105.17876199850942 40.13070393137015, -105.17873013085455 40.13071207822432, -105.1786989738613 40.13072105023332, -105.17866995379858 40.13073195014857, -105.17864092335547 40.130745046694344, -105.17861402984349 40.13076007024781, -105.1785878532218 40.13077509578964, -105.17856416904833 40.13079204933064, -105.17850203892633 40.13084705429363, -105.1784840588681 40.13086786763377, -105.17845489086814 40.13091006260262, -105.17844404912896 40.13093391475787, -105.1784339246554 40.13095694572148, -105.17842701694698 40.130981084422054, -105.1784229738302 40.13100413231251, -105.17841892564394 40.1310280042764, -105.17841809423427 40.131052983077566, -105.17841316730812 40.13194404858856, -105.17839994800136 40.13330396605977, -105.17839913968335 40.1337020124477, -105.17840487911754 40.13377395099028, -105.17839910938315 40.13408688368758, -105.17839585479788 40.13492689429661, -105.17839616185312 40.13508913406532, -105.17839489726424 40.135281017682075, -105.17839402304146 40.13644990497878, -105.17839083276404 40.137427996446306, -105.17838575697611 40.137923771941324, -105.17838569252147 40.137923753749085, -105.17838081858942 40.139384970438975, -105.17837940916303 40.139751996734944, -105.17837637846564 40.141337888516965, -105.17837637794638 40.141337998393695, -105.1783713737261 40.14226699561438, -105.1783533903674 40.143361992413006, -105.17834934368746 40.144132997148226, -105.17835476089924 40.144147645837656, -105.17835516172805 40.14414850346271, -105.17835138768633 40.14416088307052, -105.17835072303357 40.14416221146657, -105.1783483399981 40.14435999722787, -105.17833734952136 40.14522699350773, -105.17833730785604 40.14535299840424, -105.1783402810778 40.14660499955411, -105.17833436991964 40.147846834541795, -105.17833428289335 40.1478649966097, -105.17833426856191 40.147868276701345, -105.1783322539086 40.14912099754154, -105.17833168968971 40.14922173345824, -105.17832524705936 40.15034799549664, -105.17832621111188 40.151305000031016, -105.17832320441953 40.15240999729076, -105.17832331463428 40.15242367651192, -105.18052691080484 40.15242303287242, -105.18107389763443 40.15242591632405, -105.18131110690341 40.15242108043596, -105.18154799156456 40.15240910559849, -105.18178206054885 40.15238806389035, -105.18189910750931 40.15237411100617, -105.18204015821385 40.152353087384036, -105.1821801553084 40.15232794206795, -105.18231907825327 40.15230306922523, -105.18245908410674 40.15227600253172, -105.18271011297703 40.15222288694235, -105.18287306102417 40.15218600002028, -105.18379606563974 40.151951897086605, -105.18489384285515 40.151674066409896, -105.18537189612198 40.15157407225121, -105.1858548713612 40.151491933867135, -105.18618096913295 40.151449995392575, -105.18642400350559 40.151422928950666, -105.1867460425639 40.151407880869755, -105.1879138398475 40.151431809345226, -105.18806707669081 40.15143204295714, -105.1885371158692 40.15143989897324, -105.18978808664193 40.151452871927724, -105.19009599857208 40.151475933974, -105.19018216510263 40.15148687092086, -105.19026903760924 40.15150000635485, -105.19035304378754 40.1515139572273, -105.19036073190159 40.15151567733403, -105.19036855807735 40.151516977211706, -105.19053867102599 40.15155504178544, -105.19078555342985 40.151625154555546, -105.19156741059824 40.15190011247274, -105.19203451033374 40.15208391058577, -105.19231955345072 40.152181024746845, -105.19241958733224 40.152210939184165, -105.19261645327569 40.152266914452994, -105.19281060389568 40.15231163858869, -105.19308597406658 40.15235906840143, -105.19327191397227 40.152379052814425, -105.19336417292473 40.152388082490425, -105.1934589589035 40.1523919022945, -105.19364710262239 40.152398989393966, -105.19473394210193 40.15239912036138, -105.19620291021289 40.15238706996752, -105.1981951622453 40.15239887839329, -105.20039282146774 40.15239608689111, -105.2020348748597 40.15239895990317, -105.2020348288985 40.15240195080602, -105.2020503898697 40.15240197831892, -105.20203644871107 40.153297960805965, -105.20203155454175 40.15972599329237, -105.20202557456592 40.16223504358608, -105.20203749520009 40.16276176079394, -105.20270583135539 40.162757042281726, -105.20365683466991 40.16276607272876, -105.204275853226 40.1627610700721, -105.204402908596 40.162752884969485, -105.20476316783173 40.16276396317483, -105.20511901770635 40.16280193104347, -105.20543582300013 40.1628499557001, -105.20544302544447 40.16285171318667, -105.20545134054429 40.16285297365462, -105.20575944183071 40.16292815196992, -105.2060545441587 40.16303102252008, -105.20646959611061 40.16319706058182, -105.20759734849008 40.16370804603448, -105.2079663720258 40.16384596142348, -105.20847167503396 40.16399492621811, -105.20889362372097 40.164090737641146, -105.20921012074034 40.16414588869302, -105.20977199591883 40.16420302786118, -105.21024312628657 40.1642280930169, -105.21028287689401 40.164219957238956, -105.21033488501352 40.164190988912615, -105.2103420726814 40.164183045295296, -105.21034803583642 40.164043058025975, -105.21033605968876 40.16366309970188, -105.21033997745286 40.16299494039553, -105.21032505114643 40.16271901622092, -105.21045774886878 40.162711865331914, -105.21143616475884 40.16273866730598, -105.21145511286817 40.162738589423434, -105.21145419185379 40.162654886414686, -105.21144811487062 40.162101004614684, -105.21144192519867 40.16153662826254, -105.21143574507434 40.1609733461614, -105.21144520562605 40.160440742749046, -105.21145475185916 40.159903401255065, -105.21145744883538 40.1597515686144, -105.21145789710683 40.15970288667428, -105.21151286566307 40.15970204940688, -105.2129959093312 40.159698055737586, -105.2131941054505 40.15970211607535, -105.21338716799629 40.1597360861206, -105.21338884178945 40.15973666758005, -105.21340268400907 40.159739103006046, -105.21355237854544 40.15979108244539, -105.21377052442864 40.1599008801363, -105.2139196676629 40.1599989766702, -105.2161254215365 40.16163091588331, -105.21625345665245 40.161730055392965, -105.21634634185902 40.161849971754854, -105.21639838414941 40.161982965047166, -105.21640853897992 40.16212189431283, -105.21637664299655 40.16316414840772, -105.21638757091395 40.163460925162944, -105.216431672717 40.16352499570027, -105.21650339564287 40.16357211283747, -105.2165641148155 40.16359012498538, -105.21712297232476 40.16365794850347, -105.21871485164235 40.163746109776376, -105.21957181890005 40.163806463377114, -105.22043214595409 40.16385745212516, -105.22067112849773 40.163870256075704, -105.22141213802132 40.163872044534216, -105.22142256256299 40.16387457162896, -105.2239583699097 40.163882946052475, -105.22396885462149 40.163866905537986, -105.2239736138655 40.1638596199467, -105.22399035329788 40.16383283986644, -105.22399673815093 40.16382214384298, -105.22400647851899 40.1638058304559, -105.2240219812683 40.163778602503356, -105.22403686855324 40.163751165032075, -105.2240511192151 40.16372352519695, -105.2240647426128 40.163695691126236, -105.22407773048955 40.163667672707376, -105.22409007812487 40.16363947623385, -105.22410177960984 40.16361111159879, -105.22411283607892 40.163582588711975, -105.22412324164132 40.16355391296346, -105.22413299038101 40.163525096047515, -105.22414208344337 40.16349614517214, -105.22415051726007 40.16346707203724, -105.22415829064705 40.163437879342084, -105.22416539649606 40.163408583281225, -105.22417183361935 40.16337918745454, -105.22417760548844 40.16334970447931, -105.22418270268737 40.163320140637666, -105.22418457173661 40.16330764065921, -105.22418713340147 40.16329050405493, -105.22419088701537 40.16326080731471, -105.22419396818545 40.163231060335235, -105.2241973377886 40.163186050954934, -105.22443502453667 40.16315723912725, -105.2244362919172 40.16316198219946, -105.22445054064558 40.16316025452517, -105.22451442428284 40.16339939613837, -105.22470827182981 40.16363382177953, -105.22498182570828 40.163818295632446, -105.2250694176052 40.16383585388203, -105.2256663557273 40.164061374948766, -105.22566784523062 40.164132164907535, -105.22568132432586 40.16477260883281, -105.2256817332005 40.16479202842404, -105.22568187502212 40.164798779930834, -105.22568245441485 40.16482453049973, -105.22568442432446 40.164918261699064, -105.2256687399535 40.16490737000433, -105.22562272055102 40.1648754133671, -105.22552730237273 40.16482628226239, -105.2255231832839 40.16482913740503, -105.22543940761388 40.164887204198926, -105.22536767189742 40.16489314729116, -105.22527188359014 40.16493571068604, -105.22531157472422 40.164972484337746, -105.22526361879424 40.165009048773236, -105.22499236177575 40.16509398665386, -105.2248727425661 40.16511815425683, -105.2247611907744 40.16511788867045, -105.22461690096799 40.165331502852894, -105.22421778065177 40.16550782979035, -105.22385740731184 40.16595322475723, -105.22374473709303 40.16622804315812, -105.2233295249893 40.16644100787245, -105.22296179447193 40.16673355524715, -105.22257782640692 40.16709941839082, -105.22189922794989 40.16741566810365, -105.22180228280136 40.16773942785083, -105.22165845337022 40.16783689066961, -105.22161808711809 40.167965168324365, -105.22171203145805 40.16837497049304, -105.22168725044288 40.16858886861951, -105.22153532612177 40.16871687666976, -105.2210479242416 40.169039694426736, -105.22098347464978 40.1692107056338, -105.22098259709541 40.16942466038511, -105.22099587644509 40.17007267832358, -105.22099424643919 40.170752620170894, -105.22094907362384 40.170754549266825, -105.22094523799618 40.171041904941205, -105.22091803565013 40.17104304341818, -105.22092496316705 40.17173139885161, -105.21951278032704 40.17280376660269, -105.2202794070359 40.173387901259, -105.22038082156554 40.173647164846585, -105.22027077849893 40.17381279293881, -105.2202205384567 40.1738884129844, -105.22012390773622 40.17409218918033, -105.22006464443322 40.17426452904852, -105.22006222936565 40.174264520498234, -105.21999749891012 40.17450224221455, -105.21989314505738 40.17468538125315, -105.21971739654985 40.17478887776263, -105.21965291297658 40.17496599973029, -105.21946931969619 40.175038911979264, -105.21938927518171 40.17512430056305, -105.21942039533639 40.175307767937994, -105.21951567256394 40.17539358200687, -105.21966485518782 40.17546273799122, -105.21992941706546 40.17555352473044, -105.22035083056055 40.17578684214399, -105.22039024895572 40.17589085907136, -105.22034990066287 40.17601302357969, -105.22027353539048 40.1761753142792, -105.22010169589748 40.176293623653315, -105.2200605406032 40.17661140311732, -105.22017173516849 40.17670336867613, -105.22071309816359 40.17683916514571, -105.22093435735384 40.17690254127866, -105.22094988231315 40.17690698826339, -105.22095049468263 40.17720104252477, -105.22091752126646 40.177300062481336, -105.22085666660412 40.177391054395656, -105.220836538589 40.177412143691086, -105.22028640080765 40.17777893666681, -105.22011748897503 40.17786390172237, -105.2199974868583 40.17789106247914, -105.21954260203049 40.17789490160314, -105.21756857585765 40.17788213413407, -105.21685636546304 40.17788807886922, -105.21643735526327 40.17787112952691, -105.21635637044214 40.17789591176385, -105.21629961664465 40.177946009014946, -105.2162775854453 40.17799399481255, -105.21627750957944 40.178098035068174, -105.21627770061565 40.179425036243636, -105.21627361775495 40.180232097539125, -105.21631344776249 40.180293137622954, -105.21637641174132 40.18031928352345, -105.21668490325334 40.18035393351696, -105.21668954559047 40.18035572814999, -105.2167004241158 40.18035694995044, -105.21676545672523 40.18038209019546, -105.21681754217005 40.180422022234545, -105.21685061878149 40.18047206505125, -105.21692257214292 40.18081208938658, -105.21701436935116 40.18128612529975, -105.21710348395955 40.18180297880132, -105.21709142028692 40.18186389070432, -105.21704753915661 40.18191594175241, -105.21696038502029 40.18195992434277, -105.21638250313354 40.18201396018677, -105.2163093738847 40.1820420561787, -105.21625656171906 40.182089966410565, -105.21622549344433 40.182159067879326, -105.21623941350211 40.18302601656777, -105.21624155866891 40.18336998753779, -105.21624745765817 40.18350012203573, -105.21623855789477 40.18494706245082, -105.2162274413648 40.185295118468794, -105.21605266794457 40.18840712538431, -105.21603340551596 40.18881994646077, -105.21396058673602 40.188817033756294, -105.21204636681338 40.18880706586764, -105.21067151562845 40.18880802608792, -105.21063353135115 40.18898609076457, -105.21037643424418 40.18993306751391, -105.21002668064415 40.191034088826235, -105.20981556916516 40.19177007906735, -105.20949950103007 40.1928580058869, -105.2091984259771 40.193953106906356, -105.20890459438984 40.19510999151015, -105.20872342334322 40.19578703355778, -105.20866838895932 40.1959321129289, -105.20864069284279 40.19596306273813, -105.2085663813553 40.19601201399413, -105.20847356646934 40.196035113628525, -105.20778837845648 40.19603914913586, -105.20684096873286 40.19602785289616, -105.20664621685884 40.19605606126178, -105.20659344590024 40.19614203326668, -105.20652751951104 40.196468040002486, -105.20656260385412 40.197462965088796, -105.20656556384107 40.19818713874076, -105.20655838595488 40.19918689807859, -105.20652246136521 40.19921590544162, -105.2064985931352 40.200266955586685, -105.20649566986617 40.201192881676675, -105.20651137118128 40.202283013064346, -105.20651963700115 40.20302202312945, -105.20653649044662 40.203098929410814, -105.20659952119827 40.203177051621154, -105.2068616666747 40.20332512998329, -105.20701162470917 40.20341994212115, -105.20708437632969 40.20348600941636, -105.20719868863205 40.20362794753153, -105.20780551443931 40.20488098724236, -105.20803245336536 40.20547588162022, -105.20810255185675 40.20565998188825, -105.20844650860509 40.20643689730729, -105.20853642540263 40.206759128399824, -105.20854862225086 40.206837120468045, -105.2085881819834 40.20693692902196, -105.20858935569078 40.206939890552455, -105.20939456450559 40.206943015378215, -105.21122001465984 40.20694785888084, -105.21122003552136 40.206944883248056, -105.21292391727515 40.206946929417654, -105.2199621309225 40.20695787201179, -105.22067200809443 40.20698402009077, -105.22166989205364 40.20706191673026, -105.22236597336799 40.20713496297432, -105.22260395716248 40.20716188737166, -105.22305911075921 40.207228037906305, -105.22338114348749 40.20727712290655, -105.22449884147427 40.20747689105567, -105.22528690431616 40.20764896314754, -105.22546218523715 40.207697062331896, -105.22606484036743 40.20784708452415, -105.22694601531043 40.20810501482701, -105.22755890003775 40.2083041088891, -105.22786782961292 40.20840887609876, -105.22817603041958 40.20851693527186, -105.22877305720863 40.20874398709151, -105.22936394625565 40.20898501994377, -105.23028307395569 40.20933991590296, -105.23106384049854 40.209645893886965, -105.23243801275325 40.21019700803472, -105.23353405384255 40.21064287608376, -105.23438708252829 40.21097288085786, -105.23451507518247 40.211022038381614, -105.23585789613134 40.21154696105116, -105.23613283886706 40.21165107906058, -105.23666695259946 40.21186504393149, -105.23681783628166 40.21192111290259, -105.23697087102813 40.21197691277624, -105.23712499458976 40.21202887193505, -105.2374329106352 40.212125925185255, -105.23752567383883 40.212153406788424))</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
@@ -5272,7 +5296,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1590573513478 40.26121887960556, -105.1590573570404 40.26121891654797, -105.1590924124816 40.26122587265385, -105.1681541115292 40.26127286014907, -105.1681541609035 40.26127286029062, -105.1776300395872 40.26125226577008, -105.1776370908802 40.26125225028417, -105.1799331642954 40.26124727972221, -105.1809020336891 40.26124516797755, -105.1826989240208 40.26124123121768, -105.182705897719 40.26124121611084, -105.1845310811603 40.261237189768, -105.1845380266437 40.26123717447391, -105.1856946342339 40.26123460648543, -105.1857015632586 40.26123459107681, -105.1871193884505 40.26123187397589, -105.1873425473743 40.26123992604474, -105.1934085797967 40.26139700742055, -105.1934155690683 40.26139719074749, -105.1955078148134 40.26145209028402, -105.1955147758784 40.26145227431058, -105.1959353715118 40.26146337597554, -105.1974555694628 40.26067608537934, -105.1981464893336 40.26019411223952, -105.1990088615929 40.26006109067797, -105.1994597387419 40.25978578531463, -105.1997792681634 40.25962927023967, -105.1999761854271 40.2593262239081, -105.2000207747857 40.25904261606559, -105.2000748644785 40.25869858566038, -105.2008642821137 40.25762519302322, -105.2013873248839 40.25726290962486, -105.2014730596705 40.25693086456624, -105.2016532792466 40.25656638298578, -105.2020937188124 40.25649088340332, -105.2020985102739 40.25649006175851, -105.2026035359551 40.25667050722171, -105.2026072283505 40.25667182621633, -105.2028660107326 40.25670894541448, -105.20353402528 40.25655572234178, -105.2039280948155 40.25651146572446, -105.2039386748967 40.25651027784723, -105.204213565107 40.25674349021606, -105.2050861937948 40.25744193061791, -105.2050873125373 40.25744282598645, -105.2061453886893 40.25759856552384, -105.2061584405259 40.25760048636711, -105.2064410225062 40.25772515264362, -105.2067436942732 40.25788085597899, -105.2070114768788 40.25814245286414, -105.2073081950761 40.25828511842026, -105.207621112189 40.25839094630618, -105.2076312940399 40.25839438989173, -105.2081977342884 40.25834933817321, -105.2088859767249 40.25819613524021, -105.2094740958972 40.25781027378541, -105.2094472990344 40.25666285004529, -105.2094966629434 40.25645434180458, -105.2094348585935 40.25613018100962, -105.2095185749566 40.25587714568412, -105.2096715968779 40.25550883050449, -105.2101540955547 40.25553376227379, -105.2105702983742 40.25549455045693, -105.2109450285866 40.25528918197753, -105.2124903087098 40.25479991430108, -105.2128932706567 40.25463280689722, -105.2133718730392 40.25413205482123, -105.2164030018444 40.25062630659323, -105.216594930966 40.25041072509776, -105.2172405545028 40.24954584877566, -105.2175493089082 40.2491024012631, -105.21782169094 40.24849392203895, -105.2184710561619 40.24749196008531, -105.2192062160137 40.2472627512926, -105.2201614200856 40.24636299751891, -105.2213179325129 40.2455953056567, -105.2217295278817 40.24552875557625, -105.2217322305576 40.24552831896781, -105.2219590939805 40.24558935384183, -105.2222685939753 40.24579925097038, -105.2225539755656 40.24590701172082, -105.222561076526 40.24590969279355, -105.2234132855202 40.24594345550864, -105.2242533468189 40.2459686081519, -105.2248804827458 40.24603755400981, -105.2249795242437 40.24604104248748, -105.2251246908747 40.24603598724892, -105.225124418846 40.24601403657721, -105.2251246544638 40.24597612984243, -105.2251264416318 40.24569094225593, -105.2251396946851 40.24516006982153, -105.2251486824313 40.24373510434809, -105.2251655874775 40.2430098863984, -105.2251615362667 40.2422401475095, -105.2251897075283 40.24014596842481, -105.2251923741208 40.23939793128302, -105.2251866361226 40.23931089739514, -105.2251535915836 40.23915599503675, -105.2250724245328 40.23894305548698, -105.2249646736965 40.23874899464865, -105.2248367108495 40.23859304245457, -105.2241133670372 40.23792014026026, -105.2232375815495 40.23712608323071, -105.2228576305124 40.23675211280806, -105.2225646450352 40.23639701604122, -105.2223025250875 40.23602799325127, -105.2220385404729 40.23559006293472, -105.2218776819986 40.23524790936244, -105.2217555450768 40.23489706395679, -105.2214424586468 40.23368214613465, -105.2211684457862 40.23246210583308, -105.2210345366483 40.2318400144956, -105.2209816135649 40.23147011913398, -105.2209614313443 40.23097704736698, -105.2209775112241 40.23054994659705, -105.2210286816048 40.23012512524188, -105.2210955580444 40.22979999070917, -105.2212345738807 40.22935094963212, -105.221414383736 40.22890996814414, -105.2222733670456 40.22721088304503, -105.2223926121098 40.22695202984121, -105.2224814427476 40.22668596697582, -105.2224955826586 40.22655588179951, -105.2224944949933 40.22629591658432, -105.222456515767 40.22603696072321, -105.2223816240407 40.22578395587376, -105.2218874003409 40.22482087832691, -105.2217915851812 40.22460597964299, -105.2217183566255 40.22438509649398, -105.2216694950232 40.22416097651936, -105.2215166074621 40.22266698865904, -105.2214566169285 40.22183809224568, -105.2214886997248 40.22161197213887, -105.2215605121959 40.22139088759893, -105.2216734602475 40.22118088335245, -105.22180667625 40.22100606485856, -105.2219666573605 40.2208540955447, -105.2221534169228 40.22072113145052, -105.222364429915 40.22061210723617, -105.2225936070471 40.22052700996868, -105.2240474735757 40.22018597437552, -105.2253873846429 40.21986938401997, -105.2280896387928 40.2192320089863, -105.2290855042023 40.21896504863379, -105.2293046641618 40.2188741496954, -105.2295013646164 40.21875794149326, -105.2296734424702 40.21861999007856, -105.2298155142526 40.21846302630055, -105.2299595982937 40.21825006684786, -105.2300426830196 40.21806798432373, -105.2300704882472 40.21796439404318, -105.2300946371679 40.21788006507707, -105.2301086331605 40.2177820967097, -105.2301247091618 40.21652898563659, -105.23012845509 40.2158558903383, -105.2301415094318 40.21500301146425, -105.2301383637466 40.21435213555789, -105.2301504808107 40.21409604375543, -105.2301595522665 40.21163011961929, -105.2301555092061 40.21102508422261, -105.2301400093207 40.21102641251364, -105.2301399807453 40.21102206961, -105.2298742263724 40.2110448449103, -105.2294503923334 40.2111467971645, -105.2291590513998 40.21144800191435, -105.2283698152349 40.21187514808197, -105.2278753854815 40.21200919831927, -105.2277120368063 40.21224963597185, -105.2274482307357 40.21257208671688, -105.2271019703582 40.21278312088065, -105.2269009936536 40.21294153470387, -105.2268313582051 40.21307907293179, -105.2267408484977 40.21325363531842, -105.225738529839 40.21340485457109, -105.2249787260143 40.21337656924641, -105.2243483967612 40.21378817767526, -105.2239268180089 40.21382954143416, -105.2226893202231 40.21404902495213, -105.2219218867605 40.21419547745586, -105.2212997430297 40.21428931261474, -105.2209471547051 40.21435201814516, -105.2206776411029 40.21437255222598, -105.2195818740997 40.21424732969597, -105.2194172439189 40.21430823721885, -105.2193320750478 40.21449194906986, -105.2189844220926 40.21466419967764, -105.2187624035569 40.21473579059544, -105.2184958329167 40.21472540903732, -105.2183256146939 40.21453675764475, -105.2181220301564 40.21434893702349, -105.2177850704482 40.21418463216135, -105.2175902741623 40.21402067260001, -105.217510888195 40.21388083699802, -105.2170715816219 40.21375715061206, -105.2170678516254 40.21375745580795, -105.2155783456237 40.21387950723339, -105.2144270717195 40.21402993613065, -105.2136454313024 40.21396669689456, -105.2124598923856 40.21381389636853, -105.2124572607502 40.21381254158332, -105.2121407184077 40.21364961832136, -105.2121271137522 40.21364759136831, -105.2121251901466 40.21364660129154, -105.2115799573767 40.21356536342635, -105.2111923353717 40.21341104953922, -105.2111936954968 40.21334806106676, -105.2111714408698 40.21319208211123, -105.2111796372598 40.21278005888963, -105.2111863566922 40.21220991280554, -105.211211532736 40.20889605807057, -105.2112276320728 40.20805608894247, -105.2112355622117 40.20694790040265, -105.2112200146598 40.20694785888084, -105.2093945645056 40.20694301537822, -105.2085893556908 40.20693989055246, -105.2085881819834 40.20693692902196, -105.2085486222509 40.20683712046804, -105.2085364254026 40.20675912839982, -105.2084465086051 40.20643689730729, -105.2081025518568 40.20565998188825, -105.2080324533654 40.20547588162022, -105.2078055144393 40.20488098724236, -105.207198688632 40.20362794753153, -105.2070843763297 40.20348600941636, -105.2070116247092 40.20341994212115, -105.2068616666747 40.20332512998329, -105.2065995211983 40.20317705162115, -105.2065364904466 40.20309892941081, -105.2065196370012 40.20302202312945, -105.2065113711813 40.20228301306435, -105.2064956698662 40.20119288167668, -105.2064985931352 40.20026695558668, -105.2065224613652 40.19921590544162, -105.2065583859549 40.19918689807859, -105.2065655638411 40.19818713874076, -105.2065626038541 40.1974629650888, -105.206527519511 40.19646804000249, -105.2065934459002 40.19614203326668, -105.2066462168588 40.19605606126178, -105.2068409687329 40.19602785289616, -105.2077883784565 40.19603914913586, -105.2084735664693 40.19603511362853, -105.2085663813553 40.19601201399413, -105.2086406928428 40.19596306273813, -105.2086683889593 40.1959321129289, -105.2087234233432 40.19578703355778, -105.2089045943898 40.19510999151015, -105.2091984259771 40.19395310690636, -105.2094995010301 40.1928580058869, -105.2098155691652 40.19177007906735, -105.2100266806441 40.19103408882624, -105.2103764342442 40.18993306751391, -105.2106335313511 40.18898609076457, -105.2106715156284 40.18880802608792, -105.2120463668134 40.18880706586764, -105.213960586736 40.18881703375629, -105.216033405516 40.18881994646077, -105.2160526679446 40.18840712538431, -105.2162274413648 40.18529511846879, -105.2162385578948 40.18494706245082, -105.2162474576582 40.18350012203573, -105.2162415586689 40.18336998753779, -105.2162394135021 40.18302601656777, -105.2162254934443 40.18215906787933, -105.2162565617191 40.18208996641057, -105.2163093738847 40.1820420561787, -105.2163825031335 40.18201396018677, -105.2169603850203 40.18195992434277, -105.2170475391566 40.18191594175241, -105.2170914202869 40.18186389070432, -105.2171034839595 40.18180297880132, -105.2170143693512 40.18128612529975, -105.2169225721429 40.18081208938658, -105.2168506187815 40.18047206505125, -105.21681754217 40.18042202223454, -105.2167654567252 40.18038209019546, -105.2167004241158 40.18035694995044, -105.2166895455905 40.18035572814999, -105.2166849032533 40.18035393351696, -105.2163764117413 40.18031928352345, -105.2163134477625 40.18029313762295, -105.216273617755 40.18023209753913, -105.2162777006156 40.17942503624364, -105.2162775095794 40.17809803506817, -105.2162775854453 40.17799399481255, -105.2162996166446 40.17794600901495, -105.2163563704421 40.17789591176385, -105.2164373552633 40.17787112952691, -105.216856365463 40.17788807886922, -105.2175685758577 40.17788213413407, -105.2195426020305 40.17789490160314, -105.2199974868583 40.17789106247914, -105.220117488975 40.17786390172237, -105.2202864008077 40.17777893666681, -105.220836538589 40.17741214369109, -105.2208566666041 40.17739105439566, -105.2209175212665 40.17730006248134, -105.2209504946826 40.17720104252477, -105.2209498823131 40.17690698826339, -105.2209343573538 40.17690254127866, -105.2207130981636 40.17683916514571, -105.2201717351685 40.17670336867613, -105.2200605406032 40.17661140311732, -105.2201016958975 40.17629362365332, -105.2202735353905 40.1761753142792, -105.2203499006629 40.17601302357969, -105.2203902489557 40.17589085907136, -105.2203508305605 40.17578684214399, -105.2199294170655 40.17555352473044, -105.2196648551878 40.17546273799122, -105.2195156725639 40.17539358200687, -105.2194203953364 40.17530776793799, -105.2193892751817 40.17512430056305, -105.2194693196962 40.17503891197926, -105.2196529129766 40.17496599973029, -105.2197173965499 40.17478887776263, -105.2198931450574 40.17468538125315, -105.2199974989101 40.17450224221455, -105.2200622293657 40.17426452049823, -105.2200646444332 40.17426452904852, -105.2201239077362 40.17409218918033, -105.2202205384567 40.1738884129844, -105.2202707784989 40.17381279293881, -105.2203808215655 40.17364716484659, -105.2202794070359 40.173387901259, -105.219512780327 40.17280376660269, -105.2209249631671 40.17173139885161, -105.2209180356501 40.17104304341818, -105.2209452379962 40.17104190494121, -105.2209490736238 40.17075454926682, -105.2209942464392 40.17075262017089, -105.2209958764451 40.17007267832358, -105.2209825970954 40.16942466038511, -105.2209834746498 40.1692107056338, -105.2210479242416 40.16903969442674, -105.2215353261218 40.16871687666976, -105.2216872504429 40.16858886861951, -105.2217120314581 40.16837497049304, -105.2216180871181 40.16796516832436, -105.2216584533702 40.16783689066961, -105.2218022828014 40.16773942785083, -105.2218992279499 40.16741566810365, -105.2225778264069 40.16709941839082, -105.2229617944719 40.16673355524715, -105.2233295249893 40.16644100787245, -105.223744737093 40.16622804315812, -105.2238574073118 40.16595322475723, -105.2242177806518 40.16550782979035, -105.224616900968 40.16533150285289, -105.2247611907744 40.16511788867045, -105.2248727425661 40.16511815425683, -105.2249923617757 40.16509398665386, -105.2252636187942 40.16500904877324, -105.2253115747242 40.16497248433775, -105.2252718835901 40.16493571068604, -105.2253676718974 40.16489314729116, -105.2254394076139 40.16488720419893, -105.2255231832839 40.16482913740503, -105.2255273023727 40.16482628226239, -105.225622720551 40.1648754133671, -105.2256687399535 40.16490737000433, -105.2256844243245 40.16491826169906, -105.2256824544149 40.16482453049973, -105.2256818750221 40.16479877993083, -105.2256817332005 40.16479202842404, -105.2256813243259 40.16477260883281, -105.2256678452306 40.16413216490754, -105.2256663557273 40.16406137494877, -105.2250694176052 40.16383585388203, -105.2249818257083 40.16381829563245, -105.2247082718298 40.16363382177953, -105.2245144242828 40.16339939613837, -105.2244505406456 40.16316025452517, -105.2244362919172 40.16316198219946, -105.2244350245367 40.16315723912725, -105.2241973377886 40.16318605095493, -105.2241939681854 40.16323106033524, -105.2241908870154 40.16326080731471, -105.2241871334015 40.16329050405493, -105.2241845717366 40.16330764065921, -105.2241827026874 40.16332014063767, -105.2241776054884 40.16334970447931, -105.2241718336194 40.16337918745454, -105.2241653964961 40.16340858328122, -105.2241582906471 40.16343787934208, -105.2241505172601 40.16346707203724, -105.2241420834434 40.16349614517214, -105.224132990381 40.16352509604751, -105.2241232416413 40.16355391296346, -105.2241128360789 40.16358258871198, -105.2241017796098 40.16361111159879, -105.2240900781249 40.16363947623385, -105.2240777304896 40.16366767270738, -105.2240647426128 40.16369569112624, -105.2240511192151 40.16372352519695, -105.2240368685532 40.16375116503207, -105.2240219812683 40.16377860250336, -105.224006478519 40.1638058304559, -105.2239967381509 40.16382214384298, -105.2239903532979 40.16383283986644, -105.2239736138655 40.1638596199467, -105.2239688546215 40.16386690553799, -105.2239583699097 40.16388294605247, -105.221422562563 40.16387457162896, -105.2214121380213 40.16387204453422, -105.2206711284977 40.1638702560757, -105.2204321459541 40.16385745212516, -105.2195718189001 40.16380646337711, -105.2187148516423 40.16374610977638, -105.2171229723248 40.16365794850347, -105.2165641148155 40.16359012498538, -105.2165033956429 40.16357211283747, -105.216431672717 40.16352499570027, -105.216387570914 40.16346092516294, -105.2163766429966 40.16316414840772, -105.2164085389799 40.16212189431283, -105.2163983841494 40.16198296504717, -105.216346341859 40.16184997175485, -105.2162534566525 40.16173005539297, -105.2161254215365 40.16163091588331, -105.2139196676629 40.1599989766702, -105.2137705244286 40.1599008801363, -105.2135523785454 40.15979108244539, -105.2134026840091 40.15973910300605, -105.2133888417895 40.15973666758005, -105.2133871679963 40.1597360861206, -105.2131941054505 40.15970211607535, -105.2129959093312 40.15969805573759, -105.2115128656631 40.15970204940688, -105.2114578971068 40.15970288667428, -105.2114574488354 40.1597515686144, -105.2114547518592 40.15990340125506, -105.211445205626 40.16044074274905, -105.2114357450743 40.1609733461614, -105.2114419251987 40.16153662826254, -105.2114481148706 40.16210100461468, -105.2114541918538 40.16265488641469, -105.2114551128682 40.16273858942343, -105.2114361647588 40.16273866730598, -105.2104577488688 40.16271186533191, -105.2103250511464 40.16271901622092, -105.2103399774529 40.16299494039553, -105.2103360596888 40.16366309970188, -105.2103480358364 40.16404305802597, -105.2103420726814 40.1641830452953, -105.2103348850135 40.16419098891262, -105.210282876894 40.16421995723896, -105.2102431262866 40.1642280930169, -105.2097719959188 40.16420302786118, -105.2092101207403 40.16414588869302, -105.208893623721 40.16409073764115, -105.208471675034 40.16399492621811, -105.2079663720258 40.16384596142348, -105.2075973484901 40.16370804603448, -105.2064695961106 40.16319706058182, -105.2060545441587 40.16303102252008, -105.2057594418307 40.16292815196992, -105.2054513405443 40.16285297365462, -105.2054430254445 40.16285171318667, -105.2054358230001 40.1628499557001, -105.2051190177064 40.16280193104347, -105.2047631678317 40.16276396317483, -105.204402908596 40.16275288496949, -105.204275853226 40.1627610700721, -105.2036568346699 40.16276607272876, -105.2027058313554 40.16275704228173, -105.2020374952001 40.16276176079394, -105.2020255745659 40.16223504358608, -105.2020315545417 40.15972599329237, -105.2020364487111 40.15329796080596, -105.2020503898697 40.15240197831892, -105.2020348288985 40.15240195080602, -105.2020348748597 40.15239895990317, -105.2003928214677 40.15239608689111, -105.1981951622453 40.15239887839329, -105.1962029102129 40.15238706996752, -105.1947339421019 40.15239912036138, -105.1936471026224 40.15239898939397, -105.1934589589035 40.1523919022945, -105.1933641729247 40.15238808249043, -105.1932719139723 40.15237905281442, -105.1930859740666 40.15235906840143, -105.1928106038957 40.15231163858869, -105.1926164532757 40.15226691445299, -105.1924195873322 40.15221093918417, -105.1923195534507 40.15218102474685, -105.1920345103337 40.15208391058577, -105.1915674105982 40.15190011247274, -105.1907855534298 40.15162515455555, -105.190538671026 40.15155504178544, -105.1903685580774 40.15151697721171, -105.1903607319016 40.15151567733403, -105.1903530437875 40.1515139572273, -105.1902690376092 40.15150000635485, -105.1901821651026 40.15148687092086, -105.1900959985721 40.151475933974, -105.1897880866419 40.15145287192772, -105.1885371158692 40.15143989897324, -105.1880670766908 40.15143204295714, -105.1879138398475 40.15143180934523, -105.1867460425639 40.15140788086975, -105.1864240035056 40.15142292895067, -105.1861809691329 40.15144999539257, -105.1858548713612 40.15149193386713, -105.185371896122 40.15157407225121, -105.1848938428551 40.1516740664099, -105.1837960656397 40.1519518970866, -105.1828730610242 40.15218600002028, -105.182710112977 40.15222288694235, -105.1824590841067 40.15227600253172, -105.1823190782533 40.15230306922523, -105.1821801553084 40.15232794206795, -105.1820401582139 40.15235308738404, -105.1818991075093 40.15237411100617, -105.1817820605489 40.15238806389035, -105.1815479915646 40.15240910559849, -105.1813111069034 40.15242108043596, -105.1810738976344 40.15242591632405, -105.1805269108048 40.15242303287242, -105.1783233146343 40.15242367651192, -105.1783301522852 40.15303800468062, -105.1783291792601 40.15375999780937, -105.1783012893748 40.15590656871396, -105.1783011802659 40.1559149983927, -105.1783005822134 40.15597644463524, -105.1782971626988 40.15633399335119, -105.1782960871354 40.15719749425114, -105.1782960854515 40.15719884340366, -105.1782960843966 40.15719956301125, -105.1782951121814 40.15799899804473, -105.178294217315 40.15818577184383, -105.1782870964684 40.15965399674796, -105.1782862950887 40.15989422276495, -105.1782860862953 40.15995699669625, -105.1782851194905 40.16030891223458, -105.1782850786808 40.16032399691657, -105.178284679339 40.16043600372073, -105.1782749234563 40.16315591889484, -105.178274033215 40.16340399540454, -105.1782655161564 40.1650051485672, -105.1782579902131 40.16641899487397, -105.1782449702689 40.1681079937859, -105.178239767373 40.1687701694254, -105.1782249819881 40.17185948877151, -105.1781973695228 40.17705081512157, -105.1781856753826 40.1794676433639, -105.1781825181676 40.17975001998585, -105.1781812588263 40.18010303695387, -105.1781793654503 40.18059104394589, -105.1781684523568 40.18168714946533, -105.1781684669265 40.18183643617814, -105.1781660473366 40.18316294860183, -105.1781498990898 40.18620289633849, -105.1781465206755 40.1865180200456, -105.1781438093425 40.18681401520618, -105.178140520294 40.18717302076964, -105.1781444987996 40.1872194370608, -105.1781439104042 40.18733011805361, -105.1781394025259 40.18737198322795, -105.1781394746657 40.18773489066125, -105.178139841851 40.18809600032777, -105.1781305791092 40.18957200588383, -105.1781304006922 40.18958464219161, -105.1781202084915 40.1900471212033, -105.1780948944239 40.19119569292697, -105.1780936532397 40.19125198092252, -105.1780785993141 40.19253098832572, -105.1780756714483 40.19337646219445, -105.17807555733 40.19340999518588, -105.1780755436376 40.19355999935622, -105.1780754437916 40.19356992676756, -105.1780551400565 40.19491920996467, -105.1780545724636 40.19495698637294, -105.1780511446152 40.19536670668712, -105.1780475346618 40.1958009894524, -105.1780295545943 40.19680784784939, -105.1780344485064 40.19725808820253, -105.1780344787037 40.19764486805438, -105.1780338448599 40.19770630300314, -105.1780338432419 40.19770639666449, -105.1780265031893 40.19837698788592, -105.1780244953112 40.19858399017504, -105.1780244611668 40.19870778033302, -105.1780244603029 40.19882999897617, -105.1780262933825 40.19946629969199, -105.1780294225022 40.20054600094512, -105.1780177912117 40.20209443943981, -105.1780154294347 40.20240789362089, -105.1780170937183 40.20279956093896, -105.1780170986384 40.20280075429105, -105.1780171024931 40.20280167654974, -105.1780171035354 40.20280170447224, -105.1780193743578 40.20332300422022, -105.1780125892502 40.20344194989982, -105.1779985287708 40.20376896198804, -105.1779793391662 40.20578677022317, -105.1779733735186 40.20641786448409, -105.1779725180975 40.20704933316319, -105.1779724928907 40.20706829500229, -105.1779692945993 40.20951299755229, -105.1779642885702 40.21058099413643, -105.1779642880199 40.21058111031635, -105.1779548545939 40.21285325838544, -105.1779462410317 40.21411403975657, -105.1779402743808 40.21444507532357, -105.1779392003615 40.21541000119228, -105.1779391996817 40.21541064063836, -105.1779231113842 40.21602719206967, -105.1779222810411 40.216058878454, -105.1779061898209 40.21830724012914, -105.1779061013509 40.21831971271479, -105.1779001627716 40.21915299099524, -105.1778640906119 40.22388898961723, -105.177864540534 40.22467292051728, -105.1778669788484 40.22911209642017, -105.1778663526854 40.22919784805772, -105.177865003127 40.22937498989583, -105.1778569786166 40.23065399100331, -105.1778535241373 40.23095143561333, -105.1778529903291 40.23099711941484, -105.1778516407136 40.23142737115413, -105.1778499448728 40.23197999479415, -105.1778406387775 40.23204779070896, -105.1778184627386 40.23220092675904, -105.1777991760248 40.23223585886259, -105.1777990753533 40.2322360251985, -105.1777373000234 40.23228598032479, -105.1776563108877 40.23231160004515, -105.1776460005625 40.23231260073759, -105.1766870186988 40.23231559253281, -105.1762842567278 40.23231202562735, -105.1746699443099 40.2322976123188, -105.1733949514683 40.23228760767522, -105.1720667001548 40.23229148153948, -105.1720321683417 40.23229158269653, -105.1720320179274 40.2322915831708, -105.1715299999297 40.2322915883125, -105.1691109836499 40.23229392230051, -105.1684200036398 40.23229458111676, -105.1661308987598 40.2323106876401, -105.1660599158641 40.23231118707495, -105.1652950423296 40.23231656198064, -105.162829047121 40.2323355569361, -105.160993003236 40.23233656725746, -105.1596320574399 40.23234954749802, -105.159631111938 40.2326021603701, -105.159639287903 40.23489116429988, -105.1596411241535 40.23543000233618, -105.1596455377918 40.23602956648127, -105.1596490939906 40.23651103133323, -105.1596522712427 40.23722609101691, -105.1596540870133 40.23763600383838, -105.1596750332671 40.23923601341176, -105.1596793682309 40.23954562245473, -105.1596820218607 40.23973500530968, -105.1596852663667 40.24018047174287, -105.1596852684716 40.24018075544682, -105.1596864522177 40.24038181330056, -105.1597150691784 40.24686193224582, -105.1597140201794 40.24693386583294, -105.1597068877074 40.24714470682556, -105.1596630831104 40.24838283982047, -105.1596334362387 40.24898218808481, -105.1596333787975 40.24898333081097, -105.1596251227761 40.24914994405553, -105.1595390930119 40.25123381788716, -105.1595390876333 40.25123395296526, -105.159436146626 40.25319294047603, -105.1594315084507 40.25329819468507, -105.1594011116351 40.25399307586693, -105.1594193459625 40.25413204204748, -105.1594254824308 40.25417719946864, -105.1594376867242 40.25422352574407, -105.1594480492416 40.25426137441204, -105.1594480757986 40.2542614699565, -105.1595344547845 40.25439932079264, -105.1596523760393 40.25452303893846, -105.1597878147295 40.25460896776644, -105.1599382833191 40.25468036847293, -105.160341656995 40.25483557437291, -105.1603418083376 40.25483563335776, -105.1605874317561 40.25494246474813, -105.1608249922877 40.2550751577644, -105.1610305136834 40.25524053832483, -105.1610515290015 40.25526742410285, -105.1610813427591 40.25530659135412, -105.1611090626313 40.25537858837161, -105.1611188206494 40.25540469905818, -105.1611160671059 40.25552193081968, -105.1610980231822 40.25558792265264, -105.1610768827189 40.25562969209872, -105.16104190423 40.25569596936283, -105.1610295681123 40.25571325316199, -105.1609816117556 40.25576544534216, -105.160838322246 40.25591957105722, -105.1607775160145 40.25598497549689, -105.1607389143321 40.25602649736401, -105.1606064865818 40.25617027131609, -105.1605757980321 40.25620359452309, -105.1599924986764 40.25659730650925, -105.1599989720365 40.25673921994948, -105.1599547792698 40.25678485179284, -105.1598025509507 40.25693200702809, -105.1595811076893 40.2571367624378, -105.1594444833865 40.2572704528118, -105.1594442707474 40.25727066113117, -105.1593850046439 40.25732871936017, -105.1593135897142 40.25741741259193, -105.1592464000906 40.25751418241698, -105.1592073730529 40.25761787627735, -105.1592065780735 40.2576200489465, -105.1592065673312 40.25762008133739, -105.1591639582087 40.2577383241414, -105.1590671169694 40.25811957256996, -105.1588131688499 40.25926007653372, -105.1588050309629 40.25937747332689, -105.1588035176399 40.25938480355556, -105.1587867913851 40.25946585282338, -105.1587732062316 40.25970394070752, -105.1587867235447 40.25988310314099, -105.1588772703448 40.26029735125145, -105.1589371805952 40.26053541613221, -105.1589944087731 40.26086126506672, -105.1590273950741 40.26104527341096, -105.1590403258768 40.26112013450027, -105.1590548541795 40.26120439741041, -105.1590573513478 40.26121887960556))</t>
+          <t>POLYGON ((-105.15905735134784 40.26121887960556, -105.15905735704044 40.26121891654797, -105.15909241248157 40.261225872653846, -105.16815411152918 40.26127286014907, -105.16815416090354 40.261272860290624, -105.17763003958721 40.261252265770075, -105.17763709088017 40.261252250284166, -105.17993316429539 40.26124727972221, -105.18090203368908 40.26124516797755, -105.18269892402084 40.26124123121768, -105.18270589771899 40.26124121611084, -105.18453108116029 40.261237189767996, -105.18453802664372 40.261237174473905, -105.18569463423385 40.26123460648543, -105.18570156325865 40.261234591076814, -105.18711938845047 40.26123187397589, -105.18734254737434 40.261239926044745, -105.19340857979672 40.26139700742055, -105.19341556906834 40.26139719074749, -105.19550781481341 40.26145209028402, -105.19551477587835 40.26145227431058, -105.19593537151175 40.261463375975545, -105.19745556946279 40.26067608537934, -105.19814648933357 40.26019411223952, -105.19900886159286 40.260061090677965, -105.19945973874188 40.25978578531463, -105.19977926816337 40.25962927023967, -105.19997618542715 40.259326223908104, -105.20002077478567 40.25904261606559, -105.20007486447845 40.25869858566038, -105.20086428211374 40.257625193023216, -105.20138732488391 40.25726290962486, -105.2014730596705 40.256930864566236, -105.20165327924657 40.25656638298578, -105.20209371881236 40.25649088340332, -105.20209851027386 40.256490061758505, -105.20260353595509 40.256670507221706, -105.20260722835046 40.256671826216326, -105.2028660107326 40.25670894541448, -105.20353402527995 40.25655572234178, -105.20392809481547 40.25651146572446, -105.20393867489669 40.25651027784723, -105.20421356510703 40.25674349021606, -105.20508619379483 40.25744193061791, -105.20508731253726 40.25744282598645, -105.20614538868928 40.257598565523836, -105.20615844052588 40.25760048636711, -105.20644102250624 40.257725152643616, -105.20674369427319 40.25788085597899, -105.2070114768788 40.25814245286414, -105.20730819507605 40.25828511842026, -105.20762111218897 40.25839094630618, -105.20763129403989 40.25839438989173, -105.2081977342884 40.25834933817321, -105.20888597672494 40.25819613524021, -105.20947409589716 40.25781027378541, -105.20944729903435 40.256662850045295, -105.20949666294338 40.256454341804584, -105.20943485859353 40.25613018100962, -105.2095185749566 40.25587714568412, -105.20967159687791 40.25550883050449, -105.21015409555469 40.25553376227379, -105.21057029837421 40.25549455045693, -105.21094502858661 40.25528918197753, -105.21249030870977 40.25479991430108, -105.2128932706567 40.25463280689722, -105.2133718730392 40.25413205482123, -105.21640300184444 40.250626306593226, -105.21659493096602 40.25041072509776, -105.21724055450275 40.24954584877566, -105.2175493089082 40.2491024012631, -105.21782169094001 40.248493922038946, -105.2184710561619 40.24749196008531, -105.21920621601373 40.2472627512926, -105.2201614200856 40.24636299751891, -105.22131793251293 40.2455953056567, -105.22172952788173 40.24552875557625, -105.22173223055762 40.24552831896781, -105.22195909398049 40.24558935384183, -105.22226859397534 40.24579925097038, -105.22255397556557 40.245907011720824, -105.22256107652599 40.24590969279355, -105.22341328552024 40.245943455508645, -105.22425334681886 40.2459686081519, -105.22488048274585 40.24603755400981, -105.22497952424372 40.246041042487484, -105.22512469087472 40.246035987248916, -105.22512441884601 40.246014036577215, -105.2251246544638 40.24597612984243, -105.22512644163183 40.245690942255926, -105.22513969468511 40.24516006982153, -105.22514868243132 40.24373510434809, -105.22516558747753 40.2430098863984, -105.2251615362667 40.2422401475095, -105.22518970752834 40.240145968424805, -105.22519237412081 40.23939793128302, -105.22518663612263 40.23931089739514, -105.22515359158363 40.23915599503675, -105.2250724245328 40.238943055486985, -105.22496467369648 40.238748994648645, -105.22483671084952 40.23859304245457, -105.22411336703718 40.237920140260265, -105.22323758154953 40.237126083230706, -105.22285763051238 40.23675211280806, -105.2225646450352 40.236397016041224, -105.2223025250875 40.23602799325127, -105.22203854047287 40.23559006293472, -105.22187768199858 40.23524790936244, -105.2217555450768 40.234897063956794, -105.22144245864678 40.233682146134655, -105.22116844578618 40.23246210583308, -105.22103453664833 40.2318400144956, -105.22098161356493 40.23147011913398, -105.22096143134428 40.230977047366984, -105.22097751122409 40.23054994659705, -105.22102868160485 40.23012512524188, -105.22109555804444 40.22979999070917, -105.22123457388068 40.22935094963212, -105.22141438373605 40.228909968144144, -105.22227336704563 40.22721088304503, -105.22239261210979 40.226952029841215, -105.22248144274762 40.22668596697582, -105.22249558265862 40.22655588179951, -105.22249449499326 40.22629591658432, -105.222456515767 40.226036960723214, -105.22238162404068 40.22578395587376, -105.22188740034088 40.22482087832691, -105.22179158518115 40.224605979642995, -105.22171835662554 40.224385096493975, -105.22166949502325 40.22416097651936, -105.22151660746212 40.222666988659036, -105.22145661692855 40.22183809224568, -105.22148869972482 40.22161197213887, -105.22156051219594 40.22139088759893, -105.22167346024747 40.221180883352446, -105.22180667624997 40.22100606485856, -105.22196665736045 40.2208540955447, -105.22215341692281 40.220721131450524, -105.22236442991498 40.22061210723617, -105.22259360704709 40.220527009968684, -105.22404747357571 40.22018597437552, -105.22538738464291 40.21986938401997, -105.22808963879277 40.2192320089863, -105.22908550420233 40.21896504863379, -105.22930466416182 40.2188741496954, -105.2295013646164 40.21875794149326, -105.22967344247023 40.21861999007856, -105.22981551425259 40.21846302630055, -105.22995959829372 40.21825006684786, -105.23004268301958 40.21806798432373, -105.23007048824716 40.21796439404318, -105.23009463716794 40.21788006507707, -105.23010863316054 40.2177820967097, -105.2301247091618 40.21652898563659, -105.23012845508997 40.2158558903383, -105.23014150943182 40.21500301146425, -105.23013836374662 40.21435213555789, -105.23015048081075 40.214096043755426, -105.23015955226647 40.21163011961929, -105.2301555092061 40.211025084222605, -105.23014000932068 40.21102641251364, -105.2301399807453 40.21102206961, -105.22987422637239 40.211044844910305, -105.22945039233339 40.211146797164496, -105.22915905139979 40.21144800191435, -105.22836981523494 40.21187514808197, -105.22787538548151 40.212009198319265, -105.22771203680632 40.21224963597185, -105.22744823073567 40.212572086716875, -105.22710197035819 40.21278312088065, -105.22690099365356 40.21294153470387, -105.22683135820506 40.21307907293179, -105.22674084849771 40.213253635318424, -105.22573852983898 40.21340485457109, -105.22497872601426 40.21337656924641, -105.22434839676117 40.213788177675255, -105.22392681800889 40.21382954143416, -105.22268932022308 40.21404902495213, -105.22192188676053 40.21419547745586, -105.2212997430297 40.21428931261474, -105.22094715470513 40.21435201814516, -105.2206776411029 40.21437255222598, -105.21958187409975 40.21424732969597, -105.21941724391888 40.21430823721885, -105.21933207504783 40.21449194906986, -105.2189844220926 40.214664199677635, -105.21876240355685 40.21473579059544, -105.21849583291673 40.21472540903732, -105.21832561469387 40.21453675764475, -105.2181220301564 40.21434893702349, -105.21778507044816 40.21418463216135, -105.2175902741623 40.21402067260001, -105.21751088819502 40.213880836998015, -105.21707158162191 40.21375715061206, -105.21706785162542 40.21375745580795, -105.2155783456237 40.21387950723339, -105.21442707171953 40.21402993613065, -105.21364543130244 40.21396669689456, -105.2124598923856 40.213813896368535, -105.21245726075018 40.21381254158332, -105.21214071840774 40.21364961832136, -105.21212711375216 40.21364759136831, -105.21212519014664 40.213646601291536, -105.21157995737671 40.213565363426355, -105.21119233537168 40.21341104953922, -105.21119369549679 40.21334806106676, -105.21117144086983 40.213192082111235, -105.21117963725983 40.212780058889635, -105.2111863566922 40.21220991280554, -105.21121153273602 40.20889605807057, -105.21122763207279 40.20805608894247, -105.21123556221168 40.20694790040265, -105.21122001465984 40.20694785888084, -105.20939456450559 40.206943015378215, -105.20858935569078 40.206939890552455, -105.2085881819834 40.20693692902196, -105.20854862225086 40.206837120468045, -105.20853642540263 40.206759128399824, -105.20844650860509 40.20643689730729, -105.20810255185675 40.20565998188825, -105.20803245336536 40.20547588162022, -105.20780551443931 40.20488098724236, -105.20719868863205 40.20362794753153, -105.20708437632969 40.20348600941636, -105.20701162470917 40.20341994212115, -105.2068616666747 40.20332512998329, -105.20659952119827 40.203177051621154, -105.20653649044662 40.203098929410814, -105.20651963700115 40.20302202312945, -105.20651137118128 40.202283013064346, -105.20649566986617 40.201192881676675, -105.2064985931352 40.200266955586685, -105.20652246136521 40.19921590544162, -105.20655838595488 40.19918689807859, -105.20656556384107 40.19818713874076, -105.20656260385412 40.197462965088796, -105.20652751951104 40.196468040002486, -105.20659344590024 40.19614203326668, -105.20664621685884 40.19605606126178, -105.20684096873286 40.19602785289616, -105.20778837845648 40.19603914913586, -105.20847356646934 40.196035113628525, -105.2085663813553 40.19601201399413, -105.20864069284279 40.19596306273813, -105.20866838895932 40.1959321129289, -105.20872342334322 40.19578703355778, -105.20890459438984 40.19510999151015, -105.2091984259771 40.193953106906356, -105.20949950103007 40.1928580058869, -105.20981556916516 40.19177007906735, -105.21002668064415 40.191034088826235, -105.21037643424418 40.18993306751391, -105.21063353135115 40.18898609076457, -105.21067151562845 40.18880802608792, -105.21204636681338 40.18880706586764, -105.21396058673602 40.188817033756294, -105.21603340551596 40.18881994646077, -105.21605266794457 40.18840712538431, -105.2162274413648 40.185295118468794, -105.21623855789477 40.18494706245082, -105.21624745765817 40.18350012203573, -105.21624155866891 40.18336998753779, -105.21623941350211 40.18302601656777, -105.21622549344433 40.182159067879326, -105.21625656171906 40.182089966410565, -105.2163093738847 40.1820420561787, -105.21638250313354 40.18201396018677, -105.21696038502029 40.18195992434277, -105.21704753915661 40.18191594175241, -105.21709142028692 40.18186389070432, -105.21710348395955 40.18180297880132, -105.21701436935116 40.18128612529975, -105.21692257214292 40.18081208938658, -105.21685061878149 40.18047206505125, -105.21681754217005 40.180422022234545, -105.21676545672523 40.18038209019546, -105.2167004241158 40.18035694995044, -105.21668954559047 40.18035572814999, -105.21668490325334 40.18035393351696, -105.21637641174132 40.18031928352345, -105.21631344776249 40.180293137622954, -105.21627361775495 40.180232097539125, -105.21627770061565 40.179425036243636, -105.21627750957944 40.178098035068174, -105.2162775854453 40.17799399481255, -105.21629961664465 40.177946009014946, -105.21635637044214 40.17789591176385, -105.21643735526327 40.17787112952691, -105.21685636546304 40.17788807886922, -105.21756857585765 40.17788213413407, -105.21954260203049 40.17789490160314, -105.2199974868583 40.17789106247914, -105.22011748897503 40.17786390172237, -105.22028640080765 40.17777893666681, -105.220836538589 40.177412143691086, -105.22085666660412 40.177391054395656, -105.22091752126646 40.177300062481336, -105.22095049468263 40.17720104252477, -105.22094988231315 40.17690698826339, -105.22093435735384 40.17690254127866, -105.22071309816359 40.17683916514571, -105.22017173516849 40.17670336867613, -105.2200605406032 40.17661140311732, -105.22010169589748 40.176293623653315, -105.22027353539048 40.1761753142792, -105.22034990066287 40.17601302357969, -105.22039024895572 40.17589085907136, -105.22035083056055 40.17578684214399, -105.21992941706546 40.17555352473044, -105.21966485518782 40.17546273799122, -105.21951567256394 40.17539358200687, -105.21942039533639 40.175307767937994, -105.21938927518171 40.17512430056305, -105.21946931969619 40.175038911979264, -105.21965291297658 40.17496599973029, -105.21971739654985 40.17478887776263, -105.21989314505738 40.17468538125315, -105.21999749891012 40.17450224221455, -105.22006222936565 40.174264520498234, -105.22006464443322 40.17426452904852, -105.22012390773622 40.17409218918033, -105.2202205384567 40.1738884129844, -105.22027077849893 40.17381279293881, -105.22038082156554 40.173647164846585, -105.2202794070359 40.173387901259, -105.21951278032704 40.17280376660269, -105.22092496316705 40.17173139885161, -105.22091803565013 40.17104304341818, -105.22094523799618 40.171041904941205, -105.22094907362384 40.170754549266825, -105.22099424643919 40.170752620170894, -105.22099587644509 40.17007267832358, -105.22098259709541 40.16942466038511, -105.22098347464978 40.1692107056338, -105.2210479242416 40.169039694426736, -105.22153532612177 40.16871687666976, -105.22168725044288 40.16858886861951, -105.22171203145805 40.16837497049304, -105.22161808711809 40.167965168324365, -105.22165845337022 40.16783689066961, -105.22180228280136 40.16773942785083, -105.22189922794989 40.16741566810365, -105.22257782640692 40.16709941839082, -105.22296179447193 40.16673355524715, -105.2233295249893 40.16644100787245, -105.22374473709303 40.16622804315812, -105.22385740731184 40.16595322475723, -105.22421778065177 40.16550782979035, -105.22461690096799 40.165331502852894, -105.2247611907744 40.16511788867045, -105.2248727425661 40.16511815425683, -105.22499236177575 40.16509398665386, -105.22526361879424 40.165009048773236, -105.22531157472422 40.164972484337746, -105.22527188359014 40.16493571068604, -105.22536767189742 40.16489314729116, -105.22543940761388 40.164887204198926, -105.2255231832839 40.16482913740503, -105.22552730237273 40.16482628226239, -105.22562272055102 40.1648754133671, -105.2256687399535 40.16490737000433, -105.22568442432446 40.164918261699064, -105.22568245441485 40.16482453049973, -105.22568187502212 40.164798779930834, -105.2256817332005 40.16479202842404, -105.22568132432586 40.16477260883281, -105.22566784523062 40.164132164907535, -105.2256663557273 40.164061374948766, -105.2250694176052 40.16383585388203, -105.22498182570828 40.163818295632446, -105.22470827182981 40.16363382177953, -105.22451442428284 40.16339939613837, -105.22445054064558 40.16316025452517, -105.2244362919172 40.16316198219946, -105.22443502453667 40.16315723912725, -105.2241973377886 40.163186050954934, -105.22419396818545 40.163231060335235, -105.22419088701537 40.16326080731471, -105.22418713340147 40.16329050405493, -105.22418457173661 40.16330764065921, -105.22418270268737 40.163320140637666, -105.22417760548844 40.16334970447931, -105.22417183361935 40.16337918745454, -105.22416539649606 40.163408583281225, -105.22415829064705 40.163437879342084, -105.22415051726007 40.16346707203724, -105.22414208344337 40.16349614517214, -105.22413299038101 40.163525096047515, -105.22412324164132 40.16355391296346, -105.22411283607892 40.163582588711975, -105.22410177960984 40.16361111159879, -105.22409007812487 40.16363947623385, -105.22407773048955 40.163667672707376, -105.2240647426128 40.163695691126236, -105.2240511192151 40.16372352519695, -105.22403686855324 40.163751165032075, -105.2240219812683 40.163778602503356, -105.22400647851899 40.1638058304559, -105.22399673815093 40.16382214384298, -105.22399035329788 40.16383283986644, -105.2239736138655 40.1638596199467, -105.22396885462149 40.163866905537986, -105.2239583699097 40.163882946052475, -105.22142256256299 40.16387457162896, -105.22141213802132 40.163872044534216, -105.22067112849773 40.163870256075704, -105.22043214595409 40.16385745212516, -105.21957181890005 40.163806463377114, -105.21871485164235 40.163746109776376, -105.21712297232476 40.16365794850347, -105.2165641148155 40.16359012498538, -105.21650339564287 40.16357211283747, -105.216431672717 40.16352499570027, -105.21638757091395 40.163460925162944, -105.21637664299655 40.16316414840772, -105.21640853897992 40.16212189431283, -105.21639838414941 40.161982965047166, -105.21634634185902 40.161849971754854, -105.21625345665245 40.161730055392965, -105.2161254215365 40.16163091588331, -105.2139196676629 40.1599989766702, -105.21377052442864 40.1599008801363, -105.21355237854544 40.15979108244539, -105.21340268400907 40.159739103006046, -105.21338884178945 40.15973666758005, -105.21338716799629 40.1597360861206, -105.2131941054505 40.15970211607535, -105.2129959093312 40.159698055737586, -105.21151286566307 40.15970204940688, -105.21145789710683 40.15970288667428, -105.21145744883538 40.1597515686144, -105.21145475185916 40.159903401255065, -105.21144520562605 40.160440742749046, -105.21143574507434 40.1609733461614, -105.21144192519867 40.16153662826254, -105.21144811487062 40.162101004614684, -105.21145419185379 40.162654886414686, -105.21145511286817 40.162738589423434, -105.21143616475884 40.16273866730598, -105.21045774886878 40.162711865331914, -105.21032505114643 40.16271901622092, -105.21033997745286 40.16299494039553, -105.21033605968876 40.16366309970188, -105.21034803583642 40.164043058025975, -105.2103420726814 40.164183045295296, -105.21033488501352 40.164190988912615, -105.21028287689401 40.164219957238956, -105.21024312628657 40.1642280930169, -105.20977199591883 40.16420302786118, -105.20921012074034 40.16414588869302, -105.20889362372097 40.164090737641146, -105.20847167503396 40.16399492621811, -105.2079663720258 40.16384596142348, -105.20759734849008 40.16370804603448, -105.20646959611061 40.16319706058182, -105.2060545441587 40.16303102252008, -105.20575944183071 40.16292815196992, -105.20545134054429 40.16285297365462, -105.20544302544447 40.16285171318667, -105.20543582300013 40.1628499557001, -105.20511901770635 40.16280193104347, -105.20476316783173 40.16276396317483, -105.204402908596 40.162752884969485, -105.204275853226 40.1627610700721, -105.20365683466991 40.16276607272876, -105.20270583135539 40.162757042281726, -105.20203749520009 40.16276176079394, -105.20202557456592 40.16223504358608, -105.20203155454175 40.15972599329237, -105.20203644871107 40.153297960805965, -105.2020503898697 40.15240197831892, -105.2020348288985 40.15240195080602, -105.2020348748597 40.15239895990317, -105.20039282146774 40.15239608689111, -105.1981951622453 40.15239887839329, -105.19620291021289 40.15238706996752, -105.19473394210193 40.15239912036138, -105.19364710262239 40.152398989393966, -105.1934589589035 40.1523919022945, -105.19336417292473 40.152388082490425, -105.19327191397227 40.152379052814425, -105.19308597406658 40.15235906840143, -105.19281060389568 40.15231163858869, -105.19261645327569 40.152266914452994, -105.19241958733224 40.152210939184165, -105.19231955345072 40.152181024746845, -105.19203451033374 40.15208391058577, -105.19156741059824 40.15190011247274, -105.19078555342985 40.151625154555546, -105.19053867102599 40.15155504178544, -105.19036855807735 40.151516977211706, -105.19036073190159 40.15151567733403, -105.19035304378754 40.1515139572273, -105.19026903760924 40.15150000635485, -105.19018216510263 40.15148687092086, -105.19009599857208 40.151475933974, -105.18978808664193 40.151452871927724, -105.1885371158692 40.15143989897324, -105.18806707669081 40.15143204295714, -105.1879138398475 40.151431809345226, -105.1867460425639 40.151407880869755, -105.18642400350559 40.151422928950666, -105.18618096913295 40.151449995392575, -105.1858548713612 40.151491933867135, -105.18537189612198 40.15157407225121, -105.18489384285515 40.151674066409896, -105.18379606563974 40.151951897086605, -105.18287306102417 40.15218600002028, -105.18271011297703 40.15222288694235, -105.18245908410674 40.15227600253172, -105.18231907825327 40.15230306922523, -105.1821801553084 40.15232794206795, -105.18204015821385 40.152353087384036, -105.18189910750931 40.15237411100617, -105.18178206054885 40.15238806389035, -105.18154799156456 40.15240910559849, -105.18131110690341 40.15242108043596, -105.18107389763443 40.15242591632405, -105.18052691080484 40.15242303287242, -105.17832331463428 40.15242367651192, -105.17833015228523 40.153038004680624, -105.17832917926015 40.153759997809374, -105.1783012893748 40.15590656871396, -105.1783011802659 40.1559149983927, -105.17830058221338 40.155976444635236, -105.17829716269877 40.15633399335119, -105.17829608713544 40.15719749425114, -105.17829608545148 40.15719884340366, -105.17829608439656 40.15719956301125, -105.17829511218137 40.157998998044725, -105.17829421731496 40.158185771843826, -105.17828709646844 40.15965399674796, -105.17828629508872 40.159894222764954, -105.17828608629526 40.15995699669625, -105.1782851194905 40.160308912234576, -105.1782850786808 40.16032399691657, -105.17828467933904 40.16043600372073, -105.17827492345634 40.163155918894844, -105.17827403321505 40.163403995404536, -105.1782655161564 40.165005148567204, -105.17825799021314 40.16641899487397, -105.17824497026889 40.1681079937859, -105.178239767373 40.1687701694254, -105.17822498198805 40.17185948877151, -105.17819736952283 40.17705081512157, -105.17818567538262 40.1794676433639, -105.17818251816756 40.179750019985846, -105.17818125882629 40.180103036953874, -105.1781793654503 40.18059104394589, -105.17816845235684 40.18168714946533, -105.1781684669265 40.18183643617814, -105.1781660473366 40.183162948601826, -105.17814989908976 40.18620289633849, -105.17814652067545 40.1865180200456, -105.17814380934253 40.18681401520618, -105.17814052029402 40.18717302076964, -105.17814449879961 40.1872194370608, -105.17814391040417 40.18733011805361, -105.1781394025259 40.187371983227955, -105.17813947466566 40.18773489066125, -105.17813984185103 40.188096000327775, -105.17813057910922 40.189572005883825, -105.17813040069217 40.18958464219161, -105.17812020849152 40.1900471212033, -105.17809489442394 40.19119569292697, -105.17809365323973 40.191251980922516, -105.17807859931413 40.19253098832572, -105.17807567144827 40.19337646219445, -105.17807555733003 40.19340999518588, -105.1780755436376 40.193559999356225, -105.17807544379163 40.19356992676756, -105.17805514005646 40.194919209964674, -105.17805457246362 40.19495698637294, -105.17805114461522 40.195366706687125, -105.17804753466176 40.1958009894524, -105.17802955459432 40.196807847849385, -105.17803444850635 40.19725808820253, -105.17803447870367 40.19764486805438, -105.17803384485991 40.197706303003145, -105.1780338432419 40.19770639666449, -105.17802650318933 40.19837698788592, -105.17802449531118 40.19858399017504, -105.17802446116676 40.198707780333024, -105.17802446030292 40.198829998976166, -105.17802629338252 40.19946629969199, -105.17802942250223 40.200546000945124, -105.17801779121167 40.20209443943981, -105.17801542943474 40.202407893620894, -105.17801709371831 40.20279956093896, -105.1780170986384 40.202800754291054, -105.17801710249309 40.20280167654974, -105.17801710353541 40.202801704472236, -105.17801937435783 40.203323004220216, -105.17801258925016 40.20344194989982, -105.17799852877081 40.20376896198804, -105.17797933916623 40.20578677022317, -105.1779733735186 40.20641786448409, -105.17797251809748 40.20704933316319, -105.1779724928907 40.207068295002294, -105.17796929459932 40.20951299755229, -105.17796428857021 40.21058099413643, -105.17796428801988 40.210581110316355, -105.1779548545939 40.212853258385444, -105.17794624103169 40.214114039756566, -105.17794027438083 40.21444507532357, -105.17793920036152 40.21541000119228, -105.17793919968172 40.21541064063836, -105.17792311138416 40.21602719206967, -105.1779222810411 40.216058878454, -105.17790618982087 40.21830724012914, -105.17790610135093 40.21831971271479, -105.17790016277155 40.21915299099524, -105.17786409061186 40.22388898961723, -105.17786454053405 40.22467292051728, -105.17786697884839 40.229112096420174, -105.17786635268537 40.229197848057716, -105.17786500312704 40.22937498989583, -105.17785697861656 40.23065399100331, -105.1778535241373 40.23095143561333, -105.17785299032911 40.230997119414845, -105.17785164071356 40.231427371154126, -105.17784994487276 40.23197999479415, -105.17784063877747 40.23204779070896, -105.17781846273856 40.23220092675904, -105.17779917602482 40.23223585886259, -105.1777990753533 40.2322360251985, -105.17773730002344 40.23228598032479, -105.1776563108877 40.23231160004515, -105.17764600056253 40.23231260073759, -105.17668701869876 40.232315592532814, -105.17628425672778 40.23231202562735, -105.17466994430987 40.2322976123188, -105.17339495146831 40.23228760767522, -105.17206670015476 40.232291481539484, -105.17203216834172 40.23229158269653, -105.17203201792735 40.2322915831708, -105.1715299999297 40.2322915883125, -105.16911098364986 40.232293922300514, -105.1684200036398 40.23229458111676, -105.16613089875979 40.2323106876401, -105.16605991586405 40.23231118707495, -105.16529504232963 40.23231656198064, -105.16282904712098 40.2323355569361, -105.160993003236 40.23233656725746, -105.15963205743985 40.232349547498025, -105.15963111193798 40.2326021603701, -105.159639287903 40.23489116429988, -105.15964112415352 40.23543000233618, -105.15964553779179 40.23602956648127, -105.15964909399057 40.23651103133323, -105.15965227124268 40.237226091016915, -105.15965408701334 40.23763600383838, -105.15967503326708 40.239236013411755, -105.15967936823093 40.23954562245473, -105.15968202186066 40.23973500530968, -105.15968526636668 40.240180471742875, -105.1596852684716 40.24018075544682, -105.15968645221767 40.24038181330056, -105.15971506917836 40.24686193224582, -105.15971402017936 40.246933865832936, -105.15970688770742 40.24714470682556, -105.15966308311042 40.248382839820465, -105.15963343623875 40.24898218808481, -105.15963337879754 40.248983330810965, -105.15962512277606 40.24914994405553, -105.15953909301187 40.25123381788716, -105.15953908763332 40.251233952965265, -105.159436146626 40.25319294047603, -105.1594315084507 40.25329819468507, -105.15940111163513 40.25399307586693, -105.1594193459625 40.25413204204748, -105.15942548243076 40.25417719946864, -105.15943768672423 40.25422352574407, -105.15944804924163 40.25426137441204, -105.1594480757986 40.254261469956504, -105.15953445478448 40.25439932079264, -105.15965237603928 40.25452303893846, -105.15978781472954 40.254608967766444, -105.15993828331905 40.25468036847293, -105.16034165699497 40.25483557437291, -105.1603418083376 40.25483563335776, -105.16058743175611 40.25494246474813, -105.16082499228769 40.255075157764395, -105.16103051368343 40.25524053832483, -105.1610515290015 40.25526742410285, -105.16108134275909 40.25530659135412, -105.16110906263125 40.255378588371606, -105.16111882064938 40.255404699058175, -105.16111606710592 40.25552193081968, -105.16109802318218 40.255587922652644, -105.1610768827189 40.25562969209872, -105.16104190423002 40.255695969362826, -105.16102956811226 40.25571325316199, -105.16098161175556 40.255765445342156, -105.16083832224595 40.25591957105722, -105.1607775160145 40.25598497549689, -105.16073891433206 40.25602649736401, -105.1606064865818 40.256170271316094, -105.16057579803207 40.25620359452309, -105.15999249867636 40.25659730650925, -105.15999897203646 40.25673921994948, -105.15995477926982 40.25678485179284, -105.15980255095073 40.25693200702809, -105.15958110768928 40.257136762437796, -105.15944448338654 40.2572704528118, -105.1594442707474 40.25727066113117, -105.15938500464394 40.257328719360174, -105.15931358971419 40.25741741259193, -105.1592464000906 40.257514182416976, -105.15920737305285 40.25761787627735, -105.15920657807348 40.2576200489465, -105.15920656733118 40.257620081337386, -105.15916395820871 40.2577383241414, -105.15906711696941 40.25811957256996, -105.15881316884987 40.25926007653372, -105.15880503096291 40.259377473326886, -105.1588035176399 40.259384803555555, -105.15878679138505 40.25946585282338, -105.15877320623163 40.25970394070752, -105.15878672354474 40.25988310314099, -105.1588772703448 40.26029735125145, -105.15893718059517 40.26053541613221, -105.15899440877313 40.26086126506672, -105.15902739507408 40.26104527341096, -105.15904032587676 40.261120134500274, -105.15905485417952 40.26120439741041, -105.15905735134784 40.26121887960556))</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
@@ -5314,7 +5338,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1499553999603 40.19980913607915, -105.149964101196 40.20036601195144, -105.1499562482724 40.20039565687276, -105.1499662706908 40.20210364514212, -105.1499702753119 40.20243164381855, -105.1499682812303 40.20282264077071, -105.1499702876212 40.20326363768343, -105.1499712682566 40.20329697851118, -105.1777689132483 40.20332279657391, -105.1780193743578 40.20332300422022, -105.1780171035354 40.20280170447224, -105.1780171024931 40.20280167654974, -105.1780170986384 40.20280075429105, -105.1780170937183 40.20279956093896, -105.1780154294347 40.20240789362089, -105.1780177912117 40.20209443943981, -105.1780294225022 40.20054600094512, -105.1780262933825 40.19946629969199, -105.1780244603029 40.19882999897617, -105.1780244611668 40.19870778033302, -105.1780244953112 40.19858399017504, -105.1780265031893 40.19837698788592, -105.1780338432419 40.19770639666449, -105.1780338448599 40.19770630300314, -105.1780344787037 40.19764486805438, -105.1780344485064 40.19725808820253, -105.1780295545943 40.19680784784939, -105.1780475346618 40.1958009894524, -105.1780511446152 40.19536670668712, -105.1780545724636 40.19495698637294, -105.1780551400565 40.19491920996467, -105.1780754437916 40.19356992676756, -105.1780755436376 40.19355999935622, -105.17807555733 40.19340999518588, -105.1780756714483 40.19337646219445, -105.1780785993141 40.19253098832572, -105.1780936532397 40.19125198092252, -105.1780948944239 40.19119569292697, -105.1781202084915 40.1900471212033, -105.1781304006922 40.18958464219161, -105.1781305791092 40.18957200588383, -105.178139841851 40.18809600032777, -105.1781394746657 40.18773489066125, -105.1781394025259 40.18737198322795, -105.1781439104042 40.18733011805361, -105.1781444987996 40.1872194370608, -105.178140520294 40.18717302076964, -105.1781438093425 40.18681401520618, -105.1781465206755 40.1865180200456, -105.1781498990898 40.18620289633849, -105.1781660473366 40.18316294860183, -105.1781684669265 40.18183643617814, -105.1781684523568 40.18168714946533, -105.1781793654503 40.18059104394589, -105.1781812588263 40.18010303695387, -105.1781825181676 40.17975001998585, -105.1781856753826 40.1794676433639, -105.1781973695228 40.17705081512157, -105.1782249819881 40.17185948877151, -105.178239767373 40.1687701694254, -105.1782449702689 40.1681079937859, -105.1782538706628 40.16695343985297, -105.1735772011636 40.16694246349251, -105.1735112021403 40.16875746475598, -105.1735104074165 40.16876894654175, -105.1734888774345 40.16876895687698, -105.1734876717343 40.1687689579743, -105.1734767013714 40.17058610997677, -105.1734766984293 40.17058819044085, -105.1734768239046 40.17088245964705, -105.1734768197971 40.17088453830642, -105.1733657812711 40.17083213172842, -105.1733576954174 40.17082828027013, -105.1729529231051 40.17063241614367, -105.1728205681745 40.1705683728318, -105.1728195198593 40.17056786550766, -105.1687255340658 40.16858670852341, -105.1687256438738 40.1685916425322, -105.1687231045455 40.16859477217606, -105.1677518350548 40.16979169341922, -105.1677465944088 40.16979815123889, -105.167035661948 40.17067421828263, -105.167026766362 40.17067109176306, -105.1670240178124 40.17067447924944, -105.1669332093008 40.17078637943621, -105.1669304607418 40.17078976692029, -105.1668896186171 40.17084009214113, -105.1668985520034 40.17084317464879, -105.1668943955052 40.17084829540469, -105.1668849048761 40.17085999075397, -105.1665201919034 40.17073175740313, -105.1665174951051 40.17073080935722, -105.1664129896231 40.17079382714124, -105.1650199693466 40.17032183177924, -105.1642709600386 40.17007883540592, -105.1642169582605 40.17006083511097, -105.1640679558686 40.16999983608142, -105.1638209526211 40.16989583642651, -105.1637179519749 40.16985083726004, -105.1635209475333 40.16973283788921, -105.1631259398792 40.16948983996239, -105.1622709235831 40.1688868436568, -105.161120902206 40.16807485153609, -105.1602088846895 40.16741385793949, -105.1599118790576 40.16721485751804, -105.1598118775726 40.1671618596847, -105.1596798760458 40.16712085952145, -105.1595208740774 40.16707385977891, -105.1593498721462 40.16705286010649, -105.1572978539927 40.16702986225165, -105.1562688454048 40.16703286263721, -105.1551078351645 40.16704986397507, -105.1546488300367 40.16705586518081, -105.1546488353165 40.16705898771062, -105.154647999395 40.16705899872255, -105.1546530002739 40.17018099915842, -105.1546569998319 40.17225799859407, -105.1546569996872 40.17249899848197, -105.1546589995688 40.17417299912417, -105.1546599342045 40.17417298750612, -105.1546620818144 40.17647724158829, -105.1546629131087 40.17736968103145, -105.1546629770468 40.17743779821491, -105.154734010364 40.17971278356963, -105.154772043574 40.18204276868759, -105.1547760472109 40.18231676688708, -105.1547761624487 40.18231997349721, -105.1547749998258 40.18231999974654, -105.1547920001525 40.18279499845895, -105.1548391576341 40.18279499875759, -105.1548391987841 40.18280146725144, -105.1548751995001 40.18420846777963, -105.1561902006576 40.18420546794748, -105.1563442888084 40.18427100243236, -105.1568855688112 40.18450120863788, -105.1575644515808 40.1847899325708, -105.1580737797326 40.18500654159926, -105.158429101739 40.18522127318123, -105.1584622286077 40.18523943690133, -105.1584622689358 40.18524309810573, -105.1584638862964 40.18733561945109, -105.1584638890017 40.18733882211959, -105.1584640423004 40.18753722180259, -105.1584590925243 40.18753745755789, -105.158125901028 40.18755334084461, -105.156950659277 40.18760411594983, -105.1556639597298 40.18766202520918, -105.1550332835498 40.18768878906563, -105.1550295936307 40.18753811519997, -105.1550295159042 40.18753491771105, -105.1548431219606 40.18754573195616, -105.1548431080552 40.18754893457554, -105.154841999169 40.18754899881291, -105.1548369993615 40.18865397295026, -105.1548381373372 40.18865072595334, -105.1555308853084 40.18865548209631, -105.155531199946 40.18866546838077, -105.1555431997794 40.19021346870296, -105.154617200905 40.18989046922776, -105.1527832001366 40.1899674691564, -105.1526282001168 40.19021446851695, -105.1523262006294 40.19040146942321, -105.1522062000076 40.19044046900569, -105.1520391995784 40.1904544685933, -105.1520391995797 40.1904813219414, -105.1520301329908 40.190480717349, -105.151725130212 40.19045971848809, -105.1510521225241 40.19039872026119, -105.150400114481 40.19034672131698, -105.1498131075271 40.19030272138396, -105.1496481067909 40.19028072156684, -105.1493191020164 40.19026372260259, -105.1489900989153 40.19026372220461, -105.1486820954207 40.19027472289796, -105.1484240929505 40.19029072383959, -105.1479800890678 40.19036772283105, -105.1475290858815 40.19047172415833, -105.1469560824025 40.19063072326936, -105.146023039163 40.19095953422137, -105.1458950200733 40.19099873057759, -105.145556198577 40.19110246879873, -105.145540002091 40.19156738941043, -105.1454650795996 40.19166871898251, -105.1446851981676 40.19186346973615, -105.1435901972262 40.19178347003211, -105.1430128227406 40.19170322191939, -105.1422191542082 40.19159290600409, -105.1417411975476 40.19152646954736, -105.1411226446519 40.19153998197216, -105.1409890318654 40.19152972594931, -105.1409040306353 40.19154572658073, -105.1405211966407 40.19155347041578, -105.1395731959861 40.1916054697542, -105.1393233110076 40.19185722614801, -105.1388341967081 40.19234946940898, -105.1390461965723 40.19282347040903, -105.1396701978683 40.19287647006031, -105.1404581968998 40.19310846976347, -105.1420492687273 40.19332518604399, -105.1430131974055 40.19345646962464, -105.1430341800693 40.19346310723986, -105.1430150797219 40.19356771111762, -105.1430142317597 40.19356972952564, -105.1429570807157 40.19370571023295, -105.1429070803512 40.19380370978143, -105.1428790829269 40.19388670873322, -105.142879089666 40.19388676729531, -105.1428930830832 40.1940017072699, -105.142943085833 40.19412270623425, -105.1429930883901 40.19419970643524, -105.1430720899324 40.1942987058851, -105.1431220907786 40.19435370620326, -105.1431720931412 40.1944467052078, -105.1432220946501 40.19460570364041, -105.1432360974586 40.19477070269613, -105.1432721000626 40.19491870167863, -105.1433001014114 40.19499570050589, -105.1433361023987 40.19506770115726, -105.1434151044106 40.19515569999793, -105.1435081061389 40.19524369871329, -105.1438091135656 40.19546269709496, -105.1440091178666 40.1956336960499, -105.1443811252396 40.19591869385945, -105.1448041341312 40.19618269030496, -105.1452121412532 40.19636968980674, -105.1456841479397 40.19655668763392, -105.1461431546569 40.19669468522994, -105.1467441635402 40.19682668434852, -105.1473461715542 40.19692568232102, -105.1474821738625 40.19693668216285, -105.1476461753783 40.19693668305129, -105.1479411771563 40.19687668244443, -105.1483218563037 40.19709180819938, -105.1485730402104 40.19710161420416, -105.1489791994848 40.19711747053223, -105.1496263405455 40.19758894297775, -105.1499812003125 40.19784746942187, -105.1499829925106 40.19805283933351, -105.1499887946139 40.1987172693529, -105.1499949388271 40.19942660956755, -105.1499962832889 40.19959051377015, -105.1499982009238 40.19982447013613, -105.1499553999603 40.19980913607915))</t>
+          <t>POLYGON ((-105.14995539996029 40.19980913607915, -105.149964101196 40.20036601195144, -105.14995624827245 40.20039565687276, -105.14996627069075 40.202103645142124, -105.14997027531189 40.20243164381855, -105.14996828123034 40.202822640770705, -105.14997028762116 40.203263637683435, -105.14997126825659 40.203296978511176, -105.17776891324831 40.203322796573914, -105.17801937435783 40.203323004220216, -105.17801710353541 40.202801704472236, -105.17801710249309 40.20280167654974, -105.1780170986384 40.202800754291054, -105.17801709371831 40.20279956093896, -105.17801542943474 40.202407893620894, -105.17801779121167 40.20209443943981, -105.17802942250223 40.200546000945124, -105.17802629338252 40.19946629969199, -105.17802446030292 40.198829998976166, -105.17802446116676 40.198707780333024, -105.17802449531118 40.19858399017504, -105.17802650318933 40.19837698788592, -105.1780338432419 40.19770639666449, -105.17803384485991 40.197706303003145, -105.17803447870367 40.19764486805438, -105.17803444850635 40.19725808820253, -105.17802955459432 40.196807847849385, -105.17804753466176 40.1958009894524, -105.17805114461522 40.195366706687125, -105.17805457246362 40.19495698637294, -105.17805514005646 40.194919209964674, -105.17807544379163 40.19356992676756, -105.1780755436376 40.193559999356225, -105.17807555733003 40.19340999518588, -105.17807567144827 40.19337646219445, -105.17807859931413 40.19253098832572, -105.17809365323973 40.191251980922516, -105.17809489442394 40.19119569292697, -105.17812020849152 40.1900471212033, -105.17813040069217 40.18958464219161, -105.17813057910922 40.189572005883825, -105.17813984185103 40.188096000327775, -105.17813947466566 40.18773489066125, -105.1781394025259 40.187371983227955, -105.17814391040417 40.18733011805361, -105.17814449879961 40.1872194370608, -105.17814052029402 40.18717302076964, -105.17814380934253 40.18681401520618, -105.17814652067545 40.1865180200456, -105.17814989908976 40.18620289633849, -105.1781660473366 40.183162948601826, -105.1781684669265 40.18183643617814, -105.17816845235684 40.18168714946533, -105.1781793654503 40.18059104394589, -105.17818125882629 40.180103036953874, -105.17818251816756 40.179750019985846, -105.17818567538262 40.1794676433639, -105.17819736952283 40.17705081512157, -105.17822498198805 40.17185948877151, -105.178239767373 40.1687701694254, -105.17824497026889 40.1681079937859, -105.17825387066277 40.166953439852975, -105.17357720116361 40.16694246349251, -105.17351120214029 40.16875746475598, -105.17351040741647 40.168768946541746, -105.17348887743452 40.16876895687698, -105.17348767173426 40.1687689579743, -105.17347670137138 40.17058610997677, -105.17347669842927 40.17058819044085, -105.17347682390464 40.170882459647046, -105.1734768197971 40.170884538306424, -105.17336578127112 40.17083213172842, -105.1733576954174 40.17082828027013, -105.17295292310514 40.17063241614367, -105.1728205681745 40.1705683728318, -105.17281951985935 40.170567865507664, -105.16872553406576 40.16858670852341, -105.16872564387377 40.1685916425322, -105.16872310454552 40.168594772176064, -105.16775183505476 40.16979169341922, -105.16774659440881 40.16979815123889, -105.16703566194798 40.17067421828263, -105.16702676636204 40.17067109176306, -105.16702401781235 40.17067447924944, -105.16693320930081 40.17078637943621, -105.16693046074175 40.170789766920294, -105.16688961861706 40.170840092141134, -105.16689855200339 40.17084317464879, -105.16689439550517 40.17084829540469, -105.16688490487608 40.17085999075397, -105.16652019190344 40.17073175740313, -105.1665174951051 40.170730809357224, -105.16641298962311 40.17079382714124, -105.16501996934656 40.17032183177924, -105.16427096003862 40.17007883540592, -105.16421695826051 40.17006083511097, -105.16406795586859 40.169999836081416, -105.16382095262105 40.16989583642651, -105.16371795197493 40.169850837260036, -105.16352094753327 40.169732837889214, -105.16312593987924 40.16948983996239, -105.1622709235831 40.1688868436568, -105.16112090220598 40.16807485153609, -105.16020888468945 40.16741385793949, -105.15991187905757 40.16721485751804, -105.15981187757257 40.167161859684704, -105.15967987604576 40.167120859521454, -105.15952087407739 40.16707385977891, -105.15934987214617 40.16705286010649, -105.15729785399269 40.167029862251646, -105.15626884540481 40.167032862637214, -105.15510783516454 40.16704986397507, -105.15464883003673 40.167055865180814, -105.15464883531652 40.16705898771062, -105.15464799939501 40.16705899872255, -105.15465300027391 40.17018099915842, -105.15465699983194 40.17225799859407, -105.15465699968722 40.17249899848197, -105.15465899956884 40.174172999124174, -105.15465993420452 40.17417298750612, -105.15466208181435 40.17647724158829, -105.15466291310872 40.17736968103145, -105.15466297704683 40.17743779821491, -105.154734010364 40.179712783569634, -105.15477204357396 40.182042768687595, -105.1547760472109 40.182316766887084, -105.15477616244868 40.18231997349721, -105.15477499982585 40.18231999974654, -105.15479200015248 40.18279499845895, -105.15483915763413 40.18279499875759, -105.15483919878406 40.18280146725144, -105.15487519950011 40.18420846777963, -105.15619020065765 40.18420546794748, -105.15634428880844 40.18427100243236, -105.15688556881125 40.184501208637876, -105.15756445158078 40.1847899325708, -105.15807377973265 40.185006541599265, -105.15842910173899 40.18522127318123, -105.15846222860773 40.185239436901334, -105.15846226893584 40.18524309810573, -105.15846388629636 40.18733561945109, -105.15846388900172 40.187338822119585, -105.15846404230035 40.187537221802586, -105.15845909252428 40.18753745755789, -105.15812590102801 40.18755334084461, -105.15695065927703 40.18760411594983, -105.15566395972985 40.18766202520918, -105.15503328354981 40.18768878906563, -105.15502959363067 40.18753811519997, -105.15502951590416 40.18753491771105, -105.1548431219606 40.187545731956156, -105.1548431080552 40.18754893457554, -105.15484199916904 40.18754899881291, -105.15483699936152 40.18865397295026, -105.15483813733722 40.188650725953345, -105.15553088530844 40.18865548209631, -105.15553119994598 40.18866546838077, -105.15554319977937 40.19021346870296, -105.15461720090497 40.18989046922776, -105.1527832001366 40.1899674691564, -105.15262820011681 40.19021446851695, -105.15232620062943 40.19040146942321, -105.1522062000076 40.190440469005694, -105.15203919957837 40.1904544685933, -105.15203919957975 40.1904813219414, -105.15203013299082 40.190480717349, -105.151725130212 40.19045971848809, -105.15105212252408 40.190398720261186, -105.15040011448097 40.19034672131698, -105.1498131075271 40.19030272138396, -105.14964810679093 40.190280721566836, -105.14931910201645 40.19026372260259, -105.1489900989153 40.190263722204605, -105.14868209542068 40.19027472289796, -105.14842409295046 40.19029072383959, -105.14798008906776 40.19036772283105, -105.14752908588154 40.19047172415833, -105.1469560824025 40.19063072326936, -105.14602303916301 40.19095953422137, -105.14589502007333 40.19099873057759, -105.145556198577 40.191102468798725, -105.145540002091 40.19156738941043, -105.1454650795996 40.19166871898251, -105.14468519816758 40.19186346973615, -105.1435901972262 40.191783470032114, -105.14301282274063 40.19170322191939, -105.14221915420819 40.19159290600409, -105.14174119754756 40.191526469547355, -105.14112264465186 40.19153998197216, -105.14098903186539 40.19152972594931, -105.14090403063526 40.19154572658073, -105.14052119664075 40.191553470415776, -105.13957319598613 40.1916054697542, -105.13932331100759 40.19185722614801, -105.1388341967081 40.19234946940898, -105.13904619657231 40.19282347040903, -105.13967019786826 40.19287647006031, -105.14045819689983 40.19310846976347, -105.1420492687273 40.19332518604399, -105.14301319740552 40.193456469624635, -105.14303418006925 40.19346310723986, -105.14301507972189 40.193567711117616, -105.14301423175972 40.19356972952564, -105.14295708071572 40.19370571023295, -105.1429070803512 40.19380370978143, -105.14287908292691 40.193886708733224, -105.14287908966598 40.19388676729531, -105.14289308308324 40.194001707269905, -105.14294308583304 40.194122706234246, -105.14299308839014 40.19419970643524, -105.1430720899324 40.194298705885096, -105.14312209077858 40.19435370620326, -105.14317209314122 40.194446705207795, -105.14322209465014 40.194605703640406, -105.14323609745858 40.194770702696125, -105.14327210006265 40.19491870167863, -105.14330010141141 40.19499570050589, -105.14333610239869 40.195067701157264, -105.14341510441056 40.195155699997926, -105.14350810613891 40.19524369871329, -105.14380911356557 40.19546269709496, -105.14400911786664 40.1956336960499, -105.14438112523962 40.19591869385945, -105.14480413413118 40.19618269030496, -105.14521214125323 40.19636968980674, -105.14568414793975 40.196556687633915, -105.14614315465687 40.19669468522994, -105.14674416354019 40.19682668434852, -105.14734617155419 40.19692568232102, -105.14748217386251 40.19693668216285, -105.14764617537826 40.19693668305129, -105.1479411771563 40.196876682444426, -105.14832185630365 40.19709180819938, -105.1485730402104 40.19710161420416, -105.14897919948483 40.19711747053223, -105.14962634054551 40.19758894297775, -105.1499812003125 40.19784746942187, -105.14998299251059 40.198052839333506, -105.14998879461386 40.1987172693529, -105.14999493882712 40.199426609567546, -105.14999628328891 40.19959051377015, -105.14999820092376 40.19982447013613, -105.14995539996029 40.19980913607915))</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
@@ -5356,7 +5380,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1310621395053 40.20684793765957, -105.1310533021474 40.20968258961523, -105.1310514606757 40.21197482829734, -105.1310367843588 40.21778099139445, -105.1310271676941 40.22006698700108, -105.131026906522 40.22097287970463, -105.1310414344916 40.22436661806086, -105.1310435996392 40.22498920175052, -105.1310556957027 40.22876588192633, -105.1310557011318 40.228778951898, -105.1310774280237 40.23005693691376, -105.1310550515423 40.2314901091419, -105.131073843669 40.23231700085739, -105.1310791128305 40.23325996848013, -105.1311127165956 40.23593409002422, -105.1311584838377 40.23970255416663, -105.1311184824445 40.23985155552562, -105.1310744816857 40.23999555643233, -105.1305200464066 40.24078505036213, -105.1303191943012 40.24105866478993, -105.1299281089684 40.24158722768075, -105.1296491269694 40.24196427322305, -105.1291398434366 40.24265282821231, -105.1289180578097 40.24293463633306, -105.1287650707703 40.24315699900501, -105.1286197377563 40.24338015337015, -105.1285952164659 40.24350423804182, -105.1285607532926 40.243678633234, -105.1286519447919 40.24562528316412, -105.128671190133 40.24608006404942, -105.1286796589799 40.24628019911523, -105.1286864416629 40.24644047056071, -105.1287380090491 40.24689082941862, -105.1298298171615 40.24690390968819, -105.1311740975227 40.24690902238671, -105.1311900138686 40.24714487914462, -105.131150060175 40.25199702365023, -105.1311290184574 40.25356304539059, -105.1311288993839 40.25483897485558, -105.1311310871961 40.25509592524632, -105.1311351527115 40.25553488205652, -105.1311418728351 40.25627690814446, -105.1311493998935 40.25727262246063, -105.1311494053365 40.25820762303031, -105.1311494102614 40.25901562345165, -105.1311514181201 40.2604706245238, -105.1311533315791 40.26130018177933, -105.1311626635374 40.26130017098836, -105.1314776165972 40.2612997953193, -105.1314853591348 40.26129978664688, -105.1342536901744 40.26129684293716, -105.1342613927367 40.26129683485336, -105.1379208885625 40.2612928107571, -105.1379285346962 40.2612928022528, -105.1406108744983 40.26128977971715, -105.1406184806711 40.26128976910978, -105.1429377925196 40.26128640160884, -105.1429453634243 40.26128639073979, -105.1467900194693 40.26128072362639, -105.1467975327648 40.26128071323016, -105.1468465531939 40.26128064035046, -105.1500654098023 40.26127582459359, -105.150072849193 40.26127578314014, -105.1579317739117 40.26123219050455, -105.157939095726 40.26123214999929, -105.1590573513478 40.26121887960556, -105.1590548541795 40.26120439741041, -105.1590403258768 40.26112013450027, -105.1590273950741 40.26104527341096, -105.1589944087731 40.26086126506672, -105.1589371805952 40.26053541613221, -105.1588772703448 40.26029735125145, -105.1587867235447 40.25988310314099, -105.1587732062316 40.25970394070752, -105.1587867913851 40.25946585282338, -105.1588035176399 40.25938480355556, -105.1588050309629 40.25937747332689, -105.1588131688499 40.25926007653372, -105.1590671169694 40.25811957256996, -105.1591639582087 40.2577383241414, -105.1592065673312 40.25762008133739, -105.1592065780735 40.2576200489465, -105.1592073730529 40.25761787627735, -105.1592464000906 40.25751418241698, -105.1593135897142 40.25741741259193, -105.1593850046439 40.25732871936017, -105.1594442707474 40.25727066113117, -105.1594444833865 40.2572704528118, -105.1595811076893 40.2571367624378, -105.1598025509507 40.25693200702809, -105.1599547792698 40.25678485179284, -105.1599989720365 40.25673921994948, -105.1599924986764 40.25659730650925, -105.1605757980321 40.25620359452309, -105.1606064865818 40.25617027131609, -105.1607389143321 40.25602649736401, -105.1607775160145 40.25598497549689, -105.160838322246 40.25591957105722, -105.1609816117556 40.25576544534216, -105.1610295681123 40.25571325316199, -105.16104190423 40.25569596936283, -105.1610768827189 40.25562969209872, -105.1610980231822 40.25558792265264, -105.1611160671059 40.25552193081968, -105.1611188206494 40.25540469905818, -105.1611090626313 40.25537858837161, -105.1610813427591 40.25530659135412, -105.1610515290015 40.25526742410285, -105.1610305136834 40.25524053832483, -105.1608249922877 40.2550751577644, -105.1605874317561 40.25494246474813, -105.1603418083376 40.25483563335776, -105.160341656995 40.25483557437291, -105.1599382833191 40.25468036847293, -105.1597878147295 40.25460896776644, -105.1596523760393 40.25452303893846, -105.1595344547845 40.25439932079264, -105.1594480757986 40.2542614699565, -105.1594480492416 40.25426137441204, -105.1594376867242 40.25422352574407, -105.1594254824308 40.25417719946864, -105.1594193459625 40.25413204204748, -105.1594011116351 40.25399307586693, -105.1594315084507 40.25329819468507, -105.159436146626 40.25319294047603, -105.1595390876333 40.25123395296526, -105.1595390930119 40.25123381788716, -105.1596251227761 40.24914994405553, -105.1596333787975 40.24898333081097, -105.1596334362387 40.24898218808481, -105.1596630831104 40.24838283982047, -105.1597068877074 40.24714470682556, -105.1597140201794 40.24693386583294, -105.1597150691784 40.24686193224582, -105.1596864522177 40.24038181330056, -105.1596852684716 40.24018075544682, -105.1596852663667 40.24018047174287, -105.1596820218607 40.23973500530968, -105.1596793682309 40.23954562245473, -105.1596750332671 40.23923601341176, -105.1596540870133 40.23763600383838, -105.1596522712427 40.23722609101691, -105.1596490939906 40.23651103133323, -105.1596455377918 40.23602956648127, -105.1596411241535 40.23543000233618, -105.159639287903 40.23489116429988, -105.159631111938 40.2326021603701, -105.1596320574399 40.23234954749802, -105.160993003236 40.23233656725746, -105.162829047121 40.2323355569361, -105.1652950423296 40.23231656198064, -105.1660599158641 40.23231118707495, -105.1661308987598 40.2323106876401, -105.1684200036398 40.23229458111676, -105.1691109836499 40.23229392230051, -105.1715299999297 40.2322915883125, -105.1720320179274 40.2322915831708, -105.1720321683417 40.23229158269653, -105.1720667001548 40.23229148153948, -105.1733949514683 40.23228760767522, -105.1746699443099 40.2322976123188, -105.1762842567278 40.23231202562735, -105.1766870186988 40.23231559253281, -105.1776460005625 40.23231260073759, -105.1776563108877 40.23231160004515, -105.1777373000234 40.23228598032479, -105.1777990753533 40.2322360251985, -105.1777991760248 40.23223585886259, -105.1778184627386 40.23220092675904, -105.1778406387775 40.23204779070896, -105.1778499448728 40.23197999479415, -105.1778516407136 40.23142737115413, -105.1778529903291 40.23099711941484, -105.1778535241373 40.23095143561333, -105.1778569786166 40.23065399100331, -105.177865003127 40.22937498989583, -105.1778663526854 40.22919784805772, -105.1778669788484 40.22911209642017, -105.177864540534 40.22467292051728, -105.1778640906119 40.22388898961723, -105.1779001627716 40.21915299099524, -105.1779061013509 40.21831971271479, -105.1779061898209 40.21830724012914, -105.1779222810411 40.216058878454, -105.1779231113842 40.21602719206967, -105.1779391996817 40.21541064063836, -105.1779392003615 40.21541000119228, -105.1779402743808 40.21444507532357, -105.1779462410317 40.21411403975657, -105.1779548545939 40.21285325838544, -105.1779642880199 40.21058111031635, -105.1779642885702 40.21058099413643, -105.1779692945993 40.20951299755229, -105.1779724928907 40.20706829500229, -105.1779725180975 40.20704933316319, -105.1779733735186 40.20641786448409, -105.1779793391662 40.20578677022317, -105.1779985287708 40.20376896198804, -105.1780125892502 40.20344194989982, -105.1780193743578 40.20332300422022, -105.1777689132483 40.20332279657391, -105.1499712682566 40.20329697851118, -105.149971287175 40.20329763873301, -105.149969901152 40.20329763904111, -105.1494542823717 40.20329763897393, -105.1493042800662 40.20329663931438, -105.1491162779991 40.20329663915726, -105.1484382710454 40.20329264098557, -105.1480176142956 40.20329544312548, -105.1475372602013 40.20329864181809, -105.1470852547486 40.20330164222964, -105.1470359037472 40.20329266990918, -105.1470302534053 40.2032916430533, -105.1450462311085 40.20328364593188, -105.1414041879966 40.20328165160092, -105.1406181803717 40.20327465360264, -105.1405783310746 40.20327465404951, -105.1405431778102 40.20327465376817, -105.1404671774334 40.20327365378093, -105.1393501657596 40.20326465486743, -105.1370411375896 40.20324765828751, -105.1356161214376 40.2032486610788, -105.1354471192618 40.20324566162454, -105.1341401040008 40.20322766440542, -105.1338881012024 40.20322866366779, -105.1311050689144 40.20324866892156, -105.1311050050803 40.20325199115882, -105.1311000733982 40.20350866707759, -105.1311260827941 40.20434866191943, -105.1311220944714 40.20525265550346, -105.1311061048515 40.20615965121866, -105.1311011281608 40.2068508539929, -105.1310621395053 40.20684793765957))</t>
+          <t>POLYGON ((-105.13106213950535 40.206847937659575, -105.13105330214738 40.209682589615234, -105.13105146067568 40.21197482829734, -105.13103678435878 40.21778099139445, -105.13102716769413 40.220066987001076, -105.13102690652195 40.22097287970463, -105.13104143449155 40.224366618060856, -105.13104359963918 40.224989201750525, -105.13105569570268 40.22876588192633, -105.13105570113176 40.228778951898, -105.13107742802369 40.23005693691376, -105.13105505154226 40.2314901091419, -105.13107384366901 40.23231700085739, -105.13107911283052 40.23325996848013, -105.13111271659558 40.23593409002422, -105.1311584838377 40.239702554166634, -105.13111848244455 40.23985155552562, -105.13107448168569 40.23999555643233, -105.1305200464066 40.24078505036213, -105.13031919430115 40.24105866478993, -105.12992810896844 40.24158722768075, -105.1296491269694 40.241964273223054, -105.12913984343663 40.24265282821231, -105.12891805780971 40.24293463633306, -105.12876507077029 40.24315699900501, -105.12861973775632 40.24338015337015, -105.12859521646587 40.24350423804182, -105.1285607532926 40.243678633234, -105.12865194479188 40.24562528316412, -105.128671190133 40.246080064049416, -105.12867965897992 40.246280199115226, -105.12868644166295 40.24644047056071, -105.12873800904909 40.24689082941862, -105.12982981716151 40.24690390968819, -105.13117409752275 40.24690902238671, -105.13119001386862 40.24714487914462, -105.131150060175 40.25199702365023, -105.13112901845743 40.25356304539059, -105.13112889938391 40.25483897485558, -105.13113108719612 40.255095925246316, -105.13113515271147 40.255534882056516, -105.13114187283514 40.256276908144464, -105.13114939989346 40.25727262246063, -105.13114940533653 40.25820762303031, -105.13114941026139 40.259015623451646, -105.13115141812011 40.260470624523805, -105.13115333157913 40.26130018177933, -105.13116266353735 40.26130017098836, -105.13147761659718 40.261299795319296, -105.13148535913476 40.26129978664688, -105.13425369017436 40.26129684293716, -105.13426139273669 40.26129683485336, -105.13792088856253 40.2612928107571, -105.13792853469623 40.2612928022528, -105.14061087449828 40.26128977971715, -105.14061848067111 40.26128976910978, -105.1429377925196 40.26128640160884, -105.14294536342435 40.26128639073979, -105.14679001946928 40.26128072362639, -105.14679753276477 40.26128071323016, -105.14684655319391 40.261280640350456, -105.15006540980231 40.26127582459359, -105.15007284919302 40.261275783140135, -105.15793177391167 40.26123219050455, -105.15793909572595 40.261232149999294, -105.15905735134784 40.26121887960556, -105.15905485417952 40.26120439741041, -105.15904032587676 40.261120134500274, -105.15902739507408 40.26104527341096, -105.15899440877313 40.26086126506672, -105.15893718059517 40.26053541613221, -105.1588772703448 40.26029735125145, -105.15878672354474 40.25988310314099, -105.15877320623163 40.25970394070752, -105.15878679138505 40.25946585282338, -105.1588035176399 40.259384803555555, -105.15880503096291 40.259377473326886, -105.15881316884987 40.25926007653372, -105.15906711696941 40.25811957256996, -105.15916395820871 40.2577383241414, -105.15920656733118 40.257620081337386, -105.15920657807348 40.2576200489465, -105.15920737305285 40.25761787627735, -105.1592464000906 40.257514182416976, -105.15931358971419 40.25741741259193, -105.15938500464394 40.257328719360174, -105.1594442707474 40.25727066113117, -105.15944448338654 40.2572704528118, -105.15958110768928 40.257136762437796, -105.15980255095073 40.25693200702809, -105.15995477926982 40.25678485179284, -105.15999897203646 40.25673921994948, -105.15999249867636 40.25659730650925, -105.16057579803207 40.25620359452309, -105.1606064865818 40.256170271316094, -105.16073891433206 40.25602649736401, -105.1607775160145 40.25598497549689, -105.16083832224595 40.25591957105722, -105.16098161175556 40.255765445342156, -105.16102956811226 40.25571325316199, -105.16104190423002 40.255695969362826, -105.1610768827189 40.25562969209872, -105.16109802318218 40.255587922652644, -105.16111606710592 40.25552193081968, -105.16111882064938 40.255404699058175, -105.16110906263125 40.255378588371606, -105.16108134275909 40.25530659135412, -105.1610515290015 40.25526742410285, -105.16103051368343 40.25524053832483, -105.16082499228769 40.255075157764395, -105.16058743175611 40.25494246474813, -105.1603418083376 40.25483563335776, -105.16034165699497 40.25483557437291, -105.15993828331905 40.25468036847293, -105.15978781472954 40.254608967766444, -105.15965237603928 40.25452303893846, -105.15953445478448 40.25439932079264, -105.1594480757986 40.254261469956504, -105.15944804924163 40.25426137441204, -105.15943768672423 40.25422352574407, -105.15942548243076 40.25417719946864, -105.1594193459625 40.25413204204748, -105.15940111163513 40.25399307586693, -105.1594315084507 40.25329819468507, -105.159436146626 40.25319294047603, -105.15953908763332 40.251233952965265, -105.15953909301187 40.25123381788716, -105.15962512277606 40.24914994405553, -105.15963337879754 40.248983330810965, -105.15963343623875 40.24898218808481, -105.15966308311042 40.248382839820465, -105.15970688770742 40.24714470682556, -105.15971402017936 40.246933865832936, -105.15971506917836 40.24686193224582, -105.15968645221767 40.24038181330056, -105.1596852684716 40.24018075544682, -105.15968526636668 40.240180471742875, -105.15968202186066 40.23973500530968, -105.15967936823093 40.23954562245473, -105.15967503326708 40.239236013411755, -105.15965408701334 40.23763600383838, -105.15965227124268 40.237226091016915, -105.15964909399057 40.23651103133323, -105.15964553779179 40.23602956648127, -105.15964112415352 40.23543000233618, -105.159639287903 40.23489116429988, -105.15963111193798 40.2326021603701, -105.15963205743985 40.232349547498025, -105.160993003236 40.23233656725746, -105.16282904712098 40.2323355569361, -105.16529504232963 40.23231656198064, -105.16605991586405 40.23231118707495, -105.16613089875979 40.2323106876401, -105.1684200036398 40.23229458111676, -105.16911098364986 40.232293922300514, -105.1715299999297 40.2322915883125, -105.17203201792735 40.2322915831708, -105.17203216834172 40.23229158269653, -105.17206670015476 40.232291481539484, -105.17339495146831 40.23228760767522, -105.17466994430987 40.2322976123188, -105.17628425672778 40.23231202562735, -105.17668701869876 40.232315592532814, -105.17764600056253 40.23231260073759, -105.1776563108877 40.23231160004515, -105.17773730002344 40.23228598032479, -105.1777990753533 40.2322360251985, -105.17779917602482 40.23223585886259, -105.17781846273856 40.23220092675904, -105.17784063877747 40.23204779070896, -105.17784994487276 40.23197999479415, -105.17785164071356 40.231427371154126, -105.17785299032911 40.230997119414845, -105.1778535241373 40.23095143561333, -105.17785697861656 40.23065399100331, -105.17786500312704 40.22937498989583, -105.17786635268537 40.229197848057716, -105.17786697884839 40.229112096420174, -105.17786454053405 40.22467292051728, -105.17786409061186 40.22388898961723, -105.17790016277155 40.21915299099524, -105.17790610135093 40.21831971271479, -105.17790618982087 40.21830724012914, -105.1779222810411 40.216058878454, -105.17792311138416 40.21602719206967, -105.17793919968172 40.21541064063836, -105.17793920036152 40.21541000119228, -105.17794027438083 40.21444507532357, -105.17794624103169 40.214114039756566, -105.1779548545939 40.212853258385444, -105.17796428801988 40.210581110316355, -105.17796428857021 40.21058099413643, -105.17796929459932 40.20951299755229, -105.1779724928907 40.207068295002294, -105.17797251809748 40.20704933316319, -105.1779733735186 40.20641786448409, -105.17797933916623 40.20578677022317, -105.17799852877081 40.20376896198804, -105.17801258925016 40.20344194989982, -105.17801937435783 40.203323004220216, -105.17776891324831 40.203322796573914, -105.14997126825659 40.203296978511176, -105.14997128717502 40.20329763873301, -105.14996990115196 40.20329763904111, -105.14945428237165 40.20329763897393, -105.14930428006622 40.20329663931438, -105.14911627799906 40.20329663915726, -105.14843827104538 40.20329264098557, -105.14801761429563 40.203295443125484, -105.14753726020133 40.203298641818094, -105.14708525474862 40.20330164222964, -105.14703590374715 40.20329266990918, -105.14703025340529 40.2032916430533, -105.14504623110852 40.203283645931876, -105.14140418799663 40.203281651600925, -105.14061818037173 40.20327465360264, -105.14057833107458 40.20327465404951, -105.14054317781024 40.20327465376817, -105.1404671774334 40.20327365378093, -105.13935016575962 40.203264654867425, -105.13704113758965 40.20324765828751, -105.13561612143764 40.203248661078796, -105.13544711926178 40.203245661624536, -105.13414010400083 40.20322766440542, -105.13388810120243 40.20322866366779, -105.13110506891444 40.20324866892156, -105.13110500508029 40.203251991158815, -105.13110007339816 40.20350866707759, -105.13112608279408 40.20434866191943, -105.13112209447138 40.205252655503465, -105.13110610485151 40.206159651218655, -105.13110112816078 40.206850853992904, -105.13106213950535 40.206847937659575))</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
@@ -5398,7 +5422,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1025008330252 40.20329617878833, -105.1024844022742 40.20329565938531, -105.1024151901731 40.20329347428748, -105.1018971891388 40.2032814736801, -105.1018961897053 40.20421247454206, -105.1022201967591 40.20421818627374, -105.1025107002389 40.20422331812248, -105.1025210625498 40.20515181087357, -105.1025237619839 40.20539370203086, -105.1025237636843 40.20571670054039, -105.1025437709455 40.20634669622018, -105.1025137811899 40.20727069089985, -105.1025047847938 40.20772268878633, -105.102465788828 40.20820268604596, -105.102494799139 40.20914168066236, -105.1024778062865 40.2099546758207, -105.1024751480868 40.2103992398415, -105.1023781912976 40.21039966129107, -105.1020764826853 40.210400971623, -105.0978221643321 40.21038836945402, -105.0978192865362 40.20995801171471, -105.0978192638643 40.20995469549757, -105.0978192166669 40.20994758211779, -105.0977981954315 40.20680406130543, -105.0977981545344 40.20679786929404, -105.0976247893968 40.20679703029651, -105.0976247948587 40.20679491652393, -105.0971607119664 40.20679337303581, -105.0971599989639 40.20679337055231, -105.0954331146536 40.20678761374383, -105.0932545485407 40.20678031284936, -105.0932022136999 40.20678056108493, -105.0932041876712 40.206406475457, -105.0932105779957 40.2051159902964, -105.0932147345931 40.20427675894129, -105.0932201875574 40.20317547481145, -105.0930820960962 40.20317412349315, -105.0930711835685 40.20317401664741, -105.093005727191 40.20317337651804, -105.0930057234746 40.2031730162505, -105.0928657727666 40.20317203549725, -105.0926146724067 40.20317027581347, -105.0921975370513 40.20316735111282, -105.0919455217571 40.20316558314721, -105.0917522278974 40.20316422728517, -105.0914944937617 40.2031624183343, -105.0912832223234 40.20316093513956, -105.0908696894022 40.20316115619768, -105.0904716416781 40.20316441172043, -105.0897408380637 40.20317038475633, -105.0888532544556 40.20317763229867, -105.0877735888691 40.20318643920209, -105.0856452363401 40.20320449042337, -105.0856447171358 40.20320449576815, -105.0837211863008 40.203227474651, -105.0835981069327 40.20321967515504, -105.0835791856489 40.20321847582563, -105.0830682814023 40.2032196909061, -105.0822069163204 40.20323024316917, -105.0816501847357 40.20324047561559, -105.0806879610338 40.20324837306046, -105.0798893828385 40.20325404710055, -105.0790784726884 40.20326612110446, -105.0788240199679 40.20327306536132, -105.0787342713654 40.20327551513552, -105.0783672903983 40.20327647528878, -105.0783671987761 40.20327647585538, -105.0779601843807 40.2032754757722, -105.0776037795497 40.20327547779507, -105.0765138346332 40.20327584447682, -105.0747471835121 40.20329593233741, -105.074174153481 40.20330244200157, -105.0741613829224 40.20330268048043, -105.0741578445987 40.20330274940949, -105.0740449135742 40.20330506064477, -105.074014699015 40.20330567887017, -105.0690749998827 40.2033999992119, -105.067296999437 40.20343799958135, -105.0662489993874 40.20346199884766, -105.0650095092602 40.20349053724983, -105.0649459997082 40.20349199875547, -105.0647999996946 40.20349499884104, -105.0647763071737 40.20349548788953, -105.0647501006766 40.20349602781442, -105.0647029999319 40.20349699885044, -105.0625290002004 40.20354499890966, -105.0605809999359 40.20358599860956, -105.0604691792169 40.20358828730067, -105.0594589803057 40.20360895889921, -105.0594569996611 40.2036089990881, -105.0594407995711 40.20360935166872, -105.058538999233 40.20362899881254, -105.0583553984353 40.20363396552585, -105.056911999972 40.20367299893432, -105.0558368854482 40.20367580791534, -105.0557639998678 40.20367599809817, -105.0557612194496 40.20367601713887, -105.0551933208667 40.20367993430043, -105.0551658094086 40.20367990683798, -105.0551658095187 40.20368024908086, -105.0551659250086 40.20376457266076, -105.0551659295546 40.20376782758404, -105.0551748699924 40.2109485718148, -105.055174874339 40.21095185735524, -105.055175144372 40.21195298746794, -105.055175145165 40.21195627749737, -105.0551768073136 40.21818594070018, -105.0551754907823 40.21826647950752, -105.0551754375666 40.2182695846955, -105.0551754353958 40.21826973689463, -105.055165657996 40.21908808908051, -105.0551656190208 40.21909135193408, -105.055154576327 40.22001719721558, -105.0551545759616 40.22001725305361, -105.0550521966061 40.22547075966209, -105.0550521333209 40.22547414490511, -105.055084557513 40.2318932132323, -105.0550845739097 40.2318966321016, -105.0550890166748 40.23277390435145, -105.0549114469985 40.23973943660069, -105.0549113570069 40.23974294872203, -105.0549124708876 40.2398219348914, -105.0549125264558 40.23982547279036, -105.0550781606866 40.24716273015109, -105.0550786266126 40.24742526243025, -105.0550786320396 40.24742874159061, -105.0550893173981 40.25453828145123, -105.0550893227732 40.25454176871278, -105.055089102158 40.2561198963567, -105.0550882881114 40.26180786511199, -105.0550981174537 40.26181467832726, -105.0645770650161 40.26171970004614, -105.0645857591206 40.26171962647721, -105.0648359236269 40.26171750422144, -105.0740535654481 40.26163893567075, -105.0823658167984 40.26158485138247, -105.0828514814461 40.26158169068106, -105.0834070961972 40.26157807633273, -105.0834155232793 40.26157802110299, -105.0835143486308 40.2615773824463, -105.0835227733561 40.26157732810092, -105.0835787990881 40.26157696408129, -105.0835872226432 40.26157690882633, -105.085095114039 40.2615670067869, -105.0880010516577 40.26154792095951, -105.0880094105433 40.26154786605323, -105.093112518724 40.26151415207208, -105.0931208000076 40.26151409742457, -105.0998980221863 40.26146897484655, -105.0999062011835 40.26146891936003, -105.1000146066554 40.261468190755, -105.1000227844769 40.26146813525616, -105.1005771055564 40.26146440970788, -105.1005852751427 40.26146435504149, -105.100960609353 40.26146184446047, -105.1009687718798 40.26146179064328, -105.1024397379435 40.26145193344261, -105.1024478793076 40.26145187944849, -105.1026625533545 40.26145053973125, -105.1029236626631 40.26145078371452, -105.1029318436331 40.2614507919655, -105.1055683013489 40.26145324602741, -105.1055764423602 40.26145325215404, -105.1057125353351 40.26145336277992, -105.1057206751605 40.26145337069362, -105.1084594708947 40.26145588500171, -105.108467570751 40.26145589258702, -105.1100495048815 40.26145728993158, -105.1100575800509 40.26145729732243, -105.1122869928654 40.26145921342841, -105.1122949779269 40.26145914831125, -105.114256210008 40.26144303760103, -105.1142641668518 40.26144297225395, -105.1157171297533 40.26143107517082, -105.1157250642582 40.26143100964919, -105.1157347810537 40.26143093023018, -105.115742714383 40.26143086470346, -105.1177053612486 40.26141472727208, -105.121707037398 40.26138182410287, -105.1217148802063 40.26138175606975, -105.1302096472331 40.26130835111636, -105.1302173595303 40.26130828299087, -105.1302183188658 40.26130827434753, -105.1302260335092 40.26130820712956, -105.1306741940863 40.26130429907008, -105.1306819028509 40.26130423180297, -105.1310475630141 40.26130104431788, -105.1310552670561 40.26130098061338, -105.1310555398049 40.26130097878088, -105.1311533315791 40.26130018177933, -105.1311533230373 40.26129655853457, -105.1311514181201 40.2604706245238, -105.1311494102614 40.25901562345165, -105.1311494053365 40.25820762303031, -105.1311493998935 40.25727262246063, -105.1311418728351 40.25627690814446, -105.1311351527115 40.25553488205652, -105.1311310871961 40.25509592524632, -105.1311288993839 40.25483897485558, -105.1311290184574 40.25356304539059, -105.131150060175 40.25199702365023, -105.1311900138686 40.24714487914462, -105.1311740975227 40.24690902238671, -105.1298298171615 40.24690390968819, -105.1287380090491 40.24689082941862, -105.1286864416629 40.24644047056071, -105.1286796589799 40.24628019911523, -105.128671190133 40.24608006404942, -105.1286519447919 40.24562528316412, -105.1285607532926 40.243678633234, -105.1285952164659 40.24350423804182, -105.1286197377563 40.24338015337015, -105.1287650707703 40.24315699900501, -105.1289180578097 40.24293463633306, -105.1291398434366 40.24265282821231, -105.1296491269694 40.24196427322305, -105.1299281089684 40.24158722768075, -105.1303191943012 40.24105866478993, -105.1305200464066 40.24078505036213, -105.1310744816857 40.23999555643233, -105.1311184824445 40.23985155552562, -105.1311584838377 40.23970255416663, -105.1311127165956 40.23593409002422, -105.1310791128305 40.23325996848013, -105.131073843669 40.23231700085739, -105.1310550515423 40.2314901091419, -105.1310774280237 40.23005693691376, -105.1310557011318 40.228778951898, -105.1310556957027 40.22876588192633, -105.1310435996392 40.22498920175052, -105.1310414344916 40.22436661806086, -105.131026906522 40.22097287970463, -105.1310271676941 40.22006698700108, -105.1310367843588 40.21778099139445, -105.1310514606757 40.21197482829734, -105.1310533021474 40.20968258961523, -105.13106209839 40.20686114262469, -105.1308211106778 40.20685958646517, -105.1298610279341 40.20685338449566, -105.1267617702838 40.20683330727967, -105.1263251952959 40.20683047273798, -105.1263252134739 40.20681968499972, -105.1263252377158 40.20680501554748, -105.126325383258 40.20671719607243, -105.1263273198157 40.20555140862761, -105.1263288168892 40.20465044754024, -105.1263293100186 40.20435383414205, -105.1263296824622 40.20412961875567, -105.1263299835551 40.20394852101509, -105.1263302867637 40.20376618310218, -105.1263306224686 40.20356382598065, -105.1263307358341 40.20349575097127, -105.1263309880781 40.20334363097754, -105.1263310249341 40.20332110892354, -105.1263310707939 40.20329352893387, -105.1263311072719 40.20327150312825, -105.1263311477963 40.20324703121165, -105.1263311955124 40.20321847223759, -105.1263100144433 40.20321840109568, -105.1263099741148 40.20321163359582, -105.1263099548083 40.20320830748921, -105.1248379976579 40.20320367781203, -105.1248368677285 40.20320367234526, -105.1239909869865 40.20319968052207, -105.1225519696027 40.20318968180091, -105.1220259643586 40.20319068285817, -105.1215602059391 40.20318796272678, -105.1215591626463 40.20345390870822, -105.1214718525096 40.20679480657027, -105.1213741436619 40.21041936286073, -105.1159566603877 40.21041252952389, -105.1159557476378 40.21041252829438, -105.1155192744741 40.21041196710615, -105.1155087349688 40.21041195368512, -105.1155957253303 40.2034586936532, -105.1155968269777 40.20318946052415, -105.1155357402171 40.20318939435722, -105.1151857766577 40.20318901124353, -105.1134346468925 40.20318708080785, -105.1125030266368 40.20318604347585, -105.111056502299 40.20319290306869, -105.1108060990517 40.2031948859403, -105.1098898104245 40.20319715386316, -105.1091350909051 40.20319674093735, -105.1077521907158 40.20319147334009, -105.1073079789816 40.20321240066425, -105.1064851728413 40.20325111772296, -105.1054421903556 40.20329947399756, -105.1053837709425 40.20329941517127, -105.1053409606589 40.20329937175753, -105.1052308076059 40.2032992596835, -105.105123135279 40.20329915147183, -105.1043405998986 40.20329835559978, -105.1030852803135 40.20329706845792, -105.1026765488442 40.20329664572056, -105.1025008330252 40.20329617878833))</t>
+          <t>POLYGON ((-105.10250083302522 40.20329617878833, -105.10248440227421 40.20329565938531, -105.10241519017313 40.203293474287484, -105.10189718913881 40.2032814736801, -105.1018961897053 40.20421247454206, -105.10222019675915 40.20421818627374, -105.10251070023885 40.20422331812248, -105.10252106254977 40.20515181087357, -105.10252376198393 40.20539370203086, -105.1025237636843 40.205716700540385, -105.10254377094547 40.20634669622018, -105.10251378118986 40.207270690899854, -105.10250478479384 40.207722688786326, -105.102465788828 40.208202686045965, -105.10249479913901 40.209141680662356, -105.10247780628652 40.2099546758207, -105.10247514808682 40.2103992398415, -105.10237819129762 40.21039966129107, -105.10207648268533 40.210400971622995, -105.09782216433213 40.21038836945402, -105.09781928653622 40.20995801171471, -105.09781926386432 40.20995469549757, -105.09781921666689 40.20994758211779, -105.09779819543148 40.206804061305434, -105.09779815453437 40.20679786929404, -105.09762478939679 40.20679703029651, -105.09762479485875 40.206794916523926, -105.09716071196644 40.206793373035815, -105.09715999896386 40.20679337055231, -105.09543311465357 40.206787613743835, -105.09325454854073 40.20678031284936, -105.09320221369985 40.20678056108493, -105.09320418767116 40.206406475457, -105.09321057799566 40.2051159902964, -105.09321473459312 40.20427675894129, -105.0932201875574 40.203175474811445, -105.09308209609623 40.20317412349315, -105.09307118356853 40.20317401664741, -105.09300572719101 40.203173376518045, -105.09300572347459 40.203173016250496, -105.09286577276664 40.20317203549725, -105.09261467240674 40.20317027581347, -105.09219753705133 40.20316735111282, -105.09194552175714 40.20316558314721, -105.09175222789742 40.20316422728517, -105.09149449376167 40.2031624183343, -105.09128322232336 40.203160935139564, -105.09086968940224 40.20316115619768, -105.09047164167815 40.20316441172043, -105.08974083806369 40.203170384756326, -105.08885325445559 40.20317763229867, -105.08777358886908 40.203186439202085, -105.08564523634008 40.20320449042337, -105.08564471713582 40.203204495768155, -105.08372118630079 40.203227474651, -105.0835981069327 40.20321967515504, -105.0835791856489 40.20321847582563, -105.08306828140232 40.2032196909061, -105.08220691632043 40.20323024316917, -105.08165018473568 40.203240475615594, -105.0806879610338 40.20324837306046, -105.07988938283849 40.20325404710055, -105.0790784726884 40.203266121104456, -105.07882401996785 40.20327306536132, -105.07873427136538 40.203275515135516, -105.07836729039832 40.20327647528878, -105.0783671987761 40.20327647585538, -105.0779601843807 40.2032754757722, -105.07760377954972 40.203275477795074, -105.07651383463325 40.20327584447682, -105.0747471835121 40.20329593233741, -105.07417415348101 40.20330244200157, -105.07416138292244 40.20330268048043, -105.07415784459874 40.20330274940949, -105.0740449135742 40.203305060644766, -105.07401469901501 40.203305678870166, -105.06907499988272 40.2033999992119, -105.06729699943696 40.203437999581354, -105.0662489993874 40.20346199884766, -105.06500950926018 40.20349053724983, -105.06494599970824 40.20349199875547, -105.06479999969461 40.203494998841045, -105.06477630717366 40.20349548788953, -105.06475010067658 40.20349602781442, -105.06470299993185 40.20349699885044, -105.06252900020037 40.20354499890966, -105.06058099993591 40.20358599860956, -105.06046917921685 40.20358828730067, -105.05945898030575 40.20360895889921, -105.05945699966105 40.2036089990881, -105.05944079957108 40.20360935166872, -105.05853899923298 40.20362899881254, -105.05835539843525 40.203633965525846, -105.05691199997196 40.203672998934316, -105.05583688544822 40.20367580791534, -105.05576399986776 40.20367599809817, -105.05576121944962 40.20367601713887, -105.05519332086666 40.20367993430043, -105.0551658094086 40.203679906837976, -105.05516580951867 40.20368024908086, -105.05516592500855 40.20376457266076, -105.0551659295546 40.20376782758404, -105.05517486999237 40.210948571814804, -105.05517487433897 40.21095185735524, -105.055175144372 40.21195298746794, -105.055175145165 40.21195627749737, -105.05517680731361 40.21818594070018, -105.05517549078228 40.21826647950752, -105.0551754375666 40.2182695846955, -105.05517543539581 40.218269736894634, -105.05516565799599 40.21908808908051, -105.0551656190208 40.219091351934075, -105.055154576327 40.220017197215576, -105.05515457596158 40.22001725305361, -105.05505219660614 40.225470759662095, -105.05505213332091 40.22547414490511, -105.05508455751303 40.231893213232304, -105.05508457390972 40.2318966321016, -105.05508901667478 40.23277390435145, -105.05491144699855 40.239739436600686, -105.05491135700692 40.23974294872203, -105.0549124708876 40.239821934891395, -105.05491252645577 40.23982547279036, -105.05507816068665 40.24716273015109, -105.05507862661258 40.24742526243025, -105.0550786320396 40.24742874159061, -105.05508931739814 40.254538281451225, -105.05508932277324 40.254541768712784, -105.05508910215801 40.2561198963567, -105.05508828811143 40.26180786511199, -105.05509811745374 40.26181467832726, -105.06457706501607 40.261719700046136, -105.0645857591206 40.26171962647721, -105.0648359236269 40.261717504221444, -105.07405356544814 40.261638935670746, -105.08236581679843 40.26158485138247, -105.08285148144613 40.26158169068106, -105.0834070961972 40.261578076332725, -105.08341552327934 40.26157802110299, -105.08351434863081 40.261577382446305, -105.0835227733561 40.26157732810092, -105.0835787990881 40.26157696408129, -105.08358722264325 40.26157690882633, -105.085095114039 40.261567006786905, -105.08800105165774 40.26154792095951, -105.0880094105433 40.26154786605323, -105.093112518724 40.26151415207208, -105.09312080000764 40.261514097424566, -105.09989802218627 40.26146897484655, -105.09990620118354 40.261468919360034, -105.10001460665542 40.261468190755004, -105.10002278447689 40.26146813525616, -105.10057710555644 40.261464409707884, -105.1005852751427 40.26146435504149, -105.10096060935297 40.26146184446047, -105.10096877187979 40.26146179064328, -105.10243973794354 40.26145193344261, -105.10244787930759 40.261451879448494, -105.10266255335452 40.26145053973125, -105.10292366266313 40.26145078371452, -105.10293184363312 40.2614507919655, -105.10556830134885 40.261453246027415, -105.10557644236022 40.26145325215404, -105.10571253533509 40.26145336277992, -105.10572067516048 40.261453370693616, -105.10845947089472 40.26145588500171, -105.10846757075103 40.261455892587016, -105.11004950488146 40.26145728993158, -105.1100575800509 40.26145729732243, -105.11228699286545 40.26145921342841, -105.11229497792694 40.26145914831125, -105.11425621000802 40.26144303760103, -105.11426416685183 40.26144297225395, -105.11571712975328 40.26143107517082, -105.11572506425824 40.261431009649186, -105.11573478105366 40.26143093023018, -105.11574271438302 40.26143086470346, -105.11770536124857 40.26141472727208, -105.12170703739801 40.26138182410287, -105.12171488020631 40.261381756069746, -105.13020964723314 40.261308351116355, -105.13021735953032 40.26130828299087, -105.13021831886579 40.26130827434753, -105.13022603350922 40.26130820712956, -105.13067419408625 40.26130429907008, -105.13068190285092 40.261304231802974, -105.13104756301406 40.261301044317875, -105.13105526705613 40.261300980613385, -105.13105553980488 40.26130097878088, -105.13115333157913 40.26130018177933, -105.13115332303731 40.261296558534575, -105.13115141812011 40.260470624523805, -105.13114941026139 40.259015623451646, -105.13114940533653 40.25820762303031, -105.13114939989346 40.25727262246063, -105.13114187283514 40.256276908144464, -105.13113515271147 40.255534882056516, -105.13113108719612 40.255095925246316, -105.13112889938391 40.25483897485558, -105.13112901845743 40.25356304539059, -105.131150060175 40.25199702365023, -105.13119001386862 40.24714487914462, -105.13117409752275 40.24690902238671, -105.12982981716151 40.24690390968819, -105.12873800904909 40.24689082941862, -105.12868644166295 40.24644047056071, -105.12867965897992 40.246280199115226, -105.128671190133 40.246080064049416, -105.12865194479188 40.24562528316412, -105.1285607532926 40.243678633234, -105.12859521646587 40.24350423804182, -105.12861973775632 40.24338015337015, -105.12876507077029 40.24315699900501, -105.12891805780971 40.24293463633306, -105.12913984343663 40.24265282821231, -105.1296491269694 40.241964273223054, -105.12992810896844 40.24158722768075, -105.13031919430115 40.24105866478993, -105.1305200464066 40.24078505036213, -105.13107448168569 40.23999555643233, -105.13111848244455 40.23985155552562, -105.1311584838377 40.239702554166634, -105.13111271659558 40.23593409002422, -105.13107911283052 40.23325996848013, -105.13107384366901 40.23231700085739, -105.13105505154226 40.2314901091419, -105.13107742802369 40.23005693691376, -105.13105570113176 40.228778951898, -105.13105569570268 40.22876588192633, -105.13104359963918 40.224989201750525, -105.13104143449155 40.224366618060856, -105.13102690652195 40.22097287970463, -105.13102716769413 40.220066987001076, -105.13103678435878 40.21778099139445, -105.13105146067568 40.21197482829734, -105.13105330214738 40.209682589615234, -105.13106209839 40.20686114262469, -105.13082111067781 40.20685958646517, -105.12986102793406 40.20685338449566, -105.12676177028384 40.20683330727967, -105.12632519529588 40.206830472737984, -105.12632521347393 40.20681968499972, -105.12632523771585 40.20680501554748, -105.12632538325799 40.206717196072425, -105.1263273198157 40.20555140862761, -105.12632881688923 40.20465044754024, -105.12632931001856 40.20435383414205, -105.12632968246217 40.204129618755665, -105.12632998355507 40.203948521015086, -105.12633028676366 40.203766183102175, -105.12633062246864 40.20356382598065, -105.12633073583407 40.20349575097127, -105.12633098807805 40.203343630977535, -105.12633102493409 40.20332110892354, -105.12633107079388 40.20329352893387, -105.12633110727187 40.20327150312825, -105.1263311477963 40.203247031211646, -105.12633119551245 40.20321847223759, -105.1263100144433 40.20321840109568, -105.12630997411478 40.20321163359582, -105.12630995480828 40.203208307489206, -105.12483799765788 40.20320367781203, -105.12483686772846 40.20320367234526, -105.12399098698651 40.20319968052207, -105.12255196960265 40.20318968180091, -105.1220259643586 40.20319068285817, -105.12156020593909 40.20318796272678, -105.12155916264626 40.20345390870822, -105.12147185250961 40.20679480657027, -105.12137414366192 40.21041936286073, -105.11595666038768 40.210412529523886, -105.11595574763777 40.21041252829438, -105.11551927447411 40.21041196710615, -105.11550873496881 40.210411953685124, -105.11559572533034 40.2034586936532, -105.11559682697765 40.20318946052415, -105.11553574021708 40.203189394357224, -105.11518577665774 40.20318901124353, -105.11343464689254 40.20318708080785, -105.11250302663682 40.203186043475846, -105.11105650229896 40.20319290306869, -105.1108060990517 40.2031948859403, -105.10988981042452 40.20319715386316, -105.10913509090508 40.20319674093735, -105.1077521907158 40.20319147334009, -105.10730797898162 40.20321240066425, -105.10648517284133 40.20325111772296, -105.10544219035563 40.20329947399756, -105.10538377094248 40.203299415171266, -105.10534096065894 40.20329937175753, -105.10523080760592 40.2032992596835, -105.10512313527902 40.20329915147183, -105.10434059989859 40.203298355599784, -105.10308528031346 40.20329706845792, -105.10267654884422 40.20329664572056, -105.10250083302522 40.20329617878833))</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
@@ -5440,7 +5464,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.1999431444402 40.09446928464906, -105.20004901646 40.0944713051883, -105.2000942419318 40.09447216840297, -105.2004028346573 40.09447194731246, -105.2020925487541 40.09447072187066, -105.204067954345 40.09447526321931, -105.206084292794 40.09448027846468, -105.2067696857456 40.09448197611559, -105.2067688747363 40.09435139755085, -105.2069747075104 40.09435044215074, -105.2068623764414 40.07451341961843, -105.2068647486335 40.07396214178695, -105.2068677753563 40.07325874343877, -105.2068798224365 40.07280181856465, -105.2068465057981 40.07117836077267, -105.2067702438353 40.07117795720276, -105.2063513217104 40.07118051817727, -105.2062419806407 40.0711939631236, -105.2060310188561 40.07122691751993, -105.2058299486888 40.07128597501093, -105.2056899679546 40.07134793401426, -105.205479003384 40.07146406586098, -105.2052689409496 40.0716189076843, -105.2045168221222 40.07234912431174, -105.2042239527948 40.07256387047889, -105.2040609420013 40.07266200516737, -105.2038830407287 40.07273292346781, -105.2038469064714 40.07274298737001, -105.2036409100057 40.07278308778325, -105.2032059353273 40.07280695141796, -105.2030440636358 40.07280708357413, -105.2021660596678 40.07281690086156, -105.2011680960696 40.07280306606555, -105.1998038607809 40.07279101579683, -105.1982398337714 40.07278913325598, -105.1979078919024 40.07278497129465, -105.1977160136586 40.07278309635792, -105.1971160825409 40.07277713118252, -105.1970328286375 40.07277608949424, -105.1969338538223 40.07277500556847, -105.1968731121383 40.07277402287241, -105.1967158901643 40.07277306047437, -105.1965590232563 40.07277292288894, -105.195948214593 40.07277500006112, -105.1959218927785 40.07277508923514, -105.1955909649218 40.07278409976774, -105.1948670366262 40.07277889370809, -105.1942781733234 40.07277486502355, -105.194183128132 40.07277406474559, -105.1940641417293 40.07277292533653, -105.1938518906687 40.07277208786569, -105.1938520922997 40.07267139500048, -105.1917239390811 40.07265964144332, -105.1893946744375 40.07264673391924, -105.1880841936159 40.07263945058795, -105.1880706438702 40.07136436642797, -105.1880671940498 40.06913144933019, -105.185800786321 40.06912764169806, -105.1839211916622 40.06912445053024, -105.1832611922969 40.06912044991955, -105.1833961920323 40.06889744939709, -105.1837501921285 40.06857045028935, -105.1838490101667 40.06846881885282, -105.183740034292 40.06856390986091, -105.1831601619173 40.06817113054244, -105.1831270176412 40.06815292118763, -105.1829580021636 40.06807806249881, -105.1827810018886 40.06803008491246, -105.1825171400026 40.06799010278778, -105.1823828306993 40.06798204711436, -105.181714937013 40.06800107072923, -105.1812873206927 40.06800015368258, -105.181286191659 40.06800644970687, -105.1812891923216 40.06915245055091, -105.1792591686312 40.06913657318423, -105.1785051917741 40.06913045045798, -105.1784950725557 40.06913121664342, -105.1785070374569 40.06989596523194, -105.1785168294514 40.07054687553875, -105.1785170121184 40.0705839359631, -105.1785009334851 40.07240092923784, -105.1784958444745 40.07272210092214, -105.1784700126258 40.07272244957001, -105.1784681917568 40.07272945154712, -105.1784741913036 40.07290045107155, -105.1801665604356 40.07291007946497, -105.1814644385908 40.0729143637982, -105.1829851934239 40.07288645145971, -105.1835708587782 40.07288929420034, -105.1853123095948 40.07290014352606, -105.186579245816 40.07290802007324, -105.1880889785409 40.07291738748686, -105.1891170700742 40.07291393943083, -105.1910141758257 40.07290737187865, -105.1926061727062 40.07290183614763, -105.1938631961004 40.07289745028993, -105.1938671953461 40.07375044969388, -105.1939091944498 40.07392045037489, -105.1939661962362 40.07404145051328, -105.1941301947049 40.07448244993503, -105.1942701949712 40.07470545027712, -105.1944961955827 40.07523545057487, -105.1944861950927 40.07535544988587, -105.1944611949431 40.07540045034644, -105.1945641953128 40.0754304506349, -105.1942621963568 40.07595945108564, -105.1935500196004 40.07569382935834, -105.1930686556212 40.07551448774536, -105.1929101955311 40.07545545029699, -105.1924521950065 40.07516645038263, -105.1921041958643 40.07508645023321, -105.1919231953974 40.0750234505873, -105.1914101946249 40.07502445075971, -105.1910911942501 40.07506045112101, -105.1908421948001 40.07505445084159, -105.1908321947982 40.07508045099295, -105.1908181943892 40.07512045091352, -105.1908111950647 40.07514245121535, -105.1908011950725 40.07517645092222, -105.1907921949662 40.07520944998442, -105.1907811943645 40.07525545084962, -105.1907751946438 40.07528244972295, -105.190767194877 40.07532545046012, -105.1907621941908 40.07536145038617, -105.1907571945497 40.07540445015314, -105.1907541950898 40.07543245047793, -105.1907521948045 40.07546245021675, -105.1907511950104 40.07549545089397, -105.1902241265108 40.07560863429631, -105.1899641949593 40.07566445030815, -105.1896741947545 40.07570145051615, -105.1893281944698 40.07585345077683, -105.18910319508 40.0759064506717, -105.1889631943489 40.07592345061921, -105.188729194604 40.07604045081974, -105.1885141942192 40.07610945042958, -105.1882921938901 40.07615545069577, -105.188192193863 40.07618545050101, -105.1880801936184 40.07619945109983, -105.1880708562545 40.07619876208987, -105.188070113258 40.07624298911882, -105.1880671719961 40.07641702604863, -105.1880519079191 40.07733113014445, -105.1880401421608 40.07904189470351, -105.1880128391563 40.08125800461307, -105.1880109830068 40.08142902449755, -105.1880101273988 40.08153800596429, -105.1879849016488 40.08337803203136, -105.1879828820664 40.08420899185455, -105.1879580266744 40.08573387104014, -105.1879367177722 40.08684890384132, -105.1879288796204 40.08725901393426, -105.1879120318739 40.087501088446, -105.1879129845044 40.08750456571757, -105.1879211426858 40.08750728610932, -105.1880329532884 40.08791559131351, -105.1880331435849 40.08791628622662, -105.187895143864 40.09008128635119, -105.1878801447803 40.09031128629881, -105.1877841432244 40.09059128547788, -105.1836459240365 40.09435811360667, -105.1837133098082 40.09435902413936, -105.1842268610857 40.09437092141485, -105.1842313087119 40.09437102454378, -105.1847691909817 40.09436254127205, -105.1851806430128 40.0943560507158, -105.1851823083869 40.09435602463465, -105.1864923089405 40.09436502536359, -105.1869288298045 40.09436799308698, -105.1869333094328 40.09436802324625, -105.1878489982433 40.09436703406432, -105.1878583084638 40.09436702410904, -105.1878579783739 40.09437328631103, -105.1878581437286 40.09437328585741, -105.1878554742897 40.09442402015232, -105.1878551441828 40.09443028595678, -105.1914201445046 40.09443828540665, -105.1941921454042 40.0944432846204, -105.1961591443175 40.09444728514715, -105.1999431444402 40.09446928464906))</t>
+          <t>POLYGON ((-105.19994314444023 40.09446928464906, -105.20004901645996 40.0944713051883, -105.20009424193184 40.09447216840297, -105.20040283465731 40.094471947312464, -105.20209254875405 40.094470721870664, -105.20406795434502 40.09447526321931, -105.20608429279402 40.09448027846468, -105.2067696857456 40.09448197611559, -105.2067688747363 40.094351397550845, -105.20697470751037 40.09435044215074, -105.2068623764414 40.074513419618434, -105.20686474863352 40.07396214178695, -105.20686777535627 40.07325874343877, -105.20687982243646 40.07280181856465, -105.2068465057981 40.07117836077267, -105.20677024383534 40.071177957202764, -105.2063513217104 40.07118051817727, -105.20624198064074 40.0711939631236, -105.20603101885605 40.07122691751993, -105.20582994868883 40.07128597501093, -105.20568996795458 40.07134793401426, -105.20547900338396 40.07146406586098, -105.20526894094964 40.0716189076843, -105.20451682212216 40.07234912431174, -105.20422395279478 40.072563870478895, -105.2040609420013 40.072662005167366, -105.20388304072873 40.07273292346781, -105.20384690647141 40.07274298737001, -105.20364091000572 40.07278308778325, -105.2032059353273 40.07280695141796, -105.20304406363582 40.07280708357413, -105.20216605966785 40.07281690086156, -105.20116809606964 40.072803066065546, -105.19980386078092 40.07279101579683, -105.19823983377144 40.07278913325598, -105.19790789190243 40.07278497129465, -105.1977160136586 40.07278309635792, -105.19711608254087 40.07277713118252, -105.19703282863752 40.07277608949424, -105.19693385382234 40.072775005568474, -105.19687311213832 40.07277402287241, -105.19671589016426 40.07277306047437, -105.19655902325633 40.072772922888944, -105.19594821459299 40.07277500006112, -105.19592189277849 40.072775089235144, -105.19559096492179 40.07278409976774, -105.19486703662623 40.07277889370809, -105.19427817332344 40.07277486502355, -105.19418312813204 40.07277406474559, -105.19406414172929 40.07277292533653, -105.19385189066865 40.072772087865694, -105.19385209229966 40.07267139500048, -105.19172393908114 40.072659641443316, -105.18939467443747 40.07264673391924, -105.18808419361588 40.07263945058795, -105.18807064387016 40.07136436642797, -105.18806719404984 40.06913144933019, -105.18580078632104 40.06912764169806, -105.18392119166224 40.06912445053024, -105.18326119229694 40.069120449919545, -105.18339619203232 40.06889744939709, -105.18375019212854 40.06857045028935, -105.18384901016671 40.06846881885282, -105.18374003429201 40.06856390986091, -105.18316016191731 40.06817113054244, -105.18312701764117 40.068152921187625, -105.18295800216363 40.06807806249881, -105.1827810018886 40.068030084912465, -105.18251714000264 40.06799010278778, -105.1823828306993 40.067982047114356, -105.181714937013 40.06800107072923, -105.18128732069269 40.068000153682576, -105.18128619165903 40.06800644970687, -105.18128919232159 40.06915245055091, -105.17925916863116 40.06913657318423, -105.17850519177411 40.069130450457976, -105.17849507255573 40.06913121664342, -105.17850703745694 40.069895965231936, -105.17851682945137 40.07054687553875, -105.17851701211839 40.0705839359631, -105.17850093348505 40.07240092923784, -105.17849584447447 40.072722100922135, -105.1784700126258 40.07272244957001, -105.17846819175679 40.07272945154712, -105.17847419130362 40.072900451071554, -105.18016656043561 40.07291007946497, -105.18146443859081 40.072914363798205, -105.18298519342392 40.07288645145971, -105.1835708587782 40.07288929420034, -105.18531230959479 40.072900143526056, -105.18657924581603 40.07290802007324, -105.18808897854088 40.07291738748686, -105.18911707007419 40.072913939430826, -105.19101417582573 40.07290737187865, -105.19260617270622 40.07290183614763, -105.19386319610042 40.07289745028993, -105.19386719534614 40.07375044969388, -105.19390919444979 40.073920450374885, -105.19396619623618 40.074041450513285, -105.19413019470491 40.074482449935026, -105.19427019497124 40.07470545027712, -105.19449619558274 40.07523545057487, -105.19448619509271 40.07535544988587, -105.19446119494306 40.075400450346436, -105.19456419531275 40.075430450634904, -105.19426219635677 40.075959451085645, -105.1935500196004 40.075693829358336, -105.19306865562119 40.07551448774536, -105.19291019553113 40.075455450296985, -105.19245219500647 40.07516645038263, -105.1921041958643 40.07508645023321, -105.19192319539738 40.0750234505873, -105.19141019462492 40.07502445075971, -105.19109119425013 40.07506045112101, -105.19084219480007 40.07505445084159, -105.1908321947982 40.07508045099295, -105.19081819438921 40.075120450913516, -105.19081119506471 40.07514245121535, -105.19080119507251 40.07517645092222, -105.19079219496625 40.07520944998442, -105.19078119436448 40.075255450849625, -105.19077519464376 40.07528244972295, -105.19076719487695 40.07532545046012, -105.19076219419077 40.07536145038617, -105.1907571945497 40.075404450153144, -105.19075419508978 40.075432450477926, -105.19075219480449 40.075462450216754, -105.19075119501042 40.075495450893975, -105.19022412651081 40.07560863429631, -105.18996419495933 40.075664450308146, -105.18967419475453 40.07570145051615, -105.18932819446984 40.075853450776826, -105.18910319508004 40.075906450671695, -105.18896319434891 40.075923450619214, -105.188729194604 40.07604045081974, -105.18851419421918 40.07610945042958, -105.18829219389012 40.076155450695765, -105.18819219386302 40.07618545050101, -105.1880801936184 40.07619945109983, -105.18807085625447 40.076198762089874, -105.188070113258 40.076242989118825, -105.1880671719961 40.07641702604863, -105.18805190791906 40.07733113014445, -105.18804014216083 40.079041894703515, -105.18801283915626 40.08125800461307, -105.18801098300685 40.08142902449755, -105.1880101273988 40.08153800596429, -105.18798490164883 40.08337803203136, -105.18798288206645 40.08420899185455, -105.18795802667437 40.08573387104014, -105.1879367177722 40.08684890384132, -105.1879288796204 40.087259013934265, -105.18791203187388 40.087501088446, -105.18791298450441 40.087504565717566, -105.1879211426858 40.08750728610932, -105.18803295328843 40.08791559131351, -105.1880331435849 40.08791628622662, -105.18789514386395 40.09008128635119, -105.18788014478031 40.090311286298814, -105.18778414322443 40.09059128547788, -105.18364592403653 40.09435811360667, -105.1837133098082 40.09435902413936, -105.18422686108573 40.09437092141485, -105.18423130871186 40.09437102454378, -105.18476919098173 40.09436254127205, -105.18518064301284 40.0943560507158, -105.18518230838691 40.09435602463465, -105.18649230894046 40.094365025363594, -105.18692882980451 40.09436799308698, -105.18693330943276 40.094368023246254, -105.18784899824328 40.09436703406432, -105.18785830846376 40.09436702410904, -105.1878579783739 40.094373286311026, -105.18785814372862 40.09437328585741, -105.18785547428973 40.094424020152324, -105.18785514418282 40.09443028595678, -105.1914201445046 40.09443828540665, -105.19419214540423 40.094443284620404, -105.19615914431746 40.09444728514715, -105.19994314444023 40.09446928464906))</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
@@ -5482,10 +5506,14 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2068465057981 40.07117836077267, -105.2068798224365 40.07280181856465, -105.2068677753563 40.07325874343877, -105.2068647486335 40.07396214178695, -105.2068623764414 40.07451341961843, -105.2076420782932 40.07371766177889, -105.2082801606808 40.07302997161467, -105.2086245150866 40.07265908095091, -105.2099806192159 40.07132523758062, -105.2107244253088 40.07057602937812, -105.2112000554906 40.07019030381962, -105.2138871567176 40.06781106466761, -105.2161601606601 40.065676155581, -105.2161515695624 40.06476845457101, -105.2161489168033 40.06403186699564, -105.2161370889706 40.06326895154256, -105.2161351423245 40.06185481826265, -105.2160151985019 40.06185644695927, -105.2144889285572 40.06184333056139, -105.2116771982488 40.06182044730468, -105.2070381967239 40.06179344782172, -105.2068437684325 40.06179232904368, -105.2068438304768 40.06178308493803, -105.2068520652456 40.06169608423045, -105.2068749843029 40.06085309603117, -105.2068741762046 40.05938002791319, -105.2068748975684 40.0589608656869, -105.2068740084848 40.05834961512206, -105.2055541963941 40.05838544689875, -105.2052551959982 40.05847144768208, -105.2048171966658 40.05844444708361, -105.2043011952846 40.05848944735493, -105.2036141957108 40.05861644723085, -105.2030841948025 40.05879544709134, -105.2029191954679 40.05892644793907, -105.2025611961079 40.05994444774891, -105.2022581955147 40.06021544819658, -105.2020791960017 40.06027244767436, -105.2020971959404 40.06055644730947, -105.2039251968715 40.06102844726419, -105.2039191966671 40.06188244736903, -105.2023031957252 40.06217144785335, -105.2012341952632 40.06256244833814, -105.2010431953765 40.06269044755282, -105.2008701954203 40.06280544810341, -105.2004271948154 40.0631064479396, -105.1994881955361 40.06370844772376, -105.197510194433 40.06410844816937, -105.1975131946994 40.06384744877385, -105.1962251942363 40.0631234489768, -105.1960821947275 40.06189544761963, -105.1944631938403 40.06188444842264, -105.1939423130284 40.06188444891134, -105.1939389409759 40.06188596206637, -105.1935278372535 40.06188410371627, -105.1930531938404 40.06188344841224, -105.1928031939953 40.06197244919012, -105.192830194072 40.06206044878067, -105.1928621939255 40.06214444837541, -105.1928981932525 40.06221544871938, -105.1932001627259 40.06253903928965, -105.195066194525 40.06429244893643, -105.1950261937514 40.06432744874969, -105.1950591935295 40.06435544887151, -105.1950961944753 40.06438544818828, -105.1951361943555 40.06441744945245, -105.1951891945079 40.06445744948024, -105.1952181943264 40.06447744843081, -105.1952991946379 40.06453244880927, -105.1953261940917 40.06454944869287, -105.1954081943274 40.06459844880609, -105.1954221947172 40.06460744901683, -105.1954341946791 40.06461344928788, -105.1954481948594 40.06462144887348, -105.1954631949272 40.06462944929453, -105.1954741938401 40.0646354487212, -105.1954861952043 40.06464244871119, -105.1955071952751 40.06465344790787, -105.1955191940804 40.06465944816699, -105.1955361941598 40.06466844907239, -105.1955621953032 40.06468144828445, -105.1958335281126 40.06482122755254, -105.1961561946336 40.06498744839866, -105.1961811946941 40.06500444822031, -105.1962161953141 40.06502844808715, -105.1962471945175 40.0650494481572, -105.1962861947403 40.06507844902631, -105.1963061946974 40.06509244910959, -105.1963351948621 40.0651164493617, -105.1964601945655 40.06521144902592, -105.196613194153 40.06534144843442, -105.1967121942066 40.06543344785908, -105.1967491951159 40.06548244853415, -105.1967551952459 40.06549044945493, -105.1967811954029 40.06553144866818, -105.197500195574 40.06553044795643, -105.1993447543905 40.06554629272709, -105.2003585210558 40.0655549887631, -105.2022371955249 40.06554144896795, -105.2022461967158 40.06719644869614, -105.202495195546 40.06738144820481, -105.2026291967245 40.06751244885115, -105.2024761975983 40.06763844798303, -105.2023491962878 40.06777944851839, -105.2022321959824 40.06797144872966, -105.2021841960138 40.06808744821939, -105.2021581970034 40.06820744840584, -105.2021606973751 40.06883412167546, -105.2021571971997 40.06915744908764, -105.2008557060834 40.06916006349055, -105.1982481955772 40.06916644960438, -105.1983431964843 40.06969344951722, -105.1981921953054 40.0700514489731, -105.1978608565895 40.07054974585753, -105.1976471349798 40.070854867217, -105.1974891959825 40.07108844907243, -105.1974111953331 40.07173844977702, -105.1971151965505 40.07180144923354, -105.1959639747934 40.07179589531189, -105.1959629613449 40.07179313125406, -105.1955317416101 40.07179076427918, -105.1955325357656 40.0721290328372, -105.19555338647 40.07215351162139, -105.195571161459 40.0721891665423, -105.195575276256 40.07222722619021, -105.1955696351996 40.07225420104457, -105.1955552225853 40.07228173548236, -105.1955329102784 40.07230570863143, -105.1956497600617 40.07230497294984, -105.1958715408196 40.07265610430982, -105.195948214593 40.07277500006112, -105.1965590232563 40.07277292288894, -105.1967158901643 40.07277306047437, -105.1968731121383 40.07277402287241, -105.1969338538223 40.07277500556847, -105.1970328286375 40.07277608949424, -105.1971160825409 40.07277713118252, -105.1977160136586 40.07278309635792, -105.1979078919024 40.07278497129465, -105.1982398337714 40.07278913325598, -105.1998038607809 40.07279101579683, -105.2011680960696 40.07280306606555, -105.2021660596678 40.07281690086156, -105.2030440636358 40.07280708357413, -105.2032059353273 40.07280695141796, -105.2036409100057 40.07278308778325, -105.2038469064714 40.07274298737001, -105.2038830407287 40.07273292346781, -105.2040609420013 40.07266200516737, -105.2042239527948 40.07256387047889, -105.2045168221222 40.07234912431174, -105.2052689409496 40.0716189076843, -105.205479003384 40.07146406586098, -105.2056899679546 40.07134793401426, -105.2058299486888 40.07128597501093, -105.2060310188561 40.07122691751993, -105.2062419806407 40.0711939631236, -105.2063513217104 40.07118051817727, -105.2067702438353 40.07117795720276, -105.2068465057981 40.07117836077267))</t>
-        </is>
-      </c>
-      <c r="H121" t="inlineStr"/>
+          <t>POLYGON ((-105.2068465057981 40.07117836077267, -105.20687982243646 40.07280181856465, -105.20686777535627 40.07325874343877, -105.20686474863352 40.07396214178695, -105.2068623764414 40.074513419618434, -105.20764207829323 40.073717661778886, -105.20828016068076 40.073029971614666, -105.20862451508663 40.07265908095091, -105.20998061921591 40.071325237580616, -105.21072442530875 40.070576029378124, -105.21120005549055 40.07019030381962, -105.21388715671756 40.06781106466761, -105.21616016066007 40.065676155580995, -105.21615156956237 40.06476845457101, -105.21614891680326 40.06403186699564, -105.21613708897056 40.06326895154256, -105.21613514232453 40.06185481826265, -105.21601519850194 40.06185644695927, -105.21448892855722 40.061843330561395, -105.2116771982488 40.061820447304676, -105.20703819672389 40.06179344782172, -105.2068437684325 40.061792329043676, -105.20684383047684 40.06178308493803, -105.20685206524557 40.06169608423045, -105.20687498430289 40.060853096031174, -105.20687417620464 40.05938002791319, -105.20687489756837 40.0589608656869, -105.20687400848476 40.05834961512206, -105.20555419639409 40.058385446898754, -105.20525519599822 40.05847144768208, -105.20481719666584 40.05844444708361, -105.20430119528456 40.05848944735493, -105.20361419571084 40.058616447230854, -105.20308419480254 40.05879544709134, -105.20291919546786 40.05892644793907, -105.20256119610794 40.05994444774891, -105.20225819551469 40.06021544819658, -105.2020791960017 40.06027244767436, -105.20209719594037 40.060556447309466, -105.20392519687151 40.061028447264185, -105.20391919666712 40.06188244736903, -105.20230319572521 40.06217144785335, -105.2012341952632 40.06256244833814, -105.20104319537651 40.06269044755282, -105.20087019542031 40.06280544810341, -105.20042719481545 40.0631064479396, -105.1994881955361 40.06370844772376, -105.197510194433 40.06410844816937, -105.19751319469937 40.06384744877385, -105.19622519423635 40.0631234489768, -105.19608219472745 40.061895447619634, -105.1944631938403 40.06188444842264, -105.19394231302836 40.061884448911336, -105.19393894097588 40.06188596206637, -105.19352783725346 40.06188410371627, -105.19305319384037 40.06188344841224, -105.19280319399527 40.06197244919012, -105.192830194072 40.06206044878067, -105.19286219392555 40.062144448375406, -105.19289819325246 40.06221544871938, -105.19320016272589 40.06253903928965, -105.19506619452498 40.06429244893643, -105.1950261937514 40.06432744874969, -105.19505919352953 40.06435544887151, -105.19509619447527 40.064385448188276, -105.19513619435548 40.06441744945245, -105.19518919450789 40.06445744948024, -105.19521819432644 40.064477448430814, -105.19529919463793 40.064532448809274, -105.19532619409173 40.06454944869287, -105.19540819432744 40.06459844880609, -105.19542219471717 40.064607449016826, -105.19543419467907 40.06461344928788, -105.19544819485938 40.06462144887348, -105.19546319492719 40.06462944929453, -105.1954741938401 40.0646354487212, -105.19548619520427 40.06464244871119, -105.1955071952751 40.064653447907865, -105.19551919408043 40.064659448166985, -105.19553619415981 40.06466844907239, -105.19556219530322 40.064681448284446, -105.19583352811263 40.06482122755254, -105.1961561946336 40.06498744839866, -105.19618119469408 40.06500444822031, -105.19621619531407 40.065028448087155, -105.19624719451745 40.0650494481572, -105.1962861947403 40.06507844902631, -105.19630619469736 40.065092449109585, -105.19633519486206 40.065116449361696, -105.1964601945655 40.06521144902592, -105.19661319415297 40.06534144843442, -105.1967121942066 40.06543344785908, -105.19674919511594 40.06548244853415, -105.19675519524594 40.065490449454934, -105.19678119540292 40.06553144866818, -105.197500195574 40.06553044795643, -105.19934475439051 40.06554629272709, -105.20035852105578 40.065554988763104, -105.20223719552489 40.06554144896795, -105.20224619671583 40.06719644869614, -105.20249519554599 40.06738144820481, -105.20262919672446 40.06751244885115, -105.2024761975983 40.06763844798303, -105.20234919628778 40.067779448518394, -105.20223219598242 40.06797144872966, -105.2021841960138 40.068087448219394, -105.2021581970034 40.068207448405836, -105.20216069737508 40.06883412167546, -105.20215719719974 40.06915744908764, -105.20085570608342 40.06916006349055, -105.1982481955772 40.06916644960438, -105.19834319648426 40.06969344951722, -105.19819219530544 40.0700514489731, -105.19786085658947 40.07054974585753, -105.1976471349798 40.070854867217, -105.19748919598247 40.071088449072434, -105.19741119533312 40.07173844977702, -105.19711519655048 40.07180144923354, -105.19596397479337 40.07179589531189, -105.19596296134492 40.07179313125406, -105.1955317416101 40.07179076427918, -105.19553253576561 40.0721290328372, -105.19555338647001 40.072153511621394, -105.19557116145899 40.0721891665423, -105.19557527625595 40.072227226190215, -105.19556963519956 40.07225420104457, -105.19555522258528 40.072281735482356, -105.19553291027836 40.072305708631426, -105.19564976006166 40.07230497294984, -105.19587154081958 40.07265610430982, -105.19594821459299 40.07277500006112, -105.19655902325633 40.072772922888944, -105.19671589016426 40.07277306047437, -105.19687311213832 40.07277402287241, -105.19693385382234 40.072775005568474, -105.19703282863752 40.07277608949424, -105.19711608254087 40.07277713118252, -105.1977160136586 40.07278309635792, -105.19790789190243 40.07278497129465, -105.19823983377144 40.07278913325598, -105.19980386078092 40.07279101579683, -105.20116809606964 40.072803066065546, -105.20216605966785 40.07281690086156, -105.20304406363582 40.07280708357413, -105.2032059353273 40.07280695141796, -105.20364091000572 40.07278308778325, -105.20384690647141 40.07274298737001, -105.20388304072873 40.07273292346781, -105.2040609420013 40.072662005167366, -105.20422395279478 40.072563870478895, -105.20451682212216 40.07234912431174, -105.20526894094964 40.0716189076843, -105.20547900338396 40.07146406586098, -105.20568996795458 40.07134793401426, -105.20582994868883 40.07128597501093, -105.20603101885605 40.07122691751993, -105.20624198064074 40.0711939631236, -105.2063513217104 40.07118051817727, -105.20677024383534 40.071177957202764, -105.2068465057981 40.07117836077267))</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Niwot HS</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5520,7 +5548,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.208456199712 40.08891645102268, -105.2093902465011 40.08891684883024, -105.2102848781286 40.08891722303895, -105.2114362013246 40.08891745132185, -105.213437201397 40.08892445097817, -105.2143002021996 40.08892245043239, -105.2148042021617 40.08892745043244, -105.2148588360544 40.08892679371123, -105.2159742024865 40.08892045011142, -105.2163292022599 40.08892045018143, -105.216360202134 40.08892145040806, -105.2163692023297 40.08714545077098, -105.2182532019159 40.08714945059754, -105.2182432027494 40.08641344971119, -105.2211262032423 40.08639345027048, -105.2211162029895 40.08627444986659, -105.2219812039535 40.08618344991433, -105.2230462031982 40.08603244956893, -105.2246852045713 40.08554044892636, -105.2246712037403 40.08611344976358, -105.2258422045073 40.08612344890279, -105.225847257111 40.08702564690289, -105.2258442047025 40.08817345056035, -105.2258660776002 40.08846675183878, -105.2259971464311 40.08825128178296, -105.2260951784236 40.08815046645809, -105.2260799511012 40.08815043483378, -105.2260289772142 40.08815032829153, -105.2260301833774 40.08814810745953, -105.2260316128055 40.08814547826421, -105.2260330445643 40.08814285267693, -105.2260344868726 40.08814022801536, -105.226035930357 40.08813760245592, -105.2260373773409 40.08813498140795, -105.2260388290152 40.08813236037112, -105.2260402865523 40.08812973934819, -105.2260417429166 40.08812711832244, -105.2260432086508 40.08812450002085, -105.2260446767192 40.08812188442674, -105.226046152992 40.08811926975269, -105.2260476280957 40.08811665417521, -105.2260491125655 40.08811404222255, -105.2260505993841 40.08811142937476, -105.2260520885404 40.08810881833376, -105.2260535823798 40.08810620910523, -105.2260550832546 40.0881035998933, -105.2260565841257 40.08810099158206, -105.2260580920141 40.08809838779062, -105.2260596034202 40.08809578400751, -105.2260611230379 40.08809317934323, -105.2260626414721 40.08809057737804, -105.2260641669416 40.08808797542954, -105.2260656970834 40.08808537799534, -105.2260672295774 40.08808277876541, -105.2260687690924 40.08808018315465, -105.2260703097799 40.08807758754672, -105.2260718574956 40.08807499375673, -105.2260734087289 40.088072399975, -105.2260749611275 40.0880698079974, -105.2260765193853 40.08806721693423, -105.226078084664 40.08806462949036, -105.2260796499462 40.0880620411458, -105.2260812222603 40.08805945371852, -105.2260827980811 40.08805686900151, -105.2260843809301 40.08805428610243, -105.2260859637863 40.08805170140207, -105.2260875536562 40.08804912212216, -105.2260891482163 40.08804654285341, -105.2260907451214 40.08804396359018, -105.2260923455334 40.08804138703718, -105.2260939506355 40.08803881049528, -105.2260955615934 40.08803623576855, -105.2260971760652 40.08803366195077, -105.2260987916986 40.08803109083762, -105.2261004178852 40.08802851974954, -105.2261020440572 40.08802595226398, -105.2261036725816 40.08802338298269, -105.2261053092994 40.08802081732343, -105.2261069495313 40.08801825257306, -105.2261085932736 40.08801568963229, -105.2261102405372 40.08801312579922, -105.2261118948289 40.0880105637841, -105.2261135491024 40.08800800627216, -105.2261152092496 40.08800544607216, -105.2261168764069 40.08800289219328, -105.226118542406 40.08800033470907, -105.2261202165914 40.08799778264812, -105.2261218943052 40.08799522789362, -105.2261235755077 40.08799268035245, -105.2261252602387 40.08799013011774, -105.226126950829 40.08798758079754, -105.2261286460914 40.08798503599166, -105.2261303460513 40.08798248939556, -105.2261320460038 40.0879799446007, -105.2261337541534 40.08797740252725, -105.2261354658207 40.08797486046209, -105.2261371809875 40.08797232290842, -105.2261388996683 40.08796978626372, -105.2261406218776 40.08796724692545, -105.2261423475865 40.08796471209865, -105.2261440803236 40.08796217908979, -105.2261458165711 40.08795964789051, -105.2261475563434 40.08795711489833, -105.226149300777 40.08795458912228, -105.2261510475738 40.08795205884863, -105.2261528013842 40.08794953399544, -105.2261545551981 40.08794700824161, -105.2261563172056 40.08794448610973, -105.2261580815545 40.08794196488402, -105.2261598505936 40.08793944366944, -105.2261616231395 40.08793692516508, -105.2261634015482 40.08793440667458, -105.2261651799496 40.08793188998534, -105.2261669688859 40.08792937782427, -105.2261687566533 40.08792686475982, -105.2261705502725 40.0879243544111, -105.226172348582 40.08792184407345, -105.2261741480568 40.08791933553987, -105.2261759557322 40.08791682882699, -105.2261777645729 40.08791432391816, -105.2261795792655 40.08791182172511, -105.2261813974722 40.08790932044101, -105.2261832203618 40.08790682096924, -105.2261850455965 40.08790432150305, -105.2261868778629 40.08790182295415, -105.2261887112837 40.08789932891115, -105.2261905517435 40.08789683398418, -105.2261923945412 40.08789434086405, -105.2261942361589 40.08789184954237, -105.226196091833 40.08788936185654, -105.226197947507 40.08788687417072, -105.2261998043462 40.08788438828893, -105.2262016682208 40.08788190242377, -105.226203534426 40.08787942016669, -105.2262054064867 40.08787693972477, -105.2262072808852 40.08787446108968, -105.2262091611538 40.08787198066713, -105.2262110437421 40.0878695065546, -105.2262129298625 40.08786702884783, -105.2262148218203 40.0878645574594, -105.2262167161233 40.08786208607652, -105.2262186162781 40.08785961740938, -105.2262205211268 40.08785714785272, -105.226222428306 40.08785468190413, -105.2262243401755 40.08785221596659, -105.2262262543791 40.08784975273657, -105.2262281732657 40.08784729131887, -105.2262300991841 40.08784483081848, -105.226232023919 40.08784237301715, -105.2262339568581 40.08783991613592, -105.2262358933076 40.08783746106425, -105.2262378332675 40.08783500780219, -105.2262397767451 40.08783255454839, -105.2262417237222 40.08783010580613, -105.2262436742169 40.08782765707216, -105.2262456270494 40.08782521014498, -105.2262475892516 40.08782276594194, -105.2262495549714 40.08782032174722, -105.2262515195077 40.08781788025156, -105.2262534898923 40.08781544237237, -105.2262554673158 40.08781300360911, -105.226257445901 40.08781056755058, -105.2262594326977 40.0878081306108, -105.2262614183 40.08780569907206, -105.2262634085889 40.08780326844501, -105.2262654059096 40.08780083873525, -105.2262674008741 40.08779841172184, -105.2262694052227 40.08779598382996, -105.2262714142507 40.0877935586511, -105.2262734244331 40.08779113797818, -105.2262754393057 40.08778871731626, -105.2262774576886 40.08778629846402, -105.2262794831069 40.0877838796284, -105.2262815085034 40.08778146619655, -105.2262835374175 40.08777905277302, -105.2262855745432 40.08777663846826, -105.2262876128304 40.08777422686813, -105.2262896569624 40.08777181978507, -105.226291699918 40.08776941359987, -105.2262937499053 40.08776700833194, -105.2262958045756 40.08776460487633, -105.2262978662741 40.08776220323865, -105.2262999267926 40.08775980339941, -105.2263019919905 40.08775740627321, -105.2263040642092 40.08775501276614, -105.2263061352625 40.08775261745505, -105.2263082145056 40.08775022666651, -105.2263102972735 40.08774783408501, -105.2263123800232 40.08774544600666, -105.226314467456 40.08774305974064, -105.2263165619241 40.08774067349134, -105.2263186598953 40.08773829085281, -105.2263207637256 40.08773590912882, -105.226322866376 40.08773352920324, -105.2263249737094 40.08773115109006, -105.2263270845495 40.0877287756871, -105.2263292047701 40.08772640030627, -105.2263313249726 40.08772402942868, -105.226333448689 40.08772165945994, -105.2263355759121 40.08771929220145, -105.2263377078255 40.08771692495404, -105.2263398455944 40.08771455952174, -105.2263419810035 40.08771219768641, -105.2263441269622 40.08770983677667, -105.2263462740824 40.08770747857164, -105.2263484247239 40.08770511947421, -105.2263505776958 40.08770276398484, -105.2263527353471 40.08770041120849, -105.226354900023 40.08769806115065, -105.2263570647023 40.08769571019219, -105.2263592363989 40.0876933637535, -105.2263614080953 40.08769101731477, -105.2263635879888 40.08768867359738, -105.2263657702201 40.0876863316868, -105.2263679524405 40.08768399247809, -105.2263701416961 40.08768165328597, -105.2263723344585 40.0876793168041, -105.2263745307277 40.0876769830324, -105.2263767305145 40.08767464926904, -105.2263789361496 40.08767231912204, -105.2263825065714 40.08766855838156, -105.2263977138776 40.0876481506639, -105.2264158800905 40.08762967283475, -105.226434455812 40.08761141663134, -105.2264521500162 40.08759367350561, -105.2264697795498 40.08757626436348, -105.2264878009205 40.08755909752002, -105.2265062070929 40.08754217295839, -105.226524998038 40.0875254978835, -105.2265441631842 40.08750907677334, -105.2265637001611 40.08749291592657, -105.22658359957 40.0874770198241, -105.2266038602236 40.08746139206541, -105.2266244715363 40.08744604073107, -105.2266454253037 40.08743096490092, -105.2266667226549 40.08741617538511, -105.2266883530404 40.08740167125784, -105.2267103070542 40.08738745880117, -105.2267325834878 40.08737354701852, -105.2267551729715 40.08735993318564, -105.226778067272 40.08734662358735, -105.2268012569799 40.08733362540633, -105.2268247444441 40.08732093774738, -105.2268485155578 40.08730856958332, -105.2268725621166 40.08729651999401, -105.226896880574 40.08728479617606, -105.2269214580284 40.08727339899931, -105.2269462956309 40.08726233387031, -105.2269713781346 40.08725160165343, -105.226995713506 40.08724120810847, -105.2270202222304 40.08723115271041, -105.2270449570381 40.08722144459034, -105.227069908556 40.08721208192462, -105.2270950662131 40.08720306919137, -105.2271204311677 40.08719440999577, -105.2271459834793 40.08718610609185, -105.2271717266588 40.08717815928905, -105.2271977580158 40.08717057341977, -105.2272236163383 40.08716344466387, -105.2272444844378 40.08716355701311, -105.2283729549368 40.08717092525384, -105.2315411374752 40.08755923148525, -105.2315951034686 40.08756556421094, -105.2316492191852 40.08757169551478, -105.2317034632943 40.08757708676092, -105.2317578193674 40.08758174061293, -105.2318122651521 40.08758564981383, -105.2318667865754 40.08758881433079, -105.2319213672231 40.08759123322496, -105.2319759906559 40.08759291186197, -105.2320306369806 40.0875938393878, -105.2320852944376 40.08759402388102, -105.232139950141 40.08759346170912, -105.2321945759326 40.08759215640933, -105.2322491612788 40.08759010255342, -105.2323036897474 40.08758730370593, -105.2323581460858 40.0875837616329, -105.2324125138727 40.08757947719696, -105.2324667696581 40.08757444944327, -105.2325209052109 40.08756868375681, -105.2325748982646 40.08756217648359, -105.2326288764451 40.08755497475301, -105.2326832836757 40.08754720298132, -105.232737453437 40.08753868580036, -105.2327913728077 40.08752942858451, -105.2328450159892 40.08751943127434, -105.232898377103 40.08750869745924, -105.2329514268327 40.08749722707182, -105.2330041639691 40.08748502911613, -105.2330565603615 40.08747210532881, -105.2331086089517 40.08745846109794, -105.2331195646996 40.08745541432238, -105.233160289808 40.08744409547717, -105.2332115864704 40.0874290192368, -105.2332572252643 40.08741486387087, -105.2333106562827 40.0873970203308, -105.2333632162177 40.08737853169327, -105.2334153508784 40.08735934044687, -105.2334670391323 40.08733945284803, -105.2335182680553 40.08731887517195, -105.2335350154684 40.08731185997121, -105.2335198087354 40.08730061994037, -105.2334842065225 40.08728144947539, -105.233557508418 40.08725212883198, -105.2336642062275 40.0872094484582, -105.2337498879304 40.08716518662143, -105.2338752055783 40.08710044895112, -105.2340141176357 40.08701357127359, -105.2340547143473 40.08698818193187, -105.234116919408 40.08694927681879, -105.2341742062996 40.08691344866173, -105.2341886118381 40.08690464559623, -105.2342102060382 40.08689144861766, -105.2342874907976 40.08682176614175, -105.2344113616564 40.08671008020809, -105.2346296381483 40.08650825210744, -105.2347532059639 40.0863524487831, -105.2349272055709 40.08608544943124, -105.2351162069385 40.08560644881669, -105.2351382054217 40.08551144874158, -105.2350852057845 40.0846124484227, -105.2350776389745 40.08420165278985, -105.2350497203358 40.08268589163298, -105.2350032064051 40.08016044862552, -105.2299052044168 40.08008044876753, -105.2334432055741 40.07899144749057, -105.2352892054144 40.07873844737262, -105.2378132062725 40.07833444783447, -105.2384812068036 40.07833244791702, -105.2403432064991 40.07833344770941, -105.2423652076105 40.07833744689923, -105.2435522068469 40.07833844725607, -105.2446880588089 40.07833844686491, -105.2446880583013 40.07833920790986, -105.245048207299 40.07833944731037, -105.2467352086361 40.07833144715077, -105.2479762077927 40.07832544680577, -105.2509901360431 40.07831039649412, -105.2552788447606 40.07829042246069, -105.263475212196 40.07824944591677, -105.2635022120304 40.08020744623987, -105.265906623877 40.08014227963445, -105.2678107184368 40.08009626548748, -105.269120467453 40.08006436083225, -105.270773469619 40.08002883906712, -105.271602868858 40.08001390036796, -105.2722111865081 40.08000293913378, -105.2732488422515 40.07998423568615, -105.2738472151207 40.07997344533944, -105.2741904007602 40.07997698391911, -105.275236925473 40.07998199934345, -105.2760592152198 40.07997644544199, -105.2774492150437 40.079994445459, -105.2774442150245 40.07989344467622, -105.2775032146846 40.07989444554472, -105.277486220627 40.07914765992864, -105.277462333618 40.07819218232893, -105.2774232152314 40.07679644423713, -105.2774182151642 40.07662844439344, -105.277414215237 40.07647944379102, -105.2774795717141 40.0764360956394, -105.2776022148752 40.07633644500343, -105.2777612150901 40.07620044483633, -105.2779022152453 40.07603844420503, -105.2780202147794 40.07579044515734, -105.2783742148064 40.07579144511136, -105.278372214492 40.07653744417692, -105.2782532143109 40.07666244408787, -105.2821112161553 40.07666744386643, -105.2821342160606 40.0791254445771, -105.2822223466844 40.07989150774977, -105.2822690597651 40.07965201797717, -105.2823048577945 40.07952086600779, -105.2823438719979 40.07938999478642, -105.2825129694785 40.07892198794374, -105.2826709107073 40.07859011936667, -105.2838018419132 40.0763738690773, -105.2839320007679 40.07612210589992, -105.2839819795333 40.07602502070181, -105.284061438017 40.07587059340077, -105.2841729060126 40.07565395617164, -105.2843430443443 40.07530206774775, -105.2844881096322 40.07496797674111, -105.2846140488599 40.07458004438773, -105.2846558254534 40.07436407727556, -105.2846799442029 40.07408191848048, -105.2846740115247 40.07381095898337, -105.284634842972 40.07354103535643, -105.2845098877672 40.0730540823975, -105.2844238046166 40.07276114874126, -105.2844119360205 40.07272887084649, -105.2841258539786 40.07178289850857, -105.2839564523263 40.07122915445703, -105.283447132496 40.06958603676775, -105.2830899236575 40.06843101948598, -105.2828828825465 40.06781286879525, -105.2828103083754 40.06759885395986, -105.2827667487974 40.0674749475167, -105.282708682352 40.06730598772923, -105.2826287480644 40.0671032160873, -105.2824690223394 40.06665264506963, -105.2821777644898 40.06610051550977, -105.2818205276817 40.06556514578249, -105.2823076520964 40.06555737709394, -105.2826421053623 40.06555460571782, -105.2840396611971 40.06556052476189, -105.2840422155819 40.0655634422325, -105.2841102147732 40.06556744313233, -105.2841555199931 40.0655765955805, -105.2842092152591 40.06558744250346, -105.2842552150438 40.06560344292603, -105.2843132151617 40.06563044283727, -105.2844392150506 40.0657224424132, -105.2844419581037 40.06556495868456, -105.2844696482367 40.06556530130753, -105.2844750682011 40.06545646919614, -105.2844743893111 40.06528829290035, -105.2844693643109 40.06404057361777, -105.2844681111398 40.06372971757044, -105.283919471611 40.06372879883411, -105.2835079480766 40.06372864274691, -105.2832962374926 40.06372837690664, -105.282319982506 40.06372626586732, -105.282127928685 40.06372330059435, -105.2818065024136 40.0636562328228, -105.2814222747994 40.06419864439965, -105.2809515658617 40.06431108663833, -105.280571421083 40.06429735375461, -105.2802739685094 40.06411686471955, -105.2799809979885 40.06393952401127, -105.2794570843467 40.06360607635985, -105.2766818087143 40.0618889301708, -105.2764060265012 40.06171701384444, -105.2730720982822 40.05964009195046, -105.2713911776679 40.05857795867715, -105.2708018933556 40.05820399463217, -105.2704799468352 40.05801009468256, -105.269613922533 40.05749501959285, -105.2682239553873 40.05662805383557, -105.2668749737009 40.05580013493221, -105.2656519227221 40.05503202749767, -105.2651129178647 40.0547020581333, -105.2643711340155 40.05423304186316, -105.2636688880578 40.05380006284676, -105.2628900215765 40.05331696043408, -105.2624829531093 40.05306301764614, -105.2623361003706 40.0529699277751, -105.2621960311828 40.05287795048658, -105.2620028794537 40.05274495970432, -105.2617659165283 40.0525759170593, -105.2614929991048 40.05237111141436, -105.2612450666888 40.0521729459601, -105.2610698287841 40.05202599008051, -105.2609530191591 40.05192390191151, -105.2607870983266 40.05176900406456, -105.2606671334609 40.05164988950381, -105.2605749425811 40.05155608753633, -105.2603760318205 40.0513360595755, -105.2602141708121 40.05114493352249, -105.2601188264747 40.05103410417082, -105.2598741447213 40.05103112475856, -105.2596540956784 40.05103203920658, -105.2594829834554 40.05103387844358, -105.2593029494353 40.05103295453986, -105.2589768334914 40.05102705814787, -105.2587289291635 40.05102599065928, -105.2584981610342 40.05102797837995, -105.2575590331624 40.05103012676278, -105.2573100547426 40.05102987806262, -105.257231109612 40.05102998669123, -105.2569678378071 40.05103107976799, -105.2566809897506 40.05103212163024, -105.25604407166 40.05103297347731, -105.2551588691268 40.05103905939236, -105.2549531084884 40.05103999519333, -105.2542390203288 40.05104396683892, -105.2537370961487 40.05105387742171, -105.2532001644783 40.05106398564791, -105.2524199535919 40.05107796120676, -105.2510428610323 40.05108488106519, -105.2508760373014 40.05108589359897, -105.2490581462503 40.05109101404377, -105.2483851425808 40.05109311682119, -105.2475231626413 40.05109809690759, -105.2468959021357 40.05109507542115, -105.2461500947277 40.05107888798747, -105.2442429405871 40.05107302924297, -105.2428419426089 40.05107211210048, -105.2421489161141 40.05107907484076, -105.2365320855235 40.05106995573312, -105.2357508266088 40.05107695324783, -105.2348829780416 40.05109024293931, -105.2345658693909 40.0510950970329, -105.234505146494 40.05109413413817, -105.234254046906 40.05108806575161, -105.233742911622 40.05109392331027, -105.2328579827825 40.05110405832345, -105.2322589673265 40.05109498290111, -105.2313310609188 40.05105906073936, -105.2255132508242 40.05104207956713, -105.2255121997152 40.05104844465996, -105.2255131993988 40.05166644490966, -105.2255144818426 40.05233267196999, -105.2255172002856 40.05374544531903, -105.2255182005121 40.05476544570443, -105.2252621999629 40.05476044491763, -105.2250889657715 40.0547790063182, -105.2248982008678 40.05479944495026, -105.2247629796722 40.05483727490623, -105.2245622003918 40.05489344487475, -105.2244915600372 40.05491131624516, -105.2242669549185 40.05496813582263, -105.2238901992559 40.05506344591768, -105.2234611993335 40.05515144511462, -105.2226751991902 40.05523444591667, -105.2215101992092 40.05551444592377, -105.2207951986344 40.0557584459232, -105.22080819831 40.05466444502937, -105.2199480798594 40.05465482055129, -105.2178801587147 40.05464468834945, -105.2159731984142 40.05462644657686, -105.2159491981005 40.05506044566964, -105.2159399253224 40.05548742980623, -105.215927198784 40.05607344660881, -105.2159241988464 40.05654844624868, -105.2160381978682 40.05677044599801, -105.2160881989679 40.05694944610164, -105.2160991982986 40.05722244647633, -105.2150271981241 40.05721844599338, -105.2147491987564 40.05722544618729, -105.2143381982444 40.0572654468832, -105.2142531979739 40.05728144632609, -105.2139361978653 40.05733944632712, -105.213604197271 40.05742944613198, -105.2133621975794 40.05750044691125, -105.2131981981032 40.05754944636183, -105.213117197296 40.05756744624475, -105.2130431979704 40.05758444664818, -105.2128581978988 40.05759144654688, -105.212820197039 40.05823044648699, -105.2159321990569 40.05825844688626, -105.2159997620123 40.0591844562415, -105.2161151623542 40.05918488788823, -105.2161389050824 40.0607749575591, -105.2161370248116 40.06165505807027, -105.2161351368842 40.06185105984153, -105.2161370889706 40.06326895154256, -105.2161489168033 40.06403186699564, -105.2161515695624 40.06476845457101, -105.2161601606601 40.065676155581, -105.2138871567176 40.06781106466761, -105.2112000554906 40.07019030381962, -105.2107244253088 40.07057602937812, -105.2099806192159 40.07132523758062, -105.2086245150866 40.07265908095091, -105.2082801606808 40.07302997161467, -105.2076420782932 40.07371766177889, -105.2068623764414 40.07451341961843, -105.2069438669998 40.08890529265857, -105.2069481319076 40.08890527106102, -105.2075245971012 40.08890693460845, -105.208456199712 40.08891645102268))</t>
+          <t>POLYGON ((-105.20845619971197 40.088916451022676, -105.20939024650113 40.08891684883024, -105.21028487812863 40.08891722303895, -105.21143620132462 40.088917451321855, -105.21343720139699 40.08892445097817, -105.21430020219961 40.08892245043239, -105.21480420216173 40.08892745043244, -105.21485883605443 40.08892679371123, -105.21597420248646 40.08892045011142, -105.21632920225987 40.08892045018143, -105.21636020213397 40.08892145040806, -105.21636920232973 40.08714545077098, -105.21825320191593 40.087149450597536, -105.21824320274943 40.086413449711195, -105.22112620324229 40.08639345027048, -105.22111620298946 40.08627444986659, -105.22198120395349 40.08618344991433, -105.22304620319824 40.08603244956893, -105.22468520457126 40.08554044892636, -105.22467120374027 40.08611344976358, -105.22584220450734 40.08612344890279, -105.225847257111 40.08702564690289, -105.22584420470254 40.088173450560355, -105.22586607760016 40.08846675183878, -105.22599714643113 40.08825128178296, -105.22609517842363 40.08815046645809, -105.22607995110123 40.08815043483378, -105.22602897721418 40.088150328291526, -105.22603018337745 40.08814810745953, -105.22603161280553 40.08814547826421, -105.22603304456426 40.08814285267693, -105.22603448687256 40.088140228015355, -105.22603593035697 40.088137602455916, -105.22603737734094 40.088134981407954, -105.22603882901521 40.08813236037112, -105.2260402865523 40.08812973934819, -105.22604174291665 40.08812711832244, -105.22604320865081 40.088124500020854, -105.22604467671918 40.08812188442674, -105.22604615299197 40.08811926975269, -105.22604762809566 40.08811665417521, -105.22604911256549 40.08811404222255, -105.22605059938407 40.08811142937476, -105.22605208854043 40.08810881833376, -105.22605358237979 40.088106209105234, -105.2260550832546 40.0881035998933, -105.22605658412569 40.08810099158206, -105.2260580920141 40.08809838779062, -105.22605960342018 40.088095784007514, -105.22606112303788 40.08809317934323, -105.22606264147205 40.08809057737804, -105.22606416694163 40.088087975429545, -105.2260656970834 40.08808537799534, -105.22606722957744 40.08808277876541, -105.22606876909245 40.08808018315465, -105.22607030977991 40.08807758754672, -105.22607185749558 40.08807499375673, -105.22607340872892 40.088072399975005, -105.22607496112747 40.0880698079974, -105.22607651938526 40.088067216934235, -105.22607808466402 40.08806462949036, -105.22607964994621 40.0880620411458, -105.22608122226026 40.08805945371852, -105.22608279808112 40.08805686900151, -105.22608438093015 40.08805428610243, -105.2260859637863 40.088051701402065, -105.22608755365617 40.088049122122165, -105.22608914821626 40.088046542853405, -105.2260907451214 40.08804396359018, -105.22609234553337 40.08804138703718, -105.22609395063553 40.08803881049528, -105.22609556159335 40.08803623576855, -105.22609717606518 40.088033661950774, -105.22609879169858 40.088031090837625, -105.2261004178852 40.088028519749535, -105.22610204405721 40.08802595226398, -105.22610367258157 40.08802338298269, -105.22610530929944 40.088020817323425, -105.22610694953133 40.088018252573065, -105.2261085932736 40.08801568963229, -105.22611024053718 40.08801312579922, -105.22611189482893 40.088010563784096, -105.22611354910242 40.08800800627216, -105.22611520924964 40.08800544607216, -105.22611687640695 40.08800289219328, -105.226118542406 40.08800033470907, -105.22612021659137 40.08799778264812, -105.2261218943052 40.08799522789362, -105.22612357550771 40.08799268035245, -105.22612526023875 40.08799013011774, -105.22612695082901 40.08798758079754, -105.2261286460914 40.087985035991665, -105.22613034605126 40.087982489395564, -105.22613204600376 40.0879799446007, -105.22613375415338 40.08797740252725, -105.22613546582066 40.08797486046209, -105.22613718098748 40.08797232290842, -105.22613889966833 40.08796978626372, -105.22614062187763 40.08796724692545, -105.22614234758655 40.08796471209865, -105.22614408032358 40.087962179089786, -105.22614581657106 40.08795964789051, -105.2261475563434 40.08795711489833, -105.22614930077698 40.087954589122276, -105.22615104757375 40.08795205884863, -105.2261528013842 40.08794953399544, -105.22615455519815 40.087947008241606, -105.22615631720561 40.08794448610973, -105.22615808155446 40.08794196488402, -105.22615985059359 40.08793944366944, -105.22616162313946 40.08793692516508, -105.22616340154822 40.087934406674584, -105.22616517994956 40.08793188998534, -105.22616696888593 40.087929377824274, -105.22616875665327 40.08792686475982, -105.22617055027254 40.0879243544111, -105.22617234858203 40.08792184407345, -105.22617414805676 40.08791933553987, -105.22617595573219 40.08791682882699, -105.22617776457287 40.08791432391816, -105.22617957926549 40.087911821725115, -105.22618139747217 40.08790932044101, -105.22618322036178 40.087906820969245, -105.22618504559645 40.08790432150305, -105.22618687786292 40.08790182295415, -105.22618871128371 40.08789932891115, -105.22619055174354 40.08789683398418, -105.22619239454121 40.087894340864054, -105.22619423615886 40.087891849542366, -105.226196091833 40.08788936185654, -105.226197947507 40.08788687417072, -105.2261998043462 40.08788438828893, -105.22620166822081 40.087881902423774, -105.22620353442599 40.08787942016669, -105.22620540648671 40.08787693972477, -105.22620728088522 40.08787446108968, -105.22620916115385 40.08787198066713, -105.22621104374208 40.0878695065546, -105.2262129298625 40.08786702884783, -105.22621482182035 40.0878645574594, -105.22621671612326 40.08786208607652, -105.22621861627809 40.08785961740938, -105.2262205211268 40.087857147852716, -105.22622242830604 40.087854681904126, -105.22622434017549 40.08785221596659, -105.22622625437913 40.08784975273657, -105.22622817326574 40.087847291318866, -105.22623009918414 40.087844830818476, -105.22623202391895 40.087842373017146, -105.22623395685808 40.08783991613592, -105.22623589330765 40.08783746106425, -105.22623783326755 40.08783500780219, -105.22623977674515 40.08783255454839, -105.22624172372221 40.087830105806134, -105.2262436742169 40.08782765707216, -105.22624562704942 40.087825210144985, -105.22624758925161 40.087822765941944, -105.22624955497145 40.08782032174722, -105.22625151950771 40.08781788025156, -105.22625348989226 40.087815442372374, -105.22625546731582 40.087813003609114, -105.22625744590096 40.087810567550584, -105.22625943269774 40.0878081306108, -105.22626141830003 40.08780569907206, -105.2262634085889 40.08780326844501, -105.22626540590961 40.08780083873525, -105.22626740087406 40.08779841172184, -105.22626940522272 40.08779598382996, -105.22627141425073 40.0877935586511, -105.22627342443312 40.08779113797818, -105.22627543930565 40.087788717316265, -105.22627745768861 40.08778629846402, -105.22627948310692 40.0877838796284, -105.22628150850342 40.087781466196546, -105.2262835374175 40.087779052773016, -105.22628557454316 40.08777663846826, -105.22628761283043 40.08777422686813, -105.22628965696238 40.08777181978507, -105.22629169991798 40.087769413599865, -105.22629374990531 40.08776700833194, -105.22629580457564 40.08776460487633, -105.22629786627414 40.087762203238654, -105.22629992679262 40.08775980339941, -105.22630199199047 40.087757406273205, -105.2263040642092 40.08775501276614, -105.22630613526246 40.087752617455045, -105.22630821450556 40.08775022666651, -105.22631029727353 40.08774783408501, -105.22631238002324 40.087745446006664, -105.22631446745598 40.08774305974064, -105.22631656192405 40.08774067349134, -105.22631865989526 40.08773829085281, -105.2263207637256 40.08773590912882, -105.22632286637598 40.08773352920324, -105.22632497370938 40.08773115109006, -105.2263270845495 40.0877287756871, -105.22632920477012 40.08772640030627, -105.22633132497256 40.08772402942868, -105.226333448689 40.087721659459945, -105.22633557591215 40.08771929220145, -105.22633770782554 40.08771692495404, -105.22633984559444 40.08771455952174, -105.22634198100351 40.087712197686415, -105.2263441269622 40.087709836776675, -105.22634627408237 40.08770747857164, -105.22634842472385 40.08770511947421, -105.22635057769583 40.08770276398484, -105.22635273534713 40.08770041120849, -105.22635490002297 40.087698061150654, -105.22635706470228 40.08769571019219, -105.22635923639888 40.0876933637535, -105.22636140809533 40.08769101731477, -105.2263635879888 40.08768867359738, -105.22636577022014 40.0876863316868, -105.22636795244047 40.08768399247809, -105.22637014169614 40.08768165328597, -105.22637233445855 40.0876793168041, -105.22637453072771 40.0876769830324, -105.22637673051449 40.08767464926904, -105.22637893614962 40.08767231912204, -105.22638250657144 40.08766855838156, -105.22639771387756 40.087648150663895, -105.22641588009053 40.08762967283475, -105.22643445581203 40.08761141663134, -105.22645215001624 40.08759367350561, -105.22646977954976 40.087576264363484, -105.22648780092054 40.08755909752002, -105.22650620709292 40.08754217295839, -105.226524998038 40.0875254978835, -105.22654416318423 40.08750907677334, -105.22656370016112 40.08749291592657, -105.22658359956998 40.0874770198241, -105.22660386022363 40.087461392065414, -105.2266244715363 40.08744604073107, -105.22664542530366 40.08743096490092, -105.22666672265485 40.08741617538511, -105.22668835304036 40.087401671257844, -105.2267103070542 40.08738745880117, -105.22673258348783 40.087373547018515, -105.22675517297154 40.08735993318564, -105.22677806727201 40.08734662358735, -105.22680125697993 40.08733362540633, -105.22682474444414 40.08732093774738, -105.22684851555779 40.08730856958332, -105.22687256211657 40.087296519994005, -105.22689688057402 40.087284796176064, -105.22692145802843 40.08727339899931, -105.22694629563092 40.087262333870314, -105.22697137813459 40.08725160165343, -105.22699571350596 40.087241208108466, -105.22702022223042 40.08723115271041, -105.22704495703813 40.08722144459034, -105.227069908556 40.08721208192462, -105.22709506621307 40.08720306919137, -105.22712043116775 40.087194409995774, -105.22714598347935 40.08718610609185, -105.22717172665875 40.087178159289046, -105.22719775801576 40.08717057341977, -105.22722361633834 40.08716344466387, -105.22724448443779 40.08716355701311, -105.2283729549368 40.08717092525384, -105.23154113747518 40.08755923148525, -105.23159510346865 40.08756556421094, -105.23164921918521 40.087571695514775, -105.23170346329434 40.087577086760916, -105.2317578193674 40.087581740612926, -105.23181226515209 40.08758564981383, -105.23186678657542 40.08758881433079, -105.23192136722312 40.087591233224956, -105.23197599065594 40.08759291186197, -105.23203063698061 40.0875938393878, -105.23208529443761 40.087594023881024, -105.23213995014099 40.08759346170912, -105.23219457593261 40.08759215640933, -105.2322491612788 40.08759010255342, -105.23230368974735 40.08758730370593, -105.2323581460858 40.0875837616329, -105.23241251387269 40.08757947719696, -105.23246676965806 40.08757444944327, -105.23252090521092 40.087568683756814, -105.23257489826456 40.087562176483594, -105.23262887644508 40.08755497475301, -105.2326832836757 40.08754720298132, -105.23273745343701 40.08753868580036, -105.23279137280774 40.08752942858451, -105.23284501598923 40.08751943127434, -105.23289837710301 40.08750869745924, -105.23295142683274 40.08749722707182, -105.23300416396908 40.08748502911613, -105.23305656036149 40.087472105328814, -105.23310860895167 40.08745846109794, -105.2331195646996 40.08745541432238, -105.23316028980796 40.08744409547717, -105.23321158647039 40.0874290192368, -105.23325722526434 40.08741486387087, -105.23331065628268 40.0873970203308, -105.23336321621771 40.08737853169327, -105.23341535087839 40.087359340446866, -105.23346703913232 40.087339452848035, -105.23351826805532 40.087318875171945, -105.23353501546842 40.08731185997121, -105.23351980873542 40.08730061994037, -105.23348420652255 40.08728144947539, -105.23355750841804 40.087252128831985, -105.23366420622754 40.087209448458204, -105.23374988793036 40.08716518662143, -105.2338752055783 40.08710044895112, -105.23401411763574 40.08701357127359, -105.23405471434727 40.08698818193187, -105.23411691940804 40.086949276818785, -105.23417420629958 40.086913448661726, -105.2341886118381 40.08690464559623, -105.2342102060382 40.086891448617656, -105.23428749079763 40.08682176614175, -105.23441136165638 40.086710080208086, -105.23462963814833 40.08650825210744, -105.23475320596388 40.086352448783096, -105.23492720557088 40.08608544943124, -105.23511620693853 40.08560644881669, -105.23513820542169 40.08551144874158, -105.23508520578451 40.084612448422696, -105.23507763897449 40.08420165278985, -105.23504972033575 40.082685891632984, -105.23500320640507 40.08016044862552, -105.22990520441682 40.080080448767525, -105.23344320557413 40.078991447490566, -105.23528920541436 40.07873844737262, -105.2378132062725 40.07833444783447, -105.2384812068036 40.07833244791702, -105.2403432064991 40.07833344770941, -105.2423652076105 40.078337446899226, -105.2435522068469 40.07833844725607, -105.2446880588089 40.07833844686491, -105.24468805830135 40.07833920790986, -105.24504820729896 40.07833944731037, -105.24673520863611 40.078331447150774, -105.24797620779272 40.07832544680577, -105.25099013604314 40.078310396494125, -105.25527884476058 40.07829042246069, -105.26347521219596 40.07824944591677, -105.26350221203036 40.08020744623987, -105.26590662387704 40.08014227963445, -105.26781071843679 40.08009626548748, -105.26912046745295 40.08006436083225, -105.27077346961903 40.08002883906712, -105.27160286885797 40.08001390036796, -105.27221118650809 40.080002939133784, -105.27324884225148 40.079984235686155, -105.27384721512072 40.07997344533944, -105.27419040076023 40.07997698391911, -105.275236925473 40.07998199934345, -105.27605921521977 40.07997644544199, -105.27744921504366 40.079994445459, -105.27744421502449 40.07989344467622, -105.2775032146846 40.079894445544724, -105.27748622062703 40.079147659928644, -105.27746233361805 40.07819218232893, -105.27742321523138 40.076796444237125, -105.27741821516419 40.07662844439344, -105.27741421523704 40.076479443791015, -105.27747957171408 40.0764360956394, -105.2776022148752 40.076336445003435, -105.27776121509011 40.07620044483633, -105.27790221524532 40.076038444205025, -105.27802021477937 40.07579044515734, -105.27837421480645 40.07579144511136, -105.27837221449197 40.07653744417692, -105.27825321431087 40.076662444087866, -105.2821112161553 40.076667443866434, -105.28213421606061 40.0791254445771, -105.28222234668438 40.07989150774977, -105.28226905976508 40.079652017977175, -105.28230485779454 40.07952086600779, -105.28234387199792 40.079389994786425, -105.28251296947849 40.078921987943744, -105.28267091070731 40.078590119366666, -105.28380184191316 40.0763738690773, -105.28393200076792 40.07612210589992, -105.28398197953325 40.076025020701806, -105.28406143801703 40.075870593400765, -105.28417290601259 40.075653956171635, -105.28434304434431 40.07530206774775, -105.28448810963225 40.07496797674111, -105.28461404885985 40.07458004438773, -105.28465582545337 40.07436407727556, -105.28467994420292 40.07408191848048, -105.28467401152466 40.07381095898337, -105.28463484297197 40.07354103535643, -105.28450988776724 40.073054082397505, -105.28442380461658 40.072761148741264, -105.2844119360205 40.07272887084649, -105.28412585397858 40.071782898508566, -105.28395645232631 40.07122915445703, -105.28344713249602 40.06958603676775, -105.28308992365754 40.068431019485985, -105.28288288254652 40.06781286879525, -105.28281030837537 40.067598853959865, -105.28276674879744 40.0674749475167, -105.28270868235202 40.067305987729235, -105.2826287480644 40.067103216087304, -105.28246902233936 40.06665264506963, -105.28217776448983 40.06610051550977, -105.28182052768169 40.06556514578249, -105.28230765209639 40.06555737709394, -105.2826421053623 40.06555460571782, -105.28403966119708 40.065560524761885, -105.2840422155819 40.0655634422325, -105.28411021477325 40.06556744313233, -105.28415551999306 40.065576595580495, -105.28420921525914 40.065587442503464, -105.28425521504384 40.065603442926026, -105.28431321516172 40.06563044283727, -105.28443921505063 40.0657224424132, -105.28444195810373 40.06556495868456, -105.28446964823674 40.06556530130753, -105.28447506820109 40.065456469196135, -105.28447438931113 40.06528829290035, -105.28446936431091 40.064040573617774, -105.28446811113976 40.06372971757044, -105.28391947161099 40.063728798834106, -105.28350794807665 40.06372864274691, -105.28329623749258 40.06372837690664, -105.28231998250595 40.063726265867324, -105.28212792868496 40.06372330059435, -105.28180650241363 40.0636562328228, -105.28142227479943 40.06419864439965, -105.28095156586173 40.064311086638334, -105.28057142108304 40.06429735375461, -105.2802739685094 40.06411686471955, -105.27998099798846 40.063939524011275, -105.27945708434669 40.063606076359854, -105.27668180871433 40.0618889301708, -105.27640602650123 40.06171701384444, -105.27307209828221 40.059640091950456, -105.27139117766788 40.05857795867715, -105.27080189335564 40.058203994632166, -105.27047994683524 40.05801009468256, -105.26961392253298 40.05749501959285, -105.26822395538733 40.05662805383557, -105.26687497370085 40.05580013493221, -105.2656519227221 40.055032027497674, -105.26511291786467 40.0547020581333, -105.2643711340155 40.05423304186316, -105.26366888805782 40.05380006284676, -105.26289002157647 40.05331696043408, -105.26248295310934 40.05306301764614, -105.26233610037056 40.052969927775095, -105.26219603118284 40.05287795048658, -105.26200287945368 40.05274495970432, -105.26176591652835 40.0525759170593, -105.26149299910482 40.05237111141436, -105.26124506668879 40.0521729459601, -105.26106982878406 40.05202599008051, -105.26095301915907 40.051923901911515, -105.26078709832663 40.05176900406456, -105.26066713346091 40.051649889503814, -105.26057494258106 40.051556087536326, -105.26037603182047 40.0513360595755, -105.26021417081213 40.05114493352249, -105.26011882647472 40.05103410417082, -105.25987414472125 40.05103112475856, -105.25965409567844 40.05103203920658, -105.25948298345538 40.05103387844358, -105.25930294943528 40.051032954539856, -105.25897683349142 40.05102705814787, -105.2587289291635 40.051025990659284, -105.25849816103424 40.05102797837995, -105.25755903316241 40.051030126762775, -105.25731005474265 40.05102987806262, -105.25723110961195 40.05102998669123, -105.25696783780707 40.05103107976799, -105.25668098975056 40.051032121630236, -105.25604407166001 40.051032973477305, -105.25515886912677 40.05103905939236, -105.25495310848838 40.05103999519333, -105.2542390203288 40.05104396683892, -105.25373709614865 40.05105387742171, -105.25320016447833 40.051063985647914, -105.25241995359185 40.05107796120676, -105.25104286103227 40.05108488106519, -105.25087603730138 40.05108589359897, -105.24905814625026 40.05109101404377, -105.24838514258077 40.051093116821185, -105.24752316264134 40.051098096907594, -105.24689590213573 40.05109507542115, -105.2461500947277 40.051078887987465, -105.24424294058713 40.05107302924297, -105.24284194260892 40.051072112100485, -105.24214891611415 40.05107907484076, -105.23653208552355 40.05106995573312, -105.23575082660882 40.05107695324783, -105.23488297804161 40.05109024293931, -105.23456586939088 40.0510950970329, -105.23450514649396 40.05109413413817, -105.23425404690599 40.051088065751614, -105.233742911622 40.05109392331027, -105.23285798278255 40.05110405832345, -105.23225896732653 40.05109498290111, -105.23133106091885 40.051059060739355, -105.2255132508242 40.05104207956713, -105.22551219971524 40.05104844465996, -105.22551319939883 40.051666444909664, -105.22551448184258 40.052332671969985, -105.2255172002856 40.05374544531903, -105.22551820051213 40.054765445704426, -105.22526219996293 40.05476044491763, -105.22508896577155 40.0547790063182, -105.22489820086776 40.054799444950255, -105.22476297967225 40.054837274906234, -105.22456220039183 40.05489344487475, -105.22449156003717 40.05491131624516, -105.22426695491855 40.05496813582263, -105.22389019925588 40.05506344591768, -105.22346119933347 40.055151445114625, -105.2226751991902 40.055234445916675, -105.22151019920918 40.05551444592377, -105.22079519863445 40.0557584459232, -105.22080819830997 40.054664445029374, -105.21994807985942 40.05465482055129, -105.21788015871469 40.05464468834945, -105.21597319841416 40.05462644657686, -105.21594919810053 40.05506044566964, -105.21593992532243 40.05548742980623, -105.21592719878397 40.056073446608806, -105.21592419884637 40.05654844624868, -105.21603819786819 40.05677044599801, -105.2160881989679 40.05694944610164, -105.21609919829862 40.05722244647633, -105.21502719812406 40.05721844599338, -105.21474919875641 40.05722544618729, -105.21433819824436 40.0572654468832, -105.21425319797387 40.05728144632609, -105.2139361978653 40.05733944632712, -105.21360419727095 40.057429446131984, -105.21336219757937 40.05750044691125, -105.21319819810316 40.057549446361826, -105.213117197296 40.057567446244754, -105.21304319797039 40.05758444664818, -105.21285819789883 40.05759144654688, -105.21282019703902 40.05823044648699, -105.21593219905685 40.05825844688626, -105.21599976201229 40.0591844562415, -105.21611516235417 40.05918488788823, -105.21613890508245 40.060774957559104, -105.2161370248116 40.061655058070265, -105.21613513688418 40.06185105984153, -105.21613708897056 40.06326895154256, -105.21614891680326 40.06403186699564, -105.21615156956237 40.06476845457101, -105.21616016066007 40.065676155580995, -105.21388715671756 40.06781106466761, -105.21120005549055 40.07019030381962, -105.21072442530875 40.070576029378124, -105.20998061921591 40.071325237580616, -105.20862451508663 40.07265908095091, -105.20828016068076 40.073029971614666, -105.20764207829323 40.073717661778886, -105.2068623764414 40.074513419618434, -105.20694386699977 40.088905292658566, -105.20694813190755 40.088905271061016, -105.2075245971012 40.08890693460845, -105.20845619971197 40.088916451022676))</t>
         </is>
       </c>
       <c r="H122" t="inlineStr">
@@ -5562,7 +5590,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2651129178647 40.0547020581333, -105.2656519227221 40.05503202749767, -105.2668749737009 40.05580013493221, -105.2682239553873 40.05662805383557, -105.269613922533 40.05749501959285, -105.2704799468352 40.05801009468256, -105.2708018933556 40.05820399463217, -105.2713911776679 40.05857795867715, -105.2730720982822 40.05964009195046, -105.2764060265012 40.06171701384444, -105.2766818087143 40.0618889301708, -105.2794570843467 40.06360607635985, -105.2799809979885 40.06393952401127, -105.2802739685094 40.06411686471955, -105.280571421083 40.06429735375461, -105.2809515658617 40.06431108663833, -105.2814222747994 40.06419864439965, -105.2818065024136 40.0636562328228, -105.282127928685 40.06372330059435, -105.2821279542729 40.06368010832493, -105.2821240784269 40.06319387511908, -105.2821274673131 40.0629163435874, -105.2821210831339 40.06279005363829, -105.2821199255093 40.06225803662362, -105.2821208994861 40.0621770549917, -105.282124152918 40.06183007068088, -105.282129085445 40.05995210384833, -105.2821285218888 40.05958106496158, -105.2821285244142 40.05957697602803, -105.2811291285672 40.05959553140116, -105.2797971614958 40.05958806016634, -105.2797893342385 40.05923550936571, -105.2797884779981 40.05824016090641, -105.2810099891663 40.05823197123103, -105.282127839189 40.05821907062705, -105.2821289486717 40.05787208211032, -105.2821291566991 40.05780702153673, -105.2821291029179 40.05771203825965, -105.2821248835557 40.05679706254603, -105.2821221773207 40.05630292527739, -105.2821209028561 40.05614287870047, -105.2821191223585 40.05591749638784, -105.2821149073205 40.05544806278647, -105.2821118360542 40.05506812417644, -105.2821169945096 40.05457207967767, -105.2815789810369 40.05457792549657, -105.2811959688363 40.05459586760778, -105.2809251780282 40.05459809900324, -105.2805418593558 40.05460011581017, -105.2797980916086 40.05460199256783, -105.2791201089074 40.05460625740289, -105.2782424158444 40.05461177201197, -105.2776278783659 40.05461562941392, -105.2768269719381 40.05462065075204, -105.2761791738526 40.05462470900412, -105.275690884737 40.05462776515175, -105.2748409852941 40.05463303051442, -105.2743658758627 40.05463597077346, -105.2730088594046 40.05464498085863, -105.2727300726154 40.05464401602034, -105.2725639554301 40.05464506131736, -105.2724778624255 40.05464489159953, -105.272428917587 40.05464589297431, -105.2721809925417 40.05464705105311, -105.2695745880636 40.05466424885152, -105.269180883568 40.05466305040962, -105.2685039138491 40.05466608675869, -105.2682981408171 40.0546678695453, -105.2680041227128 40.05467194596278, -105.2674661100601 40.05467690189419, -105.267028132484 40.05467903835208, -105.2666369583191 40.054679895221, -105.2665258543755 40.05468104306746, -105.265755986229 40.05468909095225, -105.2651940136974 40.05470112528752, -105.2651129178647 40.0547020581333))</t>
+          <t>POLYGON ((-105.26511291786467 40.0547020581333, -105.2656519227221 40.055032027497674, -105.26687497370085 40.05580013493221, -105.26822395538733 40.05662805383557, -105.26961392253298 40.05749501959285, -105.27047994683524 40.05801009468256, -105.27080189335564 40.058203994632166, -105.27139117766788 40.05857795867715, -105.27307209828221 40.059640091950456, -105.27640602650123 40.06171701384444, -105.27668180871433 40.0618889301708, -105.27945708434669 40.063606076359854, -105.27998099798846 40.063939524011275, -105.2802739685094 40.06411686471955, -105.28057142108304 40.06429735375461, -105.28095156586173 40.064311086638334, -105.28142227479943 40.06419864439965, -105.28180650241363 40.0636562328228, -105.28212792868496 40.06372330059435, -105.28212795427294 40.06368010832493, -105.28212407842689 40.06319387511908, -105.28212746731309 40.062916343587396, -105.28212108313387 40.06279005363829, -105.28211992550935 40.06225803662362, -105.28212089948612 40.0621770549917, -105.28212415291804 40.06183007068088, -105.28212908544504 40.05995210384833, -105.28212852188875 40.059581064961584, -105.28212852441422 40.059576976028026, -105.28112912856719 40.059595531401165, -105.2797971614958 40.05958806016634, -105.27978933423847 40.05923550936571, -105.27978847799814 40.05824016090641, -105.28100998916634 40.05823197123103, -105.28212783918903 40.05821907062705, -105.28212894867168 40.05787208211032, -105.28212915669914 40.05780702153673, -105.28212910291788 40.05771203825965, -105.28212488355571 40.05679706254603, -105.28212217732066 40.056302925277386, -105.28212090285615 40.05614287870047, -105.28211912235848 40.05591749638784, -105.28211490732049 40.055448062786475, -105.28211183605417 40.055068124176444, -105.28211699450961 40.05457207967767, -105.28157898103692 40.054577925496574, -105.28119596883626 40.05459586760778, -105.28092517802817 40.054598099003236, -105.28054185935584 40.05460011581017, -105.27979809160863 40.05460199256783, -105.27912010890742 40.05460625740289, -105.27824241584442 40.05461177201197, -105.27762787836588 40.05461562941392, -105.2768269719381 40.05462065075204, -105.2761791738526 40.054624709004116, -105.27569088473705 40.05462776515175, -105.2748409852941 40.054633030514424, -105.27436587586266 40.05463597077346, -105.27300885940461 40.05464498085863, -105.27273007261545 40.05464401602034, -105.27256395543006 40.05464506131736, -105.27247786242548 40.05464489159953, -105.272428917587 40.054645892974314, -105.27218099254168 40.05464705105311, -105.2695745880636 40.05466424885152, -105.26918088356801 40.054663050409616, -105.26850391384906 40.054666086758694, -105.26829814081711 40.0546678695453, -105.26800412271278 40.05467194596278, -105.26746611006014 40.05467690189419, -105.26702813248401 40.054679038352084, -105.26663695831907 40.054679895221, -105.26652585437553 40.05468104306746, -105.265755986229 40.05468909095225, -105.26519401369744 40.054701125287515, -105.26511291786467 40.0547020581333))</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
@@ -5604,7 +5632,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2840396611971 40.06556052476189, -105.2826421053623 40.06555460571782, -105.2823076520964 40.06555737709394, -105.2818205276817 40.06556514578249, -105.2821777644898 40.06610051550977, -105.2824690223394 40.06665264506963, -105.2826287480644 40.0671032160873, -105.282708682352 40.06730598772923, -105.2827667487974 40.0674749475167, -105.2828103083754 40.06759885395986, -105.2828828825465 40.06781286879525, -105.2830899236575 40.06843101948598, -105.283447132496 40.06958603676775, -105.2839564523263 40.07122915445703, -105.2841258539786 40.07178289850857, -105.2844119360205 40.07272887084649, -105.2844238046166 40.07276114874126, -105.2845098877672 40.0730540823975, -105.284634842972 40.07354103535643, -105.2846740115247 40.07381095898337, -105.2846799442029 40.07408191848048, -105.2846558254534 40.07436407727556, -105.2846140488599 40.07458004438773, -105.2844881096322 40.07496797674111, -105.2843430443443 40.07530206774775, -105.2841729060126 40.07565395617164, -105.284061438017 40.07587059340077, -105.2839819795333 40.07602502070181, -105.2839320007679 40.07612210589992, -105.2838018419132 40.0763738690773, -105.2826709107073 40.07859011936667, -105.2825129694785 40.07892198794374, -105.2823438719979 40.07938999478642, -105.2823048577945 40.07952086600779, -105.2822690597651 40.07965201797717, -105.2822036751846 40.07998723360745, -105.2823430660183 40.07999338222898, -105.2823919994679 40.07989699918794, -105.2823952780968 40.07991484894792, -105.2824011515673 40.07990327952567, -105.282401297917 40.07990407867368, -105.2824011411118 40.07990508439865, -105.2824007327974 40.07990774683631, -105.2824003209599 40.07991041106865, -105.2823999149817 40.07991307621273, -105.2823995066586 40.07991574135234, -105.2823991053731 40.07991840560455, -105.2823987029122 40.07992107075525, -105.2823983016237 40.07992373590812, -105.2823979038555 40.07992640016695, -105.2823976774251 40.07992791372447, -105.2823975060843 40.07992906532645, -105.282397110658 40.07993173049039, -105.2823967163984 40.07993439745781, -105.2823963256647 40.0799370617299, -105.2823959384426 40.07993972780994, -105.2823955512205 40.07994239388992, -105.2823951651708 40.07994505997216, -105.2823947802935 40.0799477260566, -105.2823944012699 40.07995039485399, -105.282394021091 40.07995305824535, -105.2823936397224 40.07995572703835, -105.2823932630464 40.0799583949395, -105.2823928898907 40.07996106194668, -105.2823925179131 40.07996372715476, -105.2823921482747 40.07996639416855, -105.2823917798029 40.07996906298585, -105.2823914089919 40.0799717299974, -105.2823910440317 40.07997440062258, -105.2823906814308 40.079977066749, -105.2823903188241 40.07997973467666, -105.2823899597318 40.07998240351165, -105.2823896018177 40.07998507054752, -105.2824181042333 40.07999429284036, -105.286776370838 40.07996676963486, -105.2914711834894 40.07994775920668, -105.2963570642727 40.07992677134823, -105.29835794075 40.07992390089793, -105.2983609040826 40.07976014455694, -105.2983610203705 40.07975373487191, -105.2983672168973 40.07941148540178, -105.298374196989 40.07902591447207, -105.298383670297 40.0785026564008, -105.298398651852 40.07767504398448, -105.2984062371164 40.07725600516275, -105.2984137706934 40.07684093086841, -105.2984218454775 40.07643944552976, -105.2984230913359 40.07637737885216, -105.2984301702275 40.07602556232767, -105.2984466576848 40.0752057041428, -105.2984549189209 40.07479495861516, -105.298463156682 40.07438537756021, -105.2984794586653 40.07357484416879, -105.298488691564 40.07311568426164, -105.2984975212523 40.07267667106333, -105.2985005608829 40.07219478871703, -105.2985234482982 40.07173851752213, -105.2985730330561 40.07081656544484, -105.2986241173753 40.06991352311999, -105.2986677653263 40.06914193677803, -105.2986754958076 40.06900530517979, -105.29870025933 40.06856755163097, -105.2987192329377 40.06823210493573, -105.2987263238378 40.06810675099321, -105.2987302535221 40.06801697965914, -105.2987314888543 40.06786190499341, -105.2987225263747 40.06781885920241, -105.2986835881801 40.06763183250003, -105.2985903100406 40.06718967503565, -105.2984318069521 40.06643474608794, -105.2983516024941 40.06605274103391, -105.2983468262208 40.06603077853836, -105.2982682769369 40.06566967939599, -105.2982327825016 40.06550651392549, -105.2982014712006 40.06536256563826, -105.2981978518479 40.06534540199922, -105.2973789599828 40.06372975052703, -105.2973884290788 40.06373086323793, -105.2973402180112 40.06363444184545, -105.2965442169241 40.06353244180595, -105.2965352172466 40.06290744122514, -105.2970972181385 40.06282944126758, -105.2973032183859 40.0629314421194, -105.2977081053878 40.06286746179762, -105.2977170362547 40.06285833949234, -105.2977803364841 40.06279367683017, -105.2982490417868 40.06231488036838, -105.2985422998704 40.06165897982746, -105.2988779054747 40.06128408561559, -105.2993182269009 40.06101666839782, -105.2996941029532 40.06031562128015, -105.2999677819429 40.05966486894309, -105.2996155698368 40.05966386972095, -105.2999932869668 40.05842945264786, -105.3000911809479 40.05810952785405, -105.2991350028483 40.0581151348086, -105.2983635039619 40.05811965346847, -105.2921703812756 40.05815404431473, -105.292093210861 40.0581545069408, -105.2914999036799 40.05815926728892, -105.2913599215963 40.05815996086945, -105.2913551687225 40.05993760077276, -105.289365965576 40.06022976327775, -105.2883743746056 40.05914254968653, -105.2877547851576 40.05881224599267, -105.2868448433649 40.05833263860146, -105.285708142419 40.05830620782245, -105.2844697620174 40.05830177153683, -105.2844600273087 40.05897444858893, -105.2839918801106 40.05896469828112, -105.2825012375485 40.05895736100234, -105.2824985890428 40.05897044151475, -105.2822495295621 40.05896926932784, -105.2821288586788 40.05897133912178, -105.2821285244142 40.05957697602803, -105.2821285218888 40.05958106496158, -105.282129085445 40.05995210384833, -105.282124152918 40.06183007068088, -105.2821208994861 40.0621770549917, -105.2821199255093 40.06225803662362, -105.2821210831339 40.06279005363829, -105.2821274673131 40.0629163435874, -105.2821240784269 40.06319387511908, -105.2821279542729 40.06368010832493, -105.282127928685 40.06372330059435, -105.282319982506 40.06372626586732, -105.2832962374926 40.06372837690664, -105.2835079480766 40.06372864274691, -105.283919471611 40.06372879883411, -105.2844681111398 40.06372971757044, -105.2844693643109 40.06404057361777, -105.2844743893111 40.06528829290035, -105.2844750682011 40.06545646919614, -105.2844696482367 40.06556530130753, -105.2844419581037 40.06556495868456, -105.2844392150506 40.0657224424132, -105.2843132151617 40.06563044283727, -105.2842552150438 40.06560344292603, -105.2842092152591 40.06558744250346, -105.2841555199931 40.0655765955805, -105.2841102147732 40.06556744313233, -105.2840422155819 40.0655634422325, -105.2840396611971 40.06556052476189))</t>
+          <t>POLYGON ((-105.28403966119708 40.065560524761885, -105.2826421053623 40.06555460571782, -105.28230765209639 40.06555737709394, -105.28182052768169 40.06556514578249, -105.28217776448983 40.06610051550977, -105.28246902233936 40.06665264506963, -105.2826287480644 40.067103216087304, -105.28270868235202 40.067305987729235, -105.28276674879744 40.0674749475167, -105.28281030837537 40.067598853959865, -105.28288288254652 40.06781286879525, -105.28308992365754 40.068431019485985, -105.28344713249602 40.06958603676775, -105.28395645232631 40.07122915445703, -105.28412585397858 40.071782898508566, -105.2844119360205 40.07272887084649, -105.28442380461658 40.072761148741264, -105.28450988776724 40.073054082397505, -105.28463484297197 40.07354103535643, -105.28467401152466 40.07381095898337, -105.28467994420292 40.07408191848048, -105.28465582545337 40.07436407727556, -105.28461404885985 40.07458004438773, -105.28448810963225 40.07496797674111, -105.28434304434431 40.07530206774775, -105.28417290601259 40.075653956171635, -105.28406143801703 40.075870593400765, -105.28398197953325 40.076025020701806, -105.28393200076792 40.07612210589992, -105.28380184191316 40.0763738690773, -105.28267091070731 40.078590119366666, -105.28251296947849 40.078921987943744, -105.28234387199792 40.079389994786425, -105.28230485779454 40.07952086600779, -105.28226905976508 40.079652017977175, -105.28220367518465 40.07998723360745, -105.28234306601831 40.079993382228984, -105.28239199946788 40.07989699918794, -105.28239527809679 40.079914848947915, -105.28240115156734 40.07990327952567, -105.28240129791703 40.07990407867368, -105.2824011411118 40.079905084398646, -105.28240073279743 40.07990774683631, -105.28240032095991 40.07991041106865, -105.28239991498172 40.07991307621273, -105.28239950665863 40.07991574135234, -105.28239910537312 40.07991840560455, -105.2823987029122 40.07992107075525, -105.28239830162374 40.07992373590812, -105.28239790385547 40.079926400166954, -105.2823976774251 40.07992791372447, -105.28239750608431 40.079929065326446, -105.28239711065801 40.079931730490394, -105.28239671639837 40.079934397457805, -105.28239632566468 40.0799370617299, -105.28239593844259 40.07993972780994, -105.28239555122052 40.079942393889915, -105.2823951651708 40.07994505997216, -105.28239478029354 40.0799477260566, -105.28239440126987 40.07995039485399, -105.282394021091 40.07995305824535, -105.28239363972239 40.07995572703835, -105.28239326304644 40.079958394939496, -105.28239288989066 40.079961061946676, -105.28239251791308 40.079963727154755, -105.28239214827467 40.07996639416855, -105.28239177980291 40.07996906298585, -105.28239140899193 40.0799717299974, -105.28239104403173 40.07997440062258, -105.28239068143081 40.079977066748995, -105.28239031882407 40.079979734676655, -105.28238995973182 40.07998240351165, -105.28238960181771 40.07998507054752, -105.28241810423329 40.07999429284036, -105.28677637083796 40.079966769634865, -105.2914711834894 40.07994775920668, -105.29635706427274 40.079926771348234, -105.29835794074998 40.07992390089793, -105.29836090408264 40.07976014455694, -105.29836102037052 40.079753734871915, -105.29836721689729 40.07941148540178, -105.29837419698899 40.07902591447207, -105.29838367029699 40.0785026564008, -105.298398651852 40.077675043984485, -105.29840623711641 40.077256005162745, -105.29841377069337 40.076840930868414, -105.29842184547755 40.07643944552976, -105.29842309133593 40.07637737885216, -105.2984301702275 40.07602556232767, -105.29844665768478 40.0752057041428, -105.29845491892085 40.074794958615165, -105.29846315668199 40.07438537756021, -105.29847945866533 40.07357484416879, -105.29848869156396 40.07311568426164, -105.29849752125233 40.072676671063334, -105.29850056088293 40.07219478871703, -105.29852344829816 40.07173851752213, -105.29857303305606 40.070816565444844, -105.29862411737528 40.069913523119986, -105.29866776532633 40.06914193677803, -105.29867549580761 40.06900530517979, -105.29870025933 40.06856755163097, -105.29871923293773 40.06823210493573, -105.29872632383777 40.06810675099321, -105.29873025352208 40.06801697965914, -105.29873148885427 40.06786190499341, -105.29872252637469 40.06781885920241, -105.29868358818013 40.067631832500034, -105.29859031004062 40.06718967503565, -105.29843180695205 40.066434746087936, -105.29835160249407 40.066052741033914, -105.29834682622077 40.06603077853836, -105.29826827693685 40.06566967939599, -105.29823278250161 40.06550651392549, -105.29820147120063 40.06536256563826, -105.29819785184789 40.06534540199922, -105.29737895998284 40.06372975052703, -105.29738842907875 40.06373086323793, -105.29734021801116 40.06363444184545, -105.29654421692415 40.06353244180595, -105.2965352172466 40.06290744122514, -105.29709721813846 40.06282944126758, -105.2973032183859 40.0629314421194, -105.29770810538781 40.06286746179762, -105.29771703625465 40.062858339492344, -105.29778033648411 40.06279367683017, -105.29824904178682 40.062314880368376, -105.29854229987045 40.06165897982746, -105.29887790547468 40.06128408561559, -105.29931822690087 40.06101666839782, -105.29969410295321 40.06031562128015, -105.29996778194288 40.059664868943095, -105.29961556983679 40.05966386972095, -105.29999328696678 40.058429452647864, -105.30009118094793 40.05810952785405, -105.29913500284829 40.0581151348086, -105.29836350396188 40.05811965346847, -105.29217038127562 40.05815404431473, -105.29209321086095 40.0581545069408, -105.29149990367995 40.05815926728892, -105.29135992159628 40.058159960869446, -105.29135516872255 40.059937600772756, -105.28936596557595 40.060229763277746, -105.28837437460561 40.05914254968653, -105.28775478515759 40.05881224599267, -105.28684484336493 40.058332638601456, -105.28570814241903 40.058306207822454, -105.28446976201742 40.05830177153683, -105.2844600273087 40.058974448588934, -105.28399188011062 40.05896469828112, -105.28250123754852 40.058957361002335, -105.28249858904276 40.058970441514745, -105.28224952956214 40.05896926932784, -105.28212885867882 40.05897133912178, -105.28212852441422 40.059576976028026, -105.28212852188875 40.059581064961584, -105.28212908544504 40.05995210384833, -105.28212415291804 40.06183007068088, -105.28212089948612 40.0621770549917, -105.28211992550935 40.06225803662362, -105.28212108313387 40.06279005363829, -105.28212746731309 40.062916343587396, -105.28212407842689 40.06319387511908, -105.28212795427294 40.06368010832493, -105.28212792868496 40.06372330059435, -105.28231998250595 40.063726265867324, -105.28329623749258 40.06372837690664, -105.28350794807665 40.06372864274691, -105.28391947161099 40.063728798834106, -105.28446811113976 40.06372971757044, -105.28446936431091 40.064040573617774, -105.28447438931113 40.06528829290035, -105.28447506820109 40.065456469196135, -105.28446964823674 40.06556530130753, -105.28444195810373 40.06556495868456, -105.28443921505063 40.0657224424132, -105.28431321516172 40.06563044283727, -105.28425521504384 40.065603442926026, -105.28420921525914 40.065587442503464, -105.28415551999306 40.065576595580495, -105.28411021477325 40.06556744313233, -105.2840422155819 40.0655634422325, -105.28403966119708 40.065560524761885))</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
@@ -5646,7 +5674,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.285708142419 40.05830620782245, -105.2868448433649 40.05833263860146, -105.2877547851576 40.05881224599267, -105.2883743746056 40.05914254968653, -105.289365965576 40.06022976327775, -105.2913551687225 40.05993760077276, -105.2913599215963 40.05815996086945, -105.2914999036799 40.05815926728892, -105.292093210861 40.0581545069408, -105.2921703812756 40.05815404431473, -105.2983635039619 40.05811965346847, -105.2991350028483 40.0581151348086, -105.3000911809479 40.05810952785405, -105.3000918507764 40.0581073368398, -105.3004110715137 40.05774889241609, -105.3011622582961 40.05774407019464, -105.3012407527371 40.05774356595811, -105.3012352909331 40.05733490149893, -105.3012300813415 40.05683939706749, -105.3012242930165 40.05654311294367, -105.3012131439918 40.05580240605936, -105.3012016743867 40.05517407771591, -105.3011781566274 40.05518522413686, -105.3009725525449 40.05528267008335, -105.3004745146386 40.05460527172093, -105.3004680431854 40.0544257948489, -105.3004667791446 40.05434674915338, -105.3004811651408 40.05383857656198, -105.3011681855068 40.0538302038374, -105.3011773462785 40.05383009172997, -105.3011748535467 40.05361835784946, -105.3011733260973 40.05348832425237, -105.3011638641235 40.0529847685901, -105.3011618078404 40.0528753219722, -105.3011507208908 40.05211418188754, -105.3011279442928 40.05088702920902, -105.3011130281842 40.04998853356952, -105.3010980915397 40.0491080498573, -105.3010973598342 40.04906482920834, -105.3010754027105 40.04728861907851, -105.3010750669934 40.04726150809377, -105.3004821178877 40.04726067432208, -105.2995777074999 40.04725939327028, -105.2993785148173 40.04725911013684, -105.2984338616306 40.04725776364863, -105.2979832250498 40.04725711872771, -105.2970158594432 40.04725572806646, -105.2962874641264 40.04725467490402, -105.2956195772189 40.04725370722846, -105.2955740425528 40.04725388504762, -105.2955646637362 40.04725392156858, -105.295138592642 40.04725557509141, -105.295047096733 40.04725593047504, -105.2948781256633 40.04725736935744, -105.2948338484197 40.04725716454314, -105.2944404634873 40.04726439007469, -105.2944399091494 40.04726439989486, -105.2941419153592 40.04726664801208, -105.2939623175397 40.04747117356362, -105.2935617690094 40.04739276589242, -105.2931333735992 40.04730854635932, -105.2931351899642 40.04730587018746, -105.2931190714868 40.04730785513716, -105.2930831475293 40.0473122777485, -105.2925641480346 40.04711827748598, -105.2923231477523 40.04702627775064, -105.2919101464262 40.04687227752947, -105.2913721469993 40.04667627690404, -105.2911531463136 40.04661827793976, -105.2909281466963 40.04658027739244, -105.2906991479196 40.04656127733434, -105.2902751471324 40.04655527824723, -105.2899511476118 40.04655327844637, -105.2897911477727 40.04655927808477, -105.2897901469812 40.0465592780627, -105.2897141473675 40.04656927817304, -105.2893061469497 40.04665027849616, -105.2888621465885 40.04674327839245, -105.2882791462674 40.04678027777359, -105.2870501458672 40.0467962784804, -105.2868921471954 40.04679127727393, -105.2868061477403 40.04678647645866, -105.286746270903 40.04678767354718, -105.2866864608666 40.04678886892687, -105.2866191303324 40.0467902142856, -105.2864670367458 40.04677515236694, -105.2863934400896 40.04676641224462, -105.2861362872023 40.04670112252147, -105.2860716123038 40.04666698333216, -105.285885097885 40.04656853062735, -105.2857154248379 40.04647912979314, -105.2856533922188 40.04644895272444, -105.2856197993314 40.04643504824607, -105.2856107278606 40.04643129369941, -105.2856042908745 40.04642862932879, -105.2855920325154 40.04642355481273, -105.285576904431 40.04641729331141, -105.2855675298397 40.04641341390852, -105.2854574967038 40.04639188200418, -105.2853743746032 40.04637561661295, -105.2851725674794 40.0463753941511, -105.2846960458856 40.04637486888372, -105.2845321459332 40.04637827899764, -105.2839881453484 40.04637427796205, -105.2820953129514 40.04639418149944, -105.2820953673213 40.046387805911, -105.2820872681542 40.04638789148733, -105.2820770794491 40.04638799833468, -105.2820770792187 40.04638807038612, -105.2820800498064 40.04657612150675, -105.2820809866036 40.04661812411999, -105.2820839656067 40.04713889101917, -105.2820848286775 40.04720395369414, -105.2820858248411 40.04778593388745, -105.2820868910294 40.04801104126194, -105.2820869405271 40.04821912535708, -105.2820929716489 40.04867895465735, -105.282093962903 40.04870393781199, -105.2820991666128 40.04886399194467, -105.282110156031 40.04900209559193, -105.2821528537462 40.04961297875377, -105.2821529080917 40.05004287445905, -105.282111936332 40.0507911330381, -105.2821010018127 40.05108292507596, -105.2821001394499 40.05112904293382, -105.2820950329251 40.05160889046894, -105.2821022271971 40.05242015642738, -105.2821029972769 40.05280498132497, -105.2821050101574 40.0530690713008, -105.2821110289956 40.05386793028244, -105.282113919467 40.05419296421472, -105.2821140566117 40.05426186853085, -105.2821169945096 40.05457207967767, -105.2821118360542 40.05506812417644, -105.2821149073205 40.05544806278647, -105.2821191223585 40.05591749638784, -105.2821209028561 40.05614287870047, -105.2821221773207 40.05630292527739, -105.2821248835557 40.05679706254603, -105.2821291029179 40.05771203825965, -105.2821291566991 40.05780702153673, -105.2821289486717 40.05787208211032, -105.282127839189 40.05821907062705, -105.2810099891663 40.05823197123103, -105.2797884779981 40.05824016090641, -105.2797893342385 40.05923550936571, -105.2797971614958 40.05958806016634, -105.2798664812612 40.05958844910147, -105.2805889964471 40.0595925035874, -105.2811291285672 40.05959553140116, -105.2815719599436 40.05958731081207, -105.2821285244142 40.05957697602803, -105.2821288586788 40.05897133912178, -105.2822495295621 40.05896926932784, -105.2824985890428 40.05897044151475, -105.2825012375485 40.05895736100234, -105.2839918801106 40.05896469828112, -105.2844600273087 40.05897444858893, -105.2844697620174 40.05830177153683, -105.285708142419 40.05830620782245))</t>
+          <t>POLYGON ((-105.28570814241903 40.058306207822454, -105.28684484336493 40.058332638601456, -105.28775478515759 40.05881224599267, -105.28837437460561 40.05914254968653, -105.28936596557595 40.060229763277746, -105.29135516872255 40.059937600772756, -105.29135992159628 40.058159960869446, -105.29149990367995 40.05815926728892, -105.29209321086095 40.0581545069408, -105.29217038127562 40.05815404431473, -105.29836350396188 40.05811965346847, -105.29913500284829 40.0581151348086, -105.30009118094793 40.05810952785405, -105.3000918507764 40.058107336839804, -105.30041107151371 40.05774889241609, -105.30116225829613 40.05774407019464, -105.30124075273713 40.05774356595811, -105.30123529093312 40.05733490149893, -105.30123008134152 40.05683939706749, -105.30122429301649 40.05654311294367, -105.30121314399184 40.05580240605936, -105.3012016743867 40.05517407771591, -105.30117815662739 40.055185224136864, -105.30097255254488 40.05528267008335, -105.30047451463864 40.05460527172093, -105.30046804318536 40.0544257948489, -105.30046677914456 40.05434674915338, -105.30048116514075 40.05383857656198, -105.3011681855068 40.0538302038374, -105.30117734627855 40.05383009172997, -105.30117485354671 40.05361835784946, -105.30117332609733 40.05348832425237, -105.30116386412348 40.0529847685901, -105.30116180784037 40.0528753219722, -105.3011507208908 40.05211418188754, -105.30112794429279 40.05088702920902, -105.3011130281842 40.04998853356952, -105.30109809153974 40.049108049857296, -105.30109735983416 40.04906482920834, -105.30107540271047 40.047288619078515, -105.30107506699336 40.04726150809377, -105.3004821178877 40.047260674322075, -105.29957770749995 40.04725939327028, -105.29937851481728 40.04725911013684, -105.29843386163064 40.04725776364863, -105.29798322504976 40.047257118727714, -105.29701585944319 40.04725572806646, -105.29628746412635 40.04725467490402, -105.29561957721893 40.047253707228464, -105.29557404255284 40.04725388504762, -105.2955646637362 40.04725392156858, -105.29513859264199 40.047255575091405, -105.295047096733 40.04725593047504, -105.29487812566329 40.04725736935744, -105.29483384841966 40.04725716454314, -105.29444046348732 40.04726439007469, -105.2944399091494 40.047264399894864, -105.29414191535923 40.047266648012084, -105.29396231753974 40.04747117356362, -105.29356176900943 40.04739276589242, -105.29313337359919 40.04730854635932, -105.29313518996419 40.047305870187465, -105.29311907148684 40.04730785513716, -105.29308314752929 40.047312277748496, -105.29256414803459 40.04711827748598, -105.29232314775233 40.04702627775064, -105.2919101464262 40.046872277529474, -105.29137214699927 40.04667627690404, -105.29115314631362 40.046618277939764, -105.29092814669626 40.04658027739244, -105.29069914791957 40.04656127733434, -105.29027514713242 40.04655527824723, -105.28995114761177 40.046553278446375, -105.28979114777273 40.04655927808477, -105.28979014698116 40.0465592780627, -105.28971414736752 40.04656927817304, -105.28930614694967 40.04665027849616, -105.28886214658847 40.04674327839245, -105.28827914626736 40.046780277773586, -105.28705014586716 40.0467962784804, -105.28689214719539 40.046791277273925, -105.28680614774026 40.04678647645866, -105.28674627090295 40.04678767354718, -105.28668646086659 40.04678886892687, -105.2866191303324 40.0467902142856, -105.28646703674583 40.04677515236694, -105.28639344008961 40.046766412244615, -105.28613628720227 40.04670112252147, -105.28607161230383 40.04666698333216, -105.28588509788496 40.04656853062735, -105.28571542483787 40.04647912979314, -105.28565339221885 40.04644895272444, -105.28561979933141 40.04643504824607, -105.28561072786064 40.04643129369941, -105.2856042908745 40.046428629328794, -105.28559203251541 40.046423554812726, -105.28557690443104 40.04641729331141, -105.28556752983972 40.046413413908525, -105.28545749670384 40.04639188200418, -105.28537437460322 40.04637561661295, -105.28517256747945 40.0463753941511, -105.28469604588564 40.04637486888372, -105.2845321459332 40.04637827899764, -105.2839881453484 40.04637427796205, -105.28209531295138 40.04639418149944, -105.28209536732132 40.046387805911, -105.2820872681542 40.04638789148733, -105.28207707944905 40.04638799833468, -105.28207707921867 40.04638807038612, -105.28208004980642 40.046576121506746, -105.28208098660356 40.046618124119995, -105.28208396560674 40.047138891019166, -105.28208482867745 40.04720395369414, -105.28208582484109 40.047785933887454, -105.28208689102937 40.048011041261944, -105.28208694052707 40.04821912535708, -105.28209297164886 40.04867895465735, -105.28209396290302 40.048703937811986, -105.28209916661278 40.04886399194467, -105.28211015603097 40.04900209559193, -105.2821528537462 40.04961297875377, -105.2821529080917 40.050042874459045, -105.28211193633203 40.0507911330381, -105.28210100181266 40.05108292507596, -105.28210013944985 40.05112904293382, -105.28209503292514 40.05160889046894, -105.28210222719714 40.05242015642738, -105.28210299727688 40.05280498132497, -105.28210501015735 40.0530690713008, -105.28211102899559 40.053867930282436, -105.28211391946695 40.05419296421472, -105.28211405661175 40.05426186853085, -105.28211699450961 40.05457207967767, -105.28211183605417 40.055068124176444, -105.28211490732049 40.055448062786475, -105.28211912235848 40.05591749638784, -105.28212090285615 40.05614287870047, -105.28212217732066 40.056302925277386, -105.28212488355571 40.05679706254603, -105.28212910291788 40.05771203825965, -105.28212915669914 40.05780702153673, -105.28212894867168 40.05787208211032, -105.28212783918903 40.05821907062705, -105.28100998916634 40.05823197123103, -105.27978847799814 40.05824016090641, -105.27978933423847 40.05923550936571, -105.2797971614958 40.05958806016634, -105.2798664812612 40.05958844910147, -105.2805889964471 40.0595925035874, -105.28112912856719 40.059595531401165, -105.28157195994356 40.05958731081207, -105.28212852441422 40.059576976028026, -105.28212885867882 40.05897133912178, -105.28224952956214 40.05896926932784, -105.28249858904276 40.058970441514745, -105.28250123754852 40.058957361002335, -105.28399188011062 40.05896469828112, -105.2844600273087 40.058974448588934, -105.28446976201742 40.05830177153683, -105.28570814241903 40.058306207822454))</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
@@ -5688,7 +5716,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2727300726154 40.05464401602034, -105.2730088594046 40.05464498085863, -105.2743658758627 40.05463597077346, -105.2748409852941 40.05463303051442, -105.275690884737 40.05462776515175, -105.2761791738526 40.05462470900412, -105.2768269719381 40.05462065075204, -105.2776278783659 40.05461562941392, -105.2782424158444 40.05461177201197, -105.2791201089074 40.05460625740289, -105.2797980916086 40.05460199256783, -105.2805418593558 40.05460011581017, -105.2809251780282 40.05459809900324, -105.2811959688363 40.05459586760778, -105.2815789810369 40.05457792549657, -105.2821169945096 40.05457207967767, -105.2821140566117 40.05426186853085, -105.282113919467 40.05419296421472, -105.2821110289956 40.05386793028244, -105.2821050101574 40.0530690713008, -105.2821029972769 40.05280498132497, -105.2821022271971 40.05242015642738, -105.2820950329251 40.05160889046894, -105.2821001394499 40.05112904293382, -105.2821010018127 40.05108292507596, -105.282111936332 40.0507911330381, -105.2821529080917 40.05004287445905, -105.2821528537462 40.04961297875377, -105.282110156031 40.04900209559193, -105.2820991666128 40.04886399194467, -105.282093962903 40.04870393781199, -105.2820929716489 40.04867895465735, -105.2820869405271 40.04821912535708, -105.2820868910294 40.04801104126194, -105.2820858248411 40.04778593388745, -105.2820848286775 40.04720395369414, -105.2820839656067 40.04713889101917, -105.2820809866036 40.04661812411999, -105.2820800498064 40.04657612150675, -105.2820770792187 40.04638807038612, -105.2820770794491 40.04638799833468, -105.2820953673213 40.046387805911, -105.2820992602341 40.04592931828846, -105.2820912578224 40.04516431743618, -105.2820892588198 40.04495131835098, -105.2820842573841 40.04434731765315, -105.2820832594536 40.04409831790472, -105.2820852605044 40.04390531895158, -105.2820892596123 40.04365731844217, -105.2820891721232 40.04364509917423, -105.2820708481881 40.04364507266984, -105.2811339960779 40.04363808270838, -105.2810140330758 40.04362303129678, -105.280916842527 40.04363492538631, -105.2808521452884 40.04364990099339, -105.2805138861428 40.0436539251566, -105.2801638663687 40.04364996418393, -105.2798591715378 40.04365707025223, -105.2793880493568 40.0436589155447, -105.2786990124604 40.04367187124376, -105.2786218911866 40.04366293836192, -105.2785348284089 40.04363586799158, -105.2784508854329 40.04363790351297, -105.2783099946193 40.04368786927655, -105.2782389127541 40.04368910526165, -105.277825013327 40.04366799483049, -105.2776949977746 40.04366911697812, -105.277411038845 40.0436699420842, -105.2771699087427 40.04368100673599, -105.2771031715048 40.04366413205724, -105.2770421726654 40.04364013078624, -105.2769539577334 40.04363803919612, -105.2764819857427 40.04368104864997, -105.276330179594 40.04368295023548, -105.2760019664365 40.04367298005805, -105.275612997663 40.04367387151462, -105.2751229907905 40.04366193677129, -105.2747890229824 40.04366403053018, -105.2743839014497 40.04368904351995, -105.2742699258984 40.04370007599498, -105.2741371221832 40.04368005044567, -105.2740218735326 40.04364386275716, -105.2739200780991 40.04364393802936, -105.273753153546 40.04368094542063, -105.2731259839293 40.04367092892404, -105.2727509156415 40.04368089769377, -105.2727540573019 40.04488109794064, -105.2727519026059 40.04606289454581, -105.2727590236538 40.04714094192357, -105.2727631619907 40.04793513217358, -105.2727620283394 40.04816792149277, -105.2727588765819 40.04879189453326, -105.2727568838312 40.04917511836184, -105.2727550918599 40.05003408219484, -105.2727549655316 40.05007196592084, -105.2727550100268 40.05048703703091, -105.2727560962167 40.05080410792461, -105.2727589645644 40.05112200550927, -105.2727711990294 40.05229512756312, -105.2727729891799 40.05280812317558, -105.2727508467841 40.05387787658103, -105.2727299889079 40.0545619344025, -105.2727300726154 40.05464401602034))</t>
+          <t>POLYGON ((-105.27273007261545 40.05464401602034, -105.27300885940461 40.05464498085863, -105.27436587586266 40.05463597077346, -105.2748409852941 40.054633030514424, -105.27569088473705 40.05462776515175, -105.2761791738526 40.054624709004116, -105.2768269719381 40.05462065075204, -105.27762787836588 40.05461562941392, -105.27824241584442 40.05461177201197, -105.27912010890742 40.05460625740289, -105.27979809160863 40.05460199256783, -105.28054185935584 40.05460011581017, -105.28092517802817 40.054598099003236, -105.28119596883626 40.05459586760778, -105.28157898103692 40.054577925496574, -105.28211699450961 40.05457207967767, -105.28211405661175 40.05426186853085, -105.28211391946695 40.05419296421472, -105.28211102899559 40.053867930282436, -105.28210501015735 40.0530690713008, -105.28210299727688 40.05280498132497, -105.28210222719714 40.05242015642738, -105.28209503292514 40.05160889046894, -105.28210013944985 40.05112904293382, -105.28210100181266 40.05108292507596, -105.28211193633203 40.0507911330381, -105.2821529080917 40.050042874459045, -105.2821528537462 40.04961297875377, -105.28211015603097 40.04900209559193, -105.28209916661278 40.04886399194467, -105.28209396290302 40.048703937811986, -105.28209297164886 40.04867895465735, -105.28208694052707 40.04821912535708, -105.28208689102937 40.048011041261944, -105.28208582484109 40.047785933887454, -105.28208482867745 40.04720395369414, -105.28208396560674 40.047138891019166, -105.28208098660356 40.046618124119995, -105.28208004980642 40.046576121506746, -105.28207707921867 40.04638807038612, -105.28207707944905 40.04638799833468, -105.28209536732132 40.046387805911, -105.28209926023412 40.04592931828846, -105.28209125782237 40.04516431743618, -105.28208925881982 40.04495131835098, -105.28208425738407 40.04434731765315, -105.28208325945357 40.04409831790472, -105.28208526050436 40.04390531895158, -105.28208925961228 40.04365731844217, -105.28208917212322 40.04364509917423, -105.28207084818813 40.04364507266984, -105.28113399607793 40.043638082708384, -105.28101403307585 40.043623031296775, -105.280916842527 40.043634925386314, -105.28085214528839 40.04364990099339, -105.28051388614284 40.0436539251566, -105.28016386636871 40.043649964183935, -105.27985917153781 40.04365707025223, -105.27938804935681 40.043658915544704, -105.27869901246036 40.04367187124376, -105.27862189118657 40.04366293836192, -105.27853482840892 40.043635867991576, -105.27845088543295 40.043637903512966, -105.27830999461932 40.043687869276546, -105.27823891275412 40.04368910526165, -105.277825013327 40.04366799483049, -105.27769499777456 40.04366911697812, -105.27741103884502 40.0436699420842, -105.2771699087427 40.04368100673599, -105.27710317150485 40.04366413205724, -105.2770421726654 40.04364013078624, -105.27695395773341 40.04363803919612, -105.27648198574266 40.043681048649965, -105.27633017959401 40.04368295023548, -105.27600196643652 40.04367298005805, -105.27561299766298 40.04367387151462, -105.27512299079055 40.04366193677129, -105.27478902298239 40.04366403053018, -105.27438390144971 40.04368904351995, -105.27426992589838 40.04370007599498, -105.27413712218322 40.04368005044567, -105.27402187353265 40.043643862757165, -105.27392007809905 40.04364393802936, -105.27375315354602 40.04368094542063, -105.2731259839293 40.043670928924044, -105.2727509156415 40.04368089769377, -105.2727540573019 40.04488109794064, -105.27275190260586 40.04606289454581, -105.27275902365383 40.04714094192357, -105.27276316199067 40.047935132173585, -105.27276202833936 40.04816792149277, -105.27275887658193 40.04879189453326, -105.27275688383118 40.04917511836184, -105.27275509185988 40.05003408219484, -105.27275496553162 40.05007196592084, -105.27275501002678 40.05048703703091, -105.27275609621667 40.05080410792461, -105.27275896456437 40.05112200550927, -105.27277119902938 40.05229512756312, -105.2727729891799 40.05280812317558, -105.27275084678412 40.05387787658103, -105.27272998890791 40.0545619344025, -105.27273007261545 40.05464401602034))</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
@@ -5730,7 +5758,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2601188264747 40.05103410417082, -105.2602141708121 40.05114493352249, -105.2603760318205 40.0513360595755, -105.2605749425811 40.05155608753633, -105.2606671334609 40.05164988950381, -105.2607870983266 40.05176900406456, -105.2609530191591 40.05192390191151, -105.2610698287841 40.05202599008051, -105.2612450666888 40.0521729459601, -105.2614929991048 40.05237111141436, -105.2617659165283 40.0525759170593, -105.2620028794537 40.05274495970432, -105.2621960311828 40.05287795048658, -105.2623361003706 40.0529699277751, -105.2624829531093 40.05306301764614, -105.2628900215765 40.05331696043408, -105.2636688880578 40.05380006284676, -105.2643711340155 40.05423304186316, -105.2651129178647 40.0547020581333, -105.2651940136974 40.05470112528752, -105.265755986229 40.05468909095225, -105.2665258543755 40.05468104306746, -105.2666369583191 40.054679895221, -105.267028132484 40.05467903835208, -105.2674661100601 40.05467690189419, -105.2680041227128 40.05467194596278, -105.2682981408171 40.0546678695453, -105.2685039138491 40.05466608675869, -105.269180883568 40.05466305040962, -105.2695745880636 40.05466424885152, -105.2721809925417 40.05464705105311, -105.272428917587 40.05464589297431, -105.2724778624255 40.05464489159953, -105.2725639554301 40.05464506131736, -105.2727300726154 40.05464401602034, -105.2727299889079 40.0545619344025, -105.2727508467841 40.05387787658103, -105.2727729891799 40.05280812317558, -105.2727711990294 40.05229512756312, -105.2727589645644 40.05112200550927, -105.2727560962167 40.05080410792461, -105.2727550100268 40.05048703703091, -105.2727549655316 40.05007196592084, -105.2727550918599 40.05003408219484, -105.2727568838312 40.04917511836184, -105.2727588765819 40.04879189453326, -105.2727620283394 40.04816792149277, -105.2727631619907 40.04793513217358, -105.2727590236538 40.04714094192357, -105.2727519026059 40.04606289454581, -105.2727540573019 40.04488109794064, -105.2727509156415 40.04368089769377, -105.2724119538849 40.04368105275066, -105.2705431466196 40.04369794005434, -105.2697031199627 40.04368199106873, -105.2692694698212 40.04369157668958, -105.2689899124076 40.04369471714984, -105.2686831313114 40.04369632889271, -105.2681889710207 40.04369892437131, -105.2674581055709 40.04370276022885, -105.2674373425578 40.04370286968756, -105.2666950373309 40.04370675961066, -105.2659102649756 40.04371086932636, -105.2656216311616 40.04371237735209, -105.2656227612868 40.04430003885544, -105.2656235574844 40.0447145876716, -105.2656244520254 40.04518062047342, -105.2656250546597 40.04549539315068, -105.265627763298 40.0455709117729, -105.2655879950437 40.04557694008583, -105.265425826989 40.04557825778472, -105.2652211535706 40.04558003726618, -105.2648150348807 40.04557893545725, -105.2642131467077 40.0455870413356, -105.2637041480973 40.04558901899909, -105.2635908481951 40.0456099251388, -105.2634871236304 40.04565006704565, -105.2634008580785 40.04570287176336, -105.2633278669242 40.04563601458425, -105.2632831151267 40.04556290084826, -105.2632726527912 40.04553756123483, -105.2631531738905 40.04553645591186, -105.2631165811388 40.04553710851337, -105.2625430837086 40.04554395622243, -105.2620721242456 40.04554828991369, -105.2612685278558 40.0455556805962, -105.2611859293927 40.04555644003092, -105.2608964703001 40.04555909908301, -105.2608058840952 40.04555993265756, -105.2587244031369 40.04556793308797, -105.2585405106698 40.04557391508014, -105.2585412801613 40.04583500499989, -105.2585431409786 40.0466000914717, -105.2585491366171 40.04702505910149, -105.2585801436604 40.04744788236328, -105.2586361577098 40.04786993381616, -105.2587031080589 40.04822996778709, -105.2587330305727 40.04835411276961, -105.2588011065953 40.04859802744705, -105.2588770324828 40.04884497745633, -105.2589520194323 40.04905404325294, -105.2590968835464 40.04940298337421, -105.2592908491195 40.04980693019196, -105.2594790114012 40.05013509748598, -105.2595461504909 40.05024092674891, -105.2597039348822 40.05047294914017, -105.2598909228966 40.05073001337415, -105.2600729289857 40.05098212507661, -105.2601188264747 40.05103410417082))</t>
+          <t>POLYGON ((-105.26011882647472 40.05103410417082, -105.26021417081213 40.05114493352249, -105.26037603182047 40.0513360595755, -105.26057494258106 40.051556087536326, -105.26066713346091 40.051649889503814, -105.26078709832663 40.05176900406456, -105.26095301915907 40.051923901911515, -105.26106982878406 40.05202599008051, -105.26124506668879 40.0521729459601, -105.26149299910482 40.05237111141436, -105.26176591652835 40.0525759170593, -105.26200287945368 40.05274495970432, -105.26219603118284 40.05287795048658, -105.26233610037056 40.052969927775095, -105.26248295310934 40.05306301764614, -105.26289002157647 40.05331696043408, -105.26366888805782 40.05380006284676, -105.2643711340155 40.05423304186316, -105.26511291786467 40.0547020581333, -105.26519401369744 40.054701125287515, -105.265755986229 40.05468909095225, -105.26652585437553 40.05468104306746, -105.26663695831907 40.054679895221, -105.26702813248401 40.054679038352084, -105.26746611006014 40.05467690189419, -105.26800412271278 40.05467194596278, -105.26829814081711 40.0546678695453, -105.26850391384906 40.054666086758694, -105.26918088356801 40.054663050409616, -105.2695745880636 40.05466424885152, -105.27218099254168 40.05464705105311, -105.272428917587 40.054645892974314, -105.27247786242548 40.05464489159953, -105.27256395543006 40.05464506131736, -105.27273007261545 40.05464401602034, -105.27272998890791 40.0545619344025, -105.27275084678412 40.05387787658103, -105.2727729891799 40.05280812317558, -105.27277119902938 40.05229512756312, -105.27275896456437 40.05112200550927, -105.27275609621667 40.05080410792461, -105.27275501002678 40.05048703703091, -105.27275496553162 40.05007196592084, -105.27275509185988 40.05003408219484, -105.27275688383118 40.04917511836184, -105.27275887658193 40.04879189453326, -105.27276202833936 40.04816792149277, -105.27276316199067 40.047935132173585, -105.27275902365383 40.04714094192357, -105.27275190260586 40.04606289454581, -105.2727540573019 40.04488109794064, -105.2727509156415 40.04368089769377, -105.27241195388488 40.043681052750664, -105.27054314661963 40.043697940054344, -105.26970311996267 40.04368199106873, -105.26926946982123 40.04369157668958, -105.26898991240756 40.04369471714984, -105.26868313131145 40.043696328892715, -105.26818897102069 40.043698924371306, -105.26745810557087 40.043702760228854, -105.26743734255783 40.04370286968756, -105.26669503733093 40.043706759610664, -105.26591026497559 40.04371086932636, -105.26562163116162 40.043712377352094, -105.26562276128678 40.04430003885544, -105.26562355748445 40.0447145876716, -105.26562445202536 40.045180620473424, -105.26562505465965 40.04549539315068, -105.26562776329804 40.0455709117729, -105.26558799504372 40.04557694008583, -105.26542582698897 40.04557825778472, -105.26522115357055 40.045580037266184, -105.26481503488071 40.04557893545725, -105.26421314670772 40.0455870413356, -105.26370414809735 40.04558901899909, -105.26359084819505 40.0456099251388, -105.26348712363036 40.04565006704565, -105.26340085807854 40.04570287176336, -105.26332786692423 40.045636014584254, -105.26328311512667 40.04556290084826, -105.2632726527912 40.04553756123483, -105.26315317389049 40.045536455911865, -105.26311658113885 40.04553710851337, -105.26254308370862 40.04554395622243, -105.26207212424558 40.04554828991369, -105.2612685278558 40.0455556805962, -105.2611859293927 40.04555644003092, -105.26089647030012 40.045559099083015, -105.26080588409516 40.04555993265756, -105.25872440313694 40.045567933087966, -105.2585405106698 40.04557391508014, -105.25854128016128 40.045835004999894, -105.25854314097862 40.046600091471696, -105.25854913661706 40.047025059101486, -105.25858014366037 40.04744788236328, -105.25863615770983 40.04786993381616, -105.25870310805891 40.048229967787094, -105.25873303057266 40.04835411276961, -105.25880110659527 40.04859802744705, -105.2588770324828 40.04884497745633, -105.25895201943227 40.04905404325294, -105.25909688354645 40.04940298337421, -105.25929084911945 40.04980693019196, -105.25947901140117 40.05013509748598, -105.25954615049089 40.050240926748906, -105.25970393488221 40.05047294914017, -105.25989092289659 40.05073001337415, -105.26007292898571 40.05098212507661, -105.26011882647472 40.05103410417082))</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
@@ -5772,7 +5800,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2442429405871 40.05107302924297, -105.2461500947277 40.05107888798747, -105.2468959021357 40.05109507542115, -105.2475231626413 40.05109809690759, -105.2483851425808 40.05109311682119, -105.2490581462503 40.05109101404377, -105.2508760373014 40.05108589359897, -105.2510428610323 40.05108488106519, -105.2524199535919 40.05107796120676, -105.2532001644783 40.05106398564791, -105.2537370961487 40.05105387742171, -105.2542390203288 40.05104396683892, -105.2549531084884 40.05103999519333, -105.2551588691268 40.05103905939236, -105.25604407166 40.05103297347731, -105.2566809897506 40.05103212163024, -105.2569678378071 40.05103107976799, -105.257231109612 40.05102998669123, -105.2573100547426 40.05102987806262, -105.2575590331624 40.05103012676278, -105.2584981610342 40.05102797837995, -105.2587289291635 40.05102599065928, -105.2589768334914 40.05102705814787, -105.2593029494353 40.05103295453986, -105.2594829834554 40.05103387844358, -105.2596540956784 40.05103203920658, -105.2598741447213 40.05103112475856, -105.2601188264747 40.05103410417082, -105.2600729289857 40.05098212507661, -105.2598909228966 40.05073001337415, -105.2597039348822 40.05047294914017, -105.2595461504909 40.05024092674891, -105.2594790114012 40.05013509748598, -105.2592908491195 40.04980693019196, -105.2590968835464 40.04940298337421, -105.2589520194323 40.04905404325294, -105.2588770324828 40.04884497745633, -105.2588011065953 40.04859802744705, -105.2587330305727 40.04835411276961, -105.2587031080589 40.04822996778709, -105.2586361577098 40.04786993381616, -105.2585801436604 40.04744788236328, -105.2585491366171 40.04702505910149, -105.2585431409786 40.0466000914717, -105.2585412801613 40.04583500499989, -105.2585405106698 40.04557391508014, -105.258535903728 40.04360206066097, -105.2583951659752 40.0436050597048, -105.2575578683964 40.04362608882376, -105.2567041520336 40.04364405736783, -105.2548139134812 40.04366009530941, -105.2545631178009 40.04367603314368, -105.2542829323291 40.04371990903944, -105.2539141370445 40.04377210462879, -105.2538390884301 40.0443769837805, -105.2538328837183 40.04480906253848, -105.2538480665677 40.04594587570338, -105.2532468905064 40.04595310180906, -105.2529968297143 40.04596107698521, -105.2527069963257 40.04600300642463, -105.2524960622399 40.04605608513078, -105.2522310257654 40.04615489213785, -105.2520470613259 40.04625606857408, -105.2517450365559 40.04640887536303, -105.2515508858689 40.04650168367383, -105.2512221055394 40.04660512723049, -105.2509489322841 40.04668112912296, -105.2506518826494 40.04674197938601, -105.2503909923662 40.04678012248868, -105.2500440548153 40.0468079211004, -105.2494600286874 40.04681187006781, -105.2489260161856 40.04681400383738, -105.2487620611019 40.04681501953493, -105.2486320348659 40.04681693211568, -105.2483308885866 40.04682588377189, -105.2483318758626 40.04742900308894, -105.2475249862594 40.04742394661578, -105.2472499260496 40.04742910946336, -105.2464551624836 40.04742901213277, -105.2457400405578 40.04743292882939, -105.2448631101524 40.04743593491281, -105.2443780481382 40.04743293931372, -105.2442269113973 40.04744413449284, -105.2442209462894 40.04874808419349, -105.2442229418913 40.0491681019278, -105.2442338761105 40.05025192424335, -105.2442310841703 40.05090087990886, -105.2442429405871 40.05107302924297))</t>
+          <t>POLYGON ((-105.24424294058713 40.05107302924297, -105.2461500947277 40.051078887987465, -105.24689590213573 40.05109507542115, -105.24752316264134 40.051098096907594, -105.24838514258077 40.051093116821185, -105.24905814625026 40.05109101404377, -105.25087603730138 40.05108589359897, -105.25104286103227 40.05108488106519, -105.25241995359185 40.05107796120676, -105.25320016447833 40.051063985647914, -105.25373709614865 40.05105387742171, -105.2542390203288 40.05104396683892, -105.25495310848838 40.05103999519333, -105.25515886912677 40.05103905939236, -105.25604407166001 40.051032973477305, -105.25668098975056 40.051032121630236, -105.25696783780707 40.05103107976799, -105.25723110961195 40.05102998669123, -105.25731005474265 40.05102987806262, -105.25755903316241 40.051030126762775, -105.25849816103424 40.05102797837995, -105.2587289291635 40.051025990659284, -105.25897683349142 40.05102705814787, -105.25930294943528 40.051032954539856, -105.25948298345538 40.05103387844358, -105.25965409567844 40.05103203920658, -105.25987414472125 40.05103112475856, -105.26011882647472 40.05103410417082, -105.26007292898571 40.05098212507661, -105.25989092289659 40.05073001337415, -105.25970393488221 40.05047294914017, -105.25954615049089 40.050240926748906, -105.25947901140117 40.05013509748598, -105.25929084911945 40.04980693019196, -105.25909688354645 40.04940298337421, -105.25895201943227 40.04905404325294, -105.2588770324828 40.04884497745633, -105.25880110659527 40.04859802744705, -105.25873303057266 40.04835411276961, -105.25870310805891 40.048229967787094, -105.25863615770983 40.04786993381616, -105.25858014366037 40.04744788236328, -105.25854913661706 40.047025059101486, -105.25854314097862 40.046600091471696, -105.25854128016128 40.045835004999894, -105.2585405106698 40.04557391508014, -105.258535903728 40.043602060660966, -105.25839516597516 40.0436050597048, -105.25755786839645 40.043626088823764, -105.25670415203358 40.04364405736783, -105.25481391348117 40.043660095309406, -105.25456311780088 40.043676033143676, -105.2542829323291 40.04371990903944, -105.25391413704453 40.04377210462879, -105.2538390884301 40.0443769837805, -105.25383288371826 40.044809062538484, -105.25384806656773 40.04594587570338, -105.2532468905064 40.04595310180906, -105.2529968297143 40.045961076985215, -105.25270699632567 40.04600300642463, -105.25249606223991 40.04605608513078, -105.25223102576538 40.04615489213785, -105.2520470613259 40.04625606857408, -105.25174503655586 40.046408875363035, -105.25155088586887 40.04650168367383, -105.25122210553941 40.046605127230485, -105.25094893228412 40.04668112912296, -105.25065188264945 40.046741979386006, -105.25039099236622 40.04678012248868, -105.25004405481526 40.046807921100395, -105.24946002868742 40.04681187006781, -105.24892601618558 40.046814003837376, -105.24876206110189 40.04681501953493, -105.24863203486595 40.04681693211568, -105.24833088858662 40.046825883771895, -105.2483318758626 40.04742900308894, -105.2475249862594 40.04742394661578, -105.24724992604963 40.04742910946336, -105.2464551624836 40.047429012132774, -105.24574004055779 40.04743292882939, -105.2448631101524 40.04743593491281, -105.24437804813823 40.04743293931372, -105.24422691139728 40.04744413449284, -105.24422094628943 40.04874808419349, -105.24422294189131 40.0491681019278, -105.24423387611048 40.05025192424335, -105.24423108417032 40.05090087990886, -105.24424294058713 40.05107302924297))</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
@@ -5814,7 +5842,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2373031389998 40.04755756582615, -105.236973906076 40.04784509661621, -105.2366521446513 40.04810295900571, -105.2348717728759 40.04950637015926, -105.2348829780416 40.05109024293931, -105.2357508266088 40.05107695324783, -105.2365320855235 40.05106995573312, -105.2421489161141 40.05107907484076, -105.2428419426089 40.05107211210048, -105.2442429405871 40.05107302924297, -105.2442310841703 40.05090087990886, -105.2442338761105 40.05025192424335, -105.2442229418913 40.0491681019278, -105.2442209462894 40.04874808419349, -105.2442269113973 40.04744413449284, -105.2443780481382 40.04743293931372, -105.2448631101524 40.04743593491281, -105.2457400405578 40.04743292882939, -105.2464551624836 40.04742901213277, -105.2472499260496 40.04742910946336, -105.2475249862594 40.04742394661578, -105.2483318758626 40.04742900308894, -105.2483308885866 40.04682588377189, -105.2486320348659 40.04681693211568, -105.2487620611019 40.04681501953493, -105.2489260161856 40.04681400383738, -105.2494600286874 40.04681187006781, -105.2500440548153 40.0468079211004, -105.2503909923662 40.04678012248868, -105.2506518826494 40.04674197938601, -105.2509489322841 40.04668112912296, -105.2512221055394 40.04660512723049, -105.2515508858689 40.04650168367383, -105.2517450365559 40.04640887536303, -105.2520470613259 40.04625606857408, -105.2522310257654 40.04615489213785, -105.2524960622399 40.04605608513078, -105.2527069963257 40.04600300642463, -105.2529968297143 40.04596107698521, -105.2532468905064 40.04595310180906, -105.2538480665677 40.04594587570338, -105.2538328837183 40.04480906253848, -105.2538390884301 40.0443769837805, -105.2539141370445 40.04377210462879, -105.2542829323291 40.04371990903944, -105.2545631178009 40.04367603314368, -105.2548139134812 40.04366009530941, -105.2567041520336 40.04364405736783, -105.2575578683964 40.04362608882376, -105.2583951659752 40.0436050597048, -105.258535903728 40.04360206066097, -105.2585328883272 40.04344502971864, -105.2585200529217 40.0428339247763, -105.2585019067495 40.04140309591936, -105.2584811444412 40.04010595201317, -105.2576250499565 40.04010196086148, -105.2572561306026 40.04009487076375, -105.2570050616881 40.04009104854779, -105.2564700565923 40.04008607648185, -105.2541156704493 40.04008547509496, -105.2541114189239 40.04008556330383, -105.2541130449594 40.0400350024811, -105.2541075664353 40.03908055851134, -105.2536959323025 40.03907688210359, -105.2536949545598 40.03812015275444, -105.2535405399283 40.03814509251686, -105.2533805946551 40.03816870800271, -105.2532201543185 40.03819018946845, -105.2530592634851 40.0382095298022, -105.2528979772607 40.03822672371619, -105.2527363390311 40.03824176679848, -105.252574399222 40.03825465195054, -105.2524122082365 40.03826537837855, -105.252087273247 40.03828033297279, -105.2519246265246 40.03828456224724, -105.2517619181192 40.03828706191138, -105.2515262941062 40.03828575038629, -105.2500216866296 40.03828440663961, -105.2489428716393 40.03828342936805, -105.2476788464136 40.03828923237084, -105.2463663111993 40.03830715832521, -105.2456601157548 40.03831973388306, -105.2446044735468 40.03855084401205, -105.2437996973181 40.03858015455958, -105.2438006785438 40.03859655127737, -105.2437872024745 40.03871244225677, -105.2437532031555 40.03873044189604, -105.2435522027756 40.03885844241933, -105.2434222030257 40.03894944238947, -105.2433064056922 40.03903892199388, -105.2432242029855 40.03910244206068, -105.2431468286627 40.03917225845748, -105.2430092033677 40.03929644165687, -105.2428152033527 40.03950244199812, -105.24264120286 40.03971844241541, -105.2425142025077 40.03991144219246, -105.242371581746 40.0401394431425, -105.2423570942121 40.04013997459672, -105.242137900229 40.04049086907413, -105.2414939075501 40.04153506926259, -105.2405720149029 40.04304889223569, -105.240272135138 40.04347893719775, -105.2393799143466 40.04497195457869, -105.2390160894422 40.04558687675885, -105.2389010418821 40.04578207368654, -105.2385538760367 40.04633499171325, -105.2383869376615 40.04655505184557, -105.238130844994 40.04683008772683, -105.2379150718361 40.04702313301646, -105.2373031389998 40.04755756582615))</t>
+          <t>POLYGON ((-105.23730313899979 40.04755756582615, -105.23697390607605 40.04784509661621, -105.23665214465126 40.04810295900571, -105.23487177287592 40.04950637015926, -105.23488297804161 40.05109024293931, -105.23575082660882 40.05107695324783, -105.23653208552355 40.05106995573312, -105.24214891611415 40.05107907484076, -105.24284194260892 40.051072112100485, -105.24424294058713 40.05107302924297, -105.24423108417032 40.05090087990886, -105.24423387611048 40.05025192424335, -105.24422294189131 40.0491681019278, -105.24422094628943 40.04874808419349, -105.24422691139728 40.04744413449284, -105.24437804813823 40.04743293931372, -105.2448631101524 40.04743593491281, -105.24574004055779 40.04743292882939, -105.2464551624836 40.047429012132774, -105.24724992604963 40.04742910946336, -105.2475249862594 40.04742394661578, -105.2483318758626 40.04742900308894, -105.24833088858662 40.046825883771895, -105.24863203486595 40.04681693211568, -105.24876206110189 40.04681501953493, -105.24892601618558 40.046814003837376, -105.24946002868742 40.04681187006781, -105.25004405481526 40.046807921100395, -105.25039099236622 40.04678012248868, -105.25065188264945 40.046741979386006, -105.25094893228412 40.04668112912296, -105.25122210553941 40.046605127230485, -105.25155088586887 40.04650168367383, -105.25174503655586 40.046408875363035, -105.2520470613259 40.04625606857408, -105.25223102576538 40.04615489213785, -105.25249606223991 40.04605608513078, -105.25270699632567 40.04600300642463, -105.2529968297143 40.045961076985215, -105.2532468905064 40.04595310180906, -105.25384806656773 40.04594587570338, -105.25383288371826 40.044809062538484, -105.2538390884301 40.0443769837805, -105.25391413704453 40.04377210462879, -105.2542829323291 40.04371990903944, -105.25456311780088 40.043676033143676, -105.25481391348117 40.043660095309406, -105.25670415203358 40.04364405736783, -105.25755786839645 40.043626088823764, -105.25839516597516 40.0436050597048, -105.258535903728 40.043602060660966, -105.25853288832717 40.04344502971864, -105.2585200529217 40.0428339247763, -105.25850190674954 40.041403095919364, -105.25848114444125 40.04010595201317, -105.25762504995646 40.040101960861485, -105.25725613060256 40.040094870763745, -105.25700506168813 40.040091048547794, -105.25647005659232 40.04008607648185, -105.25411567044932 40.04008547509496, -105.2541114189239 40.04008556330383, -105.25411304495935 40.0400350024811, -105.25410756643528 40.039080558511344, -105.2536959323025 40.039076882103586, -105.25369495455983 40.03812015275444, -105.25354053992825 40.03814509251686, -105.25338059465514 40.03816870800271, -105.2532201543185 40.03819018946845, -105.25305926348506 40.0382095298022, -105.25289797726074 40.03822672371619, -105.25273633903109 40.03824176679848, -105.252574399222 40.03825465195054, -105.25241220823655 40.03826537837855, -105.25208727324699 40.03828033297279, -105.25192462652457 40.03828456224724, -105.25176191811916 40.03828706191138, -105.25152629410616 40.038285750386294, -105.25002168662955 40.03828440663961, -105.24894287163933 40.03828342936805, -105.2476788464136 40.03828923237084, -105.24636631119927 40.03830715832521, -105.24566011575476 40.038319733883064, -105.24460447354679 40.03855084401205, -105.24379969731814 40.038580154559575, -105.24380067854382 40.038596551277365, -105.24378720247454 40.038712442256774, -105.24375320315555 40.038730441896035, -105.24355220277559 40.038858442419325, -105.24342220302569 40.038949442389466, -105.24330640569224 40.03903892199388, -105.24322420298553 40.03910244206068, -105.24314682866274 40.039172258457484, -105.24300920336769 40.03929644165687, -105.24281520335269 40.03950244199812, -105.24264120285997 40.039718442415406, -105.24251420250768 40.039911442192455, -105.24237158174604 40.0401394431425, -105.24235709421208 40.04013997459672, -105.24213790022903 40.040490869074134, -105.24149390755007 40.041535069262586, -105.24057201490292 40.04304889223569, -105.24027213513796 40.043478937197754, -105.23937991434661 40.04497195457869, -105.23901608944219 40.045586876758854, -105.23890104188214 40.04578207368654, -105.23855387603672 40.04633499171325, -105.23838693766153 40.046555051845566, -105.23813084499396 40.04683008772683, -105.23791507183613 40.04702313301646, -105.23730313899979 40.04755756582615))</t>
         </is>
       </c>
       <c r="H129" t="inlineStr">
@@ -5856,7 +5884,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2541114189239 40.04008556330383, -105.2541156704493 40.04008547509496, -105.2564700565923 40.04008607648185, -105.2570050616881 40.04009104854779, -105.2572561306026 40.04009487076375, -105.2576250499565 40.04010196086148, -105.2584811444412 40.04010595201317, -105.2584653846817 40.03890912737619, -105.2584720435084 40.03753396766986, -105.258455895004 40.03685010807402, -105.258446899267 40.03646603760756, -105.2581871656926 40.03647219430682, -105.2581781645477 40.0364731940744, -105.2580461650126 40.03647319470316, -105.2571990758087 40.03646012351341, -105.2557308902084 40.03645592622264, -105.2553020091816 40.0364440365835, -105.2548091605646 40.03644299013902, -105.2536830499528 40.03645706230709, -105.2534351520261 40.03646888605991, -105.2524408934483 40.03646401156114, -105.2521169607307 40.0364660611543, -105.2512098564058 40.0364580687045, -105.2506559111753 40.03646401039433, -105.2500680520282 40.03646603287999, -105.2489469397278 40.03648006964826, -105.2489481075616 40.03616300270446, -105.2489399492534 40.03537209672879, -105.2489642566334 40.03491032664272, -105.2489496620318 40.0346936992231, -105.2489418359893 40.03437504821487, -105.2489411634529 40.0337820853754, -105.2489407326374 40.03375844776104, -105.2488220886228 40.03376027179359, -105.2480707491682 40.033764702882, -105.2475318448188 40.0337678784605, -105.2469897592641 40.0337710715639, -105.2465148034942 40.03377325231298, -105.2459253594542 40.03377474489069, -105.2453730542609 40.03402702879499, -105.2444588367812 40.03552861301022, -105.2440929793375 40.03610011054108, -105.2438753893139 40.0364924229959, -105.2432991274496 40.03743023787163, -105.2430111166943 40.0379132414562, -105.2427781086196 40.03829124483734, -105.2425780966287 40.03862463649937, -105.2446044735468 40.03855084401205, -105.2456601157548 40.03831973388306, -105.2463663111993 40.03830715832521, -105.2476788464136 40.03828923237084, -105.2489428716393 40.03828342936805, -105.2500216866296 40.03828440663961, -105.2515262941062 40.03828575038629, -105.2517619181192 40.03828706191138, -105.2519246265246 40.03828456224724, -105.252087273247 40.03828033297279, -105.2524122082365 40.03826537837855, -105.252574399222 40.03825465195054, -105.2527363390311 40.03824176679848, -105.2528979772607 40.03822672371619, -105.2530592634851 40.0382095298022, -105.2532201543185 40.03819018946845, -105.2533805946551 40.03816870800271, -105.2535405399283 40.03814509251686, -105.2536949545598 40.03812015275444, -105.2536959323025 40.03907688210359, -105.2541075664353 40.03908055851134, -105.2541130449594 40.0400350024811, -105.2541114189239 40.04008556330383))</t>
+          <t>POLYGON ((-105.2541114189239 40.04008556330383, -105.25411567044932 40.04008547509496, -105.25647005659232 40.04008607648185, -105.25700506168813 40.040091048547794, -105.25725613060256 40.040094870763745, -105.25762504995646 40.040101960861485, -105.25848114444125 40.04010595201317, -105.25846538468167 40.03890912737619, -105.25847204350838 40.03753396766986, -105.25845589500403 40.03685010807402, -105.258446899267 40.03646603760756, -105.25818716569263 40.036472194306825, -105.2581781645477 40.0364731940744, -105.25804616501259 40.03647319470316, -105.2571990758087 40.03646012351341, -105.25573089020835 40.036455926222644, -105.25530200918156 40.0364440365835, -105.2548091605646 40.036442990139015, -105.25368304995277 40.03645706230709, -105.25343515202606 40.03646888605991, -105.25244089344825 40.036464011561144, -105.25211696073075 40.0364660611543, -105.2512098564058 40.036458068704505, -105.25065591117529 40.036464010394326, -105.2500680520282 40.03646603287999, -105.2489469397278 40.036480069648256, -105.24894810756163 40.03616300270446, -105.24893994925338 40.035372096728786, -105.24896425663339 40.03491032664272, -105.2489496620318 40.0346936992231, -105.24894183598929 40.03437504821487, -105.24894116345287 40.0337820853754, -105.24894073263735 40.033758447761045, -105.24882208862277 40.03376027179359, -105.24807074916816 40.033764702881996, -105.24753184481875 40.0337678784605, -105.2469897592641 40.033771071563905, -105.24651480349418 40.03377325231298, -105.2459253594542 40.033774744890685, -105.2453730542609 40.03402702879499, -105.24445883678116 40.03552861301022, -105.24409297933748 40.03610011054108, -105.24387538931391 40.0364924229959, -105.24329912744956 40.03743023787163, -105.2430111166943 40.0379132414562, -105.2427781086196 40.03829124483734, -105.24257809662866 40.03862463649937, -105.24460447354679 40.03855084401205, -105.24566011575476 40.038319733883064, -105.24636631119927 40.03830715832521, -105.2476788464136 40.03828923237084, -105.24894287163933 40.03828342936805, -105.25002168662955 40.03828440663961, -105.25152629410616 40.038285750386294, -105.25176191811916 40.03828706191138, -105.25192462652457 40.03828456224724, -105.25208727324699 40.03828033297279, -105.25241220823655 40.03826537837855, -105.252574399222 40.03825465195054, -105.25273633903109 40.03824176679848, -105.25289797726074 40.03822672371619, -105.25305926348506 40.0382095298022, -105.2532201543185 40.03819018946845, -105.25338059465514 40.03816870800271, -105.25354053992825 40.03814509251686, -105.25369495455983 40.03812015275444, -105.2536959323025 40.039076882103586, -105.25410756643528 40.039080558511344, -105.25411304495935 40.0400350024811, -105.2541114189239 40.04008556330383))</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
@@ -5898,7 +5926,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.258535903728 40.04360206066097, -105.2585405106698 40.04557391508014, -105.2587244031369 40.04556793308797, -105.2608058840952 40.04555993265756, -105.2608964703001 40.04555909908301, -105.2611859293927 40.04555644003092, -105.2612685278558 40.0455556805962, -105.2620721242456 40.04554828991369, -105.2625430837086 40.04554395622243, -105.2631165811388 40.04553710851337, -105.2631531738905 40.04553645591186, -105.2632726527912 40.04553756123483, -105.2632619577849 40.04548407045354, -105.263255013832 40.04532401175254, -105.2632540060707 40.04510000292596, -105.2632541220282 40.04475795281136, -105.2632499281982 40.04380591470743, -105.2632480149571 40.04374002648308, -105.2632509956977 40.04339606111056, -105.2632619475292 40.04322505837643, -105.2632641432374 40.04320996439585, -105.2632719609655 40.04291295077446, -105.2632699728957 40.04255991644305, -105.2632690952054 40.04250391316108, -105.2632620035227 40.04238612968864, -105.2632519140621 40.04220602502703, -105.2632450784286 40.04191200118217, -105.2632430471918 40.04167398957392, -105.2632379358998 40.04119192443023, -105.2632361202312 40.04099509094445, -105.2632319091161 40.04066511130758, -105.26321808558 40.04042899745103, -105.2632050686902 40.04037187044779, -105.2631660657392 40.04028998347919, -105.2630888610693 40.04020390118565, -105.2631831695124 40.04009593399001, -105.2632231715832 40.03999307183668, -105.2632250066563 40.03936195792361, -105.2632229054454 40.03863008649829, -105.2632211084702 40.03791386353014, -105.2632148246484 40.03735795059089, -105.2632151403107 40.03726708556623, -105.263225170679 40.03643586385155, -105.2622890950964 40.03643997857341, -105.2612830205331 40.03644393997342, -105.2605001712293 40.03644396467524, -105.2590269395231 40.03645297536733, -105.2585008484345 40.03646011079696, -105.258446899267 40.03646603760756, -105.258455895004 40.03685010807402, -105.2584720435084 40.03753396766986, -105.2584653846817 40.03890912737619, -105.2584811444412 40.04010595201317, -105.2585019067495 40.04140309591936, -105.2585200529217 40.0428339247763, -105.2585328883272 40.04344502971864, -105.258535903728 40.04360206066097))</t>
+          <t>POLYGON ((-105.258535903728 40.043602060660966, -105.2585405106698 40.04557391508014, -105.25872440313694 40.045567933087966, -105.26080588409516 40.04555993265756, -105.26089647030012 40.045559099083015, -105.2611859293927 40.04555644003092, -105.2612685278558 40.0455556805962, -105.26207212424558 40.04554828991369, -105.26254308370862 40.04554395622243, -105.26311658113885 40.04553710851337, -105.26315317389049 40.045536455911865, -105.2632726527912 40.04553756123483, -105.26326195778489 40.04548407045354, -105.263255013832 40.04532401175254, -105.26325400607074 40.045100002925956, -105.26325412202816 40.04475795281136, -105.26324992819822 40.043805914707434, -105.26324801495714 40.04374002648308, -105.26325099569767 40.043396061110556, -105.26326194752924 40.04322505837643, -105.26326414323738 40.04320996439585, -105.26327196096545 40.04291295077446, -105.26326997289573 40.04255991644305, -105.26326909520543 40.04250391316108, -105.26326200352274 40.04238612968864, -105.26325191406207 40.042206025027035, -105.26324507842855 40.04191200118217, -105.26324304719178 40.04167398957392, -105.26323793589981 40.04119192443023, -105.2632361202312 40.04099509094445, -105.26323190911612 40.040665111307575, -105.26321808557995 40.04042899745103, -105.26320506869024 40.04037187044779, -105.26316606573921 40.04028998347919, -105.26308886106929 40.04020390118565, -105.2631831695124 40.04009593399001, -105.26322317158316 40.039993071836676, -105.26322500665634 40.03936195792361, -105.2632229054454 40.03863008649829, -105.2632211084702 40.03791386353014, -105.26321482464839 40.037357950590895, -105.26321514031072 40.03726708556623, -105.26322517067904 40.03643586385155, -105.26228909509645 40.036439978573405, -105.2612830205331 40.03644393997342, -105.26050017122925 40.036443964675236, -105.25902693952311 40.03645297536733, -105.25850084843451 40.03646011079696, -105.258446899267 40.03646603760756, -105.25845589500403 40.03685010807402, -105.25847204350838 40.03753396766986, -105.25846538468167 40.03890912737619, -105.25848114444125 40.04010595201317, -105.25850190674954 40.041403095919364, -105.2585200529217 40.0428339247763, -105.25853288832717 40.04344502971864, -105.258535903728 40.043602060660966))</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
@@ -5940,7 +5968,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2632726527912 40.04553756123483, -105.2632831151267 40.04556290084826, -105.2633278669242 40.04563601458425, -105.2634008580785 40.04570287176336, -105.2634871236304 40.04565006704565, -105.2635908481951 40.0456099251388, -105.2637041480973 40.04558901899909, -105.2642131467077 40.0455870413356, -105.2648150348807 40.04557893545725, -105.2652211535706 40.04558003726618, -105.265425826989 40.04557825778472, -105.2655879950437 40.04557694008583, -105.265627763298 40.0455709117729, -105.2656250546597 40.04549539315068, -105.2656244520254 40.04518062047342, -105.2656235574844 40.0447145876716, -105.2656227612868 40.04430003885544, -105.2656216311616 40.04371237735209, -105.2659102649756 40.04371086932636, -105.2666950373309 40.04370675961066, -105.2674373425578 40.04370286968756, -105.2674581055709 40.04370276022885, -105.2681889710207 40.04369892437131, -105.2686831313114 40.04369632889271, -105.2689899124076 40.04369471714984, -105.2692694698212 40.04369157668958, -105.2697031199627 40.04368199106873, -105.2705431466196 40.04369794005434, -105.2724119538849 40.04368105275066, -105.2727509156415 40.04368089769377, -105.2727281048552 40.04253103185214, -105.2727429988608 40.04155610930046, -105.2727511649065 40.04082096497932, -105.2727378474649 40.04010197465951, -105.2727340477568 40.03867090178024, -105.2727159762066 40.03787805675818, -105.2727101264736 40.03738308870695, -105.2727068348309 40.03719201749416, -105.272693011895 40.03641098462665, -105.2722969317176 40.03641486978847, -105.270493035731 40.03641102135016, -105.2685051665427 40.03642104917662, -105.268183023931 40.03642204958091, -105.2647380295588 40.03643099813947, -105.263225170679 40.03643586385155, -105.2632151403107 40.03726708556623, -105.2632148246484 40.03735795059089, -105.2632211084702 40.03791386353014, -105.2632229054454 40.03863008649829, -105.2632250066563 40.03936195792361, -105.2632231715832 40.03999307183668, -105.2631831695124 40.04009593399001, -105.2630888610693 40.04020390118565, -105.2631660657392 40.04028998347919, -105.2632050686902 40.04037187044779, -105.26321808558 40.04042899745103, -105.2632319091161 40.04066511130758, -105.2632361202312 40.04099509094445, -105.2632379358998 40.04119192443023, -105.2632430471918 40.04167398957392, -105.2632450784286 40.04191200118217, -105.2632519140621 40.04220602502703, -105.2632620035227 40.04238612968864, -105.2632690952054 40.04250391316108, -105.2632699728957 40.04255991644305, -105.2632719609655 40.04291295077446, -105.2632641432374 40.04320996439585, -105.2632619475292 40.04322505837643, -105.2632509956977 40.04339606111056, -105.2632480149571 40.04374002648308, -105.2632499281982 40.04380591470743, -105.2632541220282 40.04475795281136, -105.2632540060707 40.04510000292596, -105.263255013832 40.04532401175254, -105.2632619577849 40.04548407045354, -105.2632726527912 40.04553756123483))</t>
+          <t>POLYGON ((-105.2632726527912 40.04553756123483, -105.26328311512667 40.04556290084826, -105.26332786692423 40.045636014584254, -105.26340085807854 40.04570287176336, -105.26348712363036 40.04565006704565, -105.26359084819505 40.0456099251388, -105.26370414809735 40.04558901899909, -105.26421314670772 40.0455870413356, -105.26481503488071 40.04557893545725, -105.26522115357055 40.045580037266184, -105.26542582698897 40.04557825778472, -105.26558799504372 40.04557694008583, -105.26562776329804 40.0455709117729, -105.26562505465965 40.04549539315068, -105.26562445202536 40.045180620473424, -105.26562355748445 40.0447145876716, -105.26562276128678 40.04430003885544, -105.26562163116162 40.043712377352094, -105.26591026497559 40.04371086932636, -105.26669503733093 40.043706759610664, -105.26743734255783 40.04370286968756, -105.26745810557087 40.043702760228854, -105.26818897102069 40.043698924371306, -105.26868313131145 40.043696328892715, -105.26898991240756 40.04369471714984, -105.26926946982123 40.04369157668958, -105.26970311996267 40.04368199106873, -105.27054314661963 40.043697940054344, -105.27241195388488 40.043681052750664, -105.2727509156415 40.04368089769377, -105.27272810485518 40.042531031852135, -105.27274299886083 40.04155610930046, -105.27275116490645 40.040820964979325, -105.27273784746491 40.04010197465951, -105.27273404775677 40.038670901780236, -105.27271597620661 40.03787805675818, -105.2727101264736 40.03738308870695, -105.27270683483087 40.037192017494164, -105.27269301189496 40.03641098462665, -105.2722969317176 40.03641486978847, -105.27049303573101 40.03641102135016, -105.26850516654274 40.03642104917662, -105.26818302393096 40.036422049580906, -105.26473802955884 40.03643099813947, -105.26322517067904 40.03643586385155, -105.26321514031072 40.03726708556623, -105.26321482464839 40.037357950590895, -105.2632211084702 40.03791386353014, -105.2632229054454 40.03863008649829, -105.26322500665634 40.03936195792361, -105.26322317158316 40.039993071836676, -105.2631831695124 40.04009593399001, -105.26308886106929 40.04020390118565, -105.26316606573921 40.04028998347919, -105.26320506869024 40.04037187044779, -105.26321808557995 40.04042899745103, -105.26323190911612 40.040665111307575, -105.2632361202312 40.04099509094445, -105.26323793589981 40.04119192443023, -105.26324304719178 40.04167398957392, -105.26324507842855 40.04191200118217, -105.26325191406207 40.042206025027035, -105.26326200352274 40.04238612968864, -105.26326909520543 40.04250391316108, -105.26326997289573 40.04255991644305, -105.26327196096545 40.04291295077446, -105.26326414323738 40.04320996439585, -105.26326194752924 40.04322505837643, -105.26325099569767 40.043396061110556, -105.26324801495714 40.04374002648308, -105.26324992819822 40.043805914707434, -105.26325412202816 40.04475795281136, -105.26325400607074 40.045100002925956, -105.263255013832 40.04532401175254, -105.26326195778489 40.04548407045354, -105.2632726527912 40.04553756123483))</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -5982,7 +6010,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2727509156415 40.04368089769377, -105.2731259839293 40.04367092892404, -105.273753153546 40.04368094542063, -105.2739200780991 40.04364393802936, -105.2740218735326 40.04364386275716, -105.2741371221832 40.04368005044567, -105.2742699258984 40.04370007599498, -105.2743839014497 40.04368904351995, -105.2747890229824 40.04366403053018, -105.2751229907905 40.04366193677129, -105.275612997663 40.04367387151462, -105.2760019664365 40.04367298005805, -105.276330179594 40.04368295023548, -105.2764819857427 40.04368104864997, -105.2769539577334 40.04363803919612, -105.2770421726654 40.04364013078624, -105.2771031715048 40.04366413205724, -105.2771699087427 40.04368100673599, -105.277411038845 40.0436699420842, -105.2776949977746 40.04366911697812, -105.277825013327 40.04366799483049, -105.2782389127541 40.04368910526165, -105.2783099946193 40.04368786927655, -105.2784508854329 40.04363790351297, -105.2785348284089 40.04363586799158, -105.2786218911866 40.04366293836192, -105.2786990124604 40.04367187124376, -105.2793880493568 40.0436589155447, -105.2798591715378 40.04365707025223, -105.2801638663687 40.04364996418393, -105.2805138861428 40.0436539251566, -105.2808521452884 40.04364990099339, -105.280916842527 40.04363492538631, -105.2810140330758 40.04362303129678, -105.2811339960779 40.04363808270838, -105.2820708481881 40.04364507266984, -105.2820891721232 40.04364509917423, -105.2820842555383 40.04295631866731, -105.2820922578742 40.04170031755889, -105.2820972563115 40.04092931826332, -105.2820971543631 40.04091685759044, -105.2820822583888 40.03910131882655, -105.2820892579222 40.03830031885973, -105.2820932567946 40.03789431907661, -105.2820972563 40.03729531910635, -105.2820842547273 40.03642931825196, -105.2820839552159 40.03641671759907, -105.2820659978288 40.03641699440085, -105.2819750277566 40.03641791950253, -105.2817311219349 40.03641196792484, -105.2808768423087 40.03641309362312, -105.2799811160418 40.03641989901413, -105.2796861602564 40.03640698278901, -105.2793311558585 40.03640987264631, -105.2790261483974 40.03641313188791, -105.2783640460312 40.03640307771293, -105.2775490944122 40.03639107691423, -105.2770380254055 40.03639201228593, -105.2760758931834 40.0363920698398, -105.2753169540531 40.03639800655378, -105.2752880258183 40.03639795020879, -105.274691954339 40.0364000821719, -105.27282516314 40.03640795036102, -105.272693011895 40.03641098462665, -105.2727068348309 40.03719201749416, -105.2727101264736 40.03738308870695, -105.2727159762066 40.03787805675818, -105.2727340477568 40.03867090178024, -105.2727378474649 40.04010197465951, -105.2727511649065 40.04082096497932, -105.2727429988608 40.04155610930046, -105.2727281048552 40.04253103185214, -105.2727509156415 40.04368089769377))</t>
+          <t>POLYGON ((-105.2727509156415 40.04368089769377, -105.2731259839293 40.043670928924044, -105.27375315354602 40.04368094542063, -105.27392007809905 40.04364393802936, -105.27402187353265 40.043643862757165, -105.27413712218322 40.04368005044567, -105.27426992589838 40.04370007599498, -105.27438390144971 40.04368904351995, -105.27478902298239 40.04366403053018, -105.27512299079055 40.04366193677129, -105.27561299766298 40.04367387151462, -105.27600196643652 40.04367298005805, -105.27633017959401 40.04368295023548, -105.27648198574266 40.043681048649965, -105.27695395773341 40.04363803919612, -105.2770421726654 40.04364013078624, -105.27710317150485 40.04366413205724, -105.2771699087427 40.04368100673599, -105.27741103884502 40.0436699420842, -105.27769499777456 40.04366911697812, -105.277825013327 40.04366799483049, -105.27823891275412 40.04368910526165, -105.27830999461932 40.043687869276546, -105.27845088543295 40.043637903512966, -105.27853482840892 40.043635867991576, -105.27862189118657 40.04366293836192, -105.27869901246036 40.04367187124376, -105.27938804935681 40.043658915544704, -105.27985917153781 40.04365707025223, -105.28016386636871 40.043649964183935, -105.28051388614284 40.0436539251566, -105.28085214528839 40.04364990099339, -105.280916842527 40.043634925386314, -105.28101403307585 40.043623031296775, -105.28113399607793 40.043638082708384, -105.28207084818813 40.04364507266984, -105.28208917212322 40.04364509917423, -105.28208425553827 40.042956318667315, -105.28209225787417 40.04170031755889, -105.28209725631154 40.04092931826332, -105.28209715436307 40.04091685759044, -105.28208225838881 40.03910131882655, -105.2820892579222 40.038300318859726, -105.28209325679462 40.03789431907661, -105.2820972563 40.03729531910635, -105.28208425472734 40.03642931825196, -105.28208395521594 40.036416717599074, -105.28206599782881 40.036416994400845, -105.28197502775664 40.03641791950253, -105.2817311219349 40.03641196792484, -105.28087684230866 40.03641309362312, -105.27998111604178 40.036419899014135, -105.27968616025645 40.03640698278901, -105.2793311558585 40.03640987264631, -105.27902614839736 40.03641313188791, -105.2783640460312 40.03640307771293, -105.27754909441221 40.03639107691423, -105.27703802540549 40.03639201228593, -105.27607589318342 40.0363920698398, -105.27531695405307 40.03639800655378, -105.27528802581831 40.03639795020879, -105.27469195433902 40.0364000821719, -105.27282516313997 40.03640795036102, -105.27269301189496 40.03641098462665, -105.27270683483087 40.037192017494164, -105.2727101264736 40.03738308870695, -105.27271597620661 40.03787805675818, -105.27273404775677 40.038670901780236, -105.27273784746491 40.04010197465951, -105.27275116490645 40.040820964979325, -105.27274299886083 40.04155610930046, -105.27272810485518 40.042531031852135, -105.2727509156415 40.04368089769377))</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
@@ -6024,7 +6052,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2931333735992 40.04730854635932, -105.2935617690094 40.04739276589242, -105.2939623175397 40.04747117356362, -105.2941419153592 40.04726664801208, -105.2944399091494 40.04726439989486, -105.2944404634873 40.04726439007469, -105.2944194169752 40.04716467424064, -105.294385436063 40.04700367056027, -105.2944296129665 40.04678727757992, -105.2943152940317 40.04667577353722, -105.2942122476653 40.0465751981367, -105.294143304593 40.04639821125092, -105.2941108734289 40.04631495780103, -105.29414042267 40.04616746272247, -105.2941690651538 40.046024489973, -105.2941785920136 40.04597693022144, -105.294198045444 40.04587982369743, -105.2941908186116 40.04580062040248, -105.2941758419687 40.04563651717602, -105.2941750876323 40.04562825328249, -105.2941592003012 40.04545413591815, -105.2941577902834 40.04543870259427, -105.2941407062313 40.04525150567407, -105.2941232401209 40.04506008312395, -105.2941048711552 40.04485878154456, -105.2939954347525 40.04457736232708, -105.2939796379256 40.04453674099438, -105.2938811886993 40.04428358290985, -105.293864484944 40.04424530432762, -105.2937704444272 40.04396988728238, -105.2936598952786 40.04365323415506, -105.293922680682 40.04331614435128, -105.2940090412087 40.04317499221415, -105.2940521006302 40.04310461314707, -105.2940604136163 40.04309102639075, -105.2947353382417 40.04273226060973, -105.295303539671 40.04273558388315, -105.2949694223724 40.04232599975767, -105.2950445989627 40.0416958981118, -105.2950542146376 40.04169243868945, -105.2953102149488 40.04163743842137, -105.295219214638 40.04150343873349, -105.2951062149429 40.04138243859521, -105.2949712147415 40.04127443884101, -105.2948932151189 40.04122543820289, -105.2947957789681 40.04117335244502, -105.2947681997134 40.04116125630991, -105.2945507911018 40.04108965505999, -105.2944852147498 40.04106843876539, -105.2941858466411 40.04099383664246, -105.2938592146066 40.04091243917004, -105.2936387602875 40.04088251278208, -105.2936404423018 40.04090982706559, -105.2936419909393 40.04097306619047, -105.2934190202191 40.04094986543068, -105.2930040630487 40.04092798433868, -105.29268691454 40.04092412030541, -105.2920969046858 40.04091701973583, -105.2917750974063 40.04091808576007, -105.2913789966629 40.04092093945307, -105.2912833009954 40.04092752663995, -105.2910829027924 40.04092287413435, -105.2908289544505 40.04092488447498, -105.2907728790686 40.04092505749229, -105.2904721577454 40.04092204125421, -105.2895539205841 40.04091295761805, -105.2878070718198 40.04090289503355, -105.2875159710775 40.04090702642674, -105.2849108458764 40.04090192430674, -105.2834189457056 40.04091203595226, -105.2820971543631 40.04091685759044, -105.2820972563115 40.04092931826332, -105.2820922578742 40.04170031755889, -105.2820842555383 40.04295631866731, -105.2820891721232 40.04364509917423, -105.2820892596123 40.04365731844217, -105.2820852605044 40.04390531895158, -105.2820832594536 40.04409831790472, -105.2820842573841 40.04434731765315, -105.2820892588198 40.04495131835098, -105.2820912578224 40.04516431743618, -105.2820992602341 40.04592931828846, -105.2820953673213 40.046387805911, -105.2820953129514 40.04639418149944, -105.2839881453484 40.04637427796205, -105.2845321459332 40.04637827899764, -105.2846960458856 40.04637486888372, -105.2851725674794 40.0463753941511, -105.2853743746032 40.04637561661295, -105.2854574967038 40.04639188200418, -105.2855675298397 40.04641341390852, -105.285576904431 40.04641729331141, -105.2855920325154 40.04642355481273, -105.2856042908745 40.04642862932879, -105.2856107278606 40.04643129369941, -105.2856197993314 40.04643504824607, -105.2856533922188 40.04644895272444, -105.2857154248379 40.04647912979314, -105.285885097885 40.04656853062735, -105.2860716123038 40.04666698333216, -105.2861362872023 40.04670112252147, -105.2863934400896 40.04676641224462, -105.2864670367458 40.04677515236694, -105.2866191303324 40.0467902142856, -105.2866864608666 40.04678886892687, -105.286746270903 40.04678767354718, -105.2868061477403 40.04678647645866, -105.2868921471954 40.04679127727393, -105.2870501458672 40.0467962784804, -105.2882791462674 40.04678027777359, -105.2888621465885 40.04674327839245, -105.2893061469497 40.04665027849616, -105.2897141473675 40.04656927817304, -105.2897901469812 40.0465592780627, -105.2897911477727 40.04655927808477, -105.2899511476118 40.04655327844637, -105.2902751471324 40.04655527824723, -105.2906991479196 40.04656127733434, -105.2909281466963 40.04658027739244, -105.2911531463136 40.04661827793976, -105.2913721469993 40.04667627690404, -105.2919101464262 40.04687227752947, -105.2923231477523 40.04702627775064, -105.2925641480346 40.04711827748598, -105.2930831475293 40.0473122777485, -105.2931190714868 40.04730785513716, -105.2931351899642 40.04730587018746, -105.2931333735992 40.04730854635932))</t>
+          <t>POLYGON ((-105.29313337359919 40.04730854635932, -105.29356176900943 40.04739276589242, -105.29396231753974 40.04747117356362, -105.29414191535923 40.047266648012084, -105.2944399091494 40.047264399894864, -105.29444046348732 40.04726439007469, -105.2944194169752 40.04716467424064, -105.294385436063 40.04700367056027, -105.29442961296651 40.046787277579924, -105.29431529403169 40.04667577353722, -105.29421224766529 40.0465751981367, -105.29414330459304 40.04639821125092, -105.29411087342892 40.04631495780103, -105.29414042266995 40.046167462722465, -105.29416906515375 40.046024489973, -105.29417859201362 40.04597693022144, -105.29419804544403 40.045879823697426, -105.29419081861157 40.04580062040248, -105.29417584196874 40.04563651717602, -105.29417508763231 40.04562825328249, -105.29415920030118 40.04545413591815, -105.29415779028335 40.04543870259427, -105.29414070623135 40.045251505674074, -105.29412324012091 40.04506008312395, -105.29410487115521 40.04485878154456, -105.29399543475247 40.044577362327075, -105.29397963792562 40.04453674099438, -105.29388118869927 40.04428358290985, -105.29386448494402 40.044245304327625, -105.2937704444272 40.04396988728238, -105.29365989527861 40.04365323415506, -105.293922680682 40.04331614435128, -105.29400904120872 40.043174992214155, -105.29405210063024 40.04310461314707, -105.29406041361628 40.043091026390755, -105.29473533824172 40.04273226060973, -105.29530353967101 40.04273558388315, -105.2949694223724 40.042325999757665, -105.29504459896272 40.041695898111804, -105.29505421463757 40.041692438689445, -105.29531021494884 40.04163743842137, -105.29521921463797 40.041503438733486, -105.29510621494286 40.04138243859521, -105.29497121474152 40.04127443884101, -105.29489321511888 40.04122543820289, -105.29479577896805 40.04117335244502, -105.29476819971337 40.041161256309906, -105.29455079110183 40.04108965505999, -105.29448521474981 40.041068438765386, -105.29418584664107 40.040993836642464, -105.29385921460664 40.04091243917004, -105.29363876028748 40.04088251278208, -105.29364044230175 40.04090982706559, -105.29364199093926 40.040973066190475, -105.29341902021909 40.04094986543068, -105.2930040630487 40.04092798433868, -105.29268691454004 40.040924120305405, -105.2920969046858 40.04091701973583, -105.29177509740626 40.04091808576007, -105.2913789966629 40.04092093945307, -105.29128330099536 40.040927526639955, -105.29108290279238 40.040922874134345, -105.29082895445046 40.040924884474975, -105.29077287906863 40.04092505749229, -105.2904721577454 40.040922041254206, -105.28955392058408 40.04091295761805, -105.28780707181981 40.040902895033554, -105.28751597107745 40.040907026426744, -105.2849108458764 40.04090192430674, -105.2834189457056 40.04091203595226, -105.28209715436307 40.04091685759044, -105.28209725631154 40.04092931826332, -105.28209225787417 40.04170031755889, -105.28208425553827 40.042956318667315, -105.28208917212322 40.04364509917423, -105.28208925961228 40.04365731844217, -105.28208526050436 40.04390531895158, -105.28208325945357 40.04409831790472, -105.28208425738407 40.04434731765315, -105.28208925881982 40.04495131835098, -105.28209125782237 40.04516431743618, -105.28209926023412 40.04592931828846, -105.28209536732132 40.046387805911, -105.28209531295138 40.04639418149944, -105.2839881453484 40.04637427796205, -105.2845321459332 40.04637827899764, -105.28469604588564 40.04637486888372, -105.28517256747945 40.0463753941511, -105.28537437460322 40.04637561661295, -105.28545749670384 40.04639188200418, -105.28556752983972 40.046413413908525, -105.28557690443104 40.04641729331141, -105.28559203251541 40.046423554812726, -105.2856042908745 40.046428629328794, -105.28561072786064 40.04643129369941, -105.28561979933141 40.04643504824607, -105.28565339221885 40.04644895272444, -105.28571542483787 40.04647912979314, -105.28588509788496 40.04656853062735, -105.28607161230383 40.04666698333216, -105.28613628720227 40.04670112252147, -105.28639344008961 40.046766412244615, -105.28646703674583 40.04677515236694, -105.2866191303324 40.0467902142856, -105.28668646086659 40.04678886892687, -105.28674627090295 40.04678767354718, -105.28680614774026 40.04678647645866, -105.28689214719539 40.046791277273925, -105.28705014586716 40.0467962784804, -105.28827914626736 40.046780277773586, -105.28886214658847 40.04674327839245, -105.28930614694967 40.04665027849616, -105.28971414736752 40.04656927817304, -105.28979014698116 40.0465592780627, -105.28979114777273 40.04655927808477, -105.28995114761177 40.046553278446375, -105.29027514713242 40.04655527824723, -105.29069914791957 40.04656127733434, -105.29092814669626 40.04658027739244, -105.29115314631362 40.046618277939764, -105.29137214699927 40.04667627690404, -105.2919101464262 40.046872277529474, -105.29232314775233 40.04702627775064, -105.29256414803459 40.04711827748598, -105.29308314752929 40.047312277748496, -105.29311907148684 40.04730785513716, -105.29313518996419 40.047305870187465, -105.29313337359919 40.04730854635932))</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
@@ -6066,10 +6094,14 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2936404423018 40.04090982706559, -105.2936404333365 40.04090969195224, -105.2936393298994 40.04089176076243, -105.2936387602875 40.04088251278208, -105.2936382144575 40.04088243885319, -105.2936381907138 40.04087325219269, -105.2936381107935 40.04084275698107, -105.2936375293797 40.04061951931827, -105.2936362147382 40.04011443848095, -105.2934722142269 40.04010743878002, -105.2934792144789 40.03920443815797, -105.2923682131695 40.03918943861687, -105.2923892136016 40.03902243843871, -105.2924912138074 40.03896743828266, -105.2926092133786 40.0388264377026, -105.2927262144654 40.03861943834501, -105.292842214139 40.03837543840261, -105.2929572138373 40.03793343784105, -105.2929242137023 40.03785143845414, -105.2921662137698 40.03784743828271, -105.292166213115 40.03765743823374, -105.2929242141904 40.03765843834879, -105.2927792134548 40.03731343830118, -105.2932632137346 40.03730943865403, -105.2932582145944 40.03688043786936, -105.2916252132727 40.03688043864178, -105.2916242139543 40.03633843870183, -105.2930502139936 40.03635143785036, -105.2930342143154 40.03628543748766, -105.2929422134349 40.03619843809624, -105.292908213494 40.03617043802443, -105.2927832141158 40.03600443825045, -105.2927602138006 40.03597043795142, -105.2927107603088 40.03587813792029, -105.2926582136129 40.03576543800347, -105.2926232139659 40.0355924378065, -105.2925802137358 40.03543343821553, -105.2926902132874 40.03525443823721, -105.2926532134305 40.03511543756299, -105.2926922137881 40.03505743828392, -105.2927552137461 40.03499443757188, -105.2931342134192 40.03501543737434, -105.2932612136337 40.03502943777404, -105.2933812135632 40.03506143848394, -105.2934642135779 40.03506843745255, -105.293634213987 40.0348184377084, -105.2936462145961 40.03479243761252, -105.2936532138585 40.0347724377023, -105.2936592133786 40.03474943774147, -105.2936612144225 40.03473943780755, -105.2936652146541 40.03472043765701, -105.2936672133564 40.03469843746568, -105.2936672134586 40.03467943736553, -105.2936672134593 40.03466743801314, -105.2936652138936 40.03464443725404, -105.293662213805 40.0346264378129, -105.2936581157056 40.03460848684401, -105.2936542131837 40.03459443783817, -105.2936502137531 40.0345814379154, -105.2936462131523 40.03456843799037, -105.2936422133352 40.03455943695012, -105.2935046256782 40.03432954495042, -105.2933842142322 40.03413143774353, -105.2930712139342 40.03413743794434, -105.2930142135916 40.03410643800208, -105.2929952137423 40.03410643813415, -105.2929572138224 40.03408143815955, -105.2929102131477 40.03405643732565, -105.2928912131919 40.03404143802341, -105.2928792139851 40.03402643777797, -105.2928672138293 40.03400943808766, -105.2928562133356 40.0339904380472, -105.2928432126227 40.03397843786441, -105.2928422125705 40.03392543824812, -105.2928442131984 40.03390943819936, -105.2928502132125 40.03389443694749, -105.2928602128196 40.03387843775223, -105.2928772133286 40.03385543686772, -105.2928832130675 40.03383743735128, -105.2928852132439 40.03382543798608, -105.2928972826058 40.03380499689747, -105.2929052133355 40.03379043772514, -105.2929162131264 40.03378343780931, -105.292924213406 40.03377143750584, -105.292933213333 40.03375743685223, -105.2930112141034 40.03362143735369, -105.293291955493 40.03362143728865, -105.2937372138235 40.0336214372065, -105.2937382974607 40.03337909957001, -105.2937386793353 40.03329355655762, -105.2937395508468 40.03309847291506, -105.2937402132035 40.03295043792892, -105.2932286416031 40.03294919515979, -105.2931052137653 40.03294843796873, -105.2927092126049 40.03294843766469, -105.2927108121817 40.03286705423627, -105.292710907085 40.03286705440682, -105.2927122130598 40.03278743752472, -105.2936812128586 40.03278843795151, -105.2936722139328 40.03195643683105, -105.2933122135404 40.03195643722582, -105.2933122133834 40.03167943790211, -105.2936742141418 40.03167843776409, -105.2936732131968 40.03155043743585, -105.2932162129589 40.03154943719254, -105.2932342129986 40.03110243735086, -105.2932282125647 40.0310404366715, -105.293669213941 40.03104043735713, -105.2936642128336 40.03048443747013, -105.2936648818336 40.03047785401582, -105.2936537748646 40.03047788728623, -105.2927552572933 40.03049408413858, -105.29275521762 40.0304882505582, -105.2927385970148 40.03048906550561, -105.2926902128227 40.03049143643388, -105.292694024948 40.03033512199099, -105.2926953162127 40.03015092069578, -105.2926952125016 40.02997043747474, -105.2927355065977 40.02996954708772, -105.2928733794138 40.02996650196004, -105.293193212992 40.02995943740156, -105.2932232128183 40.0299614365863, -105.2932232133512 40.02983612015983, -105.2931884875867 40.02976646198516, -105.2931867492964 40.02966709736802, -105.2936473388391 40.02965363342965, -105.2936571602725 40.02965404007967, -105.293657096737 40.02964638804434, -105.2936542127414 40.02932343683928, -105.2933562129823 40.02932143711671, -105.2930897958375 40.02932328771823, -105.29278021285 40.02932543663955, -105.2927792132976 40.02925843639324, -105.2926812130856 40.02925543766246, -105.2926814065824 40.02924882814005, -105.2926819728648 40.02922943366055, -105.2926912123074 40.02891343650078, -105.2927623809299 40.0289131834094, -105.2927622187183 40.02890295353519, -105.2932416180685 40.02890518641989, -105.2932459804773 40.02805555882141, -105.2932121680632 40.02797051286821, -105.2931062443818 40.02797125870275, -105.2927482126114 40.0279784372106, -105.2926652124506 40.02798243734529, -105.2926662131555 40.02781943678586, -105.2926862126045 40.02765543642518, -105.2926882122127 40.02760543682441, -105.2926782129605 40.02736543611802, -105.2927526221468 40.0273611710597, -105.2928406316727 40.0273612309844, -105.2936104824806 40.02736175091879, -105.2936342486239 40.02736138454571, -105.293635212304 40.02716843638694, -105.2932082126097 40.02716843631173, -105.2932082128545 40.02696443724676, -105.2936352122566 40.02695443650428, -105.2936362122575 40.02682843733329, -105.2936314855515 40.02575744316506, -105.2936332128447 40.02541943670018, -105.2936339345848 40.02541515269726, -105.2926069291672 40.02543973575167, -105.2925031180585 40.02550902431486, -105.2920939363481 40.025498130862, -105.2915040127181 40.02550612476494, -105.2902481507636 40.02550796560364, -105.290043906236 40.02550594671673, -105.2887301598848 40.02552001896971, -105.2867490705732 40.02551994347327, -105.2856660543705 40.0255160131922, -105.2856812109885 40.02583443661324, -105.2856822111836 40.02592843665887, -105.2856742107215 40.02601043682525, -105.2855892107703 40.02642143748587, -105.2855692118289 40.02663843724292, -105.2855712105374 40.02672743692585, -105.2855754584629 40.02732638721953, -105.2855862117171 40.02922543814994, -105.2855863693517 40.02924870043505, -105.2855895839882 40.02975199420325, -105.2855932655471 40.03029421670868, -105.2856075598998 40.03111985202749, -105.2856121682715 40.03181337185057, -105.2856187194815 40.03279928309118, -105.2856191603849 40.03286696954467, -105.2856190537651 40.03286696934653, -105.2856233092233 40.03353419031163, -105.2856302124652 40.03499243870875, -105.2840522108804 40.03500343762658, -105.2824672114959 40.03498943845764, -105.282092223959 40.03498258560737, -105.2820922571864 40.03498831830537, -105.282084254758 40.03633731870206, -105.2820832571337 40.03638731727795, -105.2820839552159 40.03641671759907, -105.2820842547273 40.03642931825196, -105.2820972563 40.03729531910635, -105.2820932567946 40.03789431907661, -105.2820892579222 40.03830031885973, -105.2820822583888 40.03910131882655, -105.2820971543631 40.04091685759044, -105.2834189457056 40.04091203595226, -105.2849108458764 40.04090192430674, -105.2875159710775 40.04090702642674, -105.2878070718198 40.04090289503355, -105.2895539205841 40.04091295761805, -105.2904721577454 40.04092204125421, -105.2907728790686 40.04092505749229, -105.2908289544505 40.04092488447498, -105.2910829027924 40.04092287413435, -105.2912833009954 40.04092752663995, -105.2913789966629 40.04092093945307, -105.2917750974063 40.04091808576007, -105.2920969046858 40.04091701973583, -105.29268691454 40.04092412030541, -105.2930040630487 40.04092798433868, -105.2934190202191 40.04094986543068, -105.2936419909393 40.04097306619047, -105.2936404423018 40.04090982706559))</t>
-        </is>
-      </c>
-      <c r="H135" t="inlineStr"/>
+          <t>POLYGON ((-105.29364044230175 40.04090982706559, -105.29364043333648 40.040909691952244, -105.29363932989943 40.040891760762435, -105.29363876028748 40.04088251278208, -105.29363821445747 40.04088243885319, -105.29363819071385 40.04087325219269, -105.29363811079354 40.04084275698107, -105.29363752937974 40.04061951931827, -105.29363621473821 40.04011443848095, -105.29347221422685 40.04010743878002, -105.29347921447891 40.039204438157974, -105.29236821316951 40.03918943861687, -105.2923892136016 40.03902243843871, -105.29249121380744 40.03896743828266, -105.2926092133786 40.038826437702596, -105.2927262144654 40.03861943834501, -105.29284221413897 40.03837543840261, -105.29295721383734 40.037933437841055, -105.29292421370235 40.03785143845414, -105.29216621376985 40.03784743828271, -105.29216621311498 40.037657438233744, -105.29292421419035 40.037658438348785, -105.29277921345479 40.03731343830118, -105.29326321373456 40.037309438654034, -105.29325821459443 40.03688043786936, -105.2916252132727 40.03688043864178, -105.29162421395431 40.036338438701826, -105.29305021399357 40.03635143785036, -105.29303421431538 40.03628543748766, -105.29294221343488 40.036198438096235, -105.29290821349404 40.036170438024435, -105.29278321411576 40.03600443825045, -105.29276021380058 40.03597043795142, -105.29271076030881 40.03587813792029, -105.29265821361287 40.03576543800347, -105.29262321396591 40.0355924378065, -105.2925802137358 40.03543343821553, -105.29269021328741 40.03525443823721, -105.29265321343051 40.03511543756299, -105.2926922137881 40.03505743828392, -105.29275521374606 40.03499443757188, -105.2931342134192 40.03501543737434, -105.29326121363371 40.035029437774035, -105.29338121356318 40.03506143848394, -105.29346421357788 40.03506843745255, -105.29363421398698 40.0348184377084, -105.29364621459608 40.034792437612516, -105.29365321385849 40.0347724377023, -105.2936592133786 40.034749437741475, -105.29366121442253 40.03473943780755, -105.29366521465407 40.03472043765701, -105.29366721335637 40.03469843746568, -105.29366721345859 40.03467943736553, -105.29366721345934 40.03466743801314, -105.29366521389356 40.034644437254045, -105.29366221380496 40.034626437812896, -105.29365811570564 40.034608486844014, -105.29365421318374 40.03459443783817, -105.29365021375311 40.0345814379154, -105.29364621315229 40.034568437990366, -105.29364221333516 40.03455943695012, -105.29350462567824 40.034329544950424, -105.2933842142322 40.03413143774353, -105.29307121393418 40.03413743794434, -105.29301421359156 40.034106438002084, -105.29299521374229 40.03410643813415, -105.29295721382238 40.03408143815955, -105.29291021314772 40.03405643732565, -105.2928912131919 40.03404143802341, -105.29287921398506 40.03402643777797, -105.29286721382933 40.03400943808766, -105.29285621333558 40.033990438047205, -105.29284321262273 40.033978437864405, -105.29284221257052 40.03392543824812, -105.29284421319845 40.03390943819936, -105.29285021321247 40.03389443694749, -105.29286021281965 40.03387843775223, -105.29287721332857 40.03385543686772, -105.29288321306754 40.03383743735128, -105.29288521324389 40.03382543798608, -105.29289728260575 40.03380499689747, -105.2929052133355 40.033790437725145, -105.29291621312643 40.03378343780931, -105.29292421340601 40.03377143750584, -105.29293321333304 40.03375743685223, -105.29301121410336 40.033621437353695, -105.29329195549299 40.03362143728865, -105.29373721382348 40.0336214372065, -105.29373829746073 40.033379099570006, -105.29373867933535 40.03329355655762, -105.29373955084681 40.033098472915064, -105.29374021320349 40.03295043792892, -105.2932286416031 40.032949195159794, -105.29310521376533 40.032948437968734, -105.29270921260489 40.032948437664686, -105.2927108121817 40.03286705423627, -105.29271090708495 40.03286705440682, -105.29271221305977 40.03278743752472, -105.29368121285857 40.03278843795151, -105.29367221393282 40.031956436831045, -105.29331221354039 40.03195643722582, -105.2933122133834 40.031679437902106, -105.29367421414184 40.031678437764086, -105.29367321319675 40.031550437435854, -105.2932162129589 40.03154943719254, -105.2932342129986 40.03110243735086, -105.29322821256469 40.0310404366715, -105.293669213941 40.03104043735713, -105.29366421283365 40.03048443747013, -105.2936648818336 40.03047785401582, -105.29365377486457 40.03047788728623, -105.2927552572933 40.03049408413858, -105.29275521761997 40.0304882505582, -105.29273859701476 40.03048906550561, -105.2926902128227 40.03049143643388, -105.29269402494799 40.030335121990994, -105.29269531621273 40.03015092069578, -105.29269521250161 40.02997043747474, -105.29273550659772 40.029969547087724, -105.29287337941378 40.02996650196004, -105.29319321299195 40.02995943740156, -105.29322321281835 40.0299614365863, -105.29322321335115 40.02983612015983, -105.29318848758669 40.02976646198516, -105.29318674929641 40.02966709736802, -105.29364733883907 40.029653633429646, -105.29365716027247 40.02965404007967, -105.29365709673698 40.02964638804434, -105.29365421274139 40.02932343683928, -105.29335621298233 40.029321437116714, -105.29308979583755 40.029323287718235, -105.29278021285002 40.029325436639546, -105.29277921329765 40.02925843639324, -105.29268121308561 40.02925543766246, -105.2926814065824 40.02924882814005, -105.29268197286476 40.02922943366055, -105.29269121230745 40.02891343650078, -105.29276238092987 40.0289131834094, -105.29276221871832 40.028902953535194, -105.29324161806852 40.02890518641989, -105.29324598047725 40.02805555882141, -105.29321216806316 40.02797051286821, -105.29310624438185 40.02797125870275, -105.29274821261139 40.0279784372106, -105.29266521245059 40.02798243734529, -105.29266621315554 40.02781943678586, -105.29268621260448 40.02765543642518, -105.29268821221267 40.02760543682441, -105.29267821296051 40.027365436118025, -105.29275262214685 40.027361171059695, -105.29284063167269 40.0273612309844, -105.29361048248057 40.02736175091879, -105.29363424862393 40.02736138454571, -105.29363521230398 40.027168436386944, -105.29320821260971 40.027168436311726, -105.29320821285447 40.02696443724676, -105.2936352122566 40.02695443650428, -105.29363621225745 40.02682843733329, -105.29363148555154 40.02575744316506, -105.29363321284467 40.02541943670018, -105.29363393458482 40.02541515269726, -105.29260692916722 40.02543973575167, -105.2925031180585 40.025509024314864, -105.29209393634812 40.025498130862, -105.29150401271811 40.02550612476494, -105.29024815076362 40.02550796560364, -105.29004390623602 40.02550594671673, -105.28873015988484 40.025520018969715, -105.28674907057322 40.02551994347327, -105.2856660543705 40.0255160131922, -105.28568121098849 40.025834436613245, -105.28568221118361 40.02592843665887, -105.2856742107215 40.02601043682525, -105.28558921077033 40.02642143748587, -105.2855692118289 40.02663843724292, -105.28557121053741 40.02672743692585, -105.28557545846286 40.02732638721953, -105.28558621171715 40.029225438149936, -105.28558636935168 40.02924870043505, -105.28558958398824 40.029751994203245, -105.28559326554713 40.03029421670868, -105.28560755989976 40.031119852027494, -105.28561216827154 40.03181337185057, -105.2856187194815 40.03279928309118, -105.28561916038485 40.03286696954467, -105.28561905376512 40.03286696934653, -105.28562330922334 40.033534190311634, -105.28563021246521 40.03499243870875, -105.28405221088039 40.03500343762658, -105.28246721149587 40.034989438457636, -105.282092223959 40.03498258560737, -105.28209225718639 40.03498831830537, -105.28208425475798 40.03633731870206, -105.28208325713375 40.03638731727795, -105.28208395521594 40.036416717599074, -105.28208425472734 40.03642931825196, -105.2820972563 40.03729531910635, -105.28209325679462 40.03789431907661, -105.2820892579222 40.038300318859726, -105.28208225838881 40.03910131882655, -105.28209715436307 40.04091685759044, -105.2834189457056 40.04091203595226, -105.2849108458764 40.04090192430674, -105.28751597107745 40.040907026426744, -105.28780707181981 40.040902895033554, -105.28955392058408 40.04091295761805, -105.2904721577454 40.040922041254206, -105.29077287906863 40.04092505749229, -105.29082895445046 40.040924884474975, -105.29108290279238 40.040922874134345, -105.29128330099536 40.040927526639955, -105.2913789966629 40.04092093945307, -105.29177509740626 40.04091808576007, -105.2920969046858 40.04091701973583, -105.29268691454004 40.040924120305405, -105.2930040630487 40.04092798433868, -105.29341902021909 40.04094986543068, -105.29364199093926 40.040973066190475, -105.29364044230175 40.04090982706559))</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>Centennial MS</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -6104,7 +6136,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.272693011895 40.03641098462665, -105.27282516314 40.03640795036102, -105.274691954339 40.0364000821719, -105.2752880258183 40.03639795020879, -105.2753169540531 40.03639800655378, -105.2760758931834 40.0363920698398, -105.2770380254055 40.03639201228593, -105.2775490944122 40.03639107691423, -105.2783640460312 40.03640307771293, -105.2790261483974 40.03641313188791, -105.2793311558585 40.03640987264631, -105.2796861602564 40.03640698278901, -105.2799811160418 40.03641989901413, -105.2808768423087 40.03641309362312, -105.2817311219349 40.03641196792484, -105.2819750277566 40.03641791950253, -105.2820659978288 40.03641699440085, -105.2820839552159 40.03641671759907, -105.2820832571337 40.03638731727795, -105.282084254758 40.03633731870206, -105.2820922571864 40.03498831830537, -105.282092223959 40.03498258560737, -105.2824672114959 40.03498943845764, -105.2840522108804 40.03500343762658, -105.2856302124652 40.03499243870875, -105.2856233092233 40.03353419031163, -105.2856190537651 40.03286696934653, -105.2856191603849 40.03286696954467, -105.2856187194815 40.03279928309118, -105.2856121682715 40.03181337185057, -105.2856075598998 40.03111985202749, -105.2855932655471 40.03029421670868, -105.2855895839882 40.02975199420325, -105.2855863857595 40.02924869866423, -105.2855761122275 40.02924902721826, -105.2854201124465 40.02923199133771, -105.2844270167391 40.02923096285564, -105.2832689344744 40.02923208823412, -105.2821221918683 40.02925559915963, -105.28212225549 40.02926831736175, -105.2821084505153 40.03010442340204, -105.2820900004695 40.03010393732394, -105.2820898563745 40.03010393344913, -105.2805939720805 40.03009396023452, -105.2804018518184 40.030093047055, -105.2803029427175 40.03009011263436, -105.2793758908887 40.03009191253876, -105.2791998402836 40.03009102538928, -105.2784088644469 40.03008703905117, -105.2781960300691 40.03008690379698, -105.277470066055 40.03007699534945, -105.276498044355 40.03007099921356, -105.2751321551345 40.03005901118281, -105.2741701059328 40.03006097391676, -105.273645871071 40.030061869293, -105.2726510020113 40.03005387211383, -105.2726558625326 40.03073798238746, -105.2726628596342 40.03142401880926, -105.2726661710148 40.03160905132167, -105.272671164566 40.03193189473561, -105.2726760357997 40.03272004799683, -105.2726760239568 40.0331518655748, -105.2726820898275 40.03390296023866, -105.2726840628362 40.03406108764794, -105.2726881734809 40.03464911391067, -105.2726940852457 40.03630310060525, -105.272693011895 40.03641098462665))</t>
+          <t>POLYGON ((-105.27269301189496 40.03641098462665, -105.27282516313997 40.03640795036102, -105.27469195433902 40.0364000821719, -105.27528802581831 40.03639795020879, -105.27531695405307 40.03639800655378, -105.27607589318342 40.0363920698398, -105.27703802540549 40.03639201228593, -105.27754909441221 40.03639107691423, -105.2783640460312 40.03640307771293, -105.27902614839736 40.03641313188791, -105.2793311558585 40.03640987264631, -105.27968616025645 40.03640698278901, -105.27998111604178 40.036419899014135, -105.28087684230866 40.03641309362312, -105.2817311219349 40.03641196792484, -105.28197502775664 40.03641791950253, -105.28206599782881 40.036416994400845, -105.28208395521594 40.036416717599074, -105.28208325713375 40.03638731727795, -105.28208425475798 40.03633731870206, -105.28209225718639 40.03498831830537, -105.282092223959 40.03498258560737, -105.28246721149587 40.034989438457636, -105.28405221088039 40.03500343762658, -105.28563021246521 40.03499243870875, -105.28562330922334 40.033534190311634, -105.28561905376512 40.03286696934653, -105.28561916038485 40.03286696954467, -105.2856187194815 40.03279928309118, -105.28561216827154 40.03181337185057, -105.28560755989976 40.031119852027494, -105.28559326554713 40.03029421670868, -105.28558958398824 40.029751994203245, -105.28558638575949 40.029248698664226, -105.28557611222752 40.029249027218256, -105.28542011244654 40.02923199133771, -105.28442701673912 40.029230962855635, -105.28326893447445 40.02923208823412, -105.28212219186831 40.029255599159626, -105.28212225548998 40.02926831736175, -105.28210845051531 40.03010442340204, -105.28209000046947 40.030103937323936, -105.2820898563745 40.03010393344913, -105.28059397208054 40.030093960234524, -105.28040185181841 40.030093047055, -105.28030294271747 40.03009011263436, -105.27937589088867 40.03009191253876, -105.27919984028357 40.030091025389275, -105.27840886444692 40.030087039051175, -105.27819603006911 40.03008690379698, -105.27747006605496 40.03007699534945, -105.27649804435504 40.03007099921356, -105.27513215513453 40.030059011182814, -105.27417010593277 40.03006097391676, -105.27364587107101 40.030061869293, -105.2726510020113 40.03005387211383, -105.27265586253262 40.03073798238746, -105.27266285963421 40.03142401880926, -105.27266617101482 40.031609051321674, -105.272671164566 40.03193189473561, -105.27267603579966 40.03272004799683, -105.27267602395676 40.0331518655748, -105.2726820898275 40.033902960238656, -105.27268406283622 40.03406108764794, -105.27268817348092 40.034649113910675, -105.27269408524567 40.03630310060525, -105.27269301189496 40.03641098462665))</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -6146,7 +6178,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.258446899267 40.03646603760756, -105.2585008484345 40.03646011079696, -105.2590269395231 40.03645297536733, -105.2605001712293 40.03644396467524, -105.2612830205331 40.03644393997342, -105.2622890950964 40.03643997857341, -105.263225170679 40.03643586385155, -105.2647380295588 40.03643099813947, -105.268183023931 40.03642204958091, -105.2685051665427 40.03642104917662, -105.270493035731 40.03641102135016, -105.2722969317176 40.03641486978847, -105.272693011895 40.03641098462665, -105.2726940852457 40.03630310060525, -105.2726881734809 40.03464911391067, -105.2726840628362 40.03406108764794, -105.2726820898275 40.03390296023866, -105.2726760239568 40.0331518655748, -105.2726760357997 40.03272004799683, -105.272671164566 40.03193189473561, -105.2726661710148 40.03160905132167, -105.2726628596342 40.03142401880926, -105.2726558625326 40.03073798238746, -105.2726510020113 40.03005387211383, -105.2726431137961 40.02931402807485, -105.2726378711389 40.02799495559294, -105.2726248698914 40.02675410445867, -105.2724391697248 40.02675813072266, -105.2722851382764 40.02679598460758, -105.2721821366655 40.026844096625, -105.2712200627177 40.02739891617156, -105.2707191449315 40.02769302966741, -105.2705449708217 40.02777311773346, -105.2703590775048 40.02783396502272, -105.2701599867456 40.0278901194453, -105.269954176002 40.02792704383995, -105.2694618422777 40.02800292602936, -105.2687529792441 40.02811707949513, -105.2684821309878 40.02816704828201, -105.2666869661029 40.02849312791361, -105.2664928873497 40.02854407048214, -105.2663698268983 40.02860805840928, -105.2662798937188 40.02869599678734, -105.2659830419497 40.0290379943425, -105.2658878266626 40.02910396023101, -105.2657551564794 40.02915804605855, -105.2656000920418 40.02918188831284, -105.2650558597207 40.02918489888469, -105.2645041764277 40.02917389106241, -105.2641049336855 40.02917499727695, -105.2633179148443 40.02916597275626, -105.2631300554157 40.02917299949814, -105.2619208966281 40.02917709843084, -105.261397433136 40.02917401288314, -105.2607085005719 40.0291675069947, -105.2597381905843 40.02915582694323, -105.259088875901 40.0291349825795, -105.2584008552258 40.0291030718611, -105.2584230215977 40.03080897880332, -105.258422876378 40.03155512074788, -105.2584330323697 40.03282094785845, -105.2584408767324 40.03524304377068, -105.2584500008643 40.0359938719383, -105.258446899267 40.03646603760756))</t>
+          <t>POLYGON ((-105.258446899267 40.03646603760756, -105.25850084843451 40.03646011079696, -105.25902693952311 40.03645297536733, -105.26050017122925 40.036443964675236, -105.2612830205331 40.03644393997342, -105.26228909509645 40.036439978573405, -105.26322517067904 40.03643586385155, -105.26473802955884 40.03643099813947, -105.26818302393096 40.036422049580906, -105.26850516654274 40.03642104917662, -105.27049303573101 40.03641102135016, -105.2722969317176 40.03641486978847, -105.27269301189496 40.03641098462665, -105.27269408524567 40.03630310060525, -105.27268817348092 40.034649113910675, -105.27268406283622 40.03406108764794, -105.2726820898275 40.033902960238656, -105.27267602395676 40.0331518655748, -105.27267603579966 40.03272004799683, -105.272671164566 40.03193189473561, -105.27266617101482 40.031609051321674, -105.27266285963421 40.03142401880926, -105.27265586253262 40.03073798238746, -105.2726510020113 40.03005387211383, -105.27264311379614 40.02931402807485, -105.27263787113887 40.027994955592945, -105.27262486989143 40.02675410445867, -105.27243916972482 40.02675813072266, -105.27228513827643 40.02679598460758, -105.27218213666552 40.026844096625, -105.27122006271772 40.02739891617156, -105.27071914493149 40.02769302966741, -105.27054497082173 40.02777311773346, -105.27035907750484 40.027833965022715, -105.27015998674558 40.027890119445296, -105.269954176002 40.027927043839945, -105.26946184227765 40.02800292602936, -105.26875297924411 40.028117079495125, -105.26848213098779 40.028167048282015, -105.26668696610294 40.02849312791361, -105.26649288734967 40.02854407048214, -105.26636982689826 40.028608058409276, -105.26627989371885 40.02869599678734, -105.26598304194968 40.0290379943425, -105.26588782666258 40.029103960231005, -105.2657551564794 40.029158046058555, -105.26560009204181 40.02918188831284, -105.2650558597207 40.029184898884694, -105.26450417642769 40.02917389106241, -105.26410493368547 40.029174997276954, -105.26331791484425 40.02916597275626, -105.26313005541569 40.02917299949814, -105.26192089662813 40.02917709843084, -105.261397433136 40.02917401288314, -105.26070850057188 40.029167506994696, -105.25973819058426 40.02915582694323, -105.25908887590097 40.0291349825795, -105.25840085522579 40.0291030718611, -105.25842302159771 40.03080897880332, -105.25842287637805 40.03155512074788, -105.25843303236968 40.03282094785845, -105.25844087673235 40.035243043770684, -105.25845000086426 40.0359938719383, -105.258446899267 40.03646603760756))</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
@@ -6188,7 +6220,7 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2453730542609 40.03402702879499, -105.2459253594542 40.03377474489069, -105.2465148034942 40.03377325231298, -105.2469897592641 40.0337710715639, -105.2475318448188 40.0337678784605, -105.2480707491682 40.033764702882, -105.2488220886228 40.03376027179359, -105.2489407326374 40.03375844776104, -105.2489411634529 40.0337820853754, -105.2489418359893 40.03437504821487, -105.2489496620318 40.0346936992231, -105.2489642566334 40.03491032664272, -105.2489399492534 40.03537209672879, -105.2489481075616 40.03616300270446, -105.2489469397278 40.03648006964826, -105.2500680520282 40.03646603287999, -105.2506559111753 40.03646401039433, -105.2512098564058 40.0364580687045, -105.2521169607307 40.0364660611543, -105.2524408934483 40.03646401156114, -105.2534351520261 40.03646888605991, -105.2536830499528 40.03645706230709, -105.2548091605646 40.03644299013902, -105.2553020091816 40.0364440365835, -105.2557308902084 40.03645592622264, -105.2571990758087 40.03646012351341, -105.2580461650126 40.03647319470316, -105.2581781645477 40.0364731940744, -105.2581871656926 40.03647219430682, -105.258446899267 40.03646603760756, -105.2584500008643 40.0359938719383, -105.2584408767324 40.03524304377068, -105.2584330323697 40.03282094785845, -105.258422876378 40.03155512074788, -105.2584230215977 40.03080897880332, -105.2584008552258 40.0291030718611, -105.2574731748613 40.02908410461595, -105.2568789101786 40.02909795213807, -105.2560300596294 40.02910412076228, -105.2550068904213 40.02912501244828, -105.2544228360915 40.02917894797287, -105.2536750228567 40.02919107939742, -105.2482195454966 40.02920455652909, -105.2481541927388 40.02931308733002, -105.247983553166 40.0296102141241, -105.2477685658453 40.02998489963429, -105.2475764919784 40.03031963966591, -105.2474157554355 40.03059976586545, -105.2472377688188 40.03090995649731, -105.2470527888195 40.03123232722809, -105.2470384585521 40.03125730147787, -105.2468743915512 40.03153389625475, -105.2466014210446 40.03199231009842, -105.2462652351348 40.03255119866444, -105.2453730542609 40.03402702879499))</t>
+          <t>POLYGON ((-105.2453730542609 40.03402702879499, -105.2459253594542 40.033774744890685, -105.24651480349418 40.03377325231298, -105.2469897592641 40.033771071563905, -105.24753184481875 40.0337678784605, -105.24807074916816 40.033764702881996, -105.24882208862277 40.03376027179359, -105.24894073263735 40.033758447761045, -105.24894116345287 40.0337820853754, -105.24894183598929 40.03437504821487, -105.2489496620318 40.0346936992231, -105.24896425663339 40.03491032664272, -105.24893994925338 40.035372096728786, -105.24894810756163 40.03616300270446, -105.2489469397278 40.036480069648256, -105.2500680520282 40.03646603287999, -105.25065591117529 40.036464010394326, -105.2512098564058 40.036458068704505, -105.25211696073075 40.0364660611543, -105.25244089344825 40.036464011561144, -105.25343515202606 40.03646888605991, -105.25368304995277 40.03645706230709, -105.2548091605646 40.036442990139015, -105.25530200918156 40.0364440365835, -105.25573089020835 40.036455926222644, -105.2571990758087 40.03646012351341, -105.25804616501259 40.03647319470316, -105.2581781645477 40.0364731940744, -105.25818716569263 40.036472194306825, -105.258446899267 40.03646603760756, -105.25845000086426 40.0359938719383, -105.25844087673235 40.035243043770684, -105.25843303236968 40.03282094785845, -105.25842287637805 40.03155512074788, -105.25842302159771 40.03080897880332, -105.25840085522579 40.0291030718611, -105.25747317486129 40.02908410461595, -105.25687891017859 40.02909795213807, -105.25603005962941 40.029104120762284, -105.25500689042127 40.029125012448276, -105.25442283609148 40.02917894797287, -105.25367502285674 40.02919107939742, -105.24821954549657 40.029204556529095, -105.24815419273884 40.029313087330024, -105.247983553166 40.0296102141241, -105.24776856584528 40.02998489963429, -105.24757649197839 40.03031963966591, -105.24741575543554 40.030599765865446, -105.24723776881878 40.03090995649731, -105.2470527888195 40.03123232722809, -105.24703845855211 40.03125730147787, -105.24687439155124 40.03153389625475, -105.24660142104464 40.03199231009842, -105.24626523513476 40.032551198664436, -105.2453730542609 40.03402702879499))</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
@@ -6230,7 +6262,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2208591976603 40.04021944344885, -105.220913197136 40.04017644371963, -105.2209821983598 40.04014844366193, -105.2210591982608 40.04014044384326, -105.223497505316 40.04015150481216, -105.22407704741 40.04015412622703, -105.2258593874601 40.04016074121972, -105.2276746826273 40.0401621385647, -105.2286399728214 40.0401628702557, -105.2298354739006 40.04016222201453, -105.2314588703982 40.04015761180696, -105.2328302880019 40.04015369964417, -105.2335462006925 40.04015244262079, -105.2336891999156 40.04015244226186, -105.2338002012012 40.03945344235616, -105.2348372005173 40.03836744194803, -105.2348286362072 40.03708139570391, -105.2348242002542 40.03641544158987, -105.2348322862713 40.0361973792786, -105.2348572000809 40.03552544198848, -105.2356341995921 40.0350774410321, -105.2357952003409 40.03500344132726, -105.2359922007589 40.0349134417673, -105.2362041999249 40.03484844131424, -105.2367342003588 40.03483044207642, -105.2370662006303 40.03487744228755, -105.237397200161 40.0349504419565, -105.2378882000602 40.03516344213855, -105.2382342008113 40.03540544098632, -105.2391190094183 40.03621631438021, -105.2394381522089 40.03651262561413, -105.2396062009134 40.03652244116942, -105.2409032015566 40.03652344124953, -105.241018201577 40.03650844155181, -105.2404672015227 40.03726344178768, -105.2398934186792 40.03772339881659, -105.2385454852443 40.03864375463035, -105.2425769492914 40.03862654872201, -105.2425780966287 40.03862463649937, -105.2427781086196 40.03829124483734, -105.2430111166943 40.0379132414562, -105.2432991274496 40.03743023787163, -105.2438753893139 40.0364924229959, -105.2440929793375 40.03610011054108, -105.2444588367812 40.03552861301022, -105.2453730542609 40.03402702879499, -105.2462652351348 40.03255119866444, -105.2466014210446 40.03199231009842, -105.2468743915512 40.03153389625475, -105.2470384585521 40.03125730147787, -105.2470527888195 40.03123232722809, -105.2472377688188 40.03090995649731, -105.2474157554355 40.03059976586545, -105.2475764919784 40.03031963966591, -105.2477685658453 40.02998489963429, -105.247983553166 40.0296102141241, -105.2481541927388 40.02931308733002, -105.2482195454966 40.02920455652909, -105.2475199805581 40.02920302743363, -105.2471535866196 40.02920497006868, -105.2470046722872 40.02920574144774, -105.2467879073245 40.02920691310877, -105.2459758332215 40.02921391257004, -105.2448980525407 40.02922690726311, -105.2447080626234 40.02923005531607, -105.2441955801484 40.02923144538298, -105.2431311238466 40.02922408398609, -105.2400198840386 40.02917511185208, -105.2395431210193 40.02918391916977, -105.2382999573494 40.02920828260488, -105.2375975186471 40.02922070455187, -105.2365361783417 40.02922211126447, -105.2346081604372 40.02922894693484, -105.2335989823584 40.02923101313294, -105.2329054947644 40.02923023263606, -105.2326919485125 40.02923001266877, -105.2317567030328 40.02922893947044, -105.2312381944585 40.02922828192708, -105.2308360988211 40.02922789375545, -105.2303165160975 40.02922777805944, -105.2300240500278 40.02922791711205, -105.2291319973156 40.02923104149665, -105.2286845476068 40.02923108871217, -105.2275989594909 40.02923100067746, -105.2260059682783 40.02922091333762, -105.2259449032419 40.029221042971, -105.2258520567489 40.02922109704281, -105.2253944375382 40.02922698588036, -105.225394197129 40.02923344208104, -105.2253951967717 40.02932644126568, -105.2259961973092 40.0293284414642, -105.2259941979395 40.02962444223154, -105.2259931976188 40.02985144192847, -105.2259871977661 40.03029944157155, -105.2259891978973 40.03071444140571, -105.2259891973577 40.0312724419347, -105.2259870021577 40.0322697246056, -105.2259859825384 40.03291451209868, -105.225982197759 40.03347944212604, -105.2255911987063 40.03359744281072, -105.2250371980086 40.03374044312552, -105.2245743280957 40.03386447092257, -105.2241681975645 40.03399244230303, -105.2236111982574 40.03421344303411, -105.2232891976821 40.03439244202391, -105.222917197469 40.03452644327425, -105.2227431977602 40.03464544348129, -105.2227395470943 40.03558613982754, -105.2227401974629 40.03650644306278, -105.2207291969135 40.03650744297263, -105.2207471963628 40.0375574432325, -105.2207161974315 40.03835144348213, -105.218441197225 40.03832844367185, -105.2184331975993 40.04005444361138, -105.2208581977847 40.04005444358192, -105.2208591976603 40.04021944344885))</t>
+          <t>POLYGON ((-105.22085919766035 40.04021944344885, -105.220913197136 40.04017644371963, -105.2209821983598 40.040148443661934, -105.22105919826082 40.040140443843256, -105.22349750531596 40.04015150481216, -105.22407704741003 40.04015412622703, -105.22585938746009 40.040160741219715, -105.22767468262725 40.040162138564696, -105.22863997282141 40.0401628702557, -105.22983547390062 40.04016222201453, -105.2314588703982 40.04015761180696, -105.2328302880019 40.04015369964417, -105.23354620069246 40.04015244262079, -105.23368919991559 40.040152442261856, -105.23380020120116 40.039453442356155, -105.23483720051732 40.038367441948026, -105.23482863620723 40.03708139570391, -105.23482420025421 40.03641544158987, -105.23483228627128 40.036197379278605, -105.23485720008091 40.03552544198848, -105.23563419959214 40.0350774410321, -105.23579520034092 40.03500344132726, -105.23599220075887 40.0349134417673, -105.23620419992491 40.03484844131424, -105.2367342003588 40.03483044207642, -105.23706620063027 40.03487744228755, -105.23739720016104 40.034950441956504, -105.2378882000602 40.03516344213855, -105.2382342008113 40.035405440986324, -105.23911900941827 40.03621631438021, -105.23943815220889 40.03651262561413, -105.23960620091343 40.036522441169424, -105.24090320155658 40.03652344124953, -105.24101820157696 40.03650844155181, -105.24046720152272 40.03726344178768, -105.2398934186792 40.03772339881659, -105.23854548524427 40.03864375463035, -105.24257694929143 40.03862654872201, -105.24257809662866 40.03862463649937, -105.2427781086196 40.03829124483734, -105.2430111166943 40.0379132414562, -105.24329912744956 40.03743023787163, -105.24387538931391 40.0364924229959, -105.24409297933748 40.03610011054108, -105.24445883678116 40.03552861301022, -105.2453730542609 40.03402702879499, -105.24626523513476 40.032551198664436, -105.24660142104464 40.03199231009842, -105.24687439155124 40.03153389625475, -105.24703845855211 40.03125730147787, -105.2470527888195 40.03123232722809, -105.24723776881878 40.03090995649731, -105.24741575543554 40.030599765865446, -105.24757649197839 40.03031963966591, -105.24776856584528 40.02998489963429, -105.247983553166 40.0296102141241, -105.24815419273884 40.029313087330024, -105.24821954549657 40.029204556529095, -105.24751998055812 40.02920302743363, -105.24715358661965 40.029204970068676, -105.24700467228716 40.02920574144774, -105.24678790732452 40.02920691310877, -105.24597583322151 40.02921391257004, -105.24489805254075 40.02922690726311, -105.24470806262345 40.02923005531607, -105.24419558014837 40.029231445382976, -105.24313112384661 40.02922408398609, -105.24001988403863 40.02917511185208, -105.2395431210193 40.02918391916977, -105.23829995734944 40.029208282604884, -105.2375975186471 40.02922070455187, -105.23653617834171 40.02922211126447, -105.23460816043719 40.029228946934836, -105.23359898235839 40.029231013132936, -105.23290549476444 40.02923023263606, -105.23269194851247 40.02923001266877, -105.23175670303283 40.029228939470435, -105.2312381944585 40.029228281927075, -105.23083609882106 40.029227893755454, -105.2303165160975 40.02922777805944, -105.2300240500278 40.029227917112046, -105.22913199731562 40.02923104149665, -105.22868454760678 40.02923108871217, -105.22759895949092 40.02923100067746, -105.22600596827826 40.029220913337625, -105.22594490324188 40.029221042970995, -105.22585205674893 40.029221097042814, -105.22539443753824 40.02922698588036, -105.22539419712899 40.02923344208104, -105.22539519677166 40.02932644126568, -105.22599619730916 40.0293284414642, -105.22599419793946 40.029624442231544, -105.22599319761879 40.02985144192847, -105.22598719776606 40.03029944157155, -105.2259891978973 40.03071444140571, -105.2259891973577 40.031272441934696, -105.2259870021577 40.0322697246056, -105.22598598253838 40.03291451209868, -105.22598219775895 40.033479442126044, -105.22559119870633 40.03359744281072, -105.22503719800864 40.03374044312552, -105.22457432809568 40.03386447092257, -105.22416819756447 40.03399244230303, -105.22361119825736 40.03421344303411, -105.22328919768213 40.034392442023915, -105.22291719746897 40.03452644327425, -105.22274319776018 40.03464544348129, -105.22273954709433 40.035586139827544, -105.22274019746293 40.03650644306278, -105.22072919691348 40.036507442972635, -105.22074719636284 40.0375574432325, -105.2207161974315 40.03835144348213, -105.21844119722505 40.03832844367185, -105.21843319759925 40.04005444361138, -105.2208581977847 40.040054443581916, -105.22085919766035 40.04021944344885))</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
@@ -6272,7 +6304,7 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2160111955 40.02941744250101, -105.2160241944471 40.02958644314366, -105.2160301953674 40.0296674427522, -105.2160431949233 40.02976544318457, -105.2160821948466 40.029843442886, -105.2161731957375 40.02993344293114, -105.2162281958708 40.02996544241743, -105.2163231954602 40.03000344222524, -105.216393195045 40.030018442685, -105.216714195362 40.02978944179781, -105.2169183296271 40.02964944212096, -105.2170861959579 40.02953944212074, -105.2171013733368 40.02953197961455, -105.2172628810816 40.02945581657214, -105.2173882346814 40.02940610874885, -105.2175251954509 40.02935744244781, -105.2176198784911 40.0293380499647, -105.2177341859115 40.02931463718165, -105.2178571961912 40.02928944246727, -105.2180831955133 40.02926644208032, -105.2184761957898 40.02926244201551, -105.2185102178733 40.02926210714222, -105.2191025662913 40.02925881640458, -105.2199463053364 40.02925557303384, -105.22047383285 40.0292534418192, -105.2209515721532 40.02925336013067, -105.2213741961431 40.02925244173912, -105.221524196698 40.02924344258807, -105.2215368541062 40.02924212396792, -105.2216681962193 40.02922844212854, -105.2217758048782 40.02920913506678, -105.2220471963629 40.0291604417221, -105.2221531959837 40.02913544191373, -105.2227491964695 40.02893444274527, -105.2231341967773 40.02873844263139, -105.2234171967727 40.02858844157902, -105.2240448012386 40.02921896182992, -105.2240485290634 40.0292221896779, -105.2242922587597 40.02922218887095, -105.2243452592167 40.02922218854747, -105.2250902606939 40.02922118797638, -105.2253838715813 40.02922712104237, -105.2253876759348 40.02922707245764, -105.2258520567489 40.02922109704281, -105.2259449032419 40.029221042971, -105.2260059682783 40.02922091333762, -105.2275989594909 40.02923100067746, -105.2286845476068 40.02923108871217, -105.2291319973156 40.02923104149665, -105.2300240500278 40.02922791711205, -105.2303165160975 40.02922777805944, -105.2308360988211 40.02922789375545, -105.2312381944585 40.02922828192708, -105.2317567030328 40.02922893947044, -105.2326919485125 40.02923001266877, -105.2329054947644 40.02923023263606, -105.2335989823584 40.02923101313294, -105.2346081604372 40.02922894693484, -105.2365361783417 40.02922211126447, -105.2375975186471 40.02922070455187, -105.2382999573494 40.02920828260488, -105.2395431210193 40.02918391916977, -105.2400198840386 40.02917511185208, -105.2431311238466 40.02922408398609, -105.2441955801484 40.02923144538298, -105.2447080626234 40.02923005531607, -105.2448980525407 40.02922690726311, -105.2459758332215 40.02921391257004, -105.2467879073245 40.02920691310877, -105.2470046722872 40.02920574144774, -105.2471535866196 40.02920497006868, -105.2475199805581 40.02920302743363, -105.2482195454966 40.02920455652909, -105.2536750228567 40.02919107939742, -105.2544228360915 40.02917894797287, -105.2550068904213 40.02912501244828, -105.2560300596294 40.02910412076228, -105.2568789101786 40.02909795213807, -105.2574731748613 40.02908410461595, -105.2584008552258 40.0291030718611, -105.2584009719777 40.02907012989925, -105.2583971480592 40.02732802426323, -105.2583841483148 40.02615991830773, -105.258382877582 40.02551095323694, -105.2583811009352 40.02450099341501, -105.2583789356683 40.02339906985873, -105.2583830465151 40.0223399835016, -105.2584077255942 40.02163362987389, -105.2583999303681 40.02054880387701, -105.2583865082488 40.02003406862268, -105.2583845261048 40.01916806167687, -105.2583845465005 40.01820405441318, -105.2583835533824 40.017841051784, -105.2583967697713 40.01738897110558, -105.258420544823 40.01462569237854, -105.2537731835135 40.0146261868912, -105.2501120279116 40.01463197668197, -105.2489568317006 40.01463733680855, -105.2477575533147 40.0146096980253, -105.2465954644375 40.01458212939171, -105.2460469422521 40.01457377343792, -105.2449033960308 40.01456052644195, -105.2432112087095 40.01457106881134, -105.2422256658095 40.01457244483336, -105.2407671682903 40.01461834492035, -105.2401101703597 40.01465348406194, -105.239268545971 40.01470520202151, -105.2379838714334 40.01472804370003, -105.2364884675618 40.01473462743368, -105.234785953114 40.0147380290238, -105.2338293506786 40.01473924403673, -105.2319659677214 40.01469691984863, -105.2309519694455 40.01468609977, -105.230058133229 40.01466913584839, -105.22915700892 40.01466702306828, -105.2281480626285 40.01466492383204, -105.2272090327501 40.01466628746812, -105.2258513852783 40.01466824594888, -105.2254145473955 40.01466887288986, -105.2254128747107 40.01466887521181, -105.2245834902002 40.0146398382582, -105.2239170504272 40.01464087196651, -105.2191844656205 40.01463953261158, -105.217100941391 40.01463444043784, -105.2164899016262 40.01467620189562, -105.2164723909476 40.01467739814613, -105.215735902945 40.01471779606526, -105.2157340623453 40.01471789690481, -105.2148910155936 40.01473046222324, -105.2148764361527 40.01473067926249, -105.2141074361257 40.0147478477099, -105.2130981903515 40.01474897460401, -105.2130969381798 40.01474897599216, -105.2130940324873 40.01467594647242, -105.2130777016322 40.01363575086111, -105.2130740693893 40.01339608598071, -105.2130736861623 40.01323274517098, -105.2130673059102 40.01280105946651, -105.213064157268 40.01258789120162, -105.2130646768166 40.01262642336378, -105.2121356176559 40.01262468172177, -105.2101880793582 40.01262205279892, -105.2101881770135 40.0126180919686, -105.2098311921049 40.01261944051893, -105.2098292659196 40.01246736656677, -105.2098286476958 40.01241859730428, -105.2098111911977 40.01104044022411, -105.2074681901274 40.01104044140051, -105.2075011914237 40.01348844053171, -105.2078361910397 40.01348944102689, -105.2078121909381 40.01462344028587, -105.2069742231526 40.01462497172324, -105.2050431900852 40.0146034419073, -105.2050398702081 40.01392145197964, -105.2050351910883 40.01296044132123, -105.2048331905392 40.01297844102542, -105.2045691898613 40.01294644116913, -105.2043981908388 40.01288544030034, -105.2038051899005 40.01281044069496, -105.2027581900902 40.01266844174256, -105.2028090273656 40.01467798954275, -105.2036567103979 40.01467716810863, -105.2036568942967 40.01467716858118, -105.2038309998592 40.01467699888822, -105.2045197317803 40.01467615277912, -105.2046439989874 40.01467599916017, -105.2048625378809 40.01467753585545, -105.2050079696713 40.01467855822093, -105.2052129998992 40.0146799993535, -105.2052452071275 40.01468054190908, -105.2055099991169 40.01468499841905, -105.2059949427587 40.01469404259862, -105.2059949767234 40.01469404358584, -105.206367999478 40.01470099950867, -105.2066710004365 40.01470499853, -105.2067196345875 40.01470499883064, -105.2067203549632 40.0147049988613, -105.2067098058444 40.0150998456722, -105.2067183070375 40.01600540075746, -105.2066918318187 40.01639614326426, -105.2067009491717 40.01715872104394, -105.2066873211797 40.01744464479255, -105.2066417223345 40.0193985748575, -105.2066282588804 40.01964637159548, -105.2066396306025 40.01988469898361, -105.2066508805403 40.02015162089645, -105.2066866789568 40.02047579851763, -105.2067823753913 40.02074214075176, -105.2069473712818 40.02099014246873, -105.2071853679822 40.02123014325992, -105.2072853658604 40.02131414432528, -105.2073173661939 40.02133714445619, -105.2077919256969 40.02163067272885, -105.2081351092813 40.0218317118302, -105.2085064200148 40.02197920421263, -105.2089568292927 40.02211259715015, -105.2092683557341 40.02218214859246, -105.2096453553682 40.02228714891598, -105.210131353124 40.02246915041668, -105.2104213509922 40.02261115079264, -105.2106593493525 40.0227561515699, -105.2107433476153 40.02283715262609, -105.2108295770383 40.02291528432966, -105.2109051937388 40.02298744145597, -105.2109292903985 40.02301884637291, -105.2110271929919 40.02314644131605, -105.2110908591813 40.02325882755933, -105.2111421929906 40.02334944202191, -105.2111681958693 40.02340961220849, -105.2112281926976 40.02354844225731, -105.2112661927701 40.02380644202619, -105.2112831927006 40.02414744200545, -105.2112831926451 40.02472144241093, -105.2112871930142 40.02556744269105, -105.2113161932457 40.02663444274262, -105.2113071938985 40.02853044222877, -105.2113005886311 40.02886265923356, -105.2112971941228 40.02903344233737, -105.21132119374 40.02911044242671, -105.2113691942612 40.02918144297956, -105.2113901939955 40.02920244289452, -105.2114661938733 40.02925644249451, -105.2115561934457 40.02929544246373, -105.2116561945448 40.0293154428859, -105.2121779687597 40.02931370359353, -105.2132951941631 40.02931044250712, -105.2142271952085 40.02931444306602, -105.2154397747579 40.02930063641094, -105.2158601952949 40.02929244290664, -105.2159541953328 40.02928944287671, -105.2159851951632 40.0292884429292, -105.2160111955 40.02941744250101))</t>
+          <t>POLYGON ((-105.21601119549997 40.029417442501014, -105.21602419444714 40.02958644314366, -105.21603019536744 40.0296674427522, -105.21604319492326 40.029765443184566, -105.21608219484663 40.029843442886, -105.21617319573753 40.02993344293114, -105.2162281958708 40.029965442417435, -105.21632319546022 40.03000344222524, -105.21639319504503 40.030018442685, -105.21671419536204 40.02978944179781, -105.21691832962706 40.02964944212096, -105.21708619595795 40.02953944212074, -105.2171013733368 40.02953197961455, -105.21726288108155 40.02945581657214, -105.21738823468142 40.02940610874885, -105.2175251954509 40.02935744244781, -105.21761987849106 40.0293380499647, -105.21773418591154 40.02931463718165, -105.21785719619116 40.029289442467274, -105.2180831955133 40.02926644208032, -105.21847619578985 40.02926244201551, -105.21851021787334 40.02926210714222, -105.21910256629131 40.02925881640458, -105.21994630533635 40.029255573033836, -105.22047383285002 40.0292534418192, -105.22095157215317 40.029253360130674, -105.22137419614309 40.02925244173912, -105.22152419669797 40.02924344258807, -105.22153685410616 40.02924212396792, -105.22166819621934 40.02922844212854, -105.22177580487825 40.02920913506678, -105.22204719636294 40.0291604417221, -105.22215319598371 40.02913544191373, -105.2227491964695 40.028934442745275, -105.22313419677728 40.028738442631386, -105.22341719677267 40.02858844157902, -105.22404480123862 40.02921896182992, -105.22404852906344 40.029222189677895, -105.22429225875968 40.029222188870946, -105.2243452592167 40.02922218854747, -105.2250902606939 40.029221187976376, -105.22538387158134 40.029227121042375, -105.2253876759348 40.029227072457644, -105.22585205674893 40.029221097042814, -105.22594490324188 40.029221042970995, -105.22600596827826 40.029220913337625, -105.22759895949092 40.02923100067746, -105.22868454760678 40.02923108871217, -105.22913199731562 40.02923104149665, -105.2300240500278 40.029227917112046, -105.2303165160975 40.02922777805944, -105.23083609882106 40.029227893755454, -105.2312381944585 40.029228281927075, -105.23175670303283 40.029228939470435, -105.23269194851247 40.02923001266877, -105.23290549476444 40.02923023263606, -105.23359898235839 40.029231013132936, -105.23460816043719 40.029228946934836, -105.23653617834171 40.02922211126447, -105.2375975186471 40.02922070455187, -105.23829995734944 40.029208282604884, -105.2395431210193 40.02918391916977, -105.24001988403863 40.02917511185208, -105.24313112384661 40.02922408398609, -105.24419558014837 40.029231445382976, -105.24470806262345 40.02923005531607, -105.24489805254075 40.02922690726311, -105.24597583322151 40.02921391257004, -105.24678790732452 40.02920691310877, -105.24700467228716 40.02920574144774, -105.24715358661965 40.029204970068676, -105.24751998055812 40.02920302743363, -105.24821954549657 40.029204556529095, -105.25367502285674 40.02919107939742, -105.25442283609148 40.02917894797287, -105.25500689042127 40.029125012448276, -105.25603005962941 40.029104120762284, -105.25687891017859 40.02909795213807, -105.25747317486129 40.02908410461595, -105.25840085522579 40.0291030718611, -105.25840097197765 40.029070129899246, -105.25839714805917 40.02732802426323, -105.25838414831479 40.026159918307734, -105.25838287758201 40.02551095323694, -105.25838110093518 40.02450099341501, -105.25837893566833 40.023399069858726, -105.25838304651515 40.022339983501595, -105.25840772559422 40.02163362987389, -105.25839993036806 40.02054880387701, -105.25838650824882 40.02003406862268, -105.25838452610483 40.019168061676865, -105.2583845465005 40.01820405441318, -105.25838355338244 40.017841051783996, -105.25839676977125 40.017388971105575, -105.258420544823 40.014625692378544, -105.25377318351349 40.0146261868912, -105.25011202791158 40.01463197668197, -105.24895683170055 40.01463733680855, -105.24775755331466 40.0146096980253, -105.24659546443755 40.01458212939171, -105.24604694225205 40.014573773437924, -105.24490339603082 40.014560526441954, -105.24321120870951 40.014571068811335, -105.2422256658095 40.014572444833355, -105.24076716829035 40.01461834492035, -105.24011017035973 40.01465348406194, -105.23926854597097 40.01470520202151, -105.23798387143336 40.01472804370003, -105.23648846756177 40.014734627433675, -105.23478595311404 40.0147380290238, -105.2338293506786 40.01473924403673, -105.23196596772144 40.01469691984863, -105.23095196944553 40.01468609977, -105.23005813322901 40.014669135848386, -105.22915700892003 40.01466702306828, -105.22814806262855 40.01466492383204, -105.2272090327501 40.014666287468124, -105.2258513852783 40.014668245948876, -105.22541454739553 40.014668872889864, -105.22541287471071 40.01466887521181, -105.22458349020025 40.0146398382582, -105.22391705042719 40.014640871966506, -105.21918446562049 40.01463953261158, -105.21710094139102 40.01463444043784, -105.2164899016262 40.01467620189562, -105.21647239094757 40.01467739814613, -105.21573590294497 40.01471779606526, -105.2157340623453 40.01471789690481, -105.21489101559357 40.01473046222324, -105.21487643615265 40.01473067926249, -105.21410743612572 40.0147478477099, -105.21309819035152 40.01474897460401, -105.21309693817976 40.014748975992156, -105.21309403248726 40.014675946472416, -105.2130777016322 40.01363575086111, -105.2130740693893 40.01339608598071, -105.21307368616226 40.01323274517098, -105.21306730591022 40.01280105946651, -105.213064157268 40.01258789120162, -105.21306467681661 40.012626423363784, -105.21213561765589 40.012624681721775, -105.21018807935823 40.01262205279892, -105.21018817701355 40.0126180919686, -105.20983119210486 40.01261944051893, -105.20982926591964 40.012467366566774, -105.20982864769584 40.01241859730428, -105.20981119119767 40.011040440224114, -105.20746819012743 40.01104044140051, -105.20750119142375 40.01348844053171, -105.20783619103973 40.01348944102689, -105.20781219093811 40.014623440285874, -105.20697422315263 40.01462497172324, -105.20504319008523 40.0146034419073, -105.20503987020814 40.01392145197964, -105.20503519108834 40.01296044132123, -105.2048331905392 40.01297844102542, -105.20456918986132 40.012946441169134, -105.20439819083882 40.012885440300344, -105.20380518990045 40.01281044069496, -105.20275819009024 40.012668441742555, -105.20280902736565 40.014677989542754, -105.20365671039794 40.01467716810863, -105.20365689429666 40.01467716858118, -105.20383099985916 40.01467699888822, -105.20451973178025 40.01467615277912, -105.20464399898744 40.01467599916017, -105.20486253788094 40.014677535855455, -105.2050079696713 40.01467855822093, -105.20521299989923 40.0146799993535, -105.20524520712755 40.01468054190908, -105.20550999911694 40.01468499841905, -105.20599494275875 40.01469404259862, -105.20599497672345 40.01469404358584, -105.20636799947805 40.01470099950867, -105.20667100043647 40.01470499853, -105.20671963458754 40.01470499883064, -105.20672035496321 40.0147049988613, -105.20670980584435 40.0150998456722, -105.20671830703753 40.016005400757464, -105.20669183181872 40.01639614326426, -105.20670094917168 40.01715872104394, -105.20668732117969 40.01744464479255, -105.20664172233452 40.019398574857505, -105.20662825888037 40.019646371595485, -105.20663963060254 40.01988469898361, -105.2066508805403 40.02015162089645, -105.20668667895676 40.02047579851763, -105.2067823753913 40.02074214075176, -105.20694737128179 40.02099014246873, -105.20718536798223 40.02123014325992, -105.20728536586044 40.02131414432528, -105.2073173661939 40.02133714445619, -105.20779192569692 40.021630672728854, -105.20813510928129 40.021831711830195, -105.20850642001483 40.02197920421263, -105.20895682929275 40.02211259715015, -105.20926835573408 40.022182148592464, -105.20964535536818 40.02228714891598, -105.21013135312397 40.022469150416676, -105.21042135099223 40.02261115079264, -105.21065934935245 40.0227561515699, -105.21074334761526 40.02283715262609, -105.21082957703833 40.022915284329656, -105.21090519373878 40.022987441455975, -105.21092929039852 40.02301884637291, -105.2110271929919 40.02314644131605, -105.21109085918125 40.02325882755933, -105.21114219299055 40.02334944202191, -105.21116819586933 40.02340961220849, -105.21122819269765 40.02354844225731, -105.21126619277014 40.02380644202619, -105.21128319270062 40.02414744200545, -105.21128319264511 40.02472144241093, -105.21128719301419 40.02556744269105, -105.2113161932457 40.02663444274262, -105.21130719389852 40.02853044222877, -105.21130058863108 40.02886265923356, -105.21129719412276 40.029033442337365, -105.21132119373996 40.02911044242671, -105.21136919426115 40.029181442979564, -105.21139019399551 40.02920244289452, -105.21146619387335 40.029256442494514, -105.21155619344569 40.029295442463734, -105.21165619454476 40.029315442885895, -105.21217796875966 40.02931370359353, -105.21329519416307 40.029310442507125, -105.21422719520845 40.02931444306602, -105.21543977475791 40.029300636410944, -105.21586019529485 40.029292442906645, -105.21595419533278 40.02928944287671, -105.21598519516317 40.0292884429292, -105.21601119549997 40.029417442501014))</t>
         </is>
       </c>
       <c r="H140" t="inlineStr">
@@ -6314,7 +6346,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2584008552258 40.0291030718611, -105.259088875901 40.0291349825795, -105.2597381905843 40.02915582694323, -105.2607085005719 40.0291675069947, -105.261397433136 40.02917401288314, -105.2619208966281 40.02917709843084, -105.2631300554157 40.02917299949814, -105.2633179148443 40.02916597275626, -105.2641049336855 40.02917499727695, -105.2645041764277 40.02917389106241, -105.2650558597207 40.02918489888469, -105.2656000920418 40.02918188831284, -105.2657551564794 40.02915804605855, -105.2658878266626 40.02910396023101, -105.2659830419497 40.0290379943425, -105.2662798937188 40.02869599678734, -105.2663698268983 40.02860805840928, -105.2664928873497 40.02854407048214, -105.2666869661029 40.02849312791361, -105.2684821309878 40.02816704828201, -105.2687529792441 40.02811707949513, -105.2694618422777 40.02800292602936, -105.269954176002 40.02792704383995, -105.2701599867456 40.0278901194453, -105.2703590775048 40.02783396502272, -105.2705449708217 40.02777311773346, -105.2707191449315 40.02769302966741, -105.2712200627177 40.02739891617156, -105.2721821366655 40.026844096625, -105.2722851382764 40.02679598460758, -105.2724391697248 40.02675813072266, -105.2726248698914 40.02675410445867, -105.2726181274602 40.02620587677047, -105.2726178873861 40.02606394994715, -105.2726199882499 40.02575512003067, -105.2725799692758 40.02565593982267, -105.2725230499857 40.02559186516272, -105.2724079619951 40.02551696877548, -105.2716481672724 40.02506800120462, -105.2715121215238 40.02496094431037, -105.2714558843878 40.02490702710772, -105.271283153701 40.02498492246853, -105.2711960062075 40.02499106319144, -105.2711471268735 40.02497888759054, -105.2705571374207 40.02490112502463, -105.2701351511876 40.02487695076279, -105.2698180480713 40.02488208254371, -105.2695930218969 40.02490194833804, -105.2689580821212 40.02502311364085, -105.2687318382624 40.02508607416824, -105.2686079015087 40.02509488435066, -105.2685628779465 40.02510412746538, -105.268499879351 40.02514902278204, -105.2684711463209 40.02519810372616, -105.2684139123429 40.02522791115344, -105.2682411423188 40.02458107234318, -105.2679109587122 40.02360394413302, -105.2665938779832 40.02387086387858, -105.2652839000161 40.02414601860607, -105.2639678550197 40.02441702917763, -105.2637180536465 40.02447608769097, -105.2634068292216 40.02453694257784, -105.2619428416898 40.02483590064909, -105.2609680305519 40.02503593129295, -105.2603669897415 40.02515904067031, -105.2588440818718 40.02545097495982, -105.2585261275946 40.02549395801625, -105.258382877582 40.02551095323694, -105.2583841483148 40.02615991830773, -105.2583971480592 40.02732802426323, -105.2584009719777 40.02907012989925, -105.2584008552258 40.0291030718611))</t>
+          <t>POLYGON ((-105.25840085522579 40.0291030718611, -105.25908887590097 40.0291349825795, -105.25973819058426 40.02915582694323, -105.26070850057188 40.029167506994696, -105.261397433136 40.02917401288314, -105.26192089662813 40.02917709843084, -105.26313005541569 40.02917299949814, -105.26331791484425 40.02916597275626, -105.26410493368547 40.029174997276954, -105.26450417642769 40.02917389106241, -105.2650558597207 40.029184898884694, -105.26560009204181 40.02918188831284, -105.2657551564794 40.029158046058555, -105.26588782666258 40.029103960231005, -105.26598304194968 40.0290379943425, -105.26627989371885 40.02869599678734, -105.26636982689826 40.028608058409276, -105.26649288734967 40.02854407048214, -105.26668696610294 40.02849312791361, -105.26848213098779 40.028167048282015, -105.26875297924411 40.028117079495125, -105.26946184227765 40.02800292602936, -105.269954176002 40.027927043839945, -105.27015998674558 40.027890119445296, -105.27035907750484 40.027833965022715, -105.27054497082173 40.02777311773346, -105.27071914493149 40.02769302966741, -105.27122006271772 40.02739891617156, -105.27218213666552 40.026844096625, -105.27228513827643 40.02679598460758, -105.27243916972482 40.02675813072266, -105.27262486989143 40.02675410445867, -105.27261812746025 40.02620587677047, -105.27261788738606 40.02606394994715, -105.27261998824994 40.02575512003067, -105.27257996927581 40.02565593982267, -105.27252304998571 40.025591865162724, -105.27240796199514 40.025516968775484, -105.27164816727242 40.02506800120462, -105.27151212152378 40.02496094431037, -105.2714558843878 40.024907027107716, -105.27128315370099 40.024984922468526, -105.27119600620753 40.024991063191436, -105.27114712687346 40.02497888759054, -105.27055713742074 40.02490112502463, -105.27013515118762 40.02487695076279, -105.2698180480713 40.02488208254371, -105.26959302189694 40.02490194833804, -105.2689580821212 40.02502311364085, -105.26873183826243 40.02508607416824, -105.26860790150869 40.025094884350665, -105.26856287794654 40.025104127465376, -105.26849987935098 40.02514902278204, -105.26847114632093 40.02519810372616, -105.26841391234292 40.025227911153436, -105.26824114231879 40.02458107234318, -105.26791095871219 40.02360394413302, -105.2665938779832 40.02387086387858, -105.26528390001609 40.024146018606075, -105.2639678550197 40.02441702917763, -105.26371805364646 40.02447608769097, -105.26340682922162 40.02453694257784, -105.2619428416898 40.02483590064909, -105.26096803055185 40.02503593129295, -105.2603669897415 40.02515904067031, -105.25884408187184 40.025450974959824, -105.25852612759459 40.02549395801625, -105.25838287758201 40.02551095323694, -105.25838414831479 40.026159918307734, -105.25839714805917 40.02732802426323, -105.25840097197765 40.029070129899246, -105.25840085522579 40.0291030718611))</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -6356,7 +6388,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2584077255942 40.02163362987389, -105.2583830465151 40.0223399835016, -105.2583789356683 40.02339906985873, -105.2583811009352 40.02450099341501, -105.258382877582 40.02551095323694, -105.2585261275946 40.02549395801625, -105.2588440818718 40.02545097495982, -105.2603669897415 40.02515904067031, -105.2609680305519 40.02503593129295, -105.2619428416898 40.02483590064909, -105.2634068292216 40.02453694257784, -105.2637180536465 40.02447608769097, -105.2639678550197 40.02441702917763, -105.2652839000161 40.02414601860607, -105.2665938779832 40.02387086387858, -105.2679109587122 40.02360394413302, -105.2692069688962 40.02333504521185, -105.2706919552907 40.02303713466639, -105.2718350184137 40.0227980990951, -105.2731581119964 40.0225360723508, -105.2737048480964 40.02240812267149, -105.2744830821575 40.02224301388614, -105.2751429569503 40.02212900447875, -105.275791141536 40.02198586943896, -105.2756221241764 40.02148207228412, -105.2754398713189 40.02098593613955, -105.2750889786491 40.01998298339993, -105.274734155878 40.01898386577277, -105.2746429734595 40.01870093263628, -105.2745000155115 40.0183111106561, -105.274376930333 40.01795893586328, -105.2730799837011 40.01822404786218, -105.2717401463564 40.01850004115301, -105.2704370972072 40.01876895355906, -105.2700580063443 40.01884753496827, -105.2696803444062 40.01892556858872, -105.2693019661193 40.01900387333878, -105.2686122076427 40.01914450089696, -105.2680973970993 40.01925466764992, -105.2679198763101 40.01930609172816, -105.2678551656534 40.0193309428674, -105.2676828799027 40.01938604817391, -105.2674491787615 40.01944212820076, -105.2670879450382 40.01951689188036, -105.266296866458 40.01968302265511, -105.2652010009439 40.0199119427986, -105.2639081134081 40.02019378688698, -105.2631006172239 40.02034189325134, -105.2629498628668 40.02034552295202, -105.2627081080169 40.02034502581612, -105.2622897374631 40.02032986645273, -105.2620527330483 40.02030078204538, -105.2607775069657 40.02004506006818, -105.2605279034556 40.02001186733855, -105.2605288886978 40.02034101793548, -105.2602939444293 40.0203419024729, -105.2602139311204 40.02035106960302, -105.260099925642 40.02038102957353, -105.2599729567468 40.02044198359838, -105.2598481531794 40.02049607812605, -105.2597119844178 40.0205331292272, -105.2595879157173 40.02054681546718, -105.2595055587969 40.02055177658189, -105.2583999303681 40.02054880387701, -105.2584077255942 40.02163362987389))</t>
+          <t>POLYGON ((-105.25840772559422 40.02163362987389, -105.25838304651515 40.022339983501595, -105.25837893566833 40.023399069858726, -105.25838110093518 40.02450099341501, -105.25838287758201 40.02551095323694, -105.25852612759459 40.02549395801625, -105.25884408187184 40.025450974959824, -105.2603669897415 40.02515904067031, -105.26096803055185 40.02503593129295, -105.2619428416898 40.02483590064909, -105.26340682922162 40.02453694257784, -105.26371805364646 40.02447608769097, -105.2639678550197 40.02441702917763, -105.26528390001609 40.024146018606075, -105.2665938779832 40.02387086387858, -105.26791095871219 40.02360394413302, -105.26920696889621 40.02333504521185, -105.27069195529073 40.02303713466639, -105.27183501841367 40.0227980990951, -105.27315811199637 40.022536072350796, -105.27370484809641 40.02240812267149, -105.27448308215747 40.02224301388614, -105.2751429569503 40.02212900447875, -105.27579114153596 40.021985869438964, -105.27562212417635 40.02148207228412, -105.27543987131885 40.020985936139546, -105.27508897864912 40.01998298339993, -105.27473415587797 40.018983865772775, -105.27464297345955 40.01870093263628, -105.27450001551146 40.0183111106561, -105.27437693033303 40.017958935863284, -105.2730799837011 40.018224047862184, -105.27174014635642 40.01850004115301, -105.27043709720718 40.01876895355906, -105.27005800634433 40.01884753496827, -105.26968034440624 40.01892556858872, -105.26930196611934 40.019003873338775, -105.26861220764275 40.01914450089696, -105.2680973970993 40.019254667649925, -105.26791987631009 40.01930609172816, -105.26785516565336 40.0193309428674, -105.26768287990271 40.019386048173914, -105.2674491787615 40.01944212820076, -105.2670879450382 40.019516891880365, -105.26629686645802 40.01968302265511, -105.26520100094393 40.0199119427986, -105.26390811340815 40.02019378688698, -105.2631006172239 40.02034189325134, -105.26294986286676 40.02034552295202, -105.26270810801692 40.02034502581612, -105.26228973746308 40.020329866452734, -105.26205273304831 40.02030078204538, -105.26077750696568 40.020045060068185, -105.26052790345557 40.02001186733855, -105.2605288886978 40.02034101793548, -105.26029394442926 40.0203419024729, -105.26021393112042 40.02035106960302, -105.26009992564202 40.02038102957353, -105.25997295674681 40.02044198359838, -105.25984815317936 40.02049607812605, -105.25971198441779 40.0205331292272, -105.2595879157173 40.020546815467185, -105.25950555879692 40.02055177658189, -105.25839993036806 40.02054880387701, -105.25840772559422 40.02163362987389))</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
@@ -6398,7 +6430,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2583865082488 40.02003406862268, -105.2583999303681 40.02054880387701, -105.2595055587969 40.02055177658189, -105.2595879157173 40.02054681546718, -105.2597119844178 40.0205331292272, -105.2598481531794 40.02049607812605, -105.2599729567468 40.02044198359838, -105.260099925642 40.02038102957353, -105.2602139311204 40.02035106960302, -105.2602939444293 40.0203419024729, -105.2605288886978 40.02034101793548, -105.2605279034556 40.02001186733855, -105.2607775069657 40.02004506006818, -105.2620527330483 40.02030078204538, -105.2622897374631 40.02032986645273, -105.2627081080169 40.02034502581612, -105.2629498628668 40.02034552295202, -105.2631006172239 40.02034189325134, -105.2639081134081 40.02019378688698, -105.2652010009439 40.0199119427986, -105.266296866458 40.01968302265511, -105.2670879450382 40.01951689188036, -105.2674491787615 40.01944212820076, -105.2676828799027 40.01938604817391, -105.2676990767671 40.01931258403011, -105.267689766196 40.01890867348826, -105.2678383911952 40.01887780661495, -105.2678359656673 40.01865406816931, -105.2674461746455 40.01865516972585, -105.2674429838105 40.01824029343027, -105.2679035691069 40.01824071327699, -105.2678914857639 40.01728391407077, -105.2704739413353 40.01726411374025, -105.2704901696526 40.01721610437608, -105.2704270439177 40.01666501947656, -105.2703914128105 40.01633604674385, -105.2703481026559 40.01627309591758, -105.270323100022 40.01625495473562, -105.2702621077403 40.01623698954031, -105.2702128396511 40.01623606819027, -105.2690099946544 40.01623613578052, -105.2689849046278 40.01542213584512, -105.2689819637891 40.01460406242605, -105.2678219770818 40.01460804739548, -105.2662260626349 40.01461196195721, -105.2657616256185 40.01461332253763, -105.2646558644589 40.01461288522881, -105.2638765422727 40.01460508854388, -105.2630753109644 40.01461633090538, -105.2630299591908 40.01461696725389, -105.258420544823 40.01462569237854, -105.2583967697713 40.01738897110558, -105.2583835533824 40.017841051784, -105.2583845465005 40.01820405441318, -105.2583845261048 40.01916806167687, -105.2583865082488 40.02003406862268))</t>
+          <t>POLYGON ((-105.25838650824882 40.02003406862268, -105.25839993036806 40.02054880387701, -105.25950555879692 40.02055177658189, -105.2595879157173 40.020546815467185, -105.25971198441779 40.0205331292272, -105.25984815317936 40.02049607812605, -105.25997295674681 40.02044198359838, -105.26009992564202 40.02038102957353, -105.26021393112042 40.02035106960302, -105.26029394442926 40.0203419024729, -105.2605288886978 40.02034101793548, -105.26052790345557 40.02001186733855, -105.26077750696568 40.020045060068185, -105.26205273304831 40.02030078204538, -105.26228973746308 40.020329866452734, -105.26270810801692 40.02034502581612, -105.26294986286676 40.02034552295202, -105.2631006172239 40.02034189325134, -105.26390811340815 40.02019378688698, -105.26520100094393 40.0199119427986, -105.26629686645802 40.01968302265511, -105.2670879450382 40.019516891880365, -105.2674491787615 40.01944212820076, -105.26768287990271 40.019386048173914, -105.26769907676712 40.01931258403011, -105.26768976619597 40.01890867348826, -105.26783839119521 40.018877806614945, -105.26783596566729 40.01865406816931, -105.26744617464554 40.018655169725854, -105.26744298381051 40.018240293430274, -105.26790356910695 40.01824071327699, -105.26789148576385 40.01728391407077, -105.27047394133527 40.01726411374025, -105.27049016965263 40.01721610437608, -105.27042704391768 40.01666501947656, -105.27039141281045 40.01633604674385, -105.27034810265589 40.016273095917576, -105.27032310002201 40.016254954735615, -105.27026210774032 40.01623698954031, -105.27021283965111 40.01623606819027, -105.2690099946544 40.01623613578052, -105.26898490462783 40.01542213584512, -105.26898196378912 40.01460406242605, -105.26782197708182 40.01460804739548, -105.26622606263491 40.014611961957215, -105.26576162561848 40.01461332253763, -105.26465586445893 40.014612885228814, -105.2638765422727 40.01460508854388, -105.26307531096444 40.014616330905376, -105.26302995919076 40.01461696725389, -105.258420544823 40.014625692378544, -105.25839676977125 40.017388971105575, -105.25838355338244 40.017841051783996, -105.2583845465005 40.01820405441318, -105.25838452610483 40.019168061676865, -105.25838650824882 40.02003406862268))</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
@@ -6440,7 +6472,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2745000155115 40.0183111106561, -105.2746429734595 40.01870093263628, -105.274734155878 40.01898386577277, -105.2750889786491 40.01998298339993, -105.2754398713189 40.02098593613955, -105.2756221241764 40.02148207228412, -105.275791141536 40.02198586943896, -105.2771059814931 40.02172707508173, -105.2777080128257 40.02160991932885, -105.2784180042659 40.02145288802323, -105.2797088871452 40.02119786196825, -105.2803241748155 40.02106397208449, -105.2810050386895 40.02092611359631, -105.2810049992309 40.02092599823808, -105.2810182375564 40.02092314129024, -105.2806882501358 40.01992431817114, -105.2803492507365 40.01890931823954, -105.280344103938 40.01889429097838, -105.2800122511694 40.01792531871845, -105.2797922499383 40.0173063188877, -105.2796422519211 40.01688331794094, -105.2795172500427 40.01656331893992, -105.2793182480616 40.01593431868323, -105.2792882488983 40.01584331888502, -105.279283131531 40.01582838979826, -105.2790212496877 40.01506431947683, -105.2789422504309 40.01484831880367, -105.2788752505237 40.01466131864607, -105.278851249496 40.01459531880194, -105.2786822492777 40.01411631803115, -105.2786769521653 40.01410055096331, -105.278663968713 40.01410393231048, -105.2782030961592 40.01419611210767, -105.278005899344 40.01423306829994, -105.2775250367717 40.01432794849211, -105.2773539185385 40.01436001199994, -105.2764250735946 40.01453802385365, -105.2760611408061 40.01457602595389, -105.2746458800721 40.01458095527774, -105.2736219240902 40.0145838908234, -105.2725519067238 40.01458809993736, -105.2716550449331 40.01459291590101, -105.270220141546 40.01459912551402, -105.2689819637891 40.01460406242605, -105.2689849046278 40.01542213584512, -105.2690099946544 40.01623613578052, -105.2702128396511 40.01623606819027, -105.2702621077403 40.01623698954031, -105.270323100022 40.01625495473562, -105.2703481026559 40.01627309591758, -105.2703914128105 40.01633604674385, -105.2704270439177 40.01666501947656, -105.2704901696526 40.01721610437608, -105.2704739413353 40.01726411374025, -105.2678914857639 40.01728391407077, -105.2679035691069 40.01824071327699, -105.2674429838105 40.01824029343027, -105.2674461746455 40.01865516972585, -105.2678359656673 40.01865406816931, -105.2678383911952 40.01887780661495, -105.267689766196 40.01890867348826, -105.2676990767671 40.01931258403011, -105.2676828799027 40.01938604817391, -105.2678551656534 40.0193309428674, -105.2679198763101 40.01930609172816, -105.2680973970993 40.01925466764992, -105.2686122076427 40.01914450089696, -105.2693019661193 40.01900387333878, -105.2696803444062 40.01892556858872, -105.2700580063443 40.01884753496827, -105.2704370972072 40.01876895355906, -105.2717401463564 40.01850004115301, -105.2730799837011 40.01822404786218, -105.274376930333 40.01795893586328, -105.2745000155115 40.0183111106561))</t>
+          <t>POLYGON ((-105.27450001551146 40.0183111106561, -105.27464297345955 40.01870093263628, -105.27473415587797 40.018983865772775, -105.27508897864912 40.01998298339993, -105.27543987131885 40.020985936139546, -105.27562212417635 40.02148207228412, -105.27579114153596 40.021985869438964, -105.27710598149311 40.021727075081735, -105.27770801282566 40.02160991932885, -105.27841800426593 40.021452888023234, -105.27970888714518 40.021197861968254, -105.28032417481549 40.02106397208449, -105.28100503868954 40.02092611359631, -105.28100499923086 40.02092599823808, -105.28101823755642 40.02092314129024, -105.28068825013582 40.019924318171135, -105.28034925073653 40.01890931823954, -105.28034410393798 40.01889429097838, -105.28001225116941 40.01792531871845, -105.27979224993825 40.0173063188877, -105.2796422519211 40.016883317940945, -105.27951725004274 40.016563318939916, -105.27931824806156 40.01593431868323, -105.27928824889825 40.01584331888502, -105.27928313153105 40.01582838979826, -105.27902124968774 40.015064319476835, -105.27894225043093 40.01484831880367, -105.27887525052368 40.01466131864607, -105.27885124949597 40.014595318801945, -105.27868224927768 40.01411631803115, -105.27867695216533 40.014100550963306, -105.27866396871299 40.01410393231048, -105.2782030961592 40.01419611210767, -105.278005899344 40.01423306829994, -105.27752503677172 40.01432794849211, -105.27735391853847 40.01436001199994, -105.2764250735946 40.01453802385365, -105.27606114080606 40.01457602595389, -105.27464588007207 40.014580955277744, -105.27362192409025 40.0145838908234, -105.27255190672376 40.014588099937356, -105.27165504493307 40.01459291590101, -105.27022014154602 40.014599125514025, -105.26898196378912 40.01460406242605, -105.26898490462783 40.01542213584512, -105.2690099946544 40.01623613578052, -105.27021283965111 40.01623606819027, -105.27026210774032 40.01623698954031, -105.27032310002201 40.016254954735615, -105.27034810265589 40.016273095917576, -105.27039141281045 40.01633604674385, -105.27042704391768 40.01666501947656, -105.27049016965263 40.01721610437608, -105.27047394133527 40.01726411374025, -105.26789148576385 40.01728391407077, -105.26790356910695 40.01824071327699, -105.26744298381051 40.018240293430274, -105.26744617464554 40.018655169725854, -105.26783596566729 40.01865406816931, -105.26783839119521 40.018877806614945, -105.26768976619597 40.01890867348826, -105.26769907676712 40.01931258403011, -105.26768287990271 40.019386048173914, -105.26785516565336 40.0193309428674, -105.26791987631009 40.01930609172816, -105.2680973970993 40.019254667649925, -105.26861220764275 40.01914450089696, -105.26930196611934 40.019003873338775, -105.26968034440624 40.01892556858872, -105.27005800634433 40.01884753496827, -105.27043709720718 40.01876895355906, -105.27174014635642 40.01850004115301, -105.2730799837011 40.018224047862184, -105.27437693033303 40.017958935863284, -105.27450001551146 40.0183111106561))</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
@@ -6482,7 +6514,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2804018518184 40.030093047055, -105.2805939720805 40.03009396023452, -105.2820898563745 40.03010393344913, -105.2820900004695 40.03010393732394, -105.2821084505153 40.03010442340204, -105.28212225549 40.02926831736175, -105.2821221918683 40.02925559915963, -105.2832689344744 40.02923208823412, -105.2844270167391 40.02923096285564, -105.2854201124465 40.02923199133771, -105.2855761122275 40.02924902721826, -105.2855863541211 40.02924870040671, -105.2855862117171 40.02922543814994, -105.2855754584629 40.02732638721953, -105.2855712105374 40.02672743692585, -105.2855692118289 40.02663843724292, -105.2855892107703 40.02642143748587, -105.2856742107215 40.02601043682525, -105.2856822111836 40.02592843665887, -105.2856812109885 40.02583443661324, -105.2856660543705 40.0255160131922, -105.283568919774 40.02551402008966, -105.2832522926848 40.02551476930772, -105.2820799576935 40.02551691771405, -105.2820552528565 40.02447831817484, -105.2820462506693 40.02416731908562, -105.282030253746 40.02400831769852, -105.2819872512269 40.02381131814664, -105.2819012528731 40.02352531873172, -105.2817882518133 40.02320731847269, -105.2816952524114 40.02294531788972, -105.2814522517319 40.02218931788916, -105.2813222531418 40.02180131874344, -105.2810232518009 40.02093831867468, -105.2810182375564 40.02092314129024, -105.2810049992309 40.02092599823808, -105.2810050386895 40.02092611359631, -105.2803241748155 40.02106397208449, -105.2797088871452 40.02119786196825, -105.2784180042659 40.02145288802323, -105.2777080128257 40.02160991932885, -105.2771059814931 40.02172707508173, -105.275791141536 40.02198586943896, -105.2751429569503 40.02212900447875, -105.2744830821575 40.02224301388614, -105.2737048480964 40.02240812267149, -105.2731581119964 40.0225360723508, -105.2718350184137 40.0227980990951, -105.2706919552907 40.02303713466639, -105.2692069688962 40.02333504521185, -105.2679109587122 40.02360394413302, -105.2682411423188 40.02458107234318, -105.2684139123429 40.02522791115344, -105.2684711463209 40.02519810372616, -105.268499879351 40.02514902278204, -105.2685628779465 40.02510412746538, -105.2686079015087 40.02509488435066, -105.2687318382624 40.02508607416824, -105.2689580821212 40.02502311364085, -105.2695930218969 40.02490194833804, -105.2698180480713 40.02488208254371, -105.2701351511876 40.02487695076279, -105.2705571374207 40.02490112502463, -105.2711471268735 40.02497888759054, -105.2711960062075 40.02499106319144, -105.271283153701 40.02498492246853, -105.2714558843878 40.02490702710772, -105.2715121215238 40.02496094431037, -105.2716481672724 40.02506800120462, -105.2724079619951 40.02551696877548, -105.2725230499857 40.02559186516272, -105.2725799692758 40.02565593982267, -105.2726199882499 40.02575512003067, -105.2726178873861 40.02606394994715, -105.2726181274602 40.02620587677047, -105.2726248698914 40.02675410445867, -105.2726378711389 40.02799495559294, -105.2726431137961 40.02931402807485, -105.2726510020113 40.03005387211383, -105.273645871071 40.030061869293, -105.2741701059328 40.03006097391676, -105.2751321551345 40.03005901118281, -105.276498044355 40.03007099921356, -105.277470066055 40.03007699534945, -105.2781960300691 40.03008690379698, -105.2784088644469 40.03008703905117, -105.2791998402836 40.03009102538928, -105.2793758908887 40.03009191253876, -105.2803029427175 40.03009011263436, -105.2804018518184 40.030093047055))</t>
+          <t>POLYGON ((-105.28040185181841 40.030093047055, -105.28059397208054 40.030093960234524, -105.2820898563745 40.03010393344913, -105.28209000046947 40.030103937323936, -105.28210845051531 40.03010442340204, -105.28212225548998 40.02926831736175, -105.28212219186831 40.029255599159626, -105.28326893447445 40.02923208823412, -105.28442701673912 40.029230962855635, -105.28542011244654 40.02923199133771, -105.28557611222752 40.029249027218256, -105.2855863541211 40.02924870040671, -105.28558621171715 40.029225438149936, -105.28557545846286 40.02732638721953, -105.28557121053741 40.02672743692585, -105.2855692118289 40.02663843724292, -105.28558921077033 40.02642143748587, -105.2856742107215 40.02601043682525, -105.28568221118361 40.02592843665887, -105.28568121098849 40.025834436613245, -105.2856660543705 40.0255160131922, -105.28356891977397 40.02551402008966, -105.28325229268482 40.02551476930772, -105.28207995769351 40.02551691771405, -105.28205525285647 40.02447831817484, -105.28204625066932 40.02416731908562, -105.28203025374596 40.02400831769852, -105.28198725122694 40.02381131814664, -105.2819012528731 40.02352531873172, -105.28178825181327 40.023207318472686, -105.28169525241138 40.02294531788972, -105.2814522517319 40.022189317889165, -105.28132225314175 40.02180131874344, -105.28102325180092 40.02093831867468, -105.28101823755642 40.02092314129024, -105.28100499923086 40.02092599823808, -105.28100503868954 40.02092611359631, -105.28032417481549 40.02106397208449, -105.27970888714518 40.021197861968254, -105.27841800426593 40.021452888023234, -105.27770801282566 40.02160991932885, -105.27710598149311 40.021727075081735, -105.27579114153596 40.021985869438964, -105.2751429569503 40.02212900447875, -105.27448308215747 40.02224301388614, -105.27370484809641 40.02240812267149, -105.27315811199637 40.022536072350796, -105.27183501841367 40.0227980990951, -105.27069195529073 40.02303713466639, -105.26920696889621 40.02333504521185, -105.26791095871219 40.02360394413302, -105.26824114231879 40.02458107234318, -105.26841391234292 40.025227911153436, -105.26847114632093 40.02519810372616, -105.26849987935098 40.02514902278204, -105.26856287794654 40.025104127465376, -105.26860790150869 40.025094884350665, -105.26873183826243 40.02508607416824, -105.2689580821212 40.02502311364085, -105.26959302189694 40.02490194833804, -105.2698180480713 40.02488208254371, -105.27013515118762 40.02487695076279, -105.27055713742074 40.02490112502463, -105.27114712687346 40.02497888759054, -105.27119600620753 40.024991063191436, -105.27128315370099 40.024984922468526, -105.2714558843878 40.024907027107716, -105.27151212152378 40.02496094431037, -105.27164816727242 40.02506800120462, -105.27240796199514 40.025516968775484, -105.27252304998571 40.025591865162724, -105.27257996927581 40.02565593982267, -105.27261998824994 40.02575512003067, -105.27261788738606 40.02606394994715, -105.27261812746025 40.02620587677047, -105.27262486989143 40.02675410445867, -105.27263787113887 40.027994955592945, -105.27264311379614 40.02931402807485, -105.2726510020113 40.03005387211383, -105.27364587107101 40.030061869293, -105.27417010593277 40.03006097391676, -105.27513215513453 40.030059011182814, -105.27649804435504 40.03007099921356, -105.27747006605496 40.03007699534945, -105.27819603006911 40.03008690379698, -105.27840886444692 40.030087039051175, -105.27919984028357 40.030091025389275, -105.27937589088867 40.03009191253876, -105.28030294271747 40.03009011263436, -105.28040185181841 40.030093047055))</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
@@ -6524,10 +6556,14 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2810182375564 40.02092314129024, -105.2810232518009 40.02093831867468, -105.2813222531418 40.02180131874344, -105.2814522517319 40.02218931788916, -105.2816952524114 40.02294531788972, -105.2817882518133 40.02320731847269, -105.2819012528731 40.02352531873172, -105.2819872512269 40.02381131814664, -105.282030253746 40.02400831769852, -105.2820462506693 40.02416731908562, -105.2820552528565 40.02447831817484, -105.2820799576935 40.02551691771405, -105.2832522926848 40.02551476930772, -105.283568919774 40.02551402008966, -105.2856660543705 40.0255160131922, -105.2856570833245 40.024507963209, -105.2856500166217 40.02368906050599, -105.2856359777445 40.02327094245604, -105.2856281572593 40.02314602207673, -105.2855958483006 40.02297411245853, -105.285527898361 40.02278099918674, -105.2854569165297 40.02264388269615, -105.2851988391675 40.02227801733283, -105.2849598351697 40.0219788954425, -105.2849019229106 40.02188709849514, -105.2848640990607 40.02176596516206, -105.2848648315332 40.02074201109222, -105.2848861179262 40.02055894665072, -105.2849060840865 40.0204549406858, -105.2848988256668 40.02037888518526, -105.284697939107 40.01977100051715, -105.2844501492575 40.0190919268021, -105.284370977069 40.0188370251274, -105.2842460118721 40.01849803489817, -105.2840818920156 40.01812191122571, -105.280344103938 40.01889429097838, -105.2803492507365 40.01890931823954, -105.2806882501358 40.01992431817114, -105.2810182375564 40.02092314129024))</t>
-        </is>
-      </c>
-      <c r="H146" t="inlineStr"/>
+          <t>POLYGON ((-105.28101823755642 40.02092314129024, -105.28102325180092 40.02093831867468, -105.28132225314175 40.02180131874344, -105.2814522517319 40.022189317889165, -105.28169525241138 40.02294531788972, -105.28178825181327 40.023207318472686, -105.2819012528731 40.02352531873172, -105.28198725122694 40.02381131814664, -105.28203025374596 40.02400831769852, -105.28204625066932 40.02416731908562, -105.28205525285647 40.02447831817484, -105.28207995769351 40.02551691771405, -105.28325229268482 40.02551476930772, -105.28356891977397 40.02551402008966, -105.2856660543705 40.0255160131922, -105.2856570833245 40.024507963209, -105.28565001662172 40.02368906050599, -105.2856359777445 40.02327094245604, -105.28562815725932 40.02314602207673, -105.28559584830063 40.02297411245853, -105.28552789836098 40.02278099918674, -105.2854569165297 40.02264388269615, -105.28519883916746 40.02227801733283, -105.28495983516974 40.0219788954425, -105.28490192291062 40.021887098495135, -105.28486409906071 40.02176596516206, -105.28486483153323 40.02074201109222, -105.2848861179262 40.02055894665072, -105.28490608408649 40.0204549406858, -105.28489882566683 40.02037888518526, -105.28469793910703 40.019771000517146, -105.2844501492575 40.019091926802105, -105.28437097706903 40.0188370251274, -105.28424601187214 40.018498034898165, -105.28408189201564 40.018121911225705, -105.28034410393798 40.01889429097838, -105.28034925073653 40.01890931823954, -105.28068825013582 40.019924318171135, -105.28101823755642 40.02092314129024))</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Casey MS</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -6562,7 +6598,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2856660543705 40.0255160131922, -105.2867490705732 40.02551994347327, -105.2887301598848 40.02552001896971, -105.290043906236 40.02550594671673, -105.2902481507636 40.02550796560364, -105.2915040127181 40.02550612476494, -105.2920939363481 40.025498130862, -105.2925031180585 40.02550902431486, -105.2926069291672 40.02543973575167, -105.2962396867081 40.02535273730569, -105.2962396415504 40.02215067912587, -105.2965063930992 40.02212077652984, -105.296517951967 40.02170905190105, -105.2973454669022 40.02169077920819, -105.2975414845485 40.0216889150605, -105.2978286935315 40.02168380149962, -105.2985031217535 40.02167179168337, -105.2993086826939 40.02165744112135, -105.2994764234297 40.02165361239809, -105.2995578477222 40.02165092228681, -105.2999702138019 40.02163943527666, -105.3000022127899 40.02163643576153, -105.3000416495151 40.02163458305144, -105.3001512135371 40.02162943569349, -105.3003744593163 40.02186554865892, -105.300551877922 40.02205473641342, -105.3006923663629 40.02220365504299, -105.3007456372707 40.02226072043052, -105.3008132688921 40.02233316848579, -105.300850162537 40.02237268968993, -105.3009018723378 40.02242808160176, -105.300917159086 40.02244445749604, -105.3009242022055 40.02245200179229, -105.3009373752128 40.02246611250222, -105.3009452930333 40.02247459408259, -105.3009490405688 40.02247860844452, -105.3009510573917 40.02248076988352, -105.3009542338659 40.02248417171811, -105.3009547173413 40.02248469042645, -105.3009560264697 40.02248609229643, -105.300956902401 40.02248700796821, -105.3009582137961 40.02248843596094, -105.3009753391095 40.01934896424599, -105.3010112132555 40.01445143493394, -105.3010146521981 40.01412034528163, -105.3010065439604 40.01412285491573, -105.3009841703811 40.01413088704314, -105.3008359183136 40.01416110284114, -105.300684149682 40.01417292017293, -105.3005359990144 40.01416799685423, -105.300254092653 40.01412001668933, -105.300067868143 40.0140719279547, -105.3000011606622 40.01405287069223, -105.2996880626172 40.01392796986438, -105.2994309509394 40.01382595114303, -105.2990971694855 40.01369387506902, -105.2989748438362 40.01364891574665, -105.2987091069599 40.01356691986554, -105.2984361789157 40.01350193131028, -105.2981560643021 40.0134531259425, -105.2978951689382 40.01342411927098, -105.2975649848486 40.01340487234885, -105.297280077546 40.01340711706504, -105.2972629400945 40.01340708693889, -105.2968701231647 40.01343988732408, -105.2966129379867 40.013483906396, -105.2959720191087 40.01362689650804, -105.2955889946644 40.01372696689724, -105.2951188286011 40.01383593998661, -105.2948950990359 40.01391405477982, -105.2948279437313 40.01392601395955, -105.2948850709373 40.01404306065437, -105.2949111667633 40.01415099338725, -105.2949149278989 40.01420590378106, -105.2949106525785 40.01428611088715, -105.2948669406371 40.01436130597801, -105.2948050566042 40.01443646962085, -105.2945651847544 40.01463397060598, -105.2942962425791 40.01484536492688, -105.2941799322994 40.01493717604964, -105.2940456558378 40.01498431869415, -105.2935522291935 40.01508380053187, -105.2932648974691 40.01514153813964, -105.2929311934506 40.01520907552712, -105.2924838834105 40.01529960385942, -105.2916482773999 40.01546871123976, -105.2904817987244 40.01572217487955, -105.2891551001181 40.01599098183944, -105.2885419939298 40.01611983770974, -105.2878670067061 40.0162528717229, -105.2866812529073 40.01650245354258, -105.2865308262578 40.01653288651573, -105.2852128642166 40.01680605680808, -105.2850088672696 40.01684712918449, -105.2841060700353 40.01702607643248, -105.2840110981352 40.01704713596685, -105.2837991589066 40.01709413112621, -105.2838869444426 40.01755905605179, -105.2839600121989 40.01782410420856, -105.2840818920156 40.01812191122571, -105.2842460118721 40.01849803489817, -105.284370977069 40.0188370251274, -105.2844501492575 40.0190919268021, -105.284697939107 40.01977100051715, -105.2848988256668 40.02037888518526, -105.2849060840865 40.0204549406858, -105.2848861179262 40.02055894665072, -105.2848648315332 40.02074201109222, -105.2848640990607 40.02176596516206, -105.2849019229106 40.02188709849514, -105.2849598351697 40.0219788954425, -105.2851988391675 40.02227801733283, -105.2854569165297 40.02264388269615, -105.285527898361 40.02278099918674, -105.2855958483006 40.02297411245853, -105.2856281572593 40.02314602207673, -105.2856359777445 40.02327094245604, -105.2856500166217 40.02368906050599, -105.2856570833245 40.024507963209, -105.2856660543705 40.0255160131922))</t>
+          <t>POLYGON ((-105.2856660543705 40.0255160131922, -105.28674907057322 40.02551994347327, -105.28873015988484 40.025520018969715, -105.29004390623602 40.02550594671673, -105.29024815076362 40.02550796560364, -105.29150401271811 40.02550612476494, -105.29209393634812 40.025498130862, -105.2925031180585 40.025509024314864, -105.29260692916722 40.02543973575167, -105.29623968670813 40.02535273730569, -105.29623964155041 40.02215067912587, -105.29650639309915 40.02212077652984, -105.29651795196699 40.02170905190105, -105.2973454669022 40.021690779208186, -105.2975414845485 40.0216889150605, -105.29782869353146 40.02168380149962, -105.29850312175354 40.021671791683374, -105.29930868269392 40.02165744112135, -105.29947642342967 40.02165361239809, -105.2995578477222 40.02165092228681, -105.29997021380194 40.02163943527666, -105.30000221278986 40.02163643576153, -105.30004164951507 40.02163458305144, -105.30015121353712 40.02162943569349, -105.30037445931632 40.021865548658916, -105.300551877922 40.022054736413416, -105.30069236636294 40.02220365504299, -105.30074563727065 40.022260720430516, -105.30081326889211 40.02233316848579, -105.30085016253703 40.02237268968993, -105.30090187233777 40.02242808160176, -105.30091715908598 40.022444457496036, -105.3009242022055 40.02245200179229, -105.30093737521281 40.022466112502215, -105.3009452930333 40.02247459408259, -105.30094904056878 40.02247860844452, -105.30095105739174 40.02248076988352, -105.30095423386594 40.02248417171811, -105.3009547173413 40.02248469042645, -105.30095602646966 40.022486092296425, -105.30095690240098 40.02248700796821, -105.30095821379608 40.022488435960945, -105.30097533910954 40.019348964245985, -105.30101121325552 40.01445143493394, -105.30101465219812 40.014120345281626, -105.30100654396044 40.01412285491573, -105.30098417038108 40.014130887043144, -105.30083591831364 40.014161102841136, -105.30068414968203 40.01417292017293, -105.30053599901436 40.014167996854226, -105.30025409265298 40.014120016689326, -105.30006786814296 40.0140719279547, -105.30000116066219 40.014052870692225, -105.29968806261716 40.013927969864376, -105.2994309509394 40.013825951143026, -105.29909716948549 40.013693875069016, -105.29897484383618 40.01364891574665, -105.29870910695993 40.01356691986554, -105.29843617891571 40.01350193131028, -105.29815606430208 40.013453125942505, -105.2978951689382 40.01342411927098, -105.29756498484858 40.01340487234885, -105.29728007754596 40.01340711706504, -105.29726294009447 40.01340708693889, -105.29687012316467 40.01343988732408, -105.29661293798665 40.013483906396, -105.29597201910866 40.01362689650804, -105.29558899466441 40.01372696689724, -105.29511882860109 40.01383593998661, -105.29489509903587 40.013914054779825, -105.29482794373129 40.01392601395955, -105.29488507093733 40.01404306065437, -105.29491116676326 40.014150993387254, -105.29491492789886 40.01420590378106, -105.29491065257852 40.01428611088715, -105.29486694063706 40.01436130597801, -105.29480505660418 40.01443646962085, -105.29456518475438 40.01463397060598, -105.29429624257914 40.014845364926884, -105.2941799322994 40.01493717604964, -105.29404565583785 40.014984318694154, -105.29355222919354 40.01508380053187, -105.29326489746909 40.015141538139645, -105.29293119345061 40.01520907552712, -105.29248388341045 40.01529960385942, -105.29164827739994 40.01546871123976, -105.2904817987244 40.01572217487955, -105.28915510011811 40.015990981839444, -105.28854199392984 40.016119837709745, -105.28786700670614 40.0162528717229, -105.28668125290733 40.01650245354258, -105.28653082625777 40.01653288651573, -105.28521286421662 40.01680605680808, -105.28500886726961 40.01684712918449, -105.28410607003526 40.01702607643248, -105.28401109813524 40.01704713596685, -105.28379915890659 40.017094131126214, -105.28388694444259 40.017559056051795, -105.28396001219888 40.01782410420856, -105.28408189201564 40.018121911225705, -105.28424601187214 40.018498034898165, -105.28437097706903 40.0188370251274, -105.2844501492575 40.019091926802105, -105.28469793910703 40.019771000517146, -105.28489882566683 40.02037888518526, -105.28490608408649 40.0204549406858, -105.2848861179262 40.02055894665072, -105.28486483153323 40.02074201109222, -105.28486409906071 40.02176596516206, -105.28490192291062 40.021887098495135, -105.28495983516974 40.0219788954425, -105.28519883916746 40.02227801733283, -105.2854569165297 40.02264388269615, -105.28552789836098 40.02278099918674, -105.28559584830063 40.02297411245853, -105.28562815725932 40.02314602207673, -105.2856359777445 40.02327094245604, -105.28565001662172 40.02368906050599, -105.2856570833245 40.024507963209, -105.2856660543705 40.0255160131922))</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
@@ -6604,7 +6640,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2837252085129 40.01657343580141, -105.283771209105 40.01665443657647, -105.2838012090704 40.01686243610673, -105.2837991589066 40.01709413112621, -105.2838089245483 40.01709196535331, -105.2840110981352 40.01704713596685, -105.2841060700353 40.01702607643248, -105.2850088672696 40.01684712918449, -105.2852128642166 40.01680605680808, -105.2865308262578 40.01653288651573, -105.2866812529073 40.01650245354258, -105.2878670067061 40.0162528717229, -105.2885419939298 40.01611983770974, -105.2891551001181 40.01599098183944, -105.2904817987244 40.01572217487955, -105.2916482773999 40.01546871123976, -105.2924838834105 40.01529960385942, -105.2929311934506 40.01520907552712, -105.2932648974691 40.01514153813964, -105.2935522291935 40.01508380053187, -105.2940456558378 40.01498431869415, -105.2941799322994 40.01493717604964, -105.2942962425791 40.01484536492688, -105.2945651847544 40.01463397060598, -105.2948050566042 40.01443646962085, -105.2948669406371 40.01436130597801, -105.2949106525785 40.01428611088715, -105.2949149278989 40.01420590378106, -105.2949111667633 40.01415099338725, -105.2948850709373 40.01404306065437, -105.2948279437313 40.01392601395955, -105.2948950990359 40.01391405477982, -105.2951188286011 40.01383593998661, -105.2955889946644 40.01372696689724, -105.2959720191087 40.01362689650804, -105.2966129379867 40.013483906396, -105.2968701231647 40.01343988732408, -105.2972629400945 40.01340708693889, -105.297280077546 40.01340711706504, -105.2975649848486 40.01340487234885, -105.2978951689382 40.01342411927098, -105.2981560643021 40.0134531259425, -105.2984361789157 40.01350193131028, -105.2987091069599 40.01356691986554, -105.2989748438362 40.01364891574665, -105.2990971694855 40.01369387506902, -105.2994309509394 40.01382595114303, -105.2996880626172 40.01392796986438, -105.3000011606622 40.01405287069223, -105.300067868143 40.0140719279547, -105.300254092653 40.01412001668933, -105.3005359990144 40.01416799685423, -105.300684149682 40.01417292017293, -105.3008359183136 40.01416110284114, -105.3009841703811 40.01413088704314, -105.3010065439604 40.01412285491573, -105.3010143555852 40.01412043663623, -105.3010146521981 40.01412034528163, -105.3010158302282 40.01400687156732, -105.3010182134563 40.01377743388108, -105.3012511657355 40.01363978016212, -105.3012602122003 40.01363443507628, -105.3013157480595 40.01351102356379, -105.3013862127445 40.01335443432603, -105.3014422127245 40.01298943465143, -105.3014430498437 40.01295818709555, -105.3014437804599 40.01293093194339, -105.3014452129743 40.01287743392142, -105.3014602128255 40.01281143480046, -105.3013522126834 40.01290343407975, -105.3012592457636 40.01298185572877, -105.301205212717 40.01302743462566, -105.3011789468909 40.01300787493373, -105.3011764667329 40.01300603603117, -105.3011729942204 40.0130034812011, -105.3011729464176 40.01300340546396, -105.3011632841785 40.01299621061416, -105.3011419577046 40.01298029445854, -105.3011202771397 40.01296410208901, -105.3010292126056 40.01289543426423, -105.3010281067779 40.01289306454397, -105.301023340076 40.01288285103966, -105.3009735379753 40.01278267752139, -105.3009032128719 40.01264143397508, -105.3008117447473 40.01263456076815, -105.3007562324528 40.01263038942474, -105.3007216161107 40.01262785912573, -105.3007216232754 40.01262781230426, -105.3007216280422 40.01262778439228, -105.3004884530218 40.01261020130202, -105.3002518157827 40.01259380600695, -105.299705267281 40.01255424261292, -105.2993692121943 40.01253043425595, -105.2993753074033 40.01249150609813, -105.2993653365875 40.01249054937211, -105.2994896376608 40.01169225972444, -105.2992927086213 40.01167132375566, -105.2986916238546 40.01160627754996, -105.2986066136606 40.01177065292691, -105.2985718404069 40.01183568677898, -105.2984517355405 40.01181772238958, -105.298122211411 40.01176843426795, -105.2976912121973 40.01172343446013, -105.2976410500742 40.01171848383155, -105.2975392118156 40.01170843394527, -105.2974892276555 40.01192397025246, -105.2974275838077 40.01218258042406, -105.2974242114839 40.01219643372481, -105.2972624798172 40.01217012068312, -105.2969202114587 40.01211443461543, -105.2969212186651 40.01238543430799, -105.2969222108167 40.01264143451774, -105.2961832109625 40.01252843470885, -105.295809211419 40.01257043426351, -105.2957852116624 40.012505434982, -105.2957822123902 40.01218343415776, -105.2954662113391 40.01215043446568, -105.2953132109346 40.01212543471485, -105.2952052115695 40.01213443502252, -105.2948072112871 40.01214143441656, -105.2948072105055 40.01255543418904, -105.2948142108489 40.01267043461998, -105.2942141485911 40.01273466443779, -105.2938052106283 40.01277843517675, -105.2936372113 40.01280243515163, -105.2935512109194 40.0128564346988, -105.2931333503741 40.0128564352352, -105.2927912101938 40.01285643433663, -105.292694211126 40.01285243494313, -105.2926981092893 40.01260199958435, -105.2927022113221 40.01233843488738, -105.293105211251 40.01233943420036, -105.293105976447 40.01208570852052, -105.2931065501837 40.01189546581841, -105.2931072112711 40.01167643394096, -105.2926421528956 40.0116779178345, -105.292480210274 40.01167843441603, -105.2924722100788 40.01164043413667, -105.2922312110259 40.01162343450338, -105.2922312110156 40.01149543479373, -105.2921692110959 40.01143943493722, -105.2921912106079 40.01114143453822, -105.2921922106798 40.01082443486659, -105.2918546625634 40.01082371352069, -105.2916219709538 40.01082393365192, -105.2915192101345 40.01082443421697, -105.2915172102254 40.01104143452457, -105.2914002106621 40.01099343436549, -105.2913502088046 40.0109674357598, -105.2910521068837 40.01081245315488, -105.2907130561806 40.01063845205723, -105.2904481483452 40.01050448448408, -105.29015521014 40.01039243489431, -105.2900632101764 40.01038843427113, -105.2899932107029 40.01035343447901, -105.2899762105711 40.01037143456766, -105.2896527354281 40.01039073317661, -105.2892512100549 40.01041243440763, -105.2887563243114 40.0104143605715, -105.2887551645736 40.01041517623894, -105.2887237568676 40.01041448734374, -105.2884699572886 40.0104089180808, -105.2873547301276 40.01042634000402, -105.2872221087053 40.01044889807955, -105.287236185778 40.01283899620268, -105.2872368045829 40.01294398630525, -105.2872372028315 40.01294398523873, -105.2872392098854 40.01321143473722, -105.2872452095009 40.01447643612124, -105.2875272095745 40.01524743540963, -105.2871952098002 40.01524243619603, -105.2867662096611 40.01519543586925, -105.285426209528 40.01491443481696, -105.2852132098042 40.01488143563238, -105.2849552084834 40.014861435914, -105.2847062096368 40.01485943573339, -105.2843342088197 40.01488943577559, -105.2840502086252 40.01494043510699, -105.2832492082461 40.01510743623574, -105.2837252085129 40.01657343580141))</t>
+          <t>POLYGON ((-105.28372520851286 40.01657343580141, -105.283771209105 40.016654436576474, -105.28380120907043 40.016862436106734, -105.28379915890659 40.017094131126214, -105.28380892454831 40.01709196535331, -105.28401109813524 40.01704713596685, -105.28410607003526 40.01702607643248, -105.28500886726961 40.01684712918449, -105.28521286421662 40.01680605680808, -105.28653082625777 40.01653288651573, -105.28668125290733 40.01650245354258, -105.28786700670614 40.0162528717229, -105.28854199392984 40.016119837709745, -105.28915510011811 40.015990981839444, -105.2904817987244 40.01572217487955, -105.29164827739994 40.01546871123976, -105.29248388341045 40.01529960385942, -105.29293119345061 40.01520907552712, -105.29326489746909 40.015141538139645, -105.29355222919354 40.01508380053187, -105.29404565583785 40.014984318694154, -105.2941799322994 40.01493717604964, -105.29429624257914 40.014845364926884, -105.29456518475438 40.01463397060598, -105.29480505660418 40.01443646962085, -105.29486694063706 40.01436130597801, -105.29491065257852 40.01428611088715, -105.29491492789886 40.01420590378106, -105.29491116676326 40.014150993387254, -105.29488507093733 40.01404306065437, -105.29482794373129 40.01392601395955, -105.29489509903587 40.013914054779825, -105.29511882860109 40.01383593998661, -105.29558899466441 40.01372696689724, -105.29597201910866 40.01362689650804, -105.29661293798665 40.013483906396, -105.29687012316467 40.01343988732408, -105.29726294009447 40.01340708693889, -105.29728007754596 40.01340711706504, -105.29756498484858 40.01340487234885, -105.2978951689382 40.01342411927098, -105.29815606430208 40.013453125942505, -105.29843617891571 40.01350193131028, -105.29870910695993 40.01356691986554, -105.29897484383618 40.01364891574665, -105.29909716948549 40.013693875069016, -105.2994309509394 40.013825951143026, -105.29968806261716 40.013927969864376, -105.30000116066219 40.014052870692225, -105.30006786814296 40.0140719279547, -105.30025409265298 40.014120016689326, -105.30053599901436 40.014167996854226, -105.30068414968203 40.01417292017293, -105.30083591831364 40.014161102841136, -105.30098417038108 40.014130887043144, -105.30100654396044 40.01412285491573, -105.3010143555852 40.014120436636226, -105.30101465219812 40.014120345281626, -105.30101583022815 40.01400687156732, -105.30101821345626 40.01377743388108, -105.3012511657355 40.01363978016212, -105.30126021220028 40.013634435076284, -105.3013157480595 40.01351102356379, -105.30138621274452 40.01335443432603, -105.30144221272448 40.01298943465143, -105.30144304984366 40.01295818709555, -105.30144378045993 40.012930931943394, -105.30144521297427 40.01287743392142, -105.3014602128255 40.01281143480046, -105.30135221268338 40.01290343407975, -105.30125924576365 40.012981855728775, -105.30120521271697 40.013027434625656, -105.30117894689087 40.013007874933734, -105.30117646673291 40.01300603603117, -105.30117299422044 40.013003481201096, -105.30117294641758 40.013003405463955, -105.30116328417847 40.01299621061416, -105.30114195770462 40.01298029445854, -105.30112027713966 40.012964102089015, -105.30102921260556 40.01289543426423, -105.30102810677789 40.012893064543974, -105.30102334007599 40.012882851039656, -105.3009735379753 40.01278267752139, -105.3009032128719 40.012641433975084, -105.30081174474726 40.01263456076815, -105.3007562324528 40.012630389424736, -105.30072161611075 40.01262785912573, -105.30072162327542 40.01262781230426, -105.3007216280422 40.01262778439228, -105.30048845302179 40.012610201302024, -105.30025181578267 40.01259380600695, -105.29970526728098 40.01255424261292, -105.29936921219429 40.01253043425595, -105.29937530740334 40.01249150609813, -105.29936533658753 40.01249054937211, -105.29948963766081 40.01169225972444, -105.29929270862127 40.011671323755664, -105.29869162385458 40.01160627754996, -105.29860661366064 40.01177065292691, -105.29857184040688 40.01183568677898, -105.29845173554048 40.01181772238958, -105.29812221141096 40.01176843426795, -105.29769121219731 40.01172343446013, -105.2976410500742 40.01171848383155, -105.29753921181562 40.01170843394527, -105.2974892276555 40.01192397025246, -105.29742758380769 40.01218258042406, -105.29742421148386 40.01219643372481, -105.29726247981725 40.012170120683116, -105.29692021145871 40.012114434615434, -105.29692121866508 40.01238543430799, -105.2969222108167 40.01264143451774, -105.2961832109625 40.01252843470885, -105.29580921141903 40.01257043426351, -105.29578521166239 40.012505434981996, -105.2957822123902 40.01218343415776, -105.29546621133909 40.01215043446568, -105.29531321093464 40.01212543471485, -105.2952052115695 40.012134435022524, -105.29480721128711 40.012141434416556, -105.29480721050552 40.01255543418904, -105.29481421084894 40.012670434619984, -105.29421414859111 40.012734664437794, -105.2938052106283 40.01277843517675, -105.29363721130001 40.01280243515163, -105.29355121091945 40.0128564346988, -105.29313335037415 40.0128564352352, -105.29279121019383 40.012856434336626, -105.29269421112603 40.01285243494313, -105.29269810928935 40.012601999584355, -105.29270221132207 40.012338434887376, -105.29310521125096 40.012339434200356, -105.29310597644695 40.012085708520516, -105.29310655018374 40.01189546581841, -105.29310721127112 40.011676433940956, -105.2926421528956 40.0116779178345, -105.29248021027404 40.01167843441603, -105.29247221007883 40.01164043413667, -105.29223121102586 40.01162343450338, -105.29223121101562 40.01149543479373, -105.2921692110959 40.011439434937216, -105.2921912106079 40.01114143453822, -105.29219221067983 40.01082443486659, -105.29185466256342 40.010823713520686, -105.2916219709538 40.01082393365192, -105.29151921013445 40.01082443421697, -105.29151721022536 40.01104143452457, -105.2914002106621 40.01099343436549, -105.29135020880456 40.010967435759795, -105.29105210688373 40.010812453154884, -105.29071305618055 40.01063845205723, -105.29044814834525 40.01050448448408, -105.29015521014001 40.010392434894314, -105.29006321017638 40.01038843427113, -105.28999321070289 40.01035343447901, -105.28997621057111 40.01037143456766, -105.28965273542809 40.01039073317661, -105.2892512100549 40.010412434407634, -105.28875632431138 40.010414360571495, -105.28875516457364 40.01041517623894, -105.28872375686763 40.010414487343745, -105.28846995728863 40.0104089180808, -105.28735473012765 40.010426340004024, -105.28722210870525 40.01044889807955, -105.287236185778 40.01283899620268, -105.28723680458292 40.01294398630525, -105.28723720283148 40.01294398523873, -105.28723920988544 40.013211434737215, -105.28724520950092 40.014476436121235, -105.28752720957448 40.01524743540963, -105.28719520980016 40.01524243619603, -105.28676620966112 40.01519543586925, -105.28542620952801 40.01491443481696, -105.28521320980424 40.01488143563238, -105.28495520848337 40.014861435914, -105.28470620963675 40.01485943573339, -105.28433420881966 40.01488943577559, -105.2840502086252 40.01494043510699, -105.28324920824609 40.015107436235745, -105.28372520851286 40.01657343580141))</t>
         </is>
       </c>
       <c r="H148" t="inlineStr">
@@ -6646,7 +6682,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2790212496877 40.01506431947683, -105.279283131531 40.01582838979826, -105.2792882488983 40.01584331888502, -105.2793182480616 40.01593431868323, -105.2795172500427 40.01656331893992, -105.2796422519211 40.01688331794094, -105.2797922499383 40.0173063188877, -105.2800122511694 40.01792531871845, -105.280344103938 40.01889429097838, -105.2840818920156 40.01812191122571, -105.2839600121989 40.01782410420856, -105.2838869444426 40.01755905605179, -105.2837991589066 40.01709413112621, -105.2838012090704 40.01686243610673, -105.283771209105 40.01665443657647, -105.2837252085129 40.01657343580141, -105.2832492082461 40.01510743623574, -105.2840502086252 40.01494043510699, -105.2843342088197 40.01488943577559, -105.2847062096368 40.01485943573339, -105.2849552084834 40.014861435914, -105.2852132098042 40.01488143563238, -105.285426209528 40.01491443481696, -105.2867662096611 40.01519543586925, -105.2871952098002 40.01524243619603, -105.2875272095745 40.01524743540963, -105.2872452095009 40.01447643612124, -105.2872392098854 40.01321143473722, -105.2872372028315 40.01294398523873, -105.2872368045829 40.01294398630525, -105.2872221087053 40.01044889807955, -105.2873547301276 40.01042634000402, -105.2884699572886 40.0104089180808, -105.2887551645736 40.01041517623894, -105.2887563243114 40.0104143605715, -105.2892512100549 40.01041243440763, -105.2896527354309 40.01039073227599, -105.2899762105711 40.01037143456766, -105.2899932107029 40.01035343447901, -105.2900632101764 40.01038843427113, -105.2901552136538 40.0103924349007, -105.290154209284 40.01034543526126, -105.2906912104696 40.01034743433848, -105.2906906047592 40.01003956613808, -105.2906912103231 40.0098434340922, -105.2906892101524 40.00976243394203, -105.2906902700733 40.00962089482662, -105.2906912943824 40.00945966739491, -105.2906925531651 40.00929912848419, -105.2906932101914 40.00921443417534, -105.2903549358019 40.00921443393288, -105.2900702103074 40.00921343500197, -105.2900712087696 40.00893743474369, -105.2908119707734 40.00893655268581, -105.2914292099533 40.00893843358583, -105.2914292843717 40.00892559132514, -105.2908690869226 40.00844982779828, -105.2907819711598 40.00840996903745, -105.290661065552 40.00825601822979, -105.2904830588015 40.00809702258108, -105.2903059756377 40.00798607001173, -105.2901651591649 40.00792294834658, -105.2900128690378 40.00787600294159, -105.2898541047652 40.00784496816384, -105.2897431274692 40.00782994113508, -105.2896179351386 40.00779402536224, -105.2895010031458 40.00774192810649, -105.289405168331 40.00767888851305, -105.2893250772793 40.0076040727572, -105.2892639375149 40.00751913492665, -105.289223168539 40.00742709573112, -105.2891968309264 40.00728594512627, -105.2891459174028 40.00724192903881, -105.2890970445134 40.00723113361098, -105.2890631285643 40.007231894771, -105.2884758772812 40.00723493682361, -105.2876390732287 40.00724410484807, -105.2872299698913 40.0072430760162, -105.2869468595005 40.00724996565361, -105.2864738555099 40.00724909075706, -105.2855649684075 40.00724905147178, -105.284303060725 40.00723708977463, -105.2831478234024 40.00724700172137, -105.2820611343066 40.00725401178327, -105.2819728960741 40.00727388539485, -105.2819328809913 40.00728396638529, -105.2811321477586 40.00728794062378, -105.2799030378844 40.0072899927621, -105.2798991196525 40.00850391052731, -105.2798981776063 40.0086850911318, -105.2792530928789 40.00868413275619, -105.2786690288632 40.00869097407449, -105.2774331244734 40.00868887001202, -105.2773649345335 40.00869011097444, -105.2763388826292 40.00870596917193, -105.2762321354144 40.00870795787013, -105.2758060111793 40.00874609601551, -105.2758152485927 40.00875931933824, -105.2762812494074 40.00949531960137, -105.2767752494434 40.01022432000386, -105.2769412473638 40.01050232036644, -105.277468250776 40.01146031826774, -105.2775092477175 40.01155231971639, -105.2779272502179 40.01230831848352, -105.2780772507445 40.01258131833099, -105.2782442475646 40.01290131875111, -105.2783382504144 40.01312631838457, -105.2784682507316 40.01347931837473, -105.2786769521653 40.01410055096331, -105.2786822492777 40.01411631803115, -105.278851249496 40.01459531880194, -105.2788752505237 40.01466131864607, -105.2789422504309 40.01484831880367, -105.2790212496877 40.01506431947683))</t>
+          <t>POLYGON ((-105.27902124968774 40.015064319476835, -105.27928313153105 40.01582838979826, -105.27928824889825 40.01584331888502, -105.27931824806156 40.01593431868323, -105.27951725004274 40.016563318939916, -105.2796422519211 40.016883317940945, -105.27979224993825 40.0173063188877, -105.28001225116941 40.01792531871845, -105.28034410393798 40.01889429097838, -105.28408189201564 40.018121911225705, -105.28396001219888 40.01782410420856, -105.28388694444259 40.017559056051795, -105.28379915890659 40.017094131126214, -105.28380120907043 40.016862436106734, -105.283771209105 40.016654436576474, -105.28372520851286 40.01657343580141, -105.28324920824609 40.015107436235745, -105.2840502086252 40.01494043510699, -105.28433420881966 40.01488943577559, -105.28470620963675 40.01485943573339, -105.28495520848337 40.014861435914, -105.28521320980424 40.01488143563238, -105.28542620952801 40.01491443481696, -105.28676620966112 40.01519543586925, -105.28719520980016 40.01524243619603, -105.28752720957448 40.01524743540963, -105.28724520950092 40.014476436121235, -105.28723920988544 40.013211434737215, -105.28723720283148 40.01294398523873, -105.28723680458292 40.01294398630525, -105.28722210870525 40.01044889807955, -105.28735473012765 40.010426340004024, -105.28846995728863 40.0104089180808, -105.28875516457364 40.01041517623894, -105.28875632431138 40.010414360571495, -105.2892512100549 40.010412434407634, -105.28965273543086 40.01039073227599, -105.28997621057111 40.01037143456766, -105.28999321070289 40.01035343447901, -105.29006321017638 40.01038843427113, -105.29015521365379 40.0103924349007, -105.29015420928403 40.01034543526126, -105.2906912104696 40.01034743433848, -105.29069060475925 40.010039566138076, -105.2906912103231 40.009843434092204, -105.29068921015235 40.00976243394203, -105.2906902700733 40.00962089482662, -105.29069129438243 40.00945966739491, -105.29069255316507 40.00929912848419, -105.29069321019138 40.00921443417534, -105.29035493580193 40.009214433932875, -105.29007021030738 40.00921343500197, -105.29007120876958 40.008937434743686, -105.29081197077345 40.00893655268581, -105.29142920995332 40.00893843358583, -105.29142928437169 40.00892559132514, -105.29086908692258 40.00844982779828, -105.29078197115977 40.00840996903745, -105.29066106555204 40.00825601822979, -105.29048305880146 40.00809702258108, -105.29030597563766 40.007986070011725, -105.29016515916486 40.00792294834658, -105.29001286903781 40.007876002941586, -105.28985410476521 40.00784496816384, -105.28974312746922 40.00782994113508, -105.28961793513864 40.007794025362244, -105.28950100314584 40.00774192810649, -105.28940516833096 40.00767888851305, -105.28932507727932 40.0076040727572, -105.28926393751492 40.00751913492665, -105.28922316853901 40.00742709573112, -105.28919683092644 40.00728594512627, -105.28914591740282 40.007241929038805, -105.28909704451344 40.00723113361098, -105.28906312856431 40.007231894770996, -105.2884758772812 40.007234936823615, -105.28763907322869 40.00724410484807, -105.28722996989126 40.007243076016195, -105.28694685950052 40.007249965653614, -105.28647385550994 40.00724909075706, -105.28556496840748 40.00724905147178, -105.28430306072495 40.00723708977463, -105.28314782340243 40.007247001721375, -105.28206113430656 40.007254011783274, -105.28197289607405 40.007273885394845, -105.2819328809913 40.00728396638529, -105.28113214775861 40.007287940623776, -105.27990303788437 40.0072899927621, -105.27989911965251 40.00850391052731, -105.27989817760633 40.0086850911318, -105.27925309287892 40.00868413275619, -105.27866902886316 40.00869097407449, -105.27743312447345 40.00868887001202, -105.27736493453354 40.00869011097444, -105.27633888262925 40.008705969171935, -105.27623213541439 40.00870795787013, -105.27580601117927 40.008746096015514, -105.27581524859272 40.00875931933824, -105.2762812494074 40.00949531960137, -105.27677524944343 40.010224320003864, -105.27694124736375 40.01050232036644, -105.27746825077601 40.011460318267744, -105.27750924771748 40.01155231971639, -105.27792725021787 40.01230831848352, -105.27807725074447 40.01258131833099, -105.27824424756463 40.01290131875111, -105.27833825041438 40.01312631838457, -105.27846825073165 40.01347931837473, -105.27867695216533 40.014100550963306, -105.27868224927768 40.01411631803115, -105.27885124949597 40.014595318801945, -105.27887525052368 40.01466131864607, -105.27894225043093 40.01484831880367, -105.27902124968774 40.015064319476835))</t>
         </is>
       </c>
       <c r="H149" t="inlineStr">
@@ -6688,7 +6724,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2891459174028 40.00724192903881, -105.2891968309264 40.00728594512627, -105.289223168539 40.00742709573112, -105.2892639375149 40.00751913492665, -105.2893250772793 40.0076040727572, -105.289405168331 40.00767888851305, -105.2895010031458 40.00774192810649, -105.2896179351386 40.00779402536224, -105.2897431274692 40.00782994113508, -105.2898541047652 40.00784496816384, -105.2900128690378 40.00787600294159, -105.2901651591649 40.00792294834658, -105.2903059756377 40.00798607001173, -105.2904830588015 40.00809702258108, -105.290661065552 40.00825601822979, -105.2907819711598 40.00840996903745, -105.2908690869226 40.00844982779828, -105.2914292843717 40.00892559132514, -105.2914494441 40.00894271315248, -105.2914413909659 40.00838696663524, -105.291435571172 40.00799368282969, -105.291434505532 40.00792163594929, -105.2914274930992 40.00744731200101, -105.2914243985306 40.00725707878722, -105.2914186624658 40.00655926840435, -105.2914129736189 40.00586750143415, -105.2914128284874 40.0058498573957, -105.2893062940022 40.00585108026677, -105.2893072089034 40.00573843376241, -105.2891862090265 40.00573843417073, -105.289183208523 40.00569143445288, -105.2892542509013 40.00557829378603, -105.2892642092937 40.00556243348697, -105.2892802089861 40.0054494344716, -105.2892701024788 40.00539384846005, -105.2892448616018 40.00525502802683, -105.289222208486 40.0051304336159, -105.2892165752351 40.00502961420859, -105.289210260548 40.00491661583447, -105.2892046483513 40.00481619545184, -105.2892046450271 40.00481613420144, -105.2891990708099 40.00471063150589, -105.2891938451001 40.00461287325479, -105.2891892086024 40.00453743424469, -105.2891906716055 40.00448773442004, -105.2891912095267 40.0044694341479, -105.2895168917593 40.00447009575527, -105.2897786282747 40.00447043362994, -105.2898148558858 40.0044704339242, -105.2902082092732 40.00447143396809, -105.2902102089141 40.00411343370725, -105.2894660313344 40.00410981221352, -105.2891832092096 40.00410843445307, -105.289181013276 40.00397698382579, -105.2891772087631 40.00380443348672, -105.2891702087786 40.00377943388832, -105.2891467731285 40.00375699811492, -105.2891429452346 40.00373938065857, -105.2891412091127 40.0036664336449, -105.2892812090433 40.00366243309112, -105.2893447655934 40.00366262397495, -105.2894523686889 40.00366294659735, -105.2896152085675 40.00366343386199, -105.289770518014 40.00366314161278, -105.2901164327568 40.00366188130267, -105.290862209096 40.00366043353663, -105.290862209305 40.00323495363791, -105.2908622089139 40.0030464335758, -105.2908672093773 40.00300643386311, -105.2908679289755 40.00295776481137, -105.2908692895132 40.00286583498241, -105.2908722090372 40.00266843347151, -105.2913502085469 40.0026694336212, -105.2913492206836 40.00250580399706, -105.2913481910814 40.00233514830476, -105.2913476092056 40.00223863423225, -105.2913463894752 40.00203634457346, -105.2913462769537 40.00201761980421, -105.2913068970221 40.00194598899164, -105.2912431223398 40.00178994627621, -105.2911290832752 40.00149600453362, -105.2910651240601 40.00140008083691, -105.2909818640846 40.00131290798303, -105.2908892513289 40.00124347447206, -105.2908860638731 40.00124108466389, -105.2907490552145 40.00116344842886, -105.2907431735999 40.00116011614801, -105.2906398832182 40.00108608323755, -105.29055304792 40.00100109936883, -105.2904858796778 40.00090489481551, -105.2904390747612 40.00080296305709, -105.2904151097517 40.00070299478965, -105.2904099428142 40.00064204183543, -105.2904188442762 40.00053307364049, -105.2904830814278 40.00030506497129, -105.2905838398758 40.00006708752765, -105.2905880724399 40.00005708986423, -105.2905990409973 40.00003110704095, -105.2896358700064 40.00001308078038, -105.2885510767874 40.00002207724711, -105.2879659082731 40.00006410246323, -105.2877728243598 40.00005606015532, -105.2876621524141 40.0000618961723, -105.2867661455717 40.00006121170582, -105.2866469934847 40.00006112008104, -105.2854190818014 40.00006405708816, -105.284251143358 40.00006489746362, -105.2838849334417 40.00005899595487, -105.2834851123632 40.00006557896818, -105.2834014688553 40.00006695568155, -105.2832483927471 40.00006757407493, -105.2831669050245 40.00006790270817, -105.2831127752968 40.00006780089974, -105.2828547635354 40.00006592736987, -105.2827446929499 40.00006849493339, -105.2825949350523 40.00006821265478, -105.2822084318244 40.00006806235598, -105.2819370370845 40.0000679564938, -105.2810889264481 40.00006799577455, -105.2803721710106 40.00006910409878, -105.2798638671253 40.00007197783349, -105.279646841714 40.00007211177422, -105.278630959455 40.00007400981507, -105.2784039373483 40.00007494632052, -105.2773991366947 40.00007191202165, -105.2761780199424 40.00007092064759, -105.2749419062467 40.00007098586583, -105.2749419141296 40.00007746878211, -105.2749439353011 40.00183587613848, -105.2749439861859 40.0018452979681, -105.2749541445287 40.00371800203029, -105.2761939054203 40.00371410054612, -105.277421161032 40.00371400557973, -105.2774251347819 40.00413704801434, -105.2774248286698 40.00433991763281, -105.2774230429322 40.00488703093239, -105.2774240231571 40.00546187703087, -105.2778681120404 40.00545888939006, -105.2786630827622 40.00546398736055, -105.2798871783135 40.00545699704956, -105.2799030378844 40.0072899927621, -105.2811321477586 40.00728794062378, -105.2819328809913 40.00728396638529, -105.2819728960741 40.00727388539485, -105.2820611343066 40.00725401178327, -105.2831478234024 40.00724700172137, -105.284303060725 40.00723708977463, -105.2855649684075 40.00724905147178, -105.2864738555099 40.00724909075706, -105.2869468595005 40.00724996565361, -105.2872299698913 40.0072430760162, -105.2876390732287 40.00724410484807, -105.2884758772812 40.00723493682361, -105.2890631285643 40.007231894771, -105.2890970445134 40.00723113361098, -105.2891459174028 40.00724192903881))</t>
+          <t>POLYGON ((-105.28914591740282 40.007241929038805, -105.28919683092644 40.00728594512627, -105.28922316853901 40.00742709573112, -105.28926393751492 40.00751913492665, -105.28932507727932 40.0076040727572, -105.28940516833096 40.00767888851305, -105.28950100314584 40.00774192810649, -105.28961793513864 40.007794025362244, -105.28974312746922 40.00782994113508, -105.28985410476521 40.00784496816384, -105.29001286903781 40.007876002941586, -105.29016515916486 40.00792294834658, -105.29030597563766 40.007986070011725, -105.29048305880146 40.00809702258108, -105.29066106555204 40.00825601822979, -105.29078197115977 40.00840996903745, -105.29086908692258 40.00844982779828, -105.29142928437169 40.00892559132514, -105.29144944410001 40.00894271315248, -105.29144139096594 40.00838696663524, -105.29143557117204 40.007993682829685, -105.29143450553198 40.00792163594929, -105.29142749309919 40.00744731200101, -105.29142439853064 40.00725707878722, -105.29141866246584 40.00655926840435, -105.29141297361895 40.00586750143415, -105.29141282848738 40.005849857395695, -105.28930629400216 40.00585108026677, -105.28930720890335 40.00573843376241, -105.28918620902647 40.00573843417073, -105.28918320852303 40.005691434452885, -105.2892542509013 40.00557829378603, -105.28926420929366 40.00556243348697, -105.28928020898609 40.0054494344716, -105.28927010247882 40.00539384846005, -105.28924486160177 40.00525502802683, -105.28922220848595 40.0051304336159, -105.28921657523514 40.00502961420859, -105.28921026054797 40.00491661583447, -105.28920464835129 40.004816195451845, -105.28920464502711 40.00481613420144, -105.28919907080989 40.00471063150589, -105.28919384510014 40.004612873254786, -105.28918920860235 40.00453743424469, -105.28919067160547 40.00448773442004, -105.28919120952675 40.0044694341479, -105.28951689175932 40.004470095755266, -105.28977862827472 40.00447043362994, -105.28981485588578 40.0044704339242, -105.29020820927322 40.004471433968085, -105.29021020891412 40.00411343370725, -105.28946603133438 40.00410981221352, -105.28918320920957 40.004108434453066, -105.28918101327598 40.003976983825794, -105.28917720876309 40.00380443348672, -105.28917020877857 40.00377943388832, -105.28914677312846 40.003756998114916, -105.28914294523457 40.003739380658565, -105.28914120911266 40.0036664336449, -105.28928120904331 40.00366243309112, -105.28934476559341 40.003662623974954, -105.2894523686889 40.00366294659735, -105.28961520856753 40.003663433861995, -105.28977051801397 40.003663141612776, -105.29011643275683 40.00366188130267, -105.290862209096 40.00366043353663, -105.290862209305 40.00323495363791, -105.29086220891392 40.003046433575804, -105.29086720937725 40.003006433863106, -105.29086792897547 40.00295776481137, -105.29086928951321 40.00286583498241, -105.29087220903722 40.002668433471506, -105.29135020854687 40.0026694336212, -105.29134922068359 40.00250580399706, -105.29134819108137 40.00233514830476, -105.29134760920564 40.00223863423225, -105.2913463894752 40.00203634457346, -105.29134627695373 40.00201761980421, -105.29130689702207 40.00194598899164, -105.2912431223398 40.00178994627621, -105.2911290832752 40.00149600453362, -105.29106512406014 40.00140008083691, -105.29098186408459 40.00131290798303, -105.29088925132888 40.001243474472055, -105.29088606387312 40.00124108466389, -105.29074905521453 40.00116344842886, -105.29074317359994 40.001160116148014, -105.29063988321818 40.00108608323755, -105.29055304791996 40.00100109936883, -105.29048587967782 40.000904894815505, -105.29043907476122 40.00080296305709, -105.29041510975173 40.00070299478965, -105.29040994281424 40.000642041835434, -105.29041884427619 40.00053307364049, -105.29048308142782 40.00030506497129, -105.29058383987575 40.000067087527654, -105.29058807243986 40.00005708986423, -105.29059904099726 40.000031107040954, -105.28963587000638 40.00001308078038, -105.28855107678743 40.00002207724711, -105.28796590827314 40.000064102463234, -105.28777282435979 40.000056060155316, -105.2876621524141 40.000061896172305, -105.28676614557169 40.00006121170582, -105.28664699348472 40.00006112008104, -105.28541908180142 40.00006405708816, -105.28425114335796 40.00006489746362, -105.28388493344166 40.00005899595487, -105.2834851123632 40.00006557896818, -105.2834014688553 40.000066955681554, -105.28324839274713 40.000067574074926, -105.28316690502447 40.000067902708174, -105.28311277529676 40.000067800899735, -105.28285476353535 40.00006592736987, -105.28274469294988 40.000068494933394, -105.28259493505229 40.00006821265478, -105.28220843182442 40.00006806235598, -105.28193703708446 40.0000679564938, -105.2810889264481 40.00006799577455, -105.28037217101055 40.00006910409878, -105.27986386712531 40.000071977833485, -105.27964684171397 40.00007211177422, -105.27863095945504 40.000074009815066, -105.27840393734827 40.00007494632052, -105.27739913669468 40.00007191202165, -105.2761780199424 40.000070920647595, -105.27494190624671 40.00007098586583, -105.27494191412961 40.00007746878211, -105.2749439353011 40.00183587613848, -105.2749439861859 40.001845297968096, -105.27495414452875 40.00371800203029, -105.27619390542027 40.00371410054612, -105.27742116103197 40.00371400557973, -105.27742513478188 40.00413704801434, -105.27742482866984 40.00433991763281, -105.27742304293224 40.004887030932395, -105.27742402315705 40.00546187703087, -105.27786811204038 40.005458889390056, -105.27866308276221 40.00546398736055, -105.27988717831353 40.005456997049556, -105.27990303788437 40.0072899927621, -105.28113214775861 40.007287940623776, -105.2819328809913 40.00728396638529, -105.28197289607405 40.007273885394845, -105.28206113430656 40.007254011783274, -105.28314782340243 40.007247001721375, -105.28430306072495 40.00723708977463, -105.28556496840748 40.00724905147178, -105.28647385550994 40.00724909075706, -105.28694685950052 40.007249965653614, -105.28722996989126 40.007243076016195, -105.28763907322869 40.00724410484807, -105.2884758772812 40.007234936823615, -105.28906312856431 40.007231894770996, -105.28909704451344 40.00723113361098, -105.28914591740282 40.007241929038805))</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
@@ -6730,7 +6766,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2716111402284 40.00551027935118, -105.2722611403804 40.00586627888787, -105.2736911402234 40.00667128030472, -105.2742621400523 40.0069772785035, -105.2746310127811 40.00721335853029, -105.2746371404818 40.00721728023854, -105.2746386357653 40.00721845040646, -105.2746462454315 40.00722331979489, -105.2746536622742 40.00722912368327, -105.2746692471074 40.00724132015178, -105.2747272479164 40.00729731986099, -105.2748652461734 40.00743031941985, -105.275157248258 40.0078173185688, -105.2758060111793 40.00874609601551, -105.2762321354144 40.00870795787013, -105.2763388826292 40.00870596917193, -105.2773649345335 40.00869011097444, -105.2774331244734 40.00868887001202, -105.2786690288632 40.00869097407449, -105.2792530928789 40.00868413275619, -105.2798981776063 40.0086850911318, -105.2798991196525 40.00850391052731, -105.2799030378844 40.0072899927621, -105.2798871783135 40.00545699704956, -105.2786630827622 40.00546398736055, -105.2778681120404 40.00545888939006, -105.2774240231571 40.00546187703087, -105.2774230429322 40.00488703093239, -105.2774248286698 40.00433991763281, -105.2774251347819 40.00413704801434, -105.277421161032 40.00371400557973, -105.2761939054203 40.00371410054612, -105.2749541445287 40.00371800203029, -105.2749439861859 40.0018452979681, -105.2749439353011 40.00183587613848, -105.2749419062467 40.00007098586583, -105.2737168453467 40.00007490171039, -105.2724860869347 40.00007495020975, -105.2712538896729 40.0000780026072, -105.2700220559592 40.00007912146844, -105.2687848652311 40.00008103962393, -105.2677639960641 40.0000800858277, -105.2665028856773 40.00008302921293, -105.2650550950247 40.00008502916437, -105.2643058348404 40.00009201025707, -105.2637600945748 40.00008210840647, -105.2637656435806 40.0000901112732, -105.263769138599 40.00008828020039, -105.2637746374994 40.00009621091169, -105.2648501394024 40.0016472790201, -105.265172138007 40.00211927949019, -105.265314139698 40.00228927957695, -105.2654201381661 40.00239728003677, -105.265598137788 40.00254727923986, -105.2657834964632 40.00267885494259, -105.2657911393899 40.00268427978975, -105.2657941935688 40.00268602515451, -105.2659871378317 40.00279627946254, -105.2661961397833 40.00289128012255, -105.2663941397006 40.0029622800261, -105.2671601389595 40.00320627976553, -105.267351138822 40.00325728019524, -105.2676243703217 40.00334934651156, -105.2676271392426 40.00335027976428, -105.2676330588495 40.0033552479871, -105.2677333968445 40.00343945945376, -105.267739140128 40.00344427960884, -105.2677430472131 40.00344595819004, -105.2679671393481 40.00354227935713, -105.268273139198 40.00366227986972, -105.2688041396874 40.00398227958208, -105.2695381402365 40.00443327920139, -105.269724701591 40.00455130870641, -105.2697341397638 40.00455727996897, -105.2698001397925 40.0044902797896, -105.2705538001161 40.00491304065314, -105.2705631401521 40.00491828032208, -105.2716111402284 40.00551027935118))</t>
+          <t>POLYGON ((-105.27161114022844 40.005510279351185, -105.27226114038042 40.00586627888787, -105.27369114022336 40.00667128030472, -105.2742621400523 40.0069772785035, -105.27463101278107 40.007213358530294, -105.27463714048183 40.007217280238535, -105.27463863576531 40.007218450406455, -105.27464624543148 40.00722331979489, -105.27465366227423 40.007229123683274, -105.27466924710741 40.00724132015178, -105.27472724791637 40.00729731986099, -105.27486524617342 40.007430319419846, -105.27515724825803 40.0078173185688, -105.27580601117927 40.008746096015514, -105.27623213541439 40.00870795787013, -105.27633888262925 40.008705969171935, -105.27736493453354 40.00869011097444, -105.27743312447345 40.00868887001202, -105.27866902886316 40.00869097407449, -105.27925309287892 40.00868413275619, -105.27989817760633 40.0086850911318, -105.27989911965251 40.00850391052731, -105.27990303788437 40.0072899927621, -105.27988717831353 40.005456997049556, -105.27866308276221 40.00546398736055, -105.27786811204038 40.005458889390056, -105.27742402315705 40.00546187703087, -105.27742304293224 40.004887030932395, -105.27742482866984 40.00433991763281, -105.27742513478188 40.00413704801434, -105.27742116103197 40.00371400557973, -105.27619390542027 40.00371410054612, -105.27495414452875 40.00371800203029, -105.2749439861859 40.001845297968096, -105.2749439353011 40.00183587613848, -105.27494190624671 40.00007098586583, -105.2737168453467 40.00007490171039, -105.27248608693466 40.00007495020975, -105.27125388967289 40.0000780026072, -105.27002205595919 40.00007912146844, -105.26878486523107 40.00008103962393, -105.26776399606409 40.0000800858277, -105.26650288567726 40.00008302921293, -105.26505509502475 40.00008502916437, -105.26430583484039 40.00009201025707, -105.26376009457483 40.000082108406474, -105.26376564358064 40.000090111273195, -105.263769138599 40.00008828020039, -105.26377463749944 40.00009621091169, -105.2648501394024 40.001647279020105, -105.26517213800705 40.002119279490195, -105.26531413969803 40.00228927957695, -105.26542013816606 40.00239728003677, -105.26559813778803 40.00254727923986, -105.26578349646316 40.002678854942594, -105.26579113938989 40.002684279789754, -105.26579419356877 40.00268602515451, -105.26598713783166 40.00279627946254, -105.2661961397833 40.002891280122554, -105.26639413970064 40.0029622800261, -105.2671601389595 40.00320627976553, -105.267351138822 40.00325728019524, -105.26762437032166 40.00334934651156, -105.26762713924263 40.003350279764284, -105.2676330588495 40.0033552479871, -105.26773339684455 40.00343945945376, -105.26773914012801 40.00344427960884, -105.2677430472131 40.003445958190035, -105.26796713934809 40.003542279357134, -105.26827313919803 40.003662279869715, -105.2688041396874 40.003982279582075, -105.26953814023652 40.004433279201386, -105.26972470159097 40.00455130870641, -105.2697341397638 40.00455727996897, -105.26980013979248 40.0044902797896, -105.27055380011613 40.00491304065314, -105.27056314015212 40.00491828032208, -105.27161114022844 40.005510279351185))</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
@@ -6772,7 +6808,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2537731835135 40.0146261868912, -105.258420544823 40.01462569237854, -105.2630299591908 40.01461696725389, -105.2630753109644 40.01461633090538, -105.2638765422727 40.01460508854388, -105.2646558644589 40.01461288522881, -105.2657616256185 40.01461332253763, -105.2662260626349 40.01461196195721, -105.2678219770818 40.01460804739548, -105.2689819637891 40.01460406242605, -105.270220141546 40.01459912551402, -105.2716550449331 40.01459291590101, -105.2725519067238 40.01458809993736, -105.2736219240902 40.0145838908234, -105.2746458800721 40.01458095527774, -105.2760611408061 40.01457602595389, -105.2764250735946 40.01453802385365, -105.2773539185385 40.01436001199994, -105.2775250367717 40.01432794849211, -105.278005899344 40.01423306829994, -105.2782030961592 40.01419611210767, -105.278663968713 40.01410393231048, -105.2786769521653 40.01410055096331, -105.2784682507316 40.01347931837473, -105.2783382504144 40.01312631838457, -105.2782442475646 40.01290131875111, -105.2780772507445 40.01258131833099, -105.2779272502179 40.01230831848352, -105.2775092477175 40.01155231971639, -105.277468250776 40.01146031826774, -105.2769412473638 40.01050232036644, -105.2767752494434 40.01022432000386, -105.2762812494074 40.00949531960137, -105.2758152485927 40.00875931933824, -105.2758060111793 40.00874609601551, -105.275157248258 40.0078173185688, -105.2748652461734 40.00743031941985, -105.2747272479164 40.00729731986099, -105.2746692471074 40.00724132015178, -105.2746536622742 40.00722912368327, -105.2746462454315 40.00722331979489, -105.2746386357653 40.00721845040646, -105.2746371404818 40.00721728023854, -105.2746310127811 40.00721335853029, -105.2742621400523 40.0069772785035, -105.2736911402234 40.00667128030472, -105.2722611403804 40.00586627888787, -105.2716111402284 40.00551027935118, -105.2705631401521 40.00491828032208, -105.2705538001161 40.00491304065314, -105.2698001397925 40.0044902797896, -105.2697341397638 40.00455727996897, -105.269724701591 40.00455130870641, -105.2695381402365 40.00443327920139, -105.2688041396874 40.00398227958208, -105.268273139198 40.00366227986972, -105.2679671393481 40.00354227935713, -105.2677430472131 40.00344595819004, -105.267739140128 40.00344427960884, -105.2677333968445 40.00343945945376, -105.2676330588495 40.0033552479871, -105.2676271392426 40.00335027976428, -105.2676243703217 40.00334934651156, -105.267351138822 40.00325728019524, -105.2671601389595 40.00320627976553, -105.2663941397006 40.0029622800261, -105.2661961397833 40.00289128012255, -105.2659871378317 40.00279627946254, -105.2657941935688 40.00268602515451, -105.2657911393899 40.00268427978975, -105.2657834964632 40.00267885494259, -105.265598137788 40.00254727923986, -105.2654201381661 40.00239728003677, -105.265314139698 40.00228927957695, -105.265172138007 40.00211927949019, -105.2648501394024 40.0016472790201, -105.2637746374994 40.00009621091169, -105.263769138599 40.00008828020039, -105.2637656435806 40.0000901112732, -105.2636851372977 40.00013227971019, -105.2636677621977 40.00013487760815, -105.2635825036177 40.00014762629726, -105.263577605498 40.00014071094439, -105.2635362436151 40.00008232142758, -105.2635316634515 40.00008266869302, -105.2635271382638 40.00007628008433, -105.2635226869538 40.00007661770653, -105.262564137449 40.0001492804175, -105.2614471376263 40.00025428044938, -105.2613031379176 40.00026628085262, -105.2606671387836 40.00031627988058, -105.2602051376428 40.00033828032775, -105.2597321375767 40.00033028045623, -105.2595041374749 40.0003192800807, -105.2593301393748 40.00027828043822, -105.259251053428 40.00025364728025, -105.2592544037049 40.00038408331039, -105.2589195861169 40.00036267320748, -105.2581675632618 40.00029957202448, -105.2583433547495 40.00053228127841, -105.2584680337078 40.00076130850472, -105.2585687794402 40.00118688281169, -105.2586142067626 40.00148365856045, -105.2586454140996 40.00185904416556, -105.2586436430115 40.00235946687246, -105.2586556382503 40.00290996136781, -105.2586434447849 40.0037284900354, -105.2586430706025 40.00514755563273, -105.2586543381473 40.00721719960971, -105.2586277312311 40.00816795412359, -105.2586278665026 40.00917862640373, -105.2586519120392 40.00939872239886, -105.2586579820996 40.01031022620893, -105.2586461933803 40.01101437225237, -105.2582616960437 40.01101199975422, -105.2581495439637 40.01101231219729, -105.2579311542937 40.01101174589978, -105.2576567124926 40.0110110352899, -105.2575833654388 40.01101084600234, -105.257320369252 40.01101016675749, -105.2570548665784 40.01100947532786, -105.2567832592556 40.01100877131261, -105.2565201237135 40.01100808724684, -105.2561213262367 40.01100705271504, -105.2553495296632 40.01100503785093, -105.253644540834 40.0110005767994, -105.2535030853529 40.01100293505052, -105.2535019003321 40.01119789590327, -105.2535261719986 40.01169290685051, -105.2535630325855 40.01186593254538, -105.2536241596939 40.01204202995962, -105.253715823358 40.01226403757396, -105.2537806712891 40.01248002734037, -105.2538054741536 40.01274848195483, -105.2538081303951 40.01360465598484, -105.2537949903803 40.01406758669711, -105.2537731835135 40.0146261868912), (-105.2782259988166 40.01288899876749, -105.2782434257579 40.01293071174543, -105.2782259265416 40.01288889235155, -105.2782259988166 40.01288899876749))</t>
+          <t>POLYGON ((-105.25377318351349 40.0146261868912, -105.258420544823 40.014625692378544, -105.26302995919076 40.01461696725389, -105.26307531096444 40.014616330905376, -105.2638765422727 40.01460508854388, -105.26465586445893 40.014612885228814, -105.26576162561848 40.01461332253763, -105.26622606263491 40.014611961957215, -105.26782197708182 40.01460804739548, -105.26898196378912 40.01460406242605, -105.27022014154602 40.014599125514025, -105.27165504493307 40.01459291590101, -105.27255190672376 40.014588099937356, -105.27362192409025 40.0145838908234, -105.27464588007207 40.014580955277744, -105.27606114080606 40.01457602595389, -105.2764250735946 40.01453802385365, -105.27735391853847 40.01436001199994, -105.27752503677172 40.01432794849211, -105.278005899344 40.01423306829994, -105.2782030961592 40.01419611210767, -105.27866396871299 40.01410393231048, -105.27867695216533 40.014100550963306, -105.27846825073165 40.01347931837473, -105.27833825041438 40.01312631838457, -105.27824424756463 40.01290131875111, -105.27807725074447 40.01258131833099, -105.27792725021787 40.01230831848352, -105.27750924771748 40.01155231971639, -105.27746825077601 40.011460318267744, -105.27694124736375 40.01050232036644, -105.27677524944343 40.010224320003864, -105.2762812494074 40.00949531960137, -105.27581524859272 40.00875931933824, -105.27580601117927 40.008746096015514, -105.27515724825803 40.0078173185688, -105.27486524617342 40.007430319419846, -105.27472724791637 40.00729731986099, -105.27466924710741 40.00724132015178, -105.27465366227423 40.007229123683274, -105.27464624543148 40.00722331979489, -105.27463863576531 40.007218450406455, -105.27463714048183 40.007217280238535, -105.27463101278107 40.007213358530294, -105.2742621400523 40.0069772785035, -105.27369114022336 40.00667128030472, -105.27226114038042 40.00586627888787, -105.27161114022844 40.005510279351185, -105.27056314015212 40.00491828032208, -105.27055380011613 40.00491304065314, -105.26980013979248 40.0044902797896, -105.2697341397638 40.00455727996897, -105.26972470159097 40.00455130870641, -105.26953814023652 40.004433279201386, -105.2688041396874 40.003982279582075, -105.26827313919803 40.003662279869715, -105.26796713934809 40.003542279357134, -105.2677430472131 40.003445958190035, -105.26773914012801 40.00344427960884, -105.26773339684455 40.00343945945376, -105.2676330588495 40.0033552479871, -105.26762713924263 40.003350279764284, -105.26762437032166 40.00334934651156, -105.267351138822 40.00325728019524, -105.2671601389595 40.00320627976553, -105.26639413970064 40.0029622800261, -105.2661961397833 40.002891280122554, -105.26598713783166 40.00279627946254, -105.26579419356877 40.00268602515451, -105.26579113938989 40.002684279789754, -105.26578349646316 40.002678854942594, -105.26559813778803 40.00254727923986, -105.26542013816606 40.00239728003677, -105.26531413969803 40.00228927957695, -105.26517213800705 40.002119279490195, -105.2648501394024 40.001647279020105, -105.26377463749944 40.00009621091169, -105.263769138599 40.00008828020039, -105.26376564358064 40.000090111273195, -105.2636851372977 40.000132279710186, -105.26366776219774 40.000134877608154, -105.26358250361771 40.000147626297256, -105.26357760549804 40.00014071094439, -105.26353624361508 40.000082321427584, -105.26353166345149 40.00008266869302, -105.26352713826377 40.00007628008433, -105.26352268695379 40.000076617706526, -105.26256413744898 40.0001492804175, -105.26144713762633 40.00025428044938, -105.26130313791761 40.00026628085262, -105.26066713878359 40.00031627988058, -105.26020513764277 40.000338280327746, -105.25973213757672 40.000330280456225, -105.25950413747489 40.000319280080696, -105.25933013937475 40.000278280438216, -105.25925105342797 40.000253647280246, -105.2592544037049 40.00038408331039, -105.25891958611686 40.000362673207476, -105.2581675632618 40.00029957202448, -105.25834335474954 40.00053228127841, -105.25846803370776 40.00076130850472, -105.25856877944018 40.001186882811695, -105.25861420676263 40.001483658560446, -105.25864541409963 40.001859044165556, -105.25864364301147 40.002359466872456, -105.25865563825032 40.002909961367806, -105.25864344478488 40.0037284900354, -105.25864307060247 40.00514755563273, -105.2586543381473 40.00721719960971, -105.25862773123106 40.00816795412359, -105.25862786650265 40.00917862640373, -105.25865191203923 40.009398722398856, -105.25865798209963 40.01031022620893, -105.25864619338034 40.01101437225237, -105.25826169604368 40.01101199975422, -105.2581495439637 40.011012312197295, -105.2579311542937 40.01101174589978, -105.25765671249256 40.011011035289904, -105.2575833654388 40.011010846002335, -105.25732036925204 40.011010166757494, -105.25705486657837 40.01100947532786, -105.25678325925558 40.01100877131261, -105.25652012371349 40.011008087246836, -105.25612132623665 40.01100705271504, -105.25534952966318 40.01100503785093, -105.253644540834 40.0110005767994, -105.25350308535288 40.01100293505052, -105.2535019003321 40.011197895903265, -105.25352617199863 40.01169290685051, -105.25356303258555 40.011865932545376, -105.25362415969387 40.012042029959616, -105.25371582335798 40.012264037573956, -105.25378067128915 40.01248002734037, -105.25380547415362 40.01274848195483, -105.25380813039506 40.013604655984835, -105.25379499038033 40.01406758669711, -105.25377318351349 40.0146261868912), (-105.2782259988166 40.012888998767494, -105.27824342575795 40.012930711745426, -105.2782259265416 40.012888892351555, -105.2782259988166 40.012888998767494))</t>
         </is>
       </c>
       <c r="H152" t="inlineStr">
@@ -6814,7 +6850,7 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2586461933803 40.01101437225237, -105.2586579820996 40.01031022620893, -105.2586519120392 40.00939872239886, -105.2586278665026 40.00917862640373, -105.2586277312311 40.00816795412359, -105.2586543381473 40.00721719960971, -105.2586430706025 40.00514755563273, -105.2586434447849 40.0037284900354, -105.258572133868 40.00373098416479, -105.2583379493246 40.00373488608032, -105.2540440020844 40.00372910138983, -105.2531108838922 40.00373012711088, -105.2531039801196 40.00445402054249, -105.2531010238238 40.00517188259421, -105.2531028651088 40.00594493428408, -105.2531119710475 40.00658513352174, -105.2531470399376 40.00675897970751, -105.253390440773 40.00738013872348, -105.2534580881613 40.00761587168582, -105.2534788384062 40.0077021148444, -105.2535018757067 40.00784711067982, -105.2535111127166 40.00805686367984, -105.2535011689129 40.00823994697006, -105.2535068895725 40.00892900280688, -105.2535061296354 40.01032410969325, -105.2535039273517 40.01086430388367, -105.2535030853529 40.01100293505052, -105.253644540834 40.0110005767994, -105.2553495296632 40.01100503785093, -105.2561213262367 40.01100705271504, -105.2565201237135 40.01100808724684, -105.2567832592556 40.01100877131261, -105.2570548665784 40.01100947532786, -105.257320369252 40.01101016675749, -105.2575833654388 40.01101084600234, -105.2576567124926 40.0110110352899, -105.2579311542937 40.01101174589978, -105.2581495439637 40.01101231219729, -105.2582616960437 40.01101199975422, -105.2586461933803 40.01101437225237))</t>
+          <t>POLYGON ((-105.25864619338034 40.01101437225237, -105.25865798209963 40.01031022620893, -105.25865191203923 40.009398722398856, -105.25862786650265 40.00917862640373, -105.25862773123106 40.00816795412359, -105.2586543381473 40.00721719960971, -105.25864307060247 40.00514755563273, -105.25864344478488 40.0037284900354, -105.25857213386804 40.00373098416479, -105.25833794932456 40.003734886080316, -105.25404400208444 40.00372910138983, -105.25311088389222 40.003730127110884, -105.25310398011958 40.00445402054249, -105.25310102382376 40.00517188259421, -105.25310286510884 40.00594493428408, -105.25311197104755 40.00658513352174, -105.25314703993757 40.006758979707506, -105.25339044077305 40.007380138723484, -105.25345808816127 40.00761587168582, -105.25347883840624 40.0077021148444, -105.25350187570666 40.00784711067982, -105.25351111271657 40.00805686367984, -105.25350116891293 40.008239946970065, -105.25350688957249 40.00892900280688, -105.25350612963537 40.01032410969325, -105.25350392735174 40.01086430388367, -105.25350308535288 40.01100293505052, -105.253644540834 40.0110005767994, -105.25534952966318 40.01100503785093, -105.25612132623665 40.01100705271504, -105.25652012371349 40.011008087246836, -105.25678325925558 40.01100877131261, -105.25705486657837 40.01100947532786, -105.25732036925204 40.011010166757494, -105.2575833654388 40.011010846002335, -105.25765671249256 40.011011035289904, -105.2579311542937 40.01101174589978, -105.2581495439637 40.011012312197295, -105.25826169604368 40.01101199975422, -105.25864619338034 40.01101437225237))</t>
         </is>
       </c>
       <c r="H153" t="inlineStr">
@@ -6856,7 +6892,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2460469422521 40.01457377343792, -105.2465954644375 40.01458212939171, -105.2477575533147 40.0146096980253, -105.2489568317006 40.01463733680855, -105.2501120279116 40.01463197668197, -105.2537731835135 40.0146261868912, -105.2537949903803 40.01406758669711, -105.2538081303951 40.01360465598484, -105.2538054741536 40.01274848195483, -105.2537806712891 40.01248002734037, -105.253715823358 40.01226403757396, -105.2536241596939 40.01204202995962, -105.2535630325855 40.01186593254538, -105.2535261719986 40.01169290685051, -105.2535019003321 40.01119789590327, -105.2535030853529 40.01100293505052, -105.2535039273517 40.01086430388367, -105.2535061296354 40.01032410969325, -105.2535068895725 40.00892900280688, -105.2535011689129 40.00823994697006, -105.2535111127166 40.00805686367984, -105.2535018757067 40.00784711067982, -105.2534788384062 40.0077021148444, -105.2534580881613 40.00761587168582, -105.253390440773 40.00738013872348, -105.2531470399376 40.00675897970751, -105.2531119710475 40.00658513352174, -105.2531028651088 40.00594493428408, -105.2531010238238 40.00517188259421, -105.2531039801196 40.00445402054249, -105.2531108838922 40.00373012711088, -105.2512571503644 40.00372998617799, -105.2507459645829 40.00373190219263, -105.2503311673884 40.00373210269301, -105.2493891330616 40.00373088229632, -105.2492320666852 40.00373109021578, -105.2483739119415 40.00373196590926, -105.2474329370459 40.00373402643322, -105.2465258818805 40.00373395715376, -105.2464109378442 40.00373397911915, -105.2460761014417 40.00373406634042, -105.2456098973364 40.00373495983664, -105.2446710684481 40.00373590466019, -105.2444301101221 40.00373701813933, -105.2437240245236 40.00373792147855, -105.2433099373974 40.00373892239762, -105.2430249973684 40.0037599745659, -105.2424278327316 40.00384291993261, -105.2422009576195 40.0038959441677, -105.2419328825653 40.00398813164567, -105.2411529008695 40.00436494609108, -105.2401951250173 40.00483908383512, -105.2400351798579 40.00501219013716, -105.2396037895222 40.00522099519871, -105.2397183929218 40.00655542897663, -105.2397617504435 40.00716500984186, -105.2397860088713 40.00738069992978, -105.23948896571 40.0073811712716, -105.2394896630826 40.00769466327992, -105.2392875951565 40.00798585798366, -105.2396676925198 40.00852564696019, -105.2400337091165 40.00916902485668, -105.2402477007044 40.00961602752709, -105.2403746926028 40.01006703098007, -105.240420687093 40.01034203277578, -105.2404676781633 40.01073103605304, -105.2403976425554 40.01245704927243, -105.2403911251345 40.01288166363222, -105.2404060976704 40.01320570721274, -105.2404326225197 40.01344005644812, -105.240525230141 40.01384153270504, -105.2406371859685 40.01423433406529, -105.2407671682903 40.01461834492035, -105.2422256658095 40.01457244483336, -105.2432112087095 40.01457106881134, -105.2449033960308 40.01456052644195, -105.2460469422521 40.01457377343792))</t>
+          <t>POLYGON ((-105.24604694225205 40.014573773437924, -105.24659546443755 40.01458212939171, -105.24775755331466 40.0146096980253, -105.24895683170055 40.01463733680855, -105.25011202791158 40.01463197668197, -105.25377318351349 40.0146261868912, -105.25379499038033 40.01406758669711, -105.25380813039506 40.013604655984835, -105.25380547415362 40.01274848195483, -105.25378067128915 40.01248002734037, -105.25371582335798 40.012264037573956, -105.25362415969387 40.012042029959616, -105.25356303258555 40.011865932545376, -105.25352617199863 40.01169290685051, -105.2535019003321 40.011197895903265, -105.25350308535288 40.01100293505052, -105.25350392735174 40.01086430388367, -105.25350612963537 40.01032410969325, -105.25350688957249 40.00892900280688, -105.25350116891293 40.008239946970065, -105.25351111271657 40.00805686367984, -105.25350187570666 40.00784711067982, -105.25347883840624 40.0077021148444, -105.25345808816127 40.00761587168582, -105.25339044077305 40.007380138723484, -105.25314703993757 40.006758979707506, -105.25311197104755 40.00658513352174, -105.25310286510884 40.00594493428408, -105.25310102382376 40.00517188259421, -105.25310398011958 40.00445402054249, -105.25311088389222 40.003730127110884, -105.25125715036444 40.00372998617799, -105.25074596458293 40.003731902192634, -105.25033116738838 40.003732102693014, -105.2493891330616 40.00373088229632, -105.24923206668522 40.00373109021578, -105.24837391194146 40.00373196590926, -105.24743293704586 40.00373402643322, -105.24652588188049 40.003733957153756, -105.24641093784425 40.003733979119154, -105.24607610144173 40.00373406634042, -105.24560989733641 40.00373495983664, -105.24467106844806 40.00373590466019, -105.24443011012212 40.003737018139326, -105.24372402452364 40.00373792147855, -105.2433099373974 40.00373892239762, -105.24302499736841 40.0037599745659, -105.24242783273162 40.00384291993261, -105.24220095761953 40.003895944167695, -105.24193288256534 40.00398813164567, -105.24115290086948 40.00436494609108, -105.24019512501732 40.004839083835115, -105.2400351798579 40.00501219013716, -105.23960378952219 40.00522099519871, -105.23971839292183 40.006555428976625, -105.23976175044352 40.007165009841856, -105.23978600887133 40.00738069992978, -105.23948896570995 40.007381171271604, -105.23948966308264 40.00769466327992, -105.23928759515651 40.007985857983655, -105.23966769251979 40.00852564696019, -105.24003370911646 40.00916902485668, -105.24024770070437 40.00961602752709, -105.2403746926028 40.01006703098007, -105.24042068709304 40.01034203277578, -105.24046767816331 40.010731036053045, -105.24039764255537 40.01245704927243, -105.24039112513454 40.01288166363222, -105.24040609767042 40.01320570721274, -105.24043262251968 40.01344005644812, -105.24052523014103 40.01384153270504, -105.2406371859685 40.014234334065286, -105.24076716829035 40.01461834492035, -105.2422256658095 40.014572444833355, -105.24321120870951 40.014571068811335, -105.24490339603082 40.014560526441954, -105.24604694225205 40.014573773437924))</t>
         </is>
       </c>
       <c r="H154" t="inlineStr">
@@ -6898,7 +6934,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2347807798344 40.00738343141639, -105.2347861480169 40.00743690475733, -105.2347869907763 40.00777099692358, -105.234790177152 40.0085119331571, -105.2347898260397 40.0087859030241, -105.234791105128 40.00928306124879, -105.234791099499 40.00956005178001, -105.2347919282631 40.00971405910673, -105.2347919049999 40.01008713128241, -105.2347920224502 40.01088296410842, -105.2347971303825 40.01168100414004, -105.234789083746 40.01191405305922, -105.2347580306384 40.0120040235386, -105.2346801343823 40.01211310348232, -105.2346271149457 40.01215992443042, -105.2345369057483 40.01222203299974, -105.2346290374364 40.01230789445579, -105.2346709708027 40.01235795377421, -105.2347401519167 40.01247011724447, -105.2347888443759 40.01261792103272, -105.2347980207445 40.01273708322816, -105.234789858508 40.01281612648683, -105.2347951477407 40.01466887101872, -105.234785953114 40.0147380290238, -105.2364884675618 40.01473462743368, -105.2379838714334 40.01472804370003, -105.239268545971 40.01470520202151, -105.2401101703597 40.01465348406194, -105.2407671682903 40.01461834492035, -105.2406371859685 40.01423433406529, -105.240525230141 40.01384153270504, -105.2404326225197 40.01344005644812, -105.2404060976704 40.01320570721274, -105.2403911251345 40.01288166363222, -105.2403976425554 40.01245704927243, -105.2404676781633 40.01073103605304, -105.240420687093 40.01034203277578, -105.2403746926028 40.01006703098007, -105.2402477007044 40.00961602752709, -105.2400337091165 40.00916902485668, -105.2396676925198 40.00852564696019, -105.2392875951565 40.00798585798366, -105.2387427436112 40.00730801166415, -105.2387257436185 40.00728901168986, -105.2383654939881 40.00738287517316, -105.237909376571 40.00738357404163, -105.2347807798344 40.00738343141639))</t>
+          <t>POLYGON ((-105.23478077983441 40.007383431416386, -105.23478614801687 40.007436904757334, -105.23478699077631 40.007770996923576, -105.23479017715201 40.008511933157095, -105.23478982603969 40.0087859030241, -105.23479110512798 40.009283061248794, -105.23479109949899 40.00956005178001, -105.2347919282631 40.009714059106734, -105.23479190499988 40.01008713128241, -105.23479202245024 40.01088296410842, -105.23479713038247 40.01168100414004, -105.234789083746 40.01191405305922, -105.23475803063843 40.0120040235386, -105.23468013438229 40.01211310348232, -105.23462711494572 40.01215992443042, -105.23453690574831 40.012222032999745, -105.23462903743636 40.01230789445579, -105.23467097080271 40.01235795377421, -105.23474015191674 40.01247011724447, -105.23478884437587 40.01261792103272, -105.23479802074452 40.01273708322816, -105.23478985850802 40.01281612648683, -105.23479514774073 40.01466887101872, -105.23478595311404 40.0147380290238, -105.23648846756177 40.014734627433675, -105.23798387143336 40.01472804370003, -105.23926854597097 40.01470520202151, -105.24011017035973 40.01465348406194, -105.24076716829035 40.01461834492035, -105.2406371859685 40.014234334065286, -105.24052523014103 40.01384153270504, -105.24043262251968 40.01344005644812, -105.24040609767042 40.01320570721274, -105.24039112513454 40.01288166363222, -105.24039764255537 40.01245704927243, -105.24046767816331 40.010731036053045, -105.24042068709304 40.01034203277578, -105.2403746926028 40.01006703098007, -105.24024770070437 40.00961602752709, -105.24003370911646 40.00916902485668, -105.23966769251979 40.00852564696019, -105.23928759515651 40.007985857983655, -105.23874274361121 40.00730801166415, -105.23872574361852 40.007289011689856, -105.23836549398806 40.00738287517316, -105.23790937657097 40.007383574041626, -105.23478077983441 40.007383431416386))</t>
         </is>
       </c>
       <c r="H155" t="inlineStr">
@@ -6940,7 +6976,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2319659677214 40.01469691984863, -105.2338293506786 40.01473924403673, -105.234785953114 40.0147380290238, -105.2347951477407 40.01466887101872, -105.234789858508 40.01281612648683, -105.2347980207445 40.01273708322816, -105.2347888443759 40.01261792103272, -105.2347401519167 40.01247011724447, -105.2346709708027 40.01235795377421, -105.2346290374364 40.01230789445579, -105.2345369057483 40.01222203299974, -105.2346271149457 40.01215992443042, -105.2346801343823 40.01211310348232, -105.2347580306384 40.0120040235386, -105.234789083746 40.01191405305922, -105.2347971303825 40.01168100414004, -105.2347920224502 40.01088296410842, -105.2347919049999 40.01008713128241, -105.2347919282631 40.00971405910673, -105.234791099499 40.00956005178001, -105.234791105128 40.00928306124879, -105.2347898260397 40.0087859030241, -105.234790177152 40.0085119331571, -105.2347869907763 40.00777099692358, -105.2347861480169 40.00743690475733, -105.2347807798344 40.00738343141639, -105.2346783761087 40.00738394068345, -105.2346198625271 40.00738384746584, -105.2340253218562 40.00738291357975, -105.2336299662758 40.007382300914, -105.2325721352162 40.00738065588258, -105.2319770120331 40.00738251381947, -105.2316875845155 40.00738344390084, -105.231475230575 40.007384234829, -105.2314109936904 40.00738432930238, -105.2311356759831 40.00738521070436, -105.2308672814088 40.00738607068052, -105.2305913159967 40.00738695287374, -105.2303184081062 40.00738648427205, -105.2298925137825 40.00738331597374, -105.2291767246352 40.00737900718899, -105.2284624124079 40.00737383010913, -105.2280982082051 40.00737103100143, -105.2275036335946 40.00736776314012, -105.2269887934874 40.00736789905334, -105.2265732467347 40.00737299478353, -105.2254955104332 40.00737263364671, -105.2253705412734 40.00737273507742, -105.2253710771084 40.00740690445893, -105.2253779332292 40.00800894302443, -105.2256670714257 40.00801512163429, -105.225768878845 40.0079988926334, -105.2261411768403 40.00783204594692, -105.2261879939317 40.00781898055843, -105.2263458679567 40.00779794227783, -105.2264839909668 40.00780595705876, -105.2273631422155 40.00792388558138, -105.2277578650019 40.00795089747909, -105.2283318942658 40.00795389855885, -105.2287739630372 40.00792501676322, -105.2288811080015 40.00791291535942, -105.2291229407293 40.00787505099355, -105.2295851797194 40.00780091689289, -105.2298469758819 40.00776996080432, -105.2301290247384 40.00776293505575, -105.2301288653482 40.00852500114549, -105.2301379433825 40.00929807046362, -105.2301430672563 40.01007799344709, -105.230138116363 40.01087793233127, -105.2301469262573 40.0113580876576, -105.2301371693739 40.01183902271003, -105.2301780012011 40.01198598688668, -105.2302581399472 40.01212398332255, -105.2303718973232 40.012246959756, -105.2305171550157 40.01234887135718, -105.2306411542193 40.01241010465385, -105.2308219353433 40.01246707698136, -105.2310149740053 40.01249388141499, -105.2311988428679 40.01249211434547, -105.2319429004521 40.01248204139353, -105.2319810815714 40.01248707202062, -105.2321098265489 40.01252196075033, -105.2322138572192 40.01257710618241, -105.2322889323139 40.01264206717271, -105.2323489275755 40.01272895464211, -105.232207034409 40.01286011969522, -105.2321119494098 40.01298096195091, -105.2320389649344 40.01311091515174, -105.2319811230555 40.01329388531928, -105.2319670011355 40.01343495511924, -105.2319679002225 40.01347888025946, -105.2319650275997 40.01448196871915, -105.2319751403845 40.01463407558799, -105.2319659677214 40.01469691984863))</t>
+          <t>POLYGON ((-105.23196596772144 40.01469691984863, -105.2338293506786 40.01473924403673, -105.23478595311404 40.0147380290238, -105.23479514774073 40.01466887101872, -105.23478985850802 40.01281612648683, -105.23479802074452 40.01273708322816, -105.23478884437587 40.01261792103272, -105.23474015191674 40.01247011724447, -105.23467097080271 40.01235795377421, -105.23462903743636 40.01230789445579, -105.23453690574831 40.012222032999745, -105.23462711494572 40.01215992443042, -105.23468013438229 40.01211310348232, -105.23475803063843 40.0120040235386, -105.234789083746 40.01191405305922, -105.23479713038247 40.01168100414004, -105.23479202245024 40.01088296410842, -105.23479190499988 40.01008713128241, -105.2347919282631 40.009714059106734, -105.23479109949899 40.00956005178001, -105.23479110512798 40.009283061248794, -105.23478982603969 40.0087859030241, -105.23479017715201 40.008511933157095, -105.23478699077631 40.007770996923576, -105.23478614801687 40.007436904757334, -105.23478077983441 40.007383431416386, -105.23467837610872 40.00738394068345, -105.23461986252707 40.00738384746584, -105.23402532185622 40.00738291357975, -105.2336299662758 40.007382300914, -105.23257213521616 40.00738065588258, -105.23197701203313 40.00738251381947, -105.23168758451548 40.00738344390084, -105.23147523057496 40.007384234829004, -105.23141099369043 40.00738432930238, -105.23113567598311 40.007385210704356, -105.23086728140876 40.00738607068052, -105.23059131599668 40.00738695287374, -105.23031840810623 40.00738648427205, -105.2298925137825 40.00738331597374, -105.22917672463515 40.00737900718899, -105.22846241240794 40.00737383010913, -105.22809820820507 40.00737103100143, -105.22750363359458 40.007367763140124, -105.22698879348744 40.00736789905334, -105.22657324673467 40.00737299478353, -105.22549551043322 40.00737263364671, -105.22537054127343 40.007372735077425, -105.22537107710842 40.00740690445893, -105.22537793322918 40.00800894302443, -105.22566707142572 40.008015121634294, -105.22576887884497 40.0079988926334, -105.2261411768403 40.00783204594692, -105.22618799393169 40.00781898055843, -105.22634586795671 40.007797942277826, -105.22648399096678 40.007805957058764, -105.22736314221552 40.00792388558138, -105.22775786500189 40.00795089747909, -105.22833189426584 40.007953898558846, -105.22877396303724 40.007925016763224, -105.22888110800149 40.00791291535942, -105.22912294072927 40.00787505099355, -105.22958517971936 40.00780091689289, -105.22984697588187 40.007769960804325, -105.23012902473839 40.00776293505575, -105.23012886534816 40.00852500114549, -105.23013794338252 40.00929807046362, -105.23014306725628 40.01007799344709, -105.23013811636298 40.01087793233127, -105.23014692625733 40.0113580876576, -105.23013716937392 40.01183902271003, -105.23017800120114 40.01198598688668, -105.23025813994721 40.012123983322546, -105.23037189732315 40.012246959756, -105.23051715501566 40.012348871357176, -105.23064115421933 40.01241010465385, -105.23082193534327 40.01246707698136, -105.23101497400532 40.01249388141499, -105.2311988428679 40.01249211434547, -105.23194290045205 40.012482041393525, -105.2319810815714 40.01248707202062, -105.23210982654888 40.012521960750334, -105.23221385721924 40.01257710618241, -105.23228893231386 40.01264206717271, -105.23234892757547 40.012728954642114, -105.23220703440904 40.01286011969522, -105.23211194940984 40.01298096195091, -105.23203896493438 40.01311091515174, -105.23198112305548 40.01329388531928, -105.23196700113554 40.013434955119244, -105.23196790022251 40.013478880259456, -105.23196502759971 40.01448196871915, -105.23197514038453 40.01463407558799, -105.23196596772144 40.01469691984863))</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
@@ -6982,7 +7018,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2254128747107 40.01466887521181, -105.2254145473955 40.01466887288986, -105.2258513852783 40.01466824594888, -105.2272090327501 40.01466628746812, -105.2281480626285 40.01466492383204, -105.22915700892 40.01466702306828, -105.230058133229 40.01466913584839, -105.2309519694455 40.01468609977, -105.2319659677214 40.01469691984863, -105.2319751403845 40.01463407558799, -105.2319650275997 40.01448196871915, -105.2319679002225 40.01347888025946, -105.2319670011355 40.01343495511924, -105.2319811230555 40.01329388531928, -105.2320389649344 40.01311091515174, -105.2321119494098 40.01298096195091, -105.232207034409 40.01286011969522, -105.2323489275755 40.01272895464211, -105.2322889323139 40.01264206717271, -105.2322138572192 40.01257710618241, -105.2321098265489 40.01252196075033, -105.2319810815714 40.01248707202062, -105.2319429004521 40.01248204139353, -105.2311988428679 40.01249211434547, -105.2310149740053 40.01249388141499, -105.2308219353433 40.01246707698136, -105.2306411542193 40.01241010465385, -105.2305171550157 40.01234887135718, -105.2303718973232 40.012246959756, -105.2302581399472 40.01212398332255, -105.2301780012011 40.01198598688668, -105.2301371693739 40.01183902271003, -105.2301469262573 40.0113580876576, -105.230138116363 40.01087793233127, -105.2301430672563 40.01007799344709, -105.2301379433825 40.00929807046362, -105.2301288653482 40.00852500114549, -105.2301290247384 40.00776293505575, -105.2298469758819 40.00776996080432, -105.2295851797194 40.00780091689289, -105.2291229407293 40.00787505099355, -105.2288811080015 40.00791291535942, -105.2287739630372 40.00792501676322, -105.2283318942658 40.00795389855885, -105.2277578650019 40.00795089747909, -105.2273631422155 40.00792388558138, -105.2264839909668 40.00780595705876, -105.2263458679567 40.00779794227783, -105.2261879939317 40.00781898055843, -105.2261411768403 40.00783204594692, -105.225768878845 40.0079988926334, -105.2256670714257 40.00801512163429, -105.2253779332292 40.00800894302443, -105.2253839389156 40.00846795481117, -105.2253838330693 40.00955807248677, -105.2253821431884 40.01042088382555, -105.2253810146688 40.01096690145793, -105.2253809092057 40.01152499925985, -105.2253813324297 40.01154118861345, -105.2254553697515 40.01153734978604, -105.2259894631732 40.01154280090893, -105.2259836905349 40.01179242401184, -105.2254566798614 40.01178766431855, -105.225388537699 40.01178677074186, -105.2254010518784 40.01210812757141, -105.2254141427847 40.01249193706877, -105.2254161363436 40.01279501167843, -105.2254189417418 40.0131620508104, -105.2254209804249 40.0133649260246, -105.2254189733863 40.0135090437885, -105.225417110159 40.01370586992432, -105.2254160606848 40.01378904725933, -105.2254141322162 40.01400206968174, -105.2254131321368 40.01451624302689, -105.2254128747107 40.01466887521181))</t>
+          <t>POLYGON ((-105.22541287471071 40.01466887521181, -105.22541454739553 40.014668872889864, -105.2258513852783 40.014668245948876, -105.2272090327501 40.014666287468124, -105.22814806262855 40.01466492383204, -105.22915700892003 40.01466702306828, -105.23005813322901 40.014669135848386, -105.23095196944553 40.01468609977, -105.23196596772144 40.01469691984863, -105.23197514038453 40.01463407558799, -105.23196502759971 40.01448196871915, -105.23196790022251 40.013478880259456, -105.23196700113554 40.013434955119244, -105.23198112305548 40.01329388531928, -105.23203896493438 40.01311091515174, -105.23211194940984 40.01298096195091, -105.23220703440904 40.01286011969522, -105.23234892757547 40.012728954642114, -105.23228893231386 40.01264206717271, -105.23221385721924 40.01257710618241, -105.23210982654888 40.012521960750334, -105.2319810815714 40.01248707202062, -105.23194290045205 40.012482041393525, -105.2311988428679 40.01249211434547, -105.23101497400532 40.01249388141499, -105.23082193534327 40.01246707698136, -105.23064115421933 40.01241010465385, -105.23051715501566 40.012348871357176, -105.23037189732315 40.012246959756, -105.23025813994721 40.012123983322546, -105.23017800120114 40.01198598688668, -105.23013716937392 40.01183902271003, -105.23014692625733 40.0113580876576, -105.23013811636298 40.01087793233127, -105.23014306725628 40.01007799344709, -105.23013794338252 40.00929807046362, -105.23012886534816 40.00852500114549, -105.23012902473839 40.00776293505575, -105.22984697588187 40.007769960804325, -105.22958517971936 40.00780091689289, -105.22912294072927 40.00787505099355, -105.22888110800149 40.00791291535942, -105.22877396303724 40.007925016763224, -105.22833189426584 40.007953898558846, -105.22775786500189 40.00795089747909, -105.22736314221552 40.00792388558138, -105.22648399096678 40.007805957058764, -105.22634586795671 40.007797942277826, -105.22618799393169 40.00781898055843, -105.2261411768403 40.00783204594692, -105.22576887884497 40.0079988926334, -105.22566707142572 40.008015121634294, -105.22537793322918 40.00800894302443, -105.2253839389156 40.008467954811174, -105.22538383306933 40.00955807248677, -105.22538214318843 40.01042088382555, -105.22538101466881 40.01096690145793, -105.22538090920571 40.01152499925985, -105.22538133242973 40.01154118861345, -105.22545536975151 40.01153734978604, -105.22598946317318 40.01154280090893, -105.22598369053495 40.011792424011844, -105.22545667986141 40.011787664318554, -105.22538853769896 40.01178677074186, -105.22540105187835 40.01210812757141, -105.22541414278471 40.012491937068766, -105.22541613634363 40.01279501167843, -105.2254189417418 40.0131620508104, -105.22542098042493 40.0133649260246, -105.22541897338625 40.0135090437885, -105.22541711015901 40.01370586992432, -105.22541606068484 40.01378904725933, -105.22541413221622 40.014002069681744, -105.22541313213682 40.01451624302689, -105.22541287471071 40.01466887521181))</t>
         </is>
       </c>
       <c r="H157" t="inlineStr">
@@ -7024,7 +7060,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2130940324873 40.01467594647242, -105.2130969381798 40.01474897599216, -105.2130981903515 40.01474897460401, -105.2141074361257 40.0147478477099, -105.2148764361527 40.01473067926249, -105.2148910155936 40.01473046222324, -105.2157340623453 40.01471789690481, -105.215735902945 40.01471779606526, -105.2164723909476 40.01467739814613, -105.2164899016262 40.01467620189562, -105.217100941391 40.01463444043784, -105.2191844656205 40.01463953261158, -105.2239170504272 40.01464087196651, -105.2245834902002 40.0146398382582, -105.2254128747107 40.01466887521181, -105.2254131321368 40.01451624302689, -105.2254141322162 40.01400206968174, -105.2254160606848 40.01378904725933, -105.225417110159 40.01370586992432, -105.2254189733863 40.0135090437885, -105.2254209804249 40.0133649260246, -105.2254189417418 40.0131620508104, -105.2254161363436 40.01279501167843, -105.2254141427847 40.01249193706877, -105.2254010518784 40.01210812757141, -105.225388537699 40.01178677074186, -105.2254566798614 40.01178766431855, -105.2259836905349 40.01179242401184, -105.2259894631732 40.01154280090893, -105.2254553697515 40.01153734978604, -105.2253813324297 40.01154118861345, -105.2253809092057 40.01152499925985, -105.2253810146688 40.01096690145793, -105.2253821431884 40.01042088382555, -105.2253838330693 40.00955807248677, -105.2253839389156 40.00846795481117, -105.2253779332292 40.00800894302443, -105.2253710771084 40.00740690445893, -105.2253705412734 40.00737273507742, -105.2254955104332 40.00737263364671, -105.2265732467347 40.00737299478353, -105.2269887934874 40.00736789905334, -105.2275036335946 40.00736776314012, -105.2280982082051 40.00737103100143, -105.2284624124079 40.00737383010913, -105.2291767246352 40.00737900718899, -105.2298925137825 40.00738331597374, -105.2303184081062 40.00738648427205, -105.2305913159967 40.00738695287374, -105.2308672814088 40.00738607068052, -105.2311356759831 40.00738521070436, -105.2314109936904 40.00738432930238, -105.231475230575 40.007384234829, -105.2316875845155 40.00738344390084, -105.2319770120331 40.00738251381947, -105.2325721352162 40.00738065588258, -105.2336299662758 40.007382300914, -105.233617310355 40.00712050301013, -105.2335795972293 40.00658094596193, -105.2335708506883 40.00653178608862, -105.2325454181118 40.00653003820529, -105.2299623249569 40.0065233425341, -105.2289009910103 40.00652057480598, -105.2265688248415 40.00650301211288, -105.2256249335607 40.00651010353371, -105.2253661145294 40.00651154719828, -105.225369874075 40.00557805082113, -105.2253701681565 40.00550502919539, -105.2253711764782 40.00534306428025, -105.2253711554255 40.00525988522655, -105.2253710525624 40.00519702022958, -105.2253689488286 40.00483300146669, -105.2253670471577 40.0042411320881, -105.2253659339144 40.00345408017876, -105.2253670051872 40.00318807360595, -105.2253628226623 40.00289707216505, -105.2253588845966 40.00263407263947, -105.2253539877582 40.00234306948083, -105.2253430917478 40.00176902229651, -105.2253421681761 40.00137810367464, -105.2253431400887 40.00131386861644, -105.2253478593084 40.00076291802563, -105.2253502088998 40.00051594885953, -105.225354046752 40.00011286918626, -105.2253349559493 39.99909188404666, -105.2253319626453 39.99894912586416, -105.2252859486925 39.99876399025853, -105.2252498335415 39.99869088182842, -105.2251459824802 39.99850890201741, -105.2250469054067 39.9983829352995, -105.2248858227375 39.99823101590031, -105.2247950790052 39.99816299355049, -105.2246470892445 39.99803992961618, -105.224555062579 39.99793594086837, -105.224480917112 39.99782293599132, -105.2244140993091 39.99766410345214, -105.224398994631 39.99760394774227, -105.2243878308265 39.99753995745615, -105.224380027552 39.99655605899623, -105.2243809144956 39.99580689549131, -105.2243759286585 39.99492100747396, -105.224383933816 39.99426492285259, -105.2243818903101 39.99353387065675, -105.224373066493 39.99333290079716, -105.224373995855 39.99318290251038, -105.2269704853094 39.99317677606326, -105.2269745738349 39.99240084977456, -105.2269697053404 39.99030109572695, -105.2269656014882 39.98939425758067, -105.2269729632646 39.98860175680049, -105.2269788017231 39.98690004958741, -105.2269848063165 39.98666212230915, -105.2269904941112 39.98643693044628, -105.2269992934832 39.98608841196461, -105.2270013766576 39.98600585559555, -105.2259757261998 39.98599553233836, -105.2254644467161 39.98600197681813, -105.2245736987022 39.98600863702274, -105.2239582758726 39.98601323449112, -105.2237453083268 39.98601482465087, -105.223084657606 39.98601975668618, -105.2222353497503 39.98602247873587, -105.222234990267 39.98609839414738, -105.2206616558601 39.98611582894792, -105.2206587622344 39.98604446297291, -105.2185404142695 39.98606441335764, -105.2159614741359 39.98608864702656, -105.2129348461996 39.986122924, -105.2128408265147 39.98613467486216, -105.2128409991863 39.98614399888426, -105.2128199983129 39.98714499875833, -105.212819999065 39.9874409984555, -105.212820998313 39.98749399914585, -105.2128209981865 39.98794399929118, -105.2128229998723 39.98972899884425, -105.2127899996551 39.99032999898677, -105.2127249983793 39.99099299884455, -105.2126889998817 39.99139699911375, -105.2126539990297 39.99178199891079, -105.2125093588739 39.99318486329975, -105.2124779991473 39.99348899860376, -105.2124601767598 39.99431311694229, -105.2124740351865 39.99470038739478, -105.2124983315102 39.99518419448454, -105.2124925687887 39.99544869177733, -105.2124961767938 39.99569533982743, -105.2125139076481 39.9958991302809, -105.2126006533221 39.99626870887596, -105.2126844006306 39.99661445128344, -105.2127449818323 39.99692495901152, -105.2127440001071 39.99692699925155, -105.2127469993367 39.99716299909484, -105.2127455277946 39.99746149416151, -105.2127389991961 39.99878599927126, -105.2127392146961 39.99881852246104, -105.2127459994442 39.99984399810055, -105.2127829993984 40.00004099865892, -105.2127928656112 40.00007553362977, -105.2127969995393 40.00008999943838, -105.2128159836817 40.00024499989686, -105.2128159972606 40.00024511251258, -105.2128050001144 40.00042099923211, -105.2127818519077 40.00052534458408, -105.2127399996955 40.00071399866724, -105.2125852425582 40.00147525356017, -105.2125669991999 40.00156493581707, -105.212566988398 40.00156499793533, -105.2125269999105 40.00195299848955, -105.2125161427577 40.00307331652181, -105.2125117588774 40.00352564947486, -105.2117791909032 40.00354043954807, -105.2117761908399 40.0030044389501, -105.2111441915764 40.00300243863417, -105.2111711906653 40.00325443919979, -105.2111551901976 40.00343643944229, -105.21103119153 40.00352344002083, -105.2110311909939 40.00371343942365, -105.2125107894076 40.00369755140002, -105.2125059976708 40.00582199879766, -105.2125054826385 40.00647891950867, -105.2125049987698 40.00709399945863, -105.2125429989301 40.00731899837689, -105.2125739999607 40.00741399830913, -105.2126529828366 40.00758894189271, -105.2126530118967 40.00758899420312, -105.2128859992807 40.00799899844429, -105.2129235378465 40.00809508272722, -105.2129700000606 40.00821399827627, -105.2129869521706 40.00829726722127, -105.213003999585 40.0083809993364, -105.2130112852478 40.00853642174128, -105.2130189997407 40.00870099855842, -105.2130219999797 40.00890899948654, -105.2130219996678 40.00906603303326, -105.2130219997471 40.00935599951865, -105.2129829998411 40.0095709993631, -105.2129829986977 40.0095865752715, -105.2129829999123 40.00961299956395, -105.2130060003659 40.00974199894547, -105.2130180708937 40.00983143781237, -105.2130280004494 40.00990499912331, -105.2130312388504 40.01016524665692, -105.2130440003177 40.01119099898076, -105.2130454473815 40.01133281594282, -105.2130460006044 40.01138699885649, -105.2130529986013 40.01186999911342, -105.2130589996108 40.01220499962974, -105.2130592574697 40.01222416348261, -105.213064157268 40.01258789120162, -105.2130673059102 40.01280105946651, -105.2130736861623 40.01323274517098, -105.2130740693893 40.01339608598071, -105.2130777016322 40.01363575086111, -105.2130940324873 40.01467594647242))</t>
+          <t>POLYGON ((-105.21309403248726 40.014675946472416, -105.21309693817976 40.014748975992156, -105.21309819035152 40.01474897460401, -105.21410743612572 40.0147478477099, -105.21487643615265 40.01473067926249, -105.21489101559357 40.01473046222324, -105.2157340623453 40.01471789690481, -105.21573590294497 40.01471779606526, -105.21647239094757 40.01467739814613, -105.2164899016262 40.01467620189562, -105.21710094139102 40.01463444043784, -105.21918446562049 40.01463953261158, -105.22391705042719 40.014640871966506, -105.22458349020025 40.0146398382582, -105.22541287471071 40.01466887521181, -105.22541313213682 40.01451624302689, -105.22541413221622 40.014002069681744, -105.22541606068484 40.01378904725933, -105.22541711015901 40.01370586992432, -105.22541897338625 40.0135090437885, -105.22542098042493 40.0133649260246, -105.2254189417418 40.0131620508104, -105.22541613634363 40.01279501167843, -105.22541414278471 40.012491937068766, -105.22540105187835 40.01210812757141, -105.22538853769896 40.01178677074186, -105.22545667986141 40.011787664318554, -105.22598369053495 40.011792424011844, -105.22598946317318 40.01154280090893, -105.22545536975151 40.01153734978604, -105.22538133242973 40.01154118861345, -105.22538090920571 40.01152499925985, -105.22538101466881 40.01096690145793, -105.22538214318843 40.01042088382555, -105.22538383306933 40.00955807248677, -105.2253839389156 40.008467954811174, -105.22537793322918 40.00800894302443, -105.22537107710842 40.00740690445893, -105.22537054127343 40.007372735077425, -105.22549551043322 40.00737263364671, -105.22657324673467 40.00737299478353, -105.22698879348744 40.00736789905334, -105.22750363359458 40.007367763140124, -105.22809820820507 40.00737103100143, -105.22846241240794 40.00737383010913, -105.22917672463515 40.00737900718899, -105.2298925137825 40.00738331597374, -105.23031840810623 40.00738648427205, -105.23059131599668 40.00738695287374, -105.23086728140876 40.00738607068052, -105.23113567598311 40.007385210704356, -105.23141099369043 40.00738432930238, -105.23147523057496 40.007384234829004, -105.23168758451548 40.00738344390084, -105.23197701203313 40.00738251381947, -105.23257213521616 40.00738065588258, -105.2336299662758 40.007382300914, -105.23361731035496 40.00712050301013, -105.23357959722934 40.00658094596193, -105.23357085068831 40.00653178608862, -105.23254541811183 40.00653003820529, -105.22996232495693 40.0065233425341, -105.22890099101032 40.006520574805975, -105.22656882484154 40.00650301211288, -105.22562493356068 40.00651010353371, -105.2253661145294 40.00651154719828, -105.22536987407497 40.00557805082113, -105.22537016815653 40.00550502919539, -105.22537117647816 40.00534306428025, -105.22537115542546 40.00525988522655, -105.22537105256237 40.00519702022958, -105.22536894882857 40.004833001466686, -105.22536704715769 40.004241132088104, -105.22536593391445 40.003454080178756, -105.22536700518715 40.003188073605955, -105.22536282266232 40.00289707216505, -105.22535888459663 40.00263407263947, -105.2253539877582 40.00234306948083, -105.22534309174783 40.001769022296514, -105.22534216817614 40.00137810367464, -105.22534314008868 40.00131386861644, -105.22534785930836 40.00076291802563, -105.22535020889977 40.00051594885953, -105.22535404675197 40.00011286918626, -105.22533495594931 39.99909188404666, -105.22533196264533 39.998949125864165, -105.22528594869246 39.99876399025853, -105.22524983354145 39.998690881828416, -105.22514598248017 39.99850890201741, -105.22504690540674 39.9983829352995, -105.22488582273748 39.99823101590031, -105.22479507900516 39.99816299355049, -105.22464708924446 39.99803992961618, -105.22455506257897 39.997935940868366, -105.22448091711205 39.99782293599132, -105.22441409930909 39.99766410345214, -105.22439899463099 39.99760394774227, -105.22438783082652 39.99753995745615, -105.22438002755204 39.99655605899623, -105.22438091449563 39.99580689549131, -105.22437592865846 39.994921007473955, -105.22438393381603 39.994264922852594, -105.22438189031013 39.99353387065675, -105.22437306649297 39.993332900797164, -105.22437399585502 39.99318290251038, -105.22697048530941 39.99317677606326, -105.22697457383491 39.99240084977456, -105.22696970534042 39.99030109572695, -105.22696560148822 39.98939425758067, -105.22697296326457 39.98860175680049, -105.22697880172308 39.98690004958741, -105.22698480631654 39.98666212230915, -105.22699049411118 39.98643693044628, -105.2269992934832 39.98608841196461, -105.22700137665757 39.98600585559555, -105.22597572619978 39.985995532338364, -105.22546444671612 39.98600197681813, -105.22457369870224 39.98600863702274, -105.22395827587256 39.98601323449112, -105.22374530832681 39.98601482465087, -105.223084657606 39.98601975668618, -105.22223534975033 39.98602247873587, -105.22223499026695 39.986098394147376, -105.22066165586011 39.986115828947916, -105.22065876223436 39.986044462972906, -105.21854041426948 39.98606441335764, -105.21596147413587 39.98608864702656, -105.2129348461996 39.986122924, -105.21284082651475 39.98613467486216, -105.21284099918626 39.98614399888426, -105.21281999831294 39.98714499875833, -105.21281999906496 39.987440998455504, -105.212820998313 39.987493999145855, -105.2128209981865 39.98794399929118, -105.2128229998723 39.98972899884425, -105.2127899996551 39.990329998986766, -105.21272499837931 39.99099299884455, -105.21268899988175 39.991396999113746, -105.21265399902974 39.99178199891079, -105.21250935887393 39.99318486329975, -105.2124779991473 39.99348899860376, -105.2124601767598 39.99431311694229, -105.21247403518655 39.99470038739478, -105.21249833151022 39.99518419448454, -105.2124925687887 39.99544869177733, -105.21249617679379 39.99569533982743, -105.21251390764806 39.995899130280904, -105.2126006533221 39.99626870887596, -105.21268440063064 39.99661445128344, -105.21274498183229 39.996924959011515, -105.21274400010705 39.99692699925155, -105.21274699933667 39.99716299909484, -105.21274552779455 39.997461494161506, -105.2127389991961 39.99878599927126, -105.21273921469607 39.99881852246104, -105.2127459994442 39.99984399810055, -105.21278299939843 40.00004099865892, -105.2127928656112 40.00007553362977, -105.21279699953932 40.00008999943838, -105.21281598368172 40.00024499989686, -105.21281599726058 40.00024511251258, -105.2128050001144 40.000420999232105, -105.21278185190766 40.000525344584084, -105.21273999969553 40.000713998667244, -105.21258524255825 40.001475253560166, -105.21256699919985 40.00156493581707, -105.21256698839802 40.001564997935326, -105.21252699991051 40.00195299848955, -105.21251614275768 40.003073316521814, -105.21251175887738 40.00352564947486, -105.2117791909032 40.00354043954807, -105.21177619083987 40.0030044389501, -105.21114419157635 40.00300243863417, -105.21117119066528 40.00325443919979, -105.21115519019756 40.00343643944229, -105.21103119153004 40.00352344002083, -105.21103119099389 40.00371343942365, -105.21251078940765 40.003697551400016, -105.21250599767083 40.00582199879766, -105.21250548263852 40.006478919508666, -105.21250499876983 40.00709399945863, -105.21254299893013 40.00731899837689, -105.21257399996067 40.00741399830913, -105.2126529828366 40.00758894189271, -105.21265301189669 40.00758899420312, -105.21288599928072 40.00799899844429, -105.21292353784645 40.00809508272722, -105.2129700000606 40.00821399827627, -105.2129869521706 40.008297267221266, -105.21300399958496 40.0083809993364, -105.21301128524784 40.00853642174128, -105.21301899974073 40.00870099855842, -105.21302199997974 40.008908999486536, -105.21302199966782 40.009066033033264, -105.2130219997471 40.009355999518654, -105.21298299984113 40.0095709993631, -105.21298299869767 40.0095865752715, -105.2129829999123 40.00961299956395, -105.2130060003659 40.00974199894547, -105.21301807089367 40.00983143781237, -105.21302800044937 40.009904999123314, -105.21303123885042 40.010165246656925, -105.21304400031774 40.01119099898076, -105.21304544738146 40.01133281594282, -105.21304600060444 40.01138699885649, -105.21305299860126 40.01186999911342, -105.21305899961078 40.01220499962974, -105.21305925746974 40.01222416348261, -105.213064157268 40.01258789120162, -105.21306730591022 40.01280105946651, -105.21307368616226 40.01323274517098, -105.2130740693893 40.01339608598071, -105.2130777016322 40.01363575086111, -105.21309403248726 40.014675946472416))</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
@@ -7066,7 +7102,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2269704853094 39.99317677606326, -105.224373995855 39.99318290251038, -105.224373066493 39.99333290079716, -105.2243818903101 39.99353387065675, -105.224383933816 39.99426492285259, -105.2243759286585 39.99492100747396, -105.2243809144956 39.99580689549131, -105.224380027552 39.99655605899623, -105.2243878308265 39.99753995745615, -105.224398994631 39.99760394774227, -105.2244140993091 39.99766410345214, -105.224480917112 39.99782293599132, -105.224555062579 39.99793594086837, -105.2246470892445 39.99803992961618, -105.2247950790052 39.99816299355049, -105.2248858227375 39.99823101590031, -105.2250469054067 39.9983829352995, -105.2251459824802 39.99850890201741, -105.2252498335415 39.99869088182842, -105.2252859486925 39.99876399025853, -105.2253319626453 39.99894912586416, -105.2253349559493 39.99909188404666, -105.225354046752 40.00011286918626, -105.2253502088998 40.00051594885953, -105.2253478593084 40.00076291802563, -105.2253431400887 40.00131386861644, -105.2253421681761 40.00137810367464, -105.2253430917478 40.00176902229651, -105.2253539877582 40.00234306948083, -105.2253588845966 40.00263407263947, -105.2253628226623 40.00289707216505, -105.2253670051872 40.00318807360595, -105.2253659339144 40.00345408017876, -105.2253670471577 40.0042411320881, -105.2253689488286 40.00483300146669, -105.2253710525624 40.00519702022958, -105.2253711554255 40.00525988522655, -105.2253711764782 40.00534306428025, -105.2253701681565 40.00550502919539, -105.225369874075 40.00557805082113, -105.2253661145294 40.00651154719828, -105.2256249335607 40.00651010353371, -105.2265688248415 40.00650301211288, -105.2289009910103 40.00652057480598, -105.2299623249569 40.0065233425341, -105.2325454181118 40.00653003820529, -105.2335708506883 40.00653178608862, -105.2335795972293 40.00658094596193, -105.233617310355 40.00712050301013, -105.2336299662758 40.007382300914, -105.2340253218562 40.00738291357975, -105.2346198625271 40.00738384746584, -105.2346783761087 40.00738394068345, -105.2347807798344 40.00738343141639, -105.237909376571 40.00738357404163, -105.2383654939881 40.00738287517316, -105.2387257436185 40.00728901168986, -105.2387007440196 40.00725601094121, -105.234735824706 40.00256597950803, -105.2336867520658 40.00122508394391, -105.2327802357967 40.00008630243428, -105.2315727911532 40.00006603135803, -105.2312149162657 40.00006519764642, -105.230829196794 40.00005357463328, -105.2295648744829 40.00004897693059, -105.2295661712776 39.9999918793853, -105.2295580641257 39.99978597077631, -105.229524157622 39.9996049821949, -105.2293679223644 39.99921809162684, -105.2293401491907 39.99911096383681, -105.2293179557386 39.99894702324459, -105.2293189801351 39.99859893439575, -105.2293141162702 39.99766610335006, -105.2293280049977 39.99758405479982, -105.2293828985478 39.99742304033567, -105.2294709466912 39.99727198652509, -105.2296939947666 39.99701089201523, -105.229802148455 39.99682996173368, -105.2298559013762 39.99668596493536, -105.2298920220077 39.99648812079264, -105.2298980465868 39.99613812158013, -105.2299060183916 39.9951169256626, -105.2299169005759 39.9939908696123, -105.2299091280582 39.99388104265839, -105.2298770748835 39.9937730817142, -105.2297969400669 39.99364002571505, -105.229713055697 39.99355198280633, -105.2296098574216 39.99347487532473, -105.2293740232478 39.9933628668272, -105.2292899710431 39.99331792225447, -105.2291718231109 39.99323007318709, -105.2290840685852 39.99312911793925, -105.229031966724 39.99303703141354, -105.228996035092 39.99291807940918, -105.2288806839204 39.99292905828161, -105.2288649980137 39.99317226849462, -105.2269704853094 39.99317677606326))</t>
+          <t>POLYGON ((-105.22697048530941 39.99317677606326, -105.22437399585502 39.99318290251038, -105.22437306649297 39.993332900797164, -105.22438189031013 39.99353387065675, -105.22438393381603 39.994264922852594, -105.22437592865846 39.994921007473955, -105.22438091449563 39.99580689549131, -105.22438002755204 39.99655605899623, -105.22438783082652 39.99753995745615, -105.22439899463099 39.99760394774227, -105.22441409930909 39.99766410345214, -105.22448091711205 39.99782293599132, -105.22455506257897 39.997935940868366, -105.22464708924446 39.99803992961618, -105.22479507900516 39.99816299355049, -105.22488582273748 39.99823101590031, -105.22504690540674 39.9983829352995, -105.22514598248017 39.99850890201741, -105.22524983354145 39.998690881828416, -105.22528594869246 39.99876399025853, -105.22533196264533 39.998949125864165, -105.22533495594931 39.99909188404666, -105.22535404675197 40.00011286918626, -105.22535020889977 40.00051594885953, -105.22534785930836 40.00076291802563, -105.22534314008868 40.00131386861644, -105.22534216817614 40.00137810367464, -105.22534309174783 40.001769022296514, -105.2253539877582 40.00234306948083, -105.22535888459663 40.00263407263947, -105.22536282266232 40.00289707216505, -105.22536700518715 40.003188073605955, -105.22536593391445 40.003454080178756, -105.22536704715769 40.004241132088104, -105.22536894882857 40.004833001466686, -105.22537105256237 40.00519702022958, -105.22537115542546 40.00525988522655, -105.22537117647816 40.00534306428025, -105.22537016815653 40.00550502919539, -105.22536987407497 40.00557805082113, -105.2253661145294 40.00651154719828, -105.22562493356068 40.00651010353371, -105.22656882484154 40.00650301211288, -105.22890099101032 40.006520574805975, -105.22996232495693 40.0065233425341, -105.23254541811183 40.00653003820529, -105.23357085068831 40.00653178608862, -105.23357959722934 40.00658094596193, -105.23361731035496 40.00712050301013, -105.2336299662758 40.007382300914, -105.23402532185622 40.00738291357975, -105.23461986252707 40.00738384746584, -105.23467837610872 40.00738394068345, -105.23478077983441 40.007383431416386, -105.23790937657097 40.007383574041626, -105.23836549398806 40.00738287517316, -105.23872574361852 40.007289011689856, -105.23870074401964 40.007256010941205, -105.23473582470602 40.002565979508034, -105.23368675206584 40.001225083943915, -105.23278023579665 40.00008630243428, -105.2315727911532 40.00006603135803, -105.23121491626574 40.00006519764642, -105.23082919679398 40.00005357463328, -105.22956487448295 40.00004897693059, -105.2295661712776 39.9999918793853, -105.22955806412571 39.99978597077631, -105.22952415762204 39.9996049821949, -105.22936792236442 39.999218091626844, -105.22934014919069 39.99911096383681, -105.22931795573858 39.99894702324459, -105.22931898013515 39.99859893439575, -105.22931411627023 39.997666103350056, -105.22932800499767 39.997584054799816, -105.2293828985478 39.99742304033567, -105.22947094669117 39.997271986525085, -105.22969399476659 39.997010892015226, -105.22980214845495 39.99682996173368, -105.22985590137618 39.99668596493536, -105.22989202200772 39.99648812079264, -105.22989804658681 39.99613812158013, -105.2299060183916 39.9951169256626, -105.22991690057586 39.9939908696123, -105.22990912805824 39.993881042658394, -105.22987707488346 39.9937730817142, -105.22979694006688 39.993640025715045, -105.22971305569698 39.99355198280633, -105.22960985742161 39.99347487532473, -105.22937402324784 39.993362866827205, -105.22928997104306 39.99331792225447, -105.22917182311087 39.99323007318709, -105.22908406858515 39.99312911793925, -105.22903196672401 39.993037031413536, -105.22899603509195 39.99291807940918, -105.22888068392042 39.99292905828161, -105.22886499801375 39.99317226849462, -105.22697048530941 39.99317677606326))</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
@@ -7108,7 +7144,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2316456813471 39.99571605960905, -105.2316392818717 39.99734243241262, -105.2315727911532 40.00006603135803, -105.2327802357967 40.00008630243428, -105.2336867520658 40.00122508394391, -105.234735824706 40.00256597950803, -105.2387007440196 40.00725601094121, -105.2387257436185 40.00728901168986, -105.2387427436112 40.00730801166415, -105.2392875951565 40.00798585798366, -105.2394896630826 40.00769466327992, -105.23948896571 40.0073811712716, -105.2397860088713 40.00738069992978, -105.2397617504435 40.00716500984186, -105.2397183929218 40.00655542897663, -105.2396037895222 40.00522099519871, -105.2400351798579 40.00501219013716, -105.2401951250173 40.00483908383512, -105.2411529008695 40.00436494609108, -105.2419328825653 40.00398813164567, -105.2422009576195 40.0038959441677, -105.2424278327316 40.00384291993261, -105.2430249973684 40.0037599745659, -105.2433099373974 40.00373892239762, -105.2437240245236 40.00373792147855, -105.2437181670989 40.00225687443313, -105.2437131733929 40.00149589374237, -105.2437280002277 40.00087496279527, -105.2437179903998 40.00078407447747, -105.2436830323785 40.00068297402652, -105.2436031658809 40.0005639290533, -105.243511030364 40.00047999574345, -105.2434059787843 40.00041387737136, -105.243285870079 40.00036501973633, -105.2431571319965 40.00033288861193, -105.2431510732557 40.00016702329347, -105.2431493365557 40.00010980268009, -105.2422326797842 40.00009824342826, -105.2401180011096 40.00008277324998, -105.2401649392682 39.99880204982464, -105.239303991962 39.99814894509955, -105.2375229504292 39.99673606739726, -105.2373420925832 39.99661596485014, -105.2371458286437 39.99651092546517, -105.2368628612523 39.99639800170707, -105.2366179092346 39.99633100831502, -105.2364930499866 39.99631397714569, -105.2365149413456 39.9962830068348, -105.2366400583279 39.99614109106445, -105.2375070803766 39.99548076120305, -105.2379398693798 39.99515111366383, -105.2382619523008 39.9949289351124, -105.2382870629868 39.99489604977548, -105.23834494198 39.9947880206398, -105.2383368709705 39.99438006523951, -105.2383379946104 39.99399409225366, -105.2383238322312 39.99312712594978, -105.2364689106397 39.99313909730117, -105.2364661425782 39.99228505947059, -105.2364579412395 39.99126711967727, -105.2355589146679 39.99126396310474, -105.2355325627036 39.99126818617076, -105.2354221365493 39.99128588555319, -105.2352959661362 39.99133308746169, -105.2351889848636 39.99140202108246, -105.234761912102 39.99173293425835, -105.2345710429928 39.99189693204435, -105.2344139012137 39.99201488828059, -105.2342361253701 39.99211605176179, -105.2340638469615 39.99217989190147, -105.2338809414382 39.99222311828235, -105.2337859500843 39.9922368996541, -105.2319781356781 39.99225604515681, -105.2316639565938 39.99225242952157, -105.2316456813471 39.99571605960905))</t>
+          <t>POLYGON ((-105.2316456813471 39.99571605960905, -105.23163928187168 39.99734243241262, -105.2315727911532 40.00006603135803, -105.23278023579665 40.00008630243428, -105.23368675206584 40.001225083943915, -105.23473582470602 40.002565979508034, -105.23870074401964 40.007256010941205, -105.23872574361852 40.007289011689856, -105.23874274361121 40.00730801166415, -105.23928759515651 40.007985857983655, -105.23948966308264 40.00769466327992, -105.23948896570995 40.007381171271604, -105.23978600887133 40.00738069992978, -105.23976175044352 40.007165009841856, -105.23971839292183 40.006555428976625, -105.23960378952219 40.00522099519871, -105.2400351798579 40.00501219013716, -105.24019512501732 40.004839083835115, -105.24115290086948 40.00436494609108, -105.24193288256534 40.00398813164567, -105.24220095761953 40.003895944167695, -105.24242783273162 40.00384291993261, -105.24302499736841 40.0037599745659, -105.2433099373974 40.00373892239762, -105.24372402452364 40.00373792147855, -105.2437181670989 40.00225687443313, -105.24371317339295 40.001495893742366, -105.24372800022768 40.000874962795265, -105.24371799039984 40.00078407447747, -105.24368303237853 40.00068297402652, -105.24360316588087 40.0005639290533, -105.243511030364 40.00047999574345, -105.24340597878428 40.00041387737136, -105.24328587007902 40.00036501973633, -105.24315713199653 40.00033288861193, -105.24315107325569 40.00016702329347, -105.24314933655573 40.00010980268009, -105.2422326797842 40.00009824342826, -105.24011800110956 40.00008277324998, -105.24016493926817 39.99880204982464, -105.239303991962 39.99814894509955, -105.23752295042915 39.99673606739726, -105.2373420925832 39.99661596485014, -105.23714582864369 39.99651092546517, -105.23686286125229 39.99639800170707, -105.23661790923457 39.99633100831502, -105.23649304998659 39.99631397714569, -105.23651494134556 39.9962830068348, -105.23664005832785 39.99614109106445, -105.23750708037662 39.995480761203055, -105.23793986937977 39.99515111366383, -105.23826195230085 39.9949289351124, -105.2382870629868 39.994896049775484, -105.23834494197999 39.994788020639795, -105.2383368709705 39.99438006523951, -105.23833799461038 39.99399409225366, -105.23832383223122 39.99312712594978, -105.23646891063972 39.99313909730117, -105.23646614257817 39.99228505947059, -105.23645794123948 39.991267119677275, -105.23555891466789 39.991263963104736, -105.23553256270363 39.99126818617076, -105.23542213654926 39.99128588555319, -105.23529596613622 39.99133308746169, -105.23518898486363 39.991402021082465, -105.23476191210203 39.99173293425835, -105.23457104299275 39.99189693204435, -105.23441390121366 39.992014888280586, -105.23423612537013 39.99211605176179, -105.2340638469615 39.99217989190147, -105.23388094143822 39.992223118282354, -105.23378595008428 39.992236899654095, -105.23197813567813 39.99225604515681, -105.23166395659383 39.99225242952157, -105.2316456813471 39.99571605960905))</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
@@ -7150,7 +7186,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2431510732557 40.00016702329347, -105.2431571319965 40.00033288861193, -105.243285870079 40.00036501973633, -105.2434059787843 40.00041387737136, -105.243511030364 40.00047999574345, -105.2436031658809 40.0005639290533, -105.2436830323785 40.00068297402652, -105.2437179903998 40.00078407447747, -105.2437280002277 40.00087496279527, -105.2437131733929 40.00149589374237, -105.2437181670989 40.00225687443313, -105.2437240245236 40.00373792147855, -105.2444301101221 40.00373701813933, -105.2446710684481 40.00373590466019, -105.2456098973364 40.00373495983664, -105.2460761014417 40.00373406634042, -105.2464109378442 40.00373397911915, -105.2465258818805 40.00373395715376, -105.2474329370459 40.00373402643322, -105.2483739119415 40.00373196590926, -105.2492320666852 40.00373109021578, -105.2493891330616 40.00373088229632, -105.2503311673884 40.00373210269301, -105.2507459645829 40.00373190219263, -105.2512571503644 40.00372998617799, -105.2531108838922 40.00373012711088, -105.2540440020844 40.00372910138983, -105.2583379493246 40.00373488608032, -105.258572133868 40.00373098416479, -105.2586434447849 40.0037284900354, -105.2586556382503 40.00290996136781, -105.2586436430115 40.00235946687246, -105.2586454140996 40.00185904416556, -105.2586142067626 40.00148365856045, -105.2585687794402 40.00118688281169, -105.2584680337078 40.00076130850472, -105.2583433547495 40.00053228127841, -105.2581675632618 40.00029957202448, -105.2577880710165 40.00025886209083, -105.2572332229477 40.00022519510679, -105.2564991340491 40.00015215776349, -105.2559182940653 40.00011518449874, -105.2556348847636 40.00008598844521, -105.2545940488416 40.00001228844468, -105.2538457383644 40.00001784269875, -105.2530347277771 40.00000978133342, -105.2503165795159 40.00000758837528, -105.2483719392432 40.00001002208948, -105.2473977786926 40.0000083801519, -105.2470212334831 40.00002900096509, -105.2464540767689 40.00006350033268, -105.2459194677626 40.00009449394422, -105.2452919437584 40.00011455577305, -105.2447945691646 40.00013132853758, -105.2438138964199 40.00012915375532, -105.2431493365557 40.00010980268009, -105.2431510732557 40.00016702329347))</t>
+          <t>POLYGON ((-105.24315107325569 40.00016702329347, -105.24315713199653 40.00033288861193, -105.24328587007902 40.00036501973633, -105.24340597878428 40.00041387737136, -105.243511030364 40.00047999574345, -105.24360316588087 40.0005639290533, -105.24368303237853 40.00068297402652, -105.24371799039984 40.00078407447747, -105.24372800022768 40.000874962795265, -105.24371317339295 40.001495893742366, -105.2437181670989 40.00225687443313, -105.24372402452364 40.00373792147855, -105.24443011012212 40.003737018139326, -105.24467106844806 40.00373590466019, -105.24560989733641 40.00373495983664, -105.24607610144173 40.00373406634042, -105.24641093784425 40.003733979119154, -105.24652588188049 40.003733957153756, -105.24743293704586 40.00373402643322, -105.24837391194146 40.00373196590926, -105.24923206668522 40.00373109021578, -105.2493891330616 40.00373088229632, -105.25033116738838 40.003732102693014, -105.25074596458293 40.003731902192634, -105.25125715036444 40.00372998617799, -105.25311088389222 40.003730127110884, -105.25404400208444 40.00372910138983, -105.25833794932456 40.003734886080316, -105.25857213386804 40.00373098416479, -105.25864344478488 40.0037284900354, -105.25865563825032 40.002909961367806, -105.25864364301147 40.002359466872456, -105.25864541409963 40.001859044165556, -105.25861420676263 40.001483658560446, -105.25856877944018 40.001186882811695, -105.25846803370776 40.00076130850472, -105.25834335474954 40.00053228127841, -105.2581675632618 40.00029957202448, -105.25778807101649 40.00025886209083, -105.25723322294773 40.00022519510679, -105.2564991340491 40.000152157763495, -105.25591829406534 40.00011518449874, -105.25563488476364 40.000085988445214, -105.2545940488416 40.00001228844468, -105.25384573836436 40.000017842698746, -105.25303472777706 40.000009781333425, -105.2503165795159 40.000007588375276, -105.24837193924319 40.00001002208948, -105.2473977786926 40.0000083801519, -105.24702123348305 40.00002900096509, -105.24645407676893 40.00006350033268, -105.2459194677626 40.00009449394422, -105.24529194375839 40.000114555773045, -105.24479456916463 40.00013132853758, -105.24381389641991 40.000129153755324, -105.24314933655573 40.00010980268009, -105.24315107325569 40.00016702329347))</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
@@ -7192,7 +7228,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2556348847636 40.00008598844521, -105.2559182940653 40.00011518449874, -105.2564991340491 40.00015215776349, -105.2572332229477 40.00022519510679, -105.2577880710165 40.00025886209083, -105.2581675632618 40.00029957202448, -105.2589195861169 40.00036267320748, -105.2592544037049 40.00038408331039, -105.259251053428 40.00025364728025, -105.259208137926 40.00024028023068, -105.2589691389426 40.00013528073883, -105.2588631378062 40.00007828100154, -105.2586371380042 39.99996628110418, -105.2581901380272 39.99973028114304, -105.2579881380721 39.9996242809139, -105.2569711373872 39.99907628081892, -105.2554151376702 39.99826728194028, -105.2551191376442 39.99812828080001, -105.2531881376958 39.99700828020997, -105.2529616488933 39.99687856120978, -105.2526451362952 39.9966972807593, -105.252490135917 39.99676028120317, -105.2519301367892 39.99643628146383, -105.2488871359441 39.99466728119395, -105.2483721362223 39.99436828224118, -105.2466227154164 39.99335930785364, -105.2410388945943 39.99004486718228, -105.2401816972446 39.98954904272472, -105.2398431564504 39.98986597086589, -105.2398430835623 39.98986604725708, -105.239842460506 39.98986669522325, -105.2392999425185 39.99043107915255, -105.2392249466247 39.99053687428649, -105.2391079433111 39.99070790962207, -105.2390219540881 39.99088807473773, -105.2388690597486 39.99129786242749, -105.238382164903 39.99252798068977, -105.2383338522648 39.99274803609929, -105.2383238322312 39.99312712594978, -105.2383379946104 39.99399409225366, -105.2383368709705 39.99438006523951, -105.23834494198 39.9947880206398, -105.2382870629868 39.99489604977548, -105.2382619523008 39.9949289351124, -105.2379398693798 39.99515111366383, -105.2375070803766 39.99548076120305, -105.2366400583279 39.99614109106445, -105.2365149413456 39.9962830068348, -105.2364930499866 39.99631397714569, -105.2366179092346 39.99633100831502, -105.2368628612523 39.99639800170707, -105.2371458286437 39.99651092546517, -105.2373420925832 39.99661596485014, -105.2375229504292 39.99673606739726, -105.239303991962 39.99814894509955, -105.2401649392682 39.99880204982464, -105.2401180011096 40.00008277324998, -105.2422326797842 40.00009824342826, -105.2431493365557 40.00010980268009, -105.2438138964199 40.00012915375532, -105.2447945691646 40.00013132853758, -105.2452919437584 40.00011455577305, -105.2459194677626 40.00009449394422, -105.2464540767689 40.00006350033268, -105.2470212334831 40.00002900096509, -105.2473977786926 40.0000083801519, -105.2483719392432 40.00001002208948, -105.2503165795159 40.00000758837528, -105.2530347277771 40.00000978133342, -105.2538457383644 40.00001784269875, -105.2545940488416 40.00001228844468, -105.2556348847636 40.00008598844521))</t>
+          <t>POLYGON ((-105.25563488476364 40.000085988445214, -105.25591829406534 40.00011518449874, -105.2564991340491 40.000152157763495, -105.25723322294773 40.00022519510679, -105.25778807101649 40.00025886209083, -105.2581675632618 40.00029957202448, -105.25891958611686 40.000362673207476, -105.2592544037049 40.00038408331039, -105.25925105342797 40.000253647280246, -105.25920813792597 40.000240280230685, -105.25896913894256 40.00013528073883, -105.25886313780617 40.000078281001535, -105.25863713800422 39.99996628110418, -105.2581901380272 39.99973028114304, -105.25798813807206 39.9996242809139, -105.25697113738718 39.99907628081892, -105.25541513767021 39.99826728194028, -105.25511913764421 39.99812828080001, -105.25318813769576 39.99700828020997, -105.25296164889333 39.996878561209776, -105.25264513629524 39.9966972807593, -105.25249013591703 39.996760281203166, -105.25193013678921 39.99643628146383, -105.24888713594407 39.99466728119395, -105.24837213622226 39.994368282241176, -105.24662271541642 39.99335930785364, -105.24103889459431 39.99004486718228, -105.24018169724461 39.98954904272472, -105.23984315645038 39.989865970865885, -105.2398430835623 39.98986604725708, -105.23984246050595 39.98986669522325, -105.23929994251853 39.99043107915255, -105.23922494662469 39.99053687428649, -105.23910794331107 39.99070790962207, -105.23902195408814 39.990888074737725, -105.23886905974862 39.991297862427494, -105.23838216490296 39.99252798068977, -105.23833385226479 39.992748036099286, -105.23832383223122 39.99312712594978, -105.23833799461038 39.99399409225366, -105.2383368709705 39.99438006523951, -105.23834494197999 39.994788020639795, -105.2382870629868 39.994896049775484, -105.23826195230085 39.9949289351124, -105.23793986937977 39.99515111366383, -105.23750708037662 39.995480761203055, -105.23664005832785 39.99614109106445, -105.23651494134556 39.9962830068348, -105.23649304998659 39.99631397714569, -105.23661790923457 39.99633100831502, -105.23686286125229 39.99639800170707, -105.23714582864369 39.99651092546517, -105.2373420925832 39.99661596485014, -105.23752295042915 39.99673606739726, -105.239303991962 39.99814894509955, -105.24016493926817 39.99880204982464, -105.24011800110956 40.00008277324998, -105.2422326797842 40.00009824342826, -105.24314933655573 40.00010980268009, -105.24381389641991 40.000129153755324, -105.24479456916463 40.00013132853758, -105.24529194375839 40.000114555773045, -105.2459194677626 40.00009449394422, -105.24645407676893 40.00006350033268, -105.24702123348305 40.00002900096509, -105.2473977786926 40.0000083801519, -105.24837193924319 40.00001002208948, -105.2503165795159 40.000007588375276, -105.25303472777706 40.000009781333425, -105.25384573836436 40.000017842698746, -105.2545940488416 40.00001228844468, -105.25563488476364 40.000085988445214))</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
@@ -7234,7 +7270,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2466227165907 39.99335930695561, -105.2483721362223 39.99436828224118, -105.2488871359441 39.99466728119395, -105.2519301367892 39.99643628146383, -105.252490135917 39.99676028120317, -105.2526451362952 39.9966972807593, -105.2529616488933 39.99687856120978, -105.2531881376958 39.99700828020997, -105.2551191376442 39.99812828080001, -105.2554151376702 39.99826728194028, -105.2569711373872 39.99907628081892, -105.2579881380721 39.9996242809139, -105.2581901380272 39.99973028114304, -105.2586371380042 39.99996628110418, -105.2588631378062 40.00007828100154, -105.2589691389426 40.00013528073883, -105.259208137926 40.00024028023068, -105.259251053428 40.00025364728025, -105.2593301393748 40.00027828043822, -105.2595041374749 40.0003192800807, -105.2597321375767 40.00033028045623, -105.2602051376428 40.00033828032775, -105.2606671387836 40.00031627988058, -105.2613031379176 40.00026628085262, -105.2614471376263 40.00025428044938, -105.262564137449 40.0001492804175, -105.2635226869538 40.00007661770653, -105.2635271382638 40.00007628008433, -105.2635316634515 40.00008266869302, -105.2635362436151 40.00008232142758, -105.263577605498 40.00014071094439, -105.2635825036177 40.00014762629726, -105.2636677621977 40.00013487760815, -105.2636616490187 40.00012814440228, -105.2636359111153 40.00009189888685, -105.2636119128586 40.00003589839808, -105.2635339129713 39.99989289753027, -105.2633639117712 39.99966589752046, -105.2630219104211 39.99921689664917, -105.2628649097271 39.99900589659193, -105.2622529055395 39.9981348940354, -105.261640903616 39.99723789256219, -105.2611309008647 39.99652989144005, -105.2608688994295 39.99615489070485, -105.2600818936084 39.99503388793405, -105.2594518911588 39.99415388637748, -105.2584222456255 39.99269217486411, -105.2583630602698 39.99271900831015, -105.2581979196601 39.99278893921107, -105.2578890938063 39.99291704138979, -105.2568431490209 39.99347211537662, -105.2566469544573 39.99354197855802, -105.256439076781 39.99358491328484, -105.2562241597075 39.99360010701558, -105.2558879427119 39.99360104290265, -105.2549139222388 39.99360089751056, -105.2539748649406 39.99360493719707, -105.253976992119 39.99350995784211, -105.2539598245705 39.99342097709806, -105.2537680195346 39.99316389105262, -105.253481917966 39.99282809124987, -105.2532838677984 39.99262095392066, -105.2531030577065 39.99248303242634, -105.2529520429993 39.99239596059435, -105.2529160599851 39.99237803971734, -105.2525991777126 39.99226508096519, -105.2521180947648 39.99215890608932, -105.2511991538801 39.99193703631351, -105.2505979253994 39.99179600699761, -105.2499018481588 39.99163198315823, -105.2495039201496 39.99152899760701, -105.2490551479953 39.99137401601043, -105.248946097095 39.99133012926357, -105.2485859878499 39.99113498504862, -105.2478088871432 39.99068609379896, -105.2474840945791 39.99049706225706, -105.2467369290482 39.99006387816448, -105.2460040292133 39.98963593541377, -105.2452579682391 39.98919890009814, -105.2445229609886 39.98876710100529, -105.2442409753642 39.98906405572566, -105.2430880959231 39.99023286953971, -105.2430139381545 39.99030709924219, -105.24294293165 39.99040233108766, -105.2426875294299 39.99066405991451, -105.2424807589426 39.99088294639051, -105.2419808182389 39.99058968315889, -105.2410388945943 39.99004486718228, -105.2466227165907 39.99335930695561))</t>
+          <t>POLYGON ((-105.24662271659072 39.99335930695561, -105.24837213622226 39.994368282241176, -105.24888713594407 39.99466728119395, -105.25193013678921 39.99643628146383, -105.25249013591703 39.996760281203166, -105.25264513629524 39.9966972807593, -105.25296164889333 39.996878561209776, -105.25318813769576 39.99700828020997, -105.25511913764421 39.99812828080001, -105.25541513767021 39.99826728194028, -105.25697113738718 39.99907628081892, -105.25798813807206 39.9996242809139, -105.2581901380272 39.99973028114304, -105.25863713800422 39.99996628110418, -105.25886313780617 40.000078281001535, -105.25896913894256 40.00013528073883, -105.25920813792597 40.000240280230685, -105.25925105342797 40.000253647280246, -105.25933013937475 40.000278280438216, -105.25950413747489 40.000319280080696, -105.25973213757672 40.000330280456225, -105.26020513764277 40.000338280327746, -105.26066713878359 40.00031627988058, -105.26130313791761 40.00026628085262, -105.26144713762633 40.00025428044938, -105.26256413744898 40.0001492804175, -105.26352268695379 40.000076617706526, -105.26352713826377 40.00007628008433, -105.26353166345149 40.00008266869302, -105.26353624361508 40.000082321427584, -105.26357760549804 40.00014071094439, -105.26358250361771 40.000147626297256, -105.26366776219774 40.000134877608154, -105.26366164901866 40.00012814440228, -105.26363591111529 40.00009189888685, -105.2636119128586 40.00003589839808, -105.2635339129713 39.99989289753027, -105.26336391177124 39.99966589752046, -105.26302191042113 39.999216896649166, -105.26286490972711 39.99900589659193, -105.26225290553954 39.9981348940354, -105.26164090361601 39.99723789256219, -105.26113090086469 39.99652989144005, -105.26086889942945 39.99615489070485, -105.26008189360844 39.99503388793405, -105.25945189115878 39.99415388637748, -105.25842224562547 39.99269217486411, -105.2583630602698 39.99271900831015, -105.25819791966006 39.992788939211074, -105.25788909380631 39.992917041389795, -105.25684314902091 39.99347211537662, -105.25664695445731 39.99354197855802, -105.25643907678104 39.99358491328484, -105.25622415970746 39.99360010701558, -105.25588794271194 39.993601042902654, -105.25491392223877 39.99360089751056, -105.25397486494057 39.99360493719707, -105.25397699211904 39.993509957842114, -105.25395982457049 39.99342097709806, -105.25376801953456 39.99316389105262, -105.25348191796598 39.99282809124987, -105.25328386779843 39.99262095392066, -105.25310305770647 39.992483032426335, -105.2529520429993 39.99239596059435, -105.2529160599851 39.99237803971734, -105.2525991777126 39.99226508096519, -105.25211809476482 39.99215890608932, -105.25119915388011 39.99193703631351, -105.25059792539938 39.99179600699761, -105.24990184815881 39.99163198315823, -105.24950392014964 39.99152899760701, -105.24905514799526 39.991374016010425, -105.24894609709499 39.991330129263574, -105.24858598784989 39.991134985048625, -105.24780888714318 39.990686093798956, -105.24748409457912 39.990497062257056, -105.24673692904815 39.99006387816448, -105.24600402921334 39.98963593541377, -105.24525796823914 39.98919890009814, -105.2445229609886 39.98876710100529, -105.24424097536418 39.989064055725656, -105.24308809592307 39.99023286953971, -105.24301393815448 39.99030709924219, -105.24294293165002 39.99040233108766, -105.24268752942986 39.990664059914515, -105.24248075894259 39.990882946390506, -105.24198081823887 39.99058968315889, -105.24103889459431 39.99004486718228, -105.24662271659072 39.99335930695561))</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
@@ -7276,7 +7312,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2636359111153 40.00009189888685, -105.2636616490187 40.00012814440228, -105.2636677621977 40.00013487760815, -105.2636851372977 40.00013227971019, -105.2637656435806 40.0000901112732, -105.2637600945748 40.00008210840647, -105.2643058348404 40.00009201025707, -105.2650550950247 40.00008502916437, -105.2665028856773 40.00008302921293, -105.2677639960641 40.0000800858277, -105.2687848652311 40.00008103962393, -105.2700220559592 40.00007912146844, -105.2712538896729 40.0000780026072, -105.2724860869347 40.00007495020975, -105.2737168453467 40.00007490171039, -105.2749419062467 40.00007098586583, -105.2761780199424 40.00007092064759, -105.2773991366947 40.00007191202165, -105.2784039373483 40.00007494632052, -105.278630959455 40.00007400981507, -105.279646841714 40.00007211177422, -105.2798638671253 40.00007197783349, -105.2803721710106 40.00006910409878, -105.2810889264481 40.00006799577455, -105.2819370370845 40.0000679564938, -105.2825949350523 40.00006821265478, -105.2827446929499 40.00006849493339, -105.2828547635354 40.00006592736987, -105.2831127752968 40.00006780089974, -105.2831669050245 40.00006790270817, -105.2832483927471 40.00006757407493, -105.2832472068767 40.00005343339678, -105.2832492067252 39.99996843443798, -105.283001573634 39.99715502844389, -105.2827223626449 39.99403700746425, -105.2826135655954 39.99275545438949, -105.2818969261123 39.99276302544907, -105.2779829253155 39.99288181170427, -105.2774916626261 39.99289384212508, -105.27728062072 39.98929895772331, -105.272469014403 39.98928825018775, -105.2723997887415 39.98928809732546, -105.2719593156257 39.98928710617648, -105.2716223730542 39.98928634550769, -105.2714638608088 39.98928598995118, -105.2703890471504 39.9898999403625, -105.2698468464089 39.98934422916937, -105.2697863162731 39.98928219374066, -105.2695693272313 39.98928169987499, -105.2690513821612 39.98928979605612, -105.2690057951191 39.98929090439255, -105.2687604302988 39.9892966468156, -105.2684356365834 39.98930393683757, -105.2681284182476 39.98931082988264, -105.2678213991263 39.98931696866276, -105.2675174223414 39.9893223075758, -105.2672124361285 39.98932766346351, -105.266908817561 39.98933299609138, -105.266603422585 39.98933835674684, -105.2662923260879 39.98934381491483, -105.2659872541979 39.98934917008992, -105.2656825850795 39.98935451626985, -105.2653789826748 39.98935984220002, -105.2650717982035 39.98936523118273, -105.2650513892666 39.98936558767976, -105.2648373547264 39.98936934381865, -105.2647632739567 39.9893706805596, -105.2644639608202 39.98937623169154, -105.2641617801198 39.98938041799351, -105.2638595103053 39.98938429079391, -105.2635635170793 39.98938968787346, -105.2632699746576 39.98939504239177, -105.2629693208403 39.98940052204338, -105.2629691437031 39.9894198227013, -105.2627225441111 39.9894217534786, -105.2627009087332 39.98942190889128, -105.2624725175554 39.98942225453435, -105.2624366887991 39.98942230950096, -105.2622208029755 39.98942263267978, -105.2621663028471 39.98942271569812, -105.2619716046779 39.98942300826597, -105.261884822492 39.98942313887572, -105.2617216745568 39.98942338450279, -105.2616051383066 39.98942356057711, -105.2614710243243 39.9894237605091, -105.2613061563213 39.98942400649242, -105.2612196528034 39.98942413807912, -105.2610063617066 39.98942445625218, -105.2609693807718 39.98942451197681, -105.2607178722534 39.98942488726801, -105.2602818806604 39.9894271824184, -105.260173036398 39.98942793414727, -105.2601740487218 39.98945272226218, -105.2600467919094 39.98945347249305, -105.2597926037893 39.98945497231101, -105.2595416908582 39.98945775102465, -105.2592898072885 39.98945951573064, -105.2588723144116 39.98946019957963, -105.2586205327938 39.98946060845237, -105.2583666323539 39.98946119967027, -105.2581178826346 39.98946181734791, -105.2578639328738 39.98946244518267, -105.2576166222085 39.98946305669547, -105.2573661769858 39.98946367729223, -105.257119961121 39.98946428463978, -105.2568670253593 39.98946490701096, -105.2566144244698 39.98946552953418, -105.2563672403421 39.98946643765117, -105.2562075202875 39.98946711863591, -105.2559412881601 39.98947447747421, -105.2565448745829 39.99004987770695, -105.2576485940671 39.99157272394766, -105.2584222456255 39.99269217486411, -105.2594518911588 39.99415388637748, -105.2600818936084 39.99503388793405, -105.2608688994295 39.99615489070485, -105.2611309008647 39.99652989144005, -105.261640903616 39.99723789256219, -105.2622529055395 39.9981348940354, -105.2628649097271 39.99900589659193, -105.2630219104211 39.99921689664917, -105.2633639117712 39.99966589752046, -105.2635339129713 39.99989289753027, -105.2636119128586 40.00003589839808, -105.2636359111153 40.00009189888685))</t>
+          <t>POLYGON ((-105.26363591111529 40.00009189888685, -105.26366164901866 40.00012814440228, -105.26366776219774 40.000134877608154, -105.2636851372977 40.000132279710186, -105.26376564358064 40.000090111273195, -105.26376009457483 40.000082108406474, -105.26430583484039 40.00009201025707, -105.26505509502475 40.00008502916437, -105.26650288567726 40.00008302921293, -105.26776399606409 40.0000800858277, -105.26878486523107 40.00008103962393, -105.27002205595919 40.00007912146844, -105.27125388967289 40.0000780026072, -105.27248608693466 40.00007495020975, -105.2737168453467 40.00007490171039, -105.27494190624671 40.00007098586583, -105.2761780199424 40.000070920647595, -105.27739913669468 40.00007191202165, -105.27840393734827 40.00007494632052, -105.27863095945504 40.000074009815066, -105.27964684171397 40.00007211177422, -105.27986386712531 40.000071977833485, -105.28037217101055 40.00006910409878, -105.2810889264481 40.00006799577455, -105.28193703708446 40.0000679564938, -105.28259493505229 40.00006821265478, -105.28274469294988 40.000068494933394, -105.28285476353535 40.00006592736987, -105.28311277529676 40.000067800899735, -105.28316690502447 40.000067902708174, -105.28324839274713 40.000067574074926, -105.28324720687672 40.00005343339678, -105.28324920672522 39.99996843443798, -105.28300157363404 39.99715502844389, -105.28272236264492 39.99403700746425, -105.28261356559544 39.99275545438949, -105.28189692611234 39.99276302544907, -105.27798292531547 39.99288181170427, -105.27749166262615 39.992893842125085, -105.27728062071996 39.989298957723314, -105.27246901440301 39.98928825018775, -105.27239978874152 39.98928809732546, -105.27195931562566 39.989287106176484, -105.27162237305421 39.98928634550769, -105.27146386080882 39.98928598995118, -105.2703890471504 39.9898999403625, -105.26984684640885 39.98934422916937, -105.26978631627311 39.989282193740664, -105.26956932723131 39.98928169987499, -105.26905138216117 39.98928979605612, -105.2690057951191 39.98929090439255, -105.26876043029883 39.989296646815596, -105.26843563658345 39.98930393683757, -105.26812841824758 39.98931082988264, -105.26782139912633 39.989316968662756, -105.26751742234138 39.989322307575804, -105.26721243612847 39.989327663463506, -105.26690881756105 39.98933299609138, -105.26660342258495 39.98933835674684, -105.26629232608794 39.98934381491483, -105.26598725419791 39.98934917008992, -105.26568258507952 39.98935451626985, -105.26537898267483 39.98935984220002, -105.26507179820351 39.98936523118273, -105.2650513892666 39.98936558767976, -105.26483735472642 39.98936934381865, -105.26476327395672 39.9893706805596, -105.26446396082021 39.989376231691544, -105.2641617801198 39.98938041799351, -105.26385951030525 39.98938429079391, -105.26356351707929 39.98938968787346, -105.26326997465763 39.98939504239177, -105.2629693208403 39.989400522043375, -105.2629691437031 39.9894198227013, -105.26272254411109 39.9894217534786, -105.26270090873321 39.98942190889128, -105.2624725175554 39.98942225453435, -105.2624366887991 39.98942230950096, -105.26222080297555 39.98942263267978, -105.26216630284712 39.98942271569812, -105.26197160467787 39.98942300826597, -105.26188482249202 39.98942313887572, -105.26172167455678 39.98942338450279, -105.26160513830662 39.98942356057711, -105.26147102432434 39.9894237605091, -105.26130615632125 39.98942400649242, -105.26121965280342 39.989424138079116, -105.26100636170663 39.98942445625218, -105.26096938077183 39.98942451197681, -105.26071787225341 39.98942488726801, -105.26028188066039 39.9894271824184, -105.26017303639796 39.98942793414727, -105.26017404872178 39.98945272226218, -105.26004679190943 39.98945347249305, -105.25979260378934 39.98945497231101, -105.2595416908582 39.98945775102465, -105.25928980728845 39.989459515730644, -105.25887231441165 39.98946019957963, -105.25862053279376 39.98946060845237, -105.25836663235386 39.98946119967027, -105.25811788263461 39.98946181734791, -105.25786393287376 39.98946244518267, -105.25761662220854 39.98946305669547, -105.25736617698584 39.98946367729223, -105.25711996112105 39.98946428463978, -105.25686702535926 39.989464907010955, -105.25661442446984 39.98946552953418, -105.25636724034212 39.989466437651174, -105.25620752028749 39.98946711863591, -105.2559412881601 39.98947447747421, -105.25654487458293 39.99004987770695, -105.25764859406709 39.99157272394766, -105.25842224562547 39.99269217486411, -105.25945189115878 39.99415388637748, -105.26008189360844 39.99503388793405, -105.26086889942945 39.99615489070485, -105.26113090086469 39.99652989144005, -105.26164090361601 39.99723789256219, -105.26225290553954 39.9981348940354, -105.26286490972711 39.99900589659193, -105.26302191042113 39.999216896649166, -105.26336391177124 39.99966589752046, -105.2635339129713 39.99989289753027, -105.2636119128586 40.00003589839808, -105.26363591111529 40.00009189888685))</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
@@ -7318,7 +7354,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2698468464089 39.98934422916937, -105.2703890471504 39.9898999403625, -105.2714638608088 39.98928598995118, -105.2716223730542 39.98928634550769, -105.2719593156257 39.98928710617648, -105.2723997887415 39.98928809732546, -105.272469014403 39.98928825018775, -105.27728062072 39.98929895772331, -105.2770692361139 39.98569787181271, -105.2693219715217 39.98568827537257, -105.2693230565022 39.98487477127614, -105.2692050571009 39.98487402981937, -105.2689670763001 39.98485900393208, -105.2685961061897 39.98480802222888, -105.2682309574687 39.9847241095941, -105.2679329289423 39.98463209445797, -105.267683104764 39.98453194102219, -105.2672730197861 39.98433592936551, -105.2671729209081 39.98428302002201, -105.266313014888 39.98382502725105, -105.2658890858176 39.98361004180648, -105.2653939206792 39.9833559267931, -105.2647808344368 39.98304501876047, -105.264593914942 39.98292000547517, -105.2644248927018 39.98277910578437, -105.2638610800784 39.98225691251253, -105.2636771671341 39.98208907864245, -105.2632858671283 39.98173194873376, -105.2625501634418 39.98220810062183, -105.2624050298437 39.98227999986478, -105.2622488849338 39.98233705323542, -105.2620281769223 39.98238601133514, -105.2618568300338 39.98240212864589, -105.2609279514417 39.98239691129109, -105.2598249010107 39.98239901077235, -105.2595830614137 39.98236803476654, -105.2594090755475 39.98232292541489, -105.2590951262364 39.98219791177391, -105.2587659545189 39.98203909986017, -105.2585298309313 39.98190601192692, -105.2580081412259 39.98250090116355, -105.2572230666266 39.9820970781437, -105.256964863671 39.98195186270966, -105.2567530779354 39.98179988076132, -105.2566190534311 39.98165712142143, -105.2565239845004 39.98149797393191, -105.2563429162402 39.98103886783078, -105.2562962594057 39.98090963595508, -105.2560729999783 39.98097350472325, -105.2558124675118 39.98106588900765, -105.2556216049941 39.98116557073261, -105.2554632154886 39.98127961803709, -105.2553185850252 39.98144373743585, -105.255127835323 39.98163804141733, -105.2539235545214 39.98303141215703, -105.2534058854819 39.98355575438762, -105.2532753787122 39.98366628452531, -105.2530193237723 39.98380156668554, -105.2525213178784 39.98402569028387, -105.2519907553042 39.98425689199309, -105.2515999032001 39.98440260411046, -105.2514508442976 39.98450236810509, -105.2511573353756 39.98471262956502, -105.2508776457729 39.98495508973993, -105.2507192003461 39.98507985450048, -105.2505514353589 39.98521174737539, -105.250285970502 39.98537559890283, -105.2500764747387 39.98548237868278, -105.2498907386311 39.98556828381667, -105.2500878649971 39.98581688052339, -105.2503028658171 39.98605588039614, -105.2505868667575 39.9863338807198, -105.2510420594896 39.98675222905197, -105.2515148505574 39.98707852694061, -105.2519739398096 39.98734045241409, -105.2543108704154 39.98844087796657, -105.2551538717717 39.98889087686553, -105.2555178306132 39.98911024176632, -105.2557778724409 39.98932087692706, -105.2559412881601 39.98947447747421, -105.2562075202875 39.98946711863591, -105.2563672403421 39.98946643765117, -105.2566144244698 39.98946552953418, -105.2568670253593 39.98946490701096, -105.257119961121 39.98946428463978, -105.2573661769858 39.98946367729223, -105.2576166222085 39.98946305669547, -105.2578639328738 39.98946244518267, -105.2581178826346 39.98946181734791, -105.2583666323539 39.98946119967027, -105.2586205327938 39.98946060845237, -105.2588723144116 39.98946019957963, -105.2592898072885 39.98945951573064, -105.2595416908582 39.98945775102465, -105.2597926037893 39.98945497231101, -105.2600467919094 39.98945347249305, -105.2601740487218 39.98945272226218, -105.260173036398 39.98942793414727, -105.2602818806604 39.9894271824184, -105.2607178722534 39.98942488726801, -105.2609693807718 39.98942451197681, -105.2610063617066 39.98942445625218, -105.2612196528034 39.98942413807912, -105.2613061563213 39.98942400649242, -105.2614710243243 39.9894237605091, -105.2616051383066 39.98942356057711, -105.2617216745568 39.98942338450279, -105.261884822492 39.98942313887572, -105.2619716046779 39.98942300826597, -105.2621663028471 39.98942271569812, -105.2622208029755 39.98942263267978, -105.2624366887991 39.98942230950096, -105.2624725175554 39.98942225453435, -105.2627009087332 39.98942190889128, -105.2627225441111 39.9894217534786, -105.2629691437031 39.9894198227013, -105.2629693208403 39.98940052204338, -105.2632699746576 39.98939504239177, -105.2635635170793 39.98938968787346, -105.2638595103053 39.98938429079391, -105.2641617801198 39.98938041799351, -105.2644639608202 39.98937623169154, -105.2647632739567 39.9893706805596, -105.2648373547264 39.98936934381865, -105.2650513892666 39.98936558767976, -105.2650717982035 39.98936523118273, -105.2653789826748 39.98935984220002, -105.2656825850795 39.98935451626985, -105.2659872541979 39.98934917008992, -105.2662923260879 39.98934381491483, -105.266603422585 39.98933835674684, -105.266908817561 39.98933299609138, -105.2672124361285 39.98932766346351, -105.2675174223414 39.9893223075758, -105.2678213991263 39.98931696866276, -105.2681284182476 39.98931082988264, -105.2684356365834 39.98930393683757, -105.2687604302988 39.9892966468156, -105.2690057951191 39.98929090439255, -105.2690513821612 39.98928979605612, -105.2695693272313 39.98928169987499, -105.2697863162731 39.98928219374066, -105.2698468464089 39.98934422916937))</t>
+          <t>POLYGON ((-105.26984684640885 39.98934422916937, -105.2703890471504 39.9898999403625, -105.27146386080882 39.98928598995118, -105.27162237305421 39.98928634550769, -105.27195931562566 39.989287106176484, -105.27239978874152 39.98928809732546, -105.27246901440301 39.98928825018775, -105.27728062071996 39.989298957723314, -105.27706923611393 39.98569787181271, -105.2693219715217 39.98568827537257, -105.26932305650219 39.98487477127614, -105.26920505710092 39.98487402981937, -105.26896707630007 39.98485900393208, -105.2685961061897 39.984808022228876, -105.26823095746873 39.984724109594104, -105.2679329289423 39.98463209445797, -105.26768310476403 39.98453194102219, -105.2672730197861 39.984335929365514, -105.26717292090807 39.98428302002201, -105.26631301488804 39.98382502725105, -105.26588908581758 39.98361004180648, -105.26539392067917 39.983355926793095, -105.26478083443685 39.98304501876047, -105.26459391494197 39.982920005475165, -105.26442489270181 39.98277910578437, -105.26386108007839 39.98225691251253, -105.26367716713408 39.98208907864245, -105.26328586712833 39.98173194873376, -105.26255016344184 39.982208100621826, -105.26240502984375 39.98227999986478, -105.26224888493378 39.98233705323542, -105.26202817692233 39.982386011335144, -105.26185683003375 39.98240212864589, -105.26092795144172 39.98239691129109, -105.25982490101066 39.982399010772355, -105.25958306141374 39.982368034766544, -105.2594090755475 39.98232292541489, -105.25909512623639 39.98219791177391, -105.25876595451895 39.98203909986017, -105.25852983093128 39.981906011926924, -105.25800814122587 39.98250090116355, -105.25722306662664 39.9820970781437, -105.25696486367103 39.98195186270966, -105.25675307793539 39.981799880761315, -105.25661905343107 39.98165712142143, -105.2565239845004 39.98149797393191, -105.25634291624024 39.98103886783078, -105.25629625940572 39.98090963595508, -105.2560729999783 39.980973504723245, -105.25581246751177 39.98106588900765, -105.25562160499409 39.98116557073261, -105.25546321548865 39.981279618037085, -105.25531858502515 39.98144373743585, -105.25512783532298 39.98163804141733, -105.25392355452144 39.983031412157025, -105.25340588548192 39.983555754387616, -105.2532753787122 39.98366628452531, -105.25301932377232 39.983801566685536, -105.2525213178784 39.98402569028387, -105.25199075530425 39.98425689199309, -105.25159990320013 39.98440260411046, -105.25145084429761 39.98450236810509, -105.25115733537555 39.98471262956502, -105.25087764577286 39.984955089739934, -105.25071920034608 39.98507985450048, -105.25055143535891 39.98521174737539, -105.25028597050202 39.98537559890283, -105.2500764747387 39.985482378682775, -105.24989073863107 39.98556828381667, -105.25008786499713 39.98581688052339, -105.2503028658171 39.98605588039614, -105.25058686675746 39.9863338807198, -105.2510420594896 39.986752229051966, -105.25151485055741 39.987078526940614, -105.25197393980957 39.98734045241409, -105.25431087041541 39.988440877966575, -105.25515387177167 39.98889087686553, -105.25551783061321 39.98911024176632, -105.25577787244092 39.98932087692706, -105.2559412881601 39.98947447747421, -105.25620752028749 39.98946711863591, -105.25636724034212 39.989466437651174, -105.25661442446984 39.98946552953418, -105.25686702535926 39.989464907010955, -105.25711996112105 39.98946428463978, -105.25736617698584 39.98946367729223, -105.25761662220854 39.98946305669547, -105.25786393287376 39.98946244518267, -105.25811788263461 39.98946181734791, -105.25836663235386 39.98946119967027, -105.25862053279376 39.98946060845237, -105.25887231441165 39.98946019957963, -105.25928980728845 39.989459515730644, -105.2595416908582 39.98945775102465, -105.25979260378934 39.98945497231101, -105.26004679190943 39.98945347249305, -105.26017404872178 39.98945272226218, -105.26017303639796 39.98942793414727, -105.26028188066039 39.9894271824184, -105.26071787225341 39.98942488726801, -105.26096938077183 39.98942451197681, -105.26100636170663 39.98942445625218, -105.26121965280342 39.989424138079116, -105.26130615632125 39.98942400649242, -105.26147102432434 39.9894237605091, -105.26160513830662 39.98942356057711, -105.26172167455678 39.98942338450279, -105.26188482249202 39.98942313887572, -105.26197160467787 39.98942300826597, -105.26216630284712 39.98942271569812, -105.26222080297555 39.98942263267978, -105.2624366887991 39.98942230950096, -105.2624725175554 39.98942225453435, -105.26270090873321 39.98942190889128, -105.26272254411109 39.9894217534786, -105.2629691437031 39.9894198227013, -105.2629693208403 39.989400522043375, -105.26326997465763 39.98939504239177, -105.26356351707929 39.98938968787346, -105.26385951030525 39.98938429079391, -105.2641617801198 39.98938041799351, -105.26446396082021 39.989376231691544, -105.26476327395672 39.9893706805596, -105.26483735472642 39.98936934381865, -105.2650513892666 39.98936558767976, -105.26507179820351 39.98936523118273, -105.26537898267483 39.98935984220002, -105.26568258507952 39.98935451626985, -105.26598725419791 39.98934917008992, -105.26629232608794 39.98934381491483, -105.26660342258495 39.98933835674684, -105.26690881756105 39.98933299609138, -105.26721243612847 39.989327663463506, -105.26751742234138 39.989322307575804, -105.26782139912633 39.989316968662756, -105.26812841824758 39.98931082988264, -105.26843563658345 39.98930393683757, -105.26876043029883 39.989296646815596, -105.2690057951191 39.98929090439255, -105.26905138216117 39.98928979605612, -105.26956932723131 39.98928169987499, -105.26978631627311 39.989282193740664, -105.26984684640885 39.98934422916937))</t>
         </is>
       </c>
       <c r="H165" t="inlineStr">
@@ -7360,7 +7396,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2460040292133 39.98963593541377, -105.2467369290482 39.99006387816448, -105.2474840945791 39.99049706225706, -105.2478088871432 39.99068609379896, -105.2485859878499 39.99113498504862, -105.248946097095 39.99133012926357, -105.2490551479953 39.99137401601043, -105.2495039201496 39.99152899760701, -105.2499018481588 39.99163198315823, -105.2505979253994 39.99179600699761, -105.2511991538801 39.99193703631351, -105.2521180947648 39.99215890608932, -105.2525991777126 39.99226508096519, -105.2529160599851 39.99237803971734, -105.2529520429993 39.99239596059435, -105.2531030577065 39.99248303242634, -105.2532838677984 39.99262095392066, -105.253481917966 39.99282809124987, -105.2537680195346 39.99316389105262, -105.2539598245705 39.99342097709806, -105.253976992119 39.99350995784211, -105.2539748649406 39.99360493719707, -105.2549139222388 39.99360089751056, -105.2558879427119 39.99360104290265, -105.2562241597075 39.99360010701558, -105.256439076781 39.99358491328484, -105.2566469544573 39.99354197855802, -105.2568431490209 39.99347211537662, -105.2578890938063 39.99291704138979, -105.2581979196601 39.99278893921107, -105.2583630602698 39.99271900831015, -105.2584222456255 39.99269217486411, -105.2576485940671 39.99157272394766, -105.2565448745829 39.99004987770695, -105.2559412881601 39.98947447747421, -105.2557778724409 39.98932087692706, -105.2555178306132 39.98911024176632, -105.2551538717717 39.98889087686553, -105.2543108704154 39.98844087796657, -105.2519739398096 39.98734045241409, -105.2515148505574 39.98707852694061, -105.2510420594896 39.98675222905197, -105.2505868667575 39.9863338807198, -105.2503028658171 39.98605588039614, -105.2500878649971 39.98581688052339, -105.2498907386311 39.98556828381667, -105.2498308463612 39.98559293537799, -105.2496778365173 39.98566590032408, -105.2495749091305 39.98570603061875, -105.2494998736553 39.98573112375553, -105.2493458817763 39.98577992785833, -105.2492658723818 39.98579897023517, -105.2491801709455 39.98581305917854, -105.2488300693012 39.98581504208742, -105.2482519366188 39.98581405567264, -105.2473258418448 39.98581587258087, -105.2473149565125 39.98721288171633, -105.2472800705901 39.98747799228057, -105.2471981173839 39.98782809980144, -105.2470751482517 39.98817098048374, -105.246924079962 39.9884879946819, -105.2467391456733 39.98879395259649, -105.2465228491003 39.98908803727352, -105.2460040292133 39.98963593541377))</t>
+          <t>POLYGON ((-105.24600402921334 39.98963593541377, -105.24673692904815 39.99006387816448, -105.24748409457912 39.990497062257056, -105.24780888714318 39.990686093798956, -105.24858598784989 39.991134985048625, -105.24894609709499 39.991330129263574, -105.24905514799526 39.991374016010425, -105.24950392014964 39.99152899760701, -105.24990184815881 39.99163198315823, -105.25059792539938 39.99179600699761, -105.25119915388011 39.99193703631351, -105.25211809476482 39.99215890608932, -105.2525991777126 39.99226508096519, -105.2529160599851 39.99237803971734, -105.2529520429993 39.99239596059435, -105.25310305770647 39.992483032426335, -105.25328386779843 39.99262095392066, -105.25348191796598 39.99282809124987, -105.25376801953456 39.99316389105262, -105.25395982457049 39.99342097709806, -105.25397699211904 39.993509957842114, -105.25397486494057 39.99360493719707, -105.25491392223877 39.99360089751056, -105.25588794271194 39.993601042902654, -105.25622415970746 39.99360010701558, -105.25643907678104 39.99358491328484, -105.25664695445731 39.99354197855802, -105.25684314902091 39.99347211537662, -105.25788909380631 39.992917041389795, -105.25819791966006 39.992788939211074, -105.2583630602698 39.99271900831015, -105.25842224562547 39.99269217486411, -105.25764859406709 39.99157272394766, -105.25654487458293 39.99004987770695, -105.2559412881601 39.98947447747421, -105.25577787244092 39.98932087692706, -105.25551783061321 39.98911024176632, -105.25515387177167 39.98889087686553, -105.25431087041541 39.988440877966575, -105.25197393980957 39.98734045241409, -105.25151485055741 39.987078526940614, -105.2510420594896 39.986752229051966, -105.25058686675746 39.9863338807198, -105.2503028658171 39.98605588039614, -105.25008786499713 39.98581688052339, -105.24989073863107 39.98556828381667, -105.24983084636125 39.98559293537799, -105.24967783651726 39.98566590032408, -105.24957490913054 39.98570603061875, -105.24949987365528 39.98573112375553, -105.24934588177635 39.98577992785833, -105.24926587238181 39.98579897023517, -105.24918017094546 39.98581305917854, -105.24883006930116 39.98581504208742, -105.24825193661883 39.98581405567264, -105.24732584184483 39.985815872580865, -105.24731495651253 39.98721288171633, -105.24728007059007 39.98747799228057, -105.24719811738392 39.98782809980144, -105.24707514825172 39.988170980483744, -105.246924079962 39.988487994681904, -105.24673914567332 39.98879395259649, -105.24652284910034 39.98908803727352, -105.24600402921334 39.98963593541377))</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
@@ -7402,7 +7438,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2401753611049 39.98955497456853, -105.2401816972446 39.98954904272472, -105.2405530817692 39.9897638630389, -105.2419808182389 39.99058968315889, -105.2424807589426 39.99088294639051, -105.2426875294299 39.99066405991451, -105.24294293165 39.99040233108766, -105.2430139381545 39.99030709924219, -105.2430880959231 39.99023286953971, -105.2442409753642 39.98906405572566, -105.2445229609886 39.98876710100529, -105.2452579682391 39.98919890009814, -105.2460040292133 39.98963593541377, -105.2465228491003 39.98908803727352, -105.2467391456733 39.98879395259649, -105.246924079962 39.9884879946819, -105.2470751482517 39.98817098048374, -105.2471981173839 39.98782809980144, -105.2472800705901 39.98747799228057, -105.2473149565125 39.98721288171633, -105.2473258418448 39.98581587258087, -105.2463901100238 39.98581793554781, -105.245466867449 39.98582001849653, -105.2445368539037 39.98581988324903, -105.2441339418788 39.98582008755279, -105.2436068321087 39.98582193627747, -105.242676088801 39.98582590128977, -105.2424551787016 39.98582705525318, -105.2416761177718 39.98582805727749, -105.2414691317438 39.98582786795451, -105.2411996727348 39.98582803428326, -105.2407878626364 39.98582688655449, -105.2378539436258 39.98581201366842, -105.2373102997409 39.98580362670153, -105.2371104747867 39.98580674587166, -105.236868774774 39.98582406702248, -105.2365712434053 39.98585913179958, -105.236106861085 39.98588791557931, -105.2359640957165 39.98589198116586, -105.2357538722775 39.98589808776029, -105.2356450415273 39.98589399514155, -105.2346318540104 39.98589907961485, -105.2341479195462 39.98590208237118, -105.2339109478228 39.98590400611815, -105.2338788294352 39.98590393197578, -105.2333233018165 39.98589626973319, -105.2333186456079 39.98589620582294, -105.233549133973 39.98600228301675, -105.2343462575852 39.98636654917703, -105.2345601331849 39.9864642829105, -105.2347186571129 39.98653701728261, -105.2347301344601 39.98654228280646, -105.2347290390252 39.98654275943437, -105.2401753611049 39.98955497456853))</t>
+          <t>POLYGON ((-105.24017536110495 39.98955497456853, -105.24018169724461 39.98954904272472, -105.24055308176924 39.9897638630389, -105.24198081823887 39.99058968315889, -105.24248075894259 39.990882946390506, -105.24268752942986 39.990664059914515, -105.24294293165002 39.99040233108766, -105.24301393815448 39.99030709924219, -105.24308809592307 39.99023286953971, -105.24424097536418 39.989064055725656, -105.2445229609886 39.98876710100529, -105.24525796823914 39.98919890009814, -105.24600402921334 39.98963593541377, -105.24652284910034 39.98908803727352, -105.24673914567332 39.98879395259649, -105.246924079962 39.988487994681904, -105.24707514825172 39.988170980483744, -105.24719811738392 39.98782809980144, -105.24728007059007 39.98747799228057, -105.24731495651253 39.98721288171633, -105.24732584184483 39.985815872580865, -105.24639011002384 39.98581793554781, -105.24546686744904 39.98582001849653, -105.24453685390372 39.98581988324903, -105.24413394187879 39.98582008755279, -105.24360683210871 39.98582193627747, -105.242676088801 39.98582590128977, -105.24245517870163 39.98582705525318, -105.2416761177718 39.98582805727749, -105.24146913174377 39.98582786795451, -105.24119967273481 39.98582803428326, -105.24078786263638 39.98582688655449, -105.23785394362575 39.98581201366842, -105.23731029974091 39.985803626701525, -105.23711047478675 39.98580674587166, -105.23686877477401 39.98582406702248, -105.2365712434053 39.98585913179958, -105.23610686108499 39.98588791557931, -105.2359640957165 39.98589198116586, -105.23575387227753 39.98589808776029, -105.23564504152726 39.985893995141545, -105.2346318540104 39.985899079614846, -105.23414791954623 39.985902082371176, -105.23391094782285 39.98590400611815, -105.23387882943517 39.985903931975784, -105.23332330181648 39.98589626973319, -105.23331864560794 39.98589620582294, -105.23354913397304 39.986002283016745, -105.23434625758517 39.98636654917703, -105.2345601331849 39.986464282910504, -105.23471865711292 39.98653701728261, -105.23473013446012 39.98654228280646, -105.23472903902515 39.98654275943437, -105.24017536110495 39.98955497456853))</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
@@ -7444,7 +7480,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2364579412395 39.99126711967727, -105.2364661425782 39.99228505947059, -105.2364689106397 39.99313909730117, -105.2383238322312 39.99312712594978, -105.2383338522648 39.99274803609929, -105.238382164903 39.99252798068977, -105.2388690597486 39.99129786242749, -105.2390219540881 39.99088807473773, -105.2391079433111 39.99070790962207, -105.2392249466247 39.99053687428649, -105.2392999425185 39.99043107915255, -105.239842460506 39.98986669522325, -105.2398430835623 39.98986604725708, -105.2398431564504 39.98986597086589, -105.2401753611049 39.98955497456853, -105.2347290390252 39.98654275943437, -105.2347301344601 39.98654228280646, -105.2347186571129 39.98653701728261, -105.2345601331849 39.9864642829105, -105.233549133973 39.98600228301675, -105.2333186456079 39.98589620582294, -105.2331971337308 39.985840282157, -105.2330351331852 39.98576428266011, -105.2327191338569 39.98561728215761, -105.2325671332445 39.98554728283532, -105.2324551331664 39.98549528298939, -105.2323551334779 39.9854482825155, -105.2319832192942 39.98527649380193, -105.2319792472305 39.9853401131802, -105.2317468861034 39.98770945571772, -105.2316927465716 39.98847784361123, -105.2316858085995 39.98906046766875, -105.2316726259023 39.99123014769962, -105.2316639565938 39.99225242952157, -105.2319781356781 39.99225604515681, -105.2337859500843 39.9922368996541, -105.2338809414382 39.99222311828235, -105.2340638469615 39.99217989190147, -105.2342361253701 39.99211605176179, -105.2344139012137 39.99201488828059, -105.2345710429928 39.99189693204435, -105.234761912102 39.99173293425835, -105.2351889848636 39.99140202108246, -105.2352959661362 39.99133308746169, -105.2354221365493 39.99128588555319, -105.2355325627036 39.99126818617076, -105.2355589146679 39.99126396310474, -105.2364579412395 39.99126711967727))</t>
+          <t>POLYGON ((-105.23645794123948 39.991267119677275, -105.23646614257817 39.99228505947059, -105.23646891063972 39.99313909730117, -105.23832383223122 39.99312712594978, -105.23833385226479 39.992748036099286, -105.23838216490296 39.99252798068977, -105.23886905974862 39.991297862427494, -105.23902195408814 39.990888074737725, -105.23910794331107 39.99070790962207, -105.23922494662469 39.99053687428649, -105.23929994251853 39.99043107915255, -105.23984246050595 39.98986669522325, -105.2398430835623 39.98986604725708, -105.23984315645038 39.989865970865885, -105.24017536110495 39.98955497456853, -105.23472903902515 39.98654275943437, -105.23473013446012 39.98654228280646, -105.23471865711292 39.98653701728261, -105.2345601331849 39.986464282910504, -105.23354913397304 39.986002283016745, -105.23331864560794 39.98589620582294, -105.23319713373081 39.985840282157, -105.23303513318524 39.985764282660114, -105.23271913385688 39.985617282157605, -105.23256713324454 39.98554728283532, -105.23245513316638 39.98549528298939, -105.23235513347785 39.9854482825155, -105.2319832192942 39.985276493801926, -105.23197924723054 39.9853401131802, -105.23174688610335 39.98770945571772, -105.23169274657157 39.98847784361123, -105.2316858085995 39.98906046766875, -105.2316726259023 39.99123014769962, -105.23166395659383 39.99225242952157, -105.23197813567813 39.99225604515681, -105.23378595008428 39.992236899654095, -105.23388094143822 39.992223118282354, -105.2340638469615 39.99217989190147, -105.23423612537013 39.99211605176179, -105.23441390121366 39.992014888280586, -105.23457104299275 39.99189693204435, -105.23476191210203 39.99173293425835, -105.23518898486363 39.991402021082465, -105.23529596613622 39.99133308746169, -105.23542213654926 39.99128588555319, -105.23553256270363 39.99126818617076, -105.23555891466789 39.991263963104736, -105.23645794123948 39.991267119677275))</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
@@ -7486,7 +7522,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.229031966724 39.99303703141354, -105.2290840685852 39.99312911793925, -105.2291718231109 39.99323007318709, -105.2292899710431 39.99331792225447, -105.2293740232478 39.9933628668272, -105.2296098574216 39.99347487532473, -105.229713055697 39.99355198280633, -105.2297969400669 39.99364002571505, -105.2298770748835 39.9937730817142, -105.2299091280582 39.99388104265839, -105.2299169005759 39.9939908696123, -105.2299060183916 39.9951169256626, -105.2298980465868 39.99613812158013, -105.2298920220077 39.99648812079264, -105.2298559013762 39.99668596493536, -105.229802148455 39.99682996173368, -105.2296939947666 39.99701089201523, -105.2294709466912 39.99727198652509, -105.2293828985478 39.99742304033567, -105.2293280049977 39.99758405479982, -105.2293141162702 39.99766610335006, -105.2293189801351 39.99859893439575, -105.2293179557386 39.99894702324459, -105.2293401491907 39.99911096383681, -105.2293679223644 39.99921809162684, -105.229524157622 39.9996049821949, -105.2295580641257 39.99978597077631, -105.2295661712776 39.9999918793853, -105.2295648744829 40.00004897693059, -105.230829196794 40.00005357463328, -105.2312149162657 40.00006519764642, -105.2315727911532 40.00006603135803, -105.2316392818717 39.99734243241262, -105.2316456813471 39.99571605960905, -105.2316639565938 39.99225242952157, -105.2316726259023 39.99123014769962, -105.2316858085995 39.98906046766875, -105.2316927465716 39.98847784361123, -105.2317468861034 39.98770945571772, -105.2319792472305 39.9853401131802, -105.2319832192942 39.98527649380193, -105.2319351336893 39.9852542826066, -105.2311531345965 39.98489128325956, -105.2309501326586 39.98479628222291, -105.2302491328946 39.98447128245876, -105.2293111332321 39.98403928262311, -105.228734132372 39.98377128349869, -105.2276381336663 39.98326528294741, -105.2268921334482 39.98292028334055, -105.2259871327598 39.98250228293273, -105.2259021321316 39.9824632823856, -105.2233041316678 39.98126628283385, -105.221716133175 39.98053428301674, -105.2212231314078 39.9803062839601, -105.2211641313148 39.98041428305446, -105.2208531327514 39.98027028363045, -105.2205521325287 39.98013228345715, -105.2205507460672 39.98013349868391, -105.220540062076 39.98012857681351, -105.2205429995072 39.98012599905148, -105.2198569987801 39.97980999936001, -105.217670999848 39.9788049982916, -105.2175789989619 39.97876299865521, -105.216200462426 39.97812263862686, -105.2161149998271 39.9782349994438, -105.2160471505688 39.97825984715396, -105.2149131886728 39.97773343595954, -105.2128301877808 39.97808843595108, -105.2128395034223 39.98012199063935, -105.212833000599 39.98012599947322, -105.2128330007686 39.98049724201171, -105.21283300067 39.9809199993889, -105.2128303968119 39.98311209701794, -105.212830000377 39.98344599815635, -105.2128298606279 39.98346834759489, -105.2128279999043 39.98376599906238, -105.2128239999816 39.98447999876575, -105.2128219705335 39.98490281397867, -105.2128209987258 39.98510499896647, -105.2128335385606 39.98575351525029, -105.212838999747 39.98603599893198, -105.2128393984281 39.98605755172515, -105.2128408265147 39.98613467486216, -105.2129348461996 39.986122924, -105.2159614741359 39.98608864702656, -105.2185404142695 39.98606441335764, -105.2206587622344 39.98604446297291, -105.2206616558601 39.98611582894792, -105.222234990267 39.98609839414738, -105.2222353497503 39.98602247873587, -105.223084657606 39.98601975668618, -105.2237453083268 39.98601482465087, -105.2239582758726 39.98601323449112, -105.2245736987022 39.98600863702274, -105.2254644467161 39.98600197681813, -105.2259757261998 39.98599553233836, -105.2270013766576 39.98600585559555, -105.2269992934832 39.98608841196461, -105.2269904941112 39.98643693044628, -105.2269848063165 39.98666212230915, -105.2269788017231 39.98690004958741, -105.2269729632646 39.98860175680049, -105.2269656014882 39.98939425758067, -105.2269697053404 39.99030109572695, -105.2269745738349 39.99240084977456, -105.2269704853094 39.99317677606326, -105.2288649980137 39.99317226849462, -105.2288806839204 39.99292905828161, -105.228996035092 39.99291807940918, -105.229031966724 39.99303703141354))</t>
+          <t>POLYGON ((-105.22903196672401 39.993037031413536, -105.22908406858515 39.99312911793925, -105.22917182311087 39.99323007318709, -105.22928997104306 39.99331792225447, -105.22937402324784 39.993362866827205, -105.22960985742161 39.99347487532473, -105.22971305569698 39.99355198280633, -105.22979694006688 39.993640025715045, -105.22987707488346 39.9937730817142, -105.22990912805824 39.993881042658394, -105.22991690057586 39.9939908696123, -105.2299060183916 39.9951169256626, -105.22989804658681 39.99613812158013, -105.22989202200772 39.99648812079264, -105.22985590137618 39.99668596493536, -105.22980214845495 39.99682996173368, -105.22969399476659 39.997010892015226, -105.22947094669117 39.997271986525085, -105.2293828985478 39.99742304033567, -105.22932800499767 39.997584054799816, -105.22931411627023 39.997666103350056, -105.22931898013515 39.99859893439575, -105.22931795573858 39.99894702324459, -105.22934014919069 39.99911096383681, -105.22936792236442 39.999218091626844, -105.22952415762204 39.9996049821949, -105.22955806412571 39.99978597077631, -105.2295661712776 39.9999918793853, -105.22956487448295 40.00004897693059, -105.23082919679398 40.00005357463328, -105.23121491626574 40.00006519764642, -105.2315727911532 40.00006603135803, -105.23163928187168 39.99734243241262, -105.2316456813471 39.99571605960905, -105.23166395659383 39.99225242952157, -105.2316726259023 39.99123014769962, -105.2316858085995 39.98906046766875, -105.23169274657157 39.98847784361123, -105.23174688610335 39.98770945571772, -105.23197924723054 39.9853401131802, -105.2319832192942 39.985276493801926, -105.2319351336893 39.9852542826066, -105.23115313459652 39.984891283259564, -105.23095013265858 39.98479628222291, -105.23024913289461 39.98447128245876, -105.22931113323214 39.98403928262311, -105.22873413237197 39.98377128349869, -105.22763813366635 39.983265282947414, -105.22689213344817 39.982920283340555, -105.22598713275978 39.98250228293273, -105.22590213213158 39.9824632823856, -105.22330413166777 39.98126628283385, -105.22171613317498 39.98053428301674, -105.22122313140781 39.980306283960104, -105.22116413131482 39.980414283054465, -105.22085313275137 39.98027028363045, -105.22055213252868 39.980132283457145, -105.22055074606725 39.98013349868391, -105.22054006207604 39.98012857681351, -105.22054299950722 39.98012599905148, -105.21985699878006 39.97980999936001, -105.21767099984795 39.9788049982916, -105.21757899896187 39.978762998655206, -105.21620046242603 39.978122638626864, -105.21611499982714 39.9782349994438, -105.21604715056883 39.97825984715396, -105.21491318867275 39.97773343595954, -105.21283018778081 39.97808843595108, -105.21283950342234 39.980121990639354, -105.21283300059898 39.980125999473216, -105.21283300076855 39.98049724201171, -105.21283300067002 39.9809199993889, -105.21283039681194 39.98311209701794, -105.21283000037698 39.98344599815635, -105.21282986062786 39.983468347594886, -105.21282799990433 39.983765999062385, -105.21282399998162 39.98447999876575, -105.21282197053348 39.98490281397867, -105.2128209987258 39.98510499896647, -105.21283353856064 39.98575351525029, -105.21283899974702 39.98603599893198, -105.21283939842807 39.986057551725146, -105.21284082651475 39.98613467486216, -105.2129348461996 39.986122924, -105.21596147413587 39.98608864702656, -105.21854041426948 39.98606441335764, -105.22065876223436 39.986044462972906, -105.22066165586011 39.986115828947916, -105.22223499026695 39.986098394147376, -105.22223534975033 39.98602247873587, -105.223084657606 39.98601975668618, -105.22374530832681 39.98601482465087, -105.22395827587256 39.98601323449112, -105.22457369870224 39.98600863702274, -105.22546444671612 39.98600197681813, -105.22597572619978 39.985995532338364, -105.22700137665757 39.98600585559555, -105.2269992934832 39.98608841196461, -105.22699049411118 39.98643693044628, -105.22698480631654 39.98666212230915, -105.22697880172308 39.98690004958741, -105.22697296326457 39.98860175680049, -105.22696560148822 39.98939425758067, -105.22696970534042 39.99030109572695, -105.22697457383491 39.99240084977456, -105.22697048530941 39.99317677606326, -105.22886499801375 39.99317226849462, -105.22888068392042 39.99292905828161, -105.22899603509195 39.99291807940918, -105.22903196672401 39.993037031413536))</t>
         </is>
       </c>
       <c r="H169" t="inlineStr">
@@ -7528,7 +7564,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.236106861085 39.98588791557931, -105.2365712434053 39.98585913179958, -105.236868774774 39.98582406702248, -105.2371104747867 39.98580674587166, -105.2373102997409 39.98580362670153, -105.2378539436258 39.98581201366842, -105.2407878626364 39.98582688655449, -105.2411996727348 39.98582803428326, -105.2412161612756 39.98581118581514, -105.2412180325216 39.98572038955676, -105.2412176870151 39.98554419629536, -105.2412173382405 39.98536608732999, -105.2412169821173 39.98518466933762, -105.2412166236751 39.98500046831209, -105.2412162660193 39.98481914668028, -105.2412164735184 39.98463668428315, -105.2412169126676 39.98445118088985, -105.2412173609239 39.98426235049294, -105.2412177359399 39.98410424398539, -105.2412177998155 39.98407691374117, -105.2412182364348 39.98389238394111, -105.2412186923771 39.98369998245297, -105.2412191350575 39.98351354507192, -105.2412203511739 39.98332568638834, -105.2412231590182 39.98313396115834, -105.2412258748471 39.98294858714085, -105.24122868688 39.98275667547787, -105.2412314708192 39.98256661009216, -105.241234437705 39.98236380624208, -105.2412361128316 39.98225924749787, -105.2416650065276 39.9822600924146, -105.2426631056501 39.98226699125357, -105.2435809278364 39.98227013450452, -105.2445248264287 39.98226591675018, -105.2454590670426 39.9822679835349, -105.2463829480082 39.98227303985243, -105.2466499210034 39.98226099884663, -105.2468911033262 39.9822749799717, -105.2469899345277 39.98227986413753, -105.245800143718 39.98094801864188, -105.2428560147591 39.97766810735965, -105.2414479703547 39.97615811412556, -105.2409141414532 39.97559991366145, -105.2404348886767 39.97508956116814, -105.2396065640024 39.97421909272716, -105.2393131352965 39.97390608003223, -105.2388245148268 39.97340234006232, -105.2383062013195 39.97287214043273, -105.2379128811428 39.97246018080529, -105.2377694636597 39.97230257655232, -105.2375705868881 39.97206978243837, -105.2374503865781 39.97191580534781, -105.2373302280914 39.97175110590815, -105.2371871588444 39.97150413946797, -105.237145594438 39.97143970447904, -105.2367095939701 39.97148016108699, -105.2365775120796 39.97147915946314, -105.2365447584172 39.97740785472327, -105.23652737028 39.97869697347777, -105.2362905994008 39.97869735158999, -105.2361100107017 39.97869764079686, -105.2360114515747 39.97869779969002, -105.2359151507977 39.9786979519646, -105.23574588659 39.97869821791085, -105.2358082160567 39.97966765483083, -105.2358130239537 39.98052568467754, -105.2358035452942 39.98180777708973, -105.2358026320149 39.98204751514026, -105.2358045579366 39.98229842422084, -105.2358064545418 39.98254813985963, -105.235808481226 39.98279692091025, -105.2358101945944 39.98290743528528, -105.2357031936082 39.98290643525121, -105.2356141949383 39.982911435147, -105.2354961950666 39.98292443470311, -105.2354367320685 39.98293455581012, -105.2353914103151 39.98294306835437, -105.2353161938382 39.98296143476448, -105.2352661936963 39.98297443439139, -105.2351831945578 39.98300343489522, -105.2351031942518 39.98303743456508, -105.2349811943916 39.98310443492078, -105.2349301934007 39.98313843449031, -105.2348791936221 39.98317843510868, -105.2348191932734 39.98323243460499, -105.2347761939119 39.98327743510863, -105.2347301939354 39.98333743541542, -105.2346971935738 39.98338743502155, -105.2346317056057 39.98345129657835, -105.2349847390988 39.98373861991558, -105.2352982587296 39.9841027503011, -105.2355534442347 39.98455599286225, -105.2358411338562 39.98516866769616, -105.2360001678611 39.98571875967034, -105.236106861085 39.98588791557931))</t>
+          <t>POLYGON ((-105.23610686108499 39.98588791557931, -105.2365712434053 39.98585913179958, -105.23686877477401 39.98582406702248, -105.23711047478675 39.98580674587166, -105.23731029974091 39.985803626701525, -105.23785394362575 39.98581201366842, -105.24078786263638 39.98582688655449, -105.24119967273481 39.98582803428326, -105.24121616127562 39.985811185815145, -105.24121803252163 39.98572038955676, -105.24121768701507 39.98554419629536, -105.24121733824047 39.985366087329986, -105.2412169821173 39.98518466933762, -105.24121662367509 39.98500046831209, -105.24121626601926 39.98481914668028, -105.24121647351838 39.98463668428315, -105.24121691266764 39.98445118088985, -105.24121736092386 39.98426235049294, -105.24121773593991 39.98410424398539, -105.24121779981546 39.98407691374117, -105.2412182364348 39.98389238394111, -105.24121869237712 39.98369998245297, -105.24121913505755 39.983513545071915, -105.2412203511739 39.98332568638834, -105.24122315901823 39.983133961158345, -105.24122587484713 39.982948587140854, -105.24122868688002 39.982756675477866, -105.2412314708192 39.98256661009216, -105.241234437705 39.98236380624208, -105.24123611283164 39.98225924749787, -105.24166500652758 39.9822600924146, -105.24266310565008 39.982266991253574, -105.2435809278364 39.982270134504525, -105.24452482642873 39.98226591675018, -105.24545906704256 39.982267983534896, -105.24638294800822 39.98227303985243, -105.2466499210034 39.982260998846634, -105.24689110332625 39.9822749799717, -105.24698993452773 39.98227986413753, -105.24580014371804 39.980948018641875, -105.24285601475908 39.977668107359655, -105.24144797035473 39.97615811412556, -105.24091414145316 39.97559991366145, -105.2404348886767 39.97508956116814, -105.23960656400237 39.97421909272716, -105.23931313529647 39.97390608003223, -105.23882451482685 39.97340234006232, -105.23830620131949 39.97287214043273, -105.23791288114278 39.972460180805285, -105.2377694636597 39.972302576552316, -105.23757058688808 39.97206978243837, -105.2374503865781 39.97191580534781, -105.23733022809137 39.97175110590815, -105.23718715884438 39.97150413946797, -105.23714559443803 39.97143970447904, -105.23670959397008 39.971480161086994, -105.23657751207963 39.971479159463144, -105.2365447584172 39.977407854723275, -105.23652737028 39.97869697347777, -105.23629059940077 39.97869735158999, -105.23611001070167 39.97869764079686, -105.23601145157468 39.978697799690025, -105.23591515079774 39.9786979519646, -105.23574588659004 39.978698217910846, -105.23580821605674 39.97966765483083, -105.23581302395368 39.98052568467754, -105.23580354529419 39.98180777708973, -105.23580263201492 39.98204751514026, -105.23580455793662 39.98229842422084, -105.23580645454177 39.98254813985963, -105.23580848122603 39.98279692091025, -105.23581019459436 39.98290743528528, -105.23570319360816 39.98290643525121, -105.23561419493826 39.982911435147, -105.23549619506663 39.98292443470311, -105.23543673206854 39.98293455581012, -105.23539141031515 39.982943068354366, -105.23531619383822 39.982961434764476, -105.23526619369633 39.982974434391394, -105.23518319455782 39.983003434895224, -105.23510319425176 39.983037434565084, -105.23498119439161 39.983104434920776, -105.23493019340074 39.98313843449031, -105.23487919362213 39.98317843510868, -105.23481919327338 39.98323243460499, -105.2347761939119 39.98327743510863, -105.23473019393542 39.98333743541542, -105.23469719357382 39.98338743502155, -105.23463170560565 39.98345129657835, -105.23498473909878 39.98373861991558, -105.23529825872961 39.9841027503011, -105.2355534442347 39.98455599286225, -105.23584113385618 39.985168667696165, -105.23600016786109 39.98571875967034, -105.23610686108499 39.98588791557931))</t>
         </is>
       </c>
       <c r="H170" t="inlineStr">
@@ -7570,7 +7606,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2412361128316 39.98225924749787, -105.241234437705 39.98236380624208, -105.2412314708192 39.98256661009216, -105.24122868688 39.98275667547787, -105.2412258748471 39.98294858714085, -105.2412231590182 39.98313396115834, -105.2412203511739 39.98332568638834, -105.2412191350575 39.98351354507192, -105.2412186923771 39.98369998245297, -105.2412182364348 39.98389238394111, -105.2412177998155 39.98407691374117, -105.2412177359399 39.98410424398539, -105.2412173609239 39.98426235049294, -105.2412169126676 39.98445118088985, -105.2412164735184 39.98463668428315, -105.2412162660193 39.98481914668028, -105.2412166236751 39.98500046831209, -105.2412169821173 39.98518466933762, -105.2412173382405 39.98536608732999, -105.2412176870151 39.98554419629536, -105.2412180325216 39.98572038955676, -105.2412161612756 39.98581118581514, -105.2411996727348 39.98582803428326, -105.2414691317438 39.98582786795451, -105.2416761177718 39.98582805727749, -105.2424551787016 39.98582705525318, -105.242676088801 39.98582590128977, -105.2436068321087 39.98582193627747, -105.2441339418788 39.98582008755279, -105.2445368539037 39.98581988324903, -105.245466867449 39.98582001849653, -105.2463901100238 39.98581793554781, -105.2473258418448 39.98581587258087, -105.2482519366188 39.98581405567264, -105.2488300693012 39.98581504208742, -105.2491801709455 39.98581305917854, -105.2492658723818 39.98579897023517, -105.2493458817763 39.98577992785833, -105.2494998736553 39.98573112375553, -105.2495749091305 39.98570603061875, -105.2496778365173 39.98566590032408, -105.2498308463612 39.98559293537799, -105.2498907386311 39.98556828381667, -105.2490193084578 39.98459719669388, -105.2476126961791 39.98297845907786, -105.2469899345277 39.98227986413753, -105.2468911033262 39.9822749799717, -105.2466499210034 39.98226099884663, -105.2463829480082 39.98227303985243, -105.2454590670426 39.9822679835349, -105.2445248264287 39.98226591675018, -105.2435809278364 39.98227013450452, -105.2426631056501 39.98226699125357, -105.2416650065276 39.9822600924146, -105.2412361128316 39.98225924749787))</t>
+          <t>POLYGON ((-105.24123611283164 39.98225924749787, -105.241234437705 39.98236380624208, -105.2412314708192 39.98256661009216, -105.24122868688002 39.982756675477866, -105.24122587484713 39.982948587140854, -105.24122315901823 39.983133961158345, -105.2412203511739 39.98332568638834, -105.24121913505755 39.983513545071915, -105.24121869237712 39.98369998245297, -105.2412182364348 39.98389238394111, -105.24121779981546 39.98407691374117, -105.24121773593991 39.98410424398539, -105.24121736092386 39.98426235049294, -105.24121691266764 39.98445118088985, -105.24121647351838 39.98463668428315, -105.24121626601926 39.98481914668028, -105.24121662367509 39.98500046831209, -105.2412169821173 39.98518466933762, -105.24121733824047 39.985366087329986, -105.24121768701507 39.98554419629536, -105.24121803252163 39.98572038955676, -105.24121616127562 39.985811185815145, -105.24119967273481 39.98582803428326, -105.24146913174377 39.98582786795451, -105.2416761177718 39.98582805727749, -105.24245517870163 39.98582705525318, -105.242676088801 39.98582590128977, -105.24360683210871 39.98582193627747, -105.24413394187879 39.98582008755279, -105.24453685390372 39.98581988324903, -105.24546686744904 39.98582001849653, -105.24639011002384 39.98581793554781, -105.24732584184483 39.985815872580865, -105.24825193661883 39.98581405567264, -105.24883006930116 39.98581504208742, -105.24918017094546 39.98581305917854, -105.24926587238181 39.98579897023517, -105.24934588177635 39.98577992785833, -105.24949987365528 39.98573112375553, -105.24957490913054 39.98570603061875, -105.24967783651726 39.98566590032408, -105.24983084636125 39.98559293537799, -105.24989073863107 39.98556828381667, -105.24901930845785 39.984597196693876, -105.24761269617913 39.98297845907786, -105.24698993452773 39.98227986413753, -105.24689110332625 39.9822749799717, -105.2466499210034 39.982260998846634, -105.24638294800822 39.98227303985243, -105.24545906704256 39.982267983534896, -105.24452482642873 39.98226591675018, -105.2435809278364 39.982270134504525, -105.24266310565008 39.982266991253574, -105.24166500652758 39.9822600924146, -105.24123611283164 39.98225924749787))</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
@@ -7612,7 +7648,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2469899345277 39.98227986413753, -105.2476126961791 39.98297845907786, -105.2490193084578 39.98459719669388, -105.2498907386311 39.98556828381667, -105.2500764747387 39.98548237868278, -105.250285970502 39.98537559890283, -105.2505514353589 39.98521174737539, -105.2507192003461 39.98507985450048, -105.2508776457729 39.98495508973993, -105.2511573353756 39.98471262956502, -105.2514508442976 39.98450236810509, -105.2515999032001 39.98440260411046, -105.2519907553042 39.98425689199309, -105.2525213178784 39.98402569028387, -105.2530193237723 39.98380156668554, -105.2532753787122 39.98366628452531, -105.2534058854819 39.98355575438762, -105.2539235545214 39.98303141215703, -105.255127835323 39.98163804141733, -105.2553185850252 39.98144373743585, -105.2554632154886 39.98127961803709, -105.2556216049941 39.98116557073261, -105.2558124675118 39.98106588900765, -105.2560729999783 39.98097350472325, -105.2562962594057 39.98090963595508, -105.2571982901938 39.98073639001605, -105.2594349816054 39.98024065229194, -105.2596720231951 39.98021969945855, -105.2599182938995 39.98021663796225, -105.2601323605739 39.9802193019425, -105.2601270663233 39.97988805426846, -105.2601240925484 39.97971894376179, -105.2601148541277 39.97909905757952, -105.2601128299923 39.97876111940365, -105.2587978821324 39.97876194364169, -105.2574351597284 39.97875112306168, -105.2565470129442 39.97874513280774, -105.2556071116555 39.97874286908414, -105.2548084360336 39.97873894737987, -105.2546219021326 39.97873803075372, -105.2538251064159 39.97873193926058, -105.2534379337529 39.97873303370792, -105.2529308837927 39.97872892806342, -105.2520448639634 39.97872702547376, -105.2511381731693 39.97871793375031, -105.2506028915245 39.9787250123996, -105.2505029630528 39.97872891393846, -105.2504540584652 39.97873402466791, -105.2504051496909 39.97873995766609, -105.2503558798193 39.97874698866123, -105.2503069611447 39.97875594149448, -105.2502591032779 39.97876709330425, -105.2502119576847 39.97877907073762, -105.2501651609402 39.97879296910547, -105.2501190742881 39.97880796779358, -105.2500740536243 39.97882406757441, -105.2500300959376 39.9788420898406, -105.2496579462505 39.97902795654765, -105.2489968741238 39.97937488524389, -105.2482510874011 39.97975896003506, -105.2474948699503 39.98016304674198, -105.2469939547208 39.98042603675346, -105.2466978596759 39.98059504023666, -105.2465098781437 39.98067011993611, -105.2462461766525 39.98076397524878, -105.2459760636716 39.98085397183197, -105.2458591469235 39.98091493167031, -105.245800143718 39.98094801864188, -105.2469899345277 39.98227986413753))</t>
+          <t>POLYGON ((-105.24698993452773 39.98227986413753, -105.24761269617913 39.98297845907786, -105.24901930845785 39.984597196693876, -105.24989073863107 39.98556828381667, -105.2500764747387 39.985482378682775, -105.25028597050202 39.98537559890283, -105.25055143535891 39.98521174737539, -105.25071920034608 39.98507985450048, -105.25087764577286 39.984955089739934, -105.25115733537555 39.98471262956502, -105.25145084429761 39.98450236810509, -105.25159990320013 39.98440260411046, -105.25199075530425 39.98425689199309, -105.2525213178784 39.98402569028387, -105.25301932377232 39.983801566685536, -105.2532753787122 39.98366628452531, -105.25340588548192 39.983555754387616, -105.25392355452144 39.983031412157025, -105.25512783532298 39.98163804141733, -105.25531858502515 39.98144373743585, -105.25546321548865 39.981279618037085, -105.25562160499409 39.98116557073261, -105.25581246751177 39.98106588900765, -105.2560729999783 39.980973504723245, -105.25629625940572 39.98090963595508, -105.25719829019384 39.98073639001605, -105.25943498160535 39.98024065229194, -105.25967202319507 39.98021969945855, -105.25991829389952 39.98021663796225, -105.26013236057389 39.980219301942505, -105.26012706632332 39.97988805426846, -105.26012409254835 39.97971894376179, -105.2601148541277 39.97909905757952, -105.26011282999228 39.97876111940365, -105.25879788213238 39.97876194364169, -105.2574351597284 39.978751123061684, -105.25654701294424 39.97874513280774, -105.25560711165545 39.97874286908414, -105.25480843603364 39.97873894737987, -105.25462190213261 39.978738030753725, -105.25382510641593 39.97873193926058, -105.25343793375289 39.97873303370792, -105.25293088379273 39.97872892806342, -105.25204486396343 39.97872702547376, -105.25113817316925 39.97871793375031, -105.25060289152445 39.9787250123996, -105.25050296305275 39.97872891393846, -105.25045405846517 39.97873402466791, -105.25040514969093 39.978739957666086, -105.25035587981932 39.97874698866123, -105.25030696114473 39.97875594149448, -105.25025910327791 39.97876709330425, -105.25021195768473 39.978779070737616, -105.25016516094021 39.97879296910547, -105.25011907428814 39.97880796779358, -105.25007405362432 39.97882406757441, -105.2500300959376 39.978842089840605, -105.24965794625051 39.97902795654765, -105.24899687412376 39.97937488524389, -105.24825108740106 39.979758960035056, -105.24749486995034 39.98016304674198, -105.24699395472084 39.98042603675346, -105.24669785967588 39.980595040236665, -105.24650987814371 39.98067011993611, -105.24624617665252 39.98076397524878, -105.24597606367163 39.98085397183197, -105.24585914692348 39.98091493167031, -105.24580014371804 39.980948018641875, -105.24698993452773 39.98227986413753))</t>
         </is>
       </c>
       <c r="H172" t="inlineStr">
@@ -7654,10 +7690,14 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2861390115304 39.9722881143455, -105.2858238862138 39.97236126581304, -105.27937173981 39.97062142832051, -105.2725517491279 39.97264797001431, -105.271852448133 39.97308048041847, -105.2715141300797 39.97329796337442, -105.2710101713048 39.97334763678315, -105.270307086264 39.97305969060716, -105.2697051344663 39.97289908688346, -105.2692628275347 39.97275407844554, -105.2691738497955 39.97268801552585, -105.2690799989563 39.97258598049818, -105.2690168630316 39.97247494815974, -105.2689518921809 39.97237900979596, -105.2685800812342 39.97206997752857, -105.2685508772606 39.97205399709568, -105.2684250963644 39.97200405616698, -105.2682871089833 39.97197605214665, -105.2678989563334 39.97196209453039, -105.2678150881506 39.97196796449851, -105.2676519270121 39.97199810756532, -105.2674990387551 39.97204995801228, -105.2672269835133 39.97220506197835, -105.2675241635705 39.97252987079597, -105.2675699456847 39.97260188768651, -105.2676559560471 39.97301493963212, -105.2676558232941 39.97305392063711, -105.2676291675686 39.97312798814713, -105.2675718637409 39.97319101215554, -105.2666550309857 39.97366490295155, -105.2667058624657 39.97372100771231, -105.2667850117981 39.97384387860475, -105.2668418659355 39.97401694200342, -105.2668598632439 39.97418004298486, -105.2668451742927 39.97430190077704, -105.2667868299745 39.97445990631218, -105.266692839123 39.97460795677274, -105.2665689187773 39.9747430446541, -105.2664161606558 39.97485913137701, -105.2660540573271 39.97504809120751, -105.2657899058223 39.97518289262955, -105.2653280294155 39.97543506074108, -105.2649458519276 39.97564895769812, -105.2645848340075 39.97583105123501, -105.2638469416451 39.97623912559444, -105.2637739724697 39.97629003692276, -105.263615040984 39.9764349327568, -105.2633100577322 39.97681698813182, -105.2630501760598 39.97715713335895, -105.2628789145055 39.97735800467315, -105.2627520289152 39.97752108281585, -105.26252984924 39.9776900043216, -105.2623861695196 39.97775696645165, -105.2620860198477 39.97787493928896, -105.2615248868786 39.97803190413939, -105.2614059907024 39.97805197236678, -105.2611229553935 39.97807087721965, -105.2610451726245 39.97806906869406, -105.2601148835307 39.97807592132791, -105.2601128299923 39.97876111940365, -105.2601148541277 39.97909905757952, -105.2601240925484 39.97971894376179, -105.2601270663233 39.97988805426846, -105.2601323605739 39.9802193019425, -105.2599182938995 39.98021663796225, -105.2596720231951 39.98021969945855, -105.2594349816054 39.98024065229194, -105.2571982901938 39.98073639001605, -105.2562962594057 39.98090963595508, -105.2563429162402 39.98103886783078, -105.2565239845004 39.98149797393191, -105.2566190534311 39.98165712142143, -105.2567530779354 39.98179988076132, -105.256964863671 39.98195186270966, -105.2572230666266 39.9820970781437, -105.2580081412259 39.98250090116355, -105.2585298309313 39.98190601192692, -105.2587659545189 39.98203909986017, -105.2590951262364 39.98219791177391, -105.2594090755475 39.98232292541489, -105.2595830614137 39.98236803476654, -105.2598249010107 39.98239901077235, -105.2609279514417 39.98239691129109, -105.2618568300338 39.98240212864589, -105.2620281769223 39.98238601133514, -105.2622488849338 39.98233705323542, -105.2624050298437 39.98227999986478, -105.2625501634418 39.98220810062183, -105.2632858671283 39.98173194873376, -105.2636771671341 39.98208907864245, -105.2638610800784 39.98225691251253, -105.2644248927018 39.98277910578437, -105.264593914942 39.98292000547517, -105.2647808344368 39.98304501876047, -105.2653939206792 39.9833559267931, -105.2658890858176 39.98361004180648, -105.266313014888 39.98382502725105, -105.2671729209081 39.98428302002201, -105.2672730197861 39.98433592936551, -105.267683104764 39.98453194102219, -105.2679329289423 39.98463209445797, -105.2682309574687 39.9847241095941, -105.2685961061897 39.98480802222888, -105.2689670763001 39.98485900393208, -105.2692050571009 39.98487402981937, -105.2693230565022 39.98487477127614, -105.2693219715217 39.98568827537257, -105.2770692361139 39.98569787181271, -105.2821720691177 39.98569760737838, -105.2857057924208 39.98570468543087, -105.2862482059948 39.98525743155678, -105.2862071928632 39.98015902991641, -105.2861390115304 39.9722881143455))</t>
-        </is>
-      </c>
-      <c r="H173" t="inlineStr"/>
+          <t>POLYGON ((-105.2861390115304 39.9722881143455, -105.28582388621383 39.97236126581304, -105.27937173981 39.970621428320506, -105.27255174912793 39.972647970014314, -105.27185244813299 39.97308048041847, -105.27151413007972 39.97329796337442, -105.27101017130475 39.97334763678315, -105.270307086264 39.97305969060716, -105.26970513446629 39.97289908688346, -105.26926282753475 39.97275407844554, -105.26917384979545 39.972688015525854, -105.26907999895634 39.97258598049818, -105.26901686303158 39.972474948159736, -105.26895189218088 39.97237900979596, -105.26858008123418 39.97206997752857, -105.26855087726058 39.972053997095685, -105.26842509636435 39.97200405616698, -105.26828710898329 39.97197605214665, -105.26789895633335 39.97196209453039, -105.26781508815061 39.97196796449851, -105.26765192701214 39.97199810756532, -105.2674990387551 39.972049958012285, -105.26722698351328 39.97220506197835, -105.26752416357047 39.97252987079597, -105.26756994568466 39.97260188768651, -105.2676559560471 39.97301493963212, -105.26765582329409 39.97305392063711, -105.26762916756857 39.973127988147134, -105.26757186374087 39.97319101215554, -105.26665503098575 39.973664902951555, -105.26670586246574 39.973721007712314, -105.26678501179808 39.973843878604754, -105.26684186593548 39.97401694200342, -105.26685986324388 39.97418004298486, -105.26684517429265 39.97430190077704, -105.26678682997452 39.97445990631218, -105.266692839123 39.97460795677274, -105.2665689187773 39.974743044654105, -105.26641616065578 39.97485913137701, -105.26605405732714 39.97504809120751, -105.26578990582233 39.975182892629554, -105.26532802941549 39.97543506074108, -105.2649458519276 39.97564895769812, -105.26458483400752 39.97583105123501, -105.26384694164508 39.97623912559444, -105.26377397246975 39.976290036922755, -105.26361504098402 39.9764349327568, -105.26331005773221 39.97681698813182, -105.26305017605976 39.97715713335895, -105.2628789145055 39.97735800467315, -105.26275202891522 39.977521082815855, -105.26252984923995 39.9776900043216, -105.26238616951964 39.97775696645165, -105.26208601984769 39.97787493928896, -105.26152488687863 39.978031904139385, -105.26140599070239 39.97805197236678, -105.2611229553935 39.97807087721965, -105.26104517262453 39.97806906869406, -105.26011488353066 39.97807592132791, -105.26011282999228 39.97876111940365, -105.2601148541277 39.97909905757952, -105.26012409254835 39.97971894376179, -105.26012706632332 39.97988805426846, -105.26013236057389 39.980219301942505, -105.25991829389952 39.98021663796225, -105.25967202319507 39.98021969945855, -105.25943498160535 39.98024065229194, -105.25719829019384 39.98073639001605, -105.25629625940572 39.98090963595508, -105.25634291624024 39.98103886783078, -105.2565239845004 39.98149797393191, -105.25661905343107 39.98165712142143, -105.25675307793539 39.981799880761315, -105.25696486367103 39.98195186270966, -105.25722306662664 39.9820970781437, -105.25800814122587 39.98250090116355, -105.25852983093128 39.981906011926924, -105.25876595451895 39.98203909986017, -105.25909512623639 39.98219791177391, -105.2594090755475 39.98232292541489, -105.25958306141374 39.982368034766544, -105.25982490101066 39.982399010772355, -105.26092795144172 39.98239691129109, -105.26185683003375 39.98240212864589, -105.26202817692233 39.982386011335144, -105.26224888493378 39.98233705323542, -105.26240502984375 39.98227999986478, -105.26255016344184 39.982208100621826, -105.26328586712833 39.98173194873376, -105.26367716713408 39.98208907864245, -105.26386108007839 39.98225691251253, -105.26442489270181 39.98277910578437, -105.26459391494197 39.982920005475165, -105.26478083443685 39.98304501876047, -105.26539392067917 39.983355926793095, -105.26588908581758 39.98361004180648, -105.26631301488804 39.98382502725105, -105.26717292090807 39.98428302002201, -105.2672730197861 39.984335929365514, -105.26768310476403 39.98453194102219, -105.2679329289423 39.98463209445797, -105.26823095746873 39.984724109594104, -105.2685961061897 39.984808022228876, -105.26896707630007 39.98485900393208, -105.26920505710092 39.98487402981937, -105.26932305650219 39.98487477127614, -105.2693219715217 39.98568827537257, -105.27706923611393 39.98569787181271, -105.28217206911766 39.98569760737838, -105.28570579242079 39.985704685430875, -105.2862482059948 39.985257431556775, -105.28620719286317 39.98015902991641, -105.2861390115304 39.9722881143455))</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>Fairview HS</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -7692,7 +7732,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2601148835307 39.97807592132791, -105.2610451726245 39.97806906869406, -105.2611229553935 39.97807087721965, -105.2614059907024 39.97805197236678, -105.2615248868786 39.97803190413939, -105.2620860198477 39.97787493928896, -105.2623861695196 39.97775696645165, -105.26252984924 39.9776900043216, -105.2627520289152 39.97752108281585, -105.2628789145055 39.97735800467315, -105.2630501760598 39.97715713335895, -105.2633100577322 39.97681698813182, -105.263615040984 39.9764349327568, -105.2637739724697 39.97629003692276, -105.2638469416451 39.97623912559444, -105.2645848340075 39.97583105123501, -105.2649458519276 39.97564895769812, -105.2653280294155 39.97543506074108, -105.2657899058223 39.97518289262955, -105.2660540573271 39.97504809120751, -105.2664161606558 39.97485913137701, -105.2665689187773 39.9747430446541, -105.266692839123 39.97460795677274, -105.2667868299745 39.97445990631218, -105.2668451742927 39.97430190077704, -105.2668598632439 39.97418004298486, -105.2668418659355 39.97401694200342, -105.2667850117981 39.97384387860475, -105.2667058624657 39.97372100771231, -105.2666550309857 39.97366490295155, -105.2675718637409 39.97319101215554, -105.2676291675686 39.97312798814713, -105.2676558232941 39.97305392063711, -105.2676559560471 39.97301493963212, -105.2675699456847 39.97260188768651, -105.2675241635705 39.97252987079597, -105.2672269835133 39.97220506197835, -105.2674990387551 39.97204995801228, -105.2676519270121 39.97199810756532, -105.2678150881506 39.97196796449851, -105.2678989563334 39.97196209453039, -105.2682871089833 39.97197605214665, -105.2684250963644 39.97200405616698, -105.2685508772606 39.97205399709568, -105.2685800812342 39.97206997752857, -105.2689518921809 39.97237900979596, -105.2690168630316 39.97247494815974, -105.2690799989563 39.97258598049818, -105.2691738497955 39.97268801552585, -105.2692628275347 39.97275407844554, -105.2697051344663 39.97289908688346, -105.270307086264 39.97305969060716, -105.2710101713048 39.97334763678315, -105.2715141300797 39.97329796337442, -105.271852448133 39.97308048041847, -105.2725517491279 39.97264797001431, -105.27937173981 39.97062142832051, -105.2858238862138 39.97236126581304, -105.286136356992 39.97228873087183, -105.2861244007367 39.9711343731696, -105.2860942039776 39.96890542940076, -105.2769282016526 39.96887843060637, -105.2767862013965 39.96053042948035, -105.2741642004337 39.96057642842725, -105.2741021991976 39.95692142844955, -105.2600981963768 39.95726642936853, -105.2601035322989 39.96436378914595, -105.2601004030519 39.9653869868361, -105.2600958578688 39.96687345294639, -105.2600458065456 39.966888737356, -105.2597479477074 39.9668984284015, -105.2592714284939 39.96689857964134, -105.2589868313722 39.9669483999424, -105.2588497350911 39.96697561288582, -105.2587330722951 39.96700983502225, -105.2586678080136 39.96704741785576, -105.2586333804342 39.96709776089104, -105.2586330480665 39.96719171575484, -105.2586250633071 39.96734409096888, -105.2588081154157 39.9674694997124, -105.2590318963694 39.96756886259143, -105.2592378553571 39.96764204175338, -105.2593539892399 39.96769197171394, -105.2596780773968 39.96785708619387, -105.2597151123492 39.96787692921709, -105.2597510735942 39.96789786788992, -105.2597841722106 39.96792099638444, -105.2598169121108 39.96794494732139, -105.2598471463916 39.96797108972814, -105.2598748810544 39.96799805101909, -105.2599018966814 39.96802610870504, -105.2599260568495 39.96805498363604, -105.2599480711023 39.96808495199186, -105.2599679417791 39.96811601377863, -105.2599920807612 39.96815092845134, -105.2600130001009 39.96818803221404, -105.260032849595 39.96822513374512, -105.2600498451394 39.9682619555311, -105.2600650502581 39.9683009684859, -105.2600781171707 39.968338879988, -105.2600879706286 39.96837788179813, -105.2600960351647 39.96841797868385, -105.2601019599666 39.96845807111478, -105.260106103564 39.96849706193777, -105.2601070346524 39.96853686927319, -105.2601058226876 39.96857694684767, -105.2601060756537 39.96911390952305, -105.2600951642153 39.96957916662159, -105.2601008302682 39.97019990152354, -105.2600949802003 39.97105200083171, -105.2601021068224 39.97135892947309, -105.2601051226491 39.97151596149975, -105.2601118336586 39.97183990985678, -105.2601171439998 39.97256190912651, -105.2601131707291 39.97328608572666, -105.2601119682293 39.97342499135579, -105.260119906472 39.97400891196983, -105.2601010269371 39.97511601350899, -105.260105851442 39.97567192797527, -105.2601068763516 39.97629399305483, -105.2601151665028 39.97708188388466, -105.2601159707622 39.97746209543652, -105.2601158412143 39.97770202615754, -105.2601148835307 39.97807592132791))</t>
+          <t>POLYGON ((-105.26011488353066 39.97807592132791, -105.26104517262453 39.97806906869406, -105.2611229553935 39.97807087721965, -105.26140599070239 39.97805197236678, -105.26152488687863 39.978031904139385, -105.26208601984769 39.97787493928896, -105.26238616951964 39.97775696645165, -105.26252984923995 39.9776900043216, -105.26275202891522 39.977521082815855, -105.2628789145055 39.97735800467315, -105.26305017605976 39.97715713335895, -105.26331005773221 39.97681698813182, -105.26361504098402 39.9764349327568, -105.26377397246975 39.976290036922755, -105.26384694164508 39.97623912559444, -105.26458483400752 39.97583105123501, -105.2649458519276 39.97564895769812, -105.26532802941549 39.97543506074108, -105.26578990582233 39.975182892629554, -105.26605405732714 39.97504809120751, -105.26641616065578 39.97485913137701, -105.2665689187773 39.974743044654105, -105.266692839123 39.97460795677274, -105.26678682997452 39.97445990631218, -105.26684517429265 39.97430190077704, -105.26685986324388 39.97418004298486, -105.26684186593548 39.97401694200342, -105.26678501179808 39.973843878604754, -105.26670586246574 39.973721007712314, -105.26665503098575 39.973664902951555, -105.26757186374087 39.97319101215554, -105.26762916756857 39.973127988147134, -105.26765582329409 39.97305392063711, -105.2676559560471 39.97301493963212, -105.26756994568466 39.97260188768651, -105.26752416357047 39.97252987079597, -105.26722698351328 39.97220506197835, -105.2674990387551 39.972049958012285, -105.26765192701214 39.97199810756532, -105.26781508815061 39.97196796449851, -105.26789895633335 39.97196209453039, -105.26828710898329 39.97197605214665, -105.26842509636435 39.97200405616698, -105.26855087726058 39.972053997095685, -105.26858008123418 39.97206997752857, -105.26895189218088 39.97237900979596, -105.26901686303158 39.972474948159736, -105.26907999895634 39.97258598049818, -105.26917384979545 39.972688015525854, -105.26926282753475 39.97275407844554, -105.26970513446629 39.97289908688346, -105.270307086264 39.97305969060716, -105.27101017130475 39.97334763678315, -105.27151413007972 39.97329796337442, -105.27185244813299 39.97308048041847, -105.27255174912793 39.972647970014314, -105.27937173981 39.970621428320506, -105.28582388621383 39.97236126581304, -105.286136356992 39.97228873087183, -105.2861244007367 39.971134373169605, -105.28609420397757 39.96890542940076, -105.27692820165258 39.968878430606374, -105.27678620139646 39.96053042948035, -105.27416420043366 39.96057642842725, -105.27410219919763 39.956921428449554, -105.26009819637677 39.95726642936853, -105.26010353229893 39.96436378914595, -105.26010040305187 39.9653869868361, -105.2600958578688 39.966873452946395, -105.2600458065456 39.966888737356, -105.25974794770735 39.9668984284015, -105.25927142849386 39.96689857964134, -105.25898683137216 39.9669483999424, -105.25884973509115 39.96697561288582, -105.25873307229513 39.967009835022246, -105.25866780801356 39.96704741785576, -105.25863338043418 39.96709776089104, -105.2586330480665 39.96719171575484, -105.25862506330705 39.96734409096888, -105.25880811541575 39.9674694997124, -105.25903189636936 39.96756886259143, -105.25923785535707 39.96764204175338, -105.25935398923994 39.96769197171394, -105.2596780773968 39.967857086193874, -105.25971511234917 39.96787692921709, -105.25975107359416 39.967897867889924, -105.2597841722106 39.96792099638444, -105.25981691211076 39.96794494732139, -105.25984714639162 39.96797108972814, -105.25987488105439 39.967998051019094, -105.25990189668137 39.96802610870504, -105.25992605684945 39.96805498363604, -105.25994807110233 39.968084951991855, -105.25996794177914 39.968116013778626, -105.25999208076124 39.968150928451344, -105.26001300010086 39.968188032214044, -105.26003284959502 39.96822513374512, -105.26004984513936 39.968261955531105, -105.26006505025812 39.9683009684859, -105.26007811717065 39.968338879987996, -105.26008797062856 39.968377881798126, -105.26009603516472 39.96841797868385, -105.26010195996663 39.96845807111478, -105.26010610356396 39.96849706193777, -105.26010703465242 39.96853686927319, -105.26010582268763 39.96857694684767, -105.26010607565374 39.96911390952305, -105.26009516421534 39.96957916662159, -105.26010083026823 39.97019990152354, -105.26009498020028 39.97105200083171, -105.26010210682243 39.97135892947309, -105.26010512264908 39.97151596149975, -105.26011183365861 39.97183990985678, -105.26011714399975 39.97256190912651, -105.26011317072907 39.973286085726656, -105.26011196822925 39.97342499135579, -105.26011990647204 39.974008911969825, -105.26010102693708 39.97511601350899, -105.260105851442 39.97567192797527, -105.2601068763516 39.97629399305483, -105.26011516650279 39.97708188388466, -105.26011597076221 39.97746209543652, -105.26011584121433 39.977702026157544, -105.26011488353066 39.97807592132791))</t>
         </is>
       </c>
       <c r="H174" t="inlineStr">
@@ -7734,10 +7774,14 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.245800143718 39.98094801864188, -105.2458591469235 39.98091493167031, -105.2459760636716 39.98085397183197, -105.2462461766525 39.98076397524878, -105.2465098781437 39.98067011993611, -105.2466978596759 39.98059504023666, -105.2469939547208 39.98042603675346, -105.2474948699503 39.98016304674198, -105.2482510874011 39.97975896003506, -105.2489968741238 39.97937488524389, -105.2496579462505 39.97902795654765, -105.2500300959376 39.9788420898406, -105.2500740536243 39.97882406757441, -105.2501190742881 39.97880796779358, -105.2501651609402 39.97879296910547, -105.2502119576847 39.97877907073762, -105.2502591032779 39.97876709330425, -105.2503069611447 39.97875594149448, -105.2503558798193 39.97874698866123, -105.2504051496909 39.97873995766609, -105.2504540584652 39.97873402466791, -105.2505029630528 39.97872891393846, -105.2506028915245 39.9787250123996, -105.2511381731693 39.97871793375031, -105.2520448639634 39.97872702547376, -105.2529308837927 39.97872892806342, -105.2534379337529 39.97873303370792, -105.2538251064159 39.97873193926058, -105.2546219021326 39.97873803075372, -105.2548084360336 39.97873894737987, -105.2556071116555 39.97874286908414, -105.2565470129442 39.97874513280774, -105.2574351597284 39.97875112306168, -105.2587978821324 39.97876194364169, -105.2601128299923 39.97876111940365, -105.2601148835307 39.97807592132791, -105.2601158412143 39.97770202615754, -105.2601159707622 39.97746209543652, -105.2601151665028 39.97708188388466, -105.2601068763516 39.97629399305483, -105.260105851442 39.97567192797527, -105.2601010269371 39.97511601350899, -105.2581178634619 39.9751069276835, -105.2574420856145 39.9750969972116, -105.2565468246362 39.97509812957833, -105.255609828812 39.97509587190684, -105.25472492212 39.97509509007728, -105.2538379091741 39.97508496345969, -105.2529390662315 39.97508990325123, -105.252047017541 39.9750910075517, -105.2507499800561 39.9750920530555, -105.2504421226539 39.97507107259827, -105.2502709701032 39.97503803420135, -105.2501091656749 39.97498607322357, -105.2500069235402 39.97494110512169, -105.249689947461 39.97478009681639, -105.2491308613379 39.9753498844948, -105.2485418287389 39.97590999502591, -105.2482839415636 39.97617407001634, -105.2482201068636 39.97626095285669, -105.2481321091086 39.9764169631363, -105.2481198770704 39.97644411369523, -105.2480588565181 39.97663806625191, -105.2480388532614 39.97683705034323, -105.245967834937 39.97683497498167, -105.2459671126042 39.97645393922107, -105.2459720164586 39.9756161130714, -105.2451691589491 39.97561900799606, -105.2446071695026 39.97561803880048, -105.2440379798706 39.97563407057132, -105.2425921489947 39.97563194856655, -105.2424318460008 39.9756560225469, -105.242267879168 39.97570507050918, -105.2420848579998 39.97579195809596, -105.2419621656047 39.97587211837142, -105.2417741744749 39.9756691010777, -105.2415438868199 39.97542288863698, -105.2415029964935 39.97538491354085, -105.2414428800109 39.97533591360214, -105.2413428299869 39.97527886402315, -105.241233839971 39.97522700908468, -105.2411971215205 39.97531202783664, -105.2411318317776 39.97540412010915, -105.2410670165164 39.97546491831289, -105.2409581733426 39.97556212833344, -105.2409141414532 39.97559991366145, -105.2414479703547 39.97615811412556, -105.2428560147591 39.97766810735965, -105.245800143718 39.98094801864188))</t>
-        </is>
-      </c>
-      <c r="H175" t="inlineStr"/>
+          <t>POLYGON ((-105.24580014371804 39.980948018641875, -105.24585914692348 39.98091493167031, -105.24597606367163 39.98085397183197, -105.24624617665252 39.98076397524878, -105.24650987814371 39.98067011993611, -105.24669785967588 39.980595040236665, -105.24699395472084 39.98042603675346, -105.24749486995034 39.98016304674198, -105.24825108740106 39.979758960035056, -105.24899687412376 39.97937488524389, -105.24965794625051 39.97902795654765, -105.2500300959376 39.978842089840605, -105.25007405362432 39.97882406757441, -105.25011907428814 39.97880796779358, -105.25016516094021 39.97879296910547, -105.25021195768473 39.978779070737616, -105.25025910327791 39.97876709330425, -105.25030696114473 39.97875594149448, -105.25035587981932 39.97874698866123, -105.25040514969093 39.978739957666086, -105.25045405846517 39.97873402466791, -105.25050296305275 39.97872891393846, -105.25060289152445 39.9787250123996, -105.25113817316925 39.97871793375031, -105.25204486396343 39.97872702547376, -105.25293088379273 39.97872892806342, -105.25343793375289 39.97873303370792, -105.25382510641593 39.97873193926058, -105.25462190213261 39.978738030753725, -105.25480843603364 39.97873894737987, -105.25560711165545 39.97874286908414, -105.25654701294424 39.97874513280774, -105.2574351597284 39.978751123061684, -105.25879788213238 39.97876194364169, -105.26011282999228 39.97876111940365, -105.26011488353066 39.97807592132791, -105.26011584121433 39.977702026157544, -105.26011597076221 39.97746209543652, -105.26011516650279 39.97708188388466, -105.2601068763516 39.97629399305483, -105.260105851442 39.97567192797527, -105.26010102693708 39.97511601350899, -105.25811786346189 39.9751069276835, -105.25744208561446 39.9750969972116, -105.25654682463617 39.97509812957833, -105.25560982881198 39.97509587190684, -105.25472492212005 39.975095090077275, -105.25383790917412 39.97508496345969, -105.25293906623148 39.97508990325123, -105.25204701754103 39.975091007551704, -105.25074998005611 39.9750920530555, -105.25044212265385 39.97507107259827, -105.25027097010316 39.97503803420135, -105.25010916567486 39.97498607322357, -105.25000692354021 39.974941105121694, -105.24968994746102 39.97478009681639, -105.24913086133792 39.975349884494804, -105.24854182873888 39.97590999502591, -105.2482839415636 39.97617407001634, -105.24822010686358 39.97626095285669, -105.24813210910855 39.9764169631363, -105.24811987707035 39.97644411369523, -105.24805885651811 39.97663806625191, -105.24803885326142 39.97683705034323, -105.24596783493705 39.97683497498167, -105.24596711260425 39.97645393922107, -105.24597201645864 39.9756161130714, -105.24516915894907 39.97561900799606, -105.24460716950257 39.97561803880048, -105.24403797987061 39.97563407057132, -105.24259214899473 39.97563194856655, -105.24243184600077 39.9756560225469, -105.242267879168 39.97570507050918, -105.2420848579998 39.97579195809596, -105.24196216560468 39.97587211837142, -105.24177417447493 39.9756691010777, -105.24154388681988 39.975422888636984, -105.24150299649352 39.97538491354085, -105.24144288001092 39.975335913602144, -105.24134282998688 39.975278864023146, -105.24123383997104 39.97522700908468, -105.24119712152054 39.975312027836644, -105.24113183177761 39.97540412010915, -105.24106701651635 39.97546491831289, -105.24095817334262 39.97556212833344, -105.24091414145316 39.97559991366145, -105.24144797035473 39.97615811412556, -105.24285601475908 39.977668107359655, -105.24580014371804 39.980948018641875))</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>Fairview HS</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -7772,7 +7816,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2459671126042 39.97645393922107, -105.245967834937 39.97683497498167, -105.2480388532614 39.97683705034323, -105.2480588565181 39.97663806625191, -105.2481198770704 39.97644411369523, -105.2481321091086 39.9764169631363, -105.2482201068636 39.97626095285669, -105.2482839415636 39.97617407001634, -105.2485418287389 39.97590999502591, -105.2491308613379 39.9753498844948, -105.249689947461 39.97478009681639, -105.2500069235402 39.97494110512169, -105.2501091656749 39.97498607322357, -105.2502709701032 39.97503803420135, -105.2504421226539 39.97507107259827, -105.2507499800561 39.9750920530555, -105.252047017541 39.9750910075517, -105.2529390662315 39.97508990325123, -105.2538379091741 39.97508496345969, -105.25472492212 39.97509509007728, -105.255609828812 39.97509587190684, -105.2565468246362 39.97509812957833, -105.2574420856145 39.9750969972116, -105.2581178634619 39.9751069276835, -105.2601010269371 39.97511601350899, -105.260119906472 39.97400891196983, -105.2601119682293 39.97342499135579, -105.2601131707291 39.97328608572666, -105.2601171439998 39.97256190912651, -105.2601118336586 39.97183990985678, -105.2601051226491 39.97151596149975, -105.2601021068224 39.97135892947309, -105.2600949802003 39.97105200083171, -105.2601008302682 39.97019990152354, -105.2600951642153 39.96957916662159, -105.2601060756537 39.96911390952305, -105.2601058226876 39.96857694684767, -105.2601070346524 39.96853686927319, -105.260106103564 39.96849706193777, -105.2601019599666 39.96845807111478, -105.2600960351647 39.96841797868385, -105.2600879706286 39.96837788179813, -105.2600781171707 39.968338879988, -105.2600650502581 39.9683009684859, -105.2600498451394 39.9682619555311, -105.260032849595 39.96822513374512, -105.2600130001009 39.96818803221404, -105.2599920807612 39.96815092845134, -105.2599679417791 39.96811601377863, -105.2599480711023 39.96808495199186, -105.2599260568495 39.96805498363604, -105.2599018966814 39.96802610870504, -105.2598748810544 39.96799805101909, -105.2598471463916 39.96797108972814, -105.2598169121108 39.96794494732139, -105.2597841722106 39.96792099638444, -105.2597510735942 39.96789786788992, -105.2597151123492 39.96787692921709, -105.2596780773968 39.96785708619387, -105.2593539892399 39.96769197171394, -105.2592378553571 39.96764204175338, -105.2590318963694 39.96756886259143, -105.2587408854162 39.96803905646281, -105.2582999615848 39.96862697978188, -105.2582140676193 39.96870201790841, -105.2581018565284 39.96875311803667, -105.2580390091983 39.96876808470588, -105.257819872241 39.9687879387206, -105.2563248682633 39.9688089457336, -105.2560769586915 39.96879304799511, -105.2554061767933 39.96870103471698, -105.2551371756111 39.96869689419053, -105.25505289518 39.96871895139297, -105.2548441581341 39.96882309986093, -105.2544060703984 39.9690091154364, -105.2542789684686 39.96903300281312, -105.2541808491974 39.96903389147021, -105.253371152958 39.96897588496952, -105.253249993791 39.9689349961219, -105.2531549340253 39.96887906534976, -105.2530749143676 39.96880806722145, -105.25302312807 39.9687239529433, -105.2528869355109 39.96840109905034, -105.2520010553737 39.96859410627039, -105.2512640615616 39.96875613211644, -105.2485980655657 39.96936390056683, -105.2478899257956 39.96953392960094, -105.2477128990422 39.96955001341719, -105.2476240809881 39.96954405385281, -105.2473538238716 39.96949295020445, -105.2475568559756 39.96910192840829, -105.2476289839358 39.96899008164604, -105.2476659373223 39.96893498384546, -105.2477050304019 39.96887989161763, -105.2477179742688 39.9688530164449, -105.2477298511372 39.96882504103485, -105.2477388742074 39.96879706027771, -105.247746113366 39.96876907471447, -105.2477508557514 39.9687410836859, -105.2477531071436 39.96871089140461, -105.2477528578647 39.96868206625025, -105.2477501145556 39.96865186303658, -105.2477471615545 39.9685821286516, -105.2477460015975 39.9685099267895, -105.2477469763071 39.96843910310034, -105.2477500941148 39.96836800850068, -105.2477549946374 39.96829691870309, -105.2477620350404 39.96822610828865, -105.2478141349912 39.9677408693298, -105.2477729811179 39.96767791434331, -105.2474753673763 39.96769585395178, -105.2462912040428 39.97056630758622, -105.2440218599026 39.97058180202682, -105.2433014852756 39.97057892985443, -105.2426484757223 39.97057784552026, -105.2407611803397 39.97057524416711, -105.2397356341425 39.97057342905075, -105.2384541938374 39.97056943291407, -105.2373061931619 39.9705654331454, -105.2373862395304 39.97087910440568, -105.2373861130697 39.97087911402476, -105.237398193695 39.97092743295542, -105.2376861927079 39.97111743293383, -105.2378631932777 39.97149343284205, -105.2371748229859 39.9714850156177, -105.2371871588444 39.97150413946797, -105.2373302280914 39.97175110590815, -105.2374503865781 39.97191580534781, -105.2375705868881 39.97206978243837, -105.2377694636597 39.97230257655232, -105.2379128811428 39.97246018080529, -105.2383062013195 39.97287214043273, -105.2388245148268 39.97340234006232, -105.2393131352965 39.97390608003223, -105.2396065640024 39.97421909272716, -105.2404348886767 39.97508956116814, -105.2409141414532 39.97559991366145, -105.2409581733426 39.97556212833344, -105.2410670165164 39.97546491831289, -105.2411318317776 39.97540412010915, -105.2411971215205 39.97531202783664, -105.241233839971 39.97522700908468, -105.2413428299869 39.97527886402315, -105.2414428800109 39.97533591360214, -105.2415029964935 39.97538491354085, -105.2415438868199 39.97542288863698, -105.2417741744749 39.9756691010777, -105.2419621656047 39.97587211837142, -105.2420848579998 39.97579195809596, -105.242267879168 39.97570507050918, -105.2424318460008 39.9756560225469, -105.2425921489947 39.97563194856655, -105.2440379798706 39.97563407057132, -105.2446071695026 39.97561803880048, -105.2451691589491 39.97561900799606, -105.2459720164586 39.9756161130714, -105.2459671126042 39.97645393922107))</t>
+          <t>POLYGON ((-105.24596711260425 39.97645393922107, -105.24596783493705 39.97683497498167, -105.24803885326142 39.97683705034323, -105.24805885651811 39.97663806625191, -105.24811987707035 39.97644411369523, -105.24813210910855 39.9764169631363, -105.24822010686358 39.97626095285669, -105.2482839415636 39.97617407001634, -105.24854182873888 39.97590999502591, -105.24913086133792 39.975349884494804, -105.24968994746102 39.97478009681639, -105.25000692354021 39.974941105121694, -105.25010916567486 39.97498607322357, -105.25027097010316 39.97503803420135, -105.25044212265385 39.97507107259827, -105.25074998005611 39.9750920530555, -105.25204701754103 39.975091007551704, -105.25293906623148 39.97508990325123, -105.25383790917412 39.97508496345969, -105.25472492212005 39.975095090077275, -105.25560982881198 39.97509587190684, -105.25654682463617 39.97509812957833, -105.25744208561446 39.9750969972116, -105.25811786346189 39.9751069276835, -105.26010102693708 39.97511601350899, -105.26011990647204 39.974008911969825, -105.26011196822925 39.97342499135579, -105.26011317072907 39.973286085726656, -105.26011714399975 39.97256190912651, -105.26011183365861 39.97183990985678, -105.26010512264908 39.97151596149975, -105.26010210682243 39.97135892947309, -105.26009498020028 39.97105200083171, -105.26010083026823 39.97019990152354, -105.26009516421534 39.96957916662159, -105.26010607565374 39.96911390952305, -105.26010582268763 39.96857694684767, -105.26010703465242 39.96853686927319, -105.26010610356396 39.96849706193777, -105.26010195996663 39.96845807111478, -105.26009603516472 39.96841797868385, -105.26008797062856 39.968377881798126, -105.26007811717065 39.968338879987996, -105.26006505025812 39.9683009684859, -105.26004984513936 39.968261955531105, -105.26003284959502 39.96822513374512, -105.26001300010086 39.968188032214044, -105.25999208076124 39.968150928451344, -105.25996794177914 39.968116013778626, -105.25994807110233 39.968084951991855, -105.25992605684945 39.96805498363604, -105.25990189668137 39.96802610870504, -105.25987488105439 39.967998051019094, -105.25984714639162 39.96797108972814, -105.25981691211076 39.96794494732139, -105.2597841722106 39.96792099638444, -105.25975107359416 39.967897867889924, -105.25971511234917 39.96787692921709, -105.2596780773968 39.967857086193874, -105.25935398923994 39.96769197171394, -105.25923785535707 39.96764204175338, -105.25903189636936 39.96756886259143, -105.25874088541619 39.968039056462814, -105.25829996158475 39.96862697978188, -105.25821406761926 39.968702017908406, -105.25810185652836 39.968753118036666, -105.25803900919833 39.96876808470588, -105.257819872241 39.9687879387206, -105.2563248682633 39.9688089457336, -105.25607695869151 39.968793047995106, -105.25540617679334 39.96870103471698, -105.25513717561113 39.96869689419053, -105.25505289518001 39.96871895139297, -105.25484415813415 39.968823099860934, -105.25440607039845 39.9690091154364, -105.25427896846858 39.96903300281312, -105.25418084919741 39.96903389147021, -105.253371152958 39.96897588496952, -105.25324999379099 39.9689349961219, -105.25315493402535 39.96887906534976, -105.25307491436759 39.968808067221445, -105.25302312807001 39.9687239529433, -105.25288693551087 39.96840109905034, -105.2520010553737 39.968594106270395, -105.25126406156163 39.96875613211644, -105.2485980655657 39.969363900566826, -105.24788992579556 39.96953392960094, -105.24771289904224 39.96955001341719, -105.24762408098812 39.969544053852815, -105.24735382387159 39.96949295020445, -105.24755685597557 39.969101928408286, -105.24762898393577 39.96899008164604, -105.24766593732232 39.96893498384546, -105.24770503040192 39.968879891617625, -105.24771797426882 39.968853016444896, -105.2477298511372 39.968825041034854, -105.2477388742074 39.96879706027771, -105.247746113366 39.96876907471447, -105.24775085575142 39.9687410836859, -105.2477531071436 39.96871089140461, -105.24775285786474 39.96868206625025, -105.2477501145556 39.968651863036584, -105.24774716155451 39.968582128651605, -105.24774600159749 39.9685099267895, -105.24774697630711 39.96843910310034, -105.24775009411485 39.96836800850068, -105.24775499463736 39.96829691870309, -105.24776203504035 39.96822610828865, -105.24781413499116 39.9677408693298, -105.24777298111786 39.96767791434331, -105.2474753673763 39.96769585395178, -105.24629120404276 39.97056630758622, -105.2440218599026 39.97058180202682, -105.24330148527561 39.970578929854426, -105.2426484757223 39.97057784552026, -105.24076118033973 39.97057524416711, -105.2397356341425 39.97057342905075, -105.23845419383738 39.97056943291407, -105.23730619316187 39.9705654331454, -105.23738623953038 39.97087910440568, -105.23738611306975 39.97087911402476, -105.23739819369501 39.97092743295542, -105.23768619270793 39.97111743293383, -105.23786319327772 39.97149343284205, -105.23717482298593 39.9714850156177, -105.23718715884438 39.97150413946797, -105.23733022809137 39.97175110590815, -105.2374503865781 39.97191580534781, -105.23757058688808 39.97206978243837, -105.2377694636597 39.972302576552316, -105.23791288114278 39.972460180805285, -105.23830620131949 39.97287214043273, -105.23882451482685 39.97340234006232, -105.23931313529647 39.97390608003223, -105.23960656400237 39.97421909272716, -105.2404348886767 39.97508956116814, -105.24091414145316 39.97559991366145, -105.24095817334262 39.97556212833344, -105.24106701651635 39.97546491831289, -105.24113183177761 39.97540412010915, -105.24119712152054 39.975312027836644, -105.24123383997104 39.97522700908468, -105.24134282998688 39.975278864023146, -105.24144288001092 39.975335913602144, -105.24150299649352 39.97538491354085, -105.24154388681988 39.975422888636984, -105.24177417447493 39.9756691010777, -105.24196216560468 39.97587211837142, -105.2420848579998 39.97579195809596, -105.242267879168 39.97570507050918, -105.24243184600077 39.9756560225469, -105.24259214899473 39.97563194856655, -105.24403797987061 39.97563407057132, -105.24460716950257 39.97561803880048, -105.24516915894907 39.97561900799606, -105.24597201645864 39.9756161130714, -105.24596711260425 39.97645393922107))</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
@@ -7814,7 +7858,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2474753673763 39.96769585395178, -105.2477729811179 39.96767791434331, -105.2478141349912 39.9677408693298, -105.2477620350404 39.96822610828865, -105.2477549946374 39.96829691870309, -105.2477500941148 39.96836800850068, -105.2477469763071 39.96843910310034, -105.2477460015975 39.9685099267895, -105.2477471615545 39.9685821286516, -105.2477501145556 39.96865186303658, -105.2477528578647 39.96868206625025, -105.2477531071436 39.96871089140461, -105.2477508557514 39.9687410836859, -105.247746113366 39.96876907471447, -105.2477388742074 39.96879706027771, -105.2477298511372 39.96882504103485, -105.2477179742688 39.9688530164449, -105.2477050304019 39.96887989161763, -105.2476659373223 39.96893498384546, -105.2476289839358 39.96899008164604, -105.2475568559756 39.96910192840829, -105.2473538238716 39.96949295020445, -105.2476240809881 39.96954405385281, -105.2477128990422 39.96955001341719, -105.2478899257956 39.96953392960094, -105.2485980655657 39.96936390056683, -105.2512640615616 39.96875613211644, -105.2520010553737 39.96859410627039, -105.2528869355109 39.96840109905034, -105.25302312807 39.9687239529433, -105.2530749143676 39.96880806722145, -105.2531549340253 39.96887906534976, -105.253249993791 39.9689349961219, -105.253371152958 39.96897588496952, -105.2541808491974 39.96903389147021, -105.2542789684686 39.96903300281312, -105.2544060703984 39.9690091154364, -105.2548441581341 39.96882309986093, -105.25505289518 39.96871895139297, -105.2551371756111 39.96869689419053, -105.2554061767933 39.96870103471698, -105.2560769586915 39.96879304799511, -105.2563248682633 39.9688089457336, -105.257819872241 39.9687879387206, -105.2580390091983 39.96876808470588, -105.2581018565284 39.96875311803667, -105.2582140676193 39.96870201790841, -105.2582999615848 39.96862697978188, -105.2587408854162 39.96803905646281, -105.2590318963694 39.96756886259143, -105.2588081154157 39.9674694997124, -105.2586250633071 39.96734409096888, -105.2586330480665 39.96719171575484, -105.2586333804342 39.96709776089104, -105.2586678080136 39.96704741785576, -105.2587330722951 39.96700983502225, -105.2588497350911 39.96697561288582, -105.2589868313722 39.9669483999424, -105.2592714284939 39.96689857964134, -105.2597479477074 39.9668984284015, -105.2600458065456 39.966888737356, -105.2600958578688 39.96687345294639, -105.2601035322989 39.96436378914595, -105.2578771096302 39.96437291470987, -105.2518200780547 39.96434946840338, -105.2506987916678 39.96433320956193, -105.2488772311309 39.96432709656406, -105.2474753673763 39.96769585395178))</t>
+          <t>POLYGON ((-105.2474753673763 39.96769585395178, -105.24777298111786 39.96767791434331, -105.24781413499116 39.9677408693298, -105.24776203504035 39.96822610828865, -105.24775499463736 39.96829691870309, -105.24775009411485 39.96836800850068, -105.24774697630711 39.96843910310034, -105.24774600159749 39.9685099267895, -105.24774716155451 39.968582128651605, -105.2477501145556 39.968651863036584, -105.24775285786474 39.96868206625025, -105.2477531071436 39.96871089140461, -105.24775085575142 39.9687410836859, -105.247746113366 39.96876907471447, -105.2477388742074 39.96879706027771, -105.2477298511372 39.968825041034854, -105.24771797426882 39.968853016444896, -105.24770503040192 39.968879891617625, -105.24766593732232 39.96893498384546, -105.24762898393577 39.96899008164604, -105.24755685597557 39.969101928408286, -105.24735382387159 39.96949295020445, -105.24762408098812 39.969544053852815, -105.24771289904224 39.96955001341719, -105.24788992579556 39.96953392960094, -105.2485980655657 39.969363900566826, -105.25126406156163 39.96875613211644, -105.2520010553737 39.968594106270395, -105.25288693551087 39.96840109905034, -105.25302312807001 39.9687239529433, -105.25307491436759 39.968808067221445, -105.25315493402535 39.96887906534976, -105.25324999379099 39.9689349961219, -105.253371152958 39.96897588496952, -105.25418084919741 39.96903389147021, -105.25427896846858 39.96903300281312, -105.25440607039845 39.9690091154364, -105.25484415813415 39.968823099860934, -105.25505289518001 39.96871895139297, -105.25513717561113 39.96869689419053, -105.25540617679334 39.96870103471698, -105.25607695869151 39.968793047995106, -105.2563248682633 39.9688089457336, -105.257819872241 39.9687879387206, -105.25803900919833 39.96876808470588, -105.25810185652836 39.968753118036666, -105.25821406761926 39.968702017908406, -105.25829996158475 39.96862697978188, -105.25874088541619 39.968039056462814, -105.25903189636936 39.96756886259143, -105.25880811541575 39.9674694997124, -105.25862506330705 39.96734409096888, -105.2586330480665 39.96719171575484, -105.25863338043418 39.96709776089104, -105.25866780801356 39.96704741785576, -105.25873307229513 39.967009835022246, -105.25884973509115 39.96697561288582, -105.25898683137216 39.9669483999424, -105.25927142849386 39.96689857964134, -105.25974794770735 39.9668984284015, -105.2600458065456 39.966888737356, -105.2600958578688 39.966873452946395, -105.26010353229893 39.96436378914595, -105.25787710963021 39.96437291470987, -105.25182007805469 39.96434946840338, -105.25069879166776 39.96433320956193, -105.2488772311309 39.96432709656406, -105.2474753673763 39.96769585395178))</t>
         </is>
       </c>
       <c r="H177" t="inlineStr">
@@ -7856,7 +7900,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t xml:space="preserve">MULTIPOLYGON (((-105.1691971726547 39.92869943197082, -105.1689793582281 39.92870089031781, -105.1689792892025 39.92870089102008, -105.1684020970337 39.92870328012041, -105.1674080147692 39.92870738861864, -105.1666547280895 39.92871548841494, -105.1666546602336 39.92871548911919, -105.1662549995615 39.92871799924519, -105.1662549969533 39.928718054178, -105.1662548834643 39.92871805655115, -105.1658309152665 39.92871792608083, -105.1660201718075 39.92872443199441, -105.1660261074718 39.92941559118069, -105.166031494597 39.93004289540448, -105.1660381193122 39.93081421993796, -105.1660467016499 39.93181341576487, -105.166056515896 39.93295616617159, -105.1660647969186 39.93392020542746, -105.1660503453821 39.93509378069637, -105.1660326082687 39.93546115149928, -105.166003329776 39.93598570561753, -105.1660033259753 39.93598576505014, -105.1659873030505 39.93626023394562, -105.1658916104535 39.93622118475289, -105.1658739997193 39.93621399863118, -105.1659871752904 39.9362624329908, -105.1659749417947 39.93647953441914, -105.1659674910183 39.93676935921954, -105.1659572086535 39.93679429393993, -105.1659335404815 39.93685168841169, -105.1658977131763 39.93693353750162, -105.1658600197634 39.93701487859802, -105.1658204732303 39.93709568651817, -105.1657790841984 39.93717594147653, -105.1657358633377 39.93725561378023, -105.1657309930949 39.93726410639616, -105.1657314686866 39.93778700123453, -105.1657411728798 39.93778699967167, -105.1687795281632 39.93778699271773, -105.1705111261316 39.93778695271561, -105.1705041256043 39.93953147032551, -105.1705041235479 39.93953189633235, -105.170503856046 39.93959870391294, -105.1706001480141 39.93959920896221, -105.1706007611061 39.93959921251663, -105.1752061254244 39.93962327452727, -105.1752117639349 39.94144391979933, -105.1752117838299 39.94145375507232, -105.1752147521367 39.9424101139557, -105.1752173188591 39.9432381770126, -105.1761254808051 39.94324195231821, -105.1789957423668 39.94325383880542, -105.1795291232214 39.94325604071027, -105.1795857546609 39.94325627388761, -105.179680680969 39.9432566666597, -105.1799269123049 39.9432576806739, -105.1799269771434 39.9431864638202, -105.1799270111662 39.94314876676573, -105.1799270269173 39.94313068604808, -105.1799271965382 39.94293307347776, -105.1799284928579 39.94143895759951, -105.1799300690526 39.93962613628113, -105.1819970768541 39.93962050076085, -105.1825172429311 39.93962242816511, -105.1825172620205 39.9396190786604, -105.1846548192044 39.93961336109664, -105.1894029282757 39.93957558427936, -105.1893867343792 39.93594894951613, -105.1914911317678 39.93594133715856, -105.1923511717818 39.93593821445231, -105.1933688742004 39.93593450898793, -105.1933702477947 39.93593450363773, -105.1941599816869 39.93593162428242, -105.1945942211984 39.93592965200351, -105.1951635483 39.93592706564407, -105.1952762078992 39.93592655313077, -105.1972458768153 39.93591757849988, -105.1989481266646 39.93590979541442, -105.2002993179784 39.93590013495036, -105.2004456872241 39.93589909443324, -105.2005289440003 39.93589930820974, -105.2005695998748 39.93589960573908, -105.2005767561356 39.93597682174268, -105.2007855838866 39.93595828117817, -105.2016135821577 39.93571128289184, -105.2017205818092 39.93570628394144, -105.2019415807419 39.93585928284536, -105.2020485805162 39.93587628311925, -105.2022345798063 39.93581028363036, -105.2022817052154 39.93578010452304, -105.2022817218954 39.9357827182824, -105.2022819718508 39.93582278570346, -105.2022823369061 39.93589360196512, -105.203430843309 39.93588732563549, -105.2047070368473 39.93587606396571, -105.2046882733971 39.93394651148376, -105.2046864363509 39.93375887309851, -105.2046865622196 39.93375357663749, -105.2046865938261 39.93375222032397, -105.2046872617554 39.93372412053174, -105.2047298796838 39.93225646940934, -105.2047394578092 39.92861052434253, -105.20815190367 39.92859781286307, -105.2127497371948 39.92855694032826, -105.21745002281 39.92854504863909, -105.2182946341396 39.92854109387441, -105.2189537516798 39.92853800621756, -105.2189574099148 39.92853798902473, -105.2192246119665 39.92853673580493, -105.2193899800826 39.92853595984494, -105.2194595415266 39.92853648685829, -105.2221224251364 39.92852872241523, -105.2225585730252 39.92852772662706, -105.2269942832364 39.92851750262659, -105.231838615029 39.92851118067422, -105.2320906879295 39.92850933729788, -105.232244880529 39.92825937905761, -105.2322470002203 39.92825999913596, -105.2323239999907 39.92827499846799, -105.2325869997246 39.92832599949908, -105.2328459990954 39.92836499926473, -105.233193999894 39.92839699846957, -105.2333020002307 39.92840299930947, -105.2335169999823 39.92840799934192, -105.2338429992942 39.9284019990797, -105.2339589999796 39.92840599941181, -105.2342460000307 39.92840799944923, -105.2345579999572 39.92840399945201, -105.2346220868783 39.92839808298703, -105.235008498219 39.92954535037926, -105.2357094840183 39.93165934189567, -105.2360154780325 39.93263533803334, -105.236281472281 39.93344833402639, -105.2362914736262 39.93347633500713, -105.2363204718143 39.93355633311082, -105.2364244699075 39.93388233241797, -105.2365124675654 39.934211332045, -105.2365834657741 39.93454233001258, -105.2366494631262 39.9349403282457, -105.2367214605929 39.93554832524025, -105.2367244595431 39.93564532498768, -105.2367184583478 39.93593632327084, -105.2366914560335 39.93622632334893, -105.2365934533178 39.93682131971666, -105.2362604460931 39.93836731278099, -105.2361144443316 39.93896730909405, -105.2359764419444 39.93959030654941, -105.2358854385444 39.94007630426844, -105.2357694354685 39.94059430261459, -105.2356634342481 39.94112030001217, -105.2356304332279 39.94131729835097, -105.2356114323706 39.94151029746016, -105.2356014320325 39.94161229663906, -105.2355924294382 39.94190829551381, -105.2356074283079 39.94235429384504, -105.2356354249494 39.94272929243355, -105.235684424172 39.94310129046235, -105.2357704201069 39.94349128922146, -105.2358764195226 39.94388028719909, -105.2360184168766 39.9442792856082, -105.2362374114519 39.94482928352224, -105.2362994105811 39.94501728301593, -105.2363644094841 39.94521428241291, -105.2365134060399 39.94563127962134, -105.2365574053572 39.94586827954905, -105.2365854034608 39.94610727835873, -105.2365894029548 39.94626527741081, -105.2365814017142 39.9465022772988, -105.2365614007355 39.94666427533257, -105.2365313996723 39.94682527598022, -105.2364683993308 39.94706327408439, -105.2364103991369 39.94722027296941, -105.2363433979527 39.94737627311073, -105.2362663973395 39.94752527202102, -105.2361803968036 39.94767327125486, -105.2360353964538 39.94788527024479, -105.2358123949861 39.94815426851239, -105.2353373949938 39.94864726599771, -105.2349013944894 39.94908826348983, -105.2345443929722 39.94947226127717, -105.2341583927248 39.94993525893874, -105.2339843922855 39.95015925813851, -105.2338933927668 39.95028225714832, -105.2337133911016 39.95055025544299, -105.2332173879164 39.95142925195454, -105.2329263859335 39.95198824857948, -105.2328813846094 39.95204324832668, -105.2327903849929 39.95215824771139, -105.2327193862173 39.95224424719736, -105.232524383524 39.95259824508297, -105.2323133847181 39.95296324303607, -105.2320883826542 39.95329924107202, -105.2318913807338 39.95362223977587, -105.2318323814242 39.95370923934254, -105.2316703806363 39.95397423748284, -105.2314753793715 39.95433623591635, -105.2314223789011 39.95446223513391, -105.2313453770757 39.95467723363021, -105.2313003767481 39.9548462335438, -105.231253376375 39.95506123258171, -105.2312233748296 39.95522923168615, -105.2311983738348 39.95548223033251, -105.2311963731234 39.95565322998704, -105.2312023733035 39.9557382300675, -105.2312363718279 39.95601922818315, -105.2312903702832 39.95625422768943, -105.2313363694249 39.95640222747937, -105.2313723684942 39.95650822697466, -105.2313993672773 39.95657122608427, -105.2314743674655 39.95674822524581, -105.2315163654634 39.9568392256063, -105.2316053645577 39.95700022378365, -105.2317183627099 39.95718222346612, -105.2318093614744 39.95731022333126, -105.2319253601265 39.9574562223896, -105.2321203576787 39.9576752222892, -105.2321207867455 39.95767563668858, -105.2323323583044 39.95788022189713, -105.2323339852215 39.95788198466088, -105.2324863593553 39.95804721921932, -105.2334443494492 39.95875021940091, -105.233571348484 39.95868821912516, -105.233714348323 39.95861822001959, -105.2338239520144 39.95857110046063, -105.2338049737405 39.95855745128576, -105.2337782867351 39.95853826416749, -105.2336986413383 39.95848099104538, -105.2336468045691 39.95844371280378, -105.2336171748539 39.95842344796374, -105.2341725434769 39.9580392688392, -105.2347950472625 39.95760869288404, -105.2342243926122 39.95691524152589, -105.2341524978376 39.95682786948809, -105.2349909423702 39.95628870009567, -105.2376695730872 39.95553943080883, -105.237869403808 39.95544896598811, -105.2380925487423 39.95534793956568, -105.2381381075876 39.95533712804144, -105.2384707501498 39.9552581735205, -105.2387606413787 39.95522995514532, -105.2391404503259 39.95508480189946, -105.2392353862244 39.95517125116451, -105.2392371589414 39.95517286555238, -105.239258389572 39.9551921984806, -105.23927647946 39.95520867371651, -105.2394538794511 39.95516317297034, -105.2394675768633 39.95518923114921, -105.2396736377063 39.955581234407, -105.2406711572687 39.95439742475489, -105.240024053321 39.95392266004539, -105.2398894907311 39.95382393336795, -105.2398824476685 39.95381877110944, -105.2398473876931 39.95379304572359, -105.2398453407215 39.95379154330794, -105.2398296126404 39.95378000279207, -105.2399006156666 39.95375236339038, -105.2399205402457 39.95374460686801, -105.2399483505752 39.95372724911473, -105.2400416944829 39.9536974417265, -105.2400878385559 39.95367947772901, -105.240487048047 39.95352406659201, -105.2404916539113 39.95352201806195, -105.2408652368515 39.95346000915787, -105.240933089732 39.95344874590243, -105.2409499829143 39.95344750044689, -105.2409629638922 39.95344654341077, -105.2411807314999 39.95343048229564, -105.2412136382214 39.95342633392487, -105.2412244358653 39.95342464512465, -105.2412358248517 39.95342286488371, -105.2412578671857 39.95341887043079, -105.2412797394526 39.95341435681286, -105.2413014182228 39.95340933028208, -105.2413228882888 39.95340378900303, -105.2413441273671 39.95339774553509, -105.2413651120586 39.95339119802451, -105.2413858282717 39.95338415904898, -105.2414062525904 39.95337663125811, -105.2414263685928 39.95336862452243, -105.2414461540193 39.95336014509677, -105.2414655936254 39.95335120105296, -105.2414846663152 39.95334180044981, -105.2415033556772 39.9533319504559, -105.2415216464464 39.95332166454715, -105.2415395163498 39.95331095258089, -105.2415569548413 39.95329981813632, -105.2415739384536 39.9532882773729, -105.2415904554602 39.9532763365691, -105.2416064894054 39.95326401460206, -105.2416220297466 39.95325131415024, -105.24163705301 39.95323825317441, -105.241651550963 39.95322484246419, -105.2416655106915 39.95321109279873, -105.2416789145904 39.95319701764863, -105.2416924969039 39.95318372827051, -105.2417926015235 39.95306197295623, -105.2420940138068 39.95269873993102, -105.2423550234888 39.95238460880659, -105.242400847213 39.95232958199797, -105.2424229928676 39.95230461213298, -105.2424350975266 39.95228989182103, -105.2424467138614 39.95227494525179, -105.2424578289587 39.95225978320441, -105.2424684416042 39.95224441738487, -105.2424785412352 39.95222885587566, -105.2424881208034 39.95221310586636, -105.2424971779208 39.95219717996105, -105.2425056985141 39.95218108623425, -105.2425136860365 39.95216484000501, -105.2425211357905 39.95214844576619, -105.242528036016 39.9521319188029, -105.2425343843559 39.95211526361316, -105.242540178402 39.95209849820491, -105.242545419308 39.95208162708401, -105.2425500906432 39.9520646628231, -105.2425542040459 39.95204762256071, -105.2425577466438 39.95203050626817, -105.2425604849985 39.95201470223844, -105.2425631226928 39.95199611044753, -105.2425649537362 39.95197884892725, -105.2425662114527 39.95196156000681, -105.2425668899367 39.9519442580837, -105.2425669973535 39.95192695038124, -105.242566527808 39.95190964859498, -105.2425654812633 39.95189236263193, -105.2425638623396 39.95187510871434, -105.2425616698536 39.95185789044219, -105.2425589060715 39.95184072763487, -105.2425555709869 39.95182362209368, -105.2425516692268 39.95180658823951, -105.2425471983968 39.9517896404774, -105.2425469995326 39.95178899876466, -105.2425421690058 39.95177278513545, -105.2425365751554 39.9517560348095, -105.242530432015 39.95173940124199, -105.2425237313593 39.95172289342101, -105.2425164848536 39.95170652127981, -105.2425086947983 39.95169029563127, -105.2425003742863 39.95167477851509, -105.2424059484562 39.95151136733212, -105.2421494028326 39.95106741309232, -105.2421263742837 39.95102756327953, -105.2421244396496 39.95102421300519, -105.2421117923814 39.95100232933174, -105.2421532349839 39.9508776521355, -105.2422356511012 39.95062967915599, -105.2423203763545 39.95053644972544, -105.2423583595049 39.95045226550373, -105.2424326983841 39.95038139681725, -105.2424193456011 39.95036537308143, -105.2424164774736 39.95036192975837, -105.2424288673095 39.95035465582276, -105.2424902617059 39.95031861002217, -105.2428650690549 39.95009855353451, -105.2428848292195 39.95012039805992, -105.2428864176305 39.95012215428513, -105.2429218079034 39.95016127407835, -105.2432539182085 39.94997577837081, -105.2436207472383 39.94976943938573, -105.2436116776633 39.94976111333539, -105.2436098898687 39.94975947286139, -105.2435487854324 39.94970338529077, -105.2435552591411 39.94969465971476, -105.2437521608587 39.94942704577121, -105.2437723123789 39.94941200006306, -105.243901119003 39.94931583227635, -105.2439133601279 39.94929227305281, -105.2439907943965 39.94920904960991, -105.2438902370072 39.94913250436197, -105.243843496383 39.9490969244327, -105.2443336805456 39.94899766010215, -105.2450769997713 39.94893541989843, -105.2450769622432 39.94898556845416, -105.2450769407175 39.94901326183933, -105.2450769015449 39.94906353738384, -105.2450768554042 39.94912445058453, -105.2450768545068 39.94912625730254, -105.2450768068025 39.94918915554966, -105.2459288147174 39.9491932396644, -105.2459273019017 39.94880149693439, -105.2459270969151 39.94874811268062, -105.2459271138438 39.9487184180232, -105.2459271149365 39.94871560977393, -105.2459271527736 39.94865357973831, -105.2459280088195 39.94859022934073, -105.2464013539658 39.94842233398014, -105.2467081124108 39.948313522097, -105.2470891135391 39.94809851549275, -105.2472302242334 39.94801888546431, -105.2476083139154 39.94780552076305, -105.2476846981875 39.94776122618649, -105.2478094284176 39.94735633375443, -105.2478469404037 39.94723456492972, -105.2478433560362 39.94713228736064, -105.2478890047047 39.94705597092624, -105.2479304177987 39.9468527631968, -105.2479367866069 39.94684940326579, -105.2480295986053 39.94680042405117, -105.2485796528338 39.94651128238812, -105.2486454636441 39.94641330739307, -105.2487568057952 39.94624753735123, -105.248831466112 39.94598356233421, -105.249021310299 39.94563334264168, -105.249080831418 39.94552353705695, -105.2495449506102 39.94530671557963, -105.2503360267622 39.94525208564679, -105.2506537737573 39.9452363809138, -105.2509883201429 39.94522203648467, -105.2510883945363 39.94521343349978, -105.2511768961192 39.94520772446678, -105.2511800028379 39.94524977930156, -105.2511838734138 39.94530217534098, -105.2515099428432 39.94523367793365, -105.2518436376838 39.94515417827923, -105.2518477719972 39.94515670272256, -105.2518512447883 39.94515611576839, -105.2518547164191 39.94515552610967, -105.2518581857455 39.94515492653865, -105.251861651591 39.94515431885415, -105.2518651127853 39.94515370305352, -105.2518685751693 39.94515308185147, -105.2518720329022 39.94515245253334, -105.2518754918346 39.94515181511175, -105.2518789425989 39.94515117136789, -105.2518823933992 39.94515051771672, -105.2518858465593 39.94514985866664, -105.251889289211 39.9451491932892, -105.2518927354026 39.94514851981333, -105.251896174606 39.94514783731576, -105.2518996161757 39.9451471476179, -105.2519030495741 39.94514645249836, -105.2519064841721 39.94514574927545, -105.2519099141221 39.9451450370358, -105.2519133441015 39.9451443166902, -105.2519159145514 39.94514377282392, -105.2519167670797 39.94514359092548, -105.2519201889171 39.94514285705226, -105.2519236084339 39.94514211777003, -105.2519256753871 39.94514166558714, -105.2519270256396 39.94514137037679, -105.2519304405346 39.94514061487251, -105.2519338496082 39.9451398512497, -105.2519372587047 39.94513908132221, -105.2519406643201 39.94513830328125, -105.2519440664447 39.9451375198287, -105.2519474674253 39.94513672916829, -105.2519508625911 39.94513592858804, -105.2519542542693 39.94513512169561, -105.2519576448035 39.94513430759532, -105.2519610330267 39.94513348538403, -105.2519644165857 39.94513265865931, -105.2519677966735 39.94513182111915, -105.2519711744374 39.94513097907053, -105.2519745475565 39.94513012710465, -105.2519779218621 39.94512927063791, -105.2519812880159 39.94512840334556, -105.2519846541827 39.94512753245058, -105.2519880133548 39.94512665433513, -105.2519913737362 39.94512576541436, -105.2519947294501 39.94512487288078, -105.2519980781757 39.94512397132544, -105.2520014269308 39.94512306166417, -105.2520047721983 39.94512214569071, -105.2520081139781 39.94512122340501, -105.2520114487632 39.94512029389892, -105.2520147835744 39.94511935718746, -105.2520181149079 39.94511841146189, -105.2520214427504 39.94511746032477, -105.2520247647684 39.94511650196974, -105.2520280821318 39.94511553639932, -105.2520313995214 39.94511456362362, -105.2520347134299 39.94511358273439, -105.2520380226774 39.94511259643108, -105.2520413261068 39.9451116011086, -105.2520446283922 39.94511059857827, -105.2520479236795 39.94510958972817, -105.2520512201533 39.94510857637726, -105.2520545073116 39.94510755039697, -105.2520577933096 39.94510652171215, -105.2520610793434 39.94510548312004, -105.2520643572058 39.94510443910632, -105.2520676304072 39.94510338967851, -105.2520708989607 39.94510233123408, -105.2520741651999 39.94510126557928, -105.2520774291217 39.9451001936148, -105.252080686052 39.9450991135292, -105.2520839394946 39.94509802713147, -105.2520871917932 39.94509693352585, -105.2520904382705 39.94509583180172, -105.2520936765796 39.94509472375534, -105.2520969160751 39.94509361120816, -105.2521001520927 39.94509248964676, -105.2521033799521 39.94509135906114, -105.2521066054841 39.9450902248678, -105.2521098263649 39.94508908255848, -105.2521130414211 39.94508793303122, -105.2521162541663 39.94508677539298, -105.2521194610771 39.94508561323882, -105.2521226656769 39.94508444297368, -105.2521258656191 39.94508326639381, -105.2521290573995 39.9450820816904, -105.2521322515365 39.94508089248868, -105.2521354363483 39.9450796933595, -105.2521386153256 39.94507848971444, -105.2521417943322 39.94507727796344, -105.2521449663408 39.94507605989268, -105.2521481336949 39.94507483460657, -105.2521512975614 39.94507360300824, -105.2521544556032 39.945072364192, -105.2521576089873 39.9450711190611, -105.2521607588903 39.94506986581668, -105.2521639029653 39.94506860625501, -105.2521670423859 39.945067339478, -105.2521701783156 39.9450660672895, -105.2521733084173 39.9450647887837, -105.2521764326977 39.94506350215937, -105.2521795546639 39.94506220832474, -105.252182669632 39.94506090817035, -105.2521857811092 39.94505960260445, -105.2521888891053 39.94505828892499, -105.2521919901034 39.94505696892586, -105.2521950864469 39.94505564171133, -105.2521981757891 39.94505430907772, -105.2522012628204 39.94505296833312, -105.2522043451939 39.94505162127381, -105.2522074217362 39.94505026879794, -105.252210493624 39.94504890910668, -105.2522135585137 39.94504754309576, -105.2522166199256 39.94504616807063, -105.2522196755064 39.94504478762895, -105.2522227252527 39.94504340267135, -105.2522257738581 39.94504200960528, -105.2522288131219 39.94504061111508, -105.2522318465677 39.94503920360577, -105.2522348753491 39.945037791583, -105.2522379029864 39.94503637235244, -105.2522409212886 39.94503494589646, -105.2522439360999 39.94503351402893, -105.2522469450801 39.94503207674485, -105.2522499470686 39.94503063133973, -105.2522529443995 39.94502917961992, -105.2522559382492 39.94502771978662, -105.2522589250976 39.94502625453423, -105.2522619096219 39.9450247847735, -105.2522648848177 39.94502330598599, -105.2522678541855 39.94502182088132, -105.252270820056 39.94502033216641, -105.2522737789414 39.94501883352913, -105.2522767331494 39.94501733398111, -105.2522796815557 39.94501582091064, -105.2522826229475 39.94501430602371, -105.2522855596848 39.94501278392142, -105.2522884929345 39.94501125550695, -105.2522914203628 39.94500971897397, -105.2522943396065 39.94500818062199, -105.2522972530451 39.94500662964825, -105.2523001606396 39.94500507686057, -105.2523030659263 39.94500351506126, -105.2523059606881 39.94500195143796, -105.2523088519786 39.94500037699914, -105.2523117397717 39.94499879895016, -105.2523146170629 39.94499721277261, -105.252317489693 39.94499562118102, -105.2523203600023 39.94499402418045, -105.2523232186395 39.9449924190487, -105.2523260772863 39.94499081121498, -105.2523289266047 39.94498919435458, -105.2523317712685 39.94498757027878, -105.2523346100946 39.94498594258777, -105.2523374395856 39.94498430767137, -105.2523402632486 39.94498266643776, -105.2523430834208 39.9449810197926, -105.2523458965916 39.94497936772839, -105.2523487051111 39.94497770754813, -105.252351504289 39.94497604194386, -105.2523542988092 39.94497437002488, -105.2523570886649 39.94497269359248, -105.2523598726928 39.94497101084288, -105.2523626462154 39.9449693208654, -105.2523654162504 39.94496762457575, -105.252368179284 39.94496592286701, -105.2523709399968 39.9449642157493, -105.2523736890245 39.94496250410312, -105.2523764345645 39.94496078614474, -105.2523791719461 39.94495905916219, -105.2523819034965 39.94495732676307, -105.2523846303825 39.9449555898506, -105.2523873479302 39.94495384661338, -105.2523900608136 39.94495209886276, -105.2523927666989 39.94495034479245, -105.2523954667595 39.94494858350431, -105.2523981598155 39.94494681769777, -105.2524008458767 39.9449450446708, -105.2524035249366 39.94494326622485, -105.2524061993255 39.94494148506679, -105.2524088667262 39.94493969488705, -105.252411525962 39.94493789748446, -105.25241417936 39.9449360964666, -105.2524168245865 39.9449342900272, -105.2524194639786 39.94493247907191, -105.2524220987194 39.94493066000064, -105.2524247229484 39.94492883550277, -105.2524273448566 39.94492700559591, -105.2524299550862 39.94492516935929, -105.2524325618152 39.94492333041308, -105.252435161559 39.94492148154463, -105.252437754295 39.94491962905835, -105.2524403388627 39.94491777024991, -105.2524429175862 39.94491590962748, -105.2524454893214 39.94491403998344, -105.2524480563956 39.94491216492536, -105.2524506141249 39.9449102853439, -105.2524531636891 39.94490839853952, -105.2524557062489 39.94490650721674, -105.2524582453176 39.94490461048248, -105.2524607738779 39.94490270742096, -105.2524632989439 39.94490079984861, -105.2524658123281 39.94489888684717, -105.2524683198811 39.94489696842913, -105.2524708239463 39.94489504369899, -105.2524733163298 39.94489311353974, -105.2524758063826 39.94489118067343, -105.2524782847633 39.94488923967614, -105.2524807596564 39.94488729236664, -105.2524832240246 39.94488534323313, -105.2524856814013 39.94488338597866, -105.252488135287 39.94488142331268, -105.2524905786512 39.94487945792206, -105.2524930138569 39.94487748350729, -105.2524954432185 39.94487550727858, -105.2524978655852 39.94487352382955, -105.2525002797738 39.94487153676027, -105.2525026881378 39.94486954247318, -105.2525050883238 39.9448675445658, -105.252507481515 39.94486553943809, -105.2525098665282 39.94486353069011, -105.2525122433633 39.94486151832191, -105.2525146155505 39.9448594969371, -105.2525169772161 39.94485747282765, -105.2525193342173 39.94485544420483, -105.2525216818835 39.94485340835668, -105.2525240213717 39.94485136888823, -105.2525263538618 39.94484932310012, -105.2525286805207 39.94484727189551, -105.252530998995 39.94484521887192, -105.2525333069609 39.94484315952113, -105.2525356102689 39.94484109385569, -105.2525379651215 39.94483901208904, -105.252540327011 39.94483692583418, -105.2525426772219 39.94483483324961, -105.2525450250989 39.94483273885861, -105.2525473613071 39.94483063543593, -105.2525496916743 39.94482852929868, -105.25255201387 39.94482641773995, -105.2525543255507 39.94482430165525, -105.2525566337372 39.94482218105967, -105.2525589314087 39.94482005593821, -105.252561220912 39.94481792449454, -105.2525635045808 39.944815788535, -105.2525657812514 39.94481364625581, -105.2525680497376 39.94481150215764, -105.2525703088854 39.94480935173479, -105.2525725598618 39.94480719589041, -105.2525748026569 39.94480503732641, -105.2525770407876 39.94480287424906, -105.2525792695832 39.94480070394635, -105.2525814902041 39.94479852912275, -105.2525837014737 39.94479635157708, -105.2525859057418 39.94479416861237, -105.252588104182 39.94479197933045, -105.2525902920974 39.94478978822466, -105.252592475355 39.94478759080415, -105.2525946480943 39.94478538975839, -105.2525968103186 39.94478318418675, -105.2525989678786 39.94478097410168, -105.2526011161035 39.94477875679134, -105.2526032573107 39.94477653856522, -105.2526053915231 39.94477431311877, -105.2526075152075 39.94477208674897, -105.25260963074 39.94476984955378, -105.2526117392417 39.94476761504543, -105.2526138419254 39.9447653715179, -105.2526159317472 39.9447631252608, -105.2526180169046 39.94476087449035, -105.252620092714 39.94475862009717, -105.2526221591817 39.94475636027993, -105.2526242186481 39.94475409504364, -105.2526262699267 39.94475182888913, -105.2526283107066 39.94474955370541, -105.252630345639 39.94474727760847, -105.2526323723935 39.94474499789126, -105.2526343921596 39.94474270915246, -105.2526364013912 39.94474042129166, -105.2526384036213 39.94473812801186, -105.2526403953399 39.94473582930549, -105.2526423788803 39.94473352697889, -105.252645854658 39.94472532764486, -105.2526482250673 39.94472379441017, -105.2526505822722 39.94472170724234, -105.2526529371432 39.94471961826813, -105.2526552838428 39.94471752387238, -105.2526576247046 39.9447154258614, -105.2526599609021 39.94471332333708, -105.2526622877612 39.94471121448806, -105.2526646099396 39.94470910562895, -105.252666927457 39.94470699135584, -105.2526692368061 39.94470487076051, -105.252671540311 39.94470274835131, -105.2526738414853 39.94470062323507, -105.2526761321511 39.94469849179162, -105.2526784181526 39.94469635583479, -105.2526806947961 39.94469421895718, -105.2526829714558 39.94469207757631, -105.2526852364369 39.94468992986567, -105.2526874979173 39.94468777944552, -105.2526897535534 39.94468562721148, -105.2526920010115 39.94468347135717, -105.2526942414682 39.94468131008387, -105.2526964749236 39.94467914339153, -105.2526987060484 39.94467697399215, -105.2527009266517 39.9446748018682, -105.2527031425841 39.94467262703221, -105.2527053550256 39.94467044678472, -105.2527075569455 39.94466826381264, -105.2527097542044 39.94466607542657, -105.2527119456254 39.94466388342523, -105.2527141323725 39.94466168961259, -105.252716308611 39.94465948947267, -105.2527184813488 39.94465728662328, -105.2527206435618 39.94465508194988, -105.2527228057877 39.94465287367389, -105.2527249575019 39.94465065997132, -105.2527271022114 39.94464844175045, -105.252729243417 39.94464622172061, -105.2527313729374 39.94464399716241, -105.2527334989539 39.9446417707953, -105.2527356191424 39.94463953811108, -105.2527377346633 39.94463730181415, -105.2527398408296 39.94463506369574, -105.252741942325 39.94463282286537, -105.2527440344788 39.94463057661095, -105.2527461207948 39.9446283267413, -105.2527482000965 39.94462607505523, -105.2527502747306 39.94462381975652, -105.2527523447003 39.94462155994446, -105.2527544029817 39.94461929650464, -105.2527564577688 39.94461702855396, -105.2527585043682 39.94461475968507, -105.2527605451364 39.94461248539962, -105.2527625788967 39.94461020749648, -105.2527646056491 39.94460792597565, -105.2527666288943 39.94460564354662, -105.2527686416278 39.94460335569099, -105.2527706508605 39.94460106512589, -105.2527726484049 39.94459877093303, -105.2527746447953 39.94459647223439, -105.2527766318245 39.94459417351555, -105.2527786118524 39.94459186937779, -105.2527805872225 39.94458955892532, -105.2527825532282 39.94458724935342, -105.2527845122358 39.94458493346185, -105.252786468903 39.94458261756525, -105.252788412715 39.9445802971377, -105.2527903541997 39.94457797310252, -105.2527922851693 39.94457564454142, -105.2527942126317 39.94457331507218, -105.2527961330928 39.94457098018385, -105.2527980465428 39.94456864257851, -105.2527999518083 39.94456630315422, -105.2528018500691 39.94456395921164, -105.2528037424988 39.94456160985257, -105.2528056255608 39.94455926227464, -105.2528075039683 39.94455690748143, -105.252809374188 39.94455455176997, -105.2528112409167 39.94455219064704, -105.2528130971141 39.94454982950153, -105.2528149486473 39.94454746384262, -105.252816791996 39.9445450963648, -105.2528186306868 39.94454272257242, -105.2528204611833 39.94454034966305, -105.2528222811714 39.9445379704265, -105.2528240988289 39.94453558848292, -105.2528259083052 39.94453320381981, -105.2528277119405 39.94453081644217, -105.2528295038809 39.94452842723811, -105.252831291157 39.9445260335207, -105.2528330725954 39.94452363618807, -105.2528348470161 39.94452123793978, -105.2528366132654 39.94451883426994, -105.2528383736639 39.94451643058751, -105.2528401270644 39.94451402058545, -105.2528418722804 39.94451160876449, -105.2528436116555 39.94450919422898, -105.2528453416661 39.94